<commit_message>
Data updated by GitHub Bot (2020-05-26 12)
</commit_message>
<xml_diff>
--- a/output/snapshot/fdcf2531-4c3e-5c02-b63c-ee160ead6dea.xlsx
+++ b/output/snapshot/fdcf2531-4c3e-5c02-b63c-ee160ead6dea.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="I:\AKTUALNI PODATKI - KORONA\Za objavo na GOV.SI\ang\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{1E6DD62F-2BE2-47DC-A7ED-9B57C1589256}" xr6:coauthVersionLast="44" xr6:coauthVersionMax="44" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{1046414C-717E-412E-86D2-D36B031D64B3}" xr6:coauthVersionLast="44" xr6:coauthVersionMax="44" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -399,8 +399,8 @@
 </file>
 
 <file path=xl/tables/table1.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="1" xr:uid="{00000000-000C-0000-FFFF-FFFF00000000}" name="Tabela1" displayName="Tabela1" ref="A1:J75" totalsRowShown="0" headerRowDxfId="11" dataDxfId="10">
-  <autoFilter ref="A1:J75" xr:uid="{00000000-0009-0000-0100-000001000000}">
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="1" xr:uid="{00000000-000C-0000-FFFF-FFFF00000000}" name="Tabela1" displayName="Tabela1" ref="A1:J76" totalsRowShown="0" headerRowDxfId="11" dataDxfId="10">
+  <autoFilter ref="A1:J76" xr:uid="{00000000-0009-0000-0100-000001000000}">
     <filterColumn colId="0" hiddenButton="1"/>
     <filterColumn colId="1" hiddenButton="1"/>
     <filterColumn colId="2" hiddenButton="1"/>
@@ -696,10 +696,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:J75"/>
+  <dimension ref="A1:J76"/>
   <sheetViews>
     <sheetView tabSelected="1" topLeftCell="A40" zoomScale="89" zoomScaleNormal="89" workbookViewId="0">
-      <selection activeCell="J74" sqref="J74"/>
+      <selection activeCell="A76" sqref="A76:J76"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -3117,6 +3117,38 @@
         <v>0</v>
       </c>
     </row>
+    <row r="76" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A76" s="20">
+        <v>43976</v>
+      </c>
+      <c r="B76" s="21">
+        <v>75770</v>
+      </c>
+      <c r="C76" s="22">
+        <v>754</v>
+      </c>
+      <c r="D76" s="22">
+        <v>1469</v>
+      </c>
+      <c r="E76" s="22">
+        <v>0</v>
+      </c>
+      <c r="F76" s="22">
+        <v>9</v>
+      </c>
+      <c r="G76" s="22">
+        <v>2</v>
+      </c>
+      <c r="H76" s="22">
+        <v>6</v>
+      </c>
+      <c r="I76" s="22">
+        <v>108</v>
+      </c>
+      <c r="J76" s="22">
+        <v>1</v>
+      </c>
+    </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>

</xml_diff>

<commit_message>
Data updated by GitHub Bot (2020-05-26 20)
</commit_message>
<xml_diff>
--- a/output/snapshot/fdcf2531-4c3e-5c02-b63c-ee160ead6dea.xlsx
+++ b/output/snapshot/fdcf2531-4c3e-5c02-b63c-ee160ead6dea.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="I:\AKTUALNI PODATKI - KORONA\Za objavo na GOV.SI\ang\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{1E6DD62F-2BE2-47DC-A7ED-9B57C1589256}" xr6:coauthVersionLast="44" xr6:coauthVersionMax="44" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{1046414C-717E-412E-86D2-D36B031D64B3}" xr6:coauthVersionLast="44" xr6:coauthVersionMax="44" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -399,8 +399,8 @@
 </file>
 
 <file path=xl/tables/table1.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="1" xr:uid="{00000000-000C-0000-FFFF-FFFF00000000}" name="Tabela1" displayName="Tabela1" ref="A1:J75" totalsRowShown="0" headerRowDxfId="11" dataDxfId="10">
-  <autoFilter ref="A1:J75" xr:uid="{00000000-0009-0000-0100-000001000000}">
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="1" xr:uid="{00000000-000C-0000-FFFF-FFFF00000000}" name="Tabela1" displayName="Tabela1" ref="A1:J76" totalsRowShown="0" headerRowDxfId="11" dataDxfId="10">
+  <autoFilter ref="A1:J76" xr:uid="{00000000-0009-0000-0100-000001000000}">
     <filterColumn colId="0" hiddenButton="1"/>
     <filterColumn colId="1" hiddenButton="1"/>
     <filterColumn colId="2" hiddenButton="1"/>
@@ -696,10 +696,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:J75"/>
+  <dimension ref="A1:J76"/>
   <sheetViews>
     <sheetView tabSelected="1" topLeftCell="A40" zoomScale="89" zoomScaleNormal="89" workbookViewId="0">
-      <selection activeCell="J74" sqref="J74"/>
+      <selection activeCell="A76" sqref="A76:J76"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -3117,6 +3117,38 @@
         <v>0</v>
       </c>
     </row>
+    <row r="76" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A76" s="20">
+        <v>43976</v>
+      </c>
+      <c r="B76" s="21">
+        <v>75770</v>
+      </c>
+      <c r="C76" s="22">
+        <v>754</v>
+      </c>
+      <c r="D76" s="22">
+        <v>1469</v>
+      </c>
+      <c r="E76" s="22">
+        <v>0</v>
+      </c>
+      <c r="F76" s="22">
+        <v>9</v>
+      </c>
+      <c r="G76" s="22">
+        <v>2</v>
+      </c>
+      <c r="H76" s="22">
+        <v>6</v>
+      </c>
+      <c r="I76" s="22">
+        <v>108</v>
+      </c>
+      <c r="J76" s="22">
+        <v>1</v>
+      </c>
+    </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>

</xml_diff>

<commit_message>
Data updated by GitHub Bot (2020-05-27 12)
</commit_message>
<xml_diff>
--- a/output/snapshot/fdcf2531-4c3e-5c02-b63c-ee160ead6dea.xlsx
+++ b/output/snapshot/fdcf2531-4c3e-5c02-b63c-ee160ead6dea.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="I:\AKTUALNI PODATKI - KORONA\Za objavo na GOV.SI\ang\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{1E6DD62F-2BE2-47DC-A7ED-9B57C1589256}" xr6:coauthVersionLast="44" xr6:coauthVersionMax="44" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{2151A594-BD8B-437B-A4BC-094AB668C90C}" xr6:coauthVersionLast="44" xr6:coauthVersionMax="44" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -399,8 +399,8 @@
 </file>
 
 <file path=xl/tables/table1.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="1" xr:uid="{00000000-000C-0000-FFFF-FFFF00000000}" name="Tabela1" displayName="Tabela1" ref="A1:J75" totalsRowShown="0" headerRowDxfId="11" dataDxfId="10">
-  <autoFilter ref="A1:J75" xr:uid="{00000000-0009-0000-0100-000001000000}">
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="1" xr:uid="{00000000-000C-0000-FFFF-FFFF00000000}" name="Tabela1" displayName="Tabela1" ref="A1:J77" totalsRowShown="0" headerRowDxfId="11" dataDxfId="10">
+  <autoFilter ref="A1:J77" xr:uid="{00000000-0009-0000-0100-000001000000}">
     <filterColumn colId="0" hiddenButton="1"/>
     <filterColumn colId="1" hiddenButton="1"/>
     <filterColumn colId="2" hiddenButton="1"/>
@@ -696,10 +696,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:J75"/>
+  <dimension ref="A1:J77"/>
   <sheetViews>
     <sheetView tabSelected="1" topLeftCell="A40" zoomScale="89" zoomScaleNormal="89" workbookViewId="0">
-      <selection activeCell="J74" sqref="J74"/>
+      <selection activeCell="A77" sqref="A77:J77"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -3117,6 +3117,70 @@
         <v>0</v>
       </c>
     </row>
+    <row r="76" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A76" s="20">
+        <v>43976</v>
+      </c>
+      <c r="B76" s="21">
+        <v>75770</v>
+      </c>
+      <c r="C76" s="22">
+        <v>754</v>
+      </c>
+      <c r="D76" s="22">
+        <v>1469</v>
+      </c>
+      <c r="E76" s="22">
+        <v>0</v>
+      </c>
+      <c r="F76" s="22">
+        <v>9</v>
+      </c>
+      <c r="G76" s="22">
+        <v>2</v>
+      </c>
+      <c r="H76" s="22">
+        <v>6</v>
+      </c>
+      <c r="I76" s="22">
+        <v>108</v>
+      </c>
+      <c r="J76" s="22">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="77" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A77" s="20">
+        <v>43977</v>
+      </c>
+      <c r="B77" s="21">
+        <v>76579</v>
+      </c>
+      <c r="C77" s="22">
+        <v>809</v>
+      </c>
+      <c r="D77" s="22">
+        <v>1471</v>
+      </c>
+      <c r="E77" s="22">
+        <v>2</v>
+      </c>
+      <c r="F77" s="22">
+        <v>8</v>
+      </c>
+      <c r="G77" s="22">
+        <v>2</v>
+      </c>
+      <c r="H77" s="22">
+        <v>2</v>
+      </c>
+      <c r="I77" s="22">
+        <v>108</v>
+      </c>
+      <c r="J77" s="22">
+        <v>0</v>
+      </c>
+    </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>

</xml_diff>

<commit_message>
Data updated by GitHub Bot (2020-05-27 20)
</commit_message>
<xml_diff>
--- a/output/snapshot/fdcf2531-4c3e-5c02-b63c-ee160ead6dea.xlsx
+++ b/output/snapshot/fdcf2531-4c3e-5c02-b63c-ee160ead6dea.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="I:\AKTUALNI PODATKI - KORONA\Za objavo na GOV.SI\ang\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{1E6DD62F-2BE2-47DC-A7ED-9B57C1589256}" xr6:coauthVersionLast="44" xr6:coauthVersionMax="44" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{2151A594-BD8B-437B-A4BC-094AB668C90C}" xr6:coauthVersionLast="44" xr6:coauthVersionMax="44" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -399,8 +399,8 @@
 </file>
 
 <file path=xl/tables/table1.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="1" xr:uid="{00000000-000C-0000-FFFF-FFFF00000000}" name="Tabela1" displayName="Tabela1" ref="A1:J75" totalsRowShown="0" headerRowDxfId="11" dataDxfId="10">
-  <autoFilter ref="A1:J75" xr:uid="{00000000-0009-0000-0100-000001000000}">
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="1" xr:uid="{00000000-000C-0000-FFFF-FFFF00000000}" name="Tabela1" displayName="Tabela1" ref="A1:J77" totalsRowShown="0" headerRowDxfId="11" dataDxfId="10">
+  <autoFilter ref="A1:J77" xr:uid="{00000000-0009-0000-0100-000001000000}">
     <filterColumn colId="0" hiddenButton="1"/>
     <filterColumn colId="1" hiddenButton="1"/>
     <filterColumn colId="2" hiddenButton="1"/>
@@ -696,10 +696,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:J75"/>
+  <dimension ref="A1:J77"/>
   <sheetViews>
     <sheetView tabSelected="1" topLeftCell="A40" zoomScale="89" zoomScaleNormal="89" workbookViewId="0">
-      <selection activeCell="J74" sqref="J74"/>
+      <selection activeCell="A77" sqref="A77:J77"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -3117,6 +3117,70 @@
         <v>0</v>
       </c>
     </row>
+    <row r="76" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A76" s="20">
+        <v>43976</v>
+      </c>
+      <c r="B76" s="21">
+        <v>75770</v>
+      </c>
+      <c r="C76" s="22">
+        <v>754</v>
+      </c>
+      <c r="D76" s="22">
+        <v>1469</v>
+      </c>
+      <c r="E76" s="22">
+        <v>0</v>
+      </c>
+      <c r="F76" s="22">
+        <v>9</v>
+      </c>
+      <c r="G76" s="22">
+        <v>2</v>
+      </c>
+      <c r="H76" s="22">
+        <v>6</v>
+      </c>
+      <c r="I76" s="22">
+        <v>108</v>
+      </c>
+      <c r="J76" s="22">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="77" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A77" s="20">
+        <v>43977</v>
+      </c>
+      <c r="B77" s="21">
+        <v>76579</v>
+      </c>
+      <c r="C77" s="22">
+        <v>809</v>
+      </c>
+      <c r="D77" s="22">
+        <v>1471</v>
+      </c>
+      <c r="E77" s="22">
+        <v>2</v>
+      </c>
+      <c r="F77" s="22">
+        <v>8</v>
+      </c>
+      <c r="G77" s="22">
+        <v>2</v>
+      </c>
+      <c r="H77" s="22">
+        <v>2</v>
+      </c>
+      <c r="I77" s="22">
+        <v>108</v>
+      </c>
+      <c r="J77" s="22">
+        <v>0</v>
+      </c>
+    </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>

</xml_diff>

<commit_message>
Data updated by GitHub Bot (2020-05-28 12)
</commit_message>
<xml_diff>
--- a/output/snapshot/fdcf2531-4c3e-5c02-b63c-ee160ead6dea.xlsx
+++ b/output/snapshot/fdcf2531-4c3e-5c02-b63c-ee160ead6dea.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="I:\AKTUALNI PODATKI - KORONA\Za objavo na GOV.SI\ang\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{1E6DD62F-2BE2-47DC-A7ED-9B57C1589256}" xr6:coauthVersionLast="44" xr6:coauthVersionMax="44" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{682DB525-151F-46B1-8C23-B688EF458D07}" xr6:coauthVersionLast="44" xr6:coauthVersionMax="44" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -399,8 +399,8 @@
 </file>
 
 <file path=xl/tables/table1.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="1" xr:uid="{00000000-000C-0000-FFFF-FFFF00000000}" name="Tabela1" displayName="Tabela1" ref="A1:J75" totalsRowShown="0" headerRowDxfId="11" dataDxfId="10">
-  <autoFilter ref="A1:J75" xr:uid="{00000000-0009-0000-0100-000001000000}">
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="1" xr:uid="{00000000-000C-0000-FFFF-FFFF00000000}" name="Tabela1" displayName="Tabela1" ref="A1:J78" totalsRowShown="0" headerRowDxfId="11" dataDxfId="10">
+  <autoFilter ref="A1:J78" xr:uid="{00000000-0009-0000-0100-000001000000}">
     <filterColumn colId="0" hiddenButton="1"/>
     <filterColumn colId="1" hiddenButton="1"/>
     <filterColumn colId="2" hiddenButton="1"/>
@@ -696,10 +696,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:J75"/>
+  <dimension ref="A1:J78"/>
   <sheetViews>
     <sheetView tabSelected="1" topLeftCell="A40" zoomScale="89" zoomScaleNormal="89" workbookViewId="0">
-      <selection activeCell="J74" sqref="J74"/>
+      <selection activeCell="A78" sqref="A78:J78"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -3117,6 +3117,102 @@
         <v>0</v>
       </c>
     </row>
+    <row r="76" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A76" s="20">
+        <v>43976</v>
+      </c>
+      <c r="B76" s="21">
+        <v>75770</v>
+      </c>
+      <c r="C76" s="22">
+        <v>754</v>
+      </c>
+      <c r="D76" s="22">
+        <v>1469</v>
+      </c>
+      <c r="E76" s="22">
+        <v>0</v>
+      </c>
+      <c r="F76" s="22">
+        <v>9</v>
+      </c>
+      <c r="G76" s="22">
+        <v>2</v>
+      </c>
+      <c r="H76" s="22">
+        <v>6</v>
+      </c>
+      <c r="I76" s="22">
+        <v>108</v>
+      </c>
+      <c r="J76" s="22">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="77" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A77" s="20">
+        <v>43977</v>
+      </c>
+      <c r="B77" s="21">
+        <v>76579</v>
+      </c>
+      <c r="C77" s="22">
+        <v>809</v>
+      </c>
+      <c r="D77" s="22">
+        <v>1471</v>
+      </c>
+      <c r="E77" s="22">
+        <v>2</v>
+      </c>
+      <c r="F77" s="22">
+        <v>8</v>
+      </c>
+      <c r="G77" s="22">
+        <v>2</v>
+      </c>
+      <c r="H77" s="22">
+        <v>2</v>
+      </c>
+      <c r="I77" s="22">
+        <v>108</v>
+      </c>
+      <c r="J77" s="22">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="78" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A78" s="20">
+        <v>43978</v>
+      </c>
+      <c r="B78" s="21">
+        <v>77210</v>
+      </c>
+      <c r="C78" s="22">
+        <v>631</v>
+      </c>
+      <c r="D78" s="22">
+        <v>1473</v>
+      </c>
+      <c r="E78" s="22">
+        <v>2</v>
+      </c>
+      <c r="F78" s="22">
+        <v>7</v>
+      </c>
+      <c r="G78" s="22">
+        <v>2</v>
+      </c>
+      <c r="H78" s="22">
+        <v>1</v>
+      </c>
+      <c r="I78" s="22">
+        <v>108</v>
+      </c>
+      <c r="J78" s="22">
+        <v>0</v>
+      </c>
+    </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>

</xml_diff>

<commit_message>
Data updated by GitHub Bot (2020-05-28 20)
</commit_message>
<xml_diff>
--- a/output/snapshot/fdcf2531-4c3e-5c02-b63c-ee160ead6dea.xlsx
+++ b/output/snapshot/fdcf2531-4c3e-5c02-b63c-ee160ead6dea.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="I:\AKTUALNI PODATKI - KORONA\Za objavo na GOV.SI\ang\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{1E6DD62F-2BE2-47DC-A7ED-9B57C1589256}" xr6:coauthVersionLast="44" xr6:coauthVersionMax="44" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{682DB525-151F-46B1-8C23-B688EF458D07}" xr6:coauthVersionLast="44" xr6:coauthVersionMax="44" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -399,8 +399,8 @@
 </file>
 
 <file path=xl/tables/table1.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="1" xr:uid="{00000000-000C-0000-FFFF-FFFF00000000}" name="Tabela1" displayName="Tabela1" ref="A1:J75" totalsRowShown="0" headerRowDxfId="11" dataDxfId="10">
-  <autoFilter ref="A1:J75" xr:uid="{00000000-0009-0000-0100-000001000000}">
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="1" xr:uid="{00000000-000C-0000-FFFF-FFFF00000000}" name="Tabela1" displayName="Tabela1" ref="A1:J78" totalsRowShown="0" headerRowDxfId="11" dataDxfId="10">
+  <autoFilter ref="A1:J78" xr:uid="{00000000-0009-0000-0100-000001000000}">
     <filterColumn colId="0" hiddenButton="1"/>
     <filterColumn colId="1" hiddenButton="1"/>
     <filterColumn colId="2" hiddenButton="1"/>
@@ -696,10 +696,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:J75"/>
+  <dimension ref="A1:J78"/>
   <sheetViews>
     <sheetView tabSelected="1" topLeftCell="A40" zoomScale="89" zoomScaleNormal="89" workbookViewId="0">
-      <selection activeCell="J74" sqref="J74"/>
+      <selection activeCell="A78" sqref="A78:J78"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -3117,6 +3117,102 @@
         <v>0</v>
       </c>
     </row>
+    <row r="76" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A76" s="20">
+        <v>43976</v>
+      </c>
+      <c r="B76" s="21">
+        <v>75770</v>
+      </c>
+      <c r="C76" s="22">
+        <v>754</v>
+      </c>
+      <c r="D76" s="22">
+        <v>1469</v>
+      </c>
+      <c r="E76" s="22">
+        <v>0</v>
+      </c>
+      <c r="F76" s="22">
+        <v>9</v>
+      </c>
+      <c r="G76" s="22">
+        <v>2</v>
+      </c>
+      <c r="H76" s="22">
+        <v>6</v>
+      </c>
+      <c r="I76" s="22">
+        <v>108</v>
+      </c>
+      <c r="J76" s="22">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="77" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A77" s="20">
+        <v>43977</v>
+      </c>
+      <c r="B77" s="21">
+        <v>76579</v>
+      </c>
+      <c r="C77" s="22">
+        <v>809</v>
+      </c>
+      <c r="D77" s="22">
+        <v>1471</v>
+      </c>
+      <c r="E77" s="22">
+        <v>2</v>
+      </c>
+      <c r="F77" s="22">
+        <v>8</v>
+      </c>
+      <c r="G77" s="22">
+        <v>2</v>
+      </c>
+      <c r="H77" s="22">
+        <v>2</v>
+      </c>
+      <c r="I77" s="22">
+        <v>108</v>
+      </c>
+      <c r="J77" s="22">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="78" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A78" s="20">
+        <v>43978</v>
+      </c>
+      <c r="B78" s="21">
+        <v>77210</v>
+      </c>
+      <c r="C78" s="22">
+        <v>631</v>
+      </c>
+      <c r="D78" s="22">
+        <v>1473</v>
+      </c>
+      <c r="E78" s="22">
+        <v>2</v>
+      </c>
+      <c r="F78" s="22">
+        <v>7</v>
+      </c>
+      <c r="G78" s="22">
+        <v>2</v>
+      </c>
+      <c r="H78" s="22">
+        <v>1</v>
+      </c>
+      <c r="I78" s="22">
+        <v>108</v>
+      </c>
+      <c r="J78" s="22">
+        <v>0</v>
+      </c>
+    </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>

</xml_diff>

<commit_message>
Data updated by GitHub Bot (2020-05-29 12)
</commit_message>
<xml_diff>
--- a/output/snapshot/fdcf2531-4c3e-5c02-b63c-ee160ead6dea.xlsx
+++ b/output/snapshot/fdcf2531-4c3e-5c02-b63c-ee160ead6dea.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="I:\AKTUALNI PODATKI - KORONA\Za objavo na GOV.SI\ang\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{1E6DD62F-2BE2-47DC-A7ED-9B57C1589256}" xr6:coauthVersionLast="44" xr6:coauthVersionMax="44" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{730BD8E4-8830-4CB9-85DE-3D4608545396}" xr6:coauthVersionLast="44" xr6:coauthVersionMax="44" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -399,8 +399,8 @@
 </file>
 
 <file path=xl/tables/table1.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="1" xr:uid="{00000000-000C-0000-FFFF-FFFF00000000}" name="Tabela1" displayName="Tabela1" ref="A1:J75" totalsRowShown="0" headerRowDxfId="11" dataDxfId="10">
-  <autoFilter ref="A1:J75" xr:uid="{00000000-0009-0000-0100-000001000000}">
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="1" xr:uid="{00000000-000C-0000-FFFF-FFFF00000000}" name="Tabela1" displayName="Tabela1" ref="A1:J79" totalsRowShown="0" headerRowDxfId="11" dataDxfId="10">
+  <autoFilter ref="A1:J79" xr:uid="{00000000-0009-0000-0100-000001000000}">
     <filterColumn colId="0" hiddenButton="1"/>
     <filterColumn colId="1" hiddenButton="1"/>
     <filterColumn colId="2" hiddenButton="1"/>
@@ -696,10 +696,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:J75"/>
+  <dimension ref="A1:J79"/>
   <sheetViews>
     <sheetView tabSelected="1" topLeftCell="A40" zoomScale="89" zoomScaleNormal="89" workbookViewId="0">
-      <selection activeCell="J74" sqref="J74"/>
+      <selection activeCell="A79" sqref="A79:J79"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -3117,6 +3117,134 @@
         <v>0</v>
       </c>
     </row>
+    <row r="76" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A76" s="20">
+        <v>43976</v>
+      </c>
+      <c r="B76" s="21">
+        <v>75770</v>
+      </c>
+      <c r="C76" s="22">
+        <v>754</v>
+      </c>
+      <c r="D76" s="22">
+        <v>1469</v>
+      </c>
+      <c r="E76" s="22">
+        <v>0</v>
+      </c>
+      <c r="F76" s="22">
+        <v>9</v>
+      </c>
+      <c r="G76" s="22">
+        <v>2</v>
+      </c>
+      <c r="H76" s="22">
+        <v>6</v>
+      </c>
+      <c r="I76" s="22">
+        <v>108</v>
+      </c>
+      <c r="J76" s="22">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="77" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A77" s="20">
+        <v>43977</v>
+      </c>
+      <c r="B77" s="21">
+        <v>76579</v>
+      </c>
+      <c r="C77" s="22">
+        <v>809</v>
+      </c>
+      <c r="D77" s="22">
+        <v>1471</v>
+      </c>
+      <c r="E77" s="22">
+        <v>2</v>
+      </c>
+      <c r="F77" s="22">
+        <v>8</v>
+      </c>
+      <c r="G77" s="22">
+        <v>2</v>
+      </c>
+      <c r="H77" s="22">
+        <v>2</v>
+      </c>
+      <c r="I77" s="22">
+        <v>108</v>
+      </c>
+      <c r="J77" s="22">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="78" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A78" s="20">
+        <v>43978</v>
+      </c>
+      <c r="B78" s="21">
+        <v>77210</v>
+      </c>
+      <c r="C78" s="22">
+        <v>631</v>
+      </c>
+      <c r="D78" s="22">
+        <v>1473</v>
+      </c>
+      <c r="E78" s="22">
+        <v>2</v>
+      </c>
+      <c r="F78" s="22">
+        <v>7</v>
+      </c>
+      <c r="G78" s="22">
+        <v>2</v>
+      </c>
+      <c r="H78" s="22">
+        <v>1</v>
+      </c>
+      <c r="I78" s="22">
+        <v>108</v>
+      </c>
+      <c r="J78" s="22">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="79" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A79" s="20">
+        <v>43979</v>
+      </c>
+      <c r="B79" s="21">
+        <v>77916</v>
+      </c>
+      <c r="C79" s="22">
+        <v>706</v>
+      </c>
+      <c r="D79" s="22">
+        <v>1473</v>
+      </c>
+      <c r="E79" s="22">
+        <v>0</v>
+      </c>
+      <c r="F79" s="22">
+        <v>7</v>
+      </c>
+      <c r="G79" s="22">
+        <v>2</v>
+      </c>
+      <c r="H79" s="22">
+        <v>0</v>
+      </c>
+      <c r="I79" s="22">
+        <v>108</v>
+      </c>
+      <c r="J79" s="22">
+        <v>0</v>
+      </c>
+    </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>

</xml_diff>

<commit_message>
Data updated by GitHub Bot (2020-05-29 20)
</commit_message>
<xml_diff>
--- a/output/snapshot/fdcf2531-4c3e-5c02-b63c-ee160ead6dea.xlsx
+++ b/output/snapshot/fdcf2531-4c3e-5c02-b63c-ee160ead6dea.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="I:\AKTUALNI PODATKI - KORONA\Za objavo na GOV.SI\ang\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{1E6DD62F-2BE2-47DC-A7ED-9B57C1589256}" xr6:coauthVersionLast="44" xr6:coauthVersionMax="44" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{730BD8E4-8830-4CB9-85DE-3D4608545396}" xr6:coauthVersionLast="44" xr6:coauthVersionMax="44" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -399,8 +399,8 @@
 </file>
 
 <file path=xl/tables/table1.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="1" xr:uid="{00000000-000C-0000-FFFF-FFFF00000000}" name="Tabela1" displayName="Tabela1" ref="A1:J75" totalsRowShown="0" headerRowDxfId="11" dataDxfId="10">
-  <autoFilter ref="A1:J75" xr:uid="{00000000-0009-0000-0100-000001000000}">
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="1" xr:uid="{00000000-000C-0000-FFFF-FFFF00000000}" name="Tabela1" displayName="Tabela1" ref="A1:J79" totalsRowShown="0" headerRowDxfId="11" dataDxfId="10">
+  <autoFilter ref="A1:J79" xr:uid="{00000000-0009-0000-0100-000001000000}">
     <filterColumn colId="0" hiddenButton="1"/>
     <filterColumn colId="1" hiddenButton="1"/>
     <filterColumn colId="2" hiddenButton="1"/>
@@ -696,10 +696,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:J75"/>
+  <dimension ref="A1:J79"/>
   <sheetViews>
     <sheetView tabSelected="1" topLeftCell="A40" zoomScale="89" zoomScaleNormal="89" workbookViewId="0">
-      <selection activeCell="J74" sqref="J74"/>
+      <selection activeCell="A79" sqref="A79:J79"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -3117,6 +3117,134 @@
         <v>0</v>
       </c>
     </row>
+    <row r="76" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A76" s="20">
+        <v>43976</v>
+      </c>
+      <c r="B76" s="21">
+        <v>75770</v>
+      </c>
+      <c r="C76" s="22">
+        <v>754</v>
+      </c>
+      <c r="D76" s="22">
+        <v>1469</v>
+      </c>
+      <c r="E76" s="22">
+        <v>0</v>
+      </c>
+      <c r="F76" s="22">
+        <v>9</v>
+      </c>
+      <c r="G76" s="22">
+        <v>2</v>
+      </c>
+      <c r="H76" s="22">
+        <v>6</v>
+      </c>
+      <c r="I76" s="22">
+        <v>108</v>
+      </c>
+      <c r="J76" s="22">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="77" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A77" s="20">
+        <v>43977</v>
+      </c>
+      <c r="B77" s="21">
+        <v>76579</v>
+      </c>
+      <c r="C77" s="22">
+        <v>809</v>
+      </c>
+      <c r="D77" s="22">
+        <v>1471</v>
+      </c>
+      <c r="E77" s="22">
+        <v>2</v>
+      </c>
+      <c r="F77" s="22">
+        <v>8</v>
+      </c>
+      <c r="G77" s="22">
+        <v>2</v>
+      </c>
+      <c r="H77" s="22">
+        <v>2</v>
+      </c>
+      <c r="I77" s="22">
+        <v>108</v>
+      </c>
+      <c r="J77" s="22">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="78" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A78" s="20">
+        <v>43978</v>
+      </c>
+      <c r="B78" s="21">
+        <v>77210</v>
+      </c>
+      <c r="C78" s="22">
+        <v>631</v>
+      </c>
+      <c r="D78" s="22">
+        <v>1473</v>
+      </c>
+      <c r="E78" s="22">
+        <v>2</v>
+      </c>
+      <c r="F78" s="22">
+        <v>7</v>
+      </c>
+      <c r="G78" s="22">
+        <v>2</v>
+      </c>
+      <c r="H78" s="22">
+        <v>1</v>
+      </c>
+      <c r="I78" s="22">
+        <v>108</v>
+      </c>
+      <c r="J78" s="22">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="79" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A79" s="20">
+        <v>43979</v>
+      </c>
+      <c r="B79" s="21">
+        <v>77916</v>
+      </c>
+      <c r="C79" s="22">
+        <v>706</v>
+      </c>
+      <c r="D79" s="22">
+        <v>1473</v>
+      </c>
+      <c r="E79" s="22">
+        <v>0</v>
+      </c>
+      <c r="F79" s="22">
+        <v>7</v>
+      </c>
+      <c r="G79" s="22">
+        <v>2</v>
+      </c>
+      <c r="H79" s="22">
+        <v>0</v>
+      </c>
+      <c r="I79" s="22">
+        <v>108</v>
+      </c>
+      <c r="J79" s="22">
+        <v>0</v>
+      </c>
+    </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>

</xml_diff>

<commit_message>
Data updated by GitHub Bot (2020-05-30 12)
</commit_message>
<xml_diff>
--- a/output/snapshot/fdcf2531-4c3e-5c02-b63c-ee160ead6dea.xlsx
+++ b/output/snapshot/fdcf2531-4c3e-5c02-b63c-ee160ead6dea.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="I:\AKTUALNI PODATKI - KORONA\Za objavo na GOV.SI\ang\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{1E6DD62F-2BE2-47DC-A7ED-9B57C1589256}" xr6:coauthVersionLast="44" xr6:coauthVersionMax="44" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{DBBABD5B-7542-419C-99C2-1797D8CEE55F}" xr6:coauthVersionLast="44" xr6:coauthVersionMax="44" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -399,8 +399,8 @@
 </file>
 
 <file path=xl/tables/table1.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="1" xr:uid="{00000000-000C-0000-FFFF-FFFF00000000}" name="Tabela1" displayName="Tabela1" ref="A1:J75" totalsRowShown="0" headerRowDxfId="11" dataDxfId="10">
-  <autoFilter ref="A1:J75" xr:uid="{00000000-0009-0000-0100-000001000000}">
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="1" xr:uid="{00000000-000C-0000-FFFF-FFFF00000000}" name="Tabela1" displayName="Tabela1" ref="A1:J80" totalsRowShown="0" headerRowDxfId="11" dataDxfId="10">
+  <autoFilter ref="A1:J80" xr:uid="{00000000-0009-0000-0100-000001000000}">
     <filterColumn colId="0" hiddenButton="1"/>
     <filterColumn colId="1" hiddenButton="1"/>
     <filterColumn colId="2" hiddenButton="1"/>
@@ -696,10 +696,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:J75"/>
+  <dimension ref="A1:J80"/>
   <sheetViews>
     <sheetView tabSelected="1" topLeftCell="A40" zoomScale="89" zoomScaleNormal="89" workbookViewId="0">
-      <selection activeCell="J74" sqref="J74"/>
+      <selection activeCell="A80" sqref="A80:J80"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -3117,6 +3117,166 @@
         <v>0</v>
       </c>
     </row>
+    <row r="76" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A76" s="20">
+        <v>43976</v>
+      </c>
+      <c r="B76" s="21">
+        <v>75770</v>
+      </c>
+      <c r="C76" s="22">
+        <v>754</v>
+      </c>
+      <c r="D76" s="22">
+        <v>1469</v>
+      </c>
+      <c r="E76" s="22">
+        <v>0</v>
+      </c>
+      <c r="F76" s="22">
+        <v>9</v>
+      </c>
+      <c r="G76" s="22">
+        <v>2</v>
+      </c>
+      <c r="H76" s="22">
+        <v>6</v>
+      </c>
+      <c r="I76" s="22">
+        <v>108</v>
+      </c>
+      <c r="J76" s="22">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="77" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A77" s="20">
+        <v>43977</v>
+      </c>
+      <c r="B77" s="21">
+        <v>76579</v>
+      </c>
+      <c r="C77" s="22">
+        <v>809</v>
+      </c>
+      <c r="D77" s="22">
+        <v>1471</v>
+      </c>
+      <c r="E77" s="22">
+        <v>2</v>
+      </c>
+      <c r="F77" s="22">
+        <v>8</v>
+      </c>
+      <c r="G77" s="22">
+        <v>2</v>
+      </c>
+      <c r="H77" s="22">
+        <v>2</v>
+      </c>
+      <c r="I77" s="22">
+        <v>108</v>
+      </c>
+      <c r="J77" s="22">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="78" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A78" s="20">
+        <v>43978</v>
+      </c>
+      <c r="B78" s="21">
+        <v>77210</v>
+      </c>
+      <c r="C78" s="22">
+        <v>631</v>
+      </c>
+      <c r="D78" s="22">
+        <v>1473</v>
+      </c>
+      <c r="E78" s="22">
+        <v>2</v>
+      </c>
+      <c r="F78" s="22">
+        <v>7</v>
+      </c>
+      <c r="G78" s="22">
+        <v>2</v>
+      </c>
+      <c r="H78" s="22">
+        <v>1</v>
+      </c>
+      <c r="I78" s="22">
+        <v>108</v>
+      </c>
+      <c r="J78" s="22">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="79" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A79" s="20">
+        <v>43979</v>
+      </c>
+      <c r="B79" s="21">
+        <v>77916</v>
+      </c>
+      <c r="C79" s="22">
+        <v>706</v>
+      </c>
+      <c r="D79" s="22">
+        <v>1473</v>
+      </c>
+      <c r="E79" s="22">
+        <v>0</v>
+      </c>
+      <c r="F79" s="22">
+        <v>7</v>
+      </c>
+      <c r="G79" s="22">
+        <v>2</v>
+      </c>
+      <c r="H79" s="22">
+        <v>0</v>
+      </c>
+      <c r="I79" s="22">
+        <v>108</v>
+      </c>
+      <c r="J79" s="22">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="80" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A80" s="20">
+        <v>43980</v>
+      </c>
+      <c r="B80" s="21">
+        <v>78529</v>
+      </c>
+      <c r="C80" s="22">
+        <v>613</v>
+      </c>
+      <c r="D80" s="22">
+        <v>1473</v>
+      </c>
+      <c r="E80" s="22">
+        <v>0</v>
+      </c>
+      <c r="F80" s="22">
+        <v>7</v>
+      </c>
+      <c r="G80" s="22">
+        <v>2</v>
+      </c>
+      <c r="H80" s="22">
+        <v>0</v>
+      </c>
+      <c r="I80" s="22">
+        <v>108</v>
+      </c>
+      <c r="J80" s="22">
+        <v>0</v>
+      </c>
+    </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>

</xml_diff>

<commit_message>
Data updated by GitHub Bot (2020-05-30 20)
</commit_message>
<xml_diff>
--- a/output/snapshot/fdcf2531-4c3e-5c02-b63c-ee160ead6dea.xlsx
+++ b/output/snapshot/fdcf2531-4c3e-5c02-b63c-ee160ead6dea.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="I:\AKTUALNI PODATKI - KORONA\Za objavo na GOV.SI\ang\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{1E6DD62F-2BE2-47DC-A7ED-9B57C1589256}" xr6:coauthVersionLast="44" xr6:coauthVersionMax="44" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{DBBABD5B-7542-419C-99C2-1797D8CEE55F}" xr6:coauthVersionLast="44" xr6:coauthVersionMax="44" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -399,8 +399,8 @@
 </file>
 
 <file path=xl/tables/table1.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="1" xr:uid="{00000000-000C-0000-FFFF-FFFF00000000}" name="Tabela1" displayName="Tabela1" ref="A1:J75" totalsRowShown="0" headerRowDxfId="11" dataDxfId="10">
-  <autoFilter ref="A1:J75" xr:uid="{00000000-0009-0000-0100-000001000000}">
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="1" xr:uid="{00000000-000C-0000-FFFF-FFFF00000000}" name="Tabela1" displayName="Tabela1" ref="A1:J80" totalsRowShown="0" headerRowDxfId="11" dataDxfId="10">
+  <autoFilter ref="A1:J80" xr:uid="{00000000-0009-0000-0100-000001000000}">
     <filterColumn colId="0" hiddenButton="1"/>
     <filterColumn colId="1" hiddenButton="1"/>
     <filterColumn colId="2" hiddenButton="1"/>
@@ -696,10 +696,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:J75"/>
+  <dimension ref="A1:J80"/>
   <sheetViews>
     <sheetView tabSelected="1" topLeftCell="A40" zoomScale="89" zoomScaleNormal="89" workbookViewId="0">
-      <selection activeCell="J74" sqref="J74"/>
+      <selection activeCell="A80" sqref="A80:J80"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -3117,6 +3117,166 @@
         <v>0</v>
       </c>
     </row>
+    <row r="76" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A76" s="20">
+        <v>43976</v>
+      </c>
+      <c r="B76" s="21">
+        <v>75770</v>
+      </c>
+      <c r="C76" s="22">
+        <v>754</v>
+      </c>
+      <c r="D76" s="22">
+        <v>1469</v>
+      </c>
+      <c r="E76" s="22">
+        <v>0</v>
+      </c>
+      <c r="F76" s="22">
+        <v>9</v>
+      </c>
+      <c r="G76" s="22">
+        <v>2</v>
+      </c>
+      <c r="H76" s="22">
+        <v>6</v>
+      </c>
+      <c r="I76" s="22">
+        <v>108</v>
+      </c>
+      <c r="J76" s="22">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="77" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A77" s="20">
+        <v>43977</v>
+      </c>
+      <c r="B77" s="21">
+        <v>76579</v>
+      </c>
+      <c r="C77" s="22">
+        <v>809</v>
+      </c>
+      <c r="D77" s="22">
+        <v>1471</v>
+      </c>
+      <c r="E77" s="22">
+        <v>2</v>
+      </c>
+      <c r="F77" s="22">
+        <v>8</v>
+      </c>
+      <c r="G77" s="22">
+        <v>2</v>
+      </c>
+      <c r="H77" s="22">
+        <v>2</v>
+      </c>
+      <c r="I77" s="22">
+        <v>108</v>
+      </c>
+      <c r="J77" s="22">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="78" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A78" s="20">
+        <v>43978</v>
+      </c>
+      <c r="B78" s="21">
+        <v>77210</v>
+      </c>
+      <c r="C78" s="22">
+        <v>631</v>
+      </c>
+      <c r="D78" s="22">
+        <v>1473</v>
+      </c>
+      <c r="E78" s="22">
+        <v>2</v>
+      </c>
+      <c r="F78" s="22">
+        <v>7</v>
+      </c>
+      <c r="G78" s="22">
+        <v>2</v>
+      </c>
+      <c r="H78" s="22">
+        <v>1</v>
+      </c>
+      <c r="I78" s="22">
+        <v>108</v>
+      </c>
+      <c r="J78" s="22">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="79" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A79" s="20">
+        <v>43979</v>
+      </c>
+      <c r="B79" s="21">
+        <v>77916</v>
+      </c>
+      <c r="C79" s="22">
+        <v>706</v>
+      </c>
+      <c r="D79" s="22">
+        <v>1473</v>
+      </c>
+      <c r="E79" s="22">
+        <v>0</v>
+      </c>
+      <c r="F79" s="22">
+        <v>7</v>
+      </c>
+      <c r="G79" s="22">
+        <v>2</v>
+      </c>
+      <c r="H79" s="22">
+        <v>0</v>
+      </c>
+      <c r="I79" s="22">
+        <v>108</v>
+      </c>
+      <c r="J79" s="22">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="80" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A80" s="20">
+        <v>43980</v>
+      </c>
+      <c r="B80" s="21">
+        <v>78529</v>
+      </c>
+      <c r="C80" s="22">
+        <v>613</v>
+      </c>
+      <c r="D80" s="22">
+        <v>1473</v>
+      </c>
+      <c r="E80" s="22">
+        <v>0</v>
+      </c>
+      <c r="F80" s="22">
+        <v>7</v>
+      </c>
+      <c r="G80" s="22">
+        <v>2</v>
+      </c>
+      <c r="H80" s="22">
+        <v>0</v>
+      </c>
+      <c r="I80" s="22">
+        <v>108</v>
+      </c>
+      <c r="J80" s="22">
+        <v>0</v>
+      </c>
+    </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>

</xml_diff>

<commit_message>
Data updated by GitHub Bot (2020-05-31 12)
</commit_message>
<xml_diff>
--- a/output/snapshot/fdcf2531-4c3e-5c02-b63c-ee160ead6dea.xlsx
+++ b/output/snapshot/fdcf2531-4c3e-5c02-b63c-ee160ead6dea.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="I:\AKTUALNI PODATKI - KORONA\Za objavo na GOV.SI\ang\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{1E6DD62F-2BE2-47DC-A7ED-9B57C1589256}" xr6:coauthVersionLast="44" xr6:coauthVersionMax="44" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{D2DADF33-DB18-477E-B813-3DBE9A11F99A}" xr6:coauthVersionLast="44" xr6:coauthVersionMax="44" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12576" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Covid-19 podatki" sheetId="1" r:id="rId1"/>
@@ -399,8 +399,8 @@
 </file>
 
 <file path=xl/tables/table1.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="1" xr:uid="{00000000-000C-0000-FFFF-FFFF00000000}" name="Tabela1" displayName="Tabela1" ref="A1:J75" totalsRowShown="0" headerRowDxfId="11" dataDxfId="10">
-  <autoFilter ref="A1:J75" xr:uid="{00000000-0009-0000-0100-000001000000}">
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="1" xr:uid="{00000000-000C-0000-FFFF-FFFF00000000}" name="Tabela1" displayName="Tabela1" ref="A1:J81" totalsRowShown="0" headerRowDxfId="11" dataDxfId="10">
+  <autoFilter ref="A1:J81" xr:uid="{00000000-0009-0000-0100-000001000000}">
     <filterColumn colId="0" hiddenButton="1"/>
     <filterColumn colId="1" hiddenButton="1"/>
     <filterColumn colId="2" hiddenButton="1"/>
@@ -696,28 +696,28 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:J75"/>
+  <dimension ref="A1:J81"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A40" zoomScale="89" zoomScaleNormal="89" workbookViewId="0">
-      <selection activeCell="J74" sqref="J74"/>
+    <sheetView tabSelected="1" topLeftCell="A50" zoomScale="89" zoomScaleNormal="89" workbookViewId="0">
+      <selection activeCell="A81" sqref="A81:J81"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
-    <col min="1" max="1" width="12.7109375" style="1" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="13.5703125" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="16.28515625" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="15.28515625" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="17.85546875" bestFit="1" customWidth="1"/>
-    <col min="6" max="6" width="35.42578125" bestFit="1" customWidth="1"/>
-    <col min="7" max="7" width="51.140625" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="12.6640625" style="1" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="13.5546875" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="16.33203125" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="15.33203125" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="17.88671875" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="35.44140625" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="51.109375" bestFit="1" customWidth="1"/>
     <col min="8" max="8" width="14" bestFit="1" customWidth="1"/>
-    <col min="9" max="9" width="13.85546875" bestFit="1" customWidth="1"/>
-    <col min="10" max="10" width="16.5703125" bestFit="1" customWidth="1"/>
+    <col min="9" max="9" width="13.88671875" bestFit="1" customWidth="1"/>
+    <col min="10" max="10" width="16.5546875" bestFit="1" customWidth="1"/>
     <col min="11" max="11" width="29" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A1" s="2" t="s">
         <v>0</v>
       </c>
@@ -749,7 +749,7 @@
         <v>9</v>
       </c>
     </row>
-    <row r="2" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A2" s="4">
         <v>43902</v>
       </c>
@@ -781,7 +781,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="3" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A3" s="4">
         <v>43903</v>
       </c>
@@ -813,7 +813,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="4" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A4" s="4">
         <v>43904</v>
       </c>
@@ -845,7 +845,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="5" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A5" s="4">
         <v>43905</v>
       </c>
@@ -877,7 +877,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="6" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A6" s="4">
         <v>43906</v>
       </c>
@@ -909,7 +909,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="7" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A7" s="4">
         <v>43907</v>
       </c>
@@ -941,7 +941,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="8" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A8" s="4">
         <v>43908</v>
       </c>
@@ -973,7 +973,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="9" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A9" s="4">
         <v>43909</v>
       </c>
@@ -1005,7 +1005,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="10" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="10" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A10" s="4">
         <v>43910</v>
       </c>
@@ -1037,7 +1037,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="11" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="11" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A11" s="4">
         <v>43911</v>
       </c>
@@ -1069,7 +1069,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="12" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="12" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A12" s="4">
         <v>43912</v>
       </c>
@@ -1101,7 +1101,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="13" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="13" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A13" s="4">
         <v>43913</v>
       </c>
@@ -1133,7 +1133,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="14" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="14" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A14" s="4">
         <v>43914</v>
       </c>
@@ -1165,7 +1165,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="15" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="15" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A15" s="4">
         <v>43915</v>
       </c>
@@ -1197,7 +1197,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="16" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="16" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A16" s="4">
         <v>43916</v>
       </c>
@@ -1229,7 +1229,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="17" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="17" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A17" s="6">
         <v>43917</v>
       </c>
@@ -1261,7 +1261,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="18" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="18" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A18" s="4">
         <v>43918</v>
       </c>
@@ -1293,7 +1293,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="19" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="19" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A19" s="4">
         <v>43919</v>
       </c>
@@ -1325,7 +1325,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="20" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="20" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A20" s="4">
         <v>43920</v>
       </c>
@@ -1357,7 +1357,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="21" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="21" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A21" s="4">
         <v>43921</v>
       </c>
@@ -1389,7 +1389,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="22" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="22" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A22" s="4">
         <v>43922</v>
       </c>
@@ -1421,7 +1421,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="23" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="23" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A23" s="4">
         <v>43923</v>
       </c>
@@ -1453,7 +1453,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="24" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="24" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A24" s="4">
         <v>43924</v>
       </c>
@@ -1485,7 +1485,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="25" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="25" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A25" s="4">
         <v>43925</v>
       </c>
@@ -1517,7 +1517,7 @@
         <v>6</v>
       </c>
     </row>
-    <row r="26" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="26" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A26" s="4">
         <v>43926</v>
       </c>
@@ -1549,7 +1549,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="27" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="27" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A27" s="4">
         <v>43927</v>
       </c>
@@ -1581,7 +1581,7 @@
         <v>6</v>
       </c>
     </row>
-    <row r="28" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="28" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A28" s="8">
         <v>43928</v>
       </c>
@@ -1613,7 +1613,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="29" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="29" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A29" s="4">
         <v>43929</v>
       </c>
@@ -1645,7 +1645,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="30" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="30" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A30" s="4">
         <v>43930</v>
       </c>
@@ -1677,7 +1677,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="31" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="31" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A31" s="4">
         <v>43931</v>
       </c>
@@ -1709,7 +1709,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="32" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="32" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A32" s="4">
         <v>43932</v>
       </c>
@@ -1741,7 +1741,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="33" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="33" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A33" s="4">
         <v>43933</v>
       </c>
@@ -1773,7 +1773,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="34" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="34" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A34" s="4">
         <v>43934</v>
       </c>
@@ -1805,7 +1805,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="35" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="35" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A35" s="4">
         <v>43935</v>
       </c>
@@ -1837,7 +1837,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="36" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="36" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A36" s="4">
         <v>43936</v>
       </c>
@@ -1869,7 +1869,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="37" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="37" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A37" s="4">
         <v>43937</v>
       </c>
@@ -1901,7 +1901,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="38" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="38" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A38" s="4">
         <v>43938</v>
       </c>
@@ -1933,7 +1933,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="39" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="39" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A39" s="4">
         <v>43939</v>
       </c>
@@ -1965,7 +1965,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="40" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="40" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A40" s="4">
         <v>43940</v>
       </c>
@@ -1997,7 +1997,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="41" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="41" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A41" s="4">
         <v>43941</v>
       </c>
@@ -2029,7 +2029,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="42" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="42" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A42" s="11">
         <v>43942</v>
       </c>
@@ -2061,7 +2061,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="43" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="43" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A43" s="4">
         <v>43943</v>
       </c>
@@ -2093,7 +2093,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="44" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="44" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A44" s="4">
         <v>43944</v>
       </c>
@@ -2125,7 +2125,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="45" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="45" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A45" s="4">
         <v>43945</v>
       </c>
@@ -2157,7 +2157,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="46" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="46" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A46" s="4">
         <v>43946</v>
       </c>
@@ -2189,7 +2189,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="47" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="47" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A47" s="8">
         <v>43947</v>
       </c>
@@ -2221,7 +2221,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="48" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="48" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A48" s="4">
         <v>43948</v>
       </c>
@@ -2253,7 +2253,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="49" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="49" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A49" s="4">
         <v>43949</v>
       </c>
@@ -2285,7 +2285,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="50" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="50" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A50" s="4">
         <v>43950</v>
       </c>
@@ -2317,7 +2317,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="51" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="51" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A51" s="14">
         <v>43951</v>
       </c>
@@ -2349,7 +2349,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="52" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="52" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A52" s="4">
         <v>43952</v>
       </c>
@@ -2381,7 +2381,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="53" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="53" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A53" s="4">
         <v>43953</v>
       </c>
@@ -2413,7 +2413,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="54" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="54" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A54" s="11">
         <v>43954</v>
       </c>
@@ -2445,7 +2445,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="55" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="55" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A55" s="4">
         <v>43955</v>
       </c>
@@ -2477,7 +2477,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="56" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="56" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A56" s="11">
         <v>43956</v>
       </c>
@@ -2509,7 +2509,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="57" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="57" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A57" s="4">
         <v>43957</v>
       </c>
@@ -2541,7 +2541,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="58" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="58" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A58" s="4">
         <v>43958</v>
       </c>
@@ -2573,7 +2573,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="59" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="59" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A59" s="4">
         <v>43959</v>
       </c>
@@ -2605,7 +2605,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="60" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="60" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A60" s="4">
         <v>43960</v>
       </c>
@@ -2637,7 +2637,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="61" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="61" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A61" s="4">
         <v>43961</v>
       </c>
@@ -2669,7 +2669,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="62" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="62" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A62" s="4">
         <v>43962</v>
       </c>
@@ -2701,7 +2701,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="63" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="63" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A63" s="4">
         <v>43963</v>
       </c>
@@ -2733,7 +2733,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="64" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="64" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A64" s="17">
         <v>43964</v>
       </c>
@@ -2765,7 +2765,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="65" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="65" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A65" s="14">
         <v>43965</v>
       </c>
@@ -2797,7 +2797,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="66" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="66" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A66" s="11">
         <v>43966</v>
       </c>
@@ -2829,7 +2829,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="67" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="67" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A67" s="14">
         <v>43967</v>
       </c>
@@ -2861,7 +2861,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="68" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="68" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A68" s="11">
         <v>43968</v>
       </c>
@@ -2893,7 +2893,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="69" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="69" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A69" s="14">
         <v>43969</v>
       </c>
@@ -2925,7 +2925,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="70" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="70" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A70" s="11">
         <v>43970</v>
       </c>
@@ -2957,7 +2957,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="71" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="71" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A71" s="20">
         <v>43971</v>
       </c>
@@ -2989,7 +2989,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="72" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="72" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A72" s="23">
         <v>43972</v>
       </c>
@@ -3021,7 +3021,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="73" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="73" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A73" s="20">
         <v>43973</v>
       </c>
@@ -3053,7 +3053,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="74" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="74" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A74" s="17">
         <v>43974</v>
       </c>
@@ -3085,7 +3085,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="75" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="75" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A75" s="20">
         <v>43975</v>
       </c>
@@ -3114,6 +3114,198 @@
         <v>107</v>
       </c>
       <c r="J75" s="22">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="76" spans="1:10" x14ac:dyDescent="0.3">
+      <c r="A76" s="20">
+        <v>43976</v>
+      </c>
+      <c r="B76" s="21">
+        <v>75770</v>
+      </c>
+      <c r="C76" s="22">
+        <v>754</v>
+      </c>
+      <c r="D76" s="22">
+        <v>1469</v>
+      </c>
+      <c r="E76" s="22">
+        <v>0</v>
+      </c>
+      <c r="F76" s="22">
+        <v>9</v>
+      </c>
+      <c r="G76" s="22">
+        <v>2</v>
+      </c>
+      <c r="H76" s="22">
+        <v>6</v>
+      </c>
+      <c r="I76" s="22">
+        <v>108</v>
+      </c>
+      <c r="J76" s="22">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="77" spans="1:10" x14ac:dyDescent="0.3">
+      <c r="A77" s="20">
+        <v>43977</v>
+      </c>
+      <c r="B77" s="21">
+        <v>76579</v>
+      </c>
+      <c r="C77" s="22">
+        <v>809</v>
+      </c>
+      <c r="D77" s="22">
+        <v>1471</v>
+      </c>
+      <c r="E77" s="22">
+        <v>2</v>
+      </c>
+      <c r="F77" s="22">
+        <v>8</v>
+      </c>
+      <c r="G77" s="22">
+        <v>2</v>
+      </c>
+      <c r="H77" s="22">
+        <v>2</v>
+      </c>
+      <c r="I77" s="22">
+        <v>108</v>
+      </c>
+      <c r="J77" s="22">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="78" spans="1:10" x14ac:dyDescent="0.3">
+      <c r="A78" s="20">
+        <v>43978</v>
+      </c>
+      <c r="B78" s="21">
+        <v>77210</v>
+      </c>
+      <c r="C78" s="22">
+        <v>631</v>
+      </c>
+      <c r="D78" s="22">
+        <v>1473</v>
+      </c>
+      <c r="E78" s="22">
+        <v>2</v>
+      </c>
+      <c r="F78" s="22">
+        <v>7</v>
+      </c>
+      <c r="G78" s="22">
+        <v>2</v>
+      </c>
+      <c r="H78" s="22">
+        <v>1</v>
+      </c>
+      <c r="I78" s="22">
+        <v>108</v>
+      </c>
+      <c r="J78" s="22">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="79" spans="1:10" x14ac:dyDescent="0.3">
+      <c r="A79" s="20">
+        <v>43979</v>
+      </c>
+      <c r="B79" s="21">
+        <v>77916</v>
+      </c>
+      <c r="C79" s="22">
+        <v>706</v>
+      </c>
+      <c r="D79" s="22">
+        <v>1473</v>
+      </c>
+      <c r="E79" s="22">
+        <v>0</v>
+      </c>
+      <c r="F79" s="22">
+        <v>7</v>
+      </c>
+      <c r="G79" s="22">
+        <v>2</v>
+      </c>
+      <c r="H79" s="22">
+        <v>0</v>
+      </c>
+      <c r="I79" s="22">
+        <v>108</v>
+      </c>
+      <c r="J79" s="22">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="80" spans="1:10" x14ac:dyDescent="0.3">
+      <c r="A80" s="20">
+        <v>43980</v>
+      </c>
+      <c r="B80" s="21">
+        <v>78529</v>
+      </c>
+      <c r="C80" s="22">
+        <v>613</v>
+      </c>
+      <c r="D80" s="22">
+        <v>1473</v>
+      </c>
+      <c r="E80" s="22">
+        <v>0</v>
+      </c>
+      <c r="F80" s="22">
+        <v>7</v>
+      </c>
+      <c r="G80" s="22">
+        <v>2</v>
+      </c>
+      <c r="H80" s="22">
+        <v>0</v>
+      </c>
+      <c r="I80" s="22">
+        <v>108</v>
+      </c>
+      <c r="J80" s="22">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="81" spans="1:10" x14ac:dyDescent="0.3">
+      <c r="A81" s="20">
+        <v>43981</v>
+      </c>
+      <c r="B81" s="22">
+        <v>78793</v>
+      </c>
+      <c r="C81" s="22">
+        <v>264</v>
+      </c>
+      <c r="D81" s="22">
+        <v>1473</v>
+      </c>
+      <c r="E81" s="22">
+        <v>0</v>
+      </c>
+      <c r="F81" s="22">
+        <v>6</v>
+      </c>
+      <c r="G81" s="22">
+        <v>2</v>
+      </c>
+      <c r="H81" s="22">
+        <v>1</v>
+      </c>
+      <c r="I81" s="22">
+        <v>108</v>
+      </c>
+      <c r="J81" s="22">
         <v>0</v>
       </c>
     </row>

</xml_diff>

<commit_message>
Data updated by GitHub Bot (2020-05-31 20)
</commit_message>
<xml_diff>
--- a/output/snapshot/fdcf2531-4c3e-5c02-b63c-ee160ead6dea.xlsx
+++ b/output/snapshot/fdcf2531-4c3e-5c02-b63c-ee160ead6dea.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="I:\AKTUALNI PODATKI - KORONA\Za objavo na GOV.SI\ang\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{1E6DD62F-2BE2-47DC-A7ED-9B57C1589256}" xr6:coauthVersionLast="44" xr6:coauthVersionMax="44" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{D2DADF33-DB18-477E-B813-3DBE9A11F99A}" xr6:coauthVersionLast="44" xr6:coauthVersionMax="44" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12576" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Covid-19 podatki" sheetId="1" r:id="rId1"/>
@@ -399,8 +399,8 @@
 </file>
 
 <file path=xl/tables/table1.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="1" xr:uid="{00000000-000C-0000-FFFF-FFFF00000000}" name="Tabela1" displayName="Tabela1" ref="A1:J75" totalsRowShown="0" headerRowDxfId="11" dataDxfId="10">
-  <autoFilter ref="A1:J75" xr:uid="{00000000-0009-0000-0100-000001000000}">
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="1" xr:uid="{00000000-000C-0000-FFFF-FFFF00000000}" name="Tabela1" displayName="Tabela1" ref="A1:J81" totalsRowShown="0" headerRowDxfId="11" dataDxfId="10">
+  <autoFilter ref="A1:J81" xr:uid="{00000000-0009-0000-0100-000001000000}">
     <filterColumn colId="0" hiddenButton="1"/>
     <filterColumn colId="1" hiddenButton="1"/>
     <filterColumn colId="2" hiddenButton="1"/>
@@ -696,28 +696,28 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:J75"/>
+  <dimension ref="A1:J81"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A40" zoomScale="89" zoomScaleNormal="89" workbookViewId="0">
-      <selection activeCell="J74" sqref="J74"/>
+    <sheetView tabSelected="1" topLeftCell="A50" zoomScale="89" zoomScaleNormal="89" workbookViewId="0">
+      <selection activeCell="A81" sqref="A81:J81"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
-    <col min="1" max="1" width="12.7109375" style="1" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="13.5703125" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="16.28515625" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="15.28515625" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="17.85546875" bestFit="1" customWidth="1"/>
-    <col min="6" max="6" width="35.42578125" bestFit="1" customWidth="1"/>
-    <col min="7" max="7" width="51.140625" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="12.6640625" style="1" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="13.5546875" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="16.33203125" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="15.33203125" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="17.88671875" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="35.44140625" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="51.109375" bestFit="1" customWidth="1"/>
     <col min="8" max="8" width="14" bestFit="1" customWidth="1"/>
-    <col min="9" max="9" width="13.85546875" bestFit="1" customWidth="1"/>
-    <col min="10" max="10" width="16.5703125" bestFit="1" customWidth="1"/>
+    <col min="9" max="9" width="13.88671875" bestFit="1" customWidth="1"/>
+    <col min="10" max="10" width="16.5546875" bestFit="1" customWidth="1"/>
     <col min="11" max="11" width="29" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A1" s="2" t="s">
         <v>0</v>
       </c>
@@ -749,7 +749,7 @@
         <v>9</v>
       </c>
     </row>
-    <row r="2" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A2" s="4">
         <v>43902</v>
       </c>
@@ -781,7 +781,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="3" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A3" s="4">
         <v>43903</v>
       </c>
@@ -813,7 +813,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="4" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A4" s="4">
         <v>43904</v>
       </c>
@@ -845,7 +845,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="5" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A5" s="4">
         <v>43905</v>
       </c>
@@ -877,7 +877,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="6" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A6" s="4">
         <v>43906</v>
       </c>
@@ -909,7 +909,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="7" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A7" s="4">
         <v>43907</v>
       </c>
@@ -941,7 +941,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="8" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A8" s="4">
         <v>43908</v>
       </c>
@@ -973,7 +973,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="9" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A9" s="4">
         <v>43909</v>
       </c>
@@ -1005,7 +1005,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="10" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="10" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A10" s="4">
         <v>43910</v>
       </c>
@@ -1037,7 +1037,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="11" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="11" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A11" s="4">
         <v>43911</v>
       </c>
@@ -1069,7 +1069,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="12" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="12" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A12" s="4">
         <v>43912</v>
       </c>
@@ -1101,7 +1101,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="13" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="13" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A13" s="4">
         <v>43913</v>
       </c>
@@ -1133,7 +1133,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="14" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="14" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A14" s="4">
         <v>43914</v>
       </c>
@@ -1165,7 +1165,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="15" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="15" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A15" s="4">
         <v>43915</v>
       </c>
@@ -1197,7 +1197,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="16" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="16" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A16" s="4">
         <v>43916</v>
       </c>
@@ -1229,7 +1229,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="17" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="17" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A17" s="6">
         <v>43917</v>
       </c>
@@ -1261,7 +1261,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="18" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="18" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A18" s="4">
         <v>43918</v>
       </c>
@@ -1293,7 +1293,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="19" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="19" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A19" s="4">
         <v>43919</v>
       </c>
@@ -1325,7 +1325,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="20" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="20" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A20" s="4">
         <v>43920</v>
       </c>
@@ -1357,7 +1357,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="21" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="21" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A21" s="4">
         <v>43921</v>
       </c>
@@ -1389,7 +1389,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="22" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="22" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A22" s="4">
         <v>43922</v>
       </c>
@@ -1421,7 +1421,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="23" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="23" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A23" s="4">
         <v>43923</v>
       </c>
@@ -1453,7 +1453,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="24" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="24" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A24" s="4">
         <v>43924</v>
       </c>
@@ -1485,7 +1485,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="25" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="25" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A25" s="4">
         <v>43925</v>
       </c>
@@ -1517,7 +1517,7 @@
         <v>6</v>
       </c>
     </row>
-    <row r="26" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="26" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A26" s="4">
         <v>43926</v>
       </c>
@@ -1549,7 +1549,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="27" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="27" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A27" s="4">
         <v>43927</v>
       </c>
@@ -1581,7 +1581,7 @@
         <v>6</v>
       </c>
     </row>
-    <row r="28" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="28" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A28" s="8">
         <v>43928</v>
       </c>
@@ -1613,7 +1613,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="29" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="29" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A29" s="4">
         <v>43929</v>
       </c>
@@ -1645,7 +1645,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="30" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="30" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A30" s="4">
         <v>43930</v>
       </c>
@@ -1677,7 +1677,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="31" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="31" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A31" s="4">
         <v>43931</v>
       </c>
@@ -1709,7 +1709,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="32" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="32" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A32" s="4">
         <v>43932</v>
       </c>
@@ -1741,7 +1741,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="33" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="33" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A33" s="4">
         <v>43933</v>
       </c>
@@ -1773,7 +1773,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="34" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="34" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A34" s="4">
         <v>43934</v>
       </c>
@@ -1805,7 +1805,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="35" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="35" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A35" s="4">
         <v>43935</v>
       </c>
@@ -1837,7 +1837,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="36" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="36" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A36" s="4">
         <v>43936</v>
       </c>
@@ -1869,7 +1869,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="37" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="37" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A37" s="4">
         <v>43937</v>
       </c>
@@ -1901,7 +1901,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="38" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="38" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A38" s="4">
         <v>43938</v>
       </c>
@@ -1933,7 +1933,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="39" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="39" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A39" s="4">
         <v>43939</v>
       </c>
@@ -1965,7 +1965,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="40" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="40" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A40" s="4">
         <v>43940</v>
       </c>
@@ -1997,7 +1997,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="41" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="41" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A41" s="4">
         <v>43941</v>
       </c>
@@ -2029,7 +2029,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="42" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="42" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A42" s="11">
         <v>43942</v>
       </c>
@@ -2061,7 +2061,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="43" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="43" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A43" s="4">
         <v>43943</v>
       </c>
@@ -2093,7 +2093,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="44" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="44" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A44" s="4">
         <v>43944</v>
       </c>
@@ -2125,7 +2125,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="45" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="45" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A45" s="4">
         <v>43945</v>
       </c>
@@ -2157,7 +2157,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="46" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="46" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A46" s="4">
         <v>43946</v>
       </c>
@@ -2189,7 +2189,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="47" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="47" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A47" s="8">
         <v>43947</v>
       </c>
@@ -2221,7 +2221,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="48" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="48" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A48" s="4">
         <v>43948</v>
       </c>
@@ -2253,7 +2253,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="49" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="49" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A49" s="4">
         <v>43949</v>
       </c>
@@ -2285,7 +2285,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="50" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="50" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A50" s="4">
         <v>43950</v>
       </c>
@@ -2317,7 +2317,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="51" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="51" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A51" s="14">
         <v>43951</v>
       </c>
@@ -2349,7 +2349,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="52" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="52" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A52" s="4">
         <v>43952</v>
       </c>
@@ -2381,7 +2381,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="53" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="53" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A53" s="4">
         <v>43953</v>
       </c>
@@ -2413,7 +2413,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="54" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="54" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A54" s="11">
         <v>43954</v>
       </c>
@@ -2445,7 +2445,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="55" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="55" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A55" s="4">
         <v>43955</v>
       </c>
@@ -2477,7 +2477,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="56" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="56" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A56" s="11">
         <v>43956</v>
       </c>
@@ -2509,7 +2509,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="57" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="57" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A57" s="4">
         <v>43957</v>
       </c>
@@ -2541,7 +2541,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="58" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="58" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A58" s="4">
         <v>43958</v>
       </c>
@@ -2573,7 +2573,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="59" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="59" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A59" s="4">
         <v>43959</v>
       </c>
@@ -2605,7 +2605,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="60" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="60" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A60" s="4">
         <v>43960</v>
       </c>
@@ -2637,7 +2637,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="61" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="61" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A61" s="4">
         <v>43961</v>
       </c>
@@ -2669,7 +2669,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="62" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="62" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A62" s="4">
         <v>43962</v>
       </c>
@@ -2701,7 +2701,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="63" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="63" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A63" s="4">
         <v>43963</v>
       </c>
@@ -2733,7 +2733,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="64" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="64" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A64" s="17">
         <v>43964</v>
       </c>
@@ -2765,7 +2765,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="65" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="65" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A65" s="14">
         <v>43965</v>
       </c>
@@ -2797,7 +2797,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="66" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="66" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A66" s="11">
         <v>43966</v>
       </c>
@@ -2829,7 +2829,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="67" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="67" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A67" s="14">
         <v>43967</v>
       </c>
@@ -2861,7 +2861,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="68" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="68" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A68" s="11">
         <v>43968</v>
       </c>
@@ -2893,7 +2893,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="69" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="69" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A69" s="14">
         <v>43969</v>
       </c>
@@ -2925,7 +2925,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="70" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="70" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A70" s="11">
         <v>43970</v>
       </c>
@@ -2957,7 +2957,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="71" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="71" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A71" s="20">
         <v>43971</v>
       </c>
@@ -2989,7 +2989,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="72" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="72" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A72" s="23">
         <v>43972</v>
       </c>
@@ -3021,7 +3021,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="73" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="73" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A73" s="20">
         <v>43973</v>
       </c>
@@ -3053,7 +3053,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="74" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="74" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A74" s="17">
         <v>43974</v>
       </c>
@@ -3085,7 +3085,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="75" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="75" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A75" s="20">
         <v>43975</v>
       </c>
@@ -3114,6 +3114,198 @@
         <v>107</v>
       </c>
       <c r="J75" s="22">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="76" spans="1:10" x14ac:dyDescent="0.3">
+      <c r="A76" s="20">
+        <v>43976</v>
+      </c>
+      <c r="B76" s="21">
+        <v>75770</v>
+      </c>
+      <c r="C76" s="22">
+        <v>754</v>
+      </c>
+      <c r="D76" s="22">
+        <v>1469</v>
+      </c>
+      <c r="E76" s="22">
+        <v>0</v>
+      </c>
+      <c r="F76" s="22">
+        <v>9</v>
+      </c>
+      <c r="G76" s="22">
+        <v>2</v>
+      </c>
+      <c r="H76" s="22">
+        <v>6</v>
+      </c>
+      <c r="I76" s="22">
+        <v>108</v>
+      </c>
+      <c r="J76" s="22">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="77" spans="1:10" x14ac:dyDescent="0.3">
+      <c r="A77" s="20">
+        <v>43977</v>
+      </c>
+      <c r="B77" s="21">
+        <v>76579</v>
+      </c>
+      <c r="C77" s="22">
+        <v>809</v>
+      </c>
+      <c r="D77" s="22">
+        <v>1471</v>
+      </c>
+      <c r="E77" s="22">
+        <v>2</v>
+      </c>
+      <c r="F77" s="22">
+        <v>8</v>
+      </c>
+      <c r="G77" s="22">
+        <v>2</v>
+      </c>
+      <c r="H77" s="22">
+        <v>2</v>
+      </c>
+      <c r="I77" s="22">
+        <v>108</v>
+      </c>
+      <c r="J77" s="22">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="78" spans="1:10" x14ac:dyDescent="0.3">
+      <c r="A78" s="20">
+        <v>43978</v>
+      </c>
+      <c r="B78" s="21">
+        <v>77210</v>
+      </c>
+      <c r="C78" s="22">
+        <v>631</v>
+      </c>
+      <c r="D78" s="22">
+        <v>1473</v>
+      </c>
+      <c r="E78" s="22">
+        <v>2</v>
+      </c>
+      <c r="F78" s="22">
+        <v>7</v>
+      </c>
+      <c r="G78" s="22">
+        <v>2</v>
+      </c>
+      <c r="H78" s="22">
+        <v>1</v>
+      </c>
+      <c r="I78" s="22">
+        <v>108</v>
+      </c>
+      <c r="J78" s="22">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="79" spans="1:10" x14ac:dyDescent="0.3">
+      <c r="A79" s="20">
+        <v>43979</v>
+      </c>
+      <c r="B79" s="21">
+        <v>77916</v>
+      </c>
+      <c r="C79" s="22">
+        <v>706</v>
+      </c>
+      <c r="D79" s="22">
+        <v>1473</v>
+      </c>
+      <c r="E79" s="22">
+        <v>0</v>
+      </c>
+      <c r="F79" s="22">
+        <v>7</v>
+      </c>
+      <c r="G79" s="22">
+        <v>2</v>
+      </c>
+      <c r="H79" s="22">
+        <v>0</v>
+      </c>
+      <c r="I79" s="22">
+        <v>108</v>
+      </c>
+      <c r="J79" s="22">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="80" spans="1:10" x14ac:dyDescent="0.3">
+      <c r="A80" s="20">
+        <v>43980</v>
+      </c>
+      <c r="B80" s="21">
+        <v>78529</v>
+      </c>
+      <c r="C80" s="22">
+        <v>613</v>
+      </c>
+      <c r="D80" s="22">
+        <v>1473</v>
+      </c>
+      <c r="E80" s="22">
+        <v>0</v>
+      </c>
+      <c r="F80" s="22">
+        <v>7</v>
+      </c>
+      <c r="G80" s="22">
+        <v>2</v>
+      </c>
+      <c r="H80" s="22">
+        <v>0</v>
+      </c>
+      <c r="I80" s="22">
+        <v>108</v>
+      </c>
+      <c r="J80" s="22">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="81" spans="1:10" x14ac:dyDescent="0.3">
+      <c r="A81" s="20">
+        <v>43981</v>
+      </c>
+      <c r="B81" s="22">
+        <v>78793</v>
+      </c>
+      <c r="C81" s="22">
+        <v>264</v>
+      </c>
+      <c r="D81" s="22">
+        <v>1473</v>
+      </c>
+      <c r="E81" s="22">
+        <v>0</v>
+      </c>
+      <c r="F81" s="22">
+        <v>6</v>
+      </c>
+      <c r="G81" s="22">
+        <v>2</v>
+      </c>
+      <c r="H81" s="22">
+        <v>1</v>
+      </c>
+      <c r="I81" s="22">
+        <v>108</v>
+      </c>
+      <c r="J81" s="22">
         <v>0</v>
       </c>
     </row>

</xml_diff>

<commit_message>
Data updated by GitHub Bot (2020-06-01 12)
</commit_message>
<xml_diff>
--- a/output/snapshot/fdcf2531-4c3e-5c02-b63c-ee160ead6dea.xlsx
+++ b/output/snapshot/fdcf2531-4c3e-5c02-b63c-ee160ead6dea.xlsx
@@ -1,16 +1,15 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="21929"/>
-  <workbookPr/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
+  <fileVersion appName="xl" lastEdited="6" lowestEdited="6" rupBuild="14420"/>
+  <workbookPr defaultThemeVersion="164011"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="I:\AKTUALNI PODATKI - KORONA\Za objavo na GOV.SI\ang\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{1E6DD62F-2BE2-47DC-A7ED-9B57C1589256}" xr6:coauthVersionLast="44" xr6:coauthVersionMax="44" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-105" yWindow="-105" windowWidth="23250" windowHeight="12570"/>
   </bookViews>
   <sheets>
     <sheet name="Covid-19 podatki" sheetId="1" r:id="rId1"/>
@@ -60,7 +59,7 @@
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" mc:Ignorable="x14ac x16r2">
   <numFmts count="1">
     <numFmt numFmtId="164" formatCode="d/\ m/\ yyyy;@"/>
   </numFmts>
@@ -399,8 +398,8 @@
 </file>
 
 <file path=xl/tables/table1.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="1" xr:uid="{00000000-000C-0000-FFFF-FFFF00000000}" name="Tabela1" displayName="Tabela1" ref="A1:J75" totalsRowShown="0" headerRowDxfId="11" dataDxfId="10">
-  <autoFilter ref="A1:J75" xr:uid="{00000000-0009-0000-0100-000001000000}">
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="1" name="Tabela1" displayName="Tabela1" ref="A1:J82" totalsRowShown="0" headerRowDxfId="11" dataDxfId="10">
+  <autoFilter ref="A1:J82">
     <filterColumn colId="0" hiddenButton="1"/>
     <filterColumn colId="1" hiddenButton="1"/>
     <filterColumn colId="2" hiddenButton="1"/>
@@ -413,16 +412,16 @@
     <filterColumn colId="9" hiddenButton="1"/>
   </autoFilter>
   <tableColumns count="10">
-    <tableColumn id="1" xr3:uid="{00000000-0010-0000-0000-000001000000}" name="Date" dataDxfId="9"/>
-    <tableColumn id="2" xr3:uid="{00000000-0010-0000-0000-000002000000}" name="Tested (all)" dataDxfId="8"/>
-    <tableColumn id="3" xr3:uid="{00000000-0010-0000-0000-000003000000}" name="Tested (daily)" dataDxfId="7"/>
-    <tableColumn id="4" xr3:uid="{00000000-0010-0000-0000-000004000000}" name="Positive (all)" dataDxfId="6"/>
-    <tableColumn id="5" xr3:uid="{00000000-0010-0000-0000-000005000000}" name="Positive (daily)" dataDxfId="5"/>
-    <tableColumn id="6" xr3:uid="{00000000-0010-0000-0000-000006000000}" name="All hospitalized on certain day" dataDxfId="4"/>
-    <tableColumn id="7" xr3:uid="{00000000-0010-0000-0000-000007000000}" name="All persons in intensive care on certain day" dataDxfId="3"/>
-    <tableColumn id="10" xr3:uid="{00000000-0010-0000-0000-00000A000000}" name="Discharged" dataDxfId="2"/>
-    <tableColumn id="8" xr3:uid="{00000000-0010-0000-0000-000008000000}" name="Deaths (all)" dataDxfId="1"/>
-    <tableColumn id="9" xr3:uid="{00000000-0010-0000-0000-000009000000}" name="Deaths (daily)" dataDxfId="0"/>
+    <tableColumn id="1" name="Date" dataDxfId="9"/>
+    <tableColumn id="2" name="Tested (all)" dataDxfId="8"/>
+    <tableColumn id="3" name="Tested (daily)" dataDxfId="7"/>
+    <tableColumn id="4" name="Positive (all)" dataDxfId="6"/>
+    <tableColumn id="5" name="Positive (daily)" dataDxfId="5"/>
+    <tableColumn id="6" name="All hospitalized on certain day" dataDxfId="4"/>
+    <tableColumn id="7" name="All persons in intensive care on certain day" dataDxfId="3"/>
+    <tableColumn id="10" name="Discharged" dataDxfId="2"/>
+    <tableColumn id="8" name="Deaths (all)" dataDxfId="1"/>
+    <tableColumn id="9" name="Deaths (daily)" dataDxfId="0"/>
   </tableColumns>
   <tableStyleInfo name="TableStyleLight16" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
   <extLst>
@@ -695,11 +694,11 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:J75"/>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <dimension ref="A1:J82"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A40" zoomScale="89" zoomScaleNormal="89" workbookViewId="0">
-      <selection activeCell="J74" sqref="J74"/>
+    <sheetView tabSelected="1" topLeftCell="A50" zoomScale="89" zoomScaleNormal="89" workbookViewId="0">
+      <selection activeCell="A82" sqref="A82:J82"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -3117,6 +3116,230 @@
         <v>0</v>
       </c>
     </row>
+    <row r="76" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A76" s="20">
+        <v>43976</v>
+      </c>
+      <c r="B76" s="21">
+        <v>75770</v>
+      </c>
+      <c r="C76" s="22">
+        <v>754</v>
+      </c>
+      <c r="D76" s="22">
+        <v>1469</v>
+      </c>
+      <c r="E76" s="22">
+        <v>0</v>
+      </c>
+      <c r="F76" s="22">
+        <v>9</v>
+      </c>
+      <c r="G76" s="22">
+        <v>2</v>
+      </c>
+      <c r="H76" s="22">
+        <v>6</v>
+      </c>
+      <c r="I76" s="22">
+        <v>108</v>
+      </c>
+      <c r="J76" s="22">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="77" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A77" s="20">
+        <v>43977</v>
+      </c>
+      <c r="B77" s="21">
+        <v>76579</v>
+      </c>
+      <c r="C77" s="22">
+        <v>809</v>
+      </c>
+      <c r="D77" s="22">
+        <v>1471</v>
+      </c>
+      <c r="E77" s="22">
+        <v>2</v>
+      </c>
+      <c r="F77" s="22">
+        <v>8</v>
+      </c>
+      <c r="G77" s="22">
+        <v>2</v>
+      </c>
+      <c r="H77" s="22">
+        <v>2</v>
+      </c>
+      <c r="I77" s="22">
+        <v>108</v>
+      </c>
+      <c r="J77" s="22">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="78" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A78" s="20">
+        <v>43978</v>
+      </c>
+      <c r="B78" s="21">
+        <v>77210</v>
+      </c>
+      <c r="C78" s="22">
+        <v>631</v>
+      </c>
+      <c r="D78" s="22">
+        <v>1473</v>
+      </c>
+      <c r="E78" s="22">
+        <v>2</v>
+      </c>
+      <c r="F78" s="22">
+        <v>7</v>
+      </c>
+      <c r="G78" s="22">
+        <v>2</v>
+      </c>
+      <c r="H78" s="22">
+        <v>1</v>
+      </c>
+      <c r="I78" s="22">
+        <v>108</v>
+      </c>
+      <c r="J78" s="22">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="79" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A79" s="20">
+        <v>43979</v>
+      </c>
+      <c r="B79" s="21">
+        <v>77916</v>
+      </c>
+      <c r="C79" s="22">
+        <v>706</v>
+      </c>
+      <c r="D79" s="22">
+        <v>1473</v>
+      </c>
+      <c r="E79" s="22">
+        <v>0</v>
+      </c>
+      <c r="F79" s="22">
+        <v>7</v>
+      </c>
+      <c r="G79" s="22">
+        <v>2</v>
+      </c>
+      <c r="H79" s="22">
+        <v>0</v>
+      </c>
+      <c r="I79" s="22">
+        <v>108</v>
+      </c>
+      <c r="J79" s="22">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="80" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A80" s="20">
+        <v>43980</v>
+      </c>
+      <c r="B80" s="21">
+        <v>78529</v>
+      </c>
+      <c r="C80" s="22">
+        <v>613</v>
+      </c>
+      <c r="D80" s="22">
+        <v>1473</v>
+      </c>
+      <c r="E80" s="22">
+        <v>0</v>
+      </c>
+      <c r="F80" s="22">
+        <v>7</v>
+      </c>
+      <c r="G80" s="22">
+        <v>2</v>
+      </c>
+      <c r="H80" s="22">
+        <v>0</v>
+      </c>
+      <c r="I80" s="22">
+        <v>108</v>
+      </c>
+      <c r="J80" s="22">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="81" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A81" s="20">
+        <v>43981</v>
+      </c>
+      <c r="B81" s="22">
+        <v>78793</v>
+      </c>
+      <c r="C81" s="22">
+        <v>264</v>
+      </c>
+      <c r="D81" s="22">
+        <v>1473</v>
+      </c>
+      <c r="E81" s="22">
+        <v>0</v>
+      </c>
+      <c r="F81" s="22">
+        <v>6</v>
+      </c>
+      <c r="G81" s="22">
+        <v>2</v>
+      </c>
+      <c r="H81" s="22">
+        <v>1</v>
+      </c>
+      <c r="I81" s="22">
+        <v>108</v>
+      </c>
+      <c r="J81" s="22">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="82" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A82" s="20">
+        <v>43982</v>
+      </c>
+      <c r="B82" s="21">
+        <v>79039</v>
+      </c>
+      <c r="C82" s="22">
+        <v>246</v>
+      </c>
+      <c r="D82" s="22">
+        <v>1473</v>
+      </c>
+      <c r="E82" s="22">
+        <v>0</v>
+      </c>
+      <c r="F82" s="22">
+        <v>5</v>
+      </c>
+      <c r="G82" s="22">
+        <v>1</v>
+      </c>
+      <c r="H82" s="22">
+        <v>0</v>
+      </c>
+      <c r="I82" s="22">
+        <v>109</v>
+      </c>
+      <c r="J82" s="22">
+        <v>1</v>
+      </c>
+    </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>

</xml_diff>

<commit_message>
Data updated by GitHub Bot (2020-06-01 20)
</commit_message>
<xml_diff>
--- a/output/snapshot/fdcf2531-4c3e-5c02-b63c-ee160ead6dea.xlsx
+++ b/output/snapshot/fdcf2531-4c3e-5c02-b63c-ee160ead6dea.xlsx
@@ -1,16 +1,15 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="21929"/>
-  <workbookPr/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
+  <fileVersion appName="xl" lastEdited="6" lowestEdited="6" rupBuild="14420"/>
+  <workbookPr defaultThemeVersion="164011"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="I:\AKTUALNI PODATKI - KORONA\Za objavo na GOV.SI\ang\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{1E6DD62F-2BE2-47DC-A7ED-9B57C1589256}" xr6:coauthVersionLast="44" xr6:coauthVersionMax="44" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-105" yWindow="-105" windowWidth="23250" windowHeight="12570"/>
   </bookViews>
   <sheets>
     <sheet name="Covid-19 podatki" sheetId="1" r:id="rId1"/>
@@ -60,7 +59,7 @@
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" mc:Ignorable="x14ac x16r2">
   <numFmts count="1">
     <numFmt numFmtId="164" formatCode="d/\ m/\ yyyy;@"/>
   </numFmts>
@@ -399,8 +398,8 @@
 </file>
 
 <file path=xl/tables/table1.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="1" xr:uid="{00000000-000C-0000-FFFF-FFFF00000000}" name="Tabela1" displayName="Tabela1" ref="A1:J75" totalsRowShown="0" headerRowDxfId="11" dataDxfId="10">
-  <autoFilter ref="A1:J75" xr:uid="{00000000-0009-0000-0100-000001000000}">
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="1" name="Tabela1" displayName="Tabela1" ref="A1:J82" totalsRowShown="0" headerRowDxfId="11" dataDxfId="10">
+  <autoFilter ref="A1:J82">
     <filterColumn colId="0" hiddenButton="1"/>
     <filterColumn colId="1" hiddenButton="1"/>
     <filterColumn colId="2" hiddenButton="1"/>
@@ -413,16 +412,16 @@
     <filterColumn colId="9" hiddenButton="1"/>
   </autoFilter>
   <tableColumns count="10">
-    <tableColumn id="1" xr3:uid="{00000000-0010-0000-0000-000001000000}" name="Date" dataDxfId="9"/>
-    <tableColumn id="2" xr3:uid="{00000000-0010-0000-0000-000002000000}" name="Tested (all)" dataDxfId="8"/>
-    <tableColumn id="3" xr3:uid="{00000000-0010-0000-0000-000003000000}" name="Tested (daily)" dataDxfId="7"/>
-    <tableColumn id="4" xr3:uid="{00000000-0010-0000-0000-000004000000}" name="Positive (all)" dataDxfId="6"/>
-    <tableColumn id="5" xr3:uid="{00000000-0010-0000-0000-000005000000}" name="Positive (daily)" dataDxfId="5"/>
-    <tableColumn id="6" xr3:uid="{00000000-0010-0000-0000-000006000000}" name="All hospitalized on certain day" dataDxfId="4"/>
-    <tableColumn id="7" xr3:uid="{00000000-0010-0000-0000-000007000000}" name="All persons in intensive care on certain day" dataDxfId="3"/>
-    <tableColumn id="10" xr3:uid="{00000000-0010-0000-0000-00000A000000}" name="Discharged" dataDxfId="2"/>
-    <tableColumn id="8" xr3:uid="{00000000-0010-0000-0000-000008000000}" name="Deaths (all)" dataDxfId="1"/>
-    <tableColumn id="9" xr3:uid="{00000000-0010-0000-0000-000009000000}" name="Deaths (daily)" dataDxfId="0"/>
+    <tableColumn id="1" name="Date" dataDxfId="9"/>
+    <tableColumn id="2" name="Tested (all)" dataDxfId="8"/>
+    <tableColumn id="3" name="Tested (daily)" dataDxfId="7"/>
+    <tableColumn id="4" name="Positive (all)" dataDxfId="6"/>
+    <tableColumn id="5" name="Positive (daily)" dataDxfId="5"/>
+    <tableColumn id="6" name="All hospitalized on certain day" dataDxfId="4"/>
+    <tableColumn id="7" name="All persons in intensive care on certain day" dataDxfId="3"/>
+    <tableColumn id="10" name="Discharged" dataDxfId="2"/>
+    <tableColumn id="8" name="Deaths (all)" dataDxfId="1"/>
+    <tableColumn id="9" name="Deaths (daily)" dataDxfId="0"/>
   </tableColumns>
   <tableStyleInfo name="TableStyleLight16" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
   <extLst>
@@ -695,11 +694,11 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:J75"/>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <dimension ref="A1:J82"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A40" zoomScale="89" zoomScaleNormal="89" workbookViewId="0">
-      <selection activeCell="J74" sqref="J74"/>
+    <sheetView tabSelected="1" topLeftCell="A50" zoomScale="89" zoomScaleNormal="89" workbookViewId="0">
+      <selection activeCell="A82" sqref="A82:J82"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -3117,6 +3116,230 @@
         <v>0</v>
       </c>
     </row>
+    <row r="76" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A76" s="20">
+        <v>43976</v>
+      </c>
+      <c r="B76" s="21">
+        <v>75770</v>
+      </c>
+      <c r="C76" s="22">
+        <v>754</v>
+      </c>
+      <c r="D76" s="22">
+        <v>1469</v>
+      </c>
+      <c r="E76" s="22">
+        <v>0</v>
+      </c>
+      <c r="F76" s="22">
+        <v>9</v>
+      </c>
+      <c r="G76" s="22">
+        <v>2</v>
+      </c>
+      <c r="H76" s="22">
+        <v>6</v>
+      </c>
+      <c r="I76" s="22">
+        <v>108</v>
+      </c>
+      <c r="J76" s="22">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="77" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A77" s="20">
+        <v>43977</v>
+      </c>
+      <c r="B77" s="21">
+        <v>76579</v>
+      </c>
+      <c r="C77" s="22">
+        <v>809</v>
+      </c>
+      <c r="D77" s="22">
+        <v>1471</v>
+      </c>
+      <c r="E77" s="22">
+        <v>2</v>
+      </c>
+      <c r="F77" s="22">
+        <v>8</v>
+      </c>
+      <c r="G77" s="22">
+        <v>2</v>
+      </c>
+      <c r="H77" s="22">
+        <v>2</v>
+      </c>
+      <c r="I77" s="22">
+        <v>108</v>
+      </c>
+      <c r="J77" s="22">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="78" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A78" s="20">
+        <v>43978</v>
+      </c>
+      <c r="B78" s="21">
+        <v>77210</v>
+      </c>
+      <c r="C78" s="22">
+        <v>631</v>
+      </c>
+      <c r="D78" s="22">
+        <v>1473</v>
+      </c>
+      <c r="E78" s="22">
+        <v>2</v>
+      </c>
+      <c r="F78" s="22">
+        <v>7</v>
+      </c>
+      <c r="G78" s="22">
+        <v>2</v>
+      </c>
+      <c r="H78" s="22">
+        <v>1</v>
+      </c>
+      <c r="I78" s="22">
+        <v>108</v>
+      </c>
+      <c r="J78" s="22">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="79" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A79" s="20">
+        <v>43979</v>
+      </c>
+      <c r="B79" s="21">
+        <v>77916</v>
+      </c>
+      <c r="C79" s="22">
+        <v>706</v>
+      </c>
+      <c r="D79" s="22">
+        <v>1473</v>
+      </c>
+      <c r="E79" s="22">
+        <v>0</v>
+      </c>
+      <c r="F79" s="22">
+        <v>7</v>
+      </c>
+      <c r="G79" s="22">
+        <v>2</v>
+      </c>
+      <c r="H79" s="22">
+        <v>0</v>
+      </c>
+      <c r="I79" s="22">
+        <v>108</v>
+      </c>
+      <c r="J79" s="22">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="80" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A80" s="20">
+        <v>43980</v>
+      </c>
+      <c r="B80" s="21">
+        <v>78529</v>
+      </c>
+      <c r="C80" s="22">
+        <v>613</v>
+      </c>
+      <c r="D80" s="22">
+        <v>1473</v>
+      </c>
+      <c r="E80" s="22">
+        <v>0</v>
+      </c>
+      <c r="F80" s="22">
+        <v>7</v>
+      </c>
+      <c r="G80" s="22">
+        <v>2</v>
+      </c>
+      <c r="H80" s="22">
+        <v>0</v>
+      </c>
+      <c r="I80" s="22">
+        <v>108</v>
+      </c>
+      <c r="J80" s="22">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="81" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A81" s="20">
+        <v>43981</v>
+      </c>
+      <c r="B81" s="22">
+        <v>78793</v>
+      </c>
+      <c r="C81" s="22">
+        <v>264</v>
+      </c>
+      <c r="D81" s="22">
+        <v>1473</v>
+      </c>
+      <c r="E81" s="22">
+        <v>0</v>
+      </c>
+      <c r="F81" s="22">
+        <v>6</v>
+      </c>
+      <c r="G81" s="22">
+        <v>2</v>
+      </c>
+      <c r="H81" s="22">
+        <v>1</v>
+      </c>
+      <c r="I81" s="22">
+        <v>108</v>
+      </c>
+      <c r="J81" s="22">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="82" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A82" s="20">
+        <v>43982</v>
+      </c>
+      <c r="B82" s="21">
+        <v>79039</v>
+      </c>
+      <c r="C82" s="22">
+        <v>246</v>
+      </c>
+      <c r="D82" s="22">
+        <v>1473</v>
+      </c>
+      <c r="E82" s="22">
+        <v>0</v>
+      </c>
+      <c r="F82" s="22">
+        <v>5</v>
+      </c>
+      <c r="G82" s="22">
+        <v>1</v>
+      </c>
+      <c r="H82" s="22">
+        <v>0</v>
+      </c>
+      <c r="I82" s="22">
+        <v>109</v>
+      </c>
+      <c r="J82" s="22">
+        <v>1</v>
+      </c>
+    </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>

</xml_diff>

<commit_message>
Data updated by GitHub Bot (2020-06-02 12)
</commit_message>
<xml_diff>
--- a/output/snapshot/fdcf2531-4c3e-5c02-b63c-ee160ead6dea.xlsx
+++ b/output/snapshot/fdcf2531-4c3e-5c02-b63c-ee160ead6dea.xlsx
@@ -1,16 +1,15 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="21929"/>
-  <workbookPr/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
+  <fileVersion appName="xl" lastEdited="6" lowestEdited="6" rupBuild="14420"/>
+  <workbookPr defaultThemeVersion="164011"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="I:\AKTUALNI PODATKI - KORONA\Za objavo na GOV.SI\ang\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{1E6DD62F-2BE2-47DC-A7ED-9B57C1589256}" xr6:coauthVersionLast="44" xr6:coauthVersionMax="44" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-105" yWindow="-105" windowWidth="23250" windowHeight="12570"/>
   </bookViews>
   <sheets>
     <sheet name="Covid-19 podatki" sheetId="1" r:id="rId1"/>
@@ -60,7 +59,7 @@
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" mc:Ignorable="x14ac x16r2">
   <numFmts count="1">
     <numFmt numFmtId="164" formatCode="d/\ m/\ yyyy;@"/>
   </numFmts>
@@ -399,8 +398,8 @@
 </file>
 
 <file path=xl/tables/table1.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="1" xr:uid="{00000000-000C-0000-FFFF-FFFF00000000}" name="Tabela1" displayName="Tabela1" ref="A1:J75" totalsRowShown="0" headerRowDxfId="11" dataDxfId="10">
-  <autoFilter ref="A1:J75" xr:uid="{00000000-0009-0000-0100-000001000000}">
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="1" name="Tabela1" displayName="Tabela1" ref="A1:J83" totalsRowShown="0" headerRowDxfId="11" dataDxfId="10">
+  <autoFilter ref="A1:J83">
     <filterColumn colId="0" hiddenButton="1"/>
     <filterColumn colId="1" hiddenButton="1"/>
     <filterColumn colId="2" hiddenButton="1"/>
@@ -413,16 +412,16 @@
     <filterColumn colId="9" hiddenButton="1"/>
   </autoFilter>
   <tableColumns count="10">
-    <tableColumn id="1" xr3:uid="{00000000-0010-0000-0000-000001000000}" name="Date" dataDxfId="9"/>
-    <tableColumn id="2" xr3:uid="{00000000-0010-0000-0000-000002000000}" name="Tested (all)" dataDxfId="8"/>
-    <tableColumn id="3" xr3:uid="{00000000-0010-0000-0000-000003000000}" name="Tested (daily)" dataDxfId="7"/>
-    <tableColumn id="4" xr3:uid="{00000000-0010-0000-0000-000004000000}" name="Positive (all)" dataDxfId="6"/>
-    <tableColumn id="5" xr3:uid="{00000000-0010-0000-0000-000005000000}" name="Positive (daily)" dataDxfId="5"/>
-    <tableColumn id="6" xr3:uid="{00000000-0010-0000-0000-000006000000}" name="All hospitalized on certain day" dataDxfId="4"/>
-    <tableColumn id="7" xr3:uid="{00000000-0010-0000-0000-000007000000}" name="All persons in intensive care on certain day" dataDxfId="3"/>
-    <tableColumn id="10" xr3:uid="{00000000-0010-0000-0000-00000A000000}" name="Discharged" dataDxfId="2"/>
-    <tableColumn id="8" xr3:uid="{00000000-0010-0000-0000-000008000000}" name="Deaths (all)" dataDxfId="1"/>
-    <tableColumn id="9" xr3:uid="{00000000-0010-0000-0000-000009000000}" name="Deaths (daily)" dataDxfId="0"/>
+    <tableColumn id="1" name="Date" dataDxfId="9"/>
+    <tableColumn id="2" name="Tested (all)" dataDxfId="8"/>
+    <tableColumn id="3" name="Tested (daily)" dataDxfId="7"/>
+    <tableColumn id="4" name="Positive (all)" dataDxfId="6"/>
+    <tableColumn id="5" name="Positive (daily)" dataDxfId="5"/>
+    <tableColumn id="6" name="All hospitalized on certain day" dataDxfId="4"/>
+    <tableColumn id="7" name="All persons in intensive care on certain day" dataDxfId="3"/>
+    <tableColumn id="10" name="Discharged" dataDxfId="2"/>
+    <tableColumn id="8" name="Deaths (all)" dataDxfId="1"/>
+    <tableColumn id="9" name="Deaths (daily)" dataDxfId="0"/>
   </tableColumns>
   <tableStyleInfo name="TableStyleLight16" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
   <extLst>
@@ -695,11 +694,11 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:J75"/>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <dimension ref="A1:J83"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A40" zoomScale="89" zoomScaleNormal="89" workbookViewId="0">
-      <selection activeCell="J74" sqref="J74"/>
+    <sheetView tabSelected="1" topLeftCell="A50" zoomScale="89" zoomScaleNormal="89" workbookViewId="0">
+      <selection activeCell="A83" sqref="A83:J83"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -3117,6 +3116,262 @@
         <v>0</v>
       </c>
     </row>
+    <row r="76" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A76" s="20">
+        <v>43976</v>
+      </c>
+      <c r="B76" s="21">
+        <v>75770</v>
+      </c>
+      <c r="C76" s="22">
+        <v>754</v>
+      </c>
+      <c r="D76" s="22">
+        <v>1469</v>
+      </c>
+      <c r="E76" s="22">
+        <v>0</v>
+      </c>
+      <c r="F76" s="22">
+        <v>9</v>
+      </c>
+      <c r="G76" s="22">
+        <v>2</v>
+      </c>
+      <c r="H76" s="22">
+        <v>6</v>
+      </c>
+      <c r="I76" s="22">
+        <v>108</v>
+      </c>
+      <c r="J76" s="22">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="77" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A77" s="20">
+        <v>43977</v>
+      </c>
+      <c r="B77" s="21">
+        <v>76579</v>
+      </c>
+      <c r="C77" s="22">
+        <v>809</v>
+      </c>
+      <c r="D77" s="22">
+        <v>1471</v>
+      </c>
+      <c r="E77" s="22">
+        <v>2</v>
+      </c>
+      <c r="F77" s="22">
+        <v>8</v>
+      </c>
+      <c r="G77" s="22">
+        <v>2</v>
+      </c>
+      <c r="H77" s="22">
+        <v>2</v>
+      </c>
+      <c r="I77" s="22">
+        <v>108</v>
+      </c>
+      <c r="J77" s="22">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="78" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A78" s="20">
+        <v>43978</v>
+      </c>
+      <c r="B78" s="21">
+        <v>77210</v>
+      </c>
+      <c r="C78" s="22">
+        <v>631</v>
+      </c>
+      <c r="D78" s="22">
+        <v>1473</v>
+      </c>
+      <c r="E78" s="22">
+        <v>2</v>
+      </c>
+      <c r="F78" s="22">
+        <v>7</v>
+      </c>
+      <c r="G78" s="22">
+        <v>2</v>
+      </c>
+      <c r="H78" s="22">
+        <v>1</v>
+      </c>
+      <c r="I78" s="22">
+        <v>108</v>
+      </c>
+      <c r="J78" s="22">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="79" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A79" s="20">
+        <v>43979</v>
+      </c>
+      <c r="B79" s="21">
+        <v>77916</v>
+      </c>
+      <c r="C79" s="22">
+        <v>706</v>
+      </c>
+      <c r="D79" s="22">
+        <v>1473</v>
+      </c>
+      <c r="E79" s="22">
+        <v>0</v>
+      </c>
+      <c r="F79" s="22">
+        <v>7</v>
+      </c>
+      <c r="G79" s="22">
+        <v>2</v>
+      </c>
+      <c r="H79" s="22">
+        <v>0</v>
+      </c>
+      <c r="I79" s="22">
+        <v>108</v>
+      </c>
+      <c r="J79" s="22">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="80" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A80" s="20">
+        <v>43980</v>
+      </c>
+      <c r="B80" s="21">
+        <v>78529</v>
+      </c>
+      <c r="C80" s="22">
+        <v>613</v>
+      </c>
+      <c r="D80" s="22">
+        <v>1473</v>
+      </c>
+      <c r="E80" s="22">
+        <v>0</v>
+      </c>
+      <c r="F80" s="22">
+        <v>7</v>
+      </c>
+      <c r="G80" s="22">
+        <v>2</v>
+      </c>
+      <c r="H80" s="22">
+        <v>0</v>
+      </c>
+      <c r="I80" s="22">
+        <v>108</v>
+      </c>
+      <c r="J80" s="22">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="81" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A81" s="20">
+        <v>43981</v>
+      </c>
+      <c r="B81" s="22">
+        <v>78793</v>
+      </c>
+      <c r="C81" s="22">
+        <v>264</v>
+      </c>
+      <c r="D81" s="22">
+        <v>1473</v>
+      </c>
+      <c r="E81" s="22">
+        <v>0</v>
+      </c>
+      <c r="F81" s="22">
+        <v>6</v>
+      </c>
+      <c r="G81" s="22">
+        <v>2</v>
+      </c>
+      <c r="H81" s="22">
+        <v>1</v>
+      </c>
+      <c r="I81" s="22">
+        <v>108</v>
+      </c>
+      <c r="J81" s="22">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="82" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A82" s="20">
+        <v>43982</v>
+      </c>
+      <c r="B82" s="21">
+        <v>79039</v>
+      </c>
+      <c r="C82" s="22">
+        <v>246</v>
+      </c>
+      <c r="D82" s="22">
+        <v>1473</v>
+      </c>
+      <c r="E82" s="22">
+        <v>0</v>
+      </c>
+      <c r="F82" s="22">
+        <v>5</v>
+      </c>
+      <c r="G82" s="22">
+        <v>1</v>
+      </c>
+      <c r="H82" s="22">
+        <v>0</v>
+      </c>
+      <c r="I82" s="22">
+        <v>109</v>
+      </c>
+      <c r="J82" s="22">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="83" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A83" s="20">
+        <v>43983</v>
+      </c>
+      <c r="B83" s="21">
+        <v>79698</v>
+      </c>
+      <c r="C83" s="22">
+        <v>659</v>
+      </c>
+      <c r="D83" s="22">
+        <v>1475</v>
+      </c>
+      <c r="E83" s="22">
+        <v>2</v>
+      </c>
+      <c r="F83" s="22">
+        <v>5</v>
+      </c>
+      <c r="G83" s="22">
+        <v>1</v>
+      </c>
+      <c r="H83" s="22">
+        <v>0</v>
+      </c>
+      <c r="I83" s="22">
+        <v>109</v>
+      </c>
+      <c r="J83" s="22">
+        <v>0</v>
+      </c>
+    </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>

</xml_diff>

<commit_message>
Data updated by GitHub Bot (2020-06-02 20)
</commit_message>
<xml_diff>
--- a/output/snapshot/fdcf2531-4c3e-5c02-b63c-ee160ead6dea.xlsx
+++ b/output/snapshot/fdcf2531-4c3e-5c02-b63c-ee160ead6dea.xlsx
@@ -1,16 +1,15 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="21929"/>
-  <workbookPr/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
+  <fileVersion appName="xl" lastEdited="6" lowestEdited="6" rupBuild="14420"/>
+  <workbookPr defaultThemeVersion="164011"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="I:\AKTUALNI PODATKI - KORONA\Za objavo na GOV.SI\ang\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{1E6DD62F-2BE2-47DC-A7ED-9B57C1589256}" xr6:coauthVersionLast="44" xr6:coauthVersionMax="44" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-105" yWindow="-105" windowWidth="23250" windowHeight="12570"/>
   </bookViews>
   <sheets>
     <sheet name="Covid-19 podatki" sheetId="1" r:id="rId1"/>
@@ -60,7 +59,7 @@
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" mc:Ignorable="x14ac x16r2">
   <numFmts count="1">
     <numFmt numFmtId="164" formatCode="d/\ m/\ yyyy;@"/>
   </numFmts>
@@ -399,8 +398,8 @@
 </file>
 
 <file path=xl/tables/table1.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="1" xr:uid="{00000000-000C-0000-FFFF-FFFF00000000}" name="Tabela1" displayName="Tabela1" ref="A1:J75" totalsRowShown="0" headerRowDxfId="11" dataDxfId="10">
-  <autoFilter ref="A1:J75" xr:uid="{00000000-0009-0000-0100-000001000000}">
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="1" name="Tabela1" displayName="Tabela1" ref="A1:J83" totalsRowShown="0" headerRowDxfId="11" dataDxfId="10">
+  <autoFilter ref="A1:J83">
     <filterColumn colId="0" hiddenButton="1"/>
     <filterColumn colId="1" hiddenButton="1"/>
     <filterColumn colId="2" hiddenButton="1"/>
@@ -413,16 +412,16 @@
     <filterColumn colId="9" hiddenButton="1"/>
   </autoFilter>
   <tableColumns count="10">
-    <tableColumn id="1" xr3:uid="{00000000-0010-0000-0000-000001000000}" name="Date" dataDxfId="9"/>
-    <tableColumn id="2" xr3:uid="{00000000-0010-0000-0000-000002000000}" name="Tested (all)" dataDxfId="8"/>
-    <tableColumn id="3" xr3:uid="{00000000-0010-0000-0000-000003000000}" name="Tested (daily)" dataDxfId="7"/>
-    <tableColumn id="4" xr3:uid="{00000000-0010-0000-0000-000004000000}" name="Positive (all)" dataDxfId="6"/>
-    <tableColumn id="5" xr3:uid="{00000000-0010-0000-0000-000005000000}" name="Positive (daily)" dataDxfId="5"/>
-    <tableColumn id="6" xr3:uid="{00000000-0010-0000-0000-000006000000}" name="All hospitalized on certain day" dataDxfId="4"/>
-    <tableColumn id="7" xr3:uid="{00000000-0010-0000-0000-000007000000}" name="All persons in intensive care on certain day" dataDxfId="3"/>
-    <tableColumn id="10" xr3:uid="{00000000-0010-0000-0000-00000A000000}" name="Discharged" dataDxfId="2"/>
-    <tableColumn id="8" xr3:uid="{00000000-0010-0000-0000-000008000000}" name="Deaths (all)" dataDxfId="1"/>
-    <tableColumn id="9" xr3:uid="{00000000-0010-0000-0000-000009000000}" name="Deaths (daily)" dataDxfId="0"/>
+    <tableColumn id="1" name="Date" dataDxfId="9"/>
+    <tableColumn id="2" name="Tested (all)" dataDxfId="8"/>
+    <tableColumn id="3" name="Tested (daily)" dataDxfId="7"/>
+    <tableColumn id="4" name="Positive (all)" dataDxfId="6"/>
+    <tableColumn id="5" name="Positive (daily)" dataDxfId="5"/>
+    <tableColumn id="6" name="All hospitalized on certain day" dataDxfId="4"/>
+    <tableColumn id="7" name="All persons in intensive care on certain day" dataDxfId="3"/>
+    <tableColumn id="10" name="Discharged" dataDxfId="2"/>
+    <tableColumn id="8" name="Deaths (all)" dataDxfId="1"/>
+    <tableColumn id="9" name="Deaths (daily)" dataDxfId="0"/>
   </tableColumns>
   <tableStyleInfo name="TableStyleLight16" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
   <extLst>
@@ -695,11 +694,11 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:J75"/>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <dimension ref="A1:J83"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A40" zoomScale="89" zoomScaleNormal="89" workbookViewId="0">
-      <selection activeCell="J74" sqref="J74"/>
+    <sheetView tabSelected="1" topLeftCell="A50" zoomScale="89" zoomScaleNormal="89" workbookViewId="0">
+      <selection activeCell="A83" sqref="A83:J83"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -3117,6 +3116,262 @@
         <v>0</v>
       </c>
     </row>
+    <row r="76" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A76" s="20">
+        <v>43976</v>
+      </c>
+      <c r="B76" s="21">
+        <v>75770</v>
+      </c>
+      <c r="C76" s="22">
+        <v>754</v>
+      </c>
+      <c r="D76" s="22">
+        <v>1469</v>
+      </c>
+      <c r="E76" s="22">
+        <v>0</v>
+      </c>
+      <c r="F76" s="22">
+        <v>9</v>
+      </c>
+      <c r="G76" s="22">
+        <v>2</v>
+      </c>
+      <c r="H76" s="22">
+        <v>6</v>
+      </c>
+      <c r="I76" s="22">
+        <v>108</v>
+      </c>
+      <c r="J76" s="22">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="77" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A77" s="20">
+        <v>43977</v>
+      </c>
+      <c r="B77" s="21">
+        <v>76579</v>
+      </c>
+      <c r="C77" s="22">
+        <v>809</v>
+      </c>
+      <c r="D77" s="22">
+        <v>1471</v>
+      </c>
+      <c r="E77" s="22">
+        <v>2</v>
+      </c>
+      <c r="F77" s="22">
+        <v>8</v>
+      </c>
+      <c r="G77" s="22">
+        <v>2</v>
+      </c>
+      <c r="H77" s="22">
+        <v>2</v>
+      </c>
+      <c r="I77" s="22">
+        <v>108</v>
+      </c>
+      <c r="J77" s="22">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="78" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A78" s="20">
+        <v>43978</v>
+      </c>
+      <c r="B78" s="21">
+        <v>77210</v>
+      </c>
+      <c r="C78" s="22">
+        <v>631</v>
+      </c>
+      <c r="D78" s="22">
+        <v>1473</v>
+      </c>
+      <c r="E78" s="22">
+        <v>2</v>
+      </c>
+      <c r="F78" s="22">
+        <v>7</v>
+      </c>
+      <c r="G78" s="22">
+        <v>2</v>
+      </c>
+      <c r="H78" s="22">
+        <v>1</v>
+      </c>
+      <c r="I78" s="22">
+        <v>108</v>
+      </c>
+      <c r="J78" s="22">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="79" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A79" s="20">
+        <v>43979</v>
+      </c>
+      <c r="B79" s="21">
+        <v>77916</v>
+      </c>
+      <c r="C79" s="22">
+        <v>706</v>
+      </c>
+      <c r="D79" s="22">
+        <v>1473</v>
+      </c>
+      <c r="E79" s="22">
+        <v>0</v>
+      </c>
+      <c r="F79" s="22">
+        <v>7</v>
+      </c>
+      <c r="G79" s="22">
+        <v>2</v>
+      </c>
+      <c r="H79" s="22">
+        <v>0</v>
+      </c>
+      <c r="I79" s="22">
+        <v>108</v>
+      </c>
+      <c r="J79" s="22">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="80" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A80" s="20">
+        <v>43980</v>
+      </c>
+      <c r="B80" s="21">
+        <v>78529</v>
+      </c>
+      <c r="C80" s="22">
+        <v>613</v>
+      </c>
+      <c r="D80" s="22">
+        <v>1473</v>
+      </c>
+      <c r="E80" s="22">
+        <v>0</v>
+      </c>
+      <c r="F80" s="22">
+        <v>7</v>
+      </c>
+      <c r="G80" s="22">
+        <v>2</v>
+      </c>
+      <c r="H80" s="22">
+        <v>0</v>
+      </c>
+      <c r="I80" s="22">
+        <v>108</v>
+      </c>
+      <c r="J80" s="22">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="81" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A81" s="20">
+        <v>43981</v>
+      </c>
+      <c r="B81" s="22">
+        <v>78793</v>
+      </c>
+      <c r="C81" s="22">
+        <v>264</v>
+      </c>
+      <c r="D81" s="22">
+        <v>1473</v>
+      </c>
+      <c r="E81" s="22">
+        <v>0</v>
+      </c>
+      <c r="F81" s="22">
+        <v>6</v>
+      </c>
+      <c r="G81" s="22">
+        <v>2</v>
+      </c>
+      <c r="H81" s="22">
+        <v>1</v>
+      </c>
+      <c r="I81" s="22">
+        <v>108</v>
+      </c>
+      <c r="J81" s="22">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="82" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A82" s="20">
+        <v>43982</v>
+      </c>
+      <c r="B82" s="21">
+        <v>79039</v>
+      </c>
+      <c r="C82" s="22">
+        <v>246</v>
+      </c>
+      <c r="D82" s="22">
+        <v>1473</v>
+      </c>
+      <c r="E82" s="22">
+        <v>0</v>
+      </c>
+      <c r="F82" s="22">
+        <v>5</v>
+      </c>
+      <c r="G82" s="22">
+        <v>1</v>
+      </c>
+      <c r="H82" s="22">
+        <v>0</v>
+      </c>
+      <c r="I82" s="22">
+        <v>109</v>
+      </c>
+      <c r="J82" s="22">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="83" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A83" s="20">
+        <v>43983</v>
+      </c>
+      <c r="B83" s="21">
+        <v>79698</v>
+      </c>
+      <c r="C83" s="22">
+        <v>659</v>
+      </c>
+      <c r="D83" s="22">
+        <v>1475</v>
+      </c>
+      <c r="E83" s="22">
+        <v>2</v>
+      </c>
+      <c r="F83" s="22">
+        <v>5</v>
+      </c>
+      <c r="G83" s="22">
+        <v>1</v>
+      </c>
+      <c r="H83" s="22">
+        <v>0</v>
+      </c>
+      <c r="I83" s="22">
+        <v>109</v>
+      </c>
+      <c r="J83" s="22">
+        <v>0</v>
+      </c>
+    </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>

</xml_diff>

<commit_message>
Data updated by GitHub Bot (2020-06-03 12)
</commit_message>
<xml_diff>
--- a/output/snapshot/fdcf2531-4c3e-5c02-b63c-ee160ead6dea.xlsx
+++ b/output/snapshot/fdcf2531-4c3e-5c02-b63c-ee160ead6dea.xlsx
@@ -1,16 +1,15 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="21929"/>
-  <workbookPr/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
+  <fileVersion appName="xl" lastEdited="6" lowestEdited="6" rupBuild="14420"/>
+  <workbookPr defaultThemeVersion="164011"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="I:\AKTUALNI PODATKI - KORONA\Za objavo na GOV.SI\ang\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{1E6DD62F-2BE2-47DC-A7ED-9B57C1589256}" xr6:coauthVersionLast="44" xr6:coauthVersionMax="44" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-105" yWindow="-105" windowWidth="23250" windowHeight="12570"/>
   </bookViews>
   <sheets>
     <sheet name="Covid-19 podatki" sheetId="1" r:id="rId1"/>
@@ -60,7 +59,7 @@
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" mc:Ignorable="x14ac x16r2">
   <numFmts count="1">
     <numFmt numFmtId="164" formatCode="d/\ m/\ yyyy;@"/>
   </numFmts>
@@ -399,8 +398,8 @@
 </file>
 
 <file path=xl/tables/table1.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="1" xr:uid="{00000000-000C-0000-FFFF-FFFF00000000}" name="Tabela1" displayName="Tabela1" ref="A1:J75" totalsRowShown="0" headerRowDxfId="11" dataDxfId="10">
-  <autoFilter ref="A1:J75" xr:uid="{00000000-0009-0000-0100-000001000000}">
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="1" name="Tabela1" displayName="Tabela1" ref="A1:J84" totalsRowShown="0" headerRowDxfId="11" dataDxfId="10">
+  <autoFilter ref="A1:J84">
     <filterColumn colId="0" hiddenButton="1"/>
     <filterColumn colId="1" hiddenButton="1"/>
     <filterColumn colId="2" hiddenButton="1"/>
@@ -413,16 +412,16 @@
     <filterColumn colId="9" hiddenButton="1"/>
   </autoFilter>
   <tableColumns count="10">
-    <tableColumn id="1" xr3:uid="{00000000-0010-0000-0000-000001000000}" name="Date" dataDxfId="9"/>
-    <tableColumn id="2" xr3:uid="{00000000-0010-0000-0000-000002000000}" name="Tested (all)" dataDxfId="8"/>
-    <tableColumn id="3" xr3:uid="{00000000-0010-0000-0000-000003000000}" name="Tested (daily)" dataDxfId="7"/>
-    <tableColumn id="4" xr3:uid="{00000000-0010-0000-0000-000004000000}" name="Positive (all)" dataDxfId="6"/>
-    <tableColumn id="5" xr3:uid="{00000000-0010-0000-0000-000005000000}" name="Positive (daily)" dataDxfId="5"/>
-    <tableColumn id="6" xr3:uid="{00000000-0010-0000-0000-000006000000}" name="All hospitalized on certain day" dataDxfId="4"/>
-    <tableColumn id="7" xr3:uid="{00000000-0010-0000-0000-000007000000}" name="All persons in intensive care on certain day" dataDxfId="3"/>
-    <tableColumn id="10" xr3:uid="{00000000-0010-0000-0000-00000A000000}" name="Discharged" dataDxfId="2"/>
-    <tableColumn id="8" xr3:uid="{00000000-0010-0000-0000-000008000000}" name="Deaths (all)" dataDxfId="1"/>
-    <tableColumn id="9" xr3:uid="{00000000-0010-0000-0000-000009000000}" name="Deaths (daily)" dataDxfId="0"/>
+    <tableColumn id="1" name="Date" dataDxfId="9"/>
+    <tableColumn id="2" name="Tested (all)" dataDxfId="8"/>
+    <tableColumn id="3" name="Tested (daily)" dataDxfId="7"/>
+    <tableColumn id="4" name="Positive (all)" dataDxfId="6"/>
+    <tableColumn id="5" name="Positive (daily)" dataDxfId="5"/>
+    <tableColumn id="6" name="All hospitalized on certain day" dataDxfId="4"/>
+    <tableColumn id="7" name="All persons in intensive care on certain day" dataDxfId="3"/>
+    <tableColumn id="10" name="Discharged" dataDxfId="2"/>
+    <tableColumn id="8" name="Deaths (all)" dataDxfId="1"/>
+    <tableColumn id="9" name="Deaths (daily)" dataDxfId="0"/>
   </tableColumns>
   <tableStyleInfo name="TableStyleLight16" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
   <extLst>
@@ -695,11 +694,11 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:J75"/>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <dimension ref="A1:J84"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A40" zoomScale="89" zoomScaleNormal="89" workbookViewId="0">
-      <selection activeCell="J74" sqref="J74"/>
+    <sheetView tabSelected="1" topLeftCell="A50" zoomScale="89" zoomScaleNormal="89" workbookViewId="0">
+      <selection activeCell="A84" sqref="A84:J84"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -3117,6 +3116,294 @@
         <v>0</v>
       </c>
     </row>
+    <row r="76" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A76" s="20">
+        <v>43976</v>
+      </c>
+      <c r="B76" s="21">
+        <v>75770</v>
+      </c>
+      <c r="C76" s="22">
+        <v>754</v>
+      </c>
+      <c r="D76" s="22">
+        <v>1469</v>
+      </c>
+      <c r="E76" s="22">
+        <v>0</v>
+      </c>
+      <c r="F76" s="22">
+        <v>9</v>
+      </c>
+      <c r="G76" s="22">
+        <v>2</v>
+      </c>
+      <c r="H76" s="22">
+        <v>6</v>
+      </c>
+      <c r="I76" s="22">
+        <v>108</v>
+      </c>
+      <c r="J76" s="22">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="77" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A77" s="20">
+        <v>43977</v>
+      </c>
+      <c r="B77" s="21">
+        <v>76579</v>
+      </c>
+      <c r="C77" s="22">
+        <v>809</v>
+      </c>
+      <c r="D77" s="22">
+        <v>1471</v>
+      </c>
+      <c r="E77" s="22">
+        <v>2</v>
+      </c>
+      <c r="F77" s="22">
+        <v>8</v>
+      </c>
+      <c r="G77" s="22">
+        <v>2</v>
+      </c>
+      <c r="H77" s="22">
+        <v>2</v>
+      </c>
+      <c r="I77" s="22">
+        <v>108</v>
+      </c>
+      <c r="J77" s="22">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="78" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A78" s="20">
+        <v>43978</v>
+      </c>
+      <c r="B78" s="21">
+        <v>77210</v>
+      </c>
+      <c r="C78" s="22">
+        <v>631</v>
+      </c>
+      <c r="D78" s="22">
+        <v>1473</v>
+      </c>
+      <c r="E78" s="22">
+        <v>2</v>
+      </c>
+      <c r="F78" s="22">
+        <v>7</v>
+      </c>
+      <c r="G78" s="22">
+        <v>2</v>
+      </c>
+      <c r="H78" s="22">
+        <v>1</v>
+      </c>
+      <c r="I78" s="22">
+        <v>108</v>
+      </c>
+      <c r="J78" s="22">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="79" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A79" s="20">
+        <v>43979</v>
+      </c>
+      <c r="B79" s="21">
+        <v>77916</v>
+      </c>
+      <c r="C79" s="22">
+        <v>706</v>
+      </c>
+      <c r="D79" s="22">
+        <v>1473</v>
+      </c>
+      <c r="E79" s="22">
+        <v>0</v>
+      </c>
+      <c r="F79" s="22">
+        <v>7</v>
+      </c>
+      <c r="G79" s="22">
+        <v>2</v>
+      </c>
+      <c r="H79" s="22">
+        <v>0</v>
+      </c>
+      <c r="I79" s="22">
+        <v>108</v>
+      </c>
+      <c r="J79" s="22">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="80" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A80" s="20">
+        <v>43980</v>
+      </c>
+      <c r="B80" s="21">
+        <v>78529</v>
+      </c>
+      <c r="C80" s="22">
+        <v>613</v>
+      </c>
+      <c r="D80" s="22">
+        <v>1473</v>
+      </c>
+      <c r="E80" s="22">
+        <v>0</v>
+      </c>
+      <c r="F80" s="22">
+        <v>7</v>
+      </c>
+      <c r="G80" s="22">
+        <v>2</v>
+      </c>
+      <c r="H80" s="22">
+        <v>0</v>
+      </c>
+      <c r="I80" s="22">
+        <v>108</v>
+      </c>
+      <c r="J80" s="22">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="81" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A81" s="20">
+        <v>43981</v>
+      </c>
+      <c r="B81" s="22">
+        <v>78793</v>
+      </c>
+      <c r="C81" s="22">
+        <v>264</v>
+      </c>
+      <c r="D81" s="22">
+        <v>1473</v>
+      </c>
+      <c r="E81" s="22">
+        <v>0</v>
+      </c>
+      <c r="F81" s="22">
+        <v>6</v>
+      </c>
+      <c r="G81" s="22">
+        <v>2</v>
+      </c>
+      <c r="H81" s="22">
+        <v>1</v>
+      </c>
+      <c r="I81" s="22">
+        <v>108</v>
+      </c>
+      <c r="J81" s="22">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="82" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A82" s="20">
+        <v>43982</v>
+      </c>
+      <c r="B82" s="21">
+        <v>79039</v>
+      </c>
+      <c r="C82" s="22">
+        <v>246</v>
+      </c>
+      <c r="D82" s="22">
+        <v>1473</v>
+      </c>
+      <c r="E82" s="22">
+        <v>0</v>
+      </c>
+      <c r="F82" s="22">
+        <v>5</v>
+      </c>
+      <c r="G82" s="22">
+        <v>1</v>
+      </c>
+      <c r="H82" s="22">
+        <v>0</v>
+      </c>
+      <c r="I82" s="22">
+        <v>109</v>
+      </c>
+      <c r="J82" s="22">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="83" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A83" s="20">
+        <v>43983</v>
+      </c>
+      <c r="B83" s="21">
+        <v>79698</v>
+      </c>
+      <c r="C83" s="22">
+        <v>659</v>
+      </c>
+      <c r="D83" s="22">
+        <v>1475</v>
+      </c>
+      <c r="E83" s="22">
+        <v>2</v>
+      </c>
+      <c r="F83" s="22">
+        <v>5</v>
+      </c>
+      <c r="G83" s="22">
+        <v>1</v>
+      </c>
+      <c r="H83" s="22">
+        <v>0</v>
+      </c>
+      <c r="I83" s="22">
+        <v>109</v>
+      </c>
+      <c r="J83" s="22">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="84" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A84" s="20">
+        <v>43984</v>
+      </c>
+      <c r="B84" s="21">
+        <v>80505</v>
+      </c>
+      <c r="C84" s="22">
+        <v>807</v>
+      </c>
+      <c r="D84" s="22">
+        <v>1477</v>
+      </c>
+      <c r="E84" s="22">
+        <v>2</v>
+      </c>
+      <c r="F84" s="22">
+        <v>5</v>
+      </c>
+      <c r="G84" s="22">
+        <v>0</v>
+      </c>
+      <c r="H84" s="22">
+        <v>0</v>
+      </c>
+      <c r="I84" s="22">
+        <v>109</v>
+      </c>
+      <c r="J84" s="22">
+        <v>0</v>
+      </c>
+    </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>

</xml_diff>

<commit_message>
Data updated by GitHub Bot (2020-06-03 20)
</commit_message>
<xml_diff>
--- a/output/snapshot/fdcf2531-4c3e-5c02-b63c-ee160ead6dea.xlsx
+++ b/output/snapshot/fdcf2531-4c3e-5c02-b63c-ee160ead6dea.xlsx
@@ -1,16 +1,15 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="21929"/>
-  <workbookPr/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
+  <fileVersion appName="xl" lastEdited="6" lowestEdited="6" rupBuild="14420"/>
+  <workbookPr defaultThemeVersion="164011"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="I:\AKTUALNI PODATKI - KORONA\Za objavo na GOV.SI\ang\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{1E6DD62F-2BE2-47DC-A7ED-9B57C1589256}" xr6:coauthVersionLast="44" xr6:coauthVersionMax="44" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-105" yWindow="-105" windowWidth="23250" windowHeight="12570"/>
   </bookViews>
   <sheets>
     <sheet name="Covid-19 podatki" sheetId="1" r:id="rId1"/>
@@ -60,7 +59,7 @@
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" mc:Ignorable="x14ac x16r2">
   <numFmts count="1">
     <numFmt numFmtId="164" formatCode="d/\ m/\ yyyy;@"/>
   </numFmts>
@@ -399,8 +398,8 @@
 </file>
 
 <file path=xl/tables/table1.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="1" xr:uid="{00000000-000C-0000-FFFF-FFFF00000000}" name="Tabela1" displayName="Tabela1" ref="A1:J75" totalsRowShown="0" headerRowDxfId="11" dataDxfId="10">
-  <autoFilter ref="A1:J75" xr:uid="{00000000-0009-0000-0100-000001000000}">
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="1" name="Tabela1" displayName="Tabela1" ref="A1:J84" totalsRowShown="0" headerRowDxfId="11" dataDxfId="10">
+  <autoFilter ref="A1:J84">
     <filterColumn colId="0" hiddenButton="1"/>
     <filterColumn colId="1" hiddenButton="1"/>
     <filterColumn colId="2" hiddenButton="1"/>
@@ -413,16 +412,16 @@
     <filterColumn colId="9" hiddenButton="1"/>
   </autoFilter>
   <tableColumns count="10">
-    <tableColumn id="1" xr3:uid="{00000000-0010-0000-0000-000001000000}" name="Date" dataDxfId="9"/>
-    <tableColumn id="2" xr3:uid="{00000000-0010-0000-0000-000002000000}" name="Tested (all)" dataDxfId="8"/>
-    <tableColumn id="3" xr3:uid="{00000000-0010-0000-0000-000003000000}" name="Tested (daily)" dataDxfId="7"/>
-    <tableColumn id="4" xr3:uid="{00000000-0010-0000-0000-000004000000}" name="Positive (all)" dataDxfId="6"/>
-    <tableColumn id="5" xr3:uid="{00000000-0010-0000-0000-000005000000}" name="Positive (daily)" dataDxfId="5"/>
-    <tableColumn id="6" xr3:uid="{00000000-0010-0000-0000-000006000000}" name="All hospitalized on certain day" dataDxfId="4"/>
-    <tableColumn id="7" xr3:uid="{00000000-0010-0000-0000-000007000000}" name="All persons in intensive care on certain day" dataDxfId="3"/>
-    <tableColumn id="10" xr3:uid="{00000000-0010-0000-0000-00000A000000}" name="Discharged" dataDxfId="2"/>
-    <tableColumn id="8" xr3:uid="{00000000-0010-0000-0000-000008000000}" name="Deaths (all)" dataDxfId="1"/>
-    <tableColumn id="9" xr3:uid="{00000000-0010-0000-0000-000009000000}" name="Deaths (daily)" dataDxfId="0"/>
+    <tableColumn id="1" name="Date" dataDxfId="9"/>
+    <tableColumn id="2" name="Tested (all)" dataDxfId="8"/>
+    <tableColumn id="3" name="Tested (daily)" dataDxfId="7"/>
+    <tableColumn id="4" name="Positive (all)" dataDxfId="6"/>
+    <tableColumn id="5" name="Positive (daily)" dataDxfId="5"/>
+    <tableColumn id="6" name="All hospitalized on certain day" dataDxfId="4"/>
+    <tableColumn id="7" name="All persons in intensive care on certain day" dataDxfId="3"/>
+    <tableColumn id="10" name="Discharged" dataDxfId="2"/>
+    <tableColumn id="8" name="Deaths (all)" dataDxfId="1"/>
+    <tableColumn id="9" name="Deaths (daily)" dataDxfId="0"/>
   </tableColumns>
   <tableStyleInfo name="TableStyleLight16" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
   <extLst>
@@ -695,11 +694,11 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:J75"/>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <dimension ref="A1:J84"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A40" zoomScale="89" zoomScaleNormal="89" workbookViewId="0">
-      <selection activeCell="J74" sqref="J74"/>
+    <sheetView tabSelected="1" topLeftCell="A50" zoomScale="89" zoomScaleNormal="89" workbookViewId="0">
+      <selection activeCell="A84" sqref="A84:J84"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -3117,6 +3116,294 @@
         <v>0</v>
       </c>
     </row>
+    <row r="76" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A76" s="20">
+        <v>43976</v>
+      </c>
+      <c r="B76" s="21">
+        <v>75770</v>
+      </c>
+      <c r="C76" s="22">
+        <v>754</v>
+      </c>
+      <c r="D76" s="22">
+        <v>1469</v>
+      </c>
+      <c r="E76" s="22">
+        <v>0</v>
+      </c>
+      <c r="F76" s="22">
+        <v>9</v>
+      </c>
+      <c r="G76" s="22">
+        <v>2</v>
+      </c>
+      <c r="H76" s="22">
+        <v>6</v>
+      </c>
+      <c r="I76" s="22">
+        <v>108</v>
+      </c>
+      <c r="J76" s="22">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="77" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A77" s="20">
+        <v>43977</v>
+      </c>
+      <c r="B77" s="21">
+        <v>76579</v>
+      </c>
+      <c r="C77" s="22">
+        <v>809</v>
+      </c>
+      <c r="D77" s="22">
+        <v>1471</v>
+      </c>
+      <c r="E77" s="22">
+        <v>2</v>
+      </c>
+      <c r="F77" s="22">
+        <v>8</v>
+      </c>
+      <c r="G77" s="22">
+        <v>2</v>
+      </c>
+      <c r="H77" s="22">
+        <v>2</v>
+      </c>
+      <c r="I77" s="22">
+        <v>108</v>
+      </c>
+      <c r="J77" s="22">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="78" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A78" s="20">
+        <v>43978</v>
+      </c>
+      <c r="B78" s="21">
+        <v>77210</v>
+      </c>
+      <c r="C78" s="22">
+        <v>631</v>
+      </c>
+      <c r="D78" s="22">
+        <v>1473</v>
+      </c>
+      <c r="E78" s="22">
+        <v>2</v>
+      </c>
+      <c r="F78" s="22">
+        <v>7</v>
+      </c>
+      <c r="G78" s="22">
+        <v>2</v>
+      </c>
+      <c r="H78" s="22">
+        <v>1</v>
+      </c>
+      <c r="I78" s="22">
+        <v>108</v>
+      </c>
+      <c r="J78" s="22">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="79" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A79" s="20">
+        <v>43979</v>
+      </c>
+      <c r="B79" s="21">
+        <v>77916</v>
+      </c>
+      <c r="C79" s="22">
+        <v>706</v>
+      </c>
+      <c r="D79" s="22">
+        <v>1473</v>
+      </c>
+      <c r="E79" s="22">
+        <v>0</v>
+      </c>
+      <c r="F79" s="22">
+        <v>7</v>
+      </c>
+      <c r="G79" s="22">
+        <v>2</v>
+      </c>
+      <c r="H79" s="22">
+        <v>0</v>
+      </c>
+      <c r="I79" s="22">
+        <v>108</v>
+      </c>
+      <c r="J79" s="22">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="80" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A80" s="20">
+        <v>43980</v>
+      </c>
+      <c r="B80" s="21">
+        <v>78529</v>
+      </c>
+      <c r="C80" s="22">
+        <v>613</v>
+      </c>
+      <c r="D80" s="22">
+        <v>1473</v>
+      </c>
+      <c r="E80" s="22">
+        <v>0</v>
+      </c>
+      <c r="F80" s="22">
+        <v>7</v>
+      </c>
+      <c r="G80" s="22">
+        <v>2</v>
+      </c>
+      <c r="H80" s="22">
+        <v>0</v>
+      </c>
+      <c r="I80" s="22">
+        <v>108</v>
+      </c>
+      <c r="J80" s="22">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="81" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A81" s="20">
+        <v>43981</v>
+      </c>
+      <c r="B81" s="22">
+        <v>78793</v>
+      </c>
+      <c r="C81" s="22">
+        <v>264</v>
+      </c>
+      <c r="D81" s="22">
+        <v>1473</v>
+      </c>
+      <c r="E81" s="22">
+        <v>0</v>
+      </c>
+      <c r="F81" s="22">
+        <v>6</v>
+      </c>
+      <c r="G81" s="22">
+        <v>2</v>
+      </c>
+      <c r="H81" s="22">
+        <v>1</v>
+      </c>
+      <c r="I81" s="22">
+        <v>108</v>
+      </c>
+      <c r="J81" s="22">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="82" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A82" s="20">
+        <v>43982</v>
+      </c>
+      <c r="B82" s="21">
+        <v>79039</v>
+      </c>
+      <c r="C82" s="22">
+        <v>246</v>
+      </c>
+      <c r="D82" s="22">
+        <v>1473</v>
+      </c>
+      <c r="E82" s="22">
+        <v>0</v>
+      </c>
+      <c r="F82" s="22">
+        <v>5</v>
+      </c>
+      <c r="G82" s="22">
+        <v>1</v>
+      </c>
+      <c r="H82" s="22">
+        <v>0</v>
+      </c>
+      <c r="I82" s="22">
+        <v>109</v>
+      </c>
+      <c r="J82" s="22">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="83" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A83" s="20">
+        <v>43983</v>
+      </c>
+      <c r="B83" s="21">
+        <v>79698</v>
+      </c>
+      <c r="C83" s="22">
+        <v>659</v>
+      </c>
+      <c r="D83" s="22">
+        <v>1475</v>
+      </c>
+      <c r="E83" s="22">
+        <v>2</v>
+      </c>
+      <c r="F83" s="22">
+        <v>5</v>
+      </c>
+      <c r="G83" s="22">
+        <v>1</v>
+      </c>
+      <c r="H83" s="22">
+        <v>0</v>
+      </c>
+      <c r="I83" s="22">
+        <v>109</v>
+      </c>
+      <c r="J83" s="22">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="84" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A84" s="20">
+        <v>43984</v>
+      </c>
+      <c r="B84" s="21">
+        <v>80505</v>
+      </c>
+      <c r="C84" s="22">
+        <v>807</v>
+      </c>
+      <c r="D84" s="22">
+        <v>1477</v>
+      </c>
+      <c r="E84" s="22">
+        <v>2</v>
+      </c>
+      <c r="F84" s="22">
+        <v>5</v>
+      </c>
+      <c r="G84" s="22">
+        <v>0</v>
+      </c>
+      <c r="H84" s="22">
+        <v>0</v>
+      </c>
+      <c r="I84" s="22">
+        <v>109</v>
+      </c>
+      <c r="J84" s="22">
+        <v>0</v>
+      </c>
+    </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>

</xml_diff>

<commit_message>
Data updated by GitHub Bot (2020-06-04 12)
</commit_message>
<xml_diff>
--- a/output/snapshot/fdcf2531-4c3e-5c02-b63c-ee160ead6dea.xlsx
+++ b/output/snapshot/fdcf2531-4c3e-5c02-b63c-ee160ead6dea.xlsx
@@ -1,16 +1,15 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="21929"/>
-  <workbookPr/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
+  <fileVersion appName="xl" lastEdited="6" lowestEdited="6" rupBuild="14420"/>
+  <workbookPr defaultThemeVersion="164011"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="I:\AKTUALNI PODATKI - KORONA\Za objavo na GOV.SI\ang\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{1E6DD62F-2BE2-47DC-A7ED-9B57C1589256}" xr6:coauthVersionLast="44" xr6:coauthVersionMax="44" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-105" yWindow="-105" windowWidth="23250" windowHeight="12570"/>
   </bookViews>
   <sheets>
     <sheet name="Covid-19 podatki" sheetId="1" r:id="rId1"/>
@@ -60,7 +59,7 @@
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" mc:Ignorable="x14ac x16r2">
   <numFmts count="1">
     <numFmt numFmtId="164" formatCode="d/\ m/\ yyyy;@"/>
   </numFmts>
@@ -399,8 +398,8 @@
 </file>
 
 <file path=xl/tables/table1.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="1" xr:uid="{00000000-000C-0000-FFFF-FFFF00000000}" name="Tabela1" displayName="Tabela1" ref="A1:J75" totalsRowShown="0" headerRowDxfId="11" dataDxfId="10">
-  <autoFilter ref="A1:J75" xr:uid="{00000000-0009-0000-0100-000001000000}">
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="1" name="Tabela1" displayName="Tabela1" ref="A1:J85" totalsRowShown="0" headerRowDxfId="11" dataDxfId="10">
+  <autoFilter ref="A1:J85">
     <filterColumn colId="0" hiddenButton="1"/>
     <filterColumn colId="1" hiddenButton="1"/>
     <filterColumn colId="2" hiddenButton="1"/>
@@ -413,16 +412,16 @@
     <filterColumn colId="9" hiddenButton="1"/>
   </autoFilter>
   <tableColumns count="10">
-    <tableColumn id="1" xr3:uid="{00000000-0010-0000-0000-000001000000}" name="Date" dataDxfId="9"/>
-    <tableColumn id="2" xr3:uid="{00000000-0010-0000-0000-000002000000}" name="Tested (all)" dataDxfId="8"/>
-    <tableColumn id="3" xr3:uid="{00000000-0010-0000-0000-000003000000}" name="Tested (daily)" dataDxfId="7"/>
-    <tableColumn id="4" xr3:uid="{00000000-0010-0000-0000-000004000000}" name="Positive (all)" dataDxfId="6"/>
-    <tableColumn id="5" xr3:uid="{00000000-0010-0000-0000-000005000000}" name="Positive (daily)" dataDxfId="5"/>
-    <tableColumn id="6" xr3:uid="{00000000-0010-0000-0000-000006000000}" name="All hospitalized on certain day" dataDxfId="4"/>
-    <tableColumn id="7" xr3:uid="{00000000-0010-0000-0000-000007000000}" name="All persons in intensive care on certain day" dataDxfId="3"/>
-    <tableColumn id="10" xr3:uid="{00000000-0010-0000-0000-00000A000000}" name="Discharged" dataDxfId="2"/>
-    <tableColumn id="8" xr3:uid="{00000000-0010-0000-0000-000008000000}" name="Deaths (all)" dataDxfId="1"/>
-    <tableColumn id="9" xr3:uid="{00000000-0010-0000-0000-000009000000}" name="Deaths (daily)" dataDxfId="0"/>
+    <tableColumn id="1" name="Date" dataDxfId="9"/>
+    <tableColumn id="2" name="Tested (all)" dataDxfId="8"/>
+    <tableColumn id="3" name="Tested (daily)" dataDxfId="7"/>
+    <tableColumn id="4" name="Positive (all)" dataDxfId="6"/>
+    <tableColumn id="5" name="Positive (daily)" dataDxfId="5"/>
+    <tableColumn id="6" name="All hospitalized on certain day" dataDxfId="4"/>
+    <tableColumn id="7" name="All persons in intensive care on certain day" dataDxfId="3"/>
+    <tableColumn id="10" name="Discharged" dataDxfId="2"/>
+    <tableColumn id="8" name="Deaths (all)" dataDxfId="1"/>
+    <tableColumn id="9" name="Deaths (daily)" dataDxfId="0"/>
   </tableColumns>
   <tableStyleInfo name="TableStyleLight16" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
   <extLst>
@@ -695,11 +694,11 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:J75"/>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <dimension ref="A1:J85"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A40" zoomScale="89" zoomScaleNormal="89" workbookViewId="0">
-      <selection activeCell="J74" sqref="J74"/>
+    <sheetView tabSelected="1" topLeftCell="A50" zoomScale="89" zoomScaleNormal="89" workbookViewId="0">
+      <selection activeCell="J85" sqref="A85:J85"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -3117,6 +3116,326 @@
         <v>0</v>
       </c>
     </row>
+    <row r="76" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A76" s="20">
+        <v>43976</v>
+      </c>
+      <c r="B76" s="21">
+        <v>75770</v>
+      </c>
+      <c r="C76" s="22">
+        <v>754</v>
+      </c>
+      <c r="D76" s="22">
+        <v>1469</v>
+      </c>
+      <c r="E76" s="22">
+        <v>0</v>
+      </c>
+      <c r="F76" s="22">
+        <v>9</v>
+      </c>
+      <c r="G76" s="22">
+        <v>2</v>
+      </c>
+      <c r="H76" s="22">
+        <v>6</v>
+      </c>
+      <c r="I76" s="22">
+        <v>108</v>
+      </c>
+      <c r="J76" s="22">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="77" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A77" s="20">
+        <v>43977</v>
+      </c>
+      <c r="B77" s="21">
+        <v>76579</v>
+      </c>
+      <c r="C77" s="22">
+        <v>809</v>
+      </c>
+      <c r="D77" s="22">
+        <v>1471</v>
+      </c>
+      <c r="E77" s="22">
+        <v>2</v>
+      </c>
+      <c r="F77" s="22">
+        <v>8</v>
+      </c>
+      <c r="G77" s="22">
+        <v>2</v>
+      </c>
+      <c r="H77" s="22">
+        <v>2</v>
+      </c>
+      <c r="I77" s="22">
+        <v>108</v>
+      </c>
+      <c r="J77" s="22">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="78" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A78" s="20">
+        <v>43978</v>
+      </c>
+      <c r="B78" s="21">
+        <v>77210</v>
+      </c>
+      <c r="C78" s="22">
+        <v>631</v>
+      </c>
+      <c r="D78" s="22">
+        <v>1473</v>
+      </c>
+      <c r="E78" s="22">
+        <v>2</v>
+      </c>
+      <c r="F78" s="22">
+        <v>7</v>
+      </c>
+      <c r="G78" s="22">
+        <v>2</v>
+      </c>
+      <c r="H78" s="22">
+        <v>1</v>
+      </c>
+      <c r="I78" s="22">
+        <v>108</v>
+      </c>
+      <c r="J78" s="22">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="79" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A79" s="20">
+        <v>43979</v>
+      </c>
+      <c r="B79" s="21">
+        <v>77916</v>
+      </c>
+      <c r="C79" s="22">
+        <v>706</v>
+      </c>
+      <c r="D79" s="22">
+        <v>1473</v>
+      </c>
+      <c r="E79" s="22">
+        <v>0</v>
+      </c>
+      <c r="F79" s="22">
+        <v>7</v>
+      </c>
+      <c r="G79" s="22">
+        <v>2</v>
+      </c>
+      <c r="H79" s="22">
+        <v>0</v>
+      </c>
+      <c r="I79" s="22">
+        <v>108</v>
+      </c>
+      <c r="J79" s="22">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="80" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A80" s="20">
+        <v>43980</v>
+      </c>
+      <c r="B80" s="21">
+        <v>78529</v>
+      </c>
+      <c r="C80" s="22">
+        <v>613</v>
+      </c>
+      <c r="D80" s="22">
+        <v>1473</v>
+      </c>
+      <c r="E80" s="22">
+        <v>0</v>
+      </c>
+      <c r="F80" s="22">
+        <v>7</v>
+      </c>
+      <c r="G80" s="22">
+        <v>2</v>
+      </c>
+      <c r="H80" s="22">
+        <v>0</v>
+      </c>
+      <c r="I80" s="22">
+        <v>108</v>
+      </c>
+      <c r="J80" s="22">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="81" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A81" s="20">
+        <v>43981</v>
+      </c>
+      <c r="B81" s="22">
+        <v>78793</v>
+      </c>
+      <c r="C81" s="22">
+        <v>264</v>
+      </c>
+      <c r="D81" s="22">
+        <v>1473</v>
+      </c>
+      <c r="E81" s="22">
+        <v>0</v>
+      </c>
+      <c r="F81" s="22">
+        <v>6</v>
+      </c>
+      <c r="G81" s="22">
+        <v>2</v>
+      </c>
+      <c r="H81" s="22">
+        <v>1</v>
+      </c>
+      <c r="I81" s="22">
+        <v>108</v>
+      </c>
+      <c r="J81" s="22">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="82" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A82" s="20">
+        <v>43982</v>
+      </c>
+      <c r="B82" s="21">
+        <v>79039</v>
+      </c>
+      <c r="C82" s="22">
+        <v>246</v>
+      </c>
+      <c r="D82" s="22">
+        <v>1473</v>
+      </c>
+      <c r="E82" s="22">
+        <v>0</v>
+      </c>
+      <c r="F82" s="22">
+        <v>5</v>
+      </c>
+      <c r="G82" s="22">
+        <v>1</v>
+      </c>
+      <c r="H82" s="22">
+        <v>0</v>
+      </c>
+      <c r="I82" s="22">
+        <v>109</v>
+      </c>
+      <c r="J82" s="22">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="83" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A83" s="20">
+        <v>43983</v>
+      </c>
+      <c r="B83" s="21">
+        <v>79698</v>
+      </c>
+      <c r="C83" s="22">
+        <v>659</v>
+      </c>
+      <c r="D83" s="22">
+        <v>1475</v>
+      </c>
+      <c r="E83" s="22">
+        <v>2</v>
+      </c>
+      <c r="F83" s="22">
+        <v>5</v>
+      </c>
+      <c r="G83" s="22">
+        <v>1</v>
+      </c>
+      <c r="H83" s="22">
+        <v>0</v>
+      </c>
+      <c r="I83" s="22">
+        <v>109</v>
+      </c>
+      <c r="J83" s="22">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="84" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A84" s="20">
+        <v>43984</v>
+      </c>
+      <c r="B84" s="21">
+        <v>80505</v>
+      </c>
+      <c r="C84" s="22">
+        <v>807</v>
+      </c>
+      <c r="D84" s="22">
+        <v>1477</v>
+      </c>
+      <c r="E84" s="22">
+        <v>2</v>
+      </c>
+      <c r="F84" s="22">
+        <v>5</v>
+      </c>
+      <c r="G84" s="22">
+        <v>0</v>
+      </c>
+      <c r="H84" s="22">
+        <v>0</v>
+      </c>
+      <c r="I84" s="22">
+        <v>109</v>
+      </c>
+      <c r="J84" s="22">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="85" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A85" s="20">
+        <v>43985</v>
+      </c>
+      <c r="B85" s="21">
+        <v>81333</v>
+      </c>
+      <c r="C85" s="22">
+        <v>828</v>
+      </c>
+      <c r="D85" s="22">
+        <v>1477</v>
+      </c>
+      <c r="E85" s="22">
+        <v>0</v>
+      </c>
+      <c r="F85" s="22">
+        <v>5</v>
+      </c>
+      <c r="G85" s="22">
+        <v>0</v>
+      </c>
+      <c r="H85" s="22">
+        <v>0</v>
+      </c>
+      <c r="I85" s="22">
+        <v>109</v>
+      </c>
+      <c r="J85" s="22">
+        <v>0</v>
+      </c>
+    </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>

</xml_diff>

<commit_message>
Data updated by GitHub Bot (2020-06-04 20)
</commit_message>
<xml_diff>
--- a/output/snapshot/fdcf2531-4c3e-5c02-b63c-ee160ead6dea.xlsx
+++ b/output/snapshot/fdcf2531-4c3e-5c02-b63c-ee160ead6dea.xlsx
@@ -1,16 +1,15 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="21929"/>
-  <workbookPr/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
+  <fileVersion appName="xl" lastEdited="6" lowestEdited="6" rupBuild="14420"/>
+  <workbookPr defaultThemeVersion="164011"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="I:\AKTUALNI PODATKI - KORONA\Za objavo na GOV.SI\ang\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{1E6DD62F-2BE2-47DC-A7ED-9B57C1589256}" xr6:coauthVersionLast="44" xr6:coauthVersionMax="44" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-105" yWindow="-105" windowWidth="23250" windowHeight="12570"/>
   </bookViews>
   <sheets>
     <sheet name="Covid-19 podatki" sheetId="1" r:id="rId1"/>
@@ -60,7 +59,7 @@
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" mc:Ignorable="x14ac x16r2">
   <numFmts count="1">
     <numFmt numFmtId="164" formatCode="d/\ m/\ yyyy;@"/>
   </numFmts>
@@ -399,8 +398,8 @@
 </file>
 
 <file path=xl/tables/table1.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="1" xr:uid="{00000000-000C-0000-FFFF-FFFF00000000}" name="Tabela1" displayName="Tabela1" ref="A1:J75" totalsRowShown="0" headerRowDxfId="11" dataDxfId="10">
-  <autoFilter ref="A1:J75" xr:uid="{00000000-0009-0000-0100-000001000000}">
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="1" name="Tabela1" displayName="Tabela1" ref="A1:J85" totalsRowShown="0" headerRowDxfId="11" dataDxfId="10">
+  <autoFilter ref="A1:J85">
     <filterColumn colId="0" hiddenButton="1"/>
     <filterColumn colId="1" hiddenButton="1"/>
     <filterColumn colId="2" hiddenButton="1"/>
@@ -413,16 +412,16 @@
     <filterColumn colId="9" hiddenButton="1"/>
   </autoFilter>
   <tableColumns count="10">
-    <tableColumn id="1" xr3:uid="{00000000-0010-0000-0000-000001000000}" name="Date" dataDxfId="9"/>
-    <tableColumn id="2" xr3:uid="{00000000-0010-0000-0000-000002000000}" name="Tested (all)" dataDxfId="8"/>
-    <tableColumn id="3" xr3:uid="{00000000-0010-0000-0000-000003000000}" name="Tested (daily)" dataDxfId="7"/>
-    <tableColumn id="4" xr3:uid="{00000000-0010-0000-0000-000004000000}" name="Positive (all)" dataDxfId="6"/>
-    <tableColumn id="5" xr3:uid="{00000000-0010-0000-0000-000005000000}" name="Positive (daily)" dataDxfId="5"/>
-    <tableColumn id="6" xr3:uid="{00000000-0010-0000-0000-000006000000}" name="All hospitalized on certain day" dataDxfId="4"/>
-    <tableColumn id="7" xr3:uid="{00000000-0010-0000-0000-000007000000}" name="All persons in intensive care on certain day" dataDxfId="3"/>
-    <tableColumn id="10" xr3:uid="{00000000-0010-0000-0000-00000A000000}" name="Discharged" dataDxfId="2"/>
-    <tableColumn id="8" xr3:uid="{00000000-0010-0000-0000-000008000000}" name="Deaths (all)" dataDxfId="1"/>
-    <tableColumn id="9" xr3:uid="{00000000-0010-0000-0000-000009000000}" name="Deaths (daily)" dataDxfId="0"/>
+    <tableColumn id="1" name="Date" dataDxfId="9"/>
+    <tableColumn id="2" name="Tested (all)" dataDxfId="8"/>
+    <tableColumn id="3" name="Tested (daily)" dataDxfId="7"/>
+    <tableColumn id="4" name="Positive (all)" dataDxfId="6"/>
+    <tableColumn id="5" name="Positive (daily)" dataDxfId="5"/>
+    <tableColumn id="6" name="All hospitalized on certain day" dataDxfId="4"/>
+    <tableColumn id="7" name="All persons in intensive care on certain day" dataDxfId="3"/>
+    <tableColumn id="10" name="Discharged" dataDxfId="2"/>
+    <tableColumn id="8" name="Deaths (all)" dataDxfId="1"/>
+    <tableColumn id="9" name="Deaths (daily)" dataDxfId="0"/>
   </tableColumns>
   <tableStyleInfo name="TableStyleLight16" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
   <extLst>
@@ -695,11 +694,11 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:J75"/>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <dimension ref="A1:J85"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A40" zoomScale="89" zoomScaleNormal="89" workbookViewId="0">
-      <selection activeCell="J74" sqref="J74"/>
+    <sheetView tabSelected="1" topLeftCell="A50" zoomScale="89" zoomScaleNormal="89" workbookViewId="0">
+      <selection activeCell="J85" sqref="A85:J85"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -3117,6 +3116,326 @@
         <v>0</v>
       </c>
     </row>
+    <row r="76" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A76" s="20">
+        <v>43976</v>
+      </c>
+      <c r="B76" s="21">
+        <v>75770</v>
+      </c>
+      <c r="C76" s="22">
+        <v>754</v>
+      </c>
+      <c r="D76" s="22">
+        <v>1469</v>
+      </c>
+      <c r="E76" s="22">
+        <v>0</v>
+      </c>
+      <c r="F76" s="22">
+        <v>9</v>
+      </c>
+      <c r="G76" s="22">
+        <v>2</v>
+      </c>
+      <c r="H76" s="22">
+        <v>6</v>
+      </c>
+      <c r="I76" s="22">
+        <v>108</v>
+      </c>
+      <c r="J76" s="22">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="77" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A77" s="20">
+        <v>43977</v>
+      </c>
+      <c r="B77" s="21">
+        <v>76579</v>
+      </c>
+      <c r="C77" s="22">
+        <v>809</v>
+      </c>
+      <c r="D77" s="22">
+        <v>1471</v>
+      </c>
+      <c r="E77" s="22">
+        <v>2</v>
+      </c>
+      <c r="F77" s="22">
+        <v>8</v>
+      </c>
+      <c r="G77" s="22">
+        <v>2</v>
+      </c>
+      <c r="H77" s="22">
+        <v>2</v>
+      </c>
+      <c r="I77" s="22">
+        <v>108</v>
+      </c>
+      <c r="J77" s="22">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="78" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A78" s="20">
+        <v>43978</v>
+      </c>
+      <c r="B78" s="21">
+        <v>77210</v>
+      </c>
+      <c r="C78" s="22">
+        <v>631</v>
+      </c>
+      <c r="D78" s="22">
+        <v>1473</v>
+      </c>
+      <c r="E78" s="22">
+        <v>2</v>
+      </c>
+      <c r="F78" s="22">
+        <v>7</v>
+      </c>
+      <c r="G78" s="22">
+        <v>2</v>
+      </c>
+      <c r="H78" s="22">
+        <v>1</v>
+      </c>
+      <c r="I78" s="22">
+        <v>108</v>
+      </c>
+      <c r="J78" s="22">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="79" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A79" s="20">
+        <v>43979</v>
+      </c>
+      <c r="B79" s="21">
+        <v>77916</v>
+      </c>
+      <c r="C79" s="22">
+        <v>706</v>
+      </c>
+      <c r="D79" s="22">
+        <v>1473</v>
+      </c>
+      <c r="E79" s="22">
+        <v>0</v>
+      </c>
+      <c r="F79" s="22">
+        <v>7</v>
+      </c>
+      <c r="G79" s="22">
+        <v>2</v>
+      </c>
+      <c r="H79" s="22">
+        <v>0</v>
+      </c>
+      <c r="I79" s="22">
+        <v>108</v>
+      </c>
+      <c r="J79" s="22">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="80" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A80" s="20">
+        <v>43980</v>
+      </c>
+      <c r="B80" s="21">
+        <v>78529</v>
+      </c>
+      <c r="C80" s="22">
+        <v>613</v>
+      </c>
+      <c r="D80" s="22">
+        <v>1473</v>
+      </c>
+      <c r="E80" s="22">
+        <v>0</v>
+      </c>
+      <c r="F80" s="22">
+        <v>7</v>
+      </c>
+      <c r="G80" s="22">
+        <v>2</v>
+      </c>
+      <c r="H80" s="22">
+        <v>0</v>
+      </c>
+      <c r="I80" s="22">
+        <v>108</v>
+      </c>
+      <c r="J80" s="22">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="81" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A81" s="20">
+        <v>43981</v>
+      </c>
+      <c r="B81" s="22">
+        <v>78793</v>
+      </c>
+      <c r="C81" s="22">
+        <v>264</v>
+      </c>
+      <c r="D81" s="22">
+        <v>1473</v>
+      </c>
+      <c r="E81" s="22">
+        <v>0</v>
+      </c>
+      <c r="F81" s="22">
+        <v>6</v>
+      </c>
+      <c r="G81" s="22">
+        <v>2</v>
+      </c>
+      <c r="H81" s="22">
+        <v>1</v>
+      </c>
+      <c r="I81" s="22">
+        <v>108</v>
+      </c>
+      <c r="J81" s="22">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="82" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A82" s="20">
+        <v>43982</v>
+      </c>
+      <c r="B82" s="21">
+        <v>79039</v>
+      </c>
+      <c r="C82" s="22">
+        <v>246</v>
+      </c>
+      <c r="D82" s="22">
+        <v>1473</v>
+      </c>
+      <c r="E82" s="22">
+        <v>0</v>
+      </c>
+      <c r="F82" s="22">
+        <v>5</v>
+      </c>
+      <c r="G82" s="22">
+        <v>1</v>
+      </c>
+      <c r="H82" s="22">
+        <v>0</v>
+      </c>
+      <c r="I82" s="22">
+        <v>109</v>
+      </c>
+      <c r="J82" s="22">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="83" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A83" s="20">
+        <v>43983</v>
+      </c>
+      <c r="B83" s="21">
+        <v>79698</v>
+      </c>
+      <c r="C83" s="22">
+        <v>659</v>
+      </c>
+      <c r="D83" s="22">
+        <v>1475</v>
+      </c>
+      <c r="E83" s="22">
+        <v>2</v>
+      </c>
+      <c r="F83" s="22">
+        <v>5</v>
+      </c>
+      <c r="G83" s="22">
+        <v>1</v>
+      </c>
+      <c r="H83" s="22">
+        <v>0</v>
+      </c>
+      <c r="I83" s="22">
+        <v>109</v>
+      </c>
+      <c r="J83" s="22">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="84" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A84" s="20">
+        <v>43984</v>
+      </c>
+      <c r="B84" s="21">
+        <v>80505</v>
+      </c>
+      <c r="C84" s="22">
+        <v>807</v>
+      </c>
+      <c r="D84" s="22">
+        <v>1477</v>
+      </c>
+      <c r="E84" s="22">
+        <v>2</v>
+      </c>
+      <c r="F84" s="22">
+        <v>5</v>
+      </c>
+      <c r="G84" s="22">
+        <v>0</v>
+      </c>
+      <c r="H84" s="22">
+        <v>0</v>
+      </c>
+      <c r="I84" s="22">
+        <v>109</v>
+      </c>
+      <c r="J84" s="22">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="85" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A85" s="20">
+        <v>43985</v>
+      </c>
+      <c r="B85" s="21">
+        <v>81333</v>
+      </c>
+      <c r="C85" s="22">
+        <v>828</v>
+      </c>
+      <c r="D85" s="22">
+        <v>1477</v>
+      </c>
+      <c r="E85" s="22">
+        <v>0</v>
+      </c>
+      <c r="F85" s="22">
+        <v>5</v>
+      </c>
+      <c r="G85" s="22">
+        <v>0</v>
+      </c>
+      <c r="H85" s="22">
+        <v>0</v>
+      </c>
+      <c r="I85" s="22">
+        <v>109</v>
+      </c>
+      <c r="J85" s="22">
+        <v>0</v>
+      </c>
+    </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>

</xml_diff>

<commit_message>
Data updated by GitHub Bot (2020-06-05 12)
</commit_message>
<xml_diff>
--- a/output/snapshot/fdcf2531-4c3e-5c02-b63c-ee160ead6dea.xlsx
+++ b/output/snapshot/fdcf2531-4c3e-5c02-b63c-ee160ead6dea.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="I:\AKTUALNI PODATKI - KORONA\Za objavo na GOV.SI\ang\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{1E6DD62F-2BE2-47DC-A7ED-9B57C1589256}" xr6:coauthVersionLast="44" xr6:coauthVersionMax="44" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{E779F27A-C2D0-4365-A806-F279735D4FA6}" xr6:coauthVersionLast="44" xr6:coauthVersionMax="44" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="390" yWindow="390" windowWidth="21600" windowHeight="11205" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Covid-19 podatki" sheetId="1" r:id="rId1"/>
@@ -64,7 +64,7 @@
   <numFmts count="1">
     <numFmt numFmtId="164" formatCode="d/\ m/\ yyyy;@"/>
   </numFmts>
-  <fonts count="4" x14ac:knownFonts="1">
+  <fonts count="5" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -93,6 +93,13 @@
       <name val="Calibri Light"/>
       <scheme val="major"/>
     </font>
+    <font>
+      <sz val="10"/>
+      <color theme="1"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
   </fonts>
   <fills count="3">
     <fill>
@@ -108,7 +115,7 @@
       </patternFill>
     </fill>
   </fills>
-  <borders count="2">
+  <borders count="3">
     <border>
       <left/>
       <right/>
@@ -129,11 +136,26 @@
       <bottom/>
       <diagonal/>
     </border>
+    <border>
+      <left style="thin">
+        <color theme="4"/>
+      </left>
+      <right style="thin">
+        <color theme="4"/>
+      </right>
+      <top style="thin">
+        <color theme="4"/>
+      </top>
+      <bottom style="thin">
+        <color theme="4"/>
+      </bottom>
+      <diagonal/>
+    </border>
   </borders>
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="26">
+  <cellXfs count="29">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="49" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyAlignment="1" applyProtection="1">
       <alignment horizontal="left" vertical="top"/>
@@ -208,6 +230,15 @@
       <alignment horizontal="right"/>
     </xf>
     <xf numFmtId="0" fontId="3" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="right"/>
+    </xf>
+    <xf numFmtId="164" fontId="4" fillId="2" borderId="2" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="right" vertical="top"/>
+    </xf>
+    <xf numFmtId="3" fontId="4" fillId="2" borderId="2" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="right"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="2" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="right"/>
     </xf>
   </cellXfs>
@@ -399,8 +430,8 @@
 </file>
 
 <file path=xl/tables/table1.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="1" xr:uid="{00000000-000C-0000-FFFF-FFFF00000000}" name="Tabela1" displayName="Tabela1" ref="A1:J75" totalsRowShown="0" headerRowDxfId="11" dataDxfId="10">
-  <autoFilter ref="A1:J75" xr:uid="{00000000-0009-0000-0100-000001000000}">
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="1" xr:uid="{00000000-000C-0000-FFFF-FFFF00000000}" name="Tabela1" displayName="Tabela1" ref="A1:J86" totalsRowShown="0" headerRowDxfId="11" dataDxfId="10">
+  <autoFilter ref="A1:J86" xr:uid="{00000000-0009-0000-0100-000001000000}">
     <filterColumn colId="0" hiddenButton="1"/>
     <filterColumn colId="1" hiddenButton="1"/>
     <filterColumn colId="2" hiddenButton="1"/>
@@ -696,10 +727,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:J75"/>
+  <dimension ref="A1:J86"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A40" zoomScale="89" zoomScaleNormal="89" workbookViewId="0">
-      <selection activeCell="J74" sqref="J74"/>
+    <sheetView tabSelected="1" topLeftCell="A65" zoomScale="89" zoomScaleNormal="89" workbookViewId="0">
+      <selection activeCell="A86" sqref="A86:J86"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -3117,6 +3148,358 @@
         <v>0</v>
       </c>
     </row>
+    <row r="76" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A76" s="20">
+        <v>43976</v>
+      </c>
+      <c r="B76" s="21">
+        <v>75770</v>
+      </c>
+      <c r="C76" s="22">
+        <v>754</v>
+      </c>
+      <c r="D76" s="22">
+        <v>1469</v>
+      </c>
+      <c r="E76" s="22">
+        <v>0</v>
+      </c>
+      <c r="F76" s="22">
+        <v>9</v>
+      </c>
+      <c r="G76" s="22">
+        <v>2</v>
+      </c>
+      <c r="H76" s="22">
+        <v>6</v>
+      </c>
+      <c r="I76" s="22">
+        <v>108</v>
+      </c>
+      <c r="J76" s="22">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="77" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A77" s="20">
+        <v>43977</v>
+      </c>
+      <c r="B77" s="21">
+        <v>76579</v>
+      </c>
+      <c r="C77" s="22">
+        <v>809</v>
+      </c>
+      <c r="D77" s="22">
+        <v>1471</v>
+      </c>
+      <c r="E77" s="22">
+        <v>2</v>
+      </c>
+      <c r="F77" s="22">
+        <v>8</v>
+      </c>
+      <c r="G77" s="22">
+        <v>2</v>
+      </c>
+      <c r="H77" s="22">
+        <v>2</v>
+      </c>
+      <c r="I77" s="22">
+        <v>108</v>
+      </c>
+      <c r="J77" s="22">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="78" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A78" s="20">
+        <v>43978</v>
+      </c>
+      <c r="B78" s="21">
+        <v>77210</v>
+      </c>
+      <c r="C78" s="22">
+        <v>631</v>
+      </c>
+      <c r="D78" s="22">
+        <v>1473</v>
+      </c>
+      <c r="E78" s="22">
+        <v>2</v>
+      </c>
+      <c r="F78" s="22">
+        <v>7</v>
+      </c>
+      <c r="G78" s="22">
+        <v>2</v>
+      </c>
+      <c r="H78" s="22">
+        <v>1</v>
+      </c>
+      <c r="I78" s="22">
+        <v>108</v>
+      </c>
+      <c r="J78" s="22">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="79" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A79" s="20">
+        <v>43979</v>
+      </c>
+      <c r="B79" s="21">
+        <v>77916</v>
+      </c>
+      <c r="C79" s="22">
+        <v>706</v>
+      </c>
+      <c r="D79" s="22">
+        <v>1473</v>
+      </c>
+      <c r="E79" s="22">
+        <v>0</v>
+      </c>
+      <c r="F79" s="22">
+        <v>7</v>
+      </c>
+      <c r="G79" s="22">
+        <v>2</v>
+      </c>
+      <c r="H79" s="22">
+        <v>0</v>
+      </c>
+      <c r="I79" s="22">
+        <v>108</v>
+      </c>
+      <c r="J79" s="22">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="80" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A80" s="20">
+        <v>43980</v>
+      </c>
+      <c r="B80" s="21">
+        <v>78529</v>
+      </c>
+      <c r="C80" s="22">
+        <v>613</v>
+      </c>
+      <c r="D80" s="22">
+        <v>1473</v>
+      </c>
+      <c r="E80" s="22">
+        <v>0</v>
+      </c>
+      <c r="F80" s="22">
+        <v>7</v>
+      </c>
+      <c r="G80" s="22">
+        <v>2</v>
+      </c>
+      <c r="H80" s="22">
+        <v>0</v>
+      </c>
+      <c r="I80" s="22">
+        <v>108</v>
+      </c>
+      <c r="J80" s="22">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="81" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A81" s="20">
+        <v>43981</v>
+      </c>
+      <c r="B81" s="22">
+        <v>78793</v>
+      </c>
+      <c r="C81" s="22">
+        <v>264</v>
+      </c>
+      <c r="D81" s="22">
+        <v>1473</v>
+      </c>
+      <c r="E81" s="22">
+        <v>0</v>
+      </c>
+      <c r="F81" s="22">
+        <v>6</v>
+      </c>
+      <c r="G81" s="22">
+        <v>2</v>
+      </c>
+      <c r="H81" s="22">
+        <v>1</v>
+      </c>
+      <c r="I81" s="22">
+        <v>108</v>
+      </c>
+      <c r="J81" s="22">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="82" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A82" s="20">
+        <v>43982</v>
+      </c>
+      <c r="B82" s="21">
+        <v>79039</v>
+      </c>
+      <c r="C82" s="22">
+        <v>246</v>
+      </c>
+      <c r="D82" s="22">
+        <v>1473</v>
+      </c>
+      <c r="E82" s="22">
+        <v>0</v>
+      </c>
+      <c r="F82" s="22">
+        <v>5</v>
+      </c>
+      <c r="G82" s="22">
+        <v>1</v>
+      </c>
+      <c r="H82" s="22">
+        <v>0</v>
+      </c>
+      <c r="I82" s="22">
+        <v>109</v>
+      </c>
+      <c r="J82" s="22">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="83" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A83" s="20">
+        <v>43983</v>
+      </c>
+      <c r="B83" s="21">
+        <v>79698</v>
+      </c>
+      <c r="C83" s="22">
+        <v>659</v>
+      </c>
+      <c r="D83" s="22">
+        <v>1475</v>
+      </c>
+      <c r="E83" s="22">
+        <v>2</v>
+      </c>
+      <c r="F83" s="22">
+        <v>5</v>
+      </c>
+      <c r="G83" s="22">
+        <v>1</v>
+      </c>
+      <c r="H83" s="22">
+        <v>0</v>
+      </c>
+      <c r="I83" s="22">
+        <v>109</v>
+      </c>
+      <c r="J83" s="22">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="84" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A84" s="20">
+        <v>43984</v>
+      </c>
+      <c r="B84" s="21">
+        <v>80505</v>
+      </c>
+      <c r="C84" s="22">
+        <v>807</v>
+      </c>
+      <c r="D84" s="22">
+        <v>1477</v>
+      </c>
+      <c r="E84" s="22">
+        <v>2</v>
+      </c>
+      <c r="F84" s="22">
+        <v>5</v>
+      </c>
+      <c r="G84" s="22">
+        <v>0</v>
+      </c>
+      <c r="H84" s="22">
+        <v>0</v>
+      </c>
+      <c r="I84" s="22">
+        <v>109</v>
+      </c>
+      <c r="J84" s="22">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="85" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A85" s="20">
+        <v>43985</v>
+      </c>
+      <c r="B85" s="21">
+        <v>81333</v>
+      </c>
+      <c r="C85" s="22">
+        <v>828</v>
+      </c>
+      <c r="D85" s="22">
+        <v>1477</v>
+      </c>
+      <c r="E85" s="22">
+        <v>0</v>
+      </c>
+      <c r="F85" s="22">
+        <v>5</v>
+      </c>
+      <c r="G85" s="22">
+        <v>0</v>
+      </c>
+      <c r="H85" s="22">
+        <v>0</v>
+      </c>
+      <c r="I85" s="22">
+        <v>109</v>
+      </c>
+      <c r="J85" s="22">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="86" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A86" s="26">
+        <v>43986</v>
+      </c>
+      <c r="B86" s="27">
+        <v>82161</v>
+      </c>
+      <c r="C86" s="28">
+        <v>828</v>
+      </c>
+      <c r="D86" s="28">
+        <v>1479</v>
+      </c>
+      <c r="E86" s="28">
+        <v>2</v>
+      </c>
+      <c r="F86" s="28">
+        <v>6</v>
+      </c>
+      <c r="G86" s="28">
+        <v>0</v>
+      </c>
+      <c r="H86" s="28">
+        <v>0</v>
+      </c>
+      <c r="I86" s="28">
+        <v>109</v>
+      </c>
+      <c r="J86" s="28">
+        <v>0</v>
+      </c>
+    </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>

</xml_diff>

<commit_message>
Data updated by GitHub Bot (2020-06-05 20)
</commit_message>
<xml_diff>
--- a/output/snapshot/fdcf2531-4c3e-5c02-b63c-ee160ead6dea.xlsx
+++ b/output/snapshot/fdcf2531-4c3e-5c02-b63c-ee160ead6dea.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="I:\AKTUALNI PODATKI - KORONA\Za objavo na GOV.SI\ang\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{1E6DD62F-2BE2-47DC-A7ED-9B57C1589256}" xr6:coauthVersionLast="44" xr6:coauthVersionMax="44" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{E779F27A-C2D0-4365-A806-F279735D4FA6}" xr6:coauthVersionLast="44" xr6:coauthVersionMax="44" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="390" yWindow="390" windowWidth="21600" windowHeight="11205" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Covid-19 podatki" sheetId="1" r:id="rId1"/>
@@ -64,7 +64,7 @@
   <numFmts count="1">
     <numFmt numFmtId="164" formatCode="d/\ m/\ yyyy;@"/>
   </numFmts>
-  <fonts count="4" x14ac:knownFonts="1">
+  <fonts count="5" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -93,6 +93,13 @@
       <name val="Calibri Light"/>
       <scheme val="major"/>
     </font>
+    <font>
+      <sz val="10"/>
+      <color theme="1"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
   </fonts>
   <fills count="3">
     <fill>
@@ -108,7 +115,7 @@
       </patternFill>
     </fill>
   </fills>
-  <borders count="2">
+  <borders count="3">
     <border>
       <left/>
       <right/>
@@ -129,11 +136,26 @@
       <bottom/>
       <diagonal/>
     </border>
+    <border>
+      <left style="thin">
+        <color theme="4"/>
+      </left>
+      <right style="thin">
+        <color theme="4"/>
+      </right>
+      <top style="thin">
+        <color theme="4"/>
+      </top>
+      <bottom style="thin">
+        <color theme="4"/>
+      </bottom>
+      <diagonal/>
+    </border>
   </borders>
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="26">
+  <cellXfs count="29">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="49" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyAlignment="1" applyProtection="1">
       <alignment horizontal="left" vertical="top"/>
@@ -208,6 +230,15 @@
       <alignment horizontal="right"/>
     </xf>
     <xf numFmtId="0" fontId="3" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="right"/>
+    </xf>
+    <xf numFmtId="164" fontId="4" fillId="2" borderId="2" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="right" vertical="top"/>
+    </xf>
+    <xf numFmtId="3" fontId="4" fillId="2" borderId="2" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="right"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="2" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="right"/>
     </xf>
   </cellXfs>
@@ -399,8 +430,8 @@
 </file>
 
 <file path=xl/tables/table1.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="1" xr:uid="{00000000-000C-0000-FFFF-FFFF00000000}" name="Tabela1" displayName="Tabela1" ref="A1:J75" totalsRowShown="0" headerRowDxfId="11" dataDxfId="10">
-  <autoFilter ref="A1:J75" xr:uid="{00000000-0009-0000-0100-000001000000}">
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="1" xr:uid="{00000000-000C-0000-FFFF-FFFF00000000}" name="Tabela1" displayName="Tabela1" ref="A1:J86" totalsRowShown="0" headerRowDxfId="11" dataDxfId="10">
+  <autoFilter ref="A1:J86" xr:uid="{00000000-0009-0000-0100-000001000000}">
     <filterColumn colId="0" hiddenButton="1"/>
     <filterColumn colId="1" hiddenButton="1"/>
     <filterColumn colId="2" hiddenButton="1"/>
@@ -696,10 +727,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:J75"/>
+  <dimension ref="A1:J86"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A40" zoomScale="89" zoomScaleNormal="89" workbookViewId="0">
-      <selection activeCell="J74" sqref="J74"/>
+    <sheetView tabSelected="1" topLeftCell="A65" zoomScale="89" zoomScaleNormal="89" workbookViewId="0">
+      <selection activeCell="A86" sqref="A86:J86"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -3117,6 +3148,358 @@
         <v>0</v>
       </c>
     </row>
+    <row r="76" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A76" s="20">
+        <v>43976</v>
+      </c>
+      <c r="B76" s="21">
+        <v>75770</v>
+      </c>
+      <c r="C76" s="22">
+        <v>754</v>
+      </c>
+      <c r="D76" s="22">
+        <v>1469</v>
+      </c>
+      <c r="E76" s="22">
+        <v>0</v>
+      </c>
+      <c r="F76" s="22">
+        <v>9</v>
+      </c>
+      <c r="G76" s="22">
+        <v>2</v>
+      </c>
+      <c r="H76" s="22">
+        <v>6</v>
+      </c>
+      <c r="I76" s="22">
+        <v>108</v>
+      </c>
+      <c r="J76" s="22">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="77" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A77" s="20">
+        <v>43977</v>
+      </c>
+      <c r="B77" s="21">
+        <v>76579</v>
+      </c>
+      <c r="C77" s="22">
+        <v>809</v>
+      </c>
+      <c r="D77" s="22">
+        <v>1471</v>
+      </c>
+      <c r="E77" s="22">
+        <v>2</v>
+      </c>
+      <c r="F77" s="22">
+        <v>8</v>
+      </c>
+      <c r="G77" s="22">
+        <v>2</v>
+      </c>
+      <c r="H77" s="22">
+        <v>2</v>
+      </c>
+      <c r="I77" s="22">
+        <v>108</v>
+      </c>
+      <c r="J77" s="22">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="78" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A78" s="20">
+        <v>43978</v>
+      </c>
+      <c r="B78" s="21">
+        <v>77210</v>
+      </c>
+      <c r="C78" s="22">
+        <v>631</v>
+      </c>
+      <c r="D78" s="22">
+        <v>1473</v>
+      </c>
+      <c r="E78" s="22">
+        <v>2</v>
+      </c>
+      <c r="F78" s="22">
+        <v>7</v>
+      </c>
+      <c r="G78" s="22">
+        <v>2</v>
+      </c>
+      <c r="H78" s="22">
+        <v>1</v>
+      </c>
+      <c r="I78" s="22">
+        <v>108</v>
+      </c>
+      <c r="J78" s="22">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="79" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A79" s="20">
+        <v>43979</v>
+      </c>
+      <c r="B79" s="21">
+        <v>77916</v>
+      </c>
+      <c r="C79" s="22">
+        <v>706</v>
+      </c>
+      <c r="D79" s="22">
+        <v>1473</v>
+      </c>
+      <c r="E79" s="22">
+        <v>0</v>
+      </c>
+      <c r="F79" s="22">
+        <v>7</v>
+      </c>
+      <c r="G79" s="22">
+        <v>2</v>
+      </c>
+      <c r="H79" s="22">
+        <v>0</v>
+      </c>
+      <c r="I79" s="22">
+        <v>108</v>
+      </c>
+      <c r="J79" s="22">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="80" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A80" s="20">
+        <v>43980</v>
+      </c>
+      <c r="B80" s="21">
+        <v>78529</v>
+      </c>
+      <c r="C80" s="22">
+        <v>613</v>
+      </c>
+      <c r="D80" s="22">
+        <v>1473</v>
+      </c>
+      <c r="E80" s="22">
+        <v>0</v>
+      </c>
+      <c r="F80" s="22">
+        <v>7</v>
+      </c>
+      <c r="G80" s="22">
+        <v>2</v>
+      </c>
+      <c r="H80" s="22">
+        <v>0</v>
+      </c>
+      <c r="I80" s="22">
+        <v>108</v>
+      </c>
+      <c r="J80" s="22">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="81" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A81" s="20">
+        <v>43981</v>
+      </c>
+      <c r="B81" s="22">
+        <v>78793</v>
+      </c>
+      <c r="C81" s="22">
+        <v>264</v>
+      </c>
+      <c r="D81" s="22">
+        <v>1473</v>
+      </c>
+      <c r="E81" s="22">
+        <v>0</v>
+      </c>
+      <c r="F81" s="22">
+        <v>6</v>
+      </c>
+      <c r="G81" s="22">
+        <v>2</v>
+      </c>
+      <c r="H81" s="22">
+        <v>1</v>
+      </c>
+      <c r="I81" s="22">
+        <v>108</v>
+      </c>
+      <c r="J81" s="22">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="82" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A82" s="20">
+        <v>43982</v>
+      </c>
+      <c r="B82" s="21">
+        <v>79039</v>
+      </c>
+      <c r="C82" s="22">
+        <v>246</v>
+      </c>
+      <c r="D82" s="22">
+        <v>1473</v>
+      </c>
+      <c r="E82" s="22">
+        <v>0</v>
+      </c>
+      <c r="F82" s="22">
+        <v>5</v>
+      </c>
+      <c r="G82" s="22">
+        <v>1</v>
+      </c>
+      <c r="H82" s="22">
+        <v>0</v>
+      </c>
+      <c r="I82" s="22">
+        <v>109</v>
+      </c>
+      <c r="J82" s="22">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="83" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A83" s="20">
+        <v>43983</v>
+      </c>
+      <c r="B83" s="21">
+        <v>79698</v>
+      </c>
+      <c r="C83" s="22">
+        <v>659</v>
+      </c>
+      <c r="D83" s="22">
+        <v>1475</v>
+      </c>
+      <c r="E83" s="22">
+        <v>2</v>
+      </c>
+      <c r="F83" s="22">
+        <v>5</v>
+      </c>
+      <c r="G83" s="22">
+        <v>1</v>
+      </c>
+      <c r="H83" s="22">
+        <v>0</v>
+      </c>
+      <c r="I83" s="22">
+        <v>109</v>
+      </c>
+      <c r="J83" s="22">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="84" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A84" s="20">
+        <v>43984</v>
+      </c>
+      <c r="B84" s="21">
+        <v>80505</v>
+      </c>
+      <c r="C84" s="22">
+        <v>807</v>
+      </c>
+      <c r="D84" s="22">
+        <v>1477</v>
+      </c>
+      <c r="E84" s="22">
+        <v>2</v>
+      </c>
+      <c r="F84" s="22">
+        <v>5</v>
+      </c>
+      <c r="G84" s="22">
+        <v>0</v>
+      </c>
+      <c r="H84" s="22">
+        <v>0</v>
+      </c>
+      <c r="I84" s="22">
+        <v>109</v>
+      </c>
+      <c r="J84" s="22">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="85" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A85" s="20">
+        <v>43985</v>
+      </c>
+      <c r="B85" s="21">
+        <v>81333</v>
+      </c>
+      <c r="C85" s="22">
+        <v>828</v>
+      </c>
+      <c r="D85" s="22">
+        <v>1477</v>
+      </c>
+      <c r="E85" s="22">
+        <v>0</v>
+      </c>
+      <c r="F85" s="22">
+        <v>5</v>
+      </c>
+      <c r="G85" s="22">
+        <v>0</v>
+      </c>
+      <c r="H85" s="22">
+        <v>0</v>
+      </c>
+      <c r="I85" s="22">
+        <v>109</v>
+      </c>
+      <c r="J85" s="22">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="86" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A86" s="26">
+        <v>43986</v>
+      </c>
+      <c r="B86" s="27">
+        <v>82161</v>
+      </c>
+      <c r="C86" s="28">
+        <v>828</v>
+      </c>
+      <c r="D86" s="28">
+        <v>1479</v>
+      </c>
+      <c r="E86" s="28">
+        <v>2</v>
+      </c>
+      <c r="F86" s="28">
+        <v>6</v>
+      </c>
+      <c r="G86" s="28">
+        <v>0</v>
+      </c>
+      <c r="H86" s="28">
+        <v>0</v>
+      </c>
+      <c r="I86" s="28">
+        <v>109</v>
+      </c>
+      <c r="J86" s="28">
+        <v>0</v>
+      </c>
+    </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>

</xml_diff>

<commit_message>
Data updated by GitHub Bot (2020-06-06 12)
</commit_message>
<xml_diff>
--- a/output/snapshot/fdcf2531-4c3e-5c02-b63c-ee160ead6dea.xlsx
+++ b/output/snapshot/fdcf2531-4c3e-5c02-b63c-ee160ead6dea.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="I:\AKTUALNI PODATKI - KORONA\Za objavo na GOV.SI\ang\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{1E6DD62F-2BE2-47DC-A7ED-9B57C1589256}" xr6:coauthVersionLast="44" xr6:coauthVersionMax="44" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{7E8D50CD-A162-478B-944F-5BBE4BF6D68F}" xr6:coauthVersionLast="44" xr6:coauthVersionMax="44" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="4200" yWindow="4200" windowWidth="21600" windowHeight="11205" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Covid-19 podatki" sheetId="1" r:id="rId1"/>
@@ -64,7 +64,7 @@
   <numFmts count="1">
     <numFmt numFmtId="164" formatCode="d/\ m/\ yyyy;@"/>
   </numFmts>
-  <fonts count="4" x14ac:knownFonts="1">
+  <fonts count="5" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -93,6 +93,13 @@
       <name val="Calibri Light"/>
       <scheme val="major"/>
     </font>
+    <font>
+      <sz val="10"/>
+      <color theme="1"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
   </fonts>
   <fills count="3">
     <fill>
@@ -108,7 +115,7 @@
       </patternFill>
     </fill>
   </fills>
-  <borders count="2">
+  <borders count="3">
     <border>
       <left/>
       <right/>
@@ -129,11 +136,26 @@
       <bottom/>
       <diagonal/>
     </border>
+    <border>
+      <left style="thin">
+        <color theme="4"/>
+      </left>
+      <right style="thin">
+        <color theme="4"/>
+      </right>
+      <top style="thin">
+        <color theme="4"/>
+      </top>
+      <bottom style="thin">
+        <color theme="4"/>
+      </bottom>
+      <diagonal/>
+    </border>
   </borders>
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="26">
+  <cellXfs count="32">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="49" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyAlignment="1" applyProtection="1">
       <alignment horizontal="left" vertical="top"/>
@@ -208,6 +230,24 @@
       <alignment horizontal="right"/>
     </xf>
     <xf numFmtId="0" fontId="3" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="right"/>
+    </xf>
+    <xf numFmtId="164" fontId="4" fillId="2" borderId="2" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="right" vertical="top"/>
+    </xf>
+    <xf numFmtId="3" fontId="4" fillId="2" borderId="2" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="right"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="2" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="right"/>
+    </xf>
+    <xf numFmtId="164" fontId="3" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="right" vertical="top"/>
+    </xf>
+    <xf numFmtId="3" fontId="3" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="right"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="right"/>
     </xf>
   </cellXfs>
@@ -399,8 +439,8 @@
 </file>
 
 <file path=xl/tables/table1.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="1" xr:uid="{00000000-000C-0000-FFFF-FFFF00000000}" name="Tabela1" displayName="Tabela1" ref="A1:J75" totalsRowShown="0" headerRowDxfId="11" dataDxfId="10">
-  <autoFilter ref="A1:J75" xr:uid="{00000000-0009-0000-0100-000001000000}">
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="1" xr:uid="{00000000-000C-0000-FFFF-FFFF00000000}" name="Tabela1" displayName="Tabela1" ref="A1:J87" totalsRowShown="0" headerRowDxfId="11" dataDxfId="10">
+  <autoFilter ref="A1:J87" xr:uid="{00000000-0009-0000-0100-000001000000}">
     <filterColumn colId="0" hiddenButton="1"/>
     <filterColumn colId="1" hiddenButton="1"/>
     <filterColumn colId="2" hiddenButton="1"/>
@@ -696,10 +736,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:J75"/>
+  <dimension ref="A1:J87"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A40" zoomScale="89" zoomScaleNormal="89" workbookViewId="0">
-      <selection activeCell="J74" sqref="J74"/>
+    <sheetView tabSelected="1" topLeftCell="A65" zoomScale="89" zoomScaleNormal="89" workbookViewId="0">
+      <selection activeCell="A87" sqref="A87:J87"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -3117,6 +3157,390 @@
         <v>0</v>
       </c>
     </row>
+    <row r="76" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A76" s="20">
+        <v>43976</v>
+      </c>
+      <c r="B76" s="21">
+        <v>75770</v>
+      </c>
+      <c r="C76" s="22">
+        <v>754</v>
+      </c>
+      <c r="D76" s="22">
+        <v>1469</v>
+      </c>
+      <c r="E76" s="22">
+        <v>0</v>
+      </c>
+      <c r="F76" s="22">
+        <v>9</v>
+      </c>
+      <c r="G76" s="22">
+        <v>2</v>
+      </c>
+      <c r="H76" s="22">
+        <v>6</v>
+      </c>
+      <c r="I76" s="22">
+        <v>108</v>
+      </c>
+      <c r="J76" s="22">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="77" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A77" s="20">
+        <v>43977</v>
+      </c>
+      <c r="B77" s="21">
+        <v>76579</v>
+      </c>
+      <c r="C77" s="22">
+        <v>809</v>
+      </c>
+      <c r="D77" s="22">
+        <v>1471</v>
+      </c>
+      <c r="E77" s="22">
+        <v>2</v>
+      </c>
+      <c r="F77" s="22">
+        <v>8</v>
+      </c>
+      <c r="G77" s="22">
+        <v>2</v>
+      </c>
+      <c r="H77" s="22">
+        <v>2</v>
+      </c>
+      <c r="I77" s="22">
+        <v>108</v>
+      </c>
+      <c r="J77" s="22">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="78" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A78" s="20">
+        <v>43978</v>
+      </c>
+      <c r="B78" s="21">
+        <v>77210</v>
+      </c>
+      <c r="C78" s="22">
+        <v>631</v>
+      </c>
+      <c r="D78" s="22">
+        <v>1473</v>
+      </c>
+      <c r="E78" s="22">
+        <v>2</v>
+      </c>
+      <c r="F78" s="22">
+        <v>7</v>
+      </c>
+      <c r="G78" s="22">
+        <v>2</v>
+      </c>
+      <c r="H78" s="22">
+        <v>1</v>
+      </c>
+      <c r="I78" s="22">
+        <v>108</v>
+      </c>
+      <c r="J78" s="22">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="79" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A79" s="20">
+        <v>43979</v>
+      </c>
+      <c r="B79" s="21">
+        <v>77916</v>
+      </c>
+      <c r="C79" s="22">
+        <v>706</v>
+      </c>
+      <c r="D79" s="22">
+        <v>1473</v>
+      </c>
+      <c r="E79" s="22">
+        <v>0</v>
+      </c>
+      <c r="F79" s="22">
+        <v>7</v>
+      </c>
+      <c r="G79" s="22">
+        <v>2</v>
+      </c>
+      <c r="H79" s="22">
+        <v>0</v>
+      </c>
+      <c r="I79" s="22">
+        <v>108</v>
+      </c>
+      <c r="J79" s="22">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="80" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A80" s="20">
+        <v>43980</v>
+      </c>
+      <c r="B80" s="21">
+        <v>78529</v>
+      </c>
+      <c r="C80" s="22">
+        <v>613</v>
+      </c>
+      <c r="D80" s="22">
+        <v>1473</v>
+      </c>
+      <c r="E80" s="22">
+        <v>0</v>
+      </c>
+      <c r="F80" s="22">
+        <v>7</v>
+      </c>
+      <c r="G80" s="22">
+        <v>2</v>
+      </c>
+      <c r="H80" s="22">
+        <v>0</v>
+      </c>
+      <c r="I80" s="22">
+        <v>108</v>
+      </c>
+      <c r="J80" s="22">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="81" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A81" s="20">
+        <v>43981</v>
+      </c>
+      <c r="B81" s="22">
+        <v>78793</v>
+      </c>
+      <c r="C81" s="22">
+        <v>264</v>
+      </c>
+      <c r="D81" s="22">
+        <v>1473</v>
+      </c>
+      <c r="E81" s="22">
+        <v>0</v>
+      </c>
+      <c r="F81" s="22">
+        <v>6</v>
+      </c>
+      <c r="G81" s="22">
+        <v>2</v>
+      </c>
+      <c r="H81" s="22">
+        <v>1</v>
+      </c>
+      <c r="I81" s="22">
+        <v>108</v>
+      </c>
+      <c r="J81" s="22">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="82" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A82" s="20">
+        <v>43982</v>
+      </c>
+      <c r="B82" s="21">
+        <v>79039</v>
+      </c>
+      <c r="C82" s="22">
+        <v>246</v>
+      </c>
+      <c r="D82" s="22">
+        <v>1473</v>
+      </c>
+      <c r="E82" s="22">
+        <v>0</v>
+      </c>
+      <c r="F82" s="22">
+        <v>5</v>
+      </c>
+      <c r="G82" s="22">
+        <v>1</v>
+      </c>
+      <c r="H82" s="22">
+        <v>0</v>
+      </c>
+      <c r="I82" s="22">
+        <v>109</v>
+      </c>
+      <c r="J82" s="22">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="83" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A83" s="20">
+        <v>43983</v>
+      </c>
+      <c r="B83" s="21">
+        <v>79698</v>
+      </c>
+      <c r="C83" s="22">
+        <v>659</v>
+      </c>
+      <c r="D83" s="22">
+        <v>1475</v>
+      </c>
+      <c r="E83" s="22">
+        <v>2</v>
+      </c>
+      <c r="F83" s="22">
+        <v>5</v>
+      </c>
+      <c r="G83" s="22">
+        <v>1</v>
+      </c>
+      <c r="H83" s="22">
+        <v>0</v>
+      </c>
+      <c r="I83" s="22">
+        <v>109</v>
+      </c>
+      <c r="J83" s="22">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="84" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A84" s="20">
+        <v>43984</v>
+      </c>
+      <c r="B84" s="21">
+        <v>80505</v>
+      </c>
+      <c r="C84" s="22">
+        <v>807</v>
+      </c>
+      <c r="D84" s="22">
+        <v>1477</v>
+      </c>
+      <c r="E84" s="22">
+        <v>2</v>
+      </c>
+      <c r="F84" s="22">
+        <v>5</v>
+      </c>
+      <c r="G84" s="22">
+        <v>0</v>
+      </c>
+      <c r="H84" s="22">
+        <v>0</v>
+      </c>
+      <c r="I84" s="22">
+        <v>109</v>
+      </c>
+      <c r="J84" s="22">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="85" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A85" s="20">
+        <v>43985</v>
+      </c>
+      <c r="B85" s="21">
+        <v>81333</v>
+      </c>
+      <c r="C85" s="22">
+        <v>828</v>
+      </c>
+      <c r="D85" s="22">
+        <v>1477</v>
+      </c>
+      <c r="E85" s="22">
+        <v>0</v>
+      </c>
+      <c r="F85" s="22">
+        <v>5</v>
+      </c>
+      <c r="G85" s="22">
+        <v>0</v>
+      </c>
+      <c r="H85" s="22">
+        <v>0</v>
+      </c>
+      <c r="I85" s="22">
+        <v>109</v>
+      </c>
+      <c r="J85" s="22">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="86" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A86" s="26">
+        <v>43986</v>
+      </c>
+      <c r="B86" s="27">
+        <v>82161</v>
+      </c>
+      <c r="C86" s="28">
+        <v>828</v>
+      </c>
+      <c r="D86" s="28">
+        <v>1479</v>
+      </c>
+      <c r="E86" s="28">
+        <v>2</v>
+      </c>
+      <c r="F86" s="28">
+        <v>6</v>
+      </c>
+      <c r="G86" s="28">
+        <v>0</v>
+      </c>
+      <c r="H86" s="28">
+        <v>0</v>
+      </c>
+      <c r="I86" s="28">
+        <v>109</v>
+      </c>
+      <c r="J86" s="28">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="87" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A87" s="29">
+        <v>43987</v>
+      </c>
+      <c r="B87" s="30">
+        <v>82876</v>
+      </c>
+      <c r="C87" s="31">
+        <v>715</v>
+      </c>
+      <c r="D87" s="31">
+        <v>1484</v>
+      </c>
+      <c r="E87" s="31">
+        <v>5</v>
+      </c>
+      <c r="F87" s="31">
+        <v>6</v>
+      </c>
+      <c r="G87" s="31">
+        <v>0</v>
+      </c>
+      <c r="H87" s="31">
+        <v>0</v>
+      </c>
+      <c r="I87" s="31">
+        <v>109</v>
+      </c>
+      <c r="J87" s="31">
+        <v>0</v>
+      </c>
+    </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>

</xml_diff>

<commit_message>
Data updated by GitHub Bot (2020-06-06 20)
</commit_message>
<xml_diff>
--- a/output/snapshot/fdcf2531-4c3e-5c02-b63c-ee160ead6dea.xlsx
+++ b/output/snapshot/fdcf2531-4c3e-5c02-b63c-ee160ead6dea.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="I:\AKTUALNI PODATKI - KORONA\Za objavo na GOV.SI\ang\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{1E6DD62F-2BE2-47DC-A7ED-9B57C1589256}" xr6:coauthVersionLast="44" xr6:coauthVersionMax="44" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{7E8D50CD-A162-478B-944F-5BBE4BF6D68F}" xr6:coauthVersionLast="44" xr6:coauthVersionMax="44" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="4200" yWindow="4200" windowWidth="21600" windowHeight="11205" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Covid-19 podatki" sheetId="1" r:id="rId1"/>
@@ -64,7 +64,7 @@
   <numFmts count="1">
     <numFmt numFmtId="164" formatCode="d/\ m/\ yyyy;@"/>
   </numFmts>
-  <fonts count="4" x14ac:knownFonts="1">
+  <fonts count="5" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -93,6 +93,13 @@
       <name val="Calibri Light"/>
       <scheme val="major"/>
     </font>
+    <font>
+      <sz val="10"/>
+      <color theme="1"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
   </fonts>
   <fills count="3">
     <fill>
@@ -108,7 +115,7 @@
       </patternFill>
     </fill>
   </fills>
-  <borders count="2">
+  <borders count="3">
     <border>
       <left/>
       <right/>
@@ -129,11 +136,26 @@
       <bottom/>
       <diagonal/>
     </border>
+    <border>
+      <left style="thin">
+        <color theme="4"/>
+      </left>
+      <right style="thin">
+        <color theme="4"/>
+      </right>
+      <top style="thin">
+        <color theme="4"/>
+      </top>
+      <bottom style="thin">
+        <color theme="4"/>
+      </bottom>
+      <diagonal/>
+    </border>
   </borders>
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="26">
+  <cellXfs count="32">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="49" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyAlignment="1" applyProtection="1">
       <alignment horizontal="left" vertical="top"/>
@@ -208,6 +230,24 @@
       <alignment horizontal="right"/>
     </xf>
     <xf numFmtId="0" fontId="3" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="right"/>
+    </xf>
+    <xf numFmtId="164" fontId="4" fillId="2" borderId="2" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="right" vertical="top"/>
+    </xf>
+    <xf numFmtId="3" fontId="4" fillId="2" borderId="2" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="right"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="2" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="right"/>
+    </xf>
+    <xf numFmtId="164" fontId="3" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="right" vertical="top"/>
+    </xf>
+    <xf numFmtId="3" fontId="3" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="right"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="right"/>
     </xf>
   </cellXfs>
@@ -399,8 +439,8 @@
 </file>
 
 <file path=xl/tables/table1.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="1" xr:uid="{00000000-000C-0000-FFFF-FFFF00000000}" name="Tabela1" displayName="Tabela1" ref="A1:J75" totalsRowShown="0" headerRowDxfId="11" dataDxfId="10">
-  <autoFilter ref="A1:J75" xr:uid="{00000000-0009-0000-0100-000001000000}">
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="1" xr:uid="{00000000-000C-0000-FFFF-FFFF00000000}" name="Tabela1" displayName="Tabela1" ref="A1:J87" totalsRowShown="0" headerRowDxfId="11" dataDxfId="10">
+  <autoFilter ref="A1:J87" xr:uid="{00000000-0009-0000-0100-000001000000}">
     <filterColumn colId="0" hiddenButton="1"/>
     <filterColumn colId="1" hiddenButton="1"/>
     <filterColumn colId="2" hiddenButton="1"/>
@@ -696,10 +736,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:J75"/>
+  <dimension ref="A1:J87"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A40" zoomScale="89" zoomScaleNormal="89" workbookViewId="0">
-      <selection activeCell="J74" sqref="J74"/>
+    <sheetView tabSelected="1" topLeftCell="A65" zoomScale="89" zoomScaleNormal="89" workbookViewId="0">
+      <selection activeCell="A87" sqref="A87:J87"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -3117,6 +3157,390 @@
         <v>0</v>
       </c>
     </row>
+    <row r="76" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A76" s="20">
+        <v>43976</v>
+      </c>
+      <c r="B76" s="21">
+        <v>75770</v>
+      </c>
+      <c r="C76" s="22">
+        <v>754</v>
+      </c>
+      <c r="D76" s="22">
+        <v>1469</v>
+      </c>
+      <c r="E76" s="22">
+        <v>0</v>
+      </c>
+      <c r="F76" s="22">
+        <v>9</v>
+      </c>
+      <c r="G76" s="22">
+        <v>2</v>
+      </c>
+      <c r="H76" s="22">
+        <v>6</v>
+      </c>
+      <c r="I76" s="22">
+        <v>108</v>
+      </c>
+      <c r="J76" s="22">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="77" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A77" s="20">
+        <v>43977</v>
+      </c>
+      <c r="B77" s="21">
+        <v>76579</v>
+      </c>
+      <c r="C77" s="22">
+        <v>809</v>
+      </c>
+      <c r="D77" s="22">
+        <v>1471</v>
+      </c>
+      <c r="E77" s="22">
+        <v>2</v>
+      </c>
+      <c r="F77" s="22">
+        <v>8</v>
+      </c>
+      <c r="G77" s="22">
+        <v>2</v>
+      </c>
+      <c r="H77" s="22">
+        <v>2</v>
+      </c>
+      <c r="I77" s="22">
+        <v>108</v>
+      </c>
+      <c r="J77" s="22">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="78" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A78" s="20">
+        <v>43978</v>
+      </c>
+      <c r="B78" s="21">
+        <v>77210</v>
+      </c>
+      <c r="C78" s="22">
+        <v>631</v>
+      </c>
+      <c r="D78" s="22">
+        <v>1473</v>
+      </c>
+      <c r="E78" s="22">
+        <v>2</v>
+      </c>
+      <c r="F78" s="22">
+        <v>7</v>
+      </c>
+      <c r="G78" s="22">
+        <v>2</v>
+      </c>
+      <c r="H78" s="22">
+        <v>1</v>
+      </c>
+      <c r="I78" s="22">
+        <v>108</v>
+      </c>
+      <c r="J78" s="22">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="79" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A79" s="20">
+        <v>43979</v>
+      </c>
+      <c r="B79" s="21">
+        <v>77916</v>
+      </c>
+      <c r="C79" s="22">
+        <v>706</v>
+      </c>
+      <c r="D79" s="22">
+        <v>1473</v>
+      </c>
+      <c r="E79" s="22">
+        <v>0</v>
+      </c>
+      <c r="F79" s="22">
+        <v>7</v>
+      </c>
+      <c r="G79" s="22">
+        <v>2</v>
+      </c>
+      <c r="H79" s="22">
+        <v>0</v>
+      </c>
+      <c r="I79" s="22">
+        <v>108</v>
+      </c>
+      <c r="J79" s="22">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="80" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A80" s="20">
+        <v>43980</v>
+      </c>
+      <c r="B80" s="21">
+        <v>78529</v>
+      </c>
+      <c r="C80" s="22">
+        <v>613</v>
+      </c>
+      <c r="D80" s="22">
+        <v>1473</v>
+      </c>
+      <c r="E80" s="22">
+        <v>0</v>
+      </c>
+      <c r="F80" s="22">
+        <v>7</v>
+      </c>
+      <c r="G80" s="22">
+        <v>2</v>
+      </c>
+      <c r="H80" s="22">
+        <v>0</v>
+      </c>
+      <c r="I80" s="22">
+        <v>108</v>
+      </c>
+      <c r="J80" s="22">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="81" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A81" s="20">
+        <v>43981</v>
+      </c>
+      <c r="B81" s="22">
+        <v>78793</v>
+      </c>
+      <c r="C81" s="22">
+        <v>264</v>
+      </c>
+      <c r="D81" s="22">
+        <v>1473</v>
+      </c>
+      <c r="E81" s="22">
+        <v>0</v>
+      </c>
+      <c r="F81" s="22">
+        <v>6</v>
+      </c>
+      <c r="G81" s="22">
+        <v>2</v>
+      </c>
+      <c r="H81" s="22">
+        <v>1</v>
+      </c>
+      <c r="I81" s="22">
+        <v>108</v>
+      </c>
+      <c r="J81" s="22">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="82" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A82" s="20">
+        <v>43982</v>
+      </c>
+      <c r="B82" s="21">
+        <v>79039</v>
+      </c>
+      <c r="C82" s="22">
+        <v>246</v>
+      </c>
+      <c r="D82" s="22">
+        <v>1473</v>
+      </c>
+      <c r="E82" s="22">
+        <v>0</v>
+      </c>
+      <c r="F82" s="22">
+        <v>5</v>
+      </c>
+      <c r="G82" s="22">
+        <v>1</v>
+      </c>
+      <c r="H82" s="22">
+        <v>0</v>
+      </c>
+      <c r="I82" s="22">
+        <v>109</v>
+      </c>
+      <c r="J82" s="22">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="83" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A83" s="20">
+        <v>43983</v>
+      </c>
+      <c r="B83" s="21">
+        <v>79698</v>
+      </c>
+      <c r="C83" s="22">
+        <v>659</v>
+      </c>
+      <c r="D83" s="22">
+        <v>1475</v>
+      </c>
+      <c r="E83" s="22">
+        <v>2</v>
+      </c>
+      <c r="F83" s="22">
+        <v>5</v>
+      </c>
+      <c r="G83" s="22">
+        <v>1</v>
+      </c>
+      <c r="H83" s="22">
+        <v>0</v>
+      </c>
+      <c r="I83" s="22">
+        <v>109</v>
+      </c>
+      <c r="J83" s="22">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="84" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A84" s="20">
+        <v>43984</v>
+      </c>
+      <c r="B84" s="21">
+        <v>80505</v>
+      </c>
+      <c r="C84" s="22">
+        <v>807</v>
+      </c>
+      <c r="D84" s="22">
+        <v>1477</v>
+      </c>
+      <c r="E84" s="22">
+        <v>2</v>
+      </c>
+      <c r="F84" s="22">
+        <v>5</v>
+      </c>
+      <c r="G84" s="22">
+        <v>0</v>
+      </c>
+      <c r="H84" s="22">
+        <v>0</v>
+      </c>
+      <c r="I84" s="22">
+        <v>109</v>
+      </c>
+      <c r="J84" s="22">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="85" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A85" s="20">
+        <v>43985</v>
+      </c>
+      <c r="B85" s="21">
+        <v>81333</v>
+      </c>
+      <c r="C85" s="22">
+        <v>828</v>
+      </c>
+      <c r="D85" s="22">
+        <v>1477</v>
+      </c>
+      <c r="E85" s="22">
+        <v>0</v>
+      </c>
+      <c r="F85" s="22">
+        <v>5</v>
+      </c>
+      <c r="G85" s="22">
+        <v>0</v>
+      </c>
+      <c r="H85" s="22">
+        <v>0</v>
+      </c>
+      <c r="I85" s="22">
+        <v>109</v>
+      </c>
+      <c r="J85" s="22">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="86" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A86" s="26">
+        <v>43986</v>
+      </c>
+      <c r="B86" s="27">
+        <v>82161</v>
+      </c>
+      <c r="C86" s="28">
+        <v>828</v>
+      </c>
+      <c r="D86" s="28">
+        <v>1479</v>
+      </c>
+      <c r="E86" s="28">
+        <v>2</v>
+      </c>
+      <c r="F86" s="28">
+        <v>6</v>
+      </c>
+      <c r="G86" s="28">
+        <v>0</v>
+      </c>
+      <c r="H86" s="28">
+        <v>0</v>
+      </c>
+      <c r="I86" s="28">
+        <v>109</v>
+      </c>
+      <c r="J86" s="28">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="87" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A87" s="29">
+        <v>43987</v>
+      </c>
+      <c r="B87" s="30">
+        <v>82876</v>
+      </c>
+      <c r="C87" s="31">
+        <v>715</v>
+      </c>
+      <c r="D87" s="31">
+        <v>1484</v>
+      </c>
+      <c r="E87" s="31">
+        <v>5</v>
+      </c>
+      <c r="F87" s="31">
+        <v>6</v>
+      </c>
+      <c r="G87" s="31">
+        <v>0</v>
+      </c>
+      <c r="H87" s="31">
+        <v>0</v>
+      </c>
+      <c r="I87" s="31">
+        <v>109</v>
+      </c>
+      <c r="J87" s="31">
+        <v>0</v>
+      </c>
+    </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>

</xml_diff>

<commit_message>
Data updated by GitHub Bot (2020-06-07 12)
</commit_message>
<xml_diff>
--- a/output/snapshot/fdcf2531-4c3e-5c02-b63c-ee160ead6dea.xlsx
+++ b/output/snapshot/fdcf2531-4c3e-5c02-b63c-ee160ead6dea.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="I:\AKTUALNI PODATKI - KORONA\Za objavo na GOV.SI\ang\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{1E6DD62F-2BE2-47DC-A7ED-9B57C1589256}" xr6:coauthVersionLast="44" xr6:coauthVersionMax="44" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{7E8D50CD-A162-478B-944F-5BBE4BF6D68F}" xr6:coauthVersionLast="44" xr6:coauthVersionMax="44" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="4200" yWindow="4200" windowWidth="21600" windowHeight="11205" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Covid-19 podatki" sheetId="1" r:id="rId1"/>
@@ -64,7 +64,7 @@
   <numFmts count="1">
     <numFmt numFmtId="164" formatCode="d/\ m/\ yyyy;@"/>
   </numFmts>
-  <fonts count="4" x14ac:knownFonts="1">
+  <fonts count="5" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -93,6 +93,13 @@
       <name val="Calibri Light"/>
       <scheme val="major"/>
     </font>
+    <font>
+      <sz val="10"/>
+      <color theme="1"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
   </fonts>
   <fills count="3">
     <fill>
@@ -108,7 +115,7 @@
       </patternFill>
     </fill>
   </fills>
-  <borders count="2">
+  <borders count="3">
     <border>
       <left/>
       <right/>
@@ -129,11 +136,26 @@
       <bottom/>
       <diagonal/>
     </border>
+    <border>
+      <left style="thin">
+        <color theme="4"/>
+      </left>
+      <right style="thin">
+        <color theme="4"/>
+      </right>
+      <top style="thin">
+        <color theme="4"/>
+      </top>
+      <bottom style="thin">
+        <color theme="4"/>
+      </bottom>
+      <diagonal/>
+    </border>
   </borders>
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="26">
+  <cellXfs count="32">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="49" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyAlignment="1" applyProtection="1">
       <alignment horizontal="left" vertical="top"/>
@@ -208,6 +230,24 @@
       <alignment horizontal="right"/>
     </xf>
     <xf numFmtId="0" fontId="3" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="right"/>
+    </xf>
+    <xf numFmtId="164" fontId="4" fillId="2" borderId="2" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="right" vertical="top"/>
+    </xf>
+    <xf numFmtId="3" fontId="4" fillId="2" borderId="2" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="right"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="2" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="right"/>
+    </xf>
+    <xf numFmtId="164" fontId="3" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="right" vertical="top"/>
+    </xf>
+    <xf numFmtId="3" fontId="3" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="right"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="right"/>
     </xf>
   </cellXfs>
@@ -399,8 +439,8 @@
 </file>
 
 <file path=xl/tables/table1.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="1" xr:uid="{00000000-000C-0000-FFFF-FFFF00000000}" name="Tabela1" displayName="Tabela1" ref="A1:J75" totalsRowShown="0" headerRowDxfId="11" dataDxfId="10">
-  <autoFilter ref="A1:J75" xr:uid="{00000000-0009-0000-0100-000001000000}">
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="1" xr:uid="{00000000-000C-0000-FFFF-FFFF00000000}" name="Tabela1" displayName="Tabela1" ref="A1:J87" totalsRowShown="0" headerRowDxfId="11" dataDxfId="10">
+  <autoFilter ref="A1:J87" xr:uid="{00000000-0009-0000-0100-000001000000}">
     <filterColumn colId="0" hiddenButton="1"/>
     <filterColumn colId="1" hiddenButton="1"/>
     <filterColumn colId="2" hiddenButton="1"/>
@@ -696,10 +736,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:J75"/>
+  <dimension ref="A1:J87"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A40" zoomScale="89" zoomScaleNormal="89" workbookViewId="0">
-      <selection activeCell="J74" sqref="J74"/>
+    <sheetView tabSelected="1" topLeftCell="A65" zoomScale="89" zoomScaleNormal="89" workbookViewId="0">
+      <selection activeCell="A87" sqref="A87:J87"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -3117,6 +3157,390 @@
         <v>0</v>
       </c>
     </row>
+    <row r="76" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A76" s="20">
+        <v>43976</v>
+      </c>
+      <c r="B76" s="21">
+        <v>75770</v>
+      </c>
+      <c r="C76" s="22">
+        <v>754</v>
+      </c>
+      <c r="D76" s="22">
+        <v>1469</v>
+      </c>
+      <c r="E76" s="22">
+        <v>0</v>
+      </c>
+      <c r="F76" s="22">
+        <v>9</v>
+      </c>
+      <c r="G76" s="22">
+        <v>2</v>
+      </c>
+      <c r="H76" s="22">
+        <v>6</v>
+      </c>
+      <c r="I76" s="22">
+        <v>108</v>
+      </c>
+      <c r="J76" s="22">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="77" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A77" s="20">
+        <v>43977</v>
+      </c>
+      <c r="B77" s="21">
+        <v>76579</v>
+      </c>
+      <c r="C77" s="22">
+        <v>809</v>
+      </c>
+      <c r="D77" s="22">
+        <v>1471</v>
+      </c>
+      <c r="E77" s="22">
+        <v>2</v>
+      </c>
+      <c r="F77" s="22">
+        <v>8</v>
+      </c>
+      <c r="G77" s="22">
+        <v>2</v>
+      </c>
+      <c r="H77" s="22">
+        <v>2</v>
+      </c>
+      <c r="I77" s="22">
+        <v>108</v>
+      </c>
+      <c r="J77" s="22">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="78" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A78" s="20">
+        <v>43978</v>
+      </c>
+      <c r="B78" s="21">
+        <v>77210</v>
+      </c>
+      <c r="C78" s="22">
+        <v>631</v>
+      </c>
+      <c r="D78" s="22">
+        <v>1473</v>
+      </c>
+      <c r="E78" s="22">
+        <v>2</v>
+      </c>
+      <c r="F78" s="22">
+        <v>7</v>
+      </c>
+      <c r="G78" s="22">
+        <v>2</v>
+      </c>
+      <c r="H78" s="22">
+        <v>1</v>
+      </c>
+      <c r="I78" s="22">
+        <v>108</v>
+      </c>
+      <c r="J78" s="22">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="79" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A79" s="20">
+        <v>43979</v>
+      </c>
+      <c r="B79" s="21">
+        <v>77916</v>
+      </c>
+      <c r="C79" s="22">
+        <v>706</v>
+      </c>
+      <c r="D79" s="22">
+        <v>1473</v>
+      </c>
+      <c r="E79" s="22">
+        <v>0</v>
+      </c>
+      <c r="F79" s="22">
+        <v>7</v>
+      </c>
+      <c r="G79" s="22">
+        <v>2</v>
+      </c>
+      <c r="H79" s="22">
+        <v>0</v>
+      </c>
+      <c r="I79" s="22">
+        <v>108</v>
+      </c>
+      <c r="J79" s="22">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="80" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A80" s="20">
+        <v>43980</v>
+      </c>
+      <c r="B80" s="21">
+        <v>78529</v>
+      </c>
+      <c r="C80" s="22">
+        <v>613</v>
+      </c>
+      <c r="D80" s="22">
+        <v>1473</v>
+      </c>
+      <c r="E80" s="22">
+        <v>0</v>
+      </c>
+      <c r="F80" s="22">
+        <v>7</v>
+      </c>
+      <c r="G80" s="22">
+        <v>2</v>
+      </c>
+      <c r="H80" s="22">
+        <v>0</v>
+      </c>
+      <c r="I80" s="22">
+        <v>108</v>
+      </c>
+      <c r="J80" s="22">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="81" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A81" s="20">
+        <v>43981</v>
+      </c>
+      <c r="B81" s="22">
+        <v>78793</v>
+      </c>
+      <c r="C81" s="22">
+        <v>264</v>
+      </c>
+      <c r="D81" s="22">
+        <v>1473</v>
+      </c>
+      <c r="E81" s="22">
+        <v>0</v>
+      </c>
+      <c r="F81" s="22">
+        <v>6</v>
+      </c>
+      <c r="G81" s="22">
+        <v>2</v>
+      </c>
+      <c r="H81" s="22">
+        <v>1</v>
+      </c>
+      <c r="I81" s="22">
+        <v>108</v>
+      </c>
+      <c r="J81" s="22">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="82" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A82" s="20">
+        <v>43982</v>
+      </c>
+      <c r="B82" s="21">
+        <v>79039</v>
+      </c>
+      <c r="C82" s="22">
+        <v>246</v>
+      </c>
+      <c r="D82" s="22">
+        <v>1473</v>
+      </c>
+      <c r="E82" s="22">
+        <v>0</v>
+      </c>
+      <c r="F82" s="22">
+        <v>5</v>
+      </c>
+      <c r="G82" s="22">
+        <v>1</v>
+      </c>
+      <c r="H82" s="22">
+        <v>0</v>
+      </c>
+      <c r="I82" s="22">
+        <v>109</v>
+      </c>
+      <c r="J82" s="22">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="83" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A83" s="20">
+        <v>43983</v>
+      </c>
+      <c r="B83" s="21">
+        <v>79698</v>
+      </c>
+      <c r="C83" s="22">
+        <v>659</v>
+      </c>
+      <c r="D83" s="22">
+        <v>1475</v>
+      </c>
+      <c r="E83" s="22">
+        <v>2</v>
+      </c>
+      <c r="F83" s="22">
+        <v>5</v>
+      </c>
+      <c r="G83" s="22">
+        <v>1</v>
+      </c>
+      <c r="H83" s="22">
+        <v>0</v>
+      </c>
+      <c r="I83" s="22">
+        <v>109</v>
+      </c>
+      <c r="J83" s="22">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="84" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A84" s="20">
+        <v>43984</v>
+      </c>
+      <c r="B84" s="21">
+        <v>80505</v>
+      </c>
+      <c r="C84" s="22">
+        <v>807</v>
+      </c>
+      <c r="D84" s="22">
+        <v>1477</v>
+      </c>
+      <c r="E84" s="22">
+        <v>2</v>
+      </c>
+      <c r="F84" s="22">
+        <v>5</v>
+      </c>
+      <c r="G84" s="22">
+        <v>0</v>
+      </c>
+      <c r="H84" s="22">
+        <v>0</v>
+      </c>
+      <c r="I84" s="22">
+        <v>109</v>
+      </c>
+      <c r="J84" s="22">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="85" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A85" s="20">
+        <v>43985</v>
+      </c>
+      <c r="B85" s="21">
+        <v>81333</v>
+      </c>
+      <c r="C85" s="22">
+        <v>828</v>
+      </c>
+      <c r="D85" s="22">
+        <v>1477</v>
+      </c>
+      <c r="E85" s="22">
+        <v>0</v>
+      </c>
+      <c r="F85" s="22">
+        <v>5</v>
+      </c>
+      <c r="G85" s="22">
+        <v>0</v>
+      </c>
+      <c r="H85" s="22">
+        <v>0</v>
+      </c>
+      <c r="I85" s="22">
+        <v>109</v>
+      </c>
+      <c r="J85" s="22">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="86" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A86" s="26">
+        <v>43986</v>
+      </c>
+      <c r="B86" s="27">
+        <v>82161</v>
+      </c>
+      <c r="C86" s="28">
+        <v>828</v>
+      </c>
+      <c r="D86" s="28">
+        <v>1479</v>
+      </c>
+      <c r="E86" s="28">
+        <v>2</v>
+      </c>
+      <c r="F86" s="28">
+        <v>6</v>
+      </c>
+      <c r="G86" s="28">
+        <v>0</v>
+      </c>
+      <c r="H86" s="28">
+        <v>0</v>
+      </c>
+      <c r="I86" s="28">
+        <v>109</v>
+      </c>
+      <c r="J86" s="28">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="87" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A87" s="29">
+        <v>43987</v>
+      </c>
+      <c r="B87" s="30">
+        <v>82876</v>
+      </c>
+      <c r="C87" s="31">
+        <v>715</v>
+      </c>
+      <c r="D87" s="31">
+        <v>1484</v>
+      </c>
+      <c r="E87" s="31">
+        <v>5</v>
+      </c>
+      <c r="F87" s="31">
+        <v>6</v>
+      </c>
+      <c r="G87" s="31">
+        <v>0</v>
+      </c>
+      <c r="H87" s="31">
+        <v>0</v>
+      </c>
+      <c r="I87" s="31">
+        <v>109</v>
+      </c>
+      <c r="J87" s="31">
+        <v>0</v>
+      </c>
+    </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>

</xml_diff>

<commit_message>
Data updated by GitHub Bot (2020-06-07 20)
</commit_message>
<xml_diff>
--- a/output/snapshot/fdcf2531-4c3e-5c02-b63c-ee160ead6dea.xlsx
+++ b/output/snapshot/fdcf2531-4c3e-5c02-b63c-ee160ead6dea.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="I:\AKTUALNI PODATKI - KORONA\Za objavo na GOV.SI\ang\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{1E6DD62F-2BE2-47DC-A7ED-9B57C1589256}" xr6:coauthVersionLast="44" xr6:coauthVersionMax="44" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{25DD310D-C2B7-4E50-8262-5F4ACCE3A5DA}" xr6:coauthVersionLast="44" xr6:coauthVersionMax="44" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -64,7 +64,7 @@
   <numFmts count="1">
     <numFmt numFmtId="164" formatCode="d/\ m/\ yyyy;@"/>
   </numFmts>
-  <fonts count="4" x14ac:knownFonts="1">
+  <fonts count="5" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -93,6 +93,13 @@
       <name val="Calibri Light"/>
       <scheme val="major"/>
     </font>
+    <font>
+      <sz val="10"/>
+      <color theme="1"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
   </fonts>
   <fills count="3">
     <fill>
@@ -108,7 +115,7 @@
       </patternFill>
     </fill>
   </fills>
-  <borders count="2">
+  <borders count="3">
     <border>
       <left/>
       <right/>
@@ -129,11 +136,26 @@
       <bottom/>
       <diagonal/>
     </border>
+    <border>
+      <left style="thin">
+        <color theme="4"/>
+      </left>
+      <right style="thin">
+        <color theme="4"/>
+      </right>
+      <top style="thin">
+        <color theme="4"/>
+      </top>
+      <bottom style="thin">
+        <color theme="4"/>
+      </bottom>
+      <diagonal/>
+    </border>
   </borders>
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="26">
+  <cellXfs count="32">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="49" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyAlignment="1" applyProtection="1">
       <alignment horizontal="left" vertical="top"/>
@@ -208,6 +230,24 @@
       <alignment horizontal="right"/>
     </xf>
     <xf numFmtId="0" fontId="3" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="right"/>
+    </xf>
+    <xf numFmtId="164" fontId="4" fillId="2" borderId="2" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="right" vertical="top"/>
+    </xf>
+    <xf numFmtId="3" fontId="4" fillId="2" borderId="2" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="right"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="2" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="right"/>
+    </xf>
+    <xf numFmtId="164" fontId="3" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="right" vertical="top"/>
+    </xf>
+    <xf numFmtId="3" fontId="3" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="right"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="right"/>
     </xf>
   </cellXfs>
@@ -399,8 +439,8 @@
 </file>
 
 <file path=xl/tables/table1.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="1" xr:uid="{00000000-000C-0000-FFFF-FFFF00000000}" name="Tabela1" displayName="Tabela1" ref="A1:J75" totalsRowShown="0" headerRowDxfId="11" dataDxfId="10">
-  <autoFilter ref="A1:J75" xr:uid="{00000000-0009-0000-0100-000001000000}">
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="1" xr:uid="{00000000-000C-0000-FFFF-FFFF00000000}" name="Tabela1" displayName="Tabela1" ref="A1:J88" totalsRowShown="0" headerRowDxfId="11" dataDxfId="10">
+  <autoFilter ref="A1:J88" xr:uid="{00000000-0009-0000-0100-000001000000}">
     <filterColumn colId="0" hiddenButton="1"/>
     <filterColumn colId="1" hiddenButton="1"/>
     <filterColumn colId="2" hiddenButton="1"/>
@@ -696,10 +736,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:J75"/>
+  <dimension ref="A1:J88"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A40" zoomScale="89" zoomScaleNormal="89" workbookViewId="0">
-      <selection activeCell="J74" sqref="J74"/>
+    <sheetView tabSelected="1" topLeftCell="A65" zoomScale="89" zoomScaleNormal="89" workbookViewId="0">
+      <selection activeCell="A88" sqref="A88:J88"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -3117,6 +3157,422 @@
         <v>0</v>
       </c>
     </row>
+    <row r="76" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A76" s="20">
+        <v>43976</v>
+      </c>
+      <c r="B76" s="21">
+        <v>75770</v>
+      </c>
+      <c r="C76" s="22">
+        <v>754</v>
+      </c>
+      <c r="D76" s="22">
+        <v>1469</v>
+      </c>
+      <c r="E76" s="22">
+        <v>0</v>
+      </c>
+      <c r="F76" s="22">
+        <v>9</v>
+      </c>
+      <c r="G76" s="22">
+        <v>2</v>
+      </c>
+      <c r="H76" s="22">
+        <v>6</v>
+      </c>
+      <c r="I76" s="22">
+        <v>108</v>
+      </c>
+      <c r="J76" s="22">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="77" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A77" s="20">
+        <v>43977</v>
+      </c>
+      <c r="B77" s="21">
+        <v>76579</v>
+      </c>
+      <c r="C77" s="22">
+        <v>809</v>
+      </c>
+      <c r="D77" s="22">
+        <v>1471</v>
+      </c>
+      <c r="E77" s="22">
+        <v>2</v>
+      </c>
+      <c r="F77" s="22">
+        <v>8</v>
+      </c>
+      <c r="G77" s="22">
+        <v>2</v>
+      </c>
+      <c r="H77" s="22">
+        <v>2</v>
+      </c>
+      <c r="I77" s="22">
+        <v>108</v>
+      </c>
+      <c r="J77" s="22">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="78" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A78" s="20">
+        <v>43978</v>
+      </c>
+      <c r="B78" s="21">
+        <v>77210</v>
+      </c>
+      <c r="C78" s="22">
+        <v>631</v>
+      </c>
+      <c r="D78" s="22">
+        <v>1473</v>
+      </c>
+      <c r="E78" s="22">
+        <v>2</v>
+      </c>
+      <c r="F78" s="22">
+        <v>7</v>
+      </c>
+      <c r="G78" s="22">
+        <v>2</v>
+      </c>
+      <c r="H78" s="22">
+        <v>1</v>
+      </c>
+      <c r="I78" s="22">
+        <v>108</v>
+      </c>
+      <c r="J78" s="22">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="79" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A79" s="20">
+        <v>43979</v>
+      </c>
+      <c r="B79" s="21">
+        <v>77916</v>
+      </c>
+      <c r="C79" s="22">
+        <v>706</v>
+      </c>
+      <c r="D79" s="22">
+        <v>1473</v>
+      </c>
+      <c r="E79" s="22">
+        <v>0</v>
+      </c>
+      <c r="F79" s="22">
+        <v>7</v>
+      </c>
+      <c r="G79" s="22">
+        <v>2</v>
+      </c>
+      <c r="H79" s="22">
+        <v>0</v>
+      </c>
+      <c r="I79" s="22">
+        <v>108</v>
+      </c>
+      <c r="J79" s="22">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="80" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A80" s="20">
+        <v>43980</v>
+      </c>
+      <c r="B80" s="21">
+        <v>78529</v>
+      </c>
+      <c r="C80" s="22">
+        <v>613</v>
+      </c>
+      <c r="D80" s="22">
+        <v>1473</v>
+      </c>
+      <c r="E80" s="22">
+        <v>0</v>
+      </c>
+      <c r="F80" s="22">
+        <v>7</v>
+      </c>
+      <c r="G80" s="22">
+        <v>2</v>
+      </c>
+      <c r="H80" s="22">
+        <v>0</v>
+      </c>
+      <c r="I80" s="22">
+        <v>108</v>
+      </c>
+      <c r="J80" s="22">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="81" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A81" s="20">
+        <v>43981</v>
+      </c>
+      <c r="B81" s="22">
+        <v>78793</v>
+      </c>
+      <c r="C81" s="22">
+        <v>264</v>
+      </c>
+      <c r="D81" s="22">
+        <v>1473</v>
+      </c>
+      <c r="E81" s="22">
+        <v>0</v>
+      </c>
+      <c r="F81" s="22">
+        <v>6</v>
+      </c>
+      <c r="G81" s="22">
+        <v>2</v>
+      </c>
+      <c r="H81" s="22">
+        <v>1</v>
+      </c>
+      <c r="I81" s="22">
+        <v>108</v>
+      </c>
+      <c r="J81" s="22">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="82" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A82" s="20">
+        <v>43982</v>
+      </c>
+      <c r="B82" s="21">
+        <v>79039</v>
+      </c>
+      <c r="C82" s="22">
+        <v>246</v>
+      </c>
+      <c r="D82" s="22">
+        <v>1473</v>
+      </c>
+      <c r="E82" s="22">
+        <v>0</v>
+      </c>
+      <c r="F82" s="22">
+        <v>5</v>
+      </c>
+      <c r="G82" s="22">
+        <v>1</v>
+      </c>
+      <c r="H82" s="22">
+        <v>0</v>
+      </c>
+      <c r="I82" s="22">
+        <v>109</v>
+      </c>
+      <c r="J82" s="22">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="83" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A83" s="20">
+        <v>43983</v>
+      </c>
+      <c r="B83" s="21">
+        <v>79698</v>
+      </c>
+      <c r="C83" s="22">
+        <v>659</v>
+      </c>
+      <c r="D83" s="22">
+        <v>1475</v>
+      </c>
+      <c r="E83" s="22">
+        <v>2</v>
+      </c>
+      <c r="F83" s="22">
+        <v>5</v>
+      </c>
+      <c r="G83" s="22">
+        <v>1</v>
+      </c>
+      <c r="H83" s="22">
+        <v>0</v>
+      </c>
+      <c r="I83" s="22">
+        <v>109</v>
+      </c>
+      <c r="J83" s="22">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="84" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A84" s="20">
+        <v>43984</v>
+      </c>
+      <c r="B84" s="21">
+        <v>80505</v>
+      </c>
+      <c r="C84" s="22">
+        <v>807</v>
+      </c>
+      <c r="D84" s="22">
+        <v>1477</v>
+      </c>
+      <c r="E84" s="22">
+        <v>2</v>
+      </c>
+      <c r="F84" s="22">
+        <v>5</v>
+      </c>
+      <c r="G84" s="22">
+        <v>0</v>
+      </c>
+      <c r="H84" s="22">
+        <v>0</v>
+      </c>
+      <c r="I84" s="22">
+        <v>109</v>
+      </c>
+      <c r="J84" s="22">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="85" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A85" s="20">
+        <v>43985</v>
+      </c>
+      <c r="B85" s="21">
+        <v>81333</v>
+      </c>
+      <c r="C85" s="22">
+        <v>828</v>
+      </c>
+      <c r="D85" s="22">
+        <v>1477</v>
+      </c>
+      <c r="E85" s="22">
+        <v>0</v>
+      </c>
+      <c r="F85" s="22">
+        <v>5</v>
+      </c>
+      <c r="G85" s="22">
+        <v>0</v>
+      </c>
+      <c r="H85" s="22">
+        <v>0</v>
+      </c>
+      <c r="I85" s="22">
+        <v>109</v>
+      </c>
+      <c r="J85" s="22">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="86" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A86" s="26">
+        <v>43986</v>
+      </c>
+      <c r="B86" s="27">
+        <v>82161</v>
+      </c>
+      <c r="C86" s="28">
+        <v>828</v>
+      </c>
+      <c r="D86" s="28">
+        <v>1479</v>
+      </c>
+      <c r="E86" s="28">
+        <v>2</v>
+      </c>
+      <c r="F86" s="28">
+        <v>6</v>
+      </c>
+      <c r="G86" s="28">
+        <v>0</v>
+      </c>
+      <c r="H86" s="28">
+        <v>0</v>
+      </c>
+      <c r="I86" s="28">
+        <v>109</v>
+      </c>
+      <c r="J86" s="28">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="87" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A87" s="29">
+        <v>43987</v>
+      </c>
+      <c r="B87" s="30">
+        <v>82876</v>
+      </c>
+      <c r="C87" s="31">
+        <v>715</v>
+      </c>
+      <c r="D87" s="31">
+        <v>1484</v>
+      </c>
+      <c r="E87" s="31">
+        <v>5</v>
+      </c>
+      <c r="F87" s="31">
+        <v>6</v>
+      </c>
+      <c r="G87" s="31">
+        <v>0</v>
+      </c>
+      <c r="H87" s="31">
+        <v>0</v>
+      </c>
+      <c r="I87" s="31">
+        <v>109</v>
+      </c>
+      <c r="J87" s="31">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="88" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A88" s="23">
+        <v>43988</v>
+      </c>
+      <c r="B88" s="24">
+        <v>83105</v>
+      </c>
+      <c r="C88" s="25">
+        <v>229</v>
+      </c>
+      <c r="D88" s="25">
+        <v>1485</v>
+      </c>
+      <c r="E88" s="25">
+        <v>1</v>
+      </c>
+      <c r="F88" s="25">
+        <v>5</v>
+      </c>
+      <c r="G88" s="25">
+        <v>0</v>
+      </c>
+      <c r="H88" s="25">
+        <v>1</v>
+      </c>
+      <c r="I88" s="25">
+        <v>109</v>
+      </c>
+      <c r="J88" s="25">
+        <v>0</v>
+      </c>
+    </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>

</xml_diff>

<commit_message>
Data updated by GitHub Bot (2020-06-08 12)
</commit_message>
<xml_diff>
--- a/output/snapshot/fdcf2531-4c3e-5c02-b63c-ee160ead6dea.xlsx
+++ b/output/snapshot/fdcf2531-4c3e-5c02-b63c-ee160ead6dea.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="I:\AKTUALNI PODATKI - KORONA\Za objavo na GOV.SI\ang\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{1E6DD62F-2BE2-47DC-A7ED-9B57C1589256}" xr6:coauthVersionLast="44" xr6:coauthVersionMax="44" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{C707B87E-755A-497E-9D27-5A76429BCC17}" xr6:coauthVersionLast="44" xr6:coauthVersionMax="44" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -64,7 +64,7 @@
   <numFmts count="1">
     <numFmt numFmtId="164" formatCode="d/\ m/\ yyyy;@"/>
   </numFmts>
-  <fonts count="4" x14ac:knownFonts="1">
+  <fonts count="5" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -93,6 +93,13 @@
       <name val="Calibri Light"/>
       <scheme val="major"/>
     </font>
+    <font>
+      <sz val="10"/>
+      <color theme="1"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
   </fonts>
   <fills count="3">
     <fill>
@@ -108,7 +115,7 @@
       </patternFill>
     </fill>
   </fills>
-  <borders count="2">
+  <borders count="3">
     <border>
       <left/>
       <right/>
@@ -129,11 +136,26 @@
       <bottom/>
       <diagonal/>
     </border>
+    <border>
+      <left style="thin">
+        <color theme="4"/>
+      </left>
+      <right style="thin">
+        <color theme="4"/>
+      </right>
+      <top style="thin">
+        <color theme="4"/>
+      </top>
+      <bottom style="thin">
+        <color theme="4"/>
+      </bottom>
+      <diagonal/>
+    </border>
   </borders>
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="26">
+  <cellXfs count="32">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="49" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyAlignment="1" applyProtection="1">
       <alignment horizontal="left" vertical="top"/>
@@ -208,6 +230,24 @@
       <alignment horizontal="right"/>
     </xf>
     <xf numFmtId="0" fontId="3" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="right"/>
+    </xf>
+    <xf numFmtId="164" fontId="4" fillId="2" borderId="2" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="right" vertical="top"/>
+    </xf>
+    <xf numFmtId="3" fontId="4" fillId="2" borderId="2" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="right"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="2" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="right"/>
+    </xf>
+    <xf numFmtId="164" fontId="3" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="right" vertical="top"/>
+    </xf>
+    <xf numFmtId="3" fontId="3" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="right"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="right"/>
     </xf>
   </cellXfs>
@@ -399,8 +439,8 @@
 </file>
 
 <file path=xl/tables/table1.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="1" xr:uid="{00000000-000C-0000-FFFF-FFFF00000000}" name="Tabela1" displayName="Tabela1" ref="A1:J75" totalsRowShown="0" headerRowDxfId="11" dataDxfId="10">
-  <autoFilter ref="A1:J75" xr:uid="{00000000-0009-0000-0100-000001000000}">
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="1" xr:uid="{00000000-000C-0000-FFFF-FFFF00000000}" name="Tabela1" displayName="Tabela1" ref="A1:J89" totalsRowShown="0" headerRowDxfId="11" dataDxfId="10">
+  <autoFilter ref="A1:J89" xr:uid="{00000000-0009-0000-0100-000001000000}">
     <filterColumn colId="0" hiddenButton="1"/>
     <filterColumn colId="1" hiddenButton="1"/>
     <filterColumn colId="2" hiddenButton="1"/>
@@ -696,10 +736,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:J75"/>
+  <dimension ref="A1:J89"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A40" zoomScale="89" zoomScaleNormal="89" workbookViewId="0">
-      <selection activeCell="J74" sqref="J74"/>
+    <sheetView tabSelected="1" topLeftCell="A65" zoomScale="89" zoomScaleNormal="89" workbookViewId="0">
+      <selection activeCell="A89" sqref="A89:J89"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -3117,6 +3157,454 @@
         <v>0</v>
       </c>
     </row>
+    <row r="76" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A76" s="20">
+        <v>43976</v>
+      </c>
+      <c r="B76" s="21">
+        <v>75770</v>
+      </c>
+      <c r="C76" s="22">
+        <v>754</v>
+      </c>
+      <c r="D76" s="22">
+        <v>1469</v>
+      </c>
+      <c r="E76" s="22">
+        <v>0</v>
+      </c>
+      <c r="F76" s="22">
+        <v>9</v>
+      </c>
+      <c r="G76" s="22">
+        <v>2</v>
+      </c>
+      <c r="H76" s="22">
+        <v>6</v>
+      </c>
+      <c r="I76" s="22">
+        <v>108</v>
+      </c>
+      <c r="J76" s="22">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="77" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A77" s="20">
+        <v>43977</v>
+      </c>
+      <c r="B77" s="21">
+        <v>76579</v>
+      </c>
+      <c r="C77" s="22">
+        <v>809</v>
+      </c>
+      <c r="D77" s="22">
+        <v>1471</v>
+      </c>
+      <c r="E77" s="22">
+        <v>2</v>
+      </c>
+      <c r="F77" s="22">
+        <v>8</v>
+      </c>
+      <c r="G77" s="22">
+        <v>2</v>
+      </c>
+      <c r="H77" s="22">
+        <v>2</v>
+      </c>
+      <c r="I77" s="22">
+        <v>108</v>
+      </c>
+      <c r="J77" s="22">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="78" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A78" s="20">
+        <v>43978</v>
+      </c>
+      <c r="B78" s="21">
+        <v>77210</v>
+      </c>
+      <c r="C78" s="22">
+        <v>631</v>
+      </c>
+      <c r="D78" s="22">
+        <v>1473</v>
+      </c>
+      <c r="E78" s="22">
+        <v>2</v>
+      </c>
+      <c r="F78" s="22">
+        <v>7</v>
+      </c>
+      <c r="G78" s="22">
+        <v>2</v>
+      </c>
+      <c r="H78" s="22">
+        <v>1</v>
+      </c>
+      <c r="I78" s="22">
+        <v>108</v>
+      </c>
+      <c r="J78" s="22">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="79" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A79" s="20">
+        <v>43979</v>
+      </c>
+      <c r="B79" s="21">
+        <v>77916</v>
+      </c>
+      <c r="C79" s="22">
+        <v>706</v>
+      </c>
+      <c r="D79" s="22">
+        <v>1473</v>
+      </c>
+      <c r="E79" s="22">
+        <v>0</v>
+      </c>
+      <c r="F79" s="22">
+        <v>7</v>
+      </c>
+      <c r="G79" s="22">
+        <v>2</v>
+      </c>
+      <c r="H79" s="22">
+        <v>0</v>
+      </c>
+      <c r="I79" s="22">
+        <v>108</v>
+      </c>
+      <c r="J79" s="22">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="80" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A80" s="20">
+        <v>43980</v>
+      </c>
+      <c r="B80" s="21">
+        <v>78529</v>
+      </c>
+      <c r="C80" s="22">
+        <v>613</v>
+      </c>
+      <c r="D80" s="22">
+        <v>1473</v>
+      </c>
+      <c r="E80" s="22">
+        <v>0</v>
+      </c>
+      <c r="F80" s="22">
+        <v>7</v>
+      </c>
+      <c r="G80" s="22">
+        <v>2</v>
+      </c>
+      <c r="H80" s="22">
+        <v>0</v>
+      </c>
+      <c r="I80" s="22">
+        <v>108</v>
+      </c>
+      <c r="J80" s="22">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="81" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A81" s="20">
+        <v>43981</v>
+      </c>
+      <c r="B81" s="22">
+        <v>78793</v>
+      </c>
+      <c r="C81" s="22">
+        <v>264</v>
+      </c>
+      <c r="D81" s="22">
+        <v>1473</v>
+      </c>
+      <c r="E81" s="22">
+        <v>0</v>
+      </c>
+      <c r="F81" s="22">
+        <v>6</v>
+      </c>
+      <c r="G81" s="22">
+        <v>2</v>
+      </c>
+      <c r="H81" s="22">
+        <v>1</v>
+      </c>
+      <c r="I81" s="22">
+        <v>108</v>
+      </c>
+      <c r="J81" s="22">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="82" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A82" s="20">
+        <v>43982</v>
+      </c>
+      <c r="B82" s="21">
+        <v>79039</v>
+      </c>
+      <c r="C82" s="22">
+        <v>246</v>
+      </c>
+      <c r="D82" s="22">
+        <v>1473</v>
+      </c>
+      <c r="E82" s="22">
+        <v>0</v>
+      </c>
+      <c r="F82" s="22">
+        <v>5</v>
+      </c>
+      <c r="G82" s="22">
+        <v>1</v>
+      </c>
+      <c r="H82" s="22">
+        <v>0</v>
+      </c>
+      <c r="I82" s="22">
+        <v>109</v>
+      </c>
+      <c r="J82" s="22">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="83" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A83" s="20">
+        <v>43983</v>
+      </c>
+      <c r="B83" s="21">
+        <v>79698</v>
+      </c>
+      <c r="C83" s="22">
+        <v>659</v>
+      </c>
+      <c r="D83" s="22">
+        <v>1475</v>
+      </c>
+      <c r="E83" s="22">
+        <v>2</v>
+      </c>
+      <c r="F83" s="22">
+        <v>5</v>
+      </c>
+      <c r="G83" s="22">
+        <v>1</v>
+      </c>
+      <c r="H83" s="22">
+        <v>0</v>
+      </c>
+      <c r="I83" s="22">
+        <v>109</v>
+      </c>
+      <c r="J83" s="22">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="84" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A84" s="20">
+        <v>43984</v>
+      </c>
+      <c r="B84" s="21">
+        <v>80505</v>
+      </c>
+      <c r="C84" s="22">
+        <v>807</v>
+      </c>
+      <c r="D84" s="22">
+        <v>1477</v>
+      </c>
+      <c r="E84" s="22">
+        <v>2</v>
+      </c>
+      <c r="F84" s="22">
+        <v>5</v>
+      </c>
+      <c r="G84" s="22">
+        <v>0</v>
+      </c>
+      <c r="H84" s="22">
+        <v>0</v>
+      </c>
+      <c r="I84" s="22">
+        <v>109</v>
+      </c>
+      <c r="J84" s="22">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="85" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A85" s="20">
+        <v>43985</v>
+      </c>
+      <c r="B85" s="21">
+        <v>81333</v>
+      </c>
+      <c r="C85" s="22">
+        <v>828</v>
+      </c>
+      <c r="D85" s="22">
+        <v>1477</v>
+      </c>
+      <c r="E85" s="22">
+        <v>0</v>
+      </c>
+      <c r="F85" s="22">
+        <v>5</v>
+      </c>
+      <c r="G85" s="22">
+        <v>0</v>
+      </c>
+      <c r="H85" s="22">
+        <v>0</v>
+      </c>
+      <c r="I85" s="22">
+        <v>109</v>
+      </c>
+      <c r="J85" s="22">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="86" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A86" s="26">
+        <v>43986</v>
+      </c>
+      <c r="B86" s="27">
+        <v>82161</v>
+      </c>
+      <c r="C86" s="28">
+        <v>828</v>
+      </c>
+      <c r="D86" s="28">
+        <v>1479</v>
+      </c>
+      <c r="E86" s="28">
+        <v>2</v>
+      </c>
+      <c r="F86" s="28">
+        <v>6</v>
+      </c>
+      <c r="G86" s="28">
+        <v>0</v>
+      </c>
+      <c r="H86" s="28">
+        <v>0</v>
+      </c>
+      <c r="I86" s="28">
+        <v>109</v>
+      </c>
+      <c r="J86" s="28">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="87" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A87" s="29">
+        <v>43987</v>
+      </c>
+      <c r="B87" s="30">
+        <v>82876</v>
+      </c>
+      <c r="C87" s="31">
+        <v>715</v>
+      </c>
+      <c r="D87" s="31">
+        <v>1484</v>
+      </c>
+      <c r="E87" s="31">
+        <v>5</v>
+      </c>
+      <c r="F87" s="31">
+        <v>6</v>
+      </c>
+      <c r="G87" s="31">
+        <v>0</v>
+      </c>
+      <c r="H87" s="31">
+        <v>0</v>
+      </c>
+      <c r="I87" s="31">
+        <v>109</v>
+      </c>
+      <c r="J87" s="31">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="88" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A88" s="23">
+        <v>43988</v>
+      </c>
+      <c r="B88" s="24">
+        <v>83105</v>
+      </c>
+      <c r="C88" s="25">
+        <v>229</v>
+      </c>
+      <c r="D88" s="25">
+        <v>1485</v>
+      </c>
+      <c r="E88" s="25">
+        <v>1</v>
+      </c>
+      <c r="F88" s="25">
+        <v>5</v>
+      </c>
+      <c r="G88" s="25">
+        <v>0</v>
+      </c>
+      <c r="H88" s="25">
+        <v>1</v>
+      </c>
+      <c r="I88" s="25">
+        <v>109</v>
+      </c>
+      <c r="J88" s="25">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="89" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A89" s="29">
+        <v>43989</v>
+      </c>
+      <c r="B89" s="30">
+        <v>83316</v>
+      </c>
+      <c r="C89" s="31">
+        <v>211</v>
+      </c>
+      <c r="D89" s="31">
+        <v>1485</v>
+      </c>
+      <c r="E89" s="31">
+        <v>0</v>
+      </c>
+      <c r="F89" s="31">
+        <v>5</v>
+      </c>
+      <c r="G89" s="31">
+        <v>0</v>
+      </c>
+      <c r="H89" s="31">
+        <v>0</v>
+      </c>
+      <c r="I89" s="31">
+        <v>109</v>
+      </c>
+      <c r="J89" s="31">
+        <v>0</v>
+      </c>
+    </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>

</xml_diff>

<commit_message>
Data updated by GitHub Bot (2020-06-08 20)
</commit_message>
<xml_diff>
--- a/output/snapshot/fdcf2531-4c3e-5c02-b63c-ee160ead6dea.xlsx
+++ b/output/snapshot/fdcf2531-4c3e-5c02-b63c-ee160ead6dea.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="I:\AKTUALNI PODATKI - KORONA\Za objavo na GOV.SI\ang\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{1E6DD62F-2BE2-47DC-A7ED-9B57C1589256}" xr6:coauthVersionLast="44" xr6:coauthVersionMax="44" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{C707B87E-755A-497E-9D27-5A76429BCC17}" xr6:coauthVersionLast="44" xr6:coauthVersionMax="44" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -64,7 +64,7 @@
   <numFmts count="1">
     <numFmt numFmtId="164" formatCode="d/\ m/\ yyyy;@"/>
   </numFmts>
-  <fonts count="4" x14ac:knownFonts="1">
+  <fonts count="5" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -93,6 +93,13 @@
       <name val="Calibri Light"/>
       <scheme val="major"/>
     </font>
+    <font>
+      <sz val="10"/>
+      <color theme="1"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
   </fonts>
   <fills count="3">
     <fill>
@@ -108,7 +115,7 @@
       </patternFill>
     </fill>
   </fills>
-  <borders count="2">
+  <borders count="3">
     <border>
       <left/>
       <right/>
@@ -129,11 +136,26 @@
       <bottom/>
       <diagonal/>
     </border>
+    <border>
+      <left style="thin">
+        <color theme="4"/>
+      </left>
+      <right style="thin">
+        <color theme="4"/>
+      </right>
+      <top style="thin">
+        <color theme="4"/>
+      </top>
+      <bottom style="thin">
+        <color theme="4"/>
+      </bottom>
+      <diagonal/>
+    </border>
   </borders>
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="26">
+  <cellXfs count="32">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="49" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyAlignment="1" applyProtection="1">
       <alignment horizontal="left" vertical="top"/>
@@ -208,6 +230,24 @@
       <alignment horizontal="right"/>
     </xf>
     <xf numFmtId="0" fontId="3" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="right"/>
+    </xf>
+    <xf numFmtId="164" fontId="4" fillId="2" borderId="2" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="right" vertical="top"/>
+    </xf>
+    <xf numFmtId="3" fontId="4" fillId="2" borderId="2" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="right"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="2" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="right"/>
+    </xf>
+    <xf numFmtId="164" fontId="3" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="right" vertical="top"/>
+    </xf>
+    <xf numFmtId="3" fontId="3" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="right"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="right"/>
     </xf>
   </cellXfs>
@@ -399,8 +439,8 @@
 </file>
 
 <file path=xl/tables/table1.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="1" xr:uid="{00000000-000C-0000-FFFF-FFFF00000000}" name="Tabela1" displayName="Tabela1" ref="A1:J75" totalsRowShown="0" headerRowDxfId="11" dataDxfId="10">
-  <autoFilter ref="A1:J75" xr:uid="{00000000-0009-0000-0100-000001000000}">
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="1" xr:uid="{00000000-000C-0000-FFFF-FFFF00000000}" name="Tabela1" displayName="Tabela1" ref="A1:J89" totalsRowShown="0" headerRowDxfId="11" dataDxfId="10">
+  <autoFilter ref="A1:J89" xr:uid="{00000000-0009-0000-0100-000001000000}">
     <filterColumn colId="0" hiddenButton="1"/>
     <filterColumn colId="1" hiddenButton="1"/>
     <filterColumn colId="2" hiddenButton="1"/>
@@ -696,10 +736,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:J75"/>
+  <dimension ref="A1:J89"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A40" zoomScale="89" zoomScaleNormal="89" workbookViewId="0">
-      <selection activeCell="J74" sqref="J74"/>
+    <sheetView tabSelected="1" topLeftCell="A65" zoomScale="89" zoomScaleNormal="89" workbookViewId="0">
+      <selection activeCell="A89" sqref="A89:J89"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -3117,6 +3157,454 @@
         <v>0</v>
       </c>
     </row>
+    <row r="76" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A76" s="20">
+        <v>43976</v>
+      </c>
+      <c r="B76" s="21">
+        <v>75770</v>
+      </c>
+      <c r="C76" s="22">
+        <v>754</v>
+      </c>
+      <c r="D76" s="22">
+        <v>1469</v>
+      </c>
+      <c r="E76" s="22">
+        <v>0</v>
+      </c>
+      <c r="F76" s="22">
+        <v>9</v>
+      </c>
+      <c r="G76" s="22">
+        <v>2</v>
+      </c>
+      <c r="H76" s="22">
+        <v>6</v>
+      </c>
+      <c r="I76" s="22">
+        <v>108</v>
+      </c>
+      <c r="J76" s="22">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="77" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A77" s="20">
+        <v>43977</v>
+      </c>
+      <c r="B77" s="21">
+        <v>76579</v>
+      </c>
+      <c r="C77" s="22">
+        <v>809</v>
+      </c>
+      <c r="D77" s="22">
+        <v>1471</v>
+      </c>
+      <c r="E77" s="22">
+        <v>2</v>
+      </c>
+      <c r="F77" s="22">
+        <v>8</v>
+      </c>
+      <c r="G77" s="22">
+        <v>2</v>
+      </c>
+      <c r="H77" s="22">
+        <v>2</v>
+      </c>
+      <c r="I77" s="22">
+        <v>108</v>
+      </c>
+      <c r="J77" s="22">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="78" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A78" s="20">
+        <v>43978</v>
+      </c>
+      <c r="B78" s="21">
+        <v>77210</v>
+      </c>
+      <c r="C78" s="22">
+        <v>631</v>
+      </c>
+      <c r="D78" s="22">
+        <v>1473</v>
+      </c>
+      <c r="E78" s="22">
+        <v>2</v>
+      </c>
+      <c r="F78" s="22">
+        <v>7</v>
+      </c>
+      <c r="G78" s="22">
+        <v>2</v>
+      </c>
+      <c r="H78" s="22">
+        <v>1</v>
+      </c>
+      <c r="I78" s="22">
+        <v>108</v>
+      </c>
+      <c r="J78" s="22">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="79" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A79" s="20">
+        <v>43979</v>
+      </c>
+      <c r="B79" s="21">
+        <v>77916</v>
+      </c>
+      <c r="C79" s="22">
+        <v>706</v>
+      </c>
+      <c r="D79" s="22">
+        <v>1473</v>
+      </c>
+      <c r="E79" s="22">
+        <v>0</v>
+      </c>
+      <c r="F79" s="22">
+        <v>7</v>
+      </c>
+      <c r="G79" s="22">
+        <v>2</v>
+      </c>
+      <c r="H79" s="22">
+        <v>0</v>
+      </c>
+      <c r="I79" s="22">
+        <v>108</v>
+      </c>
+      <c r="J79" s="22">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="80" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A80" s="20">
+        <v>43980</v>
+      </c>
+      <c r="B80" s="21">
+        <v>78529</v>
+      </c>
+      <c r="C80" s="22">
+        <v>613</v>
+      </c>
+      <c r="D80" s="22">
+        <v>1473</v>
+      </c>
+      <c r="E80" s="22">
+        <v>0</v>
+      </c>
+      <c r="F80" s="22">
+        <v>7</v>
+      </c>
+      <c r="G80" s="22">
+        <v>2</v>
+      </c>
+      <c r="H80" s="22">
+        <v>0</v>
+      </c>
+      <c r="I80" s="22">
+        <v>108</v>
+      </c>
+      <c r="J80" s="22">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="81" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A81" s="20">
+        <v>43981</v>
+      </c>
+      <c r="B81" s="22">
+        <v>78793</v>
+      </c>
+      <c r="C81" s="22">
+        <v>264</v>
+      </c>
+      <c r="D81" s="22">
+        <v>1473</v>
+      </c>
+      <c r="E81" s="22">
+        <v>0</v>
+      </c>
+      <c r="F81" s="22">
+        <v>6</v>
+      </c>
+      <c r="G81" s="22">
+        <v>2</v>
+      </c>
+      <c r="H81" s="22">
+        <v>1</v>
+      </c>
+      <c r="I81" s="22">
+        <v>108</v>
+      </c>
+      <c r="J81" s="22">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="82" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A82" s="20">
+        <v>43982</v>
+      </c>
+      <c r="B82" s="21">
+        <v>79039</v>
+      </c>
+      <c r="C82" s="22">
+        <v>246</v>
+      </c>
+      <c r="D82" s="22">
+        <v>1473</v>
+      </c>
+      <c r="E82" s="22">
+        <v>0</v>
+      </c>
+      <c r="F82" s="22">
+        <v>5</v>
+      </c>
+      <c r="G82" s="22">
+        <v>1</v>
+      </c>
+      <c r="H82" s="22">
+        <v>0</v>
+      </c>
+      <c r="I82" s="22">
+        <v>109</v>
+      </c>
+      <c r="J82" s="22">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="83" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A83" s="20">
+        <v>43983</v>
+      </c>
+      <c r="B83" s="21">
+        <v>79698</v>
+      </c>
+      <c r="C83" s="22">
+        <v>659</v>
+      </c>
+      <c r="D83" s="22">
+        <v>1475</v>
+      </c>
+      <c r="E83" s="22">
+        <v>2</v>
+      </c>
+      <c r="F83" s="22">
+        <v>5</v>
+      </c>
+      <c r="G83" s="22">
+        <v>1</v>
+      </c>
+      <c r="H83" s="22">
+        <v>0</v>
+      </c>
+      <c r="I83" s="22">
+        <v>109</v>
+      </c>
+      <c r="J83" s="22">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="84" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A84" s="20">
+        <v>43984</v>
+      </c>
+      <c r="B84" s="21">
+        <v>80505</v>
+      </c>
+      <c r="C84" s="22">
+        <v>807</v>
+      </c>
+      <c r="D84" s="22">
+        <v>1477</v>
+      </c>
+      <c r="E84" s="22">
+        <v>2</v>
+      </c>
+      <c r="F84" s="22">
+        <v>5</v>
+      </c>
+      <c r="G84" s="22">
+        <v>0</v>
+      </c>
+      <c r="H84" s="22">
+        <v>0</v>
+      </c>
+      <c r="I84" s="22">
+        <v>109</v>
+      </c>
+      <c r="J84" s="22">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="85" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A85" s="20">
+        <v>43985</v>
+      </c>
+      <c r="B85" s="21">
+        <v>81333</v>
+      </c>
+      <c r="C85" s="22">
+        <v>828</v>
+      </c>
+      <c r="D85" s="22">
+        <v>1477</v>
+      </c>
+      <c r="E85" s="22">
+        <v>0</v>
+      </c>
+      <c r="F85" s="22">
+        <v>5</v>
+      </c>
+      <c r="G85" s="22">
+        <v>0</v>
+      </c>
+      <c r="H85" s="22">
+        <v>0</v>
+      </c>
+      <c r="I85" s="22">
+        <v>109</v>
+      </c>
+      <c r="J85" s="22">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="86" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A86" s="26">
+        <v>43986</v>
+      </c>
+      <c r="B86" s="27">
+        <v>82161</v>
+      </c>
+      <c r="C86" s="28">
+        <v>828</v>
+      </c>
+      <c r="D86" s="28">
+        <v>1479</v>
+      </c>
+      <c r="E86" s="28">
+        <v>2</v>
+      </c>
+      <c r="F86" s="28">
+        <v>6</v>
+      </c>
+      <c r="G86" s="28">
+        <v>0</v>
+      </c>
+      <c r="H86" s="28">
+        <v>0</v>
+      </c>
+      <c r="I86" s="28">
+        <v>109</v>
+      </c>
+      <c r="J86" s="28">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="87" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A87" s="29">
+        <v>43987</v>
+      </c>
+      <c r="B87" s="30">
+        <v>82876</v>
+      </c>
+      <c r="C87" s="31">
+        <v>715</v>
+      </c>
+      <c r="D87" s="31">
+        <v>1484</v>
+      </c>
+      <c r="E87" s="31">
+        <v>5</v>
+      </c>
+      <c r="F87" s="31">
+        <v>6</v>
+      </c>
+      <c r="G87" s="31">
+        <v>0</v>
+      </c>
+      <c r="H87" s="31">
+        <v>0</v>
+      </c>
+      <c r="I87" s="31">
+        <v>109</v>
+      </c>
+      <c r="J87" s="31">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="88" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A88" s="23">
+        <v>43988</v>
+      </c>
+      <c r="B88" s="24">
+        <v>83105</v>
+      </c>
+      <c r="C88" s="25">
+        <v>229</v>
+      </c>
+      <c r="D88" s="25">
+        <v>1485</v>
+      </c>
+      <c r="E88" s="25">
+        <v>1</v>
+      </c>
+      <c r="F88" s="25">
+        <v>5</v>
+      </c>
+      <c r="G88" s="25">
+        <v>0</v>
+      </c>
+      <c r="H88" s="25">
+        <v>1</v>
+      </c>
+      <c r="I88" s="25">
+        <v>109</v>
+      </c>
+      <c r="J88" s="25">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="89" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A89" s="29">
+        <v>43989</v>
+      </c>
+      <c r="B89" s="30">
+        <v>83316</v>
+      </c>
+      <c r="C89" s="31">
+        <v>211</v>
+      </c>
+      <c r="D89" s="31">
+        <v>1485</v>
+      </c>
+      <c r="E89" s="31">
+        <v>0</v>
+      </c>
+      <c r="F89" s="31">
+        <v>5</v>
+      </c>
+      <c r="G89" s="31">
+        <v>0</v>
+      </c>
+      <c r="H89" s="31">
+        <v>0</v>
+      </c>
+      <c r="I89" s="31">
+        <v>109</v>
+      </c>
+      <c r="J89" s="31">
+        <v>0</v>
+      </c>
+    </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>

</xml_diff>

<commit_message>
Data updated by GitHub Bot (2020-06-09 12)
</commit_message>
<xml_diff>
--- a/output/snapshot/fdcf2531-4c3e-5c02-b63c-ee160ead6dea.xlsx
+++ b/output/snapshot/fdcf2531-4c3e-5c02-b63c-ee160ead6dea.xlsx
@@ -1,16 +1,15 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="21929"/>
-  <workbookPr/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
+  <fileVersion appName="xl" lastEdited="6" lowestEdited="6" rupBuild="14420"/>
+  <workbookPr defaultThemeVersion="164011"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="I:\AKTUALNI PODATKI - KORONA\Za objavo na GOV.SI\ang\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{1E6DD62F-2BE2-47DC-A7ED-9B57C1589256}" xr6:coauthVersionLast="44" xr6:coauthVersionMax="44" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840"/>
   </bookViews>
   <sheets>
     <sheet name="Covid-19 podatki" sheetId="1" r:id="rId1"/>
@@ -60,11 +59,11 @@
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" mc:Ignorable="x14ac x16r2">
   <numFmts count="1">
     <numFmt numFmtId="164" formatCode="d/\ m/\ yyyy;@"/>
   </numFmts>
-  <fonts count="4" x14ac:knownFonts="1">
+  <fonts count="5" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -93,6 +92,13 @@
       <name val="Calibri Light"/>
       <scheme val="major"/>
     </font>
+    <font>
+      <sz val="10"/>
+      <color theme="1"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
   </fonts>
   <fills count="3">
     <fill>
@@ -108,7 +114,7 @@
       </patternFill>
     </fill>
   </fills>
-  <borders count="2">
+  <borders count="3">
     <border>
       <left/>
       <right/>
@@ -129,11 +135,26 @@
       <bottom/>
       <diagonal/>
     </border>
+    <border>
+      <left style="thin">
+        <color theme="4"/>
+      </left>
+      <right style="thin">
+        <color theme="4"/>
+      </right>
+      <top style="thin">
+        <color theme="4"/>
+      </top>
+      <bottom style="thin">
+        <color theme="4"/>
+      </bottom>
+      <diagonal/>
+    </border>
   </borders>
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="26">
+  <cellXfs count="32">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="49" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyAlignment="1" applyProtection="1">
       <alignment horizontal="left" vertical="top"/>
@@ -208,6 +229,24 @@
       <alignment horizontal="right"/>
     </xf>
     <xf numFmtId="0" fontId="3" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="right"/>
+    </xf>
+    <xf numFmtId="164" fontId="4" fillId="2" borderId="2" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="right" vertical="top"/>
+    </xf>
+    <xf numFmtId="3" fontId="4" fillId="2" borderId="2" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="right"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="2" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="right"/>
+    </xf>
+    <xf numFmtId="164" fontId="3" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="right" vertical="top"/>
+    </xf>
+    <xf numFmtId="3" fontId="3" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="right"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="right"/>
     </xf>
   </cellXfs>
@@ -399,8 +438,8 @@
 </file>
 
 <file path=xl/tables/table1.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="1" xr:uid="{00000000-000C-0000-FFFF-FFFF00000000}" name="Tabela1" displayName="Tabela1" ref="A1:J75" totalsRowShown="0" headerRowDxfId="11" dataDxfId="10">
-  <autoFilter ref="A1:J75" xr:uid="{00000000-0009-0000-0100-000001000000}">
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="1" name="Tabela1" displayName="Tabela1" ref="A1:J90" totalsRowShown="0" headerRowDxfId="11" dataDxfId="10">
+  <autoFilter ref="A1:J90">
     <filterColumn colId="0" hiddenButton="1"/>
     <filterColumn colId="1" hiddenButton="1"/>
     <filterColumn colId="2" hiddenButton="1"/>
@@ -413,16 +452,16 @@
     <filterColumn colId="9" hiddenButton="1"/>
   </autoFilter>
   <tableColumns count="10">
-    <tableColumn id="1" xr3:uid="{00000000-0010-0000-0000-000001000000}" name="Date" dataDxfId="9"/>
-    <tableColumn id="2" xr3:uid="{00000000-0010-0000-0000-000002000000}" name="Tested (all)" dataDxfId="8"/>
-    <tableColumn id="3" xr3:uid="{00000000-0010-0000-0000-000003000000}" name="Tested (daily)" dataDxfId="7"/>
-    <tableColumn id="4" xr3:uid="{00000000-0010-0000-0000-000004000000}" name="Positive (all)" dataDxfId="6"/>
-    <tableColumn id="5" xr3:uid="{00000000-0010-0000-0000-000005000000}" name="Positive (daily)" dataDxfId="5"/>
-    <tableColumn id="6" xr3:uid="{00000000-0010-0000-0000-000006000000}" name="All hospitalized on certain day" dataDxfId="4"/>
-    <tableColumn id="7" xr3:uid="{00000000-0010-0000-0000-000007000000}" name="All persons in intensive care on certain day" dataDxfId="3"/>
-    <tableColumn id="10" xr3:uid="{00000000-0010-0000-0000-00000A000000}" name="Discharged" dataDxfId="2"/>
-    <tableColumn id="8" xr3:uid="{00000000-0010-0000-0000-000008000000}" name="Deaths (all)" dataDxfId="1"/>
-    <tableColumn id="9" xr3:uid="{00000000-0010-0000-0000-000009000000}" name="Deaths (daily)" dataDxfId="0"/>
+    <tableColumn id="1" name="Date" dataDxfId="9"/>
+    <tableColumn id="2" name="Tested (all)" dataDxfId="8"/>
+    <tableColumn id="3" name="Tested (daily)" dataDxfId="7"/>
+    <tableColumn id="4" name="Positive (all)" dataDxfId="6"/>
+    <tableColumn id="5" name="Positive (daily)" dataDxfId="5"/>
+    <tableColumn id="6" name="All hospitalized on certain day" dataDxfId="4"/>
+    <tableColumn id="7" name="All persons in intensive care on certain day" dataDxfId="3"/>
+    <tableColumn id="10" name="Discharged" dataDxfId="2"/>
+    <tableColumn id="8" name="Deaths (all)" dataDxfId="1"/>
+    <tableColumn id="9" name="Deaths (daily)" dataDxfId="0"/>
   </tableColumns>
   <tableStyleInfo name="TableStyleLight16" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
   <extLst>
@@ -695,11 +734,11 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:J75"/>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <dimension ref="A1:J90"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A40" zoomScale="89" zoomScaleNormal="89" workbookViewId="0">
-      <selection activeCell="J74" sqref="J74"/>
+    <sheetView tabSelected="1" topLeftCell="A65" zoomScale="89" zoomScaleNormal="89" workbookViewId="0">
+      <selection activeCell="E94" sqref="E94"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -3117,6 +3156,486 @@
         <v>0</v>
       </c>
     </row>
+    <row r="76" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A76" s="20">
+        <v>43976</v>
+      </c>
+      <c r="B76" s="21">
+        <v>75770</v>
+      </c>
+      <c r="C76" s="22">
+        <v>754</v>
+      </c>
+      <c r="D76" s="22">
+        <v>1469</v>
+      </c>
+      <c r="E76" s="22">
+        <v>0</v>
+      </c>
+      <c r="F76" s="22">
+        <v>9</v>
+      </c>
+      <c r="G76" s="22">
+        <v>2</v>
+      </c>
+      <c r="H76" s="22">
+        <v>6</v>
+      </c>
+      <c r="I76" s="22">
+        <v>108</v>
+      </c>
+      <c r="J76" s="22">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="77" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A77" s="20">
+        <v>43977</v>
+      </c>
+      <c r="B77" s="21">
+        <v>76579</v>
+      </c>
+      <c r="C77" s="22">
+        <v>809</v>
+      </c>
+      <c r="D77" s="22">
+        <v>1471</v>
+      </c>
+      <c r="E77" s="22">
+        <v>2</v>
+      </c>
+      <c r="F77" s="22">
+        <v>8</v>
+      </c>
+      <c r="G77" s="22">
+        <v>2</v>
+      </c>
+      <c r="H77" s="22">
+        <v>2</v>
+      </c>
+      <c r="I77" s="22">
+        <v>108</v>
+      </c>
+      <c r="J77" s="22">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="78" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A78" s="20">
+        <v>43978</v>
+      </c>
+      <c r="B78" s="21">
+        <v>77210</v>
+      </c>
+      <c r="C78" s="22">
+        <v>631</v>
+      </c>
+      <c r="D78" s="22">
+        <v>1473</v>
+      </c>
+      <c r="E78" s="22">
+        <v>2</v>
+      </c>
+      <c r="F78" s="22">
+        <v>7</v>
+      </c>
+      <c r="G78" s="22">
+        <v>2</v>
+      </c>
+      <c r="H78" s="22">
+        <v>1</v>
+      </c>
+      <c r="I78" s="22">
+        <v>108</v>
+      </c>
+      <c r="J78" s="22">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="79" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A79" s="20">
+        <v>43979</v>
+      </c>
+      <c r="B79" s="21">
+        <v>77916</v>
+      </c>
+      <c r="C79" s="22">
+        <v>706</v>
+      </c>
+      <c r="D79" s="22">
+        <v>1473</v>
+      </c>
+      <c r="E79" s="22">
+        <v>0</v>
+      </c>
+      <c r="F79" s="22">
+        <v>7</v>
+      </c>
+      <c r="G79" s="22">
+        <v>2</v>
+      </c>
+      <c r="H79" s="22">
+        <v>0</v>
+      </c>
+      <c r="I79" s="22">
+        <v>108</v>
+      </c>
+      <c r="J79" s="22">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="80" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A80" s="20">
+        <v>43980</v>
+      </c>
+      <c r="B80" s="21">
+        <v>78529</v>
+      </c>
+      <c r="C80" s="22">
+        <v>613</v>
+      </c>
+      <c r="D80" s="22">
+        <v>1473</v>
+      </c>
+      <c r="E80" s="22">
+        <v>0</v>
+      </c>
+      <c r="F80" s="22">
+        <v>7</v>
+      </c>
+      <c r="G80" s="22">
+        <v>2</v>
+      </c>
+      <c r="H80" s="22">
+        <v>0</v>
+      </c>
+      <c r="I80" s="22">
+        <v>108</v>
+      </c>
+      <c r="J80" s="22">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="81" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A81" s="20">
+        <v>43981</v>
+      </c>
+      <c r="B81" s="22">
+        <v>78793</v>
+      </c>
+      <c r="C81" s="22">
+        <v>264</v>
+      </c>
+      <c r="D81" s="22">
+        <v>1473</v>
+      </c>
+      <c r="E81" s="22">
+        <v>0</v>
+      </c>
+      <c r="F81" s="22">
+        <v>6</v>
+      </c>
+      <c r="G81" s="22">
+        <v>2</v>
+      </c>
+      <c r="H81" s="22">
+        <v>1</v>
+      </c>
+      <c r="I81" s="22">
+        <v>108</v>
+      </c>
+      <c r="J81" s="22">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="82" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A82" s="20">
+        <v>43982</v>
+      </c>
+      <c r="B82" s="21">
+        <v>79039</v>
+      </c>
+      <c r="C82" s="22">
+        <v>246</v>
+      </c>
+      <c r="D82" s="22">
+        <v>1473</v>
+      </c>
+      <c r="E82" s="22">
+        <v>0</v>
+      </c>
+      <c r="F82" s="22">
+        <v>5</v>
+      </c>
+      <c r="G82" s="22">
+        <v>1</v>
+      </c>
+      <c r="H82" s="22">
+        <v>0</v>
+      </c>
+      <c r="I82" s="22">
+        <v>109</v>
+      </c>
+      <c r="J82" s="22">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="83" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A83" s="20">
+        <v>43983</v>
+      </c>
+      <c r="B83" s="21">
+        <v>79698</v>
+      </c>
+      <c r="C83" s="22">
+        <v>659</v>
+      </c>
+      <c r="D83" s="22">
+        <v>1475</v>
+      </c>
+      <c r="E83" s="22">
+        <v>2</v>
+      </c>
+      <c r="F83" s="22">
+        <v>5</v>
+      </c>
+      <c r="G83" s="22">
+        <v>1</v>
+      </c>
+      <c r="H83" s="22">
+        <v>0</v>
+      </c>
+      <c r="I83" s="22">
+        <v>109</v>
+      </c>
+      <c r="J83" s="22">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="84" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A84" s="20">
+        <v>43984</v>
+      </c>
+      <c r="B84" s="21">
+        <v>80505</v>
+      </c>
+      <c r="C84" s="22">
+        <v>807</v>
+      </c>
+      <c r="D84" s="22">
+        <v>1477</v>
+      </c>
+      <c r="E84" s="22">
+        <v>2</v>
+      </c>
+      <c r="F84" s="22">
+        <v>5</v>
+      </c>
+      <c r="G84" s="22">
+        <v>0</v>
+      </c>
+      <c r="H84" s="22">
+        <v>0</v>
+      </c>
+      <c r="I84" s="22">
+        <v>109</v>
+      </c>
+      <c r="J84" s="22">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="85" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A85" s="20">
+        <v>43985</v>
+      </c>
+      <c r="B85" s="21">
+        <v>81333</v>
+      </c>
+      <c r="C85" s="22">
+        <v>828</v>
+      </c>
+      <c r="D85" s="22">
+        <v>1477</v>
+      </c>
+      <c r="E85" s="22">
+        <v>0</v>
+      </c>
+      <c r="F85" s="22">
+        <v>5</v>
+      </c>
+      <c r="G85" s="22">
+        <v>0</v>
+      </c>
+      <c r="H85" s="22">
+        <v>0</v>
+      </c>
+      <c r="I85" s="22">
+        <v>109</v>
+      </c>
+      <c r="J85" s="22">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="86" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A86" s="26">
+        <v>43986</v>
+      </c>
+      <c r="B86" s="27">
+        <v>82161</v>
+      </c>
+      <c r="C86" s="28">
+        <v>828</v>
+      </c>
+      <c r="D86" s="28">
+        <v>1479</v>
+      </c>
+      <c r="E86" s="28">
+        <v>2</v>
+      </c>
+      <c r="F86" s="28">
+        <v>6</v>
+      </c>
+      <c r="G86" s="28">
+        <v>0</v>
+      </c>
+      <c r="H86" s="28">
+        <v>0</v>
+      </c>
+      <c r="I86" s="28">
+        <v>109</v>
+      </c>
+      <c r="J86" s="28">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="87" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A87" s="29">
+        <v>43987</v>
+      </c>
+      <c r="B87" s="30">
+        <v>82876</v>
+      </c>
+      <c r="C87" s="31">
+        <v>715</v>
+      </c>
+      <c r="D87" s="31">
+        <v>1484</v>
+      </c>
+      <c r="E87" s="31">
+        <v>5</v>
+      </c>
+      <c r="F87" s="31">
+        <v>6</v>
+      </c>
+      <c r="G87" s="31">
+        <v>0</v>
+      </c>
+      <c r="H87" s="31">
+        <v>0</v>
+      </c>
+      <c r="I87" s="31">
+        <v>109</v>
+      </c>
+      <c r="J87" s="31">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="88" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A88" s="23">
+        <v>43988</v>
+      </c>
+      <c r="B88" s="24">
+        <v>83105</v>
+      </c>
+      <c r="C88" s="25">
+        <v>229</v>
+      </c>
+      <c r="D88" s="25">
+        <v>1485</v>
+      </c>
+      <c r="E88" s="25">
+        <v>1</v>
+      </c>
+      <c r="F88" s="25">
+        <v>5</v>
+      </c>
+      <c r="G88" s="25">
+        <v>0</v>
+      </c>
+      <c r="H88" s="25">
+        <v>1</v>
+      </c>
+      <c r="I88" s="25">
+        <v>109</v>
+      </c>
+      <c r="J88" s="25">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="89" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A89" s="29">
+        <v>43989</v>
+      </c>
+      <c r="B89" s="30">
+        <v>83316</v>
+      </c>
+      <c r="C89" s="31">
+        <v>211</v>
+      </c>
+      <c r="D89" s="31">
+        <v>1485</v>
+      </c>
+      <c r="E89" s="31">
+        <v>0</v>
+      </c>
+      <c r="F89" s="31">
+        <v>5</v>
+      </c>
+      <c r="G89" s="31">
+        <v>0</v>
+      </c>
+      <c r="H89" s="31">
+        <v>0</v>
+      </c>
+      <c r="I89" s="31">
+        <v>109</v>
+      </c>
+      <c r="J89" s="31">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="90" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A90" s="20">
+        <v>43990</v>
+      </c>
+      <c r="B90" s="21">
+        <v>84130</v>
+      </c>
+      <c r="C90" s="22">
+        <v>814</v>
+      </c>
+      <c r="D90" s="22">
+        <v>1486</v>
+      </c>
+      <c r="E90" s="22">
+        <v>1</v>
+      </c>
+      <c r="F90" s="22">
+        <v>6</v>
+      </c>
+      <c r="G90" s="22">
+        <v>0</v>
+      </c>
+      <c r="H90" s="22">
+        <v>0</v>
+      </c>
+      <c r="I90" s="22">
+        <v>109</v>
+      </c>
+      <c r="J90" s="22">
+        <v>0</v>
+      </c>
+    </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>

</xml_diff>

<commit_message>
Data updated by GitHub Bot (2020-06-09 20)
</commit_message>
<xml_diff>
--- a/output/snapshot/fdcf2531-4c3e-5c02-b63c-ee160ead6dea.xlsx
+++ b/output/snapshot/fdcf2531-4c3e-5c02-b63c-ee160ead6dea.xlsx
@@ -1,16 +1,15 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="21929"/>
-  <workbookPr/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
+  <fileVersion appName="xl" lastEdited="6" lowestEdited="6" rupBuild="14420"/>
+  <workbookPr defaultThemeVersion="164011"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="I:\AKTUALNI PODATKI - KORONA\Za objavo na GOV.SI\ang\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{1E6DD62F-2BE2-47DC-A7ED-9B57C1589256}" xr6:coauthVersionLast="44" xr6:coauthVersionMax="44" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840"/>
   </bookViews>
   <sheets>
     <sheet name="Covid-19 podatki" sheetId="1" r:id="rId1"/>
@@ -60,11 +59,11 @@
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" mc:Ignorable="x14ac x16r2">
   <numFmts count="1">
     <numFmt numFmtId="164" formatCode="d/\ m/\ yyyy;@"/>
   </numFmts>
-  <fonts count="4" x14ac:knownFonts="1">
+  <fonts count="5" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -93,6 +92,13 @@
       <name val="Calibri Light"/>
       <scheme val="major"/>
     </font>
+    <font>
+      <sz val="10"/>
+      <color theme="1"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
   </fonts>
   <fills count="3">
     <fill>
@@ -108,7 +114,7 @@
       </patternFill>
     </fill>
   </fills>
-  <borders count="2">
+  <borders count="3">
     <border>
       <left/>
       <right/>
@@ -129,11 +135,26 @@
       <bottom/>
       <diagonal/>
     </border>
+    <border>
+      <left style="thin">
+        <color theme="4"/>
+      </left>
+      <right style="thin">
+        <color theme="4"/>
+      </right>
+      <top style="thin">
+        <color theme="4"/>
+      </top>
+      <bottom style="thin">
+        <color theme="4"/>
+      </bottom>
+      <diagonal/>
+    </border>
   </borders>
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="26">
+  <cellXfs count="32">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="49" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyAlignment="1" applyProtection="1">
       <alignment horizontal="left" vertical="top"/>
@@ -208,6 +229,24 @@
       <alignment horizontal="right"/>
     </xf>
     <xf numFmtId="0" fontId="3" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="right"/>
+    </xf>
+    <xf numFmtId="164" fontId="4" fillId="2" borderId="2" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="right" vertical="top"/>
+    </xf>
+    <xf numFmtId="3" fontId="4" fillId="2" borderId="2" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="right"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="2" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="right"/>
+    </xf>
+    <xf numFmtId="164" fontId="3" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="right" vertical="top"/>
+    </xf>
+    <xf numFmtId="3" fontId="3" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="right"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="right"/>
     </xf>
   </cellXfs>
@@ -399,8 +438,8 @@
 </file>
 
 <file path=xl/tables/table1.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="1" xr:uid="{00000000-000C-0000-FFFF-FFFF00000000}" name="Tabela1" displayName="Tabela1" ref="A1:J75" totalsRowShown="0" headerRowDxfId="11" dataDxfId="10">
-  <autoFilter ref="A1:J75" xr:uid="{00000000-0009-0000-0100-000001000000}">
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="1" name="Tabela1" displayName="Tabela1" ref="A1:J90" totalsRowShown="0" headerRowDxfId="11" dataDxfId="10">
+  <autoFilter ref="A1:J90">
     <filterColumn colId="0" hiddenButton="1"/>
     <filterColumn colId="1" hiddenButton="1"/>
     <filterColumn colId="2" hiddenButton="1"/>
@@ -413,16 +452,16 @@
     <filterColumn colId="9" hiddenButton="1"/>
   </autoFilter>
   <tableColumns count="10">
-    <tableColumn id="1" xr3:uid="{00000000-0010-0000-0000-000001000000}" name="Date" dataDxfId="9"/>
-    <tableColumn id="2" xr3:uid="{00000000-0010-0000-0000-000002000000}" name="Tested (all)" dataDxfId="8"/>
-    <tableColumn id="3" xr3:uid="{00000000-0010-0000-0000-000003000000}" name="Tested (daily)" dataDxfId="7"/>
-    <tableColumn id="4" xr3:uid="{00000000-0010-0000-0000-000004000000}" name="Positive (all)" dataDxfId="6"/>
-    <tableColumn id="5" xr3:uid="{00000000-0010-0000-0000-000005000000}" name="Positive (daily)" dataDxfId="5"/>
-    <tableColumn id="6" xr3:uid="{00000000-0010-0000-0000-000006000000}" name="All hospitalized on certain day" dataDxfId="4"/>
-    <tableColumn id="7" xr3:uid="{00000000-0010-0000-0000-000007000000}" name="All persons in intensive care on certain day" dataDxfId="3"/>
-    <tableColumn id="10" xr3:uid="{00000000-0010-0000-0000-00000A000000}" name="Discharged" dataDxfId="2"/>
-    <tableColumn id="8" xr3:uid="{00000000-0010-0000-0000-000008000000}" name="Deaths (all)" dataDxfId="1"/>
-    <tableColumn id="9" xr3:uid="{00000000-0010-0000-0000-000009000000}" name="Deaths (daily)" dataDxfId="0"/>
+    <tableColumn id="1" name="Date" dataDxfId="9"/>
+    <tableColumn id="2" name="Tested (all)" dataDxfId="8"/>
+    <tableColumn id="3" name="Tested (daily)" dataDxfId="7"/>
+    <tableColumn id="4" name="Positive (all)" dataDxfId="6"/>
+    <tableColumn id="5" name="Positive (daily)" dataDxfId="5"/>
+    <tableColumn id="6" name="All hospitalized on certain day" dataDxfId="4"/>
+    <tableColumn id="7" name="All persons in intensive care on certain day" dataDxfId="3"/>
+    <tableColumn id="10" name="Discharged" dataDxfId="2"/>
+    <tableColumn id="8" name="Deaths (all)" dataDxfId="1"/>
+    <tableColumn id="9" name="Deaths (daily)" dataDxfId="0"/>
   </tableColumns>
   <tableStyleInfo name="TableStyleLight16" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
   <extLst>
@@ -695,11 +734,11 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:J75"/>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <dimension ref="A1:J90"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A40" zoomScale="89" zoomScaleNormal="89" workbookViewId="0">
-      <selection activeCell="J74" sqref="J74"/>
+    <sheetView tabSelected="1" topLeftCell="A65" zoomScale="89" zoomScaleNormal="89" workbookViewId="0">
+      <selection activeCell="E94" sqref="E94"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -3117,6 +3156,486 @@
         <v>0</v>
       </c>
     </row>
+    <row r="76" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A76" s="20">
+        <v>43976</v>
+      </c>
+      <c r="B76" s="21">
+        <v>75770</v>
+      </c>
+      <c r="C76" s="22">
+        <v>754</v>
+      </c>
+      <c r="D76" s="22">
+        <v>1469</v>
+      </c>
+      <c r="E76" s="22">
+        <v>0</v>
+      </c>
+      <c r="F76" s="22">
+        <v>9</v>
+      </c>
+      <c r="G76" s="22">
+        <v>2</v>
+      </c>
+      <c r="H76" s="22">
+        <v>6</v>
+      </c>
+      <c r="I76" s="22">
+        <v>108</v>
+      </c>
+      <c r="J76" s="22">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="77" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A77" s="20">
+        <v>43977</v>
+      </c>
+      <c r="B77" s="21">
+        <v>76579</v>
+      </c>
+      <c r="C77" s="22">
+        <v>809</v>
+      </c>
+      <c r="D77" s="22">
+        <v>1471</v>
+      </c>
+      <c r="E77" s="22">
+        <v>2</v>
+      </c>
+      <c r="F77" s="22">
+        <v>8</v>
+      </c>
+      <c r="G77" s="22">
+        <v>2</v>
+      </c>
+      <c r="H77" s="22">
+        <v>2</v>
+      </c>
+      <c r="I77" s="22">
+        <v>108</v>
+      </c>
+      <c r="J77" s="22">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="78" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A78" s="20">
+        <v>43978</v>
+      </c>
+      <c r="B78" s="21">
+        <v>77210</v>
+      </c>
+      <c r="C78" s="22">
+        <v>631</v>
+      </c>
+      <c r="D78" s="22">
+        <v>1473</v>
+      </c>
+      <c r="E78" s="22">
+        <v>2</v>
+      </c>
+      <c r="F78" s="22">
+        <v>7</v>
+      </c>
+      <c r="G78" s="22">
+        <v>2</v>
+      </c>
+      <c r="H78" s="22">
+        <v>1</v>
+      </c>
+      <c r="I78" s="22">
+        <v>108</v>
+      </c>
+      <c r="J78" s="22">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="79" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A79" s="20">
+        <v>43979</v>
+      </c>
+      <c r="B79" s="21">
+        <v>77916</v>
+      </c>
+      <c r="C79" s="22">
+        <v>706</v>
+      </c>
+      <c r="D79" s="22">
+        <v>1473</v>
+      </c>
+      <c r="E79" s="22">
+        <v>0</v>
+      </c>
+      <c r="F79" s="22">
+        <v>7</v>
+      </c>
+      <c r="G79" s="22">
+        <v>2</v>
+      </c>
+      <c r="H79" s="22">
+        <v>0</v>
+      </c>
+      <c r="I79" s="22">
+        <v>108</v>
+      </c>
+      <c r="J79" s="22">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="80" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A80" s="20">
+        <v>43980</v>
+      </c>
+      <c r="B80" s="21">
+        <v>78529</v>
+      </c>
+      <c r="C80" s="22">
+        <v>613</v>
+      </c>
+      <c r="D80" s="22">
+        <v>1473</v>
+      </c>
+      <c r="E80" s="22">
+        <v>0</v>
+      </c>
+      <c r="F80" s="22">
+        <v>7</v>
+      </c>
+      <c r="G80" s="22">
+        <v>2</v>
+      </c>
+      <c r="H80" s="22">
+        <v>0</v>
+      </c>
+      <c r="I80" s="22">
+        <v>108</v>
+      </c>
+      <c r="J80" s="22">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="81" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A81" s="20">
+        <v>43981</v>
+      </c>
+      <c r="B81" s="22">
+        <v>78793</v>
+      </c>
+      <c r="C81" s="22">
+        <v>264</v>
+      </c>
+      <c r="D81" s="22">
+        <v>1473</v>
+      </c>
+      <c r="E81" s="22">
+        <v>0</v>
+      </c>
+      <c r="F81" s="22">
+        <v>6</v>
+      </c>
+      <c r="G81" s="22">
+        <v>2</v>
+      </c>
+      <c r="H81" s="22">
+        <v>1</v>
+      </c>
+      <c r="I81" s="22">
+        <v>108</v>
+      </c>
+      <c r="J81" s="22">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="82" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A82" s="20">
+        <v>43982</v>
+      </c>
+      <c r="B82" s="21">
+        <v>79039</v>
+      </c>
+      <c r="C82" s="22">
+        <v>246</v>
+      </c>
+      <c r="D82" s="22">
+        <v>1473</v>
+      </c>
+      <c r="E82" s="22">
+        <v>0</v>
+      </c>
+      <c r="F82" s="22">
+        <v>5</v>
+      </c>
+      <c r="G82" s="22">
+        <v>1</v>
+      </c>
+      <c r="H82" s="22">
+        <v>0</v>
+      </c>
+      <c r="I82" s="22">
+        <v>109</v>
+      </c>
+      <c r="J82" s="22">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="83" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A83" s="20">
+        <v>43983</v>
+      </c>
+      <c r="B83" s="21">
+        <v>79698</v>
+      </c>
+      <c r="C83" s="22">
+        <v>659</v>
+      </c>
+      <c r="D83" s="22">
+        <v>1475</v>
+      </c>
+      <c r="E83" s="22">
+        <v>2</v>
+      </c>
+      <c r="F83" s="22">
+        <v>5</v>
+      </c>
+      <c r="G83" s="22">
+        <v>1</v>
+      </c>
+      <c r="H83" s="22">
+        <v>0</v>
+      </c>
+      <c r="I83" s="22">
+        <v>109</v>
+      </c>
+      <c r="J83" s="22">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="84" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A84" s="20">
+        <v>43984</v>
+      </c>
+      <c r="B84" s="21">
+        <v>80505</v>
+      </c>
+      <c r="C84" s="22">
+        <v>807</v>
+      </c>
+      <c r="D84" s="22">
+        <v>1477</v>
+      </c>
+      <c r="E84" s="22">
+        <v>2</v>
+      </c>
+      <c r="F84" s="22">
+        <v>5</v>
+      </c>
+      <c r="G84" s="22">
+        <v>0</v>
+      </c>
+      <c r="H84" s="22">
+        <v>0</v>
+      </c>
+      <c r="I84" s="22">
+        <v>109</v>
+      </c>
+      <c r="J84" s="22">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="85" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A85" s="20">
+        <v>43985</v>
+      </c>
+      <c r="B85" s="21">
+        <v>81333</v>
+      </c>
+      <c r="C85" s="22">
+        <v>828</v>
+      </c>
+      <c r="D85" s="22">
+        <v>1477</v>
+      </c>
+      <c r="E85" s="22">
+        <v>0</v>
+      </c>
+      <c r="F85" s="22">
+        <v>5</v>
+      </c>
+      <c r="G85" s="22">
+        <v>0</v>
+      </c>
+      <c r="H85" s="22">
+        <v>0</v>
+      </c>
+      <c r="I85" s="22">
+        <v>109</v>
+      </c>
+      <c r="J85" s="22">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="86" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A86" s="26">
+        <v>43986</v>
+      </c>
+      <c r="B86" s="27">
+        <v>82161</v>
+      </c>
+      <c r="C86" s="28">
+        <v>828</v>
+      </c>
+      <c r="D86" s="28">
+        <v>1479</v>
+      </c>
+      <c r="E86" s="28">
+        <v>2</v>
+      </c>
+      <c r="F86" s="28">
+        <v>6</v>
+      </c>
+      <c r="G86" s="28">
+        <v>0</v>
+      </c>
+      <c r="H86" s="28">
+        <v>0</v>
+      </c>
+      <c r="I86" s="28">
+        <v>109</v>
+      </c>
+      <c r="J86" s="28">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="87" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A87" s="29">
+        <v>43987</v>
+      </c>
+      <c r="B87" s="30">
+        <v>82876</v>
+      </c>
+      <c r="C87" s="31">
+        <v>715</v>
+      </c>
+      <c r="D87" s="31">
+        <v>1484</v>
+      </c>
+      <c r="E87" s="31">
+        <v>5</v>
+      </c>
+      <c r="F87" s="31">
+        <v>6</v>
+      </c>
+      <c r="G87" s="31">
+        <v>0</v>
+      </c>
+      <c r="H87" s="31">
+        <v>0</v>
+      </c>
+      <c r="I87" s="31">
+        <v>109</v>
+      </c>
+      <c r="J87" s="31">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="88" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A88" s="23">
+        <v>43988</v>
+      </c>
+      <c r="B88" s="24">
+        <v>83105</v>
+      </c>
+      <c r="C88" s="25">
+        <v>229</v>
+      </c>
+      <c r="D88" s="25">
+        <v>1485</v>
+      </c>
+      <c r="E88" s="25">
+        <v>1</v>
+      </c>
+      <c r="F88" s="25">
+        <v>5</v>
+      </c>
+      <c r="G88" s="25">
+        <v>0</v>
+      </c>
+      <c r="H88" s="25">
+        <v>1</v>
+      </c>
+      <c r="I88" s="25">
+        <v>109</v>
+      </c>
+      <c r="J88" s="25">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="89" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A89" s="29">
+        <v>43989</v>
+      </c>
+      <c r="B89" s="30">
+        <v>83316</v>
+      </c>
+      <c r="C89" s="31">
+        <v>211</v>
+      </c>
+      <c r="D89" s="31">
+        <v>1485</v>
+      </c>
+      <c r="E89" s="31">
+        <v>0</v>
+      </c>
+      <c r="F89" s="31">
+        <v>5</v>
+      </c>
+      <c r="G89" s="31">
+        <v>0</v>
+      </c>
+      <c r="H89" s="31">
+        <v>0</v>
+      </c>
+      <c r="I89" s="31">
+        <v>109</v>
+      </c>
+      <c r="J89" s="31">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="90" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A90" s="20">
+        <v>43990</v>
+      </c>
+      <c r="B90" s="21">
+        <v>84130</v>
+      </c>
+      <c r="C90" s="22">
+        <v>814</v>
+      </c>
+      <c r="D90" s="22">
+        <v>1486</v>
+      </c>
+      <c r="E90" s="22">
+        <v>1</v>
+      </c>
+      <c r="F90" s="22">
+        <v>6</v>
+      </c>
+      <c r="G90" s="22">
+        <v>0</v>
+      </c>
+      <c r="H90" s="22">
+        <v>0</v>
+      </c>
+      <c r="I90" s="22">
+        <v>109</v>
+      </c>
+      <c r="J90" s="22">
+        <v>0</v>
+      </c>
+    </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>

</xml_diff>

<commit_message>
Data updated by GitHub Bot (2020-06-10 12)
</commit_message>
<xml_diff>
--- a/output/snapshot/fdcf2531-4c3e-5c02-b63c-ee160ead6dea.xlsx
+++ b/output/snapshot/fdcf2531-4c3e-5c02-b63c-ee160ead6dea.xlsx
@@ -1,16 +1,15 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="21929"/>
-  <workbookPr/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
+  <fileVersion appName="xl" lastEdited="6" lowestEdited="6" rupBuild="14420"/>
+  <workbookPr defaultThemeVersion="164011"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="I:\AKTUALNI PODATKI - KORONA\Za objavo na GOV.SI\ang\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{1E6DD62F-2BE2-47DC-A7ED-9B57C1589256}" xr6:coauthVersionLast="44" xr6:coauthVersionMax="44" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840"/>
   </bookViews>
   <sheets>
     <sheet name="Covid-19 podatki" sheetId="1" r:id="rId1"/>
@@ -60,11 +59,11 @@
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" mc:Ignorable="x14ac x16r2">
   <numFmts count="1">
     <numFmt numFmtId="164" formatCode="d/\ m/\ yyyy;@"/>
   </numFmts>
-  <fonts count="4" x14ac:knownFonts="1">
+  <fonts count="5" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -93,6 +92,13 @@
       <name val="Calibri Light"/>
       <scheme val="major"/>
     </font>
+    <font>
+      <sz val="10"/>
+      <color theme="1"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
   </fonts>
   <fills count="3">
     <fill>
@@ -108,7 +114,7 @@
       </patternFill>
     </fill>
   </fills>
-  <borders count="2">
+  <borders count="3">
     <border>
       <left/>
       <right/>
@@ -129,11 +135,26 @@
       <bottom/>
       <diagonal/>
     </border>
+    <border>
+      <left style="thin">
+        <color theme="4"/>
+      </left>
+      <right style="thin">
+        <color theme="4"/>
+      </right>
+      <top style="thin">
+        <color theme="4"/>
+      </top>
+      <bottom style="thin">
+        <color theme="4"/>
+      </bottom>
+      <diagonal/>
+    </border>
   </borders>
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="26">
+  <cellXfs count="32">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="49" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyAlignment="1" applyProtection="1">
       <alignment horizontal="left" vertical="top"/>
@@ -208,6 +229,24 @@
       <alignment horizontal="right"/>
     </xf>
     <xf numFmtId="0" fontId="3" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="right"/>
+    </xf>
+    <xf numFmtId="164" fontId="4" fillId="2" borderId="2" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="right" vertical="top"/>
+    </xf>
+    <xf numFmtId="3" fontId="4" fillId="2" borderId="2" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="right"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="2" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="right"/>
+    </xf>
+    <xf numFmtId="164" fontId="3" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="right" vertical="top"/>
+    </xf>
+    <xf numFmtId="3" fontId="3" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="right"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="right"/>
     </xf>
   </cellXfs>
@@ -399,8 +438,8 @@
 </file>
 
 <file path=xl/tables/table1.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="1" xr:uid="{00000000-000C-0000-FFFF-FFFF00000000}" name="Tabela1" displayName="Tabela1" ref="A1:J75" totalsRowShown="0" headerRowDxfId="11" dataDxfId="10">
-  <autoFilter ref="A1:J75" xr:uid="{00000000-0009-0000-0100-000001000000}">
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="1" name="Tabela1" displayName="Tabela1" ref="A1:J91" totalsRowShown="0" headerRowDxfId="11" dataDxfId="10">
+  <autoFilter ref="A1:J91">
     <filterColumn colId="0" hiddenButton="1"/>
     <filterColumn colId="1" hiddenButton="1"/>
     <filterColumn colId="2" hiddenButton="1"/>
@@ -413,16 +452,16 @@
     <filterColumn colId="9" hiddenButton="1"/>
   </autoFilter>
   <tableColumns count="10">
-    <tableColumn id="1" xr3:uid="{00000000-0010-0000-0000-000001000000}" name="Date" dataDxfId="9"/>
-    <tableColumn id="2" xr3:uid="{00000000-0010-0000-0000-000002000000}" name="Tested (all)" dataDxfId="8"/>
-    <tableColumn id="3" xr3:uid="{00000000-0010-0000-0000-000003000000}" name="Tested (daily)" dataDxfId="7"/>
-    <tableColumn id="4" xr3:uid="{00000000-0010-0000-0000-000004000000}" name="Positive (all)" dataDxfId="6"/>
-    <tableColumn id="5" xr3:uid="{00000000-0010-0000-0000-000005000000}" name="Positive (daily)" dataDxfId="5"/>
-    <tableColumn id="6" xr3:uid="{00000000-0010-0000-0000-000006000000}" name="All hospitalized on certain day" dataDxfId="4"/>
-    <tableColumn id="7" xr3:uid="{00000000-0010-0000-0000-000007000000}" name="All persons in intensive care on certain day" dataDxfId="3"/>
-    <tableColumn id="10" xr3:uid="{00000000-0010-0000-0000-00000A000000}" name="Discharged" dataDxfId="2"/>
-    <tableColumn id="8" xr3:uid="{00000000-0010-0000-0000-000008000000}" name="Deaths (all)" dataDxfId="1"/>
-    <tableColumn id="9" xr3:uid="{00000000-0010-0000-0000-000009000000}" name="Deaths (daily)" dataDxfId="0"/>
+    <tableColumn id="1" name="Date" dataDxfId="9"/>
+    <tableColumn id="2" name="Tested (all)" dataDxfId="8"/>
+    <tableColumn id="3" name="Tested (daily)" dataDxfId="7"/>
+    <tableColumn id="4" name="Positive (all)" dataDxfId="6"/>
+    <tableColumn id="5" name="Positive (daily)" dataDxfId="5"/>
+    <tableColumn id="6" name="All hospitalized on certain day" dataDxfId="4"/>
+    <tableColumn id="7" name="All persons in intensive care on certain day" dataDxfId="3"/>
+    <tableColumn id="10" name="Discharged" dataDxfId="2"/>
+    <tableColumn id="8" name="Deaths (all)" dataDxfId="1"/>
+    <tableColumn id="9" name="Deaths (daily)" dataDxfId="0"/>
   </tableColumns>
   <tableStyleInfo name="TableStyleLight16" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
   <extLst>
@@ -695,11 +734,11 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:J75"/>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <dimension ref="A1:J91"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A40" zoomScale="89" zoomScaleNormal="89" workbookViewId="0">
-      <selection activeCell="J74" sqref="J74"/>
+    <sheetView tabSelected="1" topLeftCell="A65" zoomScale="89" zoomScaleNormal="89" workbookViewId="0">
+      <selection activeCell="J91" sqref="A91:J91"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -3117,6 +3156,518 @@
         <v>0</v>
       </c>
     </row>
+    <row r="76" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A76" s="20">
+        <v>43976</v>
+      </c>
+      <c r="B76" s="21">
+        <v>75770</v>
+      </c>
+      <c r="C76" s="22">
+        <v>754</v>
+      </c>
+      <c r="D76" s="22">
+        <v>1469</v>
+      </c>
+      <c r="E76" s="22">
+        <v>0</v>
+      </c>
+      <c r="F76" s="22">
+        <v>9</v>
+      </c>
+      <c r="G76" s="22">
+        <v>2</v>
+      </c>
+      <c r="H76" s="22">
+        <v>6</v>
+      </c>
+      <c r="I76" s="22">
+        <v>108</v>
+      </c>
+      <c r="J76" s="22">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="77" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A77" s="20">
+        <v>43977</v>
+      </c>
+      <c r="B77" s="21">
+        <v>76579</v>
+      </c>
+      <c r="C77" s="22">
+        <v>809</v>
+      </c>
+      <c r="D77" s="22">
+        <v>1471</v>
+      </c>
+      <c r="E77" s="22">
+        <v>2</v>
+      </c>
+      <c r="F77" s="22">
+        <v>8</v>
+      </c>
+      <c r="G77" s="22">
+        <v>2</v>
+      </c>
+      <c r="H77" s="22">
+        <v>2</v>
+      </c>
+      <c r="I77" s="22">
+        <v>108</v>
+      </c>
+      <c r="J77" s="22">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="78" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A78" s="20">
+        <v>43978</v>
+      </c>
+      <c r="B78" s="21">
+        <v>77210</v>
+      </c>
+      <c r="C78" s="22">
+        <v>631</v>
+      </c>
+      <c r="D78" s="22">
+        <v>1473</v>
+      </c>
+      <c r="E78" s="22">
+        <v>2</v>
+      </c>
+      <c r="F78" s="22">
+        <v>7</v>
+      </c>
+      <c r="G78" s="22">
+        <v>2</v>
+      </c>
+      <c r="H78" s="22">
+        <v>1</v>
+      </c>
+      <c r="I78" s="22">
+        <v>108</v>
+      </c>
+      <c r="J78" s="22">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="79" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A79" s="20">
+        <v>43979</v>
+      </c>
+      <c r="B79" s="21">
+        <v>77916</v>
+      </c>
+      <c r="C79" s="22">
+        <v>706</v>
+      </c>
+      <c r="D79" s="22">
+        <v>1473</v>
+      </c>
+      <c r="E79" s="22">
+        <v>0</v>
+      </c>
+      <c r="F79" s="22">
+        <v>7</v>
+      </c>
+      <c r="G79" s="22">
+        <v>2</v>
+      </c>
+      <c r="H79" s="22">
+        <v>0</v>
+      </c>
+      <c r="I79" s="22">
+        <v>108</v>
+      </c>
+      <c r="J79" s="22">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="80" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A80" s="20">
+        <v>43980</v>
+      </c>
+      <c r="B80" s="21">
+        <v>78529</v>
+      </c>
+      <c r="C80" s="22">
+        <v>613</v>
+      </c>
+      <c r="D80" s="22">
+        <v>1473</v>
+      </c>
+      <c r="E80" s="22">
+        <v>0</v>
+      </c>
+      <c r="F80" s="22">
+        <v>7</v>
+      </c>
+      <c r="G80" s="22">
+        <v>2</v>
+      </c>
+      <c r="H80" s="22">
+        <v>0</v>
+      </c>
+      <c r="I80" s="22">
+        <v>108</v>
+      </c>
+      <c r="J80" s="22">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="81" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A81" s="20">
+        <v>43981</v>
+      </c>
+      <c r="B81" s="22">
+        <v>78793</v>
+      </c>
+      <c r="C81" s="22">
+        <v>264</v>
+      </c>
+      <c r="D81" s="22">
+        <v>1473</v>
+      </c>
+      <c r="E81" s="22">
+        <v>0</v>
+      </c>
+      <c r="F81" s="22">
+        <v>6</v>
+      </c>
+      <c r="G81" s="22">
+        <v>2</v>
+      </c>
+      <c r="H81" s="22">
+        <v>1</v>
+      </c>
+      <c r="I81" s="22">
+        <v>108</v>
+      </c>
+      <c r="J81" s="22">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="82" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A82" s="20">
+        <v>43982</v>
+      </c>
+      <c r="B82" s="21">
+        <v>79039</v>
+      </c>
+      <c r="C82" s="22">
+        <v>246</v>
+      </c>
+      <c r="D82" s="22">
+        <v>1473</v>
+      </c>
+      <c r="E82" s="22">
+        <v>0</v>
+      </c>
+      <c r="F82" s="22">
+        <v>5</v>
+      </c>
+      <c r="G82" s="22">
+        <v>1</v>
+      </c>
+      <c r="H82" s="22">
+        <v>0</v>
+      </c>
+      <c r="I82" s="22">
+        <v>109</v>
+      </c>
+      <c r="J82" s="22">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="83" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A83" s="20">
+        <v>43983</v>
+      </c>
+      <c r="B83" s="21">
+        <v>79698</v>
+      </c>
+      <c r="C83" s="22">
+        <v>659</v>
+      </c>
+      <c r="D83" s="22">
+        <v>1475</v>
+      </c>
+      <c r="E83" s="22">
+        <v>2</v>
+      </c>
+      <c r="F83" s="22">
+        <v>5</v>
+      </c>
+      <c r="G83" s="22">
+        <v>1</v>
+      </c>
+      <c r="H83" s="22">
+        <v>0</v>
+      </c>
+      <c r="I83" s="22">
+        <v>109</v>
+      </c>
+      <c r="J83" s="22">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="84" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A84" s="20">
+        <v>43984</v>
+      </c>
+      <c r="B84" s="21">
+        <v>80505</v>
+      </c>
+      <c r="C84" s="22">
+        <v>807</v>
+      </c>
+      <c r="D84" s="22">
+        <v>1477</v>
+      </c>
+      <c r="E84" s="22">
+        <v>2</v>
+      </c>
+      <c r="F84" s="22">
+        <v>5</v>
+      </c>
+      <c r="G84" s="22">
+        <v>0</v>
+      </c>
+      <c r="H84" s="22">
+        <v>0</v>
+      </c>
+      <c r="I84" s="22">
+        <v>109</v>
+      </c>
+      <c r="J84" s="22">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="85" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A85" s="20">
+        <v>43985</v>
+      </c>
+      <c r="B85" s="21">
+        <v>81333</v>
+      </c>
+      <c r="C85" s="22">
+        <v>828</v>
+      </c>
+      <c r="D85" s="22">
+        <v>1477</v>
+      </c>
+      <c r="E85" s="22">
+        <v>0</v>
+      </c>
+      <c r="F85" s="22">
+        <v>5</v>
+      </c>
+      <c r="G85" s="22">
+        <v>0</v>
+      </c>
+      <c r="H85" s="22">
+        <v>0</v>
+      </c>
+      <c r="I85" s="22">
+        <v>109</v>
+      </c>
+      <c r="J85" s="22">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="86" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A86" s="26">
+        <v>43986</v>
+      </c>
+      <c r="B86" s="27">
+        <v>82161</v>
+      </c>
+      <c r="C86" s="28">
+        <v>828</v>
+      </c>
+      <c r="D86" s="28">
+        <v>1479</v>
+      </c>
+      <c r="E86" s="28">
+        <v>2</v>
+      </c>
+      <c r="F86" s="28">
+        <v>6</v>
+      </c>
+      <c r="G86" s="28">
+        <v>0</v>
+      </c>
+      <c r="H86" s="28">
+        <v>0</v>
+      </c>
+      <c r="I86" s="28">
+        <v>109</v>
+      </c>
+      <c r="J86" s="28">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="87" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A87" s="29">
+        <v>43987</v>
+      </c>
+      <c r="B87" s="30">
+        <v>82876</v>
+      </c>
+      <c r="C87" s="31">
+        <v>715</v>
+      </c>
+      <c r="D87" s="31">
+        <v>1484</v>
+      </c>
+      <c r="E87" s="31">
+        <v>5</v>
+      </c>
+      <c r="F87" s="31">
+        <v>6</v>
+      </c>
+      <c r="G87" s="31">
+        <v>0</v>
+      </c>
+      <c r="H87" s="31">
+        <v>0</v>
+      </c>
+      <c r="I87" s="31">
+        <v>109</v>
+      </c>
+      <c r="J87" s="31">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="88" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A88" s="23">
+        <v>43988</v>
+      </c>
+      <c r="B88" s="24">
+        <v>83105</v>
+      </c>
+      <c r="C88" s="25">
+        <v>229</v>
+      </c>
+      <c r="D88" s="25">
+        <v>1485</v>
+      </c>
+      <c r="E88" s="25">
+        <v>1</v>
+      </c>
+      <c r="F88" s="25">
+        <v>5</v>
+      </c>
+      <c r="G88" s="25">
+        <v>0</v>
+      </c>
+      <c r="H88" s="25">
+        <v>1</v>
+      </c>
+      <c r="I88" s="25">
+        <v>109</v>
+      </c>
+      <c r="J88" s="25">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="89" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A89" s="29">
+        <v>43989</v>
+      </c>
+      <c r="B89" s="30">
+        <v>83316</v>
+      </c>
+      <c r="C89" s="31">
+        <v>211</v>
+      </c>
+      <c r="D89" s="31">
+        <v>1485</v>
+      </c>
+      <c r="E89" s="31">
+        <v>0</v>
+      </c>
+      <c r="F89" s="31">
+        <v>5</v>
+      </c>
+      <c r="G89" s="31">
+        <v>0</v>
+      </c>
+      <c r="H89" s="31">
+        <v>0</v>
+      </c>
+      <c r="I89" s="31">
+        <v>109</v>
+      </c>
+      <c r="J89" s="31">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="90" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A90" s="20">
+        <v>43990</v>
+      </c>
+      <c r="B90" s="21">
+        <v>84130</v>
+      </c>
+      <c r="C90" s="22">
+        <v>814</v>
+      </c>
+      <c r="D90" s="22">
+        <v>1486</v>
+      </c>
+      <c r="E90" s="22">
+        <v>1</v>
+      </c>
+      <c r="F90" s="22">
+        <v>6</v>
+      </c>
+      <c r="G90" s="22">
+        <v>0</v>
+      </c>
+      <c r="H90" s="22">
+        <v>0</v>
+      </c>
+      <c r="I90" s="22">
+        <v>109</v>
+      </c>
+      <c r="J90" s="22">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="91" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A91" s="20">
+        <v>43991</v>
+      </c>
+      <c r="B91" s="21">
+        <v>84868</v>
+      </c>
+      <c r="C91" s="22">
+        <v>738</v>
+      </c>
+      <c r="D91" s="22">
+        <v>1488</v>
+      </c>
+      <c r="E91" s="22">
+        <v>2</v>
+      </c>
+      <c r="F91" s="22">
+        <v>6</v>
+      </c>
+      <c r="G91" s="22">
+        <v>0</v>
+      </c>
+      <c r="H91" s="22">
+        <v>0</v>
+      </c>
+      <c r="I91" s="22">
+        <v>109</v>
+      </c>
+      <c r="J91" s="22">
+        <v>0</v>
+      </c>
+    </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>

</xml_diff>

<commit_message>
Data updated by GitHub Bot (2020-06-10 20)
</commit_message>
<xml_diff>
--- a/output/snapshot/fdcf2531-4c3e-5c02-b63c-ee160ead6dea.xlsx
+++ b/output/snapshot/fdcf2531-4c3e-5c02-b63c-ee160ead6dea.xlsx
@@ -1,16 +1,15 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="21929"/>
-  <workbookPr/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
+  <fileVersion appName="xl" lastEdited="6" lowestEdited="6" rupBuild="14420"/>
+  <workbookPr defaultThemeVersion="164011"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="I:\AKTUALNI PODATKI - KORONA\Za objavo na GOV.SI\ang\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{1E6DD62F-2BE2-47DC-A7ED-9B57C1589256}" xr6:coauthVersionLast="44" xr6:coauthVersionMax="44" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840"/>
   </bookViews>
   <sheets>
     <sheet name="Covid-19 podatki" sheetId="1" r:id="rId1"/>
@@ -60,11 +59,11 @@
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" mc:Ignorable="x14ac x16r2">
   <numFmts count="1">
     <numFmt numFmtId="164" formatCode="d/\ m/\ yyyy;@"/>
   </numFmts>
-  <fonts count="4" x14ac:knownFonts="1">
+  <fonts count="5" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -93,6 +92,13 @@
       <name val="Calibri Light"/>
       <scheme val="major"/>
     </font>
+    <font>
+      <sz val="10"/>
+      <color theme="1"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
   </fonts>
   <fills count="3">
     <fill>
@@ -108,7 +114,7 @@
       </patternFill>
     </fill>
   </fills>
-  <borders count="2">
+  <borders count="3">
     <border>
       <left/>
       <right/>
@@ -129,11 +135,26 @@
       <bottom/>
       <diagonal/>
     </border>
+    <border>
+      <left style="thin">
+        <color theme="4"/>
+      </left>
+      <right style="thin">
+        <color theme="4"/>
+      </right>
+      <top style="thin">
+        <color theme="4"/>
+      </top>
+      <bottom style="thin">
+        <color theme="4"/>
+      </bottom>
+      <diagonal/>
+    </border>
   </borders>
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="26">
+  <cellXfs count="32">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="49" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyAlignment="1" applyProtection="1">
       <alignment horizontal="left" vertical="top"/>
@@ -208,6 +229,24 @@
       <alignment horizontal="right"/>
     </xf>
     <xf numFmtId="0" fontId="3" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="right"/>
+    </xf>
+    <xf numFmtId="164" fontId="4" fillId="2" borderId="2" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="right" vertical="top"/>
+    </xf>
+    <xf numFmtId="3" fontId="4" fillId="2" borderId="2" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="right"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="2" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="right"/>
+    </xf>
+    <xf numFmtId="164" fontId="3" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="right" vertical="top"/>
+    </xf>
+    <xf numFmtId="3" fontId="3" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="right"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="right"/>
     </xf>
   </cellXfs>
@@ -399,8 +438,8 @@
 </file>
 
 <file path=xl/tables/table1.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="1" xr:uid="{00000000-000C-0000-FFFF-FFFF00000000}" name="Tabela1" displayName="Tabela1" ref="A1:J75" totalsRowShown="0" headerRowDxfId="11" dataDxfId="10">
-  <autoFilter ref="A1:J75" xr:uid="{00000000-0009-0000-0100-000001000000}">
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="1" name="Tabela1" displayName="Tabela1" ref="A1:J91" totalsRowShown="0" headerRowDxfId="11" dataDxfId="10">
+  <autoFilter ref="A1:J91">
     <filterColumn colId="0" hiddenButton="1"/>
     <filterColumn colId="1" hiddenButton="1"/>
     <filterColumn colId="2" hiddenButton="1"/>
@@ -413,16 +452,16 @@
     <filterColumn colId="9" hiddenButton="1"/>
   </autoFilter>
   <tableColumns count="10">
-    <tableColumn id="1" xr3:uid="{00000000-0010-0000-0000-000001000000}" name="Date" dataDxfId="9"/>
-    <tableColumn id="2" xr3:uid="{00000000-0010-0000-0000-000002000000}" name="Tested (all)" dataDxfId="8"/>
-    <tableColumn id="3" xr3:uid="{00000000-0010-0000-0000-000003000000}" name="Tested (daily)" dataDxfId="7"/>
-    <tableColumn id="4" xr3:uid="{00000000-0010-0000-0000-000004000000}" name="Positive (all)" dataDxfId="6"/>
-    <tableColumn id="5" xr3:uid="{00000000-0010-0000-0000-000005000000}" name="Positive (daily)" dataDxfId="5"/>
-    <tableColumn id="6" xr3:uid="{00000000-0010-0000-0000-000006000000}" name="All hospitalized on certain day" dataDxfId="4"/>
-    <tableColumn id="7" xr3:uid="{00000000-0010-0000-0000-000007000000}" name="All persons in intensive care on certain day" dataDxfId="3"/>
-    <tableColumn id="10" xr3:uid="{00000000-0010-0000-0000-00000A000000}" name="Discharged" dataDxfId="2"/>
-    <tableColumn id="8" xr3:uid="{00000000-0010-0000-0000-000008000000}" name="Deaths (all)" dataDxfId="1"/>
-    <tableColumn id="9" xr3:uid="{00000000-0010-0000-0000-000009000000}" name="Deaths (daily)" dataDxfId="0"/>
+    <tableColumn id="1" name="Date" dataDxfId="9"/>
+    <tableColumn id="2" name="Tested (all)" dataDxfId="8"/>
+    <tableColumn id="3" name="Tested (daily)" dataDxfId="7"/>
+    <tableColumn id="4" name="Positive (all)" dataDxfId="6"/>
+    <tableColumn id="5" name="Positive (daily)" dataDxfId="5"/>
+    <tableColumn id="6" name="All hospitalized on certain day" dataDxfId="4"/>
+    <tableColumn id="7" name="All persons in intensive care on certain day" dataDxfId="3"/>
+    <tableColumn id="10" name="Discharged" dataDxfId="2"/>
+    <tableColumn id="8" name="Deaths (all)" dataDxfId="1"/>
+    <tableColumn id="9" name="Deaths (daily)" dataDxfId="0"/>
   </tableColumns>
   <tableStyleInfo name="TableStyleLight16" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
   <extLst>
@@ -695,11 +734,11 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:J75"/>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <dimension ref="A1:J91"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A40" zoomScale="89" zoomScaleNormal="89" workbookViewId="0">
-      <selection activeCell="J74" sqref="J74"/>
+    <sheetView tabSelected="1" topLeftCell="A65" zoomScale="89" zoomScaleNormal="89" workbookViewId="0">
+      <selection activeCell="J91" sqref="A91:J91"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -3117,6 +3156,518 @@
         <v>0</v>
       </c>
     </row>
+    <row r="76" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A76" s="20">
+        <v>43976</v>
+      </c>
+      <c r="B76" s="21">
+        <v>75770</v>
+      </c>
+      <c r="C76" s="22">
+        <v>754</v>
+      </c>
+      <c r="D76" s="22">
+        <v>1469</v>
+      </c>
+      <c r="E76" s="22">
+        <v>0</v>
+      </c>
+      <c r="F76" s="22">
+        <v>9</v>
+      </c>
+      <c r="G76" s="22">
+        <v>2</v>
+      </c>
+      <c r="H76" s="22">
+        <v>6</v>
+      </c>
+      <c r="I76" s="22">
+        <v>108</v>
+      </c>
+      <c r="J76" s="22">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="77" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A77" s="20">
+        <v>43977</v>
+      </c>
+      <c r="B77" s="21">
+        <v>76579</v>
+      </c>
+      <c r="C77" s="22">
+        <v>809</v>
+      </c>
+      <c r="D77" s="22">
+        <v>1471</v>
+      </c>
+      <c r="E77" s="22">
+        <v>2</v>
+      </c>
+      <c r="F77" s="22">
+        <v>8</v>
+      </c>
+      <c r="G77" s="22">
+        <v>2</v>
+      </c>
+      <c r="H77" s="22">
+        <v>2</v>
+      </c>
+      <c r="I77" s="22">
+        <v>108</v>
+      </c>
+      <c r="J77" s="22">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="78" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A78" s="20">
+        <v>43978</v>
+      </c>
+      <c r="B78" s="21">
+        <v>77210</v>
+      </c>
+      <c r="C78" s="22">
+        <v>631</v>
+      </c>
+      <c r="D78" s="22">
+        <v>1473</v>
+      </c>
+      <c r="E78" s="22">
+        <v>2</v>
+      </c>
+      <c r="F78" s="22">
+        <v>7</v>
+      </c>
+      <c r="G78" s="22">
+        <v>2</v>
+      </c>
+      <c r="H78" s="22">
+        <v>1</v>
+      </c>
+      <c r="I78" s="22">
+        <v>108</v>
+      </c>
+      <c r="J78" s="22">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="79" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A79" s="20">
+        <v>43979</v>
+      </c>
+      <c r="B79" s="21">
+        <v>77916</v>
+      </c>
+      <c r="C79" s="22">
+        <v>706</v>
+      </c>
+      <c r="D79" s="22">
+        <v>1473</v>
+      </c>
+      <c r="E79" s="22">
+        <v>0</v>
+      </c>
+      <c r="F79" s="22">
+        <v>7</v>
+      </c>
+      <c r="G79" s="22">
+        <v>2</v>
+      </c>
+      <c r="H79" s="22">
+        <v>0</v>
+      </c>
+      <c r="I79" s="22">
+        <v>108</v>
+      </c>
+      <c r="J79" s="22">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="80" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A80" s="20">
+        <v>43980</v>
+      </c>
+      <c r="B80" s="21">
+        <v>78529</v>
+      </c>
+      <c r="C80" s="22">
+        <v>613</v>
+      </c>
+      <c r="D80" s="22">
+        <v>1473</v>
+      </c>
+      <c r="E80" s="22">
+        <v>0</v>
+      </c>
+      <c r="F80" s="22">
+        <v>7</v>
+      </c>
+      <c r="G80" s="22">
+        <v>2</v>
+      </c>
+      <c r="H80" s="22">
+        <v>0</v>
+      </c>
+      <c r="I80" s="22">
+        <v>108</v>
+      </c>
+      <c r="J80" s="22">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="81" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A81" s="20">
+        <v>43981</v>
+      </c>
+      <c r="B81" s="22">
+        <v>78793</v>
+      </c>
+      <c r="C81" s="22">
+        <v>264</v>
+      </c>
+      <c r="D81" s="22">
+        <v>1473</v>
+      </c>
+      <c r="E81" s="22">
+        <v>0</v>
+      </c>
+      <c r="F81" s="22">
+        <v>6</v>
+      </c>
+      <c r="G81" s="22">
+        <v>2</v>
+      </c>
+      <c r="H81" s="22">
+        <v>1</v>
+      </c>
+      <c r="I81" s="22">
+        <v>108</v>
+      </c>
+      <c r="J81" s="22">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="82" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A82" s="20">
+        <v>43982</v>
+      </c>
+      <c r="B82" s="21">
+        <v>79039</v>
+      </c>
+      <c r="C82" s="22">
+        <v>246</v>
+      </c>
+      <c r="D82" s="22">
+        <v>1473</v>
+      </c>
+      <c r="E82" s="22">
+        <v>0</v>
+      </c>
+      <c r="F82" s="22">
+        <v>5</v>
+      </c>
+      <c r="G82" s="22">
+        <v>1</v>
+      </c>
+      <c r="H82" s="22">
+        <v>0</v>
+      </c>
+      <c r="I82" s="22">
+        <v>109</v>
+      </c>
+      <c r="J82" s="22">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="83" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A83" s="20">
+        <v>43983</v>
+      </c>
+      <c r="B83" s="21">
+        <v>79698</v>
+      </c>
+      <c r="C83" s="22">
+        <v>659</v>
+      </c>
+      <c r="D83" s="22">
+        <v>1475</v>
+      </c>
+      <c r="E83" s="22">
+        <v>2</v>
+      </c>
+      <c r="F83" s="22">
+        <v>5</v>
+      </c>
+      <c r="G83" s="22">
+        <v>1</v>
+      </c>
+      <c r="H83" s="22">
+        <v>0</v>
+      </c>
+      <c r="I83" s="22">
+        <v>109</v>
+      </c>
+      <c r="J83" s="22">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="84" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A84" s="20">
+        <v>43984</v>
+      </c>
+      <c r="B84" s="21">
+        <v>80505</v>
+      </c>
+      <c r="C84" s="22">
+        <v>807</v>
+      </c>
+      <c r="D84" s="22">
+        <v>1477</v>
+      </c>
+      <c r="E84" s="22">
+        <v>2</v>
+      </c>
+      <c r="F84" s="22">
+        <v>5</v>
+      </c>
+      <c r="G84" s="22">
+        <v>0</v>
+      </c>
+      <c r="H84" s="22">
+        <v>0</v>
+      </c>
+      <c r="I84" s="22">
+        <v>109</v>
+      </c>
+      <c r="J84" s="22">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="85" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A85" s="20">
+        <v>43985</v>
+      </c>
+      <c r="B85" s="21">
+        <v>81333</v>
+      </c>
+      <c r="C85" s="22">
+        <v>828</v>
+      </c>
+      <c r="D85" s="22">
+        <v>1477</v>
+      </c>
+      <c r="E85" s="22">
+        <v>0</v>
+      </c>
+      <c r="F85" s="22">
+        <v>5</v>
+      </c>
+      <c r="G85" s="22">
+        <v>0</v>
+      </c>
+      <c r="H85" s="22">
+        <v>0</v>
+      </c>
+      <c r="I85" s="22">
+        <v>109</v>
+      </c>
+      <c r="J85" s="22">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="86" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A86" s="26">
+        <v>43986</v>
+      </c>
+      <c r="B86" s="27">
+        <v>82161</v>
+      </c>
+      <c r="C86" s="28">
+        <v>828</v>
+      </c>
+      <c r="D86" s="28">
+        <v>1479</v>
+      </c>
+      <c r="E86" s="28">
+        <v>2</v>
+      </c>
+      <c r="F86" s="28">
+        <v>6</v>
+      </c>
+      <c r="G86" s="28">
+        <v>0</v>
+      </c>
+      <c r="H86" s="28">
+        <v>0</v>
+      </c>
+      <c r="I86" s="28">
+        <v>109</v>
+      </c>
+      <c r="J86" s="28">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="87" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A87" s="29">
+        <v>43987</v>
+      </c>
+      <c r="B87" s="30">
+        <v>82876</v>
+      </c>
+      <c r="C87" s="31">
+        <v>715</v>
+      </c>
+      <c r="D87" s="31">
+        <v>1484</v>
+      </c>
+      <c r="E87" s="31">
+        <v>5</v>
+      </c>
+      <c r="F87" s="31">
+        <v>6</v>
+      </c>
+      <c r="G87" s="31">
+        <v>0</v>
+      </c>
+      <c r="H87" s="31">
+        <v>0</v>
+      </c>
+      <c r="I87" s="31">
+        <v>109</v>
+      </c>
+      <c r="J87" s="31">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="88" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A88" s="23">
+        <v>43988</v>
+      </c>
+      <c r="B88" s="24">
+        <v>83105</v>
+      </c>
+      <c r="C88" s="25">
+        <v>229</v>
+      </c>
+      <c r="D88" s="25">
+        <v>1485</v>
+      </c>
+      <c r="E88" s="25">
+        <v>1</v>
+      </c>
+      <c r="F88" s="25">
+        <v>5</v>
+      </c>
+      <c r="G88" s="25">
+        <v>0</v>
+      </c>
+      <c r="H88" s="25">
+        <v>1</v>
+      </c>
+      <c r="I88" s="25">
+        <v>109</v>
+      </c>
+      <c r="J88" s="25">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="89" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A89" s="29">
+        <v>43989</v>
+      </c>
+      <c r="B89" s="30">
+        <v>83316</v>
+      </c>
+      <c r="C89" s="31">
+        <v>211</v>
+      </c>
+      <c r="D89" s="31">
+        <v>1485</v>
+      </c>
+      <c r="E89" s="31">
+        <v>0</v>
+      </c>
+      <c r="F89" s="31">
+        <v>5</v>
+      </c>
+      <c r="G89" s="31">
+        <v>0</v>
+      </c>
+      <c r="H89" s="31">
+        <v>0</v>
+      </c>
+      <c r="I89" s="31">
+        <v>109</v>
+      </c>
+      <c r="J89" s="31">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="90" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A90" s="20">
+        <v>43990</v>
+      </c>
+      <c r="B90" s="21">
+        <v>84130</v>
+      </c>
+      <c r="C90" s="22">
+        <v>814</v>
+      </c>
+      <c r="D90" s="22">
+        <v>1486</v>
+      </c>
+      <c r="E90" s="22">
+        <v>1</v>
+      </c>
+      <c r="F90" s="22">
+        <v>6</v>
+      </c>
+      <c r="G90" s="22">
+        <v>0</v>
+      </c>
+      <c r="H90" s="22">
+        <v>0</v>
+      </c>
+      <c r="I90" s="22">
+        <v>109</v>
+      </c>
+      <c r="J90" s="22">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="91" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A91" s="20">
+        <v>43991</v>
+      </c>
+      <c r="B91" s="21">
+        <v>84868</v>
+      </c>
+      <c r="C91" s="22">
+        <v>738</v>
+      </c>
+      <c r="D91" s="22">
+        <v>1488</v>
+      </c>
+      <c r="E91" s="22">
+        <v>2</v>
+      </c>
+      <c r="F91" s="22">
+        <v>6</v>
+      </c>
+      <c r="G91" s="22">
+        <v>0</v>
+      </c>
+      <c r="H91" s="22">
+        <v>0</v>
+      </c>
+      <c r="I91" s="22">
+        <v>109</v>
+      </c>
+      <c r="J91" s="22">
+        <v>0</v>
+      </c>
+    </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>

</xml_diff>

<commit_message>
Data updated by GitHub Bot (2020-06-11 12)
</commit_message>
<xml_diff>
--- a/output/snapshot/fdcf2531-4c3e-5c02-b63c-ee160ead6dea.xlsx
+++ b/output/snapshot/fdcf2531-4c3e-5c02-b63c-ee160ead6dea.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="I:\AKTUALNI PODATKI - KORONA\Za objavo na GOV.SI\ang\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{1E6DD62F-2BE2-47DC-A7ED-9B57C1589256}" xr6:coauthVersionLast="44" xr6:coauthVersionMax="44" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{833B8CD9-5160-40BE-99A5-1323DC10DF9B}" xr6:coauthVersionLast="44" xr6:coauthVersionMax="44" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -64,7 +64,7 @@
   <numFmts count="1">
     <numFmt numFmtId="164" formatCode="d/\ m/\ yyyy;@"/>
   </numFmts>
-  <fonts count="4" x14ac:knownFonts="1">
+  <fonts count="5" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -93,6 +93,13 @@
       <name val="Calibri Light"/>
       <scheme val="major"/>
     </font>
+    <font>
+      <sz val="10"/>
+      <color theme="1"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
   </fonts>
   <fills count="3">
     <fill>
@@ -108,7 +115,7 @@
       </patternFill>
     </fill>
   </fills>
-  <borders count="2">
+  <borders count="3">
     <border>
       <left/>
       <right/>
@@ -129,11 +136,26 @@
       <bottom/>
       <diagonal/>
     </border>
+    <border>
+      <left style="thin">
+        <color theme="4"/>
+      </left>
+      <right style="thin">
+        <color theme="4"/>
+      </right>
+      <top style="thin">
+        <color theme="4"/>
+      </top>
+      <bottom style="thin">
+        <color theme="4"/>
+      </bottom>
+      <diagonal/>
+    </border>
   </borders>
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="26">
+  <cellXfs count="32">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="49" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyAlignment="1" applyProtection="1">
       <alignment horizontal="left" vertical="top"/>
@@ -208,6 +230,24 @@
       <alignment horizontal="right"/>
     </xf>
     <xf numFmtId="0" fontId="3" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="right"/>
+    </xf>
+    <xf numFmtId="164" fontId="4" fillId="2" borderId="2" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="right" vertical="top"/>
+    </xf>
+    <xf numFmtId="3" fontId="4" fillId="2" borderId="2" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="right"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="2" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="right"/>
+    </xf>
+    <xf numFmtId="164" fontId="3" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="right" vertical="top"/>
+    </xf>
+    <xf numFmtId="3" fontId="3" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="right"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="right"/>
     </xf>
   </cellXfs>
@@ -399,8 +439,8 @@
 </file>
 
 <file path=xl/tables/table1.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="1" xr:uid="{00000000-000C-0000-FFFF-FFFF00000000}" name="Tabela1" displayName="Tabela1" ref="A1:J75" totalsRowShown="0" headerRowDxfId="11" dataDxfId="10">
-  <autoFilter ref="A1:J75" xr:uid="{00000000-0009-0000-0100-000001000000}">
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="1" xr:uid="{00000000-000C-0000-FFFF-FFFF00000000}" name="Tabela1" displayName="Tabela1" ref="A1:J92" totalsRowShown="0" headerRowDxfId="11" dataDxfId="10">
+  <autoFilter ref="A1:J92" xr:uid="{00000000-0009-0000-0100-000001000000}">
     <filterColumn colId="0" hiddenButton="1"/>
     <filterColumn colId="1" hiddenButton="1"/>
     <filterColumn colId="2" hiddenButton="1"/>
@@ -696,10 +736,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:J75"/>
+  <dimension ref="A1:J92"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A40" zoomScale="89" zoomScaleNormal="89" workbookViewId="0">
-      <selection activeCell="J74" sqref="J74"/>
+    <sheetView tabSelected="1" topLeftCell="A65" zoomScale="89" zoomScaleNormal="89" workbookViewId="0">
+      <selection activeCell="A92" sqref="A92:J92"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -3117,6 +3157,550 @@
         <v>0</v>
       </c>
     </row>
+    <row r="76" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A76" s="20">
+        <v>43976</v>
+      </c>
+      <c r="B76" s="21">
+        <v>75770</v>
+      </c>
+      <c r="C76" s="22">
+        <v>754</v>
+      </c>
+      <c r="D76" s="22">
+        <v>1469</v>
+      </c>
+      <c r="E76" s="22">
+        <v>0</v>
+      </c>
+      <c r="F76" s="22">
+        <v>9</v>
+      </c>
+      <c r="G76" s="22">
+        <v>2</v>
+      </c>
+      <c r="H76" s="22">
+        <v>6</v>
+      </c>
+      <c r="I76" s="22">
+        <v>108</v>
+      </c>
+      <c r="J76" s="22">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="77" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A77" s="20">
+        <v>43977</v>
+      </c>
+      <c r="B77" s="21">
+        <v>76579</v>
+      </c>
+      <c r="C77" s="22">
+        <v>809</v>
+      </c>
+      <c r="D77" s="22">
+        <v>1471</v>
+      </c>
+      <c r="E77" s="22">
+        <v>2</v>
+      </c>
+      <c r="F77" s="22">
+        <v>8</v>
+      </c>
+      <c r="G77" s="22">
+        <v>2</v>
+      </c>
+      <c r="H77" s="22">
+        <v>2</v>
+      </c>
+      <c r="I77" s="22">
+        <v>108</v>
+      </c>
+      <c r="J77" s="22">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="78" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A78" s="20">
+        <v>43978</v>
+      </c>
+      <c r="B78" s="21">
+        <v>77210</v>
+      </c>
+      <c r="C78" s="22">
+        <v>631</v>
+      </c>
+      <c r="D78" s="22">
+        <v>1473</v>
+      </c>
+      <c r="E78" s="22">
+        <v>2</v>
+      </c>
+      <c r="F78" s="22">
+        <v>7</v>
+      </c>
+      <c r="G78" s="22">
+        <v>2</v>
+      </c>
+      <c r="H78" s="22">
+        <v>1</v>
+      </c>
+      <c r="I78" s="22">
+        <v>108</v>
+      </c>
+      <c r="J78" s="22">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="79" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A79" s="20">
+        <v>43979</v>
+      </c>
+      <c r="B79" s="21">
+        <v>77916</v>
+      </c>
+      <c r="C79" s="22">
+        <v>706</v>
+      </c>
+      <c r="D79" s="22">
+        <v>1473</v>
+      </c>
+      <c r="E79" s="22">
+        <v>0</v>
+      </c>
+      <c r="F79" s="22">
+        <v>7</v>
+      </c>
+      <c r="G79" s="22">
+        <v>2</v>
+      </c>
+      <c r="H79" s="22">
+        <v>0</v>
+      </c>
+      <c r="I79" s="22">
+        <v>108</v>
+      </c>
+      <c r="J79" s="22">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="80" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A80" s="20">
+        <v>43980</v>
+      </c>
+      <c r="B80" s="21">
+        <v>78529</v>
+      </c>
+      <c r="C80" s="22">
+        <v>613</v>
+      </c>
+      <c r="D80" s="22">
+        <v>1473</v>
+      </c>
+      <c r="E80" s="22">
+        <v>0</v>
+      </c>
+      <c r="F80" s="22">
+        <v>7</v>
+      </c>
+      <c r="G80" s="22">
+        <v>2</v>
+      </c>
+      <c r="H80" s="22">
+        <v>0</v>
+      </c>
+      <c r="I80" s="22">
+        <v>108</v>
+      </c>
+      <c r="J80" s="22">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="81" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A81" s="20">
+        <v>43981</v>
+      </c>
+      <c r="B81" s="22">
+        <v>78793</v>
+      </c>
+      <c r="C81" s="22">
+        <v>264</v>
+      </c>
+      <c r="D81" s="22">
+        <v>1473</v>
+      </c>
+      <c r="E81" s="22">
+        <v>0</v>
+      </c>
+      <c r="F81" s="22">
+        <v>6</v>
+      </c>
+      <c r="G81" s="22">
+        <v>2</v>
+      </c>
+      <c r="H81" s="22">
+        <v>1</v>
+      </c>
+      <c r="I81" s="22">
+        <v>108</v>
+      </c>
+      <c r="J81" s="22">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="82" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A82" s="20">
+        <v>43982</v>
+      </c>
+      <c r="B82" s="21">
+        <v>79039</v>
+      </c>
+      <c r="C82" s="22">
+        <v>246</v>
+      </c>
+      <c r="D82" s="22">
+        <v>1473</v>
+      </c>
+      <c r="E82" s="22">
+        <v>0</v>
+      </c>
+      <c r="F82" s="22">
+        <v>5</v>
+      </c>
+      <c r="G82" s="22">
+        <v>1</v>
+      </c>
+      <c r="H82" s="22">
+        <v>0</v>
+      </c>
+      <c r="I82" s="22">
+        <v>109</v>
+      </c>
+      <c r="J82" s="22">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="83" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A83" s="20">
+        <v>43983</v>
+      </c>
+      <c r="B83" s="21">
+        <v>79698</v>
+      </c>
+      <c r="C83" s="22">
+        <v>659</v>
+      </c>
+      <c r="D83" s="22">
+        <v>1475</v>
+      </c>
+      <c r="E83" s="22">
+        <v>2</v>
+      </c>
+      <c r="F83" s="22">
+        <v>5</v>
+      </c>
+      <c r="G83" s="22">
+        <v>1</v>
+      </c>
+      <c r="H83" s="22">
+        <v>0</v>
+      </c>
+      <c r="I83" s="22">
+        <v>109</v>
+      </c>
+      <c r="J83" s="22">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="84" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A84" s="20">
+        <v>43984</v>
+      </c>
+      <c r="B84" s="21">
+        <v>80505</v>
+      </c>
+      <c r="C84" s="22">
+        <v>807</v>
+      </c>
+      <c r="D84" s="22">
+        <v>1477</v>
+      </c>
+      <c r="E84" s="22">
+        <v>2</v>
+      </c>
+      <c r="F84" s="22">
+        <v>5</v>
+      </c>
+      <c r="G84" s="22">
+        <v>0</v>
+      </c>
+      <c r="H84" s="22">
+        <v>0</v>
+      </c>
+      <c r="I84" s="22">
+        <v>109</v>
+      </c>
+      <c r="J84" s="22">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="85" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A85" s="20">
+        <v>43985</v>
+      </c>
+      <c r="B85" s="21">
+        <v>81333</v>
+      </c>
+      <c r="C85" s="22">
+        <v>828</v>
+      </c>
+      <c r="D85" s="22">
+        <v>1477</v>
+      </c>
+      <c r="E85" s="22">
+        <v>0</v>
+      </c>
+      <c r="F85" s="22">
+        <v>5</v>
+      </c>
+      <c r="G85" s="22">
+        <v>0</v>
+      </c>
+      <c r="H85" s="22">
+        <v>0</v>
+      </c>
+      <c r="I85" s="22">
+        <v>109</v>
+      </c>
+      <c r="J85" s="22">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="86" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A86" s="26">
+        <v>43986</v>
+      </c>
+      <c r="B86" s="27">
+        <v>82161</v>
+      </c>
+      <c r="C86" s="28">
+        <v>828</v>
+      </c>
+      <c r="D86" s="28">
+        <v>1479</v>
+      </c>
+      <c r="E86" s="28">
+        <v>2</v>
+      </c>
+      <c r="F86" s="28">
+        <v>6</v>
+      </c>
+      <c r="G86" s="28">
+        <v>0</v>
+      </c>
+      <c r="H86" s="28">
+        <v>0</v>
+      </c>
+      <c r="I86" s="28">
+        <v>109</v>
+      </c>
+      <c r="J86" s="28">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="87" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A87" s="29">
+        <v>43987</v>
+      </c>
+      <c r="B87" s="30">
+        <v>82876</v>
+      </c>
+      <c r="C87" s="31">
+        <v>715</v>
+      </c>
+      <c r="D87" s="31">
+        <v>1484</v>
+      </c>
+      <c r="E87" s="31">
+        <v>5</v>
+      </c>
+      <c r="F87" s="31">
+        <v>6</v>
+      </c>
+      <c r="G87" s="31">
+        <v>0</v>
+      </c>
+      <c r="H87" s="31">
+        <v>0</v>
+      </c>
+      <c r="I87" s="31">
+        <v>109</v>
+      </c>
+      <c r="J87" s="31">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="88" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A88" s="23">
+        <v>43988</v>
+      </c>
+      <c r="B88" s="24">
+        <v>83105</v>
+      </c>
+      <c r="C88" s="25">
+        <v>229</v>
+      </c>
+      <c r="D88" s="25">
+        <v>1485</v>
+      </c>
+      <c r="E88" s="25">
+        <v>1</v>
+      </c>
+      <c r="F88" s="25">
+        <v>5</v>
+      </c>
+      <c r="G88" s="25">
+        <v>0</v>
+      </c>
+      <c r="H88" s="25">
+        <v>1</v>
+      </c>
+      <c r="I88" s="25">
+        <v>109</v>
+      </c>
+      <c r="J88" s="25">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="89" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A89" s="29">
+        <v>43989</v>
+      </c>
+      <c r="B89" s="30">
+        <v>83316</v>
+      </c>
+      <c r="C89" s="31">
+        <v>211</v>
+      </c>
+      <c r="D89" s="31">
+        <v>1485</v>
+      </c>
+      <c r="E89" s="31">
+        <v>0</v>
+      </c>
+      <c r="F89" s="31">
+        <v>5</v>
+      </c>
+      <c r="G89" s="31">
+        <v>0</v>
+      </c>
+      <c r="H89" s="31">
+        <v>0</v>
+      </c>
+      <c r="I89" s="31">
+        <v>109</v>
+      </c>
+      <c r="J89" s="31">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="90" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A90" s="20">
+        <v>43990</v>
+      </c>
+      <c r="B90" s="21">
+        <v>84130</v>
+      </c>
+      <c r="C90" s="22">
+        <v>814</v>
+      </c>
+      <c r="D90" s="22">
+        <v>1486</v>
+      </c>
+      <c r="E90" s="22">
+        <v>1</v>
+      </c>
+      <c r="F90" s="22">
+        <v>6</v>
+      </c>
+      <c r="G90" s="22">
+        <v>0</v>
+      </c>
+      <c r="H90" s="22">
+        <v>0</v>
+      </c>
+      <c r="I90" s="22">
+        <v>109</v>
+      </c>
+      <c r="J90" s="22">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="91" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A91" s="20">
+        <v>43991</v>
+      </c>
+      <c r="B91" s="21">
+        <v>84868</v>
+      </c>
+      <c r="C91" s="22">
+        <v>738</v>
+      </c>
+      <c r="D91" s="22">
+        <v>1488</v>
+      </c>
+      <c r="E91" s="22">
+        <v>2</v>
+      </c>
+      <c r="F91" s="22">
+        <v>6</v>
+      </c>
+      <c r="G91" s="22">
+        <v>0</v>
+      </c>
+      <c r="H91" s="22">
+        <v>0</v>
+      </c>
+      <c r="I91" s="22">
+        <v>109</v>
+      </c>
+      <c r="J91" s="22">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="92" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A92" s="23">
+        <v>43992</v>
+      </c>
+      <c r="B92" s="24">
+        <v>85626</v>
+      </c>
+      <c r="C92" s="25">
+        <v>758</v>
+      </c>
+      <c r="D92" s="25">
+        <v>1488</v>
+      </c>
+      <c r="E92" s="25">
+        <v>0</v>
+      </c>
+      <c r="F92" s="25">
+        <v>6</v>
+      </c>
+      <c r="G92" s="25">
+        <v>0</v>
+      </c>
+      <c r="H92" s="25">
+        <v>0</v>
+      </c>
+      <c r="I92" s="25">
+        <v>109</v>
+      </c>
+      <c r="J92" s="25">
+        <v>0</v>
+      </c>
+    </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>

</xml_diff>

<commit_message>
Data updated by GitHub Bot (2020-06-11 20)
</commit_message>
<xml_diff>
--- a/output/snapshot/fdcf2531-4c3e-5c02-b63c-ee160ead6dea.xlsx
+++ b/output/snapshot/fdcf2531-4c3e-5c02-b63c-ee160ead6dea.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="I:\AKTUALNI PODATKI - KORONA\Za objavo na GOV.SI\ang\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{1E6DD62F-2BE2-47DC-A7ED-9B57C1589256}" xr6:coauthVersionLast="44" xr6:coauthVersionMax="44" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{833B8CD9-5160-40BE-99A5-1323DC10DF9B}" xr6:coauthVersionLast="44" xr6:coauthVersionMax="44" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -64,7 +64,7 @@
   <numFmts count="1">
     <numFmt numFmtId="164" formatCode="d/\ m/\ yyyy;@"/>
   </numFmts>
-  <fonts count="4" x14ac:knownFonts="1">
+  <fonts count="5" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -93,6 +93,13 @@
       <name val="Calibri Light"/>
       <scheme val="major"/>
     </font>
+    <font>
+      <sz val="10"/>
+      <color theme="1"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
   </fonts>
   <fills count="3">
     <fill>
@@ -108,7 +115,7 @@
       </patternFill>
     </fill>
   </fills>
-  <borders count="2">
+  <borders count="3">
     <border>
       <left/>
       <right/>
@@ -129,11 +136,26 @@
       <bottom/>
       <diagonal/>
     </border>
+    <border>
+      <left style="thin">
+        <color theme="4"/>
+      </left>
+      <right style="thin">
+        <color theme="4"/>
+      </right>
+      <top style="thin">
+        <color theme="4"/>
+      </top>
+      <bottom style="thin">
+        <color theme="4"/>
+      </bottom>
+      <diagonal/>
+    </border>
   </borders>
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="26">
+  <cellXfs count="32">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="49" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyAlignment="1" applyProtection="1">
       <alignment horizontal="left" vertical="top"/>
@@ -208,6 +230,24 @@
       <alignment horizontal="right"/>
     </xf>
     <xf numFmtId="0" fontId="3" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="right"/>
+    </xf>
+    <xf numFmtId="164" fontId="4" fillId="2" borderId="2" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="right" vertical="top"/>
+    </xf>
+    <xf numFmtId="3" fontId="4" fillId="2" borderId="2" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="right"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="2" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="right"/>
+    </xf>
+    <xf numFmtId="164" fontId="3" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="right" vertical="top"/>
+    </xf>
+    <xf numFmtId="3" fontId="3" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="right"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="right"/>
     </xf>
   </cellXfs>
@@ -399,8 +439,8 @@
 </file>
 
 <file path=xl/tables/table1.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="1" xr:uid="{00000000-000C-0000-FFFF-FFFF00000000}" name="Tabela1" displayName="Tabela1" ref="A1:J75" totalsRowShown="0" headerRowDxfId="11" dataDxfId="10">
-  <autoFilter ref="A1:J75" xr:uid="{00000000-0009-0000-0100-000001000000}">
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="1" xr:uid="{00000000-000C-0000-FFFF-FFFF00000000}" name="Tabela1" displayName="Tabela1" ref="A1:J92" totalsRowShown="0" headerRowDxfId="11" dataDxfId="10">
+  <autoFilter ref="A1:J92" xr:uid="{00000000-0009-0000-0100-000001000000}">
     <filterColumn colId="0" hiddenButton="1"/>
     <filterColumn colId="1" hiddenButton="1"/>
     <filterColumn colId="2" hiddenButton="1"/>
@@ -696,10 +736,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:J75"/>
+  <dimension ref="A1:J92"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A40" zoomScale="89" zoomScaleNormal="89" workbookViewId="0">
-      <selection activeCell="J74" sqref="J74"/>
+    <sheetView tabSelected="1" topLeftCell="A65" zoomScale="89" zoomScaleNormal="89" workbookViewId="0">
+      <selection activeCell="A92" sqref="A92:J92"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -3117,6 +3157,550 @@
         <v>0</v>
       </c>
     </row>
+    <row r="76" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A76" s="20">
+        <v>43976</v>
+      </c>
+      <c r="B76" s="21">
+        <v>75770</v>
+      </c>
+      <c r="C76" s="22">
+        <v>754</v>
+      </c>
+      <c r="D76" s="22">
+        <v>1469</v>
+      </c>
+      <c r="E76" s="22">
+        <v>0</v>
+      </c>
+      <c r="F76" s="22">
+        <v>9</v>
+      </c>
+      <c r="G76" s="22">
+        <v>2</v>
+      </c>
+      <c r="H76" s="22">
+        <v>6</v>
+      </c>
+      <c r="I76" s="22">
+        <v>108</v>
+      </c>
+      <c r="J76" s="22">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="77" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A77" s="20">
+        <v>43977</v>
+      </c>
+      <c r="B77" s="21">
+        <v>76579</v>
+      </c>
+      <c r="C77" s="22">
+        <v>809</v>
+      </c>
+      <c r="D77" s="22">
+        <v>1471</v>
+      </c>
+      <c r="E77" s="22">
+        <v>2</v>
+      </c>
+      <c r="F77" s="22">
+        <v>8</v>
+      </c>
+      <c r="G77" s="22">
+        <v>2</v>
+      </c>
+      <c r="H77" s="22">
+        <v>2</v>
+      </c>
+      <c r="I77" s="22">
+        <v>108</v>
+      </c>
+      <c r="J77" s="22">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="78" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A78" s="20">
+        <v>43978</v>
+      </c>
+      <c r="B78" s="21">
+        <v>77210</v>
+      </c>
+      <c r="C78" s="22">
+        <v>631</v>
+      </c>
+      <c r="D78" s="22">
+        <v>1473</v>
+      </c>
+      <c r="E78" s="22">
+        <v>2</v>
+      </c>
+      <c r="F78" s="22">
+        <v>7</v>
+      </c>
+      <c r="G78" s="22">
+        <v>2</v>
+      </c>
+      <c r="H78" s="22">
+        <v>1</v>
+      </c>
+      <c r="I78" s="22">
+        <v>108</v>
+      </c>
+      <c r="J78" s="22">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="79" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A79" s="20">
+        <v>43979</v>
+      </c>
+      <c r="B79" s="21">
+        <v>77916</v>
+      </c>
+      <c r="C79" s="22">
+        <v>706</v>
+      </c>
+      <c r="D79" s="22">
+        <v>1473</v>
+      </c>
+      <c r="E79" s="22">
+        <v>0</v>
+      </c>
+      <c r="F79" s="22">
+        <v>7</v>
+      </c>
+      <c r="G79" s="22">
+        <v>2</v>
+      </c>
+      <c r="H79" s="22">
+        <v>0</v>
+      </c>
+      <c r="I79" s="22">
+        <v>108</v>
+      </c>
+      <c r="J79" s="22">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="80" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A80" s="20">
+        <v>43980</v>
+      </c>
+      <c r="B80" s="21">
+        <v>78529</v>
+      </c>
+      <c r="C80" s="22">
+        <v>613</v>
+      </c>
+      <c r="D80" s="22">
+        <v>1473</v>
+      </c>
+      <c r="E80" s="22">
+        <v>0</v>
+      </c>
+      <c r="F80" s="22">
+        <v>7</v>
+      </c>
+      <c r="G80" s="22">
+        <v>2</v>
+      </c>
+      <c r="H80" s="22">
+        <v>0</v>
+      </c>
+      <c r="I80" s="22">
+        <v>108</v>
+      </c>
+      <c r="J80" s="22">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="81" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A81" s="20">
+        <v>43981</v>
+      </c>
+      <c r="B81" s="22">
+        <v>78793</v>
+      </c>
+      <c r="C81" s="22">
+        <v>264</v>
+      </c>
+      <c r="D81" s="22">
+        <v>1473</v>
+      </c>
+      <c r="E81" s="22">
+        <v>0</v>
+      </c>
+      <c r="F81" s="22">
+        <v>6</v>
+      </c>
+      <c r="G81" s="22">
+        <v>2</v>
+      </c>
+      <c r="H81" s="22">
+        <v>1</v>
+      </c>
+      <c r="I81" s="22">
+        <v>108</v>
+      </c>
+      <c r="J81" s="22">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="82" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A82" s="20">
+        <v>43982</v>
+      </c>
+      <c r="B82" s="21">
+        <v>79039</v>
+      </c>
+      <c r="C82" s="22">
+        <v>246</v>
+      </c>
+      <c r="D82" s="22">
+        <v>1473</v>
+      </c>
+      <c r="E82" s="22">
+        <v>0</v>
+      </c>
+      <c r="F82" s="22">
+        <v>5</v>
+      </c>
+      <c r="G82" s="22">
+        <v>1</v>
+      </c>
+      <c r="H82" s="22">
+        <v>0</v>
+      </c>
+      <c r="I82" s="22">
+        <v>109</v>
+      </c>
+      <c r="J82" s="22">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="83" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A83" s="20">
+        <v>43983</v>
+      </c>
+      <c r="B83" s="21">
+        <v>79698</v>
+      </c>
+      <c r="C83" s="22">
+        <v>659</v>
+      </c>
+      <c r="D83" s="22">
+        <v>1475</v>
+      </c>
+      <c r="E83" s="22">
+        <v>2</v>
+      </c>
+      <c r="F83" s="22">
+        <v>5</v>
+      </c>
+      <c r="G83" s="22">
+        <v>1</v>
+      </c>
+      <c r="H83" s="22">
+        <v>0</v>
+      </c>
+      <c r="I83" s="22">
+        <v>109</v>
+      </c>
+      <c r="J83" s="22">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="84" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A84" s="20">
+        <v>43984</v>
+      </c>
+      <c r="B84" s="21">
+        <v>80505</v>
+      </c>
+      <c r="C84" s="22">
+        <v>807</v>
+      </c>
+      <c r="D84" s="22">
+        <v>1477</v>
+      </c>
+      <c r="E84" s="22">
+        <v>2</v>
+      </c>
+      <c r="F84" s="22">
+        <v>5</v>
+      </c>
+      <c r="G84" s="22">
+        <v>0</v>
+      </c>
+      <c r="H84" s="22">
+        <v>0</v>
+      </c>
+      <c r="I84" s="22">
+        <v>109</v>
+      </c>
+      <c r="J84" s="22">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="85" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A85" s="20">
+        <v>43985</v>
+      </c>
+      <c r="B85" s="21">
+        <v>81333</v>
+      </c>
+      <c r="C85" s="22">
+        <v>828</v>
+      </c>
+      <c r="D85" s="22">
+        <v>1477</v>
+      </c>
+      <c r="E85" s="22">
+        <v>0</v>
+      </c>
+      <c r="F85" s="22">
+        <v>5</v>
+      </c>
+      <c r="G85" s="22">
+        <v>0</v>
+      </c>
+      <c r="H85" s="22">
+        <v>0</v>
+      </c>
+      <c r="I85" s="22">
+        <v>109</v>
+      </c>
+      <c r="J85" s="22">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="86" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A86" s="26">
+        <v>43986</v>
+      </c>
+      <c r="B86" s="27">
+        <v>82161</v>
+      </c>
+      <c r="C86" s="28">
+        <v>828</v>
+      </c>
+      <c r="D86" s="28">
+        <v>1479</v>
+      </c>
+      <c r="E86" s="28">
+        <v>2</v>
+      </c>
+      <c r="F86" s="28">
+        <v>6</v>
+      </c>
+      <c r="G86" s="28">
+        <v>0</v>
+      </c>
+      <c r="H86" s="28">
+        <v>0</v>
+      </c>
+      <c r="I86" s="28">
+        <v>109</v>
+      </c>
+      <c r="J86" s="28">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="87" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A87" s="29">
+        <v>43987</v>
+      </c>
+      <c r="B87" s="30">
+        <v>82876</v>
+      </c>
+      <c r="C87" s="31">
+        <v>715</v>
+      </c>
+      <c r="D87" s="31">
+        <v>1484</v>
+      </c>
+      <c r="E87" s="31">
+        <v>5</v>
+      </c>
+      <c r="F87" s="31">
+        <v>6</v>
+      </c>
+      <c r="G87" s="31">
+        <v>0</v>
+      </c>
+      <c r="H87" s="31">
+        <v>0</v>
+      </c>
+      <c r="I87" s="31">
+        <v>109</v>
+      </c>
+      <c r="J87" s="31">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="88" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A88" s="23">
+        <v>43988</v>
+      </c>
+      <c r="B88" s="24">
+        <v>83105</v>
+      </c>
+      <c r="C88" s="25">
+        <v>229</v>
+      </c>
+      <c r="D88" s="25">
+        <v>1485</v>
+      </c>
+      <c r="E88" s="25">
+        <v>1</v>
+      </c>
+      <c r="F88" s="25">
+        <v>5</v>
+      </c>
+      <c r="G88" s="25">
+        <v>0</v>
+      </c>
+      <c r="H88" s="25">
+        <v>1</v>
+      </c>
+      <c r="I88" s="25">
+        <v>109</v>
+      </c>
+      <c r="J88" s="25">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="89" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A89" s="29">
+        <v>43989</v>
+      </c>
+      <c r="B89" s="30">
+        <v>83316</v>
+      </c>
+      <c r="C89" s="31">
+        <v>211</v>
+      </c>
+      <c r="D89" s="31">
+        <v>1485</v>
+      </c>
+      <c r="E89" s="31">
+        <v>0</v>
+      </c>
+      <c r="F89" s="31">
+        <v>5</v>
+      </c>
+      <c r="G89" s="31">
+        <v>0</v>
+      </c>
+      <c r="H89" s="31">
+        <v>0</v>
+      </c>
+      <c r="I89" s="31">
+        <v>109</v>
+      </c>
+      <c r="J89" s="31">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="90" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A90" s="20">
+        <v>43990</v>
+      </c>
+      <c r="B90" s="21">
+        <v>84130</v>
+      </c>
+      <c r="C90" s="22">
+        <v>814</v>
+      </c>
+      <c r="D90" s="22">
+        <v>1486</v>
+      </c>
+      <c r="E90" s="22">
+        <v>1</v>
+      </c>
+      <c r="F90" s="22">
+        <v>6</v>
+      </c>
+      <c r="G90" s="22">
+        <v>0</v>
+      </c>
+      <c r="H90" s="22">
+        <v>0</v>
+      </c>
+      <c r="I90" s="22">
+        <v>109</v>
+      </c>
+      <c r="J90" s="22">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="91" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A91" s="20">
+        <v>43991</v>
+      </c>
+      <c r="B91" s="21">
+        <v>84868</v>
+      </c>
+      <c r="C91" s="22">
+        <v>738</v>
+      </c>
+      <c r="D91" s="22">
+        <v>1488</v>
+      </c>
+      <c r="E91" s="22">
+        <v>2</v>
+      </c>
+      <c r="F91" s="22">
+        <v>6</v>
+      </c>
+      <c r="G91" s="22">
+        <v>0</v>
+      </c>
+      <c r="H91" s="22">
+        <v>0</v>
+      </c>
+      <c r="I91" s="22">
+        <v>109</v>
+      </c>
+      <c r="J91" s="22">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="92" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A92" s="23">
+        <v>43992</v>
+      </c>
+      <c r="B92" s="24">
+        <v>85626</v>
+      </c>
+      <c r="C92" s="25">
+        <v>758</v>
+      </c>
+      <c r="D92" s="25">
+        <v>1488</v>
+      </c>
+      <c r="E92" s="25">
+        <v>0</v>
+      </c>
+      <c r="F92" s="25">
+        <v>6</v>
+      </c>
+      <c r="G92" s="25">
+        <v>0</v>
+      </c>
+      <c r="H92" s="25">
+        <v>0</v>
+      </c>
+      <c r="I92" s="25">
+        <v>109</v>
+      </c>
+      <c r="J92" s="25">
+        <v>0</v>
+      </c>
+    </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>

</xml_diff>

<commit_message>
Data updated by GitHub Bot (2020-06-12 12)
</commit_message>
<xml_diff>
--- a/output/snapshot/fdcf2531-4c3e-5c02-b63c-ee160ead6dea.xlsx
+++ b/output/snapshot/fdcf2531-4c3e-5c02-b63c-ee160ead6dea.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="I:\AKTUALNI PODATKI - KORONA\Za objavo na GOV.SI\ang\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{1E6DD62F-2BE2-47DC-A7ED-9B57C1589256}" xr6:coauthVersionLast="44" xr6:coauthVersionMax="44" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{D3B4EFB9-DC53-44F6-8FC1-2DF445145104}" xr6:coauthVersionLast="44" xr6:coauthVersionMax="44" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -64,7 +64,7 @@
   <numFmts count="1">
     <numFmt numFmtId="164" formatCode="d/\ m/\ yyyy;@"/>
   </numFmts>
-  <fonts count="4" x14ac:knownFonts="1">
+  <fonts count="5" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -93,6 +93,13 @@
       <name val="Calibri Light"/>
       <scheme val="major"/>
     </font>
+    <font>
+      <sz val="10"/>
+      <color theme="1"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
   </fonts>
   <fills count="3">
     <fill>
@@ -108,7 +115,7 @@
       </patternFill>
     </fill>
   </fills>
-  <borders count="2">
+  <borders count="3">
     <border>
       <left/>
       <right/>
@@ -129,11 +136,26 @@
       <bottom/>
       <diagonal/>
     </border>
+    <border>
+      <left style="thin">
+        <color theme="4"/>
+      </left>
+      <right style="thin">
+        <color theme="4"/>
+      </right>
+      <top style="thin">
+        <color theme="4"/>
+      </top>
+      <bottom style="thin">
+        <color theme="4"/>
+      </bottom>
+      <diagonal/>
+    </border>
   </borders>
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="26">
+  <cellXfs count="32">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="49" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyAlignment="1" applyProtection="1">
       <alignment horizontal="left" vertical="top"/>
@@ -208,6 +230,24 @@
       <alignment horizontal="right"/>
     </xf>
     <xf numFmtId="0" fontId="3" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="right"/>
+    </xf>
+    <xf numFmtId="164" fontId="4" fillId="2" borderId="2" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="right" vertical="top"/>
+    </xf>
+    <xf numFmtId="3" fontId="4" fillId="2" borderId="2" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="right"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="2" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="right"/>
+    </xf>
+    <xf numFmtId="164" fontId="3" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="right" vertical="top"/>
+    </xf>
+    <xf numFmtId="3" fontId="3" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="right"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="right"/>
     </xf>
   </cellXfs>
@@ -399,8 +439,8 @@
 </file>
 
 <file path=xl/tables/table1.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="1" xr:uid="{00000000-000C-0000-FFFF-FFFF00000000}" name="Tabela1" displayName="Tabela1" ref="A1:J75" totalsRowShown="0" headerRowDxfId="11" dataDxfId="10">
-  <autoFilter ref="A1:J75" xr:uid="{00000000-0009-0000-0100-000001000000}">
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="1" xr:uid="{00000000-000C-0000-FFFF-FFFF00000000}" name="Tabela1" displayName="Tabela1" ref="A1:J93" totalsRowShown="0" headerRowDxfId="11" dataDxfId="10">
+  <autoFilter ref="A1:J93" xr:uid="{00000000-0009-0000-0100-000001000000}">
     <filterColumn colId="0" hiddenButton="1"/>
     <filterColumn colId="1" hiddenButton="1"/>
     <filterColumn colId="2" hiddenButton="1"/>
@@ -696,10 +736,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:J75"/>
+  <dimension ref="A1:J93"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A40" zoomScale="89" zoomScaleNormal="89" workbookViewId="0">
-      <selection activeCell="J74" sqref="J74"/>
+    <sheetView tabSelected="1" topLeftCell="A65" zoomScale="89" zoomScaleNormal="89" workbookViewId="0">
+      <selection activeCell="A93" sqref="A93:J93"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -3117,6 +3157,582 @@
         <v>0</v>
       </c>
     </row>
+    <row r="76" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A76" s="20">
+        <v>43976</v>
+      </c>
+      <c r="B76" s="21">
+        <v>75770</v>
+      </c>
+      <c r="C76" s="22">
+        <v>754</v>
+      </c>
+      <c r="D76" s="22">
+        <v>1469</v>
+      </c>
+      <c r="E76" s="22">
+        <v>0</v>
+      </c>
+      <c r="F76" s="22">
+        <v>9</v>
+      </c>
+      <c r="G76" s="22">
+        <v>2</v>
+      </c>
+      <c r="H76" s="22">
+        <v>6</v>
+      </c>
+      <c r="I76" s="22">
+        <v>108</v>
+      </c>
+      <c r="J76" s="22">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="77" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A77" s="20">
+        <v>43977</v>
+      </c>
+      <c r="B77" s="21">
+        <v>76579</v>
+      </c>
+      <c r="C77" s="22">
+        <v>809</v>
+      </c>
+      <c r="D77" s="22">
+        <v>1471</v>
+      </c>
+      <c r="E77" s="22">
+        <v>2</v>
+      </c>
+      <c r="F77" s="22">
+        <v>8</v>
+      </c>
+      <c r="G77" s="22">
+        <v>2</v>
+      </c>
+      <c r="H77" s="22">
+        <v>2</v>
+      </c>
+      <c r="I77" s="22">
+        <v>108</v>
+      </c>
+      <c r="J77" s="22">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="78" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A78" s="20">
+        <v>43978</v>
+      </c>
+      <c r="B78" s="21">
+        <v>77210</v>
+      </c>
+      <c r="C78" s="22">
+        <v>631</v>
+      </c>
+      <c r="D78" s="22">
+        <v>1473</v>
+      </c>
+      <c r="E78" s="22">
+        <v>2</v>
+      </c>
+      <c r="F78" s="22">
+        <v>7</v>
+      </c>
+      <c r="G78" s="22">
+        <v>2</v>
+      </c>
+      <c r="H78" s="22">
+        <v>1</v>
+      </c>
+      <c r="I78" s="22">
+        <v>108</v>
+      </c>
+      <c r="J78" s="22">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="79" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A79" s="20">
+        <v>43979</v>
+      </c>
+      <c r="B79" s="21">
+        <v>77916</v>
+      </c>
+      <c r="C79" s="22">
+        <v>706</v>
+      </c>
+      <c r="D79" s="22">
+        <v>1473</v>
+      </c>
+      <c r="E79" s="22">
+        <v>0</v>
+      </c>
+      <c r="F79" s="22">
+        <v>7</v>
+      </c>
+      <c r="G79" s="22">
+        <v>2</v>
+      </c>
+      <c r="H79" s="22">
+        <v>0</v>
+      </c>
+      <c r="I79" s="22">
+        <v>108</v>
+      </c>
+      <c r="J79" s="22">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="80" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A80" s="20">
+        <v>43980</v>
+      </c>
+      <c r="B80" s="21">
+        <v>78529</v>
+      </c>
+      <c r="C80" s="22">
+        <v>613</v>
+      </c>
+      <c r="D80" s="22">
+        <v>1473</v>
+      </c>
+      <c r="E80" s="22">
+        <v>0</v>
+      </c>
+      <c r="F80" s="22">
+        <v>7</v>
+      </c>
+      <c r="G80" s="22">
+        <v>2</v>
+      </c>
+      <c r="H80" s="22">
+        <v>0</v>
+      </c>
+      <c r="I80" s="22">
+        <v>108</v>
+      </c>
+      <c r="J80" s="22">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="81" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A81" s="20">
+        <v>43981</v>
+      </c>
+      <c r="B81" s="22">
+        <v>78793</v>
+      </c>
+      <c r="C81" s="22">
+        <v>264</v>
+      </c>
+      <c r="D81" s="22">
+        <v>1473</v>
+      </c>
+      <c r="E81" s="22">
+        <v>0</v>
+      </c>
+      <c r="F81" s="22">
+        <v>6</v>
+      </c>
+      <c r="G81" s="22">
+        <v>2</v>
+      </c>
+      <c r="H81" s="22">
+        <v>1</v>
+      </c>
+      <c r="I81" s="22">
+        <v>108</v>
+      </c>
+      <c r="J81" s="22">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="82" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A82" s="20">
+        <v>43982</v>
+      </c>
+      <c r="B82" s="21">
+        <v>79039</v>
+      </c>
+      <c r="C82" s="22">
+        <v>246</v>
+      </c>
+      <c r="D82" s="22">
+        <v>1473</v>
+      </c>
+      <c r="E82" s="22">
+        <v>0</v>
+      </c>
+      <c r="F82" s="22">
+        <v>5</v>
+      </c>
+      <c r="G82" s="22">
+        <v>1</v>
+      </c>
+      <c r="H82" s="22">
+        <v>0</v>
+      </c>
+      <c r="I82" s="22">
+        <v>109</v>
+      </c>
+      <c r="J82" s="22">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="83" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A83" s="20">
+        <v>43983</v>
+      </c>
+      <c r="B83" s="21">
+        <v>79698</v>
+      </c>
+      <c r="C83" s="22">
+        <v>659</v>
+      </c>
+      <c r="D83" s="22">
+        <v>1475</v>
+      </c>
+      <c r="E83" s="22">
+        <v>2</v>
+      </c>
+      <c r="F83" s="22">
+        <v>5</v>
+      </c>
+      <c r="G83" s="22">
+        <v>1</v>
+      </c>
+      <c r="H83" s="22">
+        <v>0</v>
+      </c>
+      <c r="I83" s="22">
+        <v>109</v>
+      </c>
+      <c r="J83" s="22">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="84" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A84" s="20">
+        <v>43984</v>
+      </c>
+      <c r="B84" s="21">
+        <v>80505</v>
+      </c>
+      <c r="C84" s="22">
+        <v>807</v>
+      </c>
+      <c r="D84" s="22">
+        <v>1477</v>
+      </c>
+      <c r="E84" s="22">
+        <v>2</v>
+      </c>
+      <c r="F84" s="22">
+        <v>5</v>
+      </c>
+      <c r="G84" s="22">
+        <v>0</v>
+      </c>
+      <c r="H84" s="22">
+        <v>0</v>
+      </c>
+      <c r="I84" s="22">
+        <v>109</v>
+      </c>
+      <c r="J84" s="22">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="85" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A85" s="20">
+        <v>43985</v>
+      </c>
+      <c r="B85" s="21">
+        <v>81333</v>
+      </c>
+      <c r="C85" s="22">
+        <v>828</v>
+      </c>
+      <c r="D85" s="22">
+        <v>1477</v>
+      </c>
+      <c r="E85" s="22">
+        <v>0</v>
+      </c>
+      <c r="F85" s="22">
+        <v>5</v>
+      </c>
+      <c r="G85" s="22">
+        <v>0</v>
+      </c>
+      <c r="H85" s="22">
+        <v>0</v>
+      </c>
+      <c r="I85" s="22">
+        <v>109</v>
+      </c>
+      <c r="J85" s="22">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="86" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A86" s="26">
+        <v>43986</v>
+      </c>
+      <c r="B86" s="27">
+        <v>82161</v>
+      </c>
+      <c r="C86" s="28">
+        <v>828</v>
+      </c>
+      <c r="D86" s="28">
+        <v>1479</v>
+      </c>
+      <c r="E86" s="28">
+        <v>2</v>
+      </c>
+      <c r="F86" s="28">
+        <v>6</v>
+      </c>
+      <c r="G86" s="28">
+        <v>0</v>
+      </c>
+      <c r="H86" s="28">
+        <v>0</v>
+      </c>
+      <c r="I86" s="28">
+        <v>109</v>
+      </c>
+      <c r="J86" s="28">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="87" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A87" s="29">
+        <v>43987</v>
+      </c>
+      <c r="B87" s="30">
+        <v>82876</v>
+      </c>
+      <c r="C87" s="31">
+        <v>715</v>
+      </c>
+      <c r="D87" s="31">
+        <v>1484</v>
+      </c>
+      <c r="E87" s="31">
+        <v>5</v>
+      </c>
+      <c r="F87" s="31">
+        <v>6</v>
+      </c>
+      <c r="G87" s="31">
+        <v>0</v>
+      </c>
+      <c r="H87" s="31">
+        <v>0</v>
+      </c>
+      <c r="I87" s="31">
+        <v>109</v>
+      </c>
+      <c r="J87" s="31">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="88" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A88" s="23">
+        <v>43988</v>
+      </c>
+      <c r="B88" s="24">
+        <v>83105</v>
+      </c>
+      <c r="C88" s="25">
+        <v>229</v>
+      </c>
+      <c r="D88" s="25">
+        <v>1485</v>
+      </c>
+      <c r="E88" s="25">
+        <v>1</v>
+      </c>
+      <c r="F88" s="25">
+        <v>5</v>
+      </c>
+      <c r="G88" s="25">
+        <v>0</v>
+      </c>
+      <c r="H88" s="25">
+        <v>1</v>
+      </c>
+      <c r="I88" s="25">
+        <v>109</v>
+      </c>
+      <c r="J88" s="25">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="89" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A89" s="29">
+        <v>43989</v>
+      </c>
+      <c r="B89" s="30">
+        <v>83316</v>
+      </c>
+      <c r="C89" s="31">
+        <v>211</v>
+      </c>
+      <c r="D89" s="31">
+        <v>1485</v>
+      </c>
+      <c r="E89" s="31">
+        <v>0</v>
+      </c>
+      <c r="F89" s="31">
+        <v>5</v>
+      </c>
+      <c r="G89" s="31">
+        <v>0</v>
+      </c>
+      <c r="H89" s="31">
+        <v>0</v>
+      </c>
+      <c r="I89" s="31">
+        <v>109</v>
+      </c>
+      <c r="J89" s="31">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="90" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A90" s="20">
+        <v>43990</v>
+      </c>
+      <c r="B90" s="21">
+        <v>84130</v>
+      </c>
+      <c r="C90" s="22">
+        <v>814</v>
+      </c>
+      <c r="D90" s="22">
+        <v>1486</v>
+      </c>
+      <c r="E90" s="22">
+        <v>1</v>
+      </c>
+      <c r="F90" s="22">
+        <v>6</v>
+      </c>
+      <c r="G90" s="22">
+        <v>0</v>
+      </c>
+      <c r="H90" s="22">
+        <v>0</v>
+      </c>
+      <c r="I90" s="22">
+        <v>109</v>
+      </c>
+      <c r="J90" s="22">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="91" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A91" s="20">
+        <v>43991</v>
+      </c>
+      <c r="B91" s="21">
+        <v>84868</v>
+      </c>
+      <c r="C91" s="22">
+        <v>738</v>
+      </c>
+      <c r="D91" s="22">
+        <v>1488</v>
+      </c>
+      <c r="E91" s="22">
+        <v>2</v>
+      </c>
+      <c r="F91" s="22">
+        <v>6</v>
+      </c>
+      <c r="G91" s="22">
+        <v>0</v>
+      </c>
+      <c r="H91" s="22">
+        <v>0</v>
+      </c>
+      <c r="I91" s="22">
+        <v>109</v>
+      </c>
+      <c r="J91" s="22">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="92" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A92" s="23">
+        <v>43992</v>
+      </c>
+      <c r="B92" s="24">
+        <v>85626</v>
+      </c>
+      <c r="C92" s="25">
+        <v>758</v>
+      </c>
+      <c r="D92" s="25">
+        <v>1488</v>
+      </c>
+      <c r="E92" s="25">
+        <v>0</v>
+      </c>
+      <c r="F92" s="25">
+        <v>6</v>
+      </c>
+      <c r="G92" s="25">
+        <v>0</v>
+      </c>
+      <c r="H92" s="25">
+        <v>0</v>
+      </c>
+      <c r="I92" s="25">
+        <v>109</v>
+      </c>
+      <c r="J92" s="25">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="93" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A93" s="29">
+        <v>43993</v>
+      </c>
+      <c r="B93" s="30">
+        <v>86328</v>
+      </c>
+      <c r="C93" s="31">
+        <v>702</v>
+      </c>
+      <c r="D93" s="31">
+        <v>1490</v>
+      </c>
+      <c r="E93" s="31">
+        <v>2</v>
+      </c>
+      <c r="F93" s="31">
+        <v>6</v>
+      </c>
+      <c r="G93" s="31">
+        <v>0</v>
+      </c>
+      <c r="H93" s="31">
+        <v>0</v>
+      </c>
+      <c r="I93" s="31">
+        <v>109</v>
+      </c>
+      <c r="J93" s="31">
+        <v>0</v>
+      </c>
+    </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>

</xml_diff>

<commit_message>
Data updated by GitHub Bot (2020-06-12 20)
</commit_message>
<xml_diff>
--- a/output/snapshot/fdcf2531-4c3e-5c02-b63c-ee160ead6dea.xlsx
+++ b/output/snapshot/fdcf2531-4c3e-5c02-b63c-ee160ead6dea.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="I:\AKTUALNI PODATKI - KORONA\Za objavo na GOV.SI\ang\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{1E6DD62F-2BE2-47DC-A7ED-9B57C1589256}" xr6:coauthVersionLast="44" xr6:coauthVersionMax="44" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{D3B4EFB9-DC53-44F6-8FC1-2DF445145104}" xr6:coauthVersionLast="44" xr6:coauthVersionMax="44" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -64,7 +64,7 @@
   <numFmts count="1">
     <numFmt numFmtId="164" formatCode="d/\ m/\ yyyy;@"/>
   </numFmts>
-  <fonts count="4" x14ac:knownFonts="1">
+  <fonts count="5" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -93,6 +93,13 @@
       <name val="Calibri Light"/>
       <scheme val="major"/>
     </font>
+    <font>
+      <sz val="10"/>
+      <color theme="1"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
   </fonts>
   <fills count="3">
     <fill>
@@ -108,7 +115,7 @@
       </patternFill>
     </fill>
   </fills>
-  <borders count="2">
+  <borders count="3">
     <border>
       <left/>
       <right/>
@@ -129,11 +136,26 @@
       <bottom/>
       <diagonal/>
     </border>
+    <border>
+      <left style="thin">
+        <color theme="4"/>
+      </left>
+      <right style="thin">
+        <color theme="4"/>
+      </right>
+      <top style="thin">
+        <color theme="4"/>
+      </top>
+      <bottom style="thin">
+        <color theme="4"/>
+      </bottom>
+      <diagonal/>
+    </border>
   </borders>
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="26">
+  <cellXfs count="32">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="49" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyAlignment="1" applyProtection="1">
       <alignment horizontal="left" vertical="top"/>
@@ -208,6 +230,24 @@
       <alignment horizontal="right"/>
     </xf>
     <xf numFmtId="0" fontId="3" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="right"/>
+    </xf>
+    <xf numFmtId="164" fontId="4" fillId="2" borderId="2" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="right" vertical="top"/>
+    </xf>
+    <xf numFmtId="3" fontId="4" fillId="2" borderId="2" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="right"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="2" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="right"/>
+    </xf>
+    <xf numFmtId="164" fontId="3" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="right" vertical="top"/>
+    </xf>
+    <xf numFmtId="3" fontId="3" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="right"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="right"/>
     </xf>
   </cellXfs>
@@ -399,8 +439,8 @@
 </file>
 
 <file path=xl/tables/table1.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="1" xr:uid="{00000000-000C-0000-FFFF-FFFF00000000}" name="Tabela1" displayName="Tabela1" ref="A1:J75" totalsRowShown="0" headerRowDxfId="11" dataDxfId="10">
-  <autoFilter ref="A1:J75" xr:uid="{00000000-0009-0000-0100-000001000000}">
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="1" xr:uid="{00000000-000C-0000-FFFF-FFFF00000000}" name="Tabela1" displayName="Tabela1" ref="A1:J93" totalsRowShown="0" headerRowDxfId="11" dataDxfId="10">
+  <autoFilter ref="A1:J93" xr:uid="{00000000-0009-0000-0100-000001000000}">
     <filterColumn colId="0" hiddenButton="1"/>
     <filterColumn colId="1" hiddenButton="1"/>
     <filterColumn colId="2" hiddenButton="1"/>
@@ -696,10 +736,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:J75"/>
+  <dimension ref="A1:J93"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A40" zoomScale="89" zoomScaleNormal="89" workbookViewId="0">
-      <selection activeCell="J74" sqref="J74"/>
+    <sheetView tabSelected="1" topLeftCell="A65" zoomScale="89" zoomScaleNormal="89" workbookViewId="0">
+      <selection activeCell="A93" sqref="A93:J93"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -3117,6 +3157,582 @@
         <v>0</v>
       </c>
     </row>
+    <row r="76" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A76" s="20">
+        <v>43976</v>
+      </c>
+      <c r="B76" s="21">
+        <v>75770</v>
+      </c>
+      <c r="C76" s="22">
+        <v>754</v>
+      </c>
+      <c r="D76" s="22">
+        <v>1469</v>
+      </c>
+      <c r="E76" s="22">
+        <v>0</v>
+      </c>
+      <c r="F76" s="22">
+        <v>9</v>
+      </c>
+      <c r="G76" s="22">
+        <v>2</v>
+      </c>
+      <c r="H76" s="22">
+        <v>6</v>
+      </c>
+      <c r="I76" s="22">
+        <v>108</v>
+      </c>
+      <c r="J76" s="22">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="77" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A77" s="20">
+        <v>43977</v>
+      </c>
+      <c r="B77" s="21">
+        <v>76579</v>
+      </c>
+      <c r="C77" s="22">
+        <v>809</v>
+      </c>
+      <c r="D77" s="22">
+        <v>1471</v>
+      </c>
+      <c r="E77" s="22">
+        <v>2</v>
+      </c>
+      <c r="F77" s="22">
+        <v>8</v>
+      </c>
+      <c r="G77" s="22">
+        <v>2</v>
+      </c>
+      <c r="H77" s="22">
+        <v>2</v>
+      </c>
+      <c r="I77" s="22">
+        <v>108</v>
+      </c>
+      <c r="J77" s="22">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="78" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A78" s="20">
+        <v>43978</v>
+      </c>
+      <c r="B78" s="21">
+        <v>77210</v>
+      </c>
+      <c r="C78" s="22">
+        <v>631</v>
+      </c>
+      <c r="D78" s="22">
+        <v>1473</v>
+      </c>
+      <c r="E78" s="22">
+        <v>2</v>
+      </c>
+      <c r="F78" s="22">
+        <v>7</v>
+      </c>
+      <c r="G78" s="22">
+        <v>2</v>
+      </c>
+      <c r="H78" s="22">
+        <v>1</v>
+      </c>
+      <c r="I78" s="22">
+        <v>108</v>
+      </c>
+      <c r="J78" s="22">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="79" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A79" s="20">
+        <v>43979</v>
+      </c>
+      <c r="B79" s="21">
+        <v>77916</v>
+      </c>
+      <c r="C79" s="22">
+        <v>706</v>
+      </c>
+      <c r="D79" s="22">
+        <v>1473</v>
+      </c>
+      <c r="E79" s="22">
+        <v>0</v>
+      </c>
+      <c r="F79" s="22">
+        <v>7</v>
+      </c>
+      <c r="G79" s="22">
+        <v>2</v>
+      </c>
+      <c r="H79" s="22">
+        <v>0</v>
+      </c>
+      <c r="I79" s="22">
+        <v>108</v>
+      </c>
+      <c r="J79" s="22">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="80" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A80" s="20">
+        <v>43980</v>
+      </c>
+      <c r="B80" s="21">
+        <v>78529</v>
+      </c>
+      <c r="C80" s="22">
+        <v>613</v>
+      </c>
+      <c r="D80" s="22">
+        <v>1473</v>
+      </c>
+      <c r="E80" s="22">
+        <v>0</v>
+      </c>
+      <c r="F80" s="22">
+        <v>7</v>
+      </c>
+      <c r="G80" s="22">
+        <v>2</v>
+      </c>
+      <c r="H80" s="22">
+        <v>0</v>
+      </c>
+      <c r="I80" s="22">
+        <v>108</v>
+      </c>
+      <c r="J80" s="22">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="81" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A81" s="20">
+        <v>43981</v>
+      </c>
+      <c r="B81" s="22">
+        <v>78793</v>
+      </c>
+      <c r="C81" s="22">
+        <v>264</v>
+      </c>
+      <c r="D81" s="22">
+        <v>1473</v>
+      </c>
+      <c r="E81" s="22">
+        <v>0</v>
+      </c>
+      <c r="F81" s="22">
+        <v>6</v>
+      </c>
+      <c r="G81" s="22">
+        <v>2</v>
+      </c>
+      <c r="H81" s="22">
+        <v>1</v>
+      </c>
+      <c r="I81" s="22">
+        <v>108</v>
+      </c>
+      <c r="J81" s="22">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="82" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A82" s="20">
+        <v>43982</v>
+      </c>
+      <c r="B82" s="21">
+        <v>79039</v>
+      </c>
+      <c r="C82" s="22">
+        <v>246</v>
+      </c>
+      <c r="D82" s="22">
+        <v>1473</v>
+      </c>
+      <c r="E82" s="22">
+        <v>0</v>
+      </c>
+      <c r="F82" s="22">
+        <v>5</v>
+      </c>
+      <c r="G82" s="22">
+        <v>1</v>
+      </c>
+      <c r="H82" s="22">
+        <v>0</v>
+      </c>
+      <c r="I82" s="22">
+        <v>109</v>
+      </c>
+      <c r="J82" s="22">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="83" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A83" s="20">
+        <v>43983</v>
+      </c>
+      <c r="B83" s="21">
+        <v>79698</v>
+      </c>
+      <c r="C83" s="22">
+        <v>659</v>
+      </c>
+      <c r="D83" s="22">
+        <v>1475</v>
+      </c>
+      <c r="E83" s="22">
+        <v>2</v>
+      </c>
+      <c r="F83" s="22">
+        <v>5</v>
+      </c>
+      <c r="G83" s="22">
+        <v>1</v>
+      </c>
+      <c r="H83" s="22">
+        <v>0</v>
+      </c>
+      <c r="I83" s="22">
+        <v>109</v>
+      </c>
+      <c r="J83" s="22">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="84" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A84" s="20">
+        <v>43984</v>
+      </c>
+      <c r="B84" s="21">
+        <v>80505</v>
+      </c>
+      <c r="C84" s="22">
+        <v>807</v>
+      </c>
+      <c r="D84" s="22">
+        <v>1477</v>
+      </c>
+      <c r="E84" s="22">
+        <v>2</v>
+      </c>
+      <c r="F84" s="22">
+        <v>5</v>
+      </c>
+      <c r="G84" s="22">
+        <v>0</v>
+      </c>
+      <c r="H84" s="22">
+        <v>0</v>
+      </c>
+      <c r="I84" s="22">
+        <v>109</v>
+      </c>
+      <c r="J84" s="22">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="85" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A85" s="20">
+        <v>43985</v>
+      </c>
+      <c r="B85" s="21">
+        <v>81333</v>
+      </c>
+      <c r="C85" s="22">
+        <v>828</v>
+      </c>
+      <c r="D85" s="22">
+        <v>1477</v>
+      </c>
+      <c r="E85" s="22">
+        <v>0</v>
+      </c>
+      <c r="F85" s="22">
+        <v>5</v>
+      </c>
+      <c r="G85" s="22">
+        <v>0</v>
+      </c>
+      <c r="H85" s="22">
+        <v>0</v>
+      </c>
+      <c r="I85" s="22">
+        <v>109</v>
+      </c>
+      <c r="J85" s="22">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="86" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A86" s="26">
+        <v>43986</v>
+      </c>
+      <c r="B86" s="27">
+        <v>82161</v>
+      </c>
+      <c r="C86" s="28">
+        <v>828</v>
+      </c>
+      <c r="D86" s="28">
+        <v>1479</v>
+      </c>
+      <c r="E86" s="28">
+        <v>2</v>
+      </c>
+      <c r="F86" s="28">
+        <v>6</v>
+      </c>
+      <c r="G86" s="28">
+        <v>0</v>
+      </c>
+      <c r="H86" s="28">
+        <v>0</v>
+      </c>
+      <c r="I86" s="28">
+        <v>109</v>
+      </c>
+      <c r="J86" s="28">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="87" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A87" s="29">
+        <v>43987</v>
+      </c>
+      <c r="B87" s="30">
+        <v>82876</v>
+      </c>
+      <c r="C87" s="31">
+        <v>715</v>
+      </c>
+      <c r="D87" s="31">
+        <v>1484</v>
+      </c>
+      <c r="E87" s="31">
+        <v>5</v>
+      </c>
+      <c r="F87" s="31">
+        <v>6</v>
+      </c>
+      <c r="G87" s="31">
+        <v>0</v>
+      </c>
+      <c r="H87" s="31">
+        <v>0</v>
+      </c>
+      <c r="I87" s="31">
+        <v>109</v>
+      </c>
+      <c r="J87" s="31">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="88" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A88" s="23">
+        <v>43988</v>
+      </c>
+      <c r="B88" s="24">
+        <v>83105</v>
+      </c>
+      <c r="C88" s="25">
+        <v>229</v>
+      </c>
+      <c r="D88" s="25">
+        <v>1485</v>
+      </c>
+      <c r="E88" s="25">
+        <v>1</v>
+      </c>
+      <c r="F88" s="25">
+        <v>5</v>
+      </c>
+      <c r="G88" s="25">
+        <v>0</v>
+      </c>
+      <c r="H88" s="25">
+        <v>1</v>
+      </c>
+      <c r="I88" s="25">
+        <v>109</v>
+      </c>
+      <c r="J88" s="25">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="89" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A89" s="29">
+        <v>43989</v>
+      </c>
+      <c r="B89" s="30">
+        <v>83316</v>
+      </c>
+      <c r="C89" s="31">
+        <v>211</v>
+      </c>
+      <c r="D89" s="31">
+        <v>1485</v>
+      </c>
+      <c r="E89" s="31">
+        <v>0</v>
+      </c>
+      <c r="F89" s="31">
+        <v>5</v>
+      </c>
+      <c r="G89" s="31">
+        <v>0</v>
+      </c>
+      <c r="H89" s="31">
+        <v>0</v>
+      </c>
+      <c r="I89" s="31">
+        <v>109</v>
+      </c>
+      <c r="J89" s="31">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="90" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A90" s="20">
+        <v>43990</v>
+      </c>
+      <c r="B90" s="21">
+        <v>84130</v>
+      </c>
+      <c r="C90" s="22">
+        <v>814</v>
+      </c>
+      <c r="D90" s="22">
+        <v>1486</v>
+      </c>
+      <c r="E90" s="22">
+        <v>1</v>
+      </c>
+      <c r="F90" s="22">
+        <v>6</v>
+      </c>
+      <c r="G90" s="22">
+        <v>0</v>
+      </c>
+      <c r="H90" s="22">
+        <v>0</v>
+      </c>
+      <c r="I90" s="22">
+        <v>109</v>
+      </c>
+      <c r="J90" s="22">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="91" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A91" s="20">
+        <v>43991</v>
+      </c>
+      <c r="B91" s="21">
+        <v>84868</v>
+      </c>
+      <c r="C91" s="22">
+        <v>738</v>
+      </c>
+      <c r="D91" s="22">
+        <v>1488</v>
+      </c>
+      <c r="E91" s="22">
+        <v>2</v>
+      </c>
+      <c r="F91" s="22">
+        <v>6</v>
+      </c>
+      <c r="G91" s="22">
+        <v>0</v>
+      </c>
+      <c r="H91" s="22">
+        <v>0</v>
+      </c>
+      <c r="I91" s="22">
+        <v>109</v>
+      </c>
+      <c r="J91" s="22">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="92" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A92" s="23">
+        <v>43992</v>
+      </c>
+      <c r="B92" s="24">
+        <v>85626</v>
+      </c>
+      <c r="C92" s="25">
+        <v>758</v>
+      </c>
+      <c r="D92" s="25">
+        <v>1488</v>
+      </c>
+      <c r="E92" s="25">
+        <v>0</v>
+      </c>
+      <c r="F92" s="25">
+        <v>6</v>
+      </c>
+      <c r="G92" s="25">
+        <v>0</v>
+      </c>
+      <c r="H92" s="25">
+        <v>0</v>
+      </c>
+      <c r="I92" s="25">
+        <v>109</v>
+      </c>
+      <c r="J92" s="25">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="93" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A93" s="29">
+        <v>43993</v>
+      </c>
+      <c r="B93" s="30">
+        <v>86328</v>
+      </c>
+      <c r="C93" s="31">
+        <v>702</v>
+      </c>
+      <c r="D93" s="31">
+        <v>1490</v>
+      </c>
+      <c r="E93" s="31">
+        <v>2</v>
+      </c>
+      <c r="F93" s="31">
+        <v>6</v>
+      </c>
+      <c r="G93" s="31">
+        <v>0</v>
+      </c>
+      <c r="H93" s="31">
+        <v>0</v>
+      </c>
+      <c r="I93" s="31">
+        <v>109</v>
+      </c>
+      <c r="J93" s="31">
+        <v>0</v>
+      </c>
+    </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>

</xml_diff>

<commit_message>
Data updated by GitHub Bot (2020-06-13 12)
</commit_message>
<xml_diff>
--- a/output/snapshot/fdcf2531-4c3e-5c02-b63c-ee160ead6dea.xlsx
+++ b/output/snapshot/fdcf2531-4c3e-5c02-b63c-ee160ead6dea.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="I:\AKTUALNI PODATKI - KORONA\Za objavo na GOV.SI\ang\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{1E6DD62F-2BE2-47DC-A7ED-9B57C1589256}" xr6:coauthVersionLast="44" xr6:coauthVersionMax="44" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{7D15F133-2A7A-4A5C-822D-D65F9E3FAE2B}" xr6:coauthVersionLast="44" xr6:coauthVersionMax="44" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -64,7 +64,7 @@
   <numFmts count="1">
     <numFmt numFmtId="164" formatCode="d/\ m/\ yyyy;@"/>
   </numFmts>
-  <fonts count="4" x14ac:knownFonts="1">
+  <fonts count="5" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -93,6 +93,13 @@
       <name val="Calibri Light"/>
       <scheme val="major"/>
     </font>
+    <font>
+      <sz val="10"/>
+      <color theme="1"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
   </fonts>
   <fills count="3">
     <fill>
@@ -108,7 +115,7 @@
       </patternFill>
     </fill>
   </fills>
-  <borders count="2">
+  <borders count="3">
     <border>
       <left/>
       <right/>
@@ -129,11 +136,26 @@
       <bottom/>
       <diagonal/>
     </border>
+    <border>
+      <left style="thin">
+        <color theme="4"/>
+      </left>
+      <right style="thin">
+        <color theme="4"/>
+      </right>
+      <top style="thin">
+        <color theme="4"/>
+      </top>
+      <bottom style="thin">
+        <color theme="4"/>
+      </bottom>
+      <diagonal/>
+    </border>
   </borders>
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="26">
+  <cellXfs count="32">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="49" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyAlignment="1" applyProtection="1">
       <alignment horizontal="left" vertical="top"/>
@@ -208,6 +230,24 @@
       <alignment horizontal="right"/>
     </xf>
     <xf numFmtId="0" fontId="3" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="right"/>
+    </xf>
+    <xf numFmtId="164" fontId="4" fillId="2" borderId="2" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="right" vertical="top"/>
+    </xf>
+    <xf numFmtId="3" fontId="4" fillId="2" borderId="2" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="right"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="2" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="right"/>
+    </xf>
+    <xf numFmtId="164" fontId="3" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="right" vertical="top"/>
+    </xf>
+    <xf numFmtId="3" fontId="3" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="right"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="right"/>
     </xf>
   </cellXfs>
@@ -399,8 +439,8 @@
 </file>
 
 <file path=xl/tables/table1.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="1" xr:uid="{00000000-000C-0000-FFFF-FFFF00000000}" name="Tabela1" displayName="Tabela1" ref="A1:J75" totalsRowShown="0" headerRowDxfId="11" dataDxfId="10">
-  <autoFilter ref="A1:J75" xr:uid="{00000000-0009-0000-0100-000001000000}">
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="1" xr:uid="{00000000-000C-0000-FFFF-FFFF00000000}" name="Tabela1" displayName="Tabela1" ref="A1:J94" totalsRowShown="0" headerRowDxfId="11" dataDxfId="10">
+  <autoFilter ref="A1:J94" xr:uid="{00000000-0009-0000-0100-000001000000}">
     <filterColumn colId="0" hiddenButton="1"/>
     <filterColumn colId="1" hiddenButton="1"/>
     <filterColumn colId="2" hiddenButton="1"/>
@@ -696,10 +736,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:J75"/>
+  <dimension ref="A1:J94"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A40" zoomScale="89" zoomScaleNormal="89" workbookViewId="0">
-      <selection activeCell="J74" sqref="J74"/>
+    <sheetView tabSelected="1" topLeftCell="A65" zoomScale="89" zoomScaleNormal="89" workbookViewId="0">
+      <selection activeCell="A95" sqref="A95"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -3117,6 +3157,614 @@
         <v>0</v>
       </c>
     </row>
+    <row r="76" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A76" s="20">
+        <v>43976</v>
+      </c>
+      <c r="B76" s="21">
+        <v>75770</v>
+      </c>
+      <c r="C76" s="22">
+        <v>754</v>
+      </c>
+      <c r="D76" s="22">
+        <v>1469</v>
+      </c>
+      <c r="E76" s="22">
+        <v>0</v>
+      </c>
+      <c r="F76" s="22">
+        <v>9</v>
+      </c>
+      <c r="G76" s="22">
+        <v>2</v>
+      </c>
+      <c r="H76" s="22">
+        <v>6</v>
+      </c>
+      <c r="I76" s="22">
+        <v>108</v>
+      </c>
+      <c r="J76" s="22">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="77" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A77" s="20">
+        <v>43977</v>
+      </c>
+      <c r="B77" s="21">
+        <v>76579</v>
+      </c>
+      <c r="C77" s="22">
+        <v>809</v>
+      </c>
+      <c r="D77" s="22">
+        <v>1471</v>
+      </c>
+      <c r="E77" s="22">
+        <v>2</v>
+      </c>
+      <c r="F77" s="22">
+        <v>8</v>
+      </c>
+      <c r="G77" s="22">
+        <v>2</v>
+      </c>
+      <c r="H77" s="22">
+        <v>2</v>
+      </c>
+      <c r="I77" s="22">
+        <v>108</v>
+      </c>
+      <c r="J77" s="22">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="78" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A78" s="20">
+        <v>43978</v>
+      </c>
+      <c r="B78" s="21">
+        <v>77210</v>
+      </c>
+      <c r="C78" s="22">
+        <v>631</v>
+      </c>
+      <c r="D78" s="22">
+        <v>1473</v>
+      </c>
+      <c r="E78" s="22">
+        <v>2</v>
+      </c>
+      <c r="F78" s="22">
+        <v>7</v>
+      </c>
+      <c r="G78" s="22">
+        <v>2</v>
+      </c>
+      <c r="H78" s="22">
+        <v>1</v>
+      </c>
+      <c r="I78" s="22">
+        <v>108</v>
+      </c>
+      <c r="J78" s="22">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="79" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A79" s="20">
+        <v>43979</v>
+      </c>
+      <c r="B79" s="21">
+        <v>77916</v>
+      </c>
+      <c r="C79" s="22">
+        <v>706</v>
+      </c>
+      <c r="D79" s="22">
+        <v>1473</v>
+      </c>
+      <c r="E79" s="22">
+        <v>0</v>
+      </c>
+      <c r="F79" s="22">
+        <v>7</v>
+      </c>
+      <c r="G79" s="22">
+        <v>2</v>
+      </c>
+      <c r="H79" s="22">
+        <v>0</v>
+      </c>
+      <c r="I79" s="22">
+        <v>108</v>
+      </c>
+      <c r="J79" s="22">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="80" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A80" s="20">
+        <v>43980</v>
+      </c>
+      <c r="B80" s="21">
+        <v>78529</v>
+      </c>
+      <c r="C80" s="22">
+        <v>613</v>
+      </c>
+      <c r="D80" s="22">
+        <v>1473</v>
+      </c>
+      <c r="E80" s="22">
+        <v>0</v>
+      </c>
+      <c r="F80" s="22">
+        <v>7</v>
+      </c>
+      <c r="G80" s="22">
+        <v>2</v>
+      </c>
+      <c r="H80" s="22">
+        <v>0</v>
+      </c>
+      <c r="I80" s="22">
+        <v>108</v>
+      </c>
+      <c r="J80" s="22">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="81" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A81" s="20">
+        <v>43981</v>
+      </c>
+      <c r="B81" s="22">
+        <v>78793</v>
+      </c>
+      <c r="C81" s="22">
+        <v>264</v>
+      </c>
+      <c r="D81" s="22">
+        <v>1473</v>
+      </c>
+      <c r="E81" s="22">
+        <v>0</v>
+      </c>
+      <c r="F81" s="22">
+        <v>6</v>
+      </c>
+      <c r="G81" s="22">
+        <v>2</v>
+      </c>
+      <c r="H81" s="22">
+        <v>1</v>
+      </c>
+      <c r="I81" s="22">
+        <v>108</v>
+      </c>
+      <c r="J81" s="22">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="82" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A82" s="20">
+        <v>43982</v>
+      </c>
+      <c r="B82" s="21">
+        <v>79039</v>
+      </c>
+      <c r="C82" s="22">
+        <v>246</v>
+      </c>
+      <c r="D82" s="22">
+        <v>1473</v>
+      </c>
+      <c r="E82" s="22">
+        <v>0</v>
+      </c>
+      <c r="F82" s="22">
+        <v>5</v>
+      </c>
+      <c r="G82" s="22">
+        <v>1</v>
+      </c>
+      <c r="H82" s="22">
+        <v>0</v>
+      </c>
+      <c r="I82" s="22">
+        <v>109</v>
+      </c>
+      <c r="J82" s="22">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="83" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A83" s="20">
+        <v>43983</v>
+      </c>
+      <c r="B83" s="21">
+        <v>79698</v>
+      </c>
+      <c r="C83" s="22">
+        <v>659</v>
+      </c>
+      <c r="D83" s="22">
+        <v>1475</v>
+      </c>
+      <c r="E83" s="22">
+        <v>2</v>
+      </c>
+      <c r="F83" s="22">
+        <v>5</v>
+      </c>
+      <c r="G83" s="22">
+        <v>1</v>
+      </c>
+      <c r="H83" s="22">
+        <v>0</v>
+      </c>
+      <c r="I83" s="22">
+        <v>109</v>
+      </c>
+      <c r="J83" s="22">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="84" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A84" s="20">
+        <v>43984</v>
+      </c>
+      <c r="B84" s="21">
+        <v>80505</v>
+      </c>
+      <c r="C84" s="22">
+        <v>807</v>
+      </c>
+      <c r="D84" s="22">
+        <v>1477</v>
+      </c>
+      <c r="E84" s="22">
+        <v>2</v>
+      </c>
+      <c r="F84" s="22">
+        <v>5</v>
+      </c>
+      <c r="G84" s="22">
+        <v>0</v>
+      </c>
+      <c r="H84" s="22">
+        <v>0</v>
+      </c>
+      <c r="I84" s="22">
+        <v>109</v>
+      </c>
+      <c r="J84" s="22">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="85" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A85" s="20">
+        <v>43985</v>
+      </c>
+      <c r="B85" s="21">
+        <v>81333</v>
+      </c>
+      <c r="C85" s="22">
+        <v>828</v>
+      </c>
+      <c r="D85" s="22">
+        <v>1477</v>
+      </c>
+      <c r="E85" s="22">
+        <v>0</v>
+      </c>
+      <c r="F85" s="22">
+        <v>5</v>
+      </c>
+      <c r="G85" s="22">
+        <v>0</v>
+      </c>
+      <c r="H85" s="22">
+        <v>0</v>
+      </c>
+      <c r="I85" s="22">
+        <v>109</v>
+      </c>
+      <c r="J85" s="22">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="86" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A86" s="26">
+        <v>43986</v>
+      </c>
+      <c r="B86" s="27">
+        <v>82161</v>
+      </c>
+      <c r="C86" s="28">
+        <v>828</v>
+      </c>
+      <c r="D86" s="28">
+        <v>1479</v>
+      </c>
+      <c r="E86" s="28">
+        <v>2</v>
+      </c>
+      <c r="F86" s="28">
+        <v>6</v>
+      </c>
+      <c r="G86" s="28">
+        <v>0</v>
+      </c>
+      <c r="H86" s="28">
+        <v>0</v>
+      </c>
+      <c r="I86" s="28">
+        <v>109</v>
+      </c>
+      <c r="J86" s="28">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="87" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A87" s="29">
+        <v>43987</v>
+      </c>
+      <c r="B87" s="30">
+        <v>82876</v>
+      </c>
+      <c r="C87" s="31">
+        <v>715</v>
+      </c>
+      <c r="D87" s="31">
+        <v>1484</v>
+      </c>
+      <c r="E87" s="31">
+        <v>5</v>
+      </c>
+      <c r="F87" s="31">
+        <v>6</v>
+      </c>
+      <c r="G87" s="31">
+        <v>0</v>
+      </c>
+      <c r="H87" s="31">
+        <v>0</v>
+      </c>
+      <c r="I87" s="31">
+        <v>109</v>
+      </c>
+      <c r="J87" s="31">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="88" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A88" s="23">
+        <v>43988</v>
+      </c>
+      <c r="B88" s="24">
+        <v>83105</v>
+      </c>
+      <c r="C88" s="25">
+        <v>229</v>
+      </c>
+      <c r="D88" s="25">
+        <v>1485</v>
+      </c>
+      <c r="E88" s="25">
+        <v>1</v>
+      </c>
+      <c r="F88" s="25">
+        <v>5</v>
+      </c>
+      <c r="G88" s="25">
+        <v>0</v>
+      </c>
+      <c r="H88" s="25">
+        <v>1</v>
+      </c>
+      <c r="I88" s="25">
+        <v>109</v>
+      </c>
+      <c r="J88" s="25">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="89" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A89" s="29">
+        <v>43989</v>
+      </c>
+      <c r="B89" s="30">
+        <v>83316</v>
+      </c>
+      <c r="C89" s="31">
+        <v>211</v>
+      </c>
+      <c r="D89" s="31">
+        <v>1485</v>
+      </c>
+      <c r="E89" s="31">
+        <v>0</v>
+      </c>
+      <c r="F89" s="31">
+        <v>5</v>
+      </c>
+      <c r="G89" s="31">
+        <v>0</v>
+      </c>
+      <c r="H89" s="31">
+        <v>0</v>
+      </c>
+      <c r="I89" s="31">
+        <v>109</v>
+      </c>
+      <c r="J89" s="31">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="90" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A90" s="20">
+        <v>43990</v>
+      </c>
+      <c r="B90" s="21">
+        <v>84130</v>
+      </c>
+      <c r="C90" s="22">
+        <v>814</v>
+      </c>
+      <c r="D90" s="22">
+        <v>1486</v>
+      </c>
+      <c r="E90" s="22">
+        <v>1</v>
+      </c>
+      <c r="F90" s="22">
+        <v>6</v>
+      </c>
+      <c r="G90" s="22">
+        <v>0</v>
+      </c>
+      <c r="H90" s="22">
+        <v>0</v>
+      </c>
+      <c r="I90" s="22">
+        <v>109</v>
+      </c>
+      <c r="J90" s="22">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="91" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A91" s="20">
+        <v>43991</v>
+      </c>
+      <c r="B91" s="21">
+        <v>84868</v>
+      </c>
+      <c r="C91" s="22">
+        <v>738</v>
+      </c>
+      <c r="D91" s="22">
+        <v>1488</v>
+      </c>
+      <c r="E91" s="22">
+        <v>2</v>
+      </c>
+      <c r="F91" s="22">
+        <v>6</v>
+      </c>
+      <c r="G91" s="22">
+        <v>0</v>
+      </c>
+      <c r="H91" s="22">
+        <v>0</v>
+      </c>
+      <c r="I91" s="22">
+        <v>109</v>
+      </c>
+      <c r="J91" s="22">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="92" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A92" s="23">
+        <v>43992</v>
+      </c>
+      <c r="B92" s="24">
+        <v>85626</v>
+      </c>
+      <c r="C92" s="25">
+        <v>758</v>
+      </c>
+      <c r="D92" s="25">
+        <v>1488</v>
+      </c>
+      <c r="E92" s="25">
+        <v>0</v>
+      </c>
+      <c r="F92" s="25">
+        <v>6</v>
+      </c>
+      <c r="G92" s="25">
+        <v>0</v>
+      </c>
+      <c r="H92" s="25">
+        <v>0</v>
+      </c>
+      <c r="I92" s="25">
+        <v>109</v>
+      </c>
+      <c r="J92" s="25">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="93" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A93" s="29">
+        <v>43993</v>
+      </c>
+      <c r="B93" s="30">
+        <v>86328</v>
+      </c>
+      <c r="C93" s="31">
+        <v>702</v>
+      </c>
+      <c r="D93" s="31">
+        <v>1490</v>
+      </c>
+      <c r="E93" s="31">
+        <v>2</v>
+      </c>
+      <c r="F93" s="31">
+        <v>6</v>
+      </c>
+      <c r="G93" s="31">
+        <v>0</v>
+      </c>
+      <c r="H93" s="31">
+        <v>0</v>
+      </c>
+      <c r="I93" s="31">
+        <v>109</v>
+      </c>
+      <c r="J93" s="31">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="94" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A94" s="23">
+        <v>43994</v>
+      </c>
+      <c r="B94" s="24">
+        <v>87095</v>
+      </c>
+      <c r="C94" s="25">
+        <v>767</v>
+      </c>
+      <c r="D94" s="25">
+        <v>1492</v>
+      </c>
+      <c r="E94" s="25">
+        <v>2</v>
+      </c>
+      <c r="F94" s="25">
+        <v>6</v>
+      </c>
+      <c r="G94" s="25">
+        <v>0</v>
+      </c>
+      <c r="H94" s="25">
+        <v>0</v>
+      </c>
+      <c r="I94" s="25">
+        <v>109</v>
+      </c>
+      <c r="J94" s="25">
+        <v>0</v>
+      </c>
+    </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>

</xml_diff>

<commit_message>
Data updated by GitHub Bot (2020-06-13 20)
</commit_message>
<xml_diff>
--- a/output/snapshot/fdcf2531-4c3e-5c02-b63c-ee160ead6dea.xlsx
+++ b/output/snapshot/fdcf2531-4c3e-5c02-b63c-ee160ead6dea.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="I:\AKTUALNI PODATKI - KORONA\Za objavo na GOV.SI\ang\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{1E6DD62F-2BE2-47DC-A7ED-9B57C1589256}" xr6:coauthVersionLast="44" xr6:coauthVersionMax="44" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{7D15F133-2A7A-4A5C-822D-D65F9E3FAE2B}" xr6:coauthVersionLast="44" xr6:coauthVersionMax="44" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -64,7 +64,7 @@
   <numFmts count="1">
     <numFmt numFmtId="164" formatCode="d/\ m/\ yyyy;@"/>
   </numFmts>
-  <fonts count="4" x14ac:knownFonts="1">
+  <fonts count="5" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -93,6 +93,13 @@
       <name val="Calibri Light"/>
       <scheme val="major"/>
     </font>
+    <font>
+      <sz val="10"/>
+      <color theme="1"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
   </fonts>
   <fills count="3">
     <fill>
@@ -108,7 +115,7 @@
       </patternFill>
     </fill>
   </fills>
-  <borders count="2">
+  <borders count="3">
     <border>
       <left/>
       <right/>
@@ -129,11 +136,26 @@
       <bottom/>
       <diagonal/>
     </border>
+    <border>
+      <left style="thin">
+        <color theme="4"/>
+      </left>
+      <right style="thin">
+        <color theme="4"/>
+      </right>
+      <top style="thin">
+        <color theme="4"/>
+      </top>
+      <bottom style="thin">
+        <color theme="4"/>
+      </bottom>
+      <diagonal/>
+    </border>
   </borders>
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="26">
+  <cellXfs count="32">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="49" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyAlignment="1" applyProtection="1">
       <alignment horizontal="left" vertical="top"/>
@@ -208,6 +230,24 @@
       <alignment horizontal="right"/>
     </xf>
     <xf numFmtId="0" fontId="3" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="right"/>
+    </xf>
+    <xf numFmtId="164" fontId="4" fillId="2" borderId="2" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="right" vertical="top"/>
+    </xf>
+    <xf numFmtId="3" fontId="4" fillId="2" borderId="2" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="right"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="2" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="right"/>
+    </xf>
+    <xf numFmtId="164" fontId="3" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="right" vertical="top"/>
+    </xf>
+    <xf numFmtId="3" fontId="3" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="right"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="right"/>
     </xf>
   </cellXfs>
@@ -399,8 +439,8 @@
 </file>
 
 <file path=xl/tables/table1.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="1" xr:uid="{00000000-000C-0000-FFFF-FFFF00000000}" name="Tabela1" displayName="Tabela1" ref="A1:J75" totalsRowShown="0" headerRowDxfId="11" dataDxfId="10">
-  <autoFilter ref="A1:J75" xr:uid="{00000000-0009-0000-0100-000001000000}">
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="1" xr:uid="{00000000-000C-0000-FFFF-FFFF00000000}" name="Tabela1" displayName="Tabela1" ref="A1:J94" totalsRowShown="0" headerRowDxfId="11" dataDxfId="10">
+  <autoFilter ref="A1:J94" xr:uid="{00000000-0009-0000-0100-000001000000}">
     <filterColumn colId="0" hiddenButton="1"/>
     <filterColumn colId="1" hiddenButton="1"/>
     <filterColumn colId="2" hiddenButton="1"/>
@@ -696,10 +736,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:J75"/>
+  <dimension ref="A1:J94"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A40" zoomScale="89" zoomScaleNormal="89" workbookViewId="0">
-      <selection activeCell="J74" sqref="J74"/>
+    <sheetView tabSelected="1" topLeftCell="A65" zoomScale="89" zoomScaleNormal="89" workbookViewId="0">
+      <selection activeCell="A95" sqref="A95"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -3117,6 +3157,614 @@
         <v>0</v>
       </c>
     </row>
+    <row r="76" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A76" s="20">
+        <v>43976</v>
+      </c>
+      <c r="B76" s="21">
+        <v>75770</v>
+      </c>
+      <c r="C76" s="22">
+        <v>754</v>
+      </c>
+      <c r="D76" s="22">
+        <v>1469</v>
+      </c>
+      <c r="E76" s="22">
+        <v>0</v>
+      </c>
+      <c r="F76" s="22">
+        <v>9</v>
+      </c>
+      <c r="G76" s="22">
+        <v>2</v>
+      </c>
+      <c r="H76" s="22">
+        <v>6</v>
+      </c>
+      <c r="I76" s="22">
+        <v>108</v>
+      </c>
+      <c r="J76" s="22">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="77" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A77" s="20">
+        <v>43977</v>
+      </c>
+      <c r="B77" s="21">
+        <v>76579</v>
+      </c>
+      <c r="C77" s="22">
+        <v>809</v>
+      </c>
+      <c r="D77" s="22">
+        <v>1471</v>
+      </c>
+      <c r="E77" s="22">
+        <v>2</v>
+      </c>
+      <c r="F77" s="22">
+        <v>8</v>
+      </c>
+      <c r="G77" s="22">
+        <v>2</v>
+      </c>
+      <c r="H77" s="22">
+        <v>2</v>
+      </c>
+      <c r="I77" s="22">
+        <v>108</v>
+      </c>
+      <c r="J77" s="22">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="78" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A78" s="20">
+        <v>43978</v>
+      </c>
+      <c r="B78" s="21">
+        <v>77210</v>
+      </c>
+      <c r="C78" s="22">
+        <v>631</v>
+      </c>
+      <c r="D78" s="22">
+        <v>1473</v>
+      </c>
+      <c r="E78" s="22">
+        <v>2</v>
+      </c>
+      <c r="F78" s="22">
+        <v>7</v>
+      </c>
+      <c r="G78" s="22">
+        <v>2</v>
+      </c>
+      <c r="H78" s="22">
+        <v>1</v>
+      </c>
+      <c r="I78" s="22">
+        <v>108</v>
+      </c>
+      <c r="J78" s="22">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="79" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A79" s="20">
+        <v>43979</v>
+      </c>
+      <c r="B79" s="21">
+        <v>77916</v>
+      </c>
+      <c r="C79" s="22">
+        <v>706</v>
+      </c>
+      <c r="D79" s="22">
+        <v>1473</v>
+      </c>
+      <c r="E79" s="22">
+        <v>0</v>
+      </c>
+      <c r="F79" s="22">
+        <v>7</v>
+      </c>
+      <c r="G79" s="22">
+        <v>2</v>
+      </c>
+      <c r="H79" s="22">
+        <v>0</v>
+      </c>
+      <c r="I79" s="22">
+        <v>108</v>
+      </c>
+      <c r="J79" s="22">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="80" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A80" s="20">
+        <v>43980</v>
+      </c>
+      <c r="B80" s="21">
+        <v>78529</v>
+      </c>
+      <c r="C80" s="22">
+        <v>613</v>
+      </c>
+      <c r="D80" s="22">
+        <v>1473</v>
+      </c>
+      <c r="E80" s="22">
+        <v>0</v>
+      </c>
+      <c r="F80" s="22">
+        <v>7</v>
+      </c>
+      <c r="G80" s="22">
+        <v>2</v>
+      </c>
+      <c r="H80" s="22">
+        <v>0</v>
+      </c>
+      <c r="I80" s="22">
+        <v>108</v>
+      </c>
+      <c r="J80" s="22">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="81" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A81" s="20">
+        <v>43981</v>
+      </c>
+      <c r="B81" s="22">
+        <v>78793</v>
+      </c>
+      <c r="C81" s="22">
+        <v>264</v>
+      </c>
+      <c r="D81" s="22">
+        <v>1473</v>
+      </c>
+      <c r="E81" s="22">
+        <v>0</v>
+      </c>
+      <c r="F81" s="22">
+        <v>6</v>
+      </c>
+      <c r="G81" s="22">
+        <v>2</v>
+      </c>
+      <c r="H81" s="22">
+        <v>1</v>
+      </c>
+      <c r="I81" s="22">
+        <v>108</v>
+      </c>
+      <c r="J81" s="22">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="82" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A82" s="20">
+        <v>43982</v>
+      </c>
+      <c r="B82" s="21">
+        <v>79039</v>
+      </c>
+      <c r="C82" s="22">
+        <v>246</v>
+      </c>
+      <c r="D82" s="22">
+        <v>1473</v>
+      </c>
+      <c r="E82" s="22">
+        <v>0</v>
+      </c>
+      <c r="F82" s="22">
+        <v>5</v>
+      </c>
+      <c r="G82" s="22">
+        <v>1</v>
+      </c>
+      <c r="H82" s="22">
+        <v>0</v>
+      </c>
+      <c r="I82" s="22">
+        <v>109</v>
+      </c>
+      <c r="J82" s="22">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="83" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A83" s="20">
+        <v>43983</v>
+      </c>
+      <c r="B83" s="21">
+        <v>79698</v>
+      </c>
+      <c r="C83" s="22">
+        <v>659</v>
+      </c>
+      <c r="D83" s="22">
+        <v>1475</v>
+      </c>
+      <c r="E83" s="22">
+        <v>2</v>
+      </c>
+      <c r="F83" s="22">
+        <v>5</v>
+      </c>
+      <c r="G83" s="22">
+        <v>1</v>
+      </c>
+      <c r="H83" s="22">
+        <v>0</v>
+      </c>
+      <c r="I83" s="22">
+        <v>109</v>
+      </c>
+      <c r="J83" s="22">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="84" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A84" s="20">
+        <v>43984</v>
+      </c>
+      <c r="B84" s="21">
+        <v>80505</v>
+      </c>
+      <c r="C84" s="22">
+        <v>807</v>
+      </c>
+      <c r="D84" s="22">
+        <v>1477</v>
+      </c>
+      <c r="E84" s="22">
+        <v>2</v>
+      </c>
+      <c r="F84" s="22">
+        <v>5</v>
+      </c>
+      <c r="G84" s="22">
+        <v>0</v>
+      </c>
+      <c r="H84" s="22">
+        <v>0</v>
+      </c>
+      <c r="I84" s="22">
+        <v>109</v>
+      </c>
+      <c r="J84" s="22">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="85" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A85" s="20">
+        <v>43985</v>
+      </c>
+      <c r="B85" s="21">
+        <v>81333</v>
+      </c>
+      <c r="C85" s="22">
+        <v>828</v>
+      </c>
+      <c r="D85" s="22">
+        <v>1477</v>
+      </c>
+      <c r="E85" s="22">
+        <v>0</v>
+      </c>
+      <c r="F85" s="22">
+        <v>5</v>
+      </c>
+      <c r="G85" s="22">
+        <v>0</v>
+      </c>
+      <c r="H85" s="22">
+        <v>0</v>
+      </c>
+      <c r="I85" s="22">
+        <v>109</v>
+      </c>
+      <c r="J85" s="22">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="86" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A86" s="26">
+        <v>43986</v>
+      </c>
+      <c r="B86" s="27">
+        <v>82161</v>
+      </c>
+      <c r="C86" s="28">
+        <v>828</v>
+      </c>
+      <c r="D86" s="28">
+        <v>1479</v>
+      </c>
+      <c r="E86" s="28">
+        <v>2</v>
+      </c>
+      <c r="F86" s="28">
+        <v>6</v>
+      </c>
+      <c r="G86" s="28">
+        <v>0</v>
+      </c>
+      <c r="H86" s="28">
+        <v>0</v>
+      </c>
+      <c r="I86" s="28">
+        <v>109</v>
+      </c>
+      <c r="J86" s="28">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="87" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A87" s="29">
+        <v>43987</v>
+      </c>
+      <c r="B87" s="30">
+        <v>82876</v>
+      </c>
+      <c r="C87" s="31">
+        <v>715</v>
+      </c>
+      <c r="D87" s="31">
+        <v>1484</v>
+      </c>
+      <c r="E87" s="31">
+        <v>5</v>
+      </c>
+      <c r="F87" s="31">
+        <v>6</v>
+      </c>
+      <c r="G87" s="31">
+        <v>0</v>
+      </c>
+      <c r="H87" s="31">
+        <v>0</v>
+      </c>
+      <c r="I87" s="31">
+        <v>109</v>
+      </c>
+      <c r="J87" s="31">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="88" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A88" s="23">
+        <v>43988</v>
+      </c>
+      <c r="B88" s="24">
+        <v>83105</v>
+      </c>
+      <c r="C88" s="25">
+        <v>229</v>
+      </c>
+      <c r="D88" s="25">
+        <v>1485</v>
+      </c>
+      <c r="E88" s="25">
+        <v>1</v>
+      </c>
+      <c r="F88" s="25">
+        <v>5</v>
+      </c>
+      <c r="G88" s="25">
+        <v>0</v>
+      </c>
+      <c r="H88" s="25">
+        <v>1</v>
+      </c>
+      <c r="I88" s="25">
+        <v>109</v>
+      </c>
+      <c r="J88" s="25">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="89" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A89" s="29">
+        <v>43989</v>
+      </c>
+      <c r="B89" s="30">
+        <v>83316</v>
+      </c>
+      <c r="C89" s="31">
+        <v>211</v>
+      </c>
+      <c r="D89" s="31">
+        <v>1485</v>
+      </c>
+      <c r="E89" s="31">
+        <v>0</v>
+      </c>
+      <c r="F89" s="31">
+        <v>5</v>
+      </c>
+      <c r="G89" s="31">
+        <v>0</v>
+      </c>
+      <c r="H89" s="31">
+        <v>0</v>
+      </c>
+      <c r="I89" s="31">
+        <v>109</v>
+      </c>
+      <c r="J89" s="31">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="90" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A90" s="20">
+        <v>43990</v>
+      </c>
+      <c r="B90" s="21">
+        <v>84130</v>
+      </c>
+      <c r="C90" s="22">
+        <v>814</v>
+      </c>
+      <c r="D90" s="22">
+        <v>1486</v>
+      </c>
+      <c r="E90" s="22">
+        <v>1</v>
+      </c>
+      <c r="F90" s="22">
+        <v>6</v>
+      </c>
+      <c r="G90" s="22">
+        <v>0</v>
+      </c>
+      <c r="H90" s="22">
+        <v>0</v>
+      </c>
+      <c r="I90" s="22">
+        <v>109</v>
+      </c>
+      <c r="J90" s="22">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="91" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A91" s="20">
+        <v>43991</v>
+      </c>
+      <c r="B91" s="21">
+        <v>84868</v>
+      </c>
+      <c r="C91" s="22">
+        <v>738</v>
+      </c>
+      <c r="D91" s="22">
+        <v>1488</v>
+      </c>
+      <c r="E91" s="22">
+        <v>2</v>
+      </c>
+      <c r="F91" s="22">
+        <v>6</v>
+      </c>
+      <c r="G91" s="22">
+        <v>0</v>
+      </c>
+      <c r="H91" s="22">
+        <v>0</v>
+      </c>
+      <c r="I91" s="22">
+        <v>109</v>
+      </c>
+      <c r="J91" s="22">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="92" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A92" s="23">
+        <v>43992</v>
+      </c>
+      <c r="B92" s="24">
+        <v>85626</v>
+      </c>
+      <c r="C92" s="25">
+        <v>758</v>
+      </c>
+      <c r="D92" s="25">
+        <v>1488</v>
+      </c>
+      <c r="E92" s="25">
+        <v>0</v>
+      </c>
+      <c r="F92" s="25">
+        <v>6</v>
+      </c>
+      <c r="G92" s="25">
+        <v>0</v>
+      </c>
+      <c r="H92" s="25">
+        <v>0</v>
+      </c>
+      <c r="I92" s="25">
+        <v>109</v>
+      </c>
+      <c r="J92" s="25">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="93" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A93" s="29">
+        <v>43993</v>
+      </c>
+      <c r="B93" s="30">
+        <v>86328</v>
+      </c>
+      <c r="C93" s="31">
+        <v>702</v>
+      </c>
+      <c r="D93" s="31">
+        <v>1490</v>
+      </c>
+      <c r="E93" s="31">
+        <v>2</v>
+      </c>
+      <c r="F93" s="31">
+        <v>6</v>
+      </c>
+      <c r="G93" s="31">
+        <v>0</v>
+      </c>
+      <c r="H93" s="31">
+        <v>0</v>
+      </c>
+      <c r="I93" s="31">
+        <v>109</v>
+      </c>
+      <c r="J93" s="31">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="94" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A94" s="23">
+        <v>43994</v>
+      </c>
+      <c r="B94" s="24">
+        <v>87095</v>
+      </c>
+      <c r="C94" s="25">
+        <v>767</v>
+      </c>
+      <c r="D94" s="25">
+        <v>1492</v>
+      </c>
+      <c r="E94" s="25">
+        <v>2</v>
+      </c>
+      <c r="F94" s="25">
+        <v>6</v>
+      </c>
+      <c r="G94" s="25">
+        <v>0</v>
+      </c>
+      <c r="H94" s="25">
+        <v>0</v>
+      </c>
+      <c r="I94" s="25">
+        <v>109</v>
+      </c>
+      <c r="J94" s="25">
+        <v>0</v>
+      </c>
+    </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>

</xml_diff>

<commit_message>
Data updated by GitHub Bot (2020-06-14 12)
</commit_message>
<xml_diff>
--- a/output/snapshot/fdcf2531-4c3e-5c02-b63c-ee160ead6dea.xlsx
+++ b/output/snapshot/fdcf2531-4c3e-5c02-b63c-ee160ead6dea.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="I:\AKTUALNI PODATKI - KORONA\Za objavo na GOV.SI\ang\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{1E6DD62F-2BE2-47DC-A7ED-9B57C1589256}" xr6:coauthVersionLast="44" xr6:coauthVersionMax="44" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{345DA3AE-6B75-4EC3-8AD2-163DF8D0F426}" xr6:coauthVersionLast="44" xr6:coauthVersionMax="44" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12576" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Covid-19 podatki" sheetId="1" r:id="rId1"/>
@@ -64,7 +64,7 @@
   <numFmts count="1">
     <numFmt numFmtId="164" formatCode="d/\ m/\ yyyy;@"/>
   </numFmts>
-  <fonts count="4" x14ac:knownFonts="1">
+  <fonts count="5" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -93,6 +93,13 @@
       <name val="Calibri Light"/>
       <scheme val="major"/>
     </font>
+    <font>
+      <sz val="10"/>
+      <color theme="1"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
   </fonts>
   <fills count="3">
     <fill>
@@ -108,7 +115,7 @@
       </patternFill>
     </fill>
   </fills>
-  <borders count="2">
+  <borders count="3">
     <border>
       <left/>
       <right/>
@@ -129,11 +136,26 @@
       <bottom/>
       <diagonal/>
     </border>
+    <border>
+      <left style="thin">
+        <color theme="4"/>
+      </left>
+      <right style="thin">
+        <color theme="4"/>
+      </right>
+      <top style="thin">
+        <color theme="4"/>
+      </top>
+      <bottom style="thin">
+        <color theme="4"/>
+      </bottom>
+      <diagonal/>
+    </border>
   </borders>
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="26">
+  <cellXfs count="32">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="49" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyAlignment="1" applyProtection="1">
       <alignment horizontal="left" vertical="top"/>
@@ -208,6 +230,24 @@
       <alignment horizontal="right"/>
     </xf>
     <xf numFmtId="0" fontId="3" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="right"/>
+    </xf>
+    <xf numFmtId="164" fontId="4" fillId="2" borderId="2" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="right" vertical="top"/>
+    </xf>
+    <xf numFmtId="3" fontId="4" fillId="2" borderId="2" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="right"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="2" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="right"/>
+    </xf>
+    <xf numFmtId="164" fontId="3" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="right" vertical="top"/>
+    </xf>
+    <xf numFmtId="3" fontId="3" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="right"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="right"/>
     </xf>
   </cellXfs>
@@ -399,8 +439,8 @@
 </file>
 
 <file path=xl/tables/table1.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="1" xr:uid="{00000000-000C-0000-FFFF-FFFF00000000}" name="Tabela1" displayName="Tabela1" ref="A1:J75" totalsRowShown="0" headerRowDxfId="11" dataDxfId="10">
-  <autoFilter ref="A1:J75" xr:uid="{00000000-0009-0000-0100-000001000000}">
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="1" xr:uid="{00000000-000C-0000-FFFF-FFFF00000000}" name="Tabela1" displayName="Tabela1" ref="A1:J95" totalsRowShown="0" headerRowDxfId="11" dataDxfId="10">
+  <autoFilter ref="A1:J95" xr:uid="{00000000-0009-0000-0100-000001000000}">
     <filterColumn colId="0" hiddenButton="1"/>
     <filterColumn colId="1" hiddenButton="1"/>
     <filterColumn colId="2" hiddenButton="1"/>
@@ -696,28 +736,28 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:J75"/>
+  <dimension ref="A1:J95"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A40" zoomScale="89" zoomScaleNormal="89" workbookViewId="0">
-      <selection activeCell="J74" sqref="J74"/>
+    <sheetView tabSelected="1" topLeftCell="A65" zoomScale="89" zoomScaleNormal="89" workbookViewId="0">
+      <selection activeCell="A95" sqref="A95:J95"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
-    <col min="1" max="1" width="12.7109375" style="1" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="13.5703125" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="16.28515625" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="15.28515625" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="17.85546875" bestFit="1" customWidth="1"/>
-    <col min="6" max="6" width="35.42578125" bestFit="1" customWidth="1"/>
-    <col min="7" max="7" width="51.140625" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="12.6640625" style="1" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="13.5546875" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="16.33203125" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="15.33203125" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="17.88671875" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="35.44140625" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="51.109375" bestFit="1" customWidth="1"/>
     <col min="8" max="8" width="14" bestFit="1" customWidth="1"/>
-    <col min="9" max="9" width="13.85546875" bestFit="1" customWidth="1"/>
-    <col min="10" max="10" width="16.5703125" bestFit="1" customWidth="1"/>
+    <col min="9" max="9" width="13.88671875" bestFit="1" customWidth="1"/>
+    <col min="10" max="10" width="16.5546875" bestFit="1" customWidth="1"/>
     <col min="11" max="11" width="29" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A1" s="2" t="s">
         <v>0</v>
       </c>
@@ -749,7 +789,7 @@
         <v>9</v>
       </c>
     </row>
-    <row r="2" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A2" s="4">
         <v>43902</v>
       </c>
@@ -781,7 +821,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="3" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A3" s="4">
         <v>43903</v>
       </c>
@@ -813,7 +853,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="4" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A4" s="4">
         <v>43904</v>
       </c>
@@ -845,7 +885,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="5" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A5" s="4">
         <v>43905</v>
       </c>
@@ -877,7 +917,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="6" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A6" s="4">
         <v>43906</v>
       </c>
@@ -909,7 +949,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="7" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A7" s="4">
         <v>43907</v>
       </c>
@@ -941,7 +981,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="8" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A8" s="4">
         <v>43908</v>
       </c>
@@ -973,7 +1013,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="9" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A9" s="4">
         <v>43909</v>
       </c>
@@ -1005,7 +1045,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="10" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="10" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A10" s="4">
         <v>43910</v>
       </c>
@@ -1037,7 +1077,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="11" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="11" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A11" s="4">
         <v>43911</v>
       </c>
@@ -1069,7 +1109,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="12" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="12" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A12" s="4">
         <v>43912</v>
       </c>
@@ -1101,7 +1141,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="13" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="13" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A13" s="4">
         <v>43913</v>
       </c>
@@ -1133,7 +1173,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="14" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="14" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A14" s="4">
         <v>43914</v>
       </c>
@@ -1165,7 +1205,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="15" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="15" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A15" s="4">
         <v>43915</v>
       </c>
@@ -1197,7 +1237,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="16" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="16" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A16" s="4">
         <v>43916</v>
       </c>
@@ -1229,7 +1269,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="17" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="17" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A17" s="6">
         <v>43917</v>
       </c>
@@ -1261,7 +1301,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="18" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="18" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A18" s="4">
         <v>43918</v>
       </c>
@@ -1293,7 +1333,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="19" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="19" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A19" s="4">
         <v>43919</v>
       </c>
@@ -1325,7 +1365,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="20" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="20" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A20" s="4">
         <v>43920</v>
       </c>
@@ -1357,7 +1397,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="21" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="21" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A21" s="4">
         <v>43921</v>
       </c>
@@ -1389,7 +1429,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="22" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="22" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A22" s="4">
         <v>43922</v>
       </c>
@@ -1421,7 +1461,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="23" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="23" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A23" s="4">
         <v>43923</v>
       </c>
@@ -1453,7 +1493,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="24" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="24" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A24" s="4">
         <v>43924</v>
       </c>
@@ -1485,7 +1525,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="25" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="25" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A25" s="4">
         <v>43925</v>
       </c>
@@ -1517,7 +1557,7 @@
         <v>6</v>
       </c>
     </row>
-    <row r="26" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="26" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A26" s="4">
         <v>43926</v>
       </c>
@@ -1549,7 +1589,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="27" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="27" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A27" s="4">
         <v>43927</v>
       </c>
@@ -1581,7 +1621,7 @@
         <v>6</v>
       </c>
     </row>
-    <row r="28" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="28" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A28" s="8">
         <v>43928</v>
       </c>
@@ -1613,7 +1653,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="29" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="29" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A29" s="4">
         <v>43929</v>
       </c>
@@ -1645,7 +1685,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="30" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="30" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A30" s="4">
         <v>43930</v>
       </c>
@@ -1677,7 +1717,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="31" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="31" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A31" s="4">
         <v>43931</v>
       </c>
@@ -1709,7 +1749,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="32" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="32" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A32" s="4">
         <v>43932</v>
       </c>
@@ -1741,7 +1781,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="33" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="33" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A33" s="4">
         <v>43933</v>
       </c>
@@ -1773,7 +1813,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="34" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="34" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A34" s="4">
         <v>43934</v>
       </c>
@@ -1805,7 +1845,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="35" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="35" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A35" s="4">
         <v>43935</v>
       </c>
@@ -1837,7 +1877,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="36" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="36" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A36" s="4">
         <v>43936</v>
       </c>
@@ -1869,7 +1909,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="37" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="37" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A37" s="4">
         <v>43937</v>
       </c>
@@ -1901,7 +1941,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="38" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="38" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A38" s="4">
         <v>43938</v>
       </c>
@@ -1933,7 +1973,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="39" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="39" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A39" s="4">
         <v>43939</v>
       </c>
@@ -1965,7 +2005,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="40" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="40" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A40" s="4">
         <v>43940</v>
       </c>
@@ -1997,7 +2037,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="41" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="41" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A41" s="4">
         <v>43941</v>
       </c>
@@ -2029,7 +2069,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="42" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="42" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A42" s="11">
         <v>43942</v>
       </c>
@@ -2061,7 +2101,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="43" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="43" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A43" s="4">
         <v>43943</v>
       </c>
@@ -2093,7 +2133,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="44" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="44" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A44" s="4">
         <v>43944</v>
       </c>
@@ -2125,7 +2165,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="45" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="45" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A45" s="4">
         <v>43945</v>
       </c>
@@ -2157,7 +2197,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="46" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="46" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A46" s="4">
         <v>43946</v>
       </c>
@@ -2189,7 +2229,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="47" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="47" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A47" s="8">
         <v>43947</v>
       </c>
@@ -2221,7 +2261,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="48" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="48" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A48" s="4">
         <v>43948</v>
       </c>
@@ -2253,7 +2293,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="49" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="49" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A49" s="4">
         <v>43949</v>
       </c>
@@ -2285,7 +2325,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="50" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="50" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A50" s="4">
         <v>43950</v>
       </c>
@@ -2317,7 +2357,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="51" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="51" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A51" s="14">
         <v>43951</v>
       </c>
@@ -2349,7 +2389,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="52" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="52" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A52" s="4">
         <v>43952</v>
       </c>
@@ -2381,7 +2421,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="53" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="53" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A53" s="4">
         <v>43953</v>
       </c>
@@ -2413,7 +2453,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="54" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="54" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A54" s="11">
         <v>43954</v>
       </c>
@@ -2445,7 +2485,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="55" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="55" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A55" s="4">
         <v>43955</v>
       </c>
@@ -2477,7 +2517,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="56" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="56" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A56" s="11">
         <v>43956</v>
       </c>
@@ -2509,7 +2549,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="57" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="57" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A57" s="4">
         <v>43957</v>
       </c>
@@ -2541,7 +2581,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="58" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="58" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A58" s="4">
         <v>43958</v>
       </c>
@@ -2573,7 +2613,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="59" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="59" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A59" s="4">
         <v>43959</v>
       </c>
@@ -2605,7 +2645,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="60" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="60" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A60" s="4">
         <v>43960</v>
       </c>
@@ -2637,7 +2677,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="61" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="61" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A61" s="4">
         <v>43961</v>
       </c>
@@ -2669,7 +2709,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="62" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="62" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A62" s="4">
         <v>43962</v>
       </c>
@@ -2701,7 +2741,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="63" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="63" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A63" s="4">
         <v>43963</v>
       </c>
@@ -2733,7 +2773,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="64" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="64" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A64" s="17">
         <v>43964</v>
       </c>
@@ -2765,7 +2805,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="65" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="65" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A65" s="14">
         <v>43965</v>
       </c>
@@ -2797,7 +2837,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="66" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="66" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A66" s="11">
         <v>43966</v>
       </c>
@@ -2829,7 +2869,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="67" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="67" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A67" s="14">
         <v>43967</v>
       </c>
@@ -2861,7 +2901,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="68" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="68" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A68" s="11">
         <v>43968</v>
       </c>
@@ -2893,7 +2933,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="69" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="69" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A69" s="14">
         <v>43969</v>
       </c>
@@ -2925,7 +2965,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="70" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="70" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A70" s="11">
         <v>43970</v>
       </c>
@@ -2957,7 +2997,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="71" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="71" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A71" s="20">
         <v>43971</v>
       </c>
@@ -2989,7 +3029,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="72" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="72" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A72" s="23">
         <v>43972</v>
       </c>
@@ -3021,7 +3061,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="73" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="73" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A73" s="20">
         <v>43973</v>
       </c>
@@ -3053,7 +3093,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="74" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="74" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A74" s="17">
         <v>43974</v>
       </c>
@@ -3085,7 +3125,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="75" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="75" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A75" s="20">
         <v>43975</v>
       </c>
@@ -3114,6 +3154,646 @@
         <v>107</v>
       </c>
       <c r="J75" s="22">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="76" spans="1:10" x14ac:dyDescent="0.3">
+      <c r="A76" s="20">
+        <v>43976</v>
+      </c>
+      <c r="B76" s="21">
+        <v>75770</v>
+      </c>
+      <c r="C76" s="22">
+        <v>754</v>
+      </c>
+      <c r="D76" s="22">
+        <v>1469</v>
+      </c>
+      <c r="E76" s="22">
+        <v>0</v>
+      </c>
+      <c r="F76" s="22">
+        <v>9</v>
+      </c>
+      <c r="G76" s="22">
+        <v>2</v>
+      </c>
+      <c r="H76" s="22">
+        <v>6</v>
+      </c>
+      <c r="I76" s="22">
+        <v>108</v>
+      </c>
+      <c r="J76" s="22">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="77" spans="1:10" x14ac:dyDescent="0.3">
+      <c r="A77" s="20">
+        <v>43977</v>
+      </c>
+      <c r="B77" s="21">
+        <v>76579</v>
+      </c>
+      <c r="C77" s="22">
+        <v>809</v>
+      </c>
+      <c r="D77" s="22">
+        <v>1471</v>
+      </c>
+      <c r="E77" s="22">
+        <v>2</v>
+      </c>
+      <c r="F77" s="22">
+        <v>8</v>
+      </c>
+      <c r="G77" s="22">
+        <v>2</v>
+      </c>
+      <c r="H77" s="22">
+        <v>2</v>
+      </c>
+      <c r="I77" s="22">
+        <v>108</v>
+      </c>
+      <c r="J77" s="22">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="78" spans="1:10" x14ac:dyDescent="0.3">
+      <c r="A78" s="20">
+        <v>43978</v>
+      </c>
+      <c r="B78" s="21">
+        <v>77210</v>
+      </c>
+      <c r="C78" s="22">
+        <v>631</v>
+      </c>
+      <c r="D78" s="22">
+        <v>1473</v>
+      </c>
+      <c r="E78" s="22">
+        <v>2</v>
+      </c>
+      <c r="F78" s="22">
+        <v>7</v>
+      </c>
+      <c r="G78" s="22">
+        <v>2</v>
+      </c>
+      <c r="H78" s="22">
+        <v>1</v>
+      </c>
+      <c r="I78" s="22">
+        <v>108</v>
+      </c>
+      <c r="J78" s="22">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="79" spans="1:10" x14ac:dyDescent="0.3">
+      <c r="A79" s="20">
+        <v>43979</v>
+      </c>
+      <c r="B79" s="21">
+        <v>77916</v>
+      </c>
+      <c r="C79" s="22">
+        <v>706</v>
+      </c>
+      <c r="D79" s="22">
+        <v>1473</v>
+      </c>
+      <c r="E79" s="22">
+        <v>0</v>
+      </c>
+      <c r="F79" s="22">
+        <v>7</v>
+      </c>
+      <c r="G79" s="22">
+        <v>2</v>
+      </c>
+      <c r="H79" s="22">
+        <v>0</v>
+      </c>
+      <c r="I79" s="22">
+        <v>108</v>
+      </c>
+      <c r="J79" s="22">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="80" spans="1:10" x14ac:dyDescent="0.3">
+      <c r="A80" s="20">
+        <v>43980</v>
+      </c>
+      <c r="B80" s="21">
+        <v>78529</v>
+      </c>
+      <c r="C80" s="22">
+        <v>613</v>
+      </c>
+      <c r="D80" s="22">
+        <v>1473</v>
+      </c>
+      <c r="E80" s="22">
+        <v>0</v>
+      </c>
+      <c r="F80" s="22">
+        <v>7</v>
+      </c>
+      <c r="G80" s="22">
+        <v>2</v>
+      </c>
+      <c r="H80" s="22">
+        <v>0</v>
+      </c>
+      <c r="I80" s="22">
+        <v>108</v>
+      </c>
+      <c r="J80" s="22">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="81" spans="1:10" x14ac:dyDescent="0.3">
+      <c r="A81" s="20">
+        <v>43981</v>
+      </c>
+      <c r="B81" s="22">
+        <v>78793</v>
+      </c>
+      <c r="C81" s="22">
+        <v>264</v>
+      </c>
+      <c r="D81" s="22">
+        <v>1473</v>
+      </c>
+      <c r="E81" s="22">
+        <v>0</v>
+      </c>
+      <c r="F81" s="22">
+        <v>6</v>
+      </c>
+      <c r="G81" s="22">
+        <v>2</v>
+      </c>
+      <c r="H81" s="22">
+        <v>1</v>
+      </c>
+      <c r="I81" s="22">
+        <v>108</v>
+      </c>
+      <c r="J81" s="22">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="82" spans="1:10" x14ac:dyDescent="0.3">
+      <c r="A82" s="20">
+        <v>43982</v>
+      </c>
+      <c r="B82" s="21">
+        <v>79039</v>
+      </c>
+      <c r="C82" s="22">
+        <v>246</v>
+      </c>
+      <c r="D82" s="22">
+        <v>1473</v>
+      </c>
+      <c r="E82" s="22">
+        <v>0</v>
+      </c>
+      <c r="F82" s="22">
+        <v>5</v>
+      </c>
+      <c r="G82" s="22">
+        <v>1</v>
+      </c>
+      <c r="H82" s="22">
+        <v>0</v>
+      </c>
+      <c r="I82" s="22">
+        <v>109</v>
+      </c>
+      <c r="J82" s="22">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="83" spans="1:10" x14ac:dyDescent="0.3">
+      <c r="A83" s="20">
+        <v>43983</v>
+      </c>
+      <c r="B83" s="21">
+        <v>79698</v>
+      </c>
+      <c r="C83" s="22">
+        <v>659</v>
+      </c>
+      <c r="D83" s="22">
+        <v>1475</v>
+      </c>
+      <c r="E83" s="22">
+        <v>2</v>
+      </c>
+      <c r="F83" s="22">
+        <v>5</v>
+      </c>
+      <c r="G83" s="22">
+        <v>1</v>
+      </c>
+      <c r="H83" s="22">
+        <v>0</v>
+      </c>
+      <c r="I83" s="22">
+        <v>109</v>
+      </c>
+      <c r="J83" s="22">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="84" spans="1:10" x14ac:dyDescent="0.3">
+      <c r="A84" s="20">
+        <v>43984</v>
+      </c>
+      <c r="B84" s="21">
+        <v>80505</v>
+      </c>
+      <c r="C84" s="22">
+        <v>807</v>
+      </c>
+      <c r="D84" s="22">
+        <v>1477</v>
+      </c>
+      <c r="E84" s="22">
+        <v>2</v>
+      </c>
+      <c r="F84" s="22">
+        <v>5</v>
+      </c>
+      <c r="G84" s="22">
+        <v>0</v>
+      </c>
+      <c r="H84" s="22">
+        <v>0</v>
+      </c>
+      <c r="I84" s="22">
+        <v>109</v>
+      </c>
+      <c r="J84" s="22">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="85" spans="1:10" x14ac:dyDescent="0.3">
+      <c r="A85" s="20">
+        <v>43985</v>
+      </c>
+      <c r="B85" s="21">
+        <v>81333</v>
+      </c>
+      <c r="C85" s="22">
+        <v>828</v>
+      </c>
+      <c r="D85" s="22">
+        <v>1477</v>
+      </c>
+      <c r="E85" s="22">
+        <v>0</v>
+      </c>
+      <c r="F85" s="22">
+        <v>5</v>
+      </c>
+      <c r="G85" s="22">
+        <v>0</v>
+      </c>
+      <c r="H85" s="22">
+        <v>0</v>
+      </c>
+      <c r="I85" s="22">
+        <v>109</v>
+      </c>
+      <c r="J85" s="22">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="86" spans="1:10" x14ac:dyDescent="0.3">
+      <c r="A86" s="26">
+        <v>43986</v>
+      </c>
+      <c r="B86" s="27">
+        <v>82161</v>
+      </c>
+      <c r="C86" s="28">
+        <v>828</v>
+      </c>
+      <c r="D86" s="28">
+        <v>1479</v>
+      </c>
+      <c r="E86" s="28">
+        <v>2</v>
+      </c>
+      <c r="F86" s="28">
+        <v>6</v>
+      </c>
+      <c r="G86" s="28">
+        <v>0</v>
+      </c>
+      <c r="H86" s="28">
+        <v>0</v>
+      </c>
+      <c r="I86" s="28">
+        <v>109</v>
+      </c>
+      <c r="J86" s="28">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="87" spans="1:10" x14ac:dyDescent="0.3">
+      <c r="A87" s="29">
+        <v>43987</v>
+      </c>
+      <c r="B87" s="30">
+        <v>82876</v>
+      </c>
+      <c r="C87" s="31">
+        <v>715</v>
+      </c>
+      <c r="D87" s="31">
+        <v>1484</v>
+      </c>
+      <c r="E87" s="31">
+        <v>5</v>
+      </c>
+      <c r="F87" s="31">
+        <v>6</v>
+      </c>
+      <c r="G87" s="31">
+        <v>0</v>
+      </c>
+      <c r="H87" s="31">
+        <v>0</v>
+      </c>
+      <c r="I87" s="31">
+        <v>109</v>
+      </c>
+      <c r="J87" s="31">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="88" spans="1:10" x14ac:dyDescent="0.3">
+      <c r="A88" s="23">
+        <v>43988</v>
+      </c>
+      <c r="B88" s="24">
+        <v>83105</v>
+      </c>
+      <c r="C88" s="25">
+        <v>229</v>
+      </c>
+      <c r="D88" s="25">
+        <v>1485</v>
+      </c>
+      <c r="E88" s="25">
+        <v>1</v>
+      </c>
+      <c r="F88" s="25">
+        <v>5</v>
+      </c>
+      <c r="G88" s="25">
+        <v>0</v>
+      </c>
+      <c r="H88" s="25">
+        <v>1</v>
+      </c>
+      <c r="I88" s="25">
+        <v>109</v>
+      </c>
+      <c r="J88" s="25">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="89" spans="1:10" x14ac:dyDescent="0.3">
+      <c r="A89" s="29">
+        <v>43989</v>
+      </c>
+      <c r="B89" s="30">
+        <v>83316</v>
+      </c>
+      <c r="C89" s="31">
+        <v>211</v>
+      </c>
+      <c r="D89" s="31">
+        <v>1485</v>
+      </c>
+      <c r="E89" s="31">
+        <v>0</v>
+      </c>
+      <c r="F89" s="31">
+        <v>5</v>
+      </c>
+      <c r="G89" s="31">
+        <v>0</v>
+      </c>
+      <c r="H89" s="31">
+        <v>0</v>
+      </c>
+      <c r="I89" s="31">
+        <v>109</v>
+      </c>
+      <c r="J89" s="31">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="90" spans="1:10" x14ac:dyDescent="0.3">
+      <c r="A90" s="20">
+        <v>43990</v>
+      </c>
+      <c r="B90" s="21">
+        <v>84130</v>
+      </c>
+      <c r="C90" s="22">
+        <v>814</v>
+      </c>
+      <c r="D90" s="22">
+        <v>1486</v>
+      </c>
+      <c r="E90" s="22">
+        <v>1</v>
+      </c>
+      <c r="F90" s="22">
+        <v>6</v>
+      </c>
+      <c r="G90" s="22">
+        <v>0</v>
+      </c>
+      <c r="H90" s="22">
+        <v>0</v>
+      </c>
+      <c r="I90" s="22">
+        <v>109</v>
+      </c>
+      <c r="J90" s="22">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="91" spans="1:10" x14ac:dyDescent="0.3">
+      <c r="A91" s="20">
+        <v>43991</v>
+      </c>
+      <c r="B91" s="21">
+        <v>84868</v>
+      </c>
+      <c r="C91" s="22">
+        <v>738</v>
+      </c>
+      <c r="D91" s="22">
+        <v>1488</v>
+      </c>
+      <c r="E91" s="22">
+        <v>2</v>
+      </c>
+      <c r="F91" s="22">
+        <v>6</v>
+      </c>
+      <c r="G91" s="22">
+        <v>0</v>
+      </c>
+      <c r="H91" s="22">
+        <v>0</v>
+      </c>
+      <c r="I91" s="22">
+        <v>109</v>
+      </c>
+      <c r="J91" s="22">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="92" spans="1:10" x14ac:dyDescent="0.3">
+      <c r="A92" s="23">
+        <v>43992</v>
+      </c>
+      <c r="B92" s="24">
+        <v>85626</v>
+      </c>
+      <c r="C92" s="25">
+        <v>758</v>
+      </c>
+      <c r="D92" s="25">
+        <v>1488</v>
+      </c>
+      <c r="E92" s="25">
+        <v>0</v>
+      </c>
+      <c r="F92" s="25">
+        <v>6</v>
+      </c>
+      <c r="G92" s="25">
+        <v>0</v>
+      </c>
+      <c r="H92" s="25">
+        <v>0</v>
+      </c>
+      <c r="I92" s="25">
+        <v>109</v>
+      </c>
+      <c r="J92" s="25">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="93" spans="1:10" x14ac:dyDescent="0.3">
+      <c r="A93" s="29">
+        <v>43993</v>
+      </c>
+      <c r="B93" s="30">
+        <v>86328</v>
+      </c>
+      <c r="C93" s="31">
+        <v>702</v>
+      </c>
+      <c r="D93" s="31">
+        <v>1490</v>
+      </c>
+      <c r="E93" s="31">
+        <v>2</v>
+      </c>
+      <c r="F93" s="31">
+        <v>6</v>
+      </c>
+      <c r="G93" s="31">
+        <v>0</v>
+      </c>
+      <c r="H93" s="31">
+        <v>0</v>
+      </c>
+      <c r="I93" s="31">
+        <v>109</v>
+      </c>
+      <c r="J93" s="31">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="94" spans="1:10" x14ac:dyDescent="0.3">
+      <c r="A94" s="23">
+        <v>43994</v>
+      </c>
+      <c r="B94" s="24">
+        <v>87095</v>
+      </c>
+      <c r="C94" s="25">
+        <v>767</v>
+      </c>
+      <c r="D94" s="25">
+        <v>1492</v>
+      </c>
+      <c r="E94" s="25">
+        <v>2</v>
+      </c>
+      <c r="F94" s="25">
+        <v>6</v>
+      </c>
+      <c r="G94" s="25">
+        <v>0</v>
+      </c>
+      <c r="H94" s="25">
+        <v>0</v>
+      </c>
+      <c r="I94" s="25">
+        <v>109</v>
+      </c>
+      <c r="J94" s="25">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="95" spans="1:10" x14ac:dyDescent="0.3">
+      <c r="A95" s="29">
+        <v>43995</v>
+      </c>
+      <c r="B95" s="30">
+        <v>87386</v>
+      </c>
+      <c r="C95" s="31">
+        <v>291</v>
+      </c>
+      <c r="D95" s="31">
+        <v>1495</v>
+      </c>
+      <c r="E95" s="31">
+        <v>3</v>
+      </c>
+      <c r="F95" s="31">
+        <v>6</v>
+      </c>
+      <c r="G95" s="31">
+        <v>0</v>
+      </c>
+      <c r="H95" s="31">
+        <v>0</v>
+      </c>
+      <c r="I95" s="31">
+        <v>109</v>
+      </c>
+      <c r="J95" s="31">
         <v>0</v>
       </c>
     </row>

</xml_diff>

<commit_message>
Data updated by GitHub Bot (2020-06-14 20)
</commit_message>
<xml_diff>
--- a/output/snapshot/fdcf2531-4c3e-5c02-b63c-ee160ead6dea.xlsx
+++ b/output/snapshot/fdcf2531-4c3e-5c02-b63c-ee160ead6dea.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="I:\AKTUALNI PODATKI - KORONA\Za objavo na GOV.SI\ang\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{1E6DD62F-2BE2-47DC-A7ED-9B57C1589256}" xr6:coauthVersionLast="44" xr6:coauthVersionMax="44" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{345DA3AE-6B75-4EC3-8AD2-163DF8D0F426}" xr6:coauthVersionLast="44" xr6:coauthVersionMax="44" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12576" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Covid-19 podatki" sheetId="1" r:id="rId1"/>
@@ -64,7 +64,7 @@
   <numFmts count="1">
     <numFmt numFmtId="164" formatCode="d/\ m/\ yyyy;@"/>
   </numFmts>
-  <fonts count="4" x14ac:knownFonts="1">
+  <fonts count="5" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -93,6 +93,13 @@
       <name val="Calibri Light"/>
       <scheme val="major"/>
     </font>
+    <font>
+      <sz val="10"/>
+      <color theme="1"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
   </fonts>
   <fills count="3">
     <fill>
@@ -108,7 +115,7 @@
       </patternFill>
     </fill>
   </fills>
-  <borders count="2">
+  <borders count="3">
     <border>
       <left/>
       <right/>
@@ -129,11 +136,26 @@
       <bottom/>
       <diagonal/>
     </border>
+    <border>
+      <left style="thin">
+        <color theme="4"/>
+      </left>
+      <right style="thin">
+        <color theme="4"/>
+      </right>
+      <top style="thin">
+        <color theme="4"/>
+      </top>
+      <bottom style="thin">
+        <color theme="4"/>
+      </bottom>
+      <diagonal/>
+    </border>
   </borders>
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="26">
+  <cellXfs count="32">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="49" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyAlignment="1" applyProtection="1">
       <alignment horizontal="left" vertical="top"/>
@@ -208,6 +230,24 @@
       <alignment horizontal="right"/>
     </xf>
     <xf numFmtId="0" fontId="3" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="right"/>
+    </xf>
+    <xf numFmtId="164" fontId="4" fillId="2" borderId="2" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="right" vertical="top"/>
+    </xf>
+    <xf numFmtId="3" fontId="4" fillId="2" borderId="2" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="right"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="2" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="right"/>
+    </xf>
+    <xf numFmtId="164" fontId="3" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="right" vertical="top"/>
+    </xf>
+    <xf numFmtId="3" fontId="3" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="right"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="right"/>
     </xf>
   </cellXfs>
@@ -399,8 +439,8 @@
 </file>
 
 <file path=xl/tables/table1.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="1" xr:uid="{00000000-000C-0000-FFFF-FFFF00000000}" name="Tabela1" displayName="Tabela1" ref="A1:J75" totalsRowShown="0" headerRowDxfId="11" dataDxfId="10">
-  <autoFilter ref="A1:J75" xr:uid="{00000000-0009-0000-0100-000001000000}">
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="1" xr:uid="{00000000-000C-0000-FFFF-FFFF00000000}" name="Tabela1" displayName="Tabela1" ref="A1:J95" totalsRowShown="0" headerRowDxfId="11" dataDxfId="10">
+  <autoFilter ref="A1:J95" xr:uid="{00000000-0009-0000-0100-000001000000}">
     <filterColumn colId="0" hiddenButton="1"/>
     <filterColumn colId="1" hiddenButton="1"/>
     <filterColumn colId="2" hiddenButton="1"/>
@@ -696,28 +736,28 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:J75"/>
+  <dimension ref="A1:J95"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A40" zoomScale="89" zoomScaleNormal="89" workbookViewId="0">
-      <selection activeCell="J74" sqref="J74"/>
+    <sheetView tabSelected="1" topLeftCell="A65" zoomScale="89" zoomScaleNormal="89" workbookViewId="0">
+      <selection activeCell="A95" sqref="A95:J95"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
-    <col min="1" max="1" width="12.7109375" style="1" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="13.5703125" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="16.28515625" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="15.28515625" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="17.85546875" bestFit="1" customWidth="1"/>
-    <col min="6" max="6" width="35.42578125" bestFit="1" customWidth="1"/>
-    <col min="7" max="7" width="51.140625" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="12.6640625" style="1" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="13.5546875" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="16.33203125" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="15.33203125" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="17.88671875" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="35.44140625" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="51.109375" bestFit="1" customWidth="1"/>
     <col min="8" max="8" width="14" bestFit="1" customWidth="1"/>
-    <col min="9" max="9" width="13.85546875" bestFit="1" customWidth="1"/>
-    <col min="10" max="10" width="16.5703125" bestFit="1" customWidth="1"/>
+    <col min="9" max="9" width="13.88671875" bestFit="1" customWidth="1"/>
+    <col min="10" max="10" width="16.5546875" bestFit="1" customWidth="1"/>
     <col min="11" max="11" width="29" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A1" s="2" t="s">
         <v>0</v>
       </c>
@@ -749,7 +789,7 @@
         <v>9</v>
       </c>
     </row>
-    <row r="2" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A2" s="4">
         <v>43902</v>
       </c>
@@ -781,7 +821,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="3" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A3" s="4">
         <v>43903</v>
       </c>
@@ -813,7 +853,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="4" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A4" s="4">
         <v>43904</v>
       </c>
@@ -845,7 +885,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="5" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A5" s="4">
         <v>43905</v>
       </c>
@@ -877,7 +917,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="6" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A6" s="4">
         <v>43906</v>
       </c>
@@ -909,7 +949,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="7" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A7" s="4">
         <v>43907</v>
       </c>
@@ -941,7 +981,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="8" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A8" s="4">
         <v>43908</v>
       </c>
@@ -973,7 +1013,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="9" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A9" s="4">
         <v>43909</v>
       </c>
@@ -1005,7 +1045,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="10" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="10" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A10" s="4">
         <v>43910</v>
       </c>
@@ -1037,7 +1077,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="11" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="11" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A11" s="4">
         <v>43911</v>
       </c>
@@ -1069,7 +1109,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="12" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="12" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A12" s="4">
         <v>43912</v>
       </c>
@@ -1101,7 +1141,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="13" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="13" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A13" s="4">
         <v>43913</v>
       </c>
@@ -1133,7 +1173,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="14" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="14" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A14" s="4">
         <v>43914</v>
       </c>
@@ -1165,7 +1205,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="15" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="15" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A15" s="4">
         <v>43915</v>
       </c>
@@ -1197,7 +1237,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="16" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="16" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A16" s="4">
         <v>43916</v>
       </c>
@@ -1229,7 +1269,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="17" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="17" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A17" s="6">
         <v>43917</v>
       </c>
@@ -1261,7 +1301,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="18" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="18" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A18" s="4">
         <v>43918</v>
       </c>
@@ -1293,7 +1333,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="19" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="19" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A19" s="4">
         <v>43919</v>
       </c>
@@ -1325,7 +1365,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="20" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="20" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A20" s="4">
         <v>43920</v>
       </c>
@@ -1357,7 +1397,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="21" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="21" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A21" s="4">
         <v>43921</v>
       </c>
@@ -1389,7 +1429,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="22" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="22" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A22" s="4">
         <v>43922</v>
       </c>
@@ -1421,7 +1461,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="23" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="23" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A23" s="4">
         <v>43923</v>
       </c>
@@ -1453,7 +1493,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="24" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="24" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A24" s="4">
         <v>43924</v>
       </c>
@@ -1485,7 +1525,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="25" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="25" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A25" s="4">
         <v>43925</v>
       </c>
@@ -1517,7 +1557,7 @@
         <v>6</v>
       </c>
     </row>
-    <row r="26" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="26" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A26" s="4">
         <v>43926</v>
       </c>
@@ -1549,7 +1589,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="27" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="27" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A27" s="4">
         <v>43927</v>
       </c>
@@ -1581,7 +1621,7 @@
         <v>6</v>
       </c>
     </row>
-    <row r="28" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="28" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A28" s="8">
         <v>43928</v>
       </c>
@@ -1613,7 +1653,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="29" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="29" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A29" s="4">
         <v>43929</v>
       </c>
@@ -1645,7 +1685,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="30" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="30" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A30" s="4">
         <v>43930</v>
       </c>
@@ -1677,7 +1717,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="31" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="31" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A31" s="4">
         <v>43931</v>
       </c>
@@ -1709,7 +1749,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="32" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="32" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A32" s="4">
         <v>43932</v>
       </c>
@@ -1741,7 +1781,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="33" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="33" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A33" s="4">
         <v>43933</v>
       </c>
@@ -1773,7 +1813,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="34" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="34" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A34" s="4">
         <v>43934</v>
       </c>
@@ -1805,7 +1845,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="35" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="35" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A35" s="4">
         <v>43935</v>
       </c>
@@ -1837,7 +1877,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="36" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="36" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A36" s="4">
         <v>43936</v>
       </c>
@@ -1869,7 +1909,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="37" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="37" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A37" s="4">
         <v>43937</v>
       </c>
@@ -1901,7 +1941,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="38" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="38" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A38" s="4">
         <v>43938</v>
       </c>
@@ -1933,7 +1973,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="39" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="39" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A39" s="4">
         <v>43939</v>
       </c>
@@ -1965,7 +2005,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="40" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="40" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A40" s="4">
         <v>43940</v>
       </c>
@@ -1997,7 +2037,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="41" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="41" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A41" s="4">
         <v>43941</v>
       </c>
@@ -2029,7 +2069,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="42" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="42" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A42" s="11">
         <v>43942</v>
       </c>
@@ -2061,7 +2101,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="43" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="43" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A43" s="4">
         <v>43943</v>
       </c>
@@ -2093,7 +2133,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="44" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="44" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A44" s="4">
         <v>43944</v>
       </c>
@@ -2125,7 +2165,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="45" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="45" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A45" s="4">
         <v>43945</v>
       </c>
@@ -2157,7 +2197,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="46" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="46" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A46" s="4">
         <v>43946</v>
       </c>
@@ -2189,7 +2229,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="47" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="47" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A47" s="8">
         <v>43947</v>
       </c>
@@ -2221,7 +2261,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="48" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="48" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A48" s="4">
         <v>43948</v>
       </c>
@@ -2253,7 +2293,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="49" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="49" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A49" s="4">
         <v>43949</v>
       </c>
@@ -2285,7 +2325,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="50" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="50" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A50" s="4">
         <v>43950</v>
       </c>
@@ -2317,7 +2357,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="51" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="51" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A51" s="14">
         <v>43951</v>
       </c>
@@ -2349,7 +2389,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="52" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="52" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A52" s="4">
         <v>43952</v>
       </c>
@@ -2381,7 +2421,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="53" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="53" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A53" s="4">
         <v>43953</v>
       </c>
@@ -2413,7 +2453,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="54" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="54" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A54" s="11">
         <v>43954</v>
       </c>
@@ -2445,7 +2485,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="55" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="55" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A55" s="4">
         <v>43955</v>
       </c>
@@ -2477,7 +2517,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="56" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="56" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A56" s="11">
         <v>43956</v>
       </c>
@@ -2509,7 +2549,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="57" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="57" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A57" s="4">
         <v>43957</v>
       </c>
@@ -2541,7 +2581,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="58" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="58" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A58" s="4">
         <v>43958</v>
       </c>
@@ -2573,7 +2613,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="59" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="59" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A59" s="4">
         <v>43959</v>
       </c>
@@ -2605,7 +2645,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="60" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="60" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A60" s="4">
         <v>43960</v>
       </c>
@@ -2637,7 +2677,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="61" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="61" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A61" s="4">
         <v>43961</v>
       </c>
@@ -2669,7 +2709,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="62" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="62" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A62" s="4">
         <v>43962</v>
       </c>
@@ -2701,7 +2741,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="63" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="63" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A63" s="4">
         <v>43963</v>
       </c>
@@ -2733,7 +2773,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="64" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="64" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A64" s="17">
         <v>43964</v>
       </c>
@@ -2765,7 +2805,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="65" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="65" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A65" s="14">
         <v>43965</v>
       </c>
@@ -2797,7 +2837,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="66" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="66" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A66" s="11">
         <v>43966</v>
       </c>
@@ -2829,7 +2869,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="67" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="67" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A67" s="14">
         <v>43967</v>
       </c>
@@ -2861,7 +2901,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="68" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="68" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A68" s="11">
         <v>43968</v>
       </c>
@@ -2893,7 +2933,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="69" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="69" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A69" s="14">
         <v>43969</v>
       </c>
@@ -2925,7 +2965,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="70" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="70" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A70" s="11">
         <v>43970</v>
       </c>
@@ -2957,7 +2997,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="71" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="71" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A71" s="20">
         <v>43971</v>
       </c>
@@ -2989,7 +3029,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="72" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="72" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A72" s="23">
         <v>43972</v>
       </c>
@@ -3021,7 +3061,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="73" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="73" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A73" s="20">
         <v>43973</v>
       </c>
@@ -3053,7 +3093,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="74" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="74" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A74" s="17">
         <v>43974</v>
       </c>
@@ -3085,7 +3125,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="75" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="75" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A75" s="20">
         <v>43975</v>
       </c>
@@ -3114,6 +3154,646 @@
         <v>107</v>
       </c>
       <c r="J75" s="22">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="76" spans="1:10" x14ac:dyDescent="0.3">
+      <c r="A76" s="20">
+        <v>43976</v>
+      </c>
+      <c r="B76" s="21">
+        <v>75770</v>
+      </c>
+      <c r="C76" s="22">
+        <v>754</v>
+      </c>
+      <c r="D76" s="22">
+        <v>1469</v>
+      </c>
+      <c r="E76" s="22">
+        <v>0</v>
+      </c>
+      <c r="F76" s="22">
+        <v>9</v>
+      </c>
+      <c r="G76" s="22">
+        <v>2</v>
+      </c>
+      <c r="H76" s="22">
+        <v>6</v>
+      </c>
+      <c r="I76" s="22">
+        <v>108</v>
+      </c>
+      <c r="J76" s="22">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="77" spans="1:10" x14ac:dyDescent="0.3">
+      <c r="A77" s="20">
+        <v>43977</v>
+      </c>
+      <c r="B77" s="21">
+        <v>76579</v>
+      </c>
+      <c r="C77" s="22">
+        <v>809</v>
+      </c>
+      <c r="D77" s="22">
+        <v>1471</v>
+      </c>
+      <c r="E77" s="22">
+        <v>2</v>
+      </c>
+      <c r="F77" s="22">
+        <v>8</v>
+      </c>
+      <c r="G77" s="22">
+        <v>2</v>
+      </c>
+      <c r="H77" s="22">
+        <v>2</v>
+      </c>
+      <c r="I77" s="22">
+        <v>108</v>
+      </c>
+      <c r="J77" s="22">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="78" spans="1:10" x14ac:dyDescent="0.3">
+      <c r="A78" s="20">
+        <v>43978</v>
+      </c>
+      <c r="B78" s="21">
+        <v>77210</v>
+      </c>
+      <c r="C78" s="22">
+        <v>631</v>
+      </c>
+      <c r="D78" s="22">
+        <v>1473</v>
+      </c>
+      <c r="E78" s="22">
+        <v>2</v>
+      </c>
+      <c r="F78" s="22">
+        <v>7</v>
+      </c>
+      <c r="G78" s="22">
+        <v>2</v>
+      </c>
+      <c r="H78" s="22">
+        <v>1</v>
+      </c>
+      <c r="I78" s="22">
+        <v>108</v>
+      </c>
+      <c r="J78" s="22">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="79" spans="1:10" x14ac:dyDescent="0.3">
+      <c r="A79" s="20">
+        <v>43979</v>
+      </c>
+      <c r="B79" s="21">
+        <v>77916</v>
+      </c>
+      <c r="C79" s="22">
+        <v>706</v>
+      </c>
+      <c r="D79" s="22">
+        <v>1473</v>
+      </c>
+      <c r="E79" s="22">
+        <v>0</v>
+      </c>
+      <c r="F79" s="22">
+        <v>7</v>
+      </c>
+      <c r="G79" s="22">
+        <v>2</v>
+      </c>
+      <c r="H79" s="22">
+        <v>0</v>
+      </c>
+      <c r="I79" s="22">
+        <v>108</v>
+      </c>
+      <c r="J79" s="22">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="80" spans="1:10" x14ac:dyDescent="0.3">
+      <c r="A80" s="20">
+        <v>43980</v>
+      </c>
+      <c r="B80" s="21">
+        <v>78529</v>
+      </c>
+      <c r="C80" s="22">
+        <v>613</v>
+      </c>
+      <c r="D80" s="22">
+        <v>1473</v>
+      </c>
+      <c r="E80" s="22">
+        <v>0</v>
+      </c>
+      <c r="F80" s="22">
+        <v>7</v>
+      </c>
+      <c r="G80" s="22">
+        <v>2</v>
+      </c>
+      <c r="H80" s="22">
+        <v>0</v>
+      </c>
+      <c r="I80" s="22">
+        <v>108</v>
+      </c>
+      <c r="J80" s="22">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="81" spans="1:10" x14ac:dyDescent="0.3">
+      <c r="A81" s="20">
+        <v>43981</v>
+      </c>
+      <c r="B81" s="22">
+        <v>78793</v>
+      </c>
+      <c r="C81" s="22">
+        <v>264</v>
+      </c>
+      <c r="D81" s="22">
+        <v>1473</v>
+      </c>
+      <c r="E81" s="22">
+        <v>0</v>
+      </c>
+      <c r="F81" s="22">
+        <v>6</v>
+      </c>
+      <c r="G81" s="22">
+        <v>2</v>
+      </c>
+      <c r="H81" s="22">
+        <v>1</v>
+      </c>
+      <c r="I81" s="22">
+        <v>108</v>
+      </c>
+      <c r="J81" s="22">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="82" spans="1:10" x14ac:dyDescent="0.3">
+      <c r="A82" s="20">
+        <v>43982</v>
+      </c>
+      <c r="B82" s="21">
+        <v>79039</v>
+      </c>
+      <c r="C82" s="22">
+        <v>246</v>
+      </c>
+      <c r="D82" s="22">
+        <v>1473</v>
+      </c>
+      <c r="E82" s="22">
+        <v>0</v>
+      </c>
+      <c r="F82" s="22">
+        <v>5</v>
+      </c>
+      <c r="G82" s="22">
+        <v>1</v>
+      </c>
+      <c r="H82" s="22">
+        <v>0</v>
+      </c>
+      <c r="I82" s="22">
+        <v>109</v>
+      </c>
+      <c r="J82" s="22">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="83" spans="1:10" x14ac:dyDescent="0.3">
+      <c r="A83" s="20">
+        <v>43983</v>
+      </c>
+      <c r="B83" s="21">
+        <v>79698</v>
+      </c>
+      <c r="C83" s="22">
+        <v>659</v>
+      </c>
+      <c r="D83" s="22">
+        <v>1475</v>
+      </c>
+      <c r="E83" s="22">
+        <v>2</v>
+      </c>
+      <c r="F83" s="22">
+        <v>5</v>
+      </c>
+      <c r="G83" s="22">
+        <v>1</v>
+      </c>
+      <c r="H83" s="22">
+        <v>0</v>
+      </c>
+      <c r="I83" s="22">
+        <v>109</v>
+      </c>
+      <c r="J83" s="22">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="84" spans="1:10" x14ac:dyDescent="0.3">
+      <c r="A84" s="20">
+        <v>43984</v>
+      </c>
+      <c r="B84" s="21">
+        <v>80505</v>
+      </c>
+      <c r="C84" s="22">
+        <v>807</v>
+      </c>
+      <c r="D84" s="22">
+        <v>1477</v>
+      </c>
+      <c r="E84" s="22">
+        <v>2</v>
+      </c>
+      <c r="F84" s="22">
+        <v>5</v>
+      </c>
+      <c r="G84" s="22">
+        <v>0</v>
+      </c>
+      <c r="H84" s="22">
+        <v>0</v>
+      </c>
+      <c r="I84" s="22">
+        <v>109</v>
+      </c>
+      <c r="J84" s="22">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="85" spans="1:10" x14ac:dyDescent="0.3">
+      <c r="A85" s="20">
+        <v>43985</v>
+      </c>
+      <c r="B85" s="21">
+        <v>81333</v>
+      </c>
+      <c r="C85" s="22">
+        <v>828</v>
+      </c>
+      <c r="D85" s="22">
+        <v>1477</v>
+      </c>
+      <c r="E85" s="22">
+        <v>0</v>
+      </c>
+      <c r="F85" s="22">
+        <v>5</v>
+      </c>
+      <c r="G85" s="22">
+        <v>0</v>
+      </c>
+      <c r="H85" s="22">
+        <v>0</v>
+      </c>
+      <c r="I85" s="22">
+        <v>109</v>
+      </c>
+      <c r="J85" s="22">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="86" spans="1:10" x14ac:dyDescent="0.3">
+      <c r="A86" s="26">
+        <v>43986</v>
+      </c>
+      <c r="B86" s="27">
+        <v>82161</v>
+      </c>
+      <c r="C86" s="28">
+        <v>828</v>
+      </c>
+      <c r="D86" s="28">
+        <v>1479</v>
+      </c>
+      <c r="E86" s="28">
+        <v>2</v>
+      </c>
+      <c r="F86" s="28">
+        <v>6</v>
+      </c>
+      <c r="G86" s="28">
+        <v>0</v>
+      </c>
+      <c r="H86" s="28">
+        <v>0</v>
+      </c>
+      <c r="I86" s="28">
+        <v>109</v>
+      </c>
+      <c r="J86" s="28">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="87" spans="1:10" x14ac:dyDescent="0.3">
+      <c r="A87" s="29">
+        <v>43987</v>
+      </c>
+      <c r="B87" s="30">
+        <v>82876</v>
+      </c>
+      <c r="C87" s="31">
+        <v>715</v>
+      </c>
+      <c r="D87" s="31">
+        <v>1484</v>
+      </c>
+      <c r="E87" s="31">
+        <v>5</v>
+      </c>
+      <c r="F87" s="31">
+        <v>6</v>
+      </c>
+      <c r="G87" s="31">
+        <v>0</v>
+      </c>
+      <c r="H87" s="31">
+        <v>0</v>
+      </c>
+      <c r="I87" s="31">
+        <v>109</v>
+      </c>
+      <c r="J87" s="31">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="88" spans="1:10" x14ac:dyDescent="0.3">
+      <c r="A88" s="23">
+        <v>43988</v>
+      </c>
+      <c r="B88" s="24">
+        <v>83105</v>
+      </c>
+      <c r="C88" s="25">
+        <v>229</v>
+      </c>
+      <c r="D88" s="25">
+        <v>1485</v>
+      </c>
+      <c r="E88" s="25">
+        <v>1</v>
+      </c>
+      <c r="F88" s="25">
+        <v>5</v>
+      </c>
+      <c r="G88" s="25">
+        <v>0</v>
+      </c>
+      <c r="H88" s="25">
+        <v>1</v>
+      </c>
+      <c r="I88" s="25">
+        <v>109</v>
+      </c>
+      <c r="J88" s="25">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="89" spans="1:10" x14ac:dyDescent="0.3">
+      <c r="A89" s="29">
+        <v>43989</v>
+      </c>
+      <c r="B89" s="30">
+        <v>83316</v>
+      </c>
+      <c r="C89" s="31">
+        <v>211</v>
+      </c>
+      <c r="D89" s="31">
+        <v>1485</v>
+      </c>
+      <c r="E89" s="31">
+        <v>0</v>
+      </c>
+      <c r="F89" s="31">
+        <v>5</v>
+      </c>
+      <c r="G89" s="31">
+        <v>0</v>
+      </c>
+      <c r="H89" s="31">
+        <v>0</v>
+      </c>
+      <c r="I89" s="31">
+        <v>109</v>
+      </c>
+      <c r="J89" s="31">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="90" spans="1:10" x14ac:dyDescent="0.3">
+      <c r="A90" s="20">
+        <v>43990</v>
+      </c>
+      <c r="B90" s="21">
+        <v>84130</v>
+      </c>
+      <c r="C90" s="22">
+        <v>814</v>
+      </c>
+      <c r="D90" s="22">
+        <v>1486</v>
+      </c>
+      <c r="E90" s="22">
+        <v>1</v>
+      </c>
+      <c r="F90" s="22">
+        <v>6</v>
+      </c>
+      <c r="G90" s="22">
+        <v>0</v>
+      </c>
+      <c r="H90" s="22">
+        <v>0</v>
+      </c>
+      <c r="I90" s="22">
+        <v>109</v>
+      </c>
+      <c r="J90" s="22">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="91" spans="1:10" x14ac:dyDescent="0.3">
+      <c r="A91" s="20">
+        <v>43991</v>
+      </c>
+      <c r="B91" s="21">
+        <v>84868</v>
+      </c>
+      <c r="C91" s="22">
+        <v>738</v>
+      </c>
+      <c r="D91" s="22">
+        <v>1488</v>
+      </c>
+      <c r="E91" s="22">
+        <v>2</v>
+      </c>
+      <c r="F91" s="22">
+        <v>6</v>
+      </c>
+      <c r="G91" s="22">
+        <v>0</v>
+      </c>
+      <c r="H91" s="22">
+        <v>0</v>
+      </c>
+      <c r="I91" s="22">
+        <v>109</v>
+      </c>
+      <c r="J91" s="22">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="92" spans="1:10" x14ac:dyDescent="0.3">
+      <c r="A92" s="23">
+        <v>43992</v>
+      </c>
+      <c r="B92" s="24">
+        <v>85626</v>
+      </c>
+      <c r="C92" s="25">
+        <v>758</v>
+      </c>
+      <c r="D92" s="25">
+        <v>1488</v>
+      </c>
+      <c r="E92" s="25">
+        <v>0</v>
+      </c>
+      <c r="F92" s="25">
+        <v>6</v>
+      </c>
+      <c r="G92" s="25">
+        <v>0</v>
+      </c>
+      <c r="H92" s="25">
+        <v>0</v>
+      </c>
+      <c r="I92" s="25">
+        <v>109</v>
+      </c>
+      <c r="J92" s="25">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="93" spans="1:10" x14ac:dyDescent="0.3">
+      <c r="A93" s="29">
+        <v>43993</v>
+      </c>
+      <c r="B93" s="30">
+        <v>86328</v>
+      </c>
+      <c r="C93" s="31">
+        <v>702</v>
+      </c>
+      <c r="D93" s="31">
+        <v>1490</v>
+      </c>
+      <c r="E93" s="31">
+        <v>2</v>
+      </c>
+      <c r="F93" s="31">
+        <v>6</v>
+      </c>
+      <c r="G93" s="31">
+        <v>0</v>
+      </c>
+      <c r="H93" s="31">
+        <v>0</v>
+      </c>
+      <c r="I93" s="31">
+        <v>109</v>
+      </c>
+      <c r="J93" s="31">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="94" spans="1:10" x14ac:dyDescent="0.3">
+      <c r="A94" s="23">
+        <v>43994</v>
+      </c>
+      <c r="B94" s="24">
+        <v>87095</v>
+      </c>
+      <c r="C94" s="25">
+        <v>767</v>
+      </c>
+      <c r="D94" s="25">
+        <v>1492</v>
+      </c>
+      <c r="E94" s="25">
+        <v>2</v>
+      </c>
+      <c r="F94" s="25">
+        <v>6</v>
+      </c>
+      <c r="G94" s="25">
+        <v>0</v>
+      </c>
+      <c r="H94" s="25">
+        <v>0</v>
+      </c>
+      <c r="I94" s="25">
+        <v>109</v>
+      </c>
+      <c r="J94" s="25">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="95" spans="1:10" x14ac:dyDescent="0.3">
+      <c r="A95" s="29">
+        <v>43995</v>
+      </c>
+      <c r="B95" s="30">
+        <v>87386</v>
+      </c>
+      <c r="C95" s="31">
+        <v>291</v>
+      </c>
+      <c r="D95" s="31">
+        <v>1495</v>
+      </c>
+      <c r="E95" s="31">
+        <v>3</v>
+      </c>
+      <c r="F95" s="31">
+        <v>6</v>
+      </c>
+      <c r="G95" s="31">
+        <v>0</v>
+      </c>
+      <c r="H95" s="31">
+        <v>0</v>
+      </c>
+      <c r="I95" s="31">
+        <v>109</v>
+      </c>
+      <c r="J95" s="31">
         <v>0</v>
       </c>
     </row>

</xml_diff>

<commit_message>
Data updated by GitHub Bot (2020-06-15 12)
</commit_message>
<xml_diff>
--- a/output/snapshot/fdcf2531-4c3e-5c02-b63c-ee160ead6dea.xlsx
+++ b/output/snapshot/fdcf2531-4c3e-5c02-b63c-ee160ead6dea.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="I:\AKTUALNI PODATKI - KORONA\Za objavo na GOV.SI\ang\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{1E6DD62F-2BE2-47DC-A7ED-9B57C1589256}" xr6:coauthVersionLast="44" xr6:coauthVersionMax="44" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{B641C904-F5E5-45C5-93A6-81E74361D8EC}" xr6:coauthVersionLast="44" xr6:coauthVersionMax="44" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="2295" yWindow="2295" windowWidth="21600" windowHeight="11205" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Covid-19 podatki" sheetId="1" r:id="rId1"/>
@@ -64,7 +64,7 @@
   <numFmts count="1">
     <numFmt numFmtId="164" formatCode="d/\ m/\ yyyy;@"/>
   </numFmts>
-  <fonts count="4" x14ac:knownFonts="1">
+  <fonts count="5" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -93,6 +93,13 @@
       <name val="Calibri Light"/>
       <scheme val="major"/>
     </font>
+    <font>
+      <sz val="10"/>
+      <color theme="1"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
   </fonts>
   <fills count="3">
     <fill>
@@ -108,7 +115,7 @@
       </patternFill>
     </fill>
   </fills>
-  <borders count="2">
+  <borders count="3">
     <border>
       <left/>
       <right/>
@@ -129,11 +136,26 @@
       <bottom/>
       <diagonal/>
     </border>
+    <border>
+      <left style="thin">
+        <color theme="4"/>
+      </left>
+      <right style="thin">
+        <color theme="4"/>
+      </right>
+      <top style="thin">
+        <color theme="4"/>
+      </top>
+      <bottom style="thin">
+        <color theme="4"/>
+      </bottom>
+      <diagonal/>
+    </border>
   </borders>
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="26">
+  <cellXfs count="32">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="49" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyAlignment="1" applyProtection="1">
       <alignment horizontal="left" vertical="top"/>
@@ -208,6 +230,24 @@
       <alignment horizontal="right"/>
     </xf>
     <xf numFmtId="0" fontId="3" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="right"/>
+    </xf>
+    <xf numFmtId="164" fontId="4" fillId="2" borderId="2" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="right" vertical="top"/>
+    </xf>
+    <xf numFmtId="3" fontId="4" fillId="2" borderId="2" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="right"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="2" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="right"/>
+    </xf>
+    <xf numFmtId="164" fontId="3" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="right" vertical="top"/>
+    </xf>
+    <xf numFmtId="3" fontId="3" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="right"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="right"/>
     </xf>
   </cellXfs>
@@ -399,8 +439,8 @@
 </file>
 
 <file path=xl/tables/table1.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="1" xr:uid="{00000000-000C-0000-FFFF-FFFF00000000}" name="Tabela1" displayName="Tabela1" ref="A1:J75" totalsRowShown="0" headerRowDxfId="11" dataDxfId="10">
-  <autoFilter ref="A1:J75" xr:uid="{00000000-0009-0000-0100-000001000000}">
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="1" xr:uid="{00000000-000C-0000-FFFF-FFFF00000000}" name="Tabela1" displayName="Tabela1" ref="A1:J96" totalsRowShown="0" headerRowDxfId="11" dataDxfId="10">
+  <autoFilter ref="A1:J96" xr:uid="{00000000-0009-0000-0100-000001000000}">
     <filterColumn colId="0" hiddenButton="1"/>
     <filterColumn colId="1" hiddenButton="1"/>
     <filterColumn colId="2" hiddenButton="1"/>
@@ -696,10 +736,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:J75"/>
+  <dimension ref="A1:J96"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A40" zoomScale="89" zoomScaleNormal="89" workbookViewId="0">
-      <selection activeCell="J74" sqref="J74"/>
+    <sheetView tabSelected="1" topLeftCell="A77" zoomScale="89" zoomScaleNormal="89" workbookViewId="0">
+      <selection activeCell="A96" sqref="A96:J96"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -3117,6 +3157,678 @@
         <v>0</v>
       </c>
     </row>
+    <row r="76" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A76" s="20">
+        <v>43976</v>
+      </c>
+      <c r="B76" s="21">
+        <v>75770</v>
+      </c>
+      <c r="C76" s="22">
+        <v>754</v>
+      </c>
+      <c r="D76" s="22">
+        <v>1469</v>
+      </c>
+      <c r="E76" s="22">
+        <v>0</v>
+      </c>
+      <c r="F76" s="22">
+        <v>9</v>
+      </c>
+      <c r="G76" s="22">
+        <v>2</v>
+      </c>
+      <c r="H76" s="22">
+        <v>6</v>
+      </c>
+      <c r="I76" s="22">
+        <v>108</v>
+      </c>
+      <c r="J76" s="22">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="77" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A77" s="20">
+        <v>43977</v>
+      </c>
+      <c r="B77" s="21">
+        <v>76579</v>
+      </c>
+      <c r="C77" s="22">
+        <v>809</v>
+      </c>
+      <c r="D77" s="22">
+        <v>1471</v>
+      </c>
+      <c r="E77" s="22">
+        <v>2</v>
+      </c>
+      <c r="F77" s="22">
+        <v>8</v>
+      </c>
+      <c r="G77" s="22">
+        <v>2</v>
+      </c>
+      <c r="H77" s="22">
+        <v>2</v>
+      </c>
+      <c r="I77" s="22">
+        <v>108</v>
+      </c>
+      <c r="J77" s="22">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="78" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A78" s="20">
+        <v>43978</v>
+      </c>
+      <c r="B78" s="21">
+        <v>77210</v>
+      </c>
+      <c r="C78" s="22">
+        <v>631</v>
+      </c>
+      <c r="D78" s="22">
+        <v>1473</v>
+      </c>
+      <c r="E78" s="22">
+        <v>2</v>
+      </c>
+      <c r="F78" s="22">
+        <v>7</v>
+      </c>
+      <c r="G78" s="22">
+        <v>2</v>
+      </c>
+      <c r="H78" s="22">
+        <v>1</v>
+      </c>
+      <c r="I78" s="22">
+        <v>108</v>
+      </c>
+      <c r="J78" s="22">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="79" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A79" s="20">
+        <v>43979</v>
+      </c>
+      <c r="B79" s="21">
+        <v>77916</v>
+      </c>
+      <c r="C79" s="22">
+        <v>706</v>
+      </c>
+      <c r="D79" s="22">
+        <v>1473</v>
+      </c>
+      <c r="E79" s="22">
+        <v>0</v>
+      </c>
+      <c r="F79" s="22">
+        <v>7</v>
+      </c>
+      <c r="G79" s="22">
+        <v>2</v>
+      </c>
+      <c r="H79" s="22">
+        <v>0</v>
+      </c>
+      <c r="I79" s="22">
+        <v>108</v>
+      </c>
+      <c r="J79" s="22">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="80" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A80" s="20">
+        <v>43980</v>
+      </c>
+      <c r="B80" s="21">
+        <v>78529</v>
+      </c>
+      <c r="C80" s="22">
+        <v>613</v>
+      </c>
+      <c r="D80" s="22">
+        <v>1473</v>
+      </c>
+      <c r="E80" s="22">
+        <v>0</v>
+      </c>
+      <c r="F80" s="22">
+        <v>7</v>
+      </c>
+      <c r="G80" s="22">
+        <v>2</v>
+      </c>
+      <c r="H80" s="22">
+        <v>0</v>
+      </c>
+      <c r="I80" s="22">
+        <v>108</v>
+      </c>
+      <c r="J80" s="22">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="81" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A81" s="20">
+        <v>43981</v>
+      </c>
+      <c r="B81" s="22">
+        <v>78793</v>
+      </c>
+      <c r="C81" s="22">
+        <v>264</v>
+      </c>
+      <c r="D81" s="22">
+        <v>1473</v>
+      </c>
+      <c r="E81" s="22">
+        <v>0</v>
+      </c>
+      <c r="F81" s="22">
+        <v>6</v>
+      </c>
+      <c r="G81" s="22">
+        <v>2</v>
+      </c>
+      <c r="H81" s="22">
+        <v>1</v>
+      </c>
+      <c r="I81" s="22">
+        <v>108</v>
+      </c>
+      <c r="J81" s="22">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="82" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A82" s="20">
+        <v>43982</v>
+      </c>
+      <c r="B82" s="21">
+        <v>79039</v>
+      </c>
+      <c r="C82" s="22">
+        <v>246</v>
+      </c>
+      <c r="D82" s="22">
+        <v>1473</v>
+      </c>
+      <c r="E82" s="22">
+        <v>0</v>
+      </c>
+      <c r="F82" s="22">
+        <v>5</v>
+      </c>
+      <c r="G82" s="22">
+        <v>1</v>
+      </c>
+      <c r="H82" s="22">
+        <v>0</v>
+      </c>
+      <c r="I82" s="22">
+        <v>109</v>
+      </c>
+      <c r="J82" s="22">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="83" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A83" s="20">
+        <v>43983</v>
+      </c>
+      <c r="B83" s="21">
+        <v>79698</v>
+      </c>
+      <c r="C83" s="22">
+        <v>659</v>
+      </c>
+      <c r="D83" s="22">
+        <v>1475</v>
+      </c>
+      <c r="E83" s="22">
+        <v>2</v>
+      </c>
+      <c r="F83" s="22">
+        <v>5</v>
+      </c>
+      <c r="G83" s="22">
+        <v>1</v>
+      </c>
+      <c r="H83" s="22">
+        <v>0</v>
+      </c>
+      <c r="I83" s="22">
+        <v>109</v>
+      </c>
+      <c r="J83" s="22">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="84" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A84" s="20">
+        <v>43984</v>
+      </c>
+      <c r="B84" s="21">
+        <v>80505</v>
+      </c>
+      <c r="C84" s="22">
+        <v>807</v>
+      </c>
+      <c r="D84" s="22">
+        <v>1477</v>
+      </c>
+      <c r="E84" s="22">
+        <v>2</v>
+      </c>
+      <c r="F84" s="22">
+        <v>5</v>
+      </c>
+      <c r="G84" s="22">
+        <v>0</v>
+      </c>
+      <c r="H84" s="22">
+        <v>0</v>
+      </c>
+      <c r="I84" s="22">
+        <v>109</v>
+      </c>
+      <c r="J84" s="22">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="85" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A85" s="20">
+        <v>43985</v>
+      </c>
+      <c r="B85" s="21">
+        <v>81333</v>
+      </c>
+      <c r="C85" s="22">
+        <v>828</v>
+      </c>
+      <c r="D85" s="22">
+        <v>1477</v>
+      </c>
+      <c r="E85" s="22">
+        <v>0</v>
+      </c>
+      <c r="F85" s="22">
+        <v>5</v>
+      </c>
+      <c r="G85" s="22">
+        <v>0</v>
+      </c>
+      <c r="H85" s="22">
+        <v>0</v>
+      </c>
+      <c r="I85" s="22">
+        <v>109</v>
+      </c>
+      <c r="J85" s="22">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="86" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A86" s="26">
+        <v>43986</v>
+      </c>
+      <c r="B86" s="27">
+        <v>82161</v>
+      </c>
+      <c r="C86" s="28">
+        <v>828</v>
+      </c>
+      <c r="D86" s="28">
+        <v>1479</v>
+      </c>
+      <c r="E86" s="28">
+        <v>2</v>
+      </c>
+      <c r="F86" s="28">
+        <v>6</v>
+      </c>
+      <c r="G86" s="28">
+        <v>0</v>
+      </c>
+      <c r="H86" s="28">
+        <v>0</v>
+      </c>
+      <c r="I86" s="28">
+        <v>109</v>
+      </c>
+      <c r="J86" s="28">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="87" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A87" s="29">
+        <v>43987</v>
+      </c>
+      <c r="B87" s="30">
+        <v>82876</v>
+      </c>
+      <c r="C87" s="31">
+        <v>715</v>
+      </c>
+      <c r="D87" s="31">
+        <v>1484</v>
+      </c>
+      <c r="E87" s="31">
+        <v>5</v>
+      </c>
+      <c r="F87" s="31">
+        <v>6</v>
+      </c>
+      <c r="G87" s="31">
+        <v>0</v>
+      </c>
+      <c r="H87" s="31">
+        <v>0</v>
+      </c>
+      <c r="I87" s="31">
+        <v>109</v>
+      </c>
+      <c r="J87" s="31">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="88" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A88" s="23">
+        <v>43988</v>
+      </c>
+      <c r="B88" s="24">
+        <v>83105</v>
+      </c>
+      <c r="C88" s="25">
+        <v>229</v>
+      </c>
+      <c r="D88" s="25">
+        <v>1485</v>
+      </c>
+      <c r="E88" s="25">
+        <v>1</v>
+      </c>
+      <c r="F88" s="25">
+        <v>5</v>
+      </c>
+      <c r="G88" s="25">
+        <v>0</v>
+      </c>
+      <c r="H88" s="25">
+        <v>1</v>
+      </c>
+      <c r="I88" s="25">
+        <v>109</v>
+      </c>
+      <c r="J88" s="25">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="89" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A89" s="29">
+        <v>43989</v>
+      </c>
+      <c r="B89" s="30">
+        <v>83316</v>
+      </c>
+      <c r="C89" s="31">
+        <v>211</v>
+      </c>
+      <c r="D89" s="31">
+        <v>1485</v>
+      </c>
+      <c r="E89" s="31">
+        <v>0</v>
+      </c>
+      <c r="F89" s="31">
+        <v>5</v>
+      </c>
+      <c r="G89" s="31">
+        <v>0</v>
+      </c>
+      <c r="H89" s="31">
+        <v>0</v>
+      </c>
+      <c r="I89" s="31">
+        <v>109</v>
+      </c>
+      <c r="J89" s="31">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="90" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A90" s="20">
+        <v>43990</v>
+      </c>
+      <c r="B90" s="21">
+        <v>84130</v>
+      </c>
+      <c r="C90" s="22">
+        <v>814</v>
+      </c>
+      <c r="D90" s="22">
+        <v>1486</v>
+      </c>
+      <c r="E90" s="22">
+        <v>1</v>
+      </c>
+      <c r="F90" s="22">
+        <v>6</v>
+      </c>
+      <c r="G90" s="22">
+        <v>0</v>
+      </c>
+      <c r="H90" s="22">
+        <v>0</v>
+      </c>
+      <c r="I90" s="22">
+        <v>109</v>
+      </c>
+      <c r="J90" s="22">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="91" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A91" s="20">
+        <v>43991</v>
+      </c>
+      <c r="B91" s="21">
+        <v>84868</v>
+      </c>
+      <c r="C91" s="22">
+        <v>738</v>
+      </c>
+      <c r="D91" s="22">
+        <v>1488</v>
+      </c>
+      <c r="E91" s="22">
+        <v>2</v>
+      </c>
+      <c r="F91" s="22">
+        <v>6</v>
+      </c>
+      <c r="G91" s="22">
+        <v>0</v>
+      </c>
+      <c r="H91" s="22">
+        <v>0</v>
+      </c>
+      <c r="I91" s="22">
+        <v>109</v>
+      </c>
+      <c r="J91" s="22">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="92" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A92" s="23">
+        <v>43992</v>
+      </c>
+      <c r="B92" s="24">
+        <v>85626</v>
+      </c>
+      <c r="C92" s="25">
+        <v>758</v>
+      </c>
+      <c r="D92" s="25">
+        <v>1488</v>
+      </c>
+      <c r="E92" s="25">
+        <v>0</v>
+      </c>
+      <c r="F92" s="25">
+        <v>6</v>
+      </c>
+      <c r="G92" s="25">
+        <v>0</v>
+      </c>
+      <c r="H92" s="25">
+        <v>0</v>
+      </c>
+      <c r="I92" s="25">
+        <v>109</v>
+      </c>
+      <c r="J92" s="25">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="93" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A93" s="29">
+        <v>43993</v>
+      </c>
+      <c r="B93" s="30">
+        <v>86328</v>
+      </c>
+      <c r="C93" s="31">
+        <v>702</v>
+      </c>
+      <c r="D93" s="31">
+        <v>1490</v>
+      </c>
+      <c r="E93" s="31">
+        <v>2</v>
+      </c>
+      <c r="F93" s="31">
+        <v>6</v>
+      </c>
+      <c r="G93" s="31">
+        <v>0</v>
+      </c>
+      <c r="H93" s="31">
+        <v>0</v>
+      </c>
+      <c r="I93" s="31">
+        <v>109</v>
+      </c>
+      <c r="J93" s="31">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="94" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A94" s="23">
+        <v>43994</v>
+      </c>
+      <c r="B94" s="24">
+        <v>87095</v>
+      </c>
+      <c r="C94" s="25">
+        <v>767</v>
+      </c>
+      <c r="D94" s="25">
+        <v>1492</v>
+      </c>
+      <c r="E94" s="25">
+        <v>2</v>
+      </c>
+      <c r="F94" s="25">
+        <v>6</v>
+      </c>
+      <c r="G94" s="25">
+        <v>0</v>
+      </c>
+      <c r="H94" s="25">
+        <v>0</v>
+      </c>
+      <c r="I94" s="25">
+        <v>109</v>
+      </c>
+      <c r="J94" s="25">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="95" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A95" s="29">
+        <v>43995</v>
+      </c>
+      <c r="B95" s="30">
+        <v>87386</v>
+      </c>
+      <c r="C95" s="31">
+        <v>291</v>
+      </c>
+      <c r="D95" s="31">
+        <v>1495</v>
+      </c>
+      <c r="E95" s="31">
+        <v>3</v>
+      </c>
+      <c r="F95" s="31">
+        <v>6</v>
+      </c>
+      <c r="G95" s="31">
+        <v>0</v>
+      </c>
+      <c r="H95" s="31">
+        <v>0</v>
+      </c>
+      <c r="I95" s="31">
+        <v>109</v>
+      </c>
+      <c r="J95" s="31">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="96" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A96" s="23">
+        <v>43996</v>
+      </c>
+      <c r="B96" s="24">
+        <v>87598</v>
+      </c>
+      <c r="C96" s="25">
+        <v>212</v>
+      </c>
+      <c r="D96" s="25">
+        <v>1496</v>
+      </c>
+      <c r="E96" s="25">
+        <v>1</v>
+      </c>
+      <c r="F96" s="25">
+        <v>7</v>
+      </c>
+      <c r="G96" s="25">
+        <v>1</v>
+      </c>
+      <c r="H96" s="25">
+        <v>0</v>
+      </c>
+      <c r="I96" s="25">
+        <v>109</v>
+      </c>
+      <c r="J96" s="25">
+        <v>0</v>
+      </c>
+    </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>

</xml_diff>

<commit_message>
Data updated by GitHub Bot (2020-06-15 20)
</commit_message>
<xml_diff>
--- a/output/snapshot/fdcf2531-4c3e-5c02-b63c-ee160ead6dea.xlsx
+++ b/output/snapshot/fdcf2531-4c3e-5c02-b63c-ee160ead6dea.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="I:\AKTUALNI PODATKI - KORONA\Za objavo na GOV.SI\ang\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{1E6DD62F-2BE2-47DC-A7ED-9B57C1589256}" xr6:coauthVersionLast="44" xr6:coauthVersionMax="44" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{B641C904-F5E5-45C5-93A6-81E74361D8EC}" xr6:coauthVersionLast="44" xr6:coauthVersionMax="44" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="2295" yWindow="2295" windowWidth="21600" windowHeight="11205" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Covid-19 podatki" sheetId="1" r:id="rId1"/>
@@ -64,7 +64,7 @@
   <numFmts count="1">
     <numFmt numFmtId="164" formatCode="d/\ m/\ yyyy;@"/>
   </numFmts>
-  <fonts count="4" x14ac:knownFonts="1">
+  <fonts count="5" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -93,6 +93,13 @@
       <name val="Calibri Light"/>
       <scheme val="major"/>
     </font>
+    <font>
+      <sz val="10"/>
+      <color theme="1"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
   </fonts>
   <fills count="3">
     <fill>
@@ -108,7 +115,7 @@
       </patternFill>
     </fill>
   </fills>
-  <borders count="2">
+  <borders count="3">
     <border>
       <left/>
       <right/>
@@ -129,11 +136,26 @@
       <bottom/>
       <diagonal/>
     </border>
+    <border>
+      <left style="thin">
+        <color theme="4"/>
+      </left>
+      <right style="thin">
+        <color theme="4"/>
+      </right>
+      <top style="thin">
+        <color theme="4"/>
+      </top>
+      <bottom style="thin">
+        <color theme="4"/>
+      </bottom>
+      <diagonal/>
+    </border>
   </borders>
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="26">
+  <cellXfs count="32">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="49" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyAlignment="1" applyProtection="1">
       <alignment horizontal="left" vertical="top"/>
@@ -208,6 +230,24 @@
       <alignment horizontal="right"/>
     </xf>
     <xf numFmtId="0" fontId="3" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="right"/>
+    </xf>
+    <xf numFmtId="164" fontId="4" fillId="2" borderId="2" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="right" vertical="top"/>
+    </xf>
+    <xf numFmtId="3" fontId="4" fillId="2" borderId="2" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="right"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="2" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="right"/>
+    </xf>
+    <xf numFmtId="164" fontId="3" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="right" vertical="top"/>
+    </xf>
+    <xf numFmtId="3" fontId="3" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="right"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="right"/>
     </xf>
   </cellXfs>
@@ -399,8 +439,8 @@
 </file>
 
 <file path=xl/tables/table1.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="1" xr:uid="{00000000-000C-0000-FFFF-FFFF00000000}" name="Tabela1" displayName="Tabela1" ref="A1:J75" totalsRowShown="0" headerRowDxfId="11" dataDxfId="10">
-  <autoFilter ref="A1:J75" xr:uid="{00000000-0009-0000-0100-000001000000}">
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="1" xr:uid="{00000000-000C-0000-FFFF-FFFF00000000}" name="Tabela1" displayName="Tabela1" ref="A1:J96" totalsRowShown="0" headerRowDxfId="11" dataDxfId="10">
+  <autoFilter ref="A1:J96" xr:uid="{00000000-0009-0000-0100-000001000000}">
     <filterColumn colId="0" hiddenButton="1"/>
     <filterColumn colId="1" hiddenButton="1"/>
     <filterColumn colId="2" hiddenButton="1"/>
@@ -696,10 +736,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:J75"/>
+  <dimension ref="A1:J96"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A40" zoomScale="89" zoomScaleNormal="89" workbookViewId="0">
-      <selection activeCell="J74" sqref="J74"/>
+    <sheetView tabSelected="1" topLeftCell="A77" zoomScale="89" zoomScaleNormal="89" workbookViewId="0">
+      <selection activeCell="A96" sqref="A96:J96"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -3117,6 +3157,678 @@
         <v>0</v>
       </c>
     </row>
+    <row r="76" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A76" s="20">
+        <v>43976</v>
+      </c>
+      <c r="B76" s="21">
+        <v>75770</v>
+      </c>
+      <c r="C76" s="22">
+        <v>754</v>
+      </c>
+      <c r="D76" s="22">
+        <v>1469</v>
+      </c>
+      <c r="E76" s="22">
+        <v>0</v>
+      </c>
+      <c r="F76" s="22">
+        <v>9</v>
+      </c>
+      <c r="G76" s="22">
+        <v>2</v>
+      </c>
+      <c r="H76" s="22">
+        <v>6</v>
+      </c>
+      <c r="I76" s="22">
+        <v>108</v>
+      </c>
+      <c r="J76" s="22">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="77" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A77" s="20">
+        <v>43977</v>
+      </c>
+      <c r="B77" s="21">
+        <v>76579</v>
+      </c>
+      <c r="C77" s="22">
+        <v>809</v>
+      </c>
+      <c r="D77" s="22">
+        <v>1471</v>
+      </c>
+      <c r="E77" s="22">
+        <v>2</v>
+      </c>
+      <c r="F77" s="22">
+        <v>8</v>
+      </c>
+      <c r="G77" s="22">
+        <v>2</v>
+      </c>
+      <c r="H77" s="22">
+        <v>2</v>
+      </c>
+      <c r="I77" s="22">
+        <v>108</v>
+      </c>
+      <c r="J77" s="22">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="78" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A78" s="20">
+        <v>43978</v>
+      </c>
+      <c r="B78" s="21">
+        <v>77210</v>
+      </c>
+      <c r="C78" s="22">
+        <v>631</v>
+      </c>
+      <c r="D78" s="22">
+        <v>1473</v>
+      </c>
+      <c r="E78" s="22">
+        <v>2</v>
+      </c>
+      <c r="F78" s="22">
+        <v>7</v>
+      </c>
+      <c r="G78" s="22">
+        <v>2</v>
+      </c>
+      <c r="H78" s="22">
+        <v>1</v>
+      </c>
+      <c r="I78" s="22">
+        <v>108</v>
+      </c>
+      <c r="J78" s="22">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="79" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A79" s="20">
+        <v>43979</v>
+      </c>
+      <c r="B79" s="21">
+        <v>77916</v>
+      </c>
+      <c r="C79" s="22">
+        <v>706</v>
+      </c>
+      <c r="D79" s="22">
+        <v>1473</v>
+      </c>
+      <c r="E79" s="22">
+        <v>0</v>
+      </c>
+      <c r="F79" s="22">
+        <v>7</v>
+      </c>
+      <c r="G79" s="22">
+        <v>2</v>
+      </c>
+      <c r="H79" s="22">
+        <v>0</v>
+      </c>
+      <c r="I79" s="22">
+        <v>108</v>
+      </c>
+      <c r="J79" s="22">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="80" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A80" s="20">
+        <v>43980</v>
+      </c>
+      <c r="B80" s="21">
+        <v>78529</v>
+      </c>
+      <c r="C80" s="22">
+        <v>613</v>
+      </c>
+      <c r="D80" s="22">
+        <v>1473</v>
+      </c>
+      <c r="E80" s="22">
+        <v>0</v>
+      </c>
+      <c r="F80" s="22">
+        <v>7</v>
+      </c>
+      <c r="G80" s="22">
+        <v>2</v>
+      </c>
+      <c r="H80" s="22">
+        <v>0</v>
+      </c>
+      <c r="I80" s="22">
+        <v>108</v>
+      </c>
+      <c r="J80" s="22">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="81" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A81" s="20">
+        <v>43981</v>
+      </c>
+      <c r="B81" s="22">
+        <v>78793</v>
+      </c>
+      <c r="C81" s="22">
+        <v>264</v>
+      </c>
+      <c r="D81" s="22">
+        <v>1473</v>
+      </c>
+      <c r="E81" s="22">
+        <v>0</v>
+      </c>
+      <c r="F81" s="22">
+        <v>6</v>
+      </c>
+      <c r="G81" s="22">
+        <v>2</v>
+      </c>
+      <c r="H81" s="22">
+        <v>1</v>
+      </c>
+      <c r="I81" s="22">
+        <v>108</v>
+      </c>
+      <c r="J81" s="22">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="82" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A82" s="20">
+        <v>43982</v>
+      </c>
+      <c r="B82" s="21">
+        <v>79039</v>
+      </c>
+      <c r="C82" s="22">
+        <v>246</v>
+      </c>
+      <c r="D82" s="22">
+        <v>1473</v>
+      </c>
+      <c r="E82" s="22">
+        <v>0</v>
+      </c>
+      <c r="F82" s="22">
+        <v>5</v>
+      </c>
+      <c r="G82" s="22">
+        <v>1</v>
+      </c>
+      <c r="H82" s="22">
+        <v>0</v>
+      </c>
+      <c r="I82" s="22">
+        <v>109</v>
+      </c>
+      <c r="J82" s="22">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="83" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A83" s="20">
+        <v>43983</v>
+      </c>
+      <c r="B83" s="21">
+        <v>79698</v>
+      </c>
+      <c r="C83" s="22">
+        <v>659</v>
+      </c>
+      <c r="D83" s="22">
+        <v>1475</v>
+      </c>
+      <c r="E83" s="22">
+        <v>2</v>
+      </c>
+      <c r="F83" s="22">
+        <v>5</v>
+      </c>
+      <c r="G83" s="22">
+        <v>1</v>
+      </c>
+      <c r="H83" s="22">
+        <v>0</v>
+      </c>
+      <c r="I83" s="22">
+        <v>109</v>
+      </c>
+      <c r="J83" s="22">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="84" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A84" s="20">
+        <v>43984</v>
+      </c>
+      <c r="B84" s="21">
+        <v>80505</v>
+      </c>
+      <c r="C84" s="22">
+        <v>807</v>
+      </c>
+      <c r="D84" s="22">
+        <v>1477</v>
+      </c>
+      <c r="E84" s="22">
+        <v>2</v>
+      </c>
+      <c r="F84" s="22">
+        <v>5</v>
+      </c>
+      <c r="G84" s="22">
+        <v>0</v>
+      </c>
+      <c r="H84" s="22">
+        <v>0</v>
+      </c>
+      <c r="I84" s="22">
+        <v>109</v>
+      </c>
+      <c r="J84" s="22">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="85" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A85" s="20">
+        <v>43985</v>
+      </c>
+      <c r="B85" s="21">
+        <v>81333</v>
+      </c>
+      <c r="C85" s="22">
+        <v>828</v>
+      </c>
+      <c r="D85" s="22">
+        <v>1477</v>
+      </c>
+      <c r="E85" s="22">
+        <v>0</v>
+      </c>
+      <c r="F85" s="22">
+        <v>5</v>
+      </c>
+      <c r="G85" s="22">
+        <v>0</v>
+      </c>
+      <c r="H85" s="22">
+        <v>0</v>
+      </c>
+      <c r="I85" s="22">
+        <v>109</v>
+      </c>
+      <c r="J85" s="22">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="86" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A86" s="26">
+        <v>43986</v>
+      </c>
+      <c r="B86" s="27">
+        <v>82161</v>
+      </c>
+      <c r="C86" s="28">
+        <v>828</v>
+      </c>
+      <c r="D86" s="28">
+        <v>1479</v>
+      </c>
+      <c r="E86" s="28">
+        <v>2</v>
+      </c>
+      <c r="F86" s="28">
+        <v>6</v>
+      </c>
+      <c r="G86" s="28">
+        <v>0</v>
+      </c>
+      <c r="H86" s="28">
+        <v>0</v>
+      </c>
+      <c r="I86" s="28">
+        <v>109</v>
+      </c>
+      <c r="J86" s="28">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="87" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A87" s="29">
+        <v>43987</v>
+      </c>
+      <c r="B87" s="30">
+        <v>82876</v>
+      </c>
+      <c r="C87" s="31">
+        <v>715</v>
+      </c>
+      <c r="D87" s="31">
+        <v>1484</v>
+      </c>
+      <c r="E87" s="31">
+        <v>5</v>
+      </c>
+      <c r="F87" s="31">
+        <v>6</v>
+      </c>
+      <c r="G87" s="31">
+        <v>0</v>
+      </c>
+      <c r="H87" s="31">
+        <v>0</v>
+      </c>
+      <c r="I87" s="31">
+        <v>109</v>
+      </c>
+      <c r="J87" s="31">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="88" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A88" s="23">
+        <v>43988</v>
+      </c>
+      <c r="B88" s="24">
+        <v>83105</v>
+      </c>
+      <c r="C88" s="25">
+        <v>229</v>
+      </c>
+      <c r="D88" s="25">
+        <v>1485</v>
+      </c>
+      <c r="E88" s="25">
+        <v>1</v>
+      </c>
+      <c r="F88" s="25">
+        <v>5</v>
+      </c>
+      <c r="G88" s="25">
+        <v>0</v>
+      </c>
+      <c r="H88" s="25">
+        <v>1</v>
+      </c>
+      <c r="I88" s="25">
+        <v>109</v>
+      </c>
+      <c r="J88" s="25">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="89" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A89" s="29">
+        <v>43989</v>
+      </c>
+      <c r="B89" s="30">
+        <v>83316</v>
+      </c>
+      <c r="C89" s="31">
+        <v>211</v>
+      </c>
+      <c r="D89" s="31">
+        <v>1485</v>
+      </c>
+      <c r="E89" s="31">
+        <v>0</v>
+      </c>
+      <c r="F89" s="31">
+        <v>5</v>
+      </c>
+      <c r="G89" s="31">
+        <v>0</v>
+      </c>
+      <c r="H89" s="31">
+        <v>0</v>
+      </c>
+      <c r="I89" s="31">
+        <v>109</v>
+      </c>
+      <c r="J89" s="31">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="90" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A90" s="20">
+        <v>43990</v>
+      </c>
+      <c r="B90" s="21">
+        <v>84130</v>
+      </c>
+      <c r="C90" s="22">
+        <v>814</v>
+      </c>
+      <c r="D90" s="22">
+        <v>1486</v>
+      </c>
+      <c r="E90" s="22">
+        <v>1</v>
+      </c>
+      <c r="F90" s="22">
+        <v>6</v>
+      </c>
+      <c r="G90" s="22">
+        <v>0</v>
+      </c>
+      <c r="H90" s="22">
+        <v>0</v>
+      </c>
+      <c r="I90" s="22">
+        <v>109</v>
+      </c>
+      <c r="J90" s="22">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="91" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A91" s="20">
+        <v>43991</v>
+      </c>
+      <c r="B91" s="21">
+        <v>84868</v>
+      </c>
+      <c r="C91" s="22">
+        <v>738</v>
+      </c>
+      <c r="D91" s="22">
+        <v>1488</v>
+      </c>
+      <c r="E91" s="22">
+        <v>2</v>
+      </c>
+      <c r="F91" s="22">
+        <v>6</v>
+      </c>
+      <c r="G91" s="22">
+        <v>0</v>
+      </c>
+      <c r="H91" s="22">
+        <v>0</v>
+      </c>
+      <c r="I91" s="22">
+        <v>109</v>
+      </c>
+      <c r="J91" s="22">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="92" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A92" s="23">
+        <v>43992</v>
+      </c>
+      <c r="B92" s="24">
+        <v>85626</v>
+      </c>
+      <c r="C92" s="25">
+        <v>758</v>
+      </c>
+      <c r="D92" s="25">
+        <v>1488</v>
+      </c>
+      <c r="E92" s="25">
+        <v>0</v>
+      </c>
+      <c r="F92" s="25">
+        <v>6</v>
+      </c>
+      <c r="G92" s="25">
+        <v>0</v>
+      </c>
+      <c r="H92" s="25">
+        <v>0</v>
+      </c>
+      <c r="I92" s="25">
+        <v>109</v>
+      </c>
+      <c r="J92" s="25">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="93" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A93" s="29">
+        <v>43993</v>
+      </c>
+      <c r="B93" s="30">
+        <v>86328</v>
+      </c>
+      <c r="C93" s="31">
+        <v>702</v>
+      </c>
+      <c r="D93" s="31">
+        <v>1490</v>
+      </c>
+      <c r="E93" s="31">
+        <v>2</v>
+      </c>
+      <c r="F93" s="31">
+        <v>6</v>
+      </c>
+      <c r="G93" s="31">
+        <v>0</v>
+      </c>
+      <c r="H93" s="31">
+        <v>0</v>
+      </c>
+      <c r="I93" s="31">
+        <v>109</v>
+      </c>
+      <c r="J93" s="31">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="94" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A94" s="23">
+        <v>43994</v>
+      </c>
+      <c r="B94" s="24">
+        <v>87095</v>
+      </c>
+      <c r="C94" s="25">
+        <v>767</v>
+      </c>
+      <c r="D94" s="25">
+        <v>1492</v>
+      </c>
+      <c r="E94" s="25">
+        <v>2</v>
+      </c>
+      <c r="F94" s="25">
+        <v>6</v>
+      </c>
+      <c r="G94" s="25">
+        <v>0</v>
+      </c>
+      <c r="H94" s="25">
+        <v>0</v>
+      </c>
+      <c r="I94" s="25">
+        <v>109</v>
+      </c>
+      <c r="J94" s="25">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="95" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A95" s="29">
+        <v>43995</v>
+      </c>
+      <c r="B95" s="30">
+        <v>87386</v>
+      </c>
+      <c r="C95" s="31">
+        <v>291</v>
+      </c>
+      <c r="D95" s="31">
+        <v>1495</v>
+      </c>
+      <c r="E95" s="31">
+        <v>3</v>
+      </c>
+      <c r="F95" s="31">
+        <v>6</v>
+      </c>
+      <c r="G95" s="31">
+        <v>0</v>
+      </c>
+      <c r="H95" s="31">
+        <v>0</v>
+      </c>
+      <c r="I95" s="31">
+        <v>109</v>
+      </c>
+      <c r="J95" s="31">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="96" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A96" s="23">
+        <v>43996</v>
+      </c>
+      <c r="B96" s="24">
+        <v>87598</v>
+      </c>
+      <c r="C96" s="25">
+        <v>212</v>
+      </c>
+      <c r="D96" s="25">
+        <v>1496</v>
+      </c>
+      <c r="E96" s="25">
+        <v>1</v>
+      </c>
+      <c r="F96" s="25">
+        <v>7</v>
+      </c>
+      <c r="G96" s="25">
+        <v>1</v>
+      </c>
+      <c r="H96" s="25">
+        <v>0</v>
+      </c>
+      <c r="I96" s="25">
+        <v>109</v>
+      </c>
+      <c r="J96" s="25">
+        <v>0</v>
+      </c>
+    </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>

</xml_diff>

<commit_message>
Data updated by GitHub Bot (2020-06-16 12)
</commit_message>
<xml_diff>
--- a/output/snapshot/fdcf2531-4c3e-5c02-b63c-ee160ead6dea.xlsx
+++ b/output/snapshot/fdcf2531-4c3e-5c02-b63c-ee160ead6dea.xlsx
@@ -1,16 +1,15 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="21929"/>
-  <workbookPr/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
+  <fileVersion appName="xl" lastEdited="6" lowestEdited="6" rupBuild="14420"/>
+  <workbookPr defaultThemeVersion="164011"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="I:\AKTUALNI PODATKI - KORONA\Za objavo na GOV.SI\ang\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{1E6DD62F-2BE2-47DC-A7ED-9B57C1589256}" xr6:coauthVersionLast="44" xr6:coauthVersionMax="44" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="2295" yWindow="2295" windowWidth="21600" windowHeight="11205"/>
   </bookViews>
   <sheets>
     <sheet name="Covid-19 podatki" sheetId="1" r:id="rId1"/>
@@ -60,11 +59,11 @@
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" mc:Ignorable="x14ac x16r2">
   <numFmts count="1">
     <numFmt numFmtId="164" formatCode="d/\ m/\ yyyy;@"/>
   </numFmts>
-  <fonts count="4" x14ac:knownFonts="1">
+  <fonts count="5" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -93,6 +92,13 @@
       <name val="Calibri Light"/>
       <scheme val="major"/>
     </font>
+    <font>
+      <sz val="10"/>
+      <color theme="1"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
   </fonts>
   <fills count="3">
     <fill>
@@ -108,7 +114,7 @@
       </patternFill>
     </fill>
   </fills>
-  <borders count="2">
+  <borders count="3">
     <border>
       <left/>
       <right/>
@@ -129,11 +135,26 @@
       <bottom/>
       <diagonal/>
     </border>
+    <border>
+      <left style="thin">
+        <color theme="4"/>
+      </left>
+      <right style="thin">
+        <color theme="4"/>
+      </right>
+      <top style="thin">
+        <color theme="4"/>
+      </top>
+      <bottom style="thin">
+        <color theme="4"/>
+      </bottom>
+      <diagonal/>
+    </border>
   </borders>
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="26">
+  <cellXfs count="32">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="49" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyAlignment="1" applyProtection="1">
       <alignment horizontal="left" vertical="top"/>
@@ -208,6 +229,24 @@
       <alignment horizontal="right"/>
     </xf>
     <xf numFmtId="0" fontId="3" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="right"/>
+    </xf>
+    <xf numFmtId="164" fontId="4" fillId="2" borderId="2" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="right" vertical="top"/>
+    </xf>
+    <xf numFmtId="3" fontId="4" fillId="2" borderId="2" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="right"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="2" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="right"/>
+    </xf>
+    <xf numFmtId="164" fontId="3" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="right" vertical="top"/>
+    </xf>
+    <xf numFmtId="3" fontId="3" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="right"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="right"/>
     </xf>
   </cellXfs>
@@ -399,8 +438,8 @@
 </file>
 
 <file path=xl/tables/table1.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="1" xr:uid="{00000000-000C-0000-FFFF-FFFF00000000}" name="Tabela1" displayName="Tabela1" ref="A1:J75" totalsRowShown="0" headerRowDxfId="11" dataDxfId="10">
-  <autoFilter ref="A1:J75" xr:uid="{00000000-0009-0000-0100-000001000000}">
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="1" name="Tabela1" displayName="Tabela1" ref="A1:J97" totalsRowShown="0" headerRowDxfId="11" dataDxfId="10">
+  <autoFilter ref="A1:J97">
     <filterColumn colId="0" hiddenButton="1"/>
     <filterColumn colId="1" hiddenButton="1"/>
     <filterColumn colId="2" hiddenButton="1"/>
@@ -413,16 +452,16 @@
     <filterColumn colId="9" hiddenButton="1"/>
   </autoFilter>
   <tableColumns count="10">
-    <tableColumn id="1" xr3:uid="{00000000-0010-0000-0000-000001000000}" name="Date" dataDxfId="9"/>
-    <tableColumn id="2" xr3:uid="{00000000-0010-0000-0000-000002000000}" name="Tested (all)" dataDxfId="8"/>
-    <tableColumn id="3" xr3:uid="{00000000-0010-0000-0000-000003000000}" name="Tested (daily)" dataDxfId="7"/>
-    <tableColumn id="4" xr3:uid="{00000000-0010-0000-0000-000004000000}" name="Positive (all)" dataDxfId="6"/>
-    <tableColumn id="5" xr3:uid="{00000000-0010-0000-0000-000005000000}" name="Positive (daily)" dataDxfId="5"/>
-    <tableColumn id="6" xr3:uid="{00000000-0010-0000-0000-000006000000}" name="All hospitalized on certain day" dataDxfId="4"/>
-    <tableColumn id="7" xr3:uid="{00000000-0010-0000-0000-000007000000}" name="All persons in intensive care on certain day" dataDxfId="3"/>
-    <tableColumn id="10" xr3:uid="{00000000-0010-0000-0000-00000A000000}" name="Discharged" dataDxfId="2"/>
-    <tableColumn id="8" xr3:uid="{00000000-0010-0000-0000-000008000000}" name="Deaths (all)" dataDxfId="1"/>
-    <tableColumn id="9" xr3:uid="{00000000-0010-0000-0000-000009000000}" name="Deaths (daily)" dataDxfId="0"/>
+    <tableColumn id="1" name="Date" dataDxfId="9"/>
+    <tableColumn id="2" name="Tested (all)" dataDxfId="8"/>
+    <tableColumn id="3" name="Tested (daily)" dataDxfId="7"/>
+    <tableColumn id="4" name="Positive (all)" dataDxfId="6"/>
+    <tableColumn id="5" name="Positive (daily)" dataDxfId="5"/>
+    <tableColumn id="6" name="All hospitalized on certain day" dataDxfId="4"/>
+    <tableColumn id="7" name="All persons in intensive care on certain day" dataDxfId="3"/>
+    <tableColumn id="10" name="Discharged" dataDxfId="2"/>
+    <tableColumn id="8" name="Deaths (all)" dataDxfId="1"/>
+    <tableColumn id="9" name="Deaths (daily)" dataDxfId="0"/>
   </tableColumns>
   <tableStyleInfo name="TableStyleLight16" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
   <extLst>
@@ -695,11 +734,11 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:J75"/>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <dimension ref="A1:J97"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A40" zoomScale="89" zoomScaleNormal="89" workbookViewId="0">
-      <selection activeCell="J74" sqref="J74"/>
+    <sheetView tabSelected="1" topLeftCell="A77" zoomScale="89" zoomScaleNormal="89" workbookViewId="0">
+      <selection activeCell="J97" sqref="A97:J97"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -3117,6 +3156,710 @@
         <v>0</v>
       </c>
     </row>
+    <row r="76" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A76" s="20">
+        <v>43976</v>
+      </c>
+      <c r="B76" s="21">
+        <v>75770</v>
+      </c>
+      <c r="C76" s="22">
+        <v>754</v>
+      </c>
+      <c r="D76" s="22">
+        <v>1469</v>
+      </c>
+      <c r="E76" s="22">
+        <v>0</v>
+      </c>
+      <c r="F76" s="22">
+        <v>9</v>
+      </c>
+      <c r="G76" s="22">
+        <v>2</v>
+      </c>
+      <c r="H76" s="22">
+        <v>6</v>
+      </c>
+      <c r="I76" s="22">
+        <v>108</v>
+      </c>
+      <c r="J76" s="22">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="77" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A77" s="20">
+        <v>43977</v>
+      </c>
+      <c r="B77" s="21">
+        <v>76579</v>
+      </c>
+      <c r="C77" s="22">
+        <v>809</v>
+      </c>
+      <c r="D77" s="22">
+        <v>1471</v>
+      </c>
+      <c r="E77" s="22">
+        <v>2</v>
+      </c>
+      <c r="F77" s="22">
+        <v>8</v>
+      </c>
+      <c r="G77" s="22">
+        <v>2</v>
+      </c>
+      <c r="H77" s="22">
+        <v>2</v>
+      </c>
+      <c r="I77" s="22">
+        <v>108</v>
+      </c>
+      <c r="J77" s="22">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="78" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A78" s="20">
+        <v>43978</v>
+      </c>
+      <c r="B78" s="21">
+        <v>77210</v>
+      </c>
+      <c r="C78" s="22">
+        <v>631</v>
+      </c>
+      <c r="D78" s="22">
+        <v>1473</v>
+      </c>
+      <c r="E78" s="22">
+        <v>2</v>
+      </c>
+      <c r="F78" s="22">
+        <v>7</v>
+      </c>
+      <c r="G78" s="22">
+        <v>2</v>
+      </c>
+      <c r="H78" s="22">
+        <v>1</v>
+      </c>
+      <c r="I78" s="22">
+        <v>108</v>
+      </c>
+      <c r="J78" s="22">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="79" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A79" s="20">
+        <v>43979</v>
+      </c>
+      <c r="B79" s="21">
+        <v>77916</v>
+      </c>
+      <c r="C79" s="22">
+        <v>706</v>
+      </c>
+      <c r="D79" s="22">
+        <v>1473</v>
+      </c>
+      <c r="E79" s="22">
+        <v>0</v>
+      </c>
+      <c r="F79" s="22">
+        <v>7</v>
+      </c>
+      <c r="G79" s="22">
+        <v>2</v>
+      </c>
+      <c r="H79" s="22">
+        <v>0</v>
+      </c>
+      <c r="I79" s="22">
+        <v>108</v>
+      </c>
+      <c r="J79" s="22">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="80" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A80" s="20">
+        <v>43980</v>
+      </c>
+      <c r="B80" s="21">
+        <v>78529</v>
+      </c>
+      <c r="C80" s="22">
+        <v>613</v>
+      </c>
+      <c r="D80" s="22">
+        <v>1473</v>
+      </c>
+      <c r="E80" s="22">
+        <v>0</v>
+      </c>
+      <c r="F80" s="22">
+        <v>7</v>
+      </c>
+      <c r="G80" s="22">
+        <v>2</v>
+      </c>
+      <c r="H80" s="22">
+        <v>0</v>
+      </c>
+      <c r="I80" s="22">
+        <v>108</v>
+      </c>
+      <c r="J80" s="22">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="81" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A81" s="20">
+        <v>43981</v>
+      </c>
+      <c r="B81" s="22">
+        <v>78793</v>
+      </c>
+      <c r="C81" s="22">
+        <v>264</v>
+      </c>
+      <c r="D81" s="22">
+        <v>1473</v>
+      </c>
+      <c r="E81" s="22">
+        <v>0</v>
+      </c>
+      <c r="F81" s="22">
+        <v>6</v>
+      </c>
+      <c r="G81" s="22">
+        <v>2</v>
+      </c>
+      <c r="H81" s="22">
+        <v>1</v>
+      </c>
+      <c r="I81" s="22">
+        <v>108</v>
+      </c>
+      <c r="J81" s="22">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="82" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A82" s="20">
+        <v>43982</v>
+      </c>
+      <c r="B82" s="21">
+        <v>79039</v>
+      </c>
+      <c r="C82" s="22">
+        <v>246</v>
+      </c>
+      <c r="D82" s="22">
+        <v>1473</v>
+      </c>
+      <c r="E82" s="22">
+        <v>0</v>
+      </c>
+      <c r="F82" s="22">
+        <v>5</v>
+      </c>
+      <c r="G82" s="22">
+        <v>1</v>
+      </c>
+      <c r="H82" s="22">
+        <v>0</v>
+      </c>
+      <c r="I82" s="22">
+        <v>109</v>
+      </c>
+      <c r="J82" s="22">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="83" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A83" s="20">
+        <v>43983</v>
+      </c>
+      <c r="B83" s="21">
+        <v>79698</v>
+      </c>
+      <c r="C83" s="22">
+        <v>659</v>
+      </c>
+      <c r="D83" s="22">
+        <v>1475</v>
+      </c>
+      <c r="E83" s="22">
+        <v>2</v>
+      </c>
+      <c r="F83" s="22">
+        <v>5</v>
+      </c>
+      <c r="G83" s="22">
+        <v>1</v>
+      </c>
+      <c r="H83" s="22">
+        <v>0</v>
+      </c>
+      <c r="I83" s="22">
+        <v>109</v>
+      </c>
+      <c r="J83" s="22">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="84" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A84" s="20">
+        <v>43984</v>
+      </c>
+      <c r="B84" s="21">
+        <v>80505</v>
+      </c>
+      <c r="C84" s="22">
+        <v>807</v>
+      </c>
+      <c r="D84" s="22">
+        <v>1477</v>
+      </c>
+      <c r="E84" s="22">
+        <v>2</v>
+      </c>
+      <c r="F84" s="22">
+        <v>5</v>
+      </c>
+      <c r="G84" s="22">
+        <v>0</v>
+      </c>
+      <c r="H84" s="22">
+        <v>0</v>
+      </c>
+      <c r="I84" s="22">
+        <v>109</v>
+      </c>
+      <c r="J84" s="22">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="85" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A85" s="20">
+        <v>43985</v>
+      </c>
+      <c r="B85" s="21">
+        <v>81333</v>
+      </c>
+      <c r="C85" s="22">
+        <v>828</v>
+      </c>
+      <c r="D85" s="22">
+        <v>1477</v>
+      </c>
+      <c r="E85" s="22">
+        <v>0</v>
+      </c>
+      <c r="F85" s="22">
+        <v>5</v>
+      </c>
+      <c r="G85" s="22">
+        <v>0</v>
+      </c>
+      <c r="H85" s="22">
+        <v>0</v>
+      </c>
+      <c r="I85" s="22">
+        <v>109</v>
+      </c>
+      <c r="J85" s="22">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="86" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A86" s="26">
+        <v>43986</v>
+      </c>
+      <c r="B86" s="27">
+        <v>82161</v>
+      </c>
+      <c r="C86" s="28">
+        <v>828</v>
+      </c>
+      <c r="D86" s="28">
+        <v>1479</v>
+      </c>
+      <c r="E86" s="28">
+        <v>2</v>
+      </c>
+      <c r="F86" s="28">
+        <v>6</v>
+      </c>
+      <c r="G86" s="28">
+        <v>0</v>
+      </c>
+      <c r="H86" s="28">
+        <v>0</v>
+      </c>
+      <c r="I86" s="28">
+        <v>109</v>
+      </c>
+      <c r="J86" s="28">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="87" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A87" s="29">
+        <v>43987</v>
+      </c>
+      <c r="B87" s="30">
+        <v>82876</v>
+      </c>
+      <c r="C87" s="31">
+        <v>715</v>
+      </c>
+      <c r="D87" s="31">
+        <v>1484</v>
+      </c>
+      <c r="E87" s="31">
+        <v>5</v>
+      </c>
+      <c r="F87" s="31">
+        <v>6</v>
+      </c>
+      <c r="G87" s="31">
+        <v>0</v>
+      </c>
+      <c r="H87" s="31">
+        <v>0</v>
+      </c>
+      <c r="I87" s="31">
+        <v>109</v>
+      </c>
+      <c r="J87" s="31">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="88" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A88" s="23">
+        <v>43988</v>
+      </c>
+      <c r="B88" s="24">
+        <v>83105</v>
+      </c>
+      <c r="C88" s="25">
+        <v>229</v>
+      </c>
+      <c r="D88" s="25">
+        <v>1485</v>
+      </c>
+      <c r="E88" s="25">
+        <v>1</v>
+      </c>
+      <c r="F88" s="25">
+        <v>5</v>
+      </c>
+      <c r="G88" s="25">
+        <v>0</v>
+      </c>
+      <c r="H88" s="25">
+        <v>1</v>
+      </c>
+      <c r="I88" s="25">
+        <v>109</v>
+      </c>
+      <c r="J88" s="25">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="89" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A89" s="29">
+        <v>43989</v>
+      </c>
+      <c r="B89" s="30">
+        <v>83316</v>
+      </c>
+      <c r="C89" s="31">
+        <v>211</v>
+      </c>
+      <c r="D89" s="31">
+        <v>1485</v>
+      </c>
+      <c r="E89" s="31">
+        <v>0</v>
+      </c>
+      <c r="F89" s="31">
+        <v>5</v>
+      </c>
+      <c r="G89" s="31">
+        <v>0</v>
+      </c>
+      <c r="H89" s="31">
+        <v>0</v>
+      </c>
+      <c r="I89" s="31">
+        <v>109</v>
+      </c>
+      <c r="J89" s="31">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="90" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A90" s="20">
+        <v>43990</v>
+      </c>
+      <c r="B90" s="21">
+        <v>84130</v>
+      </c>
+      <c r="C90" s="22">
+        <v>814</v>
+      </c>
+      <c r="D90" s="22">
+        <v>1486</v>
+      </c>
+      <c r="E90" s="22">
+        <v>1</v>
+      </c>
+      <c r="F90" s="22">
+        <v>6</v>
+      </c>
+      <c r="G90" s="22">
+        <v>0</v>
+      </c>
+      <c r="H90" s="22">
+        <v>0</v>
+      </c>
+      <c r="I90" s="22">
+        <v>109</v>
+      </c>
+      <c r="J90" s="22">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="91" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A91" s="20">
+        <v>43991</v>
+      </c>
+      <c r="B91" s="21">
+        <v>84868</v>
+      </c>
+      <c r="C91" s="22">
+        <v>738</v>
+      </c>
+      <c r="D91" s="22">
+        <v>1488</v>
+      </c>
+      <c r="E91" s="22">
+        <v>2</v>
+      </c>
+      <c r="F91" s="22">
+        <v>6</v>
+      </c>
+      <c r="G91" s="22">
+        <v>0</v>
+      </c>
+      <c r="H91" s="22">
+        <v>0</v>
+      </c>
+      <c r="I91" s="22">
+        <v>109</v>
+      </c>
+      <c r="J91" s="22">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="92" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A92" s="23">
+        <v>43992</v>
+      </c>
+      <c r="B92" s="24">
+        <v>85626</v>
+      </c>
+      <c r="C92" s="25">
+        <v>758</v>
+      </c>
+      <c r="D92" s="25">
+        <v>1488</v>
+      </c>
+      <c r="E92" s="25">
+        <v>0</v>
+      </c>
+      <c r="F92" s="25">
+        <v>6</v>
+      </c>
+      <c r="G92" s="25">
+        <v>0</v>
+      </c>
+      <c r="H92" s="25">
+        <v>0</v>
+      </c>
+      <c r="I92" s="25">
+        <v>109</v>
+      </c>
+      <c r="J92" s="25">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="93" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A93" s="29">
+        <v>43993</v>
+      </c>
+      <c r="B93" s="30">
+        <v>86328</v>
+      </c>
+      <c r="C93" s="31">
+        <v>702</v>
+      </c>
+      <c r="D93" s="31">
+        <v>1490</v>
+      </c>
+      <c r="E93" s="31">
+        <v>2</v>
+      </c>
+      <c r="F93" s="31">
+        <v>6</v>
+      </c>
+      <c r="G93" s="31">
+        <v>0</v>
+      </c>
+      <c r="H93" s="31">
+        <v>0</v>
+      </c>
+      <c r="I93" s="31">
+        <v>109</v>
+      </c>
+      <c r="J93" s="31">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="94" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A94" s="23">
+        <v>43994</v>
+      </c>
+      <c r="B94" s="24">
+        <v>87095</v>
+      </c>
+      <c r="C94" s="25">
+        <v>767</v>
+      </c>
+      <c r="D94" s="25">
+        <v>1492</v>
+      </c>
+      <c r="E94" s="25">
+        <v>2</v>
+      </c>
+      <c r="F94" s="25">
+        <v>6</v>
+      </c>
+      <c r="G94" s="25">
+        <v>0</v>
+      </c>
+      <c r="H94" s="25">
+        <v>0</v>
+      </c>
+      <c r="I94" s="25">
+        <v>109</v>
+      </c>
+      <c r="J94" s="25">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="95" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A95" s="29">
+        <v>43995</v>
+      </c>
+      <c r="B95" s="30">
+        <v>87386</v>
+      </c>
+      <c r="C95" s="31">
+        <v>291</v>
+      </c>
+      <c r="D95" s="31">
+        <v>1495</v>
+      </c>
+      <c r="E95" s="31">
+        <v>3</v>
+      </c>
+      <c r="F95" s="31">
+        <v>6</v>
+      </c>
+      <c r="G95" s="31">
+        <v>0</v>
+      </c>
+      <c r="H95" s="31">
+        <v>0</v>
+      </c>
+      <c r="I95" s="31">
+        <v>109</v>
+      </c>
+      <c r="J95" s="31">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="96" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A96" s="23">
+        <v>43996</v>
+      </c>
+      <c r="B96" s="24">
+        <v>87598</v>
+      </c>
+      <c r="C96" s="25">
+        <v>212</v>
+      </c>
+      <c r="D96" s="25">
+        <v>1496</v>
+      </c>
+      <c r="E96" s="25">
+        <v>1</v>
+      </c>
+      <c r="F96" s="25">
+        <v>7</v>
+      </c>
+      <c r="G96" s="25">
+        <v>1</v>
+      </c>
+      <c r="H96" s="25">
+        <v>0</v>
+      </c>
+      <c r="I96" s="25">
+        <v>109</v>
+      </c>
+      <c r="J96" s="25">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="97" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A97" s="20">
+        <v>43997</v>
+      </c>
+      <c r="B97" s="21">
+        <v>88165</v>
+      </c>
+      <c r="C97" s="22">
+        <v>567</v>
+      </c>
+      <c r="D97" s="22">
+        <v>1499</v>
+      </c>
+      <c r="E97" s="22">
+        <v>3</v>
+      </c>
+      <c r="F97" s="22">
+        <v>7</v>
+      </c>
+      <c r="G97" s="22">
+        <v>1</v>
+      </c>
+      <c r="H97" s="22">
+        <v>0</v>
+      </c>
+      <c r="I97" s="22">
+        <v>109</v>
+      </c>
+      <c r="J97" s="22">
+        <v>0</v>
+      </c>
+    </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>

</xml_diff>

<commit_message>
Data updated by GitHub Bot (2020-06-16 20)
</commit_message>
<xml_diff>
--- a/output/snapshot/fdcf2531-4c3e-5c02-b63c-ee160ead6dea.xlsx
+++ b/output/snapshot/fdcf2531-4c3e-5c02-b63c-ee160ead6dea.xlsx
@@ -1,16 +1,15 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="21929"/>
-  <workbookPr/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
+  <fileVersion appName="xl" lastEdited="6" lowestEdited="6" rupBuild="14420"/>
+  <workbookPr defaultThemeVersion="164011"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="I:\AKTUALNI PODATKI - KORONA\Za objavo na GOV.SI\ang\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{1E6DD62F-2BE2-47DC-A7ED-9B57C1589256}" xr6:coauthVersionLast="44" xr6:coauthVersionMax="44" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="2295" yWindow="2295" windowWidth="21600" windowHeight="11205"/>
   </bookViews>
   <sheets>
     <sheet name="Covid-19 podatki" sheetId="1" r:id="rId1"/>
@@ -60,11 +59,11 @@
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" mc:Ignorable="x14ac x16r2">
   <numFmts count="1">
     <numFmt numFmtId="164" formatCode="d/\ m/\ yyyy;@"/>
   </numFmts>
-  <fonts count="4" x14ac:knownFonts="1">
+  <fonts count="5" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -93,6 +92,13 @@
       <name val="Calibri Light"/>
       <scheme val="major"/>
     </font>
+    <font>
+      <sz val="10"/>
+      <color theme="1"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
   </fonts>
   <fills count="3">
     <fill>
@@ -108,7 +114,7 @@
       </patternFill>
     </fill>
   </fills>
-  <borders count="2">
+  <borders count="3">
     <border>
       <left/>
       <right/>
@@ -129,11 +135,26 @@
       <bottom/>
       <diagonal/>
     </border>
+    <border>
+      <left style="thin">
+        <color theme="4"/>
+      </left>
+      <right style="thin">
+        <color theme="4"/>
+      </right>
+      <top style="thin">
+        <color theme="4"/>
+      </top>
+      <bottom style="thin">
+        <color theme="4"/>
+      </bottom>
+      <diagonal/>
+    </border>
   </borders>
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="26">
+  <cellXfs count="32">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="49" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyAlignment="1" applyProtection="1">
       <alignment horizontal="left" vertical="top"/>
@@ -208,6 +229,24 @@
       <alignment horizontal="right"/>
     </xf>
     <xf numFmtId="0" fontId="3" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="right"/>
+    </xf>
+    <xf numFmtId="164" fontId="4" fillId="2" borderId="2" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="right" vertical="top"/>
+    </xf>
+    <xf numFmtId="3" fontId="4" fillId="2" borderId="2" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="right"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="2" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="right"/>
+    </xf>
+    <xf numFmtId="164" fontId="3" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="right" vertical="top"/>
+    </xf>
+    <xf numFmtId="3" fontId="3" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="right"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="right"/>
     </xf>
   </cellXfs>
@@ -399,8 +438,8 @@
 </file>
 
 <file path=xl/tables/table1.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="1" xr:uid="{00000000-000C-0000-FFFF-FFFF00000000}" name="Tabela1" displayName="Tabela1" ref="A1:J75" totalsRowShown="0" headerRowDxfId="11" dataDxfId="10">
-  <autoFilter ref="A1:J75" xr:uid="{00000000-0009-0000-0100-000001000000}">
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="1" name="Tabela1" displayName="Tabela1" ref="A1:J97" totalsRowShown="0" headerRowDxfId="11" dataDxfId="10">
+  <autoFilter ref="A1:J97">
     <filterColumn colId="0" hiddenButton="1"/>
     <filterColumn colId="1" hiddenButton="1"/>
     <filterColumn colId="2" hiddenButton="1"/>
@@ -413,16 +452,16 @@
     <filterColumn colId="9" hiddenButton="1"/>
   </autoFilter>
   <tableColumns count="10">
-    <tableColumn id="1" xr3:uid="{00000000-0010-0000-0000-000001000000}" name="Date" dataDxfId="9"/>
-    <tableColumn id="2" xr3:uid="{00000000-0010-0000-0000-000002000000}" name="Tested (all)" dataDxfId="8"/>
-    <tableColumn id="3" xr3:uid="{00000000-0010-0000-0000-000003000000}" name="Tested (daily)" dataDxfId="7"/>
-    <tableColumn id="4" xr3:uid="{00000000-0010-0000-0000-000004000000}" name="Positive (all)" dataDxfId="6"/>
-    <tableColumn id="5" xr3:uid="{00000000-0010-0000-0000-000005000000}" name="Positive (daily)" dataDxfId="5"/>
-    <tableColumn id="6" xr3:uid="{00000000-0010-0000-0000-000006000000}" name="All hospitalized on certain day" dataDxfId="4"/>
-    <tableColumn id="7" xr3:uid="{00000000-0010-0000-0000-000007000000}" name="All persons in intensive care on certain day" dataDxfId="3"/>
-    <tableColumn id="10" xr3:uid="{00000000-0010-0000-0000-00000A000000}" name="Discharged" dataDxfId="2"/>
-    <tableColumn id="8" xr3:uid="{00000000-0010-0000-0000-000008000000}" name="Deaths (all)" dataDxfId="1"/>
-    <tableColumn id="9" xr3:uid="{00000000-0010-0000-0000-000009000000}" name="Deaths (daily)" dataDxfId="0"/>
+    <tableColumn id="1" name="Date" dataDxfId="9"/>
+    <tableColumn id="2" name="Tested (all)" dataDxfId="8"/>
+    <tableColumn id="3" name="Tested (daily)" dataDxfId="7"/>
+    <tableColumn id="4" name="Positive (all)" dataDxfId="6"/>
+    <tableColumn id="5" name="Positive (daily)" dataDxfId="5"/>
+    <tableColumn id="6" name="All hospitalized on certain day" dataDxfId="4"/>
+    <tableColumn id="7" name="All persons in intensive care on certain day" dataDxfId="3"/>
+    <tableColumn id="10" name="Discharged" dataDxfId="2"/>
+    <tableColumn id="8" name="Deaths (all)" dataDxfId="1"/>
+    <tableColumn id="9" name="Deaths (daily)" dataDxfId="0"/>
   </tableColumns>
   <tableStyleInfo name="TableStyleLight16" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
   <extLst>
@@ -695,11 +734,11 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:J75"/>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <dimension ref="A1:J97"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A40" zoomScale="89" zoomScaleNormal="89" workbookViewId="0">
-      <selection activeCell="J74" sqref="J74"/>
+    <sheetView tabSelected="1" topLeftCell="A77" zoomScale="89" zoomScaleNormal="89" workbookViewId="0">
+      <selection activeCell="J97" sqref="A97:J97"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -3117,6 +3156,710 @@
         <v>0</v>
       </c>
     </row>
+    <row r="76" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A76" s="20">
+        <v>43976</v>
+      </c>
+      <c r="B76" s="21">
+        <v>75770</v>
+      </c>
+      <c r="C76" s="22">
+        <v>754</v>
+      </c>
+      <c r="D76" s="22">
+        <v>1469</v>
+      </c>
+      <c r="E76" s="22">
+        <v>0</v>
+      </c>
+      <c r="F76" s="22">
+        <v>9</v>
+      </c>
+      <c r="G76" s="22">
+        <v>2</v>
+      </c>
+      <c r="H76" s="22">
+        <v>6</v>
+      </c>
+      <c r="I76" s="22">
+        <v>108</v>
+      </c>
+      <c r="J76" s="22">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="77" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A77" s="20">
+        <v>43977</v>
+      </c>
+      <c r="B77" s="21">
+        <v>76579</v>
+      </c>
+      <c r="C77" s="22">
+        <v>809</v>
+      </c>
+      <c r="D77" s="22">
+        <v>1471</v>
+      </c>
+      <c r="E77" s="22">
+        <v>2</v>
+      </c>
+      <c r="F77" s="22">
+        <v>8</v>
+      </c>
+      <c r="G77" s="22">
+        <v>2</v>
+      </c>
+      <c r="H77" s="22">
+        <v>2</v>
+      </c>
+      <c r="I77" s="22">
+        <v>108</v>
+      </c>
+      <c r="J77" s="22">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="78" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A78" s="20">
+        <v>43978</v>
+      </c>
+      <c r="B78" s="21">
+        <v>77210</v>
+      </c>
+      <c r="C78" s="22">
+        <v>631</v>
+      </c>
+      <c r="D78" s="22">
+        <v>1473</v>
+      </c>
+      <c r="E78" s="22">
+        <v>2</v>
+      </c>
+      <c r="F78" s="22">
+        <v>7</v>
+      </c>
+      <c r="G78" s="22">
+        <v>2</v>
+      </c>
+      <c r="H78" s="22">
+        <v>1</v>
+      </c>
+      <c r="I78" s="22">
+        <v>108</v>
+      </c>
+      <c r="J78" s="22">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="79" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A79" s="20">
+        <v>43979</v>
+      </c>
+      <c r="B79" s="21">
+        <v>77916</v>
+      </c>
+      <c r="C79" s="22">
+        <v>706</v>
+      </c>
+      <c r="D79" s="22">
+        <v>1473</v>
+      </c>
+      <c r="E79" s="22">
+        <v>0</v>
+      </c>
+      <c r="F79" s="22">
+        <v>7</v>
+      </c>
+      <c r="G79" s="22">
+        <v>2</v>
+      </c>
+      <c r="H79" s="22">
+        <v>0</v>
+      </c>
+      <c r="I79" s="22">
+        <v>108</v>
+      </c>
+      <c r="J79" s="22">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="80" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A80" s="20">
+        <v>43980</v>
+      </c>
+      <c r="B80" s="21">
+        <v>78529</v>
+      </c>
+      <c r="C80" s="22">
+        <v>613</v>
+      </c>
+      <c r="D80" s="22">
+        <v>1473</v>
+      </c>
+      <c r="E80" s="22">
+        <v>0</v>
+      </c>
+      <c r="F80" s="22">
+        <v>7</v>
+      </c>
+      <c r="G80" s="22">
+        <v>2</v>
+      </c>
+      <c r="H80" s="22">
+        <v>0</v>
+      </c>
+      <c r="I80" s="22">
+        <v>108</v>
+      </c>
+      <c r="J80" s="22">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="81" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A81" s="20">
+        <v>43981</v>
+      </c>
+      <c r="B81" s="22">
+        <v>78793</v>
+      </c>
+      <c r="C81" s="22">
+        <v>264</v>
+      </c>
+      <c r="D81" s="22">
+        <v>1473</v>
+      </c>
+      <c r="E81" s="22">
+        <v>0</v>
+      </c>
+      <c r="F81" s="22">
+        <v>6</v>
+      </c>
+      <c r="G81" s="22">
+        <v>2</v>
+      </c>
+      <c r="H81" s="22">
+        <v>1</v>
+      </c>
+      <c r="I81" s="22">
+        <v>108</v>
+      </c>
+      <c r="J81" s="22">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="82" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A82" s="20">
+        <v>43982</v>
+      </c>
+      <c r="B82" s="21">
+        <v>79039</v>
+      </c>
+      <c r="C82" s="22">
+        <v>246</v>
+      </c>
+      <c r="D82" s="22">
+        <v>1473</v>
+      </c>
+      <c r="E82" s="22">
+        <v>0</v>
+      </c>
+      <c r="F82" s="22">
+        <v>5</v>
+      </c>
+      <c r="G82" s="22">
+        <v>1</v>
+      </c>
+      <c r="H82" s="22">
+        <v>0</v>
+      </c>
+      <c r="I82" s="22">
+        <v>109</v>
+      </c>
+      <c r="J82" s="22">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="83" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A83" s="20">
+        <v>43983</v>
+      </c>
+      <c r="B83" s="21">
+        <v>79698</v>
+      </c>
+      <c r="C83" s="22">
+        <v>659</v>
+      </c>
+      <c r="D83" s="22">
+        <v>1475</v>
+      </c>
+      <c r="E83" s="22">
+        <v>2</v>
+      </c>
+      <c r="F83" s="22">
+        <v>5</v>
+      </c>
+      <c r="G83" s="22">
+        <v>1</v>
+      </c>
+      <c r="H83" s="22">
+        <v>0</v>
+      </c>
+      <c r="I83" s="22">
+        <v>109</v>
+      </c>
+      <c r="J83" s="22">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="84" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A84" s="20">
+        <v>43984</v>
+      </c>
+      <c r="B84" s="21">
+        <v>80505</v>
+      </c>
+      <c r="C84" s="22">
+        <v>807</v>
+      </c>
+      <c r="D84" s="22">
+        <v>1477</v>
+      </c>
+      <c r="E84" s="22">
+        <v>2</v>
+      </c>
+      <c r="F84" s="22">
+        <v>5</v>
+      </c>
+      <c r="G84" s="22">
+        <v>0</v>
+      </c>
+      <c r="H84" s="22">
+        <v>0</v>
+      </c>
+      <c r="I84" s="22">
+        <v>109</v>
+      </c>
+      <c r="J84" s="22">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="85" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A85" s="20">
+        <v>43985</v>
+      </c>
+      <c r="B85" s="21">
+        <v>81333</v>
+      </c>
+      <c r="C85" s="22">
+        <v>828</v>
+      </c>
+      <c r="D85" s="22">
+        <v>1477</v>
+      </c>
+      <c r="E85" s="22">
+        <v>0</v>
+      </c>
+      <c r="F85" s="22">
+        <v>5</v>
+      </c>
+      <c r="G85" s="22">
+        <v>0</v>
+      </c>
+      <c r="H85" s="22">
+        <v>0</v>
+      </c>
+      <c r="I85" s="22">
+        <v>109</v>
+      </c>
+      <c r="J85" s="22">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="86" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A86" s="26">
+        <v>43986</v>
+      </c>
+      <c r="B86" s="27">
+        <v>82161</v>
+      </c>
+      <c r="C86" s="28">
+        <v>828</v>
+      </c>
+      <c r="D86" s="28">
+        <v>1479</v>
+      </c>
+      <c r="E86" s="28">
+        <v>2</v>
+      </c>
+      <c r="F86" s="28">
+        <v>6</v>
+      </c>
+      <c r="G86" s="28">
+        <v>0</v>
+      </c>
+      <c r="H86" s="28">
+        <v>0</v>
+      </c>
+      <c r="I86" s="28">
+        <v>109</v>
+      </c>
+      <c r="J86" s="28">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="87" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A87" s="29">
+        <v>43987</v>
+      </c>
+      <c r="B87" s="30">
+        <v>82876</v>
+      </c>
+      <c r="C87" s="31">
+        <v>715</v>
+      </c>
+      <c r="D87" s="31">
+        <v>1484</v>
+      </c>
+      <c r="E87" s="31">
+        <v>5</v>
+      </c>
+      <c r="F87" s="31">
+        <v>6</v>
+      </c>
+      <c r="G87" s="31">
+        <v>0</v>
+      </c>
+      <c r="H87" s="31">
+        <v>0</v>
+      </c>
+      <c r="I87" s="31">
+        <v>109</v>
+      </c>
+      <c r="J87" s="31">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="88" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A88" s="23">
+        <v>43988</v>
+      </c>
+      <c r="B88" s="24">
+        <v>83105</v>
+      </c>
+      <c r="C88" s="25">
+        <v>229</v>
+      </c>
+      <c r="D88" s="25">
+        <v>1485</v>
+      </c>
+      <c r="E88" s="25">
+        <v>1</v>
+      </c>
+      <c r="F88" s="25">
+        <v>5</v>
+      </c>
+      <c r="G88" s="25">
+        <v>0</v>
+      </c>
+      <c r="H88" s="25">
+        <v>1</v>
+      </c>
+      <c r="I88" s="25">
+        <v>109</v>
+      </c>
+      <c r="J88" s="25">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="89" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A89" s="29">
+        <v>43989</v>
+      </c>
+      <c r="B89" s="30">
+        <v>83316</v>
+      </c>
+      <c r="C89" s="31">
+        <v>211</v>
+      </c>
+      <c r="D89" s="31">
+        <v>1485</v>
+      </c>
+      <c r="E89" s="31">
+        <v>0</v>
+      </c>
+      <c r="F89" s="31">
+        <v>5</v>
+      </c>
+      <c r="G89" s="31">
+        <v>0</v>
+      </c>
+      <c r="H89" s="31">
+        <v>0</v>
+      </c>
+      <c r="I89" s="31">
+        <v>109</v>
+      </c>
+      <c r="J89" s="31">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="90" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A90" s="20">
+        <v>43990</v>
+      </c>
+      <c r="B90" s="21">
+        <v>84130</v>
+      </c>
+      <c r="C90" s="22">
+        <v>814</v>
+      </c>
+      <c r="D90" s="22">
+        <v>1486</v>
+      </c>
+      <c r="E90" s="22">
+        <v>1</v>
+      </c>
+      <c r="F90" s="22">
+        <v>6</v>
+      </c>
+      <c r="G90" s="22">
+        <v>0</v>
+      </c>
+      <c r="H90" s="22">
+        <v>0</v>
+      </c>
+      <c r="I90" s="22">
+        <v>109</v>
+      </c>
+      <c r="J90" s="22">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="91" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A91" s="20">
+        <v>43991</v>
+      </c>
+      <c r="B91" s="21">
+        <v>84868</v>
+      </c>
+      <c r="C91" s="22">
+        <v>738</v>
+      </c>
+      <c r="D91" s="22">
+        <v>1488</v>
+      </c>
+      <c r="E91" s="22">
+        <v>2</v>
+      </c>
+      <c r="F91" s="22">
+        <v>6</v>
+      </c>
+      <c r="G91" s="22">
+        <v>0</v>
+      </c>
+      <c r="H91" s="22">
+        <v>0</v>
+      </c>
+      <c r="I91" s="22">
+        <v>109</v>
+      </c>
+      <c r="J91" s="22">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="92" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A92" s="23">
+        <v>43992</v>
+      </c>
+      <c r="B92" s="24">
+        <v>85626</v>
+      </c>
+      <c r="C92" s="25">
+        <v>758</v>
+      </c>
+      <c r="D92" s="25">
+        <v>1488</v>
+      </c>
+      <c r="E92" s="25">
+        <v>0</v>
+      </c>
+      <c r="F92" s="25">
+        <v>6</v>
+      </c>
+      <c r="G92" s="25">
+        <v>0</v>
+      </c>
+      <c r="H92" s="25">
+        <v>0</v>
+      </c>
+      <c r="I92" s="25">
+        <v>109</v>
+      </c>
+      <c r="J92" s="25">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="93" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A93" s="29">
+        <v>43993</v>
+      </c>
+      <c r="B93" s="30">
+        <v>86328</v>
+      </c>
+      <c r="C93" s="31">
+        <v>702</v>
+      </c>
+      <c r="D93" s="31">
+        <v>1490</v>
+      </c>
+      <c r="E93" s="31">
+        <v>2</v>
+      </c>
+      <c r="F93" s="31">
+        <v>6</v>
+      </c>
+      <c r="G93" s="31">
+        <v>0</v>
+      </c>
+      <c r="H93" s="31">
+        <v>0</v>
+      </c>
+      <c r="I93" s="31">
+        <v>109</v>
+      </c>
+      <c r="J93" s="31">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="94" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A94" s="23">
+        <v>43994</v>
+      </c>
+      <c r="B94" s="24">
+        <v>87095</v>
+      </c>
+      <c r="C94" s="25">
+        <v>767</v>
+      </c>
+      <c r="D94" s="25">
+        <v>1492</v>
+      </c>
+      <c r="E94" s="25">
+        <v>2</v>
+      </c>
+      <c r="F94" s="25">
+        <v>6</v>
+      </c>
+      <c r="G94" s="25">
+        <v>0</v>
+      </c>
+      <c r="H94" s="25">
+        <v>0</v>
+      </c>
+      <c r="I94" s="25">
+        <v>109</v>
+      </c>
+      <c r="J94" s="25">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="95" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A95" s="29">
+        <v>43995</v>
+      </c>
+      <c r="B95" s="30">
+        <v>87386</v>
+      </c>
+      <c r="C95" s="31">
+        <v>291</v>
+      </c>
+      <c r="D95" s="31">
+        <v>1495</v>
+      </c>
+      <c r="E95" s="31">
+        <v>3</v>
+      </c>
+      <c r="F95" s="31">
+        <v>6</v>
+      </c>
+      <c r="G95" s="31">
+        <v>0</v>
+      </c>
+      <c r="H95" s="31">
+        <v>0</v>
+      </c>
+      <c r="I95" s="31">
+        <v>109</v>
+      </c>
+      <c r="J95" s="31">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="96" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A96" s="23">
+        <v>43996</v>
+      </c>
+      <c r="B96" s="24">
+        <v>87598</v>
+      </c>
+      <c r="C96" s="25">
+        <v>212</v>
+      </c>
+      <c r="D96" s="25">
+        <v>1496</v>
+      </c>
+      <c r="E96" s="25">
+        <v>1</v>
+      </c>
+      <c r="F96" s="25">
+        <v>7</v>
+      </c>
+      <c r="G96" s="25">
+        <v>1</v>
+      </c>
+      <c r="H96" s="25">
+        <v>0</v>
+      </c>
+      <c r="I96" s="25">
+        <v>109</v>
+      </c>
+      <c r="J96" s="25">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="97" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A97" s="20">
+        <v>43997</v>
+      </c>
+      <c r="B97" s="21">
+        <v>88165</v>
+      </c>
+      <c r="C97" s="22">
+        <v>567</v>
+      </c>
+      <c r="D97" s="22">
+        <v>1499</v>
+      </c>
+      <c r="E97" s="22">
+        <v>3</v>
+      </c>
+      <c r="F97" s="22">
+        <v>7</v>
+      </c>
+      <c r="G97" s="22">
+        <v>1</v>
+      </c>
+      <c r="H97" s="22">
+        <v>0</v>
+      </c>
+      <c r="I97" s="22">
+        <v>109</v>
+      </c>
+      <c r="J97" s="22">
+        <v>0</v>
+      </c>
+    </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>

</xml_diff>

<commit_message>
Data updated by GitHub Bot (2020-06-17 12)
</commit_message>
<xml_diff>
--- a/output/snapshot/fdcf2531-4c3e-5c02-b63c-ee160ead6dea.xlsx
+++ b/output/snapshot/fdcf2531-4c3e-5c02-b63c-ee160ead6dea.xlsx
@@ -1,16 +1,15 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="21929"/>
-  <workbookPr/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
+  <fileVersion appName="xl" lastEdited="6" lowestEdited="6" rupBuild="14420"/>
+  <workbookPr defaultThemeVersion="164011"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="I:\AKTUALNI PODATKI - KORONA\Za objavo na GOV.SI\ang\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{1E6DD62F-2BE2-47DC-A7ED-9B57C1589256}" xr6:coauthVersionLast="44" xr6:coauthVersionMax="44" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="2295" yWindow="2295" windowWidth="21600" windowHeight="11205"/>
   </bookViews>
   <sheets>
     <sheet name="Covid-19 podatki" sheetId="1" r:id="rId1"/>
@@ -60,11 +59,11 @@
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" mc:Ignorable="x14ac x16r2">
   <numFmts count="1">
     <numFmt numFmtId="164" formatCode="d/\ m/\ yyyy;@"/>
   </numFmts>
-  <fonts count="4" x14ac:knownFonts="1">
+  <fonts count="5" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -93,6 +92,13 @@
       <name val="Calibri Light"/>
       <scheme val="major"/>
     </font>
+    <font>
+      <sz val="10"/>
+      <color theme="1"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
   </fonts>
   <fills count="3">
     <fill>
@@ -108,7 +114,7 @@
       </patternFill>
     </fill>
   </fills>
-  <borders count="2">
+  <borders count="3">
     <border>
       <left/>
       <right/>
@@ -129,11 +135,26 @@
       <bottom/>
       <diagonal/>
     </border>
+    <border>
+      <left style="thin">
+        <color theme="4"/>
+      </left>
+      <right style="thin">
+        <color theme="4"/>
+      </right>
+      <top style="thin">
+        <color theme="4"/>
+      </top>
+      <bottom style="thin">
+        <color theme="4"/>
+      </bottom>
+      <diagonal/>
+    </border>
   </borders>
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="26">
+  <cellXfs count="32">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="49" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyAlignment="1" applyProtection="1">
       <alignment horizontal="left" vertical="top"/>
@@ -208,6 +229,24 @@
       <alignment horizontal="right"/>
     </xf>
     <xf numFmtId="0" fontId="3" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="right"/>
+    </xf>
+    <xf numFmtId="164" fontId="4" fillId="2" borderId="2" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="right" vertical="top"/>
+    </xf>
+    <xf numFmtId="3" fontId="4" fillId="2" borderId="2" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="right"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="2" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="right"/>
+    </xf>
+    <xf numFmtId="164" fontId="3" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="right" vertical="top"/>
+    </xf>
+    <xf numFmtId="3" fontId="3" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="right"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="right"/>
     </xf>
   </cellXfs>
@@ -399,8 +438,8 @@
 </file>
 
 <file path=xl/tables/table1.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="1" xr:uid="{00000000-000C-0000-FFFF-FFFF00000000}" name="Tabela1" displayName="Tabela1" ref="A1:J75" totalsRowShown="0" headerRowDxfId="11" dataDxfId="10">
-  <autoFilter ref="A1:J75" xr:uid="{00000000-0009-0000-0100-000001000000}">
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="1" name="Tabela1" displayName="Tabela1" ref="A1:J98" totalsRowShown="0" headerRowDxfId="11" dataDxfId="10">
+  <autoFilter ref="A1:J98">
     <filterColumn colId="0" hiddenButton="1"/>
     <filterColumn colId="1" hiddenButton="1"/>
     <filterColumn colId="2" hiddenButton="1"/>
@@ -413,16 +452,16 @@
     <filterColumn colId="9" hiddenButton="1"/>
   </autoFilter>
   <tableColumns count="10">
-    <tableColumn id="1" xr3:uid="{00000000-0010-0000-0000-000001000000}" name="Date" dataDxfId="9"/>
-    <tableColumn id="2" xr3:uid="{00000000-0010-0000-0000-000002000000}" name="Tested (all)" dataDxfId="8"/>
-    <tableColumn id="3" xr3:uid="{00000000-0010-0000-0000-000003000000}" name="Tested (daily)" dataDxfId="7"/>
-    <tableColumn id="4" xr3:uid="{00000000-0010-0000-0000-000004000000}" name="Positive (all)" dataDxfId="6"/>
-    <tableColumn id="5" xr3:uid="{00000000-0010-0000-0000-000005000000}" name="Positive (daily)" dataDxfId="5"/>
-    <tableColumn id="6" xr3:uid="{00000000-0010-0000-0000-000006000000}" name="All hospitalized on certain day" dataDxfId="4"/>
-    <tableColumn id="7" xr3:uid="{00000000-0010-0000-0000-000007000000}" name="All persons in intensive care on certain day" dataDxfId="3"/>
-    <tableColumn id="10" xr3:uid="{00000000-0010-0000-0000-00000A000000}" name="Discharged" dataDxfId="2"/>
-    <tableColumn id="8" xr3:uid="{00000000-0010-0000-0000-000008000000}" name="Deaths (all)" dataDxfId="1"/>
-    <tableColumn id="9" xr3:uid="{00000000-0010-0000-0000-000009000000}" name="Deaths (daily)" dataDxfId="0"/>
+    <tableColumn id="1" name="Date" dataDxfId="9"/>
+    <tableColumn id="2" name="Tested (all)" dataDxfId="8"/>
+    <tableColumn id="3" name="Tested (daily)" dataDxfId="7"/>
+    <tableColumn id="4" name="Positive (all)" dataDxfId="6"/>
+    <tableColumn id="5" name="Positive (daily)" dataDxfId="5"/>
+    <tableColumn id="6" name="All hospitalized on certain day" dataDxfId="4"/>
+    <tableColumn id="7" name="All persons in intensive care on certain day" dataDxfId="3"/>
+    <tableColumn id="10" name="Discharged" dataDxfId="2"/>
+    <tableColumn id="8" name="Deaths (all)" dataDxfId="1"/>
+    <tableColumn id="9" name="Deaths (daily)" dataDxfId="0"/>
   </tableColumns>
   <tableStyleInfo name="TableStyleLight16" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
   <extLst>
@@ -695,11 +734,11 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:J75"/>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <dimension ref="A1:J98"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A40" zoomScale="89" zoomScaleNormal="89" workbookViewId="0">
-      <selection activeCell="J74" sqref="J74"/>
+    <sheetView tabSelected="1" topLeftCell="A77" zoomScale="89" zoomScaleNormal="89" workbookViewId="0">
+      <selection activeCell="A98" sqref="A98:J98"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -3117,6 +3156,742 @@
         <v>0</v>
       </c>
     </row>
+    <row r="76" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A76" s="20">
+        <v>43976</v>
+      </c>
+      <c r="B76" s="21">
+        <v>75770</v>
+      </c>
+      <c r="C76" s="22">
+        <v>754</v>
+      </c>
+      <c r="D76" s="22">
+        <v>1469</v>
+      </c>
+      <c r="E76" s="22">
+        <v>0</v>
+      </c>
+      <c r="F76" s="22">
+        <v>9</v>
+      </c>
+      <c r="G76" s="22">
+        <v>2</v>
+      </c>
+      <c r="H76" s="22">
+        <v>6</v>
+      </c>
+      <c r="I76" s="22">
+        <v>108</v>
+      </c>
+      <c r="J76" s="22">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="77" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A77" s="20">
+        <v>43977</v>
+      </c>
+      <c r="B77" s="21">
+        <v>76579</v>
+      </c>
+      <c r="C77" s="22">
+        <v>809</v>
+      </c>
+      <c r="D77" s="22">
+        <v>1471</v>
+      </c>
+      <c r="E77" s="22">
+        <v>2</v>
+      </c>
+      <c r="F77" s="22">
+        <v>8</v>
+      </c>
+      <c r="G77" s="22">
+        <v>2</v>
+      </c>
+      <c r="H77" s="22">
+        <v>2</v>
+      </c>
+      <c r="I77" s="22">
+        <v>108</v>
+      </c>
+      <c r="J77" s="22">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="78" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A78" s="20">
+        <v>43978</v>
+      </c>
+      <c r="B78" s="21">
+        <v>77210</v>
+      </c>
+      <c r="C78" s="22">
+        <v>631</v>
+      </c>
+      <c r="D78" s="22">
+        <v>1473</v>
+      </c>
+      <c r="E78" s="22">
+        <v>2</v>
+      </c>
+      <c r="F78" s="22">
+        <v>7</v>
+      </c>
+      <c r="G78" s="22">
+        <v>2</v>
+      </c>
+      <c r="H78" s="22">
+        <v>1</v>
+      </c>
+      <c r="I78" s="22">
+        <v>108</v>
+      </c>
+      <c r="J78" s="22">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="79" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A79" s="20">
+        <v>43979</v>
+      </c>
+      <c r="B79" s="21">
+        <v>77916</v>
+      </c>
+      <c r="C79" s="22">
+        <v>706</v>
+      </c>
+      <c r="D79" s="22">
+        <v>1473</v>
+      </c>
+      <c r="E79" s="22">
+        <v>0</v>
+      </c>
+      <c r="F79" s="22">
+        <v>7</v>
+      </c>
+      <c r="G79" s="22">
+        <v>2</v>
+      </c>
+      <c r="H79" s="22">
+        <v>0</v>
+      </c>
+      <c r="I79" s="22">
+        <v>108</v>
+      </c>
+      <c r="J79" s="22">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="80" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A80" s="20">
+        <v>43980</v>
+      </c>
+      <c r="B80" s="21">
+        <v>78529</v>
+      </c>
+      <c r="C80" s="22">
+        <v>613</v>
+      </c>
+      <c r="D80" s="22">
+        <v>1473</v>
+      </c>
+      <c r="E80" s="22">
+        <v>0</v>
+      </c>
+      <c r="F80" s="22">
+        <v>7</v>
+      </c>
+      <c r="G80" s="22">
+        <v>2</v>
+      </c>
+      <c r="H80" s="22">
+        <v>0</v>
+      </c>
+      <c r="I80" s="22">
+        <v>108</v>
+      </c>
+      <c r="J80" s="22">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="81" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A81" s="20">
+        <v>43981</v>
+      </c>
+      <c r="B81" s="22">
+        <v>78793</v>
+      </c>
+      <c r="C81" s="22">
+        <v>264</v>
+      </c>
+      <c r="D81" s="22">
+        <v>1473</v>
+      </c>
+      <c r="E81" s="22">
+        <v>0</v>
+      </c>
+      <c r="F81" s="22">
+        <v>6</v>
+      </c>
+      <c r="G81" s="22">
+        <v>2</v>
+      </c>
+      <c r="H81" s="22">
+        <v>1</v>
+      </c>
+      <c r="I81" s="22">
+        <v>108</v>
+      </c>
+      <c r="J81" s="22">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="82" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A82" s="20">
+        <v>43982</v>
+      </c>
+      <c r="B82" s="21">
+        <v>79039</v>
+      </c>
+      <c r="C82" s="22">
+        <v>246</v>
+      </c>
+      <c r="D82" s="22">
+        <v>1473</v>
+      </c>
+      <c r="E82" s="22">
+        <v>0</v>
+      </c>
+      <c r="F82" s="22">
+        <v>5</v>
+      </c>
+      <c r="G82" s="22">
+        <v>1</v>
+      </c>
+      <c r="H82" s="22">
+        <v>0</v>
+      </c>
+      <c r="I82" s="22">
+        <v>109</v>
+      </c>
+      <c r="J82" s="22">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="83" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A83" s="20">
+        <v>43983</v>
+      </c>
+      <c r="B83" s="21">
+        <v>79698</v>
+      </c>
+      <c r="C83" s="22">
+        <v>659</v>
+      </c>
+      <c r="D83" s="22">
+        <v>1475</v>
+      </c>
+      <c r="E83" s="22">
+        <v>2</v>
+      </c>
+      <c r="F83" s="22">
+        <v>5</v>
+      </c>
+      <c r="G83" s="22">
+        <v>1</v>
+      </c>
+      <c r="H83" s="22">
+        <v>0</v>
+      </c>
+      <c r="I83" s="22">
+        <v>109</v>
+      </c>
+      <c r="J83" s="22">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="84" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A84" s="20">
+        <v>43984</v>
+      </c>
+      <c r="B84" s="21">
+        <v>80505</v>
+      </c>
+      <c r="C84" s="22">
+        <v>807</v>
+      </c>
+      <c r="D84" s="22">
+        <v>1477</v>
+      </c>
+      <c r="E84" s="22">
+        <v>2</v>
+      </c>
+      <c r="F84" s="22">
+        <v>5</v>
+      </c>
+      <c r="G84" s="22">
+        <v>0</v>
+      </c>
+      <c r="H84" s="22">
+        <v>0</v>
+      </c>
+      <c r="I84" s="22">
+        <v>109</v>
+      </c>
+      <c r="J84" s="22">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="85" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A85" s="20">
+        <v>43985</v>
+      </c>
+      <c r="B85" s="21">
+        <v>81333</v>
+      </c>
+      <c r="C85" s="22">
+        <v>828</v>
+      </c>
+      <c r="D85" s="22">
+        <v>1477</v>
+      </c>
+      <c r="E85" s="22">
+        <v>0</v>
+      </c>
+      <c r="F85" s="22">
+        <v>5</v>
+      </c>
+      <c r="G85" s="22">
+        <v>0</v>
+      </c>
+      <c r="H85" s="22">
+        <v>0</v>
+      </c>
+      <c r="I85" s="22">
+        <v>109</v>
+      </c>
+      <c r="J85" s="22">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="86" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A86" s="26">
+        <v>43986</v>
+      </c>
+      <c r="B86" s="27">
+        <v>82161</v>
+      </c>
+      <c r="C86" s="28">
+        <v>828</v>
+      </c>
+      <c r="D86" s="28">
+        <v>1479</v>
+      </c>
+      <c r="E86" s="28">
+        <v>2</v>
+      </c>
+      <c r="F86" s="28">
+        <v>6</v>
+      </c>
+      <c r="G86" s="28">
+        <v>0</v>
+      </c>
+      <c r="H86" s="28">
+        <v>0</v>
+      </c>
+      <c r="I86" s="28">
+        <v>109</v>
+      </c>
+      <c r="J86" s="28">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="87" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A87" s="29">
+        <v>43987</v>
+      </c>
+      <c r="B87" s="30">
+        <v>82876</v>
+      </c>
+      <c r="C87" s="31">
+        <v>715</v>
+      </c>
+      <c r="D87" s="31">
+        <v>1484</v>
+      </c>
+      <c r="E87" s="31">
+        <v>5</v>
+      </c>
+      <c r="F87" s="31">
+        <v>6</v>
+      </c>
+      <c r="G87" s="31">
+        <v>0</v>
+      </c>
+      <c r="H87" s="31">
+        <v>0</v>
+      </c>
+      <c r="I87" s="31">
+        <v>109</v>
+      </c>
+      <c r="J87" s="31">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="88" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A88" s="23">
+        <v>43988</v>
+      </c>
+      <c r="B88" s="24">
+        <v>83105</v>
+      </c>
+      <c r="C88" s="25">
+        <v>229</v>
+      </c>
+      <c r="D88" s="25">
+        <v>1485</v>
+      </c>
+      <c r="E88" s="25">
+        <v>1</v>
+      </c>
+      <c r="F88" s="25">
+        <v>5</v>
+      </c>
+      <c r="G88" s="25">
+        <v>0</v>
+      </c>
+      <c r="H88" s="25">
+        <v>1</v>
+      </c>
+      <c r="I88" s="25">
+        <v>109</v>
+      </c>
+      <c r="J88" s="25">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="89" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A89" s="29">
+        <v>43989</v>
+      </c>
+      <c r="B89" s="30">
+        <v>83316</v>
+      </c>
+      <c r="C89" s="31">
+        <v>211</v>
+      </c>
+      <c r="D89" s="31">
+        <v>1485</v>
+      </c>
+      <c r="E89" s="31">
+        <v>0</v>
+      </c>
+      <c r="F89" s="31">
+        <v>5</v>
+      </c>
+      <c r="G89" s="31">
+        <v>0</v>
+      </c>
+      <c r="H89" s="31">
+        <v>0</v>
+      </c>
+      <c r="I89" s="31">
+        <v>109</v>
+      </c>
+      <c r="J89" s="31">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="90" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A90" s="20">
+        <v>43990</v>
+      </c>
+      <c r="B90" s="21">
+        <v>84130</v>
+      </c>
+      <c r="C90" s="22">
+        <v>814</v>
+      </c>
+      <c r="D90" s="22">
+        <v>1486</v>
+      </c>
+      <c r="E90" s="22">
+        <v>1</v>
+      </c>
+      <c r="F90" s="22">
+        <v>6</v>
+      </c>
+      <c r="G90" s="22">
+        <v>0</v>
+      </c>
+      <c r="H90" s="22">
+        <v>0</v>
+      </c>
+      <c r="I90" s="22">
+        <v>109</v>
+      </c>
+      <c r="J90" s="22">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="91" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A91" s="20">
+        <v>43991</v>
+      </c>
+      <c r="B91" s="21">
+        <v>84868</v>
+      </c>
+      <c r="C91" s="22">
+        <v>738</v>
+      </c>
+      <c r="D91" s="22">
+        <v>1488</v>
+      </c>
+      <c r="E91" s="22">
+        <v>2</v>
+      </c>
+      <c r="F91" s="22">
+        <v>6</v>
+      </c>
+      <c r="G91" s="22">
+        <v>0</v>
+      </c>
+      <c r="H91" s="22">
+        <v>0</v>
+      </c>
+      <c r="I91" s="22">
+        <v>109</v>
+      </c>
+      <c r="J91" s="22">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="92" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A92" s="23">
+        <v>43992</v>
+      </c>
+      <c r="B92" s="24">
+        <v>85626</v>
+      </c>
+      <c r="C92" s="25">
+        <v>758</v>
+      </c>
+      <c r="D92" s="25">
+        <v>1488</v>
+      </c>
+      <c r="E92" s="25">
+        <v>0</v>
+      </c>
+      <c r="F92" s="25">
+        <v>6</v>
+      </c>
+      <c r="G92" s="25">
+        <v>0</v>
+      </c>
+      <c r="H92" s="25">
+        <v>0</v>
+      </c>
+      <c r="I92" s="25">
+        <v>109</v>
+      </c>
+      <c r="J92" s="25">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="93" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A93" s="29">
+        <v>43993</v>
+      </c>
+      <c r="B93" s="30">
+        <v>86328</v>
+      </c>
+      <c r="C93" s="31">
+        <v>702</v>
+      </c>
+      <c r="D93" s="31">
+        <v>1490</v>
+      </c>
+      <c r="E93" s="31">
+        <v>2</v>
+      </c>
+      <c r="F93" s="31">
+        <v>6</v>
+      </c>
+      <c r="G93" s="31">
+        <v>0</v>
+      </c>
+      <c r="H93" s="31">
+        <v>0</v>
+      </c>
+      <c r="I93" s="31">
+        <v>109</v>
+      </c>
+      <c r="J93" s="31">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="94" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A94" s="23">
+        <v>43994</v>
+      </c>
+      <c r="B94" s="24">
+        <v>87095</v>
+      </c>
+      <c r="C94" s="25">
+        <v>767</v>
+      </c>
+      <c r="D94" s="25">
+        <v>1492</v>
+      </c>
+      <c r="E94" s="25">
+        <v>2</v>
+      </c>
+      <c r="F94" s="25">
+        <v>6</v>
+      </c>
+      <c r="G94" s="25">
+        <v>0</v>
+      </c>
+      <c r="H94" s="25">
+        <v>0</v>
+      </c>
+      <c r="I94" s="25">
+        <v>109</v>
+      </c>
+      <c r="J94" s="25">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="95" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A95" s="29">
+        <v>43995</v>
+      </c>
+      <c r="B95" s="30">
+        <v>87386</v>
+      </c>
+      <c r="C95" s="31">
+        <v>291</v>
+      </c>
+      <c r="D95" s="31">
+        <v>1495</v>
+      </c>
+      <c r="E95" s="31">
+        <v>3</v>
+      </c>
+      <c r="F95" s="31">
+        <v>6</v>
+      </c>
+      <c r="G95" s="31">
+        <v>0</v>
+      </c>
+      <c r="H95" s="31">
+        <v>0</v>
+      </c>
+      <c r="I95" s="31">
+        <v>109</v>
+      </c>
+      <c r="J95" s="31">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="96" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A96" s="23">
+        <v>43996</v>
+      </c>
+      <c r="B96" s="24">
+        <v>87598</v>
+      </c>
+      <c r="C96" s="25">
+        <v>212</v>
+      </c>
+      <c r="D96" s="25">
+        <v>1496</v>
+      </c>
+      <c r="E96" s="25">
+        <v>1</v>
+      </c>
+      <c r="F96" s="25">
+        <v>7</v>
+      </c>
+      <c r="G96" s="25">
+        <v>1</v>
+      </c>
+      <c r="H96" s="25">
+        <v>0</v>
+      </c>
+      <c r="I96" s="25">
+        <v>109</v>
+      </c>
+      <c r="J96" s="25">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="97" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A97" s="20">
+        <v>43997</v>
+      </c>
+      <c r="B97" s="21">
+        <v>88165</v>
+      </c>
+      <c r="C97" s="22">
+        <v>567</v>
+      </c>
+      <c r="D97" s="22">
+        <v>1499</v>
+      </c>
+      <c r="E97" s="22">
+        <v>3</v>
+      </c>
+      <c r="F97" s="22">
+        <v>7</v>
+      </c>
+      <c r="G97" s="22">
+        <v>1</v>
+      </c>
+      <c r="H97" s="22">
+        <v>0</v>
+      </c>
+      <c r="I97" s="22">
+        <v>109</v>
+      </c>
+      <c r="J97" s="22">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="98" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A98" s="20">
+        <v>43998</v>
+      </c>
+      <c r="B98" s="21">
+        <v>89151</v>
+      </c>
+      <c r="C98" s="22">
+        <v>986</v>
+      </c>
+      <c r="D98" s="22">
+        <v>1503</v>
+      </c>
+      <c r="E98" s="22">
+        <v>4</v>
+      </c>
+      <c r="F98" s="22">
+        <v>7</v>
+      </c>
+      <c r="G98" s="22">
+        <v>1</v>
+      </c>
+      <c r="H98" s="22">
+        <v>0</v>
+      </c>
+      <c r="I98" s="22">
+        <v>109</v>
+      </c>
+      <c r="J98" s="22">
+        <v>0</v>
+      </c>
+    </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>

</xml_diff>

<commit_message>
Data updated by GitHub Bot (2020-06-17 20)
</commit_message>
<xml_diff>
--- a/output/snapshot/fdcf2531-4c3e-5c02-b63c-ee160ead6dea.xlsx
+++ b/output/snapshot/fdcf2531-4c3e-5c02-b63c-ee160ead6dea.xlsx
@@ -1,16 +1,15 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="21929"/>
-  <workbookPr/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
+  <fileVersion appName="xl" lastEdited="6" lowestEdited="6" rupBuild="14420"/>
+  <workbookPr defaultThemeVersion="164011"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="I:\AKTUALNI PODATKI - KORONA\Za objavo na GOV.SI\ang\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{1E6DD62F-2BE2-47DC-A7ED-9B57C1589256}" xr6:coauthVersionLast="44" xr6:coauthVersionMax="44" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="2295" yWindow="2295" windowWidth="21600" windowHeight="11205"/>
   </bookViews>
   <sheets>
     <sheet name="Covid-19 podatki" sheetId="1" r:id="rId1"/>
@@ -60,11 +59,11 @@
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" mc:Ignorable="x14ac x16r2">
   <numFmts count="1">
     <numFmt numFmtId="164" formatCode="d/\ m/\ yyyy;@"/>
   </numFmts>
-  <fonts count="4" x14ac:knownFonts="1">
+  <fonts count="5" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -93,6 +92,13 @@
       <name val="Calibri Light"/>
       <scheme val="major"/>
     </font>
+    <font>
+      <sz val="10"/>
+      <color theme="1"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
   </fonts>
   <fills count="3">
     <fill>
@@ -108,7 +114,7 @@
       </patternFill>
     </fill>
   </fills>
-  <borders count="2">
+  <borders count="3">
     <border>
       <left/>
       <right/>
@@ -129,11 +135,26 @@
       <bottom/>
       <diagonal/>
     </border>
+    <border>
+      <left style="thin">
+        <color theme="4"/>
+      </left>
+      <right style="thin">
+        <color theme="4"/>
+      </right>
+      <top style="thin">
+        <color theme="4"/>
+      </top>
+      <bottom style="thin">
+        <color theme="4"/>
+      </bottom>
+      <diagonal/>
+    </border>
   </borders>
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="26">
+  <cellXfs count="32">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="49" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyAlignment="1" applyProtection="1">
       <alignment horizontal="left" vertical="top"/>
@@ -208,6 +229,24 @@
       <alignment horizontal="right"/>
     </xf>
     <xf numFmtId="0" fontId="3" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="right"/>
+    </xf>
+    <xf numFmtId="164" fontId="4" fillId="2" borderId="2" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="right" vertical="top"/>
+    </xf>
+    <xf numFmtId="3" fontId="4" fillId="2" borderId="2" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="right"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="2" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="right"/>
+    </xf>
+    <xf numFmtId="164" fontId="3" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="right" vertical="top"/>
+    </xf>
+    <xf numFmtId="3" fontId="3" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="right"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="right"/>
     </xf>
   </cellXfs>
@@ -399,8 +438,8 @@
 </file>
 
 <file path=xl/tables/table1.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="1" xr:uid="{00000000-000C-0000-FFFF-FFFF00000000}" name="Tabela1" displayName="Tabela1" ref="A1:J75" totalsRowShown="0" headerRowDxfId="11" dataDxfId="10">
-  <autoFilter ref="A1:J75" xr:uid="{00000000-0009-0000-0100-000001000000}">
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="1" name="Tabela1" displayName="Tabela1" ref="A1:J98" totalsRowShown="0" headerRowDxfId="11" dataDxfId="10">
+  <autoFilter ref="A1:J98">
     <filterColumn colId="0" hiddenButton="1"/>
     <filterColumn colId="1" hiddenButton="1"/>
     <filterColumn colId="2" hiddenButton="1"/>
@@ -413,16 +452,16 @@
     <filterColumn colId="9" hiddenButton="1"/>
   </autoFilter>
   <tableColumns count="10">
-    <tableColumn id="1" xr3:uid="{00000000-0010-0000-0000-000001000000}" name="Date" dataDxfId="9"/>
-    <tableColumn id="2" xr3:uid="{00000000-0010-0000-0000-000002000000}" name="Tested (all)" dataDxfId="8"/>
-    <tableColumn id="3" xr3:uid="{00000000-0010-0000-0000-000003000000}" name="Tested (daily)" dataDxfId="7"/>
-    <tableColumn id="4" xr3:uid="{00000000-0010-0000-0000-000004000000}" name="Positive (all)" dataDxfId="6"/>
-    <tableColumn id="5" xr3:uid="{00000000-0010-0000-0000-000005000000}" name="Positive (daily)" dataDxfId="5"/>
-    <tableColumn id="6" xr3:uid="{00000000-0010-0000-0000-000006000000}" name="All hospitalized on certain day" dataDxfId="4"/>
-    <tableColumn id="7" xr3:uid="{00000000-0010-0000-0000-000007000000}" name="All persons in intensive care on certain day" dataDxfId="3"/>
-    <tableColumn id="10" xr3:uid="{00000000-0010-0000-0000-00000A000000}" name="Discharged" dataDxfId="2"/>
-    <tableColumn id="8" xr3:uid="{00000000-0010-0000-0000-000008000000}" name="Deaths (all)" dataDxfId="1"/>
-    <tableColumn id="9" xr3:uid="{00000000-0010-0000-0000-000009000000}" name="Deaths (daily)" dataDxfId="0"/>
+    <tableColumn id="1" name="Date" dataDxfId="9"/>
+    <tableColumn id="2" name="Tested (all)" dataDxfId="8"/>
+    <tableColumn id="3" name="Tested (daily)" dataDxfId="7"/>
+    <tableColumn id="4" name="Positive (all)" dataDxfId="6"/>
+    <tableColumn id="5" name="Positive (daily)" dataDxfId="5"/>
+    <tableColumn id="6" name="All hospitalized on certain day" dataDxfId="4"/>
+    <tableColumn id="7" name="All persons in intensive care on certain day" dataDxfId="3"/>
+    <tableColumn id="10" name="Discharged" dataDxfId="2"/>
+    <tableColumn id="8" name="Deaths (all)" dataDxfId="1"/>
+    <tableColumn id="9" name="Deaths (daily)" dataDxfId="0"/>
   </tableColumns>
   <tableStyleInfo name="TableStyleLight16" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
   <extLst>
@@ -695,11 +734,11 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:J75"/>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <dimension ref="A1:J98"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A40" zoomScale="89" zoomScaleNormal="89" workbookViewId="0">
-      <selection activeCell="J74" sqref="J74"/>
+    <sheetView tabSelected="1" topLeftCell="A77" zoomScale="89" zoomScaleNormal="89" workbookViewId="0">
+      <selection activeCell="A98" sqref="A98:J98"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -3117,6 +3156,742 @@
         <v>0</v>
       </c>
     </row>
+    <row r="76" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A76" s="20">
+        <v>43976</v>
+      </c>
+      <c r="B76" s="21">
+        <v>75770</v>
+      </c>
+      <c r="C76" s="22">
+        <v>754</v>
+      </c>
+      <c r="D76" s="22">
+        <v>1469</v>
+      </c>
+      <c r="E76" s="22">
+        <v>0</v>
+      </c>
+      <c r="F76" s="22">
+        <v>9</v>
+      </c>
+      <c r="G76" s="22">
+        <v>2</v>
+      </c>
+      <c r="H76" s="22">
+        <v>6</v>
+      </c>
+      <c r="I76" s="22">
+        <v>108</v>
+      </c>
+      <c r="J76" s="22">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="77" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A77" s="20">
+        <v>43977</v>
+      </c>
+      <c r="B77" s="21">
+        <v>76579</v>
+      </c>
+      <c r="C77" s="22">
+        <v>809</v>
+      </c>
+      <c r="D77" s="22">
+        <v>1471</v>
+      </c>
+      <c r="E77" s="22">
+        <v>2</v>
+      </c>
+      <c r="F77" s="22">
+        <v>8</v>
+      </c>
+      <c r="G77" s="22">
+        <v>2</v>
+      </c>
+      <c r="H77" s="22">
+        <v>2</v>
+      </c>
+      <c r="I77" s="22">
+        <v>108</v>
+      </c>
+      <c r="J77" s="22">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="78" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A78" s="20">
+        <v>43978</v>
+      </c>
+      <c r="B78" s="21">
+        <v>77210</v>
+      </c>
+      <c r="C78" s="22">
+        <v>631</v>
+      </c>
+      <c r="D78" s="22">
+        <v>1473</v>
+      </c>
+      <c r="E78" s="22">
+        <v>2</v>
+      </c>
+      <c r="F78" s="22">
+        <v>7</v>
+      </c>
+      <c r="G78" s="22">
+        <v>2</v>
+      </c>
+      <c r="H78" s="22">
+        <v>1</v>
+      </c>
+      <c r="I78" s="22">
+        <v>108</v>
+      </c>
+      <c r="J78" s="22">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="79" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A79" s="20">
+        <v>43979</v>
+      </c>
+      <c r="B79" s="21">
+        <v>77916</v>
+      </c>
+      <c r="C79" s="22">
+        <v>706</v>
+      </c>
+      <c r="D79" s="22">
+        <v>1473</v>
+      </c>
+      <c r="E79" s="22">
+        <v>0</v>
+      </c>
+      <c r="F79" s="22">
+        <v>7</v>
+      </c>
+      <c r="G79" s="22">
+        <v>2</v>
+      </c>
+      <c r="H79" s="22">
+        <v>0</v>
+      </c>
+      <c r="I79" s="22">
+        <v>108</v>
+      </c>
+      <c r="J79" s="22">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="80" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A80" s="20">
+        <v>43980</v>
+      </c>
+      <c r="B80" s="21">
+        <v>78529</v>
+      </c>
+      <c r="C80" s="22">
+        <v>613</v>
+      </c>
+      <c r="D80" s="22">
+        <v>1473</v>
+      </c>
+      <c r="E80" s="22">
+        <v>0</v>
+      </c>
+      <c r="F80" s="22">
+        <v>7</v>
+      </c>
+      <c r="G80" s="22">
+        <v>2</v>
+      </c>
+      <c r="H80" s="22">
+        <v>0</v>
+      </c>
+      <c r="I80" s="22">
+        <v>108</v>
+      </c>
+      <c r="J80" s="22">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="81" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A81" s="20">
+        <v>43981</v>
+      </c>
+      <c r="B81" s="22">
+        <v>78793</v>
+      </c>
+      <c r="C81" s="22">
+        <v>264</v>
+      </c>
+      <c r="D81" s="22">
+        <v>1473</v>
+      </c>
+      <c r="E81" s="22">
+        <v>0</v>
+      </c>
+      <c r="F81" s="22">
+        <v>6</v>
+      </c>
+      <c r="G81" s="22">
+        <v>2</v>
+      </c>
+      <c r="H81" s="22">
+        <v>1</v>
+      </c>
+      <c r="I81" s="22">
+        <v>108</v>
+      </c>
+      <c r="J81" s="22">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="82" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A82" s="20">
+        <v>43982</v>
+      </c>
+      <c r="B82" s="21">
+        <v>79039</v>
+      </c>
+      <c r="C82" s="22">
+        <v>246</v>
+      </c>
+      <c r="D82" s="22">
+        <v>1473</v>
+      </c>
+      <c r="E82" s="22">
+        <v>0</v>
+      </c>
+      <c r="F82" s="22">
+        <v>5</v>
+      </c>
+      <c r="G82" s="22">
+        <v>1</v>
+      </c>
+      <c r="H82" s="22">
+        <v>0</v>
+      </c>
+      <c r="I82" s="22">
+        <v>109</v>
+      </c>
+      <c r="J82" s="22">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="83" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A83" s="20">
+        <v>43983</v>
+      </c>
+      <c r="B83" s="21">
+        <v>79698</v>
+      </c>
+      <c r="C83" s="22">
+        <v>659</v>
+      </c>
+      <c r="D83" s="22">
+        <v>1475</v>
+      </c>
+      <c r="E83" s="22">
+        <v>2</v>
+      </c>
+      <c r="F83" s="22">
+        <v>5</v>
+      </c>
+      <c r="G83" s="22">
+        <v>1</v>
+      </c>
+      <c r="H83" s="22">
+        <v>0</v>
+      </c>
+      <c r="I83" s="22">
+        <v>109</v>
+      </c>
+      <c r="J83" s="22">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="84" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A84" s="20">
+        <v>43984</v>
+      </c>
+      <c r="B84" s="21">
+        <v>80505</v>
+      </c>
+      <c r="C84" s="22">
+        <v>807</v>
+      </c>
+      <c r="D84" s="22">
+        <v>1477</v>
+      </c>
+      <c r="E84" s="22">
+        <v>2</v>
+      </c>
+      <c r="F84" s="22">
+        <v>5</v>
+      </c>
+      <c r="G84" s="22">
+        <v>0</v>
+      </c>
+      <c r="H84" s="22">
+        <v>0</v>
+      </c>
+      <c r="I84" s="22">
+        <v>109</v>
+      </c>
+      <c r="J84" s="22">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="85" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A85" s="20">
+        <v>43985</v>
+      </c>
+      <c r="B85" s="21">
+        <v>81333</v>
+      </c>
+      <c r="C85" s="22">
+        <v>828</v>
+      </c>
+      <c r="D85" s="22">
+        <v>1477</v>
+      </c>
+      <c r="E85" s="22">
+        <v>0</v>
+      </c>
+      <c r="F85" s="22">
+        <v>5</v>
+      </c>
+      <c r="G85" s="22">
+        <v>0</v>
+      </c>
+      <c r="H85" s="22">
+        <v>0</v>
+      </c>
+      <c r="I85" s="22">
+        <v>109</v>
+      </c>
+      <c r="J85" s="22">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="86" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A86" s="26">
+        <v>43986</v>
+      </c>
+      <c r="B86" s="27">
+        <v>82161</v>
+      </c>
+      <c r="C86" s="28">
+        <v>828</v>
+      </c>
+      <c r="D86" s="28">
+        <v>1479</v>
+      </c>
+      <c r="E86" s="28">
+        <v>2</v>
+      </c>
+      <c r="F86" s="28">
+        <v>6</v>
+      </c>
+      <c r="G86" s="28">
+        <v>0</v>
+      </c>
+      <c r="H86" s="28">
+        <v>0</v>
+      </c>
+      <c r="I86" s="28">
+        <v>109</v>
+      </c>
+      <c r="J86" s="28">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="87" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A87" s="29">
+        <v>43987</v>
+      </c>
+      <c r="B87" s="30">
+        <v>82876</v>
+      </c>
+      <c r="C87" s="31">
+        <v>715</v>
+      </c>
+      <c r="D87" s="31">
+        <v>1484</v>
+      </c>
+      <c r="E87" s="31">
+        <v>5</v>
+      </c>
+      <c r="F87" s="31">
+        <v>6</v>
+      </c>
+      <c r="G87" s="31">
+        <v>0</v>
+      </c>
+      <c r="H87" s="31">
+        <v>0</v>
+      </c>
+      <c r="I87" s="31">
+        <v>109</v>
+      </c>
+      <c r="J87" s="31">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="88" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A88" s="23">
+        <v>43988</v>
+      </c>
+      <c r="B88" s="24">
+        <v>83105</v>
+      </c>
+      <c r="C88" s="25">
+        <v>229</v>
+      </c>
+      <c r="D88" s="25">
+        <v>1485</v>
+      </c>
+      <c r="E88" s="25">
+        <v>1</v>
+      </c>
+      <c r="F88" s="25">
+        <v>5</v>
+      </c>
+      <c r="G88" s="25">
+        <v>0</v>
+      </c>
+      <c r="H88" s="25">
+        <v>1</v>
+      </c>
+      <c r="I88" s="25">
+        <v>109</v>
+      </c>
+      <c r="J88" s="25">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="89" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A89" s="29">
+        <v>43989</v>
+      </c>
+      <c r="B89" s="30">
+        <v>83316</v>
+      </c>
+      <c r="C89" s="31">
+        <v>211</v>
+      </c>
+      <c r="D89" s="31">
+        <v>1485</v>
+      </c>
+      <c r="E89" s="31">
+        <v>0</v>
+      </c>
+      <c r="F89" s="31">
+        <v>5</v>
+      </c>
+      <c r="G89" s="31">
+        <v>0</v>
+      </c>
+      <c r="H89" s="31">
+        <v>0</v>
+      </c>
+      <c r="I89" s="31">
+        <v>109</v>
+      </c>
+      <c r="J89" s="31">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="90" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A90" s="20">
+        <v>43990</v>
+      </c>
+      <c r="B90" s="21">
+        <v>84130</v>
+      </c>
+      <c r="C90" s="22">
+        <v>814</v>
+      </c>
+      <c r="D90" s="22">
+        <v>1486</v>
+      </c>
+      <c r="E90" s="22">
+        <v>1</v>
+      </c>
+      <c r="F90" s="22">
+        <v>6</v>
+      </c>
+      <c r="G90" s="22">
+        <v>0</v>
+      </c>
+      <c r="H90" s="22">
+        <v>0</v>
+      </c>
+      <c r="I90" s="22">
+        <v>109</v>
+      </c>
+      <c r="J90" s="22">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="91" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A91" s="20">
+        <v>43991</v>
+      </c>
+      <c r="B91" s="21">
+        <v>84868</v>
+      </c>
+      <c r="C91" s="22">
+        <v>738</v>
+      </c>
+      <c r="D91" s="22">
+        <v>1488</v>
+      </c>
+      <c r="E91" s="22">
+        <v>2</v>
+      </c>
+      <c r="F91" s="22">
+        <v>6</v>
+      </c>
+      <c r="G91" s="22">
+        <v>0</v>
+      </c>
+      <c r="H91" s="22">
+        <v>0</v>
+      </c>
+      <c r="I91" s="22">
+        <v>109</v>
+      </c>
+      <c r="J91" s="22">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="92" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A92" s="23">
+        <v>43992</v>
+      </c>
+      <c r="B92" s="24">
+        <v>85626</v>
+      </c>
+      <c r="C92" s="25">
+        <v>758</v>
+      </c>
+      <c r="D92" s="25">
+        <v>1488</v>
+      </c>
+      <c r="E92" s="25">
+        <v>0</v>
+      </c>
+      <c r="F92" s="25">
+        <v>6</v>
+      </c>
+      <c r="G92" s="25">
+        <v>0</v>
+      </c>
+      <c r="H92" s="25">
+        <v>0</v>
+      </c>
+      <c r="I92" s="25">
+        <v>109</v>
+      </c>
+      <c r="J92" s="25">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="93" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A93" s="29">
+        <v>43993</v>
+      </c>
+      <c r="B93" s="30">
+        <v>86328</v>
+      </c>
+      <c r="C93" s="31">
+        <v>702</v>
+      </c>
+      <c r="D93" s="31">
+        <v>1490</v>
+      </c>
+      <c r="E93" s="31">
+        <v>2</v>
+      </c>
+      <c r="F93" s="31">
+        <v>6</v>
+      </c>
+      <c r="G93" s="31">
+        <v>0</v>
+      </c>
+      <c r="H93" s="31">
+        <v>0</v>
+      </c>
+      <c r="I93" s="31">
+        <v>109</v>
+      </c>
+      <c r="J93" s="31">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="94" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A94" s="23">
+        <v>43994</v>
+      </c>
+      <c r="B94" s="24">
+        <v>87095</v>
+      </c>
+      <c r="C94" s="25">
+        <v>767</v>
+      </c>
+      <c r="D94" s="25">
+        <v>1492</v>
+      </c>
+      <c r="E94" s="25">
+        <v>2</v>
+      </c>
+      <c r="F94" s="25">
+        <v>6</v>
+      </c>
+      <c r="G94" s="25">
+        <v>0</v>
+      </c>
+      <c r="H94" s="25">
+        <v>0</v>
+      </c>
+      <c r="I94" s="25">
+        <v>109</v>
+      </c>
+      <c r="J94" s="25">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="95" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A95" s="29">
+        <v>43995</v>
+      </c>
+      <c r="B95" s="30">
+        <v>87386</v>
+      </c>
+      <c r="C95" s="31">
+        <v>291</v>
+      </c>
+      <c r="D95" s="31">
+        <v>1495</v>
+      </c>
+      <c r="E95" s="31">
+        <v>3</v>
+      </c>
+      <c r="F95" s="31">
+        <v>6</v>
+      </c>
+      <c r="G95" s="31">
+        <v>0</v>
+      </c>
+      <c r="H95" s="31">
+        <v>0</v>
+      </c>
+      <c r="I95" s="31">
+        <v>109</v>
+      </c>
+      <c r="J95" s="31">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="96" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A96" s="23">
+        <v>43996</v>
+      </c>
+      <c r="B96" s="24">
+        <v>87598</v>
+      </c>
+      <c r="C96" s="25">
+        <v>212</v>
+      </c>
+      <c r="D96" s="25">
+        <v>1496</v>
+      </c>
+      <c r="E96" s="25">
+        <v>1</v>
+      </c>
+      <c r="F96" s="25">
+        <v>7</v>
+      </c>
+      <c r="G96" s="25">
+        <v>1</v>
+      </c>
+      <c r="H96" s="25">
+        <v>0</v>
+      </c>
+      <c r="I96" s="25">
+        <v>109</v>
+      </c>
+      <c r="J96" s="25">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="97" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A97" s="20">
+        <v>43997</v>
+      </c>
+      <c r="B97" s="21">
+        <v>88165</v>
+      </c>
+      <c r="C97" s="22">
+        <v>567</v>
+      </c>
+      <c r="D97" s="22">
+        <v>1499</v>
+      </c>
+      <c r="E97" s="22">
+        <v>3</v>
+      </c>
+      <c r="F97" s="22">
+        <v>7</v>
+      </c>
+      <c r="G97" s="22">
+        <v>1</v>
+      </c>
+      <c r="H97" s="22">
+        <v>0</v>
+      </c>
+      <c r="I97" s="22">
+        <v>109</v>
+      </c>
+      <c r="J97" s="22">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="98" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A98" s="20">
+        <v>43998</v>
+      </c>
+      <c r="B98" s="21">
+        <v>89151</v>
+      </c>
+      <c r="C98" s="22">
+        <v>986</v>
+      </c>
+      <c r="D98" s="22">
+        <v>1503</v>
+      </c>
+      <c r="E98" s="22">
+        <v>4</v>
+      </c>
+      <c r="F98" s="22">
+        <v>7</v>
+      </c>
+      <c r="G98" s="22">
+        <v>1</v>
+      </c>
+      <c r="H98" s="22">
+        <v>0</v>
+      </c>
+      <c r="I98" s="22">
+        <v>109</v>
+      </c>
+      <c r="J98" s="22">
+        <v>0</v>
+      </c>
+    </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>

</xml_diff>

<commit_message>
Data updated by GitHub Bot (2020-06-18 12)
</commit_message>
<xml_diff>
--- a/output/snapshot/fdcf2531-4c3e-5c02-b63c-ee160ead6dea.xlsx
+++ b/output/snapshot/fdcf2531-4c3e-5c02-b63c-ee160ead6dea.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="I:\AKTUALNI PODATKI - KORONA\Za objavo na GOV.SI\ang\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{1E6DD62F-2BE2-47DC-A7ED-9B57C1589256}" xr6:coauthVersionLast="44" xr6:coauthVersionMax="44" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{1F3925C0-727D-4AE3-82D9-F83297781159}" xr6:coauthVersionLast="44" xr6:coauthVersionMax="44" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -64,7 +64,7 @@
   <numFmts count="1">
     <numFmt numFmtId="164" formatCode="d/\ m/\ yyyy;@"/>
   </numFmts>
-  <fonts count="4" x14ac:knownFonts="1">
+  <fonts count="5" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -93,6 +93,13 @@
       <name val="Calibri Light"/>
       <scheme val="major"/>
     </font>
+    <font>
+      <sz val="10"/>
+      <color theme="1"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
   </fonts>
   <fills count="3">
     <fill>
@@ -108,7 +115,7 @@
       </patternFill>
     </fill>
   </fills>
-  <borders count="2">
+  <borders count="3">
     <border>
       <left/>
       <right/>
@@ -129,11 +136,26 @@
       <bottom/>
       <diagonal/>
     </border>
+    <border>
+      <left style="thin">
+        <color theme="4"/>
+      </left>
+      <right style="thin">
+        <color theme="4"/>
+      </right>
+      <top style="thin">
+        <color theme="4"/>
+      </top>
+      <bottom style="thin">
+        <color theme="4"/>
+      </bottom>
+      <diagonal/>
+    </border>
   </borders>
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="26">
+  <cellXfs count="32">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="49" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyAlignment="1" applyProtection="1">
       <alignment horizontal="left" vertical="top"/>
@@ -208,6 +230,24 @@
       <alignment horizontal="right"/>
     </xf>
     <xf numFmtId="0" fontId="3" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="right"/>
+    </xf>
+    <xf numFmtId="164" fontId="4" fillId="2" borderId="2" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="right" vertical="top"/>
+    </xf>
+    <xf numFmtId="3" fontId="4" fillId="2" borderId="2" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="right"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="2" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="right"/>
+    </xf>
+    <xf numFmtId="164" fontId="3" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="right" vertical="top"/>
+    </xf>
+    <xf numFmtId="3" fontId="3" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="right"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="right"/>
     </xf>
   </cellXfs>
@@ -399,8 +439,8 @@
 </file>
 
 <file path=xl/tables/table1.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="1" xr:uid="{00000000-000C-0000-FFFF-FFFF00000000}" name="Tabela1" displayName="Tabela1" ref="A1:J75" totalsRowShown="0" headerRowDxfId="11" dataDxfId="10">
-  <autoFilter ref="A1:J75" xr:uid="{00000000-0009-0000-0100-000001000000}">
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="1" xr:uid="{00000000-000C-0000-FFFF-FFFF00000000}" name="Tabela1" displayName="Tabela1" ref="A1:J99" totalsRowShown="0" headerRowDxfId="11" dataDxfId="10">
+  <autoFilter ref="A1:J99" xr:uid="{00000000-0009-0000-0100-000001000000}">
     <filterColumn colId="0" hiddenButton="1"/>
     <filterColumn colId="1" hiddenButton="1"/>
     <filterColumn colId="2" hiddenButton="1"/>
@@ -696,10 +736,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:J75"/>
+  <dimension ref="A1:J99"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A40" zoomScale="89" zoomScaleNormal="89" workbookViewId="0">
-      <selection activeCell="J74" sqref="J74"/>
+    <sheetView tabSelected="1" topLeftCell="A77" zoomScale="89" zoomScaleNormal="89" workbookViewId="0">
+      <selection activeCell="A99" sqref="A99:J99"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -3117,6 +3157,774 @@
         <v>0</v>
       </c>
     </row>
+    <row r="76" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A76" s="20">
+        <v>43976</v>
+      </c>
+      <c r="B76" s="21">
+        <v>75770</v>
+      </c>
+      <c r="C76" s="22">
+        <v>754</v>
+      </c>
+      <c r="D76" s="22">
+        <v>1469</v>
+      </c>
+      <c r="E76" s="22">
+        <v>0</v>
+      </c>
+      <c r="F76" s="22">
+        <v>9</v>
+      </c>
+      <c r="G76" s="22">
+        <v>2</v>
+      </c>
+      <c r="H76" s="22">
+        <v>6</v>
+      </c>
+      <c r="I76" s="22">
+        <v>108</v>
+      </c>
+      <c r="J76" s="22">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="77" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A77" s="20">
+        <v>43977</v>
+      </c>
+      <c r="B77" s="21">
+        <v>76579</v>
+      </c>
+      <c r="C77" s="22">
+        <v>809</v>
+      </c>
+      <c r="D77" s="22">
+        <v>1471</v>
+      </c>
+      <c r="E77" s="22">
+        <v>2</v>
+      </c>
+      <c r="F77" s="22">
+        <v>8</v>
+      </c>
+      <c r="G77" s="22">
+        <v>2</v>
+      </c>
+      <c r="H77" s="22">
+        <v>2</v>
+      </c>
+      <c r="I77" s="22">
+        <v>108</v>
+      </c>
+      <c r="J77" s="22">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="78" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A78" s="20">
+        <v>43978</v>
+      </c>
+      <c r="B78" s="21">
+        <v>77210</v>
+      </c>
+      <c r="C78" s="22">
+        <v>631</v>
+      </c>
+      <c r="D78" s="22">
+        <v>1473</v>
+      </c>
+      <c r="E78" s="22">
+        <v>2</v>
+      </c>
+      <c r="F78" s="22">
+        <v>7</v>
+      </c>
+      <c r="G78" s="22">
+        <v>2</v>
+      </c>
+      <c r="H78" s="22">
+        <v>1</v>
+      </c>
+      <c r="I78" s="22">
+        <v>108</v>
+      </c>
+      <c r="J78" s="22">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="79" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A79" s="20">
+        <v>43979</v>
+      </c>
+      <c r="B79" s="21">
+        <v>77916</v>
+      </c>
+      <c r="C79" s="22">
+        <v>706</v>
+      </c>
+      <c r="D79" s="22">
+        <v>1473</v>
+      </c>
+      <c r="E79" s="22">
+        <v>0</v>
+      </c>
+      <c r="F79" s="22">
+        <v>7</v>
+      </c>
+      <c r="G79" s="22">
+        <v>2</v>
+      </c>
+      <c r="H79" s="22">
+        <v>0</v>
+      </c>
+      <c r="I79" s="22">
+        <v>108</v>
+      </c>
+      <c r="J79" s="22">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="80" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A80" s="20">
+        <v>43980</v>
+      </c>
+      <c r="B80" s="21">
+        <v>78529</v>
+      </c>
+      <c r="C80" s="22">
+        <v>613</v>
+      </c>
+      <c r="D80" s="22">
+        <v>1473</v>
+      </c>
+      <c r="E80" s="22">
+        <v>0</v>
+      </c>
+      <c r="F80" s="22">
+        <v>7</v>
+      </c>
+      <c r="G80" s="22">
+        <v>2</v>
+      </c>
+      <c r="H80" s="22">
+        <v>0</v>
+      </c>
+      <c r="I80" s="22">
+        <v>108</v>
+      </c>
+      <c r="J80" s="22">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="81" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A81" s="20">
+        <v>43981</v>
+      </c>
+      <c r="B81" s="22">
+        <v>78793</v>
+      </c>
+      <c r="C81" s="22">
+        <v>264</v>
+      </c>
+      <c r="D81" s="22">
+        <v>1473</v>
+      </c>
+      <c r="E81" s="22">
+        <v>0</v>
+      </c>
+      <c r="F81" s="22">
+        <v>6</v>
+      </c>
+      <c r="G81" s="22">
+        <v>2</v>
+      </c>
+      <c r="H81" s="22">
+        <v>1</v>
+      </c>
+      <c r="I81" s="22">
+        <v>108</v>
+      </c>
+      <c r="J81" s="22">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="82" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A82" s="20">
+        <v>43982</v>
+      </c>
+      <c r="B82" s="21">
+        <v>79039</v>
+      </c>
+      <c r="C82" s="22">
+        <v>246</v>
+      </c>
+      <c r="D82" s="22">
+        <v>1473</v>
+      </c>
+      <c r="E82" s="22">
+        <v>0</v>
+      </c>
+      <c r="F82" s="22">
+        <v>5</v>
+      </c>
+      <c r="G82" s="22">
+        <v>1</v>
+      </c>
+      <c r="H82" s="22">
+        <v>0</v>
+      </c>
+      <c r="I82" s="22">
+        <v>109</v>
+      </c>
+      <c r="J82" s="22">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="83" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A83" s="20">
+        <v>43983</v>
+      </c>
+      <c r="B83" s="21">
+        <v>79698</v>
+      </c>
+      <c r="C83" s="22">
+        <v>659</v>
+      </c>
+      <c r="D83" s="22">
+        <v>1475</v>
+      </c>
+      <c r="E83" s="22">
+        <v>2</v>
+      </c>
+      <c r="F83" s="22">
+        <v>5</v>
+      </c>
+      <c r="G83" s="22">
+        <v>1</v>
+      </c>
+      <c r="H83" s="22">
+        <v>0</v>
+      </c>
+      <c r="I83" s="22">
+        <v>109</v>
+      </c>
+      <c r="J83" s="22">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="84" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A84" s="20">
+        <v>43984</v>
+      </c>
+      <c r="B84" s="21">
+        <v>80505</v>
+      </c>
+      <c r="C84" s="22">
+        <v>807</v>
+      </c>
+      <c r="D84" s="22">
+        <v>1477</v>
+      </c>
+      <c r="E84" s="22">
+        <v>2</v>
+      </c>
+      <c r="F84" s="22">
+        <v>5</v>
+      </c>
+      <c r="G84" s="22">
+        <v>0</v>
+      </c>
+      <c r="H84" s="22">
+        <v>0</v>
+      </c>
+      <c r="I84" s="22">
+        <v>109</v>
+      </c>
+      <c r="J84" s="22">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="85" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A85" s="20">
+        <v>43985</v>
+      </c>
+      <c r="B85" s="21">
+        <v>81333</v>
+      </c>
+      <c r="C85" s="22">
+        <v>828</v>
+      </c>
+      <c r="D85" s="22">
+        <v>1477</v>
+      </c>
+      <c r="E85" s="22">
+        <v>0</v>
+      </c>
+      <c r="F85" s="22">
+        <v>5</v>
+      </c>
+      <c r="G85" s="22">
+        <v>0</v>
+      </c>
+      <c r="H85" s="22">
+        <v>0</v>
+      </c>
+      <c r="I85" s="22">
+        <v>109</v>
+      </c>
+      <c r="J85" s="22">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="86" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A86" s="26">
+        <v>43986</v>
+      </c>
+      <c r="B86" s="27">
+        <v>82161</v>
+      </c>
+      <c r="C86" s="28">
+        <v>828</v>
+      </c>
+      <c r="D86" s="28">
+        <v>1479</v>
+      </c>
+      <c r="E86" s="28">
+        <v>2</v>
+      </c>
+      <c r="F86" s="28">
+        <v>6</v>
+      </c>
+      <c r="G86" s="28">
+        <v>0</v>
+      </c>
+      <c r="H86" s="28">
+        <v>0</v>
+      </c>
+      <c r="I86" s="28">
+        <v>109</v>
+      </c>
+      <c r="J86" s="28">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="87" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A87" s="29">
+        <v>43987</v>
+      </c>
+      <c r="B87" s="30">
+        <v>82876</v>
+      </c>
+      <c r="C87" s="31">
+        <v>715</v>
+      </c>
+      <c r="D87" s="31">
+        <v>1484</v>
+      </c>
+      <c r="E87" s="31">
+        <v>5</v>
+      </c>
+      <c r="F87" s="31">
+        <v>6</v>
+      </c>
+      <c r="G87" s="31">
+        <v>0</v>
+      </c>
+      <c r="H87" s="31">
+        <v>0</v>
+      </c>
+      <c r="I87" s="31">
+        <v>109</v>
+      </c>
+      <c r="J87" s="31">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="88" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A88" s="23">
+        <v>43988</v>
+      </c>
+      <c r="B88" s="24">
+        <v>83105</v>
+      </c>
+      <c r="C88" s="25">
+        <v>229</v>
+      </c>
+      <c r="D88" s="25">
+        <v>1485</v>
+      </c>
+      <c r="E88" s="25">
+        <v>1</v>
+      </c>
+      <c r="F88" s="25">
+        <v>5</v>
+      </c>
+      <c r="G88" s="25">
+        <v>0</v>
+      </c>
+      <c r="H88" s="25">
+        <v>1</v>
+      </c>
+      <c r="I88" s="25">
+        <v>109</v>
+      </c>
+      <c r="J88" s="25">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="89" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A89" s="29">
+        <v>43989</v>
+      </c>
+      <c r="B89" s="30">
+        <v>83316</v>
+      </c>
+      <c r="C89" s="31">
+        <v>211</v>
+      </c>
+      <c r="D89" s="31">
+        <v>1485</v>
+      </c>
+      <c r="E89" s="31">
+        <v>0</v>
+      </c>
+      <c r="F89" s="31">
+        <v>5</v>
+      </c>
+      <c r="G89" s="31">
+        <v>0</v>
+      </c>
+      <c r="H89" s="31">
+        <v>0</v>
+      </c>
+      <c r="I89" s="31">
+        <v>109</v>
+      </c>
+      <c r="J89" s="31">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="90" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A90" s="20">
+        <v>43990</v>
+      </c>
+      <c r="B90" s="21">
+        <v>84130</v>
+      </c>
+      <c r="C90" s="22">
+        <v>814</v>
+      </c>
+      <c r="D90" s="22">
+        <v>1486</v>
+      </c>
+      <c r="E90" s="22">
+        <v>1</v>
+      </c>
+      <c r="F90" s="22">
+        <v>6</v>
+      </c>
+      <c r="G90" s="22">
+        <v>0</v>
+      </c>
+      <c r="H90" s="22">
+        <v>0</v>
+      </c>
+      <c r="I90" s="22">
+        <v>109</v>
+      </c>
+      <c r="J90" s="22">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="91" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A91" s="20">
+        <v>43991</v>
+      </c>
+      <c r="B91" s="21">
+        <v>84868</v>
+      </c>
+      <c r="C91" s="22">
+        <v>738</v>
+      </c>
+      <c r="D91" s="22">
+        <v>1488</v>
+      </c>
+      <c r="E91" s="22">
+        <v>2</v>
+      </c>
+      <c r="F91" s="22">
+        <v>6</v>
+      </c>
+      <c r="G91" s="22">
+        <v>0</v>
+      </c>
+      <c r="H91" s="22">
+        <v>0</v>
+      </c>
+      <c r="I91" s="22">
+        <v>109</v>
+      </c>
+      <c r="J91" s="22">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="92" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A92" s="23">
+        <v>43992</v>
+      </c>
+      <c r="B92" s="24">
+        <v>85626</v>
+      </c>
+      <c r="C92" s="25">
+        <v>758</v>
+      </c>
+      <c r="D92" s="25">
+        <v>1488</v>
+      </c>
+      <c r="E92" s="25">
+        <v>0</v>
+      </c>
+      <c r="F92" s="25">
+        <v>6</v>
+      </c>
+      <c r="G92" s="25">
+        <v>0</v>
+      </c>
+      <c r="H92" s="25">
+        <v>0</v>
+      </c>
+      <c r="I92" s="25">
+        <v>109</v>
+      </c>
+      <c r="J92" s="25">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="93" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A93" s="29">
+        <v>43993</v>
+      </c>
+      <c r="B93" s="30">
+        <v>86328</v>
+      </c>
+      <c r="C93" s="31">
+        <v>702</v>
+      </c>
+      <c r="D93" s="31">
+        <v>1490</v>
+      </c>
+      <c r="E93" s="31">
+        <v>2</v>
+      </c>
+      <c r="F93" s="31">
+        <v>6</v>
+      </c>
+      <c r="G93" s="31">
+        <v>0</v>
+      </c>
+      <c r="H93" s="31">
+        <v>0</v>
+      </c>
+      <c r="I93" s="31">
+        <v>109</v>
+      </c>
+      <c r="J93" s="31">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="94" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A94" s="23">
+        <v>43994</v>
+      </c>
+      <c r="B94" s="24">
+        <v>87095</v>
+      </c>
+      <c r="C94" s="25">
+        <v>767</v>
+      </c>
+      <c r="D94" s="25">
+        <v>1492</v>
+      </c>
+      <c r="E94" s="25">
+        <v>2</v>
+      </c>
+      <c r="F94" s="25">
+        <v>6</v>
+      </c>
+      <c r="G94" s="25">
+        <v>0</v>
+      </c>
+      <c r="H94" s="25">
+        <v>0</v>
+      </c>
+      <c r="I94" s="25">
+        <v>109</v>
+      </c>
+      <c r="J94" s="25">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="95" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A95" s="29">
+        <v>43995</v>
+      </c>
+      <c r="B95" s="30">
+        <v>87386</v>
+      </c>
+      <c r="C95" s="31">
+        <v>291</v>
+      </c>
+      <c r="D95" s="31">
+        <v>1495</v>
+      </c>
+      <c r="E95" s="31">
+        <v>3</v>
+      </c>
+      <c r="F95" s="31">
+        <v>6</v>
+      </c>
+      <c r="G95" s="31">
+        <v>0</v>
+      </c>
+      <c r="H95" s="31">
+        <v>0</v>
+      </c>
+      <c r="I95" s="31">
+        <v>109</v>
+      </c>
+      <c r="J95" s="31">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="96" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A96" s="23">
+        <v>43996</v>
+      </c>
+      <c r="B96" s="24">
+        <v>87598</v>
+      </c>
+      <c r="C96" s="25">
+        <v>212</v>
+      </c>
+      <c r="D96" s="25">
+        <v>1496</v>
+      </c>
+      <c r="E96" s="25">
+        <v>1</v>
+      </c>
+      <c r="F96" s="25">
+        <v>7</v>
+      </c>
+      <c r="G96" s="25">
+        <v>1</v>
+      </c>
+      <c r="H96" s="25">
+        <v>0</v>
+      </c>
+      <c r="I96" s="25">
+        <v>109</v>
+      </c>
+      <c r="J96" s="25">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="97" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A97" s="20">
+        <v>43997</v>
+      </c>
+      <c r="B97" s="21">
+        <v>88165</v>
+      </c>
+      <c r="C97" s="22">
+        <v>567</v>
+      </c>
+      <c r="D97" s="22">
+        <v>1499</v>
+      </c>
+      <c r="E97" s="22">
+        <v>3</v>
+      </c>
+      <c r="F97" s="22">
+        <v>7</v>
+      </c>
+      <c r="G97" s="22">
+        <v>1</v>
+      </c>
+      <c r="H97" s="22">
+        <v>0</v>
+      </c>
+      <c r="I97" s="22">
+        <v>109</v>
+      </c>
+      <c r="J97" s="22">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="98" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A98" s="20">
+        <v>43998</v>
+      </c>
+      <c r="B98" s="21">
+        <v>89151</v>
+      </c>
+      <c r="C98" s="22">
+        <v>986</v>
+      </c>
+      <c r="D98" s="22">
+        <v>1503</v>
+      </c>
+      <c r="E98" s="22">
+        <v>4</v>
+      </c>
+      <c r="F98" s="22">
+        <v>7</v>
+      </c>
+      <c r="G98" s="22">
+        <v>1</v>
+      </c>
+      <c r="H98" s="22">
+        <v>0</v>
+      </c>
+      <c r="I98" s="22">
+        <v>109</v>
+      </c>
+      <c r="J98" s="22">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="99" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A99" s="29">
+        <v>43999</v>
+      </c>
+      <c r="B99" s="30">
+        <v>90103</v>
+      </c>
+      <c r="C99" s="31">
+        <v>952</v>
+      </c>
+      <c r="D99" s="31">
+        <v>1511</v>
+      </c>
+      <c r="E99" s="31">
+        <v>8</v>
+      </c>
+      <c r="F99" s="31">
+        <v>6</v>
+      </c>
+      <c r="G99" s="31">
+        <v>1</v>
+      </c>
+      <c r="H99" s="31">
+        <v>1</v>
+      </c>
+      <c r="I99" s="31">
+        <v>109</v>
+      </c>
+      <c r="J99" s="31">
+        <v>0</v>
+      </c>
+    </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>

</xml_diff>

<commit_message>
Data updated by GitHub Bot (2020-06-18 20)
</commit_message>
<xml_diff>
--- a/output/snapshot/fdcf2531-4c3e-5c02-b63c-ee160ead6dea.xlsx
+++ b/output/snapshot/fdcf2531-4c3e-5c02-b63c-ee160ead6dea.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="I:\AKTUALNI PODATKI - KORONA\Za objavo na GOV.SI\ang\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{1E6DD62F-2BE2-47DC-A7ED-9B57C1589256}" xr6:coauthVersionLast="44" xr6:coauthVersionMax="44" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{1F3925C0-727D-4AE3-82D9-F83297781159}" xr6:coauthVersionLast="44" xr6:coauthVersionMax="44" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -64,7 +64,7 @@
   <numFmts count="1">
     <numFmt numFmtId="164" formatCode="d/\ m/\ yyyy;@"/>
   </numFmts>
-  <fonts count="4" x14ac:knownFonts="1">
+  <fonts count="5" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -93,6 +93,13 @@
       <name val="Calibri Light"/>
       <scheme val="major"/>
     </font>
+    <font>
+      <sz val="10"/>
+      <color theme="1"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
   </fonts>
   <fills count="3">
     <fill>
@@ -108,7 +115,7 @@
       </patternFill>
     </fill>
   </fills>
-  <borders count="2">
+  <borders count="3">
     <border>
       <left/>
       <right/>
@@ -129,11 +136,26 @@
       <bottom/>
       <diagonal/>
     </border>
+    <border>
+      <left style="thin">
+        <color theme="4"/>
+      </left>
+      <right style="thin">
+        <color theme="4"/>
+      </right>
+      <top style="thin">
+        <color theme="4"/>
+      </top>
+      <bottom style="thin">
+        <color theme="4"/>
+      </bottom>
+      <diagonal/>
+    </border>
   </borders>
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="26">
+  <cellXfs count="32">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="49" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyAlignment="1" applyProtection="1">
       <alignment horizontal="left" vertical="top"/>
@@ -208,6 +230,24 @@
       <alignment horizontal="right"/>
     </xf>
     <xf numFmtId="0" fontId="3" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="right"/>
+    </xf>
+    <xf numFmtId="164" fontId="4" fillId="2" borderId="2" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="right" vertical="top"/>
+    </xf>
+    <xf numFmtId="3" fontId="4" fillId="2" borderId="2" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="right"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="2" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="right"/>
+    </xf>
+    <xf numFmtId="164" fontId="3" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="right" vertical="top"/>
+    </xf>
+    <xf numFmtId="3" fontId="3" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="right"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="right"/>
     </xf>
   </cellXfs>
@@ -399,8 +439,8 @@
 </file>
 
 <file path=xl/tables/table1.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="1" xr:uid="{00000000-000C-0000-FFFF-FFFF00000000}" name="Tabela1" displayName="Tabela1" ref="A1:J75" totalsRowShown="0" headerRowDxfId="11" dataDxfId="10">
-  <autoFilter ref="A1:J75" xr:uid="{00000000-0009-0000-0100-000001000000}">
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="1" xr:uid="{00000000-000C-0000-FFFF-FFFF00000000}" name="Tabela1" displayName="Tabela1" ref="A1:J99" totalsRowShown="0" headerRowDxfId="11" dataDxfId="10">
+  <autoFilter ref="A1:J99" xr:uid="{00000000-0009-0000-0100-000001000000}">
     <filterColumn colId="0" hiddenButton="1"/>
     <filterColumn colId="1" hiddenButton="1"/>
     <filterColumn colId="2" hiddenButton="1"/>
@@ -696,10 +736,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:J75"/>
+  <dimension ref="A1:J99"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A40" zoomScale="89" zoomScaleNormal="89" workbookViewId="0">
-      <selection activeCell="J74" sqref="J74"/>
+    <sheetView tabSelected="1" topLeftCell="A77" zoomScale="89" zoomScaleNormal="89" workbookViewId="0">
+      <selection activeCell="A99" sqref="A99:J99"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -3117,6 +3157,774 @@
         <v>0</v>
       </c>
     </row>
+    <row r="76" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A76" s="20">
+        <v>43976</v>
+      </c>
+      <c r="B76" s="21">
+        <v>75770</v>
+      </c>
+      <c r="C76" s="22">
+        <v>754</v>
+      </c>
+      <c r="D76" s="22">
+        <v>1469</v>
+      </c>
+      <c r="E76" s="22">
+        <v>0</v>
+      </c>
+      <c r="F76" s="22">
+        <v>9</v>
+      </c>
+      <c r="G76" s="22">
+        <v>2</v>
+      </c>
+      <c r="H76" s="22">
+        <v>6</v>
+      </c>
+      <c r="I76" s="22">
+        <v>108</v>
+      </c>
+      <c r="J76" s="22">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="77" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A77" s="20">
+        <v>43977</v>
+      </c>
+      <c r="B77" s="21">
+        <v>76579</v>
+      </c>
+      <c r="C77" s="22">
+        <v>809</v>
+      </c>
+      <c r="D77" s="22">
+        <v>1471</v>
+      </c>
+      <c r="E77" s="22">
+        <v>2</v>
+      </c>
+      <c r="F77" s="22">
+        <v>8</v>
+      </c>
+      <c r="G77" s="22">
+        <v>2</v>
+      </c>
+      <c r="H77" s="22">
+        <v>2</v>
+      </c>
+      <c r="I77" s="22">
+        <v>108</v>
+      </c>
+      <c r="J77" s="22">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="78" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A78" s="20">
+        <v>43978</v>
+      </c>
+      <c r="B78" s="21">
+        <v>77210</v>
+      </c>
+      <c r="C78" s="22">
+        <v>631</v>
+      </c>
+      <c r="D78" s="22">
+        <v>1473</v>
+      </c>
+      <c r="E78" s="22">
+        <v>2</v>
+      </c>
+      <c r="F78" s="22">
+        <v>7</v>
+      </c>
+      <c r="G78" s="22">
+        <v>2</v>
+      </c>
+      <c r="H78" s="22">
+        <v>1</v>
+      </c>
+      <c r="I78" s="22">
+        <v>108</v>
+      </c>
+      <c r="J78" s="22">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="79" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A79" s="20">
+        <v>43979</v>
+      </c>
+      <c r="B79" s="21">
+        <v>77916</v>
+      </c>
+      <c r="C79" s="22">
+        <v>706</v>
+      </c>
+      <c r="D79" s="22">
+        <v>1473</v>
+      </c>
+      <c r="E79" s="22">
+        <v>0</v>
+      </c>
+      <c r="F79" s="22">
+        <v>7</v>
+      </c>
+      <c r="G79" s="22">
+        <v>2</v>
+      </c>
+      <c r="H79" s="22">
+        <v>0</v>
+      </c>
+      <c r="I79" s="22">
+        <v>108</v>
+      </c>
+      <c r="J79" s="22">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="80" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A80" s="20">
+        <v>43980</v>
+      </c>
+      <c r="B80" s="21">
+        <v>78529</v>
+      </c>
+      <c r="C80" s="22">
+        <v>613</v>
+      </c>
+      <c r="D80" s="22">
+        <v>1473</v>
+      </c>
+      <c r="E80" s="22">
+        <v>0</v>
+      </c>
+      <c r="F80" s="22">
+        <v>7</v>
+      </c>
+      <c r="G80" s="22">
+        <v>2</v>
+      </c>
+      <c r="H80" s="22">
+        <v>0</v>
+      </c>
+      <c r="I80" s="22">
+        <v>108</v>
+      </c>
+      <c r="J80" s="22">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="81" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A81" s="20">
+        <v>43981</v>
+      </c>
+      <c r="B81" s="22">
+        <v>78793</v>
+      </c>
+      <c r="C81" s="22">
+        <v>264</v>
+      </c>
+      <c r="D81" s="22">
+        <v>1473</v>
+      </c>
+      <c r="E81" s="22">
+        <v>0</v>
+      </c>
+      <c r="F81" s="22">
+        <v>6</v>
+      </c>
+      <c r="G81" s="22">
+        <v>2</v>
+      </c>
+      <c r="H81" s="22">
+        <v>1</v>
+      </c>
+      <c r="I81" s="22">
+        <v>108</v>
+      </c>
+      <c r="J81" s="22">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="82" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A82" s="20">
+        <v>43982</v>
+      </c>
+      <c r="B82" s="21">
+        <v>79039</v>
+      </c>
+      <c r="C82" s="22">
+        <v>246</v>
+      </c>
+      <c r="D82" s="22">
+        <v>1473</v>
+      </c>
+      <c r="E82" s="22">
+        <v>0</v>
+      </c>
+      <c r="F82" s="22">
+        <v>5</v>
+      </c>
+      <c r="G82" s="22">
+        <v>1</v>
+      </c>
+      <c r="H82" s="22">
+        <v>0</v>
+      </c>
+      <c r="I82" s="22">
+        <v>109</v>
+      </c>
+      <c r="J82" s="22">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="83" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A83" s="20">
+        <v>43983</v>
+      </c>
+      <c r="B83" s="21">
+        <v>79698</v>
+      </c>
+      <c r="C83" s="22">
+        <v>659</v>
+      </c>
+      <c r="D83" s="22">
+        <v>1475</v>
+      </c>
+      <c r="E83" s="22">
+        <v>2</v>
+      </c>
+      <c r="F83" s="22">
+        <v>5</v>
+      </c>
+      <c r="G83" s="22">
+        <v>1</v>
+      </c>
+      <c r="H83" s="22">
+        <v>0</v>
+      </c>
+      <c r="I83" s="22">
+        <v>109</v>
+      </c>
+      <c r="J83" s="22">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="84" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A84" s="20">
+        <v>43984</v>
+      </c>
+      <c r="B84" s="21">
+        <v>80505</v>
+      </c>
+      <c r="C84" s="22">
+        <v>807</v>
+      </c>
+      <c r="D84" s="22">
+        <v>1477</v>
+      </c>
+      <c r="E84" s="22">
+        <v>2</v>
+      </c>
+      <c r="F84" s="22">
+        <v>5</v>
+      </c>
+      <c r="G84" s="22">
+        <v>0</v>
+      </c>
+      <c r="H84" s="22">
+        <v>0</v>
+      </c>
+      <c r="I84" s="22">
+        <v>109</v>
+      </c>
+      <c r="J84" s="22">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="85" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A85" s="20">
+        <v>43985</v>
+      </c>
+      <c r="B85" s="21">
+        <v>81333</v>
+      </c>
+      <c r="C85" s="22">
+        <v>828</v>
+      </c>
+      <c r="D85" s="22">
+        <v>1477</v>
+      </c>
+      <c r="E85" s="22">
+        <v>0</v>
+      </c>
+      <c r="F85" s="22">
+        <v>5</v>
+      </c>
+      <c r="G85" s="22">
+        <v>0</v>
+      </c>
+      <c r="H85" s="22">
+        <v>0</v>
+      </c>
+      <c r="I85" s="22">
+        <v>109</v>
+      </c>
+      <c r="J85" s="22">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="86" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A86" s="26">
+        <v>43986</v>
+      </c>
+      <c r="B86" s="27">
+        <v>82161</v>
+      </c>
+      <c r="C86" s="28">
+        <v>828</v>
+      </c>
+      <c r="D86" s="28">
+        <v>1479</v>
+      </c>
+      <c r="E86" s="28">
+        <v>2</v>
+      </c>
+      <c r="F86" s="28">
+        <v>6</v>
+      </c>
+      <c r="G86" s="28">
+        <v>0</v>
+      </c>
+      <c r="H86" s="28">
+        <v>0</v>
+      </c>
+      <c r="I86" s="28">
+        <v>109</v>
+      </c>
+      <c r="J86" s="28">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="87" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A87" s="29">
+        <v>43987</v>
+      </c>
+      <c r="B87" s="30">
+        <v>82876</v>
+      </c>
+      <c r="C87" s="31">
+        <v>715</v>
+      </c>
+      <c r="D87" s="31">
+        <v>1484</v>
+      </c>
+      <c r="E87" s="31">
+        <v>5</v>
+      </c>
+      <c r="F87" s="31">
+        <v>6</v>
+      </c>
+      <c r="G87" s="31">
+        <v>0</v>
+      </c>
+      <c r="H87" s="31">
+        <v>0</v>
+      </c>
+      <c r="I87" s="31">
+        <v>109</v>
+      </c>
+      <c r="J87" s="31">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="88" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A88" s="23">
+        <v>43988</v>
+      </c>
+      <c r="B88" s="24">
+        <v>83105</v>
+      </c>
+      <c r="C88" s="25">
+        <v>229</v>
+      </c>
+      <c r="D88" s="25">
+        <v>1485</v>
+      </c>
+      <c r="E88" s="25">
+        <v>1</v>
+      </c>
+      <c r="F88" s="25">
+        <v>5</v>
+      </c>
+      <c r="G88" s="25">
+        <v>0</v>
+      </c>
+      <c r="H88" s="25">
+        <v>1</v>
+      </c>
+      <c r="I88" s="25">
+        <v>109</v>
+      </c>
+      <c r="J88" s="25">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="89" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A89" s="29">
+        <v>43989</v>
+      </c>
+      <c r="B89" s="30">
+        <v>83316</v>
+      </c>
+      <c r="C89" s="31">
+        <v>211</v>
+      </c>
+      <c r="D89" s="31">
+        <v>1485</v>
+      </c>
+      <c r="E89" s="31">
+        <v>0</v>
+      </c>
+      <c r="F89" s="31">
+        <v>5</v>
+      </c>
+      <c r="G89" s="31">
+        <v>0</v>
+      </c>
+      <c r="H89" s="31">
+        <v>0</v>
+      </c>
+      <c r="I89" s="31">
+        <v>109</v>
+      </c>
+      <c r="J89" s="31">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="90" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A90" s="20">
+        <v>43990</v>
+      </c>
+      <c r="B90" s="21">
+        <v>84130</v>
+      </c>
+      <c r="C90" s="22">
+        <v>814</v>
+      </c>
+      <c r="D90" s="22">
+        <v>1486</v>
+      </c>
+      <c r="E90" s="22">
+        <v>1</v>
+      </c>
+      <c r="F90" s="22">
+        <v>6</v>
+      </c>
+      <c r="G90" s="22">
+        <v>0</v>
+      </c>
+      <c r="H90" s="22">
+        <v>0</v>
+      </c>
+      <c r="I90" s="22">
+        <v>109</v>
+      </c>
+      <c r="J90" s="22">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="91" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A91" s="20">
+        <v>43991</v>
+      </c>
+      <c r="B91" s="21">
+        <v>84868</v>
+      </c>
+      <c r="C91" s="22">
+        <v>738</v>
+      </c>
+      <c r="D91" s="22">
+        <v>1488</v>
+      </c>
+      <c r="E91" s="22">
+        <v>2</v>
+      </c>
+      <c r="F91" s="22">
+        <v>6</v>
+      </c>
+      <c r="G91" s="22">
+        <v>0</v>
+      </c>
+      <c r="H91" s="22">
+        <v>0</v>
+      </c>
+      <c r="I91" s="22">
+        <v>109</v>
+      </c>
+      <c r="J91" s="22">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="92" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A92" s="23">
+        <v>43992</v>
+      </c>
+      <c r="B92" s="24">
+        <v>85626</v>
+      </c>
+      <c r="C92" s="25">
+        <v>758</v>
+      </c>
+      <c r="D92" s="25">
+        <v>1488</v>
+      </c>
+      <c r="E92" s="25">
+        <v>0</v>
+      </c>
+      <c r="F92" s="25">
+        <v>6</v>
+      </c>
+      <c r="G92" s="25">
+        <v>0</v>
+      </c>
+      <c r="H92" s="25">
+        <v>0</v>
+      </c>
+      <c r="I92" s="25">
+        <v>109</v>
+      </c>
+      <c r="J92" s="25">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="93" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A93" s="29">
+        <v>43993</v>
+      </c>
+      <c r="B93" s="30">
+        <v>86328</v>
+      </c>
+      <c r="C93" s="31">
+        <v>702</v>
+      </c>
+      <c r="D93" s="31">
+        <v>1490</v>
+      </c>
+      <c r="E93" s="31">
+        <v>2</v>
+      </c>
+      <c r="F93" s="31">
+        <v>6</v>
+      </c>
+      <c r="G93" s="31">
+        <v>0</v>
+      </c>
+      <c r="H93" s="31">
+        <v>0</v>
+      </c>
+      <c r="I93" s="31">
+        <v>109</v>
+      </c>
+      <c r="J93" s="31">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="94" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A94" s="23">
+        <v>43994</v>
+      </c>
+      <c r="B94" s="24">
+        <v>87095</v>
+      </c>
+      <c r="C94" s="25">
+        <v>767</v>
+      </c>
+      <c r="D94" s="25">
+        <v>1492</v>
+      </c>
+      <c r="E94" s="25">
+        <v>2</v>
+      </c>
+      <c r="F94" s="25">
+        <v>6</v>
+      </c>
+      <c r="G94" s="25">
+        <v>0</v>
+      </c>
+      <c r="H94" s="25">
+        <v>0</v>
+      </c>
+      <c r="I94" s="25">
+        <v>109</v>
+      </c>
+      <c r="J94" s="25">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="95" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A95" s="29">
+        <v>43995</v>
+      </c>
+      <c r="B95" s="30">
+        <v>87386</v>
+      </c>
+      <c r="C95" s="31">
+        <v>291</v>
+      </c>
+      <c r="D95" s="31">
+        <v>1495</v>
+      </c>
+      <c r="E95" s="31">
+        <v>3</v>
+      </c>
+      <c r="F95" s="31">
+        <v>6</v>
+      </c>
+      <c r="G95" s="31">
+        <v>0</v>
+      </c>
+      <c r="H95" s="31">
+        <v>0</v>
+      </c>
+      <c r="I95" s="31">
+        <v>109</v>
+      </c>
+      <c r="J95" s="31">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="96" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A96" s="23">
+        <v>43996</v>
+      </c>
+      <c r="B96" s="24">
+        <v>87598</v>
+      </c>
+      <c r="C96" s="25">
+        <v>212</v>
+      </c>
+      <c r="D96" s="25">
+        <v>1496</v>
+      </c>
+      <c r="E96" s="25">
+        <v>1</v>
+      </c>
+      <c r="F96" s="25">
+        <v>7</v>
+      </c>
+      <c r="G96" s="25">
+        <v>1</v>
+      </c>
+      <c r="H96" s="25">
+        <v>0</v>
+      </c>
+      <c r="I96" s="25">
+        <v>109</v>
+      </c>
+      <c r="J96" s="25">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="97" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A97" s="20">
+        <v>43997</v>
+      </c>
+      <c r="B97" s="21">
+        <v>88165</v>
+      </c>
+      <c r="C97" s="22">
+        <v>567</v>
+      </c>
+      <c r="D97" s="22">
+        <v>1499</v>
+      </c>
+      <c r="E97" s="22">
+        <v>3</v>
+      </c>
+      <c r="F97" s="22">
+        <v>7</v>
+      </c>
+      <c r="G97" s="22">
+        <v>1</v>
+      </c>
+      <c r="H97" s="22">
+        <v>0</v>
+      </c>
+      <c r="I97" s="22">
+        <v>109</v>
+      </c>
+      <c r="J97" s="22">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="98" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A98" s="20">
+        <v>43998</v>
+      </c>
+      <c r="B98" s="21">
+        <v>89151</v>
+      </c>
+      <c r="C98" s="22">
+        <v>986</v>
+      </c>
+      <c r="D98" s="22">
+        <v>1503</v>
+      </c>
+      <c r="E98" s="22">
+        <v>4</v>
+      </c>
+      <c r="F98" s="22">
+        <v>7</v>
+      </c>
+      <c r="G98" s="22">
+        <v>1</v>
+      </c>
+      <c r="H98" s="22">
+        <v>0</v>
+      </c>
+      <c r="I98" s="22">
+        <v>109</v>
+      </c>
+      <c r="J98" s="22">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="99" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A99" s="29">
+        <v>43999</v>
+      </c>
+      <c r="B99" s="30">
+        <v>90103</v>
+      </c>
+      <c r="C99" s="31">
+        <v>952</v>
+      </c>
+      <c r="D99" s="31">
+        <v>1511</v>
+      </c>
+      <c r="E99" s="31">
+        <v>8</v>
+      </c>
+      <c r="F99" s="31">
+        <v>6</v>
+      </c>
+      <c r="G99" s="31">
+        <v>1</v>
+      </c>
+      <c r="H99" s="31">
+        <v>1</v>
+      </c>
+      <c r="I99" s="31">
+        <v>109</v>
+      </c>
+      <c r="J99" s="31">
+        <v>0</v>
+      </c>
+    </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>

</xml_diff>

<commit_message>
Data updated by GitHub Bot (2020-06-19 12)
</commit_message>
<xml_diff>
--- a/output/snapshot/fdcf2531-4c3e-5c02-b63c-ee160ead6dea.xlsx
+++ b/output/snapshot/fdcf2531-4c3e-5c02-b63c-ee160ead6dea.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="I:\AKTUALNI PODATKI - KORONA\Za objavo na GOV.SI\ang\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{1E6DD62F-2BE2-47DC-A7ED-9B57C1589256}" xr6:coauthVersionLast="44" xr6:coauthVersionMax="44" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{1F3925C0-727D-4AE3-82D9-F83297781159}" xr6:coauthVersionLast="44" xr6:coauthVersionMax="44" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -64,7 +64,7 @@
   <numFmts count="1">
     <numFmt numFmtId="164" formatCode="d/\ m/\ yyyy;@"/>
   </numFmts>
-  <fonts count="4" x14ac:knownFonts="1">
+  <fonts count="5" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -93,6 +93,13 @@
       <name val="Calibri Light"/>
       <scheme val="major"/>
     </font>
+    <font>
+      <sz val="10"/>
+      <color theme="1"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
   </fonts>
   <fills count="3">
     <fill>
@@ -108,7 +115,7 @@
       </patternFill>
     </fill>
   </fills>
-  <borders count="2">
+  <borders count="3">
     <border>
       <left/>
       <right/>
@@ -129,11 +136,26 @@
       <bottom/>
       <diagonal/>
     </border>
+    <border>
+      <left style="thin">
+        <color theme="4"/>
+      </left>
+      <right style="thin">
+        <color theme="4"/>
+      </right>
+      <top style="thin">
+        <color theme="4"/>
+      </top>
+      <bottom style="thin">
+        <color theme="4"/>
+      </bottom>
+      <diagonal/>
+    </border>
   </borders>
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="26">
+  <cellXfs count="32">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="49" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyAlignment="1" applyProtection="1">
       <alignment horizontal="left" vertical="top"/>
@@ -208,6 +230,24 @@
       <alignment horizontal="right"/>
     </xf>
     <xf numFmtId="0" fontId="3" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="right"/>
+    </xf>
+    <xf numFmtId="164" fontId="4" fillId="2" borderId="2" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="right" vertical="top"/>
+    </xf>
+    <xf numFmtId="3" fontId="4" fillId="2" borderId="2" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="right"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="2" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="right"/>
+    </xf>
+    <xf numFmtId="164" fontId="3" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="right" vertical="top"/>
+    </xf>
+    <xf numFmtId="3" fontId="3" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="right"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="right"/>
     </xf>
   </cellXfs>
@@ -399,8 +439,8 @@
 </file>
 
 <file path=xl/tables/table1.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="1" xr:uid="{00000000-000C-0000-FFFF-FFFF00000000}" name="Tabela1" displayName="Tabela1" ref="A1:J75" totalsRowShown="0" headerRowDxfId="11" dataDxfId="10">
-  <autoFilter ref="A1:J75" xr:uid="{00000000-0009-0000-0100-000001000000}">
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="1" xr:uid="{00000000-000C-0000-FFFF-FFFF00000000}" name="Tabela1" displayName="Tabela1" ref="A1:J99" totalsRowShown="0" headerRowDxfId="11" dataDxfId="10">
+  <autoFilter ref="A1:J99" xr:uid="{00000000-0009-0000-0100-000001000000}">
     <filterColumn colId="0" hiddenButton="1"/>
     <filterColumn colId="1" hiddenButton="1"/>
     <filterColumn colId="2" hiddenButton="1"/>
@@ -696,10 +736,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:J75"/>
+  <dimension ref="A1:J99"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A40" zoomScale="89" zoomScaleNormal="89" workbookViewId="0">
-      <selection activeCell="J74" sqref="J74"/>
+    <sheetView tabSelected="1" topLeftCell="A77" zoomScale="89" zoomScaleNormal="89" workbookViewId="0">
+      <selection activeCell="A99" sqref="A99:J99"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -3117,6 +3157,774 @@
         <v>0</v>
       </c>
     </row>
+    <row r="76" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A76" s="20">
+        <v>43976</v>
+      </c>
+      <c r="B76" s="21">
+        <v>75770</v>
+      </c>
+      <c r="C76" s="22">
+        <v>754</v>
+      </c>
+      <c r="D76" s="22">
+        <v>1469</v>
+      </c>
+      <c r="E76" s="22">
+        <v>0</v>
+      </c>
+      <c r="F76" s="22">
+        <v>9</v>
+      </c>
+      <c r="G76" s="22">
+        <v>2</v>
+      </c>
+      <c r="H76" s="22">
+        <v>6</v>
+      </c>
+      <c r="I76" s="22">
+        <v>108</v>
+      </c>
+      <c r="J76" s="22">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="77" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A77" s="20">
+        <v>43977</v>
+      </c>
+      <c r="B77" s="21">
+        <v>76579</v>
+      </c>
+      <c r="C77" s="22">
+        <v>809</v>
+      </c>
+      <c r="D77" s="22">
+        <v>1471</v>
+      </c>
+      <c r="E77" s="22">
+        <v>2</v>
+      </c>
+      <c r="F77" s="22">
+        <v>8</v>
+      </c>
+      <c r="G77" s="22">
+        <v>2</v>
+      </c>
+      <c r="H77" s="22">
+        <v>2</v>
+      </c>
+      <c r="I77" s="22">
+        <v>108</v>
+      </c>
+      <c r="J77" s="22">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="78" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A78" s="20">
+        <v>43978</v>
+      </c>
+      <c r="B78" s="21">
+        <v>77210</v>
+      </c>
+      <c r="C78" s="22">
+        <v>631</v>
+      </c>
+      <c r="D78" s="22">
+        <v>1473</v>
+      </c>
+      <c r="E78" s="22">
+        <v>2</v>
+      </c>
+      <c r="F78" s="22">
+        <v>7</v>
+      </c>
+      <c r="G78" s="22">
+        <v>2</v>
+      </c>
+      <c r="H78" s="22">
+        <v>1</v>
+      </c>
+      <c r="I78" s="22">
+        <v>108</v>
+      </c>
+      <c r="J78" s="22">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="79" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A79" s="20">
+        <v>43979</v>
+      </c>
+      <c r="B79" s="21">
+        <v>77916</v>
+      </c>
+      <c r="C79" s="22">
+        <v>706</v>
+      </c>
+      <c r="D79" s="22">
+        <v>1473</v>
+      </c>
+      <c r="E79" s="22">
+        <v>0</v>
+      </c>
+      <c r="F79" s="22">
+        <v>7</v>
+      </c>
+      <c r="G79" s="22">
+        <v>2</v>
+      </c>
+      <c r="H79" s="22">
+        <v>0</v>
+      </c>
+      <c r="I79" s="22">
+        <v>108</v>
+      </c>
+      <c r="J79" s="22">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="80" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A80" s="20">
+        <v>43980</v>
+      </c>
+      <c r="B80" s="21">
+        <v>78529</v>
+      </c>
+      <c r="C80" s="22">
+        <v>613</v>
+      </c>
+      <c r="D80" s="22">
+        <v>1473</v>
+      </c>
+      <c r="E80" s="22">
+        <v>0</v>
+      </c>
+      <c r="F80" s="22">
+        <v>7</v>
+      </c>
+      <c r="G80" s="22">
+        <v>2</v>
+      </c>
+      <c r="H80" s="22">
+        <v>0</v>
+      </c>
+      <c r="I80" s="22">
+        <v>108</v>
+      </c>
+      <c r="J80" s="22">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="81" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A81" s="20">
+        <v>43981</v>
+      </c>
+      <c r="B81" s="22">
+        <v>78793</v>
+      </c>
+      <c r="C81" s="22">
+        <v>264</v>
+      </c>
+      <c r="D81" s="22">
+        <v>1473</v>
+      </c>
+      <c r="E81" s="22">
+        <v>0</v>
+      </c>
+      <c r="F81" s="22">
+        <v>6</v>
+      </c>
+      <c r="G81" s="22">
+        <v>2</v>
+      </c>
+      <c r="H81" s="22">
+        <v>1</v>
+      </c>
+      <c r="I81" s="22">
+        <v>108</v>
+      </c>
+      <c r="J81" s="22">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="82" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A82" s="20">
+        <v>43982</v>
+      </c>
+      <c r="B82" s="21">
+        <v>79039</v>
+      </c>
+      <c r="C82" s="22">
+        <v>246</v>
+      </c>
+      <c r="D82" s="22">
+        <v>1473</v>
+      </c>
+      <c r="E82" s="22">
+        <v>0</v>
+      </c>
+      <c r="F82" s="22">
+        <v>5</v>
+      </c>
+      <c r="G82" s="22">
+        <v>1</v>
+      </c>
+      <c r="H82" s="22">
+        <v>0</v>
+      </c>
+      <c r="I82" s="22">
+        <v>109</v>
+      </c>
+      <c r="J82" s="22">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="83" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A83" s="20">
+        <v>43983</v>
+      </c>
+      <c r="B83" s="21">
+        <v>79698</v>
+      </c>
+      <c r="C83" s="22">
+        <v>659</v>
+      </c>
+      <c r="D83" s="22">
+        <v>1475</v>
+      </c>
+      <c r="E83" s="22">
+        <v>2</v>
+      </c>
+      <c r="F83" s="22">
+        <v>5</v>
+      </c>
+      <c r="G83" s="22">
+        <v>1</v>
+      </c>
+      <c r="H83" s="22">
+        <v>0</v>
+      </c>
+      <c r="I83" s="22">
+        <v>109</v>
+      </c>
+      <c r="J83" s="22">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="84" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A84" s="20">
+        <v>43984</v>
+      </c>
+      <c r="B84" s="21">
+        <v>80505</v>
+      </c>
+      <c r="C84" s="22">
+        <v>807</v>
+      </c>
+      <c r="D84" s="22">
+        <v>1477</v>
+      </c>
+      <c r="E84" s="22">
+        <v>2</v>
+      </c>
+      <c r="F84" s="22">
+        <v>5</v>
+      </c>
+      <c r="G84" s="22">
+        <v>0</v>
+      </c>
+      <c r="H84" s="22">
+        <v>0</v>
+      </c>
+      <c r="I84" s="22">
+        <v>109</v>
+      </c>
+      <c r="J84" s="22">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="85" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A85" s="20">
+        <v>43985</v>
+      </c>
+      <c r="B85" s="21">
+        <v>81333</v>
+      </c>
+      <c r="C85" s="22">
+        <v>828</v>
+      </c>
+      <c r="D85" s="22">
+        <v>1477</v>
+      </c>
+      <c r="E85" s="22">
+        <v>0</v>
+      </c>
+      <c r="F85" s="22">
+        <v>5</v>
+      </c>
+      <c r="G85" s="22">
+        <v>0</v>
+      </c>
+      <c r="H85" s="22">
+        <v>0</v>
+      </c>
+      <c r="I85" s="22">
+        <v>109</v>
+      </c>
+      <c r="J85" s="22">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="86" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A86" s="26">
+        <v>43986</v>
+      </c>
+      <c r="B86" s="27">
+        <v>82161</v>
+      </c>
+      <c r="C86" s="28">
+        <v>828</v>
+      </c>
+      <c r="D86" s="28">
+        <v>1479</v>
+      </c>
+      <c r="E86" s="28">
+        <v>2</v>
+      </c>
+      <c r="F86" s="28">
+        <v>6</v>
+      </c>
+      <c r="G86" s="28">
+        <v>0</v>
+      </c>
+      <c r="H86" s="28">
+        <v>0</v>
+      </c>
+      <c r="I86" s="28">
+        <v>109</v>
+      </c>
+      <c r="J86" s="28">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="87" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A87" s="29">
+        <v>43987</v>
+      </c>
+      <c r="B87" s="30">
+        <v>82876</v>
+      </c>
+      <c r="C87" s="31">
+        <v>715</v>
+      </c>
+      <c r="D87" s="31">
+        <v>1484</v>
+      </c>
+      <c r="E87" s="31">
+        <v>5</v>
+      </c>
+      <c r="F87" s="31">
+        <v>6</v>
+      </c>
+      <c r="G87" s="31">
+        <v>0</v>
+      </c>
+      <c r="H87" s="31">
+        <v>0</v>
+      </c>
+      <c r="I87" s="31">
+        <v>109</v>
+      </c>
+      <c r="J87" s="31">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="88" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A88" s="23">
+        <v>43988</v>
+      </c>
+      <c r="B88" s="24">
+        <v>83105</v>
+      </c>
+      <c r="C88" s="25">
+        <v>229</v>
+      </c>
+      <c r="D88" s="25">
+        <v>1485</v>
+      </c>
+      <c r="E88" s="25">
+        <v>1</v>
+      </c>
+      <c r="F88" s="25">
+        <v>5</v>
+      </c>
+      <c r="G88" s="25">
+        <v>0</v>
+      </c>
+      <c r="H88" s="25">
+        <v>1</v>
+      </c>
+      <c r="I88" s="25">
+        <v>109</v>
+      </c>
+      <c r="J88" s="25">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="89" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A89" s="29">
+        <v>43989</v>
+      </c>
+      <c r="B89" s="30">
+        <v>83316</v>
+      </c>
+      <c r="C89" s="31">
+        <v>211</v>
+      </c>
+      <c r="D89" s="31">
+        <v>1485</v>
+      </c>
+      <c r="E89" s="31">
+        <v>0</v>
+      </c>
+      <c r="F89" s="31">
+        <v>5</v>
+      </c>
+      <c r="G89" s="31">
+        <v>0</v>
+      </c>
+      <c r="H89" s="31">
+        <v>0</v>
+      </c>
+      <c r="I89" s="31">
+        <v>109</v>
+      </c>
+      <c r="J89" s="31">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="90" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A90" s="20">
+        <v>43990</v>
+      </c>
+      <c r="B90" s="21">
+        <v>84130</v>
+      </c>
+      <c r="C90" s="22">
+        <v>814</v>
+      </c>
+      <c r="D90" s="22">
+        <v>1486</v>
+      </c>
+      <c r="E90" s="22">
+        <v>1</v>
+      </c>
+      <c r="F90" s="22">
+        <v>6</v>
+      </c>
+      <c r="G90" s="22">
+        <v>0</v>
+      </c>
+      <c r="H90" s="22">
+        <v>0</v>
+      </c>
+      <c r="I90" s="22">
+        <v>109</v>
+      </c>
+      <c r="J90" s="22">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="91" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A91" s="20">
+        <v>43991</v>
+      </c>
+      <c r="B91" s="21">
+        <v>84868</v>
+      </c>
+      <c r="C91" s="22">
+        <v>738</v>
+      </c>
+      <c r="D91" s="22">
+        <v>1488</v>
+      </c>
+      <c r="E91" s="22">
+        <v>2</v>
+      </c>
+      <c r="F91" s="22">
+        <v>6</v>
+      </c>
+      <c r="G91" s="22">
+        <v>0</v>
+      </c>
+      <c r="H91" s="22">
+        <v>0</v>
+      </c>
+      <c r="I91" s="22">
+        <v>109</v>
+      </c>
+      <c r="J91" s="22">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="92" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A92" s="23">
+        <v>43992</v>
+      </c>
+      <c r="B92" s="24">
+        <v>85626</v>
+      </c>
+      <c r="C92" s="25">
+        <v>758</v>
+      </c>
+      <c r="D92" s="25">
+        <v>1488</v>
+      </c>
+      <c r="E92" s="25">
+        <v>0</v>
+      </c>
+      <c r="F92" s="25">
+        <v>6</v>
+      </c>
+      <c r="G92" s="25">
+        <v>0</v>
+      </c>
+      <c r="H92" s="25">
+        <v>0</v>
+      </c>
+      <c r="I92" s="25">
+        <v>109</v>
+      </c>
+      <c r="J92" s="25">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="93" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A93" s="29">
+        <v>43993</v>
+      </c>
+      <c r="B93" s="30">
+        <v>86328</v>
+      </c>
+      <c r="C93" s="31">
+        <v>702</v>
+      </c>
+      <c r="D93" s="31">
+        <v>1490</v>
+      </c>
+      <c r="E93" s="31">
+        <v>2</v>
+      </c>
+      <c r="F93" s="31">
+        <v>6</v>
+      </c>
+      <c r="G93" s="31">
+        <v>0</v>
+      </c>
+      <c r="H93" s="31">
+        <v>0</v>
+      </c>
+      <c r="I93" s="31">
+        <v>109</v>
+      </c>
+      <c r="J93" s="31">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="94" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A94" s="23">
+        <v>43994</v>
+      </c>
+      <c r="B94" s="24">
+        <v>87095</v>
+      </c>
+      <c r="C94" s="25">
+        <v>767</v>
+      </c>
+      <c r="D94" s="25">
+        <v>1492</v>
+      </c>
+      <c r="E94" s="25">
+        <v>2</v>
+      </c>
+      <c r="F94" s="25">
+        <v>6</v>
+      </c>
+      <c r="G94" s="25">
+        <v>0</v>
+      </c>
+      <c r="H94" s="25">
+        <v>0</v>
+      </c>
+      <c r="I94" s="25">
+        <v>109</v>
+      </c>
+      <c r="J94" s="25">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="95" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A95" s="29">
+        <v>43995</v>
+      </c>
+      <c r="B95" s="30">
+        <v>87386</v>
+      </c>
+      <c r="C95" s="31">
+        <v>291</v>
+      </c>
+      <c r="D95" s="31">
+        <v>1495</v>
+      </c>
+      <c r="E95" s="31">
+        <v>3</v>
+      </c>
+      <c r="F95" s="31">
+        <v>6</v>
+      </c>
+      <c r="G95" s="31">
+        <v>0</v>
+      </c>
+      <c r="H95" s="31">
+        <v>0</v>
+      </c>
+      <c r="I95" s="31">
+        <v>109</v>
+      </c>
+      <c r="J95" s="31">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="96" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A96" s="23">
+        <v>43996</v>
+      </c>
+      <c r="B96" s="24">
+        <v>87598</v>
+      </c>
+      <c r="C96" s="25">
+        <v>212</v>
+      </c>
+      <c r="D96" s="25">
+        <v>1496</v>
+      </c>
+      <c r="E96" s="25">
+        <v>1</v>
+      </c>
+      <c r="F96" s="25">
+        <v>7</v>
+      </c>
+      <c r="G96" s="25">
+        <v>1</v>
+      </c>
+      <c r="H96" s="25">
+        <v>0</v>
+      </c>
+      <c r="I96" s="25">
+        <v>109</v>
+      </c>
+      <c r="J96" s="25">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="97" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A97" s="20">
+        <v>43997</v>
+      </c>
+      <c r="B97" s="21">
+        <v>88165</v>
+      </c>
+      <c r="C97" s="22">
+        <v>567</v>
+      </c>
+      <c r="D97" s="22">
+        <v>1499</v>
+      </c>
+      <c r="E97" s="22">
+        <v>3</v>
+      </c>
+      <c r="F97" s="22">
+        <v>7</v>
+      </c>
+      <c r="G97" s="22">
+        <v>1</v>
+      </c>
+      <c r="H97" s="22">
+        <v>0</v>
+      </c>
+      <c r="I97" s="22">
+        <v>109</v>
+      </c>
+      <c r="J97" s="22">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="98" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A98" s="20">
+        <v>43998</v>
+      </c>
+      <c r="B98" s="21">
+        <v>89151</v>
+      </c>
+      <c r="C98" s="22">
+        <v>986</v>
+      </c>
+      <c r="D98" s="22">
+        <v>1503</v>
+      </c>
+      <c r="E98" s="22">
+        <v>4</v>
+      </c>
+      <c r="F98" s="22">
+        <v>7</v>
+      </c>
+      <c r="G98" s="22">
+        <v>1</v>
+      </c>
+      <c r="H98" s="22">
+        <v>0</v>
+      </c>
+      <c r="I98" s="22">
+        <v>109</v>
+      </c>
+      <c r="J98" s="22">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="99" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A99" s="29">
+        <v>43999</v>
+      </c>
+      <c r="B99" s="30">
+        <v>90103</v>
+      </c>
+      <c r="C99" s="31">
+        <v>952</v>
+      </c>
+      <c r="D99" s="31">
+        <v>1511</v>
+      </c>
+      <c r="E99" s="31">
+        <v>8</v>
+      </c>
+      <c r="F99" s="31">
+        <v>6</v>
+      </c>
+      <c r="G99" s="31">
+        <v>1</v>
+      </c>
+      <c r="H99" s="31">
+        <v>1</v>
+      </c>
+      <c r="I99" s="31">
+        <v>109</v>
+      </c>
+      <c r="J99" s="31">
+        <v>0</v>
+      </c>
+    </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>

</xml_diff>

<commit_message>
Data updated by GitHub Bot (2020-06-19 20)
</commit_message>
<xml_diff>
--- a/output/snapshot/fdcf2531-4c3e-5c02-b63c-ee160ead6dea.xlsx
+++ b/output/snapshot/fdcf2531-4c3e-5c02-b63c-ee160ead6dea.xlsx
@@ -1,16 +1,15 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="21929"/>
-  <workbookPr/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
+  <fileVersion appName="xl" lastEdited="6" lowestEdited="6" rupBuild="14420"/>
+  <workbookPr defaultThemeVersion="164011"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="I:\AKTUALNI PODATKI - KORONA\Za objavo na GOV.SI\ang\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{1E6DD62F-2BE2-47DC-A7ED-9B57C1589256}" xr6:coauthVersionLast="44" xr6:coauthVersionMax="44" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840"/>
   </bookViews>
   <sheets>
     <sheet name="Covid-19 podatki" sheetId="1" r:id="rId1"/>
@@ -60,11 +59,11 @@
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" mc:Ignorable="x14ac x16r2">
   <numFmts count="1">
     <numFmt numFmtId="164" formatCode="d/\ m/\ yyyy;@"/>
   </numFmts>
-  <fonts count="4" x14ac:knownFonts="1">
+  <fonts count="5" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -93,6 +92,13 @@
       <name val="Calibri Light"/>
       <scheme val="major"/>
     </font>
+    <font>
+      <sz val="10"/>
+      <color theme="1"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
   </fonts>
   <fills count="3">
     <fill>
@@ -108,7 +114,7 @@
       </patternFill>
     </fill>
   </fills>
-  <borders count="2">
+  <borders count="3">
     <border>
       <left/>
       <right/>
@@ -129,11 +135,26 @@
       <bottom/>
       <diagonal/>
     </border>
+    <border>
+      <left style="thin">
+        <color theme="4"/>
+      </left>
+      <right style="thin">
+        <color theme="4"/>
+      </right>
+      <top style="thin">
+        <color theme="4"/>
+      </top>
+      <bottom style="thin">
+        <color theme="4"/>
+      </bottom>
+      <diagonal/>
+    </border>
   </borders>
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="26">
+  <cellXfs count="32">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="49" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyAlignment="1" applyProtection="1">
       <alignment horizontal="left" vertical="top"/>
@@ -208,6 +229,24 @@
       <alignment horizontal="right"/>
     </xf>
     <xf numFmtId="0" fontId="3" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="right"/>
+    </xf>
+    <xf numFmtId="164" fontId="4" fillId="2" borderId="2" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="right" vertical="top"/>
+    </xf>
+    <xf numFmtId="3" fontId="4" fillId="2" borderId="2" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="right"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="2" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="right"/>
+    </xf>
+    <xf numFmtId="164" fontId="3" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="right" vertical="top"/>
+    </xf>
+    <xf numFmtId="3" fontId="3" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="right"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="right"/>
     </xf>
   </cellXfs>
@@ -399,8 +438,8 @@
 </file>
 
 <file path=xl/tables/table1.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="1" xr:uid="{00000000-000C-0000-FFFF-FFFF00000000}" name="Tabela1" displayName="Tabela1" ref="A1:J75" totalsRowShown="0" headerRowDxfId="11" dataDxfId="10">
-  <autoFilter ref="A1:J75" xr:uid="{00000000-0009-0000-0100-000001000000}">
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="1" name="Tabela1" displayName="Tabela1" ref="A1:J100" totalsRowShown="0" headerRowDxfId="11" dataDxfId="10">
+  <autoFilter ref="A1:J100">
     <filterColumn colId="0" hiddenButton="1"/>
     <filterColumn colId="1" hiddenButton="1"/>
     <filterColumn colId="2" hiddenButton="1"/>
@@ -413,16 +452,16 @@
     <filterColumn colId="9" hiddenButton="1"/>
   </autoFilter>
   <tableColumns count="10">
-    <tableColumn id="1" xr3:uid="{00000000-0010-0000-0000-000001000000}" name="Date" dataDxfId="9"/>
-    <tableColumn id="2" xr3:uid="{00000000-0010-0000-0000-000002000000}" name="Tested (all)" dataDxfId="8"/>
-    <tableColumn id="3" xr3:uid="{00000000-0010-0000-0000-000003000000}" name="Tested (daily)" dataDxfId="7"/>
-    <tableColumn id="4" xr3:uid="{00000000-0010-0000-0000-000004000000}" name="Positive (all)" dataDxfId="6"/>
-    <tableColumn id="5" xr3:uid="{00000000-0010-0000-0000-000005000000}" name="Positive (daily)" dataDxfId="5"/>
-    <tableColumn id="6" xr3:uid="{00000000-0010-0000-0000-000006000000}" name="All hospitalized on certain day" dataDxfId="4"/>
-    <tableColumn id="7" xr3:uid="{00000000-0010-0000-0000-000007000000}" name="All persons in intensive care on certain day" dataDxfId="3"/>
-    <tableColumn id="10" xr3:uid="{00000000-0010-0000-0000-00000A000000}" name="Discharged" dataDxfId="2"/>
-    <tableColumn id="8" xr3:uid="{00000000-0010-0000-0000-000008000000}" name="Deaths (all)" dataDxfId="1"/>
-    <tableColumn id="9" xr3:uid="{00000000-0010-0000-0000-000009000000}" name="Deaths (daily)" dataDxfId="0"/>
+    <tableColumn id="1" name="Date" dataDxfId="9"/>
+    <tableColumn id="2" name="Tested (all)" dataDxfId="8"/>
+    <tableColumn id="3" name="Tested (daily)" dataDxfId="7"/>
+    <tableColumn id="4" name="Positive (all)" dataDxfId="6"/>
+    <tableColumn id="5" name="Positive (daily)" dataDxfId="5"/>
+    <tableColumn id="6" name="All hospitalized on certain day" dataDxfId="4"/>
+    <tableColumn id="7" name="All persons in intensive care on certain day" dataDxfId="3"/>
+    <tableColumn id="10" name="Discharged" dataDxfId="2"/>
+    <tableColumn id="8" name="Deaths (all)" dataDxfId="1"/>
+    <tableColumn id="9" name="Deaths (daily)" dataDxfId="0"/>
   </tableColumns>
   <tableStyleInfo name="TableStyleLight16" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
   <extLst>
@@ -695,11 +734,11 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:J75"/>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <dimension ref="A1:J100"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A40" zoomScale="89" zoomScaleNormal="89" workbookViewId="0">
-      <selection activeCell="J74" sqref="J74"/>
+    <sheetView tabSelected="1" topLeftCell="A77" zoomScale="89" zoomScaleNormal="89" workbookViewId="0">
+      <selection activeCell="A100" sqref="A100:J100"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -3117,6 +3156,806 @@
         <v>0</v>
       </c>
     </row>
+    <row r="76" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A76" s="20">
+        <v>43976</v>
+      </c>
+      <c r="B76" s="21">
+        <v>75770</v>
+      </c>
+      <c r="C76" s="22">
+        <v>754</v>
+      </c>
+      <c r="D76" s="22">
+        <v>1469</v>
+      </c>
+      <c r="E76" s="22">
+        <v>0</v>
+      </c>
+      <c r="F76" s="22">
+        <v>9</v>
+      </c>
+      <c r="G76" s="22">
+        <v>2</v>
+      </c>
+      <c r="H76" s="22">
+        <v>6</v>
+      </c>
+      <c r="I76" s="22">
+        <v>108</v>
+      </c>
+      <c r="J76" s="22">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="77" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A77" s="20">
+        <v>43977</v>
+      </c>
+      <c r="B77" s="21">
+        <v>76579</v>
+      </c>
+      <c r="C77" s="22">
+        <v>809</v>
+      </c>
+      <c r="D77" s="22">
+        <v>1471</v>
+      </c>
+      <c r="E77" s="22">
+        <v>2</v>
+      </c>
+      <c r="F77" s="22">
+        <v>8</v>
+      </c>
+      <c r="G77" s="22">
+        <v>2</v>
+      </c>
+      <c r="H77" s="22">
+        <v>2</v>
+      </c>
+      <c r="I77" s="22">
+        <v>108</v>
+      </c>
+      <c r="J77" s="22">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="78" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A78" s="20">
+        <v>43978</v>
+      </c>
+      <c r="B78" s="21">
+        <v>77210</v>
+      </c>
+      <c r="C78" s="22">
+        <v>631</v>
+      </c>
+      <c r="D78" s="22">
+        <v>1473</v>
+      </c>
+      <c r="E78" s="22">
+        <v>2</v>
+      </c>
+      <c r="F78" s="22">
+        <v>7</v>
+      </c>
+      <c r="G78" s="22">
+        <v>2</v>
+      </c>
+      <c r="H78" s="22">
+        <v>1</v>
+      </c>
+      <c r="I78" s="22">
+        <v>108</v>
+      </c>
+      <c r="J78" s="22">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="79" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A79" s="20">
+        <v>43979</v>
+      </c>
+      <c r="B79" s="21">
+        <v>77916</v>
+      </c>
+      <c r="C79" s="22">
+        <v>706</v>
+      </c>
+      <c r="D79" s="22">
+        <v>1473</v>
+      </c>
+      <c r="E79" s="22">
+        <v>0</v>
+      </c>
+      <c r="F79" s="22">
+        <v>7</v>
+      </c>
+      <c r="G79" s="22">
+        <v>2</v>
+      </c>
+      <c r="H79" s="22">
+        <v>0</v>
+      </c>
+      <c r="I79" s="22">
+        <v>108</v>
+      </c>
+      <c r="J79" s="22">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="80" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A80" s="20">
+        <v>43980</v>
+      </c>
+      <c r="B80" s="21">
+        <v>78529</v>
+      </c>
+      <c r="C80" s="22">
+        <v>613</v>
+      </c>
+      <c r="D80" s="22">
+        <v>1473</v>
+      </c>
+      <c r="E80" s="22">
+        <v>0</v>
+      </c>
+      <c r="F80" s="22">
+        <v>7</v>
+      </c>
+      <c r="G80" s="22">
+        <v>2</v>
+      </c>
+      <c r="H80" s="22">
+        <v>0</v>
+      </c>
+      <c r="I80" s="22">
+        <v>108</v>
+      </c>
+      <c r="J80" s="22">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="81" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A81" s="20">
+        <v>43981</v>
+      </c>
+      <c r="B81" s="22">
+        <v>78793</v>
+      </c>
+      <c r="C81" s="22">
+        <v>264</v>
+      </c>
+      <c r="D81" s="22">
+        <v>1473</v>
+      </c>
+      <c r="E81" s="22">
+        <v>0</v>
+      </c>
+      <c r="F81" s="22">
+        <v>6</v>
+      </c>
+      <c r="G81" s="22">
+        <v>2</v>
+      </c>
+      <c r="H81" s="22">
+        <v>1</v>
+      </c>
+      <c r="I81" s="22">
+        <v>108</v>
+      </c>
+      <c r="J81" s="22">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="82" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A82" s="20">
+        <v>43982</v>
+      </c>
+      <c r="B82" s="21">
+        <v>79039</v>
+      </c>
+      <c r="C82" s="22">
+        <v>246</v>
+      </c>
+      <c r="D82" s="22">
+        <v>1473</v>
+      </c>
+      <c r="E82" s="22">
+        <v>0</v>
+      </c>
+      <c r="F82" s="22">
+        <v>5</v>
+      </c>
+      <c r="G82" s="22">
+        <v>1</v>
+      </c>
+      <c r="H82" s="22">
+        <v>0</v>
+      </c>
+      <c r="I82" s="22">
+        <v>109</v>
+      </c>
+      <c r="J82" s="22">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="83" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A83" s="20">
+        <v>43983</v>
+      </c>
+      <c r="B83" s="21">
+        <v>79698</v>
+      </c>
+      <c r="C83" s="22">
+        <v>659</v>
+      </c>
+      <c r="D83" s="22">
+        <v>1475</v>
+      </c>
+      <c r="E83" s="22">
+        <v>2</v>
+      </c>
+      <c r="F83" s="22">
+        <v>5</v>
+      </c>
+      <c r="G83" s="22">
+        <v>1</v>
+      </c>
+      <c r="H83" s="22">
+        <v>0</v>
+      </c>
+      <c r="I83" s="22">
+        <v>109</v>
+      </c>
+      <c r="J83" s="22">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="84" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A84" s="20">
+        <v>43984</v>
+      </c>
+      <c r="B84" s="21">
+        <v>80505</v>
+      </c>
+      <c r="C84" s="22">
+        <v>807</v>
+      </c>
+      <c r="D84" s="22">
+        <v>1477</v>
+      </c>
+      <c r="E84" s="22">
+        <v>2</v>
+      </c>
+      <c r="F84" s="22">
+        <v>5</v>
+      </c>
+      <c r="G84" s="22">
+        <v>0</v>
+      </c>
+      <c r="H84" s="22">
+        <v>0</v>
+      </c>
+      <c r="I84" s="22">
+        <v>109</v>
+      </c>
+      <c r="J84" s="22">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="85" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A85" s="20">
+        <v>43985</v>
+      </c>
+      <c r="B85" s="21">
+        <v>81333</v>
+      </c>
+      <c r="C85" s="22">
+        <v>828</v>
+      </c>
+      <c r="D85" s="22">
+        <v>1477</v>
+      </c>
+      <c r="E85" s="22">
+        <v>0</v>
+      </c>
+      <c r="F85" s="22">
+        <v>5</v>
+      </c>
+      <c r="G85" s="22">
+        <v>0</v>
+      </c>
+      <c r="H85" s="22">
+        <v>0</v>
+      </c>
+      <c r="I85" s="22">
+        <v>109</v>
+      </c>
+      <c r="J85" s="22">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="86" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A86" s="26">
+        <v>43986</v>
+      </c>
+      <c r="B86" s="27">
+        <v>82161</v>
+      </c>
+      <c r="C86" s="28">
+        <v>828</v>
+      </c>
+      <c r="D86" s="28">
+        <v>1479</v>
+      </c>
+      <c r="E86" s="28">
+        <v>2</v>
+      </c>
+      <c r="F86" s="28">
+        <v>6</v>
+      </c>
+      <c r="G86" s="28">
+        <v>0</v>
+      </c>
+      <c r="H86" s="28">
+        <v>0</v>
+      </c>
+      <c r="I86" s="28">
+        <v>109</v>
+      </c>
+      <c r="J86" s="28">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="87" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A87" s="29">
+        <v>43987</v>
+      </c>
+      <c r="B87" s="30">
+        <v>82876</v>
+      </c>
+      <c r="C87" s="31">
+        <v>715</v>
+      </c>
+      <c r="D87" s="31">
+        <v>1484</v>
+      </c>
+      <c r="E87" s="31">
+        <v>5</v>
+      </c>
+      <c r="F87" s="31">
+        <v>6</v>
+      </c>
+      <c r="G87" s="31">
+        <v>0</v>
+      </c>
+      <c r="H87" s="31">
+        <v>0</v>
+      </c>
+      <c r="I87" s="31">
+        <v>109</v>
+      </c>
+      <c r="J87" s="31">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="88" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A88" s="23">
+        <v>43988</v>
+      </c>
+      <c r="B88" s="24">
+        <v>83105</v>
+      </c>
+      <c r="C88" s="25">
+        <v>229</v>
+      </c>
+      <c r="D88" s="25">
+        <v>1485</v>
+      </c>
+      <c r="E88" s="25">
+        <v>1</v>
+      </c>
+      <c r="F88" s="25">
+        <v>5</v>
+      </c>
+      <c r="G88" s="25">
+        <v>0</v>
+      </c>
+      <c r="H88" s="25">
+        <v>1</v>
+      </c>
+      <c r="I88" s="25">
+        <v>109</v>
+      </c>
+      <c r="J88" s="25">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="89" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A89" s="29">
+        <v>43989</v>
+      </c>
+      <c r="B89" s="30">
+        <v>83316</v>
+      </c>
+      <c r="C89" s="31">
+        <v>211</v>
+      </c>
+      <c r="D89" s="31">
+        <v>1485</v>
+      </c>
+      <c r="E89" s="31">
+        <v>0</v>
+      </c>
+      <c r="F89" s="31">
+        <v>5</v>
+      </c>
+      <c r="G89" s="31">
+        <v>0</v>
+      </c>
+      <c r="H89" s="31">
+        <v>0</v>
+      </c>
+      <c r="I89" s="31">
+        <v>109</v>
+      </c>
+      <c r="J89" s="31">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="90" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A90" s="20">
+        <v>43990</v>
+      </c>
+      <c r="B90" s="21">
+        <v>84130</v>
+      </c>
+      <c r="C90" s="22">
+        <v>814</v>
+      </c>
+      <c r="D90" s="22">
+        <v>1486</v>
+      </c>
+      <c r="E90" s="22">
+        <v>1</v>
+      </c>
+      <c r="F90" s="22">
+        <v>6</v>
+      </c>
+      <c r="G90" s="22">
+        <v>0</v>
+      </c>
+      <c r="H90" s="22">
+        <v>0</v>
+      </c>
+      <c r="I90" s="22">
+        <v>109</v>
+      </c>
+      <c r="J90" s="22">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="91" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A91" s="20">
+        <v>43991</v>
+      </c>
+      <c r="B91" s="21">
+        <v>84868</v>
+      </c>
+      <c r="C91" s="22">
+        <v>738</v>
+      </c>
+      <c r="D91" s="22">
+        <v>1488</v>
+      </c>
+      <c r="E91" s="22">
+        <v>2</v>
+      </c>
+      <c r="F91" s="22">
+        <v>6</v>
+      </c>
+      <c r="G91" s="22">
+        <v>0</v>
+      </c>
+      <c r="H91" s="22">
+        <v>0</v>
+      </c>
+      <c r="I91" s="22">
+        <v>109</v>
+      </c>
+      <c r="J91" s="22">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="92" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A92" s="23">
+        <v>43992</v>
+      </c>
+      <c r="B92" s="24">
+        <v>85626</v>
+      </c>
+      <c r="C92" s="25">
+        <v>758</v>
+      </c>
+      <c r="D92" s="25">
+        <v>1488</v>
+      </c>
+      <c r="E92" s="25">
+        <v>0</v>
+      </c>
+      <c r="F92" s="25">
+        <v>6</v>
+      </c>
+      <c r="G92" s="25">
+        <v>0</v>
+      </c>
+      <c r="H92" s="25">
+        <v>0</v>
+      </c>
+      <c r="I92" s="25">
+        <v>109</v>
+      </c>
+      <c r="J92" s="25">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="93" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A93" s="29">
+        <v>43993</v>
+      </c>
+      <c r="B93" s="30">
+        <v>86328</v>
+      </c>
+      <c r="C93" s="31">
+        <v>702</v>
+      </c>
+      <c r="D93" s="31">
+        <v>1490</v>
+      </c>
+      <c r="E93" s="31">
+        <v>2</v>
+      </c>
+      <c r="F93" s="31">
+        <v>6</v>
+      </c>
+      <c r="G93" s="31">
+        <v>0</v>
+      </c>
+      <c r="H93" s="31">
+        <v>0</v>
+      </c>
+      <c r="I93" s="31">
+        <v>109</v>
+      </c>
+      <c r="J93" s="31">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="94" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A94" s="23">
+        <v>43994</v>
+      </c>
+      <c r="B94" s="24">
+        <v>87095</v>
+      </c>
+      <c r="C94" s="25">
+        <v>767</v>
+      </c>
+      <c r="D94" s="25">
+        <v>1492</v>
+      </c>
+      <c r="E94" s="25">
+        <v>2</v>
+      </c>
+      <c r="F94" s="25">
+        <v>6</v>
+      </c>
+      <c r="G94" s="25">
+        <v>0</v>
+      </c>
+      <c r="H94" s="25">
+        <v>0</v>
+      </c>
+      <c r="I94" s="25">
+        <v>109</v>
+      </c>
+      <c r="J94" s="25">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="95" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A95" s="29">
+        <v>43995</v>
+      </c>
+      <c r="B95" s="30">
+        <v>87386</v>
+      </c>
+      <c r="C95" s="31">
+        <v>291</v>
+      </c>
+      <c r="D95" s="31">
+        <v>1495</v>
+      </c>
+      <c r="E95" s="31">
+        <v>3</v>
+      </c>
+      <c r="F95" s="31">
+        <v>6</v>
+      </c>
+      <c r="G95" s="31">
+        <v>0</v>
+      </c>
+      <c r="H95" s="31">
+        <v>0</v>
+      </c>
+      <c r="I95" s="31">
+        <v>109</v>
+      </c>
+      <c r="J95" s="31">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="96" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A96" s="23">
+        <v>43996</v>
+      </c>
+      <c r="B96" s="24">
+        <v>87598</v>
+      </c>
+      <c r="C96" s="25">
+        <v>212</v>
+      </c>
+      <c r="D96" s="25">
+        <v>1496</v>
+      </c>
+      <c r="E96" s="25">
+        <v>1</v>
+      </c>
+      <c r="F96" s="25">
+        <v>7</v>
+      </c>
+      <c r="G96" s="25">
+        <v>1</v>
+      </c>
+      <c r="H96" s="25">
+        <v>0</v>
+      </c>
+      <c r="I96" s="25">
+        <v>109</v>
+      </c>
+      <c r="J96" s="25">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="97" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A97" s="20">
+        <v>43997</v>
+      </c>
+      <c r="B97" s="21">
+        <v>88165</v>
+      </c>
+      <c r="C97" s="22">
+        <v>567</v>
+      </c>
+      <c r="D97" s="22">
+        <v>1499</v>
+      </c>
+      <c r="E97" s="22">
+        <v>3</v>
+      </c>
+      <c r="F97" s="22">
+        <v>7</v>
+      </c>
+      <c r="G97" s="22">
+        <v>1</v>
+      </c>
+      <c r="H97" s="22">
+        <v>0</v>
+      </c>
+      <c r="I97" s="22">
+        <v>109</v>
+      </c>
+      <c r="J97" s="22">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="98" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A98" s="20">
+        <v>43998</v>
+      </c>
+      <c r="B98" s="21">
+        <v>89151</v>
+      </c>
+      <c r="C98" s="22">
+        <v>986</v>
+      </c>
+      <c r="D98" s="22">
+        <v>1503</v>
+      </c>
+      <c r="E98" s="22">
+        <v>4</v>
+      </c>
+      <c r="F98" s="22">
+        <v>7</v>
+      </c>
+      <c r="G98" s="22">
+        <v>1</v>
+      </c>
+      <c r="H98" s="22">
+        <v>0</v>
+      </c>
+      <c r="I98" s="22">
+        <v>109</v>
+      </c>
+      <c r="J98" s="22">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="99" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A99" s="29">
+        <v>43999</v>
+      </c>
+      <c r="B99" s="30">
+        <v>90103</v>
+      </c>
+      <c r="C99" s="31">
+        <v>952</v>
+      </c>
+      <c r="D99" s="31">
+        <v>1511</v>
+      </c>
+      <c r="E99" s="31">
+        <v>8</v>
+      </c>
+      <c r="F99" s="31">
+        <v>6</v>
+      </c>
+      <c r="G99" s="31">
+        <v>1</v>
+      </c>
+      <c r="H99" s="31">
+        <v>1</v>
+      </c>
+      <c r="I99" s="31">
+        <v>109</v>
+      </c>
+      <c r="J99" s="31">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="100" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A100" s="20">
+        <v>44000</v>
+      </c>
+      <c r="B100" s="21">
+        <v>91005</v>
+      </c>
+      <c r="C100" s="22">
+        <v>902</v>
+      </c>
+      <c r="D100" s="22">
+        <v>1513</v>
+      </c>
+      <c r="E100" s="22">
+        <v>2</v>
+      </c>
+      <c r="F100" s="22">
+        <v>8</v>
+      </c>
+      <c r="G100" s="22">
+        <v>1</v>
+      </c>
+      <c r="H100" s="22">
+        <v>0</v>
+      </c>
+      <c r="I100" s="22">
+        <v>109</v>
+      </c>
+      <c r="J100" s="22">
+        <v>0</v>
+      </c>
+    </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>

</xml_diff>

<commit_message>
Data updated by GitHub Bot (2020-06-20 12)
</commit_message>
<xml_diff>
--- a/output/snapshot/fdcf2531-4c3e-5c02-b63c-ee160ead6dea.xlsx
+++ b/output/snapshot/fdcf2531-4c3e-5c02-b63c-ee160ead6dea.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="I:\AKTUALNI PODATKI - KORONA\Za objavo na GOV.SI\ang\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{1E6DD62F-2BE2-47DC-A7ED-9B57C1589256}" xr6:coauthVersionLast="44" xr6:coauthVersionMax="44" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{9EE09CBD-7DAA-4C74-9BA3-7F1963AA8E06}" xr6:coauthVersionLast="44" xr6:coauthVersionMax="44" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12576" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Covid-19 podatki" sheetId="1" r:id="rId1"/>
@@ -64,7 +64,7 @@
   <numFmts count="1">
     <numFmt numFmtId="164" formatCode="d/\ m/\ yyyy;@"/>
   </numFmts>
-  <fonts count="4" x14ac:knownFonts="1">
+  <fonts count="5" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -93,6 +93,13 @@
       <name val="Calibri Light"/>
       <scheme val="major"/>
     </font>
+    <font>
+      <sz val="10"/>
+      <color theme="1"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
   </fonts>
   <fills count="3">
     <fill>
@@ -108,7 +115,7 @@
       </patternFill>
     </fill>
   </fills>
-  <borders count="2">
+  <borders count="3">
     <border>
       <left/>
       <right/>
@@ -129,11 +136,26 @@
       <bottom/>
       <diagonal/>
     </border>
+    <border>
+      <left style="thin">
+        <color theme="4"/>
+      </left>
+      <right style="thin">
+        <color theme="4"/>
+      </right>
+      <top style="thin">
+        <color theme="4"/>
+      </top>
+      <bottom style="thin">
+        <color theme="4"/>
+      </bottom>
+      <diagonal/>
+    </border>
   </borders>
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="26">
+  <cellXfs count="32">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="49" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyAlignment="1" applyProtection="1">
       <alignment horizontal="left" vertical="top"/>
@@ -208,6 +230,24 @@
       <alignment horizontal="right"/>
     </xf>
     <xf numFmtId="0" fontId="3" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="right"/>
+    </xf>
+    <xf numFmtId="164" fontId="4" fillId="2" borderId="2" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="right" vertical="top"/>
+    </xf>
+    <xf numFmtId="3" fontId="4" fillId="2" borderId="2" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="right"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="2" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="right"/>
+    </xf>
+    <xf numFmtId="164" fontId="3" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="right" vertical="top"/>
+    </xf>
+    <xf numFmtId="3" fontId="3" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="right"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="right"/>
     </xf>
   </cellXfs>
@@ -399,8 +439,8 @@
 </file>
 
 <file path=xl/tables/table1.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="1" xr:uid="{00000000-000C-0000-FFFF-FFFF00000000}" name="Tabela1" displayName="Tabela1" ref="A1:J75" totalsRowShown="0" headerRowDxfId="11" dataDxfId="10">
-  <autoFilter ref="A1:J75" xr:uid="{00000000-0009-0000-0100-000001000000}">
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="1" xr:uid="{00000000-000C-0000-FFFF-FFFF00000000}" name="Tabela1" displayName="Tabela1" ref="A1:J101" totalsRowShown="0" headerRowDxfId="11" dataDxfId="10">
+  <autoFilter ref="A1:J101" xr:uid="{00000000-0009-0000-0100-000001000000}">
     <filterColumn colId="0" hiddenButton="1"/>
     <filterColumn colId="1" hiddenButton="1"/>
     <filterColumn colId="2" hiddenButton="1"/>
@@ -696,28 +736,28 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:J75"/>
+  <dimension ref="A1:J101"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A40" zoomScale="89" zoomScaleNormal="89" workbookViewId="0">
-      <selection activeCell="J74" sqref="J74"/>
+    <sheetView tabSelected="1" topLeftCell="A77" zoomScale="89" zoomScaleNormal="89" workbookViewId="0">
+      <selection activeCell="A101" sqref="A101:J101"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
-    <col min="1" max="1" width="12.7109375" style="1" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="13.5703125" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="16.28515625" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="15.28515625" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="17.85546875" bestFit="1" customWidth="1"/>
-    <col min="6" max="6" width="35.42578125" bestFit="1" customWidth="1"/>
-    <col min="7" max="7" width="51.140625" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="12.6640625" style="1" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="13.5546875" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="16.33203125" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="15.33203125" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="17.88671875" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="35.44140625" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="51.109375" bestFit="1" customWidth="1"/>
     <col min="8" max="8" width="14" bestFit="1" customWidth="1"/>
-    <col min="9" max="9" width="13.85546875" bestFit="1" customWidth="1"/>
-    <col min="10" max="10" width="16.5703125" bestFit="1" customWidth="1"/>
+    <col min="9" max="9" width="13.88671875" bestFit="1" customWidth="1"/>
+    <col min="10" max="10" width="16.5546875" bestFit="1" customWidth="1"/>
     <col min="11" max="11" width="29" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A1" s="2" t="s">
         <v>0</v>
       </c>
@@ -749,7 +789,7 @@
         <v>9</v>
       </c>
     </row>
-    <row r="2" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A2" s="4">
         <v>43902</v>
       </c>
@@ -781,7 +821,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="3" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A3" s="4">
         <v>43903</v>
       </c>
@@ -813,7 +853,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="4" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A4" s="4">
         <v>43904</v>
       </c>
@@ -845,7 +885,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="5" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A5" s="4">
         <v>43905</v>
       </c>
@@ -877,7 +917,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="6" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A6" s="4">
         <v>43906</v>
       </c>
@@ -909,7 +949,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="7" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A7" s="4">
         <v>43907</v>
       </c>
@@ -941,7 +981,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="8" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A8" s="4">
         <v>43908</v>
       </c>
@@ -973,7 +1013,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="9" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A9" s="4">
         <v>43909</v>
       </c>
@@ -1005,7 +1045,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="10" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="10" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A10" s="4">
         <v>43910</v>
       </c>
@@ -1037,7 +1077,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="11" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="11" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A11" s="4">
         <v>43911</v>
       </c>
@@ -1069,7 +1109,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="12" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="12" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A12" s="4">
         <v>43912</v>
       </c>
@@ -1101,7 +1141,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="13" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="13" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A13" s="4">
         <v>43913</v>
       </c>
@@ -1133,7 +1173,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="14" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="14" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A14" s="4">
         <v>43914</v>
       </c>
@@ -1165,7 +1205,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="15" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="15" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A15" s="4">
         <v>43915</v>
       </c>
@@ -1197,7 +1237,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="16" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="16" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A16" s="4">
         <v>43916</v>
       </c>
@@ -1229,7 +1269,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="17" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="17" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A17" s="6">
         <v>43917</v>
       </c>
@@ -1261,7 +1301,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="18" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="18" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A18" s="4">
         <v>43918</v>
       </c>
@@ -1293,7 +1333,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="19" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="19" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A19" s="4">
         <v>43919</v>
       </c>
@@ -1325,7 +1365,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="20" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="20" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A20" s="4">
         <v>43920</v>
       </c>
@@ -1357,7 +1397,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="21" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="21" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A21" s="4">
         <v>43921</v>
       </c>
@@ -1389,7 +1429,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="22" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="22" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A22" s="4">
         <v>43922</v>
       </c>
@@ -1421,7 +1461,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="23" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="23" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A23" s="4">
         <v>43923</v>
       </c>
@@ -1453,7 +1493,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="24" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="24" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A24" s="4">
         <v>43924</v>
       </c>
@@ -1485,7 +1525,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="25" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="25" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A25" s="4">
         <v>43925</v>
       </c>
@@ -1517,7 +1557,7 @@
         <v>6</v>
       </c>
     </row>
-    <row r="26" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="26" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A26" s="4">
         <v>43926</v>
       </c>
@@ -1549,7 +1589,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="27" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="27" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A27" s="4">
         <v>43927</v>
       </c>
@@ -1581,7 +1621,7 @@
         <v>6</v>
       </c>
     </row>
-    <row r="28" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="28" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A28" s="8">
         <v>43928</v>
       </c>
@@ -1613,7 +1653,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="29" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="29" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A29" s="4">
         <v>43929</v>
       </c>
@@ -1645,7 +1685,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="30" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="30" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A30" s="4">
         <v>43930</v>
       </c>
@@ -1677,7 +1717,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="31" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="31" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A31" s="4">
         <v>43931</v>
       </c>
@@ -1709,7 +1749,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="32" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="32" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A32" s="4">
         <v>43932</v>
       </c>
@@ -1741,7 +1781,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="33" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="33" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A33" s="4">
         <v>43933</v>
       </c>
@@ -1773,7 +1813,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="34" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="34" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A34" s="4">
         <v>43934</v>
       </c>
@@ -1805,7 +1845,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="35" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="35" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A35" s="4">
         <v>43935</v>
       </c>
@@ -1837,7 +1877,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="36" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="36" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A36" s="4">
         <v>43936</v>
       </c>
@@ -1869,7 +1909,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="37" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="37" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A37" s="4">
         <v>43937</v>
       </c>
@@ -1901,7 +1941,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="38" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="38" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A38" s="4">
         <v>43938</v>
       </c>
@@ -1933,7 +1973,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="39" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="39" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A39" s="4">
         <v>43939</v>
       </c>
@@ -1965,7 +2005,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="40" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="40" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A40" s="4">
         <v>43940</v>
       </c>
@@ -1997,7 +2037,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="41" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="41" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A41" s="4">
         <v>43941</v>
       </c>
@@ -2029,7 +2069,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="42" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="42" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A42" s="11">
         <v>43942</v>
       </c>
@@ -2061,7 +2101,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="43" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="43" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A43" s="4">
         <v>43943</v>
       </c>
@@ -2093,7 +2133,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="44" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="44" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A44" s="4">
         <v>43944</v>
       </c>
@@ -2125,7 +2165,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="45" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="45" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A45" s="4">
         <v>43945</v>
       </c>
@@ -2157,7 +2197,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="46" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="46" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A46" s="4">
         <v>43946</v>
       </c>
@@ -2189,7 +2229,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="47" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="47" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A47" s="8">
         <v>43947</v>
       </c>
@@ -2221,7 +2261,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="48" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="48" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A48" s="4">
         <v>43948</v>
       </c>
@@ -2253,7 +2293,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="49" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="49" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A49" s="4">
         <v>43949</v>
       </c>
@@ -2285,7 +2325,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="50" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="50" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A50" s="4">
         <v>43950</v>
       </c>
@@ -2317,7 +2357,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="51" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="51" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A51" s="14">
         <v>43951</v>
       </c>
@@ -2349,7 +2389,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="52" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="52" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A52" s="4">
         <v>43952</v>
       </c>
@@ -2381,7 +2421,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="53" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="53" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A53" s="4">
         <v>43953</v>
       </c>
@@ -2413,7 +2453,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="54" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="54" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A54" s="11">
         <v>43954</v>
       </c>
@@ -2445,7 +2485,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="55" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="55" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A55" s="4">
         <v>43955</v>
       </c>
@@ -2477,7 +2517,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="56" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="56" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A56" s="11">
         <v>43956</v>
       </c>
@@ -2509,7 +2549,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="57" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="57" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A57" s="4">
         <v>43957</v>
       </c>
@@ -2541,7 +2581,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="58" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="58" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A58" s="4">
         <v>43958</v>
       </c>
@@ -2573,7 +2613,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="59" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="59" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A59" s="4">
         <v>43959</v>
       </c>
@@ -2605,7 +2645,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="60" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="60" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A60" s="4">
         <v>43960</v>
       </c>
@@ -2637,7 +2677,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="61" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="61" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A61" s="4">
         <v>43961</v>
       </c>
@@ -2669,7 +2709,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="62" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="62" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A62" s="4">
         <v>43962</v>
       </c>
@@ -2701,7 +2741,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="63" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="63" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A63" s="4">
         <v>43963</v>
       </c>
@@ -2733,7 +2773,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="64" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="64" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A64" s="17">
         <v>43964</v>
       </c>
@@ -2765,7 +2805,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="65" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="65" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A65" s="14">
         <v>43965</v>
       </c>
@@ -2797,7 +2837,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="66" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="66" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A66" s="11">
         <v>43966</v>
       </c>
@@ -2829,7 +2869,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="67" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="67" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A67" s="14">
         <v>43967</v>
       </c>
@@ -2861,7 +2901,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="68" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="68" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A68" s="11">
         <v>43968</v>
       </c>
@@ -2893,7 +2933,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="69" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="69" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A69" s="14">
         <v>43969</v>
       </c>
@@ -2925,7 +2965,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="70" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="70" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A70" s="11">
         <v>43970</v>
       </c>
@@ -2957,7 +2997,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="71" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="71" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A71" s="20">
         <v>43971</v>
       </c>
@@ -2989,7 +3029,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="72" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="72" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A72" s="23">
         <v>43972</v>
       </c>
@@ -3021,7 +3061,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="73" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="73" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A73" s="20">
         <v>43973</v>
       </c>
@@ -3053,7 +3093,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="74" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="74" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A74" s="17">
         <v>43974</v>
       </c>
@@ -3085,7 +3125,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="75" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="75" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A75" s="20">
         <v>43975</v>
       </c>
@@ -3114,6 +3154,838 @@
         <v>107</v>
       </c>
       <c r="J75" s="22">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="76" spans="1:10" x14ac:dyDescent="0.3">
+      <c r="A76" s="20">
+        <v>43976</v>
+      </c>
+      <c r="B76" s="21">
+        <v>75770</v>
+      </c>
+      <c r="C76" s="22">
+        <v>754</v>
+      </c>
+      <c r="D76" s="22">
+        <v>1469</v>
+      </c>
+      <c r="E76" s="22">
+        <v>0</v>
+      </c>
+      <c r="F76" s="22">
+        <v>9</v>
+      </c>
+      <c r="G76" s="22">
+        <v>2</v>
+      </c>
+      <c r="H76" s="22">
+        <v>6</v>
+      </c>
+      <c r="I76" s="22">
+        <v>108</v>
+      </c>
+      <c r="J76" s="22">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="77" spans="1:10" x14ac:dyDescent="0.3">
+      <c r="A77" s="20">
+        <v>43977</v>
+      </c>
+      <c r="B77" s="21">
+        <v>76579</v>
+      </c>
+      <c r="C77" s="22">
+        <v>809</v>
+      </c>
+      <c r="D77" s="22">
+        <v>1471</v>
+      </c>
+      <c r="E77" s="22">
+        <v>2</v>
+      </c>
+      <c r="F77" s="22">
+        <v>8</v>
+      </c>
+      <c r="G77" s="22">
+        <v>2</v>
+      </c>
+      <c r="H77" s="22">
+        <v>2</v>
+      </c>
+      <c r="I77" s="22">
+        <v>108</v>
+      </c>
+      <c r="J77" s="22">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="78" spans="1:10" x14ac:dyDescent="0.3">
+      <c r="A78" s="20">
+        <v>43978</v>
+      </c>
+      <c r="B78" s="21">
+        <v>77210</v>
+      </c>
+      <c r="C78" s="22">
+        <v>631</v>
+      </c>
+      <c r="D78" s="22">
+        <v>1473</v>
+      </c>
+      <c r="E78" s="22">
+        <v>2</v>
+      </c>
+      <c r="F78" s="22">
+        <v>7</v>
+      </c>
+      <c r="G78" s="22">
+        <v>2</v>
+      </c>
+      <c r="H78" s="22">
+        <v>1</v>
+      </c>
+      <c r="I78" s="22">
+        <v>108</v>
+      </c>
+      <c r="J78" s="22">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="79" spans="1:10" x14ac:dyDescent="0.3">
+      <c r="A79" s="20">
+        <v>43979</v>
+      </c>
+      <c r="B79" s="21">
+        <v>77916</v>
+      </c>
+      <c r="C79" s="22">
+        <v>706</v>
+      </c>
+      <c r="D79" s="22">
+        <v>1473</v>
+      </c>
+      <c r="E79" s="22">
+        <v>0</v>
+      </c>
+      <c r="F79" s="22">
+        <v>7</v>
+      </c>
+      <c r="G79" s="22">
+        <v>2</v>
+      </c>
+      <c r="H79" s="22">
+        <v>0</v>
+      </c>
+      <c r="I79" s="22">
+        <v>108</v>
+      </c>
+      <c r="J79" s="22">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="80" spans="1:10" x14ac:dyDescent="0.3">
+      <c r="A80" s="20">
+        <v>43980</v>
+      </c>
+      <c r="B80" s="21">
+        <v>78529</v>
+      </c>
+      <c r="C80" s="22">
+        <v>613</v>
+      </c>
+      <c r="D80" s="22">
+        <v>1473</v>
+      </c>
+      <c r="E80" s="22">
+        <v>0</v>
+      </c>
+      <c r="F80" s="22">
+        <v>7</v>
+      </c>
+      <c r="G80" s="22">
+        <v>2</v>
+      </c>
+      <c r="H80" s="22">
+        <v>0</v>
+      </c>
+      <c r="I80" s="22">
+        <v>108</v>
+      </c>
+      <c r="J80" s="22">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="81" spans="1:10" x14ac:dyDescent="0.3">
+      <c r="A81" s="20">
+        <v>43981</v>
+      </c>
+      <c r="B81" s="22">
+        <v>78793</v>
+      </c>
+      <c r="C81" s="22">
+        <v>264</v>
+      </c>
+      <c r="D81" s="22">
+        <v>1473</v>
+      </c>
+      <c r="E81" s="22">
+        <v>0</v>
+      </c>
+      <c r="F81" s="22">
+        <v>6</v>
+      </c>
+      <c r="G81" s="22">
+        <v>2</v>
+      </c>
+      <c r="H81" s="22">
+        <v>1</v>
+      </c>
+      <c r="I81" s="22">
+        <v>108</v>
+      </c>
+      <c r="J81" s="22">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="82" spans="1:10" x14ac:dyDescent="0.3">
+      <c r="A82" s="20">
+        <v>43982</v>
+      </c>
+      <c r="B82" s="21">
+        <v>79039</v>
+      </c>
+      <c r="C82" s="22">
+        <v>246</v>
+      </c>
+      <c r="D82" s="22">
+        <v>1473</v>
+      </c>
+      <c r="E82" s="22">
+        <v>0</v>
+      </c>
+      <c r="F82" s="22">
+        <v>5</v>
+      </c>
+      <c r="G82" s="22">
+        <v>1</v>
+      </c>
+      <c r="H82" s="22">
+        <v>0</v>
+      </c>
+      <c r="I82" s="22">
+        <v>109</v>
+      </c>
+      <c r="J82" s="22">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="83" spans="1:10" x14ac:dyDescent="0.3">
+      <c r="A83" s="20">
+        <v>43983</v>
+      </c>
+      <c r="B83" s="21">
+        <v>79698</v>
+      </c>
+      <c r="C83" s="22">
+        <v>659</v>
+      </c>
+      <c r="D83" s="22">
+        <v>1475</v>
+      </c>
+      <c r="E83" s="22">
+        <v>2</v>
+      </c>
+      <c r="F83" s="22">
+        <v>5</v>
+      </c>
+      <c r="G83" s="22">
+        <v>1</v>
+      </c>
+      <c r="H83" s="22">
+        <v>0</v>
+      </c>
+      <c r="I83" s="22">
+        <v>109</v>
+      </c>
+      <c r="J83" s="22">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="84" spans="1:10" x14ac:dyDescent="0.3">
+      <c r="A84" s="20">
+        <v>43984</v>
+      </c>
+      <c r="B84" s="21">
+        <v>80505</v>
+      </c>
+      <c r="C84" s="22">
+        <v>807</v>
+      </c>
+      <c r="D84" s="22">
+        <v>1477</v>
+      </c>
+      <c r="E84" s="22">
+        <v>2</v>
+      </c>
+      <c r="F84" s="22">
+        <v>5</v>
+      </c>
+      <c r="G84" s="22">
+        <v>0</v>
+      </c>
+      <c r="H84" s="22">
+        <v>0</v>
+      </c>
+      <c r="I84" s="22">
+        <v>109</v>
+      </c>
+      <c r="J84" s="22">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="85" spans="1:10" x14ac:dyDescent="0.3">
+      <c r="A85" s="20">
+        <v>43985</v>
+      </c>
+      <c r="B85" s="21">
+        <v>81333</v>
+      </c>
+      <c r="C85" s="22">
+        <v>828</v>
+      </c>
+      <c r="D85" s="22">
+        <v>1477</v>
+      </c>
+      <c r="E85" s="22">
+        <v>0</v>
+      </c>
+      <c r="F85" s="22">
+        <v>5</v>
+      </c>
+      <c r="G85" s="22">
+        <v>0</v>
+      </c>
+      <c r="H85" s="22">
+        <v>0</v>
+      </c>
+      <c r="I85" s="22">
+        <v>109</v>
+      </c>
+      <c r="J85" s="22">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="86" spans="1:10" x14ac:dyDescent="0.3">
+      <c r="A86" s="26">
+        <v>43986</v>
+      </c>
+      <c r="B86" s="27">
+        <v>82161</v>
+      </c>
+      <c r="C86" s="28">
+        <v>828</v>
+      </c>
+      <c r="D86" s="28">
+        <v>1479</v>
+      </c>
+      <c r="E86" s="28">
+        <v>2</v>
+      </c>
+      <c r="F86" s="28">
+        <v>6</v>
+      </c>
+      <c r="G86" s="28">
+        <v>0</v>
+      </c>
+      <c r="H86" s="28">
+        <v>0</v>
+      </c>
+      <c r="I86" s="28">
+        <v>109</v>
+      </c>
+      <c r="J86" s="28">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="87" spans="1:10" x14ac:dyDescent="0.3">
+      <c r="A87" s="29">
+        <v>43987</v>
+      </c>
+      <c r="B87" s="30">
+        <v>82876</v>
+      </c>
+      <c r="C87" s="31">
+        <v>715</v>
+      </c>
+      <c r="D87" s="31">
+        <v>1484</v>
+      </c>
+      <c r="E87" s="31">
+        <v>5</v>
+      </c>
+      <c r="F87" s="31">
+        <v>6</v>
+      </c>
+      <c r="G87" s="31">
+        <v>0</v>
+      </c>
+      <c r="H87" s="31">
+        <v>0</v>
+      </c>
+      <c r="I87" s="31">
+        <v>109</v>
+      </c>
+      <c r="J87" s="31">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="88" spans="1:10" x14ac:dyDescent="0.3">
+      <c r="A88" s="23">
+        <v>43988</v>
+      </c>
+      <c r="B88" s="24">
+        <v>83105</v>
+      </c>
+      <c r="C88" s="25">
+        <v>229</v>
+      </c>
+      <c r="D88" s="25">
+        <v>1485</v>
+      </c>
+      <c r="E88" s="25">
+        <v>1</v>
+      </c>
+      <c r="F88" s="25">
+        <v>5</v>
+      </c>
+      <c r="G88" s="25">
+        <v>0</v>
+      </c>
+      <c r="H88" s="25">
+        <v>1</v>
+      </c>
+      <c r="I88" s="25">
+        <v>109</v>
+      </c>
+      <c r="J88" s="25">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="89" spans="1:10" x14ac:dyDescent="0.3">
+      <c r="A89" s="29">
+        <v>43989</v>
+      </c>
+      <c r="B89" s="30">
+        <v>83316</v>
+      </c>
+      <c r="C89" s="31">
+        <v>211</v>
+      </c>
+      <c r="D89" s="31">
+        <v>1485</v>
+      </c>
+      <c r="E89" s="31">
+        <v>0</v>
+      </c>
+      <c r="F89" s="31">
+        <v>5</v>
+      </c>
+      <c r="G89" s="31">
+        <v>0</v>
+      </c>
+      <c r="H89" s="31">
+        <v>0</v>
+      </c>
+      <c r="I89" s="31">
+        <v>109</v>
+      </c>
+      <c r="J89" s="31">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="90" spans="1:10" x14ac:dyDescent="0.3">
+      <c r="A90" s="20">
+        <v>43990</v>
+      </c>
+      <c r="B90" s="21">
+        <v>84130</v>
+      </c>
+      <c r="C90" s="22">
+        <v>814</v>
+      </c>
+      <c r="D90" s="22">
+        <v>1486</v>
+      </c>
+      <c r="E90" s="22">
+        <v>1</v>
+      </c>
+      <c r="F90" s="22">
+        <v>6</v>
+      </c>
+      <c r="G90" s="22">
+        <v>0</v>
+      </c>
+      <c r="H90" s="22">
+        <v>0</v>
+      </c>
+      <c r="I90" s="22">
+        <v>109</v>
+      </c>
+      <c r="J90" s="22">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="91" spans="1:10" x14ac:dyDescent="0.3">
+      <c r="A91" s="20">
+        <v>43991</v>
+      </c>
+      <c r="B91" s="21">
+        <v>84868</v>
+      </c>
+      <c r="C91" s="22">
+        <v>738</v>
+      </c>
+      <c r="D91" s="22">
+        <v>1488</v>
+      </c>
+      <c r="E91" s="22">
+        <v>2</v>
+      </c>
+      <c r="F91" s="22">
+        <v>6</v>
+      </c>
+      <c r="G91" s="22">
+        <v>0</v>
+      </c>
+      <c r="H91" s="22">
+        <v>0</v>
+      </c>
+      <c r="I91" s="22">
+        <v>109</v>
+      </c>
+      <c r="J91" s="22">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="92" spans="1:10" x14ac:dyDescent="0.3">
+      <c r="A92" s="23">
+        <v>43992</v>
+      </c>
+      <c r="B92" s="24">
+        <v>85626</v>
+      </c>
+      <c r="C92" s="25">
+        <v>758</v>
+      </c>
+      <c r="D92" s="25">
+        <v>1488</v>
+      </c>
+      <c r="E92" s="25">
+        <v>0</v>
+      </c>
+      <c r="F92" s="25">
+        <v>6</v>
+      </c>
+      <c r="G92" s="25">
+        <v>0</v>
+      </c>
+      <c r="H92" s="25">
+        <v>0</v>
+      </c>
+      <c r="I92" s="25">
+        <v>109</v>
+      </c>
+      <c r="J92" s="25">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="93" spans="1:10" x14ac:dyDescent="0.3">
+      <c r="A93" s="29">
+        <v>43993</v>
+      </c>
+      <c r="B93" s="30">
+        <v>86328</v>
+      </c>
+      <c r="C93" s="31">
+        <v>702</v>
+      </c>
+      <c r="D93" s="31">
+        <v>1490</v>
+      </c>
+      <c r="E93" s="31">
+        <v>2</v>
+      </c>
+      <c r="F93" s="31">
+        <v>6</v>
+      </c>
+      <c r="G93" s="31">
+        <v>0</v>
+      </c>
+      <c r="H93" s="31">
+        <v>0</v>
+      </c>
+      <c r="I93" s="31">
+        <v>109</v>
+      </c>
+      <c r="J93" s="31">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="94" spans="1:10" x14ac:dyDescent="0.3">
+      <c r="A94" s="23">
+        <v>43994</v>
+      </c>
+      <c r="B94" s="24">
+        <v>87095</v>
+      </c>
+      <c r="C94" s="25">
+        <v>767</v>
+      </c>
+      <c r="D94" s="25">
+        <v>1492</v>
+      </c>
+      <c r="E94" s="25">
+        <v>2</v>
+      </c>
+      <c r="F94" s="25">
+        <v>6</v>
+      </c>
+      <c r="G94" s="25">
+        <v>0</v>
+      </c>
+      <c r="H94" s="25">
+        <v>0</v>
+      </c>
+      <c r="I94" s="25">
+        <v>109</v>
+      </c>
+      <c r="J94" s="25">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="95" spans="1:10" x14ac:dyDescent="0.3">
+      <c r="A95" s="29">
+        <v>43995</v>
+      </c>
+      <c r="B95" s="30">
+        <v>87386</v>
+      </c>
+      <c r="C95" s="31">
+        <v>291</v>
+      </c>
+      <c r="D95" s="31">
+        <v>1495</v>
+      </c>
+      <c r="E95" s="31">
+        <v>3</v>
+      </c>
+      <c r="F95" s="31">
+        <v>6</v>
+      </c>
+      <c r="G95" s="31">
+        <v>0</v>
+      </c>
+      <c r="H95" s="31">
+        <v>0</v>
+      </c>
+      <c r="I95" s="31">
+        <v>109</v>
+      </c>
+      <c r="J95" s="31">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="96" spans="1:10" x14ac:dyDescent="0.3">
+      <c r="A96" s="23">
+        <v>43996</v>
+      </c>
+      <c r="B96" s="24">
+        <v>87598</v>
+      </c>
+      <c r="C96" s="25">
+        <v>212</v>
+      </c>
+      <c r="D96" s="25">
+        <v>1496</v>
+      </c>
+      <c r="E96" s="25">
+        <v>1</v>
+      </c>
+      <c r="F96" s="25">
+        <v>7</v>
+      </c>
+      <c r="G96" s="25">
+        <v>1</v>
+      </c>
+      <c r="H96" s="25">
+        <v>0</v>
+      </c>
+      <c r="I96" s="25">
+        <v>109</v>
+      </c>
+      <c r="J96" s="25">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="97" spans="1:10" x14ac:dyDescent="0.3">
+      <c r="A97" s="20">
+        <v>43997</v>
+      </c>
+      <c r="B97" s="21">
+        <v>88165</v>
+      </c>
+      <c r="C97" s="22">
+        <v>567</v>
+      </c>
+      <c r="D97" s="22">
+        <v>1499</v>
+      </c>
+      <c r="E97" s="22">
+        <v>3</v>
+      </c>
+      <c r="F97" s="22">
+        <v>7</v>
+      </c>
+      <c r="G97" s="22">
+        <v>1</v>
+      </c>
+      <c r="H97" s="22">
+        <v>0</v>
+      </c>
+      <c r="I97" s="22">
+        <v>109</v>
+      </c>
+      <c r="J97" s="22">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="98" spans="1:10" x14ac:dyDescent="0.3">
+      <c r="A98" s="20">
+        <v>43998</v>
+      </c>
+      <c r="B98" s="21">
+        <v>89151</v>
+      </c>
+      <c r="C98" s="22">
+        <v>986</v>
+      </c>
+      <c r="D98" s="22">
+        <v>1503</v>
+      </c>
+      <c r="E98" s="22">
+        <v>4</v>
+      </c>
+      <c r="F98" s="22">
+        <v>7</v>
+      </c>
+      <c r="G98" s="22">
+        <v>1</v>
+      </c>
+      <c r="H98" s="22">
+        <v>0</v>
+      </c>
+      <c r="I98" s="22">
+        <v>109</v>
+      </c>
+      <c r="J98" s="22">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="99" spans="1:10" x14ac:dyDescent="0.3">
+      <c r="A99" s="29">
+        <v>43999</v>
+      </c>
+      <c r="B99" s="30">
+        <v>90103</v>
+      </c>
+      <c r="C99" s="31">
+        <v>952</v>
+      </c>
+      <c r="D99" s="31">
+        <v>1511</v>
+      </c>
+      <c r="E99" s="31">
+        <v>8</v>
+      </c>
+      <c r="F99" s="31">
+        <v>6</v>
+      </c>
+      <c r="G99" s="31">
+        <v>1</v>
+      </c>
+      <c r="H99" s="31">
+        <v>1</v>
+      </c>
+      <c r="I99" s="31">
+        <v>109</v>
+      </c>
+      <c r="J99" s="31">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="100" spans="1:10" x14ac:dyDescent="0.3">
+      <c r="A100" s="20">
+        <v>44000</v>
+      </c>
+      <c r="B100" s="21">
+        <v>91005</v>
+      </c>
+      <c r="C100" s="22">
+        <v>902</v>
+      </c>
+      <c r="D100" s="22">
+        <v>1513</v>
+      </c>
+      <c r="E100" s="22">
+        <v>2</v>
+      </c>
+      <c r="F100" s="22">
+        <v>8</v>
+      </c>
+      <c r="G100" s="22">
+        <v>1</v>
+      </c>
+      <c r="H100" s="22">
+        <v>0</v>
+      </c>
+      <c r="I100" s="22">
+        <v>109</v>
+      </c>
+      <c r="J100" s="22">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="101" spans="1:10" x14ac:dyDescent="0.3">
+      <c r="A101" s="29">
+        <v>44001</v>
+      </c>
+      <c r="B101" s="30">
+        <v>92152</v>
+      </c>
+      <c r="C101" s="31">
+        <v>1147</v>
+      </c>
+      <c r="D101" s="31">
+        <v>1519</v>
+      </c>
+      <c r="E101" s="31">
+        <v>6</v>
+      </c>
+      <c r="F101" s="31">
+        <v>6</v>
+      </c>
+      <c r="G101" s="31">
+        <v>1</v>
+      </c>
+      <c r="H101" s="31">
+        <v>2</v>
+      </c>
+      <c r="I101" s="31">
+        <v>109</v>
+      </c>
+      <c r="J101" s="31">
         <v>0</v>
       </c>
     </row>

</xml_diff>

<commit_message>
Data updated by GitHub Bot (2020-06-20 20)
</commit_message>
<xml_diff>
--- a/output/snapshot/fdcf2531-4c3e-5c02-b63c-ee160ead6dea.xlsx
+++ b/output/snapshot/fdcf2531-4c3e-5c02-b63c-ee160ead6dea.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="I:\AKTUALNI PODATKI - KORONA\Za objavo na GOV.SI\ang\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{1E6DD62F-2BE2-47DC-A7ED-9B57C1589256}" xr6:coauthVersionLast="44" xr6:coauthVersionMax="44" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{9EE09CBD-7DAA-4C74-9BA3-7F1963AA8E06}" xr6:coauthVersionLast="44" xr6:coauthVersionMax="44" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12576" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Covid-19 podatki" sheetId="1" r:id="rId1"/>
@@ -64,7 +64,7 @@
   <numFmts count="1">
     <numFmt numFmtId="164" formatCode="d/\ m/\ yyyy;@"/>
   </numFmts>
-  <fonts count="4" x14ac:knownFonts="1">
+  <fonts count="5" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -93,6 +93,13 @@
       <name val="Calibri Light"/>
       <scheme val="major"/>
     </font>
+    <font>
+      <sz val="10"/>
+      <color theme="1"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
   </fonts>
   <fills count="3">
     <fill>
@@ -108,7 +115,7 @@
       </patternFill>
     </fill>
   </fills>
-  <borders count="2">
+  <borders count="3">
     <border>
       <left/>
       <right/>
@@ -129,11 +136,26 @@
       <bottom/>
       <diagonal/>
     </border>
+    <border>
+      <left style="thin">
+        <color theme="4"/>
+      </left>
+      <right style="thin">
+        <color theme="4"/>
+      </right>
+      <top style="thin">
+        <color theme="4"/>
+      </top>
+      <bottom style="thin">
+        <color theme="4"/>
+      </bottom>
+      <diagonal/>
+    </border>
   </borders>
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="26">
+  <cellXfs count="32">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="49" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyAlignment="1" applyProtection="1">
       <alignment horizontal="left" vertical="top"/>
@@ -208,6 +230,24 @@
       <alignment horizontal="right"/>
     </xf>
     <xf numFmtId="0" fontId="3" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="right"/>
+    </xf>
+    <xf numFmtId="164" fontId="4" fillId="2" borderId="2" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="right" vertical="top"/>
+    </xf>
+    <xf numFmtId="3" fontId="4" fillId="2" borderId="2" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="right"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="2" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="right"/>
+    </xf>
+    <xf numFmtId="164" fontId="3" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="right" vertical="top"/>
+    </xf>
+    <xf numFmtId="3" fontId="3" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="right"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="right"/>
     </xf>
   </cellXfs>
@@ -399,8 +439,8 @@
 </file>
 
 <file path=xl/tables/table1.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="1" xr:uid="{00000000-000C-0000-FFFF-FFFF00000000}" name="Tabela1" displayName="Tabela1" ref="A1:J75" totalsRowShown="0" headerRowDxfId="11" dataDxfId="10">
-  <autoFilter ref="A1:J75" xr:uid="{00000000-0009-0000-0100-000001000000}">
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="1" xr:uid="{00000000-000C-0000-FFFF-FFFF00000000}" name="Tabela1" displayName="Tabela1" ref="A1:J101" totalsRowShown="0" headerRowDxfId="11" dataDxfId="10">
+  <autoFilter ref="A1:J101" xr:uid="{00000000-0009-0000-0100-000001000000}">
     <filterColumn colId="0" hiddenButton="1"/>
     <filterColumn colId="1" hiddenButton="1"/>
     <filterColumn colId="2" hiddenButton="1"/>
@@ -696,28 +736,28 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:J75"/>
+  <dimension ref="A1:J101"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A40" zoomScale="89" zoomScaleNormal="89" workbookViewId="0">
-      <selection activeCell="J74" sqref="J74"/>
+    <sheetView tabSelected="1" topLeftCell="A77" zoomScale="89" zoomScaleNormal="89" workbookViewId="0">
+      <selection activeCell="A101" sqref="A101:J101"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
-    <col min="1" max="1" width="12.7109375" style="1" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="13.5703125" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="16.28515625" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="15.28515625" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="17.85546875" bestFit="1" customWidth="1"/>
-    <col min="6" max="6" width="35.42578125" bestFit="1" customWidth="1"/>
-    <col min="7" max="7" width="51.140625" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="12.6640625" style="1" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="13.5546875" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="16.33203125" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="15.33203125" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="17.88671875" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="35.44140625" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="51.109375" bestFit="1" customWidth="1"/>
     <col min="8" max="8" width="14" bestFit="1" customWidth="1"/>
-    <col min="9" max="9" width="13.85546875" bestFit="1" customWidth="1"/>
-    <col min="10" max="10" width="16.5703125" bestFit="1" customWidth="1"/>
+    <col min="9" max="9" width="13.88671875" bestFit="1" customWidth="1"/>
+    <col min="10" max="10" width="16.5546875" bestFit="1" customWidth="1"/>
     <col min="11" max="11" width="29" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A1" s="2" t="s">
         <v>0</v>
       </c>
@@ -749,7 +789,7 @@
         <v>9</v>
       </c>
     </row>
-    <row r="2" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A2" s="4">
         <v>43902</v>
       </c>
@@ -781,7 +821,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="3" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A3" s="4">
         <v>43903</v>
       </c>
@@ -813,7 +853,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="4" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A4" s="4">
         <v>43904</v>
       </c>
@@ -845,7 +885,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="5" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A5" s="4">
         <v>43905</v>
       </c>
@@ -877,7 +917,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="6" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A6" s="4">
         <v>43906</v>
       </c>
@@ -909,7 +949,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="7" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A7" s="4">
         <v>43907</v>
       </c>
@@ -941,7 +981,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="8" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A8" s="4">
         <v>43908</v>
       </c>
@@ -973,7 +1013,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="9" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A9" s="4">
         <v>43909</v>
       </c>
@@ -1005,7 +1045,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="10" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="10" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A10" s="4">
         <v>43910</v>
       </c>
@@ -1037,7 +1077,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="11" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="11" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A11" s="4">
         <v>43911</v>
       </c>
@@ -1069,7 +1109,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="12" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="12" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A12" s="4">
         <v>43912</v>
       </c>
@@ -1101,7 +1141,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="13" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="13" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A13" s="4">
         <v>43913</v>
       </c>
@@ -1133,7 +1173,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="14" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="14" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A14" s="4">
         <v>43914</v>
       </c>
@@ -1165,7 +1205,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="15" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="15" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A15" s="4">
         <v>43915</v>
       </c>
@@ -1197,7 +1237,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="16" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="16" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A16" s="4">
         <v>43916</v>
       </c>
@@ -1229,7 +1269,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="17" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="17" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A17" s="6">
         <v>43917</v>
       </c>
@@ -1261,7 +1301,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="18" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="18" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A18" s="4">
         <v>43918</v>
       </c>
@@ -1293,7 +1333,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="19" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="19" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A19" s="4">
         <v>43919</v>
       </c>
@@ -1325,7 +1365,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="20" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="20" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A20" s="4">
         <v>43920</v>
       </c>
@@ -1357,7 +1397,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="21" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="21" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A21" s="4">
         <v>43921</v>
       </c>
@@ -1389,7 +1429,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="22" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="22" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A22" s="4">
         <v>43922</v>
       </c>
@@ -1421,7 +1461,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="23" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="23" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A23" s="4">
         <v>43923</v>
       </c>
@@ -1453,7 +1493,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="24" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="24" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A24" s="4">
         <v>43924</v>
       </c>
@@ -1485,7 +1525,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="25" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="25" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A25" s="4">
         <v>43925</v>
       </c>
@@ -1517,7 +1557,7 @@
         <v>6</v>
       </c>
     </row>
-    <row r="26" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="26" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A26" s="4">
         <v>43926</v>
       </c>
@@ -1549,7 +1589,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="27" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="27" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A27" s="4">
         <v>43927</v>
       </c>
@@ -1581,7 +1621,7 @@
         <v>6</v>
       </c>
     </row>
-    <row r="28" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="28" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A28" s="8">
         <v>43928</v>
       </c>
@@ -1613,7 +1653,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="29" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="29" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A29" s="4">
         <v>43929</v>
       </c>
@@ -1645,7 +1685,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="30" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="30" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A30" s="4">
         <v>43930</v>
       </c>
@@ -1677,7 +1717,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="31" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="31" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A31" s="4">
         <v>43931</v>
       </c>
@@ -1709,7 +1749,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="32" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="32" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A32" s="4">
         <v>43932</v>
       </c>
@@ -1741,7 +1781,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="33" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="33" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A33" s="4">
         <v>43933</v>
       </c>
@@ -1773,7 +1813,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="34" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="34" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A34" s="4">
         <v>43934</v>
       </c>
@@ -1805,7 +1845,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="35" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="35" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A35" s="4">
         <v>43935</v>
       </c>
@@ -1837,7 +1877,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="36" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="36" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A36" s="4">
         <v>43936</v>
       </c>
@@ -1869,7 +1909,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="37" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="37" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A37" s="4">
         <v>43937</v>
       </c>
@@ -1901,7 +1941,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="38" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="38" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A38" s="4">
         <v>43938</v>
       </c>
@@ -1933,7 +1973,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="39" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="39" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A39" s="4">
         <v>43939</v>
       </c>
@@ -1965,7 +2005,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="40" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="40" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A40" s="4">
         <v>43940</v>
       </c>
@@ -1997,7 +2037,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="41" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="41" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A41" s="4">
         <v>43941</v>
       </c>
@@ -2029,7 +2069,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="42" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="42" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A42" s="11">
         <v>43942</v>
       </c>
@@ -2061,7 +2101,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="43" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="43" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A43" s="4">
         <v>43943</v>
       </c>
@@ -2093,7 +2133,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="44" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="44" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A44" s="4">
         <v>43944</v>
       </c>
@@ -2125,7 +2165,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="45" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="45" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A45" s="4">
         <v>43945</v>
       </c>
@@ -2157,7 +2197,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="46" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="46" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A46" s="4">
         <v>43946</v>
       </c>
@@ -2189,7 +2229,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="47" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="47" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A47" s="8">
         <v>43947</v>
       </c>
@@ -2221,7 +2261,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="48" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="48" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A48" s="4">
         <v>43948</v>
       </c>
@@ -2253,7 +2293,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="49" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="49" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A49" s="4">
         <v>43949</v>
       </c>
@@ -2285,7 +2325,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="50" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="50" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A50" s="4">
         <v>43950</v>
       </c>
@@ -2317,7 +2357,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="51" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="51" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A51" s="14">
         <v>43951</v>
       </c>
@@ -2349,7 +2389,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="52" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="52" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A52" s="4">
         <v>43952</v>
       </c>
@@ -2381,7 +2421,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="53" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="53" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A53" s="4">
         <v>43953</v>
       </c>
@@ -2413,7 +2453,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="54" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="54" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A54" s="11">
         <v>43954</v>
       </c>
@@ -2445,7 +2485,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="55" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="55" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A55" s="4">
         <v>43955</v>
       </c>
@@ -2477,7 +2517,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="56" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="56" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A56" s="11">
         <v>43956</v>
       </c>
@@ -2509,7 +2549,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="57" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="57" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A57" s="4">
         <v>43957</v>
       </c>
@@ -2541,7 +2581,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="58" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="58" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A58" s="4">
         <v>43958</v>
       </c>
@@ -2573,7 +2613,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="59" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="59" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A59" s="4">
         <v>43959</v>
       </c>
@@ -2605,7 +2645,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="60" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="60" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A60" s="4">
         <v>43960</v>
       </c>
@@ -2637,7 +2677,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="61" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="61" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A61" s="4">
         <v>43961</v>
       </c>
@@ -2669,7 +2709,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="62" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="62" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A62" s="4">
         <v>43962</v>
       </c>
@@ -2701,7 +2741,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="63" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="63" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A63" s="4">
         <v>43963</v>
       </c>
@@ -2733,7 +2773,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="64" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="64" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A64" s="17">
         <v>43964</v>
       </c>
@@ -2765,7 +2805,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="65" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="65" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A65" s="14">
         <v>43965</v>
       </c>
@@ -2797,7 +2837,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="66" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="66" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A66" s="11">
         <v>43966</v>
       </c>
@@ -2829,7 +2869,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="67" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="67" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A67" s="14">
         <v>43967</v>
       </c>
@@ -2861,7 +2901,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="68" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="68" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A68" s="11">
         <v>43968</v>
       </c>
@@ -2893,7 +2933,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="69" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="69" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A69" s="14">
         <v>43969</v>
       </c>
@@ -2925,7 +2965,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="70" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="70" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A70" s="11">
         <v>43970</v>
       </c>
@@ -2957,7 +2997,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="71" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="71" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A71" s="20">
         <v>43971</v>
       </c>
@@ -2989,7 +3029,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="72" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="72" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A72" s="23">
         <v>43972</v>
       </c>
@@ -3021,7 +3061,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="73" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="73" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A73" s="20">
         <v>43973</v>
       </c>
@@ -3053,7 +3093,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="74" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="74" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A74" s="17">
         <v>43974</v>
       </c>
@@ -3085,7 +3125,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="75" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="75" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A75" s="20">
         <v>43975</v>
       </c>
@@ -3114,6 +3154,838 @@
         <v>107</v>
       </c>
       <c r="J75" s="22">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="76" spans="1:10" x14ac:dyDescent="0.3">
+      <c r="A76" s="20">
+        <v>43976</v>
+      </c>
+      <c r="B76" s="21">
+        <v>75770</v>
+      </c>
+      <c r="C76" s="22">
+        <v>754</v>
+      </c>
+      <c r="D76" s="22">
+        <v>1469</v>
+      </c>
+      <c r="E76" s="22">
+        <v>0</v>
+      </c>
+      <c r="F76" s="22">
+        <v>9</v>
+      </c>
+      <c r="G76" s="22">
+        <v>2</v>
+      </c>
+      <c r="H76" s="22">
+        <v>6</v>
+      </c>
+      <c r="I76" s="22">
+        <v>108</v>
+      </c>
+      <c r="J76" s="22">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="77" spans="1:10" x14ac:dyDescent="0.3">
+      <c r="A77" s="20">
+        <v>43977</v>
+      </c>
+      <c r="B77" s="21">
+        <v>76579</v>
+      </c>
+      <c r="C77" s="22">
+        <v>809</v>
+      </c>
+      <c r="D77" s="22">
+        <v>1471</v>
+      </c>
+      <c r="E77" s="22">
+        <v>2</v>
+      </c>
+      <c r="F77" s="22">
+        <v>8</v>
+      </c>
+      <c r="G77" s="22">
+        <v>2</v>
+      </c>
+      <c r="H77" s="22">
+        <v>2</v>
+      </c>
+      <c r="I77" s="22">
+        <v>108</v>
+      </c>
+      <c r="J77" s="22">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="78" spans="1:10" x14ac:dyDescent="0.3">
+      <c r="A78" s="20">
+        <v>43978</v>
+      </c>
+      <c r="B78" s="21">
+        <v>77210</v>
+      </c>
+      <c r="C78" s="22">
+        <v>631</v>
+      </c>
+      <c r="D78" s="22">
+        <v>1473</v>
+      </c>
+      <c r="E78" s="22">
+        <v>2</v>
+      </c>
+      <c r="F78" s="22">
+        <v>7</v>
+      </c>
+      <c r="G78" s="22">
+        <v>2</v>
+      </c>
+      <c r="H78" s="22">
+        <v>1</v>
+      </c>
+      <c r="I78" s="22">
+        <v>108</v>
+      </c>
+      <c r="J78" s="22">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="79" spans="1:10" x14ac:dyDescent="0.3">
+      <c r="A79" s="20">
+        <v>43979</v>
+      </c>
+      <c r="B79" s="21">
+        <v>77916</v>
+      </c>
+      <c r="C79" s="22">
+        <v>706</v>
+      </c>
+      <c r="D79" s="22">
+        <v>1473</v>
+      </c>
+      <c r="E79" s="22">
+        <v>0</v>
+      </c>
+      <c r="F79" s="22">
+        <v>7</v>
+      </c>
+      <c r="G79" s="22">
+        <v>2</v>
+      </c>
+      <c r="H79" s="22">
+        <v>0</v>
+      </c>
+      <c r="I79" s="22">
+        <v>108</v>
+      </c>
+      <c r="J79" s="22">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="80" spans="1:10" x14ac:dyDescent="0.3">
+      <c r="A80" s="20">
+        <v>43980</v>
+      </c>
+      <c r="B80" s="21">
+        <v>78529</v>
+      </c>
+      <c r="C80" s="22">
+        <v>613</v>
+      </c>
+      <c r="D80" s="22">
+        <v>1473</v>
+      </c>
+      <c r="E80" s="22">
+        <v>0</v>
+      </c>
+      <c r="F80" s="22">
+        <v>7</v>
+      </c>
+      <c r="G80" s="22">
+        <v>2</v>
+      </c>
+      <c r="H80" s="22">
+        <v>0</v>
+      </c>
+      <c r="I80" s="22">
+        <v>108</v>
+      </c>
+      <c r="J80" s="22">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="81" spans="1:10" x14ac:dyDescent="0.3">
+      <c r="A81" s="20">
+        <v>43981</v>
+      </c>
+      <c r="B81" s="22">
+        <v>78793</v>
+      </c>
+      <c r="C81" s="22">
+        <v>264</v>
+      </c>
+      <c r="D81" s="22">
+        <v>1473</v>
+      </c>
+      <c r="E81" s="22">
+        <v>0</v>
+      </c>
+      <c r="F81" s="22">
+        <v>6</v>
+      </c>
+      <c r="G81" s="22">
+        <v>2</v>
+      </c>
+      <c r="H81" s="22">
+        <v>1</v>
+      </c>
+      <c r="I81" s="22">
+        <v>108</v>
+      </c>
+      <c r="J81" s="22">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="82" spans="1:10" x14ac:dyDescent="0.3">
+      <c r="A82" s="20">
+        <v>43982</v>
+      </c>
+      <c r="B82" s="21">
+        <v>79039</v>
+      </c>
+      <c r="C82" s="22">
+        <v>246</v>
+      </c>
+      <c r="D82" s="22">
+        <v>1473</v>
+      </c>
+      <c r="E82" s="22">
+        <v>0</v>
+      </c>
+      <c r="F82" s="22">
+        <v>5</v>
+      </c>
+      <c r="G82" s="22">
+        <v>1</v>
+      </c>
+      <c r="H82" s="22">
+        <v>0</v>
+      </c>
+      <c r="I82" s="22">
+        <v>109</v>
+      </c>
+      <c r="J82" s="22">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="83" spans="1:10" x14ac:dyDescent="0.3">
+      <c r="A83" s="20">
+        <v>43983</v>
+      </c>
+      <c r="B83" s="21">
+        <v>79698</v>
+      </c>
+      <c r="C83" s="22">
+        <v>659</v>
+      </c>
+      <c r="D83" s="22">
+        <v>1475</v>
+      </c>
+      <c r="E83" s="22">
+        <v>2</v>
+      </c>
+      <c r="F83" s="22">
+        <v>5</v>
+      </c>
+      <c r="G83" s="22">
+        <v>1</v>
+      </c>
+      <c r="H83" s="22">
+        <v>0</v>
+      </c>
+      <c r="I83" s="22">
+        <v>109</v>
+      </c>
+      <c r="J83" s="22">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="84" spans="1:10" x14ac:dyDescent="0.3">
+      <c r="A84" s="20">
+        <v>43984</v>
+      </c>
+      <c r="B84" s="21">
+        <v>80505</v>
+      </c>
+      <c r="C84" s="22">
+        <v>807</v>
+      </c>
+      <c r="D84" s="22">
+        <v>1477</v>
+      </c>
+      <c r="E84" s="22">
+        <v>2</v>
+      </c>
+      <c r="F84" s="22">
+        <v>5</v>
+      </c>
+      <c r="G84" s="22">
+        <v>0</v>
+      </c>
+      <c r="H84" s="22">
+        <v>0</v>
+      </c>
+      <c r="I84" s="22">
+        <v>109</v>
+      </c>
+      <c r="J84" s="22">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="85" spans="1:10" x14ac:dyDescent="0.3">
+      <c r="A85" s="20">
+        <v>43985</v>
+      </c>
+      <c r="B85" s="21">
+        <v>81333</v>
+      </c>
+      <c r="C85" s="22">
+        <v>828</v>
+      </c>
+      <c r="D85" s="22">
+        <v>1477</v>
+      </c>
+      <c r="E85" s="22">
+        <v>0</v>
+      </c>
+      <c r="F85" s="22">
+        <v>5</v>
+      </c>
+      <c r="G85" s="22">
+        <v>0</v>
+      </c>
+      <c r="H85" s="22">
+        <v>0</v>
+      </c>
+      <c r="I85" s="22">
+        <v>109</v>
+      </c>
+      <c r="J85" s="22">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="86" spans="1:10" x14ac:dyDescent="0.3">
+      <c r="A86" s="26">
+        <v>43986</v>
+      </c>
+      <c r="B86" s="27">
+        <v>82161</v>
+      </c>
+      <c r="C86" s="28">
+        <v>828</v>
+      </c>
+      <c r="D86" s="28">
+        <v>1479</v>
+      </c>
+      <c r="E86" s="28">
+        <v>2</v>
+      </c>
+      <c r="F86" s="28">
+        <v>6</v>
+      </c>
+      <c r="G86" s="28">
+        <v>0</v>
+      </c>
+      <c r="H86" s="28">
+        <v>0</v>
+      </c>
+      <c r="I86" s="28">
+        <v>109</v>
+      </c>
+      <c r="J86" s="28">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="87" spans="1:10" x14ac:dyDescent="0.3">
+      <c r="A87" s="29">
+        <v>43987</v>
+      </c>
+      <c r="B87" s="30">
+        <v>82876</v>
+      </c>
+      <c r="C87" s="31">
+        <v>715</v>
+      </c>
+      <c r="D87" s="31">
+        <v>1484</v>
+      </c>
+      <c r="E87" s="31">
+        <v>5</v>
+      </c>
+      <c r="F87" s="31">
+        <v>6</v>
+      </c>
+      <c r="G87" s="31">
+        <v>0</v>
+      </c>
+      <c r="H87" s="31">
+        <v>0</v>
+      </c>
+      <c r="I87" s="31">
+        <v>109</v>
+      </c>
+      <c r="J87" s="31">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="88" spans="1:10" x14ac:dyDescent="0.3">
+      <c r="A88" s="23">
+        <v>43988</v>
+      </c>
+      <c r="B88" s="24">
+        <v>83105</v>
+      </c>
+      <c r="C88" s="25">
+        <v>229</v>
+      </c>
+      <c r="D88" s="25">
+        <v>1485</v>
+      </c>
+      <c r="E88" s="25">
+        <v>1</v>
+      </c>
+      <c r="F88" s="25">
+        <v>5</v>
+      </c>
+      <c r="G88" s="25">
+        <v>0</v>
+      </c>
+      <c r="H88" s="25">
+        <v>1</v>
+      </c>
+      <c r="I88" s="25">
+        <v>109</v>
+      </c>
+      <c r="J88" s="25">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="89" spans="1:10" x14ac:dyDescent="0.3">
+      <c r="A89" s="29">
+        <v>43989</v>
+      </c>
+      <c r="B89" s="30">
+        <v>83316</v>
+      </c>
+      <c r="C89" s="31">
+        <v>211</v>
+      </c>
+      <c r="D89" s="31">
+        <v>1485</v>
+      </c>
+      <c r="E89" s="31">
+        <v>0</v>
+      </c>
+      <c r="F89" s="31">
+        <v>5</v>
+      </c>
+      <c r="G89" s="31">
+        <v>0</v>
+      </c>
+      <c r="H89" s="31">
+        <v>0</v>
+      </c>
+      <c r="I89" s="31">
+        <v>109</v>
+      </c>
+      <c r="J89" s="31">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="90" spans="1:10" x14ac:dyDescent="0.3">
+      <c r="A90" s="20">
+        <v>43990</v>
+      </c>
+      <c r="B90" s="21">
+        <v>84130</v>
+      </c>
+      <c r="C90" s="22">
+        <v>814</v>
+      </c>
+      <c r="D90" s="22">
+        <v>1486</v>
+      </c>
+      <c r="E90" s="22">
+        <v>1</v>
+      </c>
+      <c r="F90" s="22">
+        <v>6</v>
+      </c>
+      <c r="G90" s="22">
+        <v>0</v>
+      </c>
+      <c r="H90" s="22">
+        <v>0</v>
+      </c>
+      <c r="I90" s="22">
+        <v>109</v>
+      </c>
+      <c r="J90" s="22">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="91" spans="1:10" x14ac:dyDescent="0.3">
+      <c r="A91" s="20">
+        <v>43991</v>
+      </c>
+      <c r="B91" s="21">
+        <v>84868</v>
+      </c>
+      <c r="C91" s="22">
+        <v>738</v>
+      </c>
+      <c r="D91" s="22">
+        <v>1488</v>
+      </c>
+      <c r="E91" s="22">
+        <v>2</v>
+      </c>
+      <c r="F91" s="22">
+        <v>6</v>
+      </c>
+      <c r="G91" s="22">
+        <v>0</v>
+      </c>
+      <c r="H91" s="22">
+        <v>0</v>
+      </c>
+      <c r="I91" s="22">
+        <v>109</v>
+      </c>
+      <c r="J91" s="22">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="92" spans="1:10" x14ac:dyDescent="0.3">
+      <c r="A92" s="23">
+        <v>43992</v>
+      </c>
+      <c r="B92" s="24">
+        <v>85626</v>
+      </c>
+      <c r="C92" s="25">
+        <v>758</v>
+      </c>
+      <c r="D92" s="25">
+        <v>1488</v>
+      </c>
+      <c r="E92" s="25">
+        <v>0</v>
+      </c>
+      <c r="F92" s="25">
+        <v>6</v>
+      </c>
+      <c r="G92" s="25">
+        <v>0</v>
+      </c>
+      <c r="H92" s="25">
+        <v>0</v>
+      </c>
+      <c r="I92" s="25">
+        <v>109</v>
+      </c>
+      <c r="J92" s="25">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="93" spans="1:10" x14ac:dyDescent="0.3">
+      <c r="A93" s="29">
+        <v>43993</v>
+      </c>
+      <c r="B93" s="30">
+        <v>86328</v>
+      </c>
+      <c r="C93" s="31">
+        <v>702</v>
+      </c>
+      <c r="D93" s="31">
+        <v>1490</v>
+      </c>
+      <c r="E93" s="31">
+        <v>2</v>
+      </c>
+      <c r="F93" s="31">
+        <v>6</v>
+      </c>
+      <c r="G93" s="31">
+        <v>0</v>
+      </c>
+      <c r="H93" s="31">
+        <v>0</v>
+      </c>
+      <c r="I93" s="31">
+        <v>109</v>
+      </c>
+      <c r="J93" s="31">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="94" spans="1:10" x14ac:dyDescent="0.3">
+      <c r="A94" s="23">
+        <v>43994</v>
+      </c>
+      <c r="B94" s="24">
+        <v>87095</v>
+      </c>
+      <c r="C94" s="25">
+        <v>767</v>
+      </c>
+      <c r="D94" s="25">
+        <v>1492</v>
+      </c>
+      <c r="E94" s="25">
+        <v>2</v>
+      </c>
+      <c r="F94" s="25">
+        <v>6</v>
+      </c>
+      <c r="G94" s="25">
+        <v>0</v>
+      </c>
+      <c r="H94" s="25">
+        <v>0</v>
+      </c>
+      <c r="I94" s="25">
+        <v>109</v>
+      </c>
+      <c r="J94" s="25">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="95" spans="1:10" x14ac:dyDescent="0.3">
+      <c r="A95" s="29">
+        <v>43995</v>
+      </c>
+      <c r="B95" s="30">
+        <v>87386</v>
+      </c>
+      <c r="C95" s="31">
+        <v>291</v>
+      </c>
+      <c r="D95" s="31">
+        <v>1495</v>
+      </c>
+      <c r="E95" s="31">
+        <v>3</v>
+      </c>
+      <c r="F95" s="31">
+        <v>6</v>
+      </c>
+      <c r="G95" s="31">
+        <v>0</v>
+      </c>
+      <c r="H95" s="31">
+        <v>0</v>
+      </c>
+      <c r="I95" s="31">
+        <v>109</v>
+      </c>
+      <c r="J95" s="31">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="96" spans="1:10" x14ac:dyDescent="0.3">
+      <c r="A96" s="23">
+        <v>43996</v>
+      </c>
+      <c r="B96" s="24">
+        <v>87598</v>
+      </c>
+      <c r="C96" s="25">
+        <v>212</v>
+      </c>
+      <c r="D96" s="25">
+        <v>1496</v>
+      </c>
+      <c r="E96" s="25">
+        <v>1</v>
+      </c>
+      <c r="F96" s="25">
+        <v>7</v>
+      </c>
+      <c r="G96" s="25">
+        <v>1</v>
+      </c>
+      <c r="H96" s="25">
+        <v>0</v>
+      </c>
+      <c r="I96" s="25">
+        <v>109</v>
+      </c>
+      <c r="J96" s="25">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="97" spans="1:10" x14ac:dyDescent="0.3">
+      <c r="A97" s="20">
+        <v>43997</v>
+      </c>
+      <c r="B97" s="21">
+        <v>88165</v>
+      </c>
+      <c r="C97" s="22">
+        <v>567</v>
+      </c>
+      <c r="D97" s="22">
+        <v>1499</v>
+      </c>
+      <c r="E97" s="22">
+        <v>3</v>
+      </c>
+      <c r="F97" s="22">
+        <v>7</v>
+      </c>
+      <c r="G97" s="22">
+        <v>1</v>
+      </c>
+      <c r="H97" s="22">
+        <v>0</v>
+      </c>
+      <c r="I97" s="22">
+        <v>109</v>
+      </c>
+      <c r="J97" s="22">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="98" spans="1:10" x14ac:dyDescent="0.3">
+      <c r="A98" s="20">
+        <v>43998</v>
+      </c>
+      <c r="B98" s="21">
+        <v>89151</v>
+      </c>
+      <c r="C98" s="22">
+        <v>986</v>
+      </c>
+      <c r="D98" s="22">
+        <v>1503</v>
+      </c>
+      <c r="E98" s="22">
+        <v>4</v>
+      </c>
+      <c r="F98" s="22">
+        <v>7</v>
+      </c>
+      <c r="G98" s="22">
+        <v>1</v>
+      </c>
+      <c r="H98" s="22">
+        <v>0</v>
+      </c>
+      <c r="I98" s="22">
+        <v>109</v>
+      </c>
+      <c r="J98" s="22">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="99" spans="1:10" x14ac:dyDescent="0.3">
+      <c r="A99" s="29">
+        <v>43999</v>
+      </c>
+      <c r="B99" s="30">
+        <v>90103</v>
+      </c>
+      <c r="C99" s="31">
+        <v>952</v>
+      </c>
+      <c r="D99" s="31">
+        <v>1511</v>
+      </c>
+      <c r="E99" s="31">
+        <v>8</v>
+      </c>
+      <c r="F99" s="31">
+        <v>6</v>
+      </c>
+      <c r="G99" s="31">
+        <v>1</v>
+      </c>
+      <c r="H99" s="31">
+        <v>1</v>
+      </c>
+      <c r="I99" s="31">
+        <v>109</v>
+      </c>
+      <c r="J99" s="31">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="100" spans="1:10" x14ac:dyDescent="0.3">
+      <c r="A100" s="20">
+        <v>44000</v>
+      </c>
+      <c r="B100" s="21">
+        <v>91005</v>
+      </c>
+      <c r="C100" s="22">
+        <v>902</v>
+      </c>
+      <c r="D100" s="22">
+        <v>1513</v>
+      </c>
+      <c r="E100" s="22">
+        <v>2</v>
+      </c>
+      <c r="F100" s="22">
+        <v>8</v>
+      </c>
+      <c r="G100" s="22">
+        <v>1</v>
+      </c>
+      <c r="H100" s="22">
+        <v>0</v>
+      </c>
+      <c r="I100" s="22">
+        <v>109</v>
+      </c>
+      <c r="J100" s="22">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="101" spans="1:10" x14ac:dyDescent="0.3">
+      <c r="A101" s="29">
+        <v>44001</v>
+      </c>
+      <c r="B101" s="30">
+        <v>92152</v>
+      </c>
+      <c r="C101" s="31">
+        <v>1147</v>
+      </c>
+      <c r="D101" s="31">
+        <v>1519</v>
+      </c>
+      <c r="E101" s="31">
+        <v>6</v>
+      </c>
+      <c r="F101" s="31">
+        <v>6</v>
+      </c>
+      <c r="G101" s="31">
+        <v>1</v>
+      </c>
+      <c r="H101" s="31">
+        <v>2</v>
+      </c>
+      <c r="I101" s="31">
+        <v>109</v>
+      </c>
+      <c r="J101" s="31">
         <v>0</v>
       </c>
     </row>

</xml_diff>

<commit_message>
Data updated by GitHub Bot (2020-06-21 12)
</commit_message>
<xml_diff>
--- a/output/snapshot/fdcf2531-4c3e-5c02-b63c-ee160ead6dea.xlsx
+++ b/output/snapshot/fdcf2531-4c3e-5c02-b63c-ee160ead6dea.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="I:\AKTUALNI PODATKI - KORONA\Za objavo na GOV.SI\ang\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{1E6DD62F-2BE2-47DC-A7ED-9B57C1589256}" xr6:coauthVersionLast="44" xr6:coauthVersionMax="44" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{9006D0F7-09D7-4EC0-A0E3-11905E8C747A}" xr6:coauthVersionLast="44" xr6:coauthVersionMax="44" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -64,7 +64,7 @@
   <numFmts count="1">
     <numFmt numFmtId="164" formatCode="d/\ m/\ yyyy;@"/>
   </numFmts>
-  <fonts count="4" x14ac:knownFonts="1">
+  <fonts count="5" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -93,6 +93,13 @@
       <name val="Calibri Light"/>
       <scheme val="major"/>
     </font>
+    <font>
+      <sz val="10"/>
+      <color theme="1"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
   </fonts>
   <fills count="3">
     <fill>
@@ -108,7 +115,7 @@
       </patternFill>
     </fill>
   </fills>
-  <borders count="2">
+  <borders count="3">
     <border>
       <left/>
       <right/>
@@ -129,11 +136,26 @@
       <bottom/>
       <diagonal/>
     </border>
+    <border>
+      <left style="thin">
+        <color theme="4"/>
+      </left>
+      <right style="thin">
+        <color theme="4"/>
+      </right>
+      <top style="thin">
+        <color theme="4"/>
+      </top>
+      <bottom style="thin">
+        <color theme="4"/>
+      </bottom>
+      <diagonal/>
+    </border>
   </borders>
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="26">
+  <cellXfs count="32">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="49" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyAlignment="1" applyProtection="1">
       <alignment horizontal="left" vertical="top"/>
@@ -208,6 +230,24 @@
       <alignment horizontal="right"/>
     </xf>
     <xf numFmtId="0" fontId="3" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="right"/>
+    </xf>
+    <xf numFmtId="164" fontId="4" fillId="2" borderId="2" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="right" vertical="top"/>
+    </xf>
+    <xf numFmtId="3" fontId="4" fillId="2" borderId="2" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="right"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="2" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="right"/>
+    </xf>
+    <xf numFmtId="164" fontId="3" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="right" vertical="top"/>
+    </xf>
+    <xf numFmtId="3" fontId="3" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="right"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="right"/>
     </xf>
   </cellXfs>
@@ -399,8 +439,8 @@
 </file>
 
 <file path=xl/tables/table1.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="1" xr:uid="{00000000-000C-0000-FFFF-FFFF00000000}" name="Tabela1" displayName="Tabela1" ref="A1:J75" totalsRowShown="0" headerRowDxfId="11" dataDxfId="10">
-  <autoFilter ref="A1:J75" xr:uid="{00000000-0009-0000-0100-000001000000}">
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="1" xr:uid="{00000000-000C-0000-FFFF-FFFF00000000}" name="Tabela1" displayName="Tabela1" ref="A1:J102" totalsRowShown="0" headerRowDxfId="11" dataDxfId="10">
+  <autoFilter ref="A1:J102" xr:uid="{00000000-0009-0000-0100-000001000000}">
     <filterColumn colId="0" hiddenButton="1"/>
     <filterColumn colId="1" hiddenButton="1"/>
     <filterColumn colId="2" hiddenButton="1"/>
@@ -696,10 +736,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:J75"/>
+  <dimension ref="A1:J102"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A40" zoomScale="89" zoomScaleNormal="89" workbookViewId="0">
-      <selection activeCell="J74" sqref="J74"/>
+    <sheetView tabSelected="1" topLeftCell="A77" zoomScale="89" zoomScaleNormal="89" workbookViewId="0">
+      <selection activeCell="A102" sqref="A102:J102"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -3117,6 +3157,870 @@
         <v>0</v>
       </c>
     </row>
+    <row r="76" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A76" s="20">
+        <v>43976</v>
+      </c>
+      <c r="B76" s="21">
+        <v>75770</v>
+      </c>
+      <c r="C76" s="22">
+        <v>754</v>
+      </c>
+      <c r="D76" s="22">
+        <v>1469</v>
+      </c>
+      <c r="E76" s="22">
+        <v>0</v>
+      </c>
+      <c r="F76" s="22">
+        <v>9</v>
+      </c>
+      <c r="G76" s="22">
+        <v>2</v>
+      </c>
+      <c r="H76" s="22">
+        <v>6</v>
+      </c>
+      <c r="I76" s="22">
+        <v>108</v>
+      </c>
+      <c r="J76" s="22">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="77" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A77" s="20">
+        <v>43977</v>
+      </c>
+      <c r="B77" s="21">
+        <v>76579</v>
+      </c>
+      <c r="C77" s="22">
+        <v>809</v>
+      </c>
+      <c r="D77" s="22">
+        <v>1471</v>
+      </c>
+      <c r="E77" s="22">
+        <v>2</v>
+      </c>
+      <c r="F77" s="22">
+        <v>8</v>
+      </c>
+      <c r="G77" s="22">
+        <v>2</v>
+      </c>
+      <c r="H77" s="22">
+        <v>2</v>
+      </c>
+      <c r="I77" s="22">
+        <v>108</v>
+      </c>
+      <c r="J77" s="22">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="78" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A78" s="20">
+        <v>43978</v>
+      </c>
+      <c r="B78" s="21">
+        <v>77210</v>
+      </c>
+      <c r="C78" s="22">
+        <v>631</v>
+      </c>
+      <c r="D78" s="22">
+        <v>1473</v>
+      </c>
+      <c r="E78" s="22">
+        <v>2</v>
+      </c>
+      <c r="F78" s="22">
+        <v>7</v>
+      </c>
+      <c r="G78" s="22">
+        <v>2</v>
+      </c>
+      <c r="H78" s="22">
+        <v>1</v>
+      </c>
+      <c r="I78" s="22">
+        <v>108</v>
+      </c>
+      <c r="J78" s="22">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="79" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A79" s="20">
+        <v>43979</v>
+      </c>
+      <c r="B79" s="21">
+        <v>77916</v>
+      </c>
+      <c r="C79" s="22">
+        <v>706</v>
+      </c>
+      <c r="D79" s="22">
+        <v>1473</v>
+      </c>
+      <c r="E79" s="22">
+        <v>0</v>
+      </c>
+      <c r="F79" s="22">
+        <v>7</v>
+      </c>
+      <c r="G79" s="22">
+        <v>2</v>
+      </c>
+      <c r="H79" s="22">
+        <v>0</v>
+      </c>
+      <c r="I79" s="22">
+        <v>108</v>
+      </c>
+      <c r="J79" s="22">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="80" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A80" s="20">
+        <v>43980</v>
+      </c>
+      <c r="B80" s="21">
+        <v>78529</v>
+      </c>
+      <c r="C80" s="22">
+        <v>613</v>
+      </c>
+      <c r="D80" s="22">
+        <v>1473</v>
+      </c>
+      <c r="E80" s="22">
+        <v>0</v>
+      </c>
+      <c r="F80" s="22">
+        <v>7</v>
+      </c>
+      <c r="G80" s="22">
+        <v>2</v>
+      </c>
+      <c r="H80" s="22">
+        <v>0</v>
+      </c>
+      <c r="I80" s="22">
+        <v>108</v>
+      </c>
+      <c r="J80" s="22">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="81" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A81" s="20">
+        <v>43981</v>
+      </c>
+      <c r="B81" s="22">
+        <v>78793</v>
+      </c>
+      <c r="C81" s="22">
+        <v>264</v>
+      </c>
+      <c r="D81" s="22">
+        <v>1473</v>
+      </c>
+      <c r="E81" s="22">
+        <v>0</v>
+      </c>
+      <c r="F81" s="22">
+        <v>6</v>
+      </c>
+      <c r="G81" s="22">
+        <v>2</v>
+      </c>
+      <c r="H81" s="22">
+        <v>1</v>
+      </c>
+      <c r="I81" s="22">
+        <v>108</v>
+      </c>
+      <c r="J81" s="22">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="82" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A82" s="20">
+        <v>43982</v>
+      </c>
+      <c r="B82" s="21">
+        <v>79039</v>
+      </c>
+      <c r="C82" s="22">
+        <v>246</v>
+      </c>
+      <c r="D82" s="22">
+        <v>1473</v>
+      </c>
+      <c r="E82" s="22">
+        <v>0</v>
+      </c>
+      <c r="F82" s="22">
+        <v>5</v>
+      </c>
+      <c r="G82" s="22">
+        <v>1</v>
+      </c>
+      <c r="H82" s="22">
+        <v>0</v>
+      </c>
+      <c r="I82" s="22">
+        <v>109</v>
+      </c>
+      <c r="J82" s="22">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="83" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A83" s="20">
+        <v>43983</v>
+      </c>
+      <c r="B83" s="21">
+        <v>79698</v>
+      </c>
+      <c r="C83" s="22">
+        <v>659</v>
+      </c>
+      <c r="D83" s="22">
+        <v>1475</v>
+      </c>
+      <c r="E83" s="22">
+        <v>2</v>
+      </c>
+      <c r="F83" s="22">
+        <v>5</v>
+      </c>
+      <c r="G83" s="22">
+        <v>1</v>
+      </c>
+      <c r="H83" s="22">
+        <v>0</v>
+      </c>
+      <c r="I83" s="22">
+        <v>109</v>
+      </c>
+      <c r="J83" s="22">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="84" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A84" s="20">
+        <v>43984</v>
+      </c>
+      <c r="B84" s="21">
+        <v>80505</v>
+      </c>
+      <c r="C84" s="22">
+        <v>807</v>
+      </c>
+      <c r="D84" s="22">
+        <v>1477</v>
+      </c>
+      <c r="E84" s="22">
+        <v>2</v>
+      </c>
+      <c r="F84" s="22">
+        <v>5</v>
+      </c>
+      <c r="G84" s="22">
+        <v>0</v>
+      </c>
+      <c r="H84" s="22">
+        <v>0</v>
+      </c>
+      <c r="I84" s="22">
+        <v>109</v>
+      </c>
+      <c r="J84" s="22">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="85" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A85" s="20">
+        <v>43985</v>
+      </c>
+      <c r="B85" s="21">
+        <v>81333</v>
+      </c>
+      <c r="C85" s="22">
+        <v>828</v>
+      </c>
+      <c r="D85" s="22">
+        <v>1477</v>
+      </c>
+      <c r="E85" s="22">
+        <v>0</v>
+      </c>
+      <c r="F85" s="22">
+        <v>5</v>
+      </c>
+      <c r="G85" s="22">
+        <v>0</v>
+      </c>
+      <c r="H85" s="22">
+        <v>0</v>
+      </c>
+      <c r="I85" s="22">
+        <v>109</v>
+      </c>
+      <c r="J85" s="22">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="86" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A86" s="26">
+        <v>43986</v>
+      </c>
+      <c r="B86" s="27">
+        <v>82161</v>
+      </c>
+      <c r="C86" s="28">
+        <v>828</v>
+      </c>
+      <c r="D86" s="28">
+        <v>1479</v>
+      </c>
+      <c r="E86" s="28">
+        <v>2</v>
+      </c>
+      <c r="F86" s="28">
+        <v>6</v>
+      </c>
+      <c r="G86" s="28">
+        <v>0</v>
+      </c>
+      <c r="H86" s="28">
+        <v>0</v>
+      </c>
+      <c r="I86" s="28">
+        <v>109</v>
+      </c>
+      <c r="J86" s="28">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="87" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A87" s="29">
+        <v>43987</v>
+      </c>
+      <c r="B87" s="30">
+        <v>82876</v>
+      </c>
+      <c r="C87" s="31">
+        <v>715</v>
+      </c>
+      <c r="D87" s="31">
+        <v>1484</v>
+      </c>
+      <c r="E87" s="31">
+        <v>5</v>
+      </c>
+      <c r="F87" s="31">
+        <v>6</v>
+      </c>
+      <c r="G87" s="31">
+        <v>0</v>
+      </c>
+      <c r="H87" s="31">
+        <v>0</v>
+      </c>
+      <c r="I87" s="31">
+        <v>109</v>
+      </c>
+      <c r="J87" s="31">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="88" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A88" s="23">
+        <v>43988</v>
+      </c>
+      <c r="B88" s="24">
+        <v>83105</v>
+      </c>
+      <c r="C88" s="25">
+        <v>229</v>
+      </c>
+      <c r="D88" s="25">
+        <v>1485</v>
+      </c>
+      <c r="E88" s="25">
+        <v>1</v>
+      </c>
+      <c r="F88" s="25">
+        <v>5</v>
+      </c>
+      <c r="G88" s="25">
+        <v>0</v>
+      </c>
+      <c r="H88" s="25">
+        <v>1</v>
+      </c>
+      <c r="I88" s="25">
+        <v>109</v>
+      </c>
+      <c r="J88" s="25">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="89" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A89" s="29">
+        <v>43989</v>
+      </c>
+      <c r="B89" s="30">
+        <v>83316</v>
+      </c>
+      <c r="C89" s="31">
+        <v>211</v>
+      </c>
+      <c r="D89" s="31">
+        <v>1485</v>
+      </c>
+      <c r="E89" s="31">
+        <v>0</v>
+      </c>
+      <c r="F89" s="31">
+        <v>5</v>
+      </c>
+      <c r="G89" s="31">
+        <v>0</v>
+      </c>
+      <c r="H89" s="31">
+        <v>0</v>
+      </c>
+      <c r="I89" s="31">
+        <v>109</v>
+      </c>
+      <c r="J89" s="31">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="90" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A90" s="20">
+        <v>43990</v>
+      </c>
+      <c r="B90" s="21">
+        <v>84130</v>
+      </c>
+      <c r="C90" s="22">
+        <v>814</v>
+      </c>
+      <c r="D90" s="22">
+        <v>1486</v>
+      </c>
+      <c r="E90" s="22">
+        <v>1</v>
+      </c>
+      <c r="F90" s="22">
+        <v>6</v>
+      </c>
+      <c r="G90" s="22">
+        <v>0</v>
+      </c>
+      <c r="H90" s="22">
+        <v>0</v>
+      </c>
+      <c r="I90" s="22">
+        <v>109</v>
+      </c>
+      <c r="J90" s="22">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="91" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A91" s="20">
+        <v>43991</v>
+      </c>
+      <c r="B91" s="21">
+        <v>84868</v>
+      </c>
+      <c r="C91" s="22">
+        <v>738</v>
+      </c>
+      <c r="D91" s="22">
+        <v>1488</v>
+      </c>
+      <c r="E91" s="22">
+        <v>2</v>
+      </c>
+      <c r="F91" s="22">
+        <v>6</v>
+      </c>
+      <c r="G91" s="22">
+        <v>0</v>
+      </c>
+      <c r="H91" s="22">
+        <v>0</v>
+      </c>
+      <c r="I91" s="22">
+        <v>109</v>
+      </c>
+      <c r="J91" s="22">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="92" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A92" s="23">
+        <v>43992</v>
+      </c>
+      <c r="B92" s="24">
+        <v>85626</v>
+      </c>
+      <c r="C92" s="25">
+        <v>758</v>
+      </c>
+      <c r="D92" s="25">
+        <v>1488</v>
+      </c>
+      <c r="E92" s="25">
+        <v>0</v>
+      </c>
+      <c r="F92" s="25">
+        <v>6</v>
+      </c>
+      <c r="G92" s="25">
+        <v>0</v>
+      </c>
+      <c r="H92" s="25">
+        <v>0</v>
+      </c>
+      <c r="I92" s="25">
+        <v>109</v>
+      </c>
+      <c r="J92" s="25">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="93" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A93" s="29">
+        <v>43993</v>
+      </c>
+      <c r="B93" s="30">
+        <v>86328</v>
+      </c>
+      <c r="C93" s="31">
+        <v>702</v>
+      </c>
+      <c r="D93" s="31">
+        <v>1490</v>
+      </c>
+      <c r="E93" s="31">
+        <v>2</v>
+      </c>
+      <c r="F93" s="31">
+        <v>6</v>
+      </c>
+      <c r="G93" s="31">
+        <v>0</v>
+      </c>
+      <c r="H93" s="31">
+        <v>0</v>
+      </c>
+      <c r="I93" s="31">
+        <v>109</v>
+      </c>
+      <c r="J93" s="31">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="94" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A94" s="23">
+        <v>43994</v>
+      </c>
+      <c r="B94" s="24">
+        <v>87095</v>
+      </c>
+      <c r="C94" s="25">
+        <v>767</v>
+      </c>
+      <c r="D94" s="25">
+        <v>1492</v>
+      </c>
+      <c r="E94" s="25">
+        <v>2</v>
+      </c>
+      <c r="F94" s="25">
+        <v>6</v>
+      </c>
+      <c r="G94" s="25">
+        <v>0</v>
+      </c>
+      <c r="H94" s="25">
+        <v>0</v>
+      </c>
+      <c r="I94" s="25">
+        <v>109</v>
+      </c>
+      <c r="J94" s="25">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="95" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A95" s="29">
+        <v>43995</v>
+      </c>
+      <c r="B95" s="30">
+        <v>87386</v>
+      </c>
+      <c r="C95" s="31">
+        <v>291</v>
+      </c>
+      <c r="D95" s="31">
+        <v>1495</v>
+      </c>
+      <c r="E95" s="31">
+        <v>3</v>
+      </c>
+      <c r="F95" s="31">
+        <v>6</v>
+      </c>
+      <c r="G95" s="31">
+        <v>0</v>
+      </c>
+      <c r="H95" s="31">
+        <v>0</v>
+      </c>
+      <c r="I95" s="31">
+        <v>109</v>
+      </c>
+      <c r="J95" s="31">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="96" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A96" s="23">
+        <v>43996</v>
+      </c>
+      <c r="B96" s="24">
+        <v>87598</v>
+      </c>
+      <c r="C96" s="25">
+        <v>212</v>
+      </c>
+      <c r="D96" s="25">
+        <v>1496</v>
+      </c>
+      <c r="E96" s="25">
+        <v>1</v>
+      </c>
+      <c r="F96" s="25">
+        <v>7</v>
+      </c>
+      <c r="G96" s="25">
+        <v>1</v>
+      </c>
+      <c r="H96" s="25">
+        <v>0</v>
+      </c>
+      <c r="I96" s="25">
+        <v>109</v>
+      </c>
+      <c r="J96" s="25">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="97" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A97" s="20">
+        <v>43997</v>
+      </c>
+      <c r="B97" s="21">
+        <v>88165</v>
+      </c>
+      <c r="C97" s="22">
+        <v>567</v>
+      </c>
+      <c r="D97" s="22">
+        <v>1499</v>
+      </c>
+      <c r="E97" s="22">
+        <v>3</v>
+      </c>
+      <c r="F97" s="22">
+        <v>7</v>
+      </c>
+      <c r="G97" s="22">
+        <v>1</v>
+      </c>
+      <c r="H97" s="22">
+        <v>0</v>
+      </c>
+      <c r="I97" s="22">
+        <v>109</v>
+      </c>
+      <c r="J97" s="22">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="98" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A98" s="20">
+        <v>43998</v>
+      </c>
+      <c r="B98" s="21">
+        <v>89151</v>
+      </c>
+      <c r="C98" s="22">
+        <v>986</v>
+      </c>
+      <c r="D98" s="22">
+        <v>1503</v>
+      </c>
+      <c r="E98" s="22">
+        <v>4</v>
+      </c>
+      <c r="F98" s="22">
+        <v>7</v>
+      </c>
+      <c r="G98" s="22">
+        <v>1</v>
+      </c>
+      <c r="H98" s="22">
+        <v>0</v>
+      </c>
+      <c r="I98" s="22">
+        <v>109</v>
+      </c>
+      <c r="J98" s="22">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="99" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A99" s="29">
+        <v>43999</v>
+      </c>
+      <c r="B99" s="30">
+        <v>90103</v>
+      </c>
+      <c r="C99" s="31">
+        <v>952</v>
+      </c>
+      <c r="D99" s="31">
+        <v>1511</v>
+      </c>
+      <c r="E99" s="31">
+        <v>8</v>
+      </c>
+      <c r="F99" s="31">
+        <v>6</v>
+      </c>
+      <c r="G99" s="31">
+        <v>1</v>
+      </c>
+      <c r="H99" s="31">
+        <v>1</v>
+      </c>
+      <c r="I99" s="31">
+        <v>109</v>
+      </c>
+      <c r="J99" s="31">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="100" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A100" s="20">
+        <v>44000</v>
+      </c>
+      <c r="B100" s="21">
+        <v>91005</v>
+      </c>
+      <c r="C100" s="22">
+        <v>902</v>
+      </c>
+      <c r="D100" s="22">
+        <v>1513</v>
+      </c>
+      <c r="E100" s="22">
+        <v>2</v>
+      </c>
+      <c r="F100" s="22">
+        <v>8</v>
+      </c>
+      <c r="G100" s="22">
+        <v>1</v>
+      </c>
+      <c r="H100" s="22">
+        <v>0</v>
+      </c>
+      <c r="I100" s="22">
+        <v>109</v>
+      </c>
+      <c r="J100" s="22">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="101" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A101" s="29">
+        <v>44001</v>
+      </c>
+      <c r="B101" s="30">
+        <v>92152</v>
+      </c>
+      <c r="C101" s="31">
+        <v>1147</v>
+      </c>
+      <c r="D101" s="31">
+        <v>1519</v>
+      </c>
+      <c r="E101" s="31">
+        <v>6</v>
+      </c>
+      <c r="F101" s="31">
+        <v>6</v>
+      </c>
+      <c r="G101" s="31">
+        <v>1</v>
+      </c>
+      <c r="H101" s="31">
+        <v>2</v>
+      </c>
+      <c r="I101" s="31">
+        <v>109</v>
+      </c>
+      <c r="J101" s="31">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="102" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A102" s="23">
+        <v>44002</v>
+      </c>
+      <c r="B102" s="24">
+        <v>92919</v>
+      </c>
+      <c r="C102" s="25">
+        <v>758</v>
+      </c>
+      <c r="D102" s="25">
+        <v>1520</v>
+      </c>
+      <c r="E102" s="25">
+        <v>1</v>
+      </c>
+      <c r="F102" s="25">
+        <v>6</v>
+      </c>
+      <c r="G102" s="25">
+        <v>1</v>
+      </c>
+      <c r="H102" s="25">
+        <v>2</v>
+      </c>
+      <c r="I102" s="25">
+        <v>109</v>
+      </c>
+      <c r="J102" s="25">
+        <v>0</v>
+      </c>
+    </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>

</xml_diff>

<commit_message>
Data updated by GitHub Bot (2020-06-21 20)
</commit_message>
<xml_diff>
--- a/output/snapshot/fdcf2531-4c3e-5c02-b63c-ee160ead6dea.xlsx
+++ b/output/snapshot/fdcf2531-4c3e-5c02-b63c-ee160ead6dea.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="I:\AKTUALNI PODATKI - KORONA\Za objavo na GOV.SI\ang\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{1E6DD62F-2BE2-47DC-A7ED-9B57C1589256}" xr6:coauthVersionLast="44" xr6:coauthVersionMax="44" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{9006D0F7-09D7-4EC0-A0E3-11905E8C747A}" xr6:coauthVersionLast="44" xr6:coauthVersionMax="44" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -64,7 +64,7 @@
   <numFmts count="1">
     <numFmt numFmtId="164" formatCode="d/\ m/\ yyyy;@"/>
   </numFmts>
-  <fonts count="4" x14ac:knownFonts="1">
+  <fonts count="5" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -93,6 +93,13 @@
       <name val="Calibri Light"/>
       <scheme val="major"/>
     </font>
+    <font>
+      <sz val="10"/>
+      <color theme="1"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
   </fonts>
   <fills count="3">
     <fill>
@@ -108,7 +115,7 @@
       </patternFill>
     </fill>
   </fills>
-  <borders count="2">
+  <borders count="3">
     <border>
       <left/>
       <right/>
@@ -129,11 +136,26 @@
       <bottom/>
       <diagonal/>
     </border>
+    <border>
+      <left style="thin">
+        <color theme="4"/>
+      </left>
+      <right style="thin">
+        <color theme="4"/>
+      </right>
+      <top style="thin">
+        <color theme="4"/>
+      </top>
+      <bottom style="thin">
+        <color theme="4"/>
+      </bottom>
+      <diagonal/>
+    </border>
   </borders>
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="26">
+  <cellXfs count="32">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="49" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyAlignment="1" applyProtection="1">
       <alignment horizontal="left" vertical="top"/>
@@ -208,6 +230,24 @@
       <alignment horizontal="right"/>
     </xf>
     <xf numFmtId="0" fontId="3" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="right"/>
+    </xf>
+    <xf numFmtId="164" fontId="4" fillId="2" borderId="2" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="right" vertical="top"/>
+    </xf>
+    <xf numFmtId="3" fontId="4" fillId="2" borderId="2" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="right"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="2" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="right"/>
+    </xf>
+    <xf numFmtId="164" fontId="3" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="right" vertical="top"/>
+    </xf>
+    <xf numFmtId="3" fontId="3" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="right"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="right"/>
     </xf>
   </cellXfs>
@@ -399,8 +439,8 @@
 </file>
 
 <file path=xl/tables/table1.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="1" xr:uid="{00000000-000C-0000-FFFF-FFFF00000000}" name="Tabela1" displayName="Tabela1" ref="A1:J75" totalsRowShown="0" headerRowDxfId="11" dataDxfId="10">
-  <autoFilter ref="A1:J75" xr:uid="{00000000-0009-0000-0100-000001000000}">
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="1" xr:uid="{00000000-000C-0000-FFFF-FFFF00000000}" name="Tabela1" displayName="Tabela1" ref="A1:J102" totalsRowShown="0" headerRowDxfId="11" dataDxfId="10">
+  <autoFilter ref="A1:J102" xr:uid="{00000000-0009-0000-0100-000001000000}">
     <filterColumn colId="0" hiddenButton="1"/>
     <filterColumn colId="1" hiddenButton="1"/>
     <filterColumn colId="2" hiddenButton="1"/>
@@ -696,10 +736,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:J75"/>
+  <dimension ref="A1:J102"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A40" zoomScale="89" zoomScaleNormal="89" workbookViewId="0">
-      <selection activeCell="J74" sqref="J74"/>
+    <sheetView tabSelected="1" topLeftCell="A77" zoomScale="89" zoomScaleNormal="89" workbookViewId="0">
+      <selection activeCell="A102" sqref="A102:J102"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -3117,6 +3157,870 @@
         <v>0</v>
       </c>
     </row>
+    <row r="76" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A76" s="20">
+        <v>43976</v>
+      </c>
+      <c r="B76" s="21">
+        <v>75770</v>
+      </c>
+      <c r="C76" s="22">
+        <v>754</v>
+      </c>
+      <c r="D76" s="22">
+        <v>1469</v>
+      </c>
+      <c r="E76" s="22">
+        <v>0</v>
+      </c>
+      <c r="F76" s="22">
+        <v>9</v>
+      </c>
+      <c r="G76" s="22">
+        <v>2</v>
+      </c>
+      <c r="H76" s="22">
+        <v>6</v>
+      </c>
+      <c r="I76" s="22">
+        <v>108</v>
+      </c>
+      <c r="J76" s="22">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="77" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A77" s="20">
+        <v>43977</v>
+      </c>
+      <c r="B77" s="21">
+        <v>76579</v>
+      </c>
+      <c r="C77" s="22">
+        <v>809</v>
+      </c>
+      <c r="D77" s="22">
+        <v>1471</v>
+      </c>
+      <c r="E77" s="22">
+        <v>2</v>
+      </c>
+      <c r="F77" s="22">
+        <v>8</v>
+      </c>
+      <c r="G77" s="22">
+        <v>2</v>
+      </c>
+      <c r="H77" s="22">
+        <v>2</v>
+      </c>
+      <c r="I77" s="22">
+        <v>108</v>
+      </c>
+      <c r="J77" s="22">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="78" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A78" s="20">
+        <v>43978</v>
+      </c>
+      <c r="B78" s="21">
+        <v>77210</v>
+      </c>
+      <c r="C78" s="22">
+        <v>631</v>
+      </c>
+      <c r="D78" s="22">
+        <v>1473</v>
+      </c>
+      <c r="E78" s="22">
+        <v>2</v>
+      </c>
+      <c r="F78" s="22">
+        <v>7</v>
+      </c>
+      <c r="G78" s="22">
+        <v>2</v>
+      </c>
+      <c r="H78" s="22">
+        <v>1</v>
+      </c>
+      <c r="I78" s="22">
+        <v>108</v>
+      </c>
+      <c r="J78" s="22">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="79" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A79" s="20">
+        <v>43979</v>
+      </c>
+      <c r="B79" s="21">
+        <v>77916</v>
+      </c>
+      <c r="C79" s="22">
+        <v>706</v>
+      </c>
+      <c r="D79" s="22">
+        <v>1473</v>
+      </c>
+      <c r="E79" s="22">
+        <v>0</v>
+      </c>
+      <c r="F79" s="22">
+        <v>7</v>
+      </c>
+      <c r="G79" s="22">
+        <v>2</v>
+      </c>
+      <c r="H79" s="22">
+        <v>0</v>
+      </c>
+      <c r="I79" s="22">
+        <v>108</v>
+      </c>
+      <c r="J79" s="22">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="80" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A80" s="20">
+        <v>43980</v>
+      </c>
+      <c r="B80" s="21">
+        <v>78529</v>
+      </c>
+      <c r="C80" s="22">
+        <v>613</v>
+      </c>
+      <c r="D80" s="22">
+        <v>1473</v>
+      </c>
+      <c r="E80" s="22">
+        <v>0</v>
+      </c>
+      <c r="F80" s="22">
+        <v>7</v>
+      </c>
+      <c r="G80" s="22">
+        <v>2</v>
+      </c>
+      <c r="H80" s="22">
+        <v>0</v>
+      </c>
+      <c r="I80" s="22">
+        <v>108</v>
+      </c>
+      <c r="J80" s="22">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="81" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A81" s="20">
+        <v>43981</v>
+      </c>
+      <c r="B81" s="22">
+        <v>78793</v>
+      </c>
+      <c r="C81" s="22">
+        <v>264</v>
+      </c>
+      <c r="D81" s="22">
+        <v>1473</v>
+      </c>
+      <c r="E81" s="22">
+        <v>0</v>
+      </c>
+      <c r="F81" s="22">
+        <v>6</v>
+      </c>
+      <c r="G81" s="22">
+        <v>2</v>
+      </c>
+      <c r="H81" s="22">
+        <v>1</v>
+      </c>
+      <c r="I81" s="22">
+        <v>108</v>
+      </c>
+      <c r="J81" s="22">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="82" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A82" s="20">
+        <v>43982</v>
+      </c>
+      <c r="B82" s="21">
+        <v>79039</v>
+      </c>
+      <c r="C82" s="22">
+        <v>246</v>
+      </c>
+      <c r="D82" s="22">
+        <v>1473</v>
+      </c>
+      <c r="E82" s="22">
+        <v>0</v>
+      </c>
+      <c r="F82" s="22">
+        <v>5</v>
+      </c>
+      <c r="G82" s="22">
+        <v>1</v>
+      </c>
+      <c r="H82" s="22">
+        <v>0</v>
+      </c>
+      <c r="I82" s="22">
+        <v>109</v>
+      </c>
+      <c r="J82" s="22">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="83" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A83" s="20">
+        <v>43983</v>
+      </c>
+      <c r="B83" s="21">
+        <v>79698</v>
+      </c>
+      <c r="C83" s="22">
+        <v>659</v>
+      </c>
+      <c r="D83" s="22">
+        <v>1475</v>
+      </c>
+      <c r="E83" s="22">
+        <v>2</v>
+      </c>
+      <c r="F83" s="22">
+        <v>5</v>
+      </c>
+      <c r="G83" s="22">
+        <v>1</v>
+      </c>
+      <c r="H83" s="22">
+        <v>0</v>
+      </c>
+      <c r="I83" s="22">
+        <v>109</v>
+      </c>
+      <c r="J83" s="22">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="84" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A84" s="20">
+        <v>43984</v>
+      </c>
+      <c r="B84" s="21">
+        <v>80505</v>
+      </c>
+      <c r="C84" s="22">
+        <v>807</v>
+      </c>
+      <c r="D84" s="22">
+        <v>1477</v>
+      </c>
+      <c r="E84" s="22">
+        <v>2</v>
+      </c>
+      <c r="F84" s="22">
+        <v>5</v>
+      </c>
+      <c r="G84" s="22">
+        <v>0</v>
+      </c>
+      <c r="H84" s="22">
+        <v>0</v>
+      </c>
+      <c r="I84" s="22">
+        <v>109</v>
+      </c>
+      <c r="J84" s="22">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="85" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A85" s="20">
+        <v>43985</v>
+      </c>
+      <c r="B85" s="21">
+        <v>81333</v>
+      </c>
+      <c r="C85" s="22">
+        <v>828</v>
+      </c>
+      <c r="D85" s="22">
+        <v>1477</v>
+      </c>
+      <c r="E85" s="22">
+        <v>0</v>
+      </c>
+      <c r="F85" s="22">
+        <v>5</v>
+      </c>
+      <c r="G85" s="22">
+        <v>0</v>
+      </c>
+      <c r="H85" s="22">
+        <v>0</v>
+      </c>
+      <c r="I85" s="22">
+        <v>109</v>
+      </c>
+      <c r="J85" s="22">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="86" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A86" s="26">
+        <v>43986</v>
+      </c>
+      <c r="B86" s="27">
+        <v>82161</v>
+      </c>
+      <c r="C86" s="28">
+        <v>828</v>
+      </c>
+      <c r="D86" s="28">
+        <v>1479</v>
+      </c>
+      <c r="E86" s="28">
+        <v>2</v>
+      </c>
+      <c r="F86" s="28">
+        <v>6</v>
+      </c>
+      <c r="G86" s="28">
+        <v>0</v>
+      </c>
+      <c r="H86" s="28">
+        <v>0</v>
+      </c>
+      <c r="I86" s="28">
+        <v>109</v>
+      </c>
+      <c r="J86" s="28">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="87" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A87" s="29">
+        <v>43987</v>
+      </c>
+      <c r="B87" s="30">
+        <v>82876</v>
+      </c>
+      <c r="C87" s="31">
+        <v>715</v>
+      </c>
+      <c r="D87" s="31">
+        <v>1484</v>
+      </c>
+      <c r="E87" s="31">
+        <v>5</v>
+      </c>
+      <c r="F87" s="31">
+        <v>6</v>
+      </c>
+      <c r="G87" s="31">
+        <v>0</v>
+      </c>
+      <c r="H87" s="31">
+        <v>0</v>
+      </c>
+      <c r="I87" s="31">
+        <v>109</v>
+      </c>
+      <c r="J87" s="31">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="88" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A88" s="23">
+        <v>43988</v>
+      </c>
+      <c r="B88" s="24">
+        <v>83105</v>
+      </c>
+      <c r="C88" s="25">
+        <v>229</v>
+      </c>
+      <c r="D88" s="25">
+        <v>1485</v>
+      </c>
+      <c r="E88" s="25">
+        <v>1</v>
+      </c>
+      <c r="F88" s="25">
+        <v>5</v>
+      </c>
+      <c r="G88" s="25">
+        <v>0</v>
+      </c>
+      <c r="H88" s="25">
+        <v>1</v>
+      </c>
+      <c r="I88" s="25">
+        <v>109</v>
+      </c>
+      <c r="J88" s="25">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="89" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A89" s="29">
+        <v>43989</v>
+      </c>
+      <c r="B89" s="30">
+        <v>83316</v>
+      </c>
+      <c r="C89" s="31">
+        <v>211</v>
+      </c>
+      <c r="D89" s="31">
+        <v>1485</v>
+      </c>
+      <c r="E89" s="31">
+        <v>0</v>
+      </c>
+      <c r="F89" s="31">
+        <v>5</v>
+      </c>
+      <c r="G89" s="31">
+        <v>0</v>
+      </c>
+      <c r="H89" s="31">
+        <v>0</v>
+      </c>
+      <c r="I89" s="31">
+        <v>109</v>
+      </c>
+      <c r="J89" s="31">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="90" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A90" s="20">
+        <v>43990</v>
+      </c>
+      <c r="B90" s="21">
+        <v>84130</v>
+      </c>
+      <c r="C90" s="22">
+        <v>814</v>
+      </c>
+      <c r="D90" s="22">
+        <v>1486</v>
+      </c>
+      <c r="E90" s="22">
+        <v>1</v>
+      </c>
+      <c r="F90" s="22">
+        <v>6</v>
+      </c>
+      <c r="G90" s="22">
+        <v>0</v>
+      </c>
+      <c r="H90" s="22">
+        <v>0</v>
+      </c>
+      <c r="I90" s="22">
+        <v>109</v>
+      </c>
+      <c r="J90" s="22">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="91" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A91" s="20">
+        <v>43991</v>
+      </c>
+      <c r="B91" s="21">
+        <v>84868</v>
+      </c>
+      <c r="C91" s="22">
+        <v>738</v>
+      </c>
+      <c r="D91" s="22">
+        <v>1488</v>
+      </c>
+      <c r="E91" s="22">
+        <v>2</v>
+      </c>
+      <c r="F91" s="22">
+        <v>6</v>
+      </c>
+      <c r="G91" s="22">
+        <v>0</v>
+      </c>
+      <c r="H91" s="22">
+        <v>0</v>
+      </c>
+      <c r="I91" s="22">
+        <v>109</v>
+      </c>
+      <c r="J91" s="22">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="92" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A92" s="23">
+        <v>43992</v>
+      </c>
+      <c r="B92" s="24">
+        <v>85626</v>
+      </c>
+      <c r="C92" s="25">
+        <v>758</v>
+      </c>
+      <c r="D92" s="25">
+        <v>1488</v>
+      </c>
+      <c r="E92" s="25">
+        <v>0</v>
+      </c>
+      <c r="F92" s="25">
+        <v>6</v>
+      </c>
+      <c r="G92" s="25">
+        <v>0</v>
+      </c>
+      <c r="H92" s="25">
+        <v>0</v>
+      </c>
+      <c r="I92" s="25">
+        <v>109</v>
+      </c>
+      <c r="J92" s="25">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="93" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A93" s="29">
+        <v>43993</v>
+      </c>
+      <c r="B93" s="30">
+        <v>86328</v>
+      </c>
+      <c r="C93" s="31">
+        <v>702</v>
+      </c>
+      <c r="D93" s="31">
+        <v>1490</v>
+      </c>
+      <c r="E93" s="31">
+        <v>2</v>
+      </c>
+      <c r="F93" s="31">
+        <v>6</v>
+      </c>
+      <c r="G93" s="31">
+        <v>0</v>
+      </c>
+      <c r="H93" s="31">
+        <v>0</v>
+      </c>
+      <c r="I93" s="31">
+        <v>109</v>
+      </c>
+      <c r="J93" s="31">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="94" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A94" s="23">
+        <v>43994</v>
+      </c>
+      <c r="B94" s="24">
+        <v>87095</v>
+      </c>
+      <c r="C94" s="25">
+        <v>767</v>
+      </c>
+      <c r="D94" s="25">
+        <v>1492</v>
+      </c>
+      <c r="E94" s="25">
+        <v>2</v>
+      </c>
+      <c r="F94" s="25">
+        <v>6</v>
+      </c>
+      <c r="G94" s="25">
+        <v>0</v>
+      </c>
+      <c r="H94" s="25">
+        <v>0</v>
+      </c>
+      <c r="I94" s="25">
+        <v>109</v>
+      </c>
+      <c r="J94" s="25">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="95" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A95" s="29">
+        <v>43995</v>
+      </c>
+      <c r="B95" s="30">
+        <v>87386</v>
+      </c>
+      <c r="C95" s="31">
+        <v>291</v>
+      </c>
+      <c r="D95" s="31">
+        <v>1495</v>
+      </c>
+      <c r="E95" s="31">
+        <v>3</v>
+      </c>
+      <c r="F95" s="31">
+        <v>6</v>
+      </c>
+      <c r="G95" s="31">
+        <v>0</v>
+      </c>
+      <c r="H95" s="31">
+        <v>0</v>
+      </c>
+      <c r="I95" s="31">
+        <v>109</v>
+      </c>
+      <c r="J95" s="31">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="96" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A96" s="23">
+        <v>43996</v>
+      </c>
+      <c r="B96" s="24">
+        <v>87598</v>
+      </c>
+      <c r="C96" s="25">
+        <v>212</v>
+      </c>
+      <c r="D96" s="25">
+        <v>1496</v>
+      </c>
+      <c r="E96" s="25">
+        <v>1</v>
+      </c>
+      <c r="F96" s="25">
+        <v>7</v>
+      </c>
+      <c r="G96" s="25">
+        <v>1</v>
+      </c>
+      <c r="H96" s="25">
+        <v>0</v>
+      </c>
+      <c r="I96" s="25">
+        <v>109</v>
+      </c>
+      <c r="J96" s="25">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="97" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A97" s="20">
+        <v>43997</v>
+      </c>
+      <c r="B97" s="21">
+        <v>88165</v>
+      </c>
+      <c r="C97" s="22">
+        <v>567</v>
+      </c>
+      <c r="D97" s="22">
+        <v>1499</v>
+      </c>
+      <c r="E97" s="22">
+        <v>3</v>
+      </c>
+      <c r="F97" s="22">
+        <v>7</v>
+      </c>
+      <c r="G97" s="22">
+        <v>1</v>
+      </c>
+      <c r="H97" s="22">
+        <v>0</v>
+      </c>
+      <c r="I97" s="22">
+        <v>109</v>
+      </c>
+      <c r="J97" s="22">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="98" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A98" s="20">
+        <v>43998</v>
+      </c>
+      <c r="B98" s="21">
+        <v>89151</v>
+      </c>
+      <c r="C98" s="22">
+        <v>986</v>
+      </c>
+      <c r="D98" s="22">
+        <v>1503</v>
+      </c>
+      <c r="E98" s="22">
+        <v>4</v>
+      </c>
+      <c r="F98" s="22">
+        <v>7</v>
+      </c>
+      <c r="G98" s="22">
+        <v>1</v>
+      </c>
+      <c r="H98" s="22">
+        <v>0</v>
+      </c>
+      <c r="I98" s="22">
+        <v>109</v>
+      </c>
+      <c r="J98" s="22">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="99" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A99" s="29">
+        <v>43999</v>
+      </c>
+      <c r="B99" s="30">
+        <v>90103</v>
+      </c>
+      <c r="C99" s="31">
+        <v>952</v>
+      </c>
+      <c r="D99" s="31">
+        <v>1511</v>
+      </c>
+      <c r="E99" s="31">
+        <v>8</v>
+      </c>
+      <c r="F99" s="31">
+        <v>6</v>
+      </c>
+      <c r="G99" s="31">
+        <v>1</v>
+      </c>
+      <c r="H99" s="31">
+        <v>1</v>
+      </c>
+      <c r="I99" s="31">
+        <v>109</v>
+      </c>
+      <c r="J99" s="31">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="100" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A100" s="20">
+        <v>44000</v>
+      </c>
+      <c r="B100" s="21">
+        <v>91005</v>
+      </c>
+      <c r="C100" s="22">
+        <v>902</v>
+      </c>
+      <c r="D100" s="22">
+        <v>1513</v>
+      </c>
+      <c r="E100" s="22">
+        <v>2</v>
+      </c>
+      <c r="F100" s="22">
+        <v>8</v>
+      </c>
+      <c r="G100" s="22">
+        <v>1</v>
+      </c>
+      <c r="H100" s="22">
+        <v>0</v>
+      </c>
+      <c r="I100" s="22">
+        <v>109</v>
+      </c>
+      <c r="J100" s="22">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="101" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A101" s="29">
+        <v>44001</v>
+      </c>
+      <c r="B101" s="30">
+        <v>92152</v>
+      </c>
+      <c r="C101" s="31">
+        <v>1147</v>
+      </c>
+      <c r="D101" s="31">
+        <v>1519</v>
+      </c>
+      <c r="E101" s="31">
+        <v>6</v>
+      </c>
+      <c r="F101" s="31">
+        <v>6</v>
+      </c>
+      <c r="G101" s="31">
+        <v>1</v>
+      </c>
+      <c r="H101" s="31">
+        <v>2</v>
+      </c>
+      <c r="I101" s="31">
+        <v>109</v>
+      </c>
+      <c r="J101" s="31">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="102" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A102" s="23">
+        <v>44002</v>
+      </c>
+      <c r="B102" s="24">
+        <v>92919</v>
+      </c>
+      <c r="C102" s="25">
+        <v>758</v>
+      </c>
+      <c r="D102" s="25">
+        <v>1520</v>
+      </c>
+      <c r="E102" s="25">
+        <v>1</v>
+      </c>
+      <c r="F102" s="25">
+        <v>6</v>
+      </c>
+      <c r="G102" s="25">
+        <v>1</v>
+      </c>
+      <c r="H102" s="25">
+        <v>2</v>
+      </c>
+      <c r="I102" s="25">
+        <v>109</v>
+      </c>
+      <c r="J102" s="25">
+        <v>0</v>
+      </c>
+    </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>

</xml_diff>

<commit_message>
Data updated by GitHub Bot (2020-06-22 12)
</commit_message>
<xml_diff>
--- a/output/snapshot/fdcf2531-4c3e-5c02-b63c-ee160ead6dea.xlsx
+++ b/output/snapshot/fdcf2531-4c3e-5c02-b63c-ee160ead6dea.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="I:\AKTUALNI PODATKI - KORONA\Za objavo na GOV.SI\ang\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{1E6DD62F-2BE2-47DC-A7ED-9B57C1589256}" xr6:coauthVersionLast="44" xr6:coauthVersionMax="44" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{CF849C95-B7BC-48B8-9AEE-FFE54D73249A}" xr6:coauthVersionLast="44" xr6:coauthVersionMax="44" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -64,7 +64,7 @@
   <numFmts count="1">
     <numFmt numFmtId="164" formatCode="d/\ m/\ yyyy;@"/>
   </numFmts>
-  <fonts count="4" x14ac:knownFonts="1">
+  <fonts count="5" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -93,6 +93,13 @@
       <name val="Calibri Light"/>
       <scheme val="major"/>
     </font>
+    <font>
+      <sz val="10"/>
+      <color theme="1"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
   </fonts>
   <fills count="3">
     <fill>
@@ -108,7 +115,7 @@
       </patternFill>
     </fill>
   </fills>
-  <borders count="2">
+  <borders count="3">
     <border>
       <left/>
       <right/>
@@ -129,11 +136,26 @@
       <bottom/>
       <diagonal/>
     </border>
+    <border>
+      <left style="thin">
+        <color theme="4"/>
+      </left>
+      <right style="thin">
+        <color theme="4"/>
+      </right>
+      <top style="thin">
+        <color theme="4"/>
+      </top>
+      <bottom style="thin">
+        <color theme="4"/>
+      </bottom>
+      <diagonal/>
+    </border>
   </borders>
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="26">
+  <cellXfs count="32">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="49" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyAlignment="1" applyProtection="1">
       <alignment horizontal="left" vertical="top"/>
@@ -208,6 +230,24 @@
       <alignment horizontal="right"/>
     </xf>
     <xf numFmtId="0" fontId="3" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="right"/>
+    </xf>
+    <xf numFmtId="164" fontId="4" fillId="2" borderId="2" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="right" vertical="top"/>
+    </xf>
+    <xf numFmtId="3" fontId="4" fillId="2" borderId="2" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="right"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="2" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="right"/>
+    </xf>
+    <xf numFmtId="164" fontId="3" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="right" vertical="top"/>
+    </xf>
+    <xf numFmtId="3" fontId="3" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="right"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="right"/>
     </xf>
   </cellXfs>
@@ -399,8 +439,8 @@
 </file>
 
 <file path=xl/tables/table1.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="1" xr:uid="{00000000-000C-0000-FFFF-FFFF00000000}" name="Tabela1" displayName="Tabela1" ref="A1:J75" totalsRowShown="0" headerRowDxfId="11" dataDxfId="10">
-  <autoFilter ref="A1:J75" xr:uid="{00000000-0009-0000-0100-000001000000}">
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="1" xr:uid="{00000000-000C-0000-FFFF-FFFF00000000}" name="Tabela1" displayName="Tabela1" ref="A1:J103" totalsRowShown="0" headerRowDxfId="11" dataDxfId="10">
+  <autoFilter ref="A1:J103" xr:uid="{00000000-0009-0000-0100-000001000000}">
     <filterColumn colId="0" hiddenButton="1"/>
     <filterColumn colId="1" hiddenButton="1"/>
     <filterColumn colId="2" hiddenButton="1"/>
@@ -696,10 +736,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:J75"/>
+  <dimension ref="A1:J103"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A40" zoomScale="89" zoomScaleNormal="89" workbookViewId="0">
-      <selection activeCell="J74" sqref="J74"/>
+    <sheetView tabSelected="1" topLeftCell="A77" zoomScale="89" zoomScaleNormal="89" workbookViewId="0">
+      <selection activeCell="A103" sqref="A103:J103"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -3117,6 +3157,902 @@
         <v>0</v>
       </c>
     </row>
+    <row r="76" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A76" s="20">
+        <v>43976</v>
+      </c>
+      <c r="B76" s="21">
+        <v>75770</v>
+      </c>
+      <c r="C76" s="22">
+        <v>754</v>
+      </c>
+      <c r="D76" s="22">
+        <v>1469</v>
+      </c>
+      <c r="E76" s="22">
+        <v>0</v>
+      </c>
+      <c r="F76" s="22">
+        <v>9</v>
+      </c>
+      <c r="G76" s="22">
+        <v>2</v>
+      </c>
+      <c r="H76" s="22">
+        <v>6</v>
+      </c>
+      <c r="I76" s="22">
+        <v>108</v>
+      </c>
+      <c r="J76" s="22">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="77" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A77" s="20">
+        <v>43977</v>
+      </c>
+      <c r="B77" s="21">
+        <v>76579</v>
+      </c>
+      <c r="C77" s="22">
+        <v>809</v>
+      </c>
+      <c r="D77" s="22">
+        <v>1471</v>
+      </c>
+      <c r="E77" s="22">
+        <v>2</v>
+      </c>
+      <c r="F77" s="22">
+        <v>8</v>
+      </c>
+      <c r="G77" s="22">
+        <v>2</v>
+      </c>
+      <c r="H77" s="22">
+        <v>2</v>
+      </c>
+      <c r="I77" s="22">
+        <v>108</v>
+      </c>
+      <c r="J77" s="22">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="78" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A78" s="20">
+        <v>43978</v>
+      </c>
+      <c r="B78" s="21">
+        <v>77210</v>
+      </c>
+      <c r="C78" s="22">
+        <v>631</v>
+      </c>
+      <c r="D78" s="22">
+        <v>1473</v>
+      </c>
+      <c r="E78" s="22">
+        <v>2</v>
+      </c>
+      <c r="F78" s="22">
+        <v>7</v>
+      </c>
+      <c r="G78" s="22">
+        <v>2</v>
+      </c>
+      <c r="H78" s="22">
+        <v>1</v>
+      </c>
+      <c r="I78" s="22">
+        <v>108</v>
+      </c>
+      <c r="J78" s="22">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="79" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A79" s="20">
+        <v>43979</v>
+      </c>
+      <c r="B79" s="21">
+        <v>77916</v>
+      </c>
+      <c r="C79" s="22">
+        <v>706</v>
+      </c>
+      <c r="D79" s="22">
+        <v>1473</v>
+      </c>
+      <c r="E79" s="22">
+        <v>0</v>
+      </c>
+      <c r="F79" s="22">
+        <v>7</v>
+      </c>
+      <c r="G79" s="22">
+        <v>2</v>
+      </c>
+      <c r="H79" s="22">
+        <v>0</v>
+      </c>
+      <c r="I79" s="22">
+        <v>108</v>
+      </c>
+      <c r="J79" s="22">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="80" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A80" s="20">
+        <v>43980</v>
+      </c>
+      <c r="B80" s="21">
+        <v>78529</v>
+      </c>
+      <c r="C80" s="22">
+        <v>613</v>
+      </c>
+      <c r="D80" s="22">
+        <v>1473</v>
+      </c>
+      <c r="E80" s="22">
+        <v>0</v>
+      </c>
+      <c r="F80" s="22">
+        <v>7</v>
+      </c>
+      <c r="G80" s="22">
+        <v>2</v>
+      </c>
+      <c r="H80" s="22">
+        <v>0</v>
+      </c>
+      <c r="I80" s="22">
+        <v>108</v>
+      </c>
+      <c r="J80" s="22">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="81" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A81" s="20">
+        <v>43981</v>
+      </c>
+      <c r="B81" s="22">
+        <v>78793</v>
+      </c>
+      <c r="C81" s="22">
+        <v>264</v>
+      </c>
+      <c r="D81" s="22">
+        <v>1473</v>
+      </c>
+      <c r="E81" s="22">
+        <v>0</v>
+      </c>
+      <c r="F81" s="22">
+        <v>6</v>
+      </c>
+      <c r="G81" s="22">
+        <v>2</v>
+      </c>
+      <c r="H81" s="22">
+        <v>1</v>
+      </c>
+      <c r="I81" s="22">
+        <v>108</v>
+      </c>
+      <c r="J81" s="22">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="82" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A82" s="20">
+        <v>43982</v>
+      </c>
+      <c r="B82" s="21">
+        <v>79039</v>
+      </c>
+      <c r="C82" s="22">
+        <v>246</v>
+      </c>
+      <c r="D82" s="22">
+        <v>1473</v>
+      </c>
+      <c r="E82" s="22">
+        <v>0</v>
+      </c>
+      <c r="F82" s="22">
+        <v>5</v>
+      </c>
+      <c r="G82" s="22">
+        <v>1</v>
+      </c>
+      <c r="H82" s="22">
+        <v>0</v>
+      </c>
+      <c r="I82" s="22">
+        <v>109</v>
+      </c>
+      <c r="J82" s="22">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="83" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A83" s="20">
+        <v>43983</v>
+      </c>
+      <c r="B83" s="21">
+        <v>79698</v>
+      </c>
+      <c r="C83" s="22">
+        <v>659</v>
+      </c>
+      <c r="D83" s="22">
+        <v>1475</v>
+      </c>
+      <c r="E83" s="22">
+        <v>2</v>
+      </c>
+      <c r="F83" s="22">
+        <v>5</v>
+      </c>
+      <c r="G83" s="22">
+        <v>1</v>
+      </c>
+      <c r="H83" s="22">
+        <v>0</v>
+      </c>
+      <c r="I83" s="22">
+        <v>109</v>
+      </c>
+      <c r="J83" s="22">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="84" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A84" s="20">
+        <v>43984</v>
+      </c>
+      <c r="B84" s="21">
+        <v>80505</v>
+      </c>
+      <c r="C84" s="22">
+        <v>807</v>
+      </c>
+      <c r="D84" s="22">
+        <v>1477</v>
+      </c>
+      <c r="E84" s="22">
+        <v>2</v>
+      </c>
+      <c r="F84" s="22">
+        <v>5</v>
+      </c>
+      <c r="G84" s="22">
+        <v>0</v>
+      </c>
+      <c r="H84" s="22">
+        <v>0</v>
+      </c>
+      <c r="I84" s="22">
+        <v>109</v>
+      </c>
+      <c r="J84" s="22">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="85" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A85" s="20">
+        <v>43985</v>
+      </c>
+      <c r="B85" s="21">
+        <v>81333</v>
+      </c>
+      <c r="C85" s="22">
+        <v>828</v>
+      </c>
+      <c r="D85" s="22">
+        <v>1477</v>
+      </c>
+      <c r="E85" s="22">
+        <v>0</v>
+      </c>
+      <c r="F85" s="22">
+        <v>5</v>
+      </c>
+      <c r="G85" s="22">
+        <v>0</v>
+      </c>
+      <c r="H85" s="22">
+        <v>0</v>
+      </c>
+      <c r="I85" s="22">
+        <v>109</v>
+      </c>
+      <c r="J85" s="22">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="86" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A86" s="26">
+        <v>43986</v>
+      </c>
+      <c r="B86" s="27">
+        <v>82161</v>
+      </c>
+      <c r="C86" s="28">
+        <v>828</v>
+      </c>
+      <c r="D86" s="28">
+        <v>1479</v>
+      </c>
+      <c r="E86" s="28">
+        <v>2</v>
+      </c>
+      <c r="F86" s="28">
+        <v>6</v>
+      </c>
+      <c r="G86" s="28">
+        <v>0</v>
+      </c>
+      <c r="H86" s="28">
+        <v>0</v>
+      </c>
+      <c r="I86" s="28">
+        <v>109</v>
+      </c>
+      <c r="J86" s="28">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="87" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A87" s="29">
+        <v>43987</v>
+      </c>
+      <c r="B87" s="30">
+        <v>82876</v>
+      </c>
+      <c r="C87" s="31">
+        <v>715</v>
+      </c>
+      <c r="D87" s="31">
+        <v>1484</v>
+      </c>
+      <c r="E87" s="31">
+        <v>5</v>
+      </c>
+      <c r="F87" s="31">
+        <v>6</v>
+      </c>
+      <c r="G87" s="31">
+        <v>0</v>
+      </c>
+      <c r="H87" s="31">
+        <v>0</v>
+      </c>
+      <c r="I87" s="31">
+        <v>109</v>
+      </c>
+      <c r="J87" s="31">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="88" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A88" s="23">
+        <v>43988</v>
+      </c>
+      <c r="B88" s="24">
+        <v>83105</v>
+      </c>
+      <c r="C88" s="25">
+        <v>229</v>
+      </c>
+      <c r="D88" s="25">
+        <v>1485</v>
+      </c>
+      <c r="E88" s="25">
+        <v>1</v>
+      </c>
+      <c r="F88" s="25">
+        <v>5</v>
+      </c>
+      <c r="G88" s="25">
+        <v>0</v>
+      </c>
+      <c r="H88" s="25">
+        <v>1</v>
+      </c>
+      <c r="I88" s="25">
+        <v>109</v>
+      </c>
+      <c r="J88" s="25">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="89" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A89" s="29">
+        <v>43989</v>
+      </c>
+      <c r="B89" s="30">
+        <v>83316</v>
+      </c>
+      <c r="C89" s="31">
+        <v>211</v>
+      </c>
+      <c r="D89" s="31">
+        <v>1485</v>
+      </c>
+      <c r="E89" s="31">
+        <v>0</v>
+      </c>
+      <c r="F89" s="31">
+        <v>5</v>
+      </c>
+      <c r="G89" s="31">
+        <v>0</v>
+      </c>
+      <c r="H89" s="31">
+        <v>0</v>
+      </c>
+      <c r="I89" s="31">
+        <v>109</v>
+      </c>
+      <c r="J89" s="31">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="90" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A90" s="20">
+        <v>43990</v>
+      </c>
+      <c r="B90" s="21">
+        <v>84130</v>
+      </c>
+      <c r="C90" s="22">
+        <v>814</v>
+      </c>
+      <c r="D90" s="22">
+        <v>1486</v>
+      </c>
+      <c r="E90" s="22">
+        <v>1</v>
+      </c>
+      <c r="F90" s="22">
+        <v>6</v>
+      </c>
+      <c r="G90" s="22">
+        <v>0</v>
+      </c>
+      <c r="H90" s="22">
+        <v>0</v>
+      </c>
+      <c r="I90" s="22">
+        <v>109</v>
+      </c>
+      <c r="J90" s="22">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="91" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A91" s="20">
+        <v>43991</v>
+      </c>
+      <c r="B91" s="21">
+        <v>84868</v>
+      </c>
+      <c r="C91" s="22">
+        <v>738</v>
+      </c>
+      <c r="D91" s="22">
+        <v>1488</v>
+      </c>
+      <c r="E91" s="22">
+        <v>2</v>
+      </c>
+      <c r="F91" s="22">
+        <v>6</v>
+      </c>
+      <c r="G91" s="22">
+        <v>0</v>
+      </c>
+      <c r="H91" s="22">
+        <v>0</v>
+      </c>
+      <c r="I91" s="22">
+        <v>109</v>
+      </c>
+      <c r="J91" s="22">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="92" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A92" s="23">
+        <v>43992</v>
+      </c>
+      <c r="B92" s="24">
+        <v>85626</v>
+      </c>
+      <c r="C92" s="25">
+        <v>758</v>
+      </c>
+      <c r="D92" s="25">
+        <v>1488</v>
+      </c>
+      <c r="E92" s="25">
+        <v>0</v>
+      </c>
+      <c r="F92" s="25">
+        <v>6</v>
+      </c>
+      <c r="G92" s="25">
+        <v>0</v>
+      </c>
+      <c r="H92" s="25">
+        <v>0</v>
+      </c>
+      <c r="I92" s="25">
+        <v>109</v>
+      </c>
+      <c r="J92" s="25">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="93" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A93" s="29">
+        <v>43993</v>
+      </c>
+      <c r="B93" s="30">
+        <v>86328</v>
+      </c>
+      <c r="C93" s="31">
+        <v>702</v>
+      </c>
+      <c r="D93" s="31">
+        <v>1490</v>
+      </c>
+      <c r="E93" s="31">
+        <v>2</v>
+      </c>
+      <c r="F93" s="31">
+        <v>6</v>
+      </c>
+      <c r="G93" s="31">
+        <v>0</v>
+      </c>
+      <c r="H93" s="31">
+        <v>0</v>
+      </c>
+      <c r="I93" s="31">
+        <v>109</v>
+      </c>
+      <c r="J93" s="31">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="94" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A94" s="23">
+        <v>43994</v>
+      </c>
+      <c r="B94" s="24">
+        <v>87095</v>
+      </c>
+      <c r="C94" s="25">
+        <v>767</v>
+      </c>
+      <c r="D94" s="25">
+        <v>1492</v>
+      </c>
+      <c r="E94" s="25">
+        <v>2</v>
+      </c>
+      <c r="F94" s="25">
+        <v>6</v>
+      </c>
+      <c r="G94" s="25">
+        <v>0</v>
+      </c>
+      <c r="H94" s="25">
+        <v>0</v>
+      </c>
+      <c r="I94" s="25">
+        <v>109</v>
+      </c>
+      <c r="J94" s="25">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="95" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A95" s="29">
+        <v>43995</v>
+      </c>
+      <c r="B95" s="30">
+        <v>87386</v>
+      </c>
+      <c r="C95" s="31">
+        <v>291</v>
+      </c>
+      <c r="D95" s="31">
+        <v>1495</v>
+      </c>
+      <c r="E95" s="31">
+        <v>3</v>
+      </c>
+      <c r="F95" s="31">
+        <v>6</v>
+      </c>
+      <c r="G95" s="31">
+        <v>0</v>
+      </c>
+      <c r="H95" s="31">
+        <v>0</v>
+      </c>
+      <c r="I95" s="31">
+        <v>109</v>
+      </c>
+      <c r="J95" s="31">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="96" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A96" s="23">
+        <v>43996</v>
+      </c>
+      <c r="B96" s="24">
+        <v>87598</v>
+      </c>
+      <c r="C96" s="25">
+        <v>212</v>
+      </c>
+      <c r="D96" s="25">
+        <v>1496</v>
+      </c>
+      <c r="E96" s="25">
+        <v>1</v>
+      </c>
+      <c r="F96" s="25">
+        <v>7</v>
+      </c>
+      <c r="G96" s="25">
+        <v>1</v>
+      </c>
+      <c r="H96" s="25">
+        <v>0</v>
+      </c>
+      <c r="I96" s="25">
+        <v>109</v>
+      </c>
+      <c r="J96" s="25">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="97" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A97" s="20">
+        <v>43997</v>
+      </c>
+      <c r="B97" s="21">
+        <v>88165</v>
+      </c>
+      <c r="C97" s="22">
+        <v>567</v>
+      </c>
+      <c r="D97" s="22">
+        <v>1499</v>
+      </c>
+      <c r="E97" s="22">
+        <v>3</v>
+      </c>
+      <c r="F97" s="22">
+        <v>7</v>
+      </c>
+      <c r="G97" s="22">
+        <v>1</v>
+      </c>
+      <c r="H97" s="22">
+        <v>0</v>
+      </c>
+      <c r="I97" s="22">
+        <v>109</v>
+      </c>
+      <c r="J97" s="22">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="98" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A98" s="20">
+        <v>43998</v>
+      </c>
+      <c r="B98" s="21">
+        <v>89151</v>
+      </c>
+      <c r="C98" s="22">
+        <v>986</v>
+      </c>
+      <c r="D98" s="22">
+        <v>1503</v>
+      </c>
+      <c r="E98" s="22">
+        <v>4</v>
+      </c>
+      <c r="F98" s="22">
+        <v>7</v>
+      </c>
+      <c r="G98" s="22">
+        <v>1</v>
+      </c>
+      <c r="H98" s="22">
+        <v>0</v>
+      </c>
+      <c r="I98" s="22">
+        <v>109</v>
+      </c>
+      <c r="J98" s="22">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="99" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A99" s="29">
+        <v>43999</v>
+      </c>
+      <c r="B99" s="30">
+        <v>90103</v>
+      </c>
+      <c r="C99" s="31">
+        <v>952</v>
+      </c>
+      <c r="D99" s="31">
+        <v>1511</v>
+      </c>
+      <c r="E99" s="31">
+        <v>8</v>
+      </c>
+      <c r="F99" s="31">
+        <v>6</v>
+      </c>
+      <c r="G99" s="31">
+        <v>1</v>
+      </c>
+      <c r="H99" s="31">
+        <v>1</v>
+      </c>
+      <c r="I99" s="31">
+        <v>109</v>
+      </c>
+      <c r="J99" s="31">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="100" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A100" s="20">
+        <v>44000</v>
+      </c>
+      <c r="B100" s="21">
+        <v>91005</v>
+      </c>
+      <c r="C100" s="22">
+        <v>902</v>
+      </c>
+      <c r="D100" s="22">
+        <v>1513</v>
+      </c>
+      <c r="E100" s="22">
+        <v>2</v>
+      </c>
+      <c r="F100" s="22">
+        <v>8</v>
+      </c>
+      <c r="G100" s="22">
+        <v>1</v>
+      </c>
+      <c r="H100" s="22">
+        <v>0</v>
+      </c>
+      <c r="I100" s="22">
+        <v>109</v>
+      </c>
+      <c r="J100" s="22">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="101" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A101" s="29">
+        <v>44001</v>
+      </c>
+      <c r="B101" s="30">
+        <v>92152</v>
+      </c>
+      <c r="C101" s="31">
+        <v>1147</v>
+      </c>
+      <c r="D101" s="31">
+        <v>1519</v>
+      </c>
+      <c r="E101" s="31">
+        <v>6</v>
+      </c>
+      <c r="F101" s="31">
+        <v>6</v>
+      </c>
+      <c r="G101" s="31">
+        <v>1</v>
+      </c>
+      <c r="H101" s="31">
+        <v>2</v>
+      </c>
+      <c r="I101" s="31">
+        <v>109</v>
+      </c>
+      <c r="J101" s="31">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="102" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A102" s="23">
+        <v>44002</v>
+      </c>
+      <c r="B102" s="24">
+        <v>92919</v>
+      </c>
+      <c r="C102" s="25">
+        <v>758</v>
+      </c>
+      <c r="D102" s="25">
+        <v>1520</v>
+      </c>
+      <c r="E102" s="25">
+        <v>1</v>
+      </c>
+      <c r="F102" s="25">
+        <v>6</v>
+      </c>
+      <c r="G102" s="25">
+        <v>1</v>
+      </c>
+      <c r="H102" s="25">
+        <v>2</v>
+      </c>
+      <c r="I102" s="25">
+        <v>109</v>
+      </c>
+      <c r="J102" s="25">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="103" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A103" s="29">
+        <v>44003</v>
+      </c>
+      <c r="B103" s="30">
+        <v>93181</v>
+      </c>
+      <c r="C103" s="31">
+        <v>271</v>
+      </c>
+      <c r="D103" s="31">
+        <v>1521</v>
+      </c>
+      <c r="E103" s="31">
+        <v>1</v>
+      </c>
+      <c r="F103" s="31">
+        <v>6</v>
+      </c>
+      <c r="G103" s="31">
+        <v>1</v>
+      </c>
+      <c r="H103" s="31">
+        <v>0</v>
+      </c>
+      <c r="I103" s="31">
+        <v>109</v>
+      </c>
+      <c r="J103" s="31">
+        <v>0</v>
+      </c>
+    </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>

</xml_diff>

<commit_message>
Data updated by GitHub Bot (2020-06-22 20)
</commit_message>
<xml_diff>
--- a/output/snapshot/fdcf2531-4c3e-5c02-b63c-ee160ead6dea.xlsx
+++ b/output/snapshot/fdcf2531-4c3e-5c02-b63c-ee160ead6dea.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="I:\AKTUALNI PODATKI - KORONA\Za objavo na GOV.SI\ang\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{1E6DD62F-2BE2-47DC-A7ED-9B57C1589256}" xr6:coauthVersionLast="44" xr6:coauthVersionMax="44" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{CF849C95-B7BC-48B8-9AEE-FFE54D73249A}" xr6:coauthVersionLast="44" xr6:coauthVersionMax="44" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -64,7 +64,7 @@
   <numFmts count="1">
     <numFmt numFmtId="164" formatCode="d/\ m/\ yyyy;@"/>
   </numFmts>
-  <fonts count="4" x14ac:knownFonts="1">
+  <fonts count="5" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -93,6 +93,13 @@
       <name val="Calibri Light"/>
       <scheme val="major"/>
     </font>
+    <font>
+      <sz val="10"/>
+      <color theme="1"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
   </fonts>
   <fills count="3">
     <fill>
@@ -108,7 +115,7 @@
       </patternFill>
     </fill>
   </fills>
-  <borders count="2">
+  <borders count="3">
     <border>
       <left/>
       <right/>
@@ -129,11 +136,26 @@
       <bottom/>
       <diagonal/>
     </border>
+    <border>
+      <left style="thin">
+        <color theme="4"/>
+      </left>
+      <right style="thin">
+        <color theme="4"/>
+      </right>
+      <top style="thin">
+        <color theme="4"/>
+      </top>
+      <bottom style="thin">
+        <color theme="4"/>
+      </bottom>
+      <diagonal/>
+    </border>
   </borders>
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="26">
+  <cellXfs count="32">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="49" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyAlignment="1" applyProtection="1">
       <alignment horizontal="left" vertical="top"/>
@@ -208,6 +230,24 @@
       <alignment horizontal="right"/>
     </xf>
     <xf numFmtId="0" fontId="3" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="right"/>
+    </xf>
+    <xf numFmtId="164" fontId="4" fillId="2" borderId="2" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="right" vertical="top"/>
+    </xf>
+    <xf numFmtId="3" fontId="4" fillId="2" borderId="2" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="right"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="2" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="right"/>
+    </xf>
+    <xf numFmtId="164" fontId="3" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="right" vertical="top"/>
+    </xf>
+    <xf numFmtId="3" fontId="3" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="right"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="right"/>
     </xf>
   </cellXfs>
@@ -399,8 +439,8 @@
 </file>
 
 <file path=xl/tables/table1.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="1" xr:uid="{00000000-000C-0000-FFFF-FFFF00000000}" name="Tabela1" displayName="Tabela1" ref="A1:J75" totalsRowShown="0" headerRowDxfId="11" dataDxfId="10">
-  <autoFilter ref="A1:J75" xr:uid="{00000000-0009-0000-0100-000001000000}">
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="1" xr:uid="{00000000-000C-0000-FFFF-FFFF00000000}" name="Tabela1" displayName="Tabela1" ref="A1:J103" totalsRowShown="0" headerRowDxfId="11" dataDxfId="10">
+  <autoFilter ref="A1:J103" xr:uid="{00000000-0009-0000-0100-000001000000}">
     <filterColumn colId="0" hiddenButton="1"/>
     <filterColumn colId="1" hiddenButton="1"/>
     <filterColumn colId="2" hiddenButton="1"/>
@@ -696,10 +736,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:J75"/>
+  <dimension ref="A1:J103"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A40" zoomScale="89" zoomScaleNormal="89" workbookViewId="0">
-      <selection activeCell="J74" sqref="J74"/>
+    <sheetView tabSelected="1" topLeftCell="A77" zoomScale="89" zoomScaleNormal="89" workbookViewId="0">
+      <selection activeCell="A103" sqref="A103:J103"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -3117,6 +3157,902 @@
         <v>0</v>
       </c>
     </row>
+    <row r="76" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A76" s="20">
+        <v>43976</v>
+      </c>
+      <c r="B76" s="21">
+        <v>75770</v>
+      </c>
+      <c r="C76" s="22">
+        <v>754</v>
+      </c>
+      <c r="D76" s="22">
+        <v>1469</v>
+      </c>
+      <c r="E76" s="22">
+        <v>0</v>
+      </c>
+      <c r="F76" s="22">
+        <v>9</v>
+      </c>
+      <c r="G76" s="22">
+        <v>2</v>
+      </c>
+      <c r="H76" s="22">
+        <v>6</v>
+      </c>
+      <c r="I76" s="22">
+        <v>108</v>
+      </c>
+      <c r="J76" s="22">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="77" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A77" s="20">
+        <v>43977</v>
+      </c>
+      <c r="B77" s="21">
+        <v>76579</v>
+      </c>
+      <c r="C77" s="22">
+        <v>809</v>
+      </c>
+      <c r="D77" s="22">
+        <v>1471</v>
+      </c>
+      <c r="E77" s="22">
+        <v>2</v>
+      </c>
+      <c r="F77" s="22">
+        <v>8</v>
+      </c>
+      <c r="G77" s="22">
+        <v>2</v>
+      </c>
+      <c r="H77" s="22">
+        <v>2</v>
+      </c>
+      <c r="I77" s="22">
+        <v>108</v>
+      </c>
+      <c r="J77" s="22">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="78" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A78" s="20">
+        <v>43978</v>
+      </c>
+      <c r="B78" s="21">
+        <v>77210</v>
+      </c>
+      <c r="C78" s="22">
+        <v>631</v>
+      </c>
+      <c r="D78" s="22">
+        <v>1473</v>
+      </c>
+      <c r="E78" s="22">
+        <v>2</v>
+      </c>
+      <c r="F78" s="22">
+        <v>7</v>
+      </c>
+      <c r="G78" s="22">
+        <v>2</v>
+      </c>
+      <c r="H78" s="22">
+        <v>1</v>
+      </c>
+      <c r="I78" s="22">
+        <v>108</v>
+      </c>
+      <c r="J78" s="22">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="79" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A79" s="20">
+        <v>43979</v>
+      </c>
+      <c r="B79" s="21">
+        <v>77916</v>
+      </c>
+      <c r="C79" s="22">
+        <v>706</v>
+      </c>
+      <c r="D79" s="22">
+        <v>1473</v>
+      </c>
+      <c r="E79" s="22">
+        <v>0</v>
+      </c>
+      <c r="F79" s="22">
+        <v>7</v>
+      </c>
+      <c r="G79" s="22">
+        <v>2</v>
+      </c>
+      <c r="H79" s="22">
+        <v>0</v>
+      </c>
+      <c r="I79" s="22">
+        <v>108</v>
+      </c>
+      <c r="J79" s="22">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="80" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A80" s="20">
+        <v>43980</v>
+      </c>
+      <c r="B80" s="21">
+        <v>78529</v>
+      </c>
+      <c r="C80" s="22">
+        <v>613</v>
+      </c>
+      <c r="D80" s="22">
+        <v>1473</v>
+      </c>
+      <c r="E80" s="22">
+        <v>0</v>
+      </c>
+      <c r="F80" s="22">
+        <v>7</v>
+      </c>
+      <c r="G80" s="22">
+        <v>2</v>
+      </c>
+      <c r="H80" s="22">
+        <v>0</v>
+      </c>
+      <c r="I80" s="22">
+        <v>108</v>
+      </c>
+      <c r="J80" s="22">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="81" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A81" s="20">
+        <v>43981</v>
+      </c>
+      <c r="B81" s="22">
+        <v>78793</v>
+      </c>
+      <c r="C81" s="22">
+        <v>264</v>
+      </c>
+      <c r="D81" s="22">
+        <v>1473</v>
+      </c>
+      <c r="E81" s="22">
+        <v>0</v>
+      </c>
+      <c r="F81" s="22">
+        <v>6</v>
+      </c>
+      <c r="G81" s="22">
+        <v>2</v>
+      </c>
+      <c r="H81" s="22">
+        <v>1</v>
+      </c>
+      <c r="I81" s="22">
+        <v>108</v>
+      </c>
+      <c r="J81" s="22">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="82" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A82" s="20">
+        <v>43982</v>
+      </c>
+      <c r="B82" s="21">
+        <v>79039</v>
+      </c>
+      <c r="C82" s="22">
+        <v>246</v>
+      </c>
+      <c r="D82" s="22">
+        <v>1473</v>
+      </c>
+      <c r="E82" s="22">
+        <v>0</v>
+      </c>
+      <c r="F82" s="22">
+        <v>5</v>
+      </c>
+      <c r="G82" s="22">
+        <v>1</v>
+      </c>
+      <c r="H82" s="22">
+        <v>0</v>
+      </c>
+      <c r="I82" s="22">
+        <v>109</v>
+      </c>
+      <c r="J82" s="22">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="83" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A83" s="20">
+        <v>43983</v>
+      </c>
+      <c r="B83" s="21">
+        <v>79698</v>
+      </c>
+      <c r="C83" s="22">
+        <v>659</v>
+      </c>
+      <c r="D83" s="22">
+        <v>1475</v>
+      </c>
+      <c r="E83" s="22">
+        <v>2</v>
+      </c>
+      <c r="F83" s="22">
+        <v>5</v>
+      </c>
+      <c r="G83" s="22">
+        <v>1</v>
+      </c>
+      <c r="H83" s="22">
+        <v>0</v>
+      </c>
+      <c r="I83" s="22">
+        <v>109</v>
+      </c>
+      <c r="J83" s="22">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="84" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A84" s="20">
+        <v>43984</v>
+      </c>
+      <c r="B84" s="21">
+        <v>80505</v>
+      </c>
+      <c r="C84" s="22">
+        <v>807</v>
+      </c>
+      <c r="D84" s="22">
+        <v>1477</v>
+      </c>
+      <c r="E84" s="22">
+        <v>2</v>
+      </c>
+      <c r="F84" s="22">
+        <v>5</v>
+      </c>
+      <c r="G84" s="22">
+        <v>0</v>
+      </c>
+      <c r="H84" s="22">
+        <v>0</v>
+      </c>
+      <c r="I84" s="22">
+        <v>109</v>
+      </c>
+      <c r="J84" s="22">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="85" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A85" s="20">
+        <v>43985</v>
+      </c>
+      <c r="B85" s="21">
+        <v>81333</v>
+      </c>
+      <c r="C85" s="22">
+        <v>828</v>
+      </c>
+      <c r="D85" s="22">
+        <v>1477</v>
+      </c>
+      <c r="E85" s="22">
+        <v>0</v>
+      </c>
+      <c r="F85" s="22">
+        <v>5</v>
+      </c>
+      <c r="G85" s="22">
+        <v>0</v>
+      </c>
+      <c r="H85" s="22">
+        <v>0</v>
+      </c>
+      <c r="I85" s="22">
+        <v>109</v>
+      </c>
+      <c r="J85" s="22">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="86" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A86" s="26">
+        <v>43986</v>
+      </c>
+      <c r="B86" s="27">
+        <v>82161</v>
+      </c>
+      <c r="C86" s="28">
+        <v>828</v>
+      </c>
+      <c r="D86" s="28">
+        <v>1479</v>
+      </c>
+      <c r="E86" s="28">
+        <v>2</v>
+      </c>
+      <c r="F86" s="28">
+        <v>6</v>
+      </c>
+      <c r="G86" s="28">
+        <v>0</v>
+      </c>
+      <c r="H86" s="28">
+        <v>0</v>
+      </c>
+      <c r="I86" s="28">
+        <v>109</v>
+      </c>
+      <c r="J86" s="28">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="87" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A87" s="29">
+        <v>43987</v>
+      </c>
+      <c r="B87" s="30">
+        <v>82876</v>
+      </c>
+      <c r="C87" s="31">
+        <v>715</v>
+      </c>
+      <c r="D87" s="31">
+        <v>1484</v>
+      </c>
+      <c r="E87" s="31">
+        <v>5</v>
+      </c>
+      <c r="F87" s="31">
+        <v>6</v>
+      </c>
+      <c r="G87" s="31">
+        <v>0</v>
+      </c>
+      <c r="H87" s="31">
+        <v>0</v>
+      </c>
+      <c r="I87" s="31">
+        <v>109</v>
+      </c>
+      <c r="J87" s="31">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="88" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A88" s="23">
+        <v>43988</v>
+      </c>
+      <c r="B88" s="24">
+        <v>83105</v>
+      </c>
+      <c r="C88" s="25">
+        <v>229</v>
+      </c>
+      <c r="D88" s="25">
+        <v>1485</v>
+      </c>
+      <c r="E88" s="25">
+        <v>1</v>
+      </c>
+      <c r="F88" s="25">
+        <v>5</v>
+      </c>
+      <c r="G88" s="25">
+        <v>0</v>
+      </c>
+      <c r="H88" s="25">
+        <v>1</v>
+      </c>
+      <c r="I88" s="25">
+        <v>109</v>
+      </c>
+      <c r="J88" s="25">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="89" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A89" s="29">
+        <v>43989</v>
+      </c>
+      <c r="B89" s="30">
+        <v>83316</v>
+      </c>
+      <c r="C89" s="31">
+        <v>211</v>
+      </c>
+      <c r="D89" s="31">
+        <v>1485</v>
+      </c>
+      <c r="E89" s="31">
+        <v>0</v>
+      </c>
+      <c r="F89" s="31">
+        <v>5</v>
+      </c>
+      <c r="G89" s="31">
+        <v>0</v>
+      </c>
+      <c r="H89" s="31">
+        <v>0</v>
+      </c>
+      <c r="I89" s="31">
+        <v>109</v>
+      </c>
+      <c r="J89" s="31">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="90" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A90" s="20">
+        <v>43990</v>
+      </c>
+      <c r="B90" s="21">
+        <v>84130</v>
+      </c>
+      <c r="C90" s="22">
+        <v>814</v>
+      </c>
+      <c r="D90" s="22">
+        <v>1486</v>
+      </c>
+      <c r="E90" s="22">
+        <v>1</v>
+      </c>
+      <c r="F90" s="22">
+        <v>6</v>
+      </c>
+      <c r="G90" s="22">
+        <v>0</v>
+      </c>
+      <c r="H90" s="22">
+        <v>0</v>
+      </c>
+      <c r="I90" s="22">
+        <v>109</v>
+      </c>
+      <c r="J90" s="22">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="91" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A91" s="20">
+        <v>43991</v>
+      </c>
+      <c r="B91" s="21">
+        <v>84868</v>
+      </c>
+      <c r="C91" s="22">
+        <v>738</v>
+      </c>
+      <c r="D91" s="22">
+        <v>1488</v>
+      </c>
+      <c r="E91" s="22">
+        <v>2</v>
+      </c>
+      <c r="F91" s="22">
+        <v>6</v>
+      </c>
+      <c r="G91" s="22">
+        <v>0</v>
+      </c>
+      <c r="H91" s="22">
+        <v>0</v>
+      </c>
+      <c r="I91" s="22">
+        <v>109</v>
+      </c>
+      <c r="J91" s="22">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="92" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A92" s="23">
+        <v>43992</v>
+      </c>
+      <c r="B92" s="24">
+        <v>85626</v>
+      </c>
+      <c r="C92" s="25">
+        <v>758</v>
+      </c>
+      <c r="D92" s="25">
+        <v>1488</v>
+      </c>
+      <c r="E92" s="25">
+        <v>0</v>
+      </c>
+      <c r="F92" s="25">
+        <v>6</v>
+      </c>
+      <c r="G92" s="25">
+        <v>0</v>
+      </c>
+      <c r="H92" s="25">
+        <v>0</v>
+      </c>
+      <c r="I92" s="25">
+        <v>109</v>
+      </c>
+      <c r="J92" s="25">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="93" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A93" s="29">
+        <v>43993</v>
+      </c>
+      <c r="B93" s="30">
+        <v>86328</v>
+      </c>
+      <c r="C93" s="31">
+        <v>702</v>
+      </c>
+      <c r="D93" s="31">
+        <v>1490</v>
+      </c>
+      <c r="E93" s="31">
+        <v>2</v>
+      </c>
+      <c r="F93" s="31">
+        <v>6</v>
+      </c>
+      <c r="G93" s="31">
+        <v>0</v>
+      </c>
+      <c r="H93" s="31">
+        <v>0</v>
+      </c>
+      <c r="I93" s="31">
+        <v>109</v>
+      </c>
+      <c r="J93" s="31">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="94" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A94" s="23">
+        <v>43994</v>
+      </c>
+      <c r="B94" s="24">
+        <v>87095</v>
+      </c>
+      <c r="C94" s="25">
+        <v>767</v>
+      </c>
+      <c r="D94" s="25">
+        <v>1492</v>
+      </c>
+      <c r="E94" s="25">
+        <v>2</v>
+      </c>
+      <c r="F94" s="25">
+        <v>6</v>
+      </c>
+      <c r="G94" s="25">
+        <v>0</v>
+      </c>
+      <c r="H94" s="25">
+        <v>0</v>
+      </c>
+      <c r="I94" s="25">
+        <v>109</v>
+      </c>
+      <c r="J94" s="25">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="95" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A95" s="29">
+        <v>43995</v>
+      </c>
+      <c r="B95" s="30">
+        <v>87386</v>
+      </c>
+      <c r="C95" s="31">
+        <v>291</v>
+      </c>
+      <c r="D95" s="31">
+        <v>1495</v>
+      </c>
+      <c r="E95" s="31">
+        <v>3</v>
+      </c>
+      <c r="F95" s="31">
+        <v>6</v>
+      </c>
+      <c r="G95" s="31">
+        <v>0</v>
+      </c>
+      <c r="H95" s="31">
+        <v>0</v>
+      </c>
+      <c r="I95" s="31">
+        <v>109</v>
+      </c>
+      <c r="J95" s="31">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="96" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A96" s="23">
+        <v>43996</v>
+      </c>
+      <c r="B96" s="24">
+        <v>87598</v>
+      </c>
+      <c r="C96" s="25">
+        <v>212</v>
+      </c>
+      <c r="D96" s="25">
+        <v>1496</v>
+      </c>
+      <c r="E96" s="25">
+        <v>1</v>
+      </c>
+      <c r="F96" s="25">
+        <v>7</v>
+      </c>
+      <c r="G96" s="25">
+        <v>1</v>
+      </c>
+      <c r="H96" s="25">
+        <v>0</v>
+      </c>
+      <c r="I96" s="25">
+        <v>109</v>
+      </c>
+      <c r="J96" s="25">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="97" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A97" s="20">
+        <v>43997</v>
+      </c>
+      <c r="B97" s="21">
+        <v>88165</v>
+      </c>
+      <c r="C97" s="22">
+        <v>567</v>
+      </c>
+      <c r="D97" s="22">
+        <v>1499</v>
+      </c>
+      <c r="E97" s="22">
+        <v>3</v>
+      </c>
+      <c r="F97" s="22">
+        <v>7</v>
+      </c>
+      <c r="G97" s="22">
+        <v>1</v>
+      </c>
+      <c r="H97" s="22">
+        <v>0</v>
+      </c>
+      <c r="I97" s="22">
+        <v>109</v>
+      </c>
+      <c r="J97" s="22">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="98" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A98" s="20">
+        <v>43998</v>
+      </c>
+      <c r="B98" s="21">
+        <v>89151</v>
+      </c>
+      <c r="C98" s="22">
+        <v>986</v>
+      </c>
+      <c r="D98" s="22">
+        <v>1503</v>
+      </c>
+      <c r="E98" s="22">
+        <v>4</v>
+      </c>
+      <c r="F98" s="22">
+        <v>7</v>
+      </c>
+      <c r="G98" s="22">
+        <v>1</v>
+      </c>
+      <c r="H98" s="22">
+        <v>0</v>
+      </c>
+      <c r="I98" s="22">
+        <v>109</v>
+      </c>
+      <c r="J98" s="22">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="99" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A99" s="29">
+        <v>43999</v>
+      </c>
+      <c r="B99" s="30">
+        <v>90103</v>
+      </c>
+      <c r="C99" s="31">
+        <v>952</v>
+      </c>
+      <c r="D99" s="31">
+        <v>1511</v>
+      </c>
+      <c r="E99" s="31">
+        <v>8</v>
+      </c>
+      <c r="F99" s="31">
+        <v>6</v>
+      </c>
+      <c r="G99" s="31">
+        <v>1</v>
+      </c>
+      <c r="H99" s="31">
+        <v>1</v>
+      </c>
+      <c r="I99" s="31">
+        <v>109</v>
+      </c>
+      <c r="J99" s="31">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="100" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A100" s="20">
+        <v>44000</v>
+      </c>
+      <c r="B100" s="21">
+        <v>91005</v>
+      </c>
+      <c r="C100" s="22">
+        <v>902</v>
+      </c>
+      <c r="D100" s="22">
+        <v>1513</v>
+      </c>
+      <c r="E100" s="22">
+        <v>2</v>
+      </c>
+      <c r="F100" s="22">
+        <v>8</v>
+      </c>
+      <c r="G100" s="22">
+        <v>1</v>
+      </c>
+      <c r="H100" s="22">
+        <v>0</v>
+      </c>
+      <c r="I100" s="22">
+        <v>109</v>
+      </c>
+      <c r="J100" s="22">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="101" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A101" s="29">
+        <v>44001</v>
+      </c>
+      <c r="B101" s="30">
+        <v>92152</v>
+      </c>
+      <c r="C101" s="31">
+        <v>1147</v>
+      </c>
+      <c r="D101" s="31">
+        <v>1519</v>
+      </c>
+      <c r="E101" s="31">
+        <v>6</v>
+      </c>
+      <c r="F101" s="31">
+        <v>6</v>
+      </c>
+      <c r="G101" s="31">
+        <v>1</v>
+      </c>
+      <c r="H101" s="31">
+        <v>2</v>
+      </c>
+      <c r="I101" s="31">
+        <v>109</v>
+      </c>
+      <c r="J101" s="31">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="102" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A102" s="23">
+        <v>44002</v>
+      </c>
+      <c r="B102" s="24">
+        <v>92919</v>
+      </c>
+      <c r="C102" s="25">
+        <v>758</v>
+      </c>
+      <c r="D102" s="25">
+        <v>1520</v>
+      </c>
+      <c r="E102" s="25">
+        <v>1</v>
+      </c>
+      <c r="F102" s="25">
+        <v>6</v>
+      </c>
+      <c r="G102" s="25">
+        <v>1</v>
+      </c>
+      <c r="H102" s="25">
+        <v>2</v>
+      </c>
+      <c r="I102" s="25">
+        <v>109</v>
+      </c>
+      <c r="J102" s="25">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="103" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A103" s="29">
+        <v>44003</v>
+      </c>
+      <c r="B103" s="30">
+        <v>93181</v>
+      </c>
+      <c r="C103" s="31">
+        <v>271</v>
+      </c>
+      <c r="D103" s="31">
+        <v>1521</v>
+      </c>
+      <c r="E103" s="31">
+        <v>1</v>
+      </c>
+      <c r="F103" s="31">
+        <v>6</v>
+      </c>
+      <c r="G103" s="31">
+        <v>1</v>
+      </c>
+      <c r="H103" s="31">
+        <v>0</v>
+      </c>
+      <c r="I103" s="31">
+        <v>109</v>
+      </c>
+      <c r="J103" s="31">
+        <v>0</v>
+      </c>
+    </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>

</xml_diff>

<commit_message>
Data updated by GitHub Bot (2020-06-23 12)
</commit_message>
<xml_diff>
--- a/output/snapshot/fdcf2531-4c3e-5c02-b63c-ee160ead6dea.xlsx
+++ b/output/snapshot/fdcf2531-4c3e-5c02-b63c-ee160ead6dea.xlsx
@@ -1,16 +1,15 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="21929"/>
-  <workbookPr/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
+  <fileVersion appName="xl" lastEdited="6" lowestEdited="6" rupBuild="14420"/>
+  <workbookPr defaultThemeVersion="164011"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="I:\AKTUALNI PODATKI - KORONA\Za objavo na GOV.SI\ang\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{1E6DD62F-2BE2-47DC-A7ED-9B57C1589256}" xr6:coauthVersionLast="44" xr6:coauthVersionMax="44" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840"/>
   </bookViews>
   <sheets>
     <sheet name="Covid-19 podatki" sheetId="1" r:id="rId1"/>
@@ -60,11 +59,11 @@
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" mc:Ignorable="x14ac x16r2">
   <numFmts count="1">
     <numFmt numFmtId="164" formatCode="d/\ m/\ yyyy;@"/>
   </numFmts>
-  <fonts count="4" x14ac:knownFonts="1">
+  <fonts count="5" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -93,6 +92,13 @@
       <name val="Calibri Light"/>
       <scheme val="major"/>
     </font>
+    <font>
+      <sz val="10"/>
+      <color theme="1"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
   </fonts>
   <fills count="3">
     <fill>
@@ -108,7 +114,7 @@
       </patternFill>
     </fill>
   </fills>
-  <borders count="2">
+  <borders count="3">
     <border>
       <left/>
       <right/>
@@ -129,11 +135,26 @@
       <bottom/>
       <diagonal/>
     </border>
+    <border>
+      <left style="thin">
+        <color theme="4"/>
+      </left>
+      <right style="thin">
+        <color theme="4"/>
+      </right>
+      <top style="thin">
+        <color theme="4"/>
+      </top>
+      <bottom style="thin">
+        <color theme="4"/>
+      </bottom>
+      <diagonal/>
+    </border>
   </borders>
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="26">
+  <cellXfs count="32">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="49" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyAlignment="1" applyProtection="1">
       <alignment horizontal="left" vertical="top"/>
@@ -208,6 +229,24 @@
       <alignment horizontal="right"/>
     </xf>
     <xf numFmtId="0" fontId="3" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="right"/>
+    </xf>
+    <xf numFmtId="164" fontId="4" fillId="2" borderId="2" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="right" vertical="top"/>
+    </xf>
+    <xf numFmtId="3" fontId="4" fillId="2" borderId="2" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="right"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="2" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="right"/>
+    </xf>
+    <xf numFmtId="164" fontId="3" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="right" vertical="top"/>
+    </xf>
+    <xf numFmtId="3" fontId="3" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="right"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="right"/>
     </xf>
   </cellXfs>
@@ -399,8 +438,8 @@
 </file>
 
 <file path=xl/tables/table1.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="1" xr:uid="{00000000-000C-0000-FFFF-FFFF00000000}" name="Tabela1" displayName="Tabela1" ref="A1:J75" totalsRowShown="0" headerRowDxfId="11" dataDxfId="10">
-  <autoFilter ref="A1:J75" xr:uid="{00000000-0009-0000-0100-000001000000}">
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="1" name="Tabela1" displayName="Tabela1" ref="A1:J104" totalsRowShown="0" headerRowDxfId="11" dataDxfId="10">
+  <autoFilter ref="A1:J104">
     <filterColumn colId="0" hiddenButton="1"/>
     <filterColumn colId="1" hiddenButton="1"/>
     <filterColumn colId="2" hiddenButton="1"/>
@@ -413,16 +452,16 @@
     <filterColumn colId="9" hiddenButton="1"/>
   </autoFilter>
   <tableColumns count="10">
-    <tableColumn id="1" xr3:uid="{00000000-0010-0000-0000-000001000000}" name="Date" dataDxfId="9"/>
-    <tableColumn id="2" xr3:uid="{00000000-0010-0000-0000-000002000000}" name="Tested (all)" dataDxfId="8"/>
-    <tableColumn id="3" xr3:uid="{00000000-0010-0000-0000-000003000000}" name="Tested (daily)" dataDxfId="7"/>
-    <tableColumn id="4" xr3:uid="{00000000-0010-0000-0000-000004000000}" name="Positive (all)" dataDxfId="6"/>
-    <tableColumn id="5" xr3:uid="{00000000-0010-0000-0000-000005000000}" name="Positive (daily)" dataDxfId="5"/>
-    <tableColumn id="6" xr3:uid="{00000000-0010-0000-0000-000006000000}" name="All hospitalized on certain day" dataDxfId="4"/>
-    <tableColumn id="7" xr3:uid="{00000000-0010-0000-0000-000007000000}" name="All persons in intensive care on certain day" dataDxfId="3"/>
-    <tableColumn id="10" xr3:uid="{00000000-0010-0000-0000-00000A000000}" name="Discharged" dataDxfId="2"/>
-    <tableColumn id="8" xr3:uid="{00000000-0010-0000-0000-000008000000}" name="Deaths (all)" dataDxfId="1"/>
-    <tableColumn id="9" xr3:uid="{00000000-0010-0000-0000-000009000000}" name="Deaths (daily)" dataDxfId="0"/>
+    <tableColumn id="1" name="Date" dataDxfId="9"/>
+    <tableColumn id="2" name="Tested (all)" dataDxfId="8"/>
+    <tableColumn id="3" name="Tested (daily)" dataDxfId="7"/>
+    <tableColumn id="4" name="Positive (all)" dataDxfId="6"/>
+    <tableColumn id="5" name="Positive (daily)" dataDxfId="5"/>
+    <tableColumn id="6" name="All hospitalized on certain day" dataDxfId="4"/>
+    <tableColumn id="7" name="All persons in intensive care on certain day" dataDxfId="3"/>
+    <tableColumn id="10" name="Discharged" dataDxfId="2"/>
+    <tableColumn id="8" name="Deaths (all)" dataDxfId="1"/>
+    <tableColumn id="9" name="Deaths (daily)" dataDxfId="0"/>
   </tableColumns>
   <tableStyleInfo name="TableStyleLight16" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
   <extLst>
@@ -695,11 +734,11 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:J75"/>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <dimension ref="A1:J104"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A40" zoomScale="89" zoomScaleNormal="89" workbookViewId="0">
-      <selection activeCell="J74" sqref="J74"/>
+    <sheetView tabSelected="1" topLeftCell="A77" zoomScale="89" zoomScaleNormal="89" workbookViewId="0">
+      <selection activeCell="A103" sqref="A103"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -3117,6 +3156,934 @@
         <v>0</v>
       </c>
     </row>
+    <row r="76" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A76" s="20">
+        <v>43976</v>
+      </c>
+      <c r="B76" s="21">
+        <v>75770</v>
+      </c>
+      <c r="C76" s="22">
+        <v>754</v>
+      </c>
+      <c r="D76" s="22">
+        <v>1469</v>
+      </c>
+      <c r="E76" s="22">
+        <v>0</v>
+      </c>
+      <c r="F76" s="22">
+        <v>9</v>
+      </c>
+      <c r="G76" s="22">
+        <v>2</v>
+      </c>
+      <c r="H76" s="22">
+        <v>6</v>
+      </c>
+      <c r="I76" s="22">
+        <v>108</v>
+      </c>
+      <c r="J76" s="22">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="77" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A77" s="20">
+        <v>43977</v>
+      </c>
+      <c r="B77" s="21">
+        <v>76579</v>
+      </c>
+      <c r="C77" s="22">
+        <v>809</v>
+      </c>
+      <c r="D77" s="22">
+        <v>1471</v>
+      </c>
+      <c r="E77" s="22">
+        <v>2</v>
+      </c>
+      <c r="F77" s="22">
+        <v>8</v>
+      </c>
+      <c r="G77" s="22">
+        <v>2</v>
+      </c>
+      <c r="H77" s="22">
+        <v>2</v>
+      </c>
+      <c r="I77" s="22">
+        <v>108</v>
+      </c>
+      <c r="J77" s="22">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="78" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A78" s="20">
+        <v>43978</v>
+      </c>
+      <c r="B78" s="21">
+        <v>77210</v>
+      </c>
+      <c r="C78" s="22">
+        <v>631</v>
+      </c>
+      <c r="D78" s="22">
+        <v>1473</v>
+      </c>
+      <c r="E78" s="22">
+        <v>2</v>
+      </c>
+      <c r="F78" s="22">
+        <v>7</v>
+      </c>
+      <c r="G78" s="22">
+        <v>2</v>
+      </c>
+      <c r="H78" s="22">
+        <v>1</v>
+      </c>
+      <c r="I78" s="22">
+        <v>108</v>
+      </c>
+      <c r="J78" s="22">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="79" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A79" s="20">
+        <v>43979</v>
+      </c>
+      <c r="B79" s="21">
+        <v>77916</v>
+      </c>
+      <c r="C79" s="22">
+        <v>706</v>
+      </c>
+      <c r="D79" s="22">
+        <v>1473</v>
+      </c>
+      <c r="E79" s="22">
+        <v>0</v>
+      </c>
+      <c r="F79" s="22">
+        <v>7</v>
+      </c>
+      <c r="G79" s="22">
+        <v>2</v>
+      </c>
+      <c r="H79" s="22">
+        <v>0</v>
+      </c>
+      <c r="I79" s="22">
+        <v>108</v>
+      </c>
+      <c r="J79" s="22">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="80" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A80" s="20">
+        <v>43980</v>
+      </c>
+      <c r="B80" s="21">
+        <v>78529</v>
+      </c>
+      <c r="C80" s="22">
+        <v>613</v>
+      </c>
+      <c r="D80" s="22">
+        <v>1473</v>
+      </c>
+      <c r="E80" s="22">
+        <v>0</v>
+      </c>
+      <c r="F80" s="22">
+        <v>7</v>
+      </c>
+      <c r="G80" s="22">
+        <v>2</v>
+      </c>
+      <c r="H80" s="22">
+        <v>0</v>
+      </c>
+      <c r="I80" s="22">
+        <v>108</v>
+      </c>
+      <c r="J80" s="22">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="81" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A81" s="20">
+        <v>43981</v>
+      </c>
+      <c r="B81" s="22">
+        <v>78793</v>
+      </c>
+      <c r="C81" s="22">
+        <v>264</v>
+      </c>
+      <c r="D81" s="22">
+        <v>1473</v>
+      </c>
+      <c r="E81" s="22">
+        <v>0</v>
+      </c>
+      <c r="F81" s="22">
+        <v>6</v>
+      </c>
+      <c r="G81" s="22">
+        <v>2</v>
+      </c>
+      <c r="H81" s="22">
+        <v>1</v>
+      </c>
+      <c r="I81" s="22">
+        <v>108</v>
+      </c>
+      <c r="J81" s="22">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="82" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A82" s="20">
+        <v>43982</v>
+      </c>
+      <c r="B82" s="21">
+        <v>79039</v>
+      </c>
+      <c r="C82" s="22">
+        <v>246</v>
+      </c>
+      <c r="D82" s="22">
+        <v>1473</v>
+      </c>
+      <c r="E82" s="22">
+        <v>0</v>
+      </c>
+      <c r="F82" s="22">
+        <v>5</v>
+      </c>
+      <c r="G82" s="22">
+        <v>1</v>
+      </c>
+      <c r="H82" s="22">
+        <v>0</v>
+      </c>
+      <c r="I82" s="22">
+        <v>109</v>
+      </c>
+      <c r="J82" s="22">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="83" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A83" s="20">
+        <v>43983</v>
+      </c>
+      <c r="B83" s="21">
+        <v>79698</v>
+      </c>
+      <c r="C83" s="22">
+        <v>659</v>
+      </c>
+      <c r="D83" s="22">
+        <v>1475</v>
+      </c>
+      <c r="E83" s="22">
+        <v>2</v>
+      </c>
+      <c r="F83" s="22">
+        <v>5</v>
+      </c>
+      <c r="G83" s="22">
+        <v>1</v>
+      </c>
+      <c r="H83" s="22">
+        <v>0</v>
+      </c>
+      <c r="I83" s="22">
+        <v>109</v>
+      </c>
+      <c r="J83" s="22">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="84" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A84" s="20">
+        <v>43984</v>
+      </c>
+      <c r="B84" s="21">
+        <v>80505</v>
+      </c>
+      <c r="C84" s="22">
+        <v>807</v>
+      </c>
+      <c r="D84" s="22">
+        <v>1477</v>
+      </c>
+      <c r="E84" s="22">
+        <v>2</v>
+      </c>
+      <c r="F84" s="22">
+        <v>5</v>
+      </c>
+      <c r="G84" s="22">
+        <v>0</v>
+      </c>
+      <c r="H84" s="22">
+        <v>0</v>
+      </c>
+      <c r="I84" s="22">
+        <v>109</v>
+      </c>
+      <c r="J84" s="22">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="85" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A85" s="20">
+        <v>43985</v>
+      </c>
+      <c r="B85" s="21">
+        <v>81333</v>
+      </c>
+      <c r="C85" s="22">
+        <v>828</v>
+      </c>
+      <c r="D85" s="22">
+        <v>1477</v>
+      </c>
+      <c r="E85" s="22">
+        <v>0</v>
+      </c>
+      <c r="F85" s="22">
+        <v>5</v>
+      </c>
+      <c r="G85" s="22">
+        <v>0</v>
+      </c>
+      <c r="H85" s="22">
+        <v>0</v>
+      </c>
+      <c r="I85" s="22">
+        <v>109</v>
+      </c>
+      <c r="J85" s="22">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="86" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A86" s="26">
+        <v>43986</v>
+      </c>
+      <c r="B86" s="27">
+        <v>82161</v>
+      </c>
+      <c r="C86" s="28">
+        <v>828</v>
+      </c>
+      <c r="D86" s="28">
+        <v>1479</v>
+      </c>
+      <c r="E86" s="28">
+        <v>2</v>
+      </c>
+      <c r="F86" s="28">
+        <v>6</v>
+      </c>
+      <c r="G86" s="28">
+        <v>0</v>
+      </c>
+      <c r="H86" s="28">
+        <v>0</v>
+      </c>
+      <c r="I86" s="28">
+        <v>109</v>
+      </c>
+      <c r="J86" s="28">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="87" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A87" s="29">
+        <v>43987</v>
+      </c>
+      <c r="B87" s="30">
+        <v>82876</v>
+      </c>
+      <c r="C87" s="31">
+        <v>715</v>
+      </c>
+      <c r="D87" s="31">
+        <v>1484</v>
+      </c>
+      <c r="E87" s="31">
+        <v>5</v>
+      </c>
+      <c r="F87" s="31">
+        <v>6</v>
+      </c>
+      <c r="G87" s="31">
+        <v>0</v>
+      </c>
+      <c r="H87" s="31">
+        <v>0</v>
+      </c>
+      <c r="I87" s="31">
+        <v>109</v>
+      </c>
+      <c r="J87" s="31">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="88" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A88" s="23">
+        <v>43988</v>
+      </c>
+      <c r="B88" s="24">
+        <v>83105</v>
+      </c>
+      <c r="C88" s="25">
+        <v>229</v>
+      </c>
+      <c r="D88" s="25">
+        <v>1485</v>
+      </c>
+      <c r="E88" s="25">
+        <v>1</v>
+      </c>
+      <c r="F88" s="25">
+        <v>5</v>
+      </c>
+      <c r="G88" s="25">
+        <v>0</v>
+      </c>
+      <c r="H88" s="25">
+        <v>1</v>
+      </c>
+      <c r="I88" s="25">
+        <v>109</v>
+      </c>
+      <c r="J88" s="25">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="89" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A89" s="29">
+        <v>43989</v>
+      </c>
+      <c r="B89" s="30">
+        <v>83316</v>
+      </c>
+      <c r="C89" s="31">
+        <v>211</v>
+      </c>
+      <c r="D89" s="31">
+        <v>1485</v>
+      </c>
+      <c r="E89" s="31">
+        <v>0</v>
+      </c>
+      <c r="F89" s="31">
+        <v>5</v>
+      </c>
+      <c r="G89" s="31">
+        <v>0</v>
+      </c>
+      <c r="H89" s="31">
+        <v>0</v>
+      </c>
+      <c r="I89" s="31">
+        <v>109</v>
+      </c>
+      <c r="J89" s="31">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="90" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A90" s="20">
+        <v>43990</v>
+      </c>
+      <c r="B90" s="21">
+        <v>84130</v>
+      </c>
+      <c r="C90" s="22">
+        <v>814</v>
+      </c>
+      <c r="D90" s="22">
+        <v>1486</v>
+      </c>
+      <c r="E90" s="22">
+        <v>1</v>
+      </c>
+      <c r="F90" s="22">
+        <v>6</v>
+      </c>
+      <c r="G90" s="22">
+        <v>0</v>
+      </c>
+      <c r="H90" s="22">
+        <v>0</v>
+      </c>
+      <c r="I90" s="22">
+        <v>109</v>
+      </c>
+      <c r="J90" s="22">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="91" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A91" s="20">
+        <v>43991</v>
+      </c>
+      <c r="B91" s="21">
+        <v>84868</v>
+      </c>
+      <c r="C91" s="22">
+        <v>738</v>
+      </c>
+      <c r="D91" s="22">
+        <v>1488</v>
+      </c>
+      <c r="E91" s="22">
+        <v>2</v>
+      </c>
+      <c r="F91" s="22">
+        <v>6</v>
+      </c>
+      <c r="G91" s="22">
+        <v>0</v>
+      </c>
+      <c r="H91" s="22">
+        <v>0</v>
+      </c>
+      <c r="I91" s="22">
+        <v>109</v>
+      </c>
+      <c r="J91" s="22">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="92" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A92" s="23">
+        <v>43992</v>
+      </c>
+      <c r="B92" s="24">
+        <v>85626</v>
+      </c>
+      <c r="C92" s="25">
+        <v>758</v>
+      </c>
+      <c r="D92" s="25">
+        <v>1488</v>
+      </c>
+      <c r="E92" s="25">
+        <v>0</v>
+      </c>
+      <c r="F92" s="25">
+        <v>6</v>
+      </c>
+      <c r="G92" s="25">
+        <v>0</v>
+      </c>
+      <c r="H92" s="25">
+        <v>0</v>
+      </c>
+      <c r="I92" s="25">
+        <v>109</v>
+      </c>
+      <c r="J92" s="25">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="93" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A93" s="29">
+        <v>43993</v>
+      </c>
+      <c r="B93" s="30">
+        <v>86328</v>
+      </c>
+      <c r="C93" s="31">
+        <v>702</v>
+      </c>
+      <c r="D93" s="31">
+        <v>1490</v>
+      </c>
+      <c r="E93" s="31">
+        <v>2</v>
+      </c>
+      <c r="F93" s="31">
+        <v>6</v>
+      </c>
+      <c r="G93" s="31">
+        <v>0</v>
+      </c>
+      <c r="H93" s="31">
+        <v>0</v>
+      </c>
+      <c r="I93" s="31">
+        <v>109</v>
+      </c>
+      <c r="J93" s="31">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="94" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A94" s="23">
+        <v>43994</v>
+      </c>
+      <c r="B94" s="24">
+        <v>87095</v>
+      </c>
+      <c r="C94" s="25">
+        <v>767</v>
+      </c>
+      <c r="D94" s="25">
+        <v>1492</v>
+      </c>
+      <c r="E94" s="25">
+        <v>2</v>
+      </c>
+      <c r="F94" s="25">
+        <v>6</v>
+      </c>
+      <c r="G94" s="25">
+        <v>0</v>
+      </c>
+      <c r="H94" s="25">
+        <v>0</v>
+      </c>
+      <c r="I94" s="25">
+        <v>109</v>
+      </c>
+      <c r="J94" s="25">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="95" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A95" s="29">
+        <v>43995</v>
+      </c>
+      <c r="B95" s="30">
+        <v>87386</v>
+      </c>
+      <c r="C95" s="31">
+        <v>291</v>
+      </c>
+      <c r="D95" s="31">
+        <v>1495</v>
+      </c>
+      <c r="E95" s="31">
+        <v>3</v>
+      </c>
+      <c r="F95" s="31">
+        <v>6</v>
+      </c>
+      <c r="G95" s="31">
+        <v>0</v>
+      </c>
+      <c r="H95" s="31">
+        <v>0</v>
+      </c>
+      <c r="I95" s="31">
+        <v>109</v>
+      </c>
+      <c r="J95" s="31">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="96" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A96" s="23">
+        <v>43996</v>
+      </c>
+      <c r="B96" s="24">
+        <v>87598</v>
+      </c>
+      <c r="C96" s="25">
+        <v>212</v>
+      </c>
+      <c r="D96" s="25">
+        <v>1496</v>
+      </c>
+      <c r="E96" s="25">
+        <v>1</v>
+      </c>
+      <c r="F96" s="25">
+        <v>7</v>
+      </c>
+      <c r="G96" s="25">
+        <v>1</v>
+      </c>
+      <c r="H96" s="25">
+        <v>0</v>
+      </c>
+      <c r="I96" s="25">
+        <v>109</v>
+      </c>
+      <c r="J96" s="25">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="97" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A97" s="20">
+        <v>43997</v>
+      </c>
+      <c r="B97" s="21">
+        <v>88165</v>
+      </c>
+      <c r="C97" s="22">
+        <v>567</v>
+      </c>
+      <c r="D97" s="22">
+        <v>1499</v>
+      </c>
+      <c r="E97" s="22">
+        <v>3</v>
+      </c>
+      <c r="F97" s="22">
+        <v>7</v>
+      </c>
+      <c r="G97" s="22">
+        <v>1</v>
+      </c>
+      <c r="H97" s="22">
+        <v>0</v>
+      </c>
+      <c r="I97" s="22">
+        <v>109</v>
+      </c>
+      <c r="J97" s="22">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="98" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A98" s="20">
+        <v>43998</v>
+      </c>
+      <c r="B98" s="21">
+        <v>89151</v>
+      </c>
+      <c r="C98" s="22">
+        <v>986</v>
+      </c>
+      <c r="D98" s="22">
+        <v>1503</v>
+      </c>
+      <c r="E98" s="22">
+        <v>4</v>
+      </c>
+      <c r="F98" s="22">
+        <v>7</v>
+      </c>
+      <c r="G98" s="22">
+        <v>1</v>
+      </c>
+      <c r="H98" s="22">
+        <v>0</v>
+      </c>
+      <c r="I98" s="22">
+        <v>109</v>
+      </c>
+      <c r="J98" s="22">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="99" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A99" s="29">
+        <v>43999</v>
+      </c>
+      <c r="B99" s="30">
+        <v>90103</v>
+      </c>
+      <c r="C99" s="31">
+        <v>952</v>
+      </c>
+      <c r="D99" s="31">
+        <v>1511</v>
+      </c>
+      <c r="E99" s="31">
+        <v>8</v>
+      </c>
+      <c r="F99" s="31">
+        <v>6</v>
+      </c>
+      <c r="G99" s="31">
+        <v>1</v>
+      </c>
+      <c r="H99" s="31">
+        <v>1</v>
+      </c>
+      <c r="I99" s="31">
+        <v>109</v>
+      </c>
+      <c r="J99" s="31">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="100" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A100" s="20">
+        <v>44000</v>
+      </c>
+      <c r="B100" s="21">
+        <v>91005</v>
+      </c>
+      <c r="C100" s="22">
+        <v>902</v>
+      </c>
+      <c r="D100" s="22">
+        <v>1513</v>
+      </c>
+      <c r="E100" s="22">
+        <v>2</v>
+      </c>
+      <c r="F100" s="22">
+        <v>8</v>
+      </c>
+      <c r="G100" s="22">
+        <v>1</v>
+      </c>
+      <c r="H100" s="22">
+        <v>0</v>
+      </c>
+      <c r="I100" s="22">
+        <v>109</v>
+      </c>
+      <c r="J100" s="22">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="101" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A101" s="29">
+        <v>44001</v>
+      </c>
+      <c r="B101" s="30">
+        <v>92152</v>
+      </c>
+      <c r="C101" s="31">
+        <v>1147</v>
+      </c>
+      <c r="D101" s="31">
+        <v>1519</v>
+      </c>
+      <c r="E101" s="31">
+        <v>6</v>
+      </c>
+      <c r="F101" s="31">
+        <v>6</v>
+      </c>
+      <c r="G101" s="31">
+        <v>1</v>
+      </c>
+      <c r="H101" s="31">
+        <v>2</v>
+      </c>
+      <c r="I101" s="31">
+        <v>109</v>
+      </c>
+      <c r="J101" s="31">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="102" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A102" s="23">
+        <v>44002</v>
+      </c>
+      <c r="B102" s="24">
+        <v>92919</v>
+      </c>
+      <c r="C102" s="25">
+        <v>758</v>
+      </c>
+      <c r="D102" s="25">
+        <v>1520</v>
+      </c>
+      <c r="E102" s="25">
+        <v>1</v>
+      </c>
+      <c r="F102" s="25">
+        <v>6</v>
+      </c>
+      <c r="G102" s="25">
+        <v>1</v>
+      </c>
+      <c r="H102" s="25">
+        <v>2</v>
+      </c>
+      <c r="I102" s="25">
+        <v>109</v>
+      </c>
+      <c r="J102" s="25">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="103" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A103" s="29">
+        <v>44003</v>
+      </c>
+      <c r="B103" s="30">
+        <v>93181</v>
+      </c>
+      <c r="C103" s="31">
+        <v>271</v>
+      </c>
+      <c r="D103" s="31">
+        <v>1521</v>
+      </c>
+      <c r="E103" s="31">
+        <v>1</v>
+      </c>
+      <c r="F103" s="31">
+        <v>6</v>
+      </c>
+      <c r="G103" s="31">
+        <v>1</v>
+      </c>
+      <c r="H103" s="31">
+        <v>0</v>
+      </c>
+      <c r="I103" s="31">
+        <v>109</v>
+      </c>
+      <c r="J103" s="31">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="104" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A104" s="29">
+        <v>44004</v>
+      </c>
+      <c r="B104" s="30">
+        <v>94165</v>
+      </c>
+      <c r="C104" s="31">
+        <v>984</v>
+      </c>
+      <c r="D104" s="31">
+        <v>1534</v>
+      </c>
+      <c r="E104" s="31">
+        <v>13</v>
+      </c>
+      <c r="F104" s="31">
+        <v>5</v>
+      </c>
+      <c r="G104" s="31">
+        <v>1</v>
+      </c>
+      <c r="H104" s="31">
+        <v>1</v>
+      </c>
+      <c r="I104" s="31">
+        <v>109</v>
+      </c>
+      <c r="J104" s="31">
+        <v>0</v>
+      </c>
+    </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>

</xml_diff>

<commit_message>
Data updated by GitHub Bot (2020-06-23 20)
</commit_message>
<xml_diff>
--- a/output/snapshot/fdcf2531-4c3e-5c02-b63c-ee160ead6dea.xlsx
+++ b/output/snapshot/fdcf2531-4c3e-5c02-b63c-ee160ead6dea.xlsx
@@ -1,16 +1,15 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="21929"/>
-  <workbookPr/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
+  <fileVersion appName="xl" lastEdited="6" lowestEdited="6" rupBuild="14420"/>
+  <workbookPr defaultThemeVersion="164011"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="I:\AKTUALNI PODATKI - KORONA\Za objavo na GOV.SI\ang\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{1E6DD62F-2BE2-47DC-A7ED-9B57C1589256}" xr6:coauthVersionLast="44" xr6:coauthVersionMax="44" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840"/>
   </bookViews>
   <sheets>
     <sheet name="Covid-19 podatki" sheetId="1" r:id="rId1"/>
@@ -60,11 +59,11 @@
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" mc:Ignorable="x14ac x16r2">
   <numFmts count="1">
     <numFmt numFmtId="164" formatCode="d/\ m/\ yyyy;@"/>
   </numFmts>
-  <fonts count="4" x14ac:knownFonts="1">
+  <fonts count="5" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -93,6 +92,13 @@
       <name val="Calibri Light"/>
       <scheme val="major"/>
     </font>
+    <font>
+      <sz val="10"/>
+      <color theme="1"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
   </fonts>
   <fills count="3">
     <fill>
@@ -108,7 +114,7 @@
       </patternFill>
     </fill>
   </fills>
-  <borders count="2">
+  <borders count="3">
     <border>
       <left/>
       <right/>
@@ -129,11 +135,26 @@
       <bottom/>
       <diagonal/>
     </border>
+    <border>
+      <left style="thin">
+        <color theme="4"/>
+      </left>
+      <right style="thin">
+        <color theme="4"/>
+      </right>
+      <top style="thin">
+        <color theme="4"/>
+      </top>
+      <bottom style="thin">
+        <color theme="4"/>
+      </bottom>
+      <diagonal/>
+    </border>
   </borders>
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="26">
+  <cellXfs count="32">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="49" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyAlignment="1" applyProtection="1">
       <alignment horizontal="left" vertical="top"/>
@@ -208,6 +229,24 @@
       <alignment horizontal="right"/>
     </xf>
     <xf numFmtId="0" fontId="3" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="right"/>
+    </xf>
+    <xf numFmtId="164" fontId="4" fillId="2" borderId="2" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="right" vertical="top"/>
+    </xf>
+    <xf numFmtId="3" fontId="4" fillId="2" borderId="2" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="right"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="2" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="right"/>
+    </xf>
+    <xf numFmtId="164" fontId="3" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="right" vertical="top"/>
+    </xf>
+    <xf numFmtId="3" fontId="3" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="right"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="right"/>
     </xf>
   </cellXfs>
@@ -399,8 +438,8 @@
 </file>
 
 <file path=xl/tables/table1.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="1" xr:uid="{00000000-000C-0000-FFFF-FFFF00000000}" name="Tabela1" displayName="Tabela1" ref="A1:J75" totalsRowShown="0" headerRowDxfId="11" dataDxfId="10">
-  <autoFilter ref="A1:J75" xr:uid="{00000000-0009-0000-0100-000001000000}">
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="1" name="Tabela1" displayName="Tabela1" ref="A1:J104" totalsRowShown="0" headerRowDxfId="11" dataDxfId="10">
+  <autoFilter ref="A1:J104">
     <filterColumn colId="0" hiddenButton="1"/>
     <filterColumn colId="1" hiddenButton="1"/>
     <filterColumn colId="2" hiddenButton="1"/>
@@ -413,16 +452,16 @@
     <filterColumn colId="9" hiddenButton="1"/>
   </autoFilter>
   <tableColumns count="10">
-    <tableColumn id="1" xr3:uid="{00000000-0010-0000-0000-000001000000}" name="Date" dataDxfId="9"/>
-    <tableColumn id="2" xr3:uid="{00000000-0010-0000-0000-000002000000}" name="Tested (all)" dataDxfId="8"/>
-    <tableColumn id="3" xr3:uid="{00000000-0010-0000-0000-000003000000}" name="Tested (daily)" dataDxfId="7"/>
-    <tableColumn id="4" xr3:uid="{00000000-0010-0000-0000-000004000000}" name="Positive (all)" dataDxfId="6"/>
-    <tableColumn id="5" xr3:uid="{00000000-0010-0000-0000-000005000000}" name="Positive (daily)" dataDxfId="5"/>
-    <tableColumn id="6" xr3:uid="{00000000-0010-0000-0000-000006000000}" name="All hospitalized on certain day" dataDxfId="4"/>
-    <tableColumn id="7" xr3:uid="{00000000-0010-0000-0000-000007000000}" name="All persons in intensive care on certain day" dataDxfId="3"/>
-    <tableColumn id="10" xr3:uid="{00000000-0010-0000-0000-00000A000000}" name="Discharged" dataDxfId="2"/>
-    <tableColumn id="8" xr3:uid="{00000000-0010-0000-0000-000008000000}" name="Deaths (all)" dataDxfId="1"/>
-    <tableColumn id="9" xr3:uid="{00000000-0010-0000-0000-000009000000}" name="Deaths (daily)" dataDxfId="0"/>
+    <tableColumn id="1" name="Date" dataDxfId="9"/>
+    <tableColumn id="2" name="Tested (all)" dataDxfId="8"/>
+    <tableColumn id="3" name="Tested (daily)" dataDxfId="7"/>
+    <tableColumn id="4" name="Positive (all)" dataDxfId="6"/>
+    <tableColumn id="5" name="Positive (daily)" dataDxfId="5"/>
+    <tableColumn id="6" name="All hospitalized on certain day" dataDxfId="4"/>
+    <tableColumn id="7" name="All persons in intensive care on certain day" dataDxfId="3"/>
+    <tableColumn id="10" name="Discharged" dataDxfId="2"/>
+    <tableColumn id="8" name="Deaths (all)" dataDxfId="1"/>
+    <tableColumn id="9" name="Deaths (daily)" dataDxfId="0"/>
   </tableColumns>
   <tableStyleInfo name="TableStyleLight16" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
   <extLst>
@@ -695,11 +734,11 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:J75"/>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <dimension ref="A1:J104"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A40" zoomScale="89" zoomScaleNormal="89" workbookViewId="0">
-      <selection activeCell="J74" sqref="J74"/>
+    <sheetView tabSelected="1" topLeftCell="A77" zoomScale="89" zoomScaleNormal="89" workbookViewId="0">
+      <selection activeCell="A103" sqref="A103"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -3117,6 +3156,934 @@
         <v>0</v>
       </c>
     </row>
+    <row r="76" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A76" s="20">
+        <v>43976</v>
+      </c>
+      <c r="B76" s="21">
+        <v>75770</v>
+      </c>
+      <c r="C76" s="22">
+        <v>754</v>
+      </c>
+      <c r="D76" s="22">
+        <v>1469</v>
+      </c>
+      <c r="E76" s="22">
+        <v>0</v>
+      </c>
+      <c r="F76" s="22">
+        <v>9</v>
+      </c>
+      <c r="G76" s="22">
+        <v>2</v>
+      </c>
+      <c r="H76" s="22">
+        <v>6</v>
+      </c>
+      <c r="I76" s="22">
+        <v>108</v>
+      </c>
+      <c r="J76" s="22">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="77" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A77" s="20">
+        <v>43977</v>
+      </c>
+      <c r="B77" s="21">
+        <v>76579</v>
+      </c>
+      <c r="C77" s="22">
+        <v>809</v>
+      </c>
+      <c r="D77" s="22">
+        <v>1471</v>
+      </c>
+      <c r="E77" s="22">
+        <v>2</v>
+      </c>
+      <c r="F77" s="22">
+        <v>8</v>
+      </c>
+      <c r="G77" s="22">
+        <v>2</v>
+      </c>
+      <c r="H77" s="22">
+        <v>2</v>
+      </c>
+      <c r="I77" s="22">
+        <v>108</v>
+      </c>
+      <c r="J77" s="22">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="78" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A78" s="20">
+        <v>43978</v>
+      </c>
+      <c r="B78" s="21">
+        <v>77210</v>
+      </c>
+      <c r="C78" s="22">
+        <v>631</v>
+      </c>
+      <c r="D78" s="22">
+        <v>1473</v>
+      </c>
+      <c r="E78" s="22">
+        <v>2</v>
+      </c>
+      <c r="F78" s="22">
+        <v>7</v>
+      </c>
+      <c r="G78" s="22">
+        <v>2</v>
+      </c>
+      <c r="H78" s="22">
+        <v>1</v>
+      </c>
+      <c r="I78" s="22">
+        <v>108</v>
+      </c>
+      <c r="J78" s="22">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="79" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A79" s="20">
+        <v>43979</v>
+      </c>
+      <c r="B79" s="21">
+        <v>77916</v>
+      </c>
+      <c r="C79" s="22">
+        <v>706</v>
+      </c>
+      <c r="D79" s="22">
+        <v>1473</v>
+      </c>
+      <c r="E79" s="22">
+        <v>0</v>
+      </c>
+      <c r="F79" s="22">
+        <v>7</v>
+      </c>
+      <c r="G79" s="22">
+        <v>2</v>
+      </c>
+      <c r="H79" s="22">
+        <v>0</v>
+      </c>
+      <c r="I79" s="22">
+        <v>108</v>
+      </c>
+      <c r="J79" s="22">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="80" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A80" s="20">
+        <v>43980</v>
+      </c>
+      <c r="B80" s="21">
+        <v>78529</v>
+      </c>
+      <c r="C80" s="22">
+        <v>613</v>
+      </c>
+      <c r="D80" s="22">
+        <v>1473</v>
+      </c>
+      <c r="E80" s="22">
+        <v>0</v>
+      </c>
+      <c r="F80" s="22">
+        <v>7</v>
+      </c>
+      <c r="G80" s="22">
+        <v>2</v>
+      </c>
+      <c r="H80" s="22">
+        <v>0</v>
+      </c>
+      <c r="I80" s="22">
+        <v>108</v>
+      </c>
+      <c r="J80" s="22">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="81" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A81" s="20">
+        <v>43981</v>
+      </c>
+      <c r="B81" s="22">
+        <v>78793</v>
+      </c>
+      <c r="C81" s="22">
+        <v>264</v>
+      </c>
+      <c r="D81" s="22">
+        <v>1473</v>
+      </c>
+      <c r="E81" s="22">
+        <v>0</v>
+      </c>
+      <c r="F81" s="22">
+        <v>6</v>
+      </c>
+      <c r="G81" s="22">
+        <v>2</v>
+      </c>
+      <c r="H81" s="22">
+        <v>1</v>
+      </c>
+      <c r="I81" s="22">
+        <v>108</v>
+      </c>
+      <c r="J81" s="22">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="82" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A82" s="20">
+        <v>43982</v>
+      </c>
+      <c r="B82" s="21">
+        <v>79039</v>
+      </c>
+      <c r="C82" s="22">
+        <v>246</v>
+      </c>
+      <c r="D82" s="22">
+        <v>1473</v>
+      </c>
+      <c r="E82" s="22">
+        <v>0</v>
+      </c>
+      <c r="F82" s="22">
+        <v>5</v>
+      </c>
+      <c r="G82" s="22">
+        <v>1</v>
+      </c>
+      <c r="H82" s="22">
+        <v>0</v>
+      </c>
+      <c r="I82" s="22">
+        <v>109</v>
+      </c>
+      <c r="J82" s="22">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="83" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A83" s="20">
+        <v>43983</v>
+      </c>
+      <c r="B83" s="21">
+        <v>79698</v>
+      </c>
+      <c r="C83" s="22">
+        <v>659</v>
+      </c>
+      <c r="D83" s="22">
+        <v>1475</v>
+      </c>
+      <c r="E83" s="22">
+        <v>2</v>
+      </c>
+      <c r="F83" s="22">
+        <v>5</v>
+      </c>
+      <c r="G83" s="22">
+        <v>1</v>
+      </c>
+      <c r="H83" s="22">
+        <v>0</v>
+      </c>
+      <c r="I83" s="22">
+        <v>109</v>
+      </c>
+      <c r="J83" s="22">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="84" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A84" s="20">
+        <v>43984</v>
+      </c>
+      <c r="B84" s="21">
+        <v>80505</v>
+      </c>
+      <c r="C84" s="22">
+        <v>807</v>
+      </c>
+      <c r="D84" s="22">
+        <v>1477</v>
+      </c>
+      <c r="E84" s="22">
+        <v>2</v>
+      </c>
+      <c r="F84" s="22">
+        <v>5</v>
+      </c>
+      <c r="G84" s="22">
+        <v>0</v>
+      </c>
+      <c r="H84" s="22">
+        <v>0</v>
+      </c>
+      <c r="I84" s="22">
+        <v>109</v>
+      </c>
+      <c r="J84" s="22">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="85" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A85" s="20">
+        <v>43985</v>
+      </c>
+      <c r="B85" s="21">
+        <v>81333</v>
+      </c>
+      <c r="C85" s="22">
+        <v>828</v>
+      </c>
+      <c r="D85" s="22">
+        <v>1477</v>
+      </c>
+      <c r="E85" s="22">
+        <v>0</v>
+      </c>
+      <c r="F85" s="22">
+        <v>5</v>
+      </c>
+      <c r="G85" s="22">
+        <v>0</v>
+      </c>
+      <c r="H85" s="22">
+        <v>0</v>
+      </c>
+      <c r="I85" s="22">
+        <v>109</v>
+      </c>
+      <c r="J85" s="22">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="86" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A86" s="26">
+        <v>43986</v>
+      </c>
+      <c r="B86" s="27">
+        <v>82161</v>
+      </c>
+      <c r="C86" s="28">
+        <v>828</v>
+      </c>
+      <c r="D86" s="28">
+        <v>1479</v>
+      </c>
+      <c r="E86" s="28">
+        <v>2</v>
+      </c>
+      <c r="F86" s="28">
+        <v>6</v>
+      </c>
+      <c r="G86" s="28">
+        <v>0</v>
+      </c>
+      <c r="H86" s="28">
+        <v>0</v>
+      </c>
+      <c r="I86" s="28">
+        <v>109</v>
+      </c>
+      <c r="J86" s="28">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="87" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A87" s="29">
+        <v>43987</v>
+      </c>
+      <c r="B87" s="30">
+        <v>82876</v>
+      </c>
+      <c r="C87" s="31">
+        <v>715</v>
+      </c>
+      <c r="D87" s="31">
+        <v>1484</v>
+      </c>
+      <c r="E87" s="31">
+        <v>5</v>
+      </c>
+      <c r="F87" s="31">
+        <v>6</v>
+      </c>
+      <c r="G87" s="31">
+        <v>0</v>
+      </c>
+      <c r="H87" s="31">
+        <v>0</v>
+      </c>
+      <c r="I87" s="31">
+        <v>109</v>
+      </c>
+      <c r="J87" s="31">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="88" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A88" s="23">
+        <v>43988</v>
+      </c>
+      <c r="B88" s="24">
+        <v>83105</v>
+      </c>
+      <c r="C88" s="25">
+        <v>229</v>
+      </c>
+      <c r="D88" s="25">
+        <v>1485</v>
+      </c>
+      <c r="E88" s="25">
+        <v>1</v>
+      </c>
+      <c r="F88" s="25">
+        <v>5</v>
+      </c>
+      <c r="G88" s="25">
+        <v>0</v>
+      </c>
+      <c r="H88" s="25">
+        <v>1</v>
+      </c>
+      <c r="I88" s="25">
+        <v>109</v>
+      </c>
+      <c r="J88" s="25">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="89" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A89" s="29">
+        <v>43989</v>
+      </c>
+      <c r="B89" s="30">
+        <v>83316</v>
+      </c>
+      <c r="C89" s="31">
+        <v>211</v>
+      </c>
+      <c r="D89" s="31">
+        <v>1485</v>
+      </c>
+      <c r="E89" s="31">
+        <v>0</v>
+      </c>
+      <c r="F89" s="31">
+        <v>5</v>
+      </c>
+      <c r="G89" s="31">
+        <v>0</v>
+      </c>
+      <c r="H89" s="31">
+        <v>0</v>
+      </c>
+      <c r="I89" s="31">
+        <v>109</v>
+      </c>
+      <c r="J89" s="31">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="90" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A90" s="20">
+        <v>43990</v>
+      </c>
+      <c r="B90" s="21">
+        <v>84130</v>
+      </c>
+      <c r="C90" s="22">
+        <v>814</v>
+      </c>
+      <c r="D90" s="22">
+        <v>1486</v>
+      </c>
+      <c r="E90" s="22">
+        <v>1</v>
+      </c>
+      <c r="F90" s="22">
+        <v>6</v>
+      </c>
+      <c r="G90" s="22">
+        <v>0</v>
+      </c>
+      <c r="H90" s="22">
+        <v>0</v>
+      </c>
+      <c r="I90" s="22">
+        <v>109</v>
+      </c>
+      <c r="J90" s="22">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="91" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A91" s="20">
+        <v>43991</v>
+      </c>
+      <c r="B91" s="21">
+        <v>84868</v>
+      </c>
+      <c r="C91" s="22">
+        <v>738</v>
+      </c>
+      <c r="D91" s="22">
+        <v>1488</v>
+      </c>
+      <c r="E91" s="22">
+        <v>2</v>
+      </c>
+      <c r="F91" s="22">
+        <v>6</v>
+      </c>
+      <c r="G91" s="22">
+        <v>0</v>
+      </c>
+      <c r="H91" s="22">
+        <v>0</v>
+      </c>
+      <c r="I91" s="22">
+        <v>109</v>
+      </c>
+      <c r="J91" s="22">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="92" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A92" s="23">
+        <v>43992</v>
+      </c>
+      <c r="B92" s="24">
+        <v>85626</v>
+      </c>
+      <c r="C92" s="25">
+        <v>758</v>
+      </c>
+      <c r="D92" s="25">
+        <v>1488</v>
+      </c>
+      <c r="E92" s="25">
+        <v>0</v>
+      </c>
+      <c r="F92" s="25">
+        <v>6</v>
+      </c>
+      <c r="G92" s="25">
+        <v>0</v>
+      </c>
+      <c r="H92" s="25">
+        <v>0</v>
+      </c>
+      <c r="I92" s="25">
+        <v>109</v>
+      </c>
+      <c r="J92" s="25">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="93" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A93" s="29">
+        <v>43993</v>
+      </c>
+      <c r="B93" s="30">
+        <v>86328</v>
+      </c>
+      <c r="C93" s="31">
+        <v>702</v>
+      </c>
+      <c r="D93" s="31">
+        <v>1490</v>
+      </c>
+      <c r="E93" s="31">
+        <v>2</v>
+      </c>
+      <c r="F93" s="31">
+        <v>6</v>
+      </c>
+      <c r="G93" s="31">
+        <v>0</v>
+      </c>
+      <c r="H93" s="31">
+        <v>0</v>
+      </c>
+      <c r="I93" s="31">
+        <v>109</v>
+      </c>
+      <c r="J93" s="31">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="94" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A94" s="23">
+        <v>43994</v>
+      </c>
+      <c r="B94" s="24">
+        <v>87095</v>
+      </c>
+      <c r="C94" s="25">
+        <v>767</v>
+      </c>
+      <c r="D94" s="25">
+        <v>1492</v>
+      </c>
+      <c r="E94" s="25">
+        <v>2</v>
+      </c>
+      <c r="F94" s="25">
+        <v>6</v>
+      </c>
+      <c r="G94" s="25">
+        <v>0</v>
+      </c>
+      <c r="H94" s="25">
+        <v>0</v>
+      </c>
+      <c r="I94" s="25">
+        <v>109</v>
+      </c>
+      <c r="J94" s="25">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="95" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A95" s="29">
+        <v>43995</v>
+      </c>
+      <c r="B95" s="30">
+        <v>87386</v>
+      </c>
+      <c r="C95" s="31">
+        <v>291</v>
+      </c>
+      <c r="D95" s="31">
+        <v>1495</v>
+      </c>
+      <c r="E95" s="31">
+        <v>3</v>
+      </c>
+      <c r="F95" s="31">
+        <v>6</v>
+      </c>
+      <c r="G95" s="31">
+        <v>0</v>
+      </c>
+      <c r="H95" s="31">
+        <v>0</v>
+      </c>
+      <c r="I95" s="31">
+        <v>109</v>
+      </c>
+      <c r="J95" s="31">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="96" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A96" s="23">
+        <v>43996</v>
+      </c>
+      <c r="B96" s="24">
+        <v>87598</v>
+      </c>
+      <c r="C96" s="25">
+        <v>212</v>
+      </c>
+      <c r="D96" s="25">
+        <v>1496</v>
+      </c>
+      <c r="E96" s="25">
+        <v>1</v>
+      </c>
+      <c r="F96" s="25">
+        <v>7</v>
+      </c>
+      <c r="G96" s="25">
+        <v>1</v>
+      </c>
+      <c r="H96" s="25">
+        <v>0</v>
+      </c>
+      <c r="I96" s="25">
+        <v>109</v>
+      </c>
+      <c r="J96" s="25">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="97" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A97" s="20">
+        <v>43997</v>
+      </c>
+      <c r="B97" s="21">
+        <v>88165</v>
+      </c>
+      <c r="C97" s="22">
+        <v>567</v>
+      </c>
+      <c r="D97" s="22">
+        <v>1499</v>
+      </c>
+      <c r="E97" s="22">
+        <v>3</v>
+      </c>
+      <c r="F97" s="22">
+        <v>7</v>
+      </c>
+      <c r="G97" s="22">
+        <v>1</v>
+      </c>
+      <c r="H97" s="22">
+        <v>0</v>
+      </c>
+      <c r="I97" s="22">
+        <v>109</v>
+      </c>
+      <c r="J97" s="22">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="98" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A98" s="20">
+        <v>43998</v>
+      </c>
+      <c r="B98" s="21">
+        <v>89151</v>
+      </c>
+      <c r="C98" s="22">
+        <v>986</v>
+      </c>
+      <c r="D98" s="22">
+        <v>1503</v>
+      </c>
+      <c r="E98" s="22">
+        <v>4</v>
+      </c>
+      <c r="F98" s="22">
+        <v>7</v>
+      </c>
+      <c r="G98" s="22">
+        <v>1</v>
+      </c>
+      <c r="H98" s="22">
+        <v>0</v>
+      </c>
+      <c r="I98" s="22">
+        <v>109</v>
+      </c>
+      <c r="J98" s="22">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="99" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A99" s="29">
+        <v>43999</v>
+      </c>
+      <c r="B99" s="30">
+        <v>90103</v>
+      </c>
+      <c r="C99" s="31">
+        <v>952</v>
+      </c>
+      <c r="D99" s="31">
+        <v>1511</v>
+      </c>
+      <c r="E99" s="31">
+        <v>8</v>
+      </c>
+      <c r="F99" s="31">
+        <v>6</v>
+      </c>
+      <c r="G99" s="31">
+        <v>1</v>
+      </c>
+      <c r="H99" s="31">
+        <v>1</v>
+      </c>
+      <c r="I99" s="31">
+        <v>109</v>
+      </c>
+      <c r="J99" s="31">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="100" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A100" s="20">
+        <v>44000</v>
+      </c>
+      <c r="B100" s="21">
+        <v>91005</v>
+      </c>
+      <c r="C100" s="22">
+        <v>902</v>
+      </c>
+      <c r="D100" s="22">
+        <v>1513</v>
+      </c>
+      <c r="E100" s="22">
+        <v>2</v>
+      </c>
+      <c r="F100" s="22">
+        <v>8</v>
+      </c>
+      <c r="G100" s="22">
+        <v>1</v>
+      </c>
+      <c r="H100" s="22">
+        <v>0</v>
+      </c>
+      <c r="I100" s="22">
+        <v>109</v>
+      </c>
+      <c r="J100" s="22">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="101" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A101" s="29">
+        <v>44001</v>
+      </c>
+      <c r="B101" s="30">
+        <v>92152</v>
+      </c>
+      <c r="C101" s="31">
+        <v>1147</v>
+      </c>
+      <c r="D101" s="31">
+        <v>1519</v>
+      </c>
+      <c r="E101" s="31">
+        <v>6</v>
+      </c>
+      <c r="F101" s="31">
+        <v>6</v>
+      </c>
+      <c r="G101" s="31">
+        <v>1</v>
+      </c>
+      <c r="H101" s="31">
+        <v>2</v>
+      </c>
+      <c r="I101" s="31">
+        <v>109</v>
+      </c>
+      <c r="J101" s="31">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="102" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A102" s="23">
+        <v>44002</v>
+      </c>
+      <c r="B102" s="24">
+        <v>92919</v>
+      </c>
+      <c r="C102" s="25">
+        <v>758</v>
+      </c>
+      <c r="D102" s="25">
+        <v>1520</v>
+      </c>
+      <c r="E102" s="25">
+        <v>1</v>
+      </c>
+      <c r="F102" s="25">
+        <v>6</v>
+      </c>
+      <c r="G102" s="25">
+        <v>1</v>
+      </c>
+      <c r="H102" s="25">
+        <v>2</v>
+      </c>
+      <c r="I102" s="25">
+        <v>109</v>
+      </c>
+      <c r="J102" s="25">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="103" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A103" s="29">
+        <v>44003</v>
+      </c>
+      <c r="B103" s="30">
+        <v>93181</v>
+      </c>
+      <c r="C103" s="31">
+        <v>271</v>
+      </c>
+      <c r="D103" s="31">
+        <v>1521</v>
+      </c>
+      <c r="E103" s="31">
+        <v>1</v>
+      </c>
+      <c r="F103" s="31">
+        <v>6</v>
+      </c>
+      <c r="G103" s="31">
+        <v>1</v>
+      </c>
+      <c r="H103" s="31">
+        <v>0</v>
+      </c>
+      <c r="I103" s="31">
+        <v>109</v>
+      </c>
+      <c r="J103" s="31">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="104" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A104" s="29">
+        <v>44004</v>
+      </c>
+      <c r="B104" s="30">
+        <v>94165</v>
+      </c>
+      <c r="C104" s="31">
+        <v>984</v>
+      </c>
+      <c r="D104" s="31">
+        <v>1534</v>
+      </c>
+      <c r="E104" s="31">
+        <v>13</v>
+      </c>
+      <c r="F104" s="31">
+        <v>5</v>
+      </c>
+      <c r="G104" s="31">
+        <v>1</v>
+      </c>
+      <c r="H104" s="31">
+        <v>1</v>
+      </c>
+      <c r="I104" s="31">
+        <v>109</v>
+      </c>
+      <c r="J104" s="31">
+        <v>0</v>
+      </c>
+    </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>

</xml_diff>

<commit_message>
Data updated by GitHub Bot (2020-06-24 12)
</commit_message>
<xml_diff>
--- a/output/snapshot/fdcf2531-4c3e-5c02-b63c-ee160ead6dea.xlsx
+++ b/output/snapshot/fdcf2531-4c3e-5c02-b63c-ee160ead6dea.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="I:\AKTUALNI PODATKI - KORONA\Za objavo na GOV.SI\ang\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{1E6DD62F-2BE2-47DC-A7ED-9B57C1589256}" xr6:coauthVersionLast="44" xr6:coauthVersionMax="44" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{6AA752B0-19CD-4160-85F2-84C90D1D3AA5}" xr6:coauthVersionLast="44" xr6:coauthVersionMax="44" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -25,7 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="10" uniqueCount="10">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="11" uniqueCount="11">
   <si>
     <t>Date</t>
   </si>
@@ -56,6 +56,9 @@
   <si>
     <t>Deaths (daily)</t>
   </si>
+  <si>
+    <t>111*</t>
+  </si>
 </sst>
 </file>
 
@@ -64,7 +67,7 @@
   <numFmts count="1">
     <numFmt numFmtId="164" formatCode="d/\ m/\ yyyy;@"/>
   </numFmts>
-  <fonts count="4" x14ac:knownFonts="1">
+  <fonts count="5" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -93,6 +96,13 @@
       <name val="Calibri Light"/>
       <scheme val="major"/>
     </font>
+    <font>
+      <sz val="10"/>
+      <color theme="1"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
   </fonts>
   <fills count="3">
     <fill>
@@ -108,7 +118,7 @@
       </patternFill>
     </fill>
   </fills>
-  <borders count="2">
+  <borders count="3">
     <border>
       <left/>
       <right/>
@@ -129,11 +139,26 @@
       <bottom/>
       <diagonal/>
     </border>
+    <border>
+      <left style="thin">
+        <color theme="4"/>
+      </left>
+      <right style="thin">
+        <color theme="4"/>
+      </right>
+      <top style="thin">
+        <color theme="4"/>
+      </top>
+      <bottom style="thin">
+        <color theme="4"/>
+      </bottom>
+      <diagonal/>
+    </border>
   </borders>
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="26">
+  <cellXfs count="32">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="49" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyAlignment="1" applyProtection="1">
       <alignment horizontal="left" vertical="top"/>
@@ -208,6 +233,24 @@
       <alignment horizontal="right"/>
     </xf>
     <xf numFmtId="0" fontId="3" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="right"/>
+    </xf>
+    <xf numFmtId="164" fontId="4" fillId="2" borderId="2" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="right" vertical="top"/>
+    </xf>
+    <xf numFmtId="3" fontId="4" fillId="2" borderId="2" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="right"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="2" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="right"/>
+    </xf>
+    <xf numFmtId="164" fontId="3" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="right" vertical="top"/>
+    </xf>
+    <xf numFmtId="3" fontId="3" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="right"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="right"/>
     </xf>
   </cellXfs>
@@ -399,8 +442,8 @@
 </file>
 
 <file path=xl/tables/table1.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="1" xr:uid="{00000000-000C-0000-FFFF-FFFF00000000}" name="Tabela1" displayName="Tabela1" ref="A1:J75" totalsRowShown="0" headerRowDxfId="11" dataDxfId="10">
-  <autoFilter ref="A1:J75" xr:uid="{00000000-0009-0000-0100-000001000000}">
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="1" xr:uid="{00000000-000C-0000-FFFF-FFFF00000000}" name="Tabela1" displayName="Tabela1" ref="A1:J105" totalsRowShown="0" headerRowDxfId="11" dataDxfId="10">
+  <autoFilter ref="A1:J105" xr:uid="{00000000-0009-0000-0100-000001000000}">
     <filterColumn colId="0" hiddenButton="1"/>
     <filterColumn colId="1" hiddenButton="1"/>
     <filterColumn colId="2" hiddenButton="1"/>
@@ -696,10 +739,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:J75"/>
+  <dimension ref="A1:J105"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A40" zoomScale="89" zoomScaleNormal="89" workbookViewId="0">
-      <selection activeCell="J74" sqref="J74"/>
+    <sheetView tabSelected="1" topLeftCell="A77" zoomScale="89" zoomScaleNormal="89" workbookViewId="0">
+      <selection activeCell="A105" sqref="A105:J105"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -3117,6 +3160,966 @@
         <v>0</v>
       </c>
     </row>
+    <row r="76" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A76" s="20">
+        <v>43976</v>
+      </c>
+      <c r="B76" s="21">
+        <v>75770</v>
+      </c>
+      <c r="C76" s="22">
+        <v>754</v>
+      </c>
+      <c r="D76" s="22">
+        <v>1469</v>
+      </c>
+      <c r="E76" s="22">
+        <v>0</v>
+      </c>
+      <c r="F76" s="22">
+        <v>9</v>
+      </c>
+      <c r="G76" s="22">
+        <v>2</v>
+      </c>
+      <c r="H76" s="22">
+        <v>6</v>
+      </c>
+      <c r="I76" s="22">
+        <v>108</v>
+      </c>
+      <c r="J76" s="22">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="77" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A77" s="20">
+        <v>43977</v>
+      </c>
+      <c r="B77" s="21">
+        <v>76579</v>
+      </c>
+      <c r="C77" s="22">
+        <v>809</v>
+      </c>
+      <c r="D77" s="22">
+        <v>1471</v>
+      </c>
+      <c r="E77" s="22">
+        <v>2</v>
+      </c>
+      <c r="F77" s="22">
+        <v>8</v>
+      </c>
+      <c r="G77" s="22">
+        <v>2</v>
+      </c>
+      <c r="H77" s="22">
+        <v>2</v>
+      </c>
+      <c r="I77" s="22">
+        <v>108</v>
+      </c>
+      <c r="J77" s="22">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="78" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A78" s="20">
+        <v>43978</v>
+      </c>
+      <c r="B78" s="21">
+        <v>77210</v>
+      </c>
+      <c r="C78" s="22">
+        <v>631</v>
+      </c>
+      <c r="D78" s="22">
+        <v>1473</v>
+      </c>
+      <c r="E78" s="22">
+        <v>2</v>
+      </c>
+      <c r="F78" s="22">
+        <v>7</v>
+      </c>
+      <c r="G78" s="22">
+        <v>2</v>
+      </c>
+      <c r="H78" s="22">
+        <v>1</v>
+      </c>
+      <c r="I78" s="22">
+        <v>108</v>
+      </c>
+      <c r="J78" s="22">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="79" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A79" s="20">
+        <v>43979</v>
+      </c>
+      <c r="B79" s="21">
+        <v>77916</v>
+      </c>
+      <c r="C79" s="22">
+        <v>706</v>
+      </c>
+      <c r="D79" s="22">
+        <v>1473</v>
+      </c>
+      <c r="E79" s="22">
+        <v>0</v>
+      </c>
+      <c r="F79" s="22">
+        <v>7</v>
+      </c>
+      <c r="G79" s="22">
+        <v>2</v>
+      </c>
+      <c r="H79" s="22">
+        <v>0</v>
+      </c>
+      <c r="I79" s="22">
+        <v>108</v>
+      </c>
+      <c r="J79" s="22">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="80" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A80" s="20">
+        <v>43980</v>
+      </c>
+      <c r="B80" s="21">
+        <v>78529</v>
+      </c>
+      <c r="C80" s="22">
+        <v>613</v>
+      </c>
+      <c r="D80" s="22">
+        <v>1473</v>
+      </c>
+      <c r="E80" s="22">
+        <v>0</v>
+      </c>
+      <c r="F80" s="22">
+        <v>7</v>
+      </c>
+      <c r="G80" s="22">
+        <v>2</v>
+      </c>
+      <c r="H80" s="22">
+        <v>0</v>
+      </c>
+      <c r="I80" s="22">
+        <v>108</v>
+      </c>
+      <c r="J80" s="22">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="81" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A81" s="20">
+        <v>43981</v>
+      </c>
+      <c r="B81" s="22">
+        <v>78793</v>
+      </c>
+      <c r="C81" s="22">
+        <v>264</v>
+      </c>
+      <c r="D81" s="22">
+        <v>1473</v>
+      </c>
+      <c r="E81" s="22">
+        <v>0</v>
+      </c>
+      <c r="F81" s="22">
+        <v>6</v>
+      </c>
+      <c r="G81" s="22">
+        <v>2</v>
+      </c>
+      <c r="H81" s="22">
+        <v>1</v>
+      </c>
+      <c r="I81" s="22">
+        <v>108</v>
+      </c>
+      <c r="J81" s="22">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="82" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A82" s="20">
+        <v>43982</v>
+      </c>
+      <c r="B82" s="21">
+        <v>79039</v>
+      </c>
+      <c r="C82" s="22">
+        <v>246</v>
+      </c>
+      <c r="D82" s="22">
+        <v>1473</v>
+      </c>
+      <c r="E82" s="22">
+        <v>0</v>
+      </c>
+      <c r="F82" s="22">
+        <v>5</v>
+      </c>
+      <c r="G82" s="22">
+        <v>1</v>
+      </c>
+      <c r="H82" s="22">
+        <v>0</v>
+      </c>
+      <c r="I82" s="22">
+        <v>109</v>
+      </c>
+      <c r="J82" s="22">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="83" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A83" s="20">
+        <v>43983</v>
+      </c>
+      <c r="B83" s="21">
+        <v>79698</v>
+      </c>
+      <c r="C83" s="22">
+        <v>659</v>
+      </c>
+      <c r="D83" s="22">
+        <v>1475</v>
+      </c>
+      <c r="E83" s="22">
+        <v>2</v>
+      </c>
+      <c r="F83" s="22">
+        <v>5</v>
+      </c>
+      <c r="G83" s="22">
+        <v>1</v>
+      </c>
+      <c r="H83" s="22">
+        <v>0</v>
+      </c>
+      <c r="I83" s="22">
+        <v>109</v>
+      </c>
+      <c r="J83" s="22">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="84" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A84" s="20">
+        <v>43984</v>
+      </c>
+      <c r="B84" s="21">
+        <v>80505</v>
+      </c>
+      <c r="C84" s="22">
+        <v>807</v>
+      </c>
+      <c r="D84" s="22">
+        <v>1477</v>
+      </c>
+      <c r="E84" s="22">
+        <v>2</v>
+      </c>
+      <c r="F84" s="22">
+        <v>5</v>
+      </c>
+      <c r="G84" s="22">
+        <v>0</v>
+      </c>
+      <c r="H84" s="22">
+        <v>0</v>
+      </c>
+      <c r="I84" s="22">
+        <v>109</v>
+      </c>
+      <c r="J84" s="22">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="85" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A85" s="20">
+        <v>43985</v>
+      </c>
+      <c r="B85" s="21">
+        <v>81333</v>
+      </c>
+      <c r="C85" s="22">
+        <v>828</v>
+      </c>
+      <c r="D85" s="22">
+        <v>1477</v>
+      </c>
+      <c r="E85" s="22">
+        <v>0</v>
+      </c>
+      <c r="F85" s="22">
+        <v>5</v>
+      </c>
+      <c r="G85" s="22">
+        <v>0</v>
+      </c>
+      <c r="H85" s="22">
+        <v>0</v>
+      </c>
+      <c r="I85" s="22">
+        <v>109</v>
+      </c>
+      <c r="J85" s="22">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="86" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A86" s="26">
+        <v>43986</v>
+      </c>
+      <c r="B86" s="27">
+        <v>82161</v>
+      </c>
+      <c r="C86" s="28">
+        <v>828</v>
+      </c>
+      <c r="D86" s="28">
+        <v>1479</v>
+      </c>
+      <c r="E86" s="28">
+        <v>2</v>
+      </c>
+      <c r="F86" s="28">
+        <v>6</v>
+      </c>
+      <c r="G86" s="28">
+        <v>0</v>
+      </c>
+      <c r="H86" s="28">
+        <v>0</v>
+      </c>
+      <c r="I86" s="28">
+        <v>109</v>
+      </c>
+      <c r="J86" s="28">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="87" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A87" s="29">
+        <v>43987</v>
+      </c>
+      <c r="B87" s="30">
+        <v>82876</v>
+      </c>
+      <c r="C87" s="31">
+        <v>715</v>
+      </c>
+      <c r="D87" s="31">
+        <v>1484</v>
+      </c>
+      <c r="E87" s="31">
+        <v>5</v>
+      </c>
+      <c r="F87" s="31">
+        <v>6</v>
+      </c>
+      <c r="G87" s="31">
+        <v>0</v>
+      </c>
+      <c r="H87" s="31">
+        <v>0</v>
+      </c>
+      <c r="I87" s="31">
+        <v>109</v>
+      </c>
+      <c r="J87" s="31">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="88" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A88" s="23">
+        <v>43988</v>
+      </c>
+      <c r="B88" s="24">
+        <v>83105</v>
+      </c>
+      <c r="C88" s="25">
+        <v>229</v>
+      </c>
+      <c r="D88" s="25">
+        <v>1485</v>
+      </c>
+      <c r="E88" s="25">
+        <v>1</v>
+      </c>
+      <c r="F88" s="25">
+        <v>5</v>
+      </c>
+      <c r="G88" s="25">
+        <v>0</v>
+      </c>
+      <c r="H88" s="25">
+        <v>1</v>
+      </c>
+      <c r="I88" s="25">
+        <v>109</v>
+      </c>
+      <c r="J88" s="25">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="89" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A89" s="29">
+        <v>43989</v>
+      </c>
+      <c r="B89" s="30">
+        <v>83316</v>
+      </c>
+      <c r="C89" s="31">
+        <v>211</v>
+      </c>
+      <c r="D89" s="31">
+        <v>1485</v>
+      </c>
+      <c r="E89" s="31">
+        <v>0</v>
+      </c>
+      <c r="F89" s="31">
+        <v>5</v>
+      </c>
+      <c r="G89" s="31">
+        <v>0</v>
+      </c>
+      <c r="H89" s="31">
+        <v>0</v>
+      </c>
+      <c r="I89" s="31">
+        <v>109</v>
+      </c>
+      <c r="J89" s="31">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="90" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A90" s="20">
+        <v>43990</v>
+      </c>
+      <c r="B90" s="21">
+        <v>84130</v>
+      </c>
+      <c r="C90" s="22">
+        <v>814</v>
+      </c>
+      <c r="D90" s="22">
+        <v>1486</v>
+      </c>
+      <c r="E90" s="22">
+        <v>1</v>
+      </c>
+      <c r="F90" s="22">
+        <v>6</v>
+      </c>
+      <c r="G90" s="22">
+        <v>0</v>
+      </c>
+      <c r="H90" s="22">
+        <v>0</v>
+      </c>
+      <c r="I90" s="22">
+        <v>109</v>
+      </c>
+      <c r="J90" s="22">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="91" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A91" s="20">
+        <v>43991</v>
+      </c>
+      <c r="B91" s="21">
+        <v>84868</v>
+      </c>
+      <c r="C91" s="22">
+        <v>738</v>
+      </c>
+      <c r="D91" s="22">
+        <v>1488</v>
+      </c>
+      <c r="E91" s="22">
+        <v>2</v>
+      </c>
+      <c r="F91" s="22">
+        <v>6</v>
+      </c>
+      <c r="G91" s="22">
+        <v>0</v>
+      </c>
+      <c r="H91" s="22">
+        <v>0</v>
+      </c>
+      <c r="I91" s="22">
+        <v>109</v>
+      </c>
+      <c r="J91" s="22">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="92" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A92" s="23">
+        <v>43992</v>
+      </c>
+      <c r="B92" s="24">
+        <v>85626</v>
+      </c>
+      <c r="C92" s="25">
+        <v>758</v>
+      </c>
+      <c r="D92" s="25">
+        <v>1488</v>
+      </c>
+      <c r="E92" s="25">
+        <v>0</v>
+      </c>
+      <c r="F92" s="25">
+        <v>6</v>
+      </c>
+      <c r="G92" s="25">
+        <v>0</v>
+      </c>
+      <c r="H92" s="25">
+        <v>0</v>
+      </c>
+      <c r="I92" s="25">
+        <v>109</v>
+      </c>
+      <c r="J92" s="25">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="93" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A93" s="29">
+        <v>43993</v>
+      </c>
+      <c r="B93" s="30">
+        <v>86328</v>
+      </c>
+      <c r="C93" s="31">
+        <v>702</v>
+      </c>
+      <c r="D93" s="31">
+        <v>1490</v>
+      </c>
+      <c r="E93" s="31">
+        <v>2</v>
+      </c>
+      <c r="F93" s="31">
+        <v>6</v>
+      </c>
+      <c r="G93" s="31">
+        <v>0</v>
+      </c>
+      <c r="H93" s="31">
+        <v>0</v>
+      </c>
+      <c r="I93" s="31">
+        <v>109</v>
+      </c>
+      <c r="J93" s="31">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="94" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A94" s="23">
+        <v>43994</v>
+      </c>
+      <c r="B94" s="24">
+        <v>87095</v>
+      </c>
+      <c r="C94" s="25">
+        <v>767</v>
+      </c>
+      <c r="D94" s="25">
+        <v>1492</v>
+      </c>
+      <c r="E94" s="25">
+        <v>2</v>
+      </c>
+      <c r="F94" s="25">
+        <v>6</v>
+      </c>
+      <c r="G94" s="25">
+        <v>0</v>
+      </c>
+      <c r="H94" s="25">
+        <v>0</v>
+      </c>
+      <c r="I94" s="25">
+        <v>109</v>
+      </c>
+      <c r="J94" s="25">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="95" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A95" s="29">
+        <v>43995</v>
+      </c>
+      <c r="B95" s="30">
+        <v>87386</v>
+      </c>
+      <c r="C95" s="31">
+        <v>291</v>
+      </c>
+      <c r="D95" s="31">
+        <v>1495</v>
+      </c>
+      <c r="E95" s="31">
+        <v>3</v>
+      </c>
+      <c r="F95" s="31">
+        <v>6</v>
+      </c>
+      <c r="G95" s="31">
+        <v>0</v>
+      </c>
+      <c r="H95" s="31">
+        <v>0</v>
+      </c>
+      <c r="I95" s="31">
+        <v>109</v>
+      </c>
+      <c r="J95" s="31">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="96" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A96" s="23">
+        <v>43996</v>
+      </c>
+      <c r="B96" s="24">
+        <v>87598</v>
+      </c>
+      <c r="C96" s="25">
+        <v>212</v>
+      </c>
+      <c r="D96" s="25">
+        <v>1496</v>
+      </c>
+      <c r="E96" s="25">
+        <v>1</v>
+      </c>
+      <c r="F96" s="25">
+        <v>7</v>
+      </c>
+      <c r="G96" s="25">
+        <v>1</v>
+      </c>
+      <c r="H96" s="25">
+        <v>0</v>
+      </c>
+      <c r="I96" s="25">
+        <v>109</v>
+      </c>
+      <c r="J96" s="25">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="97" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A97" s="20">
+        <v>43997</v>
+      </c>
+      <c r="B97" s="21">
+        <v>88165</v>
+      </c>
+      <c r="C97" s="22">
+        <v>567</v>
+      </c>
+      <c r="D97" s="22">
+        <v>1499</v>
+      </c>
+      <c r="E97" s="22">
+        <v>3</v>
+      </c>
+      <c r="F97" s="22">
+        <v>7</v>
+      </c>
+      <c r="G97" s="22">
+        <v>1</v>
+      </c>
+      <c r="H97" s="22">
+        <v>0</v>
+      </c>
+      <c r="I97" s="22">
+        <v>109</v>
+      </c>
+      <c r="J97" s="22">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="98" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A98" s="20">
+        <v>43998</v>
+      </c>
+      <c r="B98" s="21">
+        <v>89151</v>
+      </c>
+      <c r="C98" s="22">
+        <v>986</v>
+      </c>
+      <c r="D98" s="22">
+        <v>1503</v>
+      </c>
+      <c r="E98" s="22">
+        <v>4</v>
+      </c>
+      <c r="F98" s="22">
+        <v>7</v>
+      </c>
+      <c r="G98" s="22">
+        <v>1</v>
+      </c>
+      <c r="H98" s="22">
+        <v>0</v>
+      </c>
+      <c r="I98" s="22">
+        <v>109</v>
+      </c>
+      <c r="J98" s="22">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="99" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A99" s="29">
+        <v>43999</v>
+      </c>
+      <c r="B99" s="30">
+        <v>90103</v>
+      </c>
+      <c r="C99" s="31">
+        <v>952</v>
+      </c>
+      <c r="D99" s="31">
+        <v>1511</v>
+      </c>
+      <c r="E99" s="31">
+        <v>8</v>
+      </c>
+      <c r="F99" s="31">
+        <v>6</v>
+      </c>
+      <c r="G99" s="31">
+        <v>1</v>
+      </c>
+      <c r="H99" s="31">
+        <v>1</v>
+      </c>
+      <c r="I99" s="31">
+        <v>109</v>
+      </c>
+      <c r="J99" s="31">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="100" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A100" s="20">
+        <v>44000</v>
+      </c>
+      <c r="B100" s="21">
+        <v>91005</v>
+      </c>
+      <c r="C100" s="22">
+        <v>902</v>
+      </c>
+      <c r="D100" s="22">
+        <v>1513</v>
+      </c>
+      <c r="E100" s="22">
+        <v>2</v>
+      </c>
+      <c r="F100" s="22">
+        <v>8</v>
+      </c>
+      <c r="G100" s="22">
+        <v>1</v>
+      </c>
+      <c r="H100" s="22">
+        <v>0</v>
+      </c>
+      <c r="I100" s="22">
+        <v>109</v>
+      </c>
+      <c r="J100" s="22">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="101" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A101" s="29">
+        <v>44001</v>
+      </c>
+      <c r="B101" s="30">
+        <v>92152</v>
+      </c>
+      <c r="C101" s="31">
+        <v>1147</v>
+      </c>
+      <c r="D101" s="31">
+        <v>1519</v>
+      </c>
+      <c r="E101" s="31">
+        <v>6</v>
+      </c>
+      <c r="F101" s="31">
+        <v>6</v>
+      </c>
+      <c r="G101" s="31">
+        <v>1</v>
+      </c>
+      <c r="H101" s="31">
+        <v>2</v>
+      </c>
+      <c r="I101" s="31">
+        <v>109</v>
+      </c>
+      <c r="J101" s="31">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="102" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A102" s="23">
+        <v>44002</v>
+      </c>
+      <c r="B102" s="24">
+        <v>92919</v>
+      </c>
+      <c r="C102" s="25">
+        <v>758</v>
+      </c>
+      <c r="D102" s="25">
+        <v>1520</v>
+      </c>
+      <c r="E102" s="25">
+        <v>1</v>
+      </c>
+      <c r="F102" s="25">
+        <v>6</v>
+      </c>
+      <c r="G102" s="25">
+        <v>1</v>
+      </c>
+      <c r="H102" s="25">
+        <v>2</v>
+      </c>
+      <c r="I102" s="25">
+        <v>109</v>
+      </c>
+      <c r="J102" s="25">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="103" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A103" s="29">
+        <v>44003</v>
+      </c>
+      <c r="B103" s="30">
+        <v>93181</v>
+      </c>
+      <c r="C103" s="31">
+        <v>271</v>
+      </c>
+      <c r="D103" s="31">
+        <v>1521</v>
+      </c>
+      <c r="E103" s="31">
+        <v>1</v>
+      </c>
+      <c r="F103" s="31">
+        <v>6</v>
+      </c>
+      <c r="G103" s="31">
+        <v>1</v>
+      </c>
+      <c r="H103" s="31">
+        <v>0</v>
+      </c>
+      <c r="I103" s="31">
+        <v>109</v>
+      </c>
+      <c r="J103" s="31">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="104" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A104" s="29">
+        <v>44004</v>
+      </c>
+      <c r="B104" s="30">
+        <v>94165</v>
+      </c>
+      <c r="C104" s="31">
+        <v>984</v>
+      </c>
+      <c r="D104" s="31">
+        <v>1534</v>
+      </c>
+      <c r="E104" s="31">
+        <v>13</v>
+      </c>
+      <c r="F104" s="31">
+        <v>5</v>
+      </c>
+      <c r="G104" s="31">
+        <v>1</v>
+      </c>
+      <c r="H104" s="31">
+        <v>1</v>
+      </c>
+      <c r="I104" s="31">
+        <v>109</v>
+      </c>
+      <c r="J104" s="31">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="105" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A105" s="29">
+        <v>44005</v>
+      </c>
+      <c r="B105" s="30">
+        <v>95387</v>
+      </c>
+      <c r="C105" s="31">
+        <v>1222</v>
+      </c>
+      <c r="D105" s="31">
+        <v>1541</v>
+      </c>
+      <c r="E105" s="31">
+        <v>7</v>
+      </c>
+      <c r="F105" s="31">
+        <v>7</v>
+      </c>
+      <c r="G105" s="31">
+        <v>2</v>
+      </c>
+      <c r="H105" s="31">
+        <v>0</v>
+      </c>
+      <c r="I105" s="31" t="s">
+        <v>10</v>
+      </c>
+      <c r="J105" s="31">
+        <v>0</v>
+      </c>
+    </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>

</xml_diff>

<commit_message>
Data updated by GitHub Bot (2020-06-24 20)
</commit_message>
<xml_diff>
--- a/output/snapshot/fdcf2531-4c3e-5c02-b63c-ee160ead6dea.xlsx
+++ b/output/snapshot/fdcf2531-4c3e-5c02-b63c-ee160ead6dea.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="I:\AKTUALNI PODATKI - KORONA\Za objavo na GOV.SI\ang\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{1E6DD62F-2BE2-47DC-A7ED-9B57C1589256}" xr6:coauthVersionLast="44" xr6:coauthVersionMax="44" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{6AA752B0-19CD-4160-85F2-84C90D1D3AA5}" xr6:coauthVersionLast="44" xr6:coauthVersionMax="44" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -25,7 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="10" uniqueCount="10">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="11" uniqueCount="11">
   <si>
     <t>Date</t>
   </si>
@@ -56,6 +56,9 @@
   <si>
     <t>Deaths (daily)</t>
   </si>
+  <si>
+    <t>111*</t>
+  </si>
 </sst>
 </file>
 
@@ -64,7 +67,7 @@
   <numFmts count="1">
     <numFmt numFmtId="164" formatCode="d/\ m/\ yyyy;@"/>
   </numFmts>
-  <fonts count="4" x14ac:knownFonts="1">
+  <fonts count="5" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -93,6 +96,13 @@
       <name val="Calibri Light"/>
       <scheme val="major"/>
     </font>
+    <font>
+      <sz val="10"/>
+      <color theme="1"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
   </fonts>
   <fills count="3">
     <fill>
@@ -108,7 +118,7 @@
       </patternFill>
     </fill>
   </fills>
-  <borders count="2">
+  <borders count="3">
     <border>
       <left/>
       <right/>
@@ -129,11 +139,26 @@
       <bottom/>
       <diagonal/>
     </border>
+    <border>
+      <left style="thin">
+        <color theme="4"/>
+      </left>
+      <right style="thin">
+        <color theme="4"/>
+      </right>
+      <top style="thin">
+        <color theme="4"/>
+      </top>
+      <bottom style="thin">
+        <color theme="4"/>
+      </bottom>
+      <diagonal/>
+    </border>
   </borders>
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="26">
+  <cellXfs count="32">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="49" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyAlignment="1" applyProtection="1">
       <alignment horizontal="left" vertical="top"/>
@@ -208,6 +233,24 @@
       <alignment horizontal="right"/>
     </xf>
     <xf numFmtId="0" fontId="3" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="right"/>
+    </xf>
+    <xf numFmtId="164" fontId="4" fillId="2" borderId="2" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="right" vertical="top"/>
+    </xf>
+    <xf numFmtId="3" fontId="4" fillId="2" borderId="2" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="right"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="2" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="right"/>
+    </xf>
+    <xf numFmtId="164" fontId="3" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="right" vertical="top"/>
+    </xf>
+    <xf numFmtId="3" fontId="3" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="right"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="right"/>
     </xf>
   </cellXfs>
@@ -399,8 +442,8 @@
 </file>
 
 <file path=xl/tables/table1.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="1" xr:uid="{00000000-000C-0000-FFFF-FFFF00000000}" name="Tabela1" displayName="Tabela1" ref="A1:J75" totalsRowShown="0" headerRowDxfId="11" dataDxfId="10">
-  <autoFilter ref="A1:J75" xr:uid="{00000000-0009-0000-0100-000001000000}">
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="1" xr:uid="{00000000-000C-0000-FFFF-FFFF00000000}" name="Tabela1" displayName="Tabela1" ref="A1:J105" totalsRowShown="0" headerRowDxfId="11" dataDxfId="10">
+  <autoFilter ref="A1:J105" xr:uid="{00000000-0009-0000-0100-000001000000}">
     <filterColumn colId="0" hiddenButton="1"/>
     <filterColumn colId="1" hiddenButton="1"/>
     <filterColumn colId="2" hiddenButton="1"/>
@@ -696,10 +739,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:J75"/>
+  <dimension ref="A1:J105"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A40" zoomScale="89" zoomScaleNormal="89" workbookViewId="0">
-      <selection activeCell="J74" sqref="J74"/>
+    <sheetView tabSelected="1" topLeftCell="A77" zoomScale="89" zoomScaleNormal="89" workbookViewId="0">
+      <selection activeCell="A105" sqref="A105:J105"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -3117,6 +3160,966 @@
         <v>0</v>
       </c>
     </row>
+    <row r="76" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A76" s="20">
+        <v>43976</v>
+      </c>
+      <c r="B76" s="21">
+        <v>75770</v>
+      </c>
+      <c r="C76" s="22">
+        <v>754</v>
+      </c>
+      <c r="D76" s="22">
+        <v>1469</v>
+      </c>
+      <c r="E76" s="22">
+        <v>0</v>
+      </c>
+      <c r="F76" s="22">
+        <v>9</v>
+      </c>
+      <c r="G76" s="22">
+        <v>2</v>
+      </c>
+      <c r="H76" s="22">
+        <v>6</v>
+      </c>
+      <c r="I76" s="22">
+        <v>108</v>
+      </c>
+      <c r="J76" s="22">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="77" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A77" s="20">
+        <v>43977</v>
+      </c>
+      <c r="B77" s="21">
+        <v>76579</v>
+      </c>
+      <c r="C77" s="22">
+        <v>809</v>
+      </c>
+      <c r="D77" s="22">
+        <v>1471</v>
+      </c>
+      <c r="E77" s="22">
+        <v>2</v>
+      </c>
+      <c r="F77" s="22">
+        <v>8</v>
+      </c>
+      <c r="G77" s="22">
+        <v>2</v>
+      </c>
+      <c r="H77" s="22">
+        <v>2</v>
+      </c>
+      <c r="I77" s="22">
+        <v>108</v>
+      </c>
+      <c r="J77" s="22">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="78" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A78" s="20">
+        <v>43978</v>
+      </c>
+      <c r="B78" s="21">
+        <v>77210</v>
+      </c>
+      <c r="C78" s="22">
+        <v>631</v>
+      </c>
+      <c r="D78" s="22">
+        <v>1473</v>
+      </c>
+      <c r="E78" s="22">
+        <v>2</v>
+      </c>
+      <c r="F78" s="22">
+        <v>7</v>
+      </c>
+      <c r="G78" s="22">
+        <v>2</v>
+      </c>
+      <c r="H78" s="22">
+        <v>1</v>
+      </c>
+      <c r="I78" s="22">
+        <v>108</v>
+      </c>
+      <c r="J78" s="22">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="79" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A79" s="20">
+        <v>43979</v>
+      </c>
+      <c r="B79" s="21">
+        <v>77916</v>
+      </c>
+      <c r="C79" s="22">
+        <v>706</v>
+      </c>
+      <c r="D79" s="22">
+        <v>1473</v>
+      </c>
+      <c r="E79" s="22">
+        <v>0</v>
+      </c>
+      <c r="F79" s="22">
+        <v>7</v>
+      </c>
+      <c r="G79" s="22">
+        <v>2</v>
+      </c>
+      <c r="H79" s="22">
+        <v>0</v>
+      </c>
+      <c r="I79" s="22">
+        <v>108</v>
+      </c>
+      <c r="J79" s="22">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="80" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A80" s="20">
+        <v>43980</v>
+      </c>
+      <c r="B80" s="21">
+        <v>78529</v>
+      </c>
+      <c r="C80" s="22">
+        <v>613</v>
+      </c>
+      <c r="D80" s="22">
+        <v>1473</v>
+      </c>
+      <c r="E80" s="22">
+        <v>0</v>
+      </c>
+      <c r="F80" s="22">
+        <v>7</v>
+      </c>
+      <c r="G80" s="22">
+        <v>2</v>
+      </c>
+      <c r="H80" s="22">
+        <v>0</v>
+      </c>
+      <c r="I80" s="22">
+        <v>108</v>
+      </c>
+      <c r="J80" s="22">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="81" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A81" s="20">
+        <v>43981</v>
+      </c>
+      <c r="B81" s="22">
+        <v>78793</v>
+      </c>
+      <c r="C81" s="22">
+        <v>264</v>
+      </c>
+      <c r="D81" s="22">
+        <v>1473</v>
+      </c>
+      <c r="E81" s="22">
+        <v>0</v>
+      </c>
+      <c r="F81" s="22">
+        <v>6</v>
+      </c>
+      <c r="G81" s="22">
+        <v>2</v>
+      </c>
+      <c r="H81" s="22">
+        <v>1</v>
+      </c>
+      <c r="I81" s="22">
+        <v>108</v>
+      </c>
+      <c r="J81" s="22">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="82" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A82" s="20">
+        <v>43982</v>
+      </c>
+      <c r="B82" s="21">
+        <v>79039</v>
+      </c>
+      <c r="C82" s="22">
+        <v>246</v>
+      </c>
+      <c r="D82" s="22">
+        <v>1473</v>
+      </c>
+      <c r="E82" s="22">
+        <v>0</v>
+      </c>
+      <c r="F82" s="22">
+        <v>5</v>
+      </c>
+      <c r="G82" s="22">
+        <v>1</v>
+      </c>
+      <c r="H82" s="22">
+        <v>0</v>
+      </c>
+      <c r="I82" s="22">
+        <v>109</v>
+      </c>
+      <c r="J82" s="22">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="83" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A83" s="20">
+        <v>43983</v>
+      </c>
+      <c r="B83" s="21">
+        <v>79698</v>
+      </c>
+      <c r="C83" s="22">
+        <v>659</v>
+      </c>
+      <c r="D83" s="22">
+        <v>1475</v>
+      </c>
+      <c r="E83" s="22">
+        <v>2</v>
+      </c>
+      <c r="F83" s="22">
+        <v>5</v>
+      </c>
+      <c r="G83" s="22">
+        <v>1</v>
+      </c>
+      <c r="H83" s="22">
+        <v>0</v>
+      </c>
+      <c r="I83" s="22">
+        <v>109</v>
+      </c>
+      <c r="J83" s="22">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="84" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A84" s="20">
+        <v>43984</v>
+      </c>
+      <c r="B84" s="21">
+        <v>80505</v>
+      </c>
+      <c r="C84" s="22">
+        <v>807</v>
+      </c>
+      <c r="D84" s="22">
+        <v>1477</v>
+      </c>
+      <c r="E84" s="22">
+        <v>2</v>
+      </c>
+      <c r="F84" s="22">
+        <v>5</v>
+      </c>
+      <c r="G84" s="22">
+        <v>0</v>
+      </c>
+      <c r="H84" s="22">
+        <v>0</v>
+      </c>
+      <c r="I84" s="22">
+        <v>109</v>
+      </c>
+      <c r="J84" s="22">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="85" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A85" s="20">
+        <v>43985</v>
+      </c>
+      <c r="B85" s="21">
+        <v>81333</v>
+      </c>
+      <c r="C85" s="22">
+        <v>828</v>
+      </c>
+      <c r="D85" s="22">
+        <v>1477</v>
+      </c>
+      <c r="E85" s="22">
+        <v>0</v>
+      </c>
+      <c r="F85" s="22">
+        <v>5</v>
+      </c>
+      <c r="G85" s="22">
+        <v>0</v>
+      </c>
+      <c r="H85" s="22">
+        <v>0</v>
+      </c>
+      <c r="I85" s="22">
+        <v>109</v>
+      </c>
+      <c r="J85" s="22">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="86" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A86" s="26">
+        <v>43986</v>
+      </c>
+      <c r="B86" s="27">
+        <v>82161</v>
+      </c>
+      <c r="C86" s="28">
+        <v>828</v>
+      </c>
+      <c r="D86" s="28">
+        <v>1479</v>
+      </c>
+      <c r="E86" s="28">
+        <v>2</v>
+      </c>
+      <c r="F86" s="28">
+        <v>6</v>
+      </c>
+      <c r="G86" s="28">
+        <v>0</v>
+      </c>
+      <c r="H86" s="28">
+        <v>0</v>
+      </c>
+      <c r="I86" s="28">
+        <v>109</v>
+      </c>
+      <c r="J86" s="28">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="87" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A87" s="29">
+        <v>43987</v>
+      </c>
+      <c r="B87" s="30">
+        <v>82876</v>
+      </c>
+      <c r="C87" s="31">
+        <v>715</v>
+      </c>
+      <c r="D87" s="31">
+        <v>1484</v>
+      </c>
+      <c r="E87" s="31">
+        <v>5</v>
+      </c>
+      <c r="F87" s="31">
+        <v>6</v>
+      </c>
+      <c r="G87" s="31">
+        <v>0</v>
+      </c>
+      <c r="H87" s="31">
+        <v>0</v>
+      </c>
+      <c r="I87" s="31">
+        <v>109</v>
+      </c>
+      <c r="J87" s="31">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="88" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A88" s="23">
+        <v>43988</v>
+      </c>
+      <c r="B88" s="24">
+        <v>83105</v>
+      </c>
+      <c r="C88" s="25">
+        <v>229</v>
+      </c>
+      <c r="D88" s="25">
+        <v>1485</v>
+      </c>
+      <c r="E88" s="25">
+        <v>1</v>
+      </c>
+      <c r="F88" s="25">
+        <v>5</v>
+      </c>
+      <c r="G88" s="25">
+        <v>0</v>
+      </c>
+      <c r="H88" s="25">
+        <v>1</v>
+      </c>
+      <c r="I88" s="25">
+        <v>109</v>
+      </c>
+      <c r="J88" s="25">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="89" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A89" s="29">
+        <v>43989</v>
+      </c>
+      <c r="B89" s="30">
+        <v>83316</v>
+      </c>
+      <c r="C89" s="31">
+        <v>211</v>
+      </c>
+      <c r="D89" s="31">
+        <v>1485</v>
+      </c>
+      <c r="E89" s="31">
+        <v>0</v>
+      </c>
+      <c r="F89" s="31">
+        <v>5</v>
+      </c>
+      <c r="G89" s="31">
+        <v>0</v>
+      </c>
+      <c r="H89" s="31">
+        <v>0</v>
+      </c>
+      <c r="I89" s="31">
+        <v>109</v>
+      </c>
+      <c r="J89" s="31">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="90" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A90" s="20">
+        <v>43990</v>
+      </c>
+      <c r="B90" s="21">
+        <v>84130</v>
+      </c>
+      <c r="C90" s="22">
+        <v>814</v>
+      </c>
+      <c r="D90" s="22">
+        <v>1486</v>
+      </c>
+      <c r="E90" s="22">
+        <v>1</v>
+      </c>
+      <c r="F90" s="22">
+        <v>6</v>
+      </c>
+      <c r="G90" s="22">
+        <v>0</v>
+      </c>
+      <c r="H90" s="22">
+        <v>0</v>
+      </c>
+      <c r="I90" s="22">
+        <v>109</v>
+      </c>
+      <c r="J90" s="22">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="91" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A91" s="20">
+        <v>43991</v>
+      </c>
+      <c r="B91" s="21">
+        <v>84868</v>
+      </c>
+      <c r="C91" s="22">
+        <v>738</v>
+      </c>
+      <c r="D91" s="22">
+        <v>1488</v>
+      </c>
+      <c r="E91" s="22">
+        <v>2</v>
+      </c>
+      <c r="F91" s="22">
+        <v>6</v>
+      </c>
+      <c r="G91" s="22">
+        <v>0</v>
+      </c>
+      <c r="H91" s="22">
+        <v>0</v>
+      </c>
+      <c r="I91" s="22">
+        <v>109</v>
+      </c>
+      <c r="J91" s="22">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="92" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A92" s="23">
+        <v>43992</v>
+      </c>
+      <c r="B92" s="24">
+        <v>85626</v>
+      </c>
+      <c r="C92" s="25">
+        <v>758</v>
+      </c>
+      <c r="D92" s="25">
+        <v>1488</v>
+      </c>
+      <c r="E92" s="25">
+        <v>0</v>
+      </c>
+      <c r="F92" s="25">
+        <v>6</v>
+      </c>
+      <c r="G92" s="25">
+        <v>0</v>
+      </c>
+      <c r="H92" s="25">
+        <v>0</v>
+      </c>
+      <c r="I92" s="25">
+        <v>109</v>
+      </c>
+      <c r="J92" s="25">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="93" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A93" s="29">
+        <v>43993</v>
+      </c>
+      <c r="B93" s="30">
+        <v>86328</v>
+      </c>
+      <c r="C93" s="31">
+        <v>702</v>
+      </c>
+      <c r="D93" s="31">
+        <v>1490</v>
+      </c>
+      <c r="E93" s="31">
+        <v>2</v>
+      </c>
+      <c r="F93" s="31">
+        <v>6</v>
+      </c>
+      <c r="G93" s="31">
+        <v>0</v>
+      </c>
+      <c r="H93" s="31">
+        <v>0</v>
+      </c>
+      <c r="I93" s="31">
+        <v>109</v>
+      </c>
+      <c r="J93" s="31">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="94" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A94" s="23">
+        <v>43994</v>
+      </c>
+      <c r="B94" s="24">
+        <v>87095</v>
+      </c>
+      <c r="C94" s="25">
+        <v>767</v>
+      </c>
+      <c r="D94" s="25">
+        <v>1492</v>
+      </c>
+      <c r="E94" s="25">
+        <v>2</v>
+      </c>
+      <c r="F94" s="25">
+        <v>6</v>
+      </c>
+      <c r="G94" s="25">
+        <v>0</v>
+      </c>
+      <c r="H94" s="25">
+        <v>0</v>
+      </c>
+      <c r="I94" s="25">
+        <v>109</v>
+      </c>
+      <c r="J94" s="25">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="95" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A95" s="29">
+        <v>43995</v>
+      </c>
+      <c r="B95" s="30">
+        <v>87386</v>
+      </c>
+      <c r="C95" s="31">
+        <v>291</v>
+      </c>
+      <c r="D95" s="31">
+        <v>1495</v>
+      </c>
+      <c r="E95" s="31">
+        <v>3</v>
+      </c>
+      <c r="F95" s="31">
+        <v>6</v>
+      </c>
+      <c r="G95" s="31">
+        <v>0</v>
+      </c>
+      <c r="H95" s="31">
+        <v>0</v>
+      </c>
+      <c r="I95" s="31">
+        <v>109</v>
+      </c>
+      <c r="J95" s="31">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="96" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A96" s="23">
+        <v>43996</v>
+      </c>
+      <c r="B96" s="24">
+        <v>87598</v>
+      </c>
+      <c r="C96" s="25">
+        <v>212</v>
+      </c>
+      <c r="D96" s="25">
+        <v>1496</v>
+      </c>
+      <c r="E96" s="25">
+        <v>1</v>
+      </c>
+      <c r="F96" s="25">
+        <v>7</v>
+      </c>
+      <c r="G96" s="25">
+        <v>1</v>
+      </c>
+      <c r="H96" s="25">
+        <v>0</v>
+      </c>
+      <c r="I96" s="25">
+        <v>109</v>
+      </c>
+      <c r="J96" s="25">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="97" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A97" s="20">
+        <v>43997</v>
+      </c>
+      <c r="B97" s="21">
+        <v>88165</v>
+      </c>
+      <c r="C97" s="22">
+        <v>567</v>
+      </c>
+      <c r="D97" s="22">
+        <v>1499</v>
+      </c>
+      <c r="E97" s="22">
+        <v>3</v>
+      </c>
+      <c r="F97" s="22">
+        <v>7</v>
+      </c>
+      <c r="G97" s="22">
+        <v>1</v>
+      </c>
+      <c r="H97" s="22">
+        <v>0</v>
+      </c>
+      <c r="I97" s="22">
+        <v>109</v>
+      </c>
+      <c r="J97" s="22">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="98" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A98" s="20">
+        <v>43998</v>
+      </c>
+      <c r="B98" s="21">
+        <v>89151</v>
+      </c>
+      <c r="C98" s="22">
+        <v>986</v>
+      </c>
+      <c r="D98" s="22">
+        <v>1503</v>
+      </c>
+      <c r="E98" s="22">
+        <v>4</v>
+      </c>
+      <c r="F98" s="22">
+        <v>7</v>
+      </c>
+      <c r="G98" s="22">
+        <v>1</v>
+      </c>
+      <c r="H98" s="22">
+        <v>0</v>
+      </c>
+      <c r="I98" s="22">
+        <v>109</v>
+      </c>
+      <c r="J98" s="22">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="99" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A99" s="29">
+        <v>43999</v>
+      </c>
+      <c r="B99" s="30">
+        <v>90103</v>
+      </c>
+      <c r="C99" s="31">
+        <v>952</v>
+      </c>
+      <c r="D99" s="31">
+        <v>1511</v>
+      </c>
+      <c r="E99" s="31">
+        <v>8</v>
+      </c>
+      <c r="F99" s="31">
+        <v>6</v>
+      </c>
+      <c r="G99" s="31">
+        <v>1</v>
+      </c>
+      <c r="H99" s="31">
+        <v>1</v>
+      </c>
+      <c r="I99" s="31">
+        <v>109</v>
+      </c>
+      <c r="J99" s="31">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="100" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A100" s="20">
+        <v>44000</v>
+      </c>
+      <c r="B100" s="21">
+        <v>91005</v>
+      </c>
+      <c r="C100" s="22">
+        <v>902</v>
+      </c>
+      <c r="D100" s="22">
+        <v>1513</v>
+      </c>
+      <c r="E100" s="22">
+        <v>2</v>
+      </c>
+      <c r="F100" s="22">
+        <v>8</v>
+      </c>
+      <c r="G100" s="22">
+        <v>1</v>
+      </c>
+      <c r="H100" s="22">
+        <v>0</v>
+      </c>
+      <c r="I100" s="22">
+        <v>109</v>
+      </c>
+      <c r="J100" s="22">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="101" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A101" s="29">
+        <v>44001</v>
+      </c>
+      <c r="B101" s="30">
+        <v>92152</v>
+      </c>
+      <c r="C101" s="31">
+        <v>1147</v>
+      </c>
+      <c r="D101" s="31">
+        <v>1519</v>
+      </c>
+      <c r="E101" s="31">
+        <v>6</v>
+      </c>
+      <c r="F101" s="31">
+        <v>6</v>
+      </c>
+      <c r="G101" s="31">
+        <v>1</v>
+      </c>
+      <c r="H101" s="31">
+        <v>2</v>
+      </c>
+      <c r="I101" s="31">
+        <v>109</v>
+      </c>
+      <c r="J101" s="31">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="102" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A102" s="23">
+        <v>44002</v>
+      </c>
+      <c r="B102" s="24">
+        <v>92919</v>
+      </c>
+      <c r="C102" s="25">
+        <v>758</v>
+      </c>
+      <c r="D102" s="25">
+        <v>1520</v>
+      </c>
+      <c r="E102" s="25">
+        <v>1</v>
+      </c>
+      <c r="F102" s="25">
+        <v>6</v>
+      </c>
+      <c r="G102" s="25">
+        <v>1</v>
+      </c>
+      <c r="H102" s="25">
+        <v>2</v>
+      </c>
+      <c r="I102" s="25">
+        <v>109</v>
+      </c>
+      <c r="J102" s="25">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="103" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A103" s="29">
+        <v>44003</v>
+      </c>
+      <c r="B103" s="30">
+        <v>93181</v>
+      </c>
+      <c r="C103" s="31">
+        <v>271</v>
+      </c>
+      <c r="D103" s="31">
+        <v>1521</v>
+      </c>
+      <c r="E103" s="31">
+        <v>1</v>
+      </c>
+      <c r="F103" s="31">
+        <v>6</v>
+      </c>
+      <c r="G103" s="31">
+        <v>1</v>
+      </c>
+      <c r="H103" s="31">
+        <v>0</v>
+      </c>
+      <c r="I103" s="31">
+        <v>109</v>
+      </c>
+      <c r="J103" s="31">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="104" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A104" s="29">
+        <v>44004</v>
+      </c>
+      <c r="B104" s="30">
+        <v>94165</v>
+      </c>
+      <c r="C104" s="31">
+        <v>984</v>
+      </c>
+      <c r="D104" s="31">
+        <v>1534</v>
+      </c>
+      <c r="E104" s="31">
+        <v>13</v>
+      </c>
+      <c r="F104" s="31">
+        <v>5</v>
+      </c>
+      <c r="G104" s="31">
+        <v>1</v>
+      </c>
+      <c r="H104" s="31">
+        <v>1</v>
+      </c>
+      <c r="I104" s="31">
+        <v>109</v>
+      </c>
+      <c r="J104" s="31">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="105" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A105" s="29">
+        <v>44005</v>
+      </c>
+      <c r="B105" s="30">
+        <v>95387</v>
+      </c>
+      <c r="C105" s="31">
+        <v>1222</v>
+      </c>
+      <c r="D105" s="31">
+        <v>1541</v>
+      </c>
+      <c r="E105" s="31">
+        <v>7</v>
+      </c>
+      <c r="F105" s="31">
+        <v>7</v>
+      </c>
+      <c r="G105" s="31">
+        <v>2</v>
+      </c>
+      <c r="H105" s="31">
+        <v>0</v>
+      </c>
+      <c r="I105" s="31" t="s">
+        <v>10</v>
+      </c>
+      <c r="J105" s="31">
+        <v>0</v>
+      </c>
+    </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>

</xml_diff>

<commit_message>
Data updated by GitHub Bot (2020-06-25 12)
</commit_message>
<xml_diff>
--- a/output/snapshot/fdcf2531-4c3e-5c02-b63c-ee160ead6dea.xlsx
+++ b/output/snapshot/fdcf2531-4c3e-5c02-b63c-ee160ead6dea.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="I:\AKTUALNI PODATKI - KORONA\Za objavo na GOV.SI\ang\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{1E6DD62F-2BE2-47DC-A7ED-9B57C1589256}" xr6:coauthVersionLast="44" xr6:coauthVersionMax="44" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{1D5AFACD-32B5-4F54-9BDF-A42BD6F56F00}" xr6:coauthVersionLast="44" xr6:coauthVersionMax="44" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -25,7 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="10" uniqueCount="10">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="12" uniqueCount="11">
   <si>
     <t>Date</t>
   </si>
@@ -56,6 +56,9 @@
   <si>
     <t>Deaths (daily)</t>
   </si>
+  <si>
+    <t>111*</t>
+  </si>
 </sst>
 </file>
 
@@ -64,7 +67,7 @@
   <numFmts count="1">
     <numFmt numFmtId="164" formatCode="d/\ m/\ yyyy;@"/>
   </numFmts>
-  <fonts count="4" x14ac:knownFonts="1">
+  <fonts count="5" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -93,6 +96,13 @@
       <name val="Calibri Light"/>
       <scheme val="major"/>
     </font>
+    <font>
+      <sz val="10"/>
+      <color theme="1"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
   </fonts>
   <fills count="3">
     <fill>
@@ -108,7 +118,7 @@
       </patternFill>
     </fill>
   </fills>
-  <borders count="2">
+  <borders count="3">
     <border>
       <left/>
       <right/>
@@ -129,11 +139,26 @@
       <bottom/>
       <diagonal/>
     </border>
+    <border>
+      <left style="thin">
+        <color theme="4"/>
+      </left>
+      <right style="thin">
+        <color theme="4"/>
+      </right>
+      <top style="thin">
+        <color theme="4"/>
+      </top>
+      <bottom style="thin">
+        <color theme="4"/>
+      </bottom>
+      <diagonal/>
+    </border>
   </borders>
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="26">
+  <cellXfs count="32">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="49" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyAlignment="1" applyProtection="1">
       <alignment horizontal="left" vertical="top"/>
@@ -208,6 +233,24 @@
       <alignment horizontal="right"/>
     </xf>
     <xf numFmtId="0" fontId="3" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="right"/>
+    </xf>
+    <xf numFmtId="164" fontId="4" fillId="2" borderId="2" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="right" vertical="top"/>
+    </xf>
+    <xf numFmtId="3" fontId="4" fillId="2" borderId="2" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="right"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="2" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="right"/>
+    </xf>
+    <xf numFmtId="164" fontId="3" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="right" vertical="top"/>
+    </xf>
+    <xf numFmtId="3" fontId="3" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="right"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="right"/>
     </xf>
   </cellXfs>
@@ -399,8 +442,8 @@
 </file>
 
 <file path=xl/tables/table1.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="1" xr:uid="{00000000-000C-0000-FFFF-FFFF00000000}" name="Tabela1" displayName="Tabela1" ref="A1:J75" totalsRowShown="0" headerRowDxfId="11" dataDxfId="10">
-  <autoFilter ref="A1:J75" xr:uid="{00000000-0009-0000-0100-000001000000}">
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="1" xr:uid="{00000000-000C-0000-FFFF-FFFF00000000}" name="Tabela1" displayName="Tabela1" ref="A1:J106" totalsRowShown="0" headerRowDxfId="11" dataDxfId="10">
+  <autoFilter ref="A1:J106" xr:uid="{00000000-0009-0000-0100-000001000000}">
     <filterColumn colId="0" hiddenButton="1"/>
     <filterColumn colId="1" hiddenButton="1"/>
     <filterColumn colId="2" hiddenButton="1"/>
@@ -696,10 +739,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:J75"/>
+  <dimension ref="A1:J106"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A40" zoomScale="89" zoomScaleNormal="89" workbookViewId="0">
-      <selection activeCell="J74" sqref="J74"/>
+    <sheetView tabSelected="1" topLeftCell="A77" zoomScale="89" zoomScaleNormal="89" workbookViewId="0">
+      <selection activeCell="A106" sqref="A106:J106"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -3117,6 +3160,998 @@
         <v>0</v>
       </c>
     </row>
+    <row r="76" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A76" s="20">
+        <v>43976</v>
+      </c>
+      <c r="B76" s="21">
+        <v>75770</v>
+      </c>
+      <c r="C76" s="22">
+        <v>754</v>
+      </c>
+      <c r="D76" s="22">
+        <v>1469</v>
+      </c>
+      <c r="E76" s="22">
+        <v>0</v>
+      </c>
+      <c r="F76" s="22">
+        <v>9</v>
+      </c>
+      <c r="G76" s="22">
+        <v>2</v>
+      </c>
+      <c r="H76" s="22">
+        <v>6</v>
+      </c>
+      <c r="I76" s="22">
+        <v>108</v>
+      </c>
+      <c r="J76" s="22">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="77" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A77" s="20">
+        <v>43977</v>
+      </c>
+      <c r="B77" s="21">
+        <v>76579</v>
+      </c>
+      <c r="C77" s="22">
+        <v>809</v>
+      </c>
+      <c r="D77" s="22">
+        <v>1471</v>
+      </c>
+      <c r="E77" s="22">
+        <v>2</v>
+      </c>
+      <c r="F77" s="22">
+        <v>8</v>
+      </c>
+      <c r="G77" s="22">
+        <v>2</v>
+      </c>
+      <c r="H77" s="22">
+        <v>2</v>
+      </c>
+      <c r="I77" s="22">
+        <v>108</v>
+      </c>
+      <c r="J77" s="22">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="78" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A78" s="20">
+        <v>43978</v>
+      </c>
+      <c r="B78" s="21">
+        <v>77210</v>
+      </c>
+      <c r="C78" s="22">
+        <v>631</v>
+      </c>
+      <c r="D78" s="22">
+        <v>1473</v>
+      </c>
+      <c r="E78" s="22">
+        <v>2</v>
+      </c>
+      <c r="F78" s="22">
+        <v>7</v>
+      </c>
+      <c r="G78" s="22">
+        <v>2</v>
+      </c>
+      <c r="H78" s="22">
+        <v>1</v>
+      </c>
+      <c r="I78" s="22">
+        <v>108</v>
+      </c>
+      <c r="J78" s="22">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="79" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A79" s="20">
+        <v>43979</v>
+      </c>
+      <c r="B79" s="21">
+        <v>77916</v>
+      </c>
+      <c r="C79" s="22">
+        <v>706</v>
+      </c>
+      <c r="D79" s="22">
+        <v>1473</v>
+      </c>
+      <c r="E79" s="22">
+        <v>0</v>
+      </c>
+      <c r="F79" s="22">
+        <v>7</v>
+      </c>
+      <c r="G79" s="22">
+        <v>2</v>
+      </c>
+      <c r="H79" s="22">
+        <v>0</v>
+      </c>
+      <c r="I79" s="22">
+        <v>108</v>
+      </c>
+      <c r="J79" s="22">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="80" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A80" s="20">
+        <v>43980</v>
+      </c>
+      <c r="B80" s="21">
+        <v>78529</v>
+      </c>
+      <c r="C80" s="22">
+        <v>613</v>
+      </c>
+      <c r="D80" s="22">
+        <v>1473</v>
+      </c>
+      <c r="E80" s="22">
+        <v>0</v>
+      </c>
+      <c r="F80" s="22">
+        <v>7</v>
+      </c>
+      <c r="G80" s="22">
+        <v>2</v>
+      </c>
+      <c r="H80" s="22">
+        <v>0</v>
+      </c>
+      <c r="I80" s="22">
+        <v>108</v>
+      </c>
+      <c r="J80" s="22">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="81" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A81" s="20">
+        <v>43981</v>
+      </c>
+      <c r="B81" s="22">
+        <v>78793</v>
+      </c>
+      <c r="C81" s="22">
+        <v>264</v>
+      </c>
+      <c r="D81" s="22">
+        <v>1473</v>
+      </c>
+      <c r="E81" s="22">
+        <v>0</v>
+      </c>
+      <c r="F81" s="22">
+        <v>6</v>
+      </c>
+      <c r="G81" s="22">
+        <v>2</v>
+      </c>
+      <c r="H81" s="22">
+        <v>1</v>
+      </c>
+      <c r="I81" s="22">
+        <v>108</v>
+      </c>
+      <c r="J81" s="22">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="82" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A82" s="20">
+        <v>43982</v>
+      </c>
+      <c r="B82" s="21">
+        <v>79039</v>
+      </c>
+      <c r="C82" s="22">
+        <v>246</v>
+      </c>
+      <c r="D82" s="22">
+        <v>1473</v>
+      </c>
+      <c r="E82" s="22">
+        <v>0</v>
+      </c>
+      <c r="F82" s="22">
+        <v>5</v>
+      </c>
+      <c r="G82" s="22">
+        <v>1</v>
+      </c>
+      <c r="H82" s="22">
+        <v>0</v>
+      </c>
+      <c r="I82" s="22">
+        <v>109</v>
+      </c>
+      <c r="J82" s="22">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="83" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A83" s="20">
+        <v>43983</v>
+      </c>
+      <c r="B83" s="21">
+        <v>79698</v>
+      </c>
+      <c r="C83" s="22">
+        <v>659</v>
+      </c>
+      <c r="D83" s="22">
+        <v>1475</v>
+      </c>
+      <c r="E83" s="22">
+        <v>2</v>
+      </c>
+      <c r="F83" s="22">
+        <v>5</v>
+      </c>
+      <c r="G83" s="22">
+        <v>1</v>
+      </c>
+      <c r="H83" s="22">
+        <v>0</v>
+      </c>
+      <c r="I83" s="22">
+        <v>109</v>
+      </c>
+      <c r="J83" s="22">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="84" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A84" s="20">
+        <v>43984</v>
+      </c>
+      <c r="B84" s="21">
+        <v>80505</v>
+      </c>
+      <c r="C84" s="22">
+        <v>807</v>
+      </c>
+      <c r="D84" s="22">
+        <v>1477</v>
+      </c>
+      <c r="E84" s="22">
+        <v>2</v>
+      </c>
+      <c r="F84" s="22">
+        <v>5</v>
+      </c>
+      <c r="G84" s="22">
+        <v>0</v>
+      </c>
+      <c r="H84" s="22">
+        <v>0</v>
+      </c>
+      <c r="I84" s="22">
+        <v>109</v>
+      </c>
+      <c r="J84" s="22">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="85" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A85" s="20">
+        <v>43985</v>
+      </c>
+      <c r="B85" s="21">
+        <v>81333</v>
+      </c>
+      <c r="C85" s="22">
+        <v>828</v>
+      </c>
+      <c r="D85" s="22">
+        <v>1477</v>
+      </c>
+      <c r="E85" s="22">
+        <v>0</v>
+      </c>
+      <c r="F85" s="22">
+        <v>5</v>
+      </c>
+      <c r="G85" s="22">
+        <v>0</v>
+      </c>
+      <c r="H85" s="22">
+        <v>0</v>
+      </c>
+      <c r="I85" s="22">
+        <v>109</v>
+      </c>
+      <c r="J85" s="22">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="86" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A86" s="26">
+        <v>43986</v>
+      </c>
+      <c r="B86" s="27">
+        <v>82161</v>
+      </c>
+      <c r="C86" s="28">
+        <v>828</v>
+      </c>
+      <c r="D86" s="28">
+        <v>1479</v>
+      </c>
+      <c r="E86" s="28">
+        <v>2</v>
+      </c>
+      <c r="F86" s="28">
+        <v>6</v>
+      </c>
+      <c r="G86" s="28">
+        <v>0</v>
+      </c>
+      <c r="H86" s="28">
+        <v>0</v>
+      </c>
+      <c r="I86" s="28">
+        <v>109</v>
+      </c>
+      <c r="J86" s="28">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="87" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A87" s="29">
+        <v>43987</v>
+      </c>
+      <c r="B87" s="30">
+        <v>82876</v>
+      </c>
+      <c r="C87" s="31">
+        <v>715</v>
+      </c>
+      <c r="D87" s="31">
+        <v>1484</v>
+      </c>
+      <c r="E87" s="31">
+        <v>5</v>
+      </c>
+      <c r="F87" s="31">
+        <v>6</v>
+      </c>
+      <c r="G87" s="31">
+        <v>0</v>
+      </c>
+      <c r="H87" s="31">
+        <v>0</v>
+      </c>
+      <c r="I87" s="31">
+        <v>109</v>
+      </c>
+      <c r="J87" s="31">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="88" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A88" s="23">
+        <v>43988</v>
+      </c>
+      <c r="B88" s="24">
+        <v>83105</v>
+      </c>
+      <c r="C88" s="25">
+        <v>229</v>
+      </c>
+      <c r="D88" s="25">
+        <v>1485</v>
+      </c>
+      <c r="E88" s="25">
+        <v>1</v>
+      </c>
+      <c r="F88" s="25">
+        <v>5</v>
+      </c>
+      <c r="G88" s="25">
+        <v>0</v>
+      </c>
+      <c r="H88" s="25">
+        <v>1</v>
+      </c>
+      <c r="I88" s="25">
+        <v>109</v>
+      </c>
+      <c r="J88" s="25">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="89" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A89" s="29">
+        <v>43989</v>
+      </c>
+      <c r="B89" s="30">
+        <v>83316</v>
+      </c>
+      <c r="C89" s="31">
+        <v>211</v>
+      </c>
+      <c r="D89" s="31">
+        <v>1485</v>
+      </c>
+      <c r="E89" s="31">
+        <v>0</v>
+      </c>
+      <c r="F89" s="31">
+        <v>5</v>
+      </c>
+      <c r="G89" s="31">
+        <v>0</v>
+      </c>
+      <c r="H89" s="31">
+        <v>0</v>
+      </c>
+      <c r="I89" s="31">
+        <v>109</v>
+      </c>
+      <c r="J89" s="31">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="90" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A90" s="20">
+        <v>43990</v>
+      </c>
+      <c r="B90" s="21">
+        <v>84130</v>
+      </c>
+      <c r="C90" s="22">
+        <v>814</v>
+      </c>
+      <c r="D90" s="22">
+        <v>1486</v>
+      </c>
+      <c r="E90" s="22">
+        <v>1</v>
+      </c>
+      <c r="F90" s="22">
+        <v>6</v>
+      </c>
+      <c r="G90" s="22">
+        <v>0</v>
+      </c>
+      <c r="H90" s="22">
+        <v>0</v>
+      </c>
+      <c r="I90" s="22">
+        <v>109</v>
+      </c>
+      <c r="J90" s="22">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="91" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A91" s="20">
+        <v>43991</v>
+      </c>
+      <c r="B91" s="21">
+        <v>84868</v>
+      </c>
+      <c r="C91" s="22">
+        <v>738</v>
+      </c>
+      <c r="D91" s="22">
+        <v>1488</v>
+      </c>
+      <c r="E91" s="22">
+        <v>2</v>
+      </c>
+      <c r="F91" s="22">
+        <v>6</v>
+      </c>
+      <c r="G91" s="22">
+        <v>0</v>
+      </c>
+      <c r="H91" s="22">
+        <v>0</v>
+      </c>
+      <c r="I91" s="22">
+        <v>109</v>
+      </c>
+      <c r="J91" s="22">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="92" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A92" s="23">
+        <v>43992</v>
+      </c>
+      <c r="B92" s="24">
+        <v>85626</v>
+      </c>
+      <c r="C92" s="25">
+        <v>758</v>
+      </c>
+      <c r="D92" s="25">
+        <v>1488</v>
+      </c>
+      <c r="E92" s="25">
+        <v>0</v>
+      </c>
+      <c r="F92" s="25">
+        <v>6</v>
+      </c>
+      <c r="G92" s="25">
+        <v>0</v>
+      </c>
+      <c r="H92" s="25">
+        <v>0</v>
+      </c>
+      <c r="I92" s="25">
+        <v>109</v>
+      </c>
+      <c r="J92" s="25">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="93" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A93" s="29">
+        <v>43993</v>
+      </c>
+      <c r="B93" s="30">
+        <v>86328</v>
+      </c>
+      <c r="C93" s="31">
+        <v>702</v>
+      </c>
+      <c r="D93" s="31">
+        <v>1490</v>
+      </c>
+      <c r="E93" s="31">
+        <v>2</v>
+      </c>
+      <c r="F93" s="31">
+        <v>6</v>
+      </c>
+      <c r="G93" s="31">
+        <v>0</v>
+      </c>
+      <c r="H93" s="31">
+        <v>0</v>
+      </c>
+      <c r="I93" s="31">
+        <v>109</v>
+      </c>
+      <c r="J93" s="31">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="94" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A94" s="23">
+        <v>43994</v>
+      </c>
+      <c r="B94" s="24">
+        <v>87095</v>
+      </c>
+      <c r="C94" s="25">
+        <v>767</v>
+      </c>
+      <c r="D94" s="25">
+        <v>1492</v>
+      </c>
+      <c r="E94" s="25">
+        <v>2</v>
+      </c>
+      <c r="F94" s="25">
+        <v>6</v>
+      </c>
+      <c r="G94" s="25">
+        <v>0</v>
+      </c>
+      <c r="H94" s="25">
+        <v>0</v>
+      </c>
+      <c r="I94" s="25">
+        <v>109</v>
+      </c>
+      <c r="J94" s="25">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="95" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A95" s="29">
+        <v>43995</v>
+      </c>
+      <c r="B95" s="30">
+        <v>87386</v>
+      </c>
+      <c r="C95" s="31">
+        <v>291</v>
+      </c>
+      <c r="D95" s="31">
+        <v>1495</v>
+      </c>
+      <c r="E95" s="31">
+        <v>3</v>
+      </c>
+      <c r="F95" s="31">
+        <v>6</v>
+      </c>
+      <c r="G95" s="31">
+        <v>0</v>
+      </c>
+      <c r="H95" s="31">
+        <v>0</v>
+      </c>
+      <c r="I95" s="31">
+        <v>109</v>
+      </c>
+      <c r="J95" s="31">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="96" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A96" s="23">
+        <v>43996</v>
+      </c>
+      <c r="B96" s="24">
+        <v>87598</v>
+      </c>
+      <c r="C96" s="25">
+        <v>212</v>
+      </c>
+      <c r="D96" s="25">
+        <v>1496</v>
+      </c>
+      <c r="E96" s="25">
+        <v>1</v>
+      </c>
+      <c r="F96" s="25">
+        <v>7</v>
+      </c>
+      <c r="G96" s="25">
+        <v>1</v>
+      </c>
+      <c r="H96" s="25">
+        <v>0</v>
+      </c>
+      <c r="I96" s="25">
+        <v>109</v>
+      </c>
+      <c r="J96" s="25">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="97" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A97" s="20">
+        <v>43997</v>
+      </c>
+      <c r="B97" s="21">
+        <v>88165</v>
+      </c>
+      <c r="C97" s="22">
+        <v>567</v>
+      </c>
+      <c r="D97" s="22">
+        <v>1499</v>
+      </c>
+      <c r="E97" s="22">
+        <v>3</v>
+      </c>
+      <c r="F97" s="22">
+        <v>7</v>
+      </c>
+      <c r="G97" s="22">
+        <v>1</v>
+      </c>
+      <c r="H97" s="22">
+        <v>0</v>
+      </c>
+      <c r="I97" s="22">
+        <v>109</v>
+      </c>
+      <c r="J97" s="22">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="98" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A98" s="20">
+        <v>43998</v>
+      </c>
+      <c r="B98" s="21">
+        <v>89151</v>
+      </c>
+      <c r="C98" s="22">
+        <v>986</v>
+      </c>
+      <c r="D98" s="22">
+        <v>1503</v>
+      </c>
+      <c r="E98" s="22">
+        <v>4</v>
+      </c>
+      <c r="F98" s="22">
+        <v>7</v>
+      </c>
+      <c r="G98" s="22">
+        <v>1</v>
+      </c>
+      <c r="H98" s="22">
+        <v>0</v>
+      </c>
+      <c r="I98" s="22">
+        <v>109</v>
+      </c>
+      <c r="J98" s="22">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="99" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A99" s="29">
+        <v>43999</v>
+      </c>
+      <c r="B99" s="30">
+        <v>90103</v>
+      </c>
+      <c r="C99" s="31">
+        <v>952</v>
+      </c>
+      <c r="D99" s="31">
+        <v>1511</v>
+      </c>
+      <c r="E99" s="31">
+        <v>8</v>
+      </c>
+      <c r="F99" s="31">
+        <v>6</v>
+      </c>
+      <c r="G99" s="31">
+        <v>1</v>
+      </c>
+      <c r="H99" s="31">
+        <v>1</v>
+      </c>
+      <c r="I99" s="31">
+        <v>109</v>
+      </c>
+      <c r="J99" s="31">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="100" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A100" s="20">
+        <v>44000</v>
+      </c>
+      <c r="B100" s="21">
+        <v>91005</v>
+      </c>
+      <c r="C100" s="22">
+        <v>902</v>
+      </c>
+      <c r="D100" s="22">
+        <v>1513</v>
+      </c>
+      <c r="E100" s="22">
+        <v>2</v>
+      </c>
+      <c r="F100" s="22">
+        <v>8</v>
+      </c>
+      <c r="G100" s="22">
+        <v>1</v>
+      </c>
+      <c r="H100" s="22">
+        <v>0</v>
+      </c>
+      <c r="I100" s="22">
+        <v>109</v>
+      </c>
+      <c r="J100" s="22">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="101" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A101" s="29">
+        <v>44001</v>
+      </c>
+      <c r="B101" s="30">
+        <v>92152</v>
+      </c>
+      <c r="C101" s="31">
+        <v>1147</v>
+      </c>
+      <c r="D101" s="31">
+        <v>1519</v>
+      </c>
+      <c r="E101" s="31">
+        <v>6</v>
+      </c>
+      <c r="F101" s="31">
+        <v>6</v>
+      </c>
+      <c r="G101" s="31">
+        <v>1</v>
+      </c>
+      <c r="H101" s="31">
+        <v>2</v>
+      </c>
+      <c r="I101" s="31">
+        <v>109</v>
+      </c>
+      <c r="J101" s="31">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="102" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A102" s="23">
+        <v>44002</v>
+      </c>
+      <c r="B102" s="24">
+        <v>92919</v>
+      </c>
+      <c r="C102" s="25">
+        <v>758</v>
+      </c>
+      <c r="D102" s="25">
+        <v>1520</v>
+      </c>
+      <c r="E102" s="25">
+        <v>1</v>
+      </c>
+      <c r="F102" s="25">
+        <v>6</v>
+      </c>
+      <c r="G102" s="25">
+        <v>1</v>
+      </c>
+      <c r="H102" s="25">
+        <v>2</v>
+      </c>
+      <c r="I102" s="25">
+        <v>109</v>
+      </c>
+      <c r="J102" s="25">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="103" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A103" s="29">
+        <v>44003</v>
+      </c>
+      <c r="B103" s="30">
+        <v>93181</v>
+      </c>
+      <c r="C103" s="31">
+        <v>271</v>
+      </c>
+      <c r="D103" s="31">
+        <v>1521</v>
+      </c>
+      <c r="E103" s="31">
+        <v>1</v>
+      </c>
+      <c r="F103" s="31">
+        <v>6</v>
+      </c>
+      <c r="G103" s="31">
+        <v>1</v>
+      </c>
+      <c r="H103" s="31">
+        <v>0</v>
+      </c>
+      <c r="I103" s="31">
+        <v>109</v>
+      </c>
+      <c r="J103" s="31">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="104" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A104" s="29">
+        <v>44004</v>
+      </c>
+      <c r="B104" s="30">
+        <v>94165</v>
+      </c>
+      <c r="C104" s="31">
+        <v>984</v>
+      </c>
+      <c r="D104" s="31">
+        <v>1534</v>
+      </c>
+      <c r="E104" s="31">
+        <v>13</v>
+      </c>
+      <c r="F104" s="31">
+        <v>5</v>
+      </c>
+      <c r="G104" s="31">
+        <v>1</v>
+      </c>
+      <c r="H104" s="31">
+        <v>1</v>
+      </c>
+      <c r="I104" s="31">
+        <v>109</v>
+      </c>
+      <c r="J104" s="31">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="105" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A105" s="29">
+        <v>44005</v>
+      </c>
+      <c r="B105" s="30">
+        <v>95387</v>
+      </c>
+      <c r="C105" s="31">
+        <v>1222</v>
+      </c>
+      <c r="D105" s="31">
+        <v>1541</v>
+      </c>
+      <c r="E105" s="31">
+        <v>7</v>
+      </c>
+      <c r="F105" s="31">
+        <v>7</v>
+      </c>
+      <c r="G105" s="31">
+        <v>2</v>
+      </c>
+      <c r="H105" s="31">
+        <v>0</v>
+      </c>
+      <c r="I105" s="31" t="s">
+        <v>10</v>
+      </c>
+      <c r="J105" s="31">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="106" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A106" s="23">
+        <v>44006</v>
+      </c>
+      <c r="B106" s="24">
+        <v>96599</v>
+      </c>
+      <c r="C106" s="25">
+        <v>1212</v>
+      </c>
+      <c r="D106" s="25">
+        <v>1547</v>
+      </c>
+      <c r="E106" s="25">
+        <v>6</v>
+      </c>
+      <c r="F106" s="25">
+        <v>7</v>
+      </c>
+      <c r="G106" s="25">
+        <v>2</v>
+      </c>
+      <c r="H106" s="25">
+        <v>0</v>
+      </c>
+      <c r="I106" s="25" t="s">
+        <v>10</v>
+      </c>
+      <c r="J106" s="25">
+        <v>0</v>
+      </c>
+    </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>

</xml_diff>

<commit_message>
Data updated by GitHub Bot (2020-06-25 20)
</commit_message>
<xml_diff>
--- a/output/snapshot/fdcf2531-4c3e-5c02-b63c-ee160ead6dea.xlsx
+++ b/output/snapshot/fdcf2531-4c3e-5c02-b63c-ee160ead6dea.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="I:\AKTUALNI PODATKI - KORONA\Za objavo na GOV.SI\ang\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{1E6DD62F-2BE2-47DC-A7ED-9B57C1589256}" xr6:coauthVersionLast="44" xr6:coauthVersionMax="44" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{1D5AFACD-32B5-4F54-9BDF-A42BD6F56F00}" xr6:coauthVersionLast="44" xr6:coauthVersionMax="44" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -25,7 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="10" uniqueCount="10">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="12" uniqueCount="11">
   <si>
     <t>Date</t>
   </si>
@@ -56,6 +56,9 @@
   <si>
     <t>Deaths (daily)</t>
   </si>
+  <si>
+    <t>111*</t>
+  </si>
 </sst>
 </file>
 
@@ -64,7 +67,7 @@
   <numFmts count="1">
     <numFmt numFmtId="164" formatCode="d/\ m/\ yyyy;@"/>
   </numFmts>
-  <fonts count="4" x14ac:knownFonts="1">
+  <fonts count="5" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -93,6 +96,13 @@
       <name val="Calibri Light"/>
       <scheme val="major"/>
     </font>
+    <font>
+      <sz val="10"/>
+      <color theme="1"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
   </fonts>
   <fills count="3">
     <fill>
@@ -108,7 +118,7 @@
       </patternFill>
     </fill>
   </fills>
-  <borders count="2">
+  <borders count="3">
     <border>
       <left/>
       <right/>
@@ -129,11 +139,26 @@
       <bottom/>
       <diagonal/>
     </border>
+    <border>
+      <left style="thin">
+        <color theme="4"/>
+      </left>
+      <right style="thin">
+        <color theme="4"/>
+      </right>
+      <top style="thin">
+        <color theme="4"/>
+      </top>
+      <bottom style="thin">
+        <color theme="4"/>
+      </bottom>
+      <diagonal/>
+    </border>
   </borders>
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="26">
+  <cellXfs count="32">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="49" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyAlignment="1" applyProtection="1">
       <alignment horizontal="left" vertical="top"/>
@@ -208,6 +233,24 @@
       <alignment horizontal="right"/>
     </xf>
     <xf numFmtId="0" fontId="3" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="right"/>
+    </xf>
+    <xf numFmtId="164" fontId="4" fillId="2" borderId="2" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="right" vertical="top"/>
+    </xf>
+    <xf numFmtId="3" fontId="4" fillId="2" borderId="2" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="right"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="2" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="right"/>
+    </xf>
+    <xf numFmtId="164" fontId="3" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="right" vertical="top"/>
+    </xf>
+    <xf numFmtId="3" fontId="3" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="right"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="right"/>
     </xf>
   </cellXfs>
@@ -399,8 +442,8 @@
 </file>
 
 <file path=xl/tables/table1.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="1" xr:uid="{00000000-000C-0000-FFFF-FFFF00000000}" name="Tabela1" displayName="Tabela1" ref="A1:J75" totalsRowShown="0" headerRowDxfId="11" dataDxfId="10">
-  <autoFilter ref="A1:J75" xr:uid="{00000000-0009-0000-0100-000001000000}">
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="1" xr:uid="{00000000-000C-0000-FFFF-FFFF00000000}" name="Tabela1" displayName="Tabela1" ref="A1:J106" totalsRowShown="0" headerRowDxfId="11" dataDxfId="10">
+  <autoFilter ref="A1:J106" xr:uid="{00000000-0009-0000-0100-000001000000}">
     <filterColumn colId="0" hiddenButton="1"/>
     <filterColumn colId="1" hiddenButton="1"/>
     <filterColumn colId="2" hiddenButton="1"/>
@@ -696,10 +739,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:J75"/>
+  <dimension ref="A1:J106"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A40" zoomScale="89" zoomScaleNormal="89" workbookViewId="0">
-      <selection activeCell="J74" sqref="J74"/>
+    <sheetView tabSelected="1" topLeftCell="A77" zoomScale="89" zoomScaleNormal="89" workbookViewId="0">
+      <selection activeCell="A106" sqref="A106:J106"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -3117,6 +3160,998 @@
         <v>0</v>
       </c>
     </row>
+    <row r="76" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A76" s="20">
+        <v>43976</v>
+      </c>
+      <c r="B76" s="21">
+        <v>75770</v>
+      </c>
+      <c r="C76" s="22">
+        <v>754</v>
+      </c>
+      <c r="D76" s="22">
+        <v>1469</v>
+      </c>
+      <c r="E76" s="22">
+        <v>0</v>
+      </c>
+      <c r="F76" s="22">
+        <v>9</v>
+      </c>
+      <c r="G76" s="22">
+        <v>2</v>
+      </c>
+      <c r="H76" s="22">
+        <v>6</v>
+      </c>
+      <c r="I76" s="22">
+        <v>108</v>
+      </c>
+      <c r="J76" s="22">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="77" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A77" s="20">
+        <v>43977</v>
+      </c>
+      <c r="B77" s="21">
+        <v>76579</v>
+      </c>
+      <c r="C77" s="22">
+        <v>809</v>
+      </c>
+      <c r="D77" s="22">
+        <v>1471</v>
+      </c>
+      <c r="E77" s="22">
+        <v>2</v>
+      </c>
+      <c r="F77" s="22">
+        <v>8</v>
+      </c>
+      <c r="G77" s="22">
+        <v>2</v>
+      </c>
+      <c r="H77" s="22">
+        <v>2</v>
+      </c>
+      <c r="I77" s="22">
+        <v>108</v>
+      </c>
+      <c r="J77" s="22">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="78" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A78" s="20">
+        <v>43978</v>
+      </c>
+      <c r="B78" s="21">
+        <v>77210</v>
+      </c>
+      <c r="C78" s="22">
+        <v>631</v>
+      </c>
+      <c r="D78" s="22">
+        <v>1473</v>
+      </c>
+      <c r="E78" s="22">
+        <v>2</v>
+      </c>
+      <c r="F78" s="22">
+        <v>7</v>
+      </c>
+      <c r="G78" s="22">
+        <v>2</v>
+      </c>
+      <c r="H78" s="22">
+        <v>1</v>
+      </c>
+      <c r="I78" s="22">
+        <v>108</v>
+      </c>
+      <c r="J78" s="22">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="79" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A79" s="20">
+        <v>43979</v>
+      </c>
+      <c r="B79" s="21">
+        <v>77916</v>
+      </c>
+      <c r="C79" s="22">
+        <v>706</v>
+      </c>
+      <c r="D79" s="22">
+        <v>1473</v>
+      </c>
+      <c r="E79" s="22">
+        <v>0</v>
+      </c>
+      <c r="F79" s="22">
+        <v>7</v>
+      </c>
+      <c r="G79" s="22">
+        <v>2</v>
+      </c>
+      <c r="H79" s="22">
+        <v>0</v>
+      </c>
+      <c r="I79" s="22">
+        <v>108</v>
+      </c>
+      <c r="J79" s="22">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="80" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A80" s="20">
+        <v>43980</v>
+      </c>
+      <c r="B80" s="21">
+        <v>78529</v>
+      </c>
+      <c r="C80" s="22">
+        <v>613</v>
+      </c>
+      <c r="D80" s="22">
+        <v>1473</v>
+      </c>
+      <c r="E80" s="22">
+        <v>0</v>
+      </c>
+      <c r="F80" s="22">
+        <v>7</v>
+      </c>
+      <c r="G80" s="22">
+        <v>2</v>
+      </c>
+      <c r="H80" s="22">
+        <v>0</v>
+      </c>
+      <c r="I80" s="22">
+        <v>108</v>
+      </c>
+      <c r="J80" s="22">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="81" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A81" s="20">
+        <v>43981</v>
+      </c>
+      <c r="B81" s="22">
+        <v>78793</v>
+      </c>
+      <c r="C81" s="22">
+        <v>264</v>
+      </c>
+      <c r="D81" s="22">
+        <v>1473</v>
+      </c>
+      <c r="E81" s="22">
+        <v>0</v>
+      </c>
+      <c r="F81" s="22">
+        <v>6</v>
+      </c>
+      <c r="G81" s="22">
+        <v>2</v>
+      </c>
+      <c r="H81" s="22">
+        <v>1</v>
+      </c>
+      <c r="I81" s="22">
+        <v>108</v>
+      </c>
+      <c r="J81" s="22">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="82" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A82" s="20">
+        <v>43982</v>
+      </c>
+      <c r="B82" s="21">
+        <v>79039</v>
+      </c>
+      <c r="C82" s="22">
+        <v>246</v>
+      </c>
+      <c r="D82" s="22">
+        <v>1473</v>
+      </c>
+      <c r="E82" s="22">
+        <v>0</v>
+      </c>
+      <c r="F82" s="22">
+        <v>5</v>
+      </c>
+      <c r="G82" s="22">
+        <v>1</v>
+      </c>
+      <c r="H82" s="22">
+        <v>0</v>
+      </c>
+      <c r="I82" s="22">
+        <v>109</v>
+      </c>
+      <c r="J82" s="22">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="83" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A83" s="20">
+        <v>43983</v>
+      </c>
+      <c r="B83" s="21">
+        <v>79698</v>
+      </c>
+      <c r="C83" s="22">
+        <v>659</v>
+      </c>
+      <c r="D83" s="22">
+        <v>1475</v>
+      </c>
+      <c r="E83" s="22">
+        <v>2</v>
+      </c>
+      <c r="F83" s="22">
+        <v>5</v>
+      </c>
+      <c r="G83" s="22">
+        <v>1</v>
+      </c>
+      <c r="H83" s="22">
+        <v>0</v>
+      </c>
+      <c r="I83" s="22">
+        <v>109</v>
+      </c>
+      <c r="J83" s="22">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="84" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A84" s="20">
+        <v>43984</v>
+      </c>
+      <c r="B84" s="21">
+        <v>80505</v>
+      </c>
+      <c r="C84" s="22">
+        <v>807</v>
+      </c>
+      <c r="D84" s="22">
+        <v>1477</v>
+      </c>
+      <c r="E84" s="22">
+        <v>2</v>
+      </c>
+      <c r="F84" s="22">
+        <v>5</v>
+      </c>
+      <c r="G84" s="22">
+        <v>0</v>
+      </c>
+      <c r="H84" s="22">
+        <v>0</v>
+      </c>
+      <c r="I84" s="22">
+        <v>109</v>
+      </c>
+      <c r="J84" s="22">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="85" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A85" s="20">
+        <v>43985</v>
+      </c>
+      <c r="B85" s="21">
+        <v>81333</v>
+      </c>
+      <c r="C85" s="22">
+        <v>828</v>
+      </c>
+      <c r="D85" s="22">
+        <v>1477</v>
+      </c>
+      <c r="E85" s="22">
+        <v>0</v>
+      </c>
+      <c r="F85" s="22">
+        <v>5</v>
+      </c>
+      <c r="G85" s="22">
+        <v>0</v>
+      </c>
+      <c r="H85" s="22">
+        <v>0</v>
+      </c>
+      <c r="I85" s="22">
+        <v>109</v>
+      </c>
+      <c r="J85" s="22">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="86" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A86" s="26">
+        <v>43986</v>
+      </c>
+      <c r="B86" s="27">
+        <v>82161</v>
+      </c>
+      <c r="C86" s="28">
+        <v>828</v>
+      </c>
+      <c r="D86" s="28">
+        <v>1479</v>
+      </c>
+      <c r="E86" s="28">
+        <v>2</v>
+      </c>
+      <c r="F86" s="28">
+        <v>6</v>
+      </c>
+      <c r="G86" s="28">
+        <v>0</v>
+      </c>
+      <c r="H86" s="28">
+        <v>0</v>
+      </c>
+      <c r="I86" s="28">
+        <v>109</v>
+      </c>
+      <c r="J86" s="28">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="87" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A87" s="29">
+        <v>43987</v>
+      </c>
+      <c r="B87" s="30">
+        <v>82876</v>
+      </c>
+      <c r="C87" s="31">
+        <v>715</v>
+      </c>
+      <c r="D87" s="31">
+        <v>1484</v>
+      </c>
+      <c r="E87" s="31">
+        <v>5</v>
+      </c>
+      <c r="F87" s="31">
+        <v>6</v>
+      </c>
+      <c r="G87" s="31">
+        <v>0</v>
+      </c>
+      <c r="H87" s="31">
+        <v>0</v>
+      </c>
+      <c r="I87" s="31">
+        <v>109</v>
+      </c>
+      <c r="J87" s="31">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="88" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A88" s="23">
+        <v>43988</v>
+      </c>
+      <c r="B88" s="24">
+        <v>83105</v>
+      </c>
+      <c r="C88" s="25">
+        <v>229</v>
+      </c>
+      <c r="D88" s="25">
+        <v>1485</v>
+      </c>
+      <c r="E88" s="25">
+        <v>1</v>
+      </c>
+      <c r="F88" s="25">
+        <v>5</v>
+      </c>
+      <c r="G88" s="25">
+        <v>0</v>
+      </c>
+      <c r="H88" s="25">
+        <v>1</v>
+      </c>
+      <c r="I88" s="25">
+        <v>109</v>
+      </c>
+      <c r="J88" s="25">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="89" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A89" s="29">
+        <v>43989</v>
+      </c>
+      <c r="B89" s="30">
+        <v>83316</v>
+      </c>
+      <c r="C89" s="31">
+        <v>211</v>
+      </c>
+      <c r="D89" s="31">
+        <v>1485</v>
+      </c>
+      <c r="E89" s="31">
+        <v>0</v>
+      </c>
+      <c r="F89" s="31">
+        <v>5</v>
+      </c>
+      <c r="G89" s="31">
+        <v>0</v>
+      </c>
+      <c r="H89" s="31">
+        <v>0</v>
+      </c>
+      <c r="I89" s="31">
+        <v>109</v>
+      </c>
+      <c r="J89" s="31">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="90" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A90" s="20">
+        <v>43990</v>
+      </c>
+      <c r="B90" s="21">
+        <v>84130</v>
+      </c>
+      <c r="C90" s="22">
+        <v>814</v>
+      </c>
+      <c r="D90" s="22">
+        <v>1486</v>
+      </c>
+      <c r="E90" s="22">
+        <v>1</v>
+      </c>
+      <c r="F90" s="22">
+        <v>6</v>
+      </c>
+      <c r="G90" s="22">
+        <v>0</v>
+      </c>
+      <c r="H90" s="22">
+        <v>0</v>
+      </c>
+      <c r="I90" s="22">
+        <v>109</v>
+      </c>
+      <c r="J90" s="22">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="91" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A91" s="20">
+        <v>43991</v>
+      </c>
+      <c r="B91" s="21">
+        <v>84868</v>
+      </c>
+      <c r="C91" s="22">
+        <v>738</v>
+      </c>
+      <c r="D91" s="22">
+        <v>1488</v>
+      </c>
+      <c r="E91" s="22">
+        <v>2</v>
+      </c>
+      <c r="F91" s="22">
+        <v>6</v>
+      </c>
+      <c r="G91" s="22">
+        <v>0</v>
+      </c>
+      <c r="H91" s="22">
+        <v>0</v>
+      </c>
+      <c r="I91" s="22">
+        <v>109</v>
+      </c>
+      <c r="J91" s="22">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="92" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A92" s="23">
+        <v>43992</v>
+      </c>
+      <c r="B92" s="24">
+        <v>85626</v>
+      </c>
+      <c r="C92" s="25">
+        <v>758</v>
+      </c>
+      <c r="D92" s="25">
+        <v>1488</v>
+      </c>
+      <c r="E92" s="25">
+        <v>0</v>
+      </c>
+      <c r="F92" s="25">
+        <v>6</v>
+      </c>
+      <c r="G92" s="25">
+        <v>0</v>
+      </c>
+      <c r="H92" s="25">
+        <v>0</v>
+      </c>
+      <c r="I92" s="25">
+        <v>109</v>
+      </c>
+      <c r="J92" s="25">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="93" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A93" s="29">
+        <v>43993</v>
+      </c>
+      <c r="B93" s="30">
+        <v>86328</v>
+      </c>
+      <c r="C93" s="31">
+        <v>702</v>
+      </c>
+      <c r="D93" s="31">
+        <v>1490</v>
+      </c>
+      <c r="E93" s="31">
+        <v>2</v>
+      </c>
+      <c r="F93" s="31">
+        <v>6</v>
+      </c>
+      <c r="G93" s="31">
+        <v>0</v>
+      </c>
+      <c r="H93" s="31">
+        <v>0</v>
+      </c>
+      <c r="I93" s="31">
+        <v>109</v>
+      </c>
+      <c r="J93" s="31">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="94" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A94" s="23">
+        <v>43994</v>
+      </c>
+      <c r="B94" s="24">
+        <v>87095</v>
+      </c>
+      <c r="C94" s="25">
+        <v>767</v>
+      </c>
+      <c r="D94" s="25">
+        <v>1492</v>
+      </c>
+      <c r="E94" s="25">
+        <v>2</v>
+      </c>
+      <c r="F94" s="25">
+        <v>6</v>
+      </c>
+      <c r="G94" s="25">
+        <v>0</v>
+      </c>
+      <c r="H94" s="25">
+        <v>0</v>
+      </c>
+      <c r="I94" s="25">
+        <v>109</v>
+      </c>
+      <c r="J94" s="25">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="95" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A95" s="29">
+        <v>43995</v>
+      </c>
+      <c r="B95" s="30">
+        <v>87386</v>
+      </c>
+      <c r="C95" s="31">
+        <v>291</v>
+      </c>
+      <c r="D95" s="31">
+        <v>1495</v>
+      </c>
+      <c r="E95" s="31">
+        <v>3</v>
+      </c>
+      <c r="F95" s="31">
+        <v>6</v>
+      </c>
+      <c r="G95" s="31">
+        <v>0</v>
+      </c>
+      <c r="H95" s="31">
+        <v>0</v>
+      </c>
+      <c r="I95" s="31">
+        <v>109</v>
+      </c>
+      <c r="J95" s="31">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="96" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A96" s="23">
+        <v>43996</v>
+      </c>
+      <c r="B96" s="24">
+        <v>87598</v>
+      </c>
+      <c r="C96" s="25">
+        <v>212</v>
+      </c>
+      <c r="D96" s="25">
+        <v>1496</v>
+      </c>
+      <c r="E96" s="25">
+        <v>1</v>
+      </c>
+      <c r="F96" s="25">
+        <v>7</v>
+      </c>
+      <c r="G96" s="25">
+        <v>1</v>
+      </c>
+      <c r="H96" s="25">
+        <v>0</v>
+      </c>
+      <c r="I96" s="25">
+        <v>109</v>
+      </c>
+      <c r="J96" s="25">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="97" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A97" s="20">
+        <v>43997</v>
+      </c>
+      <c r="B97" s="21">
+        <v>88165</v>
+      </c>
+      <c r="C97" s="22">
+        <v>567</v>
+      </c>
+      <c r="D97" s="22">
+        <v>1499</v>
+      </c>
+      <c r="E97" s="22">
+        <v>3</v>
+      </c>
+      <c r="F97" s="22">
+        <v>7</v>
+      </c>
+      <c r="G97" s="22">
+        <v>1</v>
+      </c>
+      <c r="H97" s="22">
+        <v>0</v>
+      </c>
+      <c r="I97" s="22">
+        <v>109</v>
+      </c>
+      <c r="J97" s="22">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="98" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A98" s="20">
+        <v>43998</v>
+      </c>
+      <c r="B98" s="21">
+        <v>89151</v>
+      </c>
+      <c r="C98" s="22">
+        <v>986</v>
+      </c>
+      <c r="D98" s="22">
+        <v>1503</v>
+      </c>
+      <c r="E98" s="22">
+        <v>4</v>
+      </c>
+      <c r="F98" s="22">
+        <v>7</v>
+      </c>
+      <c r="G98" s="22">
+        <v>1</v>
+      </c>
+      <c r="H98" s="22">
+        <v>0</v>
+      </c>
+      <c r="I98" s="22">
+        <v>109</v>
+      </c>
+      <c r="J98" s="22">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="99" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A99" s="29">
+        <v>43999</v>
+      </c>
+      <c r="B99" s="30">
+        <v>90103</v>
+      </c>
+      <c r="C99" s="31">
+        <v>952</v>
+      </c>
+      <c r="D99" s="31">
+        <v>1511</v>
+      </c>
+      <c r="E99" s="31">
+        <v>8</v>
+      </c>
+      <c r="F99" s="31">
+        <v>6</v>
+      </c>
+      <c r="G99" s="31">
+        <v>1</v>
+      </c>
+      <c r="H99" s="31">
+        <v>1</v>
+      </c>
+      <c r="I99" s="31">
+        <v>109</v>
+      </c>
+      <c r="J99" s="31">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="100" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A100" s="20">
+        <v>44000</v>
+      </c>
+      <c r="B100" s="21">
+        <v>91005</v>
+      </c>
+      <c r="C100" s="22">
+        <v>902</v>
+      </c>
+      <c r="D100" s="22">
+        <v>1513</v>
+      </c>
+      <c r="E100" s="22">
+        <v>2</v>
+      </c>
+      <c r="F100" s="22">
+        <v>8</v>
+      </c>
+      <c r="G100" s="22">
+        <v>1</v>
+      </c>
+      <c r="H100" s="22">
+        <v>0</v>
+      </c>
+      <c r="I100" s="22">
+        <v>109</v>
+      </c>
+      <c r="J100" s="22">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="101" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A101" s="29">
+        <v>44001</v>
+      </c>
+      <c r="B101" s="30">
+        <v>92152</v>
+      </c>
+      <c r="C101" s="31">
+        <v>1147</v>
+      </c>
+      <c r="D101" s="31">
+        <v>1519</v>
+      </c>
+      <c r="E101" s="31">
+        <v>6</v>
+      </c>
+      <c r="F101" s="31">
+        <v>6</v>
+      </c>
+      <c r="G101" s="31">
+        <v>1</v>
+      </c>
+      <c r="H101" s="31">
+        <v>2</v>
+      </c>
+      <c r="I101" s="31">
+        <v>109</v>
+      </c>
+      <c r="J101" s="31">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="102" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A102" s="23">
+        <v>44002</v>
+      </c>
+      <c r="B102" s="24">
+        <v>92919</v>
+      </c>
+      <c r="C102" s="25">
+        <v>758</v>
+      </c>
+      <c r="D102" s="25">
+        <v>1520</v>
+      </c>
+      <c r="E102" s="25">
+        <v>1</v>
+      </c>
+      <c r="F102" s="25">
+        <v>6</v>
+      </c>
+      <c r="G102" s="25">
+        <v>1</v>
+      </c>
+      <c r="H102" s="25">
+        <v>2</v>
+      </c>
+      <c r="I102" s="25">
+        <v>109</v>
+      </c>
+      <c r="J102" s="25">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="103" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A103" s="29">
+        <v>44003</v>
+      </c>
+      <c r="B103" s="30">
+        <v>93181</v>
+      </c>
+      <c r="C103" s="31">
+        <v>271</v>
+      </c>
+      <c r="D103" s="31">
+        <v>1521</v>
+      </c>
+      <c r="E103" s="31">
+        <v>1</v>
+      </c>
+      <c r="F103" s="31">
+        <v>6</v>
+      </c>
+      <c r="G103" s="31">
+        <v>1</v>
+      </c>
+      <c r="H103" s="31">
+        <v>0</v>
+      </c>
+      <c r="I103" s="31">
+        <v>109</v>
+      </c>
+      <c r="J103" s="31">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="104" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A104" s="29">
+        <v>44004</v>
+      </c>
+      <c r="B104" s="30">
+        <v>94165</v>
+      </c>
+      <c r="C104" s="31">
+        <v>984</v>
+      </c>
+      <c r="D104" s="31">
+        <v>1534</v>
+      </c>
+      <c r="E104" s="31">
+        <v>13</v>
+      </c>
+      <c r="F104" s="31">
+        <v>5</v>
+      </c>
+      <c r="G104" s="31">
+        <v>1</v>
+      </c>
+      <c r="H104" s="31">
+        <v>1</v>
+      </c>
+      <c r="I104" s="31">
+        <v>109</v>
+      </c>
+      <c r="J104" s="31">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="105" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A105" s="29">
+        <v>44005</v>
+      </c>
+      <c r="B105" s="30">
+        <v>95387</v>
+      </c>
+      <c r="C105" s="31">
+        <v>1222</v>
+      </c>
+      <c r="D105" s="31">
+        <v>1541</v>
+      </c>
+      <c r="E105" s="31">
+        <v>7</v>
+      </c>
+      <c r="F105" s="31">
+        <v>7</v>
+      </c>
+      <c r="G105" s="31">
+        <v>2</v>
+      </c>
+      <c r="H105" s="31">
+        <v>0</v>
+      </c>
+      <c r="I105" s="31" t="s">
+        <v>10</v>
+      </c>
+      <c r="J105" s="31">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="106" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A106" s="23">
+        <v>44006</v>
+      </c>
+      <c r="B106" s="24">
+        <v>96599</v>
+      </c>
+      <c r="C106" s="25">
+        <v>1212</v>
+      </c>
+      <c r="D106" s="25">
+        <v>1547</v>
+      </c>
+      <c r="E106" s="25">
+        <v>6</v>
+      </c>
+      <c r="F106" s="25">
+        <v>7</v>
+      </c>
+      <c r="G106" s="25">
+        <v>2</v>
+      </c>
+      <c r="H106" s="25">
+        <v>0</v>
+      </c>
+      <c r="I106" s="25" t="s">
+        <v>10</v>
+      </c>
+      <c r="J106" s="25">
+        <v>0</v>
+      </c>
+    </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>

</xml_diff>

<commit_message>
Data updated by GitHub Bot (2020-06-26 12)
</commit_message>
<xml_diff>
--- a/output/snapshot/fdcf2531-4c3e-5c02-b63c-ee160ead6dea.xlsx
+++ b/output/snapshot/fdcf2531-4c3e-5c02-b63c-ee160ead6dea.xlsx
@@ -1,16 +1,15 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="21929"/>
-  <workbookPr/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
+  <fileVersion appName="xl" lastEdited="6" lowestEdited="6" rupBuild="14420"/>
+  <workbookPr defaultThemeVersion="164011"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="I:\AKTUALNI PODATKI - KORONA\Za objavo na GOV.SI\ang\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{1E6DD62F-2BE2-47DC-A7ED-9B57C1589256}" xr6:coauthVersionLast="44" xr6:coauthVersionMax="44" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840"/>
   </bookViews>
   <sheets>
     <sheet name="Covid-19 podatki" sheetId="1" r:id="rId1"/>
@@ -25,7 +24,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="10" uniqueCount="10">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="13" uniqueCount="11">
   <si>
     <t>Date</t>
   </si>
@@ -56,15 +55,18 @@
   <si>
     <t>Deaths (daily)</t>
   </si>
+  <si>
+    <t>111*</t>
+  </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" mc:Ignorable="x14ac x16r2">
   <numFmts count="1">
     <numFmt numFmtId="164" formatCode="d/\ m/\ yyyy;@"/>
   </numFmts>
-  <fonts count="4" x14ac:knownFonts="1">
+  <fonts count="5" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -93,6 +95,13 @@
       <name val="Calibri Light"/>
       <scheme val="major"/>
     </font>
+    <font>
+      <sz val="10"/>
+      <color theme="1"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
   </fonts>
   <fills count="3">
     <fill>
@@ -108,7 +117,7 @@
       </patternFill>
     </fill>
   </fills>
-  <borders count="2">
+  <borders count="3">
     <border>
       <left/>
       <right/>
@@ -129,11 +138,26 @@
       <bottom/>
       <diagonal/>
     </border>
+    <border>
+      <left style="thin">
+        <color theme="4"/>
+      </left>
+      <right style="thin">
+        <color theme="4"/>
+      </right>
+      <top style="thin">
+        <color theme="4"/>
+      </top>
+      <bottom style="thin">
+        <color theme="4"/>
+      </bottom>
+      <diagonal/>
+    </border>
   </borders>
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="26">
+  <cellXfs count="32">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="49" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyAlignment="1" applyProtection="1">
       <alignment horizontal="left" vertical="top"/>
@@ -208,6 +232,24 @@
       <alignment horizontal="right"/>
     </xf>
     <xf numFmtId="0" fontId="3" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="right"/>
+    </xf>
+    <xf numFmtId="164" fontId="4" fillId="2" borderId="2" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="right" vertical="top"/>
+    </xf>
+    <xf numFmtId="3" fontId="4" fillId="2" borderId="2" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="right"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="2" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="right"/>
+    </xf>
+    <xf numFmtId="164" fontId="3" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="right" vertical="top"/>
+    </xf>
+    <xf numFmtId="3" fontId="3" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="right"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="right"/>
     </xf>
   </cellXfs>
@@ -399,8 +441,8 @@
 </file>
 
 <file path=xl/tables/table1.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="1" xr:uid="{00000000-000C-0000-FFFF-FFFF00000000}" name="Tabela1" displayName="Tabela1" ref="A1:J75" totalsRowShown="0" headerRowDxfId="11" dataDxfId="10">
-  <autoFilter ref="A1:J75" xr:uid="{00000000-0009-0000-0100-000001000000}">
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="1" name="Tabela1" displayName="Tabela1" ref="A1:J107" totalsRowShown="0" headerRowDxfId="11" dataDxfId="10">
+  <autoFilter ref="A1:J107">
     <filterColumn colId="0" hiddenButton="1"/>
     <filterColumn colId="1" hiddenButton="1"/>
     <filterColumn colId="2" hiddenButton="1"/>
@@ -413,16 +455,16 @@
     <filterColumn colId="9" hiddenButton="1"/>
   </autoFilter>
   <tableColumns count="10">
-    <tableColumn id="1" xr3:uid="{00000000-0010-0000-0000-000001000000}" name="Date" dataDxfId="9"/>
-    <tableColumn id="2" xr3:uid="{00000000-0010-0000-0000-000002000000}" name="Tested (all)" dataDxfId="8"/>
-    <tableColumn id="3" xr3:uid="{00000000-0010-0000-0000-000003000000}" name="Tested (daily)" dataDxfId="7"/>
-    <tableColumn id="4" xr3:uid="{00000000-0010-0000-0000-000004000000}" name="Positive (all)" dataDxfId="6"/>
-    <tableColumn id="5" xr3:uid="{00000000-0010-0000-0000-000005000000}" name="Positive (daily)" dataDxfId="5"/>
-    <tableColumn id="6" xr3:uid="{00000000-0010-0000-0000-000006000000}" name="All hospitalized on certain day" dataDxfId="4"/>
-    <tableColumn id="7" xr3:uid="{00000000-0010-0000-0000-000007000000}" name="All persons in intensive care on certain day" dataDxfId="3"/>
-    <tableColumn id="10" xr3:uid="{00000000-0010-0000-0000-00000A000000}" name="Discharged" dataDxfId="2"/>
-    <tableColumn id="8" xr3:uid="{00000000-0010-0000-0000-000008000000}" name="Deaths (all)" dataDxfId="1"/>
-    <tableColumn id="9" xr3:uid="{00000000-0010-0000-0000-000009000000}" name="Deaths (daily)" dataDxfId="0"/>
+    <tableColumn id="1" name="Date" dataDxfId="9"/>
+    <tableColumn id="2" name="Tested (all)" dataDxfId="8"/>
+    <tableColumn id="3" name="Tested (daily)" dataDxfId="7"/>
+    <tableColumn id="4" name="Positive (all)" dataDxfId="6"/>
+    <tableColumn id="5" name="Positive (daily)" dataDxfId="5"/>
+    <tableColumn id="6" name="All hospitalized on certain day" dataDxfId="4"/>
+    <tableColumn id="7" name="All persons in intensive care on certain day" dataDxfId="3"/>
+    <tableColumn id="10" name="Discharged" dataDxfId="2"/>
+    <tableColumn id="8" name="Deaths (all)" dataDxfId="1"/>
+    <tableColumn id="9" name="Deaths (daily)" dataDxfId="0"/>
   </tableColumns>
   <tableStyleInfo name="TableStyleLight16" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
   <extLst>
@@ -695,11 +737,11 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:J75"/>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <dimension ref="A1:J107"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A40" zoomScale="89" zoomScaleNormal="89" workbookViewId="0">
-      <selection activeCell="J74" sqref="J74"/>
+    <sheetView tabSelected="1" topLeftCell="A23" zoomScale="89" zoomScaleNormal="89" workbookViewId="0">
+      <selection activeCell="G113" sqref="G113"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -3117,6 +3159,1030 @@
         <v>0</v>
       </c>
     </row>
+    <row r="76" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A76" s="20">
+        <v>43976</v>
+      </c>
+      <c r="B76" s="21">
+        <v>75770</v>
+      </c>
+      <c r="C76" s="22">
+        <v>754</v>
+      </c>
+      <c r="D76" s="22">
+        <v>1469</v>
+      </c>
+      <c r="E76" s="22">
+        <v>0</v>
+      </c>
+      <c r="F76" s="22">
+        <v>9</v>
+      </c>
+      <c r="G76" s="22">
+        <v>2</v>
+      </c>
+      <c r="H76" s="22">
+        <v>6</v>
+      </c>
+      <c r="I76" s="22">
+        <v>108</v>
+      </c>
+      <c r="J76" s="22">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="77" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A77" s="20">
+        <v>43977</v>
+      </c>
+      <c r="B77" s="21">
+        <v>76579</v>
+      </c>
+      <c r="C77" s="22">
+        <v>809</v>
+      </c>
+      <c r="D77" s="22">
+        <v>1471</v>
+      </c>
+      <c r="E77" s="22">
+        <v>2</v>
+      </c>
+      <c r="F77" s="22">
+        <v>8</v>
+      </c>
+      <c r="G77" s="22">
+        <v>2</v>
+      </c>
+      <c r="H77" s="22">
+        <v>2</v>
+      </c>
+      <c r="I77" s="22">
+        <v>108</v>
+      </c>
+      <c r="J77" s="22">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="78" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A78" s="20">
+        <v>43978</v>
+      </c>
+      <c r="B78" s="21">
+        <v>77210</v>
+      </c>
+      <c r="C78" s="22">
+        <v>631</v>
+      </c>
+      <c r="D78" s="22">
+        <v>1473</v>
+      </c>
+      <c r="E78" s="22">
+        <v>2</v>
+      </c>
+      <c r="F78" s="22">
+        <v>7</v>
+      </c>
+      <c r="G78" s="22">
+        <v>2</v>
+      </c>
+      <c r="H78" s="22">
+        <v>1</v>
+      </c>
+      <c r="I78" s="22">
+        <v>108</v>
+      </c>
+      <c r="J78" s="22">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="79" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A79" s="20">
+        <v>43979</v>
+      </c>
+      <c r="B79" s="21">
+        <v>77916</v>
+      </c>
+      <c r="C79" s="22">
+        <v>706</v>
+      </c>
+      <c r="D79" s="22">
+        <v>1473</v>
+      </c>
+      <c r="E79" s="22">
+        <v>0</v>
+      </c>
+      <c r="F79" s="22">
+        <v>7</v>
+      </c>
+      <c r="G79" s="22">
+        <v>2</v>
+      </c>
+      <c r="H79" s="22">
+        <v>0</v>
+      </c>
+      <c r="I79" s="22">
+        <v>108</v>
+      </c>
+      <c r="J79" s="22">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="80" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A80" s="20">
+        <v>43980</v>
+      </c>
+      <c r="B80" s="21">
+        <v>78529</v>
+      </c>
+      <c r="C80" s="22">
+        <v>613</v>
+      </c>
+      <c r="D80" s="22">
+        <v>1473</v>
+      </c>
+      <c r="E80" s="22">
+        <v>0</v>
+      </c>
+      <c r="F80" s="22">
+        <v>7</v>
+      </c>
+      <c r="G80" s="22">
+        <v>2</v>
+      </c>
+      <c r="H80" s="22">
+        <v>0</v>
+      </c>
+      <c r="I80" s="22">
+        <v>108</v>
+      </c>
+      <c r="J80" s="22">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="81" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A81" s="20">
+        <v>43981</v>
+      </c>
+      <c r="B81" s="22">
+        <v>78793</v>
+      </c>
+      <c r="C81" s="22">
+        <v>264</v>
+      </c>
+      <c r="D81" s="22">
+        <v>1473</v>
+      </c>
+      <c r="E81" s="22">
+        <v>0</v>
+      </c>
+      <c r="F81" s="22">
+        <v>6</v>
+      </c>
+      <c r="G81" s="22">
+        <v>2</v>
+      </c>
+      <c r="H81" s="22">
+        <v>1</v>
+      </c>
+      <c r="I81" s="22">
+        <v>108</v>
+      </c>
+      <c r="J81" s="22">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="82" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A82" s="20">
+        <v>43982</v>
+      </c>
+      <c r="B82" s="21">
+        <v>79039</v>
+      </c>
+      <c r="C82" s="22">
+        <v>246</v>
+      </c>
+      <c r="D82" s="22">
+        <v>1473</v>
+      </c>
+      <c r="E82" s="22">
+        <v>0</v>
+      </c>
+      <c r="F82" s="22">
+        <v>5</v>
+      </c>
+      <c r="G82" s="22">
+        <v>1</v>
+      </c>
+      <c r="H82" s="22">
+        <v>0</v>
+      </c>
+      <c r="I82" s="22">
+        <v>109</v>
+      </c>
+      <c r="J82" s="22">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="83" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A83" s="20">
+        <v>43983</v>
+      </c>
+      <c r="B83" s="21">
+        <v>79698</v>
+      </c>
+      <c r="C83" s="22">
+        <v>659</v>
+      </c>
+      <c r="D83" s="22">
+        <v>1475</v>
+      </c>
+      <c r="E83" s="22">
+        <v>2</v>
+      </c>
+      <c r="F83" s="22">
+        <v>5</v>
+      </c>
+      <c r="G83" s="22">
+        <v>1</v>
+      </c>
+      <c r="H83" s="22">
+        <v>0</v>
+      </c>
+      <c r="I83" s="22">
+        <v>109</v>
+      </c>
+      <c r="J83" s="22">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="84" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A84" s="20">
+        <v>43984</v>
+      </c>
+      <c r="B84" s="21">
+        <v>80505</v>
+      </c>
+      <c r="C84" s="22">
+        <v>807</v>
+      </c>
+      <c r="D84" s="22">
+        <v>1477</v>
+      </c>
+      <c r="E84" s="22">
+        <v>2</v>
+      </c>
+      <c r="F84" s="22">
+        <v>5</v>
+      </c>
+      <c r="G84" s="22">
+        <v>0</v>
+      </c>
+      <c r="H84" s="22">
+        <v>0</v>
+      </c>
+      <c r="I84" s="22">
+        <v>109</v>
+      </c>
+      <c r="J84" s="22">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="85" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A85" s="20">
+        <v>43985</v>
+      </c>
+      <c r="B85" s="21">
+        <v>81333</v>
+      </c>
+      <c r="C85" s="22">
+        <v>828</v>
+      </c>
+      <c r="D85" s="22">
+        <v>1477</v>
+      </c>
+      <c r="E85" s="22">
+        <v>0</v>
+      </c>
+      <c r="F85" s="22">
+        <v>5</v>
+      </c>
+      <c r="G85" s="22">
+        <v>0</v>
+      </c>
+      <c r="H85" s="22">
+        <v>0</v>
+      </c>
+      <c r="I85" s="22">
+        <v>109</v>
+      </c>
+      <c r="J85" s="22">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="86" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A86" s="26">
+        <v>43986</v>
+      </c>
+      <c r="B86" s="27">
+        <v>82161</v>
+      </c>
+      <c r="C86" s="28">
+        <v>828</v>
+      </c>
+      <c r="D86" s="28">
+        <v>1479</v>
+      </c>
+      <c r="E86" s="28">
+        <v>2</v>
+      </c>
+      <c r="F86" s="28">
+        <v>6</v>
+      </c>
+      <c r="G86" s="28">
+        <v>0</v>
+      </c>
+      <c r="H86" s="28">
+        <v>0</v>
+      </c>
+      <c r="I86" s="28">
+        <v>109</v>
+      </c>
+      <c r="J86" s="28">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="87" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A87" s="29">
+        <v>43987</v>
+      </c>
+      <c r="B87" s="30">
+        <v>82876</v>
+      </c>
+      <c r="C87" s="31">
+        <v>715</v>
+      </c>
+      <c r="D87" s="31">
+        <v>1484</v>
+      </c>
+      <c r="E87" s="31">
+        <v>5</v>
+      </c>
+      <c r="F87" s="31">
+        <v>6</v>
+      </c>
+      <c r="G87" s="31">
+        <v>0</v>
+      </c>
+      <c r="H87" s="31">
+        <v>0</v>
+      </c>
+      <c r="I87" s="31">
+        <v>109</v>
+      </c>
+      <c r="J87" s="31">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="88" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A88" s="23">
+        <v>43988</v>
+      </c>
+      <c r="B88" s="24">
+        <v>83105</v>
+      </c>
+      <c r="C88" s="25">
+        <v>229</v>
+      </c>
+      <c r="D88" s="25">
+        <v>1485</v>
+      </c>
+      <c r="E88" s="25">
+        <v>1</v>
+      </c>
+      <c r="F88" s="25">
+        <v>5</v>
+      </c>
+      <c r="G88" s="25">
+        <v>0</v>
+      </c>
+      <c r="H88" s="25">
+        <v>1</v>
+      </c>
+      <c r="I88" s="25">
+        <v>109</v>
+      </c>
+      <c r="J88" s="25">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="89" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A89" s="29">
+        <v>43989</v>
+      </c>
+      <c r="B89" s="30">
+        <v>83316</v>
+      </c>
+      <c r="C89" s="31">
+        <v>211</v>
+      </c>
+      <c r="D89" s="31">
+        <v>1485</v>
+      </c>
+      <c r="E89" s="31">
+        <v>0</v>
+      </c>
+      <c r="F89" s="31">
+        <v>5</v>
+      </c>
+      <c r="G89" s="31">
+        <v>0</v>
+      </c>
+      <c r="H89" s="31">
+        <v>0</v>
+      </c>
+      <c r="I89" s="31">
+        <v>109</v>
+      </c>
+      <c r="J89" s="31">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="90" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A90" s="20">
+        <v>43990</v>
+      </c>
+      <c r="B90" s="21">
+        <v>84130</v>
+      </c>
+      <c r="C90" s="22">
+        <v>814</v>
+      </c>
+      <c r="D90" s="22">
+        <v>1486</v>
+      </c>
+      <c r="E90" s="22">
+        <v>1</v>
+      </c>
+      <c r="F90" s="22">
+        <v>6</v>
+      </c>
+      <c r="G90" s="22">
+        <v>0</v>
+      </c>
+      <c r="H90" s="22">
+        <v>0</v>
+      </c>
+      <c r="I90" s="22">
+        <v>109</v>
+      </c>
+      <c r="J90" s="22">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="91" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A91" s="20">
+        <v>43991</v>
+      </c>
+      <c r="B91" s="21">
+        <v>84868</v>
+      </c>
+      <c r="C91" s="22">
+        <v>738</v>
+      </c>
+      <c r="D91" s="22">
+        <v>1488</v>
+      </c>
+      <c r="E91" s="22">
+        <v>2</v>
+      </c>
+      <c r="F91" s="22">
+        <v>6</v>
+      </c>
+      <c r="G91" s="22">
+        <v>0</v>
+      </c>
+      <c r="H91" s="22">
+        <v>0</v>
+      </c>
+      <c r="I91" s="22">
+        <v>109</v>
+      </c>
+      <c r="J91" s="22">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="92" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A92" s="23">
+        <v>43992</v>
+      </c>
+      <c r="B92" s="24">
+        <v>85626</v>
+      </c>
+      <c r="C92" s="25">
+        <v>758</v>
+      </c>
+      <c r="D92" s="25">
+        <v>1488</v>
+      </c>
+      <c r="E92" s="25">
+        <v>0</v>
+      </c>
+      <c r="F92" s="25">
+        <v>6</v>
+      </c>
+      <c r="G92" s="25">
+        <v>0</v>
+      </c>
+      <c r="H92" s="25">
+        <v>0</v>
+      </c>
+      <c r="I92" s="25">
+        <v>109</v>
+      </c>
+      <c r="J92" s="25">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="93" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A93" s="29">
+        <v>43993</v>
+      </c>
+      <c r="B93" s="30">
+        <v>86328</v>
+      </c>
+      <c r="C93" s="31">
+        <v>702</v>
+      </c>
+      <c r="D93" s="31">
+        <v>1490</v>
+      </c>
+      <c r="E93" s="31">
+        <v>2</v>
+      </c>
+      <c r="F93" s="31">
+        <v>6</v>
+      </c>
+      <c r="G93" s="31">
+        <v>0</v>
+      </c>
+      <c r="H93" s="31">
+        <v>0</v>
+      </c>
+      <c r="I93" s="31">
+        <v>109</v>
+      </c>
+      <c r="J93" s="31">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="94" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A94" s="23">
+        <v>43994</v>
+      </c>
+      <c r="B94" s="24">
+        <v>87095</v>
+      </c>
+      <c r="C94" s="25">
+        <v>767</v>
+      </c>
+      <c r="D94" s="25">
+        <v>1492</v>
+      </c>
+      <c r="E94" s="25">
+        <v>2</v>
+      </c>
+      <c r="F94" s="25">
+        <v>6</v>
+      </c>
+      <c r="G94" s="25">
+        <v>0</v>
+      </c>
+      <c r="H94" s="25">
+        <v>0</v>
+      </c>
+      <c r="I94" s="25">
+        <v>109</v>
+      </c>
+      <c r="J94" s="25">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="95" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A95" s="29">
+        <v>43995</v>
+      </c>
+      <c r="B95" s="30">
+        <v>87386</v>
+      </c>
+      <c r="C95" s="31">
+        <v>291</v>
+      </c>
+      <c r="D95" s="31">
+        <v>1495</v>
+      </c>
+      <c r="E95" s="31">
+        <v>3</v>
+      </c>
+      <c r="F95" s="31">
+        <v>6</v>
+      </c>
+      <c r="G95" s="31">
+        <v>0</v>
+      </c>
+      <c r="H95" s="31">
+        <v>0</v>
+      </c>
+      <c r="I95" s="31">
+        <v>109</v>
+      </c>
+      <c r="J95" s="31">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="96" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A96" s="23">
+        <v>43996</v>
+      </c>
+      <c r="B96" s="24">
+        <v>87598</v>
+      </c>
+      <c r="C96" s="25">
+        <v>212</v>
+      </c>
+      <c r="D96" s="25">
+        <v>1496</v>
+      </c>
+      <c r="E96" s="25">
+        <v>1</v>
+      </c>
+      <c r="F96" s="25">
+        <v>7</v>
+      </c>
+      <c r="G96" s="25">
+        <v>1</v>
+      </c>
+      <c r="H96" s="25">
+        <v>0</v>
+      </c>
+      <c r="I96" s="25">
+        <v>109</v>
+      </c>
+      <c r="J96" s="25">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="97" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A97" s="20">
+        <v>43997</v>
+      </c>
+      <c r="B97" s="21">
+        <v>88165</v>
+      </c>
+      <c r="C97" s="22">
+        <v>567</v>
+      </c>
+      <c r="D97" s="22">
+        <v>1499</v>
+      </c>
+      <c r="E97" s="22">
+        <v>3</v>
+      </c>
+      <c r="F97" s="22">
+        <v>7</v>
+      </c>
+      <c r="G97" s="22">
+        <v>1</v>
+      </c>
+      <c r="H97" s="22">
+        <v>0</v>
+      </c>
+      <c r="I97" s="22">
+        <v>109</v>
+      </c>
+      <c r="J97" s="22">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="98" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A98" s="20">
+        <v>43998</v>
+      </c>
+      <c r="B98" s="21">
+        <v>89151</v>
+      </c>
+      <c r="C98" s="22">
+        <v>986</v>
+      </c>
+      <c r="D98" s="22">
+        <v>1503</v>
+      </c>
+      <c r="E98" s="22">
+        <v>4</v>
+      </c>
+      <c r="F98" s="22">
+        <v>7</v>
+      </c>
+      <c r="G98" s="22">
+        <v>1</v>
+      </c>
+      <c r="H98" s="22">
+        <v>0</v>
+      </c>
+      <c r="I98" s="22">
+        <v>109</v>
+      </c>
+      <c r="J98" s="22">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="99" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A99" s="29">
+        <v>43999</v>
+      </c>
+      <c r="B99" s="30">
+        <v>90103</v>
+      </c>
+      <c r="C99" s="31">
+        <v>952</v>
+      </c>
+      <c r="D99" s="31">
+        <v>1511</v>
+      </c>
+      <c r="E99" s="31">
+        <v>8</v>
+      </c>
+      <c r="F99" s="31">
+        <v>6</v>
+      </c>
+      <c r="G99" s="31">
+        <v>1</v>
+      </c>
+      <c r="H99" s="31">
+        <v>1</v>
+      </c>
+      <c r="I99" s="31">
+        <v>109</v>
+      </c>
+      <c r="J99" s="31">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="100" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A100" s="20">
+        <v>44000</v>
+      </c>
+      <c r="B100" s="21">
+        <v>91005</v>
+      </c>
+      <c r="C100" s="22">
+        <v>902</v>
+      </c>
+      <c r="D100" s="22">
+        <v>1513</v>
+      </c>
+      <c r="E100" s="22">
+        <v>2</v>
+      </c>
+      <c r="F100" s="22">
+        <v>8</v>
+      </c>
+      <c r="G100" s="22">
+        <v>1</v>
+      </c>
+      <c r="H100" s="22">
+        <v>0</v>
+      </c>
+      <c r="I100" s="22">
+        <v>109</v>
+      </c>
+      <c r="J100" s="22">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="101" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A101" s="29">
+        <v>44001</v>
+      </c>
+      <c r="B101" s="30">
+        <v>92152</v>
+      </c>
+      <c r="C101" s="31">
+        <v>1147</v>
+      </c>
+      <c r="D101" s="31">
+        <v>1519</v>
+      </c>
+      <c r="E101" s="31">
+        <v>6</v>
+      </c>
+      <c r="F101" s="31">
+        <v>6</v>
+      </c>
+      <c r="G101" s="31">
+        <v>1</v>
+      </c>
+      <c r="H101" s="31">
+        <v>2</v>
+      </c>
+      <c r="I101" s="31">
+        <v>109</v>
+      </c>
+      <c r="J101" s="31">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="102" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A102" s="23">
+        <v>44002</v>
+      </c>
+      <c r="B102" s="24">
+        <v>92919</v>
+      </c>
+      <c r="C102" s="25">
+        <v>758</v>
+      </c>
+      <c r="D102" s="25">
+        <v>1520</v>
+      </c>
+      <c r="E102" s="25">
+        <v>1</v>
+      </c>
+      <c r="F102" s="25">
+        <v>6</v>
+      </c>
+      <c r="G102" s="25">
+        <v>1</v>
+      </c>
+      <c r="H102" s="25">
+        <v>2</v>
+      </c>
+      <c r="I102" s="25">
+        <v>109</v>
+      </c>
+      <c r="J102" s="25">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="103" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A103" s="29">
+        <v>44003</v>
+      </c>
+      <c r="B103" s="30">
+        <v>93181</v>
+      </c>
+      <c r="C103" s="31">
+        <v>271</v>
+      </c>
+      <c r="D103" s="31">
+        <v>1521</v>
+      </c>
+      <c r="E103" s="31">
+        <v>1</v>
+      </c>
+      <c r="F103" s="31">
+        <v>6</v>
+      </c>
+      <c r="G103" s="31">
+        <v>1</v>
+      </c>
+      <c r="H103" s="31">
+        <v>0</v>
+      </c>
+      <c r="I103" s="31">
+        <v>109</v>
+      </c>
+      <c r="J103" s="31">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="104" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A104" s="29">
+        <v>44004</v>
+      </c>
+      <c r="B104" s="30">
+        <v>94165</v>
+      </c>
+      <c r="C104" s="31">
+        <v>984</v>
+      </c>
+      <c r="D104" s="31">
+        <v>1534</v>
+      </c>
+      <c r="E104" s="31">
+        <v>13</v>
+      </c>
+      <c r="F104" s="31">
+        <v>5</v>
+      </c>
+      <c r="G104" s="31">
+        <v>1</v>
+      </c>
+      <c r="H104" s="31">
+        <v>1</v>
+      </c>
+      <c r="I104" s="31">
+        <v>109</v>
+      </c>
+      <c r="J104" s="31">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="105" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A105" s="29">
+        <v>44005</v>
+      </c>
+      <c r="B105" s="30">
+        <v>95387</v>
+      </c>
+      <c r="C105" s="31">
+        <v>1222</v>
+      </c>
+      <c r="D105" s="31">
+        <v>1541</v>
+      </c>
+      <c r="E105" s="31">
+        <v>7</v>
+      </c>
+      <c r="F105" s="31">
+        <v>7</v>
+      </c>
+      <c r="G105" s="31">
+        <v>2</v>
+      </c>
+      <c r="H105" s="31">
+        <v>0</v>
+      </c>
+      <c r="I105" s="31" t="s">
+        <v>10</v>
+      </c>
+      <c r="J105" s="31">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="106" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A106" s="23">
+        <v>44006</v>
+      </c>
+      <c r="B106" s="24">
+        <v>96599</v>
+      </c>
+      <c r="C106" s="25">
+        <v>1212</v>
+      </c>
+      <c r="D106" s="25">
+        <v>1547</v>
+      </c>
+      <c r="E106" s="25">
+        <v>6</v>
+      </c>
+      <c r="F106" s="25">
+        <v>7</v>
+      </c>
+      <c r="G106" s="25">
+        <v>2</v>
+      </c>
+      <c r="H106" s="25">
+        <v>0</v>
+      </c>
+      <c r="I106" s="25" t="s">
+        <v>10</v>
+      </c>
+      <c r="J106" s="25">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="107" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A107" s="29">
+        <v>44007</v>
+      </c>
+      <c r="B107" s="30">
+        <v>97442</v>
+      </c>
+      <c r="C107" s="31">
+        <v>843</v>
+      </c>
+      <c r="D107" s="31">
+        <v>1558</v>
+      </c>
+      <c r="E107" s="31">
+        <v>11</v>
+      </c>
+      <c r="F107" s="31">
+        <v>8</v>
+      </c>
+      <c r="G107" s="31">
+        <v>2</v>
+      </c>
+      <c r="H107" s="31">
+        <v>0</v>
+      </c>
+      <c r="I107" s="31" t="s">
+        <v>10</v>
+      </c>
+      <c r="J107" s="31">
+        <v>0</v>
+      </c>
+    </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>

</xml_diff>

<commit_message>
Data updated by GitHub Bot (2020-06-26 20)
</commit_message>
<xml_diff>
--- a/output/snapshot/fdcf2531-4c3e-5c02-b63c-ee160ead6dea.xlsx
+++ b/output/snapshot/fdcf2531-4c3e-5c02-b63c-ee160ead6dea.xlsx
@@ -1,16 +1,15 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="21929"/>
-  <workbookPr/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
+  <fileVersion appName="xl" lastEdited="6" lowestEdited="6" rupBuild="14420"/>
+  <workbookPr defaultThemeVersion="164011"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="I:\AKTUALNI PODATKI - KORONA\Za objavo na GOV.SI\ang\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{1E6DD62F-2BE2-47DC-A7ED-9B57C1589256}" xr6:coauthVersionLast="44" xr6:coauthVersionMax="44" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840"/>
   </bookViews>
   <sheets>
     <sheet name="Covid-19 podatki" sheetId="1" r:id="rId1"/>
@@ -25,7 +24,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="10" uniqueCount="10">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="13" uniqueCount="11">
   <si>
     <t>Date</t>
   </si>
@@ -56,15 +55,18 @@
   <si>
     <t>Deaths (daily)</t>
   </si>
+  <si>
+    <t>111*</t>
+  </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" mc:Ignorable="x14ac x16r2">
   <numFmts count="1">
     <numFmt numFmtId="164" formatCode="d/\ m/\ yyyy;@"/>
   </numFmts>
-  <fonts count="4" x14ac:knownFonts="1">
+  <fonts count="5" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -93,6 +95,13 @@
       <name val="Calibri Light"/>
       <scheme val="major"/>
     </font>
+    <font>
+      <sz val="10"/>
+      <color theme="1"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
   </fonts>
   <fills count="3">
     <fill>
@@ -108,7 +117,7 @@
       </patternFill>
     </fill>
   </fills>
-  <borders count="2">
+  <borders count="3">
     <border>
       <left/>
       <right/>
@@ -129,11 +138,26 @@
       <bottom/>
       <diagonal/>
     </border>
+    <border>
+      <left style="thin">
+        <color theme="4"/>
+      </left>
+      <right style="thin">
+        <color theme="4"/>
+      </right>
+      <top style="thin">
+        <color theme="4"/>
+      </top>
+      <bottom style="thin">
+        <color theme="4"/>
+      </bottom>
+      <diagonal/>
+    </border>
   </borders>
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="26">
+  <cellXfs count="32">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="49" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyAlignment="1" applyProtection="1">
       <alignment horizontal="left" vertical="top"/>
@@ -208,6 +232,24 @@
       <alignment horizontal="right"/>
     </xf>
     <xf numFmtId="0" fontId="3" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="right"/>
+    </xf>
+    <xf numFmtId="164" fontId="4" fillId="2" borderId="2" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="right" vertical="top"/>
+    </xf>
+    <xf numFmtId="3" fontId="4" fillId="2" borderId="2" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="right"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="2" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="right"/>
+    </xf>
+    <xf numFmtId="164" fontId="3" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="right" vertical="top"/>
+    </xf>
+    <xf numFmtId="3" fontId="3" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="right"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="right"/>
     </xf>
   </cellXfs>
@@ -399,8 +441,8 @@
 </file>
 
 <file path=xl/tables/table1.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="1" xr:uid="{00000000-000C-0000-FFFF-FFFF00000000}" name="Tabela1" displayName="Tabela1" ref="A1:J75" totalsRowShown="0" headerRowDxfId="11" dataDxfId="10">
-  <autoFilter ref="A1:J75" xr:uid="{00000000-0009-0000-0100-000001000000}">
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="1" name="Tabela1" displayName="Tabela1" ref="A1:J107" totalsRowShown="0" headerRowDxfId="11" dataDxfId="10">
+  <autoFilter ref="A1:J107">
     <filterColumn colId="0" hiddenButton="1"/>
     <filterColumn colId="1" hiddenButton="1"/>
     <filterColumn colId="2" hiddenButton="1"/>
@@ -413,16 +455,16 @@
     <filterColumn colId="9" hiddenButton="1"/>
   </autoFilter>
   <tableColumns count="10">
-    <tableColumn id="1" xr3:uid="{00000000-0010-0000-0000-000001000000}" name="Date" dataDxfId="9"/>
-    <tableColumn id="2" xr3:uid="{00000000-0010-0000-0000-000002000000}" name="Tested (all)" dataDxfId="8"/>
-    <tableColumn id="3" xr3:uid="{00000000-0010-0000-0000-000003000000}" name="Tested (daily)" dataDxfId="7"/>
-    <tableColumn id="4" xr3:uid="{00000000-0010-0000-0000-000004000000}" name="Positive (all)" dataDxfId="6"/>
-    <tableColumn id="5" xr3:uid="{00000000-0010-0000-0000-000005000000}" name="Positive (daily)" dataDxfId="5"/>
-    <tableColumn id="6" xr3:uid="{00000000-0010-0000-0000-000006000000}" name="All hospitalized on certain day" dataDxfId="4"/>
-    <tableColumn id="7" xr3:uid="{00000000-0010-0000-0000-000007000000}" name="All persons in intensive care on certain day" dataDxfId="3"/>
-    <tableColumn id="10" xr3:uid="{00000000-0010-0000-0000-00000A000000}" name="Discharged" dataDxfId="2"/>
-    <tableColumn id="8" xr3:uid="{00000000-0010-0000-0000-000008000000}" name="Deaths (all)" dataDxfId="1"/>
-    <tableColumn id="9" xr3:uid="{00000000-0010-0000-0000-000009000000}" name="Deaths (daily)" dataDxfId="0"/>
+    <tableColumn id="1" name="Date" dataDxfId="9"/>
+    <tableColumn id="2" name="Tested (all)" dataDxfId="8"/>
+    <tableColumn id="3" name="Tested (daily)" dataDxfId="7"/>
+    <tableColumn id="4" name="Positive (all)" dataDxfId="6"/>
+    <tableColumn id="5" name="Positive (daily)" dataDxfId="5"/>
+    <tableColumn id="6" name="All hospitalized on certain day" dataDxfId="4"/>
+    <tableColumn id="7" name="All persons in intensive care on certain day" dataDxfId="3"/>
+    <tableColumn id="10" name="Discharged" dataDxfId="2"/>
+    <tableColumn id="8" name="Deaths (all)" dataDxfId="1"/>
+    <tableColumn id="9" name="Deaths (daily)" dataDxfId="0"/>
   </tableColumns>
   <tableStyleInfo name="TableStyleLight16" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
   <extLst>
@@ -695,11 +737,11 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:J75"/>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <dimension ref="A1:J107"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A40" zoomScale="89" zoomScaleNormal="89" workbookViewId="0">
-      <selection activeCell="J74" sqref="J74"/>
+    <sheetView tabSelected="1" topLeftCell="A23" zoomScale="89" zoomScaleNormal="89" workbookViewId="0">
+      <selection activeCell="G113" sqref="G113"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -3117,6 +3159,1030 @@
         <v>0</v>
       </c>
     </row>
+    <row r="76" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A76" s="20">
+        <v>43976</v>
+      </c>
+      <c r="B76" s="21">
+        <v>75770</v>
+      </c>
+      <c r="C76" s="22">
+        <v>754</v>
+      </c>
+      <c r="D76" s="22">
+        <v>1469</v>
+      </c>
+      <c r="E76" s="22">
+        <v>0</v>
+      </c>
+      <c r="F76" s="22">
+        <v>9</v>
+      </c>
+      <c r="G76" s="22">
+        <v>2</v>
+      </c>
+      <c r="H76" s="22">
+        <v>6</v>
+      </c>
+      <c r="I76" s="22">
+        <v>108</v>
+      </c>
+      <c r="J76" s="22">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="77" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A77" s="20">
+        <v>43977</v>
+      </c>
+      <c r="B77" s="21">
+        <v>76579</v>
+      </c>
+      <c r="C77" s="22">
+        <v>809</v>
+      </c>
+      <c r="D77" s="22">
+        <v>1471</v>
+      </c>
+      <c r="E77" s="22">
+        <v>2</v>
+      </c>
+      <c r="F77" s="22">
+        <v>8</v>
+      </c>
+      <c r="G77" s="22">
+        <v>2</v>
+      </c>
+      <c r="H77" s="22">
+        <v>2</v>
+      </c>
+      <c r="I77" s="22">
+        <v>108</v>
+      </c>
+      <c r="J77" s="22">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="78" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A78" s="20">
+        <v>43978</v>
+      </c>
+      <c r="B78" s="21">
+        <v>77210</v>
+      </c>
+      <c r="C78" s="22">
+        <v>631</v>
+      </c>
+      <c r="D78" s="22">
+        <v>1473</v>
+      </c>
+      <c r="E78" s="22">
+        <v>2</v>
+      </c>
+      <c r="F78" s="22">
+        <v>7</v>
+      </c>
+      <c r="G78" s="22">
+        <v>2</v>
+      </c>
+      <c r="H78" s="22">
+        <v>1</v>
+      </c>
+      <c r="I78" s="22">
+        <v>108</v>
+      </c>
+      <c r="J78" s="22">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="79" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A79" s="20">
+        <v>43979</v>
+      </c>
+      <c r="B79" s="21">
+        <v>77916</v>
+      </c>
+      <c r="C79" s="22">
+        <v>706</v>
+      </c>
+      <c r="D79" s="22">
+        <v>1473</v>
+      </c>
+      <c r="E79" s="22">
+        <v>0</v>
+      </c>
+      <c r="F79" s="22">
+        <v>7</v>
+      </c>
+      <c r="G79" s="22">
+        <v>2</v>
+      </c>
+      <c r="H79" s="22">
+        <v>0</v>
+      </c>
+      <c r="I79" s="22">
+        <v>108</v>
+      </c>
+      <c r="J79" s="22">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="80" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A80" s="20">
+        <v>43980</v>
+      </c>
+      <c r="B80" s="21">
+        <v>78529</v>
+      </c>
+      <c r="C80" s="22">
+        <v>613</v>
+      </c>
+      <c r="D80" s="22">
+        <v>1473</v>
+      </c>
+      <c r="E80" s="22">
+        <v>0</v>
+      </c>
+      <c r="F80" s="22">
+        <v>7</v>
+      </c>
+      <c r="G80" s="22">
+        <v>2</v>
+      </c>
+      <c r="H80" s="22">
+        <v>0</v>
+      </c>
+      <c r="I80" s="22">
+        <v>108</v>
+      </c>
+      <c r="J80" s="22">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="81" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A81" s="20">
+        <v>43981</v>
+      </c>
+      <c r="B81" s="22">
+        <v>78793</v>
+      </c>
+      <c r="C81" s="22">
+        <v>264</v>
+      </c>
+      <c r="D81" s="22">
+        <v>1473</v>
+      </c>
+      <c r="E81" s="22">
+        <v>0</v>
+      </c>
+      <c r="F81" s="22">
+        <v>6</v>
+      </c>
+      <c r="G81" s="22">
+        <v>2</v>
+      </c>
+      <c r="H81" s="22">
+        <v>1</v>
+      </c>
+      <c r="I81" s="22">
+        <v>108</v>
+      </c>
+      <c r="J81" s="22">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="82" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A82" s="20">
+        <v>43982</v>
+      </c>
+      <c r="B82" s="21">
+        <v>79039</v>
+      </c>
+      <c r="C82" s="22">
+        <v>246</v>
+      </c>
+      <c r="D82" s="22">
+        <v>1473</v>
+      </c>
+      <c r="E82" s="22">
+        <v>0</v>
+      </c>
+      <c r="F82" s="22">
+        <v>5</v>
+      </c>
+      <c r="G82" s="22">
+        <v>1</v>
+      </c>
+      <c r="H82" s="22">
+        <v>0</v>
+      </c>
+      <c r="I82" s="22">
+        <v>109</v>
+      </c>
+      <c r="J82" s="22">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="83" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A83" s="20">
+        <v>43983</v>
+      </c>
+      <c r="B83" s="21">
+        <v>79698</v>
+      </c>
+      <c r="C83" s="22">
+        <v>659</v>
+      </c>
+      <c r="D83" s="22">
+        <v>1475</v>
+      </c>
+      <c r="E83" s="22">
+        <v>2</v>
+      </c>
+      <c r="F83" s="22">
+        <v>5</v>
+      </c>
+      <c r="G83" s="22">
+        <v>1</v>
+      </c>
+      <c r="H83" s="22">
+        <v>0</v>
+      </c>
+      <c r="I83" s="22">
+        <v>109</v>
+      </c>
+      <c r="J83" s="22">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="84" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A84" s="20">
+        <v>43984</v>
+      </c>
+      <c r="B84" s="21">
+        <v>80505</v>
+      </c>
+      <c r="C84" s="22">
+        <v>807</v>
+      </c>
+      <c r="D84" s="22">
+        <v>1477</v>
+      </c>
+      <c r="E84" s="22">
+        <v>2</v>
+      </c>
+      <c r="F84" s="22">
+        <v>5</v>
+      </c>
+      <c r="G84" s="22">
+        <v>0</v>
+      </c>
+      <c r="H84" s="22">
+        <v>0</v>
+      </c>
+      <c r="I84" s="22">
+        <v>109</v>
+      </c>
+      <c r="J84" s="22">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="85" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A85" s="20">
+        <v>43985</v>
+      </c>
+      <c r="B85" s="21">
+        <v>81333</v>
+      </c>
+      <c r="C85" s="22">
+        <v>828</v>
+      </c>
+      <c r="D85" s="22">
+        <v>1477</v>
+      </c>
+      <c r="E85" s="22">
+        <v>0</v>
+      </c>
+      <c r="F85" s="22">
+        <v>5</v>
+      </c>
+      <c r="G85" s="22">
+        <v>0</v>
+      </c>
+      <c r="H85" s="22">
+        <v>0</v>
+      </c>
+      <c r="I85" s="22">
+        <v>109</v>
+      </c>
+      <c r="J85" s="22">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="86" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A86" s="26">
+        <v>43986</v>
+      </c>
+      <c r="B86" s="27">
+        <v>82161</v>
+      </c>
+      <c r="C86" s="28">
+        <v>828</v>
+      </c>
+      <c r="D86" s="28">
+        <v>1479</v>
+      </c>
+      <c r="E86" s="28">
+        <v>2</v>
+      </c>
+      <c r="F86" s="28">
+        <v>6</v>
+      </c>
+      <c r="G86" s="28">
+        <v>0</v>
+      </c>
+      <c r="H86" s="28">
+        <v>0</v>
+      </c>
+      <c r="I86" s="28">
+        <v>109</v>
+      </c>
+      <c r="J86" s="28">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="87" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A87" s="29">
+        <v>43987</v>
+      </c>
+      <c r="B87" s="30">
+        <v>82876</v>
+      </c>
+      <c r="C87" s="31">
+        <v>715</v>
+      </c>
+      <c r="D87" s="31">
+        <v>1484</v>
+      </c>
+      <c r="E87" s="31">
+        <v>5</v>
+      </c>
+      <c r="F87" s="31">
+        <v>6</v>
+      </c>
+      <c r="G87" s="31">
+        <v>0</v>
+      </c>
+      <c r="H87" s="31">
+        <v>0</v>
+      </c>
+      <c r="I87" s="31">
+        <v>109</v>
+      </c>
+      <c r="J87" s="31">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="88" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A88" s="23">
+        <v>43988</v>
+      </c>
+      <c r="B88" s="24">
+        <v>83105</v>
+      </c>
+      <c r="C88" s="25">
+        <v>229</v>
+      </c>
+      <c r="D88" s="25">
+        <v>1485</v>
+      </c>
+      <c r="E88" s="25">
+        <v>1</v>
+      </c>
+      <c r="F88" s="25">
+        <v>5</v>
+      </c>
+      <c r="G88" s="25">
+        <v>0</v>
+      </c>
+      <c r="H88" s="25">
+        <v>1</v>
+      </c>
+      <c r="I88" s="25">
+        <v>109</v>
+      </c>
+      <c r="J88" s="25">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="89" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A89" s="29">
+        <v>43989</v>
+      </c>
+      <c r="B89" s="30">
+        <v>83316</v>
+      </c>
+      <c r="C89" s="31">
+        <v>211</v>
+      </c>
+      <c r="D89" s="31">
+        <v>1485</v>
+      </c>
+      <c r="E89" s="31">
+        <v>0</v>
+      </c>
+      <c r="F89" s="31">
+        <v>5</v>
+      </c>
+      <c r="G89" s="31">
+        <v>0</v>
+      </c>
+      <c r="H89" s="31">
+        <v>0</v>
+      </c>
+      <c r="I89" s="31">
+        <v>109</v>
+      </c>
+      <c r="J89" s="31">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="90" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A90" s="20">
+        <v>43990</v>
+      </c>
+      <c r="B90" s="21">
+        <v>84130</v>
+      </c>
+      <c r="C90" s="22">
+        <v>814</v>
+      </c>
+      <c r="D90" s="22">
+        <v>1486</v>
+      </c>
+      <c r="E90" s="22">
+        <v>1</v>
+      </c>
+      <c r="F90" s="22">
+        <v>6</v>
+      </c>
+      <c r="G90" s="22">
+        <v>0</v>
+      </c>
+      <c r="H90" s="22">
+        <v>0</v>
+      </c>
+      <c r="I90" s="22">
+        <v>109</v>
+      </c>
+      <c r="J90" s="22">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="91" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A91" s="20">
+        <v>43991</v>
+      </c>
+      <c r="B91" s="21">
+        <v>84868</v>
+      </c>
+      <c r="C91" s="22">
+        <v>738</v>
+      </c>
+      <c r="D91" s="22">
+        <v>1488</v>
+      </c>
+      <c r="E91" s="22">
+        <v>2</v>
+      </c>
+      <c r="F91" s="22">
+        <v>6</v>
+      </c>
+      <c r="G91" s="22">
+        <v>0</v>
+      </c>
+      <c r="H91" s="22">
+        <v>0</v>
+      </c>
+      <c r="I91" s="22">
+        <v>109</v>
+      </c>
+      <c r="J91" s="22">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="92" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A92" s="23">
+        <v>43992</v>
+      </c>
+      <c r="B92" s="24">
+        <v>85626</v>
+      </c>
+      <c r="C92" s="25">
+        <v>758</v>
+      </c>
+      <c r="D92" s="25">
+        <v>1488</v>
+      </c>
+      <c r="E92" s="25">
+        <v>0</v>
+      </c>
+      <c r="F92" s="25">
+        <v>6</v>
+      </c>
+      <c r="G92" s="25">
+        <v>0</v>
+      </c>
+      <c r="H92" s="25">
+        <v>0</v>
+      </c>
+      <c r="I92" s="25">
+        <v>109</v>
+      </c>
+      <c r="J92" s="25">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="93" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A93" s="29">
+        <v>43993</v>
+      </c>
+      <c r="B93" s="30">
+        <v>86328</v>
+      </c>
+      <c r="C93" s="31">
+        <v>702</v>
+      </c>
+      <c r="D93" s="31">
+        <v>1490</v>
+      </c>
+      <c r="E93" s="31">
+        <v>2</v>
+      </c>
+      <c r="F93" s="31">
+        <v>6</v>
+      </c>
+      <c r="G93" s="31">
+        <v>0</v>
+      </c>
+      <c r="H93" s="31">
+        <v>0</v>
+      </c>
+      <c r="I93" s="31">
+        <v>109</v>
+      </c>
+      <c r="J93" s="31">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="94" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A94" s="23">
+        <v>43994</v>
+      </c>
+      <c r="B94" s="24">
+        <v>87095</v>
+      </c>
+      <c r="C94" s="25">
+        <v>767</v>
+      </c>
+      <c r="D94" s="25">
+        <v>1492</v>
+      </c>
+      <c r="E94" s="25">
+        <v>2</v>
+      </c>
+      <c r="F94" s="25">
+        <v>6</v>
+      </c>
+      <c r="G94" s="25">
+        <v>0</v>
+      </c>
+      <c r="H94" s="25">
+        <v>0</v>
+      </c>
+      <c r="I94" s="25">
+        <v>109</v>
+      </c>
+      <c r="J94" s="25">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="95" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A95" s="29">
+        <v>43995</v>
+      </c>
+      <c r="B95" s="30">
+        <v>87386</v>
+      </c>
+      <c r="C95" s="31">
+        <v>291</v>
+      </c>
+      <c r="D95" s="31">
+        <v>1495</v>
+      </c>
+      <c r="E95" s="31">
+        <v>3</v>
+      </c>
+      <c r="F95" s="31">
+        <v>6</v>
+      </c>
+      <c r="G95" s="31">
+        <v>0</v>
+      </c>
+      <c r="H95" s="31">
+        <v>0</v>
+      </c>
+      <c r="I95" s="31">
+        <v>109</v>
+      </c>
+      <c r="J95" s="31">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="96" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A96" s="23">
+        <v>43996</v>
+      </c>
+      <c r="B96" s="24">
+        <v>87598</v>
+      </c>
+      <c r="C96" s="25">
+        <v>212</v>
+      </c>
+      <c r="D96" s="25">
+        <v>1496</v>
+      </c>
+      <c r="E96" s="25">
+        <v>1</v>
+      </c>
+      <c r="F96" s="25">
+        <v>7</v>
+      </c>
+      <c r="G96" s="25">
+        <v>1</v>
+      </c>
+      <c r="H96" s="25">
+        <v>0</v>
+      </c>
+      <c r="I96" s="25">
+        <v>109</v>
+      </c>
+      <c r="J96" s="25">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="97" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A97" s="20">
+        <v>43997</v>
+      </c>
+      <c r="B97" s="21">
+        <v>88165</v>
+      </c>
+      <c r="C97" s="22">
+        <v>567</v>
+      </c>
+      <c r="D97" s="22">
+        <v>1499</v>
+      </c>
+      <c r="E97" s="22">
+        <v>3</v>
+      </c>
+      <c r="F97" s="22">
+        <v>7</v>
+      </c>
+      <c r="G97" s="22">
+        <v>1</v>
+      </c>
+      <c r="H97" s="22">
+        <v>0</v>
+      </c>
+      <c r="I97" s="22">
+        <v>109</v>
+      </c>
+      <c r="J97" s="22">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="98" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A98" s="20">
+        <v>43998</v>
+      </c>
+      <c r="B98" s="21">
+        <v>89151</v>
+      </c>
+      <c r="C98" s="22">
+        <v>986</v>
+      </c>
+      <c r="D98" s="22">
+        <v>1503</v>
+      </c>
+      <c r="E98" s="22">
+        <v>4</v>
+      </c>
+      <c r="F98" s="22">
+        <v>7</v>
+      </c>
+      <c r="G98" s="22">
+        <v>1</v>
+      </c>
+      <c r="H98" s="22">
+        <v>0</v>
+      </c>
+      <c r="I98" s="22">
+        <v>109</v>
+      </c>
+      <c r="J98" s="22">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="99" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A99" s="29">
+        <v>43999</v>
+      </c>
+      <c r="B99" s="30">
+        <v>90103</v>
+      </c>
+      <c r="C99" s="31">
+        <v>952</v>
+      </c>
+      <c r="D99" s="31">
+        <v>1511</v>
+      </c>
+      <c r="E99" s="31">
+        <v>8</v>
+      </c>
+      <c r="F99" s="31">
+        <v>6</v>
+      </c>
+      <c r="G99" s="31">
+        <v>1</v>
+      </c>
+      <c r="H99" s="31">
+        <v>1</v>
+      </c>
+      <c r="I99" s="31">
+        <v>109</v>
+      </c>
+      <c r="J99" s="31">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="100" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A100" s="20">
+        <v>44000</v>
+      </c>
+      <c r="B100" s="21">
+        <v>91005</v>
+      </c>
+      <c r="C100" s="22">
+        <v>902</v>
+      </c>
+      <c r="D100" s="22">
+        <v>1513</v>
+      </c>
+      <c r="E100" s="22">
+        <v>2</v>
+      </c>
+      <c r="F100" s="22">
+        <v>8</v>
+      </c>
+      <c r="G100" s="22">
+        <v>1</v>
+      </c>
+      <c r="H100" s="22">
+        <v>0</v>
+      </c>
+      <c r="I100" s="22">
+        <v>109</v>
+      </c>
+      <c r="J100" s="22">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="101" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A101" s="29">
+        <v>44001</v>
+      </c>
+      <c r="B101" s="30">
+        <v>92152</v>
+      </c>
+      <c r="C101" s="31">
+        <v>1147</v>
+      </c>
+      <c r="D101" s="31">
+        <v>1519</v>
+      </c>
+      <c r="E101" s="31">
+        <v>6</v>
+      </c>
+      <c r="F101" s="31">
+        <v>6</v>
+      </c>
+      <c r="G101" s="31">
+        <v>1</v>
+      </c>
+      <c r="H101" s="31">
+        <v>2</v>
+      </c>
+      <c r="I101" s="31">
+        <v>109</v>
+      </c>
+      <c r="J101" s="31">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="102" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A102" s="23">
+        <v>44002</v>
+      </c>
+      <c r="B102" s="24">
+        <v>92919</v>
+      </c>
+      <c r="C102" s="25">
+        <v>758</v>
+      </c>
+      <c r="D102" s="25">
+        <v>1520</v>
+      </c>
+      <c r="E102" s="25">
+        <v>1</v>
+      </c>
+      <c r="F102" s="25">
+        <v>6</v>
+      </c>
+      <c r="G102" s="25">
+        <v>1</v>
+      </c>
+      <c r="H102" s="25">
+        <v>2</v>
+      </c>
+      <c r="I102" s="25">
+        <v>109</v>
+      </c>
+      <c r="J102" s="25">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="103" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A103" s="29">
+        <v>44003</v>
+      </c>
+      <c r="B103" s="30">
+        <v>93181</v>
+      </c>
+      <c r="C103" s="31">
+        <v>271</v>
+      </c>
+      <c r="D103" s="31">
+        <v>1521</v>
+      </c>
+      <c r="E103" s="31">
+        <v>1</v>
+      </c>
+      <c r="F103" s="31">
+        <v>6</v>
+      </c>
+      <c r="G103" s="31">
+        <v>1</v>
+      </c>
+      <c r="H103" s="31">
+        <v>0</v>
+      </c>
+      <c r="I103" s="31">
+        <v>109</v>
+      </c>
+      <c r="J103" s="31">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="104" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A104" s="29">
+        <v>44004</v>
+      </c>
+      <c r="B104" s="30">
+        <v>94165</v>
+      </c>
+      <c r="C104" s="31">
+        <v>984</v>
+      </c>
+      <c r="D104" s="31">
+        <v>1534</v>
+      </c>
+      <c r="E104" s="31">
+        <v>13</v>
+      </c>
+      <c r="F104" s="31">
+        <v>5</v>
+      </c>
+      <c r="G104" s="31">
+        <v>1</v>
+      </c>
+      <c r="H104" s="31">
+        <v>1</v>
+      </c>
+      <c r="I104" s="31">
+        <v>109</v>
+      </c>
+      <c r="J104" s="31">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="105" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A105" s="29">
+        <v>44005</v>
+      </c>
+      <c r="B105" s="30">
+        <v>95387</v>
+      </c>
+      <c r="C105" s="31">
+        <v>1222</v>
+      </c>
+      <c r="D105" s="31">
+        <v>1541</v>
+      </c>
+      <c r="E105" s="31">
+        <v>7</v>
+      </c>
+      <c r="F105" s="31">
+        <v>7</v>
+      </c>
+      <c r="G105" s="31">
+        <v>2</v>
+      </c>
+      <c r="H105" s="31">
+        <v>0</v>
+      </c>
+      <c r="I105" s="31" t="s">
+        <v>10</v>
+      </c>
+      <c r="J105" s="31">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="106" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A106" s="23">
+        <v>44006</v>
+      </c>
+      <c r="B106" s="24">
+        <v>96599</v>
+      </c>
+      <c r="C106" s="25">
+        <v>1212</v>
+      </c>
+      <c r="D106" s="25">
+        <v>1547</v>
+      </c>
+      <c r="E106" s="25">
+        <v>6</v>
+      </c>
+      <c r="F106" s="25">
+        <v>7</v>
+      </c>
+      <c r="G106" s="25">
+        <v>2</v>
+      </c>
+      <c r="H106" s="25">
+        <v>0</v>
+      </c>
+      <c r="I106" s="25" t="s">
+        <v>10</v>
+      </c>
+      <c r="J106" s="25">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="107" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A107" s="29">
+        <v>44007</v>
+      </c>
+      <c r="B107" s="30">
+        <v>97442</v>
+      </c>
+      <c r="C107" s="31">
+        <v>843</v>
+      </c>
+      <c r="D107" s="31">
+        <v>1558</v>
+      </c>
+      <c r="E107" s="31">
+        <v>11</v>
+      </c>
+      <c r="F107" s="31">
+        <v>8</v>
+      </c>
+      <c r="G107" s="31">
+        <v>2</v>
+      </c>
+      <c r="H107" s="31">
+        <v>0</v>
+      </c>
+      <c r="I107" s="31" t="s">
+        <v>10</v>
+      </c>
+      <c r="J107" s="31">
+        <v>0</v>
+      </c>
+    </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>

</xml_diff>

<commit_message>
Data updated by GitHub Bot (2020-06-27 12)
</commit_message>
<xml_diff>
--- a/output/snapshot/fdcf2531-4c3e-5c02-b63c-ee160ead6dea.xlsx
+++ b/output/snapshot/fdcf2531-4c3e-5c02-b63c-ee160ead6dea.xlsx
@@ -1,16 +1,15 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="21929"/>
-  <workbookPr/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
+  <fileVersion appName="xl" lastEdited="6" lowestEdited="6" rupBuild="14420"/>
+  <workbookPr defaultThemeVersion="164011"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="I:\AKTUALNI PODATKI - KORONA\Za objavo na GOV.SI\ang\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{1E6DD62F-2BE2-47DC-A7ED-9B57C1589256}" xr6:coauthVersionLast="44" xr6:coauthVersionMax="44" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840"/>
   </bookViews>
   <sheets>
     <sheet name="Covid-19 podatki" sheetId="1" r:id="rId1"/>
@@ -25,7 +24,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="10" uniqueCount="10">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="14" uniqueCount="11">
   <si>
     <t>Date</t>
   </si>
@@ -56,15 +55,18 @@
   <si>
     <t>Deaths (daily)</t>
   </si>
+  <si>
+    <t>111*</t>
+  </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" mc:Ignorable="x14ac x16r2">
   <numFmts count="1">
     <numFmt numFmtId="164" formatCode="d/\ m/\ yyyy;@"/>
   </numFmts>
-  <fonts count="4" x14ac:knownFonts="1">
+  <fonts count="5" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -93,6 +95,13 @@
       <name val="Calibri Light"/>
       <scheme val="major"/>
     </font>
+    <font>
+      <sz val="10"/>
+      <color theme="1"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
   </fonts>
   <fills count="3">
     <fill>
@@ -108,7 +117,7 @@
       </patternFill>
     </fill>
   </fills>
-  <borders count="2">
+  <borders count="3">
     <border>
       <left/>
       <right/>
@@ -129,11 +138,26 @@
       <bottom/>
       <diagonal/>
     </border>
+    <border>
+      <left style="thin">
+        <color theme="4"/>
+      </left>
+      <right style="thin">
+        <color theme="4"/>
+      </right>
+      <top style="thin">
+        <color theme="4"/>
+      </top>
+      <bottom style="thin">
+        <color theme="4"/>
+      </bottom>
+      <diagonal/>
+    </border>
   </borders>
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="26">
+  <cellXfs count="32">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="49" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyAlignment="1" applyProtection="1">
       <alignment horizontal="left" vertical="top"/>
@@ -208,6 +232,24 @@
       <alignment horizontal="right"/>
     </xf>
     <xf numFmtId="0" fontId="3" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="right"/>
+    </xf>
+    <xf numFmtId="164" fontId="4" fillId="2" borderId="2" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="right" vertical="top"/>
+    </xf>
+    <xf numFmtId="3" fontId="4" fillId="2" borderId="2" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="right"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="2" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="right"/>
+    </xf>
+    <xf numFmtId="164" fontId="3" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="right" vertical="top"/>
+    </xf>
+    <xf numFmtId="3" fontId="3" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="right"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="right"/>
     </xf>
   </cellXfs>
@@ -399,8 +441,8 @@
 </file>
 
 <file path=xl/tables/table1.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="1" xr:uid="{00000000-000C-0000-FFFF-FFFF00000000}" name="Tabela1" displayName="Tabela1" ref="A1:J75" totalsRowShown="0" headerRowDxfId="11" dataDxfId="10">
-  <autoFilter ref="A1:J75" xr:uid="{00000000-0009-0000-0100-000001000000}">
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="1" name="Tabela1" displayName="Tabela1" ref="A1:J108" totalsRowShown="0" headerRowDxfId="11" dataDxfId="10">
+  <autoFilter ref="A1:J108">
     <filterColumn colId="0" hiddenButton="1"/>
     <filterColumn colId="1" hiddenButton="1"/>
     <filterColumn colId="2" hiddenButton="1"/>
@@ -413,16 +455,16 @@
     <filterColumn colId="9" hiddenButton="1"/>
   </autoFilter>
   <tableColumns count="10">
-    <tableColumn id="1" xr3:uid="{00000000-0010-0000-0000-000001000000}" name="Date" dataDxfId="9"/>
-    <tableColumn id="2" xr3:uid="{00000000-0010-0000-0000-000002000000}" name="Tested (all)" dataDxfId="8"/>
-    <tableColumn id="3" xr3:uid="{00000000-0010-0000-0000-000003000000}" name="Tested (daily)" dataDxfId="7"/>
-    <tableColumn id="4" xr3:uid="{00000000-0010-0000-0000-000004000000}" name="Positive (all)" dataDxfId="6"/>
-    <tableColumn id="5" xr3:uid="{00000000-0010-0000-0000-000005000000}" name="Positive (daily)" dataDxfId="5"/>
-    <tableColumn id="6" xr3:uid="{00000000-0010-0000-0000-000006000000}" name="All hospitalized on certain day" dataDxfId="4"/>
-    <tableColumn id="7" xr3:uid="{00000000-0010-0000-0000-000007000000}" name="All persons in intensive care on certain day" dataDxfId="3"/>
-    <tableColumn id="10" xr3:uid="{00000000-0010-0000-0000-00000A000000}" name="Discharged" dataDxfId="2"/>
-    <tableColumn id="8" xr3:uid="{00000000-0010-0000-0000-000008000000}" name="Deaths (all)" dataDxfId="1"/>
-    <tableColumn id="9" xr3:uid="{00000000-0010-0000-0000-000009000000}" name="Deaths (daily)" dataDxfId="0"/>
+    <tableColumn id="1" name="Date" dataDxfId="9"/>
+    <tableColumn id="2" name="Tested (all)" dataDxfId="8"/>
+    <tableColumn id="3" name="Tested (daily)" dataDxfId="7"/>
+    <tableColumn id="4" name="Positive (all)" dataDxfId="6"/>
+    <tableColumn id="5" name="Positive (daily)" dataDxfId="5"/>
+    <tableColumn id="6" name="All hospitalized on certain day" dataDxfId="4"/>
+    <tableColumn id="7" name="All persons in intensive care on certain day" dataDxfId="3"/>
+    <tableColumn id="10" name="Discharged" dataDxfId="2"/>
+    <tableColumn id="8" name="Deaths (all)" dataDxfId="1"/>
+    <tableColumn id="9" name="Deaths (daily)" dataDxfId="0"/>
   </tableColumns>
   <tableStyleInfo name="TableStyleLight16" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
   <extLst>
@@ -695,11 +737,11 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:J75"/>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <dimension ref="A1:J108"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A40" zoomScale="89" zoomScaleNormal="89" workbookViewId="0">
-      <selection activeCell="J74" sqref="J74"/>
+    <sheetView tabSelected="1" topLeftCell="A83" zoomScale="89" zoomScaleNormal="89" workbookViewId="0">
+      <selection activeCell="J108" sqref="J108"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -3117,6 +3159,1062 @@
         <v>0</v>
       </c>
     </row>
+    <row r="76" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A76" s="20">
+        <v>43976</v>
+      </c>
+      <c r="B76" s="21">
+        <v>75770</v>
+      </c>
+      <c r="C76" s="22">
+        <v>754</v>
+      </c>
+      <c r="D76" s="22">
+        <v>1469</v>
+      </c>
+      <c r="E76" s="22">
+        <v>0</v>
+      </c>
+      <c r="F76" s="22">
+        <v>9</v>
+      </c>
+      <c r="G76" s="22">
+        <v>2</v>
+      </c>
+      <c r="H76" s="22">
+        <v>6</v>
+      </c>
+      <c r="I76" s="22">
+        <v>108</v>
+      </c>
+      <c r="J76" s="22">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="77" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A77" s="20">
+        <v>43977</v>
+      </c>
+      <c r="B77" s="21">
+        <v>76579</v>
+      </c>
+      <c r="C77" s="22">
+        <v>809</v>
+      </c>
+      <c r="D77" s="22">
+        <v>1471</v>
+      </c>
+      <c r="E77" s="22">
+        <v>2</v>
+      </c>
+      <c r="F77" s="22">
+        <v>8</v>
+      </c>
+      <c r="G77" s="22">
+        <v>2</v>
+      </c>
+      <c r="H77" s="22">
+        <v>2</v>
+      </c>
+      <c r="I77" s="22">
+        <v>108</v>
+      </c>
+      <c r="J77" s="22">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="78" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A78" s="20">
+        <v>43978</v>
+      </c>
+      <c r="B78" s="21">
+        <v>77210</v>
+      </c>
+      <c r="C78" s="22">
+        <v>631</v>
+      </c>
+      <c r="D78" s="22">
+        <v>1473</v>
+      </c>
+      <c r="E78" s="22">
+        <v>2</v>
+      </c>
+      <c r="F78" s="22">
+        <v>7</v>
+      </c>
+      <c r="G78" s="22">
+        <v>2</v>
+      </c>
+      <c r="H78" s="22">
+        <v>1</v>
+      </c>
+      <c r="I78" s="22">
+        <v>108</v>
+      </c>
+      <c r="J78" s="22">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="79" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A79" s="20">
+        <v>43979</v>
+      </c>
+      <c r="B79" s="21">
+        <v>77916</v>
+      </c>
+      <c r="C79" s="22">
+        <v>706</v>
+      </c>
+      <c r="D79" s="22">
+        <v>1473</v>
+      </c>
+      <c r="E79" s="22">
+        <v>0</v>
+      </c>
+      <c r="F79" s="22">
+        <v>7</v>
+      </c>
+      <c r="G79" s="22">
+        <v>2</v>
+      </c>
+      <c r="H79" s="22">
+        <v>0</v>
+      </c>
+      <c r="I79" s="22">
+        <v>108</v>
+      </c>
+      <c r="J79" s="22">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="80" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A80" s="20">
+        <v>43980</v>
+      </c>
+      <c r="B80" s="21">
+        <v>78529</v>
+      </c>
+      <c r="C80" s="22">
+        <v>613</v>
+      </c>
+      <c r="D80" s="22">
+        <v>1473</v>
+      </c>
+      <c r="E80" s="22">
+        <v>0</v>
+      </c>
+      <c r="F80" s="22">
+        <v>7</v>
+      </c>
+      <c r="G80" s="22">
+        <v>2</v>
+      </c>
+      <c r="H80" s="22">
+        <v>0</v>
+      </c>
+      <c r="I80" s="22">
+        <v>108</v>
+      </c>
+      <c r="J80" s="22">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="81" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A81" s="20">
+        <v>43981</v>
+      </c>
+      <c r="B81" s="22">
+        <v>78793</v>
+      </c>
+      <c r="C81" s="22">
+        <v>264</v>
+      </c>
+      <c r="D81" s="22">
+        <v>1473</v>
+      </c>
+      <c r="E81" s="22">
+        <v>0</v>
+      </c>
+      <c r="F81" s="22">
+        <v>6</v>
+      </c>
+      <c r="G81" s="22">
+        <v>2</v>
+      </c>
+      <c r="H81" s="22">
+        <v>1</v>
+      </c>
+      <c r="I81" s="22">
+        <v>108</v>
+      </c>
+      <c r="J81" s="22">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="82" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A82" s="20">
+        <v>43982</v>
+      </c>
+      <c r="B82" s="21">
+        <v>79039</v>
+      </c>
+      <c r="C82" s="22">
+        <v>246</v>
+      </c>
+      <c r="D82" s="22">
+        <v>1473</v>
+      </c>
+      <c r="E82" s="22">
+        <v>0</v>
+      </c>
+      <c r="F82" s="22">
+        <v>5</v>
+      </c>
+      <c r="G82" s="22">
+        <v>1</v>
+      </c>
+      <c r="H82" s="22">
+        <v>0</v>
+      </c>
+      <c r="I82" s="22">
+        <v>109</v>
+      </c>
+      <c r="J82" s="22">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="83" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A83" s="20">
+        <v>43983</v>
+      </c>
+      <c r="B83" s="21">
+        <v>79698</v>
+      </c>
+      <c r="C83" s="22">
+        <v>659</v>
+      </c>
+      <c r="D83" s="22">
+        <v>1475</v>
+      </c>
+      <c r="E83" s="22">
+        <v>2</v>
+      </c>
+      <c r="F83" s="22">
+        <v>5</v>
+      </c>
+      <c r="G83" s="22">
+        <v>1</v>
+      </c>
+      <c r="H83" s="22">
+        <v>0</v>
+      </c>
+      <c r="I83" s="22">
+        <v>109</v>
+      </c>
+      <c r="J83" s="22">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="84" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A84" s="20">
+        <v>43984</v>
+      </c>
+      <c r="B84" s="21">
+        <v>80505</v>
+      </c>
+      <c r="C84" s="22">
+        <v>807</v>
+      </c>
+      <c r="D84" s="22">
+        <v>1477</v>
+      </c>
+      <c r="E84" s="22">
+        <v>2</v>
+      </c>
+      <c r="F84" s="22">
+        <v>5</v>
+      </c>
+      <c r="G84" s="22">
+        <v>0</v>
+      </c>
+      <c r="H84" s="22">
+        <v>0</v>
+      </c>
+      <c r="I84" s="22">
+        <v>109</v>
+      </c>
+      <c r="J84" s="22">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="85" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A85" s="20">
+        <v>43985</v>
+      </c>
+      <c r="B85" s="21">
+        <v>81333</v>
+      </c>
+      <c r="C85" s="22">
+        <v>828</v>
+      </c>
+      <c r="D85" s="22">
+        <v>1477</v>
+      </c>
+      <c r="E85" s="22">
+        <v>0</v>
+      </c>
+      <c r="F85" s="22">
+        <v>5</v>
+      </c>
+      <c r="G85" s="22">
+        <v>0</v>
+      </c>
+      <c r="H85" s="22">
+        <v>0</v>
+      </c>
+      <c r="I85" s="22">
+        <v>109</v>
+      </c>
+      <c r="J85" s="22">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="86" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A86" s="26">
+        <v>43986</v>
+      </c>
+      <c r="B86" s="27">
+        <v>82161</v>
+      </c>
+      <c r="C86" s="28">
+        <v>828</v>
+      </c>
+      <c r="D86" s="28">
+        <v>1479</v>
+      </c>
+      <c r="E86" s="28">
+        <v>2</v>
+      </c>
+      <c r="F86" s="28">
+        <v>6</v>
+      </c>
+      <c r="G86" s="28">
+        <v>0</v>
+      </c>
+      <c r="H86" s="28">
+        <v>0</v>
+      </c>
+      <c r="I86" s="28">
+        <v>109</v>
+      </c>
+      <c r="J86" s="28">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="87" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A87" s="29">
+        <v>43987</v>
+      </c>
+      <c r="B87" s="30">
+        <v>82876</v>
+      </c>
+      <c r="C87" s="31">
+        <v>715</v>
+      </c>
+      <c r="D87" s="31">
+        <v>1484</v>
+      </c>
+      <c r="E87" s="31">
+        <v>5</v>
+      </c>
+      <c r="F87" s="31">
+        <v>6</v>
+      </c>
+      <c r="G87" s="31">
+        <v>0</v>
+      </c>
+      <c r="H87" s="31">
+        <v>0</v>
+      </c>
+      <c r="I87" s="31">
+        <v>109</v>
+      </c>
+      <c r="J87" s="31">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="88" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A88" s="23">
+        <v>43988</v>
+      </c>
+      <c r="B88" s="24">
+        <v>83105</v>
+      </c>
+      <c r="C88" s="25">
+        <v>229</v>
+      </c>
+      <c r="D88" s="25">
+        <v>1485</v>
+      </c>
+      <c r="E88" s="25">
+        <v>1</v>
+      </c>
+      <c r="F88" s="25">
+        <v>5</v>
+      </c>
+      <c r="G88" s="25">
+        <v>0</v>
+      </c>
+      <c r="H88" s="25">
+        <v>1</v>
+      </c>
+      <c r="I88" s="25">
+        <v>109</v>
+      </c>
+      <c r="J88" s="25">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="89" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A89" s="29">
+        <v>43989</v>
+      </c>
+      <c r="B89" s="30">
+        <v>83316</v>
+      </c>
+      <c r="C89" s="31">
+        <v>211</v>
+      </c>
+      <c r="D89" s="31">
+        <v>1485</v>
+      </c>
+      <c r="E89" s="31">
+        <v>0</v>
+      </c>
+      <c r="F89" s="31">
+        <v>5</v>
+      </c>
+      <c r="G89" s="31">
+        <v>0</v>
+      </c>
+      <c r="H89" s="31">
+        <v>0</v>
+      </c>
+      <c r="I89" s="31">
+        <v>109</v>
+      </c>
+      <c r="J89" s="31">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="90" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A90" s="20">
+        <v>43990</v>
+      </c>
+      <c r="B90" s="21">
+        <v>84130</v>
+      </c>
+      <c r="C90" s="22">
+        <v>814</v>
+      </c>
+      <c r="D90" s="22">
+        <v>1486</v>
+      </c>
+      <c r="E90" s="22">
+        <v>1</v>
+      </c>
+      <c r="F90" s="22">
+        <v>6</v>
+      </c>
+      <c r="G90" s="22">
+        <v>0</v>
+      </c>
+      <c r="H90" s="22">
+        <v>0</v>
+      </c>
+      <c r="I90" s="22">
+        <v>109</v>
+      </c>
+      <c r="J90" s="22">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="91" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A91" s="20">
+        <v>43991</v>
+      </c>
+      <c r="B91" s="21">
+        <v>84868</v>
+      </c>
+      <c r="C91" s="22">
+        <v>738</v>
+      </c>
+      <c r="D91" s="22">
+        <v>1488</v>
+      </c>
+      <c r="E91" s="22">
+        <v>2</v>
+      </c>
+      <c r="F91" s="22">
+        <v>6</v>
+      </c>
+      <c r="G91" s="22">
+        <v>0</v>
+      </c>
+      <c r="H91" s="22">
+        <v>0</v>
+      </c>
+      <c r="I91" s="22">
+        <v>109</v>
+      </c>
+      <c r="J91" s="22">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="92" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A92" s="23">
+        <v>43992</v>
+      </c>
+      <c r="B92" s="24">
+        <v>85626</v>
+      </c>
+      <c r="C92" s="25">
+        <v>758</v>
+      </c>
+      <c r="D92" s="25">
+        <v>1488</v>
+      </c>
+      <c r="E92" s="25">
+        <v>0</v>
+      </c>
+      <c r="F92" s="25">
+        <v>6</v>
+      </c>
+      <c r="G92" s="25">
+        <v>0</v>
+      </c>
+      <c r="H92" s="25">
+        <v>0</v>
+      </c>
+      <c r="I92" s="25">
+        <v>109</v>
+      </c>
+      <c r="J92" s="25">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="93" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A93" s="29">
+        <v>43993</v>
+      </c>
+      <c r="B93" s="30">
+        <v>86328</v>
+      </c>
+      <c r="C93" s="31">
+        <v>702</v>
+      </c>
+      <c r="D93" s="31">
+        <v>1490</v>
+      </c>
+      <c r="E93" s="31">
+        <v>2</v>
+      </c>
+      <c r="F93" s="31">
+        <v>6</v>
+      </c>
+      <c r="G93" s="31">
+        <v>0</v>
+      </c>
+      <c r="H93" s="31">
+        <v>0</v>
+      </c>
+      <c r="I93" s="31">
+        <v>109</v>
+      </c>
+      <c r="J93" s="31">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="94" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A94" s="23">
+        <v>43994</v>
+      </c>
+      <c r="B94" s="24">
+        <v>87095</v>
+      </c>
+      <c r="C94" s="25">
+        <v>767</v>
+      </c>
+      <c r="D94" s="25">
+        <v>1492</v>
+      </c>
+      <c r="E94" s="25">
+        <v>2</v>
+      </c>
+      <c r="F94" s="25">
+        <v>6</v>
+      </c>
+      <c r="G94" s="25">
+        <v>0</v>
+      </c>
+      <c r="H94" s="25">
+        <v>0</v>
+      </c>
+      <c r="I94" s="25">
+        <v>109</v>
+      </c>
+      <c r="J94" s="25">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="95" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A95" s="29">
+        <v>43995</v>
+      </c>
+      <c r="B95" s="30">
+        <v>87386</v>
+      </c>
+      <c r="C95" s="31">
+        <v>291</v>
+      </c>
+      <c r="D95" s="31">
+        <v>1495</v>
+      </c>
+      <c r="E95" s="31">
+        <v>3</v>
+      </c>
+      <c r="F95" s="31">
+        <v>6</v>
+      </c>
+      <c r="G95" s="31">
+        <v>0</v>
+      </c>
+      <c r="H95" s="31">
+        <v>0</v>
+      </c>
+      <c r="I95" s="31">
+        <v>109</v>
+      </c>
+      <c r="J95" s="31">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="96" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A96" s="23">
+        <v>43996</v>
+      </c>
+      <c r="B96" s="24">
+        <v>87598</v>
+      </c>
+      <c r="C96" s="25">
+        <v>212</v>
+      </c>
+      <c r="D96" s="25">
+        <v>1496</v>
+      </c>
+      <c r="E96" s="25">
+        <v>1</v>
+      </c>
+      <c r="F96" s="25">
+        <v>7</v>
+      </c>
+      <c r="G96" s="25">
+        <v>1</v>
+      </c>
+      <c r="H96" s="25">
+        <v>0</v>
+      </c>
+      <c r="I96" s="25">
+        <v>109</v>
+      </c>
+      <c r="J96" s="25">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="97" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A97" s="20">
+        <v>43997</v>
+      </c>
+      <c r="B97" s="21">
+        <v>88165</v>
+      </c>
+      <c r="C97" s="22">
+        <v>567</v>
+      </c>
+      <c r="D97" s="22">
+        <v>1499</v>
+      </c>
+      <c r="E97" s="22">
+        <v>3</v>
+      </c>
+      <c r="F97" s="22">
+        <v>7</v>
+      </c>
+      <c r="G97" s="22">
+        <v>1</v>
+      </c>
+      <c r="H97" s="22">
+        <v>0</v>
+      </c>
+      <c r="I97" s="22">
+        <v>109</v>
+      </c>
+      <c r="J97" s="22">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="98" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A98" s="20">
+        <v>43998</v>
+      </c>
+      <c r="B98" s="21">
+        <v>89151</v>
+      </c>
+      <c r="C98" s="22">
+        <v>986</v>
+      </c>
+      <c r="D98" s="22">
+        <v>1503</v>
+      </c>
+      <c r="E98" s="22">
+        <v>4</v>
+      </c>
+      <c r="F98" s="22">
+        <v>7</v>
+      </c>
+      <c r="G98" s="22">
+        <v>1</v>
+      </c>
+      <c r="H98" s="22">
+        <v>0</v>
+      </c>
+      <c r="I98" s="22">
+        <v>109</v>
+      </c>
+      <c r="J98" s="22">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="99" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A99" s="29">
+        <v>43999</v>
+      </c>
+      <c r="B99" s="30">
+        <v>90103</v>
+      </c>
+      <c r="C99" s="31">
+        <v>952</v>
+      </c>
+      <c r="D99" s="31">
+        <v>1511</v>
+      </c>
+      <c r="E99" s="31">
+        <v>8</v>
+      </c>
+      <c r="F99" s="31">
+        <v>6</v>
+      </c>
+      <c r="G99" s="31">
+        <v>1</v>
+      </c>
+      <c r="H99" s="31">
+        <v>1</v>
+      </c>
+      <c r="I99" s="31">
+        <v>109</v>
+      </c>
+      <c r="J99" s="31">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="100" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A100" s="20">
+        <v>44000</v>
+      </c>
+      <c r="B100" s="21">
+        <v>91005</v>
+      </c>
+      <c r="C100" s="22">
+        <v>902</v>
+      </c>
+      <c r="D100" s="22">
+        <v>1513</v>
+      </c>
+      <c r="E100" s="22">
+        <v>2</v>
+      </c>
+      <c r="F100" s="22">
+        <v>8</v>
+      </c>
+      <c r="G100" s="22">
+        <v>1</v>
+      </c>
+      <c r="H100" s="22">
+        <v>0</v>
+      </c>
+      <c r="I100" s="22">
+        <v>109</v>
+      </c>
+      <c r="J100" s="22">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="101" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A101" s="29">
+        <v>44001</v>
+      </c>
+      <c r="B101" s="30">
+        <v>92152</v>
+      </c>
+      <c r="C101" s="31">
+        <v>1147</v>
+      </c>
+      <c r="D101" s="31">
+        <v>1519</v>
+      </c>
+      <c r="E101" s="31">
+        <v>6</v>
+      </c>
+      <c r="F101" s="31">
+        <v>6</v>
+      </c>
+      <c r="G101" s="31">
+        <v>1</v>
+      </c>
+      <c r="H101" s="31">
+        <v>2</v>
+      </c>
+      <c r="I101" s="31">
+        <v>109</v>
+      </c>
+      <c r="J101" s="31">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="102" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A102" s="23">
+        <v>44002</v>
+      </c>
+      <c r="B102" s="24">
+        <v>92919</v>
+      </c>
+      <c r="C102" s="25">
+        <v>758</v>
+      </c>
+      <c r="D102" s="25">
+        <v>1520</v>
+      </c>
+      <c r="E102" s="25">
+        <v>1</v>
+      </c>
+      <c r="F102" s="25">
+        <v>6</v>
+      </c>
+      <c r="G102" s="25">
+        <v>1</v>
+      </c>
+      <c r="H102" s="25">
+        <v>2</v>
+      </c>
+      <c r="I102" s="25">
+        <v>109</v>
+      </c>
+      <c r="J102" s="25">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="103" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A103" s="29">
+        <v>44003</v>
+      </c>
+      <c r="B103" s="30">
+        <v>93181</v>
+      </c>
+      <c r="C103" s="31">
+        <v>271</v>
+      </c>
+      <c r="D103" s="31">
+        <v>1521</v>
+      </c>
+      <c r="E103" s="31">
+        <v>1</v>
+      </c>
+      <c r="F103" s="31">
+        <v>6</v>
+      </c>
+      <c r="G103" s="31">
+        <v>1</v>
+      </c>
+      <c r="H103" s="31">
+        <v>0</v>
+      </c>
+      <c r="I103" s="31">
+        <v>109</v>
+      </c>
+      <c r="J103" s="31">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="104" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A104" s="29">
+        <v>44004</v>
+      </c>
+      <c r="B104" s="30">
+        <v>94165</v>
+      </c>
+      <c r="C104" s="31">
+        <v>984</v>
+      </c>
+      <c r="D104" s="31">
+        <v>1534</v>
+      </c>
+      <c r="E104" s="31">
+        <v>13</v>
+      </c>
+      <c r="F104" s="31">
+        <v>5</v>
+      </c>
+      <c r="G104" s="31">
+        <v>1</v>
+      </c>
+      <c r="H104" s="31">
+        <v>1</v>
+      </c>
+      <c r="I104" s="31">
+        <v>109</v>
+      </c>
+      <c r="J104" s="31">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="105" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A105" s="29">
+        <v>44005</v>
+      </c>
+      <c r="B105" s="30">
+        <v>95387</v>
+      </c>
+      <c r="C105" s="31">
+        <v>1222</v>
+      </c>
+      <c r="D105" s="31">
+        <v>1541</v>
+      </c>
+      <c r="E105" s="31">
+        <v>7</v>
+      </c>
+      <c r="F105" s="31">
+        <v>7</v>
+      </c>
+      <c r="G105" s="31">
+        <v>2</v>
+      </c>
+      <c r="H105" s="31">
+        <v>0</v>
+      </c>
+      <c r="I105" s="31" t="s">
+        <v>10</v>
+      </c>
+      <c r="J105" s="31">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="106" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A106" s="23">
+        <v>44006</v>
+      </c>
+      <c r="B106" s="24">
+        <v>96599</v>
+      </c>
+      <c r="C106" s="25">
+        <v>1212</v>
+      </c>
+      <c r="D106" s="25">
+        <v>1547</v>
+      </c>
+      <c r="E106" s="25">
+        <v>6</v>
+      </c>
+      <c r="F106" s="25">
+        <v>7</v>
+      </c>
+      <c r="G106" s="25">
+        <v>2</v>
+      </c>
+      <c r="H106" s="25">
+        <v>0</v>
+      </c>
+      <c r="I106" s="25" t="s">
+        <v>10</v>
+      </c>
+      <c r="J106" s="25">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="107" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A107" s="29">
+        <v>44007</v>
+      </c>
+      <c r="B107" s="30">
+        <v>97442</v>
+      </c>
+      <c r="C107" s="31">
+        <v>843</v>
+      </c>
+      <c r="D107" s="31">
+        <v>1558</v>
+      </c>
+      <c r="E107" s="31">
+        <v>11</v>
+      </c>
+      <c r="F107" s="31">
+        <v>8</v>
+      </c>
+      <c r="G107" s="31">
+        <v>2</v>
+      </c>
+      <c r="H107" s="31">
+        <v>0</v>
+      </c>
+      <c r="I107" s="31" t="s">
+        <v>10</v>
+      </c>
+      <c r="J107" s="31">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="108" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A108" s="29">
+        <v>44008</v>
+      </c>
+      <c r="B108" s="30">
+        <v>98320</v>
+      </c>
+      <c r="C108" s="31">
+        <v>878</v>
+      </c>
+      <c r="D108" s="31">
+        <v>1572</v>
+      </c>
+      <c r="E108" s="31">
+        <v>14</v>
+      </c>
+      <c r="F108" s="31">
+        <v>8</v>
+      </c>
+      <c r="G108" s="31">
+        <v>1</v>
+      </c>
+      <c r="H108" s="31">
+        <v>0</v>
+      </c>
+      <c r="I108" s="31" t="s">
+        <v>10</v>
+      </c>
+      <c r="J108" s="31">
+        <v>0</v>
+      </c>
+    </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>

</xml_diff>

<commit_message>
Data updated by GitHub Bot (2020-06-27 20)
</commit_message>
<xml_diff>
--- a/output/snapshot/fdcf2531-4c3e-5c02-b63c-ee160ead6dea.xlsx
+++ b/output/snapshot/fdcf2531-4c3e-5c02-b63c-ee160ead6dea.xlsx
@@ -1,16 +1,15 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="21929"/>
-  <workbookPr/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
+  <fileVersion appName="xl" lastEdited="6" lowestEdited="6" rupBuild="14420"/>
+  <workbookPr defaultThemeVersion="164011"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="I:\AKTUALNI PODATKI - KORONA\Za objavo na GOV.SI\ang\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{1E6DD62F-2BE2-47DC-A7ED-9B57C1589256}" xr6:coauthVersionLast="44" xr6:coauthVersionMax="44" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840"/>
   </bookViews>
   <sheets>
     <sheet name="Covid-19 podatki" sheetId="1" r:id="rId1"/>
@@ -25,7 +24,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="10" uniqueCount="10">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="14" uniqueCount="11">
   <si>
     <t>Date</t>
   </si>
@@ -56,15 +55,18 @@
   <si>
     <t>Deaths (daily)</t>
   </si>
+  <si>
+    <t>111*</t>
+  </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" mc:Ignorable="x14ac x16r2">
   <numFmts count="1">
     <numFmt numFmtId="164" formatCode="d/\ m/\ yyyy;@"/>
   </numFmts>
-  <fonts count="4" x14ac:knownFonts="1">
+  <fonts count="5" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -93,6 +95,13 @@
       <name val="Calibri Light"/>
       <scheme val="major"/>
     </font>
+    <font>
+      <sz val="10"/>
+      <color theme="1"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
   </fonts>
   <fills count="3">
     <fill>
@@ -108,7 +117,7 @@
       </patternFill>
     </fill>
   </fills>
-  <borders count="2">
+  <borders count="3">
     <border>
       <left/>
       <right/>
@@ -129,11 +138,26 @@
       <bottom/>
       <diagonal/>
     </border>
+    <border>
+      <left style="thin">
+        <color theme="4"/>
+      </left>
+      <right style="thin">
+        <color theme="4"/>
+      </right>
+      <top style="thin">
+        <color theme="4"/>
+      </top>
+      <bottom style="thin">
+        <color theme="4"/>
+      </bottom>
+      <diagonal/>
+    </border>
   </borders>
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="26">
+  <cellXfs count="32">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="49" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyAlignment="1" applyProtection="1">
       <alignment horizontal="left" vertical="top"/>
@@ -208,6 +232,24 @@
       <alignment horizontal="right"/>
     </xf>
     <xf numFmtId="0" fontId="3" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="right"/>
+    </xf>
+    <xf numFmtId="164" fontId="4" fillId="2" borderId="2" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="right" vertical="top"/>
+    </xf>
+    <xf numFmtId="3" fontId="4" fillId="2" borderId="2" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="right"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="2" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="right"/>
+    </xf>
+    <xf numFmtId="164" fontId="3" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="right" vertical="top"/>
+    </xf>
+    <xf numFmtId="3" fontId="3" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="right"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="right"/>
     </xf>
   </cellXfs>
@@ -399,8 +441,8 @@
 </file>
 
 <file path=xl/tables/table1.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="1" xr:uid="{00000000-000C-0000-FFFF-FFFF00000000}" name="Tabela1" displayName="Tabela1" ref="A1:J75" totalsRowShown="0" headerRowDxfId="11" dataDxfId="10">
-  <autoFilter ref="A1:J75" xr:uid="{00000000-0009-0000-0100-000001000000}">
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="1" name="Tabela1" displayName="Tabela1" ref="A1:J108" totalsRowShown="0" headerRowDxfId="11" dataDxfId="10">
+  <autoFilter ref="A1:J108">
     <filterColumn colId="0" hiddenButton="1"/>
     <filterColumn colId="1" hiddenButton="1"/>
     <filterColumn colId="2" hiddenButton="1"/>
@@ -413,16 +455,16 @@
     <filterColumn colId="9" hiddenButton="1"/>
   </autoFilter>
   <tableColumns count="10">
-    <tableColumn id="1" xr3:uid="{00000000-0010-0000-0000-000001000000}" name="Date" dataDxfId="9"/>
-    <tableColumn id="2" xr3:uid="{00000000-0010-0000-0000-000002000000}" name="Tested (all)" dataDxfId="8"/>
-    <tableColumn id="3" xr3:uid="{00000000-0010-0000-0000-000003000000}" name="Tested (daily)" dataDxfId="7"/>
-    <tableColumn id="4" xr3:uid="{00000000-0010-0000-0000-000004000000}" name="Positive (all)" dataDxfId="6"/>
-    <tableColumn id="5" xr3:uid="{00000000-0010-0000-0000-000005000000}" name="Positive (daily)" dataDxfId="5"/>
-    <tableColumn id="6" xr3:uid="{00000000-0010-0000-0000-000006000000}" name="All hospitalized on certain day" dataDxfId="4"/>
-    <tableColumn id="7" xr3:uid="{00000000-0010-0000-0000-000007000000}" name="All persons in intensive care on certain day" dataDxfId="3"/>
-    <tableColumn id="10" xr3:uid="{00000000-0010-0000-0000-00000A000000}" name="Discharged" dataDxfId="2"/>
-    <tableColumn id="8" xr3:uid="{00000000-0010-0000-0000-000008000000}" name="Deaths (all)" dataDxfId="1"/>
-    <tableColumn id="9" xr3:uid="{00000000-0010-0000-0000-000009000000}" name="Deaths (daily)" dataDxfId="0"/>
+    <tableColumn id="1" name="Date" dataDxfId="9"/>
+    <tableColumn id="2" name="Tested (all)" dataDxfId="8"/>
+    <tableColumn id="3" name="Tested (daily)" dataDxfId="7"/>
+    <tableColumn id="4" name="Positive (all)" dataDxfId="6"/>
+    <tableColumn id="5" name="Positive (daily)" dataDxfId="5"/>
+    <tableColumn id="6" name="All hospitalized on certain day" dataDxfId="4"/>
+    <tableColumn id="7" name="All persons in intensive care on certain day" dataDxfId="3"/>
+    <tableColumn id="10" name="Discharged" dataDxfId="2"/>
+    <tableColumn id="8" name="Deaths (all)" dataDxfId="1"/>
+    <tableColumn id="9" name="Deaths (daily)" dataDxfId="0"/>
   </tableColumns>
   <tableStyleInfo name="TableStyleLight16" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
   <extLst>
@@ -695,11 +737,11 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:J75"/>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <dimension ref="A1:J108"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A40" zoomScale="89" zoomScaleNormal="89" workbookViewId="0">
-      <selection activeCell="J74" sqref="J74"/>
+    <sheetView tabSelected="1" topLeftCell="A83" zoomScale="89" zoomScaleNormal="89" workbookViewId="0">
+      <selection activeCell="J108" sqref="J108"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -3117,6 +3159,1062 @@
         <v>0</v>
       </c>
     </row>
+    <row r="76" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A76" s="20">
+        <v>43976</v>
+      </c>
+      <c r="B76" s="21">
+        <v>75770</v>
+      </c>
+      <c r="C76" s="22">
+        <v>754</v>
+      </c>
+      <c r="D76" s="22">
+        <v>1469</v>
+      </c>
+      <c r="E76" s="22">
+        <v>0</v>
+      </c>
+      <c r="F76" s="22">
+        <v>9</v>
+      </c>
+      <c r="G76" s="22">
+        <v>2</v>
+      </c>
+      <c r="H76" s="22">
+        <v>6</v>
+      </c>
+      <c r="I76" s="22">
+        <v>108</v>
+      </c>
+      <c r="J76" s="22">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="77" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A77" s="20">
+        <v>43977</v>
+      </c>
+      <c r="B77" s="21">
+        <v>76579</v>
+      </c>
+      <c r="C77" s="22">
+        <v>809</v>
+      </c>
+      <c r="D77" s="22">
+        <v>1471</v>
+      </c>
+      <c r="E77" s="22">
+        <v>2</v>
+      </c>
+      <c r="F77" s="22">
+        <v>8</v>
+      </c>
+      <c r="G77" s="22">
+        <v>2</v>
+      </c>
+      <c r="H77" s="22">
+        <v>2</v>
+      </c>
+      <c r="I77" s="22">
+        <v>108</v>
+      </c>
+      <c r="J77" s="22">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="78" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A78" s="20">
+        <v>43978</v>
+      </c>
+      <c r="B78" s="21">
+        <v>77210</v>
+      </c>
+      <c r="C78" s="22">
+        <v>631</v>
+      </c>
+      <c r="D78" s="22">
+        <v>1473</v>
+      </c>
+      <c r="E78" s="22">
+        <v>2</v>
+      </c>
+      <c r="F78" s="22">
+        <v>7</v>
+      </c>
+      <c r="G78" s="22">
+        <v>2</v>
+      </c>
+      <c r="H78" s="22">
+        <v>1</v>
+      </c>
+      <c r="I78" s="22">
+        <v>108</v>
+      </c>
+      <c r="J78" s="22">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="79" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A79" s="20">
+        <v>43979</v>
+      </c>
+      <c r="B79" s="21">
+        <v>77916</v>
+      </c>
+      <c r="C79" s="22">
+        <v>706</v>
+      </c>
+      <c r="D79" s="22">
+        <v>1473</v>
+      </c>
+      <c r="E79" s="22">
+        <v>0</v>
+      </c>
+      <c r="F79" s="22">
+        <v>7</v>
+      </c>
+      <c r="G79" s="22">
+        <v>2</v>
+      </c>
+      <c r="H79" s="22">
+        <v>0</v>
+      </c>
+      <c r="I79" s="22">
+        <v>108</v>
+      </c>
+      <c r="J79" s="22">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="80" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A80" s="20">
+        <v>43980</v>
+      </c>
+      <c r="B80" s="21">
+        <v>78529</v>
+      </c>
+      <c r="C80" s="22">
+        <v>613</v>
+      </c>
+      <c r="D80" s="22">
+        <v>1473</v>
+      </c>
+      <c r="E80" s="22">
+        <v>0</v>
+      </c>
+      <c r="F80" s="22">
+        <v>7</v>
+      </c>
+      <c r="G80" s="22">
+        <v>2</v>
+      </c>
+      <c r="H80" s="22">
+        <v>0</v>
+      </c>
+      <c r="I80" s="22">
+        <v>108</v>
+      </c>
+      <c r="J80" s="22">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="81" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A81" s="20">
+        <v>43981</v>
+      </c>
+      <c r="B81" s="22">
+        <v>78793</v>
+      </c>
+      <c r="C81" s="22">
+        <v>264</v>
+      </c>
+      <c r="D81" s="22">
+        <v>1473</v>
+      </c>
+      <c r="E81" s="22">
+        <v>0</v>
+      </c>
+      <c r="F81" s="22">
+        <v>6</v>
+      </c>
+      <c r="G81" s="22">
+        <v>2</v>
+      </c>
+      <c r="H81" s="22">
+        <v>1</v>
+      </c>
+      <c r="I81" s="22">
+        <v>108</v>
+      </c>
+      <c r="J81" s="22">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="82" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A82" s="20">
+        <v>43982</v>
+      </c>
+      <c r="B82" s="21">
+        <v>79039</v>
+      </c>
+      <c r="C82" s="22">
+        <v>246</v>
+      </c>
+      <c r="D82" s="22">
+        <v>1473</v>
+      </c>
+      <c r="E82" s="22">
+        <v>0</v>
+      </c>
+      <c r="F82" s="22">
+        <v>5</v>
+      </c>
+      <c r="G82" s="22">
+        <v>1</v>
+      </c>
+      <c r="H82" s="22">
+        <v>0</v>
+      </c>
+      <c r="I82" s="22">
+        <v>109</v>
+      </c>
+      <c r="J82" s="22">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="83" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A83" s="20">
+        <v>43983</v>
+      </c>
+      <c r="B83" s="21">
+        <v>79698</v>
+      </c>
+      <c r="C83" s="22">
+        <v>659</v>
+      </c>
+      <c r="D83" s="22">
+        <v>1475</v>
+      </c>
+      <c r="E83" s="22">
+        <v>2</v>
+      </c>
+      <c r="F83" s="22">
+        <v>5</v>
+      </c>
+      <c r="G83" s="22">
+        <v>1</v>
+      </c>
+      <c r="H83" s="22">
+        <v>0</v>
+      </c>
+      <c r="I83" s="22">
+        <v>109</v>
+      </c>
+      <c r="J83" s="22">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="84" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A84" s="20">
+        <v>43984</v>
+      </c>
+      <c r="B84" s="21">
+        <v>80505</v>
+      </c>
+      <c r="C84" s="22">
+        <v>807</v>
+      </c>
+      <c r="D84" s="22">
+        <v>1477</v>
+      </c>
+      <c r="E84" s="22">
+        <v>2</v>
+      </c>
+      <c r="F84" s="22">
+        <v>5</v>
+      </c>
+      <c r="G84" s="22">
+        <v>0</v>
+      </c>
+      <c r="H84" s="22">
+        <v>0</v>
+      </c>
+      <c r="I84" s="22">
+        <v>109</v>
+      </c>
+      <c r="J84" s="22">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="85" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A85" s="20">
+        <v>43985</v>
+      </c>
+      <c r="B85" s="21">
+        <v>81333</v>
+      </c>
+      <c r="C85" s="22">
+        <v>828</v>
+      </c>
+      <c r="D85" s="22">
+        <v>1477</v>
+      </c>
+      <c r="E85" s="22">
+        <v>0</v>
+      </c>
+      <c r="F85" s="22">
+        <v>5</v>
+      </c>
+      <c r="G85" s="22">
+        <v>0</v>
+      </c>
+      <c r="H85" s="22">
+        <v>0</v>
+      </c>
+      <c r="I85" s="22">
+        <v>109</v>
+      </c>
+      <c r="J85" s="22">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="86" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A86" s="26">
+        <v>43986</v>
+      </c>
+      <c r="B86" s="27">
+        <v>82161</v>
+      </c>
+      <c r="C86" s="28">
+        <v>828</v>
+      </c>
+      <c r="D86" s="28">
+        <v>1479</v>
+      </c>
+      <c r="E86" s="28">
+        <v>2</v>
+      </c>
+      <c r="F86" s="28">
+        <v>6</v>
+      </c>
+      <c r="G86" s="28">
+        <v>0</v>
+      </c>
+      <c r="H86" s="28">
+        <v>0</v>
+      </c>
+      <c r="I86" s="28">
+        <v>109</v>
+      </c>
+      <c r="J86" s="28">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="87" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A87" s="29">
+        <v>43987</v>
+      </c>
+      <c r="B87" s="30">
+        <v>82876</v>
+      </c>
+      <c r="C87" s="31">
+        <v>715</v>
+      </c>
+      <c r="D87" s="31">
+        <v>1484</v>
+      </c>
+      <c r="E87" s="31">
+        <v>5</v>
+      </c>
+      <c r="F87" s="31">
+        <v>6</v>
+      </c>
+      <c r="G87" s="31">
+        <v>0</v>
+      </c>
+      <c r="H87" s="31">
+        <v>0</v>
+      </c>
+      <c r="I87" s="31">
+        <v>109</v>
+      </c>
+      <c r="J87" s="31">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="88" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A88" s="23">
+        <v>43988</v>
+      </c>
+      <c r="B88" s="24">
+        <v>83105</v>
+      </c>
+      <c r="C88" s="25">
+        <v>229</v>
+      </c>
+      <c r="D88" s="25">
+        <v>1485</v>
+      </c>
+      <c r="E88" s="25">
+        <v>1</v>
+      </c>
+      <c r="F88" s="25">
+        <v>5</v>
+      </c>
+      <c r="G88" s="25">
+        <v>0</v>
+      </c>
+      <c r="H88" s="25">
+        <v>1</v>
+      </c>
+      <c r="I88" s="25">
+        <v>109</v>
+      </c>
+      <c r="J88" s="25">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="89" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A89" s="29">
+        <v>43989</v>
+      </c>
+      <c r="B89" s="30">
+        <v>83316</v>
+      </c>
+      <c r="C89" s="31">
+        <v>211</v>
+      </c>
+      <c r="D89" s="31">
+        <v>1485</v>
+      </c>
+      <c r="E89" s="31">
+        <v>0</v>
+      </c>
+      <c r="F89" s="31">
+        <v>5</v>
+      </c>
+      <c r="G89" s="31">
+        <v>0</v>
+      </c>
+      <c r="H89" s="31">
+        <v>0</v>
+      </c>
+      <c r="I89" s="31">
+        <v>109</v>
+      </c>
+      <c r="J89" s="31">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="90" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A90" s="20">
+        <v>43990</v>
+      </c>
+      <c r="B90" s="21">
+        <v>84130</v>
+      </c>
+      <c r="C90" s="22">
+        <v>814</v>
+      </c>
+      <c r="D90" s="22">
+        <v>1486</v>
+      </c>
+      <c r="E90" s="22">
+        <v>1</v>
+      </c>
+      <c r="F90" s="22">
+        <v>6</v>
+      </c>
+      <c r="G90" s="22">
+        <v>0</v>
+      </c>
+      <c r="H90" s="22">
+        <v>0</v>
+      </c>
+      <c r="I90" s="22">
+        <v>109</v>
+      </c>
+      <c r="J90" s="22">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="91" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A91" s="20">
+        <v>43991</v>
+      </c>
+      <c r="B91" s="21">
+        <v>84868</v>
+      </c>
+      <c r="C91" s="22">
+        <v>738</v>
+      </c>
+      <c r="D91" s="22">
+        <v>1488</v>
+      </c>
+      <c r="E91" s="22">
+        <v>2</v>
+      </c>
+      <c r="F91" s="22">
+        <v>6</v>
+      </c>
+      <c r="G91" s="22">
+        <v>0</v>
+      </c>
+      <c r="H91" s="22">
+        <v>0</v>
+      </c>
+      <c r="I91" s="22">
+        <v>109</v>
+      </c>
+      <c r="J91" s="22">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="92" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A92" s="23">
+        <v>43992</v>
+      </c>
+      <c r="B92" s="24">
+        <v>85626</v>
+      </c>
+      <c r="C92" s="25">
+        <v>758</v>
+      </c>
+      <c r="D92" s="25">
+        <v>1488</v>
+      </c>
+      <c r="E92" s="25">
+        <v>0</v>
+      </c>
+      <c r="F92" s="25">
+        <v>6</v>
+      </c>
+      <c r="G92" s="25">
+        <v>0</v>
+      </c>
+      <c r="H92" s="25">
+        <v>0</v>
+      </c>
+      <c r="I92" s="25">
+        <v>109</v>
+      </c>
+      <c r="J92" s="25">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="93" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A93" s="29">
+        <v>43993</v>
+      </c>
+      <c r="B93" s="30">
+        <v>86328</v>
+      </c>
+      <c r="C93" s="31">
+        <v>702</v>
+      </c>
+      <c r="D93" s="31">
+        <v>1490</v>
+      </c>
+      <c r="E93" s="31">
+        <v>2</v>
+      </c>
+      <c r="F93" s="31">
+        <v>6</v>
+      </c>
+      <c r="G93" s="31">
+        <v>0</v>
+      </c>
+      <c r="H93" s="31">
+        <v>0</v>
+      </c>
+      <c r="I93" s="31">
+        <v>109</v>
+      </c>
+      <c r="J93" s="31">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="94" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A94" s="23">
+        <v>43994</v>
+      </c>
+      <c r="B94" s="24">
+        <v>87095</v>
+      </c>
+      <c r="C94" s="25">
+        <v>767</v>
+      </c>
+      <c r="D94" s="25">
+        <v>1492</v>
+      </c>
+      <c r="E94" s="25">
+        <v>2</v>
+      </c>
+      <c r="F94" s="25">
+        <v>6</v>
+      </c>
+      <c r="G94" s="25">
+        <v>0</v>
+      </c>
+      <c r="H94" s="25">
+        <v>0</v>
+      </c>
+      <c r="I94" s="25">
+        <v>109</v>
+      </c>
+      <c r="J94" s="25">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="95" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A95" s="29">
+        <v>43995</v>
+      </c>
+      <c r="B95" s="30">
+        <v>87386</v>
+      </c>
+      <c r="C95" s="31">
+        <v>291</v>
+      </c>
+      <c r="D95" s="31">
+        <v>1495</v>
+      </c>
+      <c r="E95" s="31">
+        <v>3</v>
+      </c>
+      <c r="F95" s="31">
+        <v>6</v>
+      </c>
+      <c r="G95" s="31">
+        <v>0</v>
+      </c>
+      <c r="H95" s="31">
+        <v>0</v>
+      </c>
+      <c r="I95" s="31">
+        <v>109</v>
+      </c>
+      <c r="J95" s="31">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="96" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A96" s="23">
+        <v>43996</v>
+      </c>
+      <c r="B96" s="24">
+        <v>87598</v>
+      </c>
+      <c r="C96" s="25">
+        <v>212</v>
+      </c>
+      <c r="D96" s="25">
+        <v>1496</v>
+      </c>
+      <c r="E96" s="25">
+        <v>1</v>
+      </c>
+      <c r="F96" s="25">
+        <v>7</v>
+      </c>
+      <c r="G96" s="25">
+        <v>1</v>
+      </c>
+      <c r="H96" s="25">
+        <v>0</v>
+      </c>
+      <c r="I96" s="25">
+        <v>109</v>
+      </c>
+      <c r="J96" s="25">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="97" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A97" s="20">
+        <v>43997</v>
+      </c>
+      <c r="B97" s="21">
+        <v>88165</v>
+      </c>
+      <c r="C97" s="22">
+        <v>567</v>
+      </c>
+      <c r="D97" s="22">
+        <v>1499</v>
+      </c>
+      <c r="E97" s="22">
+        <v>3</v>
+      </c>
+      <c r="F97" s="22">
+        <v>7</v>
+      </c>
+      <c r="G97" s="22">
+        <v>1</v>
+      </c>
+      <c r="H97" s="22">
+        <v>0</v>
+      </c>
+      <c r="I97" s="22">
+        <v>109</v>
+      </c>
+      <c r="J97" s="22">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="98" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A98" s="20">
+        <v>43998</v>
+      </c>
+      <c r="B98" s="21">
+        <v>89151</v>
+      </c>
+      <c r="C98" s="22">
+        <v>986</v>
+      </c>
+      <c r="D98" s="22">
+        <v>1503</v>
+      </c>
+      <c r="E98" s="22">
+        <v>4</v>
+      </c>
+      <c r="F98" s="22">
+        <v>7</v>
+      </c>
+      <c r="G98" s="22">
+        <v>1</v>
+      </c>
+      <c r="H98" s="22">
+        <v>0</v>
+      </c>
+      <c r="I98" s="22">
+        <v>109</v>
+      </c>
+      <c r="J98" s="22">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="99" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A99" s="29">
+        <v>43999</v>
+      </c>
+      <c r="B99" s="30">
+        <v>90103</v>
+      </c>
+      <c r="C99" s="31">
+        <v>952</v>
+      </c>
+      <c r="D99" s="31">
+        <v>1511</v>
+      </c>
+      <c r="E99" s="31">
+        <v>8</v>
+      </c>
+      <c r="F99" s="31">
+        <v>6</v>
+      </c>
+      <c r="G99" s="31">
+        <v>1</v>
+      </c>
+      <c r="H99" s="31">
+        <v>1</v>
+      </c>
+      <c r="I99" s="31">
+        <v>109</v>
+      </c>
+      <c r="J99" s="31">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="100" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A100" s="20">
+        <v>44000</v>
+      </c>
+      <c r="B100" s="21">
+        <v>91005</v>
+      </c>
+      <c r="C100" s="22">
+        <v>902</v>
+      </c>
+      <c r="D100" s="22">
+        <v>1513</v>
+      </c>
+      <c r="E100" s="22">
+        <v>2</v>
+      </c>
+      <c r="F100" s="22">
+        <v>8</v>
+      </c>
+      <c r="G100" s="22">
+        <v>1</v>
+      </c>
+      <c r="H100" s="22">
+        <v>0</v>
+      </c>
+      <c r="I100" s="22">
+        <v>109</v>
+      </c>
+      <c r="J100" s="22">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="101" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A101" s="29">
+        <v>44001</v>
+      </c>
+      <c r="B101" s="30">
+        <v>92152</v>
+      </c>
+      <c r="C101" s="31">
+        <v>1147</v>
+      </c>
+      <c r="D101" s="31">
+        <v>1519</v>
+      </c>
+      <c r="E101" s="31">
+        <v>6</v>
+      </c>
+      <c r="F101" s="31">
+        <v>6</v>
+      </c>
+      <c r="G101" s="31">
+        <v>1</v>
+      </c>
+      <c r="H101" s="31">
+        <v>2</v>
+      </c>
+      <c r="I101" s="31">
+        <v>109</v>
+      </c>
+      <c r="J101" s="31">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="102" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A102" s="23">
+        <v>44002</v>
+      </c>
+      <c r="B102" s="24">
+        <v>92919</v>
+      </c>
+      <c r="C102" s="25">
+        <v>758</v>
+      </c>
+      <c r="D102" s="25">
+        <v>1520</v>
+      </c>
+      <c r="E102" s="25">
+        <v>1</v>
+      </c>
+      <c r="F102" s="25">
+        <v>6</v>
+      </c>
+      <c r="G102" s="25">
+        <v>1</v>
+      </c>
+      <c r="H102" s="25">
+        <v>2</v>
+      </c>
+      <c r="I102" s="25">
+        <v>109</v>
+      </c>
+      <c r="J102" s="25">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="103" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A103" s="29">
+        <v>44003</v>
+      </c>
+      <c r="B103" s="30">
+        <v>93181</v>
+      </c>
+      <c r="C103" s="31">
+        <v>271</v>
+      </c>
+      <c r="D103" s="31">
+        <v>1521</v>
+      </c>
+      <c r="E103" s="31">
+        <v>1</v>
+      </c>
+      <c r="F103" s="31">
+        <v>6</v>
+      </c>
+      <c r="G103" s="31">
+        <v>1</v>
+      </c>
+      <c r="H103" s="31">
+        <v>0</v>
+      </c>
+      <c r="I103" s="31">
+        <v>109</v>
+      </c>
+      <c r="J103" s="31">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="104" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A104" s="29">
+        <v>44004</v>
+      </c>
+      <c r="B104" s="30">
+        <v>94165</v>
+      </c>
+      <c r="C104" s="31">
+        <v>984</v>
+      </c>
+      <c r="D104" s="31">
+        <v>1534</v>
+      </c>
+      <c r="E104" s="31">
+        <v>13</v>
+      </c>
+      <c r="F104" s="31">
+        <v>5</v>
+      </c>
+      <c r="G104" s="31">
+        <v>1</v>
+      </c>
+      <c r="H104" s="31">
+        <v>1</v>
+      </c>
+      <c r="I104" s="31">
+        <v>109</v>
+      </c>
+      <c r="J104" s="31">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="105" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A105" s="29">
+        <v>44005</v>
+      </c>
+      <c r="B105" s="30">
+        <v>95387</v>
+      </c>
+      <c r="C105" s="31">
+        <v>1222</v>
+      </c>
+      <c r="D105" s="31">
+        <v>1541</v>
+      </c>
+      <c r="E105" s="31">
+        <v>7</v>
+      </c>
+      <c r="F105" s="31">
+        <v>7</v>
+      </c>
+      <c r="G105" s="31">
+        <v>2</v>
+      </c>
+      <c r="H105" s="31">
+        <v>0</v>
+      </c>
+      <c r="I105" s="31" t="s">
+        <v>10</v>
+      </c>
+      <c r="J105" s="31">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="106" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A106" s="23">
+        <v>44006</v>
+      </c>
+      <c r="B106" s="24">
+        <v>96599</v>
+      </c>
+      <c r="C106" s="25">
+        <v>1212</v>
+      </c>
+      <c r="D106" s="25">
+        <v>1547</v>
+      </c>
+      <c r="E106" s="25">
+        <v>6</v>
+      </c>
+      <c r="F106" s="25">
+        <v>7</v>
+      </c>
+      <c r="G106" s="25">
+        <v>2</v>
+      </c>
+      <c r="H106" s="25">
+        <v>0</v>
+      </c>
+      <c r="I106" s="25" t="s">
+        <v>10</v>
+      </c>
+      <c r="J106" s="25">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="107" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A107" s="29">
+        <v>44007</v>
+      </c>
+      <c r="B107" s="30">
+        <v>97442</v>
+      </c>
+      <c r="C107" s="31">
+        <v>843</v>
+      </c>
+      <c r="D107" s="31">
+        <v>1558</v>
+      </c>
+      <c r="E107" s="31">
+        <v>11</v>
+      </c>
+      <c r="F107" s="31">
+        <v>8</v>
+      </c>
+      <c r="G107" s="31">
+        <v>2</v>
+      </c>
+      <c r="H107" s="31">
+        <v>0</v>
+      </c>
+      <c r="I107" s="31" t="s">
+        <v>10</v>
+      </c>
+      <c r="J107" s="31">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="108" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A108" s="29">
+        <v>44008</v>
+      </c>
+      <c r="B108" s="30">
+        <v>98320</v>
+      </c>
+      <c r="C108" s="31">
+        <v>878</v>
+      </c>
+      <c r="D108" s="31">
+        <v>1572</v>
+      </c>
+      <c r="E108" s="31">
+        <v>14</v>
+      </c>
+      <c r="F108" s="31">
+        <v>8</v>
+      </c>
+      <c r="G108" s="31">
+        <v>1</v>
+      </c>
+      <c r="H108" s="31">
+        <v>0</v>
+      </c>
+      <c r="I108" s="31" t="s">
+        <v>10</v>
+      </c>
+      <c r="J108" s="31">
+        <v>0</v>
+      </c>
+    </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>

</xml_diff>

<commit_message>
Data updated by GitHub Bot (2020-06-28 12)
</commit_message>
<xml_diff>
--- a/output/snapshot/fdcf2531-4c3e-5c02-b63c-ee160ead6dea.xlsx
+++ b/output/snapshot/fdcf2531-4c3e-5c02-b63c-ee160ead6dea.xlsx
@@ -1,16 +1,15 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="21929"/>
-  <workbookPr/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
+  <fileVersion appName="xl" lastEdited="6" lowestEdited="6" rupBuild="14420"/>
+  <workbookPr defaultThemeVersion="164011"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="I:\AKTUALNI PODATKI - KORONA\Za objavo na GOV.SI\ang\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{1E6DD62F-2BE2-47DC-A7ED-9B57C1589256}" xr6:coauthVersionLast="44" xr6:coauthVersionMax="44" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840"/>
   </bookViews>
   <sheets>
     <sheet name="Covid-19 podatki" sheetId="1" r:id="rId1"/>
@@ -25,7 +24,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="10" uniqueCount="10">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="15" uniqueCount="11">
   <si>
     <t>Date</t>
   </si>
@@ -56,15 +55,18 @@
   <si>
     <t>Deaths (daily)</t>
   </si>
+  <si>
+    <t>111*</t>
+  </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" mc:Ignorable="x14ac x16r2">
   <numFmts count="1">
     <numFmt numFmtId="164" formatCode="d/\ m/\ yyyy;@"/>
   </numFmts>
-  <fonts count="4" x14ac:knownFonts="1">
+  <fonts count="5" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -93,6 +95,13 @@
       <name val="Calibri Light"/>
       <scheme val="major"/>
     </font>
+    <font>
+      <sz val="10"/>
+      <color theme="1"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
   </fonts>
   <fills count="3">
     <fill>
@@ -108,7 +117,7 @@
       </patternFill>
     </fill>
   </fills>
-  <borders count="2">
+  <borders count="3">
     <border>
       <left/>
       <right/>
@@ -129,11 +138,26 @@
       <bottom/>
       <diagonal/>
     </border>
+    <border>
+      <left style="thin">
+        <color theme="4"/>
+      </left>
+      <right style="thin">
+        <color theme="4"/>
+      </right>
+      <top style="thin">
+        <color theme="4"/>
+      </top>
+      <bottom style="thin">
+        <color theme="4"/>
+      </bottom>
+      <diagonal/>
+    </border>
   </borders>
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="26">
+  <cellXfs count="32">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="49" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyAlignment="1" applyProtection="1">
       <alignment horizontal="left" vertical="top"/>
@@ -208,6 +232,24 @@
       <alignment horizontal="right"/>
     </xf>
     <xf numFmtId="0" fontId="3" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="right"/>
+    </xf>
+    <xf numFmtId="164" fontId="4" fillId="2" borderId="2" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="right" vertical="top"/>
+    </xf>
+    <xf numFmtId="3" fontId="4" fillId="2" borderId="2" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="right"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="2" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="right"/>
+    </xf>
+    <xf numFmtId="164" fontId="3" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="right" vertical="top"/>
+    </xf>
+    <xf numFmtId="3" fontId="3" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="right"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="right"/>
     </xf>
   </cellXfs>
@@ -399,8 +441,8 @@
 </file>
 
 <file path=xl/tables/table1.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="1" xr:uid="{00000000-000C-0000-FFFF-FFFF00000000}" name="Tabela1" displayName="Tabela1" ref="A1:J75" totalsRowShown="0" headerRowDxfId="11" dataDxfId="10">
-  <autoFilter ref="A1:J75" xr:uid="{00000000-0009-0000-0100-000001000000}">
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="1" name="Tabela1" displayName="Tabela1" ref="A1:J109" totalsRowShown="0" headerRowDxfId="11" dataDxfId="10">
+  <autoFilter ref="A1:J109">
     <filterColumn colId="0" hiddenButton="1"/>
     <filterColumn colId="1" hiddenButton="1"/>
     <filterColumn colId="2" hiddenButton="1"/>
@@ -413,16 +455,16 @@
     <filterColumn colId="9" hiddenButton="1"/>
   </autoFilter>
   <tableColumns count="10">
-    <tableColumn id="1" xr3:uid="{00000000-0010-0000-0000-000001000000}" name="Date" dataDxfId="9"/>
-    <tableColumn id="2" xr3:uid="{00000000-0010-0000-0000-000002000000}" name="Tested (all)" dataDxfId="8"/>
-    <tableColumn id="3" xr3:uid="{00000000-0010-0000-0000-000003000000}" name="Tested (daily)" dataDxfId="7"/>
-    <tableColumn id="4" xr3:uid="{00000000-0010-0000-0000-000004000000}" name="Positive (all)" dataDxfId="6"/>
-    <tableColumn id="5" xr3:uid="{00000000-0010-0000-0000-000005000000}" name="Positive (daily)" dataDxfId="5"/>
-    <tableColumn id="6" xr3:uid="{00000000-0010-0000-0000-000006000000}" name="All hospitalized on certain day" dataDxfId="4"/>
-    <tableColumn id="7" xr3:uid="{00000000-0010-0000-0000-000007000000}" name="All persons in intensive care on certain day" dataDxfId="3"/>
-    <tableColumn id="10" xr3:uid="{00000000-0010-0000-0000-00000A000000}" name="Discharged" dataDxfId="2"/>
-    <tableColumn id="8" xr3:uid="{00000000-0010-0000-0000-000008000000}" name="Deaths (all)" dataDxfId="1"/>
-    <tableColumn id="9" xr3:uid="{00000000-0010-0000-0000-000009000000}" name="Deaths (daily)" dataDxfId="0"/>
+    <tableColumn id="1" name="Date" dataDxfId="9"/>
+    <tableColumn id="2" name="Tested (all)" dataDxfId="8"/>
+    <tableColumn id="3" name="Tested (daily)" dataDxfId="7"/>
+    <tableColumn id="4" name="Positive (all)" dataDxfId="6"/>
+    <tableColumn id="5" name="Positive (daily)" dataDxfId="5"/>
+    <tableColumn id="6" name="All hospitalized on certain day" dataDxfId="4"/>
+    <tableColumn id="7" name="All persons in intensive care on certain day" dataDxfId="3"/>
+    <tableColumn id="10" name="Discharged" dataDxfId="2"/>
+    <tableColumn id="8" name="Deaths (all)" dataDxfId="1"/>
+    <tableColumn id="9" name="Deaths (daily)" dataDxfId="0"/>
   </tableColumns>
   <tableStyleInfo name="TableStyleLight16" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
   <extLst>
@@ -695,11 +737,11 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:J75"/>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <dimension ref="A1:J109"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A40" zoomScale="89" zoomScaleNormal="89" workbookViewId="0">
-      <selection activeCell="J74" sqref="J74"/>
+    <sheetView tabSelected="1" topLeftCell="A83" zoomScale="89" zoomScaleNormal="89" workbookViewId="0">
+      <selection activeCell="A109" sqref="A109"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -3117,6 +3159,1094 @@
         <v>0</v>
       </c>
     </row>
+    <row r="76" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A76" s="20">
+        <v>43976</v>
+      </c>
+      <c r="B76" s="21">
+        <v>75770</v>
+      </c>
+      <c r="C76" s="22">
+        <v>754</v>
+      </c>
+      <c r="D76" s="22">
+        <v>1469</v>
+      </c>
+      <c r="E76" s="22">
+        <v>0</v>
+      </c>
+      <c r="F76" s="22">
+        <v>9</v>
+      </c>
+      <c r="G76" s="22">
+        <v>2</v>
+      </c>
+      <c r="H76" s="22">
+        <v>6</v>
+      </c>
+      <c r="I76" s="22">
+        <v>108</v>
+      </c>
+      <c r="J76" s="22">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="77" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A77" s="20">
+        <v>43977</v>
+      </c>
+      <c r="B77" s="21">
+        <v>76579</v>
+      </c>
+      <c r="C77" s="22">
+        <v>809</v>
+      </c>
+      <c r="D77" s="22">
+        <v>1471</v>
+      </c>
+      <c r="E77" s="22">
+        <v>2</v>
+      </c>
+      <c r="F77" s="22">
+        <v>8</v>
+      </c>
+      <c r="G77" s="22">
+        <v>2</v>
+      </c>
+      <c r="H77" s="22">
+        <v>2</v>
+      </c>
+      <c r="I77" s="22">
+        <v>108</v>
+      </c>
+      <c r="J77" s="22">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="78" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A78" s="20">
+        <v>43978</v>
+      </c>
+      <c r="B78" s="21">
+        <v>77210</v>
+      </c>
+      <c r="C78" s="22">
+        <v>631</v>
+      </c>
+      <c r="D78" s="22">
+        <v>1473</v>
+      </c>
+      <c r="E78" s="22">
+        <v>2</v>
+      </c>
+      <c r="F78" s="22">
+        <v>7</v>
+      </c>
+      <c r="G78" s="22">
+        <v>2</v>
+      </c>
+      <c r="H78" s="22">
+        <v>1</v>
+      </c>
+      <c r="I78" s="22">
+        <v>108</v>
+      </c>
+      <c r="J78" s="22">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="79" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A79" s="20">
+        <v>43979</v>
+      </c>
+      <c r="B79" s="21">
+        <v>77916</v>
+      </c>
+      <c r="C79" s="22">
+        <v>706</v>
+      </c>
+      <c r="D79" s="22">
+        <v>1473</v>
+      </c>
+      <c r="E79" s="22">
+        <v>0</v>
+      </c>
+      <c r="F79" s="22">
+        <v>7</v>
+      </c>
+      <c r="G79" s="22">
+        <v>2</v>
+      </c>
+      <c r="H79" s="22">
+        <v>0</v>
+      </c>
+      <c r="I79" s="22">
+        <v>108</v>
+      </c>
+      <c r="J79" s="22">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="80" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A80" s="20">
+        <v>43980</v>
+      </c>
+      <c r="B80" s="21">
+        <v>78529</v>
+      </c>
+      <c r="C80" s="22">
+        <v>613</v>
+      </c>
+      <c r="D80" s="22">
+        <v>1473</v>
+      </c>
+      <c r="E80" s="22">
+        <v>0</v>
+      </c>
+      <c r="F80" s="22">
+        <v>7</v>
+      </c>
+      <c r="G80" s="22">
+        <v>2</v>
+      </c>
+      <c r="H80" s="22">
+        <v>0</v>
+      </c>
+      <c r="I80" s="22">
+        <v>108</v>
+      </c>
+      <c r="J80" s="22">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="81" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A81" s="20">
+        <v>43981</v>
+      </c>
+      <c r="B81" s="22">
+        <v>78793</v>
+      </c>
+      <c r="C81" s="22">
+        <v>264</v>
+      </c>
+      <c r="D81" s="22">
+        <v>1473</v>
+      </c>
+      <c r="E81" s="22">
+        <v>0</v>
+      </c>
+      <c r="F81" s="22">
+        <v>6</v>
+      </c>
+      <c r="G81" s="22">
+        <v>2</v>
+      </c>
+      <c r="H81" s="22">
+        <v>1</v>
+      </c>
+      <c r="I81" s="22">
+        <v>108</v>
+      </c>
+      <c r="J81" s="22">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="82" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A82" s="20">
+        <v>43982</v>
+      </c>
+      <c r="B82" s="21">
+        <v>79039</v>
+      </c>
+      <c r="C82" s="22">
+        <v>246</v>
+      </c>
+      <c r="D82" s="22">
+        <v>1473</v>
+      </c>
+      <c r="E82" s="22">
+        <v>0</v>
+      </c>
+      <c r="F82" s="22">
+        <v>5</v>
+      </c>
+      <c r="G82" s="22">
+        <v>1</v>
+      </c>
+      <c r="H82" s="22">
+        <v>0</v>
+      </c>
+      <c r="I82" s="22">
+        <v>109</v>
+      </c>
+      <c r="J82" s="22">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="83" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A83" s="20">
+        <v>43983</v>
+      </c>
+      <c r="B83" s="21">
+        <v>79698</v>
+      </c>
+      <c r="C83" s="22">
+        <v>659</v>
+      </c>
+      <c r="D83" s="22">
+        <v>1475</v>
+      </c>
+      <c r="E83" s="22">
+        <v>2</v>
+      </c>
+      <c r="F83" s="22">
+        <v>5</v>
+      </c>
+      <c r="G83" s="22">
+        <v>1</v>
+      </c>
+      <c r="H83" s="22">
+        <v>0</v>
+      </c>
+      <c r="I83" s="22">
+        <v>109</v>
+      </c>
+      <c r="J83" s="22">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="84" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A84" s="20">
+        <v>43984</v>
+      </c>
+      <c r="B84" s="21">
+        <v>80505</v>
+      </c>
+      <c r="C84" s="22">
+        <v>807</v>
+      </c>
+      <c r="D84" s="22">
+        <v>1477</v>
+      </c>
+      <c r="E84" s="22">
+        <v>2</v>
+      </c>
+      <c r="F84" s="22">
+        <v>5</v>
+      </c>
+      <c r="G84" s="22">
+        <v>0</v>
+      </c>
+      <c r="H84" s="22">
+        <v>0</v>
+      </c>
+      <c r="I84" s="22">
+        <v>109</v>
+      </c>
+      <c r="J84" s="22">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="85" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A85" s="20">
+        <v>43985</v>
+      </c>
+      <c r="B85" s="21">
+        <v>81333</v>
+      </c>
+      <c r="C85" s="22">
+        <v>828</v>
+      </c>
+      <c r="D85" s="22">
+        <v>1477</v>
+      </c>
+      <c r="E85" s="22">
+        <v>0</v>
+      </c>
+      <c r="F85" s="22">
+        <v>5</v>
+      </c>
+      <c r="G85" s="22">
+        <v>0</v>
+      </c>
+      <c r="H85" s="22">
+        <v>0</v>
+      </c>
+      <c r="I85" s="22">
+        <v>109</v>
+      </c>
+      <c r="J85" s="22">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="86" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A86" s="26">
+        <v>43986</v>
+      </c>
+      <c r="B86" s="27">
+        <v>82161</v>
+      </c>
+      <c r="C86" s="28">
+        <v>828</v>
+      </c>
+      <c r="D86" s="28">
+        <v>1479</v>
+      </c>
+      <c r="E86" s="28">
+        <v>2</v>
+      </c>
+      <c r="F86" s="28">
+        <v>6</v>
+      </c>
+      <c r="G86" s="28">
+        <v>0</v>
+      </c>
+      <c r="H86" s="28">
+        <v>0</v>
+      </c>
+      <c r="I86" s="28">
+        <v>109</v>
+      </c>
+      <c r="J86" s="28">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="87" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A87" s="29">
+        <v>43987</v>
+      </c>
+      <c r="B87" s="30">
+        <v>82876</v>
+      </c>
+      <c r="C87" s="31">
+        <v>715</v>
+      </c>
+      <c r="D87" s="31">
+        <v>1484</v>
+      </c>
+      <c r="E87" s="31">
+        <v>5</v>
+      </c>
+      <c r="F87" s="31">
+        <v>6</v>
+      </c>
+      <c r="G87" s="31">
+        <v>0</v>
+      </c>
+      <c r="H87" s="31">
+        <v>0</v>
+      </c>
+      <c r="I87" s="31">
+        <v>109</v>
+      </c>
+      <c r="J87" s="31">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="88" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A88" s="23">
+        <v>43988</v>
+      </c>
+      <c r="B88" s="24">
+        <v>83105</v>
+      </c>
+      <c r="C88" s="25">
+        <v>229</v>
+      </c>
+      <c r="D88" s="25">
+        <v>1485</v>
+      </c>
+      <c r="E88" s="25">
+        <v>1</v>
+      </c>
+      <c r="F88" s="25">
+        <v>5</v>
+      </c>
+      <c r="G88" s="25">
+        <v>0</v>
+      </c>
+      <c r="H88" s="25">
+        <v>1</v>
+      </c>
+      <c r="I88" s="25">
+        <v>109</v>
+      </c>
+      <c r="J88" s="25">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="89" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A89" s="29">
+        <v>43989</v>
+      </c>
+      <c r="B89" s="30">
+        <v>83316</v>
+      </c>
+      <c r="C89" s="31">
+        <v>211</v>
+      </c>
+      <c r="D89" s="31">
+        <v>1485</v>
+      </c>
+      <c r="E89" s="31">
+        <v>0</v>
+      </c>
+      <c r="F89" s="31">
+        <v>5</v>
+      </c>
+      <c r="G89" s="31">
+        <v>0</v>
+      </c>
+      <c r="H89" s="31">
+        <v>0</v>
+      </c>
+      <c r="I89" s="31">
+        <v>109</v>
+      </c>
+      <c r="J89" s="31">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="90" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A90" s="20">
+        <v>43990</v>
+      </c>
+      <c r="B90" s="21">
+        <v>84130</v>
+      </c>
+      <c r="C90" s="22">
+        <v>814</v>
+      </c>
+      <c r="D90" s="22">
+        <v>1486</v>
+      </c>
+      <c r="E90" s="22">
+        <v>1</v>
+      </c>
+      <c r="F90" s="22">
+        <v>6</v>
+      </c>
+      <c r="G90" s="22">
+        <v>0</v>
+      </c>
+      <c r="H90" s="22">
+        <v>0</v>
+      </c>
+      <c r="I90" s="22">
+        <v>109</v>
+      </c>
+      <c r="J90" s="22">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="91" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A91" s="20">
+        <v>43991</v>
+      </c>
+      <c r="B91" s="21">
+        <v>84868</v>
+      </c>
+      <c r="C91" s="22">
+        <v>738</v>
+      </c>
+      <c r="D91" s="22">
+        <v>1488</v>
+      </c>
+      <c r="E91" s="22">
+        <v>2</v>
+      </c>
+      <c r="F91" s="22">
+        <v>6</v>
+      </c>
+      <c r="G91" s="22">
+        <v>0</v>
+      </c>
+      <c r="H91" s="22">
+        <v>0</v>
+      </c>
+      <c r="I91" s="22">
+        <v>109</v>
+      </c>
+      <c r="J91" s="22">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="92" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A92" s="23">
+        <v>43992</v>
+      </c>
+      <c r="B92" s="24">
+        <v>85626</v>
+      </c>
+      <c r="C92" s="25">
+        <v>758</v>
+      </c>
+      <c r="D92" s="25">
+        <v>1488</v>
+      </c>
+      <c r="E92" s="25">
+        <v>0</v>
+      </c>
+      <c r="F92" s="25">
+        <v>6</v>
+      </c>
+      <c r="G92" s="25">
+        <v>0</v>
+      </c>
+      <c r="H92" s="25">
+        <v>0</v>
+      </c>
+      <c r="I92" s="25">
+        <v>109</v>
+      </c>
+      <c r="J92" s="25">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="93" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A93" s="29">
+        <v>43993</v>
+      </c>
+      <c r="B93" s="30">
+        <v>86328</v>
+      </c>
+      <c r="C93" s="31">
+        <v>702</v>
+      </c>
+      <c r="D93" s="31">
+        <v>1490</v>
+      </c>
+      <c r="E93" s="31">
+        <v>2</v>
+      </c>
+      <c r="F93" s="31">
+        <v>6</v>
+      </c>
+      <c r="G93" s="31">
+        <v>0</v>
+      </c>
+      <c r="H93" s="31">
+        <v>0</v>
+      </c>
+      <c r="I93" s="31">
+        <v>109</v>
+      </c>
+      <c r="J93" s="31">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="94" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A94" s="23">
+        <v>43994</v>
+      </c>
+      <c r="B94" s="24">
+        <v>87095</v>
+      </c>
+      <c r="C94" s="25">
+        <v>767</v>
+      </c>
+      <c r="D94" s="25">
+        <v>1492</v>
+      </c>
+      <c r="E94" s="25">
+        <v>2</v>
+      </c>
+      <c r="F94" s="25">
+        <v>6</v>
+      </c>
+      <c r="G94" s="25">
+        <v>0</v>
+      </c>
+      <c r="H94" s="25">
+        <v>0</v>
+      </c>
+      <c r="I94" s="25">
+        <v>109</v>
+      </c>
+      <c r="J94" s="25">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="95" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A95" s="29">
+        <v>43995</v>
+      </c>
+      <c r="B95" s="30">
+        <v>87386</v>
+      </c>
+      <c r="C95" s="31">
+        <v>291</v>
+      </c>
+      <c r="D95" s="31">
+        <v>1495</v>
+      </c>
+      <c r="E95" s="31">
+        <v>3</v>
+      </c>
+      <c r="F95" s="31">
+        <v>6</v>
+      </c>
+      <c r="G95" s="31">
+        <v>0</v>
+      </c>
+      <c r="H95" s="31">
+        <v>0</v>
+      </c>
+      <c r="I95" s="31">
+        <v>109</v>
+      </c>
+      <c r="J95" s="31">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="96" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A96" s="23">
+        <v>43996</v>
+      </c>
+      <c r="B96" s="24">
+        <v>87598</v>
+      </c>
+      <c r="C96" s="25">
+        <v>212</v>
+      </c>
+      <c r="D96" s="25">
+        <v>1496</v>
+      </c>
+      <c r="E96" s="25">
+        <v>1</v>
+      </c>
+      <c r="F96" s="25">
+        <v>7</v>
+      </c>
+      <c r="G96" s="25">
+        <v>1</v>
+      </c>
+      <c r="H96" s="25">
+        <v>0</v>
+      </c>
+      <c r="I96" s="25">
+        <v>109</v>
+      </c>
+      <c r="J96" s="25">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="97" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A97" s="20">
+        <v>43997</v>
+      </c>
+      <c r="B97" s="21">
+        <v>88165</v>
+      </c>
+      <c r="C97" s="22">
+        <v>567</v>
+      </c>
+      <c r="D97" s="22">
+        <v>1499</v>
+      </c>
+      <c r="E97" s="22">
+        <v>3</v>
+      </c>
+      <c r="F97" s="22">
+        <v>7</v>
+      </c>
+      <c r="G97" s="22">
+        <v>1</v>
+      </c>
+      <c r="H97" s="22">
+        <v>0</v>
+      </c>
+      <c r="I97" s="22">
+        <v>109</v>
+      </c>
+      <c r="J97" s="22">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="98" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A98" s="20">
+        <v>43998</v>
+      </c>
+      <c r="B98" s="21">
+        <v>89151</v>
+      </c>
+      <c r="C98" s="22">
+        <v>986</v>
+      </c>
+      <c r="D98" s="22">
+        <v>1503</v>
+      </c>
+      <c r="E98" s="22">
+        <v>4</v>
+      </c>
+      <c r="F98" s="22">
+        <v>7</v>
+      </c>
+      <c r="G98" s="22">
+        <v>1</v>
+      </c>
+      <c r="H98" s="22">
+        <v>0</v>
+      </c>
+      <c r="I98" s="22">
+        <v>109</v>
+      </c>
+      <c r="J98" s="22">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="99" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A99" s="29">
+        <v>43999</v>
+      </c>
+      <c r="B99" s="30">
+        <v>90103</v>
+      </c>
+      <c r="C99" s="31">
+        <v>952</v>
+      </c>
+      <c r="D99" s="31">
+        <v>1511</v>
+      </c>
+      <c r="E99" s="31">
+        <v>8</v>
+      </c>
+      <c r="F99" s="31">
+        <v>6</v>
+      </c>
+      <c r="G99" s="31">
+        <v>1</v>
+      </c>
+      <c r="H99" s="31">
+        <v>1</v>
+      </c>
+      <c r="I99" s="31">
+        <v>109</v>
+      </c>
+      <c r="J99" s="31">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="100" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A100" s="20">
+        <v>44000</v>
+      </c>
+      <c r="B100" s="21">
+        <v>91005</v>
+      </c>
+      <c r="C100" s="22">
+        <v>902</v>
+      </c>
+      <c r="D100" s="22">
+        <v>1513</v>
+      </c>
+      <c r="E100" s="22">
+        <v>2</v>
+      </c>
+      <c r="F100" s="22">
+        <v>8</v>
+      </c>
+      <c r="G100" s="22">
+        <v>1</v>
+      </c>
+      <c r="H100" s="22">
+        <v>0</v>
+      </c>
+      <c r="I100" s="22">
+        <v>109</v>
+      </c>
+      <c r="J100" s="22">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="101" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A101" s="29">
+        <v>44001</v>
+      </c>
+      <c r="B101" s="30">
+        <v>92152</v>
+      </c>
+      <c r="C101" s="31">
+        <v>1147</v>
+      </c>
+      <c r="D101" s="31">
+        <v>1519</v>
+      </c>
+      <c r="E101" s="31">
+        <v>6</v>
+      </c>
+      <c r="F101" s="31">
+        <v>6</v>
+      </c>
+      <c r="G101" s="31">
+        <v>1</v>
+      </c>
+      <c r="H101" s="31">
+        <v>2</v>
+      </c>
+      <c r="I101" s="31">
+        <v>109</v>
+      </c>
+      <c r="J101" s="31">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="102" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A102" s="23">
+        <v>44002</v>
+      </c>
+      <c r="B102" s="24">
+        <v>92919</v>
+      </c>
+      <c r="C102" s="25">
+        <v>758</v>
+      </c>
+      <c r="D102" s="25">
+        <v>1520</v>
+      </c>
+      <c r="E102" s="25">
+        <v>1</v>
+      </c>
+      <c r="F102" s="25">
+        <v>6</v>
+      </c>
+      <c r="G102" s="25">
+        <v>1</v>
+      </c>
+      <c r="H102" s="25">
+        <v>2</v>
+      </c>
+      <c r="I102" s="25">
+        <v>109</v>
+      </c>
+      <c r="J102" s="25">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="103" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A103" s="29">
+        <v>44003</v>
+      </c>
+      <c r="B103" s="30">
+        <v>93181</v>
+      </c>
+      <c r="C103" s="31">
+        <v>271</v>
+      </c>
+      <c r="D103" s="31">
+        <v>1521</v>
+      </c>
+      <c r="E103" s="31">
+        <v>1</v>
+      </c>
+      <c r="F103" s="31">
+        <v>6</v>
+      </c>
+      <c r="G103" s="31">
+        <v>1</v>
+      </c>
+      <c r="H103" s="31">
+        <v>0</v>
+      </c>
+      <c r="I103" s="31">
+        <v>109</v>
+      </c>
+      <c r="J103" s="31">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="104" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A104" s="29">
+        <v>44004</v>
+      </c>
+      <c r="B104" s="30">
+        <v>94165</v>
+      </c>
+      <c r="C104" s="31">
+        <v>984</v>
+      </c>
+      <c r="D104" s="31">
+        <v>1534</v>
+      </c>
+      <c r="E104" s="31">
+        <v>13</v>
+      </c>
+      <c r="F104" s="31">
+        <v>5</v>
+      </c>
+      <c r="G104" s="31">
+        <v>1</v>
+      </c>
+      <c r="H104" s="31">
+        <v>1</v>
+      </c>
+      <c r="I104" s="31">
+        <v>109</v>
+      </c>
+      <c r="J104" s="31">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="105" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A105" s="29">
+        <v>44005</v>
+      </c>
+      <c r="B105" s="30">
+        <v>95387</v>
+      </c>
+      <c r="C105" s="31">
+        <v>1222</v>
+      </c>
+      <c r="D105" s="31">
+        <v>1541</v>
+      </c>
+      <c r="E105" s="31">
+        <v>7</v>
+      </c>
+      <c r="F105" s="31">
+        <v>7</v>
+      </c>
+      <c r="G105" s="31">
+        <v>2</v>
+      </c>
+      <c r="H105" s="31">
+        <v>0</v>
+      </c>
+      <c r="I105" s="31" t="s">
+        <v>10</v>
+      </c>
+      <c r="J105" s="31">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="106" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A106" s="23">
+        <v>44006</v>
+      </c>
+      <c r="B106" s="24">
+        <v>96599</v>
+      </c>
+      <c r="C106" s="25">
+        <v>1212</v>
+      </c>
+      <c r="D106" s="25">
+        <v>1547</v>
+      </c>
+      <c r="E106" s="25">
+        <v>6</v>
+      </c>
+      <c r="F106" s="25">
+        <v>7</v>
+      </c>
+      <c r="G106" s="25">
+        <v>2</v>
+      </c>
+      <c r="H106" s="25">
+        <v>0</v>
+      </c>
+      <c r="I106" s="25" t="s">
+        <v>10</v>
+      </c>
+      <c r="J106" s="25">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="107" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A107" s="29">
+        <v>44007</v>
+      </c>
+      <c r="B107" s="30">
+        <v>97442</v>
+      </c>
+      <c r="C107" s="31">
+        <v>843</v>
+      </c>
+      <c r="D107" s="31">
+        <v>1558</v>
+      </c>
+      <c r="E107" s="31">
+        <v>11</v>
+      </c>
+      <c r="F107" s="31">
+        <v>8</v>
+      </c>
+      <c r="G107" s="31">
+        <v>2</v>
+      </c>
+      <c r="H107" s="31">
+        <v>0</v>
+      </c>
+      <c r="I107" s="31" t="s">
+        <v>10</v>
+      </c>
+      <c r="J107" s="31">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="108" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A108" s="29">
+        <v>44008</v>
+      </c>
+      <c r="B108" s="30">
+        <v>98320</v>
+      </c>
+      <c r="C108" s="31">
+        <v>878</v>
+      </c>
+      <c r="D108" s="31">
+        <v>1572</v>
+      </c>
+      <c r="E108" s="31">
+        <v>14</v>
+      </c>
+      <c r="F108" s="31">
+        <v>8</v>
+      </c>
+      <c r="G108" s="31">
+        <v>1</v>
+      </c>
+      <c r="H108" s="31">
+        <v>0</v>
+      </c>
+      <c r="I108" s="31" t="s">
+        <v>10</v>
+      </c>
+      <c r="J108" s="31">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="109" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A109" s="29">
+        <v>44009</v>
+      </c>
+      <c r="B109" s="30">
+        <v>98945</v>
+      </c>
+      <c r="C109" s="31">
+        <v>625</v>
+      </c>
+      <c r="D109" s="31">
+        <v>1581</v>
+      </c>
+      <c r="E109" s="31">
+        <v>9</v>
+      </c>
+      <c r="F109" s="31">
+        <v>7</v>
+      </c>
+      <c r="G109" s="31">
+        <v>0</v>
+      </c>
+      <c r="H109" s="31">
+        <v>1</v>
+      </c>
+      <c r="I109" s="31" t="s">
+        <v>10</v>
+      </c>
+      <c r="J109" s="31">
+        <v>0</v>
+      </c>
+    </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>

</xml_diff>

<commit_message>
Data updated by GitHub Bot (2020-06-28 20)
</commit_message>
<xml_diff>
--- a/output/snapshot/fdcf2531-4c3e-5c02-b63c-ee160ead6dea.xlsx
+++ b/output/snapshot/fdcf2531-4c3e-5c02-b63c-ee160ead6dea.xlsx
@@ -1,16 +1,15 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="21929"/>
-  <workbookPr/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
+  <fileVersion appName="xl" lastEdited="6" lowestEdited="6" rupBuild="14420"/>
+  <workbookPr defaultThemeVersion="164011"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="I:\AKTUALNI PODATKI - KORONA\Za objavo na GOV.SI\ang\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{1E6DD62F-2BE2-47DC-A7ED-9B57C1589256}" xr6:coauthVersionLast="44" xr6:coauthVersionMax="44" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840"/>
   </bookViews>
   <sheets>
     <sheet name="Covid-19 podatki" sheetId="1" r:id="rId1"/>
@@ -25,7 +24,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="10" uniqueCount="10">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="15" uniqueCount="11">
   <si>
     <t>Date</t>
   </si>
@@ -56,15 +55,18 @@
   <si>
     <t>Deaths (daily)</t>
   </si>
+  <si>
+    <t>111*</t>
+  </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" mc:Ignorable="x14ac x16r2">
   <numFmts count="1">
     <numFmt numFmtId="164" formatCode="d/\ m/\ yyyy;@"/>
   </numFmts>
-  <fonts count="4" x14ac:knownFonts="1">
+  <fonts count="5" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -93,6 +95,13 @@
       <name val="Calibri Light"/>
       <scheme val="major"/>
     </font>
+    <font>
+      <sz val="10"/>
+      <color theme="1"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
   </fonts>
   <fills count="3">
     <fill>
@@ -108,7 +117,7 @@
       </patternFill>
     </fill>
   </fills>
-  <borders count="2">
+  <borders count="3">
     <border>
       <left/>
       <right/>
@@ -129,11 +138,26 @@
       <bottom/>
       <diagonal/>
     </border>
+    <border>
+      <left style="thin">
+        <color theme="4"/>
+      </left>
+      <right style="thin">
+        <color theme="4"/>
+      </right>
+      <top style="thin">
+        <color theme="4"/>
+      </top>
+      <bottom style="thin">
+        <color theme="4"/>
+      </bottom>
+      <diagonal/>
+    </border>
   </borders>
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="26">
+  <cellXfs count="32">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="49" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyAlignment="1" applyProtection="1">
       <alignment horizontal="left" vertical="top"/>
@@ -208,6 +232,24 @@
       <alignment horizontal="right"/>
     </xf>
     <xf numFmtId="0" fontId="3" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="right"/>
+    </xf>
+    <xf numFmtId="164" fontId="4" fillId="2" borderId="2" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="right" vertical="top"/>
+    </xf>
+    <xf numFmtId="3" fontId="4" fillId="2" borderId="2" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="right"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="2" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="right"/>
+    </xf>
+    <xf numFmtId="164" fontId="3" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="right" vertical="top"/>
+    </xf>
+    <xf numFmtId="3" fontId="3" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="right"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="right"/>
     </xf>
   </cellXfs>
@@ -399,8 +441,8 @@
 </file>
 
 <file path=xl/tables/table1.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="1" xr:uid="{00000000-000C-0000-FFFF-FFFF00000000}" name="Tabela1" displayName="Tabela1" ref="A1:J75" totalsRowShown="0" headerRowDxfId="11" dataDxfId="10">
-  <autoFilter ref="A1:J75" xr:uid="{00000000-0009-0000-0100-000001000000}">
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="1" name="Tabela1" displayName="Tabela1" ref="A1:J109" totalsRowShown="0" headerRowDxfId="11" dataDxfId="10">
+  <autoFilter ref="A1:J109">
     <filterColumn colId="0" hiddenButton="1"/>
     <filterColumn colId="1" hiddenButton="1"/>
     <filterColumn colId="2" hiddenButton="1"/>
@@ -413,16 +455,16 @@
     <filterColumn colId="9" hiddenButton="1"/>
   </autoFilter>
   <tableColumns count="10">
-    <tableColumn id="1" xr3:uid="{00000000-0010-0000-0000-000001000000}" name="Date" dataDxfId="9"/>
-    <tableColumn id="2" xr3:uid="{00000000-0010-0000-0000-000002000000}" name="Tested (all)" dataDxfId="8"/>
-    <tableColumn id="3" xr3:uid="{00000000-0010-0000-0000-000003000000}" name="Tested (daily)" dataDxfId="7"/>
-    <tableColumn id="4" xr3:uid="{00000000-0010-0000-0000-000004000000}" name="Positive (all)" dataDxfId="6"/>
-    <tableColumn id="5" xr3:uid="{00000000-0010-0000-0000-000005000000}" name="Positive (daily)" dataDxfId="5"/>
-    <tableColumn id="6" xr3:uid="{00000000-0010-0000-0000-000006000000}" name="All hospitalized on certain day" dataDxfId="4"/>
-    <tableColumn id="7" xr3:uid="{00000000-0010-0000-0000-000007000000}" name="All persons in intensive care on certain day" dataDxfId="3"/>
-    <tableColumn id="10" xr3:uid="{00000000-0010-0000-0000-00000A000000}" name="Discharged" dataDxfId="2"/>
-    <tableColumn id="8" xr3:uid="{00000000-0010-0000-0000-000008000000}" name="Deaths (all)" dataDxfId="1"/>
-    <tableColumn id="9" xr3:uid="{00000000-0010-0000-0000-000009000000}" name="Deaths (daily)" dataDxfId="0"/>
+    <tableColumn id="1" name="Date" dataDxfId="9"/>
+    <tableColumn id="2" name="Tested (all)" dataDxfId="8"/>
+    <tableColumn id="3" name="Tested (daily)" dataDxfId="7"/>
+    <tableColumn id="4" name="Positive (all)" dataDxfId="6"/>
+    <tableColumn id="5" name="Positive (daily)" dataDxfId="5"/>
+    <tableColumn id="6" name="All hospitalized on certain day" dataDxfId="4"/>
+    <tableColumn id="7" name="All persons in intensive care on certain day" dataDxfId="3"/>
+    <tableColumn id="10" name="Discharged" dataDxfId="2"/>
+    <tableColumn id="8" name="Deaths (all)" dataDxfId="1"/>
+    <tableColumn id="9" name="Deaths (daily)" dataDxfId="0"/>
   </tableColumns>
   <tableStyleInfo name="TableStyleLight16" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
   <extLst>
@@ -695,11 +737,11 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:J75"/>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <dimension ref="A1:J109"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A40" zoomScale="89" zoomScaleNormal="89" workbookViewId="0">
-      <selection activeCell="J74" sqref="J74"/>
+    <sheetView tabSelected="1" topLeftCell="A83" zoomScale="89" zoomScaleNormal="89" workbookViewId="0">
+      <selection activeCell="A109" sqref="A109"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -3117,6 +3159,1094 @@
         <v>0</v>
       </c>
     </row>
+    <row r="76" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A76" s="20">
+        <v>43976</v>
+      </c>
+      <c r="B76" s="21">
+        <v>75770</v>
+      </c>
+      <c r="C76" s="22">
+        <v>754</v>
+      </c>
+      <c r="D76" s="22">
+        <v>1469</v>
+      </c>
+      <c r="E76" s="22">
+        <v>0</v>
+      </c>
+      <c r="F76" s="22">
+        <v>9</v>
+      </c>
+      <c r="G76" s="22">
+        <v>2</v>
+      </c>
+      <c r="H76" s="22">
+        <v>6</v>
+      </c>
+      <c r="I76" s="22">
+        <v>108</v>
+      </c>
+      <c r="J76" s="22">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="77" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A77" s="20">
+        <v>43977</v>
+      </c>
+      <c r="B77" s="21">
+        <v>76579</v>
+      </c>
+      <c r="C77" s="22">
+        <v>809</v>
+      </c>
+      <c r="D77" s="22">
+        <v>1471</v>
+      </c>
+      <c r="E77" s="22">
+        <v>2</v>
+      </c>
+      <c r="F77" s="22">
+        <v>8</v>
+      </c>
+      <c r="G77" s="22">
+        <v>2</v>
+      </c>
+      <c r="H77" s="22">
+        <v>2</v>
+      </c>
+      <c r="I77" s="22">
+        <v>108</v>
+      </c>
+      <c r="J77" s="22">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="78" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A78" s="20">
+        <v>43978</v>
+      </c>
+      <c r="B78" s="21">
+        <v>77210</v>
+      </c>
+      <c r="C78" s="22">
+        <v>631</v>
+      </c>
+      <c r="D78" s="22">
+        <v>1473</v>
+      </c>
+      <c r="E78" s="22">
+        <v>2</v>
+      </c>
+      <c r="F78" s="22">
+        <v>7</v>
+      </c>
+      <c r="G78" s="22">
+        <v>2</v>
+      </c>
+      <c r="H78" s="22">
+        <v>1</v>
+      </c>
+      <c r="I78" s="22">
+        <v>108</v>
+      </c>
+      <c r="J78" s="22">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="79" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A79" s="20">
+        <v>43979</v>
+      </c>
+      <c r="B79" s="21">
+        <v>77916</v>
+      </c>
+      <c r="C79" s="22">
+        <v>706</v>
+      </c>
+      <c r="D79" s="22">
+        <v>1473</v>
+      </c>
+      <c r="E79" s="22">
+        <v>0</v>
+      </c>
+      <c r="F79" s="22">
+        <v>7</v>
+      </c>
+      <c r="G79" s="22">
+        <v>2</v>
+      </c>
+      <c r="H79" s="22">
+        <v>0</v>
+      </c>
+      <c r="I79" s="22">
+        <v>108</v>
+      </c>
+      <c r="J79" s="22">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="80" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A80" s="20">
+        <v>43980</v>
+      </c>
+      <c r="B80" s="21">
+        <v>78529</v>
+      </c>
+      <c r="C80" s="22">
+        <v>613</v>
+      </c>
+      <c r="D80" s="22">
+        <v>1473</v>
+      </c>
+      <c r="E80" s="22">
+        <v>0</v>
+      </c>
+      <c r="F80" s="22">
+        <v>7</v>
+      </c>
+      <c r="G80" s="22">
+        <v>2</v>
+      </c>
+      <c r="H80" s="22">
+        <v>0</v>
+      </c>
+      <c r="I80" s="22">
+        <v>108</v>
+      </c>
+      <c r="J80" s="22">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="81" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A81" s="20">
+        <v>43981</v>
+      </c>
+      <c r="B81" s="22">
+        <v>78793</v>
+      </c>
+      <c r="C81" s="22">
+        <v>264</v>
+      </c>
+      <c r="D81" s="22">
+        <v>1473</v>
+      </c>
+      <c r="E81" s="22">
+        <v>0</v>
+      </c>
+      <c r="F81" s="22">
+        <v>6</v>
+      </c>
+      <c r="G81" s="22">
+        <v>2</v>
+      </c>
+      <c r="H81" s="22">
+        <v>1</v>
+      </c>
+      <c r="I81" s="22">
+        <v>108</v>
+      </c>
+      <c r="J81" s="22">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="82" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A82" s="20">
+        <v>43982</v>
+      </c>
+      <c r="B82" s="21">
+        <v>79039</v>
+      </c>
+      <c r="C82" s="22">
+        <v>246</v>
+      </c>
+      <c r="D82" s="22">
+        <v>1473</v>
+      </c>
+      <c r="E82" s="22">
+        <v>0</v>
+      </c>
+      <c r="F82" s="22">
+        <v>5</v>
+      </c>
+      <c r="G82" s="22">
+        <v>1</v>
+      </c>
+      <c r="H82" s="22">
+        <v>0</v>
+      </c>
+      <c r="I82" s="22">
+        <v>109</v>
+      </c>
+      <c r="J82" s="22">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="83" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A83" s="20">
+        <v>43983</v>
+      </c>
+      <c r="B83" s="21">
+        <v>79698</v>
+      </c>
+      <c r="C83" s="22">
+        <v>659</v>
+      </c>
+      <c r="D83" s="22">
+        <v>1475</v>
+      </c>
+      <c r="E83" s="22">
+        <v>2</v>
+      </c>
+      <c r="F83" s="22">
+        <v>5</v>
+      </c>
+      <c r="G83" s="22">
+        <v>1</v>
+      </c>
+      <c r="H83" s="22">
+        <v>0</v>
+      </c>
+      <c r="I83" s="22">
+        <v>109</v>
+      </c>
+      <c r="J83" s="22">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="84" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A84" s="20">
+        <v>43984</v>
+      </c>
+      <c r="B84" s="21">
+        <v>80505</v>
+      </c>
+      <c r="C84" s="22">
+        <v>807</v>
+      </c>
+      <c r="D84" s="22">
+        <v>1477</v>
+      </c>
+      <c r="E84" s="22">
+        <v>2</v>
+      </c>
+      <c r="F84" s="22">
+        <v>5</v>
+      </c>
+      <c r="G84" s="22">
+        <v>0</v>
+      </c>
+      <c r="H84" s="22">
+        <v>0</v>
+      </c>
+      <c r="I84" s="22">
+        <v>109</v>
+      </c>
+      <c r="J84" s="22">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="85" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A85" s="20">
+        <v>43985</v>
+      </c>
+      <c r="B85" s="21">
+        <v>81333</v>
+      </c>
+      <c r="C85" s="22">
+        <v>828</v>
+      </c>
+      <c r="D85" s="22">
+        <v>1477</v>
+      </c>
+      <c r="E85" s="22">
+        <v>0</v>
+      </c>
+      <c r="F85" s="22">
+        <v>5</v>
+      </c>
+      <c r="G85" s="22">
+        <v>0</v>
+      </c>
+      <c r="H85" s="22">
+        <v>0</v>
+      </c>
+      <c r="I85" s="22">
+        <v>109</v>
+      </c>
+      <c r="J85" s="22">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="86" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A86" s="26">
+        <v>43986</v>
+      </c>
+      <c r="B86" s="27">
+        <v>82161</v>
+      </c>
+      <c r="C86" s="28">
+        <v>828</v>
+      </c>
+      <c r="D86" s="28">
+        <v>1479</v>
+      </c>
+      <c r="E86" s="28">
+        <v>2</v>
+      </c>
+      <c r="F86" s="28">
+        <v>6</v>
+      </c>
+      <c r="G86" s="28">
+        <v>0</v>
+      </c>
+      <c r="H86" s="28">
+        <v>0</v>
+      </c>
+      <c r="I86" s="28">
+        <v>109</v>
+      </c>
+      <c r="J86" s="28">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="87" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A87" s="29">
+        <v>43987</v>
+      </c>
+      <c r="B87" s="30">
+        <v>82876</v>
+      </c>
+      <c r="C87" s="31">
+        <v>715</v>
+      </c>
+      <c r="D87" s="31">
+        <v>1484</v>
+      </c>
+      <c r="E87" s="31">
+        <v>5</v>
+      </c>
+      <c r="F87" s="31">
+        <v>6</v>
+      </c>
+      <c r="G87" s="31">
+        <v>0</v>
+      </c>
+      <c r="H87" s="31">
+        <v>0</v>
+      </c>
+      <c r="I87" s="31">
+        <v>109</v>
+      </c>
+      <c r="J87" s="31">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="88" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A88" s="23">
+        <v>43988</v>
+      </c>
+      <c r="B88" s="24">
+        <v>83105</v>
+      </c>
+      <c r="C88" s="25">
+        <v>229</v>
+      </c>
+      <c r="D88" s="25">
+        <v>1485</v>
+      </c>
+      <c r="E88" s="25">
+        <v>1</v>
+      </c>
+      <c r="F88" s="25">
+        <v>5</v>
+      </c>
+      <c r="G88" s="25">
+        <v>0</v>
+      </c>
+      <c r="H88" s="25">
+        <v>1</v>
+      </c>
+      <c r="I88" s="25">
+        <v>109</v>
+      </c>
+      <c r="J88" s="25">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="89" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A89" s="29">
+        <v>43989</v>
+      </c>
+      <c r="B89" s="30">
+        <v>83316</v>
+      </c>
+      <c r="C89" s="31">
+        <v>211</v>
+      </c>
+      <c r="D89" s="31">
+        <v>1485</v>
+      </c>
+      <c r="E89" s="31">
+        <v>0</v>
+      </c>
+      <c r="F89" s="31">
+        <v>5</v>
+      </c>
+      <c r="G89" s="31">
+        <v>0</v>
+      </c>
+      <c r="H89" s="31">
+        <v>0</v>
+      </c>
+      <c r="I89" s="31">
+        <v>109</v>
+      </c>
+      <c r="J89" s="31">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="90" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A90" s="20">
+        <v>43990</v>
+      </c>
+      <c r="B90" s="21">
+        <v>84130</v>
+      </c>
+      <c r="C90" s="22">
+        <v>814</v>
+      </c>
+      <c r="D90" s="22">
+        <v>1486</v>
+      </c>
+      <c r="E90" s="22">
+        <v>1</v>
+      </c>
+      <c r="F90" s="22">
+        <v>6</v>
+      </c>
+      <c r="G90" s="22">
+        <v>0</v>
+      </c>
+      <c r="H90" s="22">
+        <v>0</v>
+      </c>
+      <c r="I90" s="22">
+        <v>109</v>
+      </c>
+      <c r="J90" s="22">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="91" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A91" s="20">
+        <v>43991</v>
+      </c>
+      <c r="B91" s="21">
+        <v>84868</v>
+      </c>
+      <c r="C91" s="22">
+        <v>738</v>
+      </c>
+      <c r="D91" s="22">
+        <v>1488</v>
+      </c>
+      <c r="E91" s="22">
+        <v>2</v>
+      </c>
+      <c r="F91" s="22">
+        <v>6</v>
+      </c>
+      <c r="G91" s="22">
+        <v>0</v>
+      </c>
+      <c r="H91" s="22">
+        <v>0</v>
+      </c>
+      <c r="I91" s="22">
+        <v>109</v>
+      </c>
+      <c r="J91" s="22">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="92" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A92" s="23">
+        <v>43992</v>
+      </c>
+      <c r="B92" s="24">
+        <v>85626</v>
+      </c>
+      <c r="C92" s="25">
+        <v>758</v>
+      </c>
+      <c r="D92" s="25">
+        <v>1488</v>
+      </c>
+      <c r="E92" s="25">
+        <v>0</v>
+      </c>
+      <c r="F92" s="25">
+        <v>6</v>
+      </c>
+      <c r="G92" s="25">
+        <v>0</v>
+      </c>
+      <c r="H92" s="25">
+        <v>0</v>
+      </c>
+      <c r="I92" s="25">
+        <v>109</v>
+      </c>
+      <c r="J92" s="25">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="93" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A93" s="29">
+        <v>43993</v>
+      </c>
+      <c r="B93" s="30">
+        <v>86328</v>
+      </c>
+      <c r="C93" s="31">
+        <v>702</v>
+      </c>
+      <c r="D93" s="31">
+        <v>1490</v>
+      </c>
+      <c r="E93" s="31">
+        <v>2</v>
+      </c>
+      <c r="F93" s="31">
+        <v>6</v>
+      </c>
+      <c r="G93" s="31">
+        <v>0</v>
+      </c>
+      <c r="H93" s="31">
+        <v>0</v>
+      </c>
+      <c r="I93" s="31">
+        <v>109</v>
+      </c>
+      <c r="J93" s="31">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="94" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A94" s="23">
+        <v>43994</v>
+      </c>
+      <c r="B94" s="24">
+        <v>87095</v>
+      </c>
+      <c r="C94" s="25">
+        <v>767</v>
+      </c>
+      <c r="D94" s="25">
+        <v>1492</v>
+      </c>
+      <c r="E94" s="25">
+        <v>2</v>
+      </c>
+      <c r="F94" s="25">
+        <v>6</v>
+      </c>
+      <c r="G94" s="25">
+        <v>0</v>
+      </c>
+      <c r="H94" s="25">
+        <v>0</v>
+      </c>
+      <c r="I94" s="25">
+        <v>109</v>
+      </c>
+      <c r="J94" s="25">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="95" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A95" s="29">
+        <v>43995</v>
+      </c>
+      <c r="B95" s="30">
+        <v>87386</v>
+      </c>
+      <c r="C95" s="31">
+        <v>291</v>
+      </c>
+      <c r="D95" s="31">
+        <v>1495</v>
+      </c>
+      <c r="E95" s="31">
+        <v>3</v>
+      </c>
+      <c r="F95" s="31">
+        <v>6</v>
+      </c>
+      <c r="G95" s="31">
+        <v>0</v>
+      </c>
+      <c r="H95" s="31">
+        <v>0</v>
+      </c>
+      <c r="I95" s="31">
+        <v>109</v>
+      </c>
+      <c r="J95" s="31">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="96" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A96" s="23">
+        <v>43996</v>
+      </c>
+      <c r="B96" s="24">
+        <v>87598</v>
+      </c>
+      <c r="C96" s="25">
+        <v>212</v>
+      </c>
+      <c r="D96" s="25">
+        <v>1496</v>
+      </c>
+      <c r="E96" s="25">
+        <v>1</v>
+      </c>
+      <c r="F96" s="25">
+        <v>7</v>
+      </c>
+      <c r="G96" s="25">
+        <v>1</v>
+      </c>
+      <c r="H96" s="25">
+        <v>0</v>
+      </c>
+      <c r="I96" s="25">
+        <v>109</v>
+      </c>
+      <c r="J96" s="25">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="97" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A97" s="20">
+        <v>43997</v>
+      </c>
+      <c r="B97" s="21">
+        <v>88165</v>
+      </c>
+      <c r="C97" s="22">
+        <v>567</v>
+      </c>
+      <c r="D97" s="22">
+        <v>1499</v>
+      </c>
+      <c r="E97" s="22">
+        <v>3</v>
+      </c>
+      <c r="F97" s="22">
+        <v>7</v>
+      </c>
+      <c r="G97" s="22">
+        <v>1</v>
+      </c>
+      <c r="H97" s="22">
+        <v>0</v>
+      </c>
+      <c r="I97" s="22">
+        <v>109</v>
+      </c>
+      <c r="J97" s="22">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="98" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A98" s="20">
+        <v>43998</v>
+      </c>
+      <c r="B98" s="21">
+        <v>89151</v>
+      </c>
+      <c r="C98" s="22">
+        <v>986</v>
+      </c>
+      <c r="D98" s="22">
+        <v>1503</v>
+      </c>
+      <c r="E98" s="22">
+        <v>4</v>
+      </c>
+      <c r="F98" s="22">
+        <v>7</v>
+      </c>
+      <c r="G98" s="22">
+        <v>1</v>
+      </c>
+      <c r="H98" s="22">
+        <v>0</v>
+      </c>
+      <c r="I98" s="22">
+        <v>109</v>
+      </c>
+      <c r="J98" s="22">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="99" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A99" s="29">
+        <v>43999</v>
+      </c>
+      <c r="B99" s="30">
+        <v>90103</v>
+      </c>
+      <c r="C99" s="31">
+        <v>952</v>
+      </c>
+      <c r="D99" s="31">
+        <v>1511</v>
+      </c>
+      <c r="E99" s="31">
+        <v>8</v>
+      </c>
+      <c r="F99" s="31">
+        <v>6</v>
+      </c>
+      <c r="G99" s="31">
+        <v>1</v>
+      </c>
+      <c r="H99" s="31">
+        <v>1</v>
+      </c>
+      <c r="I99" s="31">
+        <v>109</v>
+      </c>
+      <c r="J99" s="31">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="100" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A100" s="20">
+        <v>44000</v>
+      </c>
+      <c r="B100" s="21">
+        <v>91005</v>
+      </c>
+      <c r="C100" s="22">
+        <v>902</v>
+      </c>
+      <c r="D100" s="22">
+        <v>1513</v>
+      </c>
+      <c r="E100" s="22">
+        <v>2</v>
+      </c>
+      <c r="F100" s="22">
+        <v>8</v>
+      </c>
+      <c r="G100" s="22">
+        <v>1</v>
+      </c>
+      <c r="H100" s="22">
+        <v>0</v>
+      </c>
+      <c r="I100" s="22">
+        <v>109</v>
+      </c>
+      <c r="J100" s="22">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="101" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A101" s="29">
+        <v>44001</v>
+      </c>
+      <c r="B101" s="30">
+        <v>92152</v>
+      </c>
+      <c r="C101" s="31">
+        <v>1147</v>
+      </c>
+      <c r="D101" s="31">
+        <v>1519</v>
+      </c>
+      <c r="E101" s="31">
+        <v>6</v>
+      </c>
+      <c r="F101" s="31">
+        <v>6</v>
+      </c>
+      <c r="G101" s="31">
+        <v>1</v>
+      </c>
+      <c r="H101" s="31">
+        <v>2</v>
+      </c>
+      <c r="I101" s="31">
+        <v>109</v>
+      </c>
+      <c r="J101" s="31">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="102" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A102" s="23">
+        <v>44002</v>
+      </c>
+      <c r="B102" s="24">
+        <v>92919</v>
+      </c>
+      <c r="C102" s="25">
+        <v>758</v>
+      </c>
+      <c r="D102" s="25">
+        <v>1520</v>
+      </c>
+      <c r="E102" s="25">
+        <v>1</v>
+      </c>
+      <c r="F102" s="25">
+        <v>6</v>
+      </c>
+      <c r="G102" s="25">
+        <v>1</v>
+      </c>
+      <c r="H102" s="25">
+        <v>2</v>
+      </c>
+      <c r="I102" s="25">
+        <v>109</v>
+      </c>
+      <c r="J102" s="25">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="103" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A103" s="29">
+        <v>44003</v>
+      </c>
+      <c r="B103" s="30">
+        <v>93181</v>
+      </c>
+      <c r="C103" s="31">
+        <v>271</v>
+      </c>
+      <c r="D103" s="31">
+        <v>1521</v>
+      </c>
+      <c r="E103" s="31">
+        <v>1</v>
+      </c>
+      <c r="F103" s="31">
+        <v>6</v>
+      </c>
+      <c r="G103" s="31">
+        <v>1</v>
+      </c>
+      <c r="H103" s="31">
+        <v>0</v>
+      </c>
+      <c r="I103" s="31">
+        <v>109</v>
+      </c>
+      <c r="J103" s="31">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="104" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A104" s="29">
+        <v>44004</v>
+      </c>
+      <c r="B104" s="30">
+        <v>94165</v>
+      </c>
+      <c r="C104" s="31">
+        <v>984</v>
+      </c>
+      <c r="D104" s="31">
+        <v>1534</v>
+      </c>
+      <c r="E104" s="31">
+        <v>13</v>
+      </c>
+      <c r="F104" s="31">
+        <v>5</v>
+      </c>
+      <c r="G104" s="31">
+        <v>1</v>
+      </c>
+      <c r="H104" s="31">
+        <v>1</v>
+      </c>
+      <c r="I104" s="31">
+        <v>109</v>
+      </c>
+      <c r="J104" s="31">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="105" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A105" s="29">
+        <v>44005</v>
+      </c>
+      <c r="B105" s="30">
+        <v>95387</v>
+      </c>
+      <c r="C105" s="31">
+        <v>1222</v>
+      </c>
+      <c r="D105" s="31">
+        <v>1541</v>
+      </c>
+      <c r="E105" s="31">
+        <v>7</v>
+      </c>
+      <c r="F105" s="31">
+        <v>7</v>
+      </c>
+      <c r="G105" s="31">
+        <v>2</v>
+      </c>
+      <c r="H105" s="31">
+        <v>0</v>
+      </c>
+      <c r="I105" s="31" t="s">
+        <v>10</v>
+      </c>
+      <c r="J105" s="31">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="106" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A106" s="23">
+        <v>44006</v>
+      </c>
+      <c r="B106" s="24">
+        <v>96599</v>
+      </c>
+      <c r="C106" s="25">
+        <v>1212</v>
+      </c>
+      <c r="D106" s="25">
+        <v>1547</v>
+      </c>
+      <c r="E106" s="25">
+        <v>6</v>
+      </c>
+      <c r="F106" s="25">
+        <v>7</v>
+      </c>
+      <c r="G106" s="25">
+        <v>2</v>
+      </c>
+      <c r="H106" s="25">
+        <v>0</v>
+      </c>
+      <c r="I106" s="25" t="s">
+        <v>10</v>
+      </c>
+      <c r="J106" s="25">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="107" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A107" s="29">
+        <v>44007</v>
+      </c>
+      <c r="B107" s="30">
+        <v>97442</v>
+      </c>
+      <c r="C107" s="31">
+        <v>843</v>
+      </c>
+      <c r="D107" s="31">
+        <v>1558</v>
+      </c>
+      <c r="E107" s="31">
+        <v>11</v>
+      </c>
+      <c r="F107" s="31">
+        <v>8</v>
+      </c>
+      <c r="G107" s="31">
+        <v>2</v>
+      </c>
+      <c r="H107" s="31">
+        <v>0</v>
+      </c>
+      <c r="I107" s="31" t="s">
+        <v>10</v>
+      </c>
+      <c r="J107" s="31">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="108" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A108" s="29">
+        <v>44008</v>
+      </c>
+      <c r="B108" s="30">
+        <v>98320</v>
+      </c>
+      <c r="C108" s="31">
+        <v>878</v>
+      </c>
+      <c r="D108" s="31">
+        <v>1572</v>
+      </c>
+      <c r="E108" s="31">
+        <v>14</v>
+      </c>
+      <c r="F108" s="31">
+        <v>8</v>
+      </c>
+      <c r="G108" s="31">
+        <v>1</v>
+      </c>
+      <c r="H108" s="31">
+        <v>0</v>
+      </c>
+      <c r="I108" s="31" t="s">
+        <v>10</v>
+      </c>
+      <c r="J108" s="31">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="109" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A109" s="29">
+        <v>44009</v>
+      </c>
+      <c r="B109" s="30">
+        <v>98945</v>
+      </c>
+      <c r="C109" s="31">
+        <v>625</v>
+      </c>
+      <c r="D109" s="31">
+        <v>1581</v>
+      </c>
+      <c r="E109" s="31">
+        <v>9</v>
+      </c>
+      <c r="F109" s="31">
+        <v>7</v>
+      </c>
+      <c r="G109" s="31">
+        <v>0</v>
+      </c>
+      <c r="H109" s="31">
+        <v>1</v>
+      </c>
+      <c r="I109" s="31" t="s">
+        <v>10</v>
+      </c>
+      <c r="J109" s="31">
+        <v>0</v>
+      </c>
+    </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>

</xml_diff>

<commit_message>
Data updated by GitHub Bot (2020-06-29 12)
</commit_message>
<xml_diff>
--- a/output/snapshot/fdcf2531-4c3e-5c02-b63c-ee160ead6dea.xlsx
+++ b/output/snapshot/fdcf2531-4c3e-5c02-b63c-ee160ead6dea.xlsx
@@ -1,16 +1,15 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="21929"/>
-  <workbookPr/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
+  <fileVersion appName="xl" lastEdited="6" lowestEdited="6" rupBuild="14420"/>
+  <workbookPr defaultThemeVersion="164011"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="I:\AKTUALNI PODATKI - KORONA\Za objavo na GOV.SI\ang\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{1E6DD62F-2BE2-47DC-A7ED-9B57C1589256}" xr6:coauthVersionLast="44" xr6:coauthVersionMax="44" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840"/>
   </bookViews>
   <sheets>
     <sheet name="Covid-19 podatki" sheetId="1" r:id="rId1"/>
@@ -25,7 +24,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="10" uniqueCount="10">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="16" uniqueCount="11">
   <si>
     <t>Date</t>
   </si>
@@ -56,15 +55,18 @@
   <si>
     <t>Deaths (daily)</t>
   </si>
+  <si>
+    <t>111*</t>
+  </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" mc:Ignorable="x14ac x16r2">
   <numFmts count="1">
     <numFmt numFmtId="164" formatCode="d/\ m/\ yyyy;@"/>
   </numFmts>
-  <fonts count="4" x14ac:knownFonts="1">
+  <fonts count="5" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -93,6 +95,13 @@
       <name val="Calibri Light"/>
       <scheme val="major"/>
     </font>
+    <font>
+      <sz val="10"/>
+      <color theme="1"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
   </fonts>
   <fills count="3">
     <fill>
@@ -108,7 +117,7 @@
       </patternFill>
     </fill>
   </fills>
-  <borders count="2">
+  <borders count="3">
     <border>
       <left/>
       <right/>
@@ -129,11 +138,26 @@
       <bottom/>
       <diagonal/>
     </border>
+    <border>
+      <left style="thin">
+        <color theme="4"/>
+      </left>
+      <right style="thin">
+        <color theme="4"/>
+      </right>
+      <top style="thin">
+        <color theme="4"/>
+      </top>
+      <bottom style="thin">
+        <color theme="4"/>
+      </bottom>
+      <diagonal/>
+    </border>
   </borders>
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="26">
+  <cellXfs count="32">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="49" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyAlignment="1" applyProtection="1">
       <alignment horizontal="left" vertical="top"/>
@@ -208,6 +232,24 @@
       <alignment horizontal="right"/>
     </xf>
     <xf numFmtId="0" fontId="3" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="right"/>
+    </xf>
+    <xf numFmtId="164" fontId="4" fillId="2" borderId="2" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="right" vertical="top"/>
+    </xf>
+    <xf numFmtId="3" fontId="4" fillId="2" borderId="2" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="right"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="2" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="right"/>
+    </xf>
+    <xf numFmtId="164" fontId="3" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="right" vertical="top"/>
+    </xf>
+    <xf numFmtId="3" fontId="3" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="right"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="right"/>
     </xf>
   </cellXfs>
@@ -399,8 +441,8 @@
 </file>
 
 <file path=xl/tables/table1.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="1" xr:uid="{00000000-000C-0000-FFFF-FFFF00000000}" name="Tabela1" displayName="Tabela1" ref="A1:J75" totalsRowShown="0" headerRowDxfId="11" dataDxfId="10">
-  <autoFilter ref="A1:J75" xr:uid="{00000000-0009-0000-0100-000001000000}">
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="1" name="Tabela1" displayName="Tabela1" ref="A1:J110" totalsRowShown="0" headerRowDxfId="11" dataDxfId="10">
+  <autoFilter ref="A1:J110">
     <filterColumn colId="0" hiddenButton="1"/>
     <filterColumn colId="1" hiddenButton="1"/>
     <filterColumn colId="2" hiddenButton="1"/>
@@ -413,16 +455,16 @@
     <filterColumn colId="9" hiddenButton="1"/>
   </autoFilter>
   <tableColumns count="10">
-    <tableColumn id="1" xr3:uid="{00000000-0010-0000-0000-000001000000}" name="Date" dataDxfId="9"/>
-    <tableColumn id="2" xr3:uid="{00000000-0010-0000-0000-000002000000}" name="Tested (all)" dataDxfId="8"/>
-    <tableColumn id="3" xr3:uid="{00000000-0010-0000-0000-000003000000}" name="Tested (daily)" dataDxfId="7"/>
-    <tableColumn id="4" xr3:uid="{00000000-0010-0000-0000-000004000000}" name="Positive (all)" dataDxfId="6"/>
-    <tableColumn id="5" xr3:uid="{00000000-0010-0000-0000-000005000000}" name="Positive (daily)" dataDxfId="5"/>
-    <tableColumn id="6" xr3:uid="{00000000-0010-0000-0000-000006000000}" name="All hospitalized on certain day" dataDxfId="4"/>
-    <tableColumn id="7" xr3:uid="{00000000-0010-0000-0000-000007000000}" name="All persons in intensive care on certain day" dataDxfId="3"/>
-    <tableColumn id="10" xr3:uid="{00000000-0010-0000-0000-00000A000000}" name="Discharged" dataDxfId="2"/>
-    <tableColumn id="8" xr3:uid="{00000000-0010-0000-0000-000008000000}" name="Deaths (all)" dataDxfId="1"/>
-    <tableColumn id="9" xr3:uid="{00000000-0010-0000-0000-000009000000}" name="Deaths (daily)" dataDxfId="0"/>
+    <tableColumn id="1" name="Date" dataDxfId="9"/>
+    <tableColumn id="2" name="Tested (all)" dataDxfId="8"/>
+    <tableColumn id="3" name="Tested (daily)" dataDxfId="7"/>
+    <tableColumn id="4" name="Positive (all)" dataDxfId="6"/>
+    <tableColumn id="5" name="Positive (daily)" dataDxfId="5"/>
+    <tableColumn id="6" name="All hospitalized on certain day" dataDxfId="4"/>
+    <tableColumn id="7" name="All persons in intensive care on certain day" dataDxfId="3"/>
+    <tableColumn id="10" name="Discharged" dataDxfId="2"/>
+    <tableColumn id="8" name="Deaths (all)" dataDxfId="1"/>
+    <tableColumn id="9" name="Deaths (daily)" dataDxfId="0"/>
   </tableColumns>
   <tableStyleInfo name="TableStyleLight16" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
   <extLst>
@@ -695,11 +737,11 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:J75"/>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <dimension ref="A1:J110"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A40" zoomScale="89" zoomScaleNormal="89" workbookViewId="0">
-      <selection activeCell="J74" sqref="J74"/>
+    <sheetView tabSelected="1" topLeftCell="A83" zoomScale="89" zoomScaleNormal="89" workbookViewId="0">
+      <selection activeCell="I110" sqref="I110"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -3117,6 +3159,1126 @@
         <v>0</v>
       </c>
     </row>
+    <row r="76" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A76" s="20">
+        <v>43976</v>
+      </c>
+      <c r="B76" s="21">
+        <v>75770</v>
+      </c>
+      <c r="C76" s="22">
+        <v>754</v>
+      </c>
+      <c r="D76" s="22">
+        <v>1469</v>
+      </c>
+      <c r="E76" s="22">
+        <v>0</v>
+      </c>
+      <c r="F76" s="22">
+        <v>9</v>
+      </c>
+      <c r="G76" s="22">
+        <v>2</v>
+      </c>
+      <c r="H76" s="22">
+        <v>6</v>
+      </c>
+      <c r="I76" s="22">
+        <v>108</v>
+      </c>
+      <c r="J76" s="22">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="77" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A77" s="20">
+        <v>43977</v>
+      </c>
+      <c r="B77" s="21">
+        <v>76579</v>
+      </c>
+      <c r="C77" s="22">
+        <v>809</v>
+      </c>
+      <c r="D77" s="22">
+        <v>1471</v>
+      </c>
+      <c r="E77" s="22">
+        <v>2</v>
+      </c>
+      <c r="F77" s="22">
+        <v>8</v>
+      </c>
+      <c r="G77" s="22">
+        <v>2</v>
+      </c>
+      <c r="H77" s="22">
+        <v>2</v>
+      </c>
+      <c r="I77" s="22">
+        <v>108</v>
+      </c>
+      <c r="J77" s="22">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="78" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A78" s="20">
+        <v>43978</v>
+      </c>
+      <c r="B78" s="21">
+        <v>77210</v>
+      </c>
+      <c r="C78" s="22">
+        <v>631</v>
+      </c>
+      <c r="D78" s="22">
+        <v>1473</v>
+      </c>
+      <c r="E78" s="22">
+        <v>2</v>
+      </c>
+      <c r="F78" s="22">
+        <v>7</v>
+      </c>
+      <c r="G78" s="22">
+        <v>2</v>
+      </c>
+      <c r="H78" s="22">
+        <v>1</v>
+      </c>
+      <c r="I78" s="22">
+        <v>108</v>
+      </c>
+      <c r="J78" s="22">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="79" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A79" s="20">
+        <v>43979</v>
+      </c>
+      <c r="B79" s="21">
+        <v>77916</v>
+      </c>
+      <c r="C79" s="22">
+        <v>706</v>
+      </c>
+      <c r="D79" s="22">
+        <v>1473</v>
+      </c>
+      <c r="E79" s="22">
+        <v>0</v>
+      </c>
+      <c r="F79" s="22">
+        <v>7</v>
+      </c>
+      <c r="G79" s="22">
+        <v>2</v>
+      </c>
+      <c r="H79" s="22">
+        <v>0</v>
+      </c>
+      <c r="I79" s="22">
+        <v>108</v>
+      </c>
+      <c r="J79" s="22">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="80" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A80" s="20">
+        <v>43980</v>
+      </c>
+      <c r="B80" s="21">
+        <v>78529</v>
+      </c>
+      <c r="C80" s="22">
+        <v>613</v>
+      </c>
+      <c r="D80" s="22">
+        <v>1473</v>
+      </c>
+      <c r="E80" s="22">
+        <v>0</v>
+      </c>
+      <c r="F80" s="22">
+        <v>7</v>
+      </c>
+      <c r="G80" s="22">
+        <v>2</v>
+      </c>
+      <c r="H80" s="22">
+        <v>0</v>
+      </c>
+      <c r="I80" s="22">
+        <v>108</v>
+      </c>
+      <c r="J80" s="22">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="81" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A81" s="20">
+        <v>43981</v>
+      </c>
+      <c r="B81" s="22">
+        <v>78793</v>
+      </c>
+      <c r="C81" s="22">
+        <v>264</v>
+      </c>
+      <c r="D81" s="22">
+        <v>1473</v>
+      </c>
+      <c r="E81" s="22">
+        <v>0</v>
+      </c>
+      <c r="F81" s="22">
+        <v>6</v>
+      </c>
+      <c r="G81" s="22">
+        <v>2</v>
+      </c>
+      <c r="H81" s="22">
+        <v>1</v>
+      </c>
+      <c r="I81" s="22">
+        <v>108</v>
+      </c>
+      <c r="J81" s="22">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="82" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A82" s="20">
+        <v>43982</v>
+      </c>
+      <c r="B82" s="21">
+        <v>79039</v>
+      </c>
+      <c r="C82" s="22">
+        <v>246</v>
+      </c>
+      <c r="D82" s="22">
+        <v>1473</v>
+      </c>
+      <c r="E82" s="22">
+        <v>0</v>
+      </c>
+      <c r="F82" s="22">
+        <v>5</v>
+      </c>
+      <c r="G82" s="22">
+        <v>1</v>
+      </c>
+      <c r="H82" s="22">
+        <v>0</v>
+      </c>
+      <c r="I82" s="22">
+        <v>109</v>
+      </c>
+      <c r="J82" s="22">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="83" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A83" s="20">
+        <v>43983</v>
+      </c>
+      <c r="B83" s="21">
+        <v>79698</v>
+      </c>
+      <c r="C83" s="22">
+        <v>659</v>
+      </c>
+      <c r="D83" s="22">
+        <v>1475</v>
+      </c>
+      <c r="E83" s="22">
+        <v>2</v>
+      </c>
+      <c r="F83" s="22">
+        <v>5</v>
+      </c>
+      <c r="G83" s="22">
+        <v>1</v>
+      </c>
+      <c r="H83" s="22">
+        <v>0</v>
+      </c>
+      <c r="I83" s="22">
+        <v>109</v>
+      </c>
+      <c r="J83" s="22">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="84" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A84" s="20">
+        <v>43984</v>
+      </c>
+      <c r="B84" s="21">
+        <v>80505</v>
+      </c>
+      <c r="C84" s="22">
+        <v>807</v>
+      </c>
+      <c r="D84" s="22">
+        <v>1477</v>
+      </c>
+      <c r="E84" s="22">
+        <v>2</v>
+      </c>
+      <c r="F84" s="22">
+        <v>5</v>
+      </c>
+      <c r="G84" s="22">
+        <v>0</v>
+      </c>
+      <c r="H84" s="22">
+        <v>0</v>
+      </c>
+      <c r="I84" s="22">
+        <v>109</v>
+      </c>
+      <c r="J84" s="22">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="85" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A85" s="20">
+        <v>43985</v>
+      </c>
+      <c r="B85" s="21">
+        <v>81333</v>
+      </c>
+      <c r="C85" s="22">
+        <v>828</v>
+      </c>
+      <c r="D85" s="22">
+        <v>1477</v>
+      </c>
+      <c r="E85" s="22">
+        <v>0</v>
+      </c>
+      <c r="F85" s="22">
+        <v>5</v>
+      </c>
+      <c r="G85" s="22">
+        <v>0</v>
+      </c>
+      <c r="H85" s="22">
+        <v>0</v>
+      </c>
+      <c r="I85" s="22">
+        <v>109</v>
+      </c>
+      <c r="J85" s="22">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="86" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A86" s="26">
+        <v>43986</v>
+      </c>
+      <c r="B86" s="27">
+        <v>82161</v>
+      </c>
+      <c r="C86" s="28">
+        <v>828</v>
+      </c>
+      <c r="D86" s="28">
+        <v>1479</v>
+      </c>
+      <c r="E86" s="28">
+        <v>2</v>
+      </c>
+      <c r="F86" s="28">
+        <v>6</v>
+      </c>
+      <c r="G86" s="28">
+        <v>0</v>
+      </c>
+      <c r="H86" s="28">
+        <v>0</v>
+      </c>
+      <c r="I86" s="28">
+        <v>109</v>
+      </c>
+      <c r="J86" s="28">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="87" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A87" s="29">
+        <v>43987</v>
+      </c>
+      <c r="B87" s="30">
+        <v>82876</v>
+      </c>
+      <c r="C87" s="31">
+        <v>715</v>
+      </c>
+      <c r="D87" s="31">
+        <v>1484</v>
+      </c>
+      <c r="E87" s="31">
+        <v>5</v>
+      </c>
+      <c r="F87" s="31">
+        <v>6</v>
+      </c>
+      <c r="G87" s="31">
+        <v>0</v>
+      </c>
+      <c r="H87" s="31">
+        <v>0</v>
+      </c>
+      <c r="I87" s="31">
+        <v>109</v>
+      </c>
+      <c r="J87" s="31">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="88" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A88" s="23">
+        <v>43988</v>
+      </c>
+      <c r="B88" s="24">
+        <v>83105</v>
+      </c>
+      <c r="C88" s="25">
+        <v>229</v>
+      </c>
+      <c r="D88" s="25">
+        <v>1485</v>
+      </c>
+      <c r="E88" s="25">
+        <v>1</v>
+      </c>
+      <c r="F88" s="25">
+        <v>5</v>
+      </c>
+      <c r="G88" s="25">
+        <v>0</v>
+      </c>
+      <c r="H88" s="25">
+        <v>1</v>
+      </c>
+      <c r="I88" s="25">
+        <v>109</v>
+      </c>
+      <c r="J88" s="25">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="89" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A89" s="29">
+        <v>43989</v>
+      </c>
+      <c r="B89" s="30">
+        <v>83316</v>
+      </c>
+      <c r="C89" s="31">
+        <v>211</v>
+      </c>
+      <c r="D89" s="31">
+        <v>1485</v>
+      </c>
+      <c r="E89" s="31">
+        <v>0</v>
+      </c>
+      <c r="F89" s="31">
+        <v>5</v>
+      </c>
+      <c r="G89" s="31">
+        <v>0</v>
+      </c>
+      <c r="H89" s="31">
+        <v>0</v>
+      </c>
+      <c r="I89" s="31">
+        <v>109</v>
+      </c>
+      <c r="J89" s="31">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="90" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A90" s="20">
+        <v>43990</v>
+      </c>
+      <c r="B90" s="21">
+        <v>84130</v>
+      </c>
+      <c r="C90" s="22">
+        <v>814</v>
+      </c>
+      <c r="D90" s="22">
+        <v>1486</v>
+      </c>
+      <c r="E90" s="22">
+        <v>1</v>
+      </c>
+      <c r="F90" s="22">
+        <v>6</v>
+      </c>
+      <c r="G90" s="22">
+        <v>0</v>
+      </c>
+      <c r="H90" s="22">
+        <v>0</v>
+      </c>
+      <c r="I90" s="22">
+        <v>109</v>
+      </c>
+      <c r="J90" s="22">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="91" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A91" s="20">
+        <v>43991</v>
+      </c>
+      <c r="B91" s="21">
+        <v>84868</v>
+      </c>
+      <c r="C91" s="22">
+        <v>738</v>
+      </c>
+      <c r="D91" s="22">
+        <v>1488</v>
+      </c>
+      <c r="E91" s="22">
+        <v>2</v>
+      </c>
+      <c r="F91" s="22">
+        <v>6</v>
+      </c>
+      <c r="G91" s="22">
+        <v>0</v>
+      </c>
+      <c r="H91" s="22">
+        <v>0</v>
+      </c>
+      <c r="I91" s="22">
+        <v>109</v>
+      </c>
+      <c r="J91" s="22">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="92" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A92" s="23">
+        <v>43992</v>
+      </c>
+      <c r="B92" s="24">
+        <v>85626</v>
+      </c>
+      <c r="C92" s="25">
+        <v>758</v>
+      </c>
+      <c r="D92" s="25">
+        <v>1488</v>
+      </c>
+      <c r="E92" s="25">
+        <v>0</v>
+      </c>
+      <c r="F92" s="25">
+        <v>6</v>
+      </c>
+      <c r="G92" s="25">
+        <v>0</v>
+      </c>
+      <c r="H92" s="25">
+        <v>0</v>
+      </c>
+      <c r="I92" s="25">
+        <v>109</v>
+      </c>
+      <c r="J92" s="25">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="93" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A93" s="29">
+        <v>43993</v>
+      </c>
+      <c r="B93" s="30">
+        <v>86328</v>
+      </c>
+      <c r="C93" s="31">
+        <v>702</v>
+      </c>
+      <c r="D93" s="31">
+        <v>1490</v>
+      </c>
+      <c r="E93" s="31">
+        <v>2</v>
+      </c>
+      <c r="F93" s="31">
+        <v>6</v>
+      </c>
+      <c r="G93" s="31">
+        <v>0</v>
+      </c>
+      <c r="H93" s="31">
+        <v>0</v>
+      </c>
+      <c r="I93" s="31">
+        <v>109</v>
+      </c>
+      <c r="J93" s="31">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="94" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A94" s="23">
+        <v>43994</v>
+      </c>
+      <c r="B94" s="24">
+        <v>87095</v>
+      </c>
+      <c r="C94" s="25">
+        <v>767</v>
+      </c>
+      <c r="D94" s="25">
+        <v>1492</v>
+      </c>
+      <c r="E94" s="25">
+        <v>2</v>
+      </c>
+      <c r="F94" s="25">
+        <v>6</v>
+      </c>
+      <c r="G94" s="25">
+        <v>0</v>
+      </c>
+      <c r="H94" s="25">
+        <v>0</v>
+      </c>
+      <c r="I94" s="25">
+        <v>109</v>
+      </c>
+      <c r="J94" s="25">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="95" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A95" s="29">
+        <v>43995</v>
+      </c>
+      <c r="B95" s="30">
+        <v>87386</v>
+      </c>
+      <c r="C95" s="31">
+        <v>291</v>
+      </c>
+      <c r="D95" s="31">
+        <v>1495</v>
+      </c>
+      <c r="E95" s="31">
+        <v>3</v>
+      </c>
+      <c r="F95" s="31">
+        <v>6</v>
+      </c>
+      <c r="G95" s="31">
+        <v>0</v>
+      </c>
+      <c r="H95" s="31">
+        <v>0</v>
+      </c>
+      <c r="I95" s="31">
+        <v>109</v>
+      </c>
+      <c r="J95" s="31">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="96" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A96" s="23">
+        <v>43996</v>
+      </c>
+      <c r="B96" s="24">
+        <v>87598</v>
+      </c>
+      <c r="C96" s="25">
+        <v>212</v>
+      </c>
+      <c r="D96" s="25">
+        <v>1496</v>
+      </c>
+      <c r="E96" s="25">
+        <v>1</v>
+      </c>
+      <c r="F96" s="25">
+        <v>7</v>
+      </c>
+      <c r="G96" s="25">
+        <v>1</v>
+      </c>
+      <c r="H96" s="25">
+        <v>0</v>
+      </c>
+      <c r="I96" s="25">
+        <v>109</v>
+      </c>
+      <c r="J96" s="25">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="97" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A97" s="20">
+        <v>43997</v>
+      </c>
+      <c r="B97" s="21">
+        <v>88165</v>
+      </c>
+      <c r="C97" s="22">
+        <v>567</v>
+      </c>
+      <c r="D97" s="22">
+        <v>1499</v>
+      </c>
+      <c r="E97" s="22">
+        <v>3</v>
+      </c>
+      <c r="F97" s="22">
+        <v>7</v>
+      </c>
+      <c r="G97" s="22">
+        <v>1</v>
+      </c>
+      <c r="H97" s="22">
+        <v>0</v>
+      </c>
+      <c r="I97" s="22">
+        <v>109</v>
+      </c>
+      <c r="J97" s="22">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="98" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A98" s="20">
+        <v>43998</v>
+      </c>
+      <c r="B98" s="21">
+        <v>89151</v>
+      </c>
+      <c r="C98" s="22">
+        <v>986</v>
+      </c>
+      <c r="D98" s="22">
+        <v>1503</v>
+      </c>
+      <c r="E98" s="22">
+        <v>4</v>
+      </c>
+      <c r="F98" s="22">
+        <v>7</v>
+      </c>
+      <c r="G98" s="22">
+        <v>1</v>
+      </c>
+      <c r="H98" s="22">
+        <v>0</v>
+      </c>
+      <c r="I98" s="22">
+        <v>109</v>
+      </c>
+      <c r="J98" s="22">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="99" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A99" s="29">
+        <v>43999</v>
+      </c>
+      <c r="B99" s="30">
+        <v>90103</v>
+      </c>
+      <c r="C99" s="31">
+        <v>952</v>
+      </c>
+      <c r="D99" s="31">
+        <v>1511</v>
+      </c>
+      <c r="E99" s="31">
+        <v>8</v>
+      </c>
+      <c r="F99" s="31">
+        <v>6</v>
+      </c>
+      <c r="G99" s="31">
+        <v>1</v>
+      </c>
+      <c r="H99" s="31">
+        <v>1</v>
+      </c>
+      <c r="I99" s="31">
+        <v>109</v>
+      </c>
+      <c r="J99" s="31">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="100" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A100" s="20">
+        <v>44000</v>
+      </c>
+      <c r="B100" s="21">
+        <v>91005</v>
+      </c>
+      <c r="C100" s="22">
+        <v>902</v>
+      </c>
+      <c r="D100" s="22">
+        <v>1513</v>
+      </c>
+      <c r="E100" s="22">
+        <v>2</v>
+      </c>
+      <c r="F100" s="22">
+        <v>8</v>
+      </c>
+      <c r="G100" s="22">
+        <v>1</v>
+      </c>
+      <c r="H100" s="22">
+        <v>0</v>
+      </c>
+      <c r="I100" s="22">
+        <v>109</v>
+      </c>
+      <c r="J100" s="22">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="101" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A101" s="29">
+        <v>44001</v>
+      </c>
+      <c r="B101" s="30">
+        <v>92152</v>
+      </c>
+      <c r="C101" s="31">
+        <v>1147</v>
+      </c>
+      <c r="D101" s="31">
+        <v>1519</v>
+      </c>
+      <c r="E101" s="31">
+        <v>6</v>
+      </c>
+      <c r="F101" s="31">
+        <v>6</v>
+      </c>
+      <c r="G101" s="31">
+        <v>1</v>
+      </c>
+      <c r="H101" s="31">
+        <v>2</v>
+      </c>
+      <c r="I101" s="31">
+        <v>109</v>
+      </c>
+      <c r="J101" s="31">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="102" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A102" s="23">
+        <v>44002</v>
+      </c>
+      <c r="B102" s="24">
+        <v>92919</v>
+      </c>
+      <c r="C102" s="25">
+        <v>758</v>
+      </c>
+      <c r="D102" s="25">
+        <v>1520</v>
+      </c>
+      <c r="E102" s="25">
+        <v>1</v>
+      </c>
+      <c r="F102" s="25">
+        <v>6</v>
+      </c>
+      <c r="G102" s="25">
+        <v>1</v>
+      </c>
+      <c r="H102" s="25">
+        <v>2</v>
+      </c>
+      <c r="I102" s="25">
+        <v>109</v>
+      </c>
+      <c r="J102" s="25">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="103" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A103" s="29">
+        <v>44003</v>
+      </c>
+      <c r="B103" s="30">
+        <v>93181</v>
+      </c>
+      <c r="C103" s="31">
+        <v>271</v>
+      </c>
+      <c r="D103" s="31">
+        <v>1521</v>
+      </c>
+      <c r="E103" s="31">
+        <v>1</v>
+      </c>
+      <c r="F103" s="31">
+        <v>6</v>
+      </c>
+      <c r="G103" s="31">
+        <v>1</v>
+      </c>
+      <c r="H103" s="31">
+        <v>0</v>
+      </c>
+      <c r="I103" s="31">
+        <v>109</v>
+      </c>
+      <c r="J103" s="31">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="104" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A104" s="29">
+        <v>44004</v>
+      </c>
+      <c r="B104" s="30">
+        <v>94165</v>
+      </c>
+      <c r="C104" s="31">
+        <v>984</v>
+      </c>
+      <c r="D104" s="31">
+        <v>1534</v>
+      </c>
+      <c r="E104" s="31">
+        <v>13</v>
+      </c>
+      <c r="F104" s="31">
+        <v>5</v>
+      </c>
+      <c r="G104" s="31">
+        <v>1</v>
+      </c>
+      <c r="H104" s="31">
+        <v>1</v>
+      </c>
+      <c r="I104" s="31">
+        <v>109</v>
+      </c>
+      <c r="J104" s="31">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="105" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A105" s="29">
+        <v>44005</v>
+      </c>
+      <c r="B105" s="30">
+        <v>95387</v>
+      </c>
+      <c r="C105" s="31">
+        <v>1222</v>
+      </c>
+      <c r="D105" s="31">
+        <v>1541</v>
+      </c>
+      <c r="E105" s="31">
+        <v>7</v>
+      </c>
+      <c r="F105" s="31">
+        <v>7</v>
+      </c>
+      <c r="G105" s="31">
+        <v>2</v>
+      </c>
+      <c r="H105" s="31">
+        <v>0</v>
+      </c>
+      <c r="I105" s="31" t="s">
+        <v>10</v>
+      </c>
+      <c r="J105" s="31">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="106" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A106" s="23">
+        <v>44006</v>
+      </c>
+      <c r="B106" s="24">
+        <v>96599</v>
+      </c>
+      <c r="C106" s="25">
+        <v>1212</v>
+      </c>
+      <c r="D106" s="25">
+        <v>1547</v>
+      </c>
+      <c r="E106" s="25">
+        <v>6</v>
+      </c>
+      <c r="F106" s="25">
+        <v>7</v>
+      </c>
+      <c r="G106" s="25">
+        <v>2</v>
+      </c>
+      <c r="H106" s="25">
+        <v>0</v>
+      </c>
+      <c r="I106" s="25" t="s">
+        <v>10</v>
+      </c>
+      <c r="J106" s="25">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="107" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A107" s="29">
+        <v>44007</v>
+      </c>
+      <c r="B107" s="30">
+        <v>97442</v>
+      </c>
+      <c r="C107" s="31">
+        <v>843</v>
+      </c>
+      <c r="D107" s="31">
+        <v>1558</v>
+      </c>
+      <c r="E107" s="31">
+        <v>11</v>
+      </c>
+      <c r="F107" s="31">
+        <v>8</v>
+      </c>
+      <c r="G107" s="31">
+        <v>2</v>
+      </c>
+      <c r="H107" s="31">
+        <v>0</v>
+      </c>
+      <c r="I107" s="31" t="s">
+        <v>10</v>
+      </c>
+      <c r="J107" s="31">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="108" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A108" s="29">
+        <v>44008</v>
+      </c>
+      <c r="B108" s="30">
+        <v>98320</v>
+      </c>
+      <c r="C108" s="31">
+        <v>878</v>
+      </c>
+      <c r="D108" s="31">
+        <v>1572</v>
+      </c>
+      <c r="E108" s="31">
+        <v>14</v>
+      </c>
+      <c r="F108" s="31">
+        <v>8</v>
+      </c>
+      <c r="G108" s="31">
+        <v>1</v>
+      </c>
+      <c r="H108" s="31">
+        <v>0</v>
+      </c>
+      <c r="I108" s="31" t="s">
+        <v>10</v>
+      </c>
+      <c r="J108" s="31">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="109" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A109" s="29">
+        <v>44009</v>
+      </c>
+      <c r="B109" s="30">
+        <v>98945</v>
+      </c>
+      <c r="C109" s="31">
+        <v>625</v>
+      </c>
+      <c r="D109" s="31">
+        <v>1581</v>
+      </c>
+      <c r="E109" s="31">
+        <v>9</v>
+      </c>
+      <c r="F109" s="31">
+        <v>7</v>
+      </c>
+      <c r="G109" s="31">
+        <v>0</v>
+      </c>
+      <c r="H109" s="31">
+        <v>1</v>
+      </c>
+      <c r="I109" s="31" t="s">
+        <v>10</v>
+      </c>
+      <c r="J109" s="31">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="110" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A110" s="29">
+        <v>44010</v>
+      </c>
+      <c r="B110" s="30">
+        <v>99245</v>
+      </c>
+      <c r="C110" s="31">
+        <v>300</v>
+      </c>
+      <c r="D110" s="31">
+        <v>1585</v>
+      </c>
+      <c r="E110" s="31">
+        <v>4</v>
+      </c>
+      <c r="F110" s="31">
+        <v>8</v>
+      </c>
+      <c r="G110" s="31">
+        <v>0</v>
+      </c>
+      <c r="H110" s="31">
+        <v>0</v>
+      </c>
+      <c r="I110" s="31" t="s">
+        <v>10</v>
+      </c>
+      <c r="J110" s="31">
+        <v>0</v>
+      </c>
+    </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>

</xml_diff>

<commit_message>
Data updated by GitHub Bot (2020-06-29 20)
</commit_message>
<xml_diff>
--- a/output/snapshot/fdcf2531-4c3e-5c02-b63c-ee160ead6dea.xlsx
+++ b/output/snapshot/fdcf2531-4c3e-5c02-b63c-ee160ead6dea.xlsx
@@ -1,16 +1,15 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="21929"/>
-  <workbookPr/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
+  <fileVersion appName="xl" lastEdited="6" lowestEdited="6" rupBuild="14420"/>
+  <workbookPr defaultThemeVersion="164011"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="I:\AKTUALNI PODATKI - KORONA\Za objavo na GOV.SI\ang\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{1E6DD62F-2BE2-47DC-A7ED-9B57C1589256}" xr6:coauthVersionLast="44" xr6:coauthVersionMax="44" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840"/>
   </bookViews>
   <sheets>
     <sheet name="Covid-19 podatki" sheetId="1" r:id="rId1"/>
@@ -25,7 +24,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="10" uniqueCount="10">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="16" uniqueCount="11">
   <si>
     <t>Date</t>
   </si>
@@ -56,15 +55,18 @@
   <si>
     <t>Deaths (daily)</t>
   </si>
+  <si>
+    <t>111*</t>
+  </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" mc:Ignorable="x14ac x16r2">
   <numFmts count="1">
     <numFmt numFmtId="164" formatCode="d/\ m/\ yyyy;@"/>
   </numFmts>
-  <fonts count="4" x14ac:knownFonts="1">
+  <fonts count="5" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -93,6 +95,13 @@
       <name val="Calibri Light"/>
       <scheme val="major"/>
     </font>
+    <font>
+      <sz val="10"/>
+      <color theme="1"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
   </fonts>
   <fills count="3">
     <fill>
@@ -108,7 +117,7 @@
       </patternFill>
     </fill>
   </fills>
-  <borders count="2">
+  <borders count="3">
     <border>
       <left/>
       <right/>
@@ -129,11 +138,26 @@
       <bottom/>
       <diagonal/>
     </border>
+    <border>
+      <left style="thin">
+        <color theme="4"/>
+      </left>
+      <right style="thin">
+        <color theme="4"/>
+      </right>
+      <top style="thin">
+        <color theme="4"/>
+      </top>
+      <bottom style="thin">
+        <color theme="4"/>
+      </bottom>
+      <diagonal/>
+    </border>
   </borders>
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="26">
+  <cellXfs count="32">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="49" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyAlignment="1" applyProtection="1">
       <alignment horizontal="left" vertical="top"/>
@@ -208,6 +232,24 @@
       <alignment horizontal="right"/>
     </xf>
     <xf numFmtId="0" fontId="3" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="right"/>
+    </xf>
+    <xf numFmtId="164" fontId="4" fillId="2" borderId="2" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="right" vertical="top"/>
+    </xf>
+    <xf numFmtId="3" fontId="4" fillId="2" borderId="2" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="right"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="2" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="right"/>
+    </xf>
+    <xf numFmtId="164" fontId="3" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="right" vertical="top"/>
+    </xf>
+    <xf numFmtId="3" fontId="3" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="right"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="right"/>
     </xf>
   </cellXfs>
@@ -399,8 +441,8 @@
 </file>
 
 <file path=xl/tables/table1.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="1" xr:uid="{00000000-000C-0000-FFFF-FFFF00000000}" name="Tabela1" displayName="Tabela1" ref="A1:J75" totalsRowShown="0" headerRowDxfId="11" dataDxfId="10">
-  <autoFilter ref="A1:J75" xr:uid="{00000000-0009-0000-0100-000001000000}">
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="1" name="Tabela1" displayName="Tabela1" ref="A1:J110" totalsRowShown="0" headerRowDxfId="11" dataDxfId="10">
+  <autoFilter ref="A1:J110">
     <filterColumn colId="0" hiddenButton="1"/>
     <filterColumn colId="1" hiddenButton="1"/>
     <filterColumn colId="2" hiddenButton="1"/>
@@ -413,16 +455,16 @@
     <filterColumn colId="9" hiddenButton="1"/>
   </autoFilter>
   <tableColumns count="10">
-    <tableColumn id="1" xr3:uid="{00000000-0010-0000-0000-000001000000}" name="Date" dataDxfId="9"/>
-    <tableColumn id="2" xr3:uid="{00000000-0010-0000-0000-000002000000}" name="Tested (all)" dataDxfId="8"/>
-    <tableColumn id="3" xr3:uid="{00000000-0010-0000-0000-000003000000}" name="Tested (daily)" dataDxfId="7"/>
-    <tableColumn id="4" xr3:uid="{00000000-0010-0000-0000-000004000000}" name="Positive (all)" dataDxfId="6"/>
-    <tableColumn id="5" xr3:uid="{00000000-0010-0000-0000-000005000000}" name="Positive (daily)" dataDxfId="5"/>
-    <tableColumn id="6" xr3:uid="{00000000-0010-0000-0000-000006000000}" name="All hospitalized on certain day" dataDxfId="4"/>
-    <tableColumn id="7" xr3:uid="{00000000-0010-0000-0000-000007000000}" name="All persons in intensive care on certain day" dataDxfId="3"/>
-    <tableColumn id="10" xr3:uid="{00000000-0010-0000-0000-00000A000000}" name="Discharged" dataDxfId="2"/>
-    <tableColumn id="8" xr3:uid="{00000000-0010-0000-0000-000008000000}" name="Deaths (all)" dataDxfId="1"/>
-    <tableColumn id="9" xr3:uid="{00000000-0010-0000-0000-000009000000}" name="Deaths (daily)" dataDxfId="0"/>
+    <tableColumn id="1" name="Date" dataDxfId="9"/>
+    <tableColumn id="2" name="Tested (all)" dataDxfId="8"/>
+    <tableColumn id="3" name="Tested (daily)" dataDxfId="7"/>
+    <tableColumn id="4" name="Positive (all)" dataDxfId="6"/>
+    <tableColumn id="5" name="Positive (daily)" dataDxfId="5"/>
+    <tableColumn id="6" name="All hospitalized on certain day" dataDxfId="4"/>
+    <tableColumn id="7" name="All persons in intensive care on certain day" dataDxfId="3"/>
+    <tableColumn id="10" name="Discharged" dataDxfId="2"/>
+    <tableColumn id="8" name="Deaths (all)" dataDxfId="1"/>
+    <tableColumn id="9" name="Deaths (daily)" dataDxfId="0"/>
   </tableColumns>
   <tableStyleInfo name="TableStyleLight16" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
   <extLst>
@@ -695,11 +737,11 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:J75"/>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <dimension ref="A1:J110"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A40" zoomScale="89" zoomScaleNormal="89" workbookViewId="0">
-      <selection activeCell="J74" sqref="J74"/>
+    <sheetView tabSelected="1" topLeftCell="A83" zoomScale="89" zoomScaleNormal="89" workbookViewId="0">
+      <selection activeCell="I110" sqref="I110"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -3117,6 +3159,1126 @@
         <v>0</v>
       </c>
     </row>
+    <row r="76" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A76" s="20">
+        <v>43976</v>
+      </c>
+      <c r="B76" s="21">
+        <v>75770</v>
+      </c>
+      <c r="C76" s="22">
+        <v>754</v>
+      </c>
+      <c r="D76" s="22">
+        <v>1469</v>
+      </c>
+      <c r="E76" s="22">
+        <v>0</v>
+      </c>
+      <c r="F76" s="22">
+        <v>9</v>
+      </c>
+      <c r="G76" s="22">
+        <v>2</v>
+      </c>
+      <c r="H76" s="22">
+        <v>6</v>
+      </c>
+      <c r="I76" s="22">
+        <v>108</v>
+      </c>
+      <c r="J76" s="22">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="77" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A77" s="20">
+        <v>43977</v>
+      </c>
+      <c r="B77" s="21">
+        <v>76579</v>
+      </c>
+      <c r="C77" s="22">
+        <v>809</v>
+      </c>
+      <c r="D77" s="22">
+        <v>1471</v>
+      </c>
+      <c r="E77" s="22">
+        <v>2</v>
+      </c>
+      <c r="F77" s="22">
+        <v>8</v>
+      </c>
+      <c r="G77" s="22">
+        <v>2</v>
+      </c>
+      <c r="H77" s="22">
+        <v>2</v>
+      </c>
+      <c r="I77" s="22">
+        <v>108</v>
+      </c>
+      <c r="J77" s="22">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="78" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A78" s="20">
+        <v>43978</v>
+      </c>
+      <c r="B78" s="21">
+        <v>77210</v>
+      </c>
+      <c r="C78" s="22">
+        <v>631</v>
+      </c>
+      <c r="D78" s="22">
+        <v>1473</v>
+      </c>
+      <c r="E78" s="22">
+        <v>2</v>
+      </c>
+      <c r="F78" s="22">
+        <v>7</v>
+      </c>
+      <c r="G78" s="22">
+        <v>2</v>
+      </c>
+      <c r="H78" s="22">
+        <v>1</v>
+      </c>
+      <c r="I78" s="22">
+        <v>108</v>
+      </c>
+      <c r="J78" s="22">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="79" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A79" s="20">
+        <v>43979</v>
+      </c>
+      <c r="B79" s="21">
+        <v>77916</v>
+      </c>
+      <c r="C79" s="22">
+        <v>706</v>
+      </c>
+      <c r="D79" s="22">
+        <v>1473</v>
+      </c>
+      <c r="E79" s="22">
+        <v>0</v>
+      </c>
+      <c r="F79" s="22">
+        <v>7</v>
+      </c>
+      <c r="G79" s="22">
+        <v>2</v>
+      </c>
+      <c r="H79" s="22">
+        <v>0</v>
+      </c>
+      <c r="I79" s="22">
+        <v>108</v>
+      </c>
+      <c r="J79" s="22">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="80" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A80" s="20">
+        <v>43980</v>
+      </c>
+      <c r="B80" s="21">
+        <v>78529</v>
+      </c>
+      <c r="C80" s="22">
+        <v>613</v>
+      </c>
+      <c r="D80" s="22">
+        <v>1473</v>
+      </c>
+      <c r="E80" s="22">
+        <v>0</v>
+      </c>
+      <c r="F80" s="22">
+        <v>7</v>
+      </c>
+      <c r="G80" s="22">
+        <v>2</v>
+      </c>
+      <c r="H80" s="22">
+        <v>0</v>
+      </c>
+      <c r="I80" s="22">
+        <v>108</v>
+      </c>
+      <c r="J80" s="22">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="81" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A81" s="20">
+        <v>43981</v>
+      </c>
+      <c r="B81" s="22">
+        <v>78793</v>
+      </c>
+      <c r="C81" s="22">
+        <v>264</v>
+      </c>
+      <c r="D81" s="22">
+        <v>1473</v>
+      </c>
+      <c r="E81" s="22">
+        <v>0</v>
+      </c>
+      <c r="F81" s="22">
+        <v>6</v>
+      </c>
+      <c r="G81" s="22">
+        <v>2</v>
+      </c>
+      <c r="H81" s="22">
+        <v>1</v>
+      </c>
+      <c r="I81" s="22">
+        <v>108</v>
+      </c>
+      <c r="J81" s="22">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="82" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A82" s="20">
+        <v>43982</v>
+      </c>
+      <c r="B82" s="21">
+        <v>79039</v>
+      </c>
+      <c r="C82" s="22">
+        <v>246</v>
+      </c>
+      <c r="D82" s="22">
+        <v>1473</v>
+      </c>
+      <c r="E82" s="22">
+        <v>0</v>
+      </c>
+      <c r="F82" s="22">
+        <v>5</v>
+      </c>
+      <c r="G82" s="22">
+        <v>1</v>
+      </c>
+      <c r="H82" s="22">
+        <v>0</v>
+      </c>
+      <c r="I82" s="22">
+        <v>109</v>
+      </c>
+      <c r="J82" s="22">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="83" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A83" s="20">
+        <v>43983</v>
+      </c>
+      <c r="B83" s="21">
+        <v>79698</v>
+      </c>
+      <c r="C83" s="22">
+        <v>659</v>
+      </c>
+      <c r="D83" s="22">
+        <v>1475</v>
+      </c>
+      <c r="E83" s="22">
+        <v>2</v>
+      </c>
+      <c r="F83" s="22">
+        <v>5</v>
+      </c>
+      <c r="G83" s="22">
+        <v>1</v>
+      </c>
+      <c r="H83" s="22">
+        <v>0</v>
+      </c>
+      <c r="I83" s="22">
+        <v>109</v>
+      </c>
+      <c r="J83" s="22">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="84" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A84" s="20">
+        <v>43984</v>
+      </c>
+      <c r="B84" s="21">
+        <v>80505</v>
+      </c>
+      <c r="C84" s="22">
+        <v>807</v>
+      </c>
+      <c r="D84" s="22">
+        <v>1477</v>
+      </c>
+      <c r="E84" s="22">
+        <v>2</v>
+      </c>
+      <c r="F84" s="22">
+        <v>5</v>
+      </c>
+      <c r="G84" s="22">
+        <v>0</v>
+      </c>
+      <c r="H84" s="22">
+        <v>0</v>
+      </c>
+      <c r="I84" s="22">
+        <v>109</v>
+      </c>
+      <c r="J84" s="22">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="85" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A85" s="20">
+        <v>43985</v>
+      </c>
+      <c r="B85" s="21">
+        <v>81333</v>
+      </c>
+      <c r="C85" s="22">
+        <v>828</v>
+      </c>
+      <c r="D85" s="22">
+        <v>1477</v>
+      </c>
+      <c r="E85" s="22">
+        <v>0</v>
+      </c>
+      <c r="F85" s="22">
+        <v>5</v>
+      </c>
+      <c r="G85" s="22">
+        <v>0</v>
+      </c>
+      <c r="H85" s="22">
+        <v>0</v>
+      </c>
+      <c r="I85" s="22">
+        <v>109</v>
+      </c>
+      <c r="J85" s="22">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="86" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A86" s="26">
+        <v>43986</v>
+      </c>
+      <c r="B86" s="27">
+        <v>82161</v>
+      </c>
+      <c r="C86" s="28">
+        <v>828</v>
+      </c>
+      <c r="D86" s="28">
+        <v>1479</v>
+      </c>
+      <c r="E86" s="28">
+        <v>2</v>
+      </c>
+      <c r="F86" s="28">
+        <v>6</v>
+      </c>
+      <c r="G86" s="28">
+        <v>0</v>
+      </c>
+      <c r="H86" s="28">
+        <v>0</v>
+      </c>
+      <c r="I86" s="28">
+        <v>109</v>
+      </c>
+      <c r="J86" s="28">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="87" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A87" s="29">
+        <v>43987</v>
+      </c>
+      <c r="B87" s="30">
+        <v>82876</v>
+      </c>
+      <c r="C87" s="31">
+        <v>715</v>
+      </c>
+      <c r="D87" s="31">
+        <v>1484</v>
+      </c>
+      <c r="E87" s="31">
+        <v>5</v>
+      </c>
+      <c r="F87" s="31">
+        <v>6</v>
+      </c>
+      <c r="G87" s="31">
+        <v>0</v>
+      </c>
+      <c r="H87" s="31">
+        <v>0</v>
+      </c>
+      <c r="I87" s="31">
+        <v>109</v>
+      </c>
+      <c r="J87" s="31">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="88" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A88" s="23">
+        <v>43988</v>
+      </c>
+      <c r="B88" s="24">
+        <v>83105</v>
+      </c>
+      <c r="C88" s="25">
+        <v>229</v>
+      </c>
+      <c r="D88" s="25">
+        <v>1485</v>
+      </c>
+      <c r="E88" s="25">
+        <v>1</v>
+      </c>
+      <c r="F88" s="25">
+        <v>5</v>
+      </c>
+      <c r="G88" s="25">
+        <v>0</v>
+      </c>
+      <c r="H88" s="25">
+        <v>1</v>
+      </c>
+      <c r="I88" s="25">
+        <v>109</v>
+      </c>
+      <c r="J88" s="25">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="89" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A89" s="29">
+        <v>43989</v>
+      </c>
+      <c r="B89" s="30">
+        <v>83316</v>
+      </c>
+      <c r="C89" s="31">
+        <v>211</v>
+      </c>
+      <c r="D89" s="31">
+        <v>1485</v>
+      </c>
+      <c r="E89" s="31">
+        <v>0</v>
+      </c>
+      <c r="F89" s="31">
+        <v>5</v>
+      </c>
+      <c r="G89" s="31">
+        <v>0</v>
+      </c>
+      <c r="H89" s="31">
+        <v>0</v>
+      </c>
+      <c r="I89" s="31">
+        <v>109</v>
+      </c>
+      <c r="J89" s="31">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="90" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A90" s="20">
+        <v>43990</v>
+      </c>
+      <c r="B90" s="21">
+        <v>84130</v>
+      </c>
+      <c r="C90" s="22">
+        <v>814</v>
+      </c>
+      <c r="D90" s="22">
+        <v>1486</v>
+      </c>
+      <c r="E90" s="22">
+        <v>1</v>
+      </c>
+      <c r="F90" s="22">
+        <v>6</v>
+      </c>
+      <c r="G90" s="22">
+        <v>0</v>
+      </c>
+      <c r="H90" s="22">
+        <v>0</v>
+      </c>
+      <c r="I90" s="22">
+        <v>109</v>
+      </c>
+      <c r="J90" s="22">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="91" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A91" s="20">
+        <v>43991</v>
+      </c>
+      <c r="B91" s="21">
+        <v>84868</v>
+      </c>
+      <c r="C91" s="22">
+        <v>738</v>
+      </c>
+      <c r="D91" s="22">
+        <v>1488</v>
+      </c>
+      <c r="E91" s="22">
+        <v>2</v>
+      </c>
+      <c r="F91" s="22">
+        <v>6</v>
+      </c>
+      <c r="G91" s="22">
+        <v>0</v>
+      </c>
+      <c r="H91" s="22">
+        <v>0</v>
+      </c>
+      <c r="I91" s="22">
+        <v>109</v>
+      </c>
+      <c r="J91" s="22">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="92" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A92" s="23">
+        <v>43992</v>
+      </c>
+      <c r="B92" s="24">
+        <v>85626</v>
+      </c>
+      <c r="C92" s="25">
+        <v>758</v>
+      </c>
+      <c r="D92" s="25">
+        <v>1488</v>
+      </c>
+      <c r="E92" s="25">
+        <v>0</v>
+      </c>
+      <c r="F92" s="25">
+        <v>6</v>
+      </c>
+      <c r="G92" s="25">
+        <v>0</v>
+      </c>
+      <c r="H92" s="25">
+        <v>0</v>
+      </c>
+      <c r="I92" s="25">
+        <v>109</v>
+      </c>
+      <c r="J92" s="25">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="93" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A93" s="29">
+        <v>43993</v>
+      </c>
+      <c r="B93" s="30">
+        <v>86328</v>
+      </c>
+      <c r="C93" s="31">
+        <v>702</v>
+      </c>
+      <c r="D93" s="31">
+        <v>1490</v>
+      </c>
+      <c r="E93" s="31">
+        <v>2</v>
+      </c>
+      <c r="F93" s="31">
+        <v>6</v>
+      </c>
+      <c r="G93" s="31">
+        <v>0</v>
+      </c>
+      <c r="H93" s="31">
+        <v>0</v>
+      </c>
+      <c r="I93" s="31">
+        <v>109</v>
+      </c>
+      <c r="J93" s="31">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="94" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A94" s="23">
+        <v>43994</v>
+      </c>
+      <c r="B94" s="24">
+        <v>87095</v>
+      </c>
+      <c r="C94" s="25">
+        <v>767</v>
+      </c>
+      <c r="D94" s="25">
+        <v>1492</v>
+      </c>
+      <c r="E94" s="25">
+        <v>2</v>
+      </c>
+      <c r="F94" s="25">
+        <v>6</v>
+      </c>
+      <c r="G94" s="25">
+        <v>0</v>
+      </c>
+      <c r="H94" s="25">
+        <v>0</v>
+      </c>
+      <c r="I94" s="25">
+        <v>109</v>
+      </c>
+      <c r="J94" s="25">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="95" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A95" s="29">
+        <v>43995</v>
+      </c>
+      <c r="B95" s="30">
+        <v>87386</v>
+      </c>
+      <c r="C95" s="31">
+        <v>291</v>
+      </c>
+      <c r="D95" s="31">
+        <v>1495</v>
+      </c>
+      <c r="E95" s="31">
+        <v>3</v>
+      </c>
+      <c r="F95" s="31">
+        <v>6</v>
+      </c>
+      <c r="G95" s="31">
+        <v>0</v>
+      </c>
+      <c r="H95" s="31">
+        <v>0</v>
+      </c>
+      <c r="I95" s="31">
+        <v>109</v>
+      </c>
+      <c r="J95" s="31">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="96" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A96" s="23">
+        <v>43996</v>
+      </c>
+      <c r="B96" s="24">
+        <v>87598</v>
+      </c>
+      <c r="C96" s="25">
+        <v>212</v>
+      </c>
+      <c r="D96" s="25">
+        <v>1496</v>
+      </c>
+      <c r="E96" s="25">
+        <v>1</v>
+      </c>
+      <c r="F96" s="25">
+        <v>7</v>
+      </c>
+      <c r="G96" s="25">
+        <v>1</v>
+      </c>
+      <c r="H96" s="25">
+        <v>0</v>
+      </c>
+      <c r="I96" s="25">
+        <v>109</v>
+      </c>
+      <c r="J96" s="25">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="97" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A97" s="20">
+        <v>43997</v>
+      </c>
+      <c r="B97" s="21">
+        <v>88165</v>
+      </c>
+      <c r="C97" s="22">
+        <v>567</v>
+      </c>
+      <c r="D97" s="22">
+        <v>1499</v>
+      </c>
+      <c r="E97" s="22">
+        <v>3</v>
+      </c>
+      <c r="F97" s="22">
+        <v>7</v>
+      </c>
+      <c r="G97" s="22">
+        <v>1</v>
+      </c>
+      <c r="H97" s="22">
+        <v>0</v>
+      </c>
+      <c r="I97" s="22">
+        <v>109</v>
+      </c>
+      <c r="J97" s="22">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="98" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A98" s="20">
+        <v>43998</v>
+      </c>
+      <c r="B98" s="21">
+        <v>89151</v>
+      </c>
+      <c r="C98" s="22">
+        <v>986</v>
+      </c>
+      <c r="D98" s="22">
+        <v>1503</v>
+      </c>
+      <c r="E98" s="22">
+        <v>4</v>
+      </c>
+      <c r="F98" s="22">
+        <v>7</v>
+      </c>
+      <c r="G98" s="22">
+        <v>1</v>
+      </c>
+      <c r="H98" s="22">
+        <v>0</v>
+      </c>
+      <c r="I98" s="22">
+        <v>109</v>
+      </c>
+      <c r="J98" s="22">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="99" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A99" s="29">
+        <v>43999</v>
+      </c>
+      <c r="B99" s="30">
+        <v>90103</v>
+      </c>
+      <c r="C99" s="31">
+        <v>952</v>
+      </c>
+      <c r="D99" s="31">
+        <v>1511</v>
+      </c>
+      <c r="E99" s="31">
+        <v>8</v>
+      </c>
+      <c r="F99" s="31">
+        <v>6</v>
+      </c>
+      <c r="G99" s="31">
+        <v>1</v>
+      </c>
+      <c r="H99" s="31">
+        <v>1</v>
+      </c>
+      <c r="I99" s="31">
+        <v>109</v>
+      </c>
+      <c r="J99" s="31">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="100" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A100" s="20">
+        <v>44000</v>
+      </c>
+      <c r="B100" s="21">
+        <v>91005</v>
+      </c>
+      <c r="C100" s="22">
+        <v>902</v>
+      </c>
+      <c r="D100" s="22">
+        <v>1513</v>
+      </c>
+      <c r="E100" s="22">
+        <v>2</v>
+      </c>
+      <c r="F100" s="22">
+        <v>8</v>
+      </c>
+      <c r="G100" s="22">
+        <v>1</v>
+      </c>
+      <c r="H100" s="22">
+        <v>0</v>
+      </c>
+      <c r="I100" s="22">
+        <v>109</v>
+      </c>
+      <c r="J100" s="22">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="101" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A101" s="29">
+        <v>44001</v>
+      </c>
+      <c r="B101" s="30">
+        <v>92152</v>
+      </c>
+      <c r="C101" s="31">
+        <v>1147</v>
+      </c>
+      <c r="D101" s="31">
+        <v>1519</v>
+      </c>
+      <c r="E101" s="31">
+        <v>6</v>
+      </c>
+      <c r="F101" s="31">
+        <v>6</v>
+      </c>
+      <c r="G101" s="31">
+        <v>1</v>
+      </c>
+      <c r="H101" s="31">
+        <v>2</v>
+      </c>
+      <c r="I101" s="31">
+        <v>109</v>
+      </c>
+      <c r="J101" s="31">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="102" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A102" s="23">
+        <v>44002</v>
+      </c>
+      <c r="B102" s="24">
+        <v>92919</v>
+      </c>
+      <c r="C102" s="25">
+        <v>758</v>
+      </c>
+      <c r="D102" s="25">
+        <v>1520</v>
+      </c>
+      <c r="E102" s="25">
+        <v>1</v>
+      </c>
+      <c r="F102" s="25">
+        <v>6</v>
+      </c>
+      <c r="G102" s="25">
+        <v>1</v>
+      </c>
+      <c r="H102" s="25">
+        <v>2</v>
+      </c>
+      <c r="I102" s="25">
+        <v>109</v>
+      </c>
+      <c r="J102" s="25">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="103" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A103" s="29">
+        <v>44003</v>
+      </c>
+      <c r="B103" s="30">
+        <v>93181</v>
+      </c>
+      <c r="C103" s="31">
+        <v>271</v>
+      </c>
+      <c r="D103" s="31">
+        <v>1521</v>
+      </c>
+      <c r="E103" s="31">
+        <v>1</v>
+      </c>
+      <c r="F103" s="31">
+        <v>6</v>
+      </c>
+      <c r="G103" s="31">
+        <v>1</v>
+      </c>
+      <c r="H103" s="31">
+        <v>0</v>
+      </c>
+      <c r="I103" s="31">
+        <v>109</v>
+      </c>
+      <c r="J103" s="31">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="104" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A104" s="29">
+        <v>44004</v>
+      </c>
+      <c r="B104" s="30">
+        <v>94165</v>
+      </c>
+      <c r="C104" s="31">
+        <v>984</v>
+      </c>
+      <c r="D104" s="31">
+        <v>1534</v>
+      </c>
+      <c r="E104" s="31">
+        <v>13</v>
+      </c>
+      <c r="F104" s="31">
+        <v>5</v>
+      </c>
+      <c r="G104" s="31">
+        <v>1</v>
+      </c>
+      <c r="H104" s="31">
+        <v>1</v>
+      </c>
+      <c r="I104" s="31">
+        <v>109</v>
+      </c>
+      <c r="J104" s="31">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="105" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A105" s="29">
+        <v>44005</v>
+      </c>
+      <c r="B105" s="30">
+        <v>95387</v>
+      </c>
+      <c r="C105" s="31">
+        <v>1222</v>
+      </c>
+      <c r="D105" s="31">
+        <v>1541</v>
+      </c>
+      <c r="E105" s="31">
+        <v>7</v>
+      </c>
+      <c r="F105" s="31">
+        <v>7</v>
+      </c>
+      <c r="G105" s="31">
+        <v>2</v>
+      </c>
+      <c r="H105" s="31">
+        <v>0</v>
+      </c>
+      <c r="I105" s="31" t="s">
+        <v>10</v>
+      </c>
+      <c r="J105" s="31">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="106" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A106" s="23">
+        <v>44006</v>
+      </c>
+      <c r="B106" s="24">
+        <v>96599</v>
+      </c>
+      <c r="C106" s="25">
+        <v>1212</v>
+      </c>
+      <c r="D106" s="25">
+        <v>1547</v>
+      </c>
+      <c r="E106" s="25">
+        <v>6</v>
+      </c>
+      <c r="F106" s="25">
+        <v>7</v>
+      </c>
+      <c r="G106" s="25">
+        <v>2</v>
+      </c>
+      <c r="H106" s="25">
+        <v>0</v>
+      </c>
+      <c r="I106" s="25" t="s">
+        <v>10</v>
+      </c>
+      <c r="J106" s="25">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="107" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A107" s="29">
+        <v>44007</v>
+      </c>
+      <c r="B107" s="30">
+        <v>97442</v>
+      </c>
+      <c r="C107" s="31">
+        <v>843</v>
+      </c>
+      <c r="D107" s="31">
+        <v>1558</v>
+      </c>
+      <c r="E107" s="31">
+        <v>11</v>
+      </c>
+      <c r="F107" s="31">
+        <v>8</v>
+      </c>
+      <c r="G107" s="31">
+        <v>2</v>
+      </c>
+      <c r="H107" s="31">
+        <v>0</v>
+      </c>
+      <c r="I107" s="31" t="s">
+        <v>10</v>
+      </c>
+      <c r="J107" s="31">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="108" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A108" s="29">
+        <v>44008</v>
+      </c>
+      <c r="B108" s="30">
+        <v>98320</v>
+      </c>
+      <c r="C108" s="31">
+        <v>878</v>
+      </c>
+      <c r="D108" s="31">
+        <v>1572</v>
+      </c>
+      <c r="E108" s="31">
+        <v>14</v>
+      </c>
+      <c r="F108" s="31">
+        <v>8</v>
+      </c>
+      <c r="G108" s="31">
+        <v>1</v>
+      </c>
+      <c r="H108" s="31">
+        <v>0</v>
+      </c>
+      <c r="I108" s="31" t="s">
+        <v>10</v>
+      </c>
+      <c r="J108" s="31">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="109" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A109" s="29">
+        <v>44009</v>
+      </c>
+      <c r="B109" s="30">
+        <v>98945</v>
+      </c>
+      <c r="C109" s="31">
+        <v>625</v>
+      </c>
+      <c r="D109" s="31">
+        <v>1581</v>
+      </c>
+      <c r="E109" s="31">
+        <v>9</v>
+      </c>
+      <c r="F109" s="31">
+        <v>7</v>
+      </c>
+      <c r="G109" s="31">
+        <v>0</v>
+      </c>
+      <c r="H109" s="31">
+        <v>1</v>
+      </c>
+      <c r="I109" s="31" t="s">
+        <v>10</v>
+      </c>
+      <c r="J109" s="31">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="110" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A110" s="29">
+        <v>44010</v>
+      </c>
+      <c r="B110" s="30">
+        <v>99245</v>
+      </c>
+      <c r="C110" s="31">
+        <v>300</v>
+      </c>
+      <c r="D110" s="31">
+        <v>1585</v>
+      </c>
+      <c r="E110" s="31">
+        <v>4</v>
+      </c>
+      <c r="F110" s="31">
+        <v>8</v>
+      </c>
+      <c r="G110" s="31">
+        <v>0</v>
+      </c>
+      <c r="H110" s="31">
+        <v>0</v>
+      </c>
+      <c r="I110" s="31" t="s">
+        <v>10</v>
+      </c>
+      <c r="J110" s="31">
+        <v>0</v>
+      </c>
+    </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>

</xml_diff>

<commit_message>
Data updated by GitHub Bot (2020-06-30 12)
</commit_message>
<xml_diff>
--- a/output/snapshot/fdcf2531-4c3e-5c02-b63c-ee160ead6dea.xlsx
+++ b/output/snapshot/fdcf2531-4c3e-5c02-b63c-ee160ead6dea.xlsx
@@ -1,16 +1,15 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="21929"/>
-  <workbookPr/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
+  <fileVersion appName="xl" lastEdited="6" lowestEdited="6" rupBuild="14420"/>
+  <workbookPr defaultThemeVersion="164011"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="I:\AKTUALNI PODATKI - KORONA\Za objavo na GOV.SI\ang\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{1E6DD62F-2BE2-47DC-A7ED-9B57C1589256}" xr6:coauthVersionLast="44" xr6:coauthVersionMax="44" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840"/>
   </bookViews>
   <sheets>
     <sheet name="Covid-19 podatki" sheetId="1" r:id="rId1"/>
@@ -25,7 +24,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="10" uniqueCount="10">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="17" uniqueCount="11">
   <si>
     <t>Date</t>
   </si>
@@ -56,15 +55,18 @@
   <si>
     <t>Deaths (daily)</t>
   </si>
+  <si>
+    <t>111*</t>
+  </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" mc:Ignorable="x14ac x16r2">
   <numFmts count="1">
     <numFmt numFmtId="164" formatCode="d/\ m/\ yyyy;@"/>
   </numFmts>
-  <fonts count="4" x14ac:knownFonts="1">
+  <fonts count="5" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -93,6 +95,13 @@
       <name val="Calibri Light"/>
       <scheme val="major"/>
     </font>
+    <font>
+      <sz val="10"/>
+      <color theme="1"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
   </fonts>
   <fills count="3">
     <fill>
@@ -108,7 +117,7 @@
       </patternFill>
     </fill>
   </fills>
-  <borders count="2">
+  <borders count="3">
     <border>
       <left/>
       <right/>
@@ -129,11 +138,26 @@
       <bottom/>
       <diagonal/>
     </border>
+    <border>
+      <left style="thin">
+        <color theme="4"/>
+      </left>
+      <right style="thin">
+        <color theme="4"/>
+      </right>
+      <top style="thin">
+        <color theme="4"/>
+      </top>
+      <bottom style="thin">
+        <color theme="4"/>
+      </bottom>
+      <diagonal/>
+    </border>
   </borders>
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="26">
+  <cellXfs count="32">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="49" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyAlignment="1" applyProtection="1">
       <alignment horizontal="left" vertical="top"/>
@@ -208,6 +232,24 @@
       <alignment horizontal="right"/>
     </xf>
     <xf numFmtId="0" fontId="3" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="right"/>
+    </xf>
+    <xf numFmtId="164" fontId="4" fillId="2" borderId="2" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="right" vertical="top"/>
+    </xf>
+    <xf numFmtId="3" fontId="4" fillId="2" borderId="2" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="right"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="2" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="right"/>
+    </xf>
+    <xf numFmtId="164" fontId="3" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="right" vertical="top"/>
+    </xf>
+    <xf numFmtId="3" fontId="3" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="right"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="right"/>
     </xf>
   </cellXfs>
@@ -399,8 +441,8 @@
 </file>
 
 <file path=xl/tables/table1.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="1" xr:uid="{00000000-000C-0000-FFFF-FFFF00000000}" name="Tabela1" displayName="Tabela1" ref="A1:J75" totalsRowShown="0" headerRowDxfId="11" dataDxfId="10">
-  <autoFilter ref="A1:J75" xr:uid="{00000000-0009-0000-0100-000001000000}">
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="1" name="Tabela1" displayName="Tabela1" ref="A1:J111" totalsRowShown="0" headerRowDxfId="11" dataDxfId="10">
+  <autoFilter ref="A1:J111">
     <filterColumn colId="0" hiddenButton="1"/>
     <filterColumn colId="1" hiddenButton="1"/>
     <filterColumn colId="2" hiddenButton="1"/>
@@ -413,16 +455,16 @@
     <filterColumn colId="9" hiddenButton="1"/>
   </autoFilter>
   <tableColumns count="10">
-    <tableColumn id="1" xr3:uid="{00000000-0010-0000-0000-000001000000}" name="Date" dataDxfId="9"/>
-    <tableColumn id="2" xr3:uid="{00000000-0010-0000-0000-000002000000}" name="Tested (all)" dataDxfId="8"/>
-    <tableColumn id="3" xr3:uid="{00000000-0010-0000-0000-000003000000}" name="Tested (daily)" dataDxfId="7"/>
-    <tableColumn id="4" xr3:uid="{00000000-0010-0000-0000-000004000000}" name="Positive (all)" dataDxfId="6"/>
-    <tableColumn id="5" xr3:uid="{00000000-0010-0000-0000-000005000000}" name="Positive (daily)" dataDxfId="5"/>
-    <tableColumn id="6" xr3:uid="{00000000-0010-0000-0000-000006000000}" name="All hospitalized on certain day" dataDxfId="4"/>
-    <tableColumn id="7" xr3:uid="{00000000-0010-0000-0000-000007000000}" name="All persons in intensive care on certain day" dataDxfId="3"/>
-    <tableColumn id="10" xr3:uid="{00000000-0010-0000-0000-00000A000000}" name="Discharged" dataDxfId="2"/>
-    <tableColumn id="8" xr3:uid="{00000000-0010-0000-0000-000008000000}" name="Deaths (all)" dataDxfId="1"/>
-    <tableColumn id="9" xr3:uid="{00000000-0010-0000-0000-000009000000}" name="Deaths (daily)" dataDxfId="0"/>
+    <tableColumn id="1" name="Date" dataDxfId="9"/>
+    <tableColumn id="2" name="Tested (all)" dataDxfId="8"/>
+    <tableColumn id="3" name="Tested (daily)" dataDxfId="7"/>
+    <tableColumn id="4" name="Positive (all)" dataDxfId="6"/>
+    <tableColumn id="5" name="Positive (daily)" dataDxfId="5"/>
+    <tableColumn id="6" name="All hospitalized on certain day" dataDxfId="4"/>
+    <tableColumn id="7" name="All persons in intensive care on certain day" dataDxfId="3"/>
+    <tableColumn id="10" name="Discharged" dataDxfId="2"/>
+    <tableColumn id="8" name="Deaths (all)" dataDxfId="1"/>
+    <tableColumn id="9" name="Deaths (daily)" dataDxfId="0"/>
   </tableColumns>
   <tableStyleInfo name="TableStyleLight16" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
   <extLst>
@@ -695,11 +737,11 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:J75"/>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <dimension ref="A1:J111"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A40" zoomScale="89" zoomScaleNormal="89" workbookViewId="0">
-      <selection activeCell="J74" sqref="J74"/>
+    <sheetView tabSelected="1" topLeftCell="A83" zoomScale="89" zoomScaleNormal="89" workbookViewId="0">
+      <selection activeCell="C114" sqref="C114"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -3117,6 +3159,1158 @@
         <v>0</v>
       </c>
     </row>
+    <row r="76" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A76" s="20">
+        <v>43976</v>
+      </c>
+      <c r="B76" s="21">
+        <v>75770</v>
+      </c>
+      <c r="C76" s="22">
+        <v>754</v>
+      </c>
+      <c r="D76" s="22">
+        <v>1469</v>
+      </c>
+      <c r="E76" s="22">
+        <v>0</v>
+      </c>
+      <c r="F76" s="22">
+        <v>9</v>
+      </c>
+      <c r="G76" s="22">
+        <v>2</v>
+      </c>
+      <c r="H76" s="22">
+        <v>6</v>
+      </c>
+      <c r="I76" s="22">
+        <v>108</v>
+      </c>
+      <c r="J76" s="22">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="77" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A77" s="20">
+        <v>43977</v>
+      </c>
+      <c r="B77" s="21">
+        <v>76579</v>
+      </c>
+      <c r="C77" s="22">
+        <v>809</v>
+      </c>
+      <c r="D77" s="22">
+        <v>1471</v>
+      </c>
+      <c r="E77" s="22">
+        <v>2</v>
+      </c>
+      <c r="F77" s="22">
+        <v>8</v>
+      </c>
+      <c r="G77" s="22">
+        <v>2</v>
+      </c>
+      <c r="H77" s="22">
+        <v>2</v>
+      </c>
+      <c r="I77" s="22">
+        <v>108</v>
+      </c>
+      <c r="J77" s="22">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="78" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A78" s="20">
+        <v>43978</v>
+      </c>
+      <c r="B78" s="21">
+        <v>77210</v>
+      </c>
+      <c r="C78" s="22">
+        <v>631</v>
+      </c>
+      <c r="D78" s="22">
+        <v>1473</v>
+      </c>
+      <c r="E78" s="22">
+        <v>2</v>
+      </c>
+      <c r="F78" s="22">
+        <v>7</v>
+      </c>
+      <c r="G78" s="22">
+        <v>2</v>
+      </c>
+      <c r="H78" s="22">
+        <v>1</v>
+      </c>
+      <c r="I78" s="22">
+        <v>108</v>
+      </c>
+      <c r="J78" s="22">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="79" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A79" s="20">
+        <v>43979</v>
+      </c>
+      <c r="B79" s="21">
+        <v>77916</v>
+      </c>
+      <c r="C79" s="22">
+        <v>706</v>
+      </c>
+      <c r="D79" s="22">
+        <v>1473</v>
+      </c>
+      <c r="E79" s="22">
+        <v>0</v>
+      </c>
+      <c r="F79" s="22">
+        <v>7</v>
+      </c>
+      <c r="G79" s="22">
+        <v>2</v>
+      </c>
+      <c r="H79" s="22">
+        <v>0</v>
+      </c>
+      <c r="I79" s="22">
+        <v>108</v>
+      </c>
+      <c r="J79" s="22">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="80" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A80" s="20">
+        <v>43980</v>
+      </c>
+      <c r="B80" s="21">
+        <v>78529</v>
+      </c>
+      <c r="C80" s="22">
+        <v>613</v>
+      </c>
+      <c r="D80" s="22">
+        <v>1473</v>
+      </c>
+      <c r="E80" s="22">
+        <v>0</v>
+      </c>
+      <c r="F80" s="22">
+        <v>7</v>
+      </c>
+      <c r="G80" s="22">
+        <v>2</v>
+      </c>
+      <c r="H80" s="22">
+        <v>0</v>
+      </c>
+      <c r="I80" s="22">
+        <v>108</v>
+      </c>
+      <c r="J80" s="22">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="81" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A81" s="20">
+        <v>43981</v>
+      </c>
+      <c r="B81" s="22">
+        <v>78793</v>
+      </c>
+      <c r="C81" s="22">
+        <v>264</v>
+      </c>
+      <c r="D81" s="22">
+        <v>1473</v>
+      </c>
+      <c r="E81" s="22">
+        <v>0</v>
+      </c>
+      <c r="F81" s="22">
+        <v>6</v>
+      </c>
+      <c r="G81" s="22">
+        <v>2</v>
+      </c>
+      <c r="H81" s="22">
+        <v>1</v>
+      </c>
+      <c r="I81" s="22">
+        <v>108</v>
+      </c>
+      <c r="J81" s="22">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="82" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A82" s="20">
+        <v>43982</v>
+      </c>
+      <c r="B82" s="21">
+        <v>79039</v>
+      </c>
+      <c r="C82" s="22">
+        <v>246</v>
+      </c>
+      <c r="D82" s="22">
+        <v>1473</v>
+      </c>
+      <c r="E82" s="22">
+        <v>0</v>
+      </c>
+      <c r="F82" s="22">
+        <v>5</v>
+      </c>
+      <c r="G82" s="22">
+        <v>1</v>
+      </c>
+      <c r="H82" s="22">
+        <v>0</v>
+      </c>
+      <c r="I82" s="22">
+        <v>109</v>
+      </c>
+      <c r="J82" s="22">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="83" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A83" s="20">
+        <v>43983</v>
+      </c>
+      <c r="B83" s="21">
+        <v>79698</v>
+      </c>
+      <c r="C83" s="22">
+        <v>659</v>
+      </c>
+      <c r="D83" s="22">
+        <v>1475</v>
+      </c>
+      <c r="E83" s="22">
+        <v>2</v>
+      </c>
+      <c r="F83" s="22">
+        <v>5</v>
+      </c>
+      <c r="G83" s="22">
+        <v>1</v>
+      </c>
+      <c r="H83" s="22">
+        <v>0</v>
+      </c>
+      <c r="I83" s="22">
+        <v>109</v>
+      </c>
+      <c r="J83" s="22">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="84" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A84" s="20">
+        <v>43984</v>
+      </c>
+      <c r="B84" s="21">
+        <v>80505</v>
+      </c>
+      <c r="C84" s="22">
+        <v>807</v>
+      </c>
+      <c r="D84" s="22">
+        <v>1477</v>
+      </c>
+      <c r="E84" s="22">
+        <v>2</v>
+      </c>
+      <c r="F84" s="22">
+        <v>5</v>
+      </c>
+      <c r="G84" s="22">
+        <v>0</v>
+      </c>
+      <c r="H84" s="22">
+        <v>0</v>
+      </c>
+      <c r="I84" s="22">
+        <v>109</v>
+      </c>
+      <c r="J84" s="22">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="85" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A85" s="20">
+        <v>43985</v>
+      </c>
+      <c r="B85" s="21">
+        <v>81333</v>
+      </c>
+      <c r="C85" s="22">
+        <v>828</v>
+      </c>
+      <c r="D85" s="22">
+        <v>1477</v>
+      </c>
+      <c r="E85" s="22">
+        <v>0</v>
+      </c>
+      <c r="F85" s="22">
+        <v>5</v>
+      </c>
+      <c r="G85" s="22">
+        <v>0</v>
+      </c>
+      <c r="H85" s="22">
+        <v>0</v>
+      </c>
+      <c r="I85" s="22">
+        <v>109</v>
+      </c>
+      <c r="J85" s="22">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="86" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A86" s="26">
+        <v>43986</v>
+      </c>
+      <c r="B86" s="27">
+        <v>82161</v>
+      </c>
+      <c r="C86" s="28">
+        <v>828</v>
+      </c>
+      <c r="D86" s="28">
+        <v>1479</v>
+      </c>
+      <c r="E86" s="28">
+        <v>2</v>
+      </c>
+      <c r="F86" s="28">
+        <v>6</v>
+      </c>
+      <c r="G86" s="28">
+        <v>0</v>
+      </c>
+      <c r="H86" s="28">
+        <v>0</v>
+      </c>
+      <c r="I86" s="28">
+        <v>109</v>
+      </c>
+      <c r="J86" s="28">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="87" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A87" s="29">
+        <v>43987</v>
+      </c>
+      <c r="B87" s="30">
+        <v>82876</v>
+      </c>
+      <c r="C87" s="31">
+        <v>715</v>
+      </c>
+      <c r="D87" s="31">
+        <v>1484</v>
+      </c>
+      <c r="E87" s="31">
+        <v>5</v>
+      </c>
+      <c r="F87" s="31">
+        <v>6</v>
+      </c>
+      <c r="G87" s="31">
+        <v>0</v>
+      </c>
+      <c r="H87" s="31">
+        <v>0</v>
+      </c>
+      <c r="I87" s="31">
+        <v>109</v>
+      </c>
+      <c r="J87" s="31">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="88" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A88" s="23">
+        <v>43988</v>
+      </c>
+      <c r="B88" s="24">
+        <v>83105</v>
+      </c>
+      <c r="C88" s="25">
+        <v>229</v>
+      </c>
+      <c r="D88" s="25">
+        <v>1485</v>
+      </c>
+      <c r="E88" s="25">
+        <v>1</v>
+      </c>
+      <c r="F88" s="25">
+        <v>5</v>
+      </c>
+      <c r="G88" s="25">
+        <v>0</v>
+      </c>
+      <c r="H88" s="25">
+        <v>1</v>
+      </c>
+      <c r="I88" s="25">
+        <v>109</v>
+      </c>
+      <c r="J88" s="25">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="89" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A89" s="29">
+        <v>43989</v>
+      </c>
+      <c r="B89" s="30">
+        <v>83316</v>
+      </c>
+      <c r="C89" s="31">
+        <v>211</v>
+      </c>
+      <c r="D89" s="31">
+        <v>1485</v>
+      </c>
+      <c r="E89" s="31">
+        <v>0</v>
+      </c>
+      <c r="F89" s="31">
+        <v>5</v>
+      </c>
+      <c r="G89" s="31">
+        <v>0</v>
+      </c>
+      <c r="H89" s="31">
+        <v>0</v>
+      </c>
+      <c r="I89" s="31">
+        <v>109</v>
+      </c>
+      <c r="J89" s="31">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="90" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A90" s="20">
+        <v>43990</v>
+      </c>
+      <c r="B90" s="21">
+        <v>84130</v>
+      </c>
+      <c r="C90" s="22">
+        <v>814</v>
+      </c>
+      <c r="D90" s="22">
+        <v>1486</v>
+      </c>
+      <c r="E90" s="22">
+        <v>1</v>
+      </c>
+      <c r="F90" s="22">
+        <v>6</v>
+      </c>
+      <c r="G90" s="22">
+        <v>0</v>
+      </c>
+      <c r="H90" s="22">
+        <v>0</v>
+      </c>
+      <c r="I90" s="22">
+        <v>109</v>
+      </c>
+      <c r="J90" s="22">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="91" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A91" s="20">
+        <v>43991</v>
+      </c>
+      <c r="B91" s="21">
+        <v>84868</v>
+      </c>
+      <c r="C91" s="22">
+        <v>738</v>
+      </c>
+      <c r="D91" s="22">
+        <v>1488</v>
+      </c>
+      <c r="E91" s="22">
+        <v>2</v>
+      </c>
+      <c r="F91" s="22">
+        <v>6</v>
+      </c>
+      <c r="G91" s="22">
+        <v>0</v>
+      </c>
+      <c r="H91" s="22">
+        <v>0</v>
+      </c>
+      <c r="I91" s="22">
+        <v>109</v>
+      </c>
+      <c r="J91" s="22">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="92" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A92" s="23">
+        <v>43992</v>
+      </c>
+      <c r="B92" s="24">
+        <v>85626</v>
+      </c>
+      <c r="C92" s="25">
+        <v>758</v>
+      </c>
+      <c r="D92" s="25">
+        <v>1488</v>
+      </c>
+      <c r="E92" s="25">
+        <v>0</v>
+      </c>
+      <c r="F92" s="25">
+        <v>6</v>
+      </c>
+      <c r="G92" s="25">
+        <v>0</v>
+      </c>
+      <c r="H92" s="25">
+        <v>0</v>
+      </c>
+      <c r="I92" s="25">
+        <v>109</v>
+      </c>
+      <c r="J92" s="25">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="93" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A93" s="29">
+        <v>43993</v>
+      </c>
+      <c r="B93" s="30">
+        <v>86328</v>
+      </c>
+      <c r="C93" s="31">
+        <v>702</v>
+      </c>
+      <c r="D93" s="31">
+        <v>1490</v>
+      </c>
+      <c r="E93" s="31">
+        <v>2</v>
+      </c>
+      <c r="F93" s="31">
+        <v>6</v>
+      </c>
+      <c r="G93" s="31">
+        <v>0</v>
+      </c>
+      <c r="H93" s="31">
+        <v>0</v>
+      </c>
+      <c r="I93" s="31">
+        <v>109</v>
+      </c>
+      <c r="J93" s="31">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="94" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A94" s="23">
+        <v>43994</v>
+      </c>
+      <c r="B94" s="24">
+        <v>87095</v>
+      </c>
+      <c r="C94" s="25">
+        <v>767</v>
+      </c>
+      <c r="D94" s="25">
+        <v>1492</v>
+      </c>
+      <c r="E94" s="25">
+        <v>2</v>
+      </c>
+      <c r="F94" s="25">
+        <v>6</v>
+      </c>
+      <c r="G94" s="25">
+        <v>0</v>
+      </c>
+      <c r="H94" s="25">
+        <v>0</v>
+      </c>
+      <c r="I94" s="25">
+        <v>109</v>
+      </c>
+      <c r="J94" s="25">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="95" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A95" s="29">
+        <v>43995</v>
+      </c>
+      <c r="B95" s="30">
+        <v>87386</v>
+      </c>
+      <c r="C95" s="31">
+        <v>291</v>
+      </c>
+      <c r="D95" s="31">
+        <v>1495</v>
+      </c>
+      <c r="E95" s="31">
+        <v>3</v>
+      </c>
+      <c r="F95" s="31">
+        <v>6</v>
+      </c>
+      <c r="G95" s="31">
+        <v>0</v>
+      </c>
+      <c r="H95" s="31">
+        <v>0</v>
+      </c>
+      <c r="I95" s="31">
+        <v>109</v>
+      </c>
+      <c r="J95" s="31">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="96" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A96" s="23">
+        <v>43996</v>
+      </c>
+      <c r="B96" s="24">
+        <v>87598</v>
+      </c>
+      <c r="C96" s="25">
+        <v>212</v>
+      </c>
+      <c r="D96" s="25">
+        <v>1496</v>
+      </c>
+      <c r="E96" s="25">
+        <v>1</v>
+      </c>
+      <c r="F96" s="25">
+        <v>7</v>
+      </c>
+      <c r="G96" s="25">
+        <v>1</v>
+      </c>
+      <c r="H96" s="25">
+        <v>0</v>
+      </c>
+      <c r="I96" s="25">
+        <v>109</v>
+      </c>
+      <c r="J96" s="25">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="97" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A97" s="20">
+        <v>43997</v>
+      </c>
+      <c r="B97" s="21">
+        <v>88165</v>
+      </c>
+      <c r="C97" s="22">
+        <v>567</v>
+      </c>
+      <c r="D97" s="22">
+        <v>1499</v>
+      </c>
+      <c r="E97" s="22">
+        <v>3</v>
+      </c>
+      <c r="F97" s="22">
+        <v>7</v>
+      </c>
+      <c r="G97" s="22">
+        <v>1</v>
+      </c>
+      <c r="H97" s="22">
+        <v>0</v>
+      </c>
+      <c r="I97" s="22">
+        <v>109</v>
+      </c>
+      <c r="J97" s="22">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="98" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A98" s="20">
+        <v>43998</v>
+      </c>
+      <c r="B98" s="21">
+        <v>89151</v>
+      </c>
+      <c r="C98" s="22">
+        <v>986</v>
+      </c>
+      <c r="D98" s="22">
+        <v>1503</v>
+      </c>
+      <c r="E98" s="22">
+        <v>4</v>
+      </c>
+      <c r="F98" s="22">
+        <v>7</v>
+      </c>
+      <c r="G98" s="22">
+        <v>1</v>
+      </c>
+      <c r="H98" s="22">
+        <v>0</v>
+      </c>
+      <c r="I98" s="22">
+        <v>109</v>
+      </c>
+      <c r="J98" s="22">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="99" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A99" s="29">
+        <v>43999</v>
+      </c>
+      <c r="B99" s="30">
+        <v>90103</v>
+      </c>
+      <c r="C99" s="31">
+        <v>952</v>
+      </c>
+      <c r="D99" s="31">
+        <v>1511</v>
+      </c>
+      <c r="E99" s="31">
+        <v>8</v>
+      </c>
+      <c r="F99" s="31">
+        <v>6</v>
+      </c>
+      <c r="G99" s="31">
+        <v>1</v>
+      </c>
+      <c r="H99" s="31">
+        <v>1</v>
+      </c>
+      <c r="I99" s="31">
+        <v>109</v>
+      </c>
+      <c r="J99" s="31">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="100" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A100" s="20">
+        <v>44000</v>
+      </c>
+      <c r="B100" s="21">
+        <v>91005</v>
+      </c>
+      <c r="C100" s="22">
+        <v>902</v>
+      </c>
+      <c r="D100" s="22">
+        <v>1513</v>
+      </c>
+      <c r="E100" s="22">
+        <v>2</v>
+      </c>
+      <c r="F100" s="22">
+        <v>8</v>
+      </c>
+      <c r="G100" s="22">
+        <v>1</v>
+      </c>
+      <c r="H100" s="22">
+        <v>0</v>
+      </c>
+      <c r="I100" s="22">
+        <v>109</v>
+      </c>
+      <c r="J100" s="22">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="101" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A101" s="29">
+        <v>44001</v>
+      </c>
+      <c r="B101" s="30">
+        <v>92152</v>
+      </c>
+      <c r="C101" s="31">
+        <v>1147</v>
+      </c>
+      <c r="D101" s="31">
+        <v>1519</v>
+      </c>
+      <c r="E101" s="31">
+        <v>6</v>
+      </c>
+      <c r="F101" s="31">
+        <v>6</v>
+      </c>
+      <c r="G101" s="31">
+        <v>1</v>
+      </c>
+      <c r="H101" s="31">
+        <v>2</v>
+      </c>
+      <c r="I101" s="31">
+        <v>109</v>
+      </c>
+      <c r="J101" s="31">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="102" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A102" s="23">
+        <v>44002</v>
+      </c>
+      <c r="B102" s="24">
+        <v>92919</v>
+      </c>
+      <c r="C102" s="25">
+        <v>758</v>
+      </c>
+      <c r="D102" s="25">
+        <v>1520</v>
+      </c>
+      <c r="E102" s="25">
+        <v>1</v>
+      </c>
+      <c r="F102" s="25">
+        <v>6</v>
+      </c>
+      <c r="G102" s="25">
+        <v>1</v>
+      </c>
+      <c r="H102" s="25">
+        <v>2</v>
+      </c>
+      <c r="I102" s="25">
+        <v>109</v>
+      </c>
+      <c r="J102" s="25">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="103" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A103" s="29">
+        <v>44003</v>
+      </c>
+      <c r="B103" s="30">
+        <v>93181</v>
+      </c>
+      <c r="C103" s="31">
+        <v>271</v>
+      </c>
+      <c r="D103" s="31">
+        <v>1521</v>
+      </c>
+      <c r="E103" s="31">
+        <v>1</v>
+      </c>
+      <c r="F103" s="31">
+        <v>6</v>
+      </c>
+      <c r="G103" s="31">
+        <v>1</v>
+      </c>
+      <c r="H103" s="31">
+        <v>0</v>
+      </c>
+      <c r="I103" s="31">
+        <v>109</v>
+      </c>
+      <c r="J103" s="31">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="104" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A104" s="29">
+        <v>44004</v>
+      </c>
+      <c r="B104" s="30">
+        <v>94165</v>
+      </c>
+      <c r="C104" s="31">
+        <v>984</v>
+      </c>
+      <c r="D104" s="31">
+        <v>1534</v>
+      </c>
+      <c r="E104" s="31">
+        <v>13</v>
+      </c>
+      <c r="F104" s="31">
+        <v>5</v>
+      </c>
+      <c r="G104" s="31">
+        <v>1</v>
+      </c>
+      <c r="H104" s="31">
+        <v>1</v>
+      </c>
+      <c r="I104" s="31">
+        <v>109</v>
+      </c>
+      <c r="J104" s="31">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="105" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A105" s="29">
+        <v>44005</v>
+      </c>
+      <c r="B105" s="30">
+        <v>95387</v>
+      </c>
+      <c r="C105" s="31">
+        <v>1222</v>
+      </c>
+      <c r="D105" s="31">
+        <v>1541</v>
+      </c>
+      <c r="E105" s="31">
+        <v>7</v>
+      </c>
+      <c r="F105" s="31">
+        <v>7</v>
+      </c>
+      <c r="G105" s="31">
+        <v>2</v>
+      </c>
+      <c r="H105" s="31">
+        <v>0</v>
+      </c>
+      <c r="I105" s="31" t="s">
+        <v>10</v>
+      </c>
+      <c r="J105" s="31">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="106" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A106" s="23">
+        <v>44006</v>
+      </c>
+      <c r="B106" s="24">
+        <v>96599</v>
+      </c>
+      <c r="C106" s="25">
+        <v>1212</v>
+      </c>
+      <c r="D106" s="25">
+        <v>1547</v>
+      </c>
+      <c r="E106" s="25">
+        <v>6</v>
+      </c>
+      <c r="F106" s="25">
+        <v>7</v>
+      </c>
+      <c r="G106" s="25">
+        <v>2</v>
+      </c>
+      <c r="H106" s="25">
+        <v>0</v>
+      </c>
+      <c r="I106" s="25" t="s">
+        <v>10</v>
+      </c>
+      <c r="J106" s="25">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="107" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A107" s="29">
+        <v>44007</v>
+      </c>
+      <c r="B107" s="30">
+        <v>97442</v>
+      </c>
+      <c r="C107" s="31">
+        <v>843</v>
+      </c>
+      <c r="D107" s="31">
+        <v>1558</v>
+      </c>
+      <c r="E107" s="31">
+        <v>11</v>
+      </c>
+      <c r="F107" s="31">
+        <v>8</v>
+      </c>
+      <c r="G107" s="31">
+        <v>2</v>
+      </c>
+      <c r="H107" s="31">
+        <v>0</v>
+      </c>
+      <c r="I107" s="31" t="s">
+        <v>10</v>
+      </c>
+      <c r="J107" s="31">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="108" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A108" s="29">
+        <v>44008</v>
+      </c>
+      <c r="B108" s="30">
+        <v>98320</v>
+      </c>
+      <c r="C108" s="31">
+        <v>878</v>
+      </c>
+      <c r="D108" s="31">
+        <v>1572</v>
+      </c>
+      <c r="E108" s="31">
+        <v>14</v>
+      </c>
+      <c r="F108" s="31">
+        <v>8</v>
+      </c>
+      <c r="G108" s="31">
+        <v>1</v>
+      </c>
+      <c r="H108" s="31">
+        <v>0</v>
+      </c>
+      <c r="I108" s="31" t="s">
+        <v>10</v>
+      </c>
+      <c r="J108" s="31">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="109" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A109" s="29">
+        <v>44009</v>
+      </c>
+      <c r="B109" s="30">
+        <v>98945</v>
+      </c>
+      <c r="C109" s="31">
+        <v>625</v>
+      </c>
+      <c r="D109" s="31">
+        <v>1581</v>
+      </c>
+      <c r="E109" s="31">
+        <v>9</v>
+      </c>
+      <c r="F109" s="31">
+        <v>7</v>
+      </c>
+      <c r="G109" s="31">
+        <v>0</v>
+      </c>
+      <c r="H109" s="31">
+        <v>1</v>
+      </c>
+      <c r="I109" s="31" t="s">
+        <v>10</v>
+      </c>
+      <c r="J109" s="31">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="110" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A110" s="29">
+        <v>44010</v>
+      </c>
+      <c r="B110" s="30">
+        <v>99245</v>
+      </c>
+      <c r="C110" s="31">
+        <v>300</v>
+      </c>
+      <c r="D110" s="31">
+        <v>1585</v>
+      </c>
+      <c r="E110" s="31">
+        <v>4</v>
+      </c>
+      <c r="F110" s="31">
+        <v>8</v>
+      </c>
+      <c r="G110" s="31">
+        <v>0</v>
+      </c>
+      <c r="H110" s="31">
+        <v>0</v>
+      </c>
+      <c r="I110" s="31" t="s">
+        <v>10</v>
+      </c>
+      <c r="J110" s="31">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="111" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A111" s="29">
+        <v>44011</v>
+      </c>
+      <c r="B111" s="30">
+        <v>100330</v>
+      </c>
+      <c r="C111" s="31">
+        <v>1085</v>
+      </c>
+      <c r="D111" s="31">
+        <v>1600</v>
+      </c>
+      <c r="E111" s="31">
+        <v>15</v>
+      </c>
+      <c r="F111" s="31">
+        <v>8</v>
+      </c>
+      <c r="G111" s="31">
+        <v>0</v>
+      </c>
+      <c r="H111" s="31">
+        <v>0</v>
+      </c>
+      <c r="I111" s="31" t="s">
+        <v>10</v>
+      </c>
+      <c r="J111" s="31">
+        <v>0</v>
+      </c>
+    </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>

</xml_diff>

<commit_message>
Data updated by GitHub Bot (2020-06-30 20)
</commit_message>
<xml_diff>
--- a/output/snapshot/fdcf2531-4c3e-5c02-b63c-ee160ead6dea.xlsx
+++ b/output/snapshot/fdcf2531-4c3e-5c02-b63c-ee160ead6dea.xlsx
@@ -1,16 +1,15 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="21929"/>
-  <workbookPr/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
+  <fileVersion appName="xl" lastEdited="6" lowestEdited="6" rupBuild="14420"/>
+  <workbookPr defaultThemeVersion="164011"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="I:\AKTUALNI PODATKI - KORONA\Za objavo na GOV.SI\ang\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{1E6DD62F-2BE2-47DC-A7ED-9B57C1589256}" xr6:coauthVersionLast="44" xr6:coauthVersionMax="44" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840"/>
   </bookViews>
   <sheets>
     <sheet name="Covid-19 podatki" sheetId="1" r:id="rId1"/>
@@ -25,7 +24,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="10" uniqueCount="10">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="17" uniqueCount="11">
   <si>
     <t>Date</t>
   </si>
@@ -56,15 +55,18 @@
   <si>
     <t>Deaths (daily)</t>
   </si>
+  <si>
+    <t>111*</t>
+  </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" mc:Ignorable="x14ac x16r2">
   <numFmts count="1">
     <numFmt numFmtId="164" formatCode="d/\ m/\ yyyy;@"/>
   </numFmts>
-  <fonts count="4" x14ac:knownFonts="1">
+  <fonts count="5" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -93,6 +95,13 @@
       <name val="Calibri Light"/>
       <scheme val="major"/>
     </font>
+    <font>
+      <sz val="10"/>
+      <color theme="1"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
   </fonts>
   <fills count="3">
     <fill>
@@ -108,7 +117,7 @@
       </patternFill>
     </fill>
   </fills>
-  <borders count="2">
+  <borders count="3">
     <border>
       <left/>
       <right/>
@@ -129,11 +138,26 @@
       <bottom/>
       <diagonal/>
     </border>
+    <border>
+      <left style="thin">
+        <color theme="4"/>
+      </left>
+      <right style="thin">
+        <color theme="4"/>
+      </right>
+      <top style="thin">
+        <color theme="4"/>
+      </top>
+      <bottom style="thin">
+        <color theme="4"/>
+      </bottom>
+      <diagonal/>
+    </border>
   </borders>
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="26">
+  <cellXfs count="32">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="49" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyAlignment="1" applyProtection="1">
       <alignment horizontal="left" vertical="top"/>
@@ -208,6 +232,24 @@
       <alignment horizontal="right"/>
     </xf>
     <xf numFmtId="0" fontId="3" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="right"/>
+    </xf>
+    <xf numFmtId="164" fontId="4" fillId="2" borderId="2" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="right" vertical="top"/>
+    </xf>
+    <xf numFmtId="3" fontId="4" fillId="2" borderId="2" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="right"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="2" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="right"/>
+    </xf>
+    <xf numFmtId="164" fontId="3" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="right" vertical="top"/>
+    </xf>
+    <xf numFmtId="3" fontId="3" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="right"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="right"/>
     </xf>
   </cellXfs>
@@ -399,8 +441,8 @@
 </file>
 
 <file path=xl/tables/table1.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="1" xr:uid="{00000000-000C-0000-FFFF-FFFF00000000}" name="Tabela1" displayName="Tabela1" ref="A1:J75" totalsRowShown="0" headerRowDxfId="11" dataDxfId="10">
-  <autoFilter ref="A1:J75" xr:uid="{00000000-0009-0000-0100-000001000000}">
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="1" name="Tabela1" displayName="Tabela1" ref="A1:J111" totalsRowShown="0" headerRowDxfId="11" dataDxfId="10">
+  <autoFilter ref="A1:J111">
     <filterColumn colId="0" hiddenButton="1"/>
     <filterColumn colId="1" hiddenButton="1"/>
     <filterColumn colId="2" hiddenButton="1"/>
@@ -413,16 +455,16 @@
     <filterColumn colId="9" hiddenButton="1"/>
   </autoFilter>
   <tableColumns count="10">
-    <tableColumn id="1" xr3:uid="{00000000-0010-0000-0000-000001000000}" name="Date" dataDxfId="9"/>
-    <tableColumn id="2" xr3:uid="{00000000-0010-0000-0000-000002000000}" name="Tested (all)" dataDxfId="8"/>
-    <tableColumn id="3" xr3:uid="{00000000-0010-0000-0000-000003000000}" name="Tested (daily)" dataDxfId="7"/>
-    <tableColumn id="4" xr3:uid="{00000000-0010-0000-0000-000004000000}" name="Positive (all)" dataDxfId="6"/>
-    <tableColumn id="5" xr3:uid="{00000000-0010-0000-0000-000005000000}" name="Positive (daily)" dataDxfId="5"/>
-    <tableColumn id="6" xr3:uid="{00000000-0010-0000-0000-000006000000}" name="All hospitalized on certain day" dataDxfId="4"/>
-    <tableColumn id="7" xr3:uid="{00000000-0010-0000-0000-000007000000}" name="All persons in intensive care on certain day" dataDxfId="3"/>
-    <tableColumn id="10" xr3:uid="{00000000-0010-0000-0000-00000A000000}" name="Discharged" dataDxfId="2"/>
-    <tableColumn id="8" xr3:uid="{00000000-0010-0000-0000-000008000000}" name="Deaths (all)" dataDxfId="1"/>
-    <tableColumn id="9" xr3:uid="{00000000-0010-0000-0000-000009000000}" name="Deaths (daily)" dataDxfId="0"/>
+    <tableColumn id="1" name="Date" dataDxfId="9"/>
+    <tableColumn id="2" name="Tested (all)" dataDxfId="8"/>
+    <tableColumn id="3" name="Tested (daily)" dataDxfId="7"/>
+    <tableColumn id="4" name="Positive (all)" dataDxfId="6"/>
+    <tableColumn id="5" name="Positive (daily)" dataDxfId="5"/>
+    <tableColumn id="6" name="All hospitalized on certain day" dataDxfId="4"/>
+    <tableColumn id="7" name="All persons in intensive care on certain day" dataDxfId="3"/>
+    <tableColumn id="10" name="Discharged" dataDxfId="2"/>
+    <tableColumn id="8" name="Deaths (all)" dataDxfId="1"/>
+    <tableColumn id="9" name="Deaths (daily)" dataDxfId="0"/>
   </tableColumns>
   <tableStyleInfo name="TableStyleLight16" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
   <extLst>
@@ -695,11 +737,11 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:J75"/>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <dimension ref="A1:J111"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A40" zoomScale="89" zoomScaleNormal="89" workbookViewId="0">
-      <selection activeCell="J74" sqref="J74"/>
+    <sheetView tabSelected="1" topLeftCell="A83" zoomScale="89" zoomScaleNormal="89" workbookViewId="0">
+      <selection activeCell="C114" sqref="C114"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -3117,6 +3159,1158 @@
         <v>0</v>
       </c>
     </row>
+    <row r="76" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A76" s="20">
+        <v>43976</v>
+      </c>
+      <c r="B76" s="21">
+        <v>75770</v>
+      </c>
+      <c r="C76" s="22">
+        <v>754</v>
+      </c>
+      <c r="D76" s="22">
+        <v>1469</v>
+      </c>
+      <c r="E76" s="22">
+        <v>0</v>
+      </c>
+      <c r="F76" s="22">
+        <v>9</v>
+      </c>
+      <c r="G76" s="22">
+        <v>2</v>
+      </c>
+      <c r="H76" s="22">
+        <v>6</v>
+      </c>
+      <c r="I76" s="22">
+        <v>108</v>
+      </c>
+      <c r="J76" s="22">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="77" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A77" s="20">
+        <v>43977</v>
+      </c>
+      <c r="B77" s="21">
+        <v>76579</v>
+      </c>
+      <c r="C77" s="22">
+        <v>809</v>
+      </c>
+      <c r="D77" s="22">
+        <v>1471</v>
+      </c>
+      <c r="E77" s="22">
+        <v>2</v>
+      </c>
+      <c r="F77" s="22">
+        <v>8</v>
+      </c>
+      <c r="G77" s="22">
+        <v>2</v>
+      </c>
+      <c r="H77" s="22">
+        <v>2</v>
+      </c>
+      <c r="I77" s="22">
+        <v>108</v>
+      </c>
+      <c r="J77" s="22">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="78" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A78" s="20">
+        <v>43978</v>
+      </c>
+      <c r="B78" s="21">
+        <v>77210</v>
+      </c>
+      <c r="C78" s="22">
+        <v>631</v>
+      </c>
+      <c r="D78" s="22">
+        <v>1473</v>
+      </c>
+      <c r="E78" s="22">
+        <v>2</v>
+      </c>
+      <c r="F78" s="22">
+        <v>7</v>
+      </c>
+      <c r="G78" s="22">
+        <v>2</v>
+      </c>
+      <c r="H78" s="22">
+        <v>1</v>
+      </c>
+      <c r="I78" s="22">
+        <v>108</v>
+      </c>
+      <c r="J78" s="22">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="79" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A79" s="20">
+        <v>43979</v>
+      </c>
+      <c r="B79" s="21">
+        <v>77916</v>
+      </c>
+      <c r="C79" s="22">
+        <v>706</v>
+      </c>
+      <c r="D79" s="22">
+        <v>1473</v>
+      </c>
+      <c r="E79" s="22">
+        <v>0</v>
+      </c>
+      <c r="F79" s="22">
+        <v>7</v>
+      </c>
+      <c r="G79" s="22">
+        <v>2</v>
+      </c>
+      <c r="H79" s="22">
+        <v>0</v>
+      </c>
+      <c r="I79" s="22">
+        <v>108</v>
+      </c>
+      <c r="J79" s="22">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="80" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A80" s="20">
+        <v>43980</v>
+      </c>
+      <c r="B80" s="21">
+        <v>78529</v>
+      </c>
+      <c r="C80" s="22">
+        <v>613</v>
+      </c>
+      <c r="D80" s="22">
+        <v>1473</v>
+      </c>
+      <c r="E80" s="22">
+        <v>0</v>
+      </c>
+      <c r="F80" s="22">
+        <v>7</v>
+      </c>
+      <c r="G80" s="22">
+        <v>2</v>
+      </c>
+      <c r="H80" s="22">
+        <v>0</v>
+      </c>
+      <c r="I80" s="22">
+        <v>108</v>
+      </c>
+      <c r="J80" s="22">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="81" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A81" s="20">
+        <v>43981</v>
+      </c>
+      <c r="B81" s="22">
+        <v>78793</v>
+      </c>
+      <c r="C81" s="22">
+        <v>264</v>
+      </c>
+      <c r="D81" s="22">
+        <v>1473</v>
+      </c>
+      <c r="E81" s="22">
+        <v>0</v>
+      </c>
+      <c r="F81" s="22">
+        <v>6</v>
+      </c>
+      <c r="G81" s="22">
+        <v>2</v>
+      </c>
+      <c r="H81" s="22">
+        <v>1</v>
+      </c>
+      <c r="I81" s="22">
+        <v>108</v>
+      </c>
+      <c r="J81" s="22">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="82" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A82" s="20">
+        <v>43982</v>
+      </c>
+      <c r="B82" s="21">
+        <v>79039</v>
+      </c>
+      <c r="C82" s="22">
+        <v>246</v>
+      </c>
+      <c r="D82" s="22">
+        <v>1473</v>
+      </c>
+      <c r="E82" s="22">
+        <v>0</v>
+      </c>
+      <c r="F82" s="22">
+        <v>5</v>
+      </c>
+      <c r="G82" s="22">
+        <v>1</v>
+      </c>
+      <c r="H82" s="22">
+        <v>0</v>
+      </c>
+      <c r="I82" s="22">
+        <v>109</v>
+      </c>
+      <c r="J82" s="22">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="83" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A83" s="20">
+        <v>43983</v>
+      </c>
+      <c r="B83" s="21">
+        <v>79698</v>
+      </c>
+      <c r="C83" s="22">
+        <v>659</v>
+      </c>
+      <c r="D83" s="22">
+        <v>1475</v>
+      </c>
+      <c r="E83" s="22">
+        <v>2</v>
+      </c>
+      <c r="F83" s="22">
+        <v>5</v>
+      </c>
+      <c r="G83" s="22">
+        <v>1</v>
+      </c>
+      <c r="H83" s="22">
+        <v>0</v>
+      </c>
+      <c r="I83" s="22">
+        <v>109</v>
+      </c>
+      <c r="J83" s="22">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="84" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A84" s="20">
+        <v>43984</v>
+      </c>
+      <c r="B84" s="21">
+        <v>80505</v>
+      </c>
+      <c r="C84" s="22">
+        <v>807</v>
+      </c>
+      <c r="D84" s="22">
+        <v>1477</v>
+      </c>
+      <c r="E84" s="22">
+        <v>2</v>
+      </c>
+      <c r="F84" s="22">
+        <v>5</v>
+      </c>
+      <c r="G84" s="22">
+        <v>0</v>
+      </c>
+      <c r="H84" s="22">
+        <v>0</v>
+      </c>
+      <c r="I84" s="22">
+        <v>109</v>
+      </c>
+      <c r="J84" s="22">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="85" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A85" s="20">
+        <v>43985</v>
+      </c>
+      <c r="B85" s="21">
+        <v>81333</v>
+      </c>
+      <c r="C85" s="22">
+        <v>828</v>
+      </c>
+      <c r="D85" s="22">
+        <v>1477</v>
+      </c>
+      <c r="E85" s="22">
+        <v>0</v>
+      </c>
+      <c r="F85" s="22">
+        <v>5</v>
+      </c>
+      <c r="G85" s="22">
+        <v>0</v>
+      </c>
+      <c r="H85" s="22">
+        <v>0</v>
+      </c>
+      <c r="I85" s="22">
+        <v>109</v>
+      </c>
+      <c r="J85" s="22">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="86" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A86" s="26">
+        <v>43986</v>
+      </c>
+      <c r="B86" s="27">
+        <v>82161</v>
+      </c>
+      <c r="C86" s="28">
+        <v>828</v>
+      </c>
+      <c r="D86" s="28">
+        <v>1479</v>
+      </c>
+      <c r="E86" s="28">
+        <v>2</v>
+      </c>
+      <c r="F86" s="28">
+        <v>6</v>
+      </c>
+      <c r="G86" s="28">
+        <v>0</v>
+      </c>
+      <c r="H86" s="28">
+        <v>0</v>
+      </c>
+      <c r="I86" s="28">
+        <v>109</v>
+      </c>
+      <c r="J86" s="28">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="87" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A87" s="29">
+        <v>43987</v>
+      </c>
+      <c r="B87" s="30">
+        <v>82876</v>
+      </c>
+      <c r="C87" s="31">
+        <v>715</v>
+      </c>
+      <c r="D87" s="31">
+        <v>1484</v>
+      </c>
+      <c r="E87" s="31">
+        <v>5</v>
+      </c>
+      <c r="F87" s="31">
+        <v>6</v>
+      </c>
+      <c r="G87" s="31">
+        <v>0</v>
+      </c>
+      <c r="H87" s="31">
+        <v>0</v>
+      </c>
+      <c r="I87" s="31">
+        <v>109</v>
+      </c>
+      <c r="J87" s="31">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="88" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A88" s="23">
+        <v>43988</v>
+      </c>
+      <c r="B88" s="24">
+        <v>83105</v>
+      </c>
+      <c r="C88" s="25">
+        <v>229</v>
+      </c>
+      <c r="D88" s="25">
+        <v>1485</v>
+      </c>
+      <c r="E88" s="25">
+        <v>1</v>
+      </c>
+      <c r="F88" s="25">
+        <v>5</v>
+      </c>
+      <c r="G88" s="25">
+        <v>0</v>
+      </c>
+      <c r="H88" s="25">
+        <v>1</v>
+      </c>
+      <c r="I88" s="25">
+        <v>109</v>
+      </c>
+      <c r="J88" s="25">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="89" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A89" s="29">
+        <v>43989</v>
+      </c>
+      <c r="B89" s="30">
+        <v>83316</v>
+      </c>
+      <c r="C89" s="31">
+        <v>211</v>
+      </c>
+      <c r="D89" s="31">
+        <v>1485</v>
+      </c>
+      <c r="E89" s="31">
+        <v>0</v>
+      </c>
+      <c r="F89" s="31">
+        <v>5</v>
+      </c>
+      <c r="G89" s="31">
+        <v>0</v>
+      </c>
+      <c r="H89" s="31">
+        <v>0</v>
+      </c>
+      <c r="I89" s="31">
+        <v>109</v>
+      </c>
+      <c r="J89" s="31">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="90" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A90" s="20">
+        <v>43990</v>
+      </c>
+      <c r="B90" s="21">
+        <v>84130</v>
+      </c>
+      <c r="C90" s="22">
+        <v>814</v>
+      </c>
+      <c r="D90" s="22">
+        <v>1486</v>
+      </c>
+      <c r="E90" s="22">
+        <v>1</v>
+      </c>
+      <c r="F90" s="22">
+        <v>6</v>
+      </c>
+      <c r="G90" s="22">
+        <v>0</v>
+      </c>
+      <c r="H90" s="22">
+        <v>0</v>
+      </c>
+      <c r="I90" s="22">
+        <v>109</v>
+      </c>
+      <c r="J90" s="22">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="91" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A91" s="20">
+        <v>43991</v>
+      </c>
+      <c r="B91" s="21">
+        <v>84868</v>
+      </c>
+      <c r="C91" s="22">
+        <v>738</v>
+      </c>
+      <c r="D91" s="22">
+        <v>1488</v>
+      </c>
+      <c r="E91" s="22">
+        <v>2</v>
+      </c>
+      <c r="F91" s="22">
+        <v>6</v>
+      </c>
+      <c r="G91" s="22">
+        <v>0</v>
+      </c>
+      <c r="H91" s="22">
+        <v>0</v>
+      </c>
+      <c r="I91" s="22">
+        <v>109</v>
+      </c>
+      <c r="J91" s="22">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="92" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A92" s="23">
+        <v>43992</v>
+      </c>
+      <c r="B92" s="24">
+        <v>85626</v>
+      </c>
+      <c r="C92" s="25">
+        <v>758</v>
+      </c>
+      <c r="D92" s="25">
+        <v>1488</v>
+      </c>
+      <c r="E92" s="25">
+        <v>0</v>
+      </c>
+      <c r="F92" s="25">
+        <v>6</v>
+      </c>
+      <c r="G92" s="25">
+        <v>0</v>
+      </c>
+      <c r="H92" s="25">
+        <v>0</v>
+      </c>
+      <c r="I92" s="25">
+        <v>109</v>
+      </c>
+      <c r="J92" s="25">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="93" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A93" s="29">
+        <v>43993</v>
+      </c>
+      <c r="B93" s="30">
+        <v>86328</v>
+      </c>
+      <c r="C93" s="31">
+        <v>702</v>
+      </c>
+      <c r="D93" s="31">
+        <v>1490</v>
+      </c>
+      <c r="E93" s="31">
+        <v>2</v>
+      </c>
+      <c r="F93" s="31">
+        <v>6</v>
+      </c>
+      <c r="G93" s="31">
+        <v>0</v>
+      </c>
+      <c r="H93" s="31">
+        <v>0</v>
+      </c>
+      <c r="I93" s="31">
+        <v>109</v>
+      </c>
+      <c r="J93" s="31">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="94" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A94" s="23">
+        <v>43994</v>
+      </c>
+      <c r="B94" s="24">
+        <v>87095</v>
+      </c>
+      <c r="C94" s="25">
+        <v>767</v>
+      </c>
+      <c r="D94" s="25">
+        <v>1492</v>
+      </c>
+      <c r="E94" s="25">
+        <v>2</v>
+      </c>
+      <c r="F94" s="25">
+        <v>6</v>
+      </c>
+      <c r="G94" s="25">
+        <v>0</v>
+      </c>
+      <c r="H94" s="25">
+        <v>0</v>
+      </c>
+      <c r="I94" s="25">
+        <v>109</v>
+      </c>
+      <c r="J94" s="25">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="95" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A95" s="29">
+        <v>43995</v>
+      </c>
+      <c r="B95" s="30">
+        <v>87386</v>
+      </c>
+      <c r="C95" s="31">
+        <v>291</v>
+      </c>
+      <c r="D95" s="31">
+        <v>1495</v>
+      </c>
+      <c r="E95" s="31">
+        <v>3</v>
+      </c>
+      <c r="F95" s="31">
+        <v>6</v>
+      </c>
+      <c r="G95" s="31">
+        <v>0</v>
+      </c>
+      <c r="H95" s="31">
+        <v>0</v>
+      </c>
+      <c r="I95" s="31">
+        <v>109</v>
+      </c>
+      <c r="J95" s="31">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="96" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A96" s="23">
+        <v>43996</v>
+      </c>
+      <c r="B96" s="24">
+        <v>87598</v>
+      </c>
+      <c r="C96" s="25">
+        <v>212</v>
+      </c>
+      <c r="D96" s="25">
+        <v>1496</v>
+      </c>
+      <c r="E96" s="25">
+        <v>1</v>
+      </c>
+      <c r="F96" s="25">
+        <v>7</v>
+      </c>
+      <c r="G96" s="25">
+        <v>1</v>
+      </c>
+      <c r="H96" s="25">
+        <v>0</v>
+      </c>
+      <c r="I96" s="25">
+        <v>109</v>
+      </c>
+      <c r="J96" s="25">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="97" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A97" s="20">
+        <v>43997</v>
+      </c>
+      <c r="B97" s="21">
+        <v>88165</v>
+      </c>
+      <c r="C97" s="22">
+        <v>567</v>
+      </c>
+      <c r="D97" s="22">
+        <v>1499</v>
+      </c>
+      <c r="E97" s="22">
+        <v>3</v>
+      </c>
+      <c r="F97" s="22">
+        <v>7</v>
+      </c>
+      <c r="G97" s="22">
+        <v>1</v>
+      </c>
+      <c r="H97" s="22">
+        <v>0</v>
+      </c>
+      <c r="I97" s="22">
+        <v>109</v>
+      </c>
+      <c r="J97" s="22">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="98" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A98" s="20">
+        <v>43998</v>
+      </c>
+      <c r="B98" s="21">
+        <v>89151</v>
+      </c>
+      <c r="C98" s="22">
+        <v>986</v>
+      </c>
+      <c r="D98" s="22">
+        <v>1503</v>
+      </c>
+      <c r="E98" s="22">
+        <v>4</v>
+      </c>
+      <c r="F98" s="22">
+        <v>7</v>
+      </c>
+      <c r="G98" s="22">
+        <v>1</v>
+      </c>
+      <c r="H98" s="22">
+        <v>0</v>
+      </c>
+      <c r="I98" s="22">
+        <v>109</v>
+      </c>
+      <c r="J98" s="22">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="99" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A99" s="29">
+        <v>43999</v>
+      </c>
+      <c r="B99" s="30">
+        <v>90103</v>
+      </c>
+      <c r="C99" s="31">
+        <v>952</v>
+      </c>
+      <c r="D99" s="31">
+        <v>1511</v>
+      </c>
+      <c r="E99" s="31">
+        <v>8</v>
+      </c>
+      <c r="F99" s="31">
+        <v>6</v>
+      </c>
+      <c r="G99" s="31">
+        <v>1</v>
+      </c>
+      <c r="H99" s="31">
+        <v>1</v>
+      </c>
+      <c r="I99" s="31">
+        <v>109</v>
+      </c>
+      <c r="J99" s="31">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="100" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A100" s="20">
+        <v>44000</v>
+      </c>
+      <c r="B100" s="21">
+        <v>91005</v>
+      </c>
+      <c r="C100" s="22">
+        <v>902</v>
+      </c>
+      <c r="D100" s="22">
+        <v>1513</v>
+      </c>
+      <c r="E100" s="22">
+        <v>2</v>
+      </c>
+      <c r="F100" s="22">
+        <v>8</v>
+      </c>
+      <c r="G100" s="22">
+        <v>1</v>
+      </c>
+      <c r="H100" s="22">
+        <v>0</v>
+      </c>
+      <c r="I100" s="22">
+        <v>109</v>
+      </c>
+      <c r="J100" s="22">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="101" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A101" s="29">
+        <v>44001</v>
+      </c>
+      <c r="B101" s="30">
+        <v>92152</v>
+      </c>
+      <c r="C101" s="31">
+        <v>1147</v>
+      </c>
+      <c r="D101" s="31">
+        <v>1519</v>
+      </c>
+      <c r="E101" s="31">
+        <v>6</v>
+      </c>
+      <c r="F101" s="31">
+        <v>6</v>
+      </c>
+      <c r="G101" s="31">
+        <v>1</v>
+      </c>
+      <c r="H101" s="31">
+        <v>2</v>
+      </c>
+      <c r="I101" s="31">
+        <v>109</v>
+      </c>
+      <c r="J101" s="31">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="102" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A102" s="23">
+        <v>44002</v>
+      </c>
+      <c r="B102" s="24">
+        <v>92919</v>
+      </c>
+      <c r="C102" s="25">
+        <v>758</v>
+      </c>
+      <c r="D102" s="25">
+        <v>1520</v>
+      </c>
+      <c r="E102" s="25">
+        <v>1</v>
+      </c>
+      <c r="F102" s="25">
+        <v>6</v>
+      </c>
+      <c r="G102" s="25">
+        <v>1</v>
+      </c>
+      <c r="H102" s="25">
+        <v>2</v>
+      </c>
+      <c r="I102" s="25">
+        <v>109</v>
+      </c>
+      <c r="J102" s="25">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="103" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A103" s="29">
+        <v>44003</v>
+      </c>
+      <c r="B103" s="30">
+        <v>93181</v>
+      </c>
+      <c r="C103" s="31">
+        <v>271</v>
+      </c>
+      <c r="D103" s="31">
+        <v>1521</v>
+      </c>
+      <c r="E103" s="31">
+        <v>1</v>
+      </c>
+      <c r="F103" s="31">
+        <v>6</v>
+      </c>
+      <c r="G103" s="31">
+        <v>1</v>
+      </c>
+      <c r="H103" s="31">
+        <v>0</v>
+      </c>
+      <c r="I103" s="31">
+        <v>109</v>
+      </c>
+      <c r="J103" s="31">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="104" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A104" s="29">
+        <v>44004</v>
+      </c>
+      <c r="B104" s="30">
+        <v>94165</v>
+      </c>
+      <c r="C104" s="31">
+        <v>984</v>
+      </c>
+      <c r="D104" s="31">
+        <v>1534</v>
+      </c>
+      <c r="E104" s="31">
+        <v>13</v>
+      </c>
+      <c r="F104" s="31">
+        <v>5</v>
+      </c>
+      <c r="G104" s="31">
+        <v>1</v>
+      </c>
+      <c r="H104" s="31">
+        <v>1</v>
+      </c>
+      <c r="I104" s="31">
+        <v>109</v>
+      </c>
+      <c r="J104" s="31">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="105" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A105" s="29">
+        <v>44005</v>
+      </c>
+      <c r="B105" s="30">
+        <v>95387</v>
+      </c>
+      <c r="C105" s="31">
+        <v>1222</v>
+      </c>
+      <c r="D105" s="31">
+        <v>1541</v>
+      </c>
+      <c r="E105" s="31">
+        <v>7</v>
+      </c>
+      <c r="F105" s="31">
+        <v>7</v>
+      </c>
+      <c r="G105" s="31">
+        <v>2</v>
+      </c>
+      <c r="H105" s="31">
+        <v>0</v>
+      </c>
+      <c r="I105" s="31" t="s">
+        <v>10</v>
+      </c>
+      <c r="J105" s="31">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="106" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A106" s="23">
+        <v>44006</v>
+      </c>
+      <c r="B106" s="24">
+        <v>96599</v>
+      </c>
+      <c r="C106" s="25">
+        <v>1212</v>
+      </c>
+      <c r="D106" s="25">
+        <v>1547</v>
+      </c>
+      <c r="E106" s="25">
+        <v>6</v>
+      </c>
+      <c r="F106" s="25">
+        <v>7</v>
+      </c>
+      <c r="G106" s="25">
+        <v>2</v>
+      </c>
+      <c r="H106" s="25">
+        <v>0</v>
+      </c>
+      <c r="I106" s="25" t="s">
+        <v>10</v>
+      </c>
+      <c r="J106" s="25">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="107" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A107" s="29">
+        <v>44007</v>
+      </c>
+      <c r="B107" s="30">
+        <v>97442</v>
+      </c>
+      <c r="C107" s="31">
+        <v>843</v>
+      </c>
+      <c r="D107" s="31">
+        <v>1558</v>
+      </c>
+      <c r="E107" s="31">
+        <v>11</v>
+      </c>
+      <c r="F107" s="31">
+        <v>8</v>
+      </c>
+      <c r="G107" s="31">
+        <v>2</v>
+      </c>
+      <c r="H107" s="31">
+        <v>0</v>
+      </c>
+      <c r="I107" s="31" t="s">
+        <v>10</v>
+      </c>
+      <c r="J107" s="31">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="108" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A108" s="29">
+        <v>44008</v>
+      </c>
+      <c r="B108" s="30">
+        <v>98320</v>
+      </c>
+      <c r="C108" s="31">
+        <v>878</v>
+      </c>
+      <c r="D108" s="31">
+        <v>1572</v>
+      </c>
+      <c r="E108" s="31">
+        <v>14</v>
+      </c>
+      <c r="F108" s="31">
+        <v>8</v>
+      </c>
+      <c r="G108" s="31">
+        <v>1</v>
+      </c>
+      <c r="H108" s="31">
+        <v>0</v>
+      </c>
+      <c r="I108" s="31" t="s">
+        <v>10</v>
+      </c>
+      <c r="J108" s="31">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="109" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A109" s="29">
+        <v>44009</v>
+      </c>
+      <c r="B109" s="30">
+        <v>98945</v>
+      </c>
+      <c r="C109" s="31">
+        <v>625</v>
+      </c>
+      <c r="D109" s="31">
+        <v>1581</v>
+      </c>
+      <c r="E109" s="31">
+        <v>9</v>
+      </c>
+      <c r="F109" s="31">
+        <v>7</v>
+      </c>
+      <c r="G109" s="31">
+        <v>0</v>
+      </c>
+      <c r="H109" s="31">
+        <v>1</v>
+      </c>
+      <c r="I109" s="31" t="s">
+        <v>10</v>
+      </c>
+      <c r="J109" s="31">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="110" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A110" s="29">
+        <v>44010</v>
+      </c>
+      <c r="B110" s="30">
+        <v>99245</v>
+      </c>
+      <c r="C110" s="31">
+        <v>300</v>
+      </c>
+      <c r="D110" s="31">
+        <v>1585</v>
+      </c>
+      <c r="E110" s="31">
+        <v>4</v>
+      </c>
+      <c r="F110" s="31">
+        <v>8</v>
+      </c>
+      <c r="G110" s="31">
+        <v>0</v>
+      </c>
+      <c r="H110" s="31">
+        <v>0</v>
+      </c>
+      <c r="I110" s="31" t="s">
+        <v>10</v>
+      </c>
+      <c r="J110" s="31">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="111" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A111" s="29">
+        <v>44011</v>
+      </c>
+      <c r="B111" s="30">
+        <v>100330</v>
+      </c>
+      <c r="C111" s="31">
+        <v>1085</v>
+      </c>
+      <c r="D111" s="31">
+        <v>1600</v>
+      </c>
+      <c r="E111" s="31">
+        <v>15</v>
+      </c>
+      <c r="F111" s="31">
+        <v>8</v>
+      </c>
+      <c r="G111" s="31">
+        <v>0</v>
+      </c>
+      <c r="H111" s="31">
+        <v>0</v>
+      </c>
+      <c r="I111" s="31" t="s">
+        <v>10</v>
+      </c>
+      <c r="J111" s="31">
+        <v>0</v>
+      </c>
+    </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>

</xml_diff>

<commit_message>
Data updated by GitHub Bot (2020-07-01 12)
</commit_message>
<xml_diff>
--- a/output/snapshot/fdcf2531-4c3e-5c02-b63c-ee160ead6dea.xlsx
+++ b/output/snapshot/fdcf2531-4c3e-5c02-b63c-ee160ead6dea.xlsx
@@ -1,16 +1,15 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="21929"/>
-  <workbookPr/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
+  <fileVersion appName="xl" lastEdited="6" lowestEdited="6" rupBuild="14420"/>
+  <workbookPr defaultThemeVersion="164011"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="I:\AKTUALNI PODATKI - KORONA\Za objavo na GOV.SI\ang\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{1E6DD62F-2BE2-47DC-A7ED-9B57C1589256}" xr6:coauthVersionLast="44" xr6:coauthVersionMax="44" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840"/>
   </bookViews>
   <sheets>
     <sheet name="Covid-19 podatki" sheetId="1" r:id="rId1"/>
@@ -25,7 +24,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="10" uniqueCount="10">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="18" uniqueCount="11">
   <si>
     <t>Date</t>
   </si>
@@ -56,15 +55,18 @@
   <si>
     <t>Deaths (daily)</t>
   </si>
+  <si>
+    <t>111*</t>
+  </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" mc:Ignorable="x14ac x16r2">
   <numFmts count="1">
     <numFmt numFmtId="164" formatCode="d/\ m/\ yyyy;@"/>
   </numFmts>
-  <fonts count="4" x14ac:knownFonts="1">
+  <fonts count="5" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -93,6 +95,13 @@
       <name val="Calibri Light"/>
       <scheme val="major"/>
     </font>
+    <font>
+      <sz val="10"/>
+      <color theme="1"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
   </fonts>
   <fills count="3">
     <fill>
@@ -108,7 +117,7 @@
       </patternFill>
     </fill>
   </fills>
-  <borders count="2">
+  <borders count="3">
     <border>
       <left/>
       <right/>
@@ -129,11 +138,26 @@
       <bottom/>
       <diagonal/>
     </border>
+    <border>
+      <left style="thin">
+        <color theme="4"/>
+      </left>
+      <right style="thin">
+        <color theme="4"/>
+      </right>
+      <top style="thin">
+        <color theme="4"/>
+      </top>
+      <bottom style="thin">
+        <color theme="4"/>
+      </bottom>
+      <diagonal/>
+    </border>
   </borders>
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="26">
+  <cellXfs count="32">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="49" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyAlignment="1" applyProtection="1">
       <alignment horizontal="left" vertical="top"/>
@@ -208,6 +232,24 @@
       <alignment horizontal="right"/>
     </xf>
     <xf numFmtId="0" fontId="3" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="right"/>
+    </xf>
+    <xf numFmtId="164" fontId="4" fillId="2" borderId="2" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="right" vertical="top"/>
+    </xf>
+    <xf numFmtId="3" fontId="4" fillId="2" borderId="2" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="right"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="2" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="right"/>
+    </xf>
+    <xf numFmtId="164" fontId="3" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="right" vertical="top"/>
+    </xf>
+    <xf numFmtId="3" fontId="3" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="right"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="right"/>
     </xf>
   </cellXfs>
@@ -399,8 +441,8 @@
 </file>
 
 <file path=xl/tables/table1.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="1" xr:uid="{00000000-000C-0000-FFFF-FFFF00000000}" name="Tabela1" displayName="Tabela1" ref="A1:J75" totalsRowShown="0" headerRowDxfId="11" dataDxfId="10">
-  <autoFilter ref="A1:J75" xr:uid="{00000000-0009-0000-0100-000001000000}">
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="1" name="Tabela1" displayName="Tabela1" ref="A1:J112" totalsRowShown="0" headerRowDxfId="11" dataDxfId="10">
+  <autoFilter ref="A1:J112">
     <filterColumn colId="0" hiddenButton="1"/>
     <filterColumn colId="1" hiddenButton="1"/>
     <filterColumn colId="2" hiddenButton="1"/>
@@ -413,16 +455,16 @@
     <filterColumn colId="9" hiddenButton="1"/>
   </autoFilter>
   <tableColumns count="10">
-    <tableColumn id="1" xr3:uid="{00000000-0010-0000-0000-000001000000}" name="Date" dataDxfId="9"/>
-    <tableColumn id="2" xr3:uid="{00000000-0010-0000-0000-000002000000}" name="Tested (all)" dataDxfId="8"/>
-    <tableColumn id="3" xr3:uid="{00000000-0010-0000-0000-000003000000}" name="Tested (daily)" dataDxfId="7"/>
-    <tableColumn id="4" xr3:uid="{00000000-0010-0000-0000-000004000000}" name="Positive (all)" dataDxfId="6"/>
-    <tableColumn id="5" xr3:uid="{00000000-0010-0000-0000-000005000000}" name="Positive (daily)" dataDxfId="5"/>
-    <tableColumn id="6" xr3:uid="{00000000-0010-0000-0000-000006000000}" name="All hospitalized on certain day" dataDxfId="4"/>
-    <tableColumn id="7" xr3:uid="{00000000-0010-0000-0000-000007000000}" name="All persons in intensive care on certain day" dataDxfId="3"/>
-    <tableColumn id="10" xr3:uid="{00000000-0010-0000-0000-00000A000000}" name="Discharged" dataDxfId="2"/>
-    <tableColumn id="8" xr3:uid="{00000000-0010-0000-0000-000008000000}" name="Deaths (all)" dataDxfId="1"/>
-    <tableColumn id="9" xr3:uid="{00000000-0010-0000-0000-000009000000}" name="Deaths (daily)" dataDxfId="0"/>
+    <tableColumn id="1" name="Date" dataDxfId="9"/>
+    <tableColumn id="2" name="Tested (all)" dataDxfId="8"/>
+    <tableColumn id="3" name="Tested (daily)" dataDxfId="7"/>
+    <tableColumn id="4" name="Positive (all)" dataDxfId="6"/>
+    <tableColumn id="5" name="Positive (daily)" dataDxfId="5"/>
+    <tableColumn id="6" name="All hospitalized on certain day" dataDxfId="4"/>
+    <tableColumn id="7" name="All persons in intensive care on certain day" dataDxfId="3"/>
+    <tableColumn id="10" name="Discharged" dataDxfId="2"/>
+    <tableColumn id="8" name="Deaths (all)" dataDxfId="1"/>
+    <tableColumn id="9" name="Deaths (daily)" dataDxfId="0"/>
   </tableColumns>
   <tableStyleInfo name="TableStyleLight16" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
   <extLst>
@@ -695,11 +737,11 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:J75"/>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <dimension ref="A1:J112"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A40" zoomScale="89" zoomScaleNormal="89" workbookViewId="0">
-      <selection activeCell="J74" sqref="J74"/>
+    <sheetView tabSelected="1" topLeftCell="A83" zoomScale="89" zoomScaleNormal="89" workbookViewId="0">
+      <selection activeCell="J112" sqref="J112"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -3117,6 +3159,1190 @@
         <v>0</v>
       </c>
     </row>
+    <row r="76" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A76" s="20">
+        <v>43976</v>
+      </c>
+      <c r="B76" s="21">
+        <v>75770</v>
+      </c>
+      <c r="C76" s="22">
+        <v>754</v>
+      </c>
+      <c r="D76" s="22">
+        <v>1469</v>
+      </c>
+      <c r="E76" s="22">
+        <v>0</v>
+      </c>
+      <c r="F76" s="22">
+        <v>9</v>
+      </c>
+      <c r="G76" s="22">
+        <v>2</v>
+      </c>
+      <c r="H76" s="22">
+        <v>6</v>
+      </c>
+      <c r="I76" s="22">
+        <v>108</v>
+      </c>
+      <c r="J76" s="22">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="77" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A77" s="20">
+        <v>43977</v>
+      </c>
+      <c r="B77" s="21">
+        <v>76579</v>
+      </c>
+      <c r="C77" s="22">
+        <v>809</v>
+      </c>
+      <c r="D77" s="22">
+        <v>1471</v>
+      </c>
+      <c r="E77" s="22">
+        <v>2</v>
+      </c>
+      <c r="F77" s="22">
+        <v>8</v>
+      </c>
+      <c r="G77" s="22">
+        <v>2</v>
+      </c>
+      <c r="H77" s="22">
+        <v>2</v>
+      </c>
+      <c r="I77" s="22">
+        <v>108</v>
+      </c>
+      <c r="J77" s="22">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="78" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A78" s="20">
+        <v>43978</v>
+      </c>
+      <c r="B78" s="21">
+        <v>77210</v>
+      </c>
+      <c r="C78" s="22">
+        <v>631</v>
+      </c>
+      <c r="D78" s="22">
+        <v>1473</v>
+      </c>
+      <c r="E78" s="22">
+        <v>2</v>
+      </c>
+      <c r="F78" s="22">
+        <v>7</v>
+      </c>
+      <c r="G78" s="22">
+        <v>2</v>
+      </c>
+      <c r="H78" s="22">
+        <v>1</v>
+      </c>
+      <c r="I78" s="22">
+        <v>108</v>
+      </c>
+      <c r="J78" s="22">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="79" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A79" s="20">
+        <v>43979</v>
+      </c>
+      <c r="B79" s="21">
+        <v>77916</v>
+      </c>
+      <c r="C79" s="22">
+        <v>706</v>
+      </c>
+      <c r="D79" s="22">
+        <v>1473</v>
+      </c>
+      <c r="E79" s="22">
+        <v>0</v>
+      </c>
+      <c r="F79" s="22">
+        <v>7</v>
+      </c>
+      <c r="G79" s="22">
+        <v>2</v>
+      </c>
+      <c r="H79" s="22">
+        <v>0</v>
+      </c>
+      <c r="I79" s="22">
+        <v>108</v>
+      </c>
+      <c r="J79" s="22">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="80" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A80" s="20">
+        <v>43980</v>
+      </c>
+      <c r="B80" s="21">
+        <v>78529</v>
+      </c>
+      <c r="C80" s="22">
+        <v>613</v>
+      </c>
+      <c r="D80" s="22">
+        <v>1473</v>
+      </c>
+      <c r="E80" s="22">
+        <v>0</v>
+      </c>
+      <c r="F80" s="22">
+        <v>7</v>
+      </c>
+      <c r="G80" s="22">
+        <v>2</v>
+      </c>
+      <c r="H80" s="22">
+        <v>0</v>
+      </c>
+      <c r="I80" s="22">
+        <v>108</v>
+      </c>
+      <c r="J80" s="22">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="81" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A81" s="20">
+        <v>43981</v>
+      </c>
+      <c r="B81" s="22">
+        <v>78793</v>
+      </c>
+      <c r="C81" s="22">
+        <v>264</v>
+      </c>
+      <c r="D81" s="22">
+        <v>1473</v>
+      </c>
+      <c r="E81" s="22">
+        <v>0</v>
+      </c>
+      <c r="F81" s="22">
+        <v>6</v>
+      </c>
+      <c r="G81" s="22">
+        <v>2</v>
+      </c>
+      <c r="H81" s="22">
+        <v>1</v>
+      </c>
+      <c r="I81" s="22">
+        <v>108</v>
+      </c>
+      <c r="J81" s="22">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="82" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A82" s="20">
+        <v>43982</v>
+      </c>
+      <c r="B82" s="21">
+        <v>79039</v>
+      </c>
+      <c r="C82" s="22">
+        <v>246</v>
+      </c>
+      <c r="D82" s="22">
+        <v>1473</v>
+      </c>
+      <c r="E82" s="22">
+        <v>0</v>
+      </c>
+      <c r="F82" s="22">
+        <v>5</v>
+      </c>
+      <c r="G82" s="22">
+        <v>1</v>
+      </c>
+      <c r="H82" s="22">
+        <v>0</v>
+      </c>
+      <c r="I82" s="22">
+        <v>109</v>
+      </c>
+      <c r="J82" s="22">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="83" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A83" s="20">
+        <v>43983</v>
+      </c>
+      <c r="B83" s="21">
+        <v>79698</v>
+      </c>
+      <c r="C83" s="22">
+        <v>659</v>
+      </c>
+      <c r="D83" s="22">
+        <v>1475</v>
+      </c>
+      <c r="E83" s="22">
+        <v>2</v>
+      </c>
+      <c r="F83" s="22">
+        <v>5</v>
+      </c>
+      <c r="G83" s="22">
+        <v>1</v>
+      </c>
+      <c r="H83" s="22">
+        <v>0</v>
+      </c>
+      <c r="I83" s="22">
+        <v>109</v>
+      </c>
+      <c r="J83" s="22">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="84" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A84" s="20">
+        <v>43984</v>
+      </c>
+      <c r="B84" s="21">
+        <v>80505</v>
+      </c>
+      <c r="C84" s="22">
+        <v>807</v>
+      </c>
+      <c r="D84" s="22">
+        <v>1477</v>
+      </c>
+      <c r="E84" s="22">
+        <v>2</v>
+      </c>
+      <c r="F84" s="22">
+        <v>5</v>
+      </c>
+      <c r="G84" s="22">
+        <v>0</v>
+      </c>
+      <c r="H84" s="22">
+        <v>0</v>
+      </c>
+      <c r="I84" s="22">
+        <v>109</v>
+      </c>
+      <c r="J84" s="22">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="85" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A85" s="20">
+        <v>43985</v>
+      </c>
+      <c r="B85" s="21">
+        <v>81333</v>
+      </c>
+      <c r="C85" s="22">
+        <v>828</v>
+      </c>
+      <c r="D85" s="22">
+        <v>1477</v>
+      </c>
+      <c r="E85" s="22">
+        <v>0</v>
+      </c>
+      <c r="F85" s="22">
+        <v>5</v>
+      </c>
+      <c r="G85" s="22">
+        <v>0</v>
+      </c>
+      <c r="H85" s="22">
+        <v>0</v>
+      </c>
+      <c r="I85" s="22">
+        <v>109</v>
+      </c>
+      <c r="J85" s="22">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="86" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A86" s="26">
+        <v>43986</v>
+      </c>
+      <c r="B86" s="27">
+        <v>82161</v>
+      </c>
+      <c r="C86" s="28">
+        <v>828</v>
+      </c>
+      <c r="D86" s="28">
+        <v>1479</v>
+      </c>
+      <c r="E86" s="28">
+        <v>2</v>
+      </c>
+      <c r="F86" s="28">
+        <v>6</v>
+      </c>
+      <c r="G86" s="28">
+        <v>0</v>
+      </c>
+      <c r="H86" s="28">
+        <v>0</v>
+      </c>
+      <c r="I86" s="28">
+        <v>109</v>
+      </c>
+      <c r="J86" s="28">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="87" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A87" s="29">
+        <v>43987</v>
+      </c>
+      <c r="B87" s="30">
+        <v>82876</v>
+      </c>
+      <c r="C87" s="31">
+        <v>715</v>
+      </c>
+      <c r="D87" s="31">
+        <v>1484</v>
+      </c>
+      <c r="E87" s="31">
+        <v>5</v>
+      </c>
+      <c r="F87" s="31">
+        <v>6</v>
+      </c>
+      <c r="G87" s="31">
+        <v>0</v>
+      </c>
+      <c r="H87" s="31">
+        <v>0</v>
+      </c>
+      <c r="I87" s="31">
+        <v>109</v>
+      </c>
+      <c r="J87" s="31">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="88" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A88" s="23">
+        <v>43988</v>
+      </c>
+      <c r="B88" s="24">
+        <v>83105</v>
+      </c>
+      <c r="C88" s="25">
+        <v>229</v>
+      </c>
+      <c r="D88" s="25">
+        <v>1485</v>
+      </c>
+      <c r="E88" s="25">
+        <v>1</v>
+      </c>
+      <c r="F88" s="25">
+        <v>5</v>
+      </c>
+      <c r="G88" s="25">
+        <v>0</v>
+      </c>
+      <c r="H88" s="25">
+        <v>1</v>
+      </c>
+      <c r="I88" s="25">
+        <v>109</v>
+      </c>
+      <c r="J88" s="25">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="89" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A89" s="29">
+        <v>43989</v>
+      </c>
+      <c r="B89" s="30">
+        <v>83316</v>
+      </c>
+      <c r="C89" s="31">
+        <v>211</v>
+      </c>
+      <c r="D89" s="31">
+        <v>1485</v>
+      </c>
+      <c r="E89" s="31">
+        <v>0</v>
+      </c>
+      <c r="F89" s="31">
+        <v>5</v>
+      </c>
+      <c r="G89" s="31">
+        <v>0</v>
+      </c>
+      <c r="H89" s="31">
+        <v>0</v>
+      </c>
+      <c r="I89" s="31">
+        <v>109</v>
+      </c>
+      <c r="J89" s="31">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="90" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A90" s="20">
+        <v>43990</v>
+      </c>
+      <c r="B90" s="21">
+        <v>84130</v>
+      </c>
+      <c r="C90" s="22">
+        <v>814</v>
+      </c>
+      <c r="D90" s="22">
+        <v>1486</v>
+      </c>
+      <c r="E90" s="22">
+        <v>1</v>
+      </c>
+      <c r="F90" s="22">
+        <v>6</v>
+      </c>
+      <c r="G90" s="22">
+        <v>0</v>
+      </c>
+      <c r="H90" s="22">
+        <v>0</v>
+      </c>
+      <c r="I90" s="22">
+        <v>109</v>
+      </c>
+      <c r="J90" s="22">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="91" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A91" s="20">
+        <v>43991</v>
+      </c>
+      <c r="B91" s="21">
+        <v>84868</v>
+      </c>
+      <c r="C91" s="22">
+        <v>738</v>
+      </c>
+      <c r="D91" s="22">
+        <v>1488</v>
+      </c>
+      <c r="E91" s="22">
+        <v>2</v>
+      </c>
+      <c r="F91" s="22">
+        <v>6</v>
+      </c>
+      <c r="G91" s="22">
+        <v>0</v>
+      </c>
+      <c r="H91" s="22">
+        <v>0</v>
+      </c>
+      <c r="I91" s="22">
+        <v>109</v>
+      </c>
+      <c r="J91" s="22">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="92" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A92" s="23">
+        <v>43992</v>
+      </c>
+      <c r="B92" s="24">
+        <v>85626</v>
+      </c>
+      <c r="C92" s="25">
+        <v>758</v>
+      </c>
+      <c r="D92" s="25">
+        <v>1488</v>
+      </c>
+      <c r="E92" s="25">
+        <v>0</v>
+      </c>
+      <c r="F92" s="25">
+        <v>6</v>
+      </c>
+      <c r="G92" s="25">
+        <v>0</v>
+      </c>
+      <c r="H92" s="25">
+        <v>0</v>
+      </c>
+      <c r="I92" s="25">
+        <v>109</v>
+      </c>
+      <c r="J92" s="25">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="93" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A93" s="29">
+        <v>43993</v>
+      </c>
+      <c r="B93" s="30">
+        <v>86328</v>
+      </c>
+      <c r="C93" s="31">
+        <v>702</v>
+      </c>
+      <c r="D93" s="31">
+        <v>1490</v>
+      </c>
+      <c r="E93" s="31">
+        <v>2</v>
+      </c>
+      <c r="F93" s="31">
+        <v>6</v>
+      </c>
+      <c r="G93" s="31">
+        <v>0</v>
+      </c>
+      <c r="H93" s="31">
+        <v>0</v>
+      </c>
+      <c r="I93" s="31">
+        <v>109</v>
+      </c>
+      <c r="J93" s="31">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="94" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A94" s="23">
+        <v>43994</v>
+      </c>
+      <c r="B94" s="24">
+        <v>87095</v>
+      </c>
+      <c r="C94" s="25">
+        <v>767</v>
+      </c>
+      <c r="D94" s="25">
+        <v>1492</v>
+      </c>
+      <c r="E94" s="25">
+        <v>2</v>
+      </c>
+      <c r="F94" s="25">
+        <v>6</v>
+      </c>
+      <c r="G94" s="25">
+        <v>0</v>
+      </c>
+      <c r="H94" s="25">
+        <v>0</v>
+      </c>
+      <c r="I94" s="25">
+        <v>109</v>
+      </c>
+      <c r="J94" s="25">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="95" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A95" s="29">
+        <v>43995</v>
+      </c>
+      <c r="B95" s="30">
+        <v>87386</v>
+      </c>
+      <c r="C95" s="31">
+        <v>291</v>
+      </c>
+      <c r="D95" s="31">
+        <v>1495</v>
+      </c>
+      <c r="E95" s="31">
+        <v>3</v>
+      </c>
+      <c r="F95" s="31">
+        <v>6</v>
+      </c>
+      <c r="G95" s="31">
+        <v>0</v>
+      </c>
+      <c r="H95" s="31">
+        <v>0</v>
+      </c>
+      <c r="I95" s="31">
+        <v>109</v>
+      </c>
+      <c r="J95" s="31">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="96" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A96" s="23">
+        <v>43996</v>
+      </c>
+      <c r="B96" s="24">
+        <v>87598</v>
+      </c>
+      <c r="C96" s="25">
+        <v>212</v>
+      </c>
+      <c r="D96" s="25">
+        <v>1496</v>
+      </c>
+      <c r="E96" s="25">
+        <v>1</v>
+      </c>
+      <c r="F96" s="25">
+        <v>7</v>
+      </c>
+      <c r="G96" s="25">
+        <v>1</v>
+      </c>
+      <c r="H96" s="25">
+        <v>0</v>
+      </c>
+      <c r="I96" s="25">
+        <v>109</v>
+      </c>
+      <c r="J96" s="25">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="97" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A97" s="20">
+        <v>43997</v>
+      </c>
+      <c r="B97" s="21">
+        <v>88165</v>
+      </c>
+      <c r="C97" s="22">
+        <v>567</v>
+      </c>
+      <c r="D97" s="22">
+        <v>1499</v>
+      </c>
+      <c r="E97" s="22">
+        <v>3</v>
+      </c>
+      <c r="F97" s="22">
+        <v>7</v>
+      </c>
+      <c r="G97" s="22">
+        <v>1</v>
+      </c>
+      <c r="H97" s="22">
+        <v>0</v>
+      </c>
+      <c r="I97" s="22">
+        <v>109</v>
+      </c>
+      <c r="J97" s="22">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="98" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A98" s="20">
+        <v>43998</v>
+      </c>
+      <c r="B98" s="21">
+        <v>89151</v>
+      </c>
+      <c r="C98" s="22">
+        <v>986</v>
+      </c>
+      <c r="D98" s="22">
+        <v>1503</v>
+      </c>
+      <c r="E98" s="22">
+        <v>4</v>
+      </c>
+      <c r="F98" s="22">
+        <v>7</v>
+      </c>
+      <c r="G98" s="22">
+        <v>1</v>
+      </c>
+      <c r="H98" s="22">
+        <v>0</v>
+      </c>
+      <c r="I98" s="22">
+        <v>109</v>
+      </c>
+      <c r="J98" s="22">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="99" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A99" s="29">
+        <v>43999</v>
+      </c>
+      <c r="B99" s="30">
+        <v>90103</v>
+      </c>
+      <c r="C99" s="31">
+        <v>952</v>
+      </c>
+      <c r="D99" s="31">
+        <v>1511</v>
+      </c>
+      <c r="E99" s="31">
+        <v>8</v>
+      </c>
+      <c r="F99" s="31">
+        <v>6</v>
+      </c>
+      <c r="G99" s="31">
+        <v>1</v>
+      </c>
+      <c r="H99" s="31">
+        <v>1</v>
+      </c>
+      <c r="I99" s="31">
+        <v>109</v>
+      </c>
+      <c r="J99" s="31">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="100" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A100" s="20">
+        <v>44000</v>
+      </c>
+      <c r="B100" s="21">
+        <v>91005</v>
+      </c>
+      <c r="C100" s="22">
+        <v>902</v>
+      </c>
+      <c r="D100" s="22">
+        <v>1513</v>
+      </c>
+      <c r="E100" s="22">
+        <v>2</v>
+      </c>
+      <c r="F100" s="22">
+        <v>8</v>
+      </c>
+      <c r="G100" s="22">
+        <v>1</v>
+      </c>
+      <c r="H100" s="22">
+        <v>0</v>
+      </c>
+      <c r="I100" s="22">
+        <v>109</v>
+      </c>
+      <c r="J100" s="22">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="101" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A101" s="29">
+        <v>44001</v>
+      </c>
+      <c r="B101" s="30">
+        <v>92152</v>
+      </c>
+      <c r="C101" s="31">
+        <v>1147</v>
+      </c>
+      <c r="D101" s="31">
+        <v>1519</v>
+      </c>
+      <c r="E101" s="31">
+        <v>6</v>
+      </c>
+      <c r="F101" s="31">
+        <v>6</v>
+      </c>
+      <c r="G101" s="31">
+        <v>1</v>
+      </c>
+      <c r="H101" s="31">
+        <v>2</v>
+      </c>
+      <c r="I101" s="31">
+        <v>109</v>
+      </c>
+      <c r="J101" s="31">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="102" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A102" s="23">
+        <v>44002</v>
+      </c>
+      <c r="B102" s="24">
+        <v>92919</v>
+      </c>
+      <c r="C102" s="25">
+        <v>758</v>
+      </c>
+      <c r="D102" s="25">
+        <v>1520</v>
+      </c>
+      <c r="E102" s="25">
+        <v>1</v>
+      </c>
+      <c r="F102" s="25">
+        <v>6</v>
+      </c>
+      <c r="G102" s="25">
+        <v>1</v>
+      </c>
+      <c r="H102" s="25">
+        <v>2</v>
+      </c>
+      <c r="I102" s="25">
+        <v>109</v>
+      </c>
+      <c r="J102" s="25">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="103" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A103" s="29">
+        <v>44003</v>
+      </c>
+      <c r="B103" s="30">
+        <v>93181</v>
+      </c>
+      <c r="C103" s="31">
+        <v>271</v>
+      </c>
+      <c r="D103" s="31">
+        <v>1521</v>
+      </c>
+      <c r="E103" s="31">
+        <v>1</v>
+      </c>
+      <c r="F103" s="31">
+        <v>6</v>
+      </c>
+      <c r="G103" s="31">
+        <v>1</v>
+      </c>
+      <c r="H103" s="31">
+        <v>0</v>
+      </c>
+      <c r="I103" s="31">
+        <v>109</v>
+      </c>
+      <c r="J103" s="31">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="104" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A104" s="29">
+        <v>44004</v>
+      </c>
+      <c r="B104" s="30">
+        <v>94165</v>
+      </c>
+      <c r="C104" s="31">
+        <v>984</v>
+      </c>
+      <c r="D104" s="31">
+        <v>1534</v>
+      </c>
+      <c r="E104" s="31">
+        <v>13</v>
+      </c>
+      <c r="F104" s="31">
+        <v>5</v>
+      </c>
+      <c r="G104" s="31">
+        <v>1</v>
+      </c>
+      <c r="H104" s="31">
+        <v>1</v>
+      </c>
+      <c r="I104" s="31">
+        <v>109</v>
+      </c>
+      <c r="J104" s="31">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="105" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A105" s="29">
+        <v>44005</v>
+      </c>
+      <c r="B105" s="30">
+        <v>95387</v>
+      </c>
+      <c r="C105" s="31">
+        <v>1222</v>
+      </c>
+      <c r="D105" s="31">
+        <v>1541</v>
+      </c>
+      <c r="E105" s="31">
+        <v>7</v>
+      </c>
+      <c r="F105" s="31">
+        <v>7</v>
+      </c>
+      <c r="G105" s="31">
+        <v>2</v>
+      </c>
+      <c r="H105" s="31">
+        <v>0</v>
+      </c>
+      <c r="I105" s="31" t="s">
+        <v>10</v>
+      </c>
+      <c r="J105" s="31">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="106" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A106" s="23">
+        <v>44006</v>
+      </c>
+      <c r="B106" s="24">
+        <v>96599</v>
+      </c>
+      <c r="C106" s="25">
+        <v>1212</v>
+      </c>
+      <c r="D106" s="25">
+        <v>1547</v>
+      </c>
+      <c r="E106" s="25">
+        <v>6</v>
+      </c>
+      <c r="F106" s="25">
+        <v>7</v>
+      </c>
+      <c r="G106" s="25">
+        <v>2</v>
+      </c>
+      <c r="H106" s="25">
+        <v>0</v>
+      </c>
+      <c r="I106" s="25" t="s">
+        <v>10</v>
+      </c>
+      <c r="J106" s="25">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="107" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A107" s="29">
+        <v>44007</v>
+      </c>
+      <c r="B107" s="30">
+        <v>97442</v>
+      </c>
+      <c r="C107" s="31">
+        <v>843</v>
+      </c>
+      <c r="D107" s="31">
+        <v>1558</v>
+      </c>
+      <c r="E107" s="31">
+        <v>11</v>
+      </c>
+      <c r="F107" s="31">
+        <v>8</v>
+      </c>
+      <c r="G107" s="31">
+        <v>2</v>
+      </c>
+      <c r="H107" s="31">
+        <v>0</v>
+      </c>
+      <c r="I107" s="31" t="s">
+        <v>10</v>
+      </c>
+      <c r="J107" s="31">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="108" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A108" s="29">
+        <v>44008</v>
+      </c>
+      <c r="B108" s="30">
+        <v>98320</v>
+      </c>
+      <c r="C108" s="31">
+        <v>878</v>
+      </c>
+      <c r="D108" s="31">
+        <v>1572</v>
+      </c>
+      <c r="E108" s="31">
+        <v>14</v>
+      </c>
+      <c r="F108" s="31">
+        <v>8</v>
+      </c>
+      <c r="G108" s="31">
+        <v>1</v>
+      </c>
+      <c r="H108" s="31">
+        <v>0</v>
+      </c>
+      <c r="I108" s="31" t="s">
+        <v>10</v>
+      </c>
+      <c r="J108" s="31">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="109" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A109" s="29">
+        <v>44009</v>
+      </c>
+      <c r="B109" s="30">
+        <v>98945</v>
+      </c>
+      <c r="C109" s="31">
+        <v>625</v>
+      </c>
+      <c r="D109" s="31">
+        <v>1581</v>
+      </c>
+      <c r="E109" s="31">
+        <v>9</v>
+      </c>
+      <c r="F109" s="31">
+        <v>7</v>
+      </c>
+      <c r="G109" s="31">
+        <v>0</v>
+      </c>
+      <c r="H109" s="31">
+        <v>1</v>
+      </c>
+      <c r="I109" s="31" t="s">
+        <v>10</v>
+      </c>
+      <c r="J109" s="31">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="110" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A110" s="29">
+        <v>44010</v>
+      </c>
+      <c r="B110" s="30">
+        <v>99245</v>
+      </c>
+      <c r="C110" s="31">
+        <v>300</v>
+      </c>
+      <c r="D110" s="31">
+        <v>1585</v>
+      </c>
+      <c r="E110" s="31">
+        <v>4</v>
+      </c>
+      <c r="F110" s="31">
+        <v>8</v>
+      </c>
+      <c r="G110" s="31">
+        <v>0</v>
+      </c>
+      <c r="H110" s="31">
+        <v>0</v>
+      </c>
+      <c r="I110" s="31" t="s">
+        <v>10</v>
+      </c>
+      <c r="J110" s="31">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="111" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A111" s="29">
+        <v>44011</v>
+      </c>
+      <c r="B111" s="30">
+        <v>100330</v>
+      </c>
+      <c r="C111" s="31">
+        <v>1085</v>
+      </c>
+      <c r="D111" s="31">
+        <v>1600</v>
+      </c>
+      <c r="E111" s="31">
+        <v>15</v>
+      </c>
+      <c r="F111" s="31">
+        <v>8</v>
+      </c>
+      <c r="G111" s="31">
+        <v>0</v>
+      </c>
+      <c r="H111" s="31">
+        <v>0</v>
+      </c>
+      <c r="I111" s="31" t="s">
+        <v>10</v>
+      </c>
+      <c r="J111" s="31">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="112" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A112" s="20">
+        <v>44012</v>
+      </c>
+      <c r="B112" s="21">
+        <v>101729</v>
+      </c>
+      <c r="C112" s="22">
+        <v>1399</v>
+      </c>
+      <c r="D112" s="22">
+        <v>1613</v>
+      </c>
+      <c r="E112" s="22">
+        <v>13</v>
+      </c>
+      <c r="F112" s="22">
+        <v>8</v>
+      </c>
+      <c r="G112" s="22">
+        <v>0</v>
+      </c>
+      <c r="H112" s="22">
+        <v>0</v>
+      </c>
+      <c r="I112" s="22" t="s">
+        <v>10</v>
+      </c>
+      <c r="J112" s="22">
+        <v>0</v>
+      </c>
+    </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>

</xml_diff>

<commit_message>
Data updated by GitHub Bot (2020-07-01 20)
</commit_message>
<xml_diff>
--- a/output/snapshot/fdcf2531-4c3e-5c02-b63c-ee160ead6dea.xlsx
+++ b/output/snapshot/fdcf2531-4c3e-5c02-b63c-ee160ead6dea.xlsx
@@ -1,16 +1,15 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="21929"/>
-  <workbookPr/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
+  <fileVersion appName="xl" lastEdited="6" lowestEdited="6" rupBuild="14420"/>
+  <workbookPr defaultThemeVersion="164011"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="I:\AKTUALNI PODATKI - KORONA\Za objavo na GOV.SI\ang\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{1E6DD62F-2BE2-47DC-A7ED-9B57C1589256}" xr6:coauthVersionLast="44" xr6:coauthVersionMax="44" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840"/>
   </bookViews>
   <sheets>
     <sheet name="Covid-19 podatki" sheetId="1" r:id="rId1"/>
@@ -25,7 +24,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="10" uniqueCount="10">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="18" uniqueCount="11">
   <si>
     <t>Date</t>
   </si>
@@ -56,15 +55,18 @@
   <si>
     <t>Deaths (daily)</t>
   </si>
+  <si>
+    <t>111*</t>
+  </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" mc:Ignorable="x14ac x16r2">
   <numFmts count="1">
     <numFmt numFmtId="164" formatCode="d/\ m/\ yyyy;@"/>
   </numFmts>
-  <fonts count="4" x14ac:knownFonts="1">
+  <fonts count="5" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -93,6 +95,13 @@
       <name val="Calibri Light"/>
       <scheme val="major"/>
     </font>
+    <font>
+      <sz val="10"/>
+      <color theme="1"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
   </fonts>
   <fills count="3">
     <fill>
@@ -108,7 +117,7 @@
       </patternFill>
     </fill>
   </fills>
-  <borders count="2">
+  <borders count="3">
     <border>
       <left/>
       <right/>
@@ -129,11 +138,26 @@
       <bottom/>
       <diagonal/>
     </border>
+    <border>
+      <left style="thin">
+        <color theme="4"/>
+      </left>
+      <right style="thin">
+        <color theme="4"/>
+      </right>
+      <top style="thin">
+        <color theme="4"/>
+      </top>
+      <bottom style="thin">
+        <color theme="4"/>
+      </bottom>
+      <diagonal/>
+    </border>
   </borders>
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="26">
+  <cellXfs count="32">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="49" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyAlignment="1" applyProtection="1">
       <alignment horizontal="left" vertical="top"/>
@@ -208,6 +232,24 @@
       <alignment horizontal="right"/>
     </xf>
     <xf numFmtId="0" fontId="3" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="right"/>
+    </xf>
+    <xf numFmtId="164" fontId="4" fillId="2" borderId="2" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="right" vertical="top"/>
+    </xf>
+    <xf numFmtId="3" fontId="4" fillId="2" borderId="2" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="right"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="2" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="right"/>
+    </xf>
+    <xf numFmtId="164" fontId="3" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="right" vertical="top"/>
+    </xf>
+    <xf numFmtId="3" fontId="3" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="right"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="right"/>
     </xf>
   </cellXfs>
@@ -399,8 +441,8 @@
 </file>
 
 <file path=xl/tables/table1.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="1" xr:uid="{00000000-000C-0000-FFFF-FFFF00000000}" name="Tabela1" displayName="Tabela1" ref="A1:J75" totalsRowShown="0" headerRowDxfId="11" dataDxfId="10">
-  <autoFilter ref="A1:J75" xr:uid="{00000000-0009-0000-0100-000001000000}">
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="1" name="Tabela1" displayName="Tabela1" ref="A1:J112" totalsRowShown="0" headerRowDxfId="11" dataDxfId="10">
+  <autoFilter ref="A1:J112">
     <filterColumn colId="0" hiddenButton="1"/>
     <filterColumn colId="1" hiddenButton="1"/>
     <filterColumn colId="2" hiddenButton="1"/>
@@ -413,16 +455,16 @@
     <filterColumn colId="9" hiddenButton="1"/>
   </autoFilter>
   <tableColumns count="10">
-    <tableColumn id="1" xr3:uid="{00000000-0010-0000-0000-000001000000}" name="Date" dataDxfId="9"/>
-    <tableColumn id="2" xr3:uid="{00000000-0010-0000-0000-000002000000}" name="Tested (all)" dataDxfId="8"/>
-    <tableColumn id="3" xr3:uid="{00000000-0010-0000-0000-000003000000}" name="Tested (daily)" dataDxfId="7"/>
-    <tableColumn id="4" xr3:uid="{00000000-0010-0000-0000-000004000000}" name="Positive (all)" dataDxfId="6"/>
-    <tableColumn id="5" xr3:uid="{00000000-0010-0000-0000-000005000000}" name="Positive (daily)" dataDxfId="5"/>
-    <tableColumn id="6" xr3:uid="{00000000-0010-0000-0000-000006000000}" name="All hospitalized on certain day" dataDxfId="4"/>
-    <tableColumn id="7" xr3:uid="{00000000-0010-0000-0000-000007000000}" name="All persons in intensive care on certain day" dataDxfId="3"/>
-    <tableColumn id="10" xr3:uid="{00000000-0010-0000-0000-00000A000000}" name="Discharged" dataDxfId="2"/>
-    <tableColumn id="8" xr3:uid="{00000000-0010-0000-0000-000008000000}" name="Deaths (all)" dataDxfId="1"/>
-    <tableColumn id="9" xr3:uid="{00000000-0010-0000-0000-000009000000}" name="Deaths (daily)" dataDxfId="0"/>
+    <tableColumn id="1" name="Date" dataDxfId="9"/>
+    <tableColumn id="2" name="Tested (all)" dataDxfId="8"/>
+    <tableColumn id="3" name="Tested (daily)" dataDxfId="7"/>
+    <tableColumn id="4" name="Positive (all)" dataDxfId="6"/>
+    <tableColumn id="5" name="Positive (daily)" dataDxfId="5"/>
+    <tableColumn id="6" name="All hospitalized on certain day" dataDxfId="4"/>
+    <tableColumn id="7" name="All persons in intensive care on certain day" dataDxfId="3"/>
+    <tableColumn id="10" name="Discharged" dataDxfId="2"/>
+    <tableColumn id="8" name="Deaths (all)" dataDxfId="1"/>
+    <tableColumn id="9" name="Deaths (daily)" dataDxfId="0"/>
   </tableColumns>
   <tableStyleInfo name="TableStyleLight16" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
   <extLst>
@@ -695,11 +737,11 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:J75"/>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <dimension ref="A1:J112"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A40" zoomScale="89" zoomScaleNormal="89" workbookViewId="0">
-      <selection activeCell="J74" sqref="J74"/>
+    <sheetView tabSelected="1" topLeftCell="A83" zoomScale="89" zoomScaleNormal="89" workbookViewId="0">
+      <selection activeCell="J112" sqref="J112"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -3117,6 +3159,1190 @@
         <v>0</v>
       </c>
     </row>
+    <row r="76" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A76" s="20">
+        <v>43976</v>
+      </c>
+      <c r="B76" s="21">
+        <v>75770</v>
+      </c>
+      <c r="C76" s="22">
+        <v>754</v>
+      </c>
+      <c r="D76" s="22">
+        <v>1469</v>
+      </c>
+      <c r="E76" s="22">
+        <v>0</v>
+      </c>
+      <c r="F76" s="22">
+        <v>9</v>
+      </c>
+      <c r="G76" s="22">
+        <v>2</v>
+      </c>
+      <c r="H76" s="22">
+        <v>6</v>
+      </c>
+      <c r="I76" s="22">
+        <v>108</v>
+      </c>
+      <c r="J76" s="22">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="77" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A77" s="20">
+        <v>43977</v>
+      </c>
+      <c r="B77" s="21">
+        <v>76579</v>
+      </c>
+      <c r="C77" s="22">
+        <v>809</v>
+      </c>
+      <c r="D77" s="22">
+        <v>1471</v>
+      </c>
+      <c r="E77" s="22">
+        <v>2</v>
+      </c>
+      <c r="F77" s="22">
+        <v>8</v>
+      </c>
+      <c r="G77" s="22">
+        <v>2</v>
+      </c>
+      <c r="H77" s="22">
+        <v>2</v>
+      </c>
+      <c r="I77" s="22">
+        <v>108</v>
+      </c>
+      <c r="J77" s="22">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="78" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A78" s="20">
+        <v>43978</v>
+      </c>
+      <c r="B78" s="21">
+        <v>77210</v>
+      </c>
+      <c r="C78" s="22">
+        <v>631</v>
+      </c>
+      <c r="D78" s="22">
+        <v>1473</v>
+      </c>
+      <c r="E78" s="22">
+        <v>2</v>
+      </c>
+      <c r="F78" s="22">
+        <v>7</v>
+      </c>
+      <c r="G78" s="22">
+        <v>2</v>
+      </c>
+      <c r="H78" s="22">
+        <v>1</v>
+      </c>
+      <c r="I78" s="22">
+        <v>108</v>
+      </c>
+      <c r="J78" s="22">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="79" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A79" s="20">
+        <v>43979</v>
+      </c>
+      <c r="B79" s="21">
+        <v>77916</v>
+      </c>
+      <c r="C79" s="22">
+        <v>706</v>
+      </c>
+      <c r="D79" s="22">
+        <v>1473</v>
+      </c>
+      <c r="E79" s="22">
+        <v>0</v>
+      </c>
+      <c r="F79" s="22">
+        <v>7</v>
+      </c>
+      <c r="G79" s="22">
+        <v>2</v>
+      </c>
+      <c r="H79" s="22">
+        <v>0</v>
+      </c>
+      <c r="I79" s="22">
+        <v>108</v>
+      </c>
+      <c r="J79" s="22">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="80" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A80" s="20">
+        <v>43980</v>
+      </c>
+      <c r="B80" s="21">
+        <v>78529</v>
+      </c>
+      <c r="C80" s="22">
+        <v>613</v>
+      </c>
+      <c r="D80" s="22">
+        <v>1473</v>
+      </c>
+      <c r="E80" s="22">
+        <v>0</v>
+      </c>
+      <c r="F80" s="22">
+        <v>7</v>
+      </c>
+      <c r="G80" s="22">
+        <v>2</v>
+      </c>
+      <c r="H80" s="22">
+        <v>0</v>
+      </c>
+      <c r="I80" s="22">
+        <v>108</v>
+      </c>
+      <c r="J80" s="22">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="81" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A81" s="20">
+        <v>43981</v>
+      </c>
+      <c r="B81" s="22">
+        <v>78793</v>
+      </c>
+      <c r="C81" s="22">
+        <v>264</v>
+      </c>
+      <c r="D81" s="22">
+        <v>1473</v>
+      </c>
+      <c r="E81" s="22">
+        <v>0</v>
+      </c>
+      <c r="F81" s="22">
+        <v>6</v>
+      </c>
+      <c r="G81" s="22">
+        <v>2</v>
+      </c>
+      <c r="H81" s="22">
+        <v>1</v>
+      </c>
+      <c r="I81" s="22">
+        <v>108</v>
+      </c>
+      <c r="J81" s="22">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="82" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A82" s="20">
+        <v>43982</v>
+      </c>
+      <c r="B82" s="21">
+        <v>79039</v>
+      </c>
+      <c r="C82" s="22">
+        <v>246</v>
+      </c>
+      <c r="D82" s="22">
+        <v>1473</v>
+      </c>
+      <c r="E82" s="22">
+        <v>0</v>
+      </c>
+      <c r="F82" s="22">
+        <v>5</v>
+      </c>
+      <c r="G82" s="22">
+        <v>1</v>
+      </c>
+      <c r="H82" s="22">
+        <v>0</v>
+      </c>
+      <c r="I82" s="22">
+        <v>109</v>
+      </c>
+      <c r="J82" s="22">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="83" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A83" s="20">
+        <v>43983</v>
+      </c>
+      <c r="B83" s="21">
+        <v>79698</v>
+      </c>
+      <c r="C83" s="22">
+        <v>659</v>
+      </c>
+      <c r="D83" s="22">
+        <v>1475</v>
+      </c>
+      <c r="E83" s="22">
+        <v>2</v>
+      </c>
+      <c r="F83" s="22">
+        <v>5</v>
+      </c>
+      <c r="G83" s="22">
+        <v>1</v>
+      </c>
+      <c r="H83" s="22">
+        <v>0</v>
+      </c>
+      <c r="I83" s="22">
+        <v>109</v>
+      </c>
+      <c r="J83" s="22">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="84" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A84" s="20">
+        <v>43984</v>
+      </c>
+      <c r="B84" s="21">
+        <v>80505</v>
+      </c>
+      <c r="C84" s="22">
+        <v>807</v>
+      </c>
+      <c r="D84" s="22">
+        <v>1477</v>
+      </c>
+      <c r="E84" s="22">
+        <v>2</v>
+      </c>
+      <c r="F84" s="22">
+        <v>5</v>
+      </c>
+      <c r="G84" s="22">
+        <v>0</v>
+      </c>
+      <c r="H84" s="22">
+        <v>0</v>
+      </c>
+      <c r="I84" s="22">
+        <v>109</v>
+      </c>
+      <c r="J84" s="22">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="85" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A85" s="20">
+        <v>43985</v>
+      </c>
+      <c r="B85" s="21">
+        <v>81333</v>
+      </c>
+      <c r="C85" s="22">
+        <v>828</v>
+      </c>
+      <c r="D85" s="22">
+        <v>1477</v>
+      </c>
+      <c r="E85" s="22">
+        <v>0</v>
+      </c>
+      <c r="F85" s="22">
+        <v>5</v>
+      </c>
+      <c r="G85" s="22">
+        <v>0</v>
+      </c>
+      <c r="H85" s="22">
+        <v>0</v>
+      </c>
+      <c r="I85" s="22">
+        <v>109</v>
+      </c>
+      <c r="J85" s="22">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="86" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A86" s="26">
+        <v>43986</v>
+      </c>
+      <c r="B86" s="27">
+        <v>82161</v>
+      </c>
+      <c r="C86" s="28">
+        <v>828</v>
+      </c>
+      <c r="D86" s="28">
+        <v>1479</v>
+      </c>
+      <c r="E86" s="28">
+        <v>2</v>
+      </c>
+      <c r="F86" s="28">
+        <v>6</v>
+      </c>
+      <c r="G86" s="28">
+        <v>0</v>
+      </c>
+      <c r="H86" s="28">
+        <v>0</v>
+      </c>
+      <c r="I86" s="28">
+        <v>109</v>
+      </c>
+      <c r="J86" s="28">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="87" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A87" s="29">
+        <v>43987</v>
+      </c>
+      <c r="B87" s="30">
+        <v>82876</v>
+      </c>
+      <c r="C87" s="31">
+        <v>715</v>
+      </c>
+      <c r="D87" s="31">
+        <v>1484</v>
+      </c>
+      <c r="E87" s="31">
+        <v>5</v>
+      </c>
+      <c r="F87" s="31">
+        <v>6</v>
+      </c>
+      <c r="G87" s="31">
+        <v>0</v>
+      </c>
+      <c r="H87" s="31">
+        <v>0</v>
+      </c>
+      <c r="I87" s="31">
+        <v>109</v>
+      </c>
+      <c r="J87" s="31">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="88" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A88" s="23">
+        <v>43988</v>
+      </c>
+      <c r="B88" s="24">
+        <v>83105</v>
+      </c>
+      <c r="C88" s="25">
+        <v>229</v>
+      </c>
+      <c r="D88" s="25">
+        <v>1485</v>
+      </c>
+      <c r="E88" s="25">
+        <v>1</v>
+      </c>
+      <c r="F88" s="25">
+        <v>5</v>
+      </c>
+      <c r="G88" s="25">
+        <v>0</v>
+      </c>
+      <c r="H88" s="25">
+        <v>1</v>
+      </c>
+      <c r="I88" s="25">
+        <v>109</v>
+      </c>
+      <c r="J88" s="25">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="89" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A89" s="29">
+        <v>43989</v>
+      </c>
+      <c r="B89" s="30">
+        <v>83316</v>
+      </c>
+      <c r="C89" s="31">
+        <v>211</v>
+      </c>
+      <c r="D89" s="31">
+        <v>1485</v>
+      </c>
+      <c r="E89" s="31">
+        <v>0</v>
+      </c>
+      <c r="F89" s="31">
+        <v>5</v>
+      </c>
+      <c r="G89" s="31">
+        <v>0</v>
+      </c>
+      <c r="H89" s="31">
+        <v>0</v>
+      </c>
+      <c r="I89" s="31">
+        <v>109</v>
+      </c>
+      <c r="J89" s="31">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="90" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A90" s="20">
+        <v>43990</v>
+      </c>
+      <c r="B90" s="21">
+        <v>84130</v>
+      </c>
+      <c r="C90" s="22">
+        <v>814</v>
+      </c>
+      <c r="D90" s="22">
+        <v>1486</v>
+      </c>
+      <c r="E90" s="22">
+        <v>1</v>
+      </c>
+      <c r="F90" s="22">
+        <v>6</v>
+      </c>
+      <c r="G90" s="22">
+        <v>0</v>
+      </c>
+      <c r="H90" s="22">
+        <v>0</v>
+      </c>
+      <c r="I90" s="22">
+        <v>109</v>
+      </c>
+      <c r="J90" s="22">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="91" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A91" s="20">
+        <v>43991</v>
+      </c>
+      <c r="B91" s="21">
+        <v>84868</v>
+      </c>
+      <c r="C91" s="22">
+        <v>738</v>
+      </c>
+      <c r="D91" s="22">
+        <v>1488</v>
+      </c>
+      <c r="E91" s="22">
+        <v>2</v>
+      </c>
+      <c r="F91" s="22">
+        <v>6</v>
+      </c>
+      <c r="G91" s="22">
+        <v>0</v>
+      </c>
+      <c r="H91" s="22">
+        <v>0</v>
+      </c>
+      <c r="I91" s="22">
+        <v>109</v>
+      </c>
+      <c r="J91" s="22">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="92" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A92" s="23">
+        <v>43992</v>
+      </c>
+      <c r="B92" s="24">
+        <v>85626</v>
+      </c>
+      <c r="C92" s="25">
+        <v>758</v>
+      </c>
+      <c r="D92" s="25">
+        <v>1488</v>
+      </c>
+      <c r="E92" s="25">
+        <v>0</v>
+      </c>
+      <c r="F92" s="25">
+        <v>6</v>
+      </c>
+      <c r="G92" s="25">
+        <v>0</v>
+      </c>
+      <c r="H92" s="25">
+        <v>0</v>
+      </c>
+      <c r="I92" s="25">
+        <v>109</v>
+      </c>
+      <c r="J92" s="25">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="93" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A93" s="29">
+        <v>43993</v>
+      </c>
+      <c r="B93" s="30">
+        <v>86328</v>
+      </c>
+      <c r="C93" s="31">
+        <v>702</v>
+      </c>
+      <c r="D93" s="31">
+        <v>1490</v>
+      </c>
+      <c r="E93" s="31">
+        <v>2</v>
+      </c>
+      <c r="F93" s="31">
+        <v>6</v>
+      </c>
+      <c r="G93" s="31">
+        <v>0</v>
+      </c>
+      <c r="H93" s="31">
+        <v>0</v>
+      </c>
+      <c r="I93" s="31">
+        <v>109</v>
+      </c>
+      <c r="J93" s="31">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="94" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A94" s="23">
+        <v>43994</v>
+      </c>
+      <c r="B94" s="24">
+        <v>87095</v>
+      </c>
+      <c r="C94" s="25">
+        <v>767</v>
+      </c>
+      <c r="D94" s="25">
+        <v>1492</v>
+      </c>
+      <c r="E94" s="25">
+        <v>2</v>
+      </c>
+      <c r="F94" s="25">
+        <v>6</v>
+      </c>
+      <c r="G94" s="25">
+        <v>0</v>
+      </c>
+      <c r="H94" s="25">
+        <v>0</v>
+      </c>
+      <c r="I94" s="25">
+        <v>109</v>
+      </c>
+      <c r="J94" s="25">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="95" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A95" s="29">
+        <v>43995</v>
+      </c>
+      <c r="B95" s="30">
+        <v>87386</v>
+      </c>
+      <c r="C95" s="31">
+        <v>291</v>
+      </c>
+      <c r="D95" s="31">
+        <v>1495</v>
+      </c>
+      <c r="E95" s="31">
+        <v>3</v>
+      </c>
+      <c r="F95" s="31">
+        <v>6</v>
+      </c>
+      <c r="G95" s="31">
+        <v>0</v>
+      </c>
+      <c r="H95" s="31">
+        <v>0</v>
+      </c>
+      <c r="I95" s="31">
+        <v>109</v>
+      </c>
+      <c r="J95" s="31">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="96" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A96" s="23">
+        <v>43996</v>
+      </c>
+      <c r="B96" s="24">
+        <v>87598</v>
+      </c>
+      <c r="C96" s="25">
+        <v>212</v>
+      </c>
+      <c r="D96" s="25">
+        <v>1496</v>
+      </c>
+      <c r="E96" s="25">
+        <v>1</v>
+      </c>
+      <c r="F96" s="25">
+        <v>7</v>
+      </c>
+      <c r="G96" s="25">
+        <v>1</v>
+      </c>
+      <c r="H96" s="25">
+        <v>0</v>
+      </c>
+      <c r="I96" s="25">
+        <v>109</v>
+      </c>
+      <c r="J96" s="25">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="97" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A97" s="20">
+        <v>43997</v>
+      </c>
+      <c r="B97" s="21">
+        <v>88165</v>
+      </c>
+      <c r="C97" s="22">
+        <v>567</v>
+      </c>
+      <c r="D97" s="22">
+        <v>1499</v>
+      </c>
+      <c r="E97" s="22">
+        <v>3</v>
+      </c>
+      <c r="F97" s="22">
+        <v>7</v>
+      </c>
+      <c r="G97" s="22">
+        <v>1</v>
+      </c>
+      <c r="H97" s="22">
+        <v>0</v>
+      </c>
+      <c r="I97" s="22">
+        <v>109</v>
+      </c>
+      <c r="J97" s="22">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="98" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A98" s="20">
+        <v>43998</v>
+      </c>
+      <c r="B98" s="21">
+        <v>89151</v>
+      </c>
+      <c r="C98" s="22">
+        <v>986</v>
+      </c>
+      <c r="D98" s="22">
+        <v>1503</v>
+      </c>
+      <c r="E98" s="22">
+        <v>4</v>
+      </c>
+      <c r="F98" s="22">
+        <v>7</v>
+      </c>
+      <c r="G98" s="22">
+        <v>1</v>
+      </c>
+      <c r="H98" s="22">
+        <v>0</v>
+      </c>
+      <c r="I98" s="22">
+        <v>109</v>
+      </c>
+      <c r="J98" s="22">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="99" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A99" s="29">
+        <v>43999</v>
+      </c>
+      <c r="B99" s="30">
+        <v>90103</v>
+      </c>
+      <c r="C99" s="31">
+        <v>952</v>
+      </c>
+      <c r="D99" s="31">
+        <v>1511</v>
+      </c>
+      <c r="E99" s="31">
+        <v>8</v>
+      </c>
+      <c r="F99" s="31">
+        <v>6</v>
+      </c>
+      <c r="G99" s="31">
+        <v>1</v>
+      </c>
+      <c r="H99" s="31">
+        <v>1</v>
+      </c>
+      <c r="I99" s="31">
+        <v>109</v>
+      </c>
+      <c r="J99" s="31">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="100" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A100" s="20">
+        <v>44000</v>
+      </c>
+      <c r="B100" s="21">
+        <v>91005</v>
+      </c>
+      <c r="C100" s="22">
+        <v>902</v>
+      </c>
+      <c r="D100" s="22">
+        <v>1513</v>
+      </c>
+      <c r="E100" s="22">
+        <v>2</v>
+      </c>
+      <c r="F100" s="22">
+        <v>8</v>
+      </c>
+      <c r="G100" s="22">
+        <v>1</v>
+      </c>
+      <c r="H100" s="22">
+        <v>0</v>
+      </c>
+      <c r="I100" s="22">
+        <v>109</v>
+      </c>
+      <c r="J100" s="22">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="101" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A101" s="29">
+        <v>44001</v>
+      </c>
+      <c r="B101" s="30">
+        <v>92152</v>
+      </c>
+      <c r="C101" s="31">
+        <v>1147</v>
+      </c>
+      <c r="D101" s="31">
+        <v>1519</v>
+      </c>
+      <c r="E101" s="31">
+        <v>6</v>
+      </c>
+      <c r="F101" s="31">
+        <v>6</v>
+      </c>
+      <c r="G101" s="31">
+        <v>1</v>
+      </c>
+      <c r="H101" s="31">
+        <v>2</v>
+      </c>
+      <c r="I101" s="31">
+        <v>109</v>
+      </c>
+      <c r="J101" s="31">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="102" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A102" s="23">
+        <v>44002</v>
+      </c>
+      <c r="B102" s="24">
+        <v>92919</v>
+      </c>
+      <c r="C102" s="25">
+        <v>758</v>
+      </c>
+      <c r="D102" s="25">
+        <v>1520</v>
+      </c>
+      <c r="E102" s="25">
+        <v>1</v>
+      </c>
+      <c r="F102" s="25">
+        <v>6</v>
+      </c>
+      <c r="G102" s="25">
+        <v>1</v>
+      </c>
+      <c r="H102" s="25">
+        <v>2</v>
+      </c>
+      <c r="I102" s="25">
+        <v>109</v>
+      </c>
+      <c r="J102" s="25">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="103" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A103" s="29">
+        <v>44003</v>
+      </c>
+      <c r="B103" s="30">
+        <v>93181</v>
+      </c>
+      <c r="C103" s="31">
+        <v>271</v>
+      </c>
+      <c r="D103" s="31">
+        <v>1521</v>
+      </c>
+      <c r="E103" s="31">
+        <v>1</v>
+      </c>
+      <c r="F103" s="31">
+        <v>6</v>
+      </c>
+      <c r="G103" s="31">
+        <v>1</v>
+      </c>
+      <c r="H103" s="31">
+        <v>0</v>
+      </c>
+      <c r="I103" s="31">
+        <v>109</v>
+      </c>
+      <c r="J103" s="31">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="104" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A104" s="29">
+        <v>44004</v>
+      </c>
+      <c r="B104" s="30">
+        <v>94165</v>
+      </c>
+      <c r="C104" s="31">
+        <v>984</v>
+      </c>
+      <c r="D104" s="31">
+        <v>1534</v>
+      </c>
+      <c r="E104" s="31">
+        <v>13</v>
+      </c>
+      <c r="F104" s="31">
+        <v>5</v>
+      </c>
+      <c r="G104" s="31">
+        <v>1</v>
+      </c>
+      <c r="H104" s="31">
+        <v>1</v>
+      </c>
+      <c r="I104" s="31">
+        <v>109</v>
+      </c>
+      <c r="J104" s="31">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="105" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A105" s="29">
+        <v>44005</v>
+      </c>
+      <c r="B105" s="30">
+        <v>95387</v>
+      </c>
+      <c r="C105" s="31">
+        <v>1222</v>
+      </c>
+      <c r="D105" s="31">
+        <v>1541</v>
+      </c>
+      <c r="E105" s="31">
+        <v>7</v>
+      </c>
+      <c r="F105" s="31">
+        <v>7</v>
+      </c>
+      <c r="G105" s="31">
+        <v>2</v>
+      </c>
+      <c r="H105" s="31">
+        <v>0</v>
+      </c>
+      <c r="I105" s="31" t="s">
+        <v>10</v>
+      </c>
+      <c r="J105" s="31">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="106" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A106" s="23">
+        <v>44006</v>
+      </c>
+      <c r="B106" s="24">
+        <v>96599</v>
+      </c>
+      <c r="C106" s="25">
+        <v>1212</v>
+      </c>
+      <c r="D106" s="25">
+        <v>1547</v>
+      </c>
+      <c r="E106" s="25">
+        <v>6</v>
+      </c>
+      <c r="F106" s="25">
+        <v>7</v>
+      </c>
+      <c r="G106" s="25">
+        <v>2</v>
+      </c>
+      <c r="H106" s="25">
+        <v>0</v>
+      </c>
+      <c r="I106" s="25" t="s">
+        <v>10</v>
+      </c>
+      <c r="J106" s="25">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="107" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A107" s="29">
+        <v>44007</v>
+      </c>
+      <c r="B107" s="30">
+        <v>97442</v>
+      </c>
+      <c r="C107" s="31">
+        <v>843</v>
+      </c>
+      <c r="D107" s="31">
+        <v>1558</v>
+      </c>
+      <c r="E107" s="31">
+        <v>11</v>
+      </c>
+      <c r="F107" s="31">
+        <v>8</v>
+      </c>
+      <c r="G107" s="31">
+        <v>2</v>
+      </c>
+      <c r="H107" s="31">
+        <v>0</v>
+      </c>
+      <c r="I107" s="31" t="s">
+        <v>10</v>
+      </c>
+      <c r="J107" s="31">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="108" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A108" s="29">
+        <v>44008</v>
+      </c>
+      <c r="B108" s="30">
+        <v>98320</v>
+      </c>
+      <c r="C108" s="31">
+        <v>878</v>
+      </c>
+      <c r="D108" s="31">
+        <v>1572</v>
+      </c>
+      <c r="E108" s="31">
+        <v>14</v>
+      </c>
+      <c r="F108" s="31">
+        <v>8</v>
+      </c>
+      <c r="G108" s="31">
+        <v>1</v>
+      </c>
+      <c r="H108" s="31">
+        <v>0</v>
+      </c>
+      <c r="I108" s="31" t="s">
+        <v>10</v>
+      </c>
+      <c r="J108" s="31">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="109" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A109" s="29">
+        <v>44009</v>
+      </c>
+      <c r="B109" s="30">
+        <v>98945</v>
+      </c>
+      <c r="C109" s="31">
+        <v>625</v>
+      </c>
+      <c r="D109" s="31">
+        <v>1581</v>
+      </c>
+      <c r="E109" s="31">
+        <v>9</v>
+      </c>
+      <c r="F109" s="31">
+        <v>7</v>
+      </c>
+      <c r="G109" s="31">
+        <v>0</v>
+      </c>
+      <c r="H109" s="31">
+        <v>1</v>
+      </c>
+      <c r="I109" s="31" t="s">
+        <v>10</v>
+      </c>
+      <c r="J109" s="31">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="110" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A110" s="29">
+        <v>44010</v>
+      </c>
+      <c r="B110" s="30">
+        <v>99245</v>
+      </c>
+      <c r="C110" s="31">
+        <v>300</v>
+      </c>
+      <c r="D110" s="31">
+        <v>1585</v>
+      </c>
+      <c r="E110" s="31">
+        <v>4</v>
+      </c>
+      <c r="F110" s="31">
+        <v>8</v>
+      </c>
+      <c r="G110" s="31">
+        <v>0</v>
+      </c>
+      <c r="H110" s="31">
+        <v>0</v>
+      </c>
+      <c r="I110" s="31" t="s">
+        <v>10</v>
+      </c>
+      <c r="J110" s="31">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="111" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A111" s="29">
+        <v>44011</v>
+      </c>
+      <c r="B111" s="30">
+        <v>100330</v>
+      </c>
+      <c r="C111" s="31">
+        <v>1085</v>
+      </c>
+      <c r="D111" s="31">
+        <v>1600</v>
+      </c>
+      <c r="E111" s="31">
+        <v>15</v>
+      </c>
+      <c r="F111" s="31">
+        <v>8</v>
+      </c>
+      <c r="G111" s="31">
+        <v>0</v>
+      </c>
+      <c r="H111" s="31">
+        <v>0</v>
+      </c>
+      <c r="I111" s="31" t="s">
+        <v>10</v>
+      </c>
+      <c r="J111" s="31">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="112" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A112" s="20">
+        <v>44012</v>
+      </c>
+      <c r="B112" s="21">
+        <v>101729</v>
+      </c>
+      <c r="C112" s="22">
+        <v>1399</v>
+      </c>
+      <c r="D112" s="22">
+        <v>1613</v>
+      </c>
+      <c r="E112" s="22">
+        <v>13</v>
+      </c>
+      <c r="F112" s="22">
+        <v>8</v>
+      </c>
+      <c r="G112" s="22">
+        <v>0</v>
+      </c>
+      <c r="H112" s="22">
+        <v>0</v>
+      </c>
+      <c r="I112" s="22" t="s">
+        <v>10</v>
+      </c>
+      <c r="J112" s="22">
+        <v>0</v>
+      </c>
+    </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>

</xml_diff>

<commit_message>
Data updated by GitHub Bot (2020-07-02 12)
</commit_message>
<xml_diff>
--- a/output/snapshot/fdcf2531-4c3e-5c02-b63c-ee160ead6dea.xlsx
+++ b/output/snapshot/fdcf2531-4c3e-5c02-b63c-ee160ead6dea.xlsx
@@ -1,16 +1,15 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="21929"/>
-  <workbookPr/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
+  <fileVersion appName="xl" lastEdited="6" lowestEdited="6" rupBuild="14420"/>
+  <workbookPr defaultThemeVersion="164011"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="I:\AKTUALNI PODATKI - KORONA\Za objavo na GOV.SI\ang\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{1E6DD62F-2BE2-47DC-A7ED-9B57C1589256}" xr6:coauthVersionLast="44" xr6:coauthVersionMax="44" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840"/>
   </bookViews>
   <sheets>
     <sheet name="Covid-19 podatki" sheetId="1" r:id="rId1"/>
@@ -25,7 +24,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="10" uniqueCount="10">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="19" uniqueCount="11">
   <si>
     <t>Date</t>
   </si>
@@ -56,15 +55,18 @@
   <si>
     <t>Deaths (daily)</t>
   </si>
+  <si>
+    <t>111*</t>
+  </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" mc:Ignorable="x14ac x16r2">
   <numFmts count="1">
     <numFmt numFmtId="164" formatCode="d/\ m/\ yyyy;@"/>
   </numFmts>
-  <fonts count="4" x14ac:knownFonts="1">
+  <fonts count="5" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -93,6 +95,13 @@
       <name val="Calibri Light"/>
       <scheme val="major"/>
     </font>
+    <font>
+      <sz val="10"/>
+      <color theme="1"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
   </fonts>
   <fills count="3">
     <fill>
@@ -108,7 +117,7 @@
       </patternFill>
     </fill>
   </fills>
-  <borders count="2">
+  <borders count="3">
     <border>
       <left/>
       <right/>
@@ -129,11 +138,26 @@
       <bottom/>
       <diagonal/>
     </border>
+    <border>
+      <left style="thin">
+        <color theme="4"/>
+      </left>
+      <right style="thin">
+        <color theme="4"/>
+      </right>
+      <top style="thin">
+        <color theme="4"/>
+      </top>
+      <bottom style="thin">
+        <color theme="4"/>
+      </bottom>
+      <diagonal/>
+    </border>
   </borders>
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="26">
+  <cellXfs count="32">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="49" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyAlignment="1" applyProtection="1">
       <alignment horizontal="left" vertical="top"/>
@@ -208,6 +232,24 @@
       <alignment horizontal="right"/>
     </xf>
     <xf numFmtId="0" fontId="3" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="right"/>
+    </xf>
+    <xf numFmtId="164" fontId="4" fillId="2" borderId="2" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="right" vertical="top"/>
+    </xf>
+    <xf numFmtId="3" fontId="4" fillId="2" borderId="2" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="right"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="2" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="right"/>
+    </xf>
+    <xf numFmtId="164" fontId="3" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="right" vertical="top"/>
+    </xf>
+    <xf numFmtId="3" fontId="3" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="right"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="right"/>
     </xf>
   </cellXfs>
@@ -399,8 +441,8 @@
 </file>
 
 <file path=xl/tables/table1.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="1" xr:uid="{00000000-000C-0000-FFFF-FFFF00000000}" name="Tabela1" displayName="Tabela1" ref="A1:J75" totalsRowShown="0" headerRowDxfId="11" dataDxfId="10">
-  <autoFilter ref="A1:J75" xr:uid="{00000000-0009-0000-0100-000001000000}">
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="1" name="Tabela1" displayName="Tabela1" ref="A1:J113" totalsRowShown="0" headerRowDxfId="11" dataDxfId="10">
+  <autoFilter ref="A1:J113">
     <filterColumn colId="0" hiddenButton="1"/>
     <filterColumn colId="1" hiddenButton="1"/>
     <filterColumn colId="2" hiddenButton="1"/>
@@ -413,16 +455,16 @@
     <filterColumn colId="9" hiddenButton="1"/>
   </autoFilter>
   <tableColumns count="10">
-    <tableColumn id="1" xr3:uid="{00000000-0010-0000-0000-000001000000}" name="Date" dataDxfId="9"/>
-    <tableColumn id="2" xr3:uid="{00000000-0010-0000-0000-000002000000}" name="Tested (all)" dataDxfId="8"/>
-    <tableColumn id="3" xr3:uid="{00000000-0010-0000-0000-000003000000}" name="Tested (daily)" dataDxfId="7"/>
-    <tableColumn id="4" xr3:uid="{00000000-0010-0000-0000-000004000000}" name="Positive (all)" dataDxfId="6"/>
-    <tableColumn id="5" xr3:uid="{00000000-0010-0000-0000-000005000000}" name="Positive (daily)" dataDxfId="5"/>
-    <tableColumn id="6" xr3:uid="{00000000-0010-0000-0000-000006000000}" name="All hospitalized on certain day" dataDxfId="4"/>
-    <tableColumn id="7" xr3:uid="{00000000-0010-0000-0000-000007000000}" name="All persons in intensive care on certain day" dataDxfId="3"/>
-    <tableColumn id="10" xr3:uid="{00000000-0010-0000-0000-00000A000000}" name="Discharged" dataDxfId="2"/>
-    <tableColumn id="8" xr3:uid="{00000000-0010-0000-0000-000008000000}" name="Deaths (all)" dataDxfId="1"/>
-    <tableColumn id="9" xr3:uid="{00000000-0010-0000-0000-000009000000}" name="Deaths (daily)" dataDxfId="0"/>
+    <tableColumn id="1" name="Date" dataDxfId="9"/>
+    <tableColumn id="2" name="Tested (all)" dataDxfId="8"/>
+    <tableColumn id="3" name="Tested (daily)" dataDxfId="7"/>
+    <tableColumn id="4" name="Positive (all)" dataDxfId="6"/>
+    <tableColumn id="5" name="Positive (daily)" dataDxfId="5"/>
+    <tableColumn id="6" name="All hospitalized on certain day" dataDxfId="4"/>
+    <tableColumn id="7" name="All persons in intensive care on certain day" dataDxfId="3"/>
+    <tableColumn id="10" name="Discharged" dataDxfId="2"/>
+    <tableColumn id="8" name="Deaths (all)" dataDxfId="1"/>
+    <tableColumn id="9" name="Deaths (daily)" dataDxfId="0"/>
   </tableColumns>
   <tableStyleInfo name="TableStyleLight16" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
   <extLst>
@@ -695,11 +737,11 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:J75"/>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <dimension ref="A1:J113"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A40" zoomScale="89" zoomScaleNormal="89" workbookViewId="0">
-      <selection activeCell="J74" sqref="J74"/>
+    <sheetView tabSelected="1" topLeftCell="A83" zoomScale="89" zoomScaleNormal="89" workbookViewId="0">
+      <selection activeCell="I113" sqref="I113"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -3117,6 +3159,1222 @@
         <v>0</v>
       </c>
     </row>
+    <row r="76" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A76" s="20">
+        <v>43976</v>
+      </c>
+      <c r="B76" s="21">
+        <v>75770</v>
+      </c>
+      <c r="C76" s="22">
+        <v>754</v>
+      </c>
+      <c r="D76" s="22">
+        <v>1469</v>
+      </c>
+      <c r="E76" s="22">
+        <v>0</v>
+      </c>
+      <c r="F76" s="22">
+        <v>9</v>
+      </c>
+      <c r="G76" s="22">
+        <v>2</v>
+      </c>
+      <c r="H76" s="22">
+        <v>6</v>
+      </c>
+      <c r="I76" s="22">
+        <v>108</v>
+      </c>
+      <c r="J76" s="22">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="77" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A77" s="20">
+        <v>43977</v>
+      </c>
+      <c r="B77" s="21">
+        <v>76579</v>
+      </c>
+      <c r="C77" s="22">
+        <v>809</v>
+      </c>
+      <c r="D77" s="22">
+        <v>1471</v>
+      </c>
+      <c r="E77" s="22">
+        <v>2</v>
+      </c>
+      <c r="F77" s="22">
+        <v>8</v>
+      </c>
+      <c r="G77" s="22">
+        <v>2</v>
+      </c>
+      <c r="H77" s="22">
+        <v>2</v>
+      </c>
+      <c r="I77" s="22">
+        <v>108</v>
+      </c>
+      <c r="J77" s="22">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="78" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A78" s="20">
+        <v>43978</v>
+      </c>
+      <c r="B78" s="21">
+        <v>77210</v>
+      </c>
+      <c r="C78" s="22">
+        <v>631</v>
+      </c>
+      <c r="D78" s="22">
+        <v>1473</v>
+      </c>
+      <c r="E78" s="22">
+        <v>2</v>
+      </c>
+      <c r="F78" s="22">
+        <v>7</v>
+      </c>
+      <c r="G78" s="22">
+        <v>2</v>
+      </c>
+      <c r="H78" s="22">
+        <v>1</v>
+      </c>
+      <c r="I78" s="22">
+        <v>108</v>
+      </c>
+      <c r="J78" s="22">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="79" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A79" s="20">
+        <v>43979</v>
+      </c>
+      <c r="B79" s="21">
+        <v>77916</v>
+      </c>
+      <c r="C79" s="22">
+        <v>706</v>
+      </c>
+      <c r="D79" s="22">
+        <v>1473</v>
+      </c>
+      <c r="E79" s="22">
+        <v>0</v>
+      </c>
+      <c r="F79" s="22">
+        <v>7</v>
+      </c>
+      <c r="G79" s="22">
+        <v>2</v>
+      </c>
+      <c r="H79" s="22">
+        <v>0</v>
+      </c>
+      <c r="I79" s="22">
+        <v>108</v>
+      </c>
+      <c r="J79" s="22">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="80" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A80" s="20">
+        <v>43980</v>
+      </c>
+      <c r="B80" s="21">
+        <v>78529</v>
+      </c>
+      <c r="C80" s="22">
+        <v>613</v>
+      </c>
+      <c r="D80" s="22">
+        <v>1473</v>
+      </c>
+      <c r="E80" s="22">
+        <v>0</v>
+      </c>
+      <c r="F80" s="22">
+        <v>7</v>
+      </c>
+      <c r="G80" s="22">
+        <v>2</v>
+      </c>
+      <c r="H80" s="22">
+        <v>0</v>
+      </c>
+      <c r="I80" s="22">
+        <v>108</v>
+      </c>
+      <c r="J80" s="22">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="81" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A81" s="20">
+        <v>43981</v>
+      </c>
+      <c r="B81" s="22">
+        <v>78793</v>
+      </c>
+      <c r="C81" s="22">
+        <v>264</v>
+      </c>
+      <c r="D81" s="22">
+        <v>1473</v>
+      </c>
+      <c r="E81" s="22">
+        <v>0</v>
+      </c>
+      <c r="F81" s="22">
+        <v>6</v>
+      </c>
+      <c r="G81" s="22">
+        <v>2</v>
+      </c>
+      <c r="H81" s="22">
+        <v>1</v>
+      </c>
+      <c r="I81" s="22">
+        <v>108</v>
+      </c>
+      <c r="J81" s="22">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="82" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A82" s="20">
+        <v>43982</v>
+      </c>
+      <c r="B82" s="21">
+        <v>79039</v>
+      </c>
+      <c r="C82" s="22">
+        <v>246</v>
+      </c>
+      <c r="D82" s="22">
+        <v>1473</v>
+      </c>
+      <c r="E82" s="22">
+        <v>0</v>
+      </c>
+      <c r="F82" s="22">
+        <v>5</v>
+      </c>
+      <c r="G82" s="22">
+        <v>1</v>
+      </c>
+      <c r="H82" s="22">
+        <v>0</v>
+      </c>
+      <c r="I82" s="22">
+        <v>109</v>
+      </c>
+      <c r="J82" s="22">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="83" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A83" s="20">
+        <v>43983</v>
+      </c>
+      <c r="B83" s="21">
+        <v>79698</v>
+      </c>
+      <c r="C83" s="22">
+        <v>659</v>
+      </c>
+      <c r="D83" s="22">
+        <v>1475</v>
+      </c>
+      <c r="E83" s="22">
+        <v>2</v>
+      </c>
+      <c r="F83" s="22">
+        <v>5</v>
+      </c>
+      <c r="G83" s="22">
+        <v>1</v>
+      </c>
+      <c r="H83" s="22">
+        <v>0</v>
+      </c>
+      <c r="I83" s="22">
+        <v>109</v>
+      </c>
+      <c r="J83" s="22">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="84" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A84" s="20">
+        <v>43984</v>
+      </c>
+      <c r="B84" s="21">
+        <v>80505</v>
+      </c>
+      <c r="C84" s="22">
+        <v>807</v>
+      </c>
+      <c r="D84" s="22">
+        <v>1477</v>
+      </c>
+      <c r="E84" s="22">
+        <v>2</v>
+      </c>
+      <c r="F84" s="22">
+        <v>5</v>
+      </c>
+      <c r="G84" s="22">
+        <v>0</v>
+      </c>
+      <c r="H84" s="22">
+        <v>0</v>
+      </c>
+      <c r="I84" s="22">
+        <v>109</v>
+      </c>
+      <c r="J84" s="22">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="85" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A85" s="20">
+        <v>43985</v>
+      </c>
+      <c r="B85" s="21">
+        <v>81333</v>
+      </c>
+      <c r="C85" s="22">
+        <v>828</v>
+      </c>
+      <c r="D85" s="22">
+        <v>1477</v>
+      </c>
+      <c r="E85" s="22">
+        <v>0</v>
+      </c>
+      <c r="F85" s="22">
+        <v>5</v>
+      </c>
+      <c r="G85" s="22">
+        <v>0</v>
+      </c>
+      <c r="H85" s="22">
+        <v>0</v>
+      </c>
+      <c r="I85" s="22">
+        <v>109</v>
+      </c>
+      <c r="J85" s="22">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="86" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A86" s="26">
+        <v>43986</v>
+      </c>
+      <c r="B86" s="27">
+        <v>82161</v>
+      </c>
+      <c r="C86" s="28">
+        <v>828</v>
+      </c>
+      <c r="D86" s="28">
+        <v>1479</v>
+      </c>
+      <c r="E86" s="28">
+        <v>2</v>
+      </c>
+      <c r="F86" s="28">
+        <v>6</v>
+      </c>
+      <c r="G86" s="28">
+        <v>0</v>
+      </c>
+      <c r="H86" s="28">
+        <v>0</v>
+      </c>
+      <c r="I86" s="28">
+        <v>109</v>
+      </c>
+      <c r="J86" s="28">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="87" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A87" s="29">
+        <v>43987</v>
+      </c>
+      <c r="B87" s="30">
+        <v>82876</v>
+      </c>
+      <c r="C87" s="31">
+        <v>715</v>
+      </c>
+      <c r="D87" s="31">
+        <v>1484</v>
+      </c>
+      <c r="E87" s="31">
+        <v>5</v>
+      </c>
+      <c r="F87" s="31">
+        <v>6</v>
+      </c>
+      <c r="G87" s="31">
+        <v>0</v>
+      </c>
+      <c r="H87" s="31">
+        <v>0</v>
+      </c>
+      <c r="I87" s="31">
+        <v>109</v>
+      </c>
+      <c r="J87" s="31">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="88" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A88" s="23">
+        <v>43988</v>
+      </c>
+      <c r="B88" s="24">
+        <v>83105</v>
+      </c>
+      <c r="C88" s="25">
+        <v>229</v>
+      </c>
+      <c r="D88" s="25">
+        <v>1485</v>
+      </c>
+      <c r="E88" s="25">
+        <v>1</v>
+      </c>
+      <c r="F88" s="25">
+        <v>5</v>
+      </c>
+      <c r="G88" s="25">
+        <v>0</v>
+      </c>
+      <c r="H88" s="25">
+        <v>1</v>
+      </c>
+      <c r="I88" s="25">
+        <v>109</v>
+      </c>
+      <c r="J88" s="25">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="89" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A89" s="29">
+        <v>43989</v>
+      </c>
+      <c r="B89" s="30">
+        <v>83316</v>
+      </c>
+      <c r="C89" s="31">
+        <v>211</v>
+      </c>
+      <c r="D89" s="31">
+        <v>1485</v>
+      </c>
+      <c r="E89" s="31">
+        <v>0</v>
+      </c>
+      <c r="F89" s="31">
+        <v>5</v>
+      </c>
+      <c r="G89" s="31">
+        <v>0</v>
+      </c>
+      <c r="H89" s="31">
+        <v>0</v>
+      </c>
+      <c r="I89" s="31">
+        <v>109</v>
+      </c>
+      <c r="J89" s="31">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="90" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A90" s="20">
+        <v>43990</v>
+      </c>
+      <c r="B90" s="21">
+        <v>84130</v>
+      </c>
+      <c r="C90" s="22">
+        <v>814</v>
+      </c>
+      <c r="D90" s="22">
+        <v>1486</v>
+      </c>
+      <c r="E90" s="22">
+        <v>1</v>
+      </c>
+      <c r="F90" s="22">
+        <v>6</v>
+      </c>
+      <c r="G90" s="22">
+        <v>0</v>
+      </c>
+      <c r="H90" s="22">
+        <v>0</v>
+      </c>
+      <c r="I90" s="22">
+        <v>109</v>
+      </c>
+      <c r="J90" s="22">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="91" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A91" s="20">
+        <v>43991</v>
+      </c>
+      <c r="B91" s="21">
+        <v>84868</v>
+      </c>
+      <c r="C91" s="22">
+        <v>738</v>
+      </c>
+      <c r="D91" s="22">
+        <v>1488</v>
+      </c>
+      <c r="E91" s="22">
+        <v>2</v>
+      </c>
+      <c r="F91" s="22">
+        <v>6</v>
+      </c>
+      <c r="G91" s="22">
+        <v>0</v>
+      </c>
+      <c r="H91" s="22">
+        <v>0</v>
+      </c>
+      <c r="I91" s="22">
+        <v>109</v>
+      </c>
+      <c r="J91" s="22">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="92" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A92" s="23">
+        <v>43992</v>
+      </c>
+      <c r="B92" s="24">
+        <v>85626</v>
+      </c>
+      <c r="C92" s="25">
+        <v>758</v>
+      </c>
+      <c r="D92" s="25">
+        <v>1488</v>
+      </c>
+      <c r="E92" s="25">
+        <v>0</v>
+      </c>
+      <c r="F92" s="25">
+        <v>6</v>
+      </c>
+      <c r="G92" s="25">
+        <v>0</v>
+      </c>
+      <c r="H92" s="25">
+        <v>0</v>
+      </c>
+      <c r="I92" s="25">
+        <v>109</v>
+      </c>
+      <c r="J92" s="25">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="93" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A93" s="29">
+        <v>43993</v>
+      </c>
+      <c r="B93" s="30">
+        <v>86328</v>
+      </c>
+      <c r="C93" s="31">
+        <v>702</v>
+      </c>
+      <c r="D93" s="31">
+        <v>1490</v>
+      </c>
+      <c r="E93" s="31">
+        <v>2</v>
+      </c>
+      <c r="F93" s="31">
+        <v>6</v>
+      </c>
+      <c r="G93" s="31">
+        <v>0</v>
+      </c>
+      <c r="H93" s="31">
+        <v>0</v>
+      </c>
+      <c r="I93" s="31">
+        <v>109</v>
+      </c>
+      <c r="J93" s="31">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="94" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A94" s="23">
+        <v>43994</v>
+      </c>
+      <c r="B94" s="24">
+        <v>87095</v>
+      </c>
+      <c r="C94" s="25">
+        <v>767</v>
+      </c>
+      <c r="D94" s="25">
+        <v>1492</v>
+      </c>
+      <c r="E94" s="25">
+        <v>2</v>
+      </c>
+      <c r="F94" s="25">
+        <v>6</v>
+      </c>
+      <c r="G94" s="25">
+        <v>0</v>
+      </c>
+      <c r="H94" s="25">
+        <v>0</v>
+      </c>
+      <c r="I94" s="25">
+        <v>109</v>
+      </c>
+      <c r="J94" s="25">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="95" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A95" s="29">
+        <v>43995</v>
+      </c>
+      <c r="B95" s="30">
+        <v>87386</v>
+      </c>
+      <c r="C95" s="31">
+        <v>291</v>
+      </c>
+      <c r="D95" s="31">
+        <v>1495</v>
+      </c>
+      <c r="E95" s="31">
+        <v>3</v>
+      </c>
+      <c r="F95" s="31">
+        <v>6</v>
+      </c>
+      <c r="G95" s="31">
+        <v>0</v>
+      </c>
+      <c r="H95" s="31">
+        <v>0</v>
+      </c>
+      <c r="I95" s="31">
+        <v>109</v>
+      </c>
+      <c r="J95" s="31">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="96" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A96" s="23">
+        <v>43996</v>
+      </c>
+      <c r="B96" s="24">
+        <v>87598</v>
+      </c>
+      <c r="C96" s="25">
+        <v>212</v>
+      </c>
+      <c r="D96" s="25">
+        <v>1496</v>
+      </c>
+      <c r="E96" s="25">
+        <v>1</v>
+      </c>
+      <c r="F96" s="25">
+        <v>7</v>
+      </c>
+      <c r="G96" s="25">
+        <v>1</v>
+      </c>
+      <c r="H96" s="25">
+        <v>0</v>
+      </c>
+      <c r="I96" s="25">
+        <v>109</v>
+      </c>
+      <c r="J96" s="25">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="97" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A97" s="20">
+        <v>43997</v>
+      </c>
+      <c r="B97" s="21">
+        <v>88165</v>
+      </c>
+      <c r="C97" s="22">
+        <v>567</v>
+      </c>
+      <c r="D97" s="22">
+        <v>1499</v>
+      </c>
+      <c r="E97" s="22">
+        <v>3</v>
+      </c>
+      <c r="F97" s="22">
+        <v>7</v>
+      </c>
+      <c r="G97" s="22">
+        <v>1</v>
+      </c>
+      <c r="H97" s="22">
+        <v>0</v>
+      </c>
+      <c r="I97" s="22">
+        <v>109</v>
+      </c>
+      <c r="J97" s="22">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="98" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A98" s="20">
+        <v>43998</v>
+      </c>
+      <c r="B98" s="21">
+        <v>89151</v>
+      </c>
+      <c r="C98" s="22">
+        <v>986</v>
+      </c>
+      <c r="D98" s="22">
+        <v>1503</v>
+      </c>
+      <c r="E98" s="22">
+        <v>4</v>
+      </c>
+      <c r="F98" s="22">
+        <v>7</v>
+      </c>
+      <c r="G98" s="22">
+        <v>1</v>
+      </c>
+      <c r="H98" s="22">
+        <v>0</v>
+      </c>
+      <c r="I98" s="22">
+        <v>109</v>
+      </c>
+      <c r="J98" s="22">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="99" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A99" s="29">
+        <v>43999</v>
+      </c>
+      <c r="B99" s="30">
+        <v>90103</v>
+      </c>
+      <c r="C99" s="31">
+        <v>952</v>
+      </c>
+      <c r="D99" s="31">
+        <v>1511</v>
+      </c>
+      <c r="E99" s="31">
+        <v>8</v>
+      </c>
+      <c r="F99" s="31">
+        <v>6</v>
+      </c>
+      <c r="G99" s="31">
+        <v>1</v>
+      </c>
+      <c r="H99" s="31">
+        <v>1</v>
+      </c>
+      <c r="I99" s="31">
+        <v>109</v>
+      </c>
+      <c r="J99" s="31">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="100" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A100" s="20">
+        <v>44000</v>
+      </c>
+      <c r="B100" s="21">
+        <v>91005</v>
+      </c>
+      <c r="C100" s="22">
+        <v>902</v>
+      </c>
+      <c r="D100" s="22">
+        <v>1513</v>
+      </c>
+      <c r="E100" s="22">
+        <v>2</v>
+      </c>
+      <c r="F100" s="22">
+        <v>8</v>
+      </c>
+      <c r="G100" s="22">
+        <v>1</v>
+      </c>
+      <c r="H100" s="22">
+        <v>0</v>
+      </c>
+      <c r="I100" s="22">
+        <v>109</v>
+      </c>
+      <c r="J100" s="22">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="101" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A101" s="29">
+        <v>44001</v>
+      </c>
+      <c r="B101" s="30">
+        <v>92152</v>
+      </c>
+      <c r="C101" s="31">
+        <v>1147</v>
+      </c>
+      <c r="D101" s="31">
+        <v>1519</v>
+      </c>
+      <c r="E101" s="31">
+        <v>6</v>
+      </c>
+      <c r="F101" s="31">
+        <v>6</v>
+      </c>
+      <c r="G101" s="31">
+        <v>1</v>
+      </c>
+      <c r="H101" s="31">
+        <v>2</v>
+      </c>
+      <c r="I101" s="31">
+        <v>109</v>
+      </c>
+      <c r="J101" s="31">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="102" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A102" s="23">
+        <v>44002</v>
+      </c>
+      <c r="B102" s="24">
+        <v>92919</v>
+      </c>
+      <c r="C102" s="25">
+        <v>758</v>
+      </c>
+      <c r="D102" s="25">
+        <v>1520</v>
+      </c>
+      <c r="E102" s="25">
+        <v>1</v>
+      </c>
+      <c r="F102" s="25">
+        <v>6</v>
+      </c>
+      <c r="G102" s="25">
+        <v>1</v>
+      </c>
+      <c r="H102" s="25">
+        <v>2</v>
+      </c>
+      <c r="I102" s="25">
+        <v>109</v>
+      </c>
+      <c r="J102" s="25">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="103" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A103" s="29">
+        <v>44003</v>
+      </c>
+      <c r="B103" s="30">
+        <v>93181</v>
+      </c>
+      <c r="C103" s="31">
+        <v>271</v>
+      </c>
+      <c r="D103" s="31">
+        <v>1521</v>
+      </c>
+      <c r="E103" s="31">
+        <v>1</v>
+      </c>
+      <c r="F103" s="31">
+        <v>6</v>
+      </c>
+      <c r="G103" s="31">
+        <v>1</v>
+      </c>
+      <c r="H103" s="31">
+        <v>0</v>
+      </c>
+      <c r="I103" s="31">
+        <v>109</v>
+      </c>
+      <c r="J103" s="31">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="104" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A104" s="29">
+        <v>44004</v>
+      </c>
+      <c r="B104" s="30">
+        <v>94165</v>
+      </c>
+      <c r="C104" s="31">
+        <v>984</v>
+      </c>
+      <c r="D104" s="31">
+        <v>1534</v>
+      </c>
+      <c r="E104" s="31">
+        <v>13</v>
+      </c>
+      <c r="F104" s="31">
+        <v>5</v>
+      </c>
+      <c r="G104" s="31">
+        <v>1</v>
+      </c>
+      <c r="H104" s="31">
+        <v>1</v>
+      </c>
+      <c r="I104" s="31">
+        <v>109</v>
+      </c>
+      <c r="J104" s="31">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="105" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A105" s="29">
+        <v>44005</v>
+      </c>
+      <c r="B105" s="30">
+        <v>95387</v>
+      </c>
+      <c r="C105" s="31">
+        <v>1222</v>
+      </c>
+      <c r="D105" s="31">
+        <v>1541</v>
+      </c>
+      <c r="E105" s="31">
+        <v>7</v>
+      </c>
+      <c r="F105" s="31">
+        <v>7</v>
+      </c>
+      <c r="G105" s="31">
+        <v>2</v>
+      </c>
+      <c r="H105" s="31">
+        <v>0</v>
+      </c>
+      <c r="I105" s="31" t="s">
+        <v>10</v>
+      </c>
+      <c r="J105" s="31">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="106" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A106" s="23">
+        <v>44006</v>
+      </c>
+      <c r="B106" s="24">
+        <v>96599</v>
+      </c>
+      <c r="C106" s="25">
+        <v>1212</v>
+      </c>
+      <c r="D106" s="25">
+        <v>1547</v>
+      </c>
+      <c r="E106" s="25">
+        <v>6</v>
+      </c>
+      <c r="F106" s="25">
+        <v>7</v>
+      </c>
+      <c r="G106" s="25">
+        <v>2</v>
+      </c>
+      <c r="H106" s="25">
+        <v>0</v>
+      </c>
+      <c r="I106" s="25" t="s">
+        <v>10</v>
+      </c>
+      <c r="J106" s="25">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="107" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A107" s="29">
+        <v>44007</v>
+      </c>
+      <c r="B107" s="30">
+        <v>97442</v>
+      </c>
+      <c r="C107" s="31">
+        <v>843</v>
+      </c>
+      <c r="D107" s="31">
+        <v>1558</v>
+      </c>
+      <c r="E107" s="31">
+        <v>11</v>
+      </c>
+      <c r="F107" s="31">
+        <v>8</v>
+      </c>
+      <c r="G107" s="31">
+        <v>2</v>
+      </c>
+      <c r="H107" s="31">
+        <v>0</v>
+      </c>
+      <c r="I107" s="31" t="s">
+        <v>10</v>
+      </c>
+      <c r="J107" s="31">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="108" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A108" s="29">
+        <v>44008</v>
+      </c>
+      <c r="B108" s="30">
+        <v>98320</v>
+      </c>
+      <c r="C108" s="31">
+        <v>878</v>
+      </c>
+      <c r="D108" s="31">
+        <v>1572</v>
+      </c>
+      <c r="E108" s="31">
+        <v>14</v>
+      </c>
+      <c r="F108" s="31">
+        <v>8</v>
+      </c>
+      <c r="G108" s="31">
+        <v>1</v>
+      </c>
+      <c r="H108" s="31">
+        <v>0</v>
+      </c>
+      <c r="I108" s="31" t="s">
+        <v>10</v>
+      </c>
+      <c r="J108" s="31">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="109" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A109" s="29">
+        <v>44009</v>
+      </c>
+      <c r="B109" s="30">
+        <v>98945</v>
+      </c>
+      <c r="C109" s="31">
+        <v>625</v>
+      </c>
+      <c r="D109" s="31">
+        <v>1581</v>
+      </c>
+      <c r="E109" s="31">
+        <v>9</v>
+      </c>
+      <c r="F109" s="31">
+        <v>7</v>
+      </c>
+      <c r="G109" s="31">
+        <v>0</v>
+      </c>
+      <c r="H109" s="31">
+        <v>1</v>
+      </c>
+      <c r="I109" s="31" t="s">
+        <v>10</v>
+      </c>
+      <c r="J109" s="31">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="110" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A110" s="29">
+        <v>44010</v>
+      </c>
+      <c r="B110" s="30">
+        <v>99245</v>
+      </c>
+      <c r="C110" s="31">
+        <v>300</v>
+      </c>
+      <c r="D110" s="31">
+        <v>1585</v>
+      </c>
+      <c r="E110" s="31">
+        <v>4</v>
+      </c>
+      <c r="F110" s="31">
+        <v>8</v>
+      </c>
+      <c r="G110" s="31">
+        <v>0</v>
+      </c>
+      <c r="H110" s="31">
+        <v>0</v>
+      </c>
+      <c r="I110" s="31" t="s">
+        <v>10</v>
+      </c>
+      <c r="J110" s="31">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="111" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A111" s="29">
+        <v>44011</v>
+      </c>
+      <c r="B111" s="30">
+        <v>100330</v>
+      </c>
+      <c r="C111" s="31">
+        <v>1085</v>
+      </c>
+      <c r="D111" s="31">
+        <v>1600</v>
+      </c>
+      <c r="E111" s="31">
+        <v>15</v>
+      </c>
+      <c r="F111" s="31">
+        <v>8</v>
+      </c>
+      <c r="G111" s="31">
+        <v>0</v>
+      </c>
+      <c r="H111" s="31">
+        <v>0</v>
+      </c>
+      <c r="I111" s="31" t="s">
+        <v>10</v>
+      </c>
+      <c r="J111" s="31">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="112" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A112" s="20">
+        <v>44012</v>
+      </c>
+      <c r="B112" s="21">
+        <v>101729</v>
+      </c>
+      <c r="C112" s="22">
+        <v>1399</v>
+      </c>
+      <c r="D112" s="22">
+        <v>1613</v>
+      </c>
+      <c r="E112" s="22">
+        <v>13</v>
+      </c>
+      <c r="F112" s="22">
+        <v>8</v>
+      </c>
+      <c r="G112" s="22">
+        <v>0</v>
+      </c>
+      <c r="H112" s="22">
+        <v>0</v>
+      </c>
+      <c r="I112" s="22" t="s">
+        <v>10</v>
+      </c>
+      <c r="J112" s="22">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="113" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A113" s="20">
+        <v>44013</v>
+      </c>
+      <c r="B113" s="21">
+        <v>102927</v>
+      </c>
+      <c r="C113" s="22">
+        <v>1198</v>
+      </c>
+      <c r="D113" s="22">
+        <v>1663</v>
+      </c>
+      <c r="E113" s="22">
+        <v>21</v>
+      </c>
+      <c r="F113" s="22">
+        <v>9</v>
+      </c>
+      <c r="G113" s="22">
+        <v>0</v>
+      </c>
+      <c r="H113" s="22">
+        <v>0</v>
+      </c>
+      <c r="I113" s="22" t="s">
+        <v>10</v>
+      </c>
+      <c r="J113" s="22">
+        <v>0</v>
+      </c>
+    </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>

</xml_diff>

<commit_message>
Data updated by GitHub Bot (2020-07-02 20)
</commit_message>
<xml_diff>
--- a/output/snapshot/fdcf2531-4c3e-5c02-b63c-ee160ead6dea.xlsx
+++ b/output/snapshot/fdcf2531-4c3e-5c02-b63c-ee160ead6dea.xlsx
@@ -1,16 +1,15 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="21929"/>
-  <workbookPr/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
+  <fileVersion appName="xl" lastEdited="6" lowestEdited="6" rupBuild="14420"/>
+  <workbookPr defaultThemeVersion="164011"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="I:\AKTUALNI PODATKI - KORONA\Za objavo na GOV.SI\ang\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{1E6DD62F-2BE2-47DC-A7ED-9B57C1589256}" xr6:coauthVersionLast="44" xr6:coauthVersionMax="44" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840"/>
   </bookViews>
   <sheets>
     <sheet name="Covid-19 podatki" sheetId="1" r:id="rId1"/>
@@ -25,7 +24,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="10" uniqueCount="10">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="19" uniqueCount="11">
   <si>
     <t>Date</t>
   </si>
@@ -56,15 +55,18 @@
   <si>
     <t>Deaths (daily)</t>
   </si>
+  <si>
+    <t>111*</t>
+  </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" mc:Ignorable="x14ac x16r2">
   <numFmts count="1">
     <numFmt numFmtId="164" formatCode="d/\ m/\ yyyy;@"/>
   </numFmts>
-  <fonts count="4" x14ac:knownFonts="1">
+  <fonts count="5" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -93,6 +95,13 @@
       <name val="Calibri Light"/>
       <scheme val="major"/>
     </font>
+    <font>
+      <sz val="10"/>
+      <color theme="1"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
   </fonts>
   <fills count="3">
     <fill>
@@ -108,7 +117,7 @@
       </patternFill>
     </fill>
   </fills>
-  <borders count="2">
+  <borders count="3">
     <border>
       <left/>
       <right/>
@@ -129,11 +138,26 @@
       <bottom/>
       <diagonal/>
     </border>
+    <border>
+      <left style="thin">
+        <color theme="4"/>
+      </left>
+      <right style="thin">
+        <color theme="4"/>
+      </right>
+      <top style="thin">
+        <color theme="4"/>
+      </top>
+      <bottom style="thin">
+        <color theme="4"/>
+      </bottom>
+      <diagonal/>
+    </border>
   </borders>
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="26">
+  <cellXfs count="32">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="49" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyAlignment="1" applyProtection="1">
       <alignment horizontal="left" vertical="top"/>
@@ -208,6 +232,24 @@
       <alignment horizontal="right"/>
     </xf>
     <xf numFmtId="0" fontId="3" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="right"/>
+    </xf>
+    <xf numFmtId="164" fontId="4" fillId="2" borderId="2" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="right" vertical="top"/>
+    </xf>
+    <xf numFmtId="3" fontId="4" fillId="2" borderId="2" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="right"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="2" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="right"/>
+    </xf>
+    <xf numFmtId="164" fontId="3" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="right" vertical="top"/>
+    </xf>
+    <xf numFmtId="3" fontId="3" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="right"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="right"/>
     </xf>
   </cellXfs>
@@ -399,8 +441,8 @@
 </file>
 
 <file path=xl/tables/table1.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="1" xr:uid="{00000000-000C-0000-FFFF-FFFF00000000}" name="Tabela1" displayName="Tabela1" ref="A1:J75" totalsRowShown="0" headerRowDxfId="11" dataDxfId="10">
-  <autoFilter ref="A1:J75" xr:uid="{00000000-0009-0000-0100-000001000000}">
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="1" name="Tabela1" displayName="Tabela1" ref="A1:J113" totalsRowShown="0" headerRowDxfId="11" dataDxfId="10">
+  <autoFilter ref="A1:J113">
     <filterColumn colId="0" hiddenButton="1"/>
     <filterColumn colId="1" hiddenButton="1"/>
     <filterColumn colId="2" hiddenButton="1"/>
@@ -413,16 +455,16 @@
     <filterColumn colId="9" hiddenButton="1"/>
   </autoFilter>
   <tableColumns count="10">
-    <tableColumn id="1" xr3:uid="{00000000-0010-0000-0000-000001000000}" name="Date" dataDxfId="9"/>
-    <tableColumn id="2" xr3:uid="{00000000-0010-0000-0000-000002000000}" name="Tested (all)" dataDxfId="8"/>
-    <tableColumn id="3" xr3:uid="{00000000-0010-0000-0000-000003000000}" name="Tested (daily)" dataDxfId="7"/>
-    <tableColumn id="4" xr3:uid="{00000000-0010-0000-0000-000004000000}" name="Positive (all)" dataDxfId="6"/>
-    <tableColumn id="5" xr3:uid="{00000000-0010-0000-0000-000005000000}" name="Positive (daily)" dataDxfId="5"/>
-    <tableColumn id="6" xr3:uid="{00000000-0010-0000-0000-000006000000}" name="All hospitalized on certain day" dataDxfId="4"/>
-    <tableColumn id="7" xr3:uid="{00000000-0010-0000-0000-000007000000}" name="All persons in intensive care on certain day" dataDxfId="3"/>
-    <tableColumn id="10" xr3:uid="{00000000-0010-0000-0000-00000A000000}" name="Discharged" dataDxfId="2"/>
-    <tableColumn id="8" xr3:uid="{00000000-0010-0000-0000-000008000000}" name="Deaths (all)" dataDxfId="1"/>
-    <tableColumn id="9" xr3:uid="{00000000-0010-0000-0000-000009000000}" name="Deaths (daily)" dataDxfId="0"/>
+    <tableColumn id="1" name="Date" dataDxfId="9"/>
+    <tableColumn id="2" name="Tested (all)" dataDxfId="8"/>
+    <tableColumn id="3" name="Tested (daily)" dataDxfId="7"/>
+    <tableColumn id="4" name="Positive (all)" dataDxfId="6"/>
+    <tableColumn id="5" name="Positive (daily)" dataDxfId="5"/>
+    <tableColumn id="6" name="All hospitalized on certain day" dataDxfId="4"/>
+    <tableColumn id="7" name="All persons in intensive care on certain day" dataDxfId="3"/>
+    <tableColumn id="10" name="Discharged" dataDxfId="2"/>
+    <tableColumn id="8" name="Deaths (all)" dataDxfId="1"/>
+    <tableColumn id="9" name="Deaths (daily)" dataDxfId="0"/>
   </tableColumns>
   <tableStyleInfo name="TableStyleLight16" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
   <extLst>
@@ -695,11 +737,11 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:J75"/>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <dimension ref="A1:J113"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A40" zoomScale="89" zoomScaleNormal="89" workbookViewId="0">
-      <selection activeCell="J74" sqref="J74"/>
+    <sheetView tabSelected="1" topLeftCell="A83" zoomScale="89" zoomScaleNormal="89" workbookViewId="0">
+      <selection activeCell="I113" sqref="I113"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -3117,6 +3159,1222 @@
         <v>0</v>
       </c>
     </row>
+    <row r="76" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A76" s="20">
+        <v>43976</v>
+      </c>
+      <c r="B76" s="21">
+        <v>75770</v>
+      </c>
+      <c r="C76" s="22">
+        <v>754</v>
+      </c>
+      <c r="D76" s="22">
+        <v>1469</v>
+      </c>
+      <c r="E76" s="22">
+        <v>0</v>
+      </c>
+      <c r="F76" s="22">
+        <v>9</v>
+      </c>
+      <c r="G76" s="22">
+        <v>2</v>
+      </c>
+      <c r="H76" s="22">
+        <v>6</v>
+      </c>
+      <c r="I76" s="22">
+        <v>108</v>
+      </c>
+      <c r="J76" s="22">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="77" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A77" s="20">
+        <v>43977</v>
+      </c>
+      <c r="B77" s="21">
+        <v>76579</v>
+      </c>
+      <c r="C77" s="22">
+        <v>809</v>
+      </c>
+      <c r="D77" s="22">
+        <v>1471</v>
+      </c>
+      <c r="E77" s="22">
+        <v>2</v>
+      </c>
+      <c r="F77" s="22">
+        <v>8</v>
+      </c>
+      <c r="G77" s="22">
+        <v>2</v>
+      </c>
+      <c r="H77" s="22">
+        <v>2</v>
+      </c>
+      <c r="I77" s="22">
+        <v>108</v>
+      </c>
+      <c r="J77" s="22">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="78" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A78" s="20">
+        <v>43978</v>
+      </c>
+      <c r="B78" s="21">
+        <v>77210</v>
+      </c>
+      <c r="C78" s="22">
+        <v>631</v>
+      </c>
+      <c r="D78" s="22">
+        <v>1473</v>
+      </c>
+      <c r="E78" s="22">
+        <v>2</v>
+      </c>
+      <c r="F78" s="22">
+        <v>7</v>
+      </c>
+      <c r="G78" s="22">
+        <v>2</v>
+      </c>
+      <c r="H78" s="22">
+        <v>1</v>
+      </c>
+      <c r="I78" s="22">
+        <v>108</v>
+      </c>
+      <c r="J78" s="22">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="79" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A79" s="20">
+        <v>43979</v>
+      </c>
+      <c r="B79" s="21">
+        <v>77916</v>
+      </c>
+      <c r="C79" s="22">
+        <v>706</v>
+      </c>
+      <c r="D79" s="22">
+        <v>1473</v>
+      </c>
+      <c r="E79" s="22">
+        <v>0</v>
+      </c>
+      <c r="F79" s="22">
+        <v>7</v>
+      </c>
+      <c r="G79" s="22">
+        <v>2</v>
+      </c>
+      <c r="H79" s="22">
+        <v>0</v>
+      </c>
+      <c r="I79" s="22">
+        <v>108</v>
+      </c>
+      <c r="J79" s="22">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="80" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A80" s="20">
+        <v>43980</v>
+      </c>
+      <c r="B80" s="21">
+        <v>78529</v>
+      </c>
+      <c r="C80" s="22">
+        <v>613</v>
+      </c>
+      <c r="D80" s="22">
+        <v>1473</v>
+      </c>
+      <c r="E80" s="22">
+        <v>0</v>
+      </c>
+      <c r="F80" s="22">
+        <v>7</v>
+      </c>
+      <c r="G80" s="22">
+        <v>2</v>
+      </c>
+      <c r="H80" s="22">
+        <v>0</v>
+      </c>
+      <c r="I80" s="22">
+        <v>108</v>
+      </c>
+      <c r="J80" s="22">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="81" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A81" s="20">
+        <v>43981</v>
+      </c>
+      <c r="B81" s="22">
+        <v>78793</v>
+      </c>
+      <c r="C81" s="22">
+        <v>264</v>
+      </c>
+      <c r="D81" s="22">
+        <v>1473</v>
+      </c>
+      <c r="E81" s="22">
+        <v>0</v>
+      </c>
+      <c r="F81" s="22">
+        <v>6</v>
+      </c>
+      <c r="G81" s="22">
+        <v>2</v>
+      </c>
+      <c r="H81" s="22">
+        <v>1</v>
+      </c>
+      <c r="I81" s="22">
+        <v>108</v>
+      </c>
+      <c r="J81" s="22">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="82" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A82" s="20">
+        <v>43982</v>
+      </c>
+      <c r="B82" s="21">
+        <v>79039</v>
+      </c>
+      <c r="C82" s="22">
+        <v>246</v>
+      </c>
+      <c r="D82" s="22">
+        <v>1473</v>
+      </c>
+      <c r="E82" s="22">
+        <v>0</v>
+      </c>
+      <c r="F82" s="22">
+        <v>5</v>
+      </c>
+      <c r="G82" s="22">
+        <v>1</v>
+      </c>
+      <c r="H82" s="22">
+        <v>0</v>
+      </c>
+      <c r="I82" s="22">
+        <v>109</v>
+      </c>
+      <c r="J82" s="22">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="83" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A83" s="20">
+        <v>43983</v>
+      </c>
+      <c r="B83" s="21">
+        <v>79698</v>
+      </c>
+      <c r="C83" s="22">
+        <v>659</v>
+      </c>
+      <c r="D83" s="22">
+        <v>1475</v>
+      </c>
+      <c r="E83" s="22">
+        <v>2</v>
+      </c>
+      <c r="F83" s="22">
+        <v>5</v>
+      </c>
+      <c r="G83" s="22">
+        <v>1</v>
+      </c>
+      <c r="H83" s="22">
+        <v>0</v>
+      </c>
+      <c r="I83" s="22">
+        <v>109</v>
+      </c>
+      <c r="J83" s="22">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="84" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A84" s="20">
+        <v>43984</v>
+      </c>
+      <c r="B84" s="21">
+        <v>80505</v>
+      </c>
+      <c r="C84" s="22">
+        <v>807</v>
+      </c>
+      <c r="D84" s="22">
+        <v>1477</v>
+      </c>
+      <c r="E84" s="22">
+        <v>2</v>
+      </c>
+      <c r="F84" s="22">
+        <v>5</v>
+      </c>
+      <c r="G84" s="22">
+        <v>0</v>
+      </c>
+      <c r="H84" s="22">
+        <v>0</v>
+      </c>
+      <c r="I84" s="22">
+        <v>109</v>
+      </c>
+      <c r="J84" s="22">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="85" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A85" s="20">
+        <v>43985</v>
+      </c>
+      <c r="B85" s="21">
+        <v>81333</v>
+      </c>
+      <c r="C85" s="22">
+        <v>828</v>
+      </c>
+      <c r="D85" s="22">
+        <v>1477</v>
+      </c>
+      <c r="E85" s="22">
+        <v>0</v>
+      </c>
+      <c r="F85" s="22">
+        <v>5</v>
+      </c>
+      <c r="G85" s="22">
+        <v>0</v>
+      </c>
+      <c r="H85" s="22">
+        <v>0</v>
+      </c>
+      <c r="I85" s="22">
+        <v>109</v>
+      </c>
+      <c r="J85" s="22">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="86" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A86" s="26">
+        <v>43986</v>
+      </c>
+      <c r="B86" s="27">
+        <v>82161</v>
+      </c>
+      <c r="C86" s="28">
+        <v>828</v>
+      </c>
+      <c r="D86" s="28">
+        <v>1479</v>
+      </c>
+      <c r="E86" s="28">
+        <v>2</v>
+      </c>
+      <c r="F86" s="28">
+        <v>6</v>
+      </c>
+      <c r="G86" s="28">
+        <v>0</v>
+      </c>
+      <c r="H86" s="28">
+        <v>0</v>
+      </c>
+      <c r="I86" s="28">
+        <v>109</v>
+      </c>
+      <c r="J86" s="28">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="87" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A87" s="29">
+        <v>43987</v>
+      </c>
+      <c r="B87" s="30">
+        <v>82876</v>
+      </c>
+      <c r="C87" s="31">
+        <v>715</v>
+      </c>
+      <c r="D87" s="31">
+        <v>1484</v>
+      </c>
+      <c r="E87" s="31">
+        <v>5</v>
+      </c>
+      <c r="F87" s="31">
+        <v>6</v>
+      </c>
+      <c r="G87" s="31">
+        <v>0</v>
+      </c>
+      <c r="H87" s="31">
+        <v>0</v>
+      </c>
+      <c r="I87" s="31">
+        <v>109</v>
+      </c>
+      <c r="J87" s="31">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="88" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A88" s="23">
+        <v>43988</v>
+      </c>
+      <c r="B88" s="24">
+        <v>83105</v>
+      </c>
+      <c r="C88" s="25">
+        <v>229</v>
+      </c>
+      <c r="D88" s="25">
+        <v>1485</v>
+      </c>
+      <c r="E88" s="25">
+        <v>1</v>
+      </c>
+      <c r="F88" s="25">
+        <v>5</v>
+      </c>
+      <c r="G88" s="25">
+        <v>0</v>
+      </c>
+      <c r="H88" s="25">
+        <v>1</v>
+      </c>
+      <c r="I88" s="25">
+        <v>109</v>
+      </c>
+      <c r="J88" s="25">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="89" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A89" s="29">
+        <v>43989</v>
+      </c>
+      <c r="B89" s="30">
+        <v>83316</v>
+      </c>
+      <c r="C89" s="31">
+        <v>211</v>
+      </c>
+      <c r="D89" s="31">
+        <v>1485</v>
+      </c>
+      <c r="E89" s="31">
+        <v>0</v>
+      </c>
+      <c r="F89" s="31">
+        <v>5</v>
+      </c>
+      <c r="G89" s="31">
+        <v>0</v>
+      </c>
+      <c r="H89" s="31">
+        <v>0</v>
+      </c>
+      <c r="I89" s="31">
+        <v>109</v>
+      </c>
+      <c r="J89" s="31">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="90" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A90" s="20">
+        <v>43990</v>
+      </c>
+      <c r="B90" s="21">
+        <v>84130</v>
+      </c>
+      <c r="C90" s="22">
+        <v>814</v>
+      </c>
+      <c r="D90" s="22">
+        <v>1486</v>
+      </c>
+      <c r="E90" s="22">
+        <v>1</v>
+      </c>
+      <c r="F90" s="22">
+        <v>6</v>
+      </c>
+      <c r="G90" s="22">
+        <v>0</v>
+      </c>
+      <c r="H90" s="22">
+        <v>0</v>
+      </c>
+      <c r="I90" s="22">
+        <v>109</v>
+      </c>
+      <c r="J90" s="22">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="91" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A91" s="20">
+        <v>43991</v>
+      </c>
+      <c r="B91" s="21">
+        <v>84868</v>
+      </c>
+      <c r="C91" s="22">
+        <v>738</v>
+      </c>
+      <c r="D91" s="22">
+        <v>1488</v>
+      </c>
+      <c r="E91" s="22">
+        <v>2</v>
+      </c>
+      <c r="F91" s="22">
+        <v>6</v>
+      </c>
+      <c r="G91" s="22">
+        <v>0</v>
+      </c>
+      <c r="H91" s="22">
+        <v>0</v>
+      </c>
+      <c r="I91" s="22">
+        <v>109</v>
+      </c>
+      <c r="J91" s="22">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="92" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A92" s="23">
+        <v>43992</v>
+      </c>
+      <c r="B92" s="24">
+        <v>85626</v>
+      </c>
+      <c r="C92" s="25">
+        <v>758</v>
+      </c>
+      <c r="D92" s="25">
+        <v>1488</v>
+      </c>
+      <c r="E92" s="25">
+        <v>0</v>
+      </c>
+      <c r="F92" s="25">
+        <v>6</v>
+      </c>
+      <c r="G92" s="25">
+        <v>0</v>
+      </c>
+      <c r="H92" s="25">
+        <v>0</v>
+      </c>
+      <c r="I92" s="25">
+        <v>109</v>
+      </c>
+      <c r="J92" s="25">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="93" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A93" s="29">
+        <v>43993</v>
+      </c>
+      <c r="B93" s="30">
+        <v>86328</v>
+      </c>
+      <c r="C93" s="31">
+        <v>702</v>
+      </c>
+      <c r="D93" s="31">
+        <v>1490</v>
+      </c>
+      <c r="E93" s="31">
+        <v>2</v>
+      </c>
+      <c r="F93" s="31">
+        <v>6</v>
+      </c>
+      <c r="G93" s="31">
+        <v>0</v>
+      </c>
+      <c r="H93" s="31">
+        <v>0</v>
+      </c>
+      <c r="I93" s="31">
+        <v>109</v>
+      </c>
+      <c r="J93" s="31">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="94" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A94" s="23">
+        <v>43994</v>
+      </c>
+      <c r="B94" s="24">
+        <v>87095</v>
+      </c>
+      <c r="C94" s="25">
+        <v>767</v>
+      </c>
+      <c r="D94" s="25">
+        <v>1492</v>
+      </c>
+      <c r="E94" s="25">
+        <v>2</v>
+      </c>
+      <c r="F94" s="25">
+        <v>6</v>
+      </c>
+      <c r="G94" s="25">
+        <v>0</v>
+      </c>
+      <c r="H94" s="25">
+        <v>0</v>
+      </c>
+      <c r="I94" s="25">
+        <v>109</v>
+      </c>
+      <c r="J94" s="25">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="95" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A95" s="29">
+        <v>43995</v>
+      </c>
+      <c r="B95" s="30">
+        <v>87386</v>
+      </c>
+      <c r="C95" s="31">
+        <v>291</v>
+      </c>
+      <c r="D95" s="31">
+        <v>1495</v>
+      </c>
+      <c r="E95" s="31">
+        <v>3</v>
+      </c>
+      <c r="F95" s="31">
+        <v>6</v>
+      </c>
+      <c r="G95" s="31">
+        <v>0</v>
+      </c>
+      <c r="H95" s="31">
+        <v>0</v>
+      </c>
+      <c r="I95" s="31">
+        <v>109</v>
+      </c>
+      <c r="J95" s="31">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="96" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A96" s="23">
+        <v>43996</v>
+      </c>
+      <c r="B96" s="24">
+        <v>87598</v>
+      </c>
+      <c r="C96" s="25">
+        <v>212</v>
+      </c>
+      <c r="D96" s="25">
+        <v>1496</v>
+      </c>
+      <c r="E96" s="25">
+        <v>1</v>
+      </c>
+      <c r="F96" s="25">
+        <v>7</v>
+      </c>
+      <c r="G96" s="25">
+        <v>1</v>
+      </c>
+      <c r="H96" s="25">
+        <v>0</v>
+      </c>
+      <c r="I96" s="25">
+        <v>109</v>
+      </c>
+      <c r="J96" s="25">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="97" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A97" s="20">
+        <v>43997</v>
+      </c>
+      <c r="B97" s="21">
+        <v>88165</v>
+      </c>
+      <c r="C97" s="22">
+        <v>567</v>
+      </c>
+      <c r="D97" s="22">
+        <v>1499</v>
+      </c>
+      <c r="E97" s="22">
+        <v>3</v>
+      </c>
+      <c r="F97" s="22">
+        <v>7</v>
+      </c>
+      <c r="G97" s="22">
+        <v>1</v>
+      </c>
+      <c r="H97" s="22">
+        <v>0</v>
+      </c>
+      <c r="I97" s="22">
+        <v>109</v>
+      </c>
+      <c r="J97" s="22">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="98" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A98" s="20">
+        <v>43998</v>
+      </c>
+      <c r="B98" s="21">
+        <v>89151</v>
+      </c>
+      <c r="C98" s="22">
+        <v>986</v>
+      </c>
+      <c r="D98" s="22">
+        <v>1503</v>
+      </c>
+      <c r="E98" s="22">
+        <v>4</v>
+      </c>
+      <c r="F98" s="22">
+        <v>7</v>
+      </c>
+      <c r="G98" s="22">
+        <v>1</v>
+      </c>
+      <c r="H98" s="22">
+        <v>0</v>
+      </c>
+      <c r="I98" s="22">
+        <v>109</v>
+      </c>
+      <c r="J98" s="22">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="99" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A99" s="29">
+        <v>43999</v>
+      </c>
+      <c r="B99" s="30">
+        <v>90103</v>
+      </c>
+      <c r="C99" s="31">
+        <v>952</v>
+      </c>
+      <c r="D99" s="31">
+        <v>1511</v>
+      </c>
+      <c r="E99" s="31">
+        <v>8</v>
+      </c>
+      <c r="F99" s="31">
+        <v>6</v>
+      </c>
+      <c r="G99" s="31">
+        <v>1</v>
+      </c>
+      <c r="H99" s="31">
+        <v>1</v>
+      </c>
+      <c r="I99" s="31">
+        <v>109</v>
+      </c>
+      <c r="J99" s="31">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="100" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A100" s="20">
+        <v>44000</v>
+      </c>
+      <c r="B100" s="21">
+        <v>91005</v>
+      </c>
+      <c r="C100" s="22">
+        <v>902</v>
+      </c>
+      <c r="D100" s="22">
+        <v>1513</v>
+      </c>
+      <c r="E100" s="22">
+        <v>2</v>
+      </c>
+      <c r="F100" s="22">
+        <v>8</v>
+      </c>
+      <c r="G100" s="22">
+        <v>1</v>
+      </c>
+      <c r="H100" s="22">
+        <v>0</v>
+      </c>
+      <c r="I100" s="22">
+        <v>109</v>
+      </c>
+      <c r="J100" s="22">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="101" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A101" s="29">
+        <v>44001</v>
+      </c>
+      <c r="B101" s="30">
+        <v>92152</v>
+      </c>
+      <c r="C101" s="31">
+        <v>1147</v>
+      </c>
+      <c r="D101" s="31">
+        <v>1519</v>
+      </c>
+      <c r="E101" s="31">
+        <v>6</v>
+      </c>
+      <c r="F101" s="31">
+        <v>6</v>
+      </c>
+      <c r="G101" s="31">
+        <v>1</v>
+      </c>
+      <c r="H101" s="31">
+        <v>2</v>
+      </c>
+      <c r="I101" s="31">
+        <v>109</v>
+      </c>
+      <c r="J101" s="31">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="102" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A102" s="23">
+        <v>44002</v>
+      </c>
+      <c r="B102" s="24">
+        <v>92919</v>
+      </c>
+      <c r="C102" s="25">
+        <v>758</v>
+      </c>
+      <c r="D102" s="25">
+        <v>1520</v>
+      </c>
+      <c r="E102" s="25">
+        <v>1</v>
+      </c>
+      <c r="F102" s="25">
+        <v>6</v>
+      </c>
+      <c r="G102" s="25">
+        <v>1</v>
+      </c>
+      <c r="H102" s="25">
+        <v>2</v>
+      </c>
+      <c r="I102" s="25">
+        <v>109</v>
+      </c>
+      <c r="J102" s="25">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="103" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A103" s="29">
+        <v>44003</v>
+      </c>
+      <c r="B103" s="30">
+        <v>93181</v>
+      </c>
+      <c r="C103" s="31">
+        <v>271</v>
+      </c>
+      <c r="D103" s="31">
+        <v>1521</v>
+      </c>
+      <c r="E103" s="31">
+        <v>1</v>
+      </c>
+      <c r="F103" s="31">
+        <v>6</v>
+      </c>
+      <c r="G103" s="31">
+        <v>1</v>
+      </c>
+      <c r="H103" s="31">
+        <v>0</v>
+      </c>
+      <c r="I103" s="31">
+        <v>109</v>
+      </c>
+      <c r="J103" s="31">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="104" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A104" s="29">
+        <v>44004</v>
+      </c>
+      <c r="B104" s="30">
+        <v>94165</v>
+      </c>
+      <c r="C104" s="31">
+        <v>984</v>
+      </c>
+      <c r="D104" s="31">
+        <v>1534</v>
+      </c>
+      <c r="E104" s="31">
+        <v>13</v>
+      </c>
+      <c r="F104" s="31">
+        <v>5</v>
+      </c>
+      <c r="G104" s="31">
+        <v>1</v>
+      </c>
+      <c r="H104" s="31">
+        <v>1</v>
+      </c>
+      <c r="I104" s="31">
+        <v>109</v>
+      </c>
+      <c r="J104" s="31">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="105" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A105" s="29">
+        <v>44005</v>
+      </c>
+      <c r="B105" s="30">
+        <v>95387</v>
+      </c>
+      <c r="C105" s="31">
+        <v>1222</v>
+      </c>
+      <c r="D105" s="31">
+        <v>1541</v>
+      </c>
+      <c r="E105" s="31">
+        <v>7</v>
+      </c>
+      <c r="F105" s="31">
+        <v>7</v>
+      </c>
+      <c r="G105" s="31">
+        <v>2</v>
+      </c>
+      <c r="H105" s="31">
+        <v>0</v>
+      </c>
+      <c r="I105" s="31" t="s">
+        <v>10</v>
+      </c>
+      <c r="J105" s="31">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="106" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A106" s="23">
+        <v>44006</v>
+      </c>
+      <c r="B106" s="24">
+        <v>96599</v>
+      </c>
+      <c r="C106" s="25">
+        <v>1212</v>
+      </c>
+      <c r="D106" s="25">
+        <v>1547</v>
+      </c>
+      <c r="E106" s="25">
+        <v>6</v>
+      </c>
+      <c r="F106" s="25">
+        <v>7</v>
+      </c>
+      <c r="G106" s="25">
+        <v>2</v>
+      </c>
+      <c r="H106" s="25">
+        <v>0</v>
+      </c>
+      <c r="I106" s="25" t="s">
+        <v>10</v>
+      </c>
+      <c r="J106" s="25">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="107" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A107" s="29">
+        <v>44007</v>
+      </c>
+      <c r="B107" s="30">
+        <v>97442</v>
+      </c>
+      <c r="C107" s="31">
+        <v>843</v>
+      </c>
+      <c r="D107" s="31">
+        <v>1558</v>
+      </c>
+      <c r="E107" s="31">
+        <v>11</v>
+      </c>
+      <c r="F107" s="31">
+        <v>8</v>
+      </c>
+      <c r="G107" s="31">
+        <v>2</v>
+      </c>
+      <c r="H107" s="31">
+        <v>0</v>
+      </c>
+      <c r="I107" s="31" t="s">
+        <v>10</v>
+      </c>
+      <c r="J107" s="31">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="108" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A108" s="29">
+        <v>44008</v>
+      </c>
+      <c r="B108" s="30">
+        <v>98320</v>
+      </c>
+      <c r="C108" s="31">
+        <v>878</v>
+      </c>
+      <c r="D108" s="31">
+        <v>1572</v>
+      </c>
+      <c r="E108" s="31">
+        <v>14</v>
+      </c>
+      <c r="F108" s="31">
+        <v>8</v>
+      </c>
+      <c r="G108" s="31">
+        <v>1</v>
+      </c>
+      <c r="H108" s="31">
+        <v>0</v>
+      </c>
+      <c r="I108" s="31" t="s">
+        <v>10</v>
+      </c>
+      <c r="J108" s="31">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="109" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A109" s="29">
+        <v>44009</v>
+      </c>
+      <c r="B109" s="30">
+        <v>98945</v>
+      </c>
+      <c r="C109" s="31">
+        <v>625</v>
+      </c>
+      <c r="D109" s="31">
+        <v>1581</v>
+      </c>
+      <c r="E109" s="31">
+        <v>9</v>
+      </c>
+      <c r="F109" s="31">
+        <v>7</v>
+      </c>
+      <c r="G109" s="31">
+        <v>0</v>
+      </c>
+      <c r="H109" s="31">
+        <v>1</v>
+      </c>
+      <c r="I109" s="31" t="s">
+        <v>10</v>
+      </c>
+      <c r="J109" s="31">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="110" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A110" s="29">
+        <v>44010</v>
+      </c>
+      <c r="B110" s="30">
+        <v>99245</v>
+      </c>
+      <c r="C110" s="31">
+        <v>300</v>
+      </c>
+      <c r="D110" s="31">
+        <v>1585</v>
+      </c>
+      <c r="E110" s="31">
+        <v>4</v>
+      </c>
+      <c r="F110" s="31">
+        <v>8</v>
+      </c>
+      <c r="G110" s="31">
+        <v>0</v>
+      </c>
+      <c r="H110" s="31">
+        <v>0</v>
+      </c>
+      <c r="I110" s="31" t="s">
+        <v>10</v>
+      </c>
+      <c r="J110" s="31">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="111" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A111" s="29">
+        <v>44011</v>
+      </c>
+      <c r="B111" s="30">
+        <v>100330</v>
+      </c>
+      <c r="C111" s="31">
+        <v>1085</v>
+      </c>
+      <c r="D111" s="31">
+        <v>1600</v>
+      </c>
+      <c r="E111" s="31">
+        <v>15</v>
+      </c>
+      <c r="F111" s="31">
+        <v>8</v>
+      </c>
+      <c r="G111" s="31">
+        <v>0</v>
+      </c>
+      <c r="H111" s="31">
+        <v>0</v>
+      </c>
+      <c r="I111" s="31" t="s">
+        <v>10</v>
+      </c>
+      <c r="J111" s="31">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="112" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A112" s="20">
+        <v>44012</v>
+      </c>
+      <c r="B112" s="21">
+        <v>101729</v>
+      </c>
+      <c r="C112" s="22">
+        <v>1399</v>
+      </c>
+      <c r="D112" s="22">
+        <v>1613</v>
+      </c>
+      <c r="E112" s="22">
+        <v>13</v>
+      </c>
+      <c r="F112" s="22">
+        <v>8</v>
+      </c>
+      <c r="G112" s="22">
+        <v>0</v>
+      </c>
+      <c r="H112" s="22">
+        <v>0</v>
+      </c>
+      <c r="I112" s="22" t="s">
+        <v>10</v>
+      </c>
+      <c r="J112" s="22">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="113" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A113" s="20">
+        <v>44013</v>
+      </c>
+      <c r="B113" s="21">
+        <v>102927</v>
+      </c>
+      <c r="C113" s="22">
+        <v>1198</v>
+      </c>
+      <c r="D113" s="22">
+        <v>1663</v>
+      </c>
+      <c r="E113" s="22">
+        <v>21</v>
+      </c>
+      <c r="F113" s="22">
+        <v>9</v>
+      </c>
+      <c r="G113" s="22">
+        <v>0</v>
+      </c>
+      <c r="H113" s="22">
+        <v>0</v>
+      </c>
+      <c r="I113" s="22" t="s">
+        <v>10</v>
+      </c>
+      <c r="J113" s="22">
+        <v>0</v>
+      </c>
+    </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>

</xml_diff>

<commit_message>
Data updated by GitHub Bot (2020-07-03 12)
</commit_message>
<xml_diff>
--- a/output/snapshot/fdcf2531-4c3e-5c02-b63c-ee160ead6dea.xlsx
+++ b/output/snapshot/fdcf2531-4c3e-5c02-b63c-ee160ead6dea.xlsx
@@ -1,16 +1,15 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="21929"/>
-  <workbookPr/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
+  <fileVersion appName="xl" lastEdited="6" lowestEdited="6" rupBuild="14420"/>
+  <workbookPr defaultThemeVersion="164011"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="I:\AKTUALNI PODATKI - KORONA\Za objavo na GOV.SI\ang\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{1E6DD62F-2BE2-47DC-A7ED-9B57C1589256}" xr6:coauthVersionLast="44" xr6:coauthVersionMax="44" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840"/>
   </bookViews>
   <sheets>
     <sheet name="Covid-19 podatki" sheetId="1" r:id="rId1"/>
@@ -25,7 +24,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="10" uniqueCount="10">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="19" uniqueCount="11">
   <si>
     <t>Date</t>
   </si>
@@ -56,15 +55,18 @@
   <si>
     <t>Deaths (daily)</t>
   </si>
+  <si>
+    <t>111*</t>
+  </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" mc:Ignorable="x14ac x16r2">
   <numFmts count="1">
     <numFmt numFmtId="164" formatCode="d/\ m/\ yyyy;@"/>
   </numFmts>
-  <fonts count="4" x14ac:knownFonts="1">
+  <fonts count="5" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -93,6 +95,13 @@
       <name val="Calibri Light"/>
       <scheme val="major"/>
     </font>
+    <font>
+      <sz val="10"/>
+      <color theme="1"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
   </fonts>
   <fills count="3">
     <fill>
@@ -108,7 +117,7 @@
       </patternFill>
     </fill>
   </fills>
-  <borders count="2">
+  <borders count="3">
     <border>
       <left/>
       <right/>
@@ -129,11 +138,26 @@
       <bottom/>
       <diagonal/>
     </border>
+    <border>
+      <left style="thin">
+        <color theme="4"/>
+      </left>
+      <right style="thin">
+        <color theme="4"/>
+      </right>
+      <top style="thin">
+        <color theme="4"/>
+      </top>
+      <bottom style="thin">
+        <color theme="4"/>
+      </bottom>
+      <diagonal/>
+    </border>
   </borders>
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="26">
+  <cellXfs count="32">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="49" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyAlignment="1" applyProtection="1">
       <alignment horizontal="left" vertical="top"/>
@@ -208,6 +232,24 @@
       <alignment horizontal="right"/>
     </xf>
     <xf numFmtId="0" fontId="3" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="right"/>
+    </xf>
+    <xf numFmtId="164" fontId="4" fillId="2" borderId="2" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="right" vertical="top"/>
+    </xf>
+    <xf numFmtId="3" fontId="4" fillId="2" borderId="2" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="right"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="2" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="right"/>
+    </xf>
+    <xf numFmtId="164" fontId="3" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="right" vertical="top"/>
+    </xf>
+    <xf numFmtId="3" fontId="3" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="right"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="right"/>
     </xf>
   </cellXfs>
@@ -399,8 +441,8 @@
 </file>
 
 <file path=xl/tables/table1.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="1" xr:uid="{00000000-000C-0000-FFFF-FFFF00000000}" name="Tabela1" displayName="Tabela1" ref="A1:J75" totalsRowShown="0" headerRowDxfId="11" dataDxfId="10">
-  <autoFilter ref="A1:J75" xr:uid="{00000000-0009-0000-0100-000001000000}">
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="1" name="Tabela1" displayName="Tabela1" ref="A1:J114" totalsRowShown="0" headerRowDxfId="11" dataDxfId="10">
+  <autoFilter ref="A1:J114">
     <filterColumn colId="0" hiddenButton="1"/>
     <filterColumn colId="1" hiddenButton="1"/>
     <filterColumn colId="2" hiddenButton="1"/>
@@ -413,16 +455,16 @@
     <filterColumn colId="9" hiddenButton="1"/>
   </autoFilter>
   <tableColumns count="10">
-    <tableColumn id="1" xr3:uid="{00000000-0010-0000-0000-000001000000}" name="Date" dataDxfId="9"/>
-    <tableColumn id="2" xr3:uid="{00000000-0010-0000-0000-000002000000}" name="Tested (all)" dataDxfId="8"/>
-    <tableColumn id="3" xr3:uid="{00000000-0010-0000-0000-000003000000}" name="Tested (daily)" dataDxfId="7"/>
-    <tableColumn id="4" xr3:uid="{00000000-0010-0000-0000-000004000000}" name="Positive (all)" dataDxfId="6"/>
-    <tableColumn id="5" xr3:uid="{00000000-0010-0000-0000-000005000000}" name="Positive (daily)" dataDxfId="5"/>
-    <tableColumn id="6" xr3:uid="{00000000-0010-0000-0000-000006000000}" name="All hospitalized on certain day" dataDxfId="4"/>
-    <tableColumn id="7" xr3:uid="{00000000-0010-0000-0000-000007000000}" name="All persons in intensive care on certain day" dataDxfId="3"/>
-    <tableColumn id="10" xr3:uid="{00000000-0010-0000-0000-00000A000000}" name="Discharged" dataDxfId="2"/>
-    <tableColumn id="8" xr3:uid="{00000000-0010-0000-0000-000008000000}" name="Deaths (all)" dataDxfId="1"/>
-    <tableColumn id="9" xr3:uid="{00000000-0010-0000-0000-000009000000}" name="Deaths (daily)" dataDxfId="0"/>
+    <tableColumn id="1" name="Date" dataDxfId="9"/>
+    <tableColumn id="2" name="Tested (all)" dataDxfId="8"/>
+    <tableColumn id="3" name="Tested (daily)" dataDxfId="7"/>
+    <tableColumn id="4" name="Positive (all)" dataDxfId="6"/>
+    <tableColumn id="5" name="Positive (daily)" dataDxfId="5"/>
+    <tableColumn id="6" name="All hospitalized on certain day" dataDxfId="4"/>
+    <tableColumn id="7" name="All persons in intensive care on certain day" dataDxfId="3"/>
+    <tableColumn id="10" name="Discharged" dataDxfId="2"/>
+    <tableColumn id="8" name="Deaths (all)" dataDxfId="1"/>
+    <tableColumn id="9" name="Deaths (daily)" dataDxfId="0"/>
   </tableColumns>
   <tableStyleInfo name="TableStyleLight16" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
   <extLst>
@@ -695,11 +737,11 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:J75"/>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <dimension ref="A1:J114"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A40" zoomScale="89" zoomScaleNormal="89" workbookViewId="0">
-      <selection activeCell="J74" sqref="J74"/>
+    <sheetView tabSelected="1" topLeftCell="A83" zoomScale="89" zoomScaleNormal="89" workbookViewId="0">
+      <selection activeCell="I114" sqref="I114"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -3117,6 +3159,1254 @@
         <v>0</v>
       </c>
     </row>
+    <row r="76" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A76" s="20">
+        <v>43976</v>
+      </c>
+      <c r="B76" s="21">
+        <v>75770</v>
+      </c>
+      <c r="C76" s="22">
+        <v>754</v>
+      </c>
+      <c r="D76" s="22">
+        <v>1469</v>
+      </c>
+      <c r="E76" s="22">
+        <v>0</v>
+      </c>
+      <c r="F76" s="22">
+        <v>9</v>
+      </c>
+      <c r="G76" s="22">
+        <v>2</v>
+      </c>
+      <c r="H76" s="22">
+        <v>6</v>
+      </c>
+      <c r="I76" s="22">
+        <v>108</v>
+      </c>
+      <c r="J76" s="22">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="77" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A77" s="20">
+        <v>43977</v>
+      </c>
+      <c r="B77" s="21">
+        <v>76579</v>
+      </c>
+      <c r="C77" s="22">
+        <v>809</v>
+      </c>
+      <c r="D77" s="22">
+        <v>1471</v>
+      </c>
+      <c r="E77" s="22">
+        <v>2</v>
+      </c>
+      <c r="F77" s="22">
+        <v>8</v>
+      </c>
+      <c r="G77" s="22">
+        <v>2</v>
+      </c>
+      <c r="H77" s="22">
+        <v>2</v>
+      </c>
+      <c r="I77" s="22">
+        <v>108</v>
+      </c>
+      <c r="J77" s="22">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="78" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A78" s="20">
+        <v>43978</v>
+      </c>
+      <c r="B78" s="21">
+        <v>77210</v>
+      </c>
+      <c r="C78" s="22">
+        <v>631</v>
+      </c>
+      <c r="D78" s="22">
+        <v>1473</v>
+      </c>
+      <c r="E78" s="22">
+        <v>2</v>
+      </c>
+      <c r="F78" s="22">
+        <v>7</v>
+      </c>
+      <c r="G78" s="22">
+        <v>2</v>
+      </c>
+      <c r="H78" s="22">
+        <v>1</v>
+      </c>
+      <c r="I78" s="22">
+        <v>108</v>
+      </c>
+      <c r="J78" s="22">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="79" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A79" s="20">
+        <v>43979</v>
+      </c>
+      <c r="B79" s="21">
+        <v>77916</v>
+      </c>
+      <c r="C79" s="22">
+        <v>706</v>
+      </c>
+      <c r="D79" s="22">
+        <v>1473</v>
+      </c>
+      <c r="E79" s="22">
+        <v>0</v>
+      </c>
+      <c r="F79" s="22">
+        <v>7</v>
+      </c>
+      <c r="G79" s="22">
+        <v>2</v>
+      </c>
+      <c r="H79" s="22">
+        <v>0</v>
+      </c>
+      <c r="I79" s="22">
+        <v>108</v>
+      </c>
+      <c r="J79" s="22">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="80" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A80" s="20">
+        <v>43980</v>
+      </c>
+      <c r="B80" s="21">
+        <v>78529</v>
+      </c>
+      <c r="C80" s="22">
+        <v>613</v>
+      </c>
+      <c r="D80" s="22">
+        <v>1473</v>
+      </c>
+      <c r="E80" s="22">
+        <v>0</v>
+      </c>
+      <c r="F80" s="22">
+        <v>7</v>
+      </c>
+      <c r="G80" s="22">
+        <v>2</v>
+      </c>
+      <c r="H80" s="22">
+        <v>0</v>
+      </c>
+      <c r="I80" s="22">
+        <v>108</v>
+      </c>
+      <c r="J80" s="22">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="81" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A81" s="20">
+        <v>43981</v>
+      </c>
+      <c r="B81" s="22">
+        <v>78793</v>
+      </c>
+      <c r="C81" s="22">
+        <v>264</v>
+      </c>
+      <c r="D81" s="22">
+        <v>1473</v>
+      </c>
+      <c r="E81" s="22">
+        <v>0</v>
+      </c>
+      <c r="F81" s="22">
+        <v>6</v>
+      </c>
+      <c r="G81" s="22">
+        <v>2</v>
+      </c>
+      <c r="H81" s="22">
+        <v>1</v>
+      </c>
+      <c r="I81" s="22">
+        <v>108</v>
+      </c>
+      <c r="J81" s="22">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="82" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A82" s="20">
+        <v>43982</v>
+      </c>
+      <c r="B82" s="21">
+        <v>79039</v>
+      </c>
+      <c r="C82" s="22">
+        <v>246</v>
+      </c>
+      <c r="D82" s="22">
+        <v>1473</v>
+      </c>
+      <c r="E82" s="22">
+        <v>0</v>
+      </c>
+      <c r="F82" s="22">
+        <v>5</v>
+      </c>
+      <c r="G82" s="22">
+        <v>1</v>
+      </c>
+      <c r="H82" s="22">
+        <v>0</v>
+      </c>
+      <c r="I82" s="22">
+        <v>109</v>
+      </c>
+      <c r="J82" s="22">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="83" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A83" s="20">
+        <v>43983</v>
+      </c>
+      <c r="B83" s="21">
+        <v>79698</v>
+      </c>
+      <c r="C83" s="22">
+        <v>659</v>
+      </c>
+      <c r="D83" s="22">
+        <v>1475</v>
+      </c>
+      <c r="E83" s="22">
+        <v>2</v>
+      </c>
+      <c r="F83" s="22">
+        <v>5</v>
+      </c>
+      <c r="G83" s="22">
+        <v>1</v>
+      </c>
+      <c r="H83" s="22">
+        <v>0</v>
+      </c>
+      <c r="I83" s="22">
+        <v>109</v>
+      </c>
+      <c r="J83" s="22">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="84" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A84" s="20">
+        <v>43984</v>
+      </c>
+      <c r="B84" s="21">
+        <v>80505</v>
+      </c>
+      <c r="C84" s="22">
+        <v>807</v>
+      </c>
+      <c r="D84" s="22">
+        <v>1477</v>
+      </c>
+      <c r="E84" s="22">
+        <v>2</v>
+      </c>
+      <c r="F84" s="22">
+        <v>5</v>
+      </c>
+      <c r="G84" s="22">
+        <v>0</v>
+      </c>
+      <c r="H84" s="22">
+        <v>0</v>
+      </c>
+      <c r="I84" s="22">
+        <v>109</v>
+      </c>
+      <c r="J84" s="22">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="85" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A85" s="20">
+        <v>43985</v>
+      </c>
+      <c r="B85" s="21">
+        <v>81333</v>
+      </c>
+      <c r="C85" s="22">
+        <v>828</v>
+      </c>
+      <c r="D85" s="22">
+        <v>1477</v>
+      </c>
+      <c r="E85" s="22">
+        <v>0</v>
+      </c>
+      <c r="F85" s="22">
+        <v>5</v>
+      </c>
+      <c r="G85" s="22">
+        <v>0</v>
+      </c>
+      <c r="H85" s="22">
+        <v>0</v>
+      </c>
+      <c r="I85" s="22">
+        <v>109</v>
+      </c>
+      <c r="J85" s="22">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="86" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A86" s="26">
+        <v>43986</v>
+      </c>
+      <c r="B86" s="27">
+        <v>82161</v>
+      </c>
+      <c r="C86" s="28">
+        <v>828</v>
+      </c>
+      <c r="D86" s="28">
+        <v>1479</v>
+      </c>
+      <c r="E86" s="28">
+        <v>2</v>
+      </c>
+      <c r="F86" s="28">
+        <v>6</v>
+      </c>
+      <c r="G86" s="28">
+        <v>0</v>
+      </c>
+      <c r="H86" s="28">
+        <v>0</v>
+      </c>
+      <c r="I86" s="28">
+        <v>109</v>
+      </c>
+      <c r="J86" s="28">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="87" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A87" s="29">
+        <v>43987</v>
+      </c>
+      <c r="B87" s="30">
+        <v>82876</v>
+      </c>
+      <c r="C87" s="31">
+        <v>715</v>
+      </c>
+      <c r="D87" s="31">
+        <v>1484</v>
+      </c>
+      <c r="E87" s="31">
+        <v>5</v>
+      </c>
+      <c r="F87" s="31">
+        <v>6</v>
+      </c>
+      <c r="G87" s="31">
+        <v>0</v>
+      </c>
+      <c r="H87" s="31">
+        <v>0</v>
+      </c>
+      <c r="I87" s="31">
+        <v>109</v>
+      </c>
+      <c r="J87" s="31">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="88" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A88" s="23">
+        <v>43988</v>
+      </c>
+      <c r="B88" s="24">
+        <v>83105</v>
+      </c>
+      <c r="C88" s="25">
+        <v>229</v>
+      </c>
+      <c r="D88" s="25">
+        <v>1485</v>
+      </c>
+      <c r="E88" s="25">
+        <v>1</v>
+      </c>
+      <c r="F88" s="25">
+        <v>5</v>
+      </c>
+      <c r="G88" s="25">
+        <v>0</v>
+      </c>
+      <c r="H88" s="25">
+        <v>1</v>
+      </c>
+      <c r="I88" s="25">
+        <v>109</v>
+      </c>
+      <c r="J88" s="25">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="89" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A89" s="29">
+        <v>43989</v>
+      </c>
+      <c r="B89" s="30">
+        <v>83316</v>
+      </c>
+      <c r="C89" s="31">
+        <v>211</v>
+      </c>
+      <c r="D89" s="31">
+        <v>1485</v>
+      </c>
+      <c r="E89" s="31">
+        <v>0</v>
+      </c>
+      <c r="F89" s="31">
+        <v>5</v>
+      </c>
+      <c r="G89" s="31">
+        <v>0</v>
+      </c>
+      <c r="H89" s="31">
+        <v>0</v>
+      </c>
+      <c r="I89" s="31">
+        <v>109</v>
+      </c>
+      <c r="J89" s="31">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="90" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A90" s="20">
+        <v>43990</v>
+      </c>
+      <c r="B90" s="21">
+        <v>84130</v>
+      </c>
+      <c r="C90" s="22">
+        <v>814</v>
+      </c>
+      <c r="D90" s="22">
+        <v>1486</v>
+      </c>
+      <c r="E90" s="22">
+        <v>1</v>
+      </c>
+      <c r="F90" s="22">
+        <v>6</v>
+      </c>
+      <c r="G90" s="22">
+        <v>0</v>
+      </c>
+      <c r="H90" s="22">
+        <v>0</v>
+      </c>
+      <c r="I90" s="22">
+        <v>109</v>
+      </c>
+      <c r="J90" s="22">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="91" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A91" s="20">
+        <v>43991</v>
+      </c>
+      <c r="B91" s="21">
+        <v>84868</v>
+      </c>
+      <c r="C91" s="22">
+        <v>738</v>
+      </c>
+      <c r="D91" s="22">
+        <v>1488</v>
+      </c>
+      <c r="E91" s="22">
+        <v>2</v>
+      </c>
+      <c r="F91" s="22">
+        <v>6</v>
+      </c>
+      <c r="G91" s="22">
+        <v>0</v>
+      </c>
+      <c r="H91" s="22">
+        <v>0</v>
+      </c>
+      <c r="I91" s="22">
+        <v>109</v>
+      </c>
+      <c r="J91" s="22">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="92" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A92" s="23">
+        <v>43992</v>
+      </c>
+      <c r="B92" s="24">
+        <v>85626</v>
+      </c>
+      <c r="C92" s="25">
+        <v>758</v>
+      </c>
+      <c r="D92" s="25">
+        <v>1488</v>
+      </c>
+      <c r="E92" s="25">
+        <v>0</v>
+      </c>
+      <c r="F92" s="25">
+        <v>6</v>
+      </c>
+      <c r="G92" s="25">
+        <v>0</v>
+      </c>
+      <c r="H92" s="25">
+        <v>0</v>
+      </c>
+      <c r="I92" s="25">
+        <v>109</v>
+      </c>
+      <c r="J92" s="25">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="93" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A93" s="29">
+        <v>43993</v>
+      </c>
+      <c r="B93" s="30">
+        <v>86328</v>
+      </c>
+      <c r="C93" s="31">
+        <v>702</v>
+      </c>
+      <c r="D93" s="31">
+        <v>1490</v>
+      </c>
+      <c r="E93" s="31">
+        <v>2</v>
+      </c>
+      <c r="F93" s="31">
+        <v>6</v>
+      </c>
+      <c r="G93" s="31">
+        <v>0</v>
+      </c>
+      <c r="H93" s="31">
+        <v>0</v>
+      </c>
+      <c r="I93" s="31">
+        <v>109</v>
+      </c>
+      <c r="J93" s="31">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="94" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A94" s="23">
+        <v>43994</v>
+      </c>
+      <c r="B94" s="24">
+        <v>87095</v>
+      </c>
+      <c r="C94" s="25">
+        <v>767</v>
+      </c>
+      <c r="D94" s="25">
+        <v>1492</v>
+      </c>
+      <c r="E94" s="25">
+        <v>2</v>
+      </c>
+      <c r="F94" s="25">
+        <v>6</v>
+      </c>
+      <c r="G94" s="25">
+        <v>0</v>
+      </c>
+      <c r="H94" s="25">
+        <v>0</v>
+      </c>
+      <c r="I94" s="25">
+        <v>109</v>
+      </c>
+      <c r="J94" s="25">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="95" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A95" s="29">
+        <v>43995</v>
+      </c>
+      <c r="B95" s="30">
+        <v>87386</v>
+      </c>
+      <c r="C95" s="31">
+        <v>291</v>
+      </c>
+      <c r="D95" s="31">
+        <v>1495</v>
+      </c>
+      <c r="E95" s="31">
+        <v>3</v>
+      </c>
+      <c r="F95" s="31">
+        <v>6</v>
+      </c>
+      <c r="G95" s="31">
+        <v>0</v>
+      </c>
+      <c r="H95" s="31">
+        <v>0</v>
+      </c>
+      <c r="I95" s="31">
+        <v>109</v>
+      </c>
+      <c r="J95" s="31">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="96" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A96" s="23">
+        <v>43996</v>
+      </c>
+      <c r="B96" s="24">
+        <v>87598</v>
+      </c>
+      <c r="C96" s="25">
+        <v>212</v>
+      </c>
+      <c r="D96" s="25">
+        <v>1496</v>
+      </c>
+      <c r="E96" s="25">
+        <v>1</v>
+      </c>
+      <c r="F96" s="25">
+        <v>7</v>
+      </c>
+      <c r="G96" s="25">
+        <v>1</v>
+      </c>
+      <c r="H96" s="25">
+        <v>0</v>
+      </c>
+      <c r="I96" s="25">
+        <v>109</v>
+      </c>
+      <c r="J96" s="25">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="97" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A97" s="20">
+        <v>43997</v>
+      </c>
+      <c r="B97" s="21">
+        <v>88165</v>
+      </c>
+      <c r="C97" s="22">
+        <v>567</v>
+      </c>
+      <c r="D97" s="22">
+        <v>1499</v>
+      </c>
+      <c r="E97" s="22">
+        <v>3</v>
+      </c>
+      <c r="F97" s="22">
+        <v>7</v>
+      </c>
+      <c r="G97" s="22">
+        <v>1</v>
+      </c>
+      <c r="H97" s="22">
+        <v>0</v>
+      </c>
+      <c r="I97" s="22">
+        <v>109</v>
+      </c>
+      <c r="J97" s="22">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="98" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A98" s="20">
+        <v>43998</v>
+      </c>
+      <c r="B98" s="21">
+        <v>89151</v>
+      </c>
+      <c r="C98" s="22">
+        <v>986</v>
+      </c>
+      <c r="D98" s="22">
+        <v>1503</v>
+      </c>
+      <c r="E98" s="22">
+        <v>4</v>
+      </c>
+      <c r="F98" s="22">
+        <v>7</v>
+      </c>
+      <c r="G98" s="22">
+        <v>1</v>
+      </c>
+      <c r="H98" s="22">
+        <v>0</v>
+      </c>
+      <c r="I98" s="22">
+        <v>109</v>
+      </c>
+      <c r="J98" s="22">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="99" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A99" s="29">
+        <v>43999</v>
+      </c>
+      <c r="B99" s="30">
+        <v>90103</v>
+      </c>
+      <c r="C99" s="31">
+        <v>952</v>
+      </c>
+      <c r="D99" s="31">
+        <v>1511</v>
+      </c>
+      <c r="E99" s="31">
+        <v>8</v>
+      </c>
+      <c r="F99" s="31">
+        <v>6</v>
+      </c>
+      <c r="G99" s="31">
+        <v>1</v>
+      </c>
+      <c r="H99" s="31">
+        <v>1</v>
+      </c>
+      <c r="I99" s="31">
+        <v>109</v>
+      </c>
+      <c r="J99" s="31">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="100" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A100" s="20">
+        <v>44000</v>
+      </c>
+      <c r="B100" s="21">
+        <v>91005</v>
+      </c>
+      <c r="C100" s="22">
+        <v>902</v>
+      </c>
+      <c r="D100" s="22">
+        <v>1513</v>
+      </c>
+      <c r="E100" s="22">
+        <v>2</v>
+      </c>
+      <c r="F100" s="22">
+        <v>8</v>
+      </c>
+      <c r="G100" s="22">
+        <v>1</v>
+      </c>
+      <c r="H100" s="22">
+        <v>0</v>
+      </c>
+      <c r="I100" s="22">
+        <v>109</v>
+      </c>
+      <c r="J100" s="22">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="101" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A101" s="29">
+        <v>44001</v>
+      </c>
+      <c r="B101" s="30">
+        <v>92152</v>
+      </c>
+      <c r="C101" s="31">
+        <v>1147</v>
+      </c>
+      <c r="D101" s="31">
+        <v>1519</v>
+      </c>
+      <c r="E101" s="31">
+        <v>6</v>
+      </c>
+      <c r="F101" s="31">
+        <v>6</v>
+      </c>
+      <c r="G101" s="31">
+        <v>1</v>
+      </c>
+      <c r="H101" s="31">
+        <v>2</v>
+      </c>
+      <c r="I101" s="31">
+        <v>109</v>
+      </c>
+      <c r="J101" s="31">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="102" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A102" s="23">
+        <v>44002</v>
+      </c>
+      <c r="B102" s="24">
+        <v>92919</v>
+      </c>
+      <c r="C102" s="25">
+        <v>758</v>
+      </c>
+      <c r="D102" s="25">
+        <v>1520</v>
+      </c>
+      <c r="E102" s="25">
+        <v>1</v>
+      </c>
+      <c r="F102" s="25">
+        <v>6</v>
+      </c>
+      <c r="G102" s="25">
+        <v>1</v>
+      </c>
+      <c r="H102" s="25">
+        <v>2</v>
+      </c>
+      <c r="I102" s="25">
+        <v>109</v>
+      </c>
+      <c r="J102" s="25">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="103" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A103" s="29">
+        <v>44003</v>
+      </c>
+      <c r="B103" s="30">
+        <v>93181</v>
+      </c>
+      <c r="C103" s="31">
+        <v>271</v>
+      </c>
+      <c r="D103" s="31">
+        <v>1521</v>
+      </c>
+      <c r="E103" s="31">
+        <v>1</v>
+      </c>
+      <c r="F103" s="31">
+        <v>6</v>
+      </c>
+      <c r="G103" s="31">
+        <v>1</v>
+      </c>
+      <c r="H103" s="31">
+        <v>0</v>
+      </c>
+      <c r="I103" s="31">
+        <v>109</v>
+      </c>
+      <c r="J103" s="31">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="104" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A104" s="29">
+        <v>44004</v>
+      </c>
+      <c r="B104" s="30">
+        <v>94165</v>
+      </c>
+      <c r="C104" s="31">
+        <v>984</v>
+      </c>
+      <c r="D104" s="31">
+        <v>1534</v>
+      </c>
+      <c r="E104" s="31">
+        <v>13</v>
+      </c>
+      <c r="F104" s="31">
+        <v>5</v>
+      </c>
+      <c r="G104" s="31">
+        <v>1</v>
+      </c>
+      <c r="H104" s="31">
+        <v>1</v>
+      </c>
+      <c r="I104" s="31">
+        <v>109</v>
+      </c>
+      <c r="J104" s="31">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="105" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A105" s="29">
+        <v>44005</v>
+      </c>
+      <c r="B105" s="30">
+        <v>95387</v>
+      </c>
+      <c r="C105" s="31">
+        <v>1222</v>
+      </c>
+      <c r="D105" s="31">
+        <v>1541</v>
+      </c>
+      <c r="E105" s="31">
+        <v>7</v>
+      </c>
+      <c r="F105" s="31">
+        <v>7</v>
+      </c>
+      <c r="G105" s="31">
+        <v>2</v>
+      </c>
+      <c r="H105" s="31">
+        <v>0</v>
+      </c>
+      <c r="I105" s="31" t="s">
+        <v>10</v>
+      </c>
+      <c r="J105" s="31">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="106" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A106" s="23">
+        <v>44006</v>
+      </c>
+      <c r="B106" s="24">
+        <v>96599</v>
+      </c>
+      <c r="C106" s="25">
+        <v>1212</v>
+      </c>
+      <c r="D106" s="25">
+        <v>1547</v>
+      </c>
+      <c r="E106" s="25">
+        <v>6</v>
+      </c>
+      <c r="F106" s="25">
+        <v>7</v>
+      </c>
+      <c r="G106" s="25">
+        <v>2</v>
+      </c>
+      <c r="H106" s="25">
+        <v>0</v>
+      </c>
+      <c r="I106" s="25" t="s">
+        <v>10</v>
+      </c>
+      <c r="J106" s="25">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="107" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A107" s="29">
+        <v>44007</v>
+      </c>
+      <c r="B107" s="30">
+        <v>97442</v>
+      </c>
+      <c r="C107" s="31">
+        <v>843</v>
+      </c>
+      <c r="D107" s="31">
+        <v>1558</v>
+      </c>
+      <c r="E107" s="31">
+        <v>11</v>
+      </c>
+      <c r="F107" s="31">
+        <v>8</v>
+      </c>
+      <c r="G107" s="31">
+        <v>2</v>
+      </c>
+      <c r="H107" s="31">
+        <v>0</v>
+      </c>
+      <c r="I107" s="31" t="s">
+        <v>10</v>
+      </c>
+      <c r="J107" s="31">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="108" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A108" s="29">
+        <v>44008</v>
+      </c>
+      <c r="B108" s="30">
+        <v>98320</v>
+      </c>
+      <c r="C108" s="31">
+        <v>878</v>
+      </c>
+      <c r="D108" s="31">
+        <v>1572</v>
+      </c>
+      <c r="E108" s="31">
+        <v>14</v>
+      </c>
+      <c r="F108" s="31">
+        <v>8</v>
+      </c>
+      <c r="G108" s="31">
+        <v>1</v>
+      </c>
+      <c r="H108" s="31">
+        <v>0</v>
+      </c>
+      <c r="I108" s="31" t="s">
+        <v>10</v>
+      </c>
+      <c r="J108" s="31">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="109" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A109" s="29">
+        <v>44009</v>
+      </c>
+      <c r="B109" s="30">
+        <v>98945</v>
+      </c>
+      <c r="C109" s="31">
+        <v>625</v>
+      </c>
+      <c r="D109" s="31">
+        <v>1581</v>
+      </c>
+      <c r="E109" s="31">
+        <v>9</v>
+      </c>
+      <c r="F109" s="31">
+        <v>7</v>
+      </c>
+      <c r="G109" s="31">
+        <v>0</v>
+      </c>
+      <c r="H109" s="31">
+        <v>1</v>
+      </c>
+      <c r="I109" s="31" t="s">
+        <v>10</v>
+      </c>
+      <c r="J109" s="31">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="110" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A110" s="29">
+        <v>44010</v>
+      </c>
+      <c r="B110" s="30">
+        <v>99245</v>
+      </c>
+      <c r="C110" s="31">
+        <v>300</v>
+      </c>
+      <c r="D110" s="31">
+        <v>1585</v>
+      </c>
+      <c r="E110" s="31">
+        <v>4</v>
+      </c>
+      <c r="F110" s="31">
+        <v>8</v>
+      </c>
+      <c r="G110" s="31">
+        <v>0</v>
+      </c>
+      <c r="H110" s="31">
+        <v>0</v>
+      </c>
+      <c r="I110" s="31" t="s">
+        <v>10</v>
+      </c>
+      <c r="J110" s="31">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="111" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A111" s="29">
+        <v>44011</v>
+      </c>
+      <c r="B111" s="30">
+        <v>100330</v>
+      </c>
+      <c r="C111" s="31">
+        <v>1085</v>
+      </c>
+      <c r="D111" s="31">
+        <v>1600</v>
+      </c>
+      <c r="E111" s="31">
+        <v>15</v>
+      </c>
+      <c r="F111" s="31">
+        <v>8</v>
+      </c>
+      <c r="G111" s="31">
+        <v>0</v>
+      </c>
+      <c r="H111" s="31">
+        <v>0</v>
+      </c>
+      <c r="I111" s="31" t="s">
+        <v>10</v>
+      </c>
+      <c r="J111" s="31">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="112" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A112" s="20">
+        <v>44012</v>
+      </c>
+      <c r="B112" s="21">
+        <v>101729</v>
+      </c>
+      <c r="C112" s="22">
+        <v>1399</v>
+      </c>
+      <c r="D112" s="22">
+        <v>1613</v>
+      </c>
+      <c r="E112" s="22">
+        <v>13</v>
+      </c>
+      <c r="F112" s="22">
+        <v>8</v>
+      </c>
+      <c r="G112" s="22">
+        <v>0</v>
+      </c>
+      <c r="H112" s="22">
+        <v>0</v>
+      </c>
+      <c r="I112" s="22" t="s">
+        <v>10</v>
+      </c>
+      <c r="J112" s="22">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="113" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A113" s="20">
+        <v>44013</v>
+      </c>
+      <c r="B113" s="21">
+        <v>102927</v>
+      </c>
+      <c r="C113" s="22">
+        <v>1198</v>
+      </c>
+      <c r="D113" s="22">
+        <v>1663</v>
+      </c>
+      <c r="E113" s="22">
+        <v>21</v>
+      </c>
+      <c r="F113" s="22">
+        <v>9</v>
+      </c>
+      <c r="G113" s="22">
+        <v>0</v>
+      </c>
+      <c r="H113" s="22">
+        <v>0</v>
+      </c>
+      <c r="I113" s="22" t="s">
+        <v>10</v>
+      </c>
+      <c r="J113" s="22">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="114" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A114" s="20">
+        <v>44014</v>
+      </c>
+      <c r="B114" s="21">
+        <v>104201</v>
+      </c>
+      <c r="C114" s="22">
+        <v>1274</v>
+      </c>
+      <c r="D114" s="22">
+        <v>1649</v>
+      </c>
+      <c r="E114" s="22">
+        <v>16</v>
+      </c>
+      <c r="F114" s="22">
+        <v>10</v>
+      </c>
+      <c r="G114" s="22">
+        <v>0</v>
+      </c>
+      <c r="H114" s="22">
+        <v>0</v>
+      </c>
+      <c r="I114" s="22">
+        <v>111</v>
+      </c>
+      <c r="J114" s="22">
+        <v>0</v>
+      </c>
+    </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>

</xml_diff>

<commit_message>
Data updated by GitHub Bot (2020-07-03 20)
</commit_message>
<xml_diff>
--- a/output/snapshot/fdcf2531-4c3e-5c02-b63c-ee160ead6dea.xlsx
+++ b/output/snapshot/fdcf2531-4c3e-5c02-b63c-ee160ead6dea.xlsx
@@ -1,16 +1,15 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="21929"/>
-  <workbookPr/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
+  <fileVersion appName="xl" lastEdited="6" lowestEdited="6" rupBuild="14420"/>
+  <workbookPr defaultThemeVersion="164011"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="I:\AKTUALNI PODATKI - KORONA\Za objavo na GOV.SI\ang\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{1E6DD62F-2BE2-47DC-A7ED-9B57C1589256}" xr6:coauthVersionLast="44" xr6:coauthVersionMax="44" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840"/>
   </bookViews>
   <sheets>
     <sheet name="Covid-19 podatki" sheetId="1" r:id="rId1"/>
@@ -25,7 +24,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="10" uniqueCount="10">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="19" uniqueCount="11">
   <si>
     <t>Date</t>
   </si>
@@ -56,15 +55,18 @@
   <si>
     <t>Deaths (daily)</t>
   </si>
+  <si>
+    <t>111*</t>
+  </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" mc:Ignorable="x14ac x16r2">
   <numFmts count="1">
     <numFmt numFmtId="164" formatCode="d/\ m/\ yyyy;@"/>
   </numFmts>
-  <fonts count="4" x14ac:knownFonts="1">
+  <fonts count="5" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -93,6 +95,13 @@
       <name val="Calibri Light"/>
       <scheme val="major"/>
     </font>
+    <font>
+      <sz val="10"/>
+      <color theme="1"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
   </fonts>
   <fills count="3">
     <fill>
@@ -108,7 +117,7 @@
       </patternFill>
     </fill>
   </fills>
-  <borders count="2">
+  <borders count="3">
     <border>
       <left/>
       <right/>
@@ -129,11 +138,26 @@
       <bottom/>
       <diagonal/>
     </border>
+    <border>
+      <left style="thin">
+        <color theme="4"/>
+      </left>
+      <right style="thin">
+        <color theme="4"/>
+      </right>
+      <top style="thin">
+        <color theme="4"/>
+      </top>
+      <bottom style="thin">
+        <color theme="4"/>
+      </bottom>
+      <diagonal/>
+    </border>
   </borders>
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="26">
+  <cellXfs count="32">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="49" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyAlignment="1" applyProtection="1">
       <alignment horizontal="left" vertical="top"/>
@@ -208,6 +232,24 @@
       <alignment horizontal="right"/>
     </xf>
     <xf numFmtId="0" fontId="3" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="right"/>
+    </xf>
+    <xf numFmtId="164" fontId="4" fillId="2" borderId="2" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="right" vertical="top"/>
+    </xf>
+    <xf numFmtId="3" fontId="4" fillId="2" borderId="2" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="right"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="2" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="right"/>
+    </xf>
+    <xf numFmtId="164" fontId="3" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="right" vertical="top"/>
+    </xf>
+    <xf numFmtId="3" fontId="3" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="right"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="right"/>
     </xf>
   </cellXfs>
@@ -399,8 +441,8 @@
 </file>
 
 <file path=xl/tables/table1.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="1" xr:uid="{00000000-000C-0000-FFFF-FFFF00000000}" name="Tabela1" displayName="Tabela1" ref="A1:J75" totalsRowShown="0" headerRowDxfId="11" dataDxfId="10">
-  <autoFilter ref="A1:J75" xr:uid="{00000000-0009-0000-0100-000001000000}">
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="1" name="Tabela1" displayName="Tabela1" ref="A1:J114" totalsRowShown="0" headerRowDxfId="11" dataDxfId="10">
+  <autoFilter ref="A1:J114">
     <filterColumn colId="0" hiddenButton="1"/>
     <filterColumn colId="1" hiddenButton="1"/>
     <filterColumn colId="2" hiddenButton="1"/>
@@ -413,16 +455,16 @@
     <filterColumn colId="9" hiddenButton="1"/>
   </autoFilter>
   <tableColumns count="10">
-    <tableColumn id="1" xr3:uid="{00000000-0010-0000-0000-000001000000}" name="Date" dataDxfId="9"/>
-    <tableColumn id="2" xr3:uid="{00000000-0010-0000-0000-000002000000}" name="Tested (all)" dataDxfId="8"/>
-    <tableColumn id="3" xr3:uid="{00000000-0010-0000-0000-000003000000}" name="Tested (daily)" dataDxfId="7"/>
-    <tableColumn id="4" xr3:uid="{00000000-0010-0000-0000-000004000000}" name="Positive (all)" dataDxfId="6"/>
-    <tableColumn id="5" xr3:uid="{00000000-0010-0000-0000-000005000000}" name="Positive (daily)" dataDxfId="5"/>
-    <tableColumn id="6" xr3:uid="{00000000-0010-0000-0000-000006000000}" name="All hospitalized on certain day" dataDxfId="4"/>
-    <tableColumn id="7" xr3:uid="{00000000-0010-0000-0000-000007000000}" name="All persons in intensive care on certain day" dataDxfId="3"/>
-    <tableColumn id="10" xr3:uid="{00000000-0010-0000-0000-00000A000000}" name="Discharged" dataDxfId="2"/>
-    <tableColumn id="8" xr3:uid="{00000000-0010-0000-0000-000008000000}" name="Deaths (all)" dataDxfId="1"/>
-    <tableColumn id="9" xr3:uid="{00000000-0010-0000-0000-000009000000}" name="Deaths (daily)" dataDxfId="0"/>
+    <tableColumn id="1" name="Date" dataDxfId="9"/>
+    <tableColumn id="2" name="Tested (all)" dataDxfId="8"/>
+    <tableColumn id="3" name="Tested (daily)" dataDxfId="7"/>
+    <tableColumn id="4" name="Positive (all)" dataDxfId="6"/>
+    <tableColumn id="5" name="Positive (daily)" dataDxfId="5"/>
+    <tableColumn id="6" name="All hospitalized on certain day" dataDxfId="4"/>
+    <tableColumn id="7" name="All persons in intensive care on certain day" dataDxfId="3"/>
+    <tableColumn id="10" name="Discharged" dataDxfId="2"/>
+    <tableColumn id="8" name="Deaths (all)" dataDxfId="1"/>
+    <tableColumn id="9" name="Deaths (daily)" dataDxfId="0"/>
   </tableColumns>
   <tableStyleInfo name="TableStyleLight16" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
   <extLst>
@@ -695,11 +737,11 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:J75"/>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <dimension ref="A1:J114"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A40" zoomScale="89" zoomScaleNormal="89" workbookViewId="0">
-      <selection activeCell="J74" sqref="J74"/>
+    <sheetView tabSelected="1" topLeftCell="A83" zoomScale="89" zoomScaleNormal="89" workbookViewId="0">
+      <selection activeCell="I114" sqref="I114"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -3117,6 +3159,1254 @@
         <v>0</v>
       </c>
     </row>
+    <row r="76" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A76" s="20">
+        <v>43976</v>
+      </c>
+      <c r="B76" s="21">
+        <v>75770</v>
+      </c>
+      <c r="C76" s="22">
+        <v>754</v>
+      </c>
+      <c r="D76" s="22">
+        <v>1469</v>
+      </c>
+      <c r="E76" s="22">
+        <v>0</v>
+      </c>
+      <c r="F76" s="22">
+        <v>9</v>
+      </c>
+      <c r="G76" s="22">
+        <v>2</v>
+      </c>
+      <c r="H76" s="22">
+        <v>6</v>
+      </c>
+      <c r="I76" s="22">
+        <v>108</v>
+      </c>
+      <c r="J76" s="22">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="77" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A77" s="20">
+        <v>43977</v>
+      </c>
+      <c r="B77" s="21">
+        <v>76579</v>
+      </c>
+      <c r="C77" s="22">
+        <v>809</v>
+      </c>
+      <c r="D77" s="22">
+        <v>1471</v>
+      </c>
+      <c r="E77" s="22">
+        <v>2</v>
+      </c>
+      <c r="F77" s="22">
+        <v>8</v>
+      </c>
+      <c r="G77" s="22">
+        <v>2</v>
+      </c>
+      <c r="H77" s="22">
+        <v>2</v>
+      </c>
+      <c r="I77" s="22">
+        <v>108</v>
+      </c>
+      <c r="J77" s="22">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="78" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A78" s="20">
+        <v>43978</v>
+      </c>
+      <c r="B78" s="21">
+        <v>77210</v>
+      </c>
+      <c r="C78" s="22">
+        <v>631</v>
+      </c>
+      <c r="D78" s="22">
+        <v>1473</v>
+      </c>
+      <c r="E78" s="22">
+        <v>2</v>
+      </c>
+      <c r="F78" s="22">
+        <v>7</v>
+      </c>
+      <c r="G78" s="22">
+        <v>2</v>
+      </c>
+      <c r="H78" s="22">
+        <v>1</v>
+      </c>
+      <c r="I78" s="22">
+        <v>108</v>
+      </c>
+      <c r="J78" s="22">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="79" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A79" s="20">
+        <v>43979</v>
+      </c>
+      <c r="B79" s="21">
+        <v>77916</v>
+      </c>
+      <c r="C79" s="22">
+        <v>706</v>
+      </c>
+      <c r="D79" s="22">
+        <v>1473</v>
+      </c>
+      <c r="E79" s="22">
+        <v>0</v>
+      </c>
+      <c r="F79" s="22">
+        <v>7</v>
+      </c>
+      <c r="G79" s="22">
+        <v>2</v>
+      </c>
+      <c r="H79" s="22">
+        <v>0</v>
+      </c>
+      <c r="I79" s="22">
+        <v>108</v>
+      </c>
+      <c r="J79" s="22">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="80" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A80" s="20">
+        <v>43980</v>
+      </c>
+      <c r="B80" s="21">
+        <v>78529</v>
+      </c>
+      <c r="C80" s="22">
+        <v>613</v>
+      </c>
+      <c r="D80" s="22">
+        <v>1473</v>
+      </c>
+      <c r="E80" s="22">
+        <v>0</v>
+      </c>
+      <c r="F80" s="22">
+        <v>7</v>
+      </c>
+      <c r="G80" s="22">
+        <v>2</v>
+      </c>
+      <c r="H80" s="22">
+        <v>0</v>
+      </c>
+      <c r="I80" s="22">
+        <v>108</v>
+      </c>
+      <c r="J80" s="22">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="81" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A81" s="20">
+        <v>43981</v>
+      </c>
+      <c r="B81" s="22">
+        <v>78793</v>
+      </c>
+      <c r="C81" s="22">
+        <v>264</v>
+      </c>
+      <c r="D81" s="22">
+        <v>1473</v>
+      </c>
+      <c r="E81" s="22">
+        <v>0</v>
+      </c>
+      <c r="F81" s="22">
+        <v>6</v>
+      </c>
+      <c r="G81" s="22">
+        <v>2</v>
+      </c>
+      <c r="H81" s="22">
+        <v>1</v>
+      </c>
+      <c r="I81" s="22">
+        <v>108</v>
+      </c>
+      <c r="J81" s="22">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="82" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A82" s="20">
+        <v>43982</v>
+      </c>
+      <c r="B82" s="21">
+        <v>79039</v>
+      </c>
+      <c r="C82" s="22">
+        <v>246</v>
+      </c>
+      <c r="D82" s="22">
+        <v>1473</v>
+      </c>
+      <c r="E82" s="22">
+        <v>0</v>
+      </c>
+      <c r="F82" s="22">
+        <v>5</v>
+      </c>
+      <c r="G82" s="22">
+        <v>1</v>
+      </c>
+      <c r="H82" s="22">
+        <v>0</v>
+      </c>
+      <c r="I82" s="22">
+        <v>109</v>
+      </c>
+      <c r="J82" s="22">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="83" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A83" s="20">
+        <v>43983</v>
+      </c>
+      <c r="B83" s="21">
+        <v>79698</v>
+      </c>
+      <c r="C83" s="22">
+        <v>659</v>
+      </c>
+      <c r="D83" s="22">
+        <v>1475</v>
+      </c>
+      <c r="E83" s="22">
+        <v>2</v>
+      </c>
+      <c r="F83" s="22">
+        <v>5</v>
+      </c>
+      <c r="G83" s="22">
+        <v>1</v>
+      </c>
+      <c r="H83" s="22">
+        <v>0</v>
+      </c>
+      <c r="I83" s="22">
+        <v>109</v>
+      </c>
+      <c r="J83" s="22">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="84" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A84" s="20">
+        <v>43984</v>
+      </c>
+      <c r="B84" s="21">
+        <v>80505</v>
+      </c>
+      <c r="C84" s="22">
+        <v>807</v>
+      </c>
+      <c r="D84" s="22">
+        <v>1477</v>
+      </c>
+      <c r="E84" s="22">
+        <v>2</v>
+      </c>
+      <c r="F84" s="22">
+        <v>5</v>
+      </c>
+      <c r="G84" s="22">
+        <v>0</v>
+      </c>
+      <c r="H84" s="22">
+        <v>0</v>
+      </c>
+      <c r="I84" s="22">
+        <v>109</v>
+      </c>
+      <c r="J84" s="22">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="85" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A85" s="20">
+        <v>43985</v>
+      </c>
+      <c r="B85" s="21">
+        <v>81333</v>
+      </c>
+      <c r="C85" s="22">
+        <v>828</v>
+      </c>
+      <c r="D85" s="22">
+        <v>1477</v>
+      </c>
+      <c r="E85" s="22">
+        <v>0</v>
+      </c>
+      <c r="F85" s="22">
+        <v>5</v>
+      </c>
+      <c r="G85" s="22">
+        <v>0</v>
+      </c>
+      <c r="H85" s="22">
+        <v>0</v>
+      </c>
+      <c r="I85" s="22">
+        <v>109</v>
+      </c>
+      <c r="J85" s="22">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="86" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A86" s="26">
+        <v>43986</v>
+      </c>
+      <c r="B86" s="27">
+        <v>82161</v>
+      </c>
+      <c r="C86" s="28">
+        <v>828</v>
+      </c>
+      <c r="D86" s="28">
+        <v>1479</v>
+      </c>
+      <c r="E86" s="28">
+        <v>2</v>
+      </c>
+      <c r="F86" s="28">
+        <v>6</v>
+      </c>
+      <c r="G86" s="28">
+        <v>0</v>
+      </c>
+      <c r="H86" s="28">
+        <v>0</v>
+      </c>
+      <c r="I86" s="28">
+        <v>109</v>
+      </c>
+      <c r="J86" s="28">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="87" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A87" s="29">
+        <v>43987</v>
+      </c>
+      <c r="B87" s="30">
+        <v>82876</v>
+      </c>
+      <c r="C87" s="31">
+        <v>715</v>
+      </c>
+      <c r="D87" s="31">
+        <v>1484</v>
+      </c>
+      <c r="E87" s="31">
+        <v>5</v>
+      </c>
+      <c r="F87" s="31">
+        <v>6</v>
+      </c>
+      <c r="G87" s="31">
+        <v>0</v>
+      </c>
+      <c r="H87" s="31">
+        <v>0</v>
+      </c>
+      <c r="I87" s="31">
+        <v>109</v>
+      </c>
+      <c r="J87" s="31">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="88" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A88" s="23">
+        <v>43988</v>
+      </c>
+      <c r="B88" s="24">
+        <v>83105</v>
+      </c>
+      <c r="C88" s="25">
+        <v>229</v>
+      </c>
+      <c r="D88" s="25">
+        <v>1485</v>
+      </c>
+      <c r="E88" s="25">
+        <v>1</v>
+      </c>
+      <c r="F88" s="25">
+        <v>5</v>
+      </c>
+      <c r="G88" s="25">
+        <v>0</v>
+      </c>
+      <c r="H88" s="25">
+        <v>1</v>
+      </c>
+      <c r="I88" s="25">
+        <v>109</v>
+      </c>
+      <c r="J88" s="25">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="89" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A89" s="29">
+        <v>43989</v>
+      </c>
+      <c r="B89" s="30">
+        <v>83316</v>
+      </c>
+      <c r="C89" s="31">
+        <v>211</v>
+      </c>
+      <c r="D89" s="31">
+        <v>1485</v>
+      </c>
+      <c r="E89" s="31">
+        <v>0</v>
+      </c>
+      <c r="F89" s="31">
+        <v>5</v>
+      </c>
+      <c r="G89" s="31">
+        <v>0</v>
+      </c>
+      <c r="H89" s="31">
+        <v>0</v>
+      </c>
+      <c r="I89" s="31">
+        <v>109</v>
+      </c>
+      <c r="J89" s="31">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="90" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A90" s="20">
+        <v>43990</v>
+      </c>
+      <c r="B90" s="21">
+        <v>84130</v>
+      </c>
+      <c r="C90" s="22">
+        <v>814</v>
+      </c>
+      <c r="D90" s="22">
+        <v>1486</v>
+      </c>
+      <c r="E90" s="22">
+        <v>1</v>
+      </c>
+      <c r="F90" s="22">
+        <v>6</v>
+      </c>
+      <c r="G90" s="22">
+        <v>0</v>
+      </c>
+      <c r="H90" s="22">
+        <v>0</v>
+      </c>
+      <c r="I90" s="22">
+        <v>109</v>
+      </c>
+      <c r="J90" s="22">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="91" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A91" s="20">
+        <v>43991</v>
+      </c>
+      <c r="B91" s="21">
+        <v>84868</v>
+      </c>
+      <c r="C91" s="22">
+        <v>738</v>
+      </c>
+      <c r="D91" s="22">
+        <v>1488</v>
+      </c>
+      <c r="E91" s="22">
+        <v>2</v>
+      </c>
+      <c r="F91" s="22">
+        <v>6</v>
+      </c>
+      <c r="G91" s="22">
+        <v>0</v>
+      </c>
+      <c r="H91" s="22">
+        <v>0</v>
+      </c>
+      <c r="I91" s="22">
+        <v>109</v>
+      </c>
+      <c r="J91" s="22">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="92" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A92" s="23">
+        <v>43992</v>
+      </c>
+      <c r="B92" s="24">
+        <v>85626</v>
+      </c>
+      <c r="C92" s="25">
+        <v>758</v>
+      </c>
+      <c r="D92" s="25">
+        <v>1488</v>
+      </c>
+      <c r="E92" s="25">
+        <v>0</v>
+      </c>
+      <c r="F92" s="25">
+        <v>6</v>
+      </c>
+      <c r="G92" s="25">
+        <v>0</v>
+      </c>
+      <c r="H92" s="25">
+        <v>0</v>
+      </c>
+      <c r="I92" s="25">
+        <v>109</v>
+      </c>
+      <c r="J92" s="25">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="93" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A93" s="29">
+        <v>43993</v>
+      </c>
+      <c r="B93" s="30">
+        <v>86328</v>
+      </c>
+      <c r="C93" s="31">
+        <v>702</v>
+      </c>
+      <c r="D93" s="31">
+        <v>1490</v>
+      </c>
+      <c r="E93" s="31">
+        <v>2</v>
+      </c>
+      <c r="F93" s="31">
+        <v>6</v>
+      </c>
+      <c r="G93" s="31">
+        <v>0</v>
+      </c>
+      <c r="H93" s="31">
+        <v>0</v>
+      </c>
+      <c r="I93" s="31">
+        <v>109</v>
+      </c>
+      <c r="J93" s="31">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="94" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A94" s="23">
+        <v>43994</v>
+      </c>
+      <c r="B94" s="24">
+        <v>87095</v>
+      </c>
+      <c r="C94" s="25">
+        <v>767</v>
+      </c>
+      <c r="D94" s="25">
+        <v>1492</v>
+      </c>
+      <c r="E94" s="25">
+        <v>2</v>
+      </c>
+      <c r="F94" s="25">
+        <v>6</v>
+      </c>
+      <c r="G94" s="25">
+        <v>0</v>
+      </c>
+      <c r="H94" s="25">
+        <v>0</v>
+      </c>
+      <c r="I94" s="25">
+        <v>109</v>
+      </c>
+      <c r="J94" s="25">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="95" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A95" s="29">
+        <v>43995</v>
+      </c>
+      <c r="B95" s="30">
+        <v>87386</v>
+      </c>
+      <c r="C95" s="31">
+        <v>291</v>
+      </c>
+      <c r="D95" s="31">
+        <v>1495</v>
+      </c>
+      <c r="E95" s="31">
+        <v>3</v>
+      </c>
+      <c r="F95" s="31">
+        <v>6</v>
+      </c>
+      <c r="G95" s="31">
+        <v>0</v>
+      </c>
+      <c r="H95" s="31">
+        <v>0</v>
+      </c>
+      <c r="I95" s="31">
+        <v>109</v>
+      </c>
+      <c r="J95" s="31">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="96" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A96" s="23">
+        <v>43996</v>
+      </c>
+      <c r="B96" s="24">
+        <v>87598</v>
+      </c>
+      <c r="C96" s="25">
+        <v>212</v>
+      </c>
+      <c r="D96" s="25">
+        <v>1496</v>
+      </c>
+      <c r="E96" s="25">
+        <v>1</v>
+      </c>
+      <c r="F96" s="25">
+        <v>7</v>
+      </c>
+      <c r="G96" s="25">
+        <v>1</v>
+      </c>
+      <c r="H96" s="25">
+        <v>0</v>
+      </c>
+      <c r="I96" s="25">
+        <v>109</v>
+      </c>
+      <c r="J96" s="25">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="97" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A97" s="20">
+        <v>43997</v>
+      </c>
+      <c r="B97" s="21">
+        <v>88165</v>
+      </c>
+      <c r="C97" s="22">
+        <v>567</v>
+      </c>
+      <c r="D97" s="22">
+        <v>1499</v>
+      </c>
+      <c r="E97" s="22">
+        <v>3</v>
+      </c>
+      <c r="F97" s="22">
+        <v>7</v>
+      </c>
+      <c r="G97" s="22">
+        <v>1</v>
+      </c>
+      <c r="H97" s="22">
+        <v>0</v>
+      </c>
+      <c r="I97" s="22">
+        <v>109</v>
+      </c>
+      <c r="J97" s="22">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="98" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A98" s="20">
+        <v>43998</v>
+      </c>
+      <c r="B98" s="21">
+        <v>89151</v>
+      </c>
+      <c r="C98" s="22">
+        <v>986</v>
+      </c>
+      <c r="D98" s="22">
+        <v>1503</v>
+      </c>
+      <c r="E98" s="22">
+        <v>4</v>
+      </c>
+      <c r="F98" s="22">
+        <v>7</v>
+      </c>
+      <c r="G98" s="22">
+        <v>1</v>
+      </c>
+      <c r="H98" s="22">
+        <v>0</v>
+      </c>
+      <c r="I98" s="22">
+        <v>109</v>
+      </c>
+      <c r="J98" s="22">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="99" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A99" s="29">
+        <v>43999</v>
+      </c>
+      <c r="B99" s="30">
+        <v>90103</v>
+      </c>
+      <c r="C99" s="31">
+        <v>952</v>
+      </c>
+      <c r="D99" s="31">
+        <v>1511</v>
+      </c>
+      <c r="E99" s="31">
+        <v>8</v>
+      </c>
+      <c r="F99" s="31">
+        <v>6</v>
+      </c>
+      <c r="G99" s="31">
+        <v>1</v>
+      </c>
+      <c r="H99" s="31">
+        <v>1</v>
+      </c>
+      <c r="I99" s="31">
+        <v>109</v>
+      </c>
+      <c r="J99" s="31">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="100" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A100" s="20">
+        <v>44000</v>
+      </c>
+      <c r="B100" s="21">
+        <v>91005</v>
+      </c>
+      <c r="C100" s="22">
+        <v>902</v>
+      </c>
+      <c r="D100" s="22">
+        <v>1513</v>
+      </c>
+      <c r="E100" s="22">
+        <v>2</v>
+      </c>
+      <c r="F100" s="22">
+        <v>8</v>
+      </c>
+      <c r="G100" s="22">
+        <v>1</v>
+      </c>
+      <c r="H100" s="22">
+        <v>0</v>
+      </c>
+      <c r="I100" s="22">
+        <v>109</v>
+      </c>
+      <c r="J100" s="22">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="101" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A101" s="29">
+        <v>44001</v>
+      </c>
+      <c r="B101" s="30">
+        <v>92152</v>
+      </c>
+      <c r="C101" s="31">
+        <v>1147</v>
+      </c>
+      <c r="D101" s="31">
+        <v>1519</v>
+      </c>
+      <c r="E101" s="31">
+        <v>6</v>
+      </c>
+      <c r="F101" s="31">
+        <v>6</v>
+      </c>
+      <c r="G101" s="31">
+        <v>1</v>
+      </c>
+      <c r="H101" s="31">
+        <v>2</v>
+      </c>
+      <c r="I101" s="31">
+        <v>109</v>
+      </c>
+      <c r="J101" s="31">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="102" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A102" s="23">
+        <v>44002</v>
+      </c>
+      <c r="B102" s="24">
+        <v>92919</v>
+      </c>
+      <c r="C102" s="25">
+        <v>758</v>
+      </c>
+      <c r="D102" s="25">
+        <v>1520</v>
+      </c>
+      <c r="E102" s="25">
+        <v>1</v>
+      </c>
+      <c r="F102" s="25">
+        <v>6</v>
+      </c>
+      <c r="G102" s="25">
+        <v>1</v>
+      </c>
+      <c r="H102" s="25">
+        <v>2</v>
+      </c>
+      <c r="I102" s="25">
+        <v>109</v>
+      </c>
+      <c r="J102" s="25">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="103" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A103" s="29">
+        <v>44003</v>
+      </c>
+      <c r="B103" s="30">
+        <v>93181</v>
+      </c>
+      <c r="C103" s="31">
+        <v>271</v>
+      </c>
+      <c r="D103" s="31">
+        <v>1521</v>
+      </c>
+      <c r="E103" s="31">
+        <v>1</v>
+      </c>
+      <c r="F103" s="31">
+        <v>6</v>
+      </c>
+      <c r="G103" s="31">
+        <v>1</v>
+      </c>
+      <c r="H103" s="31">
+        <v>0</v>
+      </c>
+      <c r="I103" s="31">
+        <v>109</v>
+      </c>
+      <c r="J103" s="31">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="104" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A104" s="29">
+        <v>44004</v>
+      </c>
+      <c r="B104" s="30">
+        <v>94165</v>
+      </c>
+      <c r="C104" s="31">
+        <v>984</v>
+      </c>
+      <c r="D104" s="31">
+        <v>1534</v>
+      </c>
+      <c r="E104" s="31">
+        <v>13</v>
+      </c>
+      <c r="F104" s="31">
+        <v>5</v>
+      </c>
+      <c r="G104" s="31">
+        <v>1</v>
+      </c>
+      <c r="H104" s="31">
+        <v>1</v>
+      </c>
+      <c r="I104" s="31">
+        <v>109</v>
+      </c>
+      <c r="J104" s="31">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="105" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A105" s="29">
+        <v>44005</v>
+      </c>
+      <c r="B105" s="30">
+        <v>95387</v>
+      </c>
+      <c r="C105" s="31">
+        <v>1222</v>
+      </c>
+      <c r="D105" s="31">
+        <v>1541</v>
+      </c>
+      <c r="E105" s="31">
+        <v>7</v>
+      </c>
+      <c r="F105" s="31">
+        <v>7</v>
+      </c>
+      <c r="G105" s="31">
+        <v>2</v>
+      </c>
+      <c r="H105" s="31">
+        <v>0</v>
+      </c>
+      <c r="I105" s="31" t="s">
+        <v>10</v>
+      </c>
+      <c r="J105" s="31">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="106" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A106" s="23">
+        <v>44006</v>
+      </c>
+      <c r="B106" s="24">
+        <v>96599</v>
+      </c>
+      <c r="C106" s="25">
+        <v>1212</v>
+      </c>
+      <c r="D106" s="25">
+        <v>1547</v>
+      </c>
+      <c r="E106" s="25">
+        <v>6</v>
+      </c>
+      <c r="F106" s="25">
+        <v>7</v>
+      </c>
+      <c r="G106" s="25">
+        <v>2</v>
+      </c>
+      <c r="H106" s="25">
+        <v>0</v>
+      </c>
+      <c r="I106" s="25" t="s">
+        <v>10</v>
+      </c>
+      <c r="J106" s="25">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="107" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A107" s="29">
+        <v>44007</v>
+      </c>
+      <c r="B107" s="30">
+        <v>97442</v>
+      </c>
+      <c r="C107" s="31">
+        <v>843</v>
+      </c>
+      <c r="D107" s="31">
+        <v>1558</v>
+      </c>
+      <c r="E107" s="31">
+        <v>11</v>
+      </c>
+      <c r="F107" s="31">
+        <v>8</v>
+      </c>
+      <c r="G107" s="31">
+        <v>2</v>
+      </c>
+      <c r="H107" s="31">
+        <v>0</v>
+      </c>
+      <c r="I107" s="31" t="s">
+        <v>10</v>
+      </c>
+      <c r="J107" s="31">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="108" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A108" s="29">
+        <v>44008</v>
+      </c>
+      <c r="B108" s="30">
+        <v>98320</v>
+      </c>
+      <c r="C108" s="31">
+        <v>878</v>
+      </c>
+      <c r="D108" s="31">
+        <v>1572</v>
+      </c>
+      <c r="E108" s="31">
+        <v>14</v>
+      </c>
+      <c r="F108" s="31">
+        <v>8</v>
+      </c>
+      <c r="G108" s="31">
+        <v>1</v>
+      </c>
+      <c r="H108" s="31">
+        <v>0</v>
+      </c>
+      <c r="I108" s="31" t="s">
+        <v>10</v>
+      </c>
+      <c r="J108" s="31">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="109" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A109" s="29">
+        <v>44009</v>
+      </c>
+      <c r="B109" s="30">
+        <v>98945</v>
+      </c>
+      <c r="C109" s="31">
+        <v>625</v>
+      </c>
+      <c r="D109" s="31">
+        <v>1581</v>
+      </c>
+      <c r="E109" s="31">
+        <v>9</v>
+      </c>
+      <c r="F109" s="31">
+        <v>7</v>
+      </c>
+      <c r="G109" s="31">
+        <v>0</v>
+      </c>
+      <c r="H109" s="31">
+        <v>1</v>
+      </c>
+      <c r="I109" s="31" t="s">
+        <v>10</v>
+      </c>
+      <c r="J109" s="31">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="110" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A110" s="29">
+        <v>44010</v>
+      </c>
+      <c r="B110" s="30">
+        <v>99245</v>
+      </c>
+      <c r="C110" s="31">
+        <v>300</v>
+      </c>
+      <c r="D110" s="31">
+        <v>1585</v>
+      </c>
+      <c r="E110" s="31">
+        <v>4</v>
+      </c>
+      <c r="F110" s="31">
+        <v>8</v>
+      </c>
+      <c r="G110" s="31">
+        <v>0</v>
+      </c>
+      <c r="H110" s="31">
+        <v>0</v>
+      </c>
+      <c r="I110" s="31" t="s">
+        <v>10</v>
+      </c>
+      <c r="J110" s="31">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="111" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A111" s="29">
+        <v>44011</v>
+      </c>
+      <c r="B111" s="30">
+        <v>100330</v>
+      </c>
+      <c r="C111" s="31">
+        <v>1085</v>
+      </c>
+      <c r="D111" s="31">
+        <v>1600</v>
+      </c>
+      <c r="E111" s="31">
+        <v>15</v>
+      </c>
+      <c r="F111" s="31">
+        <v>8</v>
+      </c>
+      <c r="G111" s="31">
+        <v>0</v>
+      </c>
+      <c r="H111" s="31">
+        <v>0</v>
+      </c>
+      <c r="I111" s="31" t="s">
+        <v>10</v>
+      </c>
+      <c r="J111" s="31">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="112" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A112" s="20">
+        <v>44012</v>
+      </c>
+      <c r="B112" s="21">
+        <v>101729</v>
+      </c>
+      <c r="C112" s="22">
+        <v>1399</v>
+      </c>
+      <c r="D112" s="22">
+        <v>1613</v>
+      </c>
+      <c r="E112" s="22">
+        <v>13</v>
+      </c>
+      <c r="F112" s="22">
+        <v>8</v>
+      </c>
+      <c r="G112" s="22">
+        <v>0</v>
+      </c>
+      <c r="H112" s="22">
+        <v>0</v>
+      </c>
+      <c r="I112" s="22" t="s">
+        <v>10</v>
+      </c>
+      <c r="J112" s="22">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="113" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A113" s="20">
+        <v>44013</v>
+      </c>
+      <c r="B113" s="21">
+        <v>102927</v>
+      </c>
+      <c r="C113" s="22">
+        <v>1198</v>
+      </c>
+      <c r="D113" s="22">
+        <v>1663</v>
+      </c>
+      <c r="E113" s="22">
+        <v>21</v>
+      </c>
+      <c r="F113" s="22">
+        <v>9</v>
+      </c>
+      <c r="G113" s="22">
+        <v>0</v>
+      </c>
+      <c r="H113" s="22">
+        <v>0</v>
+      </c>
+      <c r="I113" s="22" t="s">
+        <v>10</v>
+      </c>
+      <c r="J113" s="22">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="114" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A114" s="20">
+        <v>44014</v>
+      </c>
+      <c r="B114" s="21">
+        <v>104201</v>
+      </c>
+      <c r="C114" s="22">
+        <v>1274</v>
+      </c>
+      <c r="D114" s="22">
+        <v>1649</v>
+      </c>
+      <c r="E114" s="22">
+        <v>16</v>
+      </c>
+      <c r="F114" s="22">
+        <v>10</v>
+      </c>
+      <c r="G114" s="22">
+        <v>0</v>
+      </c>
+      <c r="H114" s="22">
+        <v>0</v>
+      </c>
+      <c r="I114" s="22">
+        <v>111</v>
+      </c>
+      <c r="J114" s="22">
+        <v>0</v>
+      </c>
+    </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>

</xml_diff>

<commit_message>
Data updated by GitHub Bot (2020-07-04 12)
</commit_message>
<xml_diff>
--- a/output/snapshot/fdcf2531-4c3e-5c02-b63c-ee160ead6dea.xlsx
+++ b/output/snapshot/fdcf2531-4c3e-5c02-b63c-ee160ead6dea.xlsx
@@ -1,16 +1,15 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="21929"/>
-  <workbookPr/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
+  <fileVersion appName="xl" lastEdited="6" lowestEdited="6" rupBuild="14420"/>
+  <workbookPr defaultThemeVersion="164011"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="I:\AKTUALNI PODATKI - KORONA\Za objavo na GOV.SI\ang\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{1E6DD62F-2BE2-47DC-A7ED-9B57C1589256}" xr6:coauthVersionLast="44" xr6:coauthVersionMax="44" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840"/>
   </bookViews>
   <sheets>
     <sheet name="Covid-19 podatki" sheetId="1" r:id="rId1"/>
@@ -25,7 +24,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="10" uniqueCount="10">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="21" uniqueCount="11">
   <si>
     <t>Date</t>
   </si>
@@ -56,15 +55,18 @@
   <si>
     <t>Deaths (daily)</t>
   </si>
+  <si>
+    <t>111*</t>
+  </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" mc:Ignorable="x14ac x16r2">
   <numFmts count="1">
     <numFmt numFmtId="164" formatCode="d/\ m/\ yyyy;@"/>
   </numFmts>
-  <fonts count="4" x14ac:knownFonts="1">
+  <fonts count="5" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -93,6 +95,13 @@
       <name val="Calibri Light"/>
       <scheme val="major"/>
     </font>
+    <font>
+      <sz val="10"/>
+      <color theme="1"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
   </fonts>
   <fills count="3">
     <fill>
@@ -108,7 +117,7 @@
       </patternFill>
     </fill>
   </fills>
-  <borders count="2">
+  <borders count="3">
     <border>
       <left/>
       <right/>
@@ -129,11 +138,26 @@
       <bottom/>
       <diagonal/>
     </border>
+    <border>
+      <left style="thin">
+        <color theme="4"/>
+      </left>
+      <right style="thin">
+        <color theme="4"/>
+      </right>
+      <top style="thin">
+        <color theme="4"/>
+      </top>
+      <bottom style="thin">
+        <color theme="4"/>
+      </bottom>
+      <diagonal/>
+    </border>
   </borders>
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="26">
+  <cellXfs count="32">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="49" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyAlignment="1" applyProtection="1">
       <alignment horizontal="left" vertical="top"/>
@@ -208,6 +232,24 @@
       <alignment horizontal="right"/>
     </xf>
     <xf numFmtId="0" fontId="3" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="right"/>
+    </xf>
+    <xf numFmtId="164" fontId="4" fillId="2" borderId="2" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="right" vertical="top"/>
+    </xf>
+    <xf numFmtId="3" fontId="4" fillId="2" borderId="2" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="right"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="2" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="right"/>
+    </xf>
+    <xf numFmtId="164" fontId="3" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="right" vertical="top"/>
+    </xf>
+    <xf numFmtId="3" fontId="3" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="right"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="right"/>
     </xf>
   </cellXfs>
@@ -399,8 +441,8 @@
 </file>
 
 <file path=xl/tables/table1.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="1" xr:uid="{00000000-000C-0000-FFFF-FFFF00000000}" name="Tabela1" displayName="Tabela1" ref="A1:J75" totalsRowShown="0" headerRowDxfId="11" dataDxfId="10">
-  <autoFilter ref="A1:J75" xr:uid="{00000000-0009-0000-0100-000001000000}">
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="1" name="Tabela1" displayName="Tabela1" ref="A1:J115" totalsRowShown="0" headerRowDxfId="11" dataDxfId="10">
+  <autoFilter ref="A1:J115">
     <filterColumn colId="0" hiddenButton="1"/>
     <filterColumn colId="1" hiddenButton="1"/>
     <filterColumn colId="2" hiddenButton="1"/>
@@ -413,16 +455,16 @@
     <filterColumn colId="9" hiddenButton="1"/>
   </autoFilter>
   <tableColumns count="10">
-    <tableColumn id="1" xr3:uid="{00000000-0010-0000-0000-000001000000}" name="Date" dataDxfId="9"/>
-    <tableColumn id="2" xr3:uid="{00000000-0010-0000-0000-000002000000}" name="Tested (all)" dataDxfId="8"/>
-    <tableColumn id="3" xr3:uid="{00000000-0010-0000-0000-000003000000}" name="Tested (daily)" dataDxfId="7"/>
-    <tableColumn id="4" xr3:uid="{00000000-0010-0000-0000-000004000000}" name="Positive (all)" dataDxfId="6"/>
-    <tableColumn id="5" xr3:uid="{00000000-0010-0000-0000-000005000000}" name="Positive (daily)" dataDxfId="5"/>
-    <tableColumn id="6" xr3:uid="{00000000-0010-0000-0000-000006000000}" name="All hospitalized on certain day" dataDxfId="4"/>
-    <tableColumn id="7" xr3:uid="{00000000-0010-0000-0000-000007000000}" name="All persons in intensive care on certain day" dataDxfId="3"/>
-    <tableColumn id="10" xr3:uid="{00000000-0010-0000-0000-00000A000000}" name="Discharged" dataDxfId="2"/>
-    <tableColumn id="8" xr3:uid="{00000000-0010-0000-0000-000008000000}" name="Deaths (all)" dataDxfId="1"/>
-    <tableColumn id="9" xr3:uid="{00000000-0010-0000-0000-000009000000}" name="Deaths (daily)" dataDxfId="0"/>
+    <tableColumn id="1" name="Date" dataDxfId="9"/>
+    <tableColumn id="2" name="Tested (all)" dataDxfId="8"/>
+    <tableColumn id="3" name="Tested (daily)" dataDxfId="7"/>
+    <tableColumn id="4" name="Positive (all)" dataDxfId="6"/>
+    <tableColumn id="5" name="Positive (daily)" dataDxfId="5"/>
+    <tableColumn id="6" name="All hospitalized on certain day" dataDxfId="4"/>
+    <tableColumn id="7" name="All persons in intensive care on certain day" dataDxfId="3"/>
+    <tableColumn id="10" name="Discharged" dataDxfId="2"/>
+    <tableColumn id="8" name="Deaths (all)" dataDxfId="1"/>
+    <tableColumn id="9" name="Deaths (daily)" dataDxfId="0"/>
   </tableColumns>
   <tableStyleInfo name="TableStyleLight16" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
   <extLst>
@@ -695,11 +737,11 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:J75"/>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <dimension ref="A1:J115"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A40" zoomScale="89" zoomScaleNormal="89" workbookViewId="0">
-      <selection activeCell="J74" sqref="J74"/>
+    <sheetView tabSelected="1" topLeftCell="A83" zoomScale="89" zoomScaleNormal="89" workbookViewId="0">
+      <selection activeCell="D113" sqref="D113"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -3117,6 +3159,1286 @@
         <v>0</v>
       </c>
     </row>
+    <row r="76" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A76" s="20">
+        <v>43976</v>
+      </c>
+      <c r="B76" s="21">
+        <v>75770</v>
+      </c>
+      <c r="C76" s="22">
+        <v>754</v>
+      </c>
+      <c r="D76" s="22">
+        <v>1469</v>
+      </c>
+      <c r="E76" s="22">
+        <v>0</v>
+      </c>
+      <c r="F76" s="22">
+        <v>9</v>
+      </c>
+      <c r="G76" s="22">
+        <v>2</v>
+      </c>
+      <c r="H76" s="22">
+        <v>6</v>
+      </c>
+      <c r="I76" s="22">
+        <v>108</v>
+      </c>
+      <c r="J76" s="22">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="77" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A77" s="20">
+        <v>43977</v>
+      </c>
+      <c r="B77" s="21">
+        <v>76579</v>
+      </c>
+      <c r="C77" s="22">
+        <v>809</v>
+      </c>
+      <c r="D77" s="22">
+        <v>1471</v>
+      </c>
+      <c r="E77" s="22">
+        <v>2</v>
+      </c>
+      <c r="F77" s="22">
+        <v>8</v>
+      </c>
+      <c r="G77" s="22">
+        <v>2</v>
+      </c>
+      <c r="H77" s="22">
+        <v>2</v>
+      </c>
+      <c r="I77" s="22">
+        <v>108</v>
+      </c>
+      <c r="J77" s="22">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="78" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A78" s="20">
+        <v>43978</v>
+      </c>
+      <c r="B78" s="21">
+        <v>77210</v>
+      </c>
+      <c r="C78" s="22">
+        <v>631</v>
+      </c>
+      <c r="D78" s="22">
+        <v>1473</v>
+      </c>
+      <c r="E78" s="22">
+        <v>2</v>
+      </c>
+      <c r="F78" s="22">
+        <v>7</v>
+      </c>
+      <c r="G78" s="22">
+        <v>2</v>
+      </c>
+      <c r="H78" s="22">
+        <v>1</v>
+      </c>
+      <c r="I78" s="22">
+        <v>108</v>
+      </c>
+      <c r="J78" s="22">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="79" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A79" s="20">
+        <v>43979</v>
+      </c>
+      <c r="B79" s="21">
+        <v>77916</v>
+      </c>
+      <c r="C79" s="22">
+        <v>706</v>
+      </c>
+      <c r="D79" s="22">
+        <v>1473</v>
+      </c>
+      <c r="E79" s="22">
+        <v>0</v>
+      </c>
+      <c r="F79" s="22">
+        <v>7</v>
+      </c>
+      <c r="G79" s="22">
+        <v>2</v>
+      </c>
+      <c r="H79" s="22">
+        <v>0</v>
+      </c>
+      <c r="I79" s="22">
+        <v>108</v>
+      </c>
+      <c r="J79" s="22">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="80" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A80" s="20">
+        <v>43980</v>
+      </c>
+      <c r="B80" s="21">
+        <v>78529</v>
+      </c>
+      <c r="C80" s="22">
+        <v>613</v>
+      </c>
+      <c r="D80" s="22">
+        <v>1473</v>
+      </c>
+      <c r="E80" s="22">
+        <v>0</v>
+      </c>
+      <c r="F80" s="22">
+        <v>7</v>
+      </c>
+      <c r="G80" s="22">
+        <v>2</v>
+      </c>
+      <c r="H80" s="22">
+        <v>0</v>
+      </c>
+      <c r="I80" s="22">
+        <v>108</v>
+      </c>
+      <c r="J80" s="22">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="81" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A81" s="20">
+        <v>43981</v>
+      </c>
+      <c r="B81" s="22">
+        <v>78793</v>
+      </c>
+      <c r="C81" s="22">
+        <v>264</v>
+      </c>
+      <c r="D81" s="22">
+        <v>1473</v>
+      </c>
+      <c r="E81" s="22">
+        <v>0</v>
+      </c>
+      <c r="F81" s="22">
+        <v>6</v>
+      </c>
+      <c r="G81" s="22">
+        <v>2</v>
+      </c>
+      <c r="H81" s="22">
+        <v>1</v>
+      </c>
+      <c r="I81" s="22">
+        <v>108</v>
+      </c>
+      <c r="J81" s="22">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="82" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A82" s="20">
+        <v>43982</v>
+      </c>
+      <c r="B82" s="21">
+        <v>79039</v>
+      </c>
+      <c r="C82" s="22">
+        <v>246</v>
+      </c>
+      <c r="D82" s="22">
+        <v>1473</v>
+      </c>
+      <c r="E82" s="22">
+        <v>0</v>
+      </c>
+      <c r="F82" s="22">
+        <v>5</v>
+      </c>
+      <c r="G82" s="22">
+        <v>1</v>
+      </c>
+      <c r="H82" s="22">
+        <v>0</v>
+      </c>
+      <c r="I82" s="22">
+        <v>109</v>
+      </c>
+      <c r="J82" s="22">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="83" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A83" s="20">
+        <v>43983</v>
+      </c>
+      <c r="B83" s="21">
+        <v>79698</v>
+      </c>
+      <c r="C83" s="22">
+        <v>659</v>
+      </c>
+      <c r="D83" s="22">
+        <v>1475</v>
+      </c>
+      <c r="E83" s="22">
+        <v>2</v>
+      </c>
+      <c r="F83" s="22">
+        <v>5</v>
+      </c>
+      <c r="G83" s="22">
+        <v>1</v>
+      </c>
+      <c r="H83" s="22">
+        <v>0</v>
+      </c>
+      <c r="I83" s="22">
+        <v>109</v>
+      </c>
+      <c r="J83" s="22">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="84" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A84" s="20">
+        <v>43984</v>
+      </c>
+      <c r="B84" s="21">
+        <v>80505</v>
+      </c>
+      <c r="C84" s="22">
+        <v>807</v>
+      </c>
+      <c r="D84" s="22">
+        <v>1477</v>
+      </c>
+      <c r="E84" s="22">
+        <v>2</v>
+      </c>
+      <c r="F84" s="22">
+        <v>5</v>
+      </c>
+      <c r="G84" s="22">
+        <v>0</v>
+      </c>
+      <c r="H84" s="22">
+        <v>0</v>
+      </c>
+      <c r="I84" s="22">
+        <v>109</v>
+      </c>
+      <c r="J84" s="22">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="85" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A85" s="20">
+        <v>43985</v>
+      </c>
+      <c r="B85" s="21">
+        <v>81333</v>
+      </c>
+      <c r="C85" s="22">
+        <v>828</v>
+      </c>
+      <c r="D85" s="22">
+        <v>1477</v>
+      </c>
+      <c r="E85" s="22">
+        <v>0</v>
+      </c>
+      <c r="F85" s="22">
+        <v>5</v>
+      </c>
+      <c r="G85" s="22">
+        <v>0</v>
+      </c>
+      <c r="H85" s="22">
+        <v>0</v>
+      </c>
+      <c r="I85" s="22">
+        <v>109</v>
+      </c>
+      <c r="J85" s="22">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="86" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A86" s="26">
+        <v>43986</v>
+      </c>
+      <c r="B86" s="27">
+        <v>82161</v>
+      </c>
+      <c r="C86" s="28">
+        <v>828</v>
+      </c>
+      <c r="D86" s="28">
+        <v>1479</v>
+      </c>
+      <c r="E86" s="28">
+        <v>2</v>
+      </c>
+      <c r="F86" s="28">
+        <v>6</v>
+      </c>
+      <c r="G86" s="28">
+        <v>0</v>
+      </c>
+      <c r="H86" s="28">
+        <v>0</v>
+      </c>
+      <c r="I86" s="28">
+        <v>109</v>
+      </c>
+      <c r="J86" s="28">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="87" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A87" s="29">
+        <v>43987</v>
+      </c>
+      <c r="B87" s="30">
+        <v>82876</v>
+      </c>
+      <c r="C87" s="31">
+        <v>715</v>
+      </c>
+      <c r="D87" s="31">
+        <v>1484</v>
+      </c>
+      <c r="E87" s="31">
+        <v>5</v>
+      </c>
+      <c r="F87" s="31">
+        <v>6</v>
+      </c>
+      <c r="G87" s="31">
+        <v>0</v>
+      </c>
+      <c r="H87" s="31">
+        <v>0</v>
+      </c>
+      <c r="I87" s="31">
+        <v>109</v>
+      </c>
+      <c r="J87" s="31">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="88" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A88" s="23">
+        <v>43988</v>
+      </c>
+      <c r="B88" s="24">
+        <v>83105</v>
+      </c>
+      <c r="C88" s="25">
+        <v>229</v>
+      </c>
+      <c r="D88" s="25">
+        <v>1485</v>
+      </c>
+      <c r="E88" s="25">
+        <v>1</v>
+      </c>
+      <c r="F88" s="25">
+        <v>5</v>
+      </c>
+      <c r="G88" s="25">
+        <v>0</v>
+      </c>
+      <c r="H88" s="25">
+        <v>1</v>
+      </c>
+      <c r="I88" s="25">
+        <v>109</v>
+      </c>
+      <c r="J88" s="25">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="89" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A89" s="29">
+        <v>43989</v>
+      </c>
+      <c r="B89" s="30">
+        <v>83316</v>
+      </c>
+      <c r="C89" s="31">
+        <v>211</v>
+      </c>
+      <c r="D89" s="31">
+        <v>1485</v>
+      </c>
+      <c r="E89" s="31">
+        <v>0</v>
+      </c>
+      <c r="F89" s="31">
+        <v>5</v>
+      </c>
+      <c r="G89" s="31">
+        <v>0</v>
+      </c>
+      <c r="H89" s="31">
+        <v>0</v>
+      </c>
+      <c r="I89" s="31">
+        <v>109</v>
+      </c>
+      <c r="J89" s="31">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="90" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A90" s="20">
+        <v>43990</v>
+      </c>
+      <c r="B90" s="21">
+        <v>84130</v>
+      </c>
+      <c r="C90" s="22">
+        <v>814</v>
+      </c>
+      <c r="D90" s="22">
+        <v>1486</v>
+      </c>
+      <c r="E90" s="22">
+        <v>1</v>
+      </c>
+      <c r="F90" s="22">
+        <v>6</v>
+      </c>
+      <c r="G90" s="22">
+        <v>0</v>
+      </c>
+      <c r="H90" s="22">
+        <v>0</v>
+      </c>
+      <c r="I90" s="22">
+        <v>109</v>
+      </c>
+      <c r="J90" s="22">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="91" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A91" s="20">
+        <v>43991</v>
+      </c>
+      <c r="B91" s="21">
+        <v>84868</v>
+      </c>
+      <c r="C91" s="22">
+        <v>738</v>
+      </c>
+      <c r="D91" s="22">
+        <v>1488</v>
+      </c>
+      <c r="E91" s="22">
+        <v>2</v>
+      </c>
+      <c r="F91" s="22">
+        <v>6</v>
+      </c>
+      <c r="G91" s="22">
+        <v>0</v>
+      </c>
+      <c r="H91" s="22">
+        <v>0</v>
+      </c>
+      <c r="I91" s="22">
+        <v>109</v>
+      </c>
+      <c r="J91" s="22">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="92" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A92" s="23">
+        <v>43992</v>
+      </c>
+      <c r="B92" s="24">
+        <v>85626</v>
+      </c>
+      <c r="C92" s="25">
+        <v>758</v>
+      </c>
+      <c r="D92" s="25">
+        <v>1488</v>
+      </c>
+      <c r="E92" s="25">
+        <v>0</v>
+      </c>
+      <c r="F92" s="25">
+        <v>6</v>
+      </c>
+      <c r="G92" s="25">
+        <v>0</v>
+      </c>
+      <c r="H92" s="25">
+        <v>0</v>
+      </c>
+      <c r="I92" s="25">
+        <v>109</v>
+      </c>
+      <c r="J92" s="25">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="93" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A93" s="29">
+        <v>43993</v>
+      </c>
+      <c r="B93" s="30">
+        <v>86328</v>
+      </c>
+      <c r="C93" s="31">
+        <v>702</v>
+      </c>
+      <c r="D93" s="31">
+        <v>1490</v>
+      </c>
+      <c r="E93" s="31">
+        <v>2</v>
+      </c>
+      <c r="F93" s="31">
+        <v>6</v>
+      </c>
+      <c r="G93" s="31">
+        <v>0</v>
+      </c>
+      <c r="H93" s="31">
+        <v>0</v>
+      </c>
+      <c r="I93" s="31">
+        <v>109</v>
+      </c>
+      <c r="J93" s="31">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="94" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A94" s="23">
+        <v>43994</v>
+      </c>
+      <c r="B94" s="24">
+        <v>87095</v>
+      </c>
+      <c r="C94" s="25">
+        <v>767</v>
+      </c>
+      <c r="D94" s="25">
+        <v>1492</v>
+      </c>
+      <c r="E94" s="25">
+        <v>2</v>
+      </c>
+      <c r="F94" s="25">
+        <v>6</v>
+      </c>
+      <c r="G94" s="25">
+        <v>0</v>
+      </c>
+      <c r="H94" s="25">
+        <v>0</v>
+      </c>
+      <c r="I94" s="25">
+        <v>109</v>
+      </c>
+      <c r="J94" s="25">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="95" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A95" s="29">
+        <v>43995</v>
+      </c>
+      <c r="B95" s="30">
+        <v>87386</v>
+      </c>
+      <c r="C95" s="31">
+        <v>291</v>
+      </c>
+      <c r="D95" s="31">
+        <v>1495</v>
+      </c>
+      <c r="E95" s="31">
+        <v>3</v>
+      </c>
+      <c r="F95" s="31">
+        <v>6</v>
+      </c>
+      <c r="G95" s="31">
+        <v>0</v>
+      </c>
+      <c r="H95" s="31">
+        <v>0</v>
+      </c>
+      <c r="I95" s="31">
+        <v>109</v>
+      </c>
+      <c r="J95" s="31">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="96" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A96" s="23">
+        <v>43996</v>
+      </c>
+      <c r="B96" s="24">
+        <v>87598</v>
+      </c>
+      <c r="C96" s="25">
+        <v>212</v>
+      </c>
+      <c r="D96" s="25">
+        <v>1496</v>
+      </c>
+      <c r="E96" s="25">
+        <v>1</v>
+      </c>
+      <c r="F96" s="25">
+        <v>7</v>
+      </c>
+      <c r="G96" s="25">
+        <v>1</v>
+      </c>
+      <c r="H96" s="25">
+        <v>0</v>
+      </c>
+      <c r="I96" s="25">
+        <v>109</v>
+      </c>
+      <c r="J96" s="25">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="97" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A97" s="20">
+        <v>43997</v>
+      </c>
+      <c r="B97" s="21">
+        <v>88165</v>
+      </c>
+      <c r="C97" s="22">
+        <v>567</v>
+      </c>
+      <c r="D97" s="22">
+        <v>1499</v>
+      </c>
+      <c r="E97" s="22">
+        <v>3</v>
+      </c>
+      <c r="F97" s="22">
+        <v>7</v>
+      </c>
+      <c r="G97" s="22">
+        <v>1</v>
+      </c>
+      <c r="H97" s="22">
+        <v>0</v>
+      </c>
+      <c r="I97" s="22">
+        <v>109</v>
+      </c>
+      <c r="J97" s="22">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="98" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A98" s="20">
+        <v>43998</v>
+      </c>
+      <c r="B98" s="21">
+        <v>89151</v>
+      </c>
+      <c r="C98" s="22">
+        <v>986</v>
+      </c>
+      <c r="D98" s="22">
+        <v>1503</v>
+      </c>
+      <c r="E98" s="22">
+        <v>4</v>
+      </c>
+      <c r="F98" s="22">
+        <v>7</v>
+      </c>
+      <c r="G98" s="22">
+        <v>1</v>
+      </c>
+      <c r="H98" s="22">
+        <v>0</v>
+      </c>
+      <c r="I98" s="22">
+        <v>109</v>
+      </c>
+      <c r="J98" s="22">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="99" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A99" s="29">
+        <v>43999</v>
+      </c>
+      <c r="B99" s="30">
+        <v>90103</v>
+      </c>
+      <c r="C99" s="31">
+        <v>952</v>
+      </c>
+      <c r="D99" s="31">
+        <v>1511</v>
+      </c>
+      <c r="E99" s="31">
+        <v>8</v>
+      </c>
+      <c r="F99" s="31">
+        <v>6</v>
+      </c>
+      <c r="G99" s="31">
+        <v>1</v>
+      </c>
+      <c r="H99" s="31">
+        <v>1</v>
+      </c>
+      <c r="I99" s="31">
+        <v>109</v>
+      </c>
+      <c r="J99" s="31">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="100" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A100" s="20">
+        <v>44000</v>
+      </c>
+      <c r="B100" s="21">
+        <v>91005</v>
+      </c>
+      <c r="C100" s="22">
+        <v>902</v>
+      </c>
+      <c r="D100" s="22">
+        <v>1513</v>
+      </c>
+      <c r="E100" s="22">
+        <v>2</v>
+      </c>
+      <c r="F100" s="22">
+        <v>8</v>
+      </c>
+      <c r="G100" s="22">
+        <v>1</v>
+      </c>
+      <c r="H100" s="22">
+        <v>0</v>
+      </c>
+      <c r="I100" s="22">
+        <v>109</v>
+      </c>
+      <c r="J100" s="22">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="101" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A101" s="29">
+        <v>44001</v>
+      </c>
+      <c r="B101" s="30">
+        <v>92152</v>
+      </c>
+      <c r="C101" s="31">
+        <v>1147</v>
+      </c>
+      <c r="D101" s="31">
+        <v>1519</v>
+      </c>
+      <c r="E101" s="31">
+        <v>6</v>
+      </c>
+      <c r="F101" s="31">
+        <v>6</v>
+      </c>
+      <c r="G101" s="31">
+        <v>1</v>
+      </c>
+      <c r="H101" s="31">
+        <v>2</v>
+      </c>
+      <c r="I101" s="31">
+        <v>109</v>
+      </c>
+      <c r="J101" s="31">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="102" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A102" s="23">
+        <v>44002</v>
+      </c>
+      <c r="B102" s="24">
+        <v>92919</v>
+      </c>
+      <c r="C102" s="25">
+        <v>758</v>
+      </c>
+      <c r="D102" s="25">
+        <v>1520</v>
+      </c>
+      <c r="E102" s="25">
+        <v>1</v>
+      </c>
+      <c r="F102" s="25">
+        <v>6</v>
+      </c>
+      <c r="G102" s="25">
+        <v>1</v>
+      </c>
+      <c r="H102" s="25">
+        <v>2</v>
+      </c>
+      <c r="I102" s="25">
+        <v>109</v>
+      </c>
+      <c r="J102" s="25">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="103" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A103" s="29">
+        <v>44003</v>
+      </c>
+      <c r="B103" s="30">
+        <v>93181</v>
+      </c>
+      <c r="C103" s="31">
+        <v>271</v>
+      </c>
+      <c r="D103" s="31">
+        <v>1521</v>
+      </c>
+      <c r="E103" s="31">
+        <v>1</v>
+      </c>
+      <c r="F103" s="31">
+        <v>6</v>
+      </c>
+      <c r="G103" s="31">
+        <v>1</v>
+      </c>
+      <c r="H103" s="31">
+        <v>0</v>
+      </c>
+      <c r="I103" s="31">
+        <v>109</v>
+      </c>
+      <c r="J103" s="31">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="104" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A104" s="29">
+        <v>44004</v>
+      </c>
+      <c r="B104" s="30">
+        <v>94165</v>
+      </c>
+      <c r="C104" s="31">
+        <v>984</v>
+      </c>
+      <c r="D104" s="31">
+        <v>1534</v>
+      </c>
+      <c r="E104" s="31">
+        <v>13</v>
+      </c>
+      <c r="F104" s="31">
+        <v>5</v>
+      </c>
+      <c r="G104" s="31">
+        <v>1</v>
+      </c>
+      <c r="H104" s="31">
+        <v>1</v>
+      </c>
+      <c r="I104" s="31">
+        <v>109</v>
+      </c>
+      <c r="J104" s="31">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="105" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A105" s="29">
+        <v>44005</v>
+      </c>
+      <c r="B105" s="30">
+        <v>95387</v>
+      </c>
+      <c r="C105" s="31">
+        <v>1222</v>
+      </c>
+      <c r="D105" s="31">
+        <v>1541</v>
+      </c>
+      <c r="E105" s="31">
+        <v>7</v>
+      </c>
+      <c r="F105" s="31">
+        <v>7</v>
+      </c>
+      <c r="G105" s="31">
+        <v>2</v>
+      </c>
+      <c r="H105" s="31">
+        <v>0</v>
+      </c>
+      <c r="I105" s="31" t="s">
+        <v>10</v>
+      </c>
+      <c r="J105" s="31">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="106" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A106" s="23">
+        <v>44006</v>
+      </c>
+      <c r="B106" s="24">
+        <v>96599</v>
+      </c>
+      <c r="C106" s="25">
+        <v>1212</v>
+      </c>
+      <c r="D106" s="25">
+        <v>1547</v>
+      </c>
+      <c r="E106" s="25">
+        <v>6</v>
+      </c>
+      <c r="F106" s="25">
+        <v>7</v>
+      </c>
+      <c r="G106" s="25">
+        <v>2</v>
+      </c>
+      <c r="H106" s="25">
+        <v>0</v>
+      </c>
+      <c r="I106" s="25" t="s">
+        <v>10</v>
+      </c>
+      <c r="J106" s="25">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="107" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A107" s="29">
+        <v>44007</v>
+      </c>
+      <c r="B107" s="30">
+        <v>97442</v>
+      </c>
+      <c r="C107" s="31">
+        <v>843</v>
+      </c>
+      <c r="D107" s="31">
+        <v>1558</v>
+      </c>
+      <c r="E107" s="31">
+        <v>11</v>
+      </c>
+      <c r="F107" s="31">
+        <v>8</v>
+      </c>
+      <c r="G107" s="31">
+        <v>2</v>
+      </c>
+      <c r="H107" s="31">
+        <v>0</v>
+      </c>
+      <c r="I107" s="31" t="s">
+        <v>10</v>
+      </c>
+      <c r="J107" s="31">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="108" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A108" s="29">
+        <v>44008</v>
+      </c>
+      <c r="B108" s="30">
+        <v>98320</v>
+      </c>
+      <c r="C108" s="31">
+        <v>878</v>
+      </c>
+      <c r="D108" s="31">
+        <v>1572</v>
+      </c>
+      <c r="E108" s="31">
+        <v>14</v>
+      </c>
+      <c r="F108" s="31">
+        <v>8</v>
+      </c>
+      <c r="G108" s="31">
+        <v>1</v>
+      </c>
+      <c r="H108" s="31">
+        <v>0</v>
+      </c>
+      <c r="I108" s="31" t="s">
+        <v>10</v>
+      </c>
+      <c r="J108" s="31">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="109" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A109" s="29">
+        <v>44009</v>
+      </c>
+      <c r="B109" s="30">
+        <v>98945</v>
+      </c>
+      <c r="C109" s="31">
+        <v>625</v>
+      </c>
+      <c r="D109" s="31">
+        <v>1581</v>
+      </c>
+      <c r="E109" s="31">
+        <v>9</v>
+      </c>
+      <c r="F109" s="31">
+        <v>7</v>
+      </c>
+      <c r="G109" s="31">
+        <v>0</v>
+      </c>
+      <c r="H109" s="31">
+        <v>1</v>
+      </c>
+      <c r="I109" s="31" t="s">
+        <v>10</v>
+      </c>
+      <c r="J109" s="31">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="110" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A110" s="29">
+        <v>44010</v>
+      </c>
+      <c r="B110" s="30">
+        <v>99245</v>
+      </c>
+      <c r="C110" s="31">
+        <v>300</v>
+      </c>
+      <c r="D110" s="31">
+        <v>1585</v>
+      </c>
+      <c r="E110" s="31">
+        <v>4</v>
+      </c>
+      <c r="F110" s="31">
+        <v>8</v>
+      </c>
+      <c r="G110" s="31">
+        <v>0</v>
+      </c>
+      <c r="H110" s="31">
+        <v>0</v>
+      </c>
+      <c r="I110" s="31" t="s">
+        <v>10</v>
+      </c>
+      <c r="J110" s="31">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="111" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A111" s="29">
+        <v>44011</v>
+      </c>
+      <c r="B111" s="30">
+        <v>100330</v>
+      </c>
+      <c r="C111" s="31">
+        <v>1085</v>
+      </c>
+      <c r="D111" s="31">
+        <v>1600</v>
+      </c>
+      <c r="E111" s="31">
+        <v>15</v>
+      </c>
+      <c r="F111" s="31">
+        <v>8</v>
+      </c>
+      <c r="G111" s="31">
+        <v>0</v>
+      </c>
+      <c r="H111" s="31">
+        <v>0</v>
+      </c>
+      <c r="I111" s="31" t="s">
+        <v>10</v>
+      </c>
+      <c r="J111" s="31">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="112" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A112" s="20">
+        <v>44012</v>
+      </c>
+      <c r="B112" s="21">
+        <v>101729</v>
+      </c>
+      <c r="C112" s="22">
+        <v>1399</v>
+      </c>
+      <c r="D112" s="22">
+        <v>1613</v>
+      </c>
+      <c r="E112" s="22">
+        <v>13</v>
+      </c>
+      <c r="F112" s="22">
+        <v>8</v>
+      </c>
+      <c r="G112" s="22">
+        <v>0</v>
+      </c>
+      <c r="H112" s="22">
+        <v>0</v>
+      </c>
+      <c r="I112" s="22" t="s">
+        <v>10</v>
+      </c>
+      <c r="J112" s="22">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="113" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A113" s="20">
+        <v>44013</v>
+      </c>
+      <c r="B113" s="21">
+        <v>102927</v>
+      </c>
+      <c r="C113" s="22">
+        <v>1198</v>
+      </c>
+      <c r="D113" s="22">
+        <v>1633</v>
+      </c>
+      <c r="E113" s="22">
+        <v>21</v>
+      </c>
+      <c r="F113" s="22">
+        <v>9</v>
+      </c>
+      <c r="G113" s="22">
+        <v>0</v>
+      </c>
+      <c r="H113" s="22">
+        <v>0</v>
+      </c>
+      <c r="I113" s="22" t="s">
+        <v>10</v>
+      </c>
+      <c r="J113" s="22">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="114" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A114" s="20">
+        <v>44014</v>
+      </c>
+      <c r="B114" s="21">
+        <v>104201</v>
+      </c>
+      <c r="C114" s="22">
+        <v>1274</v>
+      </c>
+      <c r="D114" s="22">
+        <v>1649</v>
+      </c>
+      <c r="E114" s="22">
+        <v>16</v>
+      </c>
+      <c r="F114" s="22">
+        <v>10</v>
+      </c>
+      <c r="G114" s="22">
+        <v>0</v>
+      </c>
+      <c r="H114" s="22">
+        <v>0</v>
+      </c>
+      <c r="I114" s="22" t="s">
+        <v>10</v>
+      </c>
+      <c r="J114" s="22">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="115" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A115" s="20">
+        <v>44015</v>
+      </c>
+      <c r="B115" s="21">
+        <v>105652</v>
+      </c>
+      <c r="C115" s="22">
+        <v>1456</v>
+      </c>
+      <c r="D115" s="22">
+        <v>1679</v>
+      </c>
+      <c r="E115" s="22">
+        <v>30</v>
+      </c>
+      <c r="F115" s="22">
+        <v>6</v>
+      </c>
+      <c r="G115" s="22">
+        <v>0</v>
+      </c>
+      <c r="H115" s="22">
+        <v>4</v>
+      </c>
+      <c r="I115" s="22" t="s">
+        <v>10</v>
+      </c>
+      <c r="J115" s="22">
+        <v>0</v>
+      </c>
+    </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>

</xml_diff>

<commit_message>
Data updated by GitHub Bot (2020-07-04 20)
</commit_message>
<xml_diff>
--- a/output/snapshot/fdcf2531-4c3e-5c02-b63c-ee160ead6dea.xlsx
+++ b/output/snapshot/fdcf2531-4c3e-5c02-b63c-ee160ead6dea.xlsx
@@ -1,16 +1,15 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="21929"/>
-  <workbookPr/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
+  <fileVersion appName="xl" lastEdited="6" lowestEdited="6" rupBuild="14420"/>
+  <workbookPr defaultThemeVersion="164011"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="I:\AKTUALNI PODATKI - KORONA\Za objavo na GOV.SI\ang\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{1E6DD62F-2BE2-47DC-A7ED-9B57C1589256}" xr6:coauthVersionLast="44" xr6:coauthVersionMax="44" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840"/>
   </bookViews>
   <sheets>
     <sheet name="Covid-19 podatki" sheetId="1" r:id="rId1"/>
@@ -25,7 +24,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="10" uniqueCount="10">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="21" uniqueCount="11">
   <si>
     <t>Date</t>
   </si>
@@ -56,15 +55,18 @@
   <si>
     <t>Deaths (daily)</t>
   </si>
+  <si>
+    <t>111*</t>
+  </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" mc:Ignorable="x14ac x16r2">
   <numFmts count="1">
     <numFmt numFmtId="164" formatCode="d/\ m/\ yyyy;@"/>
   </numFmts>
-  <fonts count="4" x14ac:knownFonts="1">
+  <fonts count="5" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -93,6 +95,13 @@
       <name val="Calibri Light"/>
       <scheme val="major"/>
     </font>
+    <font>
+      <sz val="10"/>
+      <color theme="1"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
   </fonts>
   <fills count="3">
     <fill>
@@ -108,7 +117,7 @@
       </patternFill>
     </fill>
   </fills>
-  <borders count="2">
+  <borders count="3">
     <border>
       <left/>
       <right/>
@@ -129,11 +138,26 @@
       <bottom/>
       <diagonal/>
     </border>
+    <border>
+      <left style="thin">
+        <color theme="4"/>
+      </left>
+      <right style="thin">
+        <color theme="4"/>
+      </right>
+      <top style="thin">
+        <color theme="4"/>
+      </top>
+      <bottom style="thin">
+        <color theme="4"/>
+      </bottom>
+      <diagonal/>
+    </border>
   </borders>
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="26">
+  <cellXfs count="32">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="49" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyAlignment="1" applyProtection="1">
       <alignment horizontal="left" vertical="top"/>
@@ -208,6 +232,24 @@
       <alignment horizontal="right"/>
     </xf>
     <xf numFmtId="0" fontId="3" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="right"/>
+    </xf>
+    <xf numFmtId="164" fontId="4" fillId="2" borderId="2" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="right" vertical="top"/>
+    </xf>
+    <xf numFmtId="3" fontId="4" fillId="2" borderId="2" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="right"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="2" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="right"/>
+    </xf>
+    <xf numFmtId="164" fontId="3" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="right" vertical="top"/>
+    </xf>
+    <xf numFmtId="3" fontId="3" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="right"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="right"/>
     </xf>
   </cellXfs>
@@ -399,8 +441,8 @@
 </file>
 
 <file path=xl/tables/table1.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="1" xr:uid="{00000000-000C-0000-FFFF-FFFF00000000}" name="Tabela1" displayName="Tabela1" ref="A1:J75" totalsRowShown="0" headerRowDxfId="11" dataDxfId="10">
-  <autoFilter ref="A1:J75" xr:uid="{00000000-0009-0000-0100-000001000000}">
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="1" name="Tabela1" displayName="Tabela1" ref="A1:J115" totalsRowShown="0" headerRowDxfId="11" dataDxfId="10">
+  <autoFilter ref="A1:J115">
     <filterColumn colId="0" hiddenButton="1"/>
     <filterColumn colId="1" hiddenButton="1"/>
     <filterColumn colId="2" hiddenButton="1"/>
@@ -413,16 +455,16 @@
     <filterColumn colId="9" hiddenButton="1"/>
   </autoFilter>
   <tableColumns count="10">
-    <tableColumn id="1" xr3:uid="{00000000-0010-0000-0000-000001000000}" name="Date" dataDxfId="9"/>
-    <tableColumn id="2" xr3:uid="{00000000-0010-0000-0000-000002000000}" name="Tested (all)" dataDxfId="8"/>
-    <tableColumn id="3" xr3:uid="{00000000-0010-0000-0000-000003000000}" name="Tested (daily)" dataDxfId="7"/>
-    <tableColumn id="4" xr3:uid="{00000000-0010-0000-0000-000004000000}" name="Positive (all)" dataDxfId="6"/>
-    <tableColumn id="5" xr3:uid="{00000000-0010-0000-0000-000005000000}" name="Positive (daily)" dataDxfId="5"/>
-    <tableColumn id="6" xr3:uid="{00000000-0010-0000-0000-000006000000}" name="All hospitalized on certain day" dataDxfId="4"/>
-    <tableColumn id="7" xr3:uid="{00000000-0010-0000-0000-000007000000}" name="All persons in intensive care on certain day" dataDxfId="3"/>
-    <tableColumn id="10" xr3:uid="{00000000-0010-0000-0000-00000A000000}" name="Discharged" dataDxfId="2"/>
-    <tableColumn id="8" xr3:uid="{00000000-0010-0000-0000-000008000000}" name="Deaths (all)" dataDxfId="1"/>
-    <tableColumn id="9" xr3:uid="{00000000-0010-0000-0000-000009000000}" name="Deaths (daily)" dataDxfId="0"/>
+    <tableColumn id="1" name="Date" dataDxfId="9"/>
+    <tableColumn id="2" name="Tested (all)" dataDxfId="8"/>
+    <tableColumn id="3" name="Tested (daily)" dataDxfId="7"/>
+    <tableColumn id="4" name="Positive (all)" dataDxfId="6"/>
+    <tableColumn id="5" name="Positive (daily)" dataDxfId="5"/>
+    <tableColumn id="6" name="All hospitalized on certain day" dataDxfId="4"/>
+    <tableColumn id="7" name="All persons in intensive care on certain day" dataDxfId="3"/>
+    <tableColumn id="10" name="Discharged" dataDxfId="2"/>
+    <tableColumn id="8" name="Deaths (all)" dataDxfId="1"/>
+    <tableColumn id="9" name="Deaths (daily)" dataDxfId="0"/>
   </tableColumns>
   <tableStyleInfo name="TableStyleLight16" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
   <extLst>
@@ -695,11 +737,11 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:J75"/>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <dimension ref="A1:J115"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A40" zoomScale="89" zoomScaleNormal="89" workbookViewId="0">
-      <selection activeCell="J74" sqref="J74"/>
+    <sheetView tabSelected="1" topLeftCell="A83" zoomScale="89" zoomScaleNormal="89" workbookViewId="0">
+      <selection activeCell="D113" sqref="D113"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -3117,6 +3159,1286 @@
         <v>0</v>
       </c>
     </row>
+    <row r="76" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A76" s="20">
+        <v>43976</v>
+      </c>
+      <c r="B76" s="21">
+        <v>75770</v>
+      </c>
+      <c r="C76" s="22">
+        <v>754</v>
+      </c>
+      <c r="D76" s="22">
+        <v>1469</v>
+      </c>
+      <c r="E76" s="22">
+        <v>0</v>
+      </c>
+      <c r="F76" s="22">
+        <v>9</v>
+      </c>
+      <c r="G76" s="22">
+        <v>2</v>
+      </c>
+      <c r="H76" s="22">
+        <v>6</v>
+      </c>
+      <c r="I76" s="22">
+        <v>108</v>
+      </c>
+      <c r="J76" s="22">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="77" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A77" s="20">
+        <v>43977</v>
+      </c>
+      <c r="B77" s="21">
+        <v>76579</v>
+      </c>
+      <c r="C77" s="22">
+        <v>809</v>
+      </c>
+      <c r="D77" s="22">
+        <v>1471</v>
+      </c>
+      <c r="E77" s="22">
+        <v>2</v>
+      </c>
+      <c r="F77" s="22">
+        <v>8</v>
+      </c>
+      <c r="G77" s="22">
+        <v>2</v>
+      </c>
+      <c r="H77" s="22">
+        <v>2</v>
+      </c>
+      <c r="I77" s="22">
+        <v>108</v>
+      </c>
+      <c r="J77" s="22">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="78" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A78" s="20">
+        <v>43978</v>
+      </c>
+      <c r="B78" s="21">
+        <v>77210</v>
+      </c>
+      <c r="C78" s="22">
+        <v>631</v>
+      </c>
+      <c r="D78" s="22">
+        <v>1473</v>
+      </c>
+      <c r="E78" s="22">
+        <v>2</v>
+      </c>
+      <c r="F78" s="22">
+        <v>7</v>
+      </c>
+      <c r="G78" s="22">
+        <v>2</v>
+      </c>
+      <c r="H78" s="22">
+        <v>1</v>
+      </c>
+      <c r="I78" s="22">
+        <v>108</v>
+      </c>
+      <c r="J78" s="22">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="79" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A79" s="20">
+        <v>43979</v>
+      </c>
+      <c r="B79" s="21">
+        <v>77916</v>
+      </c>
+      <c r="C79" s="22">
+        <v>706</v>
+      </c>
+      <c r="D79" s="22">
+        <v>1473</v>
+      </c>
+      <c r="E79" s="22">
+        <v>0</v>
+      </c>
+      <c r="F79" s="22">
+        <v>7</v>
+      </c>
+      <c r="G79" s="22">
+        <v>2</v>
+      </c>
+      <c r="H79" s="22">
+        <v>0</v>
+      </c>
+      <c r="I79" s="22">
+        <v>108</v>
+      </c>
+      <c r="J79" s="22">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="80" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A80" s="20">
+        <v>43980</v>
+      </c>
+      <c r="B80" s="21">
+        <v>78529</v>
+      </c>
+      <c r="C80" s="22">
+        <v>613</v>
+      </c>
+      <c r="D80" s="22">
+        <v>1473</v>
+      </c>
+      <c r="E80" s="22">
+        <v>0</v>
+      </c>
+      <c r="F80" s="22">
+        <v>7</v>
+      </c>
+      <c r="G80" s="22">
+        <v>2</v>
+      </c>
+      <c r="H80" s="22">
+        <v>0</v>
+      </c>
+      <c r="I80" s="22">
+        <v>108</v>
+      </c>
+      <c r="J80" s="22">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="81" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A81" s="20">
+        <v>43981</v>
+      </c>
+      <c r="B81" s="22">
+        <v>78793</v>
+      </c>
+      <c r="C81" s="22">
+        <v>264</v>
+      </c>
+      <c r="D81" s="22">
+        <v>1473</v>
+      </c>
+      <c r="E81" s="22">
+        <v>0</v>
+      </c>
+      <c r="F81" s="22">
+        <v>6</v>
+      </c>
+      <c r="G81" s="22">
+        <v>2</v>
+      </c>
+      <c r="H81" s="22">
+        <v>1</v>
+      </c>
+      <c r="I81" s="22">
+        <v>108</v>
+      </c>
+      <c r="J81" s="22">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="82" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A82" s="20">
+        <v>43982</v>
+      </c>
+      <c r="B82" s="21">
+        <v>79039</v>
+      </c>
+      <c r="C82" s="22">
+        <v>246</v>
+      </c>
+      <c r="D82" s="22">
+        <v>1473</v>
+      </c>
+      <c r="E82" s="22">
+        <v>0</v>
+      </c>
+      <c r="F82" s="22">
+        <v>5</v>
+      </c>
+      <c r="G82" s="22">
+        <v>1</v>
+      </c>
+      <c r="H82" s="22">
+        <v>0</v>
+      </c>
+      <c r="I82" s="22">
+        <v>109</v>
+      </c>
+      <c r="J82" s="22">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="83" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A83" s="20">
+        <v>43983</v>
+      </c>
+      <c r="B83" s="21">
+        <v>79698</v>
+      </c>
+      <c r="C83" s="22">
+        <v>659</v>
+      </c>
+      <c r="D83" s="22">
+        <v>1475</v>
+      </c>
+      <c r="E83" s="22">
+        <v>2</v>
+      </c>
+      <c r="F83" s="22">
+        <v>5</v>
+      </c>
+      <c r="G83" s="22">
+        <v>1</v>
+      </c>
+      <c r="H83" s="22">
+        <v>0</v>
+      </c>
+      <c r="I83" s="22">
+        <v>109</v>
+      </c>
+      <c r="J83" s="22">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="84" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A84" s="20">
+        <v>43984</v>
+      </c>
+      <c r="B84" s="21">
+        <v>80505</v>
+      </c>
+      <c r="C84" s="22">
+        <v>807</v>
+      </c>
+      <c r="D84" s="22">
+        <v>1477</v>
+      </c>
+      <c r="E84" s="22">
+        <v>2</v>
+      </c>
+      <c r="F84" s="22">
+        <v>5</v>
+      </c>
+      <c r="G84" s="22">
+        <v>0</v>
+      </c>
+      <c r="H84" s="22">
+        <v>0</v>
+      </c>
+      <c r="I84" s="22">
+        <v>109</v>
+      </c>
+      <c r="J84" s="22">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="85" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A85" s="20">
+        <v>43985</v>
+      </c>
+      <c r="B85" s="21">
+        <v>81333</v>
+      </c>
+      <c r="C85" s="22">
+        <v>828</v>
+      </c>
+      <c r="D85" s="22">
+        <v>1477</v>
+      </c>
+      <c r="E85" s="22">
+        <v>0</v>
+      </c>
+      <c r="F85" s="22">
+        <v>5</v>
+      </c>
+      <c r="G85" s="22">
+        <v>0</v>
+      </c>
+      <c r="H85" s="22">
+        <v>0</v>
+      </c>
+      <c r="I85" s="22">
+        <v>109</v>
+      </c>
+      <c r="J85" s="22">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="86" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A86" s="26">
+        <v>43986</v>
+      </c>
+      <c r="B86" s="27">
+        <v>82161</v>
+      </c>
+      <c r="C86" s="28">
+        <v>828</v>
+      </c>
+      <c r="D86" s="28">
+        <v>1479</v>
+      </c>
+      <c r="E86" s="28">
+        <v>2</v>
+      </c>
+      <c r="F86" s="28">
+        <v>6</v>
+      </c>
+      <c r="G86" s="28">
+        <v>0</v>
+      </c>
+      <c r="H86" s="28">
+        <v>0</v>
+      </c>
+      <c r="I86" s="28">
+        <v>109</v>
+      </c>
+      <c r="J86" s="28">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="87" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A87" s="29">
+        <v>43987</v>
+      </c>
+      <c r="B87" s="30">
+        <v>82876</v>
+      </c>
+      <c r="C87" s="31">
+        <v>715</v>
+      </c>
+      <c r="D87" s="31">
+        <v>1484</v>
+      </c>
+      <c r="E87" s="31">
+        <v>5</v>
+      </c>
+      <c r="F87" s="31">
+        <v>6</v>
+      </c>
+      <c r="G87" s="31">
+        <v>0</v>
+      </c>
+      <c r="H87" s="31">
+        <v>0</v>
+      </c>
+      <c r="I87" s="31">
+        <v>109</v>
+      </c>
+      <c r="J87" s="31">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="88" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A88" s="23">
+        <v>43988</v>
+      </c>
+      <c r="B88" s="24">
+        <v>83105</v>
+      </c>
+      <c r="C88" s="25">
+        <v>229</v>
+      </c>
+      <c r="D88" s="25">
+        <v>1485</v>
+      </c>
+      <c r="E88" s="25">
+        <v>1</v>
+      </c>
+      <c r="F88" s="25">
+        <v>5</v>
+      </c>
+      <c r="G88" s="25">
+        <v>0</v>
+      </c>
+      <c r="H88" s="25">
+        <v>1</v>
+      </c>
+      <c r="I88" s="25">
+        <v>109</v>
+      </c>
+      <c r="J88" s="25">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="89" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A89" s="29">
+        <v>43989</v>
+      </c>
+      <c r="B89" s="30">
+        <v>83316</v>
+      </c>
+      <c r="C89" s="31">
+        <v>211</v>
+      </c>
+      <c r="D89" s="31">
+        <v>1485</v>
+      </c>
+      <c r="E89" s="31">
+        <v>0</v>
+      </c>
+      <c r="F89" s="31">
+        <v>5</v>
+      </c>
+      <c r="G89" s="31">
+        <v>0</v>
+      </c>
+      <c r="H89" s="31">
+        <v>0</v>
+      </c>
+      <c r="I89" s="31">
+        <v>109</v>
+      </c>
+      <c r="J89" s="31">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="90" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A90" s="20">
+        <v>43990</v>
+      </c>
+      <c r="B90" s="21">
+        <v>84130</v>
+      </c>
+      <c r="C90" s="22">
+        <v>814</v>
+      </c>
+      <c r="D90" s="22">
+        <v>1486</v>
+      </c>
+      <c r="E90" s="22">
+        <v>1</v>
+      </c>
+      <c r="F90" s="22">
+        <v>6</v>
+      </c>
+      <c r="G90" s="22">
+        <v>0</v>
+      </c>
+      <c r="H90" s="22">
+        <v>0</v>
+      </c>
+      <c r="I90" s="22">
+        <v>109</v>
+      </c>
+      <c r="J90" s="22">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="91" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A91" s="20">
+        <v>43991</v>
+      </c>
+      <c r="B91" s="21">
+        <v>84868</v>
+      </c>
+      <c r="C91" s="22">
+        <v>738</v>
+      </c>
+      <c r="D91" s="22">
+        <v>1488</v>
+      </c>
+      <c r="E91" s="22">
+        <v>2</v>
+      </c>
+      <c r="F91" s="22">
+        <v>6</v>
+      </c>
+      <c r="G91" s="22">
+        <v>0</v>
+      </c>
+      <c r="H91" s="22">
+        <v>0</v>
+      </c>
+      <c r="I91" s="22">
+        <v>109</v>
+      </c>
+      <c r="J91" s="22">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="92" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A92" s="23">
+        <v>43992</v>
+      </c>
+      <c r="B92" s="24">
+        <v>85626</v>
+      </c>
+      <c r="C92" s="25">
+        <v>758</v>
+      </c>
+      <c r="D92" s="25">
+        <v>1488</v>
+      </c>
+      <c r="E92" s="25">
+        <v>0</v>
+      </c>
+      <c r="F92" s="25">
+        <v>6</v>
+      </c>
+      <c r="G92" s="25">
+        <v>0</v>
+      </c>
+      <c r="H92" s="25">
+        <v>0</v>
+      </c>
+      <c r="I92" s="25">
+        <v>109</v>
+      </c>
+      <c r="J92" s="25">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="93" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A93" s="29">
+        <v>43993</v>
+      </c>
+      <c r="B93" s="30">
+        <v>86328</v>
+      </c>
+      <c r="C93" s="31">
+        <v>702</v>
+      </c>
+      <c r="D93" s="31">
+        <v>1490</v>
+      </c>
+      <c r="E93" s="31">
+        <v>2</v>
+      </c>
+      <c r="F93" s="31">
+        <v>6</v>
+      </c>
+      <c r="G93" s="31">
+        <v>0</v>
+      </c>
+      <c r="H93" s="31">
+        <v>0</v>
+      </c>
+      <c r="I93" s="31">
+        <v>109</v>
+      </c>
+      <c r="J93" s="31">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="94" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A94" s="23">
+        <v>43994</v>
+      </c>
+      <c r="B94" s="24">
+        <v>87095</v>
+      </c>
+      <c r="C94" s="25">
+        <v>767</v>
+      </c>
+      <c r="D94" s="25">
+        <v>1492</v>
+      </c>
+      <c r="E94" s="25">
+        <v>2</v>
+      </c>
+      <c r="F94" s="25">
+        <v>6</v>
+      </c>
+      <c r="G94" s="25">
+        <v>0</v>
+      </c>
+      <c r="H94" s="25">
+        <v>0</v>
+      </c>
+      <c r="I94" s="25">
+        <v>109</v>
+      </c>
+      <c r="J94" s="25">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="95" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A95" s="29">
+        <v>43995</v>
+      </c>
+      <c r="B95" s="30">
+        <v>87386</v>
+      </c>
+      <c r="C95" s="31">
+        <v>291</v>
+      </c>
+      <c r="D95" s="31">
+        <v>1495</v>
+      </c>
+      <c r="E95" s="31">
+        <v>3</v>
+      </c>
+      <c r="F95" s="31">
+        <v>6</v>
+      </c>
+      <c r="G95" s="31">
+        <v>0</v>
+      </c>
+      <c r="H95" s="31">
+        <v>0</v>
+      </c>
+      <c r="I95" s="31">
+        <v>109</v>
+      </c>
+      <c r="J95" s="31">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="96" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A96" s="23">
+        <v>43996</v>
+      </c>
+      <c r="B96" s="24">
+        <v>87598</v>
+      </c>
+      <c r="C96" s="25">
+        <v>212</v>
+      </c>
+      <c r="D96" s="25">
+        <v>1496</v>
+      </c>
+      <c r="E96" s="25">
+        <v>1</v>
+      </c>
+      <c r="F96" s="25">
+        <v>7</v>
+      </c>
+      <c r="G96" s="25">
+        <v>1</v>
+      </c>
+      <c r="H96" s="25">
+        <v>0</v>
+      </c>
+      <c r="I96" s="25">
+        <v>109</v>
+      </c>
+      <c r="J96" s="25">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="97" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A97" s="20">
+        <v>43997</v>
+      </c>
+      <c r="B97" s="21">
+        <v>88165</v>
+      </c>
+      <c r="C97" s="22">
+        <v>567</v>
+      </c>
+      <c r="D97" s="22">
+        <v>1499</v>
+      </c>
+      <c r="E97" s="22">
+        <v>3</v>
+      </c>
+      <c r="F97" s="22">
+        <v>7</v>
+      </c>
+      <c r="G97" s="22">
+        <v>1</v>
+      </c>
+      <c r="H97" s="22">
+        <v>0</v>
+      </c>
+      <c r="I97" s="22">
+        <v>109</v>
+      </c>
+      <c r="J97" s="22">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="98" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A98" s="20">
+        <v>43998</v>
+      </c>
+      <c r="B98" s="21">
+        <v>89151</v>
+      </c>
+      <c r="C98" s="22">
+        <v>986</v>
+      </c>
+      <c r="D98" s="22">
+        <v>1503</v>
+      </c>
+      <c r="E98" s="22">
+        <v>4</v>
+      </c>
+      <c r="F98" s="22">
+        <v>7</v>
+      </c>
+      <c r="G98" s="22">
+        <v>1</v>
+      </c>
+      <c r="H98" s="22">
+        <v>0</v>
+      </c>
+      <c r="I98" s="22">
+        <v>109</v>
+      </c>
+      <c r="J98" s="22">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="99" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A99" s="29">
+        <v>43999</v>
+      </c>
+      <c r="B99" s="30">
+        <v>90103</v>
+      </c>
+      <c r="C99" s="31">
+        <v>952</v>
+      </c>
+      <c r="D99" s="31">
+        <v>1511</v>
+      </c>
+      <c r="E99" s="31">
+        <v>8</v>
+      </c>
+      <c r="F99" s="31">
+        <v>6</v>
+      </c>
+      <c r="G99" s="31">
+        <v>1</v>
+      </c>
+      <c r="H99" s="31">
+        <v>1</v>
+      </c>
+      <c r="I99" s="31">
+        <v>109</v>
+      </c>
+      <c r="J99" s="31">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="100" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A100" s="20">
+        <v>44000</v>
+      </c>
+      <c r="B100" s="21">
+        <v>91005</v>
+      </c>
+      <c r="C100" s="22">
+        <v>902</v>
+      </c>
+      <c r="D100" s="22">
+        <v>1513</v>
+      </c>
+      <c r="E100" s="22">
+        <v>2</v>
+      </c>
+      <c r="F100" s="22">
+        <v>8</v>
+      </c>
+      <c r="G100" s="22">
+        <v>1</v>
+      </c>
+      <c r="H100" s="22">
+        <v>0</v>
+      </c>
+      <c r="I100" s="22">
+        <v>109</v>
+      </c>
+      <c r="J100" s="22">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="101" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A101" s="29">
+        <v>44001</v>
+      </c>
+      <c r="B101" s="30">
+        <v>92152</v>
+      </c>
+      <c r="C101" s="31">
+        <v>1147</v>
+      </c>
+      <c r="D101" s="31">
+        <v>1519</v>
+      </c>
+      <c r="E101" s="31">
+        <v>6</v>
+      </c>
+      <c r="F101" s="31">
+        <v>6</v>
+      </c>
+      <c r="G101" s="31">
+        <v>1</v>
+      </c>
+      <c r="H101" s="31">
+        <v>2</v>
+      </c>
+      <c r="I101" s="31">
+        <v>109</v>
+      </c>
+      <c r="J101" s="31">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="102" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A102" s="23">
+        <v>44002</v>
+      </c>
+      <c r="B102" s="24">
+        <v>92919</v>
+      </c>
+      <c r="C102" s="25">
+        <v>758</v>
+      </c>
+      <c r="D102" s="25">
+        <v>1520</v>
+      </c>
+      <c r="E102" s="25">
+        <v>1</v>
+      </c>
+      <c r="F102" s="25">
+        <v>6</v>
+      </c>
+      <c r="G102" s="25">
+        <v>1</v>
+      </c>
+      <c r="H102" s="25">
+        <v>2</v>
+      </c>
+      <c r="I102" s="25">
+        <v>109</v>
+      </c>
+      <c r="J102" s="25">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="103" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A103" s="29">
+        <v>44003</v>
+      </c>
+      <c r="B103" s="30">
+        <v>93181</v>
+      </c>
+      <c r="C103" s="31">
+        <v>271</v>
+      </c>
+      <c r="D103" s="31">
+        <v>1521</v>
+      </c>
+      <c r="E103" s="31">
+        <v>1</v>
+      </c>
+      <c r="F103" s="31">
+        <v>6</v>
+      </c>
+      <c r="G103" s="31">
+        <v>1</v>
+      </c>
+      <c r="H103" s="31">
+        <v>0</v>
+      </c>
+      <c r="I103" s="31">
+        <v>109</v>
+      </c>
+      <c r="J103" s="31">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="104" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A104" s="29">
+        <v>44004</v>
+      </c>
+      <c r="B104" s="30">
+        <v>94165</v>
+      </c>
+      <c r="C104" s="31">
+        <v>984</v>
+      </c>
+      <c r="D104" s="31">
+        <v>1534</v>
+      </c>
+      <c r="E104" s="31">
+        <v>13</v>
+      </c>
+      <c r="F104" s="31">
+        <v>5</v>
+      </c>
+      <c r="G104" s="31">
+        <v>1</v>
+      </c>
+      <c r="H104" s="31">
+        <v>1</v>
+      </c>
+      <c r="I104" s="31">
+        <v>109</v>
+      </c>
+      <c r="J104" s="31">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="105" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A105" s="29">
+        <v>44005</v>
+      </c>
+      <c r="B105" s="30">
+        <v>95387</v>
+      </c>
+      <c r="C105" s="31">
+        <v>1222</v>
+      </c>
+      <c r="D105" s="31">
+        <v>1541</v>
+      </c>
+      <c r="E105" s="31">
+        <v>7</v>
+      </c>
+      <c r="F105" s="31">
+        <v>7</v>
+      </c>
+      <c r="G105" s="31">
+        <v>2</v>
+      </c>
+      <c r="H105" s="31">
+        <v>0</v>
+      </c>
+      <c r="I105" s="31" t="s">
+        <v>10</v>
+      </c>
+      <c r="J105" s="31">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="106" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A106" s="23">
+        <v>44006</v>
+      </c>
+      <c r="B106" s="24">
+        <v>96599</v>
+      </c>
+      <c r="C106" s="25">
+        <v>1212</v>
+      </c>
+      <c r="D106" s="25">
+        <v>1547</v>
+      </c>
+      <c r="E106" s="25">
+        <v>6</v>
+      </c>
+      <c r="F106" s="25">
+        <v>7</v>
+      </c>
+      <c r="G106" s="25">
+        <v>2</v>
+      </c>
+      <c r="H106" s="25">
+        <v>0</v>
+      </c>
+      <c r="I106" s="25" t="s">
+        <v>10</v>
+      </c>
+      <c r="J106" s="25">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="107" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A107" s="29">
+        <v>44007</v>
+      </c>
+      <c r="B107" s="30">
+        <v>97442</v>
+      </c>
+      <c r="C107" s="31">
+        <v>843</v>
+      </c>
+      <c r="D107" s="31">
+        <v>1558</v>
+      </c>
+      <c r="E107" s="31">
+        <v>11</v>
+      </c>
+      <c r="F107" s="31">
+        <v>8</v>
+      </c>
+      <c r="G107" s="31">
+        <v>2</v>
+      </c>
+      <c r="H107" s="31">
+        <v>0</v>
+      </c>
+      <c r="I107" s="31" t="s">
+        <v>10</v>
+      </c>
+      <c r="J107" s="31">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="108" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A108" s="29">
+        <v>44008</v>
+      </c>
+      <c r="B108" s="30">
+        <v>98320</v>
+      </c>
+      <c r="C108" s="31">
+        <v>878</v>
+      </c>
+      <c r="D108" s="31">
+        <v>1572</v>
+      </c>
+      <c r="E108" s="31">
+        <v>14</v>
+      </c>
+      <c r="F108" s="31">
+        <v>8</v>
+      </c>
+      <c r="G108" s="31">
+        <v>1</v>
+      </c>
+      <c r="H108" s="31">
+        <v>0</v>
+      </c>
+      <c r="I108" s="31" t="s">
+        <v>10</v>
+      </c>
+      <c r="J108" s="31">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="109" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A109" s="29">
+        <v>44009</v>
+      </c>
+      <c r="B109" s="30">
+        <v>98945</v>
+      </c>
+      <c r="C109" s="31">
+        <v>625</v>
+      </c>
+      <c r="D109" s="31">
+        <v>1581</v>
+      </c>
+      <c r="E109" s="31">
+        <v>9</v>
+      </c>
+      <c r="F109" s="31">
+        <v>7</v>
+      </c>
+      <c r="G109" s="31">
+        <v>0</v>
+      </c>
+      <c r="H109" s="31">
+        <v>1</v>
+      </c>
+      <c r="I109" s="31" t="s">
+        <v>10</v>
+      </c>
+      <c r="J109" s="31">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="110" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A110" s="29">
+        <v>44010</v>
+      </c>
+      <c r="B110" s="30">
+        <v>99245</v>
+      </c>
+      <c r="C110" s="31">
+        <v>300</v>
+      </c>
+      <c r="D110" s="31">
+        <v>1585</v>
+      </c>
+      <c r="E110" s="31">
+        <v>4</v>
+      </c>
+      <c r="F110" s="31">
+        <v>8</v>
+      </c>
+      <c r="G110" s="31">
+        <v>0</v>
+      </c>
+      <c r="H110" s="31">
+        <v>0</v>
+      </c>
+      <c r="I110" s="31" t="s">
+        <v>10</v>
+      </c>
+      <c r="J110" s="31">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="111" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A111" s="29">
+        <v>44011</v>
+      </c>
+      <c r="B111" s="30">
+        <v>100330</v>
+      </c>
+      <c r="C111" s="31">
+        <v>1085</v>
+      </c>
+      <c r="D111" s="31">
+        <v>1600</v>
+      </c>
+      <c r="E111" s="31">
+        <v>15</v>
+      </c>
+      <c r="F111" s="31">
+        <v>8</v>
+      </c>
+      <c r="G111" s="31">
+        <v>0</v>
+      </c>
+      <c r="H111" s="31">
+        <v>0</v>
+      </c>
+      <c r="I111" s="31" t="s">
+        <v>10</v>
+      </c>
+      <c r="J111" s="31">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="112" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A112" s="20">
+        <v>44012</v>
+      </c>
+      <c r="B112" s="21">
+        <v>101729</v>
+      </c>
+      <c r="C112" s="22">
+        <v>1399</v>
+      </c>
+      <c r="D112" s="22">
+        <v>1613</v>
+      </c>
+      <c r="E112" s="22">
+        <v>13</v>
+      </c>
+      <c r="F112" s="22">
+        <v>8</v>
+      </c>
+      <c r="G112" s="22">
+        <v>0</v>
+      </c>
+      <c r="H112" s="22">
+        <v>0</v>
+      </c>
+      <c r="I112" s="22" t="s">
+        <v>10</v>
+      </c>
+      <c r="J112" s="22">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="113" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A113" s="20">
+        <v>44013</v>
+      </c>
+      <c r="B113" s="21">
+        <v>102927</v>
+      </c>
+      <c r="C113" s="22">
+        <v>1198</v>
+      </c>
+      <c r="D113" s="22">
+        <v>1633</v>
+      </c>
+      <c r="E113" s="22">
+        <v>21</v>
+      </c>
+      <c r="F113" s="22">
+        <v>9</v>
+      </c>
+      <c r="G113" s="22">
+        <v>0</v>
+      </c>
+      <c r="H113" s="22">
+        <v>0</v>
+      </c>
+      <c r="I113" s="22" t="s">
+        <v>10</v>
+      </c>
+      <c r="J113" s="22">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="114" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A114" s="20">
+        <v>44014</v>
+      </c>
+      <c r="B114" s="21">
+        <v>104201</v>
+      </c>
+      <c r="C114" s="22">
+        <v>1274</v>
+      </c>
+      <c r="D114" s="22">
+        <v>1649</v>
+      </c>
+      <c r="E114" s="22">
+        <v>16</v>
+      </c>
+      <c r="F114" s="22">
+        <v>10</v>
+      </c>
+      <c r="G114" s="22">
+        <v>0</v>
+      </c>
+      <c r="H114" s="22">
+        <v>0</v>
+      </c>
+      <c r="I114" s="22" t="s">
+        <v>10</v>
+      </c>
+      <c r="J114" s="22">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="115" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A115" s="20">
+        <v>44015</v>
+      </c>
+      <c r="B115" s="21">
+        <v>105652</v>
+      </c>
+      <c r="C115" s="22">
+        <v>1456</v>
+      </c>
+      <c r="D115" s="22">
+        <v>1679</v>
+      </c>
+      <c r="E115" s="22">
+        <v>30</v>
+      </c>
+      <c r="F115" s="22">
+        <v>6</v>
+      </c>
+      <c r="G115" s="22">
+        <v>0</v>
+      </c>
+      <c r="H115" s="22">
+        <v>4</v>
+      </c>
+      <c r="I115" s="22" t="s">
+        <v>10</v>
+      </c>
+      <c r="J115" s="22">
+        <v>0</v>
+      </c>
+    </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>

</xml_diff>

<commit_message>
Data updated by GitHub Bot (2020-07-05 12)
</commit_message>
<xml_diff>
--- a/output/snapshot/fdcf2531-4c3e-5c02-b63c-ee160ead6dea.xlsx
+++ b/output/snapshot/fdcf2531-4c3e-5c02-b63c-ee160ead6dea.xlsx
@@ -1,16 +1,15 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="21929"/>
-  <workbookPr/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
+  <fileVersion appName="xl" lastEdited="6" lowestEdited="6" rupBuild="14420"/>
+  <workbookPr defaultThemeVersion="164011"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="I:\AKTUALNI PODATKI - KORONA\Za objavo na GOV.SI\ang\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{1E6DD62F-2BE2-47DC-A7ED-9B57C1589256}" xr6:coauthVersionLast="44" xr6:coauthVersionMax="44" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840"/>
   </bookViews>
   <sheets>
     <sheet name="Covid-19 podatki" sheetId="1" r:id="rId1"/>
@@ -25,7 +24,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="10" uniqueCount="10">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="22" uniqueCount="11">
   <si>
     <t>Date</t>
   </si>
@@ -56,15 +55,18 @@
   <si>
     <t>Deaths (daily)</t>
   </si>
+  <si>
+    <t>111*</t>
+  </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" mc:Ignorable="x14ac x16r2">
   <numFmts count="1">
     <numFmt numFmtId="164" formatCode="d/\ m/\ yyyy;@"/>
   </numFmts>
-  <fonts count="4" x14ac:knownFonts="1">
+  <fonts count="5" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -93,6 +95,13 @@
       <name val="Calibri Light"/>
       <scheme val="major"/>
     </font>
+    <font>
+      <sz val="10"/>
+      <color theme="1"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
   </fonts>
   <fills count="3">
     <fill>
@@ -108,7 +117,7 @@
       </patternFill>
     </fill>
   </fills>
-  <borders count="2">
+  <borders count="3">
     <border>
       <left/>
       <right/>
@@ -129,11 +138,26 @@
       <bottom/>
       <diagonal/>
     </border>
+    <border>
+      <left style="thin">
+        <color theme="4"/>
+      </left>
+      <right style="thin">
+        <color theme="4"/>
+      </right>
+      <top style="thin">
+        <color theme="4"/>
+      </top>
+      <bottom style="thin">
+        <color theme="4"/>
+      </bottom>
+      <diagonal/>
+    </border>
   </borders>
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="26">
+  <cellXfs count="32">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="49" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyAlignment="1" applyProtection="1">
       <alignment horizontal="left" vertical="top"/>
@@ -208,6 +232,24 @@
       <alignment horizontal="right"/>
     </xf>
     <xf numFmtId="0" fontId="3" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="right"/>
+    </xf>
+    <xf numFmtId="164" fontId="4" fillId="2" borderId="2" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="right" vertical="top"/>
+    </xf>
+    <xf numFmtId="3" fontId="4" fillId="2" borderId="2" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="right"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="2" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="right"/>
+    </xf>
+    <xf numFmtId="164" fontId="3" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="right" vertical="top"/>
+    </xf>
+    <xf numFmtId="3" fontId="3" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="right"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="right"/>
     </xf>
   </cellXfs>
@@ -399,8 +441,8 @@
 </file>
 
 <file path=xl/tables/table1.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="1" xr:uid="{00000000-000C-0000-FFFF-FFFF00000000}" name="Tabela1" displayName="Tabela1" ref="A1:J75" totalsRowShown="0" headerRowDxfId="11" dataDxfId="10">
-  <autoFilter ref="A1:J75" xr:uid="{00000000-0009-0000-0100-000001000000}">
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="1" name="Tabela1" displayName="Tabela1" ref="A1:J116" totalsRowShown="0" headerRowDxfId="11" dataDxfId="10">
+  <autoFilter ref="A1:J116">
     <filterColumn colId="0" hiddenButton="1"/>
     <filterColumn colId="1" hiddenButton="1"/>
     <filterColumn colId="2" hiddenButton="1"/>
@@ -413,16 +455,16 @@
     <filterColumn colId="9" hiddenButton="1"/>
   </autoFilter>
   <tableColumns count="10">
-    <tableColumn id="1" xr3:uid="{00000000-0010-0000-0000-000001000000}" name="Date" dataDxfId="9"/>
-    <tableColumn id="2" xr3:uid="{00000000-0010-0000-0000-000002000000}" name="Tested (all)" dataDxfId="8"/>
-    <tableColumn id="3" xr3:uid="{00000000-0010-0000-0000-000003000000}" name="Tested (daily)" dataDxfId="7"/>
-    <tableColumn id="4" xr3:uid="{00000000-0010-0000-0000-000004000000}" name="Positive (all)" dataDxfId="6"/>
-    <tableColumn id="5" xr3:uid="{00000000-0010-0000-0000-000005000000}" name="Positive (daily)" dataDxfId="5"/>
-    <tableColumn id="6" xr3:uid="{00000000-0010-0000-0000-000006000000}" name="All hospitalized on certain day" dataDxfId="4"/>
-    <tableColumn id="7" xr3:uid="{00000000-0010-0000-0000-000007000000}" name="All persons in intensive care on certain day" dataDxfId="3"/>
-    <tableColumn id="10" xr3:uid="{00000000-0010-0000-0000-00000A000000}" name="Discharged" dataDxfId="2"/>
-    <tableColumn id="8" xr3:uid="{00000000-0010-0000-0000-000008000000}" name="Deaths (all)" dataDxfId="1"/>
-    <tableColumn id="9" xr3:uid="{00000000-0010-0000-0000-000009000000}" name="Deaths (daily)" dataDxfId="0"/>
+    <tableColumn id="1" name="Date" dataDxfId="9"/>
+    <tableColumn id="2" name="Tested (all)" dataDxfId="8"/>
+    <tableColumn id="3" name="Tested (daily)" dataDxfId="7"/>
+    <tableColumn id="4" name="Positive (all)" dataDxfId="6"/>
+    <tableColumn id="5" name="Positive (daily)" dataDxfId="5"/>
+    <tableColumn id="6" name="All hospitalized on certain day" dataDxfId="4"/>
+    <tableColumn id="7" name="All persons in intensive care on certain day" dataDxfId="3"/>
+    <tableColumn id="10" name="Discharged" dataDxfId="2"/>
+    <tableColumn id="8" name="Deaths (all)" dataDxfId="1"/>
+    <tableColumn id="9" name="Deaths (daily)" dataDxfId="0"/>
   </tableColumns>
   <tableStyleInfo name="TableStyleLight16" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
   <extLst>
@@ -695,11 +737,11 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:J75"/>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <dimension ref="A1:J116"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A40" zoomScale="89" zoomScaleNormal="89" workbookViewId="0">
-      <selection activeCell="J74" sqref="J74"/>
+    <sheetView tabSelected="1" topLeftCell="A83" zoomScale="89" zoomScaleNormal="89" workbookViewId="0">
+      <selection activeCell="H116" sqref="H116"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -3117,6 +3159,1318 @@
         <v>0</v>
       </c>
     </row>
+    <row r="76" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A76" s="20">
+        <v>43976</v>
+      </c>
+      <c r="B76" s="21">
+        <v>75770</v>
+      </c>
+      <c r="C76" s="22">
+        <v>754</v>
+      </c>
+      <c r="D76" s="22">
+        <v>1469</v>
+      </c>
+      <c r="E76" s="22">
+        <v>0</v>
+      </c>
+      <c r="F76" s="22">
+        <v>9</v>
+      </c>
+      <c r="G76" s="22">
+        <v>2</v>
+      </c>
+      <c r="H76" s="22">
+        <v>6</v>
+      </c>
+      <c r="I76" s="22">
+        <v>108</v>
+      </c>
+      <c r="J76" s="22">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="77" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A77" s="20">
+        <v>43977</v>
+      </c>
+      <c r="B77" s="21">
+        <v>76579</v>
+      </c>
+      <c r="C77" s="22">
+        <v>809</v>
+      </c>
+      <c r="D77" s="22">
+        <v>1471</v>
+      </c>
+      <c r="E77" s="22">
+        <v>2</v>
+      </c>
+      <c r="F77" s="22">
+        <v>8</v>
+      </c>
+      <c r="G77" s="22">
+        <v>2</v>
+      </c>
+      <c r="H77" s="22">
+        <v>2</v>
+      </c>
+      <c r="I77" s="22">
+        <v>108</v>
+      </c>
+      <c r="J77" s="22">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="78" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A78" s="20">
+        <v>43978</v>
+      </c>
+      <c r="B78" s="21">
+        <v>77210</v>
+      </c>
+      <c r="C78" s="22">
+        <v>631</v>
+      </c>
+      <c r="D78" s="22">
+        <v>1473</v>
+      </c>
+      <c r="E78" s="22">
+        <v>2</v>
+      </c>
+      <c r="F78" s="22">
+        <v>7</v>
+      </c>
+      <c r="G78" s="22">
+        <v>2</v>
+      </c>
+      <c r="H78" s="22">
+        <v>1</v>
+      </c>
+      <c r="I78" s="22">
+        <v>108</v>
+      </c>
+      <c r="J78" s="22">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="79" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A79" s="20">
+        <v>43979</v>
+      </c>
+      <c r="B79" s="21">
+        <v>77916</v>
+      </c>
+      <c r="C79" s="22">
+        <v>706</v>
+      </c>
+      <c r="D79" s="22">
+        <v>1473</v>
+      </c>
+      <c r="E79" s="22">
+        <v>0</v>
+      </c>
+      <c r="F79" s="22">
+        <v>7</v>
+      </c>
+      <c r="G79" s="22">
+        <v>2</v>
+      </c>
+      <c r="H79" s="22">
+        <v>0</v>
+      </c>
+      <c r="I79" s="22">
+        <v>108</v>
+      </c>
+      <c r="J79" s="22">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="80" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A80" s="20">
+        <v>43980</v>
+      </c>
+      <c r="B80" s="21">
+        <v>78529</v>
+      </c>
+      <c r="C80" s="22">
+        <v>613</v>
+      </c>
+      <c r="D80" s="22">
+        <v>1473</v>
+      </c>
+      <c r="E80" s="22">
+        <v>0</v>
+      </c>
+      <c r="F80" s="22">
+        <v>7</v>
+      </c>
+      <c r="G80" s="22">
+        <v>2</v>
+      </c>
+      <c r="H80" s="22">
+        <v>0</v>
+      </c>
+      <c r="I80" s="22">
+        <v>108</v>
+      </c>
+      <c r="J80" s="22">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="81" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A81" s="20">
+        <v>43981</v>
+      </c>
+      <c r="B81" s="22">
+        <v>78793</v>
+      </c>
+      <c r="C81" s="22">
+        <v>264</v>
+      </c>
+      <c r="D81" s="22">
+        <v>1473</v>
+      </c>
+      <c r="E81" s="22">
+        <v>0</v>
+      </c>
+      <c r="F81" s="22">
+        <v>6</v>
+      </c>
+      <c r="G81" s="22">
+        <v>2</v>
+      </c>
+      <c r="H81" s="22">
+        <v>1</v>
+      </c>
+      <c r="I81" s="22">
+        <v>108</v>
+      </c>
+      <c r="J81" s="22">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="82" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A82" s="20">
+        <v>43982</v>
+      </c>
+      <c r="B82" s="21">
+        <v>79039</v>
+      </c>
+      <c r="C82" s="22">
+        <v>246</v>
+      </c>
+      <c r="D82" s="22">
+        <v>1473</v>
+      </c>
+      <c r="E82" s="22">
+        <v>0</v>
+      </c>
+      <c r="F82" s="22">
+        <v>5</v>
+      </c>
+      <c r="G82" s="22">
+        <v>1</v>
+      </c>
+      <c r="H82" s="22">
+        <v>0</v>
+      </c>
+      <c r="I82" s="22">
+        <v>109</v>
+      </c>
+      <c r="J82" s="22">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="83" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A83" s="20">
+        <v>43983</v>
+      </c>
+      <c r="B83" s="21">
+        <v>79698</v>
+      </c>
+      <c r="C83" s="22">
+        <v>659</v>
+      </c>
+      <c r="D83" s="22">
+        <v>1475</v>
+      </c>
+      <c r="E83" s="22">
+        <v>2</v>
+      </c>
+      <c r="F83" s="22">
+        <v>5</v>
+      </c>
+      <c r="G83" s="22">
+        <v>1</v>
+      </c>
+      <c r="H83" s="22">
+        <v>0</v>
+      </c>
+      <c r="I83" s="22">
+        <v>109</v>
+      </c>
+      <c r="J83" s="22">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="84" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A84" s="20">
+        <v>43984</v>
+      </c>
+      <c r="B84" s="21">
+        <v>80505</v>
+      </c>
+      <c r="C84" s="22">
+        <v>807</v>
+      </c>
+      <c r="D84" s="22">
+        <v>1477</v>
+      </c>
+      <c r="E84" s="22">
+        <v>2</v>
+      </c>
+      <c r="F84" s="22">
+        <v>5</v>
+      </c>
+      <c r="G84" s="22">
+        <v>0</v>
+      </c>
+      <c r="H84" s="22">
+        <v>0</v>
+      </c>
+      <c r="I84" s="22">
+        <v>109</v>
+      </c>
+      <c r="J84" s="22">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="85" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A85" s="20">
+        <v>43985</v>
+      </c>
+      <c r="B85" s="21">
+        <v>81333</v>
+      </c>
+      <c r="C85" s="22">
+        <v>828</v>
+      </c>
+      <c r="D85" s="22">
+        <v>1477</v>
+      </c>
+      <c r="E85" s="22">
+        <v>0</v>
+      </c>
+      <c r="F85" s="22">
+        <v>5</v>
+      </c>
+      <c r="G85" s="22">
+        <v>0</v>
+      </c>
+      <c r="H85" s="22">
+        <v>0</v>
+      </c>
+      <c r="I85" s="22">
+        <v>109</v>
+      </c>
+      <c r="J85" s="22">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="86" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A86" s="26">
+        <v>43986</v>
+      </c>
+      <c r="B86" s="27">
+        <v>82161</v>
+      </c>
+      <c r="C86" s="28">
+        <v>828</v>
+      </c>
+      <c r="D86" s="28">
+        <v>1479</v>
+      </c>
+      <c r="E86" s="28">
+        <v>2</v>
+      </c>
+      <c r="F86" s="28">
+        <v>6</v>
+      </c>
+      <c r="G86" s="28">
+        <v>0</v>
+      </c>
+      <c r="H86" s="28">
+        <v>0</v>
+      </c>
+      <c r="I86" s="28">
+        <v>109</v>
+      </c>
+      <c r="J86" s="28">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="87" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A87" s="29">
+        <v>43987</v>
+      </c>
+      <c r="B87" s="30">
+        <v>82876</v>
+      </c>
+      <c r="C87" s="31">
+        <v>715</v>
+      </c>
+      <c r="D87" s="31">
+        <v>1484</v>
+      </c>
+      <c r="E87" s="31">
+        <v>5</v>
+      </c>
+      <c r="F87" s="31">
+        <v>6</v>
+      </c>
+      <c r="G87" s="31">
+        <v>0</v>
+      </c>
+      <c r="H87" s="31">
+        <v>0</v>
+      </c>
+      <c r="I87" s="31">
+        <v>109</v>
+      </c>
+      <c r="J87" s="31">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="88" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A88" s="23">
+        <v>43988</v>
+      </c>
+      <c r="B88" s="24">
+        <v>83105</v>
+      </c>
+      <c r="C88" s="25">
+        <v>229</v>
+      </c>
+      <c r="D88" s="25">
+        <v>1485</v>
+      </c>
+      <c r="E88" s="25">
+        <v>1</v>
+      </c>
+      <c r="F88" s="25">
+        <v>5</v>
+      </c>
+      <c r="G88" s="25">
+        <v>0</v>
+      </c>
+      <c r="H88" s="25">
+        <v>1</v>
+      </c>
+      <c r="I88" s="25">
+        <v>109</v>
+      </c>
+      <c r="J88" s="25">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="89" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A89" s="29">
+        <v>43989</v>
+      </c>
+      <c r="B89" s="30">
+        <v>83316</v>
+      </c>
+      <c r="C89" s="31">
+        <v>211</v>
+      </c>
+      <c r="D89" s="31">
+        <v>1485</v>
+      </c>
+      <c r="E89" s="31">
+        <v>0</v>
+      </c>
+      <c r="F89" s="31">
+        <v>5</v>
+      </c>
+      <c r="G89" s="31">
+        <v>0</v>
+      </c>
+      <c r="H89" s="31">
+        <v>0</v>
+      </c>
+      <c r="I89" s="31">
+        <v>109</v>
+      </c>
+      <c r="J89" s="31">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="90" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A90" s="20">
+        <v>43990</v>
+      </c>
+      <c r="B90" s="21">
+        <v>84130</v>
+      </c>
+      <c r="C90" s="22">
+        <v>814</v>
+      </c>
+      <c r="D90" s="22">
+        <v>1486</v>
+      </c>
+      <c r="E90" s="22">
+        <v>1</v>
+      </c>
+      <c r="F90" s="22">
+        <v>6</v>
+      </c>
+      <c r="G90" s="22">
+        <v>0</v>
+      </c>
+      <c r="H90" s="22">
+        <v>0</v>
+      </c>
+      <c r="I90" s="22">
+        <v>109</v>
+      </c>
+      <c r="J90" s="22">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="91" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A91" s="20">
+        <v>43991</v>
+      </c>
+      <c r="B91" s="21">
+        <v>84868</v>
+      </c>
+      <c r="C91" s="22">
+        <v>738</v>
+      </c>
+      <c r="D91" s="22">
+        <v>1488</v>
+      </c>
+      <c r="E91" s="22">
+        <v>2</v>
+      </c>
+      <c r="F91" s="22">
+        <v>6</v>
+      </c>
+      <c r="G91" s="22">
+        <v>0</v>
+      </c>
+      <c r="H91" s="22">
+        <v>0</v>
+      </c>
+      <c r="I91" s="22">
+        <v>109</v>
+      </c>
+      <c r="J91" s="22">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="92" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A92" s="23">
+        <v>43992</v>
+      </c>
+      <c r="B92" s="24">
+        <v>85626</v>
+      </c>
+      <c r="C92" s="25">
+        <v>758</v>
+      </c>
+      <c r="D92" s="25">
+        <v>1488</v>
+      </c>
+      <c r="E92" s="25">
+        <v>0</v>
+      </c>
+      <c r="F92" s="25">
+        <v>6</v>
+      </c>
+      <c r="G92" s="25">
+        <v>0</v>
+      </c>
+      <c r="H92" s="25">
+        <v>0</v>
+      </c>
+      <c r="I92" s="25">
+        <v>109</v>
+      </c>
+      <c r="J92" s="25">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="93" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A93" s="29">
+        <v>43993</v>
+      </c>
+      <c r="B93" s="30">
+        <v>86328</v>
+      </c>
+      <c r="C93" s="31">
+        <v>702</v>
+      </c>
+      <c r="D93" s="31">
+        <v>1490</v>
+      </c>
+      <c r="E93" s="31">
+        <v>2</v>
+      </c>
+      <c r="F93" s="31">
+        <v>6</v>
+      </c>
+      <c r="G93" s="31">
+        <v>0</v>
+      </c>
+      <c r="H93" s="31">
+        <v>0</v>
+      </c>
+      <c r="I93" s="31">
+        <v>109</v>
+      </c>
+      <c r="J93" s="31">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="94" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A94" s="23">
+        <v>43994</v>
+      </c>
+      <c r="B94" s="24">
+        <v>87095</v>
+      </c>
+      <c r="C94" s="25">
+        <v>767</v>
+      </c>
+      <c r="D94" s="25">
+        <v>1492</v>
+      </c>
+      <c r="E94" s="25">
+        <v>2</v>
+      </c>
+      <c r="F94" s="25">
+        <v>6</v>
+      </c>
+      <c r="G94" s="25">
+        <v>0</v>
+      </c>
+      <c r="H94" s="25">
+        <v>0</v>
+      </c>
+      <c r="I94" s="25">
+        <v>109</v>
+      </c>
+      <c r="J94" s="25">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="95" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A95" s="29">
+        <v>43995</v>
+      </c>
+      <c r="B95" s="30">
+        <v>87386</v>
+      </c>
+      <c r="C95" s="31">
+        <v>291</v>
+      </c>
+      <c r="D95" s="31">
+        <v>1495</v>
+      </c>
+      <c r="E95" s="31">
+        <v>3</v>
+      </c>
+      <c r="F95" s="31">
+        <v>6</v>
+      </c>
+      <c r="G95" s="31">
+        <v>0</v>
+      </c>
+      <c r="H95" s="31">
+        <v>0</v>
+      </c>
+      <c r="I95" s="31">
+        <v>109</v>
+      </c>
+      <c r="J95" s="31">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="96" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A96" s="23">
+        <v>43996</v>
+      </c>
+      <c r="B96" s="24">
+        <v>87598</v>
+      </c>
+      <c r="C96" s="25">
+        <v>212</v>
+      </c>
+      <c r="D96" s="25">
+        <v>1496</v>
+      </c>
+      <c r="E96" s="25">
+        <v>1</v>
+      </c>
+      <c r="F96" s="25">
+        <v>7</v>
+      </c>
+      <c r="G96" s="25">
+        <v>1</v>
+      </c>
+      <c r="H96" s="25">
+        <v>0</v>
+      </c>
+      <c r="I96" s="25">
+        <v>109</v>
+      </c>
+      <c r="J96" s="25">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="97" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A97" s="20">
+        <v>43997</v>
+      </c>
+      <c r="B97" s="21">
+        <v>88165</v>
+      </c>
+      <c r="C97" s="22">
+        <v>567</v>
+      </c>
+      <c r="D97" s="22">
+        <v>1499</v>
+      </c>
+      <c r="E97" s="22">
+        <v>3</v>
+      </c>
+      <c r="F97" s="22">
+        <v>7</v>
+      </c>
+      <c r="G97" s="22">
+        <v>1</v>
+      </c>
+      <c r="H97" s="22">
+        <v>0</v>
+      </c>
+      <c r="I97" s="22">
+        <v>109</v>
+      </c>
+      <c r="J97" s="22">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="98" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A98" s="20">
+        <v>43998</v>
+      </c>
+      <c r="B98" s="21">
+        <v>89151</v>
+      </c>
+      <c r="C98" s="22">
+        <v>986</v>
+      </c>
+      <c r="D98" s="22">
+        <v>1503</v>
+      </c>
+      <c r="E98" s="22">
+        <v>4</v>
+      </c>
+      <c r="F98" s="22">
+        <v>7</v>
+      </c>
+      <c r="G98" s="22">
+        <v>1</v>
+      </c>
+      <c r="H98" s="22">
+        <v>0</v>
+      </c>
+      <c r="I98" s="22">
+        <v>109</v>
+      </c>
+      <c r="J98" s="22">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="99" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A99" s="29">
+        <v>43999</v>
+      </c>
+      <c r="B99" s="30">
+        <v>90103</v>
+      </c>
+      <c r="C99" s="31">
+        <v>952</v>
+      </c>
+      <c r="D99" s="31">
+        <v>1511</v>
+      </c>
+      <c r="E99" s="31">
+        <v>8</v>
+      </c>
+      <c r="F99" s="31">
+        <v>6</v>
+      </c>
+      <c r="G99" s="31">
+        <v>1</v>
+      </c>
+      <c r="H99" s="31">
+        <v>1</v>
+      </c>
+      <c r="I99" s="31">
+        <v>109</v>
+      </c>
+      <c r="J99" s="31">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="100" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A100" s="20">
+        <v>44000</v>
+      </c>
+      <c r="B100" s="21">
+        <v>91005</v>
+      </c>
+      <c r="C100" s="22">
+        <v>902</v>
+      </c>
+      <c r="D100" s="22">
+        <v>1513</v>
+      </c>
+      <c r="E100" s="22">
+        <v>2</v>
+      </c>
+      <c r="F100" s="22">
+        <v>8</v>
+      </c>
+      <c r="G100" s="22">
+        <v>1</v>
+      </c>
+      <c r="H100" s="22">
+        <v>0</v>
+      </c>
+      <c r="I100" s="22">
+        <v>109</v>
+      </c>
+      <c r="J100" s="22">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="101" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A101" s="29">
+        <v>44001</v>
+      </c>
+      <c r="B101" s="30">
+        <v>92152</v>
+      </c>
+      <c r="C101" s="31">
+        <v>1147</v>
+      </c>
+      <c r="D101" s="31">
+        <v>1519</v>
+      </c>
+      <c r="E101" s="31">
+        <v>6</v>
+      </c>
+      <c r="F101" s="31">
+        <v>6</v>
+      </c>
+      <c r="G101" s="31">
+        <v>1</v>
+      </c>
+      <c r="H101" s="31">
+        <v>2</v>
+      </c>
+      <c r="I101" s="31">
+        <v>109</v>
+      </c>
+      <c r="J101" s="31">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="102" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A102" s="23">
+        <v>44002</v>
+      </c>
+      <c r="B102" s="24">
+        <v>92919</v>
+      </c>
+      <c r="C102" s="25">
+        <v>758</v>
+      </c>
+      <c r="D102" s="25">
+        <v>1520</v>
+      </c>
+      <c r="E102" s="25">
+        <v>1</v>
+      </c>
+      <c r="F102" s="25">
+        <v>6</v>
+      </c>
+      <c r="G102" s="25">
+        <v>1</v>
+      </c>
+      <c r="H102" s="25">
+        <v>2</v>
+      </c>
+      <c r="I102" s="25">
+        <v>109</v>
+      </c>
+      <c r="J102" s="25">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="103" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A103" s="29">
+        <v>44003</v>
+      </c>
+      <c r="B103" s="30">
+        <v>93181</v>
+      </c>
+      <c r="C103" s="31">
+        <v>271</v>
+      </c>
+      <c r="D103" s="31">
+        <v>1521</v>
+      </c>
+      <c r="E103" s="31">
+        <v>1</v>
+      </c>
+      <c r="F103" s="31">
+        <v>6</v>
+      </c>
+      <c r="G103" s="31">
+        <v>1</v>
+      </c>
+      <c r="H103" s="31">
+        <v>0</v>
+      </c>
+      <c r="I103" s="31">
+        <v>109</v>
+      </c>
+      <c r="J103" s="31">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="104" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A104" s="29">
+        <v>44004</v>
+      </c>
+      <c r="B104" s="30">
+        <v>94165</v>
+      </c>
+      <c r="C104" s="31">
+        <v>984</v>
+      </c>
+      <c r="D104" s="31">
+        <v>1534</v>
+      </c>
+      <c r="E104" s="31">
+        <v>13</v>
+      </c>
+      <c r="F104" s="31">
+        <v>5</v>
+      </c>
+      <c r="G104" s="31">
+        <v>1</v>
+      </c>
+      <c r="H104" s="31">
+        <v>1</v>
+      </c>
+      <c r="I104" s="31">
+        <v>109</v>
+      </c>
+      <c r="J104" s="31">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="105" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A105" s="29">
+        <v>44005</v>
+      </c>
+      <c r="B105" s="30">
+        <v>95387</v>
+      </c>
+      <c r="C105" s="31">
+        <v>1222</v>
+      </c>
+      <c r="D105" s="31">
+        <v>1541</v>
+      </c>
+      <c r="E105" s="31">
+        <v>7</v>
+      </c>
+      <c r="F105" s="31">
+        <v>7</v>
+      </c>
+      <c r="G105" s="31">
+        <v>2</v>
+      </c>
+      <c r="H105" s="31">
+        <v>0</v>
+      </c>
+      <c r="I105" s="31" t="s">
+        <v>10</v>
+      </c>
+      <c r="J105" s="31">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="106" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A106" s="23">
+        <v>44006</v>
+      </c>
+      <c r="B106" s="24">
+        <v>96599</v>
+      </c>
+      <c r="C106" s="25">
+        <v>1212</v>
+      </c>
+      <c r="D106" s="25">
+        <v>1547</v>
+      </c>
+      <c r="E106" s="25">
+        <v>6</v>
+      </c>
+      <c r="F106" s="25">
+        <v>7</v>
+      </c>
+      <c r="G106" s="25">
+        <v>2</v>
+      </c>
+      <c r="H106" s="25">
+        <v>0</v>
+      </c>
+      <c r="I106" s="25" t="s">
+        <v>10</v>
+      </c>
+      <c r="J106" s="25">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="107" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A107" s="29">
+        <v>44007</v>
+      </c>
+      <c r="B107" s="30">
+        <v>97442</v>
+      </c>
+      <c r="C107" s="31">
+        <v>843</v>
+      </c>
+      <c r="D107" s="31">
+        <v>1558</v>
+      </c>
+      <c r="E107" s="31">
+        <v>11</v>
+      </c>
+      <c r="F107" s="31">
+        <v>8</v>
+      </c>
+      <c r="G107" s="31">
+        <v>2</v>
+      </c>
+      <c r="H107" s="31">
+        <v>0</v>
+      </c>
+      <c r="I107" s="31" t="s">
+        <v>10</v>
+      </c>
+      <c r="J107" s="31">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="108" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A108" s="29">
+        <v>44008</v>
+      </c>
+      <c r="B108" s="30">
+        <v>98320</v>
+      </c>
+      <c r="C108" s="31">
+        <v>878</v>
+      </c>
+      <c r="D108" s="31">
+        <v>1572</v>
+      </c>
+      <c r="E108" s="31">
+        <v>14</v>
+      </c>
+      <c r="F108" s="31">
+        <v>8</v>
+      </c>
+      <c r="G108" s="31">
+        <v>1</v>
+      </c>
+      <c r="H108" s="31">
+        <v>0</v>
+      </c>
+      <c r="I108" s="31" t="s">
+        <v>10</v>
+      </c>
+      <c r="J108" s="31">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="109" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A109" s="29">
+        <v>44009</v>
+      </c>
+      <c r="B109" s="30">
+        <v>98945</v>
+      </c>
+      <c r="C109" s="31">
+        <v>625</v>
+      </c>
+      <c r="D109" s="31">
+        <v>1581</v>
+      </c>
+      <c r="E109" s="31">
+        <v>9</v>
+      </c>
+      <c r="F109" s="31">
+        <v>7</v>
+      </c>
+      <c r="G109" s="31">
+        <v>0</v>
+      </c>
+      <c r="H109" s="31">
+        <v>1</v>
+      </c>
+      <c r="I109" s="31" t="s">
+        <v>10</v>
+      </c>
+      <c r="J109" s="31">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="110" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A110" s="29">
+        <v>44010</v>
+      </c>
+      <c r="B110" s="30">
+        <v>99245</v>
+      </c>
+      <c r="C110" s="31">
+        <v>300</v>
+      </c>
+      <c r="D110" s="31">
+        <v>1585</v>
+      </c>
+      <c r="E110" s="31">
+        <v>4</v>
+      </c>
+      <c r="F110" s="31">
+        <v>8</v>
+      </c>
+      <c r="G110" s="31">
+        <v>0</v>
+      </c>
+      <c r="H110" s="31">
+        <v>0</v>
+      </c>
+      <c r="I110" s="31" t="s">
+        <v>10</v>
+      </c>
+      <c r="J110" s="31">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="111" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A111" s="29">
+        <v>44011</v>
+      </c>
+      <c r="B111" s="30">
+        <v>100330</v>
+      </c>
+      <c r="C111" s="31">
+        <v>1085</v>
+      </c>
+      <c r="D111" s="31">
+        <v>1600</v>
+      </c>
+      <c r="E111" s="31">
+        <v>15</v>
+      </c>
+      <c r="F111" s="31">
+        <v>8</v>
+      </c>
+      <c r="G111" s="31">
+        <v>0</v>
+      </c>
+      <c r="H111" s="31">
+        <v>0</v>
+      </c>
+      <c r="I111" s="31" t="s">
+        <v>10</v>
+      </c>
+      <c r="J111" s="31">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="112" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A112" s="20">
+        <v>44012</v>
+      </c>
+      <c r="B112" s="21">
+        <v>101729</v>
+      </c>
+      <c r="C112" s="22">
+        <v>1399</v>
+      </c>
+      <c r="D112" s="22">
+        <v>1613</v>
+      </c>
+      <c r="E112" s="22">
+        <v>13</v>
+      </c>
+      <c r="F112" s="22">
+        <v>8</v>
+      </c>
+      <c r="G112" s="22">
+        <v>0</v>
+      </c>
+      <c r="H112" s="22">
+        <v>0</v>
+      </c>
+      <c r="I112" s="22" t="s">
+        <v>10</v>
+      </c>
+      <c r="J112" s="22">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="113" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A113" s="20">
+        <v>44013</v>
+      </c>
+      <c r="B113" s="21">
+        <v>102927</v>
+      </c>
+      <c r="C113" s="22">
+        <v>1198</v>
+      </c>
+      <c r="D113" s="22">
+        <v>1633</v>
+      </c>
+      <c r="E113" s="22">
+        <v>21</v>
+      </c>
+      <c r="F113" s="22">
+        <v>9</v>
+      </c>
+      <c r="G113" s="22">
+        <v>0</v>
+      </c>
+      <c r="H113" s="22">
+        <v>0</v>
+      </c>
+      <c r="I113" s="22" t="s">
+        <v>10</v>
+      </c>
+      <c r="J113" s="22">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="114" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A114" s="20">
+        <v>44014</v>
+      </c>
+      <c r="B114" s="21">
+        <v>104201</v>
+      </c>
+      <c r="C114" s="22">
+        <v>1274</v>
+      </c>
+      <c r="D114" s="22">
+        <v>1649</v>
+      </c>
+      <c r="E114" s="22">
+        <v>16</v>
+      </c>
+      <c r="F114" s="22">
+        <v>10</v>
+      </c>
+      <c r="G114" s="22">
+        <v>0</v>
+      </c>
+      <c r="H114" s="22">
+        <v>0</v>
+      </c>
+      <c r="I114" s="22" t="s">
+        <v>10</v>
+      </c>
+      <c r="J114" s="22">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="115" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A115" s="20">
+        <v>44015</v>
+      </c>
+      <c r="B115" s="21">
+        <v>105652</v>
+      </c>
+      <c r="C115" s="22">
+        <v>1456</v>
+      </c>
+      <c r="D115" s="22">
+        <v>1679</v>
+      </c>
+      <c r="E115" s="22">
+        <v>30</v>
+      </c>
+      <c r="F115" s="22">
+        <v>6</v>
+      </c>
+      <c r="G115" s="22">
+        <v>0</v>
+      </c>
+      <c r="H115" s="22">
+        <v>4</v>
+      </c>
+      <c r="I115" s="22" t="s">
+        <v>10</v>
+      </c>
+      <c r="J115" s="22">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="116" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A116" s="20">
+        <v>44016</v>
+      </c>
+      <c r="B116" s="21">
+        <v>106368</v>
+      </c>
+      <c r="C116" s="22">
+        <v>716</v>
+      </c>
+      <c r="D116" s="22">
+        <v>1700</v>
+      </c>
+      <c r="E116" s="22">
+        <v>21</v>
+      </c>
+      <c r="F116" s="22">
+        <v>6</v>
+      </c>
+      <c r="G116" s="22">
+        <v>0</v>
+      </c>
+      <c r="H116" s="22">
+        <v>1</v>
+      </c>
+      <c r="I116" s="22" t="s">
+        <v>10</v>
+      </c>
+      <c r="J116" s="22">
+        <v>0</v>
+      </c>
+    </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>

</xml_diff>

<commit_message>
Data updated by GitHub Bot (2020-07-05 20)
</commit_message>
<xml_diff>
--- a/output/snapshot/fdcf2531-4c3e-5c02-b63c-ee160ead6dea.xlsx
+++ b/output/snapshot/fdcf2531-4c3e-5c02-b63c-ee160ead6dea.xlsx
@@ -1,16 +1,15 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="21929"/>
-  <workbookPr/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
+  <fileVersion appName="xl" lastEdited="6" lowestEdited="6" rupBuild="14420"/>
+  <workbookPr defaultThemeVersion="164011"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="I:\AKTUALNI PODATKI - KORONA\Za objavo na GOV.SI\ang\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{1E6DD62F-2BE2-47DC-A7ED-9B57C1589256}" xr6:coauthVersionLast="44" xr6:coauthVersionMax="44" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840"/>
   </bookViews>
   <sheets>
     <sheet name="Covid-19 podatki" sheetId="1" r:id="rId1"/>
@@ -25,7 +24,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="10" uniqueCount="10">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="22" uniqueCount="11">
   <si>
     <t>Date</t>
   </si>
@@ -56,15 +55,18 @@
   <si>
     <t>Deaths (daily)</t>
   </si>
+  <si>
+    <t>111*</t>
+  </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" mc:Ignorable="x14ac x16r2">
   <numFmts count="1">
     <numFmt numFmtId="164" formatCode="d/\ m/\ yyyy;@"/>
   </numFmts>
-  <fonts count="4" x14ac:knownFonts="1">
+  <fonts count="5" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -93,6 +95,13 @@
       <name val="Calibri Light"/>
       <scheme val="major"/>
     </font>
+    <font>
+      <sz val="10"/>
+      <color theme="1"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
   </fonts>
   <fills count="3">
     <fill>
@@ -108,7 +117,7 @@
       </patternFill>
     </fill>
   </fills>
-  <borders count="2">
+  <borders count="3">
     <border>
       <left/>
       <right/>
@@ -129,11 +138,26 @@
       <bottom/>
       <diagonal/>
     </border>
+    <border>
+      <left style="thin">
+        <color theme="4"/>
+      </left>
+      <right style="thin">
+        <color theme="4"/>
+      </right>
+      <top style="thin">
+        <color theme="4"/>
+      </top>
+      <bottom style="thin">
+        <color theme="4"/>
+      </bottom>
+      <diagonal/>
+    </border>
   </borders>
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="26">
+  <cellXfs count="32">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="49" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyAlignment="1" applyProtection="1">
       <alignment horizontal="left" vertical="top"/>
@@ -208,6 +232,24 @@
       <alignment horizontal="right"/>
     </xf>
     <xf numFmtId="0" fontId="3" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="right"/>
+    </xf>
+    <xf numFmtId="164" fontId="4" fillId="2" borderId="2" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="right" vertical="top"/>
+    </xf>
+    <xf numFmtId="3" fontId="4" fillId="2" borderId="2" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="right"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="2" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="right"/>
+    </xf>
+    <xf numFmtId="164" fontId="3" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="right" vertical="top"/>
+    </xf>
+    <xf numFmtId="3" fontId="3" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="right"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="right"/>
     </xf>
   </cellXfs>
@@ -399,8 +441,8 @@
 </file>
 
 <file path=xl/tables/table1.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="1" xr:uid="{00000000-000C-0000-FFFF-FFFF00000000}" name="Tabela1" displayName="Tabela1" ref="A1:J75" totalsRowShown="0" headerRowDxfId="11" dataDxfId="10">
-  <autoFilter ref="A1:J75" xr:uid="{00000000-0009-0000-0100-000001000000}">
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="1" name="Tabela1" displayName="Tabela1" ref="A1:J116" totalsRowShown="0" headerRowDxfId="11" dataDxfId="10">
+  <autoFilter ref="A1:J116">
     <filterColumn colId="0" hiddenButton="1"/>
     <filterColumn colId="1" hiddenButton="1"/>
     <filterColumn colId="2" hiddenButton="1"/>
@@ -413,16 +455,16 @@
     <filterColumn colId="9" hiddenButton="1"/>
   </autoFilter>
   <tableColumns count="10">
-    <tableColumn id="1" xr3:uid="{00000000-0010-0000-0000-000001000000}" name="Date" dataDxfId="9"/>
-    <tableColumn id="2" xr3:uid="{00000000-0010-0000-0000-000002000000}" name="Tested (all)" dataDxfId="8"/>
-    <tableColumn id="3" xr3:uid="{00000000-0010-0000-0000-000003000000}" name="Tested (daily)" dataDxfId="7"/>
-    <tableColumn id="4" xr3:uid="{00000000-0010-0000-0000-000004000000}" name="Positive (all)" dataDxfId="6"/>
-    <tableColumn id="5" xr3:uid="{00000000-0010-0000-0000-000005000000}" name="Positive (daily)" dataDxfId="5"/>
-    <tableColumn id="6" xr3:uid="{00000000-0010-0000-0000-000006000000}" name="All hospitalized on certain day" dataDxfId="4"/>
-    <tableColumn id="7" xr3:uid="{00000000-0010-0000-0000-000007000000}" name="All persons in intensive care on certain day" dataDxfId="3"/>
-    <tableColumn id="10" xr3:uid="{00000000-0010-0000-0000-00000A000000}" name="Discharged" dataDxfId="2"/>
-    <tableColumn id="8" xr3:uid="{00000000-0010-0000-0000-000008000000}" name="Deaths (all)" dataDxfId="1"/>
-    <tableColumn id="9" xr3:uid="{00000000-0010-0000-0000-000009000000}" name="Deaths (daily)" dataDxfId="0"/>
+    <tableColumn id="1" name="Date" dataDxfId="9"/>
+    <tableColumn id="2" name="Tested (all)" dataDxfId="8"/>
+    <tableColumn id="3" name="Tested (daily)" dataDxfId="7"/>
+    <tableColumn id="4" name="Positive (all)" dataDxfId="6"/>
+    <tableColumn id="5" name="Positive (daily)" dataDxfId="5"/>
+    <tableColumn id="6" name="All hospitalized on certain day" dataDxfId="4"/>
+    <tableColumn id="7" name="All persons in intensive care on certain day" dataDxfId="3"/>
+    <tableColumn id="10" name="Discharged" dataDxfId="2"/>
+    <tableColumn id="8" name="Deaths (all)" dataDxfId="1"/>
+    <tableColumn id="9" name="Deaths (daily)" dataDxfId="0"/>
   </tableColumns>
   <tableStyleInfo name="TableStyleLight16" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
   <extLst>
@@ -695,11 +737,11 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:J75"/>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <dimension ref="A1:J116"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A40" zoomScale="89" zoomScaleNormal="89" workbookViewId="0">
-      <selection activeCell="J74" sqref="J74"/>
+    <sheetView tabSelected="1" topLeftCell="A83" zoomScale="89" zoomScaleNormal="89" workbookViewId="0">
+      <selection activeCell="H116" sqref="H116"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -3117,6 +3159,1318 @@
         <v>0</v>
       </c>
     </row>
+    <row r="76" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A76" s="20">
+        <v>43976</v>
+      </c>
+      <c r="B76" s="21">
+        <v>75770</v>
+      </c>
+      <c r="C76" s="22">
+        <v>754</v>
+      </c>
+      <c r="D76" s="22">
+        <v>1469</v>
+      </c>
+      <c r="E76" s="22">
+        <v>0</v>
+      </c>
+      <c r="F76" s="22">
+        <v>9</v>
+      </c>
+      <c r="G76" s="22">
+        <v>2</v>
+      </c>
+      <c r="H76" s="22">
+        <v>6</v>
+      </c>
+      <c r="I76" s="22">
+        <v>108</v>
+      </c>
+      <c r="J76" s="22">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="77" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A77" s="20">
+        <v>43977</v>
+      </c>
+      <c r="B77" s="21">
+        <v>76579</v>
+      </c>
+      <c r="C77" s="22">
+        <v>809</v>
+      </c>
+      <c r="D77" s="22">
+        <v>1471</v>
+      </c>
+      <c r="E77" s="22">
+        <v>2</v>
+      </c>
+      <c r="F77" s="22">
+        <v>8</v>
+      </c>
+      <c r="G77" s="22">
+        <v>2</v>
+      </c>
+      <c r="H77" s="22">
+        <v>2</v>
+      </c>
+      <c r="I77" s="22">
+        <v>108</v>
+      </c>
+      <c r="J77" s="22">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="78" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A78" s="20">
+        <v>43978</v>
+      </c>
+      <c r="B78" s="21">
+        <v>77210</v>
+      </c>
+      <c r="C78" s="22">
+        <v>631</v>
+      </c>
+      <c r="D78" s="22">
+        <v>1473</v>
+      </c>
+      <c r="E78" s="22">
+        <v>2</v>
+      </c>
+      <c r="F78" s="22">
+        <v>7</v>
+      </c>
+      <c r="G78" s="22">
+        <v>2</v>
+      </c>
+      <c r="H78" s="22">
+        <v>1</v>
+      </c>
+      <c r="I78" s="22">
+        <v>108</v>
+      </c>
+      <c r="J78" s="22">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="79" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A79" s="20">
+        <v>43979</v>
+      </c>
+      <c r="B79" s="21">
+        <v>77916</v>
+      </c>
+      <c r="C79" s="22">
+        <v>706</v>
+      </c>
+      <c r="D79" s="22">
+        <v>1473</v>
+      </c>
+      <c r="E79" s="22">
+        <v>0</v>
+      </c>
+      <c r="F79" s="22">
+        <v>7</v>
+      </c>
+      <c r="G79" s="22">
+        <v>2</v>
+      </c>
+      <c r="H79" s="22">
+        <v>0</v>
+      </c>
+      <c r="I79" s="22">
+        <v>108</v>
+      </c>
+      <c r="J79" s="22">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="80" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A80" s="20">
+        <v>43980</v>
+      </c>
+      <c r="B80" s="21">
+        <v>78529</v>
+      </c>
+      <c r="C80" s="22">
+        <v>613</v>
+      </c>
+      <c r="D80" s="22">
+        <v>1473</v>
+      </c>
+      <c r="E80" s="22">
+        <v>0</v>
+      </c>
+      <c r="F80" s="22">
+        <v>7</v>
+      </c>
+      <c r="G80" s="22">
+        <v>2</v>
+      </c>
+      <c r="H80" s="22">
+        <v>0</v>
+      </c>
+      <c r="I80" s="22">
+        <v>108</v>
+      </c>
+      <c r="J80" s="22">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="81" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A81" s="20">
+        <v>43981</v>
+      </c>
+      <c r="B81" s="22">
+        <v>78793</v>
+      </c>
+      <c r="C81" s="22">
+        <v>264</v>
+      </c>
+      <c r="D81" s="22">
+        <v>1473</v>
+      </c>
+      <c r="E81" s="22">
+        <v>0</v>
+      </c>
+      <c r="F81" s="22">
+        <v>6</v>
+      </c>
+      <c r="G81" s="22">
+        <v>2</v>
+      </c>
+      <c r="H81" s="22">
+        <v>1</v>
+      </c>
+      <c r="I81" s="22">
+        <v>108</v>
+      </c>
+      <c r="J81" s="22">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="82" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A82" s="20">
+        <v>43982</v>
+      </c>
+      <c r="B82" s="21">
+        <v>79039</v>
+      </c>
+      <c r="C82" s="22">
+        <v>246</v>
+      </c>
+      <c r="D82" s="22">
+        <v>1473</v>
+      </c>
+      <c r="E82" s="22">
+        <v>0</v>
+      </c>
+      <c r="F82" s="22">
+        <v>5</v>
+      </c>
+      <c r="G82" s="22">
+        <v>1</v>
+      </c>
+      <c r="H82" s="22">
+        <v>0</v>
+      </c>
+      <c r="I82" s="22">
+        <v>109</v>
+      </c>
+      <c r="J82" s="22">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="83" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A83" s="20">
+        <v>43983</v>
+      </c>
+      <c r="B83" s="21">
+        <v>79698</v>
+      </c>
+      <c r="C83" s="22">
+        <v>659</v>
+      </c>
+      <c r="D83" s="22">
+        <v>1475</v>
+      </c>
+      <c r="E83" s="22">
+        <v>2</v>
+      </c>
+      <c r="F83" s="22">
+        <v>5</v>
+      </c>
+      <c r="G83" s="22">
+        <v>1</v>
+      </c>
+      <c r="H83" s="22">
+        <v>0</v>
+      </c>
+      <c r="I83" s="22">
+        <v>109</v>
+      </c>
+      <c r="J83" s="22">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="84" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A84" s="20">
+        <v>43984</v>
+      </c>
+      <c r="B84" s="21">
+        <v>80505</v>
+      </c>
+      <c r="C84" s="22">
+        <v>807</v>
+      </c>
+      <c r="D84" s="22">
+        <v>1477</v>
+      </c>
+      <c r="E84" s="22">
+        <v>2</v>
+      </c>
+      <c r="F84" s="22">
+        <v>5</v>
+      </c>
+      <c r="G84" s="22">
+        <v>0</v>
+      </c>
+      <c r="H84" s="22">
+        <v>0</v>
+      </c>
+      <c r="I84" s="22">
+        <v>109</v>
+      </c>
+      <c r="J84" s="22">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="85" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A85" s="20">
+        <v>43985</v>
+      </c>
+      <c r="B85" s="21">
+        <v>81333</v>
+      </c>
+      <c r="C85" s="22">
+        <v>828</v>
+      </c>
+      <c r="D85" s="22">
+        <v>1477</v>
+      </c>
+      <c r="E85" s="22">
+        <v>0</v>
+      </c>
+      <c r="F85" s="22">
+        <v>5</v>
+      </c>
+      <c r="G85" s="22">
+        <v>0</v>
+      </c>
+      <c r="H85" s="22">
+        <v>0</v>
+      </c>
+      <c r="I85" s="22">
+        <v>109</v>
+      </c>
+      <c r="J85" s="22">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="86" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A86" s="26">
+        <v>43986</v>
+      </c>
+      <c r="B86" s="27">
+        <v>82161</v>
+      </c>
+      <c r="C86" s="28">
+        <v>828</v>
+      </c>
+      <c r="D86" s="28">
+        <v>1479</v>
+      </c>
+      <c r="E86" s="28">
+        <v>2</v>
+      </c>
+      <c r="F86" s="28">
+        <v>6</v>
+      </c>
+      <c r="G86" s="28">
+        <v>0</v>
+      </c>
+      <c r="H86" s="28">
+        <v>0</v>
+      </c>
+      <c r="I86" s="28">
+        <v>109</v>
+      </c>
+      <c r="J86" s="28">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="87" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A87" s="29">
+        <v>43987</v>
+      </c>
+      <c r="B87" s="30">
+        <v>82876</v>
+      </c>
+      <c r="C87" s="31">
+        <v>715</v>
+      </c>
+      <c r="D87" s="31">
+        <v>1484</v>
+      </c>
+      <c r="E87" s="31">
+        <v>5</v>
+      </c>
+      <c r="F87" s="31">
+        <v>6</v>
+      </c>
+      <c r="G87" s="31">
+        <v>0</v>
+      </c>
+      <c r="H87" s="31">
+        <v>0</v>
+      </c>
+      <c r="I87" s="31">
+        <v>109</v>
+      </c>
+      <c r="J87" s="31">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="88" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A88" s="23">
+        <v>43988</v>
+      </c>
+      <c r="B88" s="24">
+        <v>83105</v>
+      </c>
+      <c r="C88" s="25">
+        <v>229</v>
+      </c>
+      <c r="D88" s="25">
+        <v>1485</v>
+      </c>
+      <c r="E88" s="25">
+        <v>1</v>
+      </c>
+      <c r="F88" s="25">
+        <v>5</v>
+      </c>
+      <c r="G88" s="25">
+        <v>0</v>
+      </c>
+      <c r="H88" s="25">
+        <v>1</v>
+      </c>
+      <c r="I88" s="25">
+        <v>109</v>
+      </c>
+      <c r="J88" s="25">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="89" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A89" s="29">
+        <v>43989</v>
+      </c>
+      <c r="B89" s="30">
+        <v>83316</v>
+      </c>
+      <c r="C89" s="31">
+        <v>211</v>
+      </c>
+      <c r="D89" s="31">
+        <v>1485</v>
+      </c>
+      <c r="E89" s="31">
+        <v>0</v>
+      </c>
+      <c r="F89" s="31">
+        <v>5</v>
+      </c>
+      <c r="G89" s="31">
+        <v>0</v>
+      </c>
+      <c r="H89" s="31">
+        <v>0</v>
+      </c>
+      <c r="I89" s="31">
+        <v>109</v>
+      </c>
+      <c r="J89" s="31">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="90" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A90" s="20">
+        <v>43990</v>
+      </c>
+      <c r="B90" s="21">
+        <v>84130</v>
+      </c>
+      <c r="C90" s="22">
+        <v>814</v>
+      </c>
+      <c r="D90" s="22">
+        <v>1486</v>
+      </c>
+      <c r="E90" s="22">
+        <v>1</v>
+      </c>
+      <c r="F90" s="22">
+        <v>6</v>
+      </c>
+      <c r="G90" s="22">
+        <v>0</v>
+      </c>
+      <c r="H90" s="22">
+        <v>0</v>
+      </c>
+      <c r="I90" s="22">
+        <v>109</v>
+      </c>
+      <c r="J90" s="22">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="91" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A91" s="20">
+        <v>43991</v>
+      </c>
+      <c r="B91" s="21">
+        <v>84868</v>
+      </c>
+      <c r="C91" s="22">
+        <v>738</v>
+      </c>
+      <c r="D91" s="22">
+        <v>1488</v>
+      </c>
+      <c r="E91" s="22">
+        <v>2</v>
+      </c>
+      <c r="F91" s="22">
+        <v>6</v>
+      </c>
+      <c r="G91" s="22">
+        <v>0</v>
+      </c>
+      <c r="H91" s="22">
+        <v>0</v>
+      </c>
+      <c r="I91" s="22">
+        <v>109</v>
+      </c>
+      <c r="J91" s="22">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="92" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A92" s="23">
+        <v>43992</v>
+      </c>
+      <c r="B92" s="24">
+        <v>85626</v>
+      </c>
+      <c r="C92" s="25">
+        <v>758</v>
+      </c>
+      <c r="D92" s="25">
+        <v>1488</v>
+      </c>
+      <c r="E92" s="25">
+        <v>0</v>
+      </c>
+      <c r="F92" s="25">
+        <v>6</v>
+      </c>
+      <c r="G92" s="25">
+        <v>0</v>
+      </c>
+      <c r="H92" s="25">
+        <v>0</v>
+      </c>
+      <c r="I92" s="25">
+        <v>109</v>
+      </c>
+      <c r="J92" s="25">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="93" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A93" s="29">
+        <v>43993</v>
+      </c>
+      <c r="B93" s="30">
+        <v>86328</v>
+      </c>
+      <c r="C93" s="31">
+        <v>702</v>
+      </c>
+      <c r="D93" s="31">
+        <v>1490</v>
+      </c>
+      <c r="E93" s="31">
+        <v>2</v>
+      </c>
+      <c r="F93" s="31">
+        <v>6</v>
+      </c>
+      <c r="G93" s="31">
+        <v>0</v>
+      </c>
+      <c r="H93" s="31">
+        <v>0</v>
+      </c>
+      <c r="I93" s="31">
+        <v>109</v>
+      </c>
+      <c r="J93" s="31">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="94" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A94" s="23">
+        <v>43994</v>
+      </c>
+      <c r="B94" s="24">
+        <v>87095</v>
+      </c>
+      <c r="C94" s="25">
+        <v>767</v>
+      </c>
+      <c r="D94" s="25">
+        <v>1492</v>
+      </c>
+      <c r="E94" s="25">
+        <v>2</v>
+      </c>
+      <c r="F94" s="25">
+        <v>6</v>
+      </c>
+      <c r="G94" s="25">
+        <v>0</v>
+      </c>
+      <c r="H94" s="25">
+        <v>0</v>
+      </c>
+      <c r="I94" s="25">
+        <v>109</v>
+      </c>
+      <c r="J94" s="25">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="95" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A95" s="29">
+        <v>43995</v>
+      </c>
+      <c r="B95" s="30">
+        <v>87386</v>
+      </c>
+      <c r="C95" s="31">
+        <v>291</v>
+      </c>
+      <c r="D95" s="31">
+        <v>1495</v>
+      </c>
+      <c r="E95" s="31">
+        <v>3</v>
+      </c>
+      <c r="F95" s="31">
+        <v>6</v>
+      </c>
+      <c r="G95" s="31">
+        <v>0</v>
+      </c>
+      <c r="H95" s="31">
+        <v>0</v>
+      </c>
+      <c r="I95" s="31">
+        <v>109</v>
+      </c>
+      <c r="J95" s="31">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="96" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A96" s="23">
+        <v>43996</v>
+      </c>
+      <c r="B96" s="24">
+        <v>87598</v>
+      </c>
+      <c r="C96" s="25">
+        <v>212</v>
+      </c>
+      <c r="D96" s="25">
+        <v>1496</v>
+      </c>
+      <c r="E96" s="25">
+        <v>1</v>
+      </c>
+      <c r="F96" s="25">
+        <v>7</v>
+      </c>
+      <c r="G96" s="25">
+        <v>1</v>
+      </c>
+      <c r="H96" s="25">
+        <v>0</v>
+      </c>
+      <c r="I96" s="25">
+        <v>109</v>
+      </c>
+      <c r="J96" s="25">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="97" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A97" s="20">
+        <v>43997</v>
+      </c>
+      <c r="B97" s="21">
+        <v>88165</v>
+      </c>
+      <c r="C97" s="22">
+        <v>567</v>
+      </c>
+      <c r="D97" s="22">
+        <v>1499</v>
+      </c>
+      <c r="E97" s="22">
+        <v>3</v>
+      </c>
+      <c r="F97" s="22">
+        <v>7</v>
+      </c>
+      <c r="G97" s="22">
+        <v>1</v>
+      </c>
+      <c r="H97" s="22">
+        <v>0</v>
+      </c>
+      <c r="I97" s="22">
+        <v>109</v>
+      </c>
+      <c r="J97" s="22">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="98" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A98" s="20">
+        <v>43998</v>
+      </c>
+      <c r="B98" s="21">
+        <v>89151</v>
+      </c>
+      <c r="C98" s="22">
+        <v>986</v>
+      </c>
+      <c r="D98" s="22">
+        <v>1503</v>
+      </c>
+      <c r="E98" s="22">
+        <v>4</v>
+      </c>
+      <c r="F98" s="22">
+        <v>7</v>
+      </c>
+      <c r="G98" s="22">
+        <v>1</v>
+      </c>
+      <c r="H98" s="22">
+        <v>0</v>
+      </c>
+      <c r="I98" s="22">
+        <v>109</v>
+      </c>
+      <c r="J98" s="22">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="99" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A99" s="29">
+        <v>43999</v>
+      </c>
+      <c r="B99" s="30">
+        <v>90103</v>
+      </c>
+      <c r="C99" s="31">
+        <v>952</v>
+      </c>
+      <c r="D99" s="31">
+        <v>1511</v>
+      </c>
+      <c r="E99" s="31">
+        <v>8</v>
+      </c>
+      <c r="F99" s="31">
+        <v>6</v>
+      </c>
+      <c r="G99" s="31">
+        <v>1</v>
+      </c>
+      <c r="H99" s="31">
+        <v>1</v>
+      </c>
+      <c r="I99" s="31">
+        <v>109</v>
+      </c>
+      <c r="J99" s="31">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="100" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A100" s="20">
+        <v>44000</v>
+      </c>
+      <c r="B100" s="21">
+        <v>91005</v>
+      </c>
+      <c r="C100" s="22">
+        <v>902</v>
+      </c>
+      <c r="D100" s="22">
+        <v>1513</v>
+      </c>
+      <c r="E100" s="22">
+        <v>2</v>
+      </c>
+      <c r="F100" s="22">
+        <v>8</v>
+      </c>
+      <c r="G100" s="22">
+        <v>1</v>
+      </c>
+      <c r="H100" s="22">
+        <v>0</v>
+      </c>
+      <c r="I100" s="22">
+        <v>109</v>
+      </c>
+      <c r="J100" s="22">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="101" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A101" s="29">
+        <v>44001</v>
+      </c>
+      <c r="B101" s="30">
+        <v>92152</v>
+      </c>
+      <c r="C101" s="31">
+        <v>1147</v>
+      </c>
+      <c r="D101" s="31">
+        <v>1519</v>
+      </c>
+      <c r="E101" s="31">
+        <v>6</v>
+      </c>
+      <c r="F101" s="31">
+        <v>6</v>
+      </c>
+      <c r="G101" s="31">
+        <v>1</v>
+      </c>
+      <c r="H101" s="31">
+        <v>2</v>
+      </c>
+      <c r="I101" s="31">
+        <v>109</v>
+      </c>
+      <c r="J101" s="31">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="102" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A102" s="23">
+        <v>44002</v>
+      </c>
+      <c r="B102" s="24">
+        <v>92919</v>
+      </c>
+      <c r="C102" s="25">
+        <v>758</v>
+      </c>
+      <c r="D102" s="25">
+        <v>1520</v>
+      </c>
+      <c r="E102" s="25">
+        <v>1</v>
+      </c>
+      <c r="F102" s="25">
+        <v>6</v>
+      </c>
+      <c r="G102" s="25">
+        <v>1</v>
+      </c>
+      <c r="H102" s="25">
+        <v>2</v>
+      </c>
+      <c r="I102" s="25">
+        <v>109</v>
+      </c>
+      <c r="J102" s="25">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="103" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A103" s="29">
+        <v>44003</v>
+      </c>
+      <c r="B103" s="30">
+        <v>93181</v>
+      </c>
+      <c r="C103" s="31">
+        <v>271</v>
+      </c>
+      <c r="D103" s="31">
+        <v>1521</v>
+      </c>
+      <c r="E103" s="31">
+        <v>1</v>
+      </c>
+      <c r="F103" s="31">
+        <v>6</v>
+      </c>
+      <c r="G103" s="31">
+        <v>1</v>
+      </c>
+      <c r="H103" s="31">
+        <v>0</v>
+      </c>
+      <c r="I103" s="31">
+        <v>109</v>
+      </c>
+      <c r="J103" s="31">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="104" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A104" s="29">
+        <v>44004</v>
+      </c>
+      <c r="B104" s="30">
+        <v>94165</v>
+      </c>
+      <c r="C104" s="31">
+        <v>984</v>
+      </c>
+      <c r="D104" s="31">
+        <v>1534</v>
+      </c>
+      <c r="E104" s="31">
+        <v>13</v>
+      </c>
+      <c r="F104" s="31">
+        <v>5</v>
+      </c>
+      <c r="G104" s="31">
+        <v>1</v>
+      </c>
+      <c r="H104" s="31">
+        <v>1</v>
+      </c>
+      <c r="I104" s="31">
+        <v>109</v>
+      </c>
+      <c r="J104" s="31">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="105" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A105" s="29">
+        <v>44005</v>
+      </c>
+      <c r="B105" s="30">
+        <v>95387</v>
+      </c>
+      <c r="C105" s="31">
+        <v>1222</v>
+      </c>
+      <c r="D105" s="31">
+        <v>1541</v>
+      </c>
+      <c r="E105" s="31">
+        <v>7</v>
+      </c>
+      <c r="F105" s="31">
+        <v>7</v>
+      </c>
+      <c r="G105" s="31">
+        <v>2</v>
+      </c>
+      <c r="H105" s="31">
+        <v>0</v>
+      </c>
+      <c r="I105" s="31" t="s">
+        <v>10</v>
+      </c>
+      <c r="J105" s="31">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="106" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A106" s="23">
+        <v>44006</v>
+      </c>
+      <c r="B106" s="24">
+        <v>96599</v>
+      </c>
+      <c r="C106" s="25">
+        <v>1212</v>
+      </c>
+      <c r="D106" s="25">
+        <v>1547</v>
+      </c>
+      <c r="E106" s="25">
+        <v>6</v>
+      </c>
+      <c r="F106" s="25">
+        <v>7</v>
+      </c>
+      <c r="G106" s="25">
+        <v>2</v>
+      </c>
+      <c r="H106" s="25">
+        <v>0</v>
+      </c>
+      <c r="I106" s="25" t="s">
+        <v>10</v>
+      </c>
+      <c r="J106" s="25">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="107" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A107" s="29">
+        <v>44007</v>
+      </c>
+      <c r="B107" s="30">
+        <v>97442</v>
+      </c>
+      <c r="C107" s="31">
+        <v>843</v>
+      </c>
+      <c r="D107" s="31">
+        <v>1558</v>
+      </c>
+      <c r="E107" s="31">
+        <v>11</v>
+      </c>
+      <c r="F107" s="31">
+        <v>8</v>
+      </c>
+      <c r="G107" s="31">
+        <v>2</v>
+      </c>
+      <c r="H107" s="31">
+        <v>0</v>
+      </c>
+      <c r="I107" s="31" t="s">
+        <v>10</v>
+      </c>
+      <c r="J107" s="31">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="108" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A108" s="29">
+        <v>44008</v>
+      </c>
+      <c r="B108" s="30">
+        <v>98320</v>
+      </c>
+      <c r="C108" s="31">
+        <v>878</v>
+      </c>
+      <c r="D108" s="31">
+        <v>1572</v>
+      </c>
+      <c r="E108" s="31">
+        <v>14</v>
+      </c>
+      <c r="F108" s="31">
+        <v>8</v>
+      </c>
+      <c r="G108" s="31">
+        <v>1</v>
+      </c>
+      <c r="H108" s="31">
+        <v>0</v>
+      </c>
+      <c r="I108" s="31" t="s">
+        <v>10</v>
+      </c>
+      <c r="J108" s="31">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="109" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A109" s="29">
+        <v>44009</v>
+      </c>
+      <c r="B109" s="30">
+        <v>98945</v>
+      </c>
+      <c r="C109" s="31">
+        <v>625</v>
+      </c>
+      <c r="D109" s="31">
+        <v>1581</v>
+      </c>
+      <c r="E109" s="31">
+        <v>9</v>
+      </c>
+      <c r="F109" s="31">
+        <v>7</v>
+      </c>
+      <c r="G109" s="31">
+        <v>0</v>
+      </c>
+      <c r="H109" s="31">
+        <v>1</v>
+      </c>
+      <c r="I109" s="31" t="s">
+        <v>10</v>
+      </c>
+      <c r="J109" s="31">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="110" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A110" s="29">
+        <v>44010</v>
+      </c>
+      <c r="B110" s="30">
+        <v>99245</v>
+      </c>
+      <c r="C110" s="31">
+        <v>300</v>
+      </c>
+      <c r="D110" s="31">
+        <v>1585</v>
+      </c>
+      <c r="E110" s="31">
+        <v>4</v>
+      </c>
+      <c r="F110" s="31">
+        <v>8</v>
+      </c>
+      <c r="G110" s="31">
+        <v>0</v>
+      </c>
+      <c r="H110" s="31">
+        <v>0</v>
+      </c>
+      <c r="I110" s="31" t="s">
+        <v>10</v>
+      </c>
+      <c r="J110" s="31">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="111" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A111" s="29">
+        <v>44011</v>
+      </c>
+      <c r="B111" s="30">
+        <v>100330</v>
+      </c>
+      <c r="C111" s="31">
+        <v>1085</v>
+      </c>
+      <c r="D111" s="31">
+        <v>1600</v>
+      </c>
+      <c r="E111" s="31">
+        <v>15</v>
+      </c>
+      <c r="F111" s="31">
+        <v>8</v>
+      </c>
+      <c r="G111" s="31">
+        <v>0</v>
+      </c>
+      <c r="H111" s="31">
+        <v>0</v>
+      </c>
+      <c r="I111" s="31" t="s">
+        <v>10</v>
+      </c>
+      <c r="J111" s="31">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="112" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A112" s="20">
+        <v>44012</v>
+      </c>
+      <c r="B112" s="21">
+        <v>101729</v>
+      </c>
+      <c r="C112" s="22">
+        <v>1399</v>
+      </c>
+      <c r="D112" s="22">
+        <v>1613</v>
+      </c>
+      <c r="E112" s="22">
+        <v>13</v>
+      </c>
+      <c r="F112" s="22">
+        <v>8</v>
+      </c>
+      <c r="G112" s="22">
+        <v>0</v>
+      </c>
+      <c r="H112" s="22">
+        <v>0</v>
+      </c>
+      <c r="I112" s="22" t="s">
+        <v>10</v>
+      </c>
+      <c r="J112" s="22">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="113" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A113" s="20">
+        <v>44013</v>
+      </c>
+      <c r="B113" s="21">
+        <v>102927</v>
+      </c>
+      <c r="C113" s="22">
+        <v>1198</v>
+      </c>
+      <c r="D113" s="22">
+        <v>1633</v>
+      </c>
+      <c r="E113" s="22">
+        <v>21</v>
+      </c>
+      <c r="F113" s="22">
+        <v>9</v>
+      </c>
+      <c r="G113" s="22">
+        <v>0</v>
+      </c>
+      <c r="H113" s="22">
+        <v>0</v>
+      </c>
+      <c r="I113" s="22" t="s">
+        <v>10</v>
+      </c>
+      <c r="J113" s="22">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="114" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A114" s="20">
+        <v>44014</v>
+      </c>
+      <c r="B114" s="21">
+        <v>104201</v>
+      </c>
+      <c r="C114" s="22">
+        <v>1274</v>
+      </c>
+      <c r="D114" s="22">
+        <v>1649</v>
+      </c>
+      <c r="E114" s="22">
+        <v>16</v>
+      </c>
+      <c r="F114" s="22">
+        <v>10</v>
+      </c>
+      <c r="G114" s="22">
+        <v>0</v>
+      </c>
+      <c r="H114" s="22">
+        <v>0</v>
+      </c>
+      <c r="I114" s="22" t="s">
+        <v>10</v>
+      </c>
+      <c r="J114" s="22">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="115" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A115" s="20">
+        <v>44015</v>
+      </c>
+      <c r="B115" s="21">
+        <v>105652</v>
+      </c>
+      <c r="C115" s="22">
+        <v>1456</v>
+      </c>
+      <c r="D115" s="22">
+        <v>1679</v>
+      </c>
+      <c r="E115" s="22">
+        <v>30</v>
+      </c>
+      <c r="F115" s="22">
+        <v>6</v>
+      </c>
+      <c r="G115" s="22">
+        <v>0</v>
+      </c>
+      <c r="H115" s="22">
+        <v>4</v>
+      </c>
+      <c r="I115" s="22" t="s">
+        <v>10</v>
+      </c>
+      <c r="J115" s="22">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="116" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A116" s="20">
+        <v>44016</v>
+      </c>
+      <c r="B116" s="21">
+        <v>106368</v>
+      </c>
+      <c r="C116" s="22">
+        <v>716</v>
+      </c>
+      <c r="D116" s="22">
+        <v>1700</v>
+      </c>
+      <c r="E116" s="22">
+        <v>21</v>
+      </c>
+      <c r="F116" s="22">
+        <v>6</v>
+      </c>
+      <c r="G116" s="22">
+        <v>0</v>
+      </c>
+      <c r="H116" s="22">
+        <v>1</v>
+      </c>
+      <c r="I116" s="22" t="s">
+        <v>10</v>
+      </c>
+      <c r="J116" s="22">
+        <v>0</v>
+      </c>
+    </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>

</xml_diff>

<commit_message>
Data updated by GitHub Bot (2020-07-06 12)
</commit_message>
<xml_diff>
--- a/output/snapshot/fdcf2531-4c3e-5c02-b63c-ee160ead6dea.xlsx
+++ b/output/snapshot/fdcf2531-4c3e-5c02-b63c-ee160ead6dea.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="I:\AKTUALNI PODATKI - KORONA\Za objavo na GOV.SI\ang\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{1E6DD62F-2BE2-47DC-A7ED-9B57C1589256}" xr6:coauthVersionLast="44" xr6:coauthVersionMax="44" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{6DAB2626-7145-4C8B-A441-894C65A6357B}" xr6:coauthVersionLast="44" xr6:coauthVersionMax="44" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -25,7 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="10" uniqueCount="10">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="23" uniqueCount="11">
   <si>
     <t>Date</t>
   </si>
@@ -56,6 +56,9 @@
   <si>
     <t>Deaths (daily)</t>
   </si>
+  <si>
+    <t>111*</t>
+  </si>
 </sst>
 </file>
 
@@ -64,7 +67,7 @@
   <numFmts count="1">
     <numFmt numFmtId="164" formatCode="d/\ m/\ yyyy;@"/>
   </numFmts>
-  <fonts count="4" x14ac:knownFonts="1">
+  <fonts count="5" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -93,6 +96,13 @@
       <name val="Calibri Light"/>
       <scheme val="major"/>
     </font>
+    <font>
+      <sz val="10"/>
+      <color theme="1"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
   </fonts>
   <fills count="3">
     <fill>
@@ -108,7 +118,7 @@
       </patternFill>
     </fill>
   </fills>
-  <borders count="2">
+  <borders count="3">
     <border>
       <left/>
       <right/>
@@ -129,11 +139,26 @@
       <bottom/>
       <diagonal/>
     </border>
+    <border>
+      <left style="thin">
+        <color theme="4"/>
+      </left>
+      <right style="thin">
+        <color theme="4"/>
+      </right>
+      <top style="thin">
+        <color theme="4"/>
+      </top>
+      <bottom style="thin">
+        <color theme="4"/>
+      </bottom>
+      <diagonal/>
+    </border>
   </borders>
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="26">
+  <cellXfs count="32">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="49" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyAlignment="1" applyProtection="1">
       <alignment horizontal="left" vertical="top"/>
@@ -208,6 +233,24 @@
       <alignment horizontal="right"/>
     </xf>
     <xf numFmtId="0" fontId="3" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="right"/>
+    </xf>
+    <xf numFmtId="164" fontId="4" fillId="2" borderId="2" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="right" vertical="top"/>
+    </xf>
+    <xf numFmtId="3" fontId="4" fillId="2" borderId="2" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="right"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="2" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="right"/>
+    </xf>
+    <xf numFmtId="164" fontId="3" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="right" vertical="top"/>
+    </xf>
+    <xf numFmtId="3" fontId="3" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="right"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="right"/>
     </xf>
   </cellXfs>
@@ -399,8 +442,8 @@
 </file>
 
 <file path=xl/tables/table1.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="1" xr:uid="{00000000-000C-0000-FFFF-FFFF00000000}" name="Tabela1" displayName="Tabela1" ref="A1:J75" totalsRowShown="0" headerRowDxfId="11" dataDxfId="10">
-  <autoFilter ref="A1:J75" xr:uid="{00000000-0009-0000-0100-000001000000}">
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="1" xr:uid="{00000000-000C-0000-FFFF-FFFF00000000}" name="Tabela1" displayName="Tabela1" ref="A1:J117" totalsRowShown="0" headerRowDxfId="11" dataDxfId="10">
+  <autoFilter ref="A1:J117" xr:uid="{00000000-0009-0000-0100-000001000000}">
     <filterColumn colId="0" hiddenButton="1"/>
     <filterColumn colId="1" hiddenButton="1"/>
     <filterColumn colId="2" hiddenButton="1"/>
@@ -696,10 +739,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:J75"/>
+  <dimension ref="A1:J117"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A40" zoomScale="89" zoomScaleNormal="89" workbookViewId="0">
-      <selection activeCell="J74" sqref="J74"/>
+    <sheetView tabSelected="1" topLeftCell="A83" zoomScale="89" zoomScaleNormal="89" workbookViewId="0">
+      <selection activeCell="A117" sqref="A117:J117"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -3117,6 +3160,1350 @@
         <v>0</v>
       </c>
     </row>
+    <row r="76" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A76" s="20">
+        <v>43976</v>
+      </c>
+      <c r="B76" s="21">
+        <v>75770</v>
+      </c>
+      <c r="C76" s="22">
+        <v>754</v>
+      </c>
+      <c r="D76" s="22">
+        <v>1469</v>
+      </c>
+      <c r="E76" s="22">
+        <v>0</v>
+      </c>
+      <c r="F76" s="22">
+        <v>9</v>
+      </c>
+      <c r="G76" s="22">
+        <v>2</v>
+      </c>
+      <c r="H76" s="22">
+        <v>6</v>
+      </c>
+      <c r="I76" s="22">
+        <v>108</v>
+      </c>
+      <c r="J76" s="22">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="77" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A77" s="20">
+        <v>43977</v>
+      </c>
+      <c r="B77" s="21">
+        <v>76579</v>
+      </c>
+      <c r="C77" s="22">
+        <v>809</v>
+      </c>
+      <c r="D77" s="22">
+        <v>1471</v>
+      </c>
+      <c r="E77" s="22">
+        <v>2</v>
+      </c>
+      <c r="F77" s="22">
+        <v>8</v>
+      </c>
+      <c r="G77" s="22">
+        <v>2</v>
+      </c>
+      <c r="H77" s="22">
+        <v>2</v>
+      </c>
+      <c r="I77" s="22">
+        <v>108</v>
+      </c>
+      <c r="J77" s="22">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="78" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A78" s="20">
+        <v>43978</v>
+      </c>
+      <c r="B78" s="21">
+        <v>77210</v>
+      </c>
+      <c r="C78" s="22">
+        <v>631</v>
+      </c>
+      <c r="D78" s="22">
+        <v>1473</v>
+      </c>
+      <c r="E78" s="22">
+        <v>2</v>
+      </c>
+      <c r="F78" s="22">
+        <v>7</v>
+      </c>
+      <c r="G78" s="22">
+        <v>2</v>
+      </c>
+      <c r="H78" s="22">
+        <v>1</v>
+      </c>
+      <c r="I78" s="22">
+        <v>108</v>
+      </c>
+      <c r="J78" s="22">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="79" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A79" s="20">
+        <v>43979</v>
+      </c>
+      <c r="B79" s="21">
+        <v>77916</v>
+      </c>
+      <c r="C79" s="22">
+        <v>706</v>
+      </c>
+      <c r="D79" s="22">
+        <v>1473</v>
+      </c>
+      <c r="E79" s="22">
+        <v>0</v>
+      </c>
+      <c r="F79" s="22">
+        <v>7</v>
+      </c>
+      <c r="G79" s="22">
+        <v>2</v>
+      </c>
+      <c r="H79" s="22">
+        <v>0</v>
+      </c>
+      <c r="I79" s="22">
+        <v>108</v>
+      </c>
+      <c r="J79" s="22">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="80" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A80" s="20">
+        <v>43980</v>
+      </c>
+      <c r="B80" s="21">
+        <v>78529</v>
+      </c>
+      <c r="C80" s="22">
+        <v>613</v>
+      </c>
+      <c r="D80" s="22">
+        <v>1473</v>
+      </c>
+      <c r="E80" s="22">
+        <v>0</v>
+      </c>
+      <c r="F80" s="22">
+        <v>7</v>
+      </c>
+      <c r="G80" s="22">
+        <v>2</v>
+      </c>
+      <c r="H80" s="22">
+        <v>0</v>
+      </c>
+      <c r="I80" s="22">
+        <v>108</v>
+      </c>
+      <c r="J80" s="22">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="81" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A81" s="20">
+        <v>43981</v>
+      </c>
+      <c r="B81" s="22">
+        <v>78793</v>
+      </c>
+      <c r="C81" s="22">
+        <v>264</v>
+      </c>
+      <c r="D81" s="22">
+        <v>1473</v>
+      </c>
+      <c r="E81" s="22">
+        <v>0</v>
+      </c>
+      <c r="F81" s="22">
+        <v>6</v>
+      </c>
+      <c r="G81" s="22">
+        <v>2</v>
+      </c>
+      <c r="H81" s="22">
+        <v>1</v>
+      </c>
+      <c r="I81" s="22">
+        <v>108</v>
+      </c>
+      <c r="J81" s="22">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="82" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A82" s="20">
+        <v>43982</v>
+      </c>
+      <c r="B82" s="21">
+        <v>79039</v>
+      </c>
+      <c r="C82" s="22">
+        <v>246</v>
+      </c>
+      <c r="D82" s="22">
+        <v>1473</v>
+      </c>
+      <c r="E82" s="22">
+        <v>0</v>
+      </c>
+      <c r="F82" s="22">
+        <v>5</v>
+      </c>
+      <c r="G82" s="22">
+        <v>1</v>
+      </c>
+      <c r="H82" s="22">
+        <v>0</v>
+      </c>
+      <c r="I82" s="22">
+        <v>109</v>
+      </c>
+      <c r="J82" s="22">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="83" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A83" s="20">
+        <v>43983</v>
+      </c>
+      <c r="B83" s="21">
+        <v>79698</v>
+      </c>
+      <c r="C83" s="22">
+        <v>659</v>
+      </c>
+      <c r="D83" s="22">
+        <v>1475</v>
+      </c>
+      <c r="E83" s="22">
+        <v>2</v>
+      </c>
+      <c r="F83" s="22">
+        <v>5</v>
+      </c>
+      <c r="G83" s="22">
+        <v>1</v>
+      </c>
+      <c r="H83" s="22">
+        <v>0</v>
+      </c>
+      <c r="I83" s="22">
+        <v>109</v>
+      </c>
+      <c r="J83" s="22">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="84" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A84" s="20">
+        <v>43984</v>
+      </c>
+      <c r="B84" s="21">
+        <v>80505</v>
+      </c>
+      <c r="C84" s="22">
+        <v>807</v>
+      </c>
+      <c r="D84" s="22">
+        <v>1477</v>
+      </c>
+      <c r="E84" s="22">
+        <v>2</v>
+      </c>
+      <c r="F84" s="22">
+        <v>5</v>
+      </c>
+      <c r="G84" s="22">
+        <v>0</v>
+      </c>
+      <c r="H84" s="22">
+        <v>0</v>
+      </c>
+      <c r="I84" s="22">
+        <v>109</v>
+      </c>
+      <c r="J84" s="22">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="85" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A85" s="20">
+        <v>43985</v>
+      </c>
+      <c r="B85" s="21">
+        <v>81333</v>
+      </c>
+      <c r="C85" s="22">
+        <v>828</v>
+      </c>
+      <c r="D85" s="22">
+        <v>1477</v>
+      </c>
+      <c r="E85" s="22">
+        <v>0</v>
+      </c>
+      <c r="F85" s="22">
+        <v>5</v>
+      </c>
+      <c r="G85" s="22">
+        <v>0</v>
+      </c>
+      <c r="H85" s="22">
+        <v>0</v>
+      </c>
+      <c r="I85" s="22">
+        <v>109</v>
+      </c>
+      <c r="J85" s="22">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="86" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A86" s="26">
+        <v>43986</v>
+      </c>
+      <c r="B86" s="27">
+        <v>82161</v>
+      </c>
+      <c r="C86" s="28">
+        <v>828</v>
+      </c>
+      <c r="D86" s="28">
+        <v>1479</v>
+      </c>
+      <c r="E86" s="28">
+        <v>2</v>
+      </c>
+      <c r="F86" s="28">
+        <v>6</v>
+      </c>
+      <c r="G86" s="28">
+        <v>0</v>
+      </c>
+      <c r="H86" s="28">
+        <v>0</v>
+      </c>
+      <c r="I86" s="28">
+        <v>109</v>
+      </c>
+      <c r="J86" s="28">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="87" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A87" s="29">
+        <v>43987</v>
+      </c>
+      <c r="B87" s="30">
+        <v>82876</v>
+      </c>
+      <c r="C87" s="31">
+        <v>715</v>
+      </c>
+      <c r="D87" s="31">
+        <v>1484</v>
+      </c>
+      <c r="E87" s="31">
+        <v>5</v>
+      </c>
+      <c r="F87" s="31">
+        <v>6</v>
+      </c>
+      <c r="G87" s="31">
+        <v>0</v>
+      </c>
+      <c r="H87" s="31">
+        <v>0</v>
+      </c>
+      <c r="I87" s="31">
+        <v>109</v>
+      </c>
+      <c r="J87" s="31">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="88" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A88" s="23">
+        <v>43988</v>
+      </c>
+      <c r="B88" s="24">
+        <v>83105</v>
+      </c>
+      <c r="C88" s="25">
+        <v>229</v>
+      </c>
+      <c r="D88" s="25">
+        <v>1485</v>
+      </c>
+      <c r="E88" s="25">
+        <v>1</v>
+      </c>
+      <c r="F88" s="25">
+        <v>5</v>
+      </c>
+      <c r="G88" s="25">
+        <v>0</v>
+      </c>
+      <c r="H88" s="25">
+        <v>1</v>
+      </c>
+      <c r="I88" s="25">
+        <v>109</v>
+      </c>
+      <c r="J88" s="25">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="89" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A89" s="29">
+        <v>43989</v>
+      </c>
+      <c r="B89" s="30">
+        <v>83316</v>
+      </c>
+      <c r="C89" s="31">
+        <v>211</v>
+      </c>
+      <c r="D89" s="31">
+        <v>1485</v>
+      </c>
+      <c r="E89" s="31">
+        <v>0</v>
+      </c>
+      <c r="F89" s="31">
+        <v>5</v>
+      </c>
+      <c r="G89" s="31">
+        <v>0</v>
+      </c>
+      <c r="H89" s="31">
+        <v>0</v>
+      </c>
+      <c r="I89" s="31">
+        <v>109</v>
+      </c>
+      <c r="J89" s="31">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="90" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A90" s="20">
+        <v>43990</v>
+      </c>
+      <c r="B90" s="21">
+        <v>84130</v>
+      </c>
+      <c r="C90" s="22">
+        <v>814</v>
+      </c>
+      <c r="D90" s="22">
+        <v>1486</v>
+      </c>
+      <c r="E90" s="22">
+        <v>1</v>
+      </c>
+      <c r="F90" s="22">
+        <v>6</v>
+      </c>
+      <c r="G90" s="22">
+        <v>0</v>
+      </c>
+      <c r="H90" s="22">
+        <v>0</v>
+      </c>
+      <c r="I90" s="22">
+        <v>109</v>
+      </c>
+      <c r="J90" s="22">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="91" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A91" s="20">
+        <v>43991</v>
+      </c>
+      <c r="B91" s="21">
+        <v>84868</v>
+      </c>
+      <c r="C91" s="22">
+        <v>738</v>
+      </c>
+      <c r="D91" s="22">
+        <v>1488</v>
+      </c>
+      <c r="E91" s="22">
+        <v>2</v>
+      </c>
+      <c r="F91" s="22">
+        <v>6</v>
+      </c>
+      <c r="G91" s="22">
+        <v>0</v>
+      </c>
+      <c r="H91" s="22">
+        <v>0</v>
+      </c>
+      <c r="I91" s="22">
+        <v>109</v>
+      </c>
+      <c r="J91" s="22">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="92" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A92" s="23">
+        <v>43992</v>
+      </c>
+      <c r="B92" s="24">
+        <v>85626</v>
+      </c>
+      <c r="C92" s="25">
+        <v>758</v>
+      </c>
+      <c r="D92" s="25">
+        <v>1488</v>
+      </c>
+      <c r="E92" s="25">
+        <v>0</v>
+      </c>
+      <c r="F92" s="25">
+        <v>6</v>
+      </c>
+      <c r="G92" s="25">
+        <v>0</v>
+      </c>
+      <c r="H92" s="25">
+        <v>0</v>
+      </c>
+      <c r="I92" s="25">
+        <v>109</v>
+      </c>
+      <c r="J92" s="25">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="93" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A93" s="29">
+        <v>43993</v>
+      </c>
+      <c r="B93" s="30">
+        <v>86328</v>
+      </c>
+      <c r="C93" s="31">
+        <v>702</v>
+      </c>
+      <c r="D93" s="31">
+        <v>1490</v>
+      </c>
+      <c r="E93" s="31">
+        <v>2</v>
+      </c>
+      <c r="F93" s="31">
+        <v>6</v>
+      </c>
+      <c r="G93" s="31">
+        <v>0</v>
+      </c>
+      <c r="H93" s="31">
+        <v>0</v>
+      </c>
+      <c r="I93" s="31">
+        <v>109</v>
+      </c>
+      <c r="J93" s="31">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="94" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A94" s="23">
+        <v>43994</v>
+      </c>
+      <c r="B94" s="24">
+        <v>87095</v>
+      </c>
+      <c r="C94" s="25">
+        <v>767</v>
+      </c>
+      <c r="D94" s="25">
+        <v>1492</v>
+      </c>
+      <c r="E94" s="25">
+        <v>2</v>
+      </c>
+      <c r="F94" s="25">
+        <v>6</v>
+      </c>
+      <c r="G94" s="25">
+        <v>0</v>
+      </c>
+      <c r="H94" s="25">
+        <v>0</v>
+      </c>
+      <c r="I94" s="25">
+        <v>109</v>
+      </c>
+      <c r="J94" s="25">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="95" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A95" s="29">
+        <v>43995</v>
+      </c>
+      <c r="B95" s="30">
+        <v>87386</v>
+      </c>
+      <c r="C95" s="31">
+        <v>291</v>
+      </c>
+      <c r="D95" s="31">
+        <v>1495</v>
+      </c>
+      <c r="E95" s="31">
+        <v>3</v>
+      </c>
+      <c r="F95" s="31">
+        <v>6</v>
+      </c>
+      <c r="G95" s="31">
+        <v>0</v>
+      </c>
+      <c r="H95" s="31">
+        <v>0</v>
+      </c>
+      <c r="I95" s="31">
+        <v>109</v>
+      </c>
+      <c r="J95" s="31">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="96" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A96" s="23">
+        <v>43996</v>
+      </c>
+      <c r="B96" s="24">
+        <v>87598</v>
+      </c>
+      <c r="C96" s="25">
+        <v>212</v>
+      </c>
+      <c r="D96" s="25">
+        <v>1496</v>
+      </c>
+      <c r="E96" s="25">
+        <v>1</v>
+      </c>
+      <c r="F96" s="25">
+        <v>7</v>
+      </c>
+      <c r="G96" s="25">
+        <v>1</v>
+      </c>
+      <c r="H96" s="25">
+        <v>0</v>
+      </c>
+      <c r="I96" s="25">
+        <v>109</v>
+      </c>
+      <c r="J96" s="25">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="97" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A97" s="20">
+        <v>43997</v>
+      </c>
+      <c r="B97" s="21">
+        <v>88165</v>
+      </c>
+      <c r="C97" s="22">
+        <v>567</v>
+      </c>
+      <c r="D97" s="22">
+        <v>1499</v>
+      </c>
+      <c r="E97" s="22">
+        <v>3</v>
+      </c>
+      <c r="F97" s="22">
+        <v>7</v>
+      </c>
+      <c r="G97" s="22">
+        <v>1</v>
+      </c>
+      <c r="H97" s="22">
+        <v>0</v>
+      </c>
+      <c r="I97" s="22">
+        <v>109</v>
+      </c>
+      <c r="J97" s="22">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="98" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A98" s="20">
+        <v>43998</v>
+      </c>
+      <c r="B98" s="21">
+        <v>89151</v>
+      </c>
+      <c r="C98" s="22">
+        <v>986</v>
+      </c>
+      <c r="D98" s="22">
+        <v>1503</v>
+      </c>
+      <c r="E98" s="22">
+        <v>4</v>
+      </c>
+      <c r="F98" s="22">
+        <v>7</v>
+      </c>
+      <c r="G98" s="22">
+        <v>1</v>
+      </c>
+      <c r="H98" s="22">
+        <v>0</v>
+      </c>
+      <c r="I98" s="22">
+        <v>109</v>
+      </c>
+      <c r="J98" s="22">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="99" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A99" s="29">
+        <v>43999</v>
+      </c>
+      <c r="B99" s="30">
+        <v>90103</v>
+      </c>
+      <c r="C99" s="31">
+        <v>952</v>
+      </c>
+      <c r="D99" s="31">
+        <v>1511</v>
+      </c>
+      <c r="E99" s="31">
+        <v>8</v>
+      </c>
+      <c r="F99" s="31">
+        <v>6</v>
+      </c>
+      <c r="G99" s="31">
+        <v>1</v>
+      </c>
+      <c r="H99" s="31">
+        <v>1</v>
+      </c>
+      <c r="I99" s="31">
+        <v>109</v>
+      </c>
+      <c r="J99" s="31">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="100" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A100" s="20">
+        <v>44000</v>
+      </c>
+      <c r="B100" s="21">
+        <v>91005</v>
+      </c>
+      <c r="C100" s="22">
+        <v>902</v>
+      </c>
+      <c r="D100" s="22">
+        <v>1513</v>
+      </c>
+      <c r="E100" s="22">
+        <v>2</v>
+      </c>
+      <c r="F100" s="22">
+        <v>8</v>
+      </c>
+      <c r="G100" s="22">
+        <v>1</v>
+      </c>
+      <c r="H100" s="22">
+        <v>0</v>
+      </c>
+      <c r="I100" s="22">
+        <v>109</v>
+      </c>
+      <c r="J100" s="22">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="101" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A101" s="29">
+        <v>44001</v>
+      </c>
+      <c r="B101" s="30">
+        <v>92152</v>
+      </c>
+      <c r="C101" s="31">
+        <v>1147</v>
+      </c>
+      <c r="D101" s="31">
+        <v>1519</v>
+      </c>
+      <c r="E101" s="31">
+        <v>6</v>
+      </c>
+      <c r="F101" s="31">
+        <v>6</v>
+      </c>
+      <c r="G101" s="31">
+        <v>1</v>
+      </c>
+      <c r="H101" s="31">
+        <v>2</v>
+      </c>
+      <c r="I101" s="31">
+        <v>109</v>
+      </c>
+      <c r="J101" s="31">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="102" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A102" s="23">
+        <v>44002</v>
+      </c>
+      <c r="B102" s="24">
+        <v>92919</v>
+      </c>
+      <c r="C102" s="25">
+        <v>758</v>
+      </c>
+      <c r="D102" s="25">
+        <v>1520</v>
+      </c>
+      <c r="E102" s="25">
+        <v>1</v>
+      </c>
+      <c r="F102" s="25">
+        <v>6</v>
+      </c>
+      <c r="G102" s="25">
+        <v>1</v>
+      </c>
+      <c r="H102" s="25">
+        <v>2</v>
+      </c>
+      <c r="I102" s="25">
+        <v>109</v>
+      </c>
+      <c r="J102" s="25">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="103" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A103" s="29">
+        <v>44003</v>
+      </c>
+      <c r="B103" s="30">
+        <v>93181</v>
+      </c>
+      <c r="C103" s="31">
+        <v>271</v>
+      </c>
+      <c r="D103" s="31">
+        <v>1521</v>
+      </c>
+      <c r="E103" s="31">
+        <v>1</v>
+      </c>
+      <c r="F103" s="31">
+        <v>6</v>
+      </c>
+      <c r="G103" s="31">
+        <v>1</v>
+      </c>
+      <c r="H103" s="31">
+        <v>0</v>
+      </c>
+      <c r="I103" s="31">
+        <v>109</v>
+      </c>
+      <c r="J103" s="31">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="104" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A104" s="29">
+        <v>44004</v>
+      </c>
+      <c r="B104" s="30">
+        <v>94165</v>
+      </c>
+      <c r="C104" s="31">
+        <v>984</v>
+      </c>
+      <c r="D104" s="31">
+        <v>1534</v>
+      </c>
+      <c r="E104" s="31">
+        <v>13</v>
+      </c>
+      <c r="F104" s="31">
+        <v>5</v>
+      </c>
+      <c r="G104" s="31">
+        <v>1</v>
+      </c>
+      <c r="H104" s="31">
+        <v>1</v>
+      </c>
+      <c r="I104" s="31">
+        <v>109</v>
+      </c>
+      <c r="J104" s="31">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="105" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A105" s="29">
+        <v>44005</v>
+      </c>
+      <c r="B105" s="30">
+        <v>95387</v>
+      </c>
+      <c r="C105" s="31">
+        <v>1222</v>
+      </c>
+      <c r="D105" s="31">
+        <v>1541</v>
+      </c>
+      <c r="E105" s="31">
+        <v>7</v>
+      </c>
+      <c r="F105" s="31">
+        <v>7</v>
+      </c>
+      <c r="G105" s="31">
+        <v>2</v>
+      </c>
+      <c r="H105" s="31">
+        <v>0</v>
+      </c>
+      <c r="I105" s="31" t="s">
+        <v>10</v>
+      </c>
+      <c r="J105" s="31">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="106" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A106" s="23">
+        <v>44006</v>
+      </c>
+      <c r="B106" s="24">
+        <v>96599</v>
+      </c>
+      <c r="C106" s="25">
+        <v>1212</v>
+      </c>
+      <c r="D106" s="25">
+        <v>1547</v>
+      </c>
+      <c r="E106" s="25">
+        <v>6</v>
+      </c>
+      <c r="F106" s="25">
+        <v>7</v>
+      </c>
+      <c r="G106" s="25">
+        <v>2</v>
+      </c>
+      <c r="H106" s="25">
+        <v>0</v>
+      </c>
+      <c r="I106" s="25" t="s">
+        <v>10</v>
+      </c>
+      <c r="J106" s="25">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="107" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A107" s="29">
+        <v>44007</v>
+      </c>
+      <c r="B107" s="30">
+        <v>97442</v>
+      </c>
+      <c r="C107" s="31">
+        <v>843</v>
+      </c>
+      <c r="D107" s="31">
+        <v>1558</v>
+      </c>
+      <c r="E107" s="31">
+        <v>11</v>
+      </c>
+      <c r="F107" s="31">
+        <v>8</v>
+      </c>
+      <c r="G107" s="31">
+        <v>2</v>
+      </c>
+      <c r="H107" s="31">
+        <v>0</v>
+      </c>
+      <c r="I107" s="31" t="s">
+        <v>10</v>
+      </c>
+      <c r="J107" s="31">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="108" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A108" s="29">
+        <v>44008</v>
+      </c>
+      <c r="B108" s="30">
+        <v>98320</v>
+      </c>
+      <c r="C108" s="31">
+        <v>878</v>
+      </c>
+      <c r="D108" s="31">
+        <v>1572</v>
+      </c>
+      <c r="E108" s="31">
+        <v>14</v>
+      </c>
+      <c r="F108" s="31">
+        <v>8</v>
+      </c>
+      <c r="G108" s="31">
+        <v>1</v>
+      </c>
+      <c r="H108" s="31">
+        <v>0</v>
+      </c>
+      <c r="I108" s="31" t="s">
+        <v>10</v>
+      </c>
+      <c r="J108" s="31">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="109" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A109" s="29">
+        <v>44009</v>
+      </c>
+      <c r="B109" s="30">
+        <v>98945</v>
+      </c>
+      <c r="C109" s="31">
+        <v>625</v>
+      </c>
+      <c r="D109" s="31">
+        <v>1581</v>
+      </c>
+      <c r="E109" s="31">
+        <v>9</v>
+      </c>
+      <c r="F109" s="31">
+        <v>7</v>
+      </c>
+      <c r="G109" s="31">
+        <v>0</v>
+      </c>
+      <c r="H109" s="31">
+        <v>1</v>
+      </c>
+      <c r="I109" s="31" t="s">
+        <v>10</v>
+      </c>
+      <c r="J109" s="31">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="110" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A110" s="29">
+        <v>44010</v>
+      </c>
+      <c r="B110" s="30">
+        <v>99245</v>
+      </c>
+      <c r="C110" s="31">
+        <v>300</v>
+      </c>
+      <c r="D110" s="31">
+        <v>1585</v>
+      </c>
+      <c r="E110" s="31">
+        <v>4</v>
+      </c>
+      <c r="F110" s="31">
+        <v>8</v>
+      </c>
+      <c r="G110" s="31">
+        <v>0</v>
+      </c>
+      <c r="H110" s="31">
+        <v>0</v>
+      </c>
+      <c r="I110" s="31" t="s">
+        <v>10</v>
+      </c>
+      <c r="J110" s="31">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="111" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A111" s="29">
+        <v>44011</v>
+      </c>
+      <c r="B111" s="30">
+        <v>100330</v>
+      </c>
+      <c r="C111" s="31">
+        <v>1085</v>
+      </c>
+      <c r="D111" s="31">
+        <v>1600</v>
+      </c>
+      <c r="E111" s="31">
+        <v>15</v>
+      </c>
+      <c r="F111" s="31">
+        <v>8</v>
+      </c>
+      <c r="G111" s="31">
+        <v>0</v>
+      </c>
+      <c r="H111" s="31">
+        <v>0</v>
+      </c>
+      <c r="I111" s="31" t="s">
+        <v>10</v>
+      </c>
+      <c r="J111" s="31">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="112" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A112" s="20">
+        <v>44012</v>
+      </c>
+      <c r="B112" s="21">
+        <v>101729</v>
+      </c>
+      <c r="C112" s="22">
+        <v>1399</v>
+      </c>
+      <c r="D112" s="22">
+        <v>1613</v>
+      </c>
+      <c r="E112" s="22">
+        <v>13</v>
+      </c>
+      <c r="F112" s="22">
+        <v>8</v>
+      </c>
+      <c r="G112" s="22">
+        <v>0</v>
+      </c>
+      <c r="H112" s="22">
+        <v>0</v>
+      </c>
+      <c r="I112" s="22" t="s">
+        <v>10</v>
+      </c>
+      <c r="J112" s="22">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="113" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A113" s="20">
+        <v>44013</v>
+      </c>
+      <c r="B113" s="21">
+        <v>102927</v>
+      </c>
+      <c r="C113" s="22">
+        <v>1198</v>
+      </c>
+      <c r="D113" s="22">
+        <v>1633</v>
+      </c>
+      <c r="E113" s="22">
+        <v>21</v>
+      </c>
+      <c r="F113" s="22">
+        <v>9</v>
+      </c>
+      <c r="G113" s="22">
+        <v>0</v>
+      </c>
+      <c r="H113" s="22">
+        <v>0</v>
+      </c>
+      <c r="I113" s="22" t="s">
+        <v>10</v>
+      </c>
+      <c r="J113" s="22">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="114" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A114" s="20">
+        <v>44014</v>
+      </c>
+      <c r="B114" s="21">
+        <v>104201</v>
+      </c>
+      <c r="C114" s="22">
+        <v>1274</v>
+      </c>
+      <c r="D114" s="22">
+        <v>1649</v>
+      </c>
+      <c r="E114" s="22">
+        <v>16</v>
+      </c>
+      <c r="F114" s="22">
+        <v>10</v>
+      </c>
+      <c r="G114" s="22">
+        <v>0</v>
+      </c>
+      <c r="H114" s="22">
+        <v>0</v>
+      </c>
+      <c r="I114" s="22" t="s">
+        <v>10</v>
+      </c>
+      <c r="J114" s="22">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="115" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A115" s="20">
+        <v>44015</v>
+      </c>
+      <c r="B115" s="21">
+        <v>105652</v>
+      </c>
+      <c r="C115" s="22">
+        <v>1456</v>
+      </c>
+      <c r="D115" s="22">
+        <v>1679</v>
+      </c>
+      <c r="E115" s="22">
+        <v>30</v>
+      </c>
+      <c r="F115" s="22">
+        <v>6</v>
+      </c>
+      <c r="G115" s="22">
+        <v>0</v>
+      </c>
+      <c r="H115" s="22">
+        <v>4</v>
+      </c>
+      <c r="I115" s="22" t="s">
+        <v>10</v>
+      </c>
+      <c r="J115" s="22">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="116" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A116" s="20">
+        <v>44016</v>
+      </c>
+      <c r="B116" s="21">
+        <v>106368</v>
+      </c>
+      <c r="C116" s="22">
+        <v>716</v>
+      </c>
+      <c r="D116" s="22">
+        <v>1700</v>
+      </c>
+      <c r="E116" s="22">
+        <v>21</v>
+      </c>
+      <c r="F116" s="22">
+        <v>6</v>
+      </c>
+      <c r="G116" s="22">
+        <v>0</v>
+      </c>
+      <c r="H116" s="22">
+        <v>1</v>
+      </c>
+      <c r="I116" s="22" t="s">
+        <v>10</v>
+      </c>
+      <c r="J116" s="22">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="117" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A117" s="29">
+        <v>44017</v>
+      </c>
+      <c r="B117" s="30">
+        <v>106898</v>
+      </c>
+      <c r="C117" s="31">
+        <v>530</v>
+      </c>
+      <c r="D117" s="31">
+        <v>1716</v>
+      </c>
+      <c r="E117" s="31">
+        <v>16</v>
+      </c>
+      <c r="F117" s="31">
+        <v>11</v>
+      </c>
+      <c r="G117" s="31">
+        <v>0</v>
+      </c>
+      <c r="H117" s="31">
+        <v>0</v>
+      </c>
+      <c r="I117" s="31" t="s">
+        <v>10</v>
+      </c>
+      <c r="J117" s="31">
+        <v>0</v>
+      </c>
+    </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>

</xml_diff>

<commit_message>
Data updated by GitHub Bot (2020-07-06 20)
</commit_message>
<xml_diff>
--- a/output/snapshot/fdcf2531-4c3e-5c02-b63c-ee160ead6dea.xlsx
+++ b/output/snapshot/fdcf2531-4c3e-5c02-b63c-ee160ead6dea.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="I:\AKTUALNI PODATKI - KORONA\Za objavo na GOV.SI\ang\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{1E6DD62F-2BE2-47DC-A7ED-9B57C1589256}" xr6:coauthVersionLast="44" xr6:coauthVersionMax="44" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{6DAB2626-7145-4C8B-A441-894C65A6357B}" xr6:coauthVersionLast="44" xr6:coauthVersionMax="44" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -25,7 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="10" uniqueCount="10">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="23" uniqueCount="11">
   <si>
     <t>Date</t>
   </si>
@@ -56,6 +56,9 @@
   <si>
     <t>Deaths (daily)</t>
   </si>
+  <si>
+    <t>111*</t>
+  </si>
 </sst>
 </file>
 
@@ -64,7 +67,7 @@
   <numFmts count="1">
     <numFmt numFmtId="164" formatCode="d/\ m/\ yyyy;@"/>
   </numFmts>
-  <fonts count="4" x14ac:knownFonts="1">
+  <fonts count="5" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -93,6 +96,13 @@
       <name val="Calibri Light"/>
       <scheme val="major"/>
     </font>
+    <font>
+      <sz val="10"/>
+      <color theme="1"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
   </fonts>
   <fills count="3">
     <fill>
@@ -108,7 +118,7 @@
       </patternFill>
     </fill>
   </fills>
-  <borders count="2">
+  <borders count="3">
     <border>
       <left/>
       <right/>
@@ -129,11 +139,26 @@
       <bottom/>
       <diagonal/>
     </border>
+    <border>
+      <left style="thin">
+        <color theme="4"/>
+      </left>
+      <right style="thin">
+        <color theme="4"/>
+      </right>
+      <top style="thin">
+        <color theme="4"/>
+      </top>
+      <bottom style="thin">
+        <color theme="4"/>
+      </bottom>
+      <diagonal/>
+    </border>
   </borders>
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="26">
+  <cellXfs count="32">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="49" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyAlignment="1" applyProtection="1">
       <alignment horizontal="left" vertical="top"/>
@@ -208,6 +233,24 @@
       <alignment horizontal="right"/>
     </xf>
     <xf numFmtId="0" fontId="3" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="right"/>
+    </xf>
+    <xf numFmtId="164" fontId="4" fillId="2" borderId="2" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="right" vertical="top"/>
+    </xf>
+    <xf numFmtId="3" fontId="4" fillId="2" borderId="2" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="right"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="2" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="right"/>
+    </xf>
+    <xf numFmtId="164" fontId="3" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="right" vertical="top"/>
+    </xf>
+    <xf numFmtId="3" fontId="3" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="right"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="right"/>
     </xf>
   </cellXfs>
@@ -399,8 +442,8 @@
 </file>
 
 <file path=xl/tables/table1.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="1" xr:uid="{00000000-000C-0000-FFFF-FFFF00000000}" name="Tabela1" displayName="Tabela1" ref="A1:J75" totalsRowShown="0" headerRowDxfId="11" dataDxfId="10">
-  <autoFilter ref="A1:J75" xr:uid="{00000000-0009-0000-0100-000001000000}">
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="1" xr:uid="{00000000-000C-0000-FFFF-FFFF00000000}" name="Tabela1" displayName="Tabela1" ref="A1:J117" totalsRowShown="0" headerRowDxfId="11" dataDxfId="10">
+  <autoFilter ref="A1:J117" xr:uid="{00000000-0009-0000-0100-000001000000}">
     <filterColumn colId="0" hiddenButton="1"/>
     <filterColumn colId="1" hiddenButton="1"/>
     <filterColumn colId="2" hiddenButton="1"/>
@@ -696,10 +739,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:J75"/>
+  <dimension ref="A1:J117"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A40" zoomScale="89" zoomScaleNormal="89" workbookViewId="0">
-      <selection activeCell="J74" sqref="J74"/>
+    <sheetView tabSelected="1" topLeftCell="A83" zoomScale="89" zoomScaleNormal="89" workbookViewId="0">
+      <selection activeCell="A117" sqref="A117:J117"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -3117,6 +3160,1350 @@
         <v>0</v>
       </c>
     </row>
+    <row r="76" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A76" s="20">
+        <v>43976</v>
+      </c>
+      <c r="B76" s="21">
+        <v>75770</v>
+      </c>
+      <c r="C76" s="22">
+        <v>754</v>
+      </c>
+      <c r="D76" s="22">
+        <v>1469</v>
+      </c>
+      <c r="E76" s="22">
+        <v>0</v>
+      </c>
+      <c r="F76" s="22">
+        <v>9</v>
+      </c>
+      <c r="G76" s="22">
+        <v>2</v>
+      </c>
+      <c r="H76" s="22">
+        <v>6</v>
+      </c>
+      <c r="I76" s="22">
+        <v>108</v>
+      </c>
+      <c r="J76" s="22">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="77" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A77" s="20">
+        <v>43977</v>
+      </c>
+      <c r="B77" s="21">
+        <v>76579</v>
+      </c>
+      <c r="C77" s="22">
+        <v>809</v>
+      </c>
+      <c r="D77" s="22">
+        <v>1471</v>
+      </c>
+      <c r="E77" s="22">
+        <v>2</v>
+      </c>
+      <c r="F77" s="22">
+        <v>8</v>
+      </c>
+      <c r="G77" s="22">
+        <v>2</v>
+      </c>
+      <c r="H77" s="22">
+        <v>2</v>
+      </c>
+      <c r="I77" s="22">
+        <v>108</v>
+      </c>
+      <c r="J77" s="22">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="78" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A78" s="20">
+        <v>43978</v>
+      </c>
+      <c r="B78" s="21">
+        <v>77210</v>
+      </c>
+      <c r="C78" s="22">
+        <v>631</v>
+      </c>
+      <c r="D78" s="22">
+        <v>1473</v>
+      </c>
+      <c r="E78" s="22">
+        <v>2</v>
+      </c>
+      <c r="F78" s="22">
+        <v>7</v>
+      </c>
+      <c r="G78" s="22">
+        <v>2</v>
+      </c>
+      <c r="H78" s="22">
+        <v>1</v>
+      </c>
+      <c r="I78" s="22">
+        <v>108</v>
+      </c>
+      <c r="J78" s="22">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="79" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A79" s="20">
+        <v>43979</v>
+      </c>
+      <c r="B79" s="21">
+        <v>77916</v>
+      </c>
+      <c r="C79" s="22">
+        <v>706</v>
+      </c>
+      <c r="D79" s="22">
+        <v>1473</v>
+      </c>
+      <c r="E79" s="22">
+        <v>0</v>
+      </c>
+      <c r="F79" s="22">
+        <v>7</v>
+      </c>
+      <c r="G79" s="22">
+        <v>2</v>
+      </c>
+      <c r="H79" s="22">
+        <v>0</v>
+      </c>
+      <c r="I79" s="22">
+        <v>108</v>
+      </c>
+      <c r="J79" s="22">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="80" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A80" s="20">
+        <v>43980</v>
+      </c>
+      <c r="B80" s="21">
+        <v>78529</v>
+      </c>
+      <c r="C80" s="22">
+        <v>613</v>
+      </c>
+      <c r="D80" s="22">
+        <v>1473</v>
+      </c>
+      <c r="E80" s="22">
+        <v>0</v>
+      </c>
+      <c r="F80" s="22">
+        <v>7</v>
+      </c>
+      <c r="G80" s="22">
+        <v>2</v>
+      </c>
+      <c r="H80" s="22">
+        <v>0</v>
+      </c>
+      <c r="I80" s="22">
+        <v>108</v>
+      </c>
+      <c r="J80" s="22">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="81" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A81" s="20">
+        <v>43981</v>
+      </c>
+      <c r="B81" s="22">
+        <v>78793</v>
+      </c>
+      <c r="C81" s="22">
+        <v>264</v>
+      </c>
+      <c r="D81" s="22">
+        <v>1473</v>
+      </c>
+      <c r="E81" s="22">
+        <v>0</v>
+      </c>
+      <c r="F81" s="22">
+        <v>6</v>
+      </c>
+      <c r="G81" s="22">
+        <v>2</v>
+      </c>
+      <c r="H81" s="22">
+        <v>1</v>
+      </c>
+      <c r="I81" s="22">
+        <v>108</v>
+      </c>
+      <c r="J81" s="22">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="82" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A82" s="20">
+        <v>43982</v>
+      </c>
+      <c r="B82" s="21">
+        <v>79039</v>
+      </c>
+      <c r="C82" s="22">
+        <v>246</v>
+      </c>
+      <c r="D82" s="22">
+        <v>1473</v>
+      </c>
+      <c r="E82" s="22">
+        <v>0</v>
+      </c>
+      <c r="F82" s="22">
+        <v>5</v>
+      </c>
+      <c r="G82" s="22">
+        <v>1</v>
+      </c>
+      <c r="H82" s="22">
+        <v>0</v>
+      </c>
+      <c r="I82" s="22">
+        <v>109</v>
+      </c>
+      <c r="J82" s="22">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="83" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A83" s="20">
+        <v>43983</v>
+      </c>
+      <c r="B83" s="21">
+        <v>79698</v>
+      </c>
+      <c r="C83" s="22">
+        <v>659</v>
+      </c>
+      <c r="D83" s="22">
+        <v>1475</v>
+      </c>
+      <c r="E83" s="22">
+        <v>2</v>
+      </c>
+      <c r="F83" s="22">
+        <v>5</v>
+      </c>
+      <c r="G83" s="22">
+        <v>1</v>
+      </c>
+      <c r="H83" s="22">
+        <v>0</v>
+      </c>
+      <c r="I83" s="22">
+        <v>109</v>
+      </c>
+      <c r="J83" s="22">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="84" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A84" s="20">
+        <v>43984</v>
+      </c>
+      <c r="B84" s="21">
+        <v>80505</v>
+      </c>
+      <c r="C84" s="22">
+        <v>807</v>
+      </c>
+      <c r="D84" s="22">
+        <v>1477</v>
+      </c>
+      <c r="E84" s="22">
+        <v>2</v>
+      </c>
+      <c r="F84" s="22">
+        <v>5</v>
+      </c>
+      <c r="G84" s="22">
+        <v>0</v>
+      </c>
+      <c r="H84" s="22">
+        <v>0</v>
+      </c>
+      <c r="I84" s="22">
+        <v>109</v>
+      </c>
+      <c r="J84" s="22">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="85" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A85" s="20">
+        <v>43985</v>
+      </c>
+      <c r="B85" s="21">
+        <v>81333</v>
+      </c>
+      <c r="C85" s="22">
+        <v>828</v>
+      </c>
+      <c r="D85" s="22">
+        <v>1477</v>
+      </c>
+      <c r="E85" s="22">
+        <v>0</v>
+      </c>
+      <c r="F85" s="22">
+        <v>5</v>
+      </c>
+      <c r="G85" s="22">
+        <v>0</v>
+      </c>
+      <c r="H85" s="22">
+        <v>0</v>
+      </c>
+      <c r="I85" s="22">
+        <v>109</v>
+      </c>
+      <c r="J85" s="22">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="86" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A86" s="26">
+        <v>43986</v>
+      </c>
+      <c r="B86" s="27">
+        <v>82161</v>
+      </c>
+      <c r="C86" s="28">
+        <v>828</v>
+      </c>
+      <c r="D86" s="28">
+        <v>1479</v>
+      </c>
+      <c r="E86" s="28">
+        <v>2</v>
+      </c>
+      <c r="F86" s="28">
+        <v>6</v>
+      </c>
+      <c r="G86" s="28">
+        <v>0</v>
+      </c>
+      <c r="H86" s="28">
+        <v>0</v>
+      </c>
+      <c r="I86" s="28">
+        <v>109</v>
+      </c>
+      <c r="J86" s="28">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="87" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A87" s="29">
+        <v>43987</v>
+      </c>
+      <c r="B87" s="30">
+        <v>82876</v>
+      </c>
+      <c r="C87" s="31">
+        <v>715</v>
+      </c>
+      <c r="D87" s="31">
+        <v>1484</v>
+      </c>
+      <c r="E87" s="31">
+        <v>5</v>
+      </c>
+      <c r="F87" s="31">
+        <v>6</v>
+      </c>
+      <c r="G87" s="31">
+        <v>0</v>
+      </c>
+      <c r="H87" s="31">
+        <v>0</v>
+      </c>
+      <c r="I87" s="31">
+        <v>109</v>
+      </c>
+      <c r="J87" s="31">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="88" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A88" s="23">
+        <v>43988</v>
+      </c>
+      <c r="B88" s="24">
+        <v>83105</v>
+      </c>
+      <c r="C88" s="25">
+        <v>229</v>
+      </c>
+      <c r="D88" s="25">
+        <v>1485</v>
+      </c>
+      <c r="E88" s="25">
+        <v>1</v>
+      </c>
+      <c r="F88" s="25">
+        <v>5</v>
+      </c>
+      <c r="G88" s="25">
+        <v>0</v>
+      </c>
+      <c r="H88" s="25">
+        <v>1</v>
+      </c>
+      <c r="I88" s="25">
+        <v>109</v>
+      </c>
+      <c r="J88" s="25">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="89" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A89" s="29">
+        <v>43989</v>
+      </c>
+      <c r="B89" s="30">
+        <v>83316</v>
+      </c>
+      <c r="C89" s="31">
+        <v>211</v>
+      </c>
+      <c r="D89" s="31">
+        <v>1485</v>
+      </c>
+      <c r="E89" s="31">
+        <v>0</v>
+      </c>
+      <c r="F89" s="31">
+        <v>5</v>
+      </c>
+      <c r="G89" s="31">
+        <v>0</v>
+      </c>
+      <c r="H89" s="31">
+        <v>0</v>
+      </c>
+      <c r="I89" s="31">
+        <v>109</v>
+      </c>
+      <c r="J89" s="31">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="90" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A90" s="20">
+        <v>43990</v>
+      </c>
+      <c r="B90" s="21">
+        <v>84130</v>
+      </c>
+      <c r="C90" s="22">
+        <v>814</v>
+      </c>
+      <c r="D90" s="22">
+        <v>1486</v>
+      </c>
+      <c r="E90" s="22">
+        <v>1</v>
+      </c>
+      <c r="F90" s="22">
+        <v>6</v>
+      </c>
+      <c r="G90" s="22">
+        <v>0</v>
+      </c>
+      <c r="H90" s="22">
+        <v>0</v>
+      </c>
+      <c r="I90" s="22">
+        <v>109</v>
+      </c>
+      <c r="J90" s="22">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="91" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A91" s="20">
+        <v>43991</v>
+      </c>
+      <c r="B91" s="21">
+        <v>84868</v>
+      </c>
+      <c r="C91" s="22">
+        <v>738</v>
+      </c>
+      <c r="D91" s="22">
+        <v>1488</v>
+      </c>
+      <c r="E91" s="22">
+        <v>2</v>
+      </c>
+      <c r="F91" s="22">
+        <v>6</v>
+      </c>
+      <c r="G91" s="22">
+        <v>0</v>
+      </c>
+      <c r="H91" s="22">
+        <v>0</v>
+      </c>
+      <c r="I91" s="22">
+        <v>109</v>
+      </c>
+      <c r="J91" s="22">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="92" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A92" s="23">
+        <v>43992</v>
+      </c>
+      <c r="B92" s="24">
+        <v>85626</v>
+      </c>
+      <c r="C92" s="25">
+        <v>758</v>
+      </c>
+      <c r="D92" s="25">
+        <v>1488</v>
+      </c>
+      <c r="E92" s="25">
+        <v>0</v>
+      </c>
+      <c r="F92" s="25">
+        <v>6</v>
+      </c>
+      <c r="G92" s="25">
+        <v>0</v>
+      </c>
+      <c r="H92" s="25">
+        <v>0</v>
+      </c>
+      <c r="I92" s="25">
+        <v>109</v>
+      </c>
+      <c r="J92" s="25">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="93" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A93" s="29">
+        <v>43993</v>
+      </c>
+      <c r="B93" s="30">
+        <v>86328</v>
+      </c>
+      <c r="C93" s="31">
+        <v>702</v>
+      </c>
+      <c r="D93" s="31">
+        <v>1490</v>
+      </c>
+      <c r="E93" s="31">
+        <v>2</v>
+      </c>
+      <c r="F93" s="31">
+        <v>6</v>
+      </c>
+      <c r="G93" s="31">
+        <v>0</v>
+      </c>
+      <c r="H93" s="31">
+        <v>0</v>
+      </c>
+      <c r="I93" s="31">
+        <v>109</v>
+      </c>
+      <c r="J93" s="31">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="94" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A94" s="23">
+        <v>43994</v>
+      </c>
+      <c r="B94" s="24">
+        <v>87095</v>
+      </c>
+      <c r="C94" s="25">
+        <v>767</v>
+      </c>
+      <c r="D94" s="25">
+        <v>1492</v>
+      </c>
+      <c r="E94" s="25">
+        <v>2</v>
+      </c>
+      <c r="F94" s="25">
+        <v>6</v>
+      </c>
+      <c r="G94" s="25">
+        <v>0</v>
+      </c>
+      <c r="H94" s="25">
+        <v>0</v>
+      </c>
+      <c r="I94" s="25">
+        <v>109</v>
+      </c>
+      <c r="J94" s="25">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="95" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A95" s="29">
+        <v>43995</v>
+      </c>
+      <c r="B95" s="30">
+        <v>87386</v>
+      </c>
+      <c r="C95" s="31">
+        <v>291</v>
+      </c>
+      <c r="D95" s="31">
+        <v>1495</v>
+      </c>
+      <c r="E95" s="31">
+        <v>3</v>
+      </c>
+      <c r="F95" s="31">
+        <v>6</v>
+      </c>
+      <c r="G95" s="31">
+        <v>0</v>
+      </c>
+      <c r="H95" s="31">
+        <v>0</v>
+      </c>
+      <c r="I95" s="31">
+        <v>109</v>
+      </c>
+      <c r="J95" s="31">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="96" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A96" s="23">
+        <v>43996</v>
+      </c>
+      <c r="B96" s="24">
+        <v>87598</v>
+      </c>
+      <c r="C96" s="25">
+        <v>212</v>
+      </c>
+      <c r="D96" s="25">
+        <v>1496</v>
+      </c>
+      <c r="E96" s="25">
+        <v>1</v>
+      </c>
+      <c r="F96" s="25">
+        <v>7</v>
+      </c>
+      <c r="G96" s="25">
+        <v>1</v>
+      </c>
+      <c r="H96" s="25">
+        <v>0</v>
+      </c>
+      <c r="I96" s="25">
+        <v>109</v>
+      </c>
+      <c r="J96" s="25">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="97" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A97" s="20">
+        <v>43997</v>
+      </c>
+      <c r="B97" s="21">
+        <v>88165</v>
+      </c>
+      <c r="C97" s="22">
+        <v>567</v>
+      </c>
+      <c r="D97" s="22">
+        <v>1499</v>
+      </c>
+      <c r="E97" s="22">
+        <v>3</v>
+      </c>
+      <c r="F97" s="22">
+        <v>7</v>
+      </c>
+      <c r="G97" s="22">
+        <v>1</v>
+      </c>
+      <c r="H97" s="22">
+        <v>0</v>
+      </c>
+      <c r="I97" s="22">
+        <v>109</v>
+      </c>
+      <c r="J97" s="22">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="98" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A98" s="20">
+        <v>43998</v>
+      </c>
+      <c r="B98" s="21">
+        <v>89151</v>
+      </c>
+      <c r="C98" s="22">
+        <v>986</v>
+      </c>
+      <c r="D98" s="22">
+        <v>1503</v>
+      </c>
+      <c r="E98" s="22">
+        <v>4</v>
+      </c>
+      <c r="F98" s="22">
+        <v>7</v>
+      </c>
+      <c r="G98" s="22">
+        <v>1</v>
+      </c>
+      <c r="H98" s="22">
+        <v>0</v>
+      </c>
+      <c r="I98" s="22">
+        <v>109</v>
+      </c>
+      <c r="J98" s="22">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="99" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A99" s="29">
+        <v>43999</v>
+      </c>
+      <c r="B99" s="30">
+        <v>90103</v>
+      </c>
+      <c r="C99" s="31">
+        <v>952</v>
+      </c>
+      <c r="D99" s="31">
+        <v>1511</v>
+      </c>
+      <c r="E99" s="31">
+        <v>8</v>
+      </c>
+      <c r="F99" s="31">
+        <v>6</v>
+      </c>
+      <c r="G99" s="31">
+        <v>1</v>
+      </c>
+      <c r="H99" s="31">
+        <v>1</v>
+      </c>
+      <c r="I99" s="31">
+        <v>109</v>
+      </c>
+      <c r="J99" s="31">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="100" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A100" s="20">
+        <v>44000</v>
+      </c>
+      <c r="B100" s="21">
+        <v>91005</v>
+      </c>
+      <c r="C100" s="22">
+        <v>902</v>
+      </c>
+      <c r="D100" s="22">
+        <v>1513</v>
+      </c>
+      <c r="E100" s="22">
+        <v>2</v>
+      </c>
+      <c r="F100" s="22">
+        <v>8</v>
+      </c>
+      <c r="G100" s="22">
+        <v>1</v>
+      </c>
+      <c r="H100" s="22">
+        <v>0</v>
+      </c>
+      <c r="I100" s="22">
+        <v>109</v>
+      </c>
+      <c r="J100" s="22">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="101" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A101" s="29">
+        <v>44001</v>
+      </c>
+      <c r="B101" s="30">
+        <v>92152</v>
+      </c>
+      <c r="C101" s="31">
+        <v>1147</v>
+      </c>
+      <c r="D101" s="31">
+        <v>1519</v>
+      </c>
+      <c r="E101" s="31">
+        <v>6</v>
+      </c>
+      <c r="F101" s="31">
+        <v>6</v>
+      </c>
+      <c r="G101" s="31">
+        <v>1</v>
+      </c>
+      <c r="H101" s="31">
+        <v>2</v>
+      </c>
+      <c r="I101" s="31">
+        <v>109</v>
+      </c>
+      <c r="J101" s="31">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="102" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A102" s="23">
+        <v>44002</v>
+      </c>
+      <c r="B102" s="24">
+        <v>92919</v>
+      </c>
+      <c r="C102" s="25">
+        <v>758</v>
+      </c>
+      <c r="D102" s="25">
+        <v>1520</v>
+      </c>
+      <c r="E102" s="25">
+        <v>1</v>
+      </c>
+      <c r="F102" s="25">
+        <v>6</v>
+      </c>
+      <c r="G102" s="25">
+        <v>1</v>
+      </c>
+      <c r="H102" s="25">
+        <v>2</v>
+      </c>
+      <c r="I102" s="25">
+        <v>109</v>
+      </c>
+      <c r="J102" s="25">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="103" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A103" s="29">
+        <v>44003</v>
+      </c>
+      <c r="B103" s="30">
+        <v>93181</v>
+      </c>
+      <c r="C103" s="31">
+        <v>271</v>
+      </c>
+      <c r="D103" s="31">
+        <v>1521</v>
+      </c>
+      <c r="E103" s="31">
+        <v>1</v>
+      </c>
+      <c r="F103" s="31">
+        <v>6</v>
+      </c>
+      <c r="G103" s="31">
+        <v>1</v>
+      </c>
+      <c r="H103" s="31">
+        <v>0</v>
+      </c>
+      <c r="I103" s="31">
+        <v>109</v>
+      </c>
+      <c r="J103" s="31">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="104" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A104" s="29">
+        <v>44004</v>
+      </c>
+      <c r="B104" s="30">
+        <v>94165</v>
+      </c>
+      <c r="C104" s="31">
+        <v>984</v>
+      </c>
+      <c r="D104" s="31">
+        <v>1534</v>
+      </c>
+      <c r="E104" s="31">
+        <v>13</v>
+      </c>
+      <c r="F104" s="31">
+        <v>5</v>
+      </c>
+      <c r="G104" s="31">
+        <v>1</v>
+      </c>
+      <c r="H104" s="31">
+        <v>1</v>
+      </c>
+      <c r="I104" s="31">
+        <v>109</v>
+      </c>
+      <c r="J104" s="31">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="105" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A105" s="29">
+        <v>44005</v>
+      </c>
+      <c r="B105" s="30">
+        <v>95387</v>
+      </c>
+      <c r="C105" s="31">
+        <v>1222</v>
+      </c>
+      <c r="D105" s="31">
+        <v>1541</v>
+      </c>
+      <c r="E105" s="31">
+        <v>7</v>
+      </c>
+      <c r="F105" s="31">
+        <v>7</v>
+      </c>
+      <c r="G105" s="31">
+        <v>2</v>
+      </c>
+      <c r="H105" s="31">
+        <v>0</v>
+      </c>
+      <c r="I105" s="31" t="s">
+        <v>10</v>
+      </c>
+      <c r="J105" s="31">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="106" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A106" s="23">
+        <v>44006</v>
+      </c>
+      <c r="B106" s="24">
+        <v>96599</v>
+      </c>
+      <c r="C106" s="25">
+        <v>1212</v>
+      </c>
+      <c r="D106" s="25">
+        <v>1547</v>
+      </c>
+      <c r="E106" s="25">
+        <v>6</v>
+      </c>
+      <c r="F106" s="25">
+        <v>7</v>
+      </c>
+      <c r="G106" s="25">
+        <v>2</v>
+      </c>
+      <c r="H106" s="25">
+        <v>0</v>
+      </c>
+      <c r="I106" s="25" t="s">
+        <v>10</v>
+      </c>
+      <c r="J106" s="25">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="107" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A107" s="29">
+        <v>44007</v>
+      </c>
+      <c r="B107" s="30">
+        <v>97442</v>
+      </c>
+      <c r="C107" s="31">
+        <v>843</v>
+      </c>
+      <c r="D107" s="31">
+        <v>1558</v>
+      </c>
+      <c r="E107" s="31">
+        <v>11</v>
+      </c>
+      <c r="F107" s="31">
+        <v>8</v>
+      </c>
+      <c r="G107" s="31">
+        <v>2</v>
+      </c>
+      <c r="H107" s="31">
+        <v>0</v>
+      </c>
+      <c r="I107" s="31" t="s">
+        <v>10</v>
+      </c>
+      <c r="J107" s="31">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="108" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A108" s="29">
+        <v>44008</v>
+      </c>
+      <c r="B108" s="30">
+        <v>98320</v>
+      </c>
+      <c r="C108" s="31">
+        <v>878</v>
+      </c>
+      <c r="D108" s="31">
+        <v>1572</v>
+      </c>
+      <c r="E108" s="31">
+        <v>14</v>
+      </c>
+      <c r="F108" s="31">
+        <v>8</v>
+      </c>
+      <c r="G108" s="31">
+        <v>1</v>
+      </c>
+      <c r="H108" s="31">
+        <v>0</v>
+      </c>
+      <c r="I108" s="31" t="s">
+        <v>10</v>
+      </c>
+      <c r="J108" s="31">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="109" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A109" s="29">
+        <v>44009</v>
+      </c>
+      <c r="B109" s="30">
+        <v>98945</v>
+      </c>
+      <c r="C109" s="31">
+        <v>625</v>
+      </c>
+      <c r="D109" s="31">
+        <v>1581</v>
+      </c>
+      <c r="E109" s="31">
+        <v>9</v>
+      </c>
+      <c r="F109" s="31">
+        <v>7</v>
+      </c>
+      <c r="G109" s="31">
+        <v>0</v>
+      </c>
+      <c r="H109" s="31">
+        <v>1</v>
+      </c>
+      <c r="I109" s="31" t="s">
+        <v>10</v>
+      </c>
+      <c r="J109" s="31">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="110" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A110" s="29">
+        <v>44010</v>
+      </c>
+      <c r="B110" s="30">
+        <v>99245</v>
+      </c>
+      <c r="C110" s="31">
+        <v>300</v>
+      </c>
+      <c r="D110" s="31">
+        <v>1585</v>
+      </c>
+      <c r="E110" s="31">
+        <v>4</v>
+      </c>
+      <c r="F110" s="31">
+        <v>8</v>
+      </c>
+      <c r="G110" s="31">
+        <v>0</v>
+      </c>
+      <c r="H110" s="31">
+        <v>0</v>
+      </c>
+      <c r="I110" s="31" t="s">
+        <v>10</v>
+      </c>
+      <c r="J110" s="31">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="111" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A111" s="29">
+        <v>44011</v>
+      </c>
+      <c r="B111" s="30">
+        <v>100330</v>
+      </c>
+      <c r="C111" s="31">
+        <v>1085</v>
+      </c>
+      <c r="D111" s="31">
+        <v>1600</v>
+      </c>
+      <c r="E111" s="31">
+        <v>15</v>
+      </c>
+      <c r="F111" s="31">
+        <v>8</v>
+      </c>
+      <c r="G111" s="31">
+        <v>0</v>
+      </c>
+      <c r="H111" s="31">
+        <v>0</v>
+      </c>
+      <c r="I111" s="31" t="s">
+        <v>10</v>
+      </c>
+      <c r="J111" s="31">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="112" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A112" s="20">
+        <v>44012</v>
+      </c>
+      <c r="B112" s="21">
+        <v>101729</v>
+      </c>
+      <c r="C112" s="22">
+        <v>1399</v>
+      </c>
+      <c r="D112" s="22">
+        <v>1613</v>
+      </c>
+      <c r="E112" s="22">
+        <v>13</v>
+      </c>
+      <c r="F112" s="22">
+        <v>8</v>
+      </c>
+      <c r="G112" s="22">
+        <v>0</v>
+      </c>
+      <c r="H112" s="22">
+        <v>0</v>
+      </c>
+      <c r="I112" s="22" t="s">
+        <v>10</v>
+      </c>
+      <c r="J112" s="22">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="113" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A113" s="20">
+        <v>44013</v>
+      </c>
+      <c r="B113" s="21">
+        <v>102927</v>
+      </c>
+      <c r="C113" s="22">
+        <v>1198</v>
+      </c>
+      <c r="D113" s="22">
+        <v>1633</v>
+      </c>
+      <c r="E113" s="22">
+        <v>21</v>
+      </c>
+      <c r="F113" s="22">
+        <v>9</v>
+      </c>
+      <c r="G113" s="22">
+        <v>0</v>
+      </c>
+      <c r="H113" s="22">
+        <v>0</v>
+      </c>
+      <c r="I113" s="22" t="s">
+        <v>10</v>
+      </c>
+      <c r="J113" s="22">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="114" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A114" s="20">
+        <v>44014</v>
+      </c>
+      <c r="B114" s="21">
+        <v>104201</v>
+      </c>
+      <c r="C114" s="22">
+        <v>1274</v>
+      </c>
+      <c r="D114" s="22">
+        <v>1649</v>
+      </c>
+      <c r="E114" s="22">
+        <v>16</v>
+      </c>
+      <c r="F114" s="22">
+        <v>10</v>
+      </c>
+      <c r="G114" s="22">
+        <v>0</v>
+      </c>
+      <c r="H114" s="22">
+        <v>0</v>
+      </c>
+      <c r="I114" s="22" t="s">
+        <v>10</v>
+      </c>
+      <c r="J114" s="22">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="115" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A115" s="20">
+        <v>44015</v>
+      </c>
+      <c r="B115" s="21">
+        <v>105652</v>
+      </c>
+      <c r="C115" s="22">
+        <v>1456</v>
+      </c>
+      <c r="D115" s="22">
+        <v>1679</v>
+      </c>
+      <c r="E115" s="22">
+        <v>30</v>
+      </c>
+      <c r="F115" s="22">
+        <v>6</v>
+      </c>
+      <c r="G115" s="22">
+        <v>0</v>
+      </c>
+      <c r="H115" s="22">
+        <v>4</v>
+      </c>
+      <c r="I115" s="22" t="s">
+        <v>10</v>
+      </c>
+      <c r="J115" s="22">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="116" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A116" s="20">
+        <v>44016</v>
+      </c>
+      <c r="B116" s="21">
+        <v>106368</v>
+      </c>
+      <c r="C116" s="22">
+        <v>716</v>
+      </c>
+      <c r="D116" s="22">
+        <v>1700</v>
+      </c>
+      <c r="E116" s="22">
+        <v>21</v>
+      </c>
+      <c r="F116" s="22">
+        <v>6</v>
+      </c>
+      <c r="G116" s="22">
+        <v>0</v>
+      </c>
+      <c r="H116" s="22">
+        <v>1</v>
+      </c>
+      <c r="I116" s="22" t="s">
+        <v>10</v>
+      </c>
+      <c r="J116" s="22">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="117" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A117" s="29">
+        <v>44017</v>
+      </c>
+      <c r="B117" s="30">
+        <v>106898</v>
+      </c>
+      <c r="C117" s="31">
+        <v>530</v>
+      </c>
+      <c r="D117" s="31">
+        <v>1716</v>
+      </c>
+      <c r="E117" s="31">
+        <v>16</v>
+      </c>
+      <c r="F117" s="31">
+        <v>11</v>
+      </c>
+      <c r="G117" s="31">
+        <v>0</v>
+      </c>
+      <c r="H117" s="31">
+        <v>0</v>
+      </c>
+      <c r="I117" s="31" t="s">
+        <v>10</v>
+      </c>
+      <c r="J117" s="31">
+        <v>0</v>
+      </c>
+    </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>

</xml_diff>

<commit_message>
Data updated by GitHub Bot (2020-07-07 12)
</commit_message>
<xml_diff>
--- a/output/snapshot/fdcf2531-4c3e-5c02-b63c-ee160ead6dea.xlsx
+++ b/output/snapshot/fdcf2531-4c3e-5c02-b63c-ee160ead6dea.xlsx
@@ -1,16 +1,15 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="21929"/>
-  <workbookPr/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
+  <fileVersion appName="xl" lastEdited="6" lowestEdited="6" rupBuild="14420"/>
+  <workbookPr defaultThemeVersion="164011"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="I:\AKTUALNI PODATKI - KORONA\Za objavo na GOV.SI\ang\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{1E6DD62F-2BE2-47DC-A7ED-9B57C1589256}" xr6:coauthVersionLast="44" xr6:coauthVersionMax="44" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840"/>
   </bookViews>
   <sheets>
     <sheet name="Covid-19 podatki" sheetId="1" r:id="rId1"/>
@@ -60,11 +59,11 @@
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" mc:Ignorable="x14ac x16r2">
   <numFmts count="1">
     <numFmt numFmtId="164" formatCode="d/\ m/\ yyyy;@"/>
   </numFmts>
-  <fonts count="4" x14ac:knownFonts="1">
+  <fonts count="5" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -93,6 +92,13 @@
       <name val="Calibri Light"/>
       <scheme val="major"/>
     </font>
+    <font>
+      <sz val="10"/>
+      <color theme="1"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
   </fonts>
   <fills count="3">
     <fill>
@@ -108,7 +114,7 @@
       </patternFill>
     </fill>
   </fills>
-  <borders count="2">
+  <borders count="3">
     <border>
       <left/>
       <right/>
@@ -129,11 +135,26 @@
       <bottom/>
       <diagonal/>
     </border>
+    <border>
+      <left style="thin">
+        <color theme="4"/>
+      </left>
+      <right style="thin">
+        <color theme="4"/>
+      </right>
+      <top style="thin">
+        <color theme="4"/>
+      </top>
+      <bottom style="thin">
+        <color theme="4"/>
+      </bottom>
+      <diagonal/>
+    </border>
   </borders>
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="26">
+  <cellXfs count="32">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="49" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyAlignment="1" applyProtection="1">
       <alignment horizontal="left" vertical="top"/>
@@ -208,6 +229,24 @@
       <alignment horizontal="right"/>
     </xf>
     <xf numFmtId="0" fontId="3" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="right"/>
+    </xf>
+    <xf numFmtId="164" fontId="4" fillId="2" borderId="2" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="right" vertical="top"/>
+    </xf>
+    <xf numFmtId="3" fontId="4" fillId="2" borderId="2" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="right"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="2" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="right"/>
+    </xf>
+    <xf numFmtId="164" fontId="3" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="right" vertical="top"/>
+    </xf>
+    <xf numFmtId="3" fontId="3" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="right"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="right"/>
     </xf>
   </cellXfs>
@@ -399,8 +438,8 @@
 </file>
 
 <file path=xl/tables/table1.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="1" xr:uid="{00000000-000C-0000-FFFF-FFFF00000000}" name="Tabela1" displayName="Tabela1" ref="A1:J75" totalsRowShown="0" headerRowDxfId="11" dataDxfId="10">
-  <autoFilter ref="A1:J75" xr:uid="{00000000-0009-0000-0100-000001000000}">
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="1" name="Tabela1" displayName="Tabela1" ref="A1:J118" totalsRowShown="0" headerRowDxfId="11" dataDxfId="10">
+  <autoFilter ref="A1:J118">
     <filterColumn colId="0" hiddenButton="1"/>
     <filterColumn colId="1" hiddenButton="1"/>
     <filterColumn colId="2" hiddenButton="1"/>
@@ -413,16 +452,16 @@
     <filterColumn colId="9" hiddenButton="1"/>
   </autoFilter>
   <tableColumns count="10">
-    <tableColumn id="1" xr3:uid="{00000000-0010-0000-0000-000001000000}" name="Date" dataDxfId="9"/>
-    <tableColumn id="2" xr3:uid="{00000000-0010-0000-0000-000002000000}" name="Tested (all)" dataDxfId="8"/>
-    <tableColumn id="3" xr3:uid="{00000000-0010-0000-0000-000003000000}" name="Tested (daily)" dataDxfId="7"/>
-    <tableColumn id="4" xr3:uid="{00000000-0010-0000-0000-000004000000}" name="Positive (all)" dataDxfId="6"/>
-    <tableColumn id="5" xr3:uid="{00000000-0010-0000-0000-000005000000}" name="Positive (daily)" dataDxfId="5"/>
-    <tableColumn id="6" xr3:uid="{00000000-0010-0000-0000-000006000000}" name="All hospitalized on certain day" dataDxfId="4"/>
-    <tableColumn id="7" xr3:uid="{00000000-0010-0000-0000-000007000000}" name="All persons in intensive care on certain day" dataDxfId="3"/>
-    <tableColumn id="10" xr3:uid="{00000000-0010-0000-0000-00000A000000}" name="Discharged" dataDxfId="2"/>
-    <tableColumn id="8" xr3:uid="{00000000-0010-0000-0000-000008000000}" name="Deaths (all)" dataDxfId="1"/>
-    <tableColumn id="9" xr3:uid="{00000000-0010-0000-0000-000009000000}" name="Deaths (daily)" dataDxfId="0"/>
+    <tableColumn id="1" name="Date" dataDxfId="9"/>
+    <tableColumn id="2" name="Tested (all)" dataDxfId="8"/>
+    <tableColumn id="3" name="Tested (daily)" dataDxfId="7"/>
+    <tableColumn id="4" name="Positive (all)" dataDxfId="6"/>
+    <tableColumn id="5" name="Positive (daily)" dataDxfId="5"/>
+    <tableColumn id="6" name="All hospitalized on certain day" dataDxfId="4"/>
+    <tableColumn id="7" name="All persons in intensive care on certain day" dataDxfId="3"/>
+    <tableColumn id="10" name="Discharged" dataDxfId="2"/>
+    <tableColumn id="8" name="Deaths (all)" dataDxfId="1"/>
+    <tableColumn id="9" name="Deaths (daily)" dataDxfId="0"/>
   </tableColumns>
   <tableStyleInfo name="TableStyleLight16" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
   <extLst>
@@ -695,11 +734,11 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:J75"/>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <dimension ref="A1:J118"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A40" zoomScale="89" zoomScaleNormal="89" workbookViewId="0">
-      <selection activeCell="J74" sqref="J74"/>
+    <sheetView tabSelected="1" topLeftCell="A83" zoomScale="89" zoomScaleNormal="89" workbookViewId="0">
+      <selection activeCell="I117" sqref="I117"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -3117,6 +3156,1382 @@
         <v>0</v>
       </c>
     </row>
+    <row r="76" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A76" s="20">
+        <v>43976</v>
+      </c>
+      <c r="B76" s="21">
+        <v>75770</v>
+      </c>
+      <c r="C76" s="22">
+        <v>754</v>
+      </c>
+      <c r="D76" s="22">
+        <v>1469</v>
+      </c>
+      <c r="E76" s="22">
+        <v>0</v>
+      </c>
+      <c r="F76" s="22">
+        <v>9</v>
+      </c>
+      <c r="G76" s="22">
+        <v>2</v>
+      </c>
+      <c r="H76" s="22">
+        <v>6</v>
+      </c>
+      <c r="I76" s="22">
+        <v>108</v>
+      </c>
+      <c r="J76" s="22">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="77" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A77" s="20">
+        <v>43977</v>
+      </c>
+      <c r="B77" s="21">
+        <v>76579</v>
+      </c>
+      <c r="C77" s="22">
+        <v>809</v>
+      </c>
+      <c r="D77" s="22">
+        <v>1471</v>
+      </c>
+      <c r="E77" s="22">
+        <v>2</v>
+      </c>
+      <c r="F77" s="22">
+        <v>8</v>
+      </c>
+      <c r="G77" s="22">
+        <v>2</v>
+      </c>
+      <c r="H77" s="22">
+        <v>2</v>
+      </c>
+      <c r="I77" s="22">
+        <v>108</v>
+      </c>
+      <c r="J77" s="22">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="78" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A78" s="20">
+        <v>43978</v>
+      </c>
+      <c r="B78" s="21">
+        <v>77210</v>
+      </c>
+      <c r="C78" s="22">
+        <v>631</v>
+      </c>
+      <c r="D78" s="22">
+        <v>1473</v>
+      </c>
+      <c r="E78" s="22">
+        <v>2</v>
+      </c>
+      <c r="F78" s="22">
+        <v>7</v>
+      </c>
+      <c r="G78" s="22">
+        <v>2</v>
+      </c>
+      <c r="H78" s="22">
+        <v>1</v>
+      </c>
+      <c r="I78" s="22">
+        <v>108</v>
+      </c>
+      <c r="J78" s="22">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="79" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A79" s="20">
+        <v>43979</v>
+      </c>
+      <c r="B79" s="21">
+        <v>77916</v>
+      </c>
+      <c r="C79" s="22">
+        <v>706</v>
+      </c>
+      <c r="D79" s="22">
+        <v>1473</v>
+      </c>
+      <c r="E79" s="22">
+        <v>0</v>
+      </c>
+      <c r="F79" s="22">
+        <v>7</v>
+      </c>
+      <c r="G79" s="22">
+        <v>2</v>
+      </c>
+      <c r="H79" s="22">
+        <v>0</v>
+      </c>
+      <c r="I79" s="22">
+        <v>108</v>
+      </c>
+      <c r="J79" s="22">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="80" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A80" s="20">
+        <v>43980</v>
+      </c>
+      <c r="B80" s="21">
+        <v>78529</v>
+      </c>
+      <c r="C80" s="22">
+        <v>613</v>
+      </c>
+      <c r="D80" s="22">
+        <v>1473</v>
+      </c>
+      <c r="E80" s="22">
+        <v>0</v>
+      </c>
+      <c r="F80" s="22">
+        <v>7</v>
+      </c>
+      <c r="G80" s="22">
+        <v>2</v>
+      </c>
+      <c r="H80" s="22">
+        <v>0</v>
+      </c>
+      <c r="I80" s="22">
+        <v>108</v>
+      </c>
+      <c r="J80" s="22">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="81" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A81" s="20">
+        <v>43981</v>
+      </c>
+      <c r="B81" s="22">
+        <v>78793</v>
+      </c>
+      <c r="C81" s="22">
+        <v>264</v>
+      </c>
+      <c r="D81" s="22">
+        <v>1473</v>
+      </c>
+      <c r="E81" s="22">
+        <v>0</v>
+      </c>
+      <c r="F81" s="22">
+        <v>6</v>
+      </c>
+      <c r="G81" s="22">
+        <v>2</v>
+      </c>
+      <c r="H81" s="22">
+        <v>1</v>
+      </c>
+      <c r="I81" s="22">
+        <v>108</v>
+      </c>
+      <c r="J81" s="22">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="82" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A82" s="20">
+        <v>43982</v>
+      </c>
+      <c r="B82" s="21">
+        <v>79039</v>
+      </c>
+      <c r="C82" s="22">
+        <v>246</v>
+      </c>
+      <c r="D82" s="22">
+        <v>1473</v>
+      </c>
+      <c r="E82" s="22">
+        <v>0</v>
+      </c>
+      <c r="F82" s="22">
+        <v>5</v>
+      </c>
+      <c r="G82" s="22">
+        <v>1</v>
+      </c>
+      <c r="H82" s="22">
+        <v>0</v>
+      </c>
+      <c r="I82" s="22">
+        <v>109</v>
+      </c>
+      <c r="J82" s="22">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="83" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A83" s="20">
+        <v>43983</v>
+      </c>
+      <c r="B83" s="21">
+        <v>79698</v>
+      </c>
+      <c r="C83" s="22">
+        <v>659</v>
+      </c>
+      <c r="D83" s="22">
+        <v>1475</v>
+      </c>
+      <c r="E83" s="22">
+        <v>2</v>
+      </c>
+      <c r="F83" s="22">
+        <v>5</v>
+      </c>
+      <c r="G83" s="22">
+        <v>1</v>
+      </c>
+      <c r="H83" s="22">
+        <v>0</v>
+      </c>
+      <c r="I83" s="22">
+        <v>109</v>
+      </c>
+      <c r="J83" s="22">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="84" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A84" s="20">
+        <v>43984</v>
+      </c>
+      <c r="B84" s="21">
+        <v>80505</v>
+      </c>
+      <c r="C84" s="22">
+        <v>807</v>
+      </c>
+      <c r="D84" s="22">
+        <v>1477</v>
+      </c>
+      <c r="E84" s="22">
+        <v>2</v>
+      </c>
+      <c r="F84" s="22">
+        <v>5</v>
+      </c>
+      <c r="G84" s="22">
+        <v>0</v>
+      </c>
+      <c r="H84" s="22">
+        <v>0</v>
+      </c>
+      <c r="I84" s="22">
+        <v>109</v>
+      </c>
+      <c r="J84" s="22">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="85" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A85" s="20">
+        <v>43985</v>
+      </c>
+      <c r="B85" s="21">
+        <v>81333</v>
+      </c>
+      <c r="C85" s="22">
+        <v>828</v>
+      </c>
+      <c r="D85" s="22">
+        <v>1477</v>
+      </c>
+      <c r="E85" s="22">
+        <v>0</v>
+      </c>
+      <c r="F85" s="22">
+        <v>5</v>
+      </c>
+      <c r="G85" s="22">
+        <v>0</v>
+      </c>
+      <c r="H85" s="22">
+        <v>0</v>
+      </c>
+      <c r="I85" s="22">
+        <v>109</v>
+      </c>
+      <c r="J85" s="22">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="86" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A86" s="26">
+        <v>43986</v>
+      </c>
+      <c r="B86" s="27">
+        <v>82161</v>
+      </c>
+      <c r="C86" s="28">
+        <v>828</v>
+      </c>
+      <c r="D86" s="28">
+        <v>1479</v>
+      </c>
+      <c r="E86" s="28">
+        <v>2</v>
+      </c>
+      <c r="F86" s="28">
+        <v>6</v>
+      </c>
+      <c r="G86" s="28">
+        <v>0</v>
+      </c>
+      <c r="H86" s="28">
+        <v>0</v>
+      </c>
+      <c r="I86" s="28">
+        <v>109</v>
+      </c>
+      <c r="J86" s="28">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="87" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A87" s="29">
+        <v>43987</v>
+      </c>
+      <c r="B87" s="30">
+        <v>82876</v>
+      </c>
+      <c r="C87" s="31">
+        <v>715</v>
+      </c>
+      <c r="D87" s="31">
+        <v>1484</v>
+      </c>
+      <c r="E87" s="31">
+        <v>5</v>
+      </c>
+      <c r="F87" s="31">
+        <v>6</v>
+      </c>
+      <c r="G87" s="31">
+        <v>0</v>
+      </c>
+      <c r="H87" s="31">
+        <v>0</v>
+      </c>
+      <c r="I87" s="31">
+        <v>109</v>
+      </c>
+      <c r="J87" s="31">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="88" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A88" s="23">
+        <v>43988</v>
+      </c>
+      <c r="B88" s="24">
+        <v>83105</v>
+      </c>
+      <c r="C88" s="25">
+        <v>229</v>
+      </c>
+      <c r="D88" s="25">
+        <v>1485</v>
+      </c>
+      <c r="E88" s="25">
+        <v>1</v>
+      </c>
+      <c r="F88" s="25">
+        <v>5</v>
+      </c>
+      <c r="G88" s="25">
+        <v>0</v>
+      </c>
+      <c r="H88" s="25">
+        <v>1</v>
+      </c>
+      <c r="I88" s="25">
+        <v>109</v>
+      </c>
+      <c r="J88" s="25">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="89" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A89" s="29">
+        <v>43989</v>
+      </c>
+      <c r="B89" s="30">
+        <v>83316</v>
+      </c>
+      <c r="C89" s="31">
+        <v>211</v>
+      </c>
+      <c r="D89" s="31">
+        <v>1485</v>
+      </c>
+      <c r="E89" s="31">
+        <v>0</v>
+      </c>
+      <c r="F89" s="31">
+        <v>5</v>
+      </c>
+      <c r="G89" s="31">
+        <v>0</v>
+      </c>
+      <c r="H89" s="31">
+        <v>0</v>
+      </c>
+      <c r="I89" s="31">
+        <v>109</v>
+      </c>
+      <c r="J89" s="31">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="90" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A90" s="20">
+        <v>43990</v>
+      </c>
+      <c r="B90" s="21">
+        <v>84130</v>
+      </c>
+      <c r="C90" s="22">
+        <v>814</v>
+      </c>
+      <c r="D90" s="22">
+        <v>1486</v>
+      </c>
+      <c r="E90" s="22">
+        <v>1</v>
+      </c>
+      <c r="F90" s="22">
+        <v>6</v>
+      </c>
+      <c r="G90" s="22">
+        <v>0</v>
+      </c>
+      <c r="H90" s="22">
+        <v>0</v>
+      </c>
+      <c r="I90" s="22">
+        <v>109</v>
+      </c>
+      <c r="J90" s="22">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="91" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A91" s="20">
+        <v>43991</v>
+      </c>
+      <c r="B91" s="21">
+        <v>84868</v>
+      </c>
+      <c r="C91" s="22">
+        <v>738</v>
+      </c>
+      <c r="D91" s="22">
+        <v>1488</v>
+      </c>
+      <c r="E91" s="22">
+        <v>2</v>
+      </c>
+      <c r="F91" s="22">
+        <v>6</v>
+      </c>
+      <c r="G91" s="22">
+        <v>0</v>
+      </c>
+      <c r="H91" s="22">
+        <v>0</v>
+      </c>
+      <c r="I91" s="22">
+        <v>109</v>
+      </c>
+      <c r="J91" s="22">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="92" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A92" s="23">
+        <v>43992</v>
+      </c>
+      <c r="B92" s="24">
+        <v>85626</v>
+      </c>
+      <c r="C92" s="25">
+        <v>758</v>
+      </c>
+      <c r="D92" s="25">
+        <v>1488</v>
+      </c>
+      <c r="E92" s="25">
+        <v>0</v>
+      </c>
+      <c r="F92" s="25">
+        <v>6</v>
+      </c>
+      <c r="G92" s="25">
+        <v>0</v>
+      </c>
+      <c r="H92" s="25">
+        <v>0</v>
+      </c>
+      <c r="I92" s="25">
+        <v>109</v>
+      </c>
+      <c r="J92" s="25">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="93" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A93" s="29">
+        <v>43993</v>
+      </c>
+      <c r="B93" s="30">
+        <v>86328</v>
+      </c>
+      <c r="C93" s="31">
+        <v>702</v>
+      </c>
+      <c r="D93" s="31">
+        <v>1490</v>
+      </c>
+      <c r="E93" s="31">
+        <v>2</v>
+      </c>
+      <c r="F93" s="31">
+        <v>6</v>
+      </c>
+      <c r="G93" s="31">
+        <v>0</v>
+      </c>
+      <c r="H93" s="31">
+        <v>0</v>
+      </c>
+      <c r="I93" s="31">
+        <v>109</v>
+      </c>
+      <c r="J93" s="31">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="94" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A94" s="23">
+        <v>43994</v>
+      </c>
+      <c r="B94" s="24">
+        <v>87095</v>
+      </c>
+      <c r="C94" s="25">
+        <v>767</v>
+      </c>
+      <c r="D94" s="25">
+        <v>1492</v>
+      </c>
+      <c r="E94" s="25">
+        <v>2</v>
+      </c>
+      <c r="F94" s="25">
+        <v>6</v>
+      </c>
+      <c r="G94" s="25">
+        <v>0</v>
+      </c>
+      <c r="H94" s="25">
+        <v>0</v>
+      </c>
+      <c r="I94" s="25">
+        <v>109</v>
+      </c>
+      <c r="J94" s="25">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="95" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A95" s="29">
+        <v>43995</v>
+      </c>
+      <c r="B95" s="30">
+        <v>87386</v>
+      </c>
+      <c r="C95" s="31">
+        <v>291</v>
+      </c>
+      <c r="D95" s="31">
+        <v>1495</v>
+      </c>
+      <c r="E95" s="31">
+        <v>3</v>
+      </c>
+      <c r="F95" s="31">
+        <v>6</v>
+      </c>
+      <c r="G95" s="31">
+        <v>0</v>
+      </c>
+      <c r="H95" s="31">
+        <v>0</v>
+      </c>
+      <c r="I95" s="31">
+        <v>109</v>
+      </c>
+      <c r="J95" s="31">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="96" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A96" s="23">
+        <v>43996</v>
+      </c>
+      <c r="B96" s="24">
+        <v>87598</v>
+      </c>
+      <c r="C96" s="25">
+        <v>212</v>
+      </c>
+      <c r="D96" s="25">
+        <v>1496</v>
+      </c>
+      <c r="E96" s="25">
+        <v>1</v>
+      </c>
+      <c r="F96" s="25">
+        <v>7</v>
+      </c>
+      <c r="G96" s="25">
+        <v>1</v>
+      </c>
+      <c r="H96" s="25">
+        <v>0</v>
+      </c>
+      <c r="I96" s="25">
+        <v>109</v>
+      </c>
+      <c r="J96" s="25">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="97" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A97" s="20">
+        <v>43997</v>
+      </c>
+      <c r="B97" s="21">
+        <v>88165</v>
+      </c>
+      <c r="C97" s="22">
+        <v>567</v>
+      </c>
+      <c r="D97" s="22">
+        <v>1499</v>
+      </c>
+      <c r="E97" s="22">
+        <v>3</v>
+      </c>
+      <c r="F97" s="22">
+        <v>7</v>
+      </c>
+      <c r="G97" s="22">
+        <v>1</v>
+      </c>
+      <c r="H97" s="22">
+        <v>0</v>
+      </c>
+      <c r="I97" s="22">
+        <v>109</v>
+      </c>
+      <c r="J97" s="22">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="98" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A98" s="20">
+        <v>43998</v>
+      </c>
+      <c r="B98" s="21">
+        <v>89151</v>
+      </c>
+      <c r="C98" s="22">
+        <v>986</v>
+      </c>
+      <c r="D98" s="22">
+        <v>1503</v>
+      </c>
+      <c r="E98" s="22">
+        <v>4</v>
+      </c>
+      <c r="F98" s="22">
+        <v>7</v>
+      </c>
+      <c r="G98" s="22">
+        <v>1</v>
+      </c>
+      <c r="H98" s="22">
+        <v>0</v>
+      </c>
+      <c r="I98" s="22">
+        <v>109</v>
+      </c>
+      <c r="J98" s="22">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="99" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A99" s="29">
+        <v>43999</v>
+      </c>
+      <c r="B99" s="30">
+        <v>90103</v>
+      </c>
+      <c r="C99" s="31">
+        <v>952</v>
+      </c>
+      <c r="D99" s="31">
+        <v>1511</v>
+      </c>
+      <c r="E99" s="31">
+        <v>8</v>
+      </c>
+      <c r="F99" s="31">
+        <v>6</v>
+      </c>
+      <c r="G99" s="31">
+        <v>1</v>
+      </c>
+      <c r="H99" s="31">
+        <v>1</v>
+      </c>
+      <c r="I99" s="31">
+        <v>109</v>
+      </c>
+      <c r="J99" s="31">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="100" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A100" s="20">
+        <v>44000</v>
+      </c>
+      <c r="B100" s="21">
+        <v>91005</v>
+      </c>
+      <c r="C100" s="22">
+        <v>902</v>
+      </c>
+      <c r="D100" s="22">
+        <v>1513</v>
+      </c>
+      <c r="E100" s="22">
+        <v>2</v>
+      </c>
+      <c r="F100" s="22">
+        <v>8</v>
+      </c>
+      <c r="G100" s="22">
+        <v>1</v>
+      </c>
+      <c r="H100" s="22">
+        <v>0</v>
+      </c>
+      <c r="I100" s="22">
+        <v>109</v>
+      </c>
+      <c r="J100" s="22">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="101" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A101" s="29">
+        <v>44001</v>
+      </c>
+      <c r="B101" s="30">
+        <v>92152</v>
+      </c>
+      <c r="C101" s="31">
+        <v>1147</v>
+      </c>
+      <c r="D101" s="31">
+        <v>1519</v>
+      </c>
+      <c r="E101" s="31">
+        <v>6</v>
+      </c>
+      <c r="F101" s="31">
+        <v>6</v>
+      </c>
+      <c r="G101" s="31">
+        <v>1</v>
+      </c>
+      <c r="H101" s="31">
+        <v>2</v>
+      </c>
+      <c r="I101" s="31">
+        <v>109</v>
+      </c>
+      <c r="J101" s="31">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="102" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A102" s="23">
+        <v>44002</v>
+      </c>
+      <c r="B102" s="24">
+        <v>92919</v>
+      </c>
+      <c r="C102" s="25">
+        <v>758</v>
+      </c>
+      <c r="D102" s="25">
+        <v>1520</v>
+      </c>
+      <c r="E102" s="25">
+        <v>1</v>
+      </c>
+      <c r="F102" s="25">
+        <v>6</v>
+      </c>
+      <c r="G102" s="25">
+        <v>1</v>
+      </c>
+      <c r="H102" s="25">
+        <v>2</v>
+      </c>
+      <c r="I102" s="25">
+        <v>109</v>
+      </c>
+      <c r="J102" s="25">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="103" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A103" s="29">
+        <v>44003</v>
+      </c>
+      <c r="B103" s="30">
+        <v>93181</v>
+      </c>
+      <c r="C103" s="31">
+        <v>271</v>
+      </c>
+      <c r="D103" s="31">
+        <v>1521</v>
+      </c>
+      <c r="E103" s="31">
+        <v>1</v>
+      </c>
+      <c r="F103" s="31">
+        <v>6</v>
+      </c>
+      <c r="G103" s="31">
+        <v>1</v>
+      </c>
+      <c r="H103" s="31">
+        <v>0</v>
+      </c>
+      <c r="I103" s="31">
+        <v>109</v>
+      </c>
+      <c r="J103" s="31">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="104" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A104" s="29">
+        <v>44004</v>
+      </c>
+      <c r="B104" s="30">
+        <v>94165</v>
+      </c>
+      <c r="C104" s="31">
+        <v>984</v>
+      </c>
+      <c r="D104" s="31">
+        <v>1534</v>
+      </c>
+      <c r="E104" s="31">
+        <v>13</v>
+      </c>
+      <c r="F104" s="31">
+        <v>5</v>
+      </c>
+      <c r="G104" s="31">
+        <v>1</v>
+      </c>
+      <c r="H104" s="31">
+        <v>1</v>
+      </c>
+      <c r="I104" s="31">
+        <v>109</v>
+      </c>
+      <c r="J104" s="31">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="105" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A105" s="29">
+        <v>44005</v>
+      </c>
+      <c r="B105" s="30">
+        <v>95387</v>
+      </c>
+      <c r="C105" s="31">
+        <v>1222</v>
+      </c>
+      <c r="D105" s="31">
+        <v>1541</v>
+      </c>
+      <c r="E105" s="31">
+        <v>7</v>
+      </c>
+      <c r="F105" s="31">
+        <v>7</v>
+      </c>
+      <c r="G105" s="31">
+        <v>2</v>
+      </c>
+      <c r="H105" s="31">
+        <v>0</v>
+      </c>
+      <c r="I105" s="31">
+        <v>111</v>
+      </c>
+      <c r="J105" s="31">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="106" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A106" s="23">
+        <v>44006</v>
+      </c>
+      <c r="B106" s="24">
+        <v>96599</v>
+      </c>
+      <c r="C106" s="25">
+        <v>1212</v>
+      </c>
+      <c r="D106" s="25">
+        <v>1547</v>
+      </c>
+      <c r="E106" s="25">
+        <v>6</v>
+      </c>
+      <c r="F106" s="25">
+        <v>7</v>
+      </c>
+      <c r="G106" s="25">
+        <v>2</v>
+      </c>
+      <c r="H106" s="25">
+        <v>0</v>
+      </c>
+      <c r="I106" s="25">
+        <v>111</v>
+      </c>
+      <c r="J106" s="25">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="107" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A107" s="29">
+        <v>44007</v>
+      </c>
+      <c r="B107" s="30">
+        <v>97442</v>
+      </c>
+      <c r="C107" s="31">
+        <v>843</v>
+      </c>
+      <c r="D107" s="31">
+        <v>1558</v>
+      </c>
+      <c r="E107" s="31">
+        <v>11</v>
+      </c>
+      <c r="F107" s="31">
+        <v>8</v>
+      </c>
+      <c r="G107" s="31">
+        <v>2</v>
+      </c>
+      <c r="H107" s="31">
+        <v>0</v>
+      </c>
+      <c r="I107" s="31">
+        <v>111</v>
+      </c>
+      <c r="J107" s="31">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="108" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A108" s="29">
+        <v>44008</v>
+      </c>
+      <c r="B108" s="30">
+        <v>98320</v>
+      </c>
+      <c r="C108" s="31">
+        <v>878</v>
+      </c>
+      <c r="D108" s="31">
+        <v>1572</v>
+      </c>
+      <c r="E108" s="31">
+        <v>14</v>
+      </c>
+      <c r="F108" s="31">
+        <v>8</v>
+      </c>
+      <c r="G108" s="31">
+        <v>1</v>
+      </c>
+      <c r="H108" s="31">
+        <v>0</v>
+      </c>
+      <c r="I108" s="31">
+        <v>111</v>
+      </c>
+      <c r="J108" s="31">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="109" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A109" s="29">
+        <v>44009</v>
+      </c>
+      <c r="B109" s="30">
+        <v>98945</v>
+      </c>
+      <c r="C109" s="31">
+        <v>625</v>
+      </c>
+      <c r="D109" s="31">
+        <v>1581</v>
+      </c>
+      <c r="E109" s="31">
+        <v>9</v>
+      </c>
+      <c r="F109" s="31">
+        <v>7</v>
+      </c>
+      <c r="G109" s="31">
+        <v>0</v>
+      </c>
+      <c r="H109" s="31">
+        <v>1</v>
+      </c>
+      <c r="I109" s="31">
+        <v>111</v>
+      </c>
+      <c r="J109" s="31">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="110" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A110" s="29">
+        <v>44010</v>
+      </c>
+      <c r="B110" s="30">
+        <v>99245</v>
+      </c>
+      <c r="C110" s="31">
+        <v>300</v>
+      </c>
+      <c r="D110" s="31">
+        <v>1585</v>
+      </c>
+      <c r="E110" s="31">
+        <v>4</v>
+      </c>
+      <c r="F110" s="31">
+        <v>8</v>
+      </c>
+      <c r="G110" s="31">
+        <v>0</v>
+      </c>
+      <c r="H110" s="31">
+        <v>0</v>
+      </c>
+      <c r="I110" s="31">
+        <v>111</v>
+      </c>
+      <c r="J110" s="31">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="111" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A111" s="29">
+        <v>44011</v>
+      </c>
+      <c r="B111" s="30">
+        <v>100330</v>
+      </c>
+      <c r="C111" s="31">
+        <v>1085</v>
+      </c>
+      <c r="D111" s="31">
+        <v>1600</v>
+      </c>
+      <c r="E111" s="31">
+        <v>15</v>
+      </c>
+      <c r="F111" s="31">
+        <v>8</v>
+      </c>
+      <c r="G111" s="31">
+        <v>0</v>
+      </c>
+      <c r="H111" s="31">
+        <v>0</v>
+      </c>
+      <c r="I111" s="31">
+        <v>111</v>
+      </c>
+      <c r="J111" s="31">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="112" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A112" s="20">
+        <v>44012</v>
+      </c>
+      <c r="B112" s="21">
+        <v>101729</v>
+      </c>
+      <c r="C112" s="22">
+        <v>1399</v>
+      </c>
+      <c r="D112" s="22">
+        <v>1613</v>
+      </c>
+      <c r="E112" s="22">
+        <v>13</v>
+      </c>
+      <c r="F112" s="22">
+        <v>8</v>
+      </c>
+      <c r="G112" s="22">
+        <v>0</v>
+      </c>
+      <c r="H112" s="22">
+        <v>0</v>
+      </c>
+      <c r="I112" s="22">
+        <v>111</v>
+      </c>
+      <c r="J112" s="22">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="113" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A113" s="20">
+        <v>44013</v>
+      </c>
+      <c r="B113" s="21">
+        <v>102927</v>
+      </c>
+      <c r="C113" s="22">
+        <v>1198</v>
+      </c>
+      <c r="D113" s="22">
+        <v>1633</v>
+      </c>
+      <c r="E113" s="22">
+        <v>21</v>
+      </c>
+      <c r="F113" s="22">
+        <v>9</v>
+      </c>
+      <c r="G113" s="22">
+        <v>0</v>
+      </c>
+      <c r="H113" s="22">
+        <v>0</v>
+      </c>
+      <c r="I113" s="22">
+        <v>111</v>
+      </c>
+      <c r="J113" s="22">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="114" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A114" s="20">
+        <v>44014</